<commit_message>
Bootstrap static files, Add file loading
</commit_message>
<xml_diff>
--- a/src/question_answer_site/tokens.xlsx
+++ b/src/question_answer_site/tokens.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C539"/>
+  <dimension ref="A1:C532"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7311,7 +7311,7 @@
     </row>
     <row r="530">
       <c r="A530" s="1" t="n">
-        <v>528</v>
+        <v>0</v>
       </c>
       <c r="B530" t="inlineStr">
         <is>
@@ -7324,7 +7324,7 @@
     </row>
     <row r="531">
       <c r="A531" s="1" t="n">
-        <v>529</v>
+        <v>1</v>
       </c>
       <c r="B531" t="inlineStr">
         <is>
@@ -7337,7 +7337,7 @@
     </row>
     <row r="532">
       <c r="A532" s="1" t="n">
-        <v>530</v>
+        <v>2</v>
       </c>
       <c r="B532" t="inlineStr">
         <is>
@@ -7346,97 +7346,6 @@
       </c>
       <c r="C532" t="n">
         <v>531</v>
-      </c>
-    </row>
-    <row r="533">
-      <c r="A533" s="1" t="n">
-        <v>531</v>
-      </c>
-      <c r="B533" t="inlineStr">
-        <is>
-          <t>['Ġk', 'os', 'mos', 'Ġwik', 'ipedia', 'Ġk', 'os', 'mos', 'Ġoperator', 'Ġr', 'ussia', 'Ġcos', 'par', 'Ġid', '028', 'e', 'Ġsat', 'cat', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġmay', 'Ġ05', 'Ġrocket', 'Ġro', 'k', 'ot', 'b', 'riz', 'km', 'Ġlaunch', 'Ġsite', 'Ġpl', 'es', 'etsk', 'Ġend', 'Ġmission', 'Ġdestroyed', 'Ġjan', 'uary', 'Ġ03', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġge', 'oc', 'entric', 'Ġregime', 'Ġlow', 'Ġearth', 'Ġper', 'ig', 'ee', 'Ġaltitude', 'Ġkilometres', 'Ġap', 'gee', 'Ġaltitude', 'Ġkilometres', 'Ġinclination', 'Ġdegrees', 'Ġperiod', 'Ġminutes', 'Ġepoch', 'Ġjan', 'uary', 'Ġ03', 'Ġk', 'os', 'mos', 'Ġk', 'os', 'mos', 'Ġr', 'ussian', 'Ġsatellite', 'Ġorbiting', 'Ġearth', 'Ġbreaking', 'Ġjan', 'uary', 'Ġsatellite', 'Ġlaunched', 'Ġmay', 'Ġpl', 'es', 'etsk', 'Ġr', 'ussia', 'Ġro', 'k', 'ot', 'b', 'riz', 'km', 'Ġlaunch', 'Ġvehicle', 'Ġalong', 'Ġrod', 'nik', 'Ġsatellites', 'Ġfollowing', 'Ġlaunch', 'Ġspacecraft', 'Ġprovision', 'ally', 'Ġdescribed', 'Ġn', 'asa', 'Ġorbital', 'Ġdebris', 'Ġprogram', 'Ġoffice', 'Ġobject', 'Ġidentity', 'Ġconfirmed', 'Ġus', 'space', 'Ġtracked', 'Ġsatellite', 'Ġcatalog', 'Ġnumber', 'Ġreports', 'Ġspeculated', 'Ġbased', 'Ġunusual', 'Ġpowered', 'Ġmaneuvers', 'Ġmay', 'Ġexperimental', 'Ġanti', 'atellite', 'Ġweapon', 'Ġsatellite', 'Ġmaintenance', 'Ġvehicle', 'Ġcollector', 'Ġspace', 'Ġdebris', 'Ġch', 'atham', 'Ġhouse', 'Ġresearch', 'Ġdirector', 'Ġspace', 'Ġsecurity', 'Ġexpert', 'Ġpat', 'ricia', 'Ġle', 'w', 'Ġstated', 'whatever', 'object', '028', 'e', 'Ġlooks', 'Ġexperimental', '."[', 'Ġmission', 'Ġk', 'os', 'mos', 'Ġwik', 'ipedia', 'Ġr', 'ussian', 'Ġstationary', 'Ġplasma', 'Ġthr', 'usters', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġaccording', 'Ġarticle', 'Ġpublished', 'Ġofficial', 'Ġmos', 'cow', 'Ġinstitute', 'Ġphysics', 'Ġtechnology', 'Ġwebsite', 'Ġcongrat', 'ulating', 'Ġdevelopers', 'Ġsuccessful', 'Ġlaunch', 'Ġdeployment', 'Ġsatellite', 'Ġdesigned', 'Ġtest', 'Ġexperimental', 'Ġplasma', 'Ġpropulsion', 'Ġengines', 'ion', 'Ġthr', 'usters', 'Ġdesigned', 'Ġres', 'het', 'ne', 'v', 'Ġcompany', 'Ġke', 'ld', 'ys', 'h', 'Ġresearch', 'Ġcenter', 'Ġarticle', 'Ġstates', 'Ġengines', 'Ġpart', 'Ġnew', 'Ġgeneration', 'Ġhall', 'Ġeffect', 'Ġthr', 'usters', 'Ġdesigned', 'Ġable', 'Ġshift', 'Ġspacecraft', 'Ġeast']</t>
-        </is>
-      </c>
-      <c r="C533" t="n">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="534">
-      <c r="A534" s="1" t="n">
-        <v>532</v>
-      </c>
-      <c r="B534" t="inlineStr">
-        <is>
-          <t>['west', 'Ġnorth', 'south', 'Ġaxis', 'Ġusing', 'Ġfraction', 'Ġenergy', 'Ġrequired', 'Ġcurrent', 'Ġpropulsion', 'Ġsystems', 'Ġde', 'cember', 'Ġus', 'space', 'Ġcatalog', 'ued', 'Ġdebris', 'Ġassociated', 'Ġk', 'os', 'mos', 'Ġfe', 'b', 'ruary', 'Ġus', 'Ġspace', 'Ġcommand', 'Ġconfirmed', 'Ġbreakup', 'Ġk', 'os', 'mos', 'Ġoccurred', 'Ġjan', 'uary', 'Ġ03', 'Ġut', 'c', 'Ġcatalog', 'ued', 'Ġassociated', 'Ġpieces', 'Ġorbiting', 'Ġkilometres', 'Ġmi', 'Ġaltitude', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġcold', 'Ġwar', 'tre', 'bit', 'el', 'Ġsp', 'ut', 'nikov', 'cd', 'owell', 'Ġj', 'athan', 'launch', 'Ġlog', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'mber', 'cos', 'mos', 'Ġsatellite', 'Ġdetails', '028', 'e', 'ad', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġpost', 'mission', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġk', 'os', 'mos', 'Ġwik', 'ipedia', 'Ġbrid', 'aine', 'Ġp', 'arn', 'ell', 'mber', 'call', 'Ġ00', 'Ġsecret', 'Ġr', 'ussian', 'Ġorbital', 'Ġweapon', 'Ġtracked', 'ad', 'Ġregister', 'Ġretrieved', 'mber', 'orb', 'ital', 'Ġdebris', 'Ġquarterly', 'Ġnews', 'Ġvolume', 'Ġissue', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġretrieved', 'Ġsam', 'Ġj', 'ones', 'object', 'e', 'Ġspace', 'Ġjunk', 'Ġr', 'ussian', 'Ġsatellite', 'Ġkiller', '?"', 'Ġfinancial', 'Ġtimes', 'Ġgra', 'ff', 'Ġgar', 'rett', 'j', 'une', 'Ġnew', 'Ġarms', 'Ġrace', 'Ġthreatening', 'Ġexplode', 'Ġspace', 'Ġwired', 'Ġyears', 'Ġsince', 'Ġobject', 'e', 'Ġjoined', 'Ġsimilar', 'Ġspace', 'Ġobjects', 'Ġr', 'ussian', 'Ġproven', 'ance', 'Ġanalysts', 'Ġfear', 'Ġmight', 'Ġmark', 'Ġrevival', 'Ġr', 'ussian', 'Ġprogram', 'Ġknown', 'Ġsatellite', 'Ġkiller', 'Ġshut', 'Ġcold', 'Ġwar', '."', 'rew', 'Ġgr', 'ï', '¬', 'ģ', 'n', 'Ġr', 'ussia', 'Ġï', '¬', 'Ĥ', 'ying', 'Ġsatellite', 'Ġkiller', 'Ġaround', 'Ġspace', 'Ġun', 'ident', 'ï', '¬', 'ģ', 'ed', 'Ġr', 'ussian', 'Ġsatellite', 'Ġprompts', 'Ġspace']</t>
-        </is>
-      </c>
-      <c r="C534" t="n">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="535">
-      <c r="A535" s="1" t="n">
-        <v>533</v>
-      </c>
-      <c r="B535" t="inlineStr">
-        <is>
-          <t>['Ġweapon', 'Ġworries', 'html', 'Ġir', 'ish', 'Ġindependent', 'Ð¾Ð', '±', 'Ñ', 'Ĭ', 'Ðµ', 'Ðº', 'ÑĤ', 'âĪĴ', 'e', 'Ġ', 'Ñģ', 'Ð´', 'Ðµ', 'Ð»', 'Ð°', 'Ð½', 'Ð¾', 'ĠÐ', '½', 'Ð°', 'Ñģ', 'mber', 'Ð', '¿', 'Ð»', 'Ð°', 'Ð', '·', 'Ð¼', 'Ðµ', 'Ð½', 'Ð½', 'Ñĭ', 'Ðµ', 'ĠÐ', '´', 'Ð²', 'Ð¸', 'Ð', '³', 'Ð°', 'ÑĤ', 'Ðµ', 'Ð»', 'Ð¸', 'ĠÐ', '½', 'Ð¾Ð', '²', 'Ð¾Ð', '³', 'Ð¾', 'ĠÐ', '¿', 'Ð¾Ð', 'º', 'Ð¾Ð', '»', 'Ðµ', 'Ð½', 'Ð¸', 'Ñı', 'Ġ', 'Ñĥ', 'Ñģ', 'Ð', '¿', 'Ðµ', 'Ñ', 'Ī', 'Ð½', 'Ð¾', 'ĠÐ', '½', 'Ð°', 'Ñ', 'ĩ', 'Ð°', 'Ð»', 'Ð¸', 'Ġ', 'Ñ', 'Ī', 'ÑĤ', 'Ð°', 'ÑĤ', 'Ð½', 'Ñĥ', 'Ñ', 'İ', 'Ġ', 'ÑĢ', 'Ð°', 'Ð', '±', 'Ð¾', 'ÑĤ', 'Ñĥ', 'ĠÐ', 'º', 'Ð¾', 'Ñģ', 'Ð¼', 'Ð¾', 'Ñģ', 'Ðµ', 'htt', 'ipt', 'ru', 'Ġke', 'l', 'ts', 'kel', 'Ġde', 'cember', 'cel', 'est', 'rak', 'les', 'Ġobjects', 'Ġappear', 'Ġassociated', 'Ġdebris', 'Ġevent', 'Ġinvolving', 'Ġdead', 'Ġcosmos', 'Ġsatellite', 'Ġlaunched', '05', 'Ġbased', 'les', 'Ġevent', 'Ġappears', 'Ġoccurred', 'Ġsometime', 'twitter', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'th', 'Ġspace', 'Ġdefense', 'Ġsquadron', 'ths', 'ds', 'Ġfe', 'b', 'ruary', 'ds', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġbreakup', 'Ġcosmos', 'weet', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'Ġj', 'ones', 'Ġsam', 'mber', 'atellite', 'Ġwars', 'Ġfinancial', 'Ġtimes', 'Ġonline', 'Ġretrieved', 'mber', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
-        </is>
-      </c>
-      <c r="C535" t="n">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="536">
-      <c r="A536" s="1" t="n">
-        <v>534</v>
-      </c>
-      <c r="B536" t="inlineStr">
-        <is>
-          <t>['Ġk', 'os', 'mos', '01', 'Ġwik', 'ipedia', 'Ġk', 'os', 'mos', '01', 'Ġmodel', 'Ġgl', 'ass', 'k', 'Ġsatellite', 'Ġmission', 'Ġtype', 'Ġnavigation', 'Ġoperator', 'Ġcos', 'par', 'Ġid', '075', 'Ġsat', 'cat', 'Ġmission', 'Ġduration', 'Ġyears', 'Ġspacecraft', 'Ġproperties', 'Ġspacecraft', 'Ġgl', 'ass', 'Ġur', 'agan', 'k', 'Ġspacecraft', 'Ġtype', 'Ġur', 'agan', 'k', 'Ġbus', 'Ġe', 'ks', 'press', 'Ġmanufacturer', 'Ġiss', 'Ġres', 'het', 'ne', 'v', 'Ġlaunch', 'Ġmass', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'mber', 'Ġut', 'c', 'Ġrocket', 'Ġfre', 'gat', 'Ġlaunch', 'Ġsite', 'Ġpl', 'es', 'etsk', 'Ġsite', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġge', 'oc', 'entric', 'Ġregime', 'Ġmedium', 'Ġearth', 'Ġper', 'ig', 'ee', 'Ġaltitude', 'Ġk', 'os', 'mos', '01', 'Ġk', 'os', 'mos', '01', 'Ġwik', 'ipedia', 'Ġap', 'gee', 'Ġaltitude', 'Ġinclination', 'Â°', 'Ġperiod', 'Ġminutes', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġk', 'os', 'mos', '01', 'r', 'ussian', 'ĠÐ', 'º', 'Ð¾', 'Ñģ', 'Ð¼', 'Ð¾', 'Ñģ', '01', 'Ġmeaning', 'Ġcosmos', '01', 'Ġalso', 'Ġknown', 'Ġgl', 'ass', 'k', 'Ġr', 'ussian', 'Ġnavigation', 'Ġsatellite', 'Ġlaunched', 'Ġsecond', 'Ġgl', 'ass', 'k', 'Ġsatellite', 'Ġlaunched', 'Ġsecond', 'Ġtwo', 'Ġgl', 'ass', 'k', 'Ġspacecraft', 'Ġserve', 'Ġprototypes', 'Ġoperational', 'Ġgl', 'ass', 'k', 'Ġspacecraft', 'Ġk', 'os', 'mos', '01', 'kil', 'ogram', '06', 'Ġsatellite', 'Ġbuilt', 'Ġiss', 'Ġres', 'het', 'ne', 'v', 'Ġbased', 'Ġe', 'ks', 'press', 'Ġsatellite', 'Ġbus', 'Ġspacecraft', 'Ġthree', 'axis', 'Ġstabil', 'isation', 'Ġkeep', 'Ġcorrect', 'Ġorientation', 'Ġbroadcast', 'Ġsignals', 'Ġnavigation', 'Ġbands', 'Ġr', 'ussian', 'Ġmilitary', 'Ġcommercial', 'Ġusers', 'Ġaddition', 'Ġnavigation', 'Ġpayload', 'Ġsatellite', 'Ġalso', 'Ġcarries', 'Ġc', 'osp', 'ars', 'Ġsearch', 'Ġrescue', 'Ġpayload', 'Ġsatellite', 'Ġlocated', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġper', 'ig', 'ee', 'Ġkilometres', '02', 'Ġmi', 'Ġap', 'gee', 'Ġkilometres', 'Ġmi', 'Â°', 'Ġinclination', 'Ġequipped', 'Ġtwo', 'Ġsolar', 'Ġpanels', 'Ġgenerate', 'Ġpower', 'Ġexpected', 'Ġremain', 'Ġservice', 'Ġten', 'Ġyears', 'Ġk', 'os', 'mos', '01']</t>
-        </is>
-      </c>
-      <c r="C536" t="n">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="537">
-      <c r="A537" s="1" t="n">
-        <v>535</v>
-      </c>
-      <c r="B537" t="inlineStr">
-        <is>
-          <t>['Ġlaunched', 'Ġsite', 'Ġpl', 'es', 'etsk', 'Ġcos', 'mod', 'rome', 'Ġnorthwest', 'Ġr', 'ussia', 'Ġcarrier', 'Ġrocket', 'Ġfre', 'gat', 'Ġupper', 'Ġstage', 'Ġused', 'Ġperform', 'Ġlaunch', 'Ġtook', 'Ġplace', 'Ġut', 'c', 'mber', 'Ġlaunch', 'Ġsuccessfully', 'Ġplaced', 'Ġsatellite', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsubsequently', 'Ġreceived', 'Ġk', 'os', 'mos', 'Ġdesignation', 'Ġinternational', 'Ġdesign', 'ator', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġcommand', 'Ġassigned', 'Ġsatellite', 'Ġcatalog', 'Ġnumber', 'cd', 'owell', 'Ġj', 'athan', 'atellite', 'Ġcatalog', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġmarch', 'Ġk', 'bs', 'Ġgun', 'ter', 'ur', 'agan', 'k', 'gl', 'ass', 'k', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'mber', 'cd', 'owell', 'Ġj', 'athan', 'jon', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġissue', '06', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'mber', 'Ġz', 'ak', 'Ġanat', 'oly', 'gl', 'ass', 'k', 'Ġsatellite', 'Ġr', 'uss', 'ians', 'pac', 'ew', 'eb', 'Ġretrieved', 'mber', 'Ġretrieved', 'Ġreferences']</t>
-        </is>
-      </c>
-      <c r="C537" t="n">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="538">
-      <c r="A538" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B538" t="inlineStr">
-        <is>
-          <t>['Ġk', 'os', 'mos', 'Ġwik', 'ipedia', 'Ġk', 'os', 'mos', 'Ġgl', 'ass', 'Ġsatellite', 'Ġmodel', 'Ġmission', 'Ġtype', 'Ġnavigation', 'Ġoperator', 'Ġr', 'ussian', 'Ġaerospace', 'Ġdefence', 'Ġforces', 'Ġcos', 'par', 'Ġid', '032', 'Ġsat', 'cat', 'Ġwebsite', 'Ġgl', 'ass', 'Ġstatus', 'h', 'Ġg', 'web', 'http', 'gl', 'Ġl', 'ass', 'Ġmission', 'Ġduration', 'Ġplanned', 'Ġyears', 'Ġactual', 'Ġyears', 'Ġmonths', 'Ġspacecraft', 'Ġproperties', 'Ġspacecraft', 'Ġgl', 'ass', 'Ġspacecraft', 'Ġtype', 'Ġur', 'agan', 'Ġmanufacturer', 'Ġres', 'het', 'ne', 'v', 'Ġlaunch', 'Ġmass', 'Ġkilograms', 'Ġdry', 'Ġmass', 'Ġdimensions', 'Ġmetres', 'Ġft', 'Ġdiameter', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġmay', 'Ġ08', 'Ġut', 'c', 'Ġk', 'os', 'mos', 'Ġk', 'os', 'mos', 'r', 'ussian', 'ĠÐ', 'º', 'Ð¾', 'Ñģ', 'Ð¼', 'Ð¾', 'Ñģ', 'Ġmeaning', 'Ġspace', 'Ġr', 'ussian', 'Ġmilitary', 'Ġsatellite', 'Ġlaunched', 'Ġpart', 'Ġgl', 'ass', 'Ġsatellite', 'Ġnavigation', 'Ġsystem', 'Ġsatellite', 'Ġgl', 'ass', 'Ġsatellite', 'Ġalso', 'Ġknown', 'Ġur', 'agan', 'Ġnumbered', 'Ġur', 'agan', 'Ġk', 'os', 'mos', 'Ġlaunched', 'Ġsite', 'Ġpl', 'es', 'etsk', 'Ġcos', 'mod', 'rome', 'Ġnorthern', 'Ġr', 'ussia', 'Ġcarrier', 'Ġrocket', 'Ġfre', 'gat', 'Ġupper', 'Ġstage', 'Ġused', 'Ġperform', 'Ġlaunch', 'Ġtook', 'Ġplace', 'Ġ08', 'Ġut', 'c', 'Ġmay', 'Ġlaunch', 'Ġsuccessfully', 'Ġplaced', 'Ġsatellite', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsubsequently', 'Ġreceived', 'Ġk', 'os', 'mos', 'Ġdesignation', 'Ġinternational', 'Ġdesign', 'ator', '032', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġcommand', 'Ġassigned', 'Ġsatellite', 'Ġcatalog', 'Ġnumber', 'Ġsatellite', 'Ġorbital', 'Ġplane', 'Ġorbital', 'Ġslot', 'Ġk', 'os', 'mos', 'Ġexperienced', 'Ġdepress', 'ur', 'ization', 'Ġevent', 'mber', 'Ġpermanently', 'Ġdisabled', 'Ġsatellite', 'Ġfour', 'Ġyears', 'Ġservice', 'Ġgl', 'ass', 'k', '05', 'Ġlaunched', 'Ġoct', 'ober', 'Ġrep', 'ur', 'posed', 'Ġreplacement', 'Ġk', 'os', 'mos', 'Ġwik', 'ipedia', 'Ġrocket', 'Ġlaunch', 'Ġsite', 'Ġpl', 'es', 'etsk', 'Ġcontractor', 'Ġr', 'ussian', 'Ġaerospace', 'Ġdefence', 'Ġforces', 'Ġend']</t>
-        </is>
-      </c>
-      <c r="C538" t="n">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="539">
-      <c r="A539" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B539" t="inlineStr">
-        <is>
-          <t>['Ġmission', 'Ġlast', 'Ġcontact', 'mber', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġge', 'oc', 'entric', 'Ġregime', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsemi', 'major', 'Ġaxis', 'Ġeccentric', 'ity', '00', 'Ġper', 'ig', 'ee', 'Ġaltitude', 'Ġap', 'gee', 'Ġaltitude', 'Ġinclination', 'Ġdegrees', 'Ġperiod', 'Ġminutes', 'Ġepoch', 'Ġjan', 'uary', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġlist', 'Ġk', 'os', 'mos', 'Ġsatellites', '01', 'âĢĵ', 'Ġlist', 'Ġlaunches', 'âĢĵ', 'live', 'Ġreal', 'Ġtime', 'Ġsatellite', 'Ġtracking', 'Ġpredictions', 'Ġcosmos', 'gl', 'ass', ')"', 'ht', 'Ġretrieved', 'Ġjan', 'uary', 'Ð½', 'Ð¾Ð', '²', 'Ðµ', 'Ð', '¹', 'Ñ', 'Ī', 'Ð¸', 'Ð', '¹', 'Ð', '³', 'Ð»', 'Ð¾', 'Ð½', 'Ð°', 'Ñģ', 'Ñģ', 'Ðº', 'Ġ', 'Ñģ', 'Ð¼', 'Ðµ', 'Ð½', 'Ð¸', 'ÑĤ', 'ĠÐ', '²', 'Ñĭ', 'Ñ', 'Ī', 'Ðµ', 'Ð´', 'Ñ', 'Ī', 'Ð¸', 'Ð', '¹', 'ĠÐ', '¸', 'Ð', '·', 'Ġ', 'Ñģ', 'ÑĤ', 'ÑĢ', 'Ð¾', 'Ñı', 'ĠÐ', '°', 'Ð', '¿', 'Ð', '¿', 'Ð°', 'ÑĢ', 'Ð°', 'ÑĤ', 'Ġ', 'ÑĢ', 'Ð°', 'Ñģ', 'Ñģ', 'Ðº', 'Ð°', 'Ð', '·', 'Ð°', 'Ð»', 'ĠÐ', '¸', 'Ñģ', 'ÑĤ', 'Ð¾', 'Ñ', 'ĩ', 'Ð½', 'Ð¸', 'Ðº', 'ri', 'new', 'est', 'Ġgl', 'ass', 'k', 'Ġreplace', 'Ġfailed', 'Ġsatellite', 'Ġsource', 'Ġsays', '].', 'Ġr', 'ia', 'v', 'ost', 'Ġr', 'ussian', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġanat', 'oly', 'Ġz', 'ak', 'gl', 'ass', 'Ġnetwork', 'Ġr', 'uss', 'ias', 'pac', 'ew', 'eb', 'Ġretrieved', 'Ġjan', 'uary', 'Ġstep', 'hen', 'Ġcl', 'ark', 'may', 'r', 'ussia', "'s", 'Ġnavigation', 'Ġnetwork', 'Ġreceives', 'Ġnew', 'Ġsatellite', 'http', 'space', 'ï', '¬', 'Ĥ', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġjan', 'uary', 'gl', 'ass', 'Ġconstellation', 'Ġstatus', '01', 'Ġcentre', 'Ġk', 'oly', 'ov', 'Ġr', 'ussia', 'Ġjan', 'uary', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġk', 'os', 'mos', 'Ġwik', 'ipedia', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'Ġretrieved']</t>
-        </is>
-      </c>
-      <c r="C539" t="n">
-        <v>538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding proxy and Aerospace mongo credentials
</commit_message>
<xml_diff>
--- a/src/question_answer_site/tokens.xlsx
+++ b/src/question_answer_site/tokens.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C504"/>
+  <dimension ref="A1:C510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['Ġgalaxy', 'Ġwik', 'ipedia', 'Ġgalaxy', 'Ġanimation', 'Ġgalaxy', 'Ġtrajectory', 'Ġoct', 'ober', 'Ġoct', 'ober', 'Ġgalaxy', 'Ġearth', 'Ġmission', 'Ġtype', 'Ġcommunication', 'Ġnavigation', 'Ġoperator', 'Ġpan', 'ams', 'âĢĵ', 'Ġint', 'els', '-)', 'Ġcos', 'par', 'Ġid', '041', 'Ġsat', 'cat', 'Ġmission', 'Ġduration', 'Ġyears', 'planned', 'Ġspacecraft', 'Ġproperties', 'Ġbus', 'Ġge', 'ost', 'ar', 'Ġmanufacturer', 'Ġorbital', 'Ġsciences', 'Ġlaunch', 'Ġmass', '033', 'Ġkilograms', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġoct', 'ober', 'Ġut', 'c', 'Ġrocket', 'ri', 'ane', 'Ġlaunch', 'Ġsite', 'Ġk', 'ou', 'Ġcontractor', 'rian', 'esp', 'ace', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġge', 'oc', 'entric', 'Ġregime', 'Ġge', 'ost', 'ation', 'ary', 'Ġlong', 'itude', 'Â°', 'Ġwest', 'Ġper', 'ig', 'ee', 'Ġaltitude', 'Ġkilometres', 'Ġmi', 'Ġap', 'gee', 'Ġaltitude', 'Ġkilometres', 'Ġmi', 'Ġgalaxy', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġinclination', '06', 'Ġdegrees', 'Ġperiod', 'Ġhours', 'Ġminutes', 'Ġtrans', 'p', 'ond', 'ers', 'Ġband', 'Ġg', 'h', 'Ġband', 'ie', 'ee', 'Ġband', 'Ġband', 'ie', 'ee', 'Ġband', 'Ġgalaxy', 'Ġameric', 'Ġtelecommunications', 'Ġsatellite', 'Ġowned', 'Ġint', 'els', 'Ġlaunched', 'Ġoriginally', 'Ġoperated', 'Ġpan', 'ams', 'Ġsubsequently', 'Ġtransferred', 'Ġint', 'els', 'Ġtwo', 'Ġcompanies', 'Ġmerged', 'Ġoriginally', 'Ġpositioned', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġlong', 'itude', 'Â°', 'Ġwest', 'Ġused', 'Ġprovide', 'Ġcommunication', 'Ġservices', 'Ġnorth', 'Ġameric', 'Ġapr', 'il', 'Ġint', 'els', 'Ġlost', 'Ġcontrol', 'Ġsatellite', 'Ġbegan', 'Ġdrift', 'Ġaway', 'Ġorbital', 'Ġslot', 'Ġpotential', 'Ġcause', 'Ġdisruption', 'Ġsatellites', 'Ġpath', 'Ġde', 'cember', 'Ġint', 'els', 'Ġreported', 'Ġsatellite', 'Ġreboot', 'ed', 'Ġper', 'Ġdesign', 'Ġcommand', 'Ġunit', 'Ġresponding', 'Ġcommands', 'Ġaddition', 'Ġsatellite', 'Ġsecured', 'Ġsafe', 'Ġmode', 'Ġpotential', 'Ġinterference', 'Ġissues', 'Ġgalaxy', 'Ġceased', 'Ġint', 'els', 'Ġrep', 'osition', 'ed', 'Ġgalaxy', 'Ġback', 'Ġoriginal', 'Ġlocation', 'Ġapr', 'il', 'Ġaug', 'ust', 'Ġint', 'els', 'Ġlost', 'Ġcontrol', 'Ġgalaxy', 'Ġattribut', 'ing', 'Ġspace', 'Ġweather', 'Ġevent', 'Ġgalaxy', 'Ġconstructed', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'Ġbased']</t>
+          <t>['Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġartist', "'s", 'Ġimpression', 'Ġsatellite', 'Ġmanufacturer', 'Ġlock', 'heed', 'Ġmart', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġoperator', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġapplications', 'Ġmilitary', 'Ġcommunications', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġbus', '00', 'Ġlaunch', 'Ġmass', 'Ġregime', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġdesign', 'Ġlife', 'Ġyears', 'planned', 'Ġdimensions', 'Ġproduction', 'Ġstatus', 'Ġoperational', 'Ġactive', 'Ġorder', 'Ġbuilt', 'Ġlaunched', 'Ġoperational', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġconstellation', 'Ġcommunications', 'Ġsatellites', 'Ġoperated', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġused', 'Ġrelay', 'Ġsecure', 'Ġcommunications', 'Ġunited', 'Ġstates', 'Ġarmed', 'Ġforces', 'Ġb', 'rit', 'ish', 'Ġarmed', 'Ġforces', 'adian', 'Ġarmed', 'Ġforces', 'Ġnet', 'lands', 'Ġarmed', 'Ġforces', 'Ġaust', 'ral', 'ian', 'Ġdefence', 'Ġforce', 'Ġsystem', 'Ġconsists', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġfinal', 'Ġsatellite', 'Ġlaunched', 'Ġmarch', 'Ġbackward', 'Ġcompatible', 'Ġreplaces', 'Ġolder', 'Ġmil', 'star', 'Ġsystem', 'Ġoperate', 'Ġupl', 'ink', 'extremely', 'Ġhigh', 'Ġfrequency', 'Ġband', 'link', 'super', 'Ġhigh', 'Ġfrequency', 'Ġband', ').[', 'Ġsystem', 'Ġjoint', 'Ġservice', 'Ġcommunications', 'Ġsystem', 'Ġprovides', 'Ġsurviv', 'able', 'Ġglobal', 'Ġsecure', 'Ġprotected', 'Ġjam', 'resistant', 'Ġcommunications', 'Ġhigh', 'priority', 'Ġmilitary', 'Ġground', 'Ġsea', 'Ġair', 'Ġassets', 'Ġsatellites', 'Ġuse', 'Ġmany', 'Ġnarrow', 'Ġspot', 'Ġbeams', 'Ġdirected', 'Ġtowards', 'Ġearth', 'Ġrelay', 'Ġcommunications', 'Ġusers', 'Ġcross', 'links', 'Ġsatellites', 'Ġallow', 'Ġrelay', 'Ġcommunications', 'Ġdirectly', 'Ġrather', 'Ġvia', 'Ġground', 'Ġstation', 'Ġsatellites', 'Ġdesigned', 'Ġprovide', 'Ġjam', 'resistant', 'Ġcommunications', 'Ġlow', 'Ġprobability', 'Ġinterception', 'Ġincorporate', 'Ġfrequency', 'ho', 'pping', 'Ġradio', 'Ġtechnology', 'Ġwell', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġadapt', 'Ġradiation', 'Ġpatterns', 'Ġorder', 'Ġblock', 'Ġpotential', 'Ġsources', 'Ġjam', 'ming', 'Ġincorporates', 'Ġexisting', 'Ġmil', 'star', 'Ġlow', 'Ġdata', 'rate', 'Ġmedium', 'Ġdata', 'rate', 'Ġsignals', 'Ġproviding', 'âĢĵ', '00', 'Ġbit', 'Ġk', 'bit', 'âĢĵ', 'bit', 'Ġrespectively', 'Ġalso', 'Ġincorporates', 'Ġnew', 'Ġsignal', 'Ġallowing', 'Ġdata', 'Ġrates', 'bit', 'Ġcomplete', 'Ġspace', 'Ġsegment', 'Ġsystem', 'Ġconsist', 'Ġsatellites', 'Ġprovides', 'Ġcoverage', 'Ġsurface', 'Ġearth', 'Ġlat', 'itudes', 'Â°', 'Ġnorth', 'Â°', 'Ġsouth', 'Ġnorthern', 'Ġpolar', 'Ġregions']</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -464,7 +464,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['Ġaround', 'Ġge', 'ost', 'ar', 'Ġsatellite', 'Ġbus', 'Ġcontract', 'Ġmanufacture', 'Ġsigned', 'Ġtime', 'Ġidentical', 'Ġgalaxy', 'Ġgalaxy', 'Ġsatellites', 'Ġalso', 'Ġorder', 'Ġcontract', 'Ġchanged', 'Ġallow', 'Ġaddition', 'Ġtrans', 'p', 'ond', 'ers', 'Ġsupport', 'Ġus', 'Ġgovernment', "'s", 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġcontrol', 'Ġsegment', 'Ġwide', 'Ġarea', 'Ġaug', 'mentation', 'Ġsystem', 'wa', 'Ġus', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġnavigation', 'Ġprogram', 'Ġcommunications', 'Ġpayload', 'Ġaboard', 'Ġgalaxy', 'Ġconsisted', 'Ġtrans', 'p', 'ond', 'ers', 'Ġoperating', 'Ġbands', 'Ġn', 'ato', 'Ġelectromagnetic', 'Ġspectrum', 'Ġband', 'Ġus', 'Ġie', 'ee', 'Ġspectrum', 'Ġalso', 'Ġcarried', 'Ġtwo', 'Ġband', 'ie', 'ee', 'Ġband', 'Ġtrans', 'p', 'ond', 'ers', 'Ġform', 'Ġpart', 'Ġus', 'Ġgovernment', "'s", 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġcontrol', 'Ġsegment', 'Ġused', 'Ġaircraft', 'Ġnavigation', 'Ġlaunch', 'Ġgalaxy', 'Ġsatellite', 'Ġmass', '033', 'Ġkilograms', 'Ġexpected', 'Ġoperational', 'Ġlifespan', 'Ġaround', 'Ġyears', 'Ġlaunch', 'Ġgalaxy', 'Ġconducted', 'rian', 'esp', 'ace', 'Ġusing', 'ri', 'ane', 'Ġcarrier', 'Ġrocket', 'Ġflying', 'Ġgu', 'iana', 'Ġspace', 'Ġcentre', 'Ġk', 'ou', 'Ġfrench', 'Ġlaunch', 'Ġoccurred', 'Ġg', 'mt', 'Ġoct', 'ober', 'Ġopening', 'minute', 'Ġlaunch', 'Ġwindow', 'Ġsuccessfully', 'Ġplaced', 'Ġgalaxy', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'Ġfrench', 'Ġsy', 'racuse', 'Ġmilitary', 'Ġcommunications', 'Ġsatellite', 'Ġlaunched', 'Ġrocket', 'Ġlaunch', 'Ġgalaxy', 'Ġlocated', 'Ġbeneath', 'Ġsy', 'racuse', 'Ġspacecraft', 'Ġmounted', 'Ġatop', 'Ġsy', 'lda', 'Ġadapt', 'Ġsatellite', 'Ġlaunch', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġfollowing', 'Ġseparation', 'Ġcarrier', 'Ġrocket', 'Ġgalaxy', 'Ġraised', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġmeans', 'Ġap', 'gee', 'Ġmotor', 'Ġinsertion', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġoccurred', 'Ġaround', '00', 'Ġoct', 'ober', 'Ġapr', 'il', 'Ġgalaxy', 'Ġceased', 'Ġresponding', 'Ġcommands', 'Ġsent', 'Ġcontrollers', 'Ġground', 'Ġhowever', 'Ġunclear', 'Ġactual', 'Ġinitial', 'Ġfailure', 'Ġdate', 'Ġcommands', 'Ġoften', 'Ġsent', 'Ġsatellite', 'Ġoperators', 'Ġdays', 'Ġeven', 'Ġweeks', 'Ġapart', 'Ġwithout', 'Ġcommands', 'Ġnecessary', 'Ġstation', 'keeping', 'Ġbegan', 'Ġdrift', 'Ġeast', 'Ġaway', 'Ġallotted', 'Ġorbital', 'Ġslot']</t>
+          <t>['Ġenhanced', 'Ġpolar', 'Ġsystem', 'Ġacts', 'Ġadjunct', 'Ġprovide', 'Ġcoverage', 'Ġinitial', 'Ġcontract', 'Ġdesign', 'Ġdevelopment', 'Ġsatellites', 'Ġawarded', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'Ġsystems', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġtechnology', 'mber', 'Ġcovered', 'Ġsystem', 'Ġdevelopment', 'Ġdemonstration', 'Ġphase', 'Ġprogram', 'Ġcontract', 'Ġcovered', 'Ġoverview', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġmaiden', 'Ġlaunch', 'Ġaug', 'ust', 'usa', 'Ġlast', 'Ġlaunch', 'Ġmarch', 'usa', 'Ġconstruction', 'Ġlaunch', 'Ġthree', 'Ġsatellites', 'Ġconstruction', 'Ġmission', 'Ġcontrol', 'Ġsegment', 'Ġcontract', 'Ġmanaged', 'Ġmil', 'sat', 'Ġprogram', 'Ġoffice', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'Ġlike', 'Ġmil', 'star', 'Ġsystem', 'Ġoperated', 'th', 'Ġspace', 'Ġoperations', 'Ġsquadron', 'Ġlocated', 'Ġsch', 'ri', 'ever', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġextends', 'cross', 'links', 'Ġamong', 'Ġearlier', 'Ġmil', 'star', 'Ġsatellites', 'Ġmakes', 'Ġmuch', 'Ġless', 'Ġvulnerable', 'Ġattacks', 'Ġground', 'Ġstations', 'Ġge', 'os', 'ynchronous', 'Ġsatellite', 'Ġequ', 'ator', 'Ġstill', 'Ġneeds', 'Ġsupplemented', 'Ġadditional', 'Ġsystems', 'Ġoptimized', 'Ġpolar', 'Ġcoverage', 'Ġhigh', 'Ġlat', 'itudes', 'Ġapr', 'il', 'Ġdefense', 'Ġdepartment', 'Ġbudget', 'Ġrequest', 'Ġsecretary', 'Ġdefense', 'Ġro', 'bert', 'Ġgates', 'Ġsaid', 'Ġplanned', 'Ġcancel', 'Ġtransform', 'ational', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'Ġstill', 'Ġdesign', 'Ġphase', 'Ġfavor', 'Ġadditional', 'Ġcapacity', 'Ġindividual', 'Ġsatellites', 'Ġexclusive', 'Ġlaunch', 'Ġexpenses', 'Ġcost', 'Ġmillion', 'Ġprior', 'Ġunited', 'Ġstates', 'Ġallied', 'Ġmilitary', 'Ġsatellite', 'Ġcommunications', 'Ġsystems', 'Ġfell', 'Ġone', 'Ġthree', 'Ġcategories', ':[', 'Ġwide', 'band', 'Ġmaximum', 'Ġbandwidth', 'Ġamong', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġsemi', 'ï', '¬', 'ģ', 'x', 'ed', 'Ġearth', 'Ġstations', 'Ġprotected', 'Ġsurviv', 'able', 'Ġelectronic', 'Ġwarfare', 'Ġattacks', 'Ġeven', 'Ġbandwidth', 'Ġsac', 'ri', 'ï', '¬', 'ģ', 'ced', 'Ġnarrow', 'band', 'Ġprincipally', 'Ġtactical', 'Ġuse', 'Ġsac', 'ri', 'ï', '¬', 'ģ', 'cing', 'Ġbandwidth', 'Ġsimplicity', 'Ġreliability', 'Ġlight', 'Ġweight', 'Ġterrestrial', 'Ġequipment', 'Ġhowever', 'Ġconver', 'ges', 'Ġrole', 'Ġwide', 'band', 'Ġdefense', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'sc', 'Ġprotected', 'Ġmil', 'star', 'Ġpredecessors', 'Ġincreasing', 'Ġbandwidth', 'Ġstill', 'Ġneed', 'Ġspecialized', 'Ġsatellite', 'Ġcommunications', 'Ġextremely', 'Ġhigh', 'Ġdata', 'Ġrate', 'Ġspace', 'Ġsensors', 'Ġge', 'osp', 'atial', 'Ġsignals', 'Ġintelligence', 'Ġsatellites', 'linked', 'Ġdata', 'Ġtypically', 'Ġgo', 'Ġspecialized', 'Ġreceiver', 'Ġprocessed', 'Ġsmaller', 'Ġamounts', 'Ġprocessed', 'Ġdata', 'Ġflow', 'Ġsatellites', 'Ġsent', 'Ġspace', 'Ġusing', 'Ġevolved']</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>['Ġtelevision', 'Ġsignals', 'Ġtransferred', 'Ġsatellites', 'Ġintentional', 'Ġtransmissions', 'Ġceased', 'Ġgalaxy', 'Ġsatellite', 'Ġremoved', 'orbit', 'Ġstorage', 'Â°', 'Ġwest', 'Ġreplace', 'Ġgalaxy', 'Â°', 'Ġwest', 'Ġorbital', 'Ġslot', 'Ġgalaxy', 'Ġoriginally', 'Ġslated', 'Ġreplace', 'Ġanother', 'Ġsatellite', 'Ġgalaxy', 'Ġrelocated', 'Â°', 'Ġeast', 'Ġstart', 'Ġmission', 'Ġcritical', 'Ġservice', 'Ġunited', 'Ġstates', 'Ġgovernment', 'Ġdue', 'Ġnecessity', 'Ġrel', 'ocating', 'Ġgalaxy', 'Â°', 'Ġwest', 'Ġint', 'els', 'Ġforced', 'Ġleave', 'Â°', 'Ġwest', 'Ġvacant', 'Ġapr', 'il', 'Ġorbital', 'Ġsciences', 'Ġtheor', 'ized', 'Ġbelieved', 'Ġsolar', 'Ġactivity', 'Ġresponsible', 'Ġsatellite', 'Ġmalfunction', 'ing', 'Ġalthough', 'Ġlater', 'Ġstatement', 'Ġcompany', 'Ġsaid', 'Ġcompany', 'Ġunable', 'Ġactually', 'Ġsettle', 'Ġsingle', 'Ġroot', 'Ġcause', '."[', 'Ġmay', 'Ġattempt', 'Ġmoment', 'ary', 'Ġseries', 'Ġstrong', 'Ġpulses', 'Ġintended', 'Ġcause', 'Ġpower', 'Ġsystem', 'Ġmalfunction', 'Ġsent', 'Ġgalaxy', 'Ġunfortunately', 'Ġdesired', 'Ġeffect', 'Ġcausing', 'Ġpower', 'Ġsystem', 'Ġoverload', 'Ġsubsequent', 'Ġshut', 'Ġactive', 'Ġtrans', 'p', 'ond', 'ers', 'Ġconcern', 'Ġneighboring', 'Ġsatellite', 'Ġoperators', 'Ġtype', 'Ġrecovery', 'Ġattempt', 'Ġwould', 'Ġpotential', 'Ġpermanently', 'Ġdamage', 'Ġsensitive', 'Ġhardware', 'Ġboard', 'Ġsatellite', 'Ġcould', 'Ġcontributed', 'Ġplacing', 'Ġsatellite', 'Ġpermanent', 'Ġunre', 'cover', 'able', 'Ġcontrol', 'Ġstate', 'Ġmay', 'Ġint', 'els', 'es', 'Ġworld', 'Ġskies', 'Ġconfirmed', 'Ġgalaxy', 'Ġwould', 'Ġpass', 'Ġclose', 'Ġlatter', "'s", 'Ġsatellite', 'Ġpotentially', 'Ġcausing', 'Ġinterference', 'Ġcable', 'Ġprogramming', 'Ġunited', 'Ġstates', 'Ġtwo', 'Ġsatellites', 'Ġbroadcast', 'Ġsimilar', 'Ġfrequencies', 'Ġmay', 'Ġj', 'une', 'Ġgalaxy', 'Ġpassed', 'Ġwithin', 'Ġhalf', 'Ġdegree', 'Ġtwo', 'Ġsatellites', 'Ġpassed', 'Ġclose', 'Ġparticularly', 'Ġclosest', 'Ġapproach', 'Ġmay', 'Ġj', 'une', 'Ġsignals', 'Ġgalaxy', 'Ġstill', 'active', 'Ġtrans', 'p', 'ond', 'ers', 'Ġcould', 'Ġinterfered', 'Ġsignals', 'Ġbroadcast', 'es', 'Ġmaneu', 'vered', 'Ġsatellite', 'Ġreduce', 'Ġpossibility', 'Ġinterference', 'es', 'Ġsatellite', 'Ġfollowed', 'Ġbehind', 'Ġgalaxy', 'Ġpass', 'Ġprovide', 'Ġbackup', 'Ġneeded', 'Ġj', 'une', 'Ġint', 'els', 'es', 'Ġreported', 'Ġinterference', 'Ġoccurred', 'Ġclosest', 'Ġapproach', 'Ġsatellites', 'Ġpassing', 'Ġwithin', 'Ġdegrees', 'Ġpassed', 'Ġgalaxy', 'Ġcontinued', 'Ġdrift', 'Ġeast', 'wards', 'Ġj', 'uly']</t>
+          <t>['Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'e', 'el', 'v', 'Ġpayload', 'Ġweight', 'Ġlaunch', 'Ġapproximately', '000', '000', 'Ġtime', 'Ġexp', 'ends', 'Ġpropell', 'ants', 'Ġachieve', 'Ġproper', 'Ġorbit', 'Ġweight', 'Ġapproximately', 'Ġsatellites', 'Ġoperate', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'ge', 'Ġorbit', 'Ġtakes', 'Ġdays', 'Ġorbital', 'Ġadjustments', 'Ġreach', 'Ġstable', 'Ġgeo', 'position', 'Ġlaunch', 'Ġupl', 'inks', 'Ġcross', 'links', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'links', 'Ġuse', 'Ġsuper', 'Ġhigh', 'Ġfrequency', 'Ġvariety', 'Ġfrequencies', 'Ġused', 'Ġwell', 'Ġdesire', 'Ġtightly', 'Ġfocused', 'links', 'Ġsecurity', 'Ġrequire', 'Ġrange', 'Ġantennas', 'Ġseen', 'Ġpicture', 'link', 'Ġphased', 'Ġarrays', 'Ġcross', 'links', 'Ġupl', 'ink', 'link', 'Ġnull', 'ing', 'Ġantennas', 'Ġbands', 'Ġlaunch', 'Ġpositioning', 'Ġelectronics', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġupl', 'ink', 'Ġphased', 'Ġarray', 'Ġupl', 'ink', 'link', 'Ġg', 'imb', 'aled', 'Ġdish', 'Ġantenna', 'Ġupl', 'ink', 'link', 'Ġearth', 'Ġcoverage', 'Ġhorns', 'Ġphased', 'Ġarray', 'Ġtechnology', 'Ġnew', 'Ġcommunications', 'Ġsatellites', 'Ġincreases', 'Ġreliability', 'Ġremoving', 'Ġmechanical', 'Ġmovement', 'Ġrequired', 'Ġg', 'imb', 'aled', 'Ġmotor', 'driven', 'Ġantennas', 'Ġlow', 'Ġgain', 'Ġearth', 'Ġcoverage', 'Ġantennas', 'Ġsend', 'Ġinformation', 'Ġanywhere', 'Ġthird', 'Ġearth', 'Ġcovered', 'Ġsatellite', "'s", 'Ġfootprint', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġprovide', 'Ġsuper', 'Ġhigh', 'gain', 'Ġearth', 'Ġcover', 'ages', 'Ġenabling', 'Ġworldwide', 'Ġunsc', 'hed', 'uled', 'Ġaccess', 'Ġusers', 'Ġincluding', 'Ġsmall', 'Ġportable', 'Ġterminals', 'Ġsubmarines', 'Ġmedium', 'Ġresolution', 'Ġcoverage', 'Ġantennas', 'rc', 'Ġhighly', 'Ġdirectional', 'spot', 'Ġcoverage', 'Ġtime', 'shared', 'Ġcover', 'Ġtargets', 'Ġtwo', 'Ġhigh', 'resolution', 'Ġcoverage', 'Ġarea', 'Ġantennas', 'Ġenable', 'Ġoperations', 'Ġpresence', 'beam', 'Ġjam', 'ming', 'Ġnull', 'ing', 'Ġantennas', 'Ġpart', 'Ġelectronic', 'Ġdefense', 'Ġhelps', 'Ġdiscriminate', 'Ġtrue', 'Ġsignals', 'Ġelectronic', 'Ġattack', 'Ġanother', 'Ġchange', 'Ġexisting', 'Ġsatellites', 'Ġusing', 'Ġsolid', 'state', 'Ġtransmit', 'ters', 'Ġrather', 'Ġtraveling', 'Ġwave', 'Ġtubes', 'Ġused', 'Ġhigh', 'power', 'Ġmilitary', 'Ġapplications', 'Ġtw', 'ts', 'Ġfixed', 'Ġpower', 'Ġoutput', 'Ġnewer', 'Ġdevices', 'Ġallow', 'Ġvarying', 'Ġtransmitted', 'Ġpower', 'Ġlowering', 'Ġprobability', 'Ġintercept', 'Ġoverall', 'Ġpower', 'Ġefficiency', 'Ġpayload', 'Ġflight', 'Ġsoftware', 'Ġcontains', 'Ġapproximately', '000', 'Ġlines', 'Ġreal', 'time', 'Ġdistributed', 'Ġembedded', 'Ġcode', 'Ġexecuting', 'Ġsimultaneously', 'board', 'Ġprocessors', 'Ġprovides', 'Ġindividual', 'Ġdigital', 'Ġdata', 'Ġstreams', 'Ġrates', 'Ġbits', 'second', 'Ġmeg', 'ab', 'second', 'Ġinclude']</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -490,7 +490,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>['Ġpassed', 'Ġgalaxy', 'hor', 'izons', 'Ġsatellite', 'Ġlocated', 'Â°', 'Ġwest', 'Ġowned', 'Ġjointly', 'Ġint', 'els', 'Ġperfect', 'Ġjs', 'Ġgroup', 'Ġpass', 'Ġreported', 'Ġcaused', 'Ġdisruption', 'Ġbroadcasts', 'Ġmade', 'Ġgalaxy', 'hor', 'izons', 'Ġj', 'uly', 'Ġgalaxy', 'Ġpassed', 'Ġanother', 'Ġint', 'els', 'Ġspacecraft', 'Ġgalaxy', 'Ġlocated', 'Â°', 'Ġwest', 'Ġclosest', 'Ġapproach', 'Ġoccurred', 'Ġj', 'uly', 'Ġaug', 'ust', 'Ġsatellite', 'Ġdrifted', 'Ġtoward', 'Ġsatellite', 'Ġowned', 'Ġg', 'ci', 'Ġcommunications', 'Ġcompany', 'Ġbroadcasting', 'Ġrural', 'Ġal', 'aska', 'Ġgalaxy', 'Ġpassed', 'ik', 'Ġfailure', 'Ġrecovery', 'Ġfailure', 'Ġreported', 'Ġpasses', 'Ġinterference', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġorbital', 'Ġslot', 'Â°', 'Ġwest', 'Ġnear', 'Ġoct', 'ober', 'Ġsatellite', 'Ġcontinued', 'Ġwatched', 'Ġtelecommunications', 'Ġcompanies', 'Ġdue', 'Ġpotential', 'Ġinterfering', 'Ġc', 'band', 'Ġfrequencies', 'Ġde', 'cember', 'Ġreported', 'Ġgalaxy', 'Ġpotentially', 'Ġcaused', 'Ġoutage', 'Ġnational', 'Ġweather', 'Ġservice', 'ap', 'ort', 'Ġfeed', 'Ġvia', 'es', 'Ġlocated', 'Ġwest', 'Ġde', 'cember', 'Ġfollowing', 'Ġadvisory', 'Ġissued', 'Ġrisk', 'Ġidentified', 'Ġgalaxy', 'Ġrogue', 'Ġsatellite', 'Ġtravers', 'es', 'es', 'Ġorbital', 'Ġposition', 'Ġmay', 'Ġresult', 'Ġpossible', 'Ġloss', 'Ġdata', 'Ġvia', 'Ġaw', 'ips', 'bn', 'ap', 'ort', 'Ġfeed', 'Ġpotential', 'Ġinterference', 'Ġmay', 'Ġtake', 'Ġplace', 'Ġinclusive', 'Ġminimize', 'Ġinterference', 'Ġsignals', 'Ġintended', 'es', 'Ġwest', 'Ġrouted', 'Ġupl', 'ink', 'ed', 'Ġvia', 'meter', 'Ġdish', 'es', 'Ġameric', 'om', 'Ġmaster', 'Ġground', 'Ġstation', 'Ġhaw', 'aii', 'Ġoutside', 'Ġgalaxy', 'Ġupl', 'ink', 'Ġfootprint', 'Ġthroughout', 'Ġfailure', 'Ġdrift', 'Ġperiod', 'Ġgalaxy', 'Ġstatus', 'Ġinformation', 'Ġregarding', 'Ġcontinued', 'Ġoperation', 'Ġtwo', 'Ġl', 'band', 'Ġwide', 'Ġarea', 'Ġaug', 'mentation', 'Ġsystem', 'Ġspace', 'Ġsegment', 'Ġtrans', 'p', 'ond', 'ers', 'Ġutilized', 'Ġaircraft', 'Ġprecision', 'Ġlocation', 'Ġremained', 'Ġunknown', 'Ġprior', 'Ġrecovery', 'Ġgalaxy', 'Ġexpected', 'Ġpass', 'ars', 'Ġdegrees', 'Ġwest', 'Ġlate', 'Ġde', 'cember', 'ars', 'Ġsince', 'Ġperformed', 'Ġwa', 'Ġmission', 'Ġdegrees', 'Ġwest', 'Ġgalaxy']</t>
+          <t>['Ġgo', 'Ġbeyond', 'Ġmil', 'star', "'s", 'Ġlow', 'Ġdata', 'Ġrate', 'ld', 'r', 'Ġmedium', 'Ġdata', 'Ġrate', 'Ġwell', 'Ġactually', 'Ġfairly', 'Ġslow', 'Ġhigh', 'Ġdata', 'Ġrate', 'Ġsubmarines', 'Ġfaster', 'Ġlinks', 'Ġdesignated', 'Ġextended', 'Ġdata', 'Ġrates', 'Ġnumber', 'Ġground', 'Ġterminals', 'Ġairborne', 'Ġterminal', 'Ġpart', 'Ġfamily', 'Ġadvanced', 'Ġbeyond', 'fab', 'Ġproject', 'Ġground', 'Ġstations', 'Ġinclude', 'Ġsingle', 'channel', 'Ġant', 'ij', 'Ġman', 'port', 'able', 'Ġterminal', 'sc', 'amp', 'Ġsecure', 'Ġmobile', 'Ġanti', 'jam', 'Ġreliable', 'Ġtactical', 'Ġterminal', 'smart', 'Ġsubmarine', 'Ġhigh', 'Ġdata', 'Ġrate', 'sub', 'Ġsystem', 'Ġbo', 'e', 'ing', 'Ġprime', 'Ġcontractor', 'Ġcommunications', 'Ġrock', 'well', 'Ġmajor', 'Ġsubcontract', 'ors', 'Ġfirst', 'Ġfab', 'incre', 'ment', 'Ġdelivered', 'Ġuse', 'Ġspirit', 'Ġaircraft', 'Ġfe', 'b', 'ruary', 'Ġplanned', 'Ġaircraft', 'Ġincluding', 'Ġaircraft', 'Ġinstallations', 'Ġgo', 'Ġfixed', 'Ġtransport', 'able', 'Ġcommand', 'Ġposts', 'Ġsuccessfully', 'Ġinter', 'operated', 'Ġlegacy', 'Ġcommunications', 'Ġusing', 'Ġcommand', 'Ġpost', 'Ġterminal', 'Ġarmy', 'Ġsingle', 'Ġchannel', 'Ġanti', 'jam', 'Ġman', 'Ġportable', 'Ġterminal', 'Ġfirst', 'Ġsatellite', 'Ġus', 'Ġsuccessfully', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġaug', 'ust', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġoccurred', 'Ġfour', 'Ġyears', 'Ġbehind', 'Ġschedule', 'Ġcontract', 'Ġawarded', 'Ġfirst', 'Ġlaunch', 'Ġexpected', 'Ġservices', 'Ġsatellites', 'usa', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġtaken', 'Ġplace', 'Ġprogram', 'Ġrestruct', 'ured', 'Ġoct', 'ober', 'Ġnational', 'Ġsecurity', 'Ġagency', 'ns', 'Ġdeliver', 'Ġkey', 'Ġcryptographic', 'Ġequipment', 'Ġpayload', 'Ġcontractor', 'Ġtime', 'Ġmeet', 'Ġlaunch', 'Ġschedule', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġsuccessfully', 'Ġplaced', 'Ġsatellite', 'Ġtransfer', 'Ġorbit', 'Ġper', 'ig', 'ee', 'Ġap', 'gee', '000', 'Ġinclination', 'Â°', 'Ġsatellite', 'Ġvehicle', "'s", 'Ġliquid', 'Ġap', 'gee', 'Ġengine', 'Ġprovided', 'Ġfailed', 'Ġraise', 'Ġorbit', 'Ġtwo', 'Ġattempts', 'Ġsolve', 'Ġproblem', 'Ġper', 'ig', 'ee', 'Ġaltitude', 'Ġraised', '00', 'Ġtwelve', 'Ġfir', 'ings', 'Ġsmaller', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'provided', 'Ġreaction', 'Ġengine', 'Ġassembly', 'Ġthr', 'usters', 'Ġoriginally', 'Ġintended', 'Ġattitude', 'Ġcontrol', 'Ġengine', 'Ġburns', 'Ġaltitude', 'Ġsolar', 'Ġpanels']</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -503,7 +503,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>['Ġperformed', 'Ġwest', 'Ġgalaxy', 'Ġlike', 'Ġmany', 'Ġcommunications', 'Ġsatellites', 'Ġreb', 'road', 'casts', 'Ġsignals', 'Ġreceives', 'Ġupl', 'ink', 'Ġfrequencies', 'Ġcorresponding', 'Ġc', 'band', 'link', 'Ġfrequencies', 'Ġtherefore', 'Ġpotential', 'Ġinterference', 'Ġexisted', 'Ġgalaxy', 'Ġdrifted', 'Ġline', 'Ġsight', 'Ġground', 'Ġupl', 'ink', 'Ġsegment', 'Ġintended', 'Ġanother', 'Ġcommunications', 'Ġsatellite', 'Ġoperating', 'Ġupl', 'ink', 'Ġfrequency', 'Ġrange', 'Ġpath', 'Ġgalaxy', 'Ġmagnitude', 'Ġinterference', 'Ġrisk', 'Ġdepended', 'Ġlarge', 'Ġnumber', 'Ġvariables', 'Ġincluding', 'Ġsize', 'Ġupl', 'ink', 'Ġantenna', 'Ġused', 'Ġlarger', 'Ġantenna', 'Ġlower', 'Ġrisk', 'Ġhit', 'Ġgalaxy', 'Ġlocation', 'Ġupl', 'ink', 'Ġwhether', 'Ġinside', 'Ġgalaxy', 'Ġfootprint', 'Ġonboard', 'Ġgain', 'Ġcapabilities', 'Ġsatellite', 'Ġprox', 'imate', 'Ġgalaxy', 'Ġsatellite', 'Ġoperators', 'Ġdevised', 'Ġvariety', 'Ġstrategies', 'Ġmitigate', 'Ġpotential', 'Ġinterference', 'Ġbirds', 'link', 'Ġtransmissions', 'Ġincluding', 'Ġtemporarily', 'Ġtransferring', 'Ġupl', 'inks', 'Ġlarger', 'Ġupl', 'ink', 'Ġantenna', 'Ġdeliberately', 'point', 'ing', 'Ġupl', 'ink', 'Ġantennas', 'Ġput', 'Ġgalaxy', 'Ġnull', 'Ġmaneuver', 'ing', 'Ġsatellite', 'Ġpassed', 'Ġmaintain', 'Ġminimum', 'Ġangular', 'Ġseparation', 'Ġincreasing', 'Ġsatellite', "'s", 'Ġgain', 'Ġsensitivity', 'Ġsettings', 'Ġallowing', 'Ġlowering', 'Ġupl', 'ink', 'Ġpower', 'Ġneeded', 'Ġlatter', 'ly', 'Ġmoving', 'Ġupl', 'ink', 'Ġlocation', 'Ġgalaxy', 'Ġupl', 'ink', 'Ġcoverage', 'e', 'Ġhaw', 'aii', 'Ġtechniques', 'Ġsuccessfully', 'Ġable', 'Ġreduce', 'Ġmitigate', 'Ġminimize', 'Ġcommercial', 'Ġsatellite', 'Ġoperations', 'Ġinterference', 'Ġpotential', 'Ġgalaxy', 'Ġfly', 'Ġsmaller', 'Ġsized', 'Ġstationary', 'Ġreceive', 'Ġsites', 'Ġlike', 'Ġused', 'ateurs', 'Ġsm', 'v', 'Ġwider', 'Ġbeam', 'Ġwidth', 'Ġreception', 'Ġpotential', 'Ġmay', 'Ġexperienced', 'Ġinterference', 'Ġpart', 'Ġcommercial', 'Ġoperators', 'Ġexperienced', 'Ġadverse', 'Ġeffects', 'Ġgalaxy', 'Ġfailure', 'Ġperiod', 'Ġthanks', 'Ġexecution', 'Ġmitigation', 'Ġpractices', 'Ġdevised', 'Ġwake', 'Ġcrisis', 'Ġsatellite', 'Ġtheor', 'ized', 'Ġlose', 'Ġattitude', 'Ġcontrol', 'Ġreaction', 'Ġwheels', 'Ġbecame', 'Ġsaturated', 'Ġevent', 'Ġoccurred', 'Ġwould', 'Ġprevent', 'Ġspacecraft', "'s", 'Ġsolar', 'Ġpanels', 'Ġtracking', 'Ġsun', 'Ġwould', 'Ġshut', 'Ġpower', 'Ġreset', 'Ġevent', 'Ġattempts', 'Ġwould', 'Ġmade', 'Ġrecover', 'Ġcontrol', 'Ġsatellite', 'Ġevent', 'Ġoriginally', 'Ġpredicted', 'Ġlate', 'Ġaug', 'ust', 'Ġearly', 'Ġse', 'pt', 'ember', 'Ġupl', 'ink', 'Ġsignal', 'Ġavoidance', 'Ġmitigation', 'Ġpower', 'Ġloss', 'Ġpredictions', 'Ġcriticism', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġint', 'els', 'Ġrevised', 'Ġestimate', 'Ġsometime', 'mber', 'Ġde', 'cember']</t>
+          <t>['Ġdeployed', 'Ġorbit', 'Ġraised', 'Ġtoward', 'Ġoperational', 'Ġorbit', 'Ġcourse', 'Ġnine', 'Ġmonths', 'Ġusing', 'Ġnew', 'ton', 'Ġhall', 'Ġthr', 'usters', 'Ġalso', 'Ġprovided', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġform', 'Ġelectric', 'Ġpropulsion', 'Ġhighly', 'Ġefficient', 'Ġlow', 'Ġthrust', 'Ġtook', 'Ġmuch', 'Ġlonger', 'Ġinitially', 'Ġintended', 'Ġdue', 'Ġlower', 'Ġstarting', 'Ġaltitude', 'Ġmaneuvers', 'Ġled', 'Ġprogram', 'Ġdelays', 'Ġsecond', 'Ġthird', 'Ġsatellite', 'Ġvehicle', 'Ġla', 'es', 'Ġanalyzed', 'Ġgovernment', 'Ġaccountability', 'Ġoffice', 'Ġreport', 'Ġreleased', 'Ġj', 'uly', 'Ġstated', 'Ġblocked', 'Ġfuel', 'Ġline', 'Ġliquid', 'Ġap', 'gee', 'Ġengine', 'Ġlikely', 'Ġcaused', 'Ġpiece', 'Ġcloth', 'Ġinadvertently', 'Ġleft', 'Ġline', 'Ġmanufacturing', 'Ġprocess', 'Ġbelieved', 'Ġprimary', 'Ġcause', 'Ġfailure', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġselected', 'Ġacquisition', 'Ġreport', 'Ġadds', 'Ġfuel', 'Ġloading', 'Ġprocedures', 'Ġun', 'met', 'Ġthermal', 'Ġcontrol', 'Ġrequirements', 'Ġcould', 'Ġalso', 'Ġcontributed', 'Ġremaining', 'Ġsatellites', 'Ġdeclared', 'Ġflight', 'ready', 'Ġmonth', 'Ġprior', 'Ġrelease', 'Ġreport', 'Ġlike', 'Ġfirst', 'Ġsatellite', 'Ġsecond', 'Ġlaunched', 'las', 'Ġflying', 'Ġconfiguration', 'Ġlaunch', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġtook', 'Ġplace', 'Ġmay', 'Ġthree', 'Ġmonths', 'Ġmaneuver', 'ing', 'Ġreached', 'Ġproper', 'Ġposition', 'Ġtesting', 'Ġprocedures', 'Ġstarted', 'Ġcompletion', 'Ġcheckout', 'Ġannounced', 'mber', 'Ġcontrol', 'Ġturned', 'th', 'Ġair', 'Ġforce', 'Ġoperations', 'Ġexpected', 'year', 'Ġservice', 'Ġlife', 'Ġthird', 'Ġsatellite', 'Ġlaunched', 'Ġcape', 'aver', 'al', 'Ġse', 'pt', 'ember', 'Ġ08', 'Ġtwo', 'hour', 'Ġwindow', 'Ġlaunch', 'Ġsatellite', 'Ġopened', 'Ġ07', '04', 'Ġut', 'c', 'Ġlaunch', 'Ġoccurred', 'Ġsoon', 'Ġweather', 'related', 'Ġclouds', 'Ġhigh', 'alt', 'itude', 'Ġwinds', 'Ġcleared', 'Ġsufficiently', 'Ġmeet', 'Ġlaunch', 'Ġcriteria', 'Ġsuccessful', 'Ġlaunch', 'Ġfailure', 'Ġkick', 'Ġmotor', 'Ġrecovery', 'Ġusing', 'Ġhall', 'effect', 'Ġthr', 'usters', 'usa', 'usa', 'usa', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġfourth', 'Ġsatellite', 'Ġlaunched', 'Ġoct', 'ober', 'Ġcape', 'aver', 'al', 'Ġ04', 'Ġut', 'c', 'Ġusing', 'las', 'Ġrocket', 'Ġoperated', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', ').[', 'Ġfifth', 'Ġsatellite']</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -516,7 +516,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['Ġsubsequent', 'Ġcriticism', 'Ġactual', 'Ġscience', 'Ġbehind', 'Ġorbital', 'Ġsciences', 'Ġpredictions', 'Ġint', 'els', 'Ġcompletely', 'Ġabandoned', 'Ġpublished', 'Ġtimeline', 'Ġmethod', 'Ġinstead', 'Ġperiod', 'Ġint', 'els', 'Ġstated', 'Ġbased', 'Ġrevised', 'Ġanalysis', 'Ġestimated', 'Ġwindow', 'Ġgalaxy', 'point', 'Ġloss', 'Ġpower', 'Ġcould', 'Ġoccur', 'Ġearly', 'Ġmonth', 'Ġwithout', 'Ġclar', 'ifying', 'Ġmonth', 'Ġindicated', 'Ġhypothesis', 'Ġused', 'Ġcalculate', 'Ġtimeline', 'Ġpotential', 'Ġoccurrence', 'Ġloss', 'Ġpower', 'Ġimp', 'rec', 'ise', 'Ġdue', 'Ġfact', 'Ġsatellite', 'Ġexperienced', 'Ġerratic', 'Ġloading', 'Ġconditions', 'Ġradio', 'Ġfrequency', 'Ġsignals', 'Ġsince', 'Ġbegan', 'Ġdrift', 'Ġmonths', 'Ġinitial', 'Ġfailure', 'Ġdate', 'Ġpublished', 'Ġtimelines', 'Ġshut', 'Ġproved', 'Ġhopes', 'Ġpublic', 'Ġrelations', 'Ġcampaign', 'Ġbased', 'Ġtheory', 'Ġinterview', 'Ġconducted', 'Ġoct', 'ober', 'Ġsat', 'con', 'Ġconference', 'Ġint', 'els', 'Ġorbital', 'Ġadmitted', 'Ġhoped', 'Ġtimeline', 'Ġscenario', 'Ġtheory', 'Ġunprecedented', 'Ġsituation', 'Ġlearning', 'Ġde', 'cember', 'Ġint', 'els', 'Ġsuccessfully', 'Ġregained', 'Ġcontrol', 'Ġsatellite', 'Ġbase', 'band', 'Ġequipment', 'Ġcommand', 'Ġunit', 'Ġreset', 'Ġfollowing', 'Ġloss', 'Ġlock', 'Ġfull', 'Ġdischarge', 'Ġbatteries', 'Ġreportedly', 'Ġcritical', 'Ġphases', 'Ġrecovery', 'Ġgalaxy', 'Ġcompleted', 'Ġemergency', 'Ġcommand', 'Ġpatch', 'Ġwould', 'Ġallow', 'Ġground', 'Ġcontrollers', 'Ġgain', 'Ġaccess', 'Ġredundant', 'Ġb', 'bes', 'Ġevent', 'Ġsimilar', 'Ġfailure', 'Ġfuture', 'Ġalso', 'Ġsuccessfully', 'Ġapplied', 'Ġgalaxy', 'Ġaccording', 'Ġint', 'els', 'Ġgalaxy', 'Ġrelocated', 'Â°', 'Ġwest', 'Ġorder', 'Ġconduct', 'Ġorbit', 'Ġtesting', 'Ġviability', 'Ġpayload', 'Ġreturn', 'Ġservice', 'Ġsatellite', 'Ġgalaxy', 'Ġfully', 'Ġrecovered', 'Ġmoved', 'Ġback', 'Â°', 'Ġwest', 'Ġgalaxy', 'Ġspacecraft', 'Ġrelocated', 'Ġintended', 'Ġmission', 'Â°', 'Ġwest', 'Ġoct', 'ober', 'Ġint', 'els', 'Ġtransitioned', 'Â°', 'Ġwest', 'Ġcustomers', 'Ġback', 'Ġgalaxy', 'Ġgalaxy', 'Ġaug', 'ust', 'Ġint', 'els', 'Ġsubmitted', 'Ġfiling', 'Ġrequesting', 'Ġpermission', 'Ġsatellite', 'Ġexceed', 'Ġstation', 'Ġkeeping', 'Ġlimits', 'Ġindicating', 'Ġcontrol', 'Ġlost', 'Ġaug', 'ust', 'Ġspacecraft', 'Ġmuted', 'Ġtrans', 'p', 'onder', 'Ġpayload', 'Ġprogrammed', 'Ġautomatically', 'Ġcase', 'Ġloss', 'Ġground', 'Ġcontrol', 'Ġdays', 'Ġlast', 'Ġcommand', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġlist', 'Ġint', 'els', 'Ġsatellites', 'Ġzombie', 'Ġsatellite']</t>
+          <t>['Ġlaunched', 'Ġaug', 'ust', 'Ġcape', 'aver', 'al', 'Ġut', 'c', 'Ġusing', 'las', 'Ġrocket', 'Ġsecondary', 'Ġpayload', 'Ġnamed', 'Ġaccompanied', 'Ġsatellite', 'Ġorbit', 'Ġsixth', 'Ġsatellite', 'Ġlaunched', 'Ġmarch', 'Ġut', 'c', 'las', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġfirst', 'Ġlaunch', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmission', 'Ġsince', 'Ġestablishment', 'Ġnew', 'Ġmilitary', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġsystem', 'Ġachieves', 'Ġinitial', 'Ġoperational', 'Ġcapability', 'Ġlos', 'Ġangel', 'es', 'Ġair', 'Ġforce', 'Ġbase', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'two', 'Ġu', 'Ġmilitary', 'Ġsatellite', 'Ġlaunches', 'Ġdelayed', 'Ġnext', 'Ġyear', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġretrieved', 'Ġjan', 'uary', 'Ġready', 'Ġlaunch', 'Ġlos', 'Ġangel', 'es', 'Ġair', 'Ġforce', 'Ġbase', 'Ġretrieved', 'Ġaug', 'ust', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġretrieved', 'Ġj', 'une', 'adv', 'anced', 'Ġpayload', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġarchived', 'Ġoriginal', 'ht', 'Ġmarch', 'Ġretrieved', 'mber', 'Ġwhite', 'rew', 'us', 'mc', 'Ġeyes', 'Ġimproved', 'Ġar', 'ctic', 'Ġcommunications', 'Ġsystems', 'Ġprocedures', 'Ġj', 'ane', "'s", 'Ġinformation', 'Ġgroup', 'Ġcapt', 'Ġhill', 'Ġwarned', 'Ġus', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', "'s", 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġsat', 'Ġconstellation', 'Ġineffective', 'th', 'Ġparallel', 'Ġnorth', 'Ġ[...]', 'lock', 'heed', 'Ġmart', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'enh', 'anced', 'Ġpolar', 'Ġsystem', 'usa', 'usa', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġlore', 'ike', 'jan', 'uary', 'extreme', 'Ġcost', 'Ġgrowth', 'Ġthemes', 'Ġus', 'Ġair', 'Ġforce', 'Ġmajor', 'Ġdefense', 'Ġacquisition', 'Ġprograms', 'Ġresearch', 'Ġgate', 'Ġretrieved', 'Ġapr', 'il', 'Ġelf', 'ers', 'Ġg', 'Ġmill', 'er', 'winter', 'future', 'Ġu', 'Ġmilitary', 'Ġsatellite', 'Ġcommunication', 'Ġsystems', 'Ġaerospace', 'Ġcorporation', 'Ġcross', 'link', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġaug', 'ust', 'ag', 'ile', 'Ġantennas', 'Ġaid', 'Ġwarriors', 'Ġaf', 'ce', 'Ġsignal', 'Ġj', 'uly']</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -529,7 +529,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['gal', 'axy', 'Ġint', 'els', 'Ġarchived', 'Ġoriginal', '08', 'Ġretrieved', 'Ġrecovery', 'Ġfailure', 'Ġrecovery', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġgalaxy', 'Ġint', 'els', 'Ġarchived', 'Ġoriginal', '07', 'Ġretrieved', '07', 'wa', 'Ġpr', 'n', 'Ġresumes', 'Ġnormal', 'Ġoperation', 'Ġg', 'Ġge', 'osp', 'atial', 'Ġworld', 'web', 'arch', 'Ġarchived', 'Ġoriginal', '07', 'Ġretrieved', '03', 'Ġrac', 'hel', 'Ġjew', 'ett', '08', 'int', 'els', 'Ġloses', 'Ġcommand', 'Ġgalaxy', 'Ġsatellite', 'Ġvia', 'Ġsatellite', 'ge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġcontrol', 'Ġsegment', 'Ġgoogle', 'Ġsearch', 'google', 'Ġretrieved', 'Ġapr', 'il', 'Ġsatellite', 'Ġdatabase', 'Ġunion', 'Ġconcerned', 'Ġscientists', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'gal', 'axy', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġmay', 'orb', 'ital', 'built', 'Ġgalaxy', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġpan', 'ams', 'Ġcompany', 'Ġlaunches', 'Ġsecond', 'Ġgalaxy', 'Ġsatellite', 'Ġpan', 'ams', 'Ġpast', 'Ġtwo', 'Ġmonths', 'business', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'cd', 'owell', 'Ġj', 'athan', 'launch', 'Ġlog', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġmay', 'Ġboost', 'Ġcivil', 'Ġmilitary', 'Ġcommunications', 'Ġsy', 'racuse', 'Ġgalaxy', 'Ġlaunch', 'Ġkit', 'rian', 'esp', 'ace', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'http', 'arian', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'cd', 'owell', 'Ġj', 'athan', 'index', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcatalog', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġfer', 'ster', 'Ġwar', 'ren', 'Ġapr', 'il', 'int', 'els', 'Ġloses', 'Ġcontact', 'Ġgalaxy', 'Ġsatellite', 'web', 'ci', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'gal', 'axy', 'eb', 'au', 'Ġretrieved', 'Ġapr', 'il', 'Ġgalaxy', 'Ġsaga', 'Ġcontinues']</t>
+          <t>['north', 'rop', 'Ġgr', 'um', 'man', 'Ġqual', 'ï', '¬', 'ģ', 'es', 'Ġextended', 'Ġdata', 'Ġrate', 'Ġsoftware', 'Ġadvanced', 'Ġmilitary', 'Ġcommunications', 'Ġsatellite', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġtechnology', 'mber', 'Ġarchived', 'Ġoriginal', 'es', 'html', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġbomber', 'Ġreceives', 'Ġfirst', 'Ġfab', 'Ġsatellite', 'Ġcommunication', 'Ġterminal', 'Ġde', 'ag', 'el', 'Ġfe', 'b', 'ruary', 'Ġro', 'bert', 'ud', 'ney', 'oct', 'ober', 'game', 'Ġchang', 'ers', 'Ġspace', 'Ġair', 'Ġforce', 'Ġmagazine', 'Ġretrieved', 'Ġapr', 'il', 'Ġdefense', 'Ġacquisitions', 'Ġassessments', 'Ġselected', 'Ġweapon', 'Ġprograms', 'web', 'ar', 'Ġunited', 'Ġstates', 'Ġgovernment', 'Ġaccountability', 'ï', '¬', 'ģ', 'ce', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġray', 'Ġspace', 'flight', 'Ġair', 'Ġforce', 'Ġsatellite', "'s", 'Ġepic', 'Ġascent', 'Ġï', '¬', 'ģ', 'n', 'ish', 'Ġsoon', 'http', 'space', 'ï', '¬', 'Ĥ', 'Ġoct', 'ober', 'access', 'ed', 'Ġde', 'cember', 'main', 'Ġengine', 'Ġprobably', 'Ġblame', 'Ġtrouble', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġray', 'Ġoct', 'ober', 'air', 'Ġforce', 'Ġsatellite', "'s", 'Ġepic', 'Ġascent', 'Ġï', '¬', 'ģ', 'n', 'ish', 'Ġsoon', 'space', 'ï', '¬', 'Ĥ', 'ig', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'dep', 'artment', 'Ġdefense', 'Ġselected', 'Ġacquisition', 'Ġreport', 'Ġde', 'cember', 'web', 'arch', 'es', 'wh', 'mil', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'air', 'Ġforce', 'Ġrec', 'ou', 'ps', 'Ġcosts', 'Ġsave', 'Ġstranded', 'Ġsatellite', 'http', 'Ġretrieved', 'Ġj', 'une', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġmission', 'Ġstatus', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġmission', 'Ġstatus', 'Ġcenter', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'mber', 'Ġadvanced']</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -542,7 +542,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['Ġdou', 'g', 'Ġlung', 'Ġtv', 'technology', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġapr', 'il', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġapr', 'il', 'orb', 'ital', 'Ġblames', 'Ġgalaxy', 'Ġfailure', 'Ġsolar', 'Ġstorm', 'ww', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', '.,', 'Ġspace', 'Ġnews', 'Ġj', 'uly', 'Ġp', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmay', 'att', 'empt', 'Ġshut', 'Ġzombie', 'Ġsatellite', 'Ġgalaxy', 'Ġfails', 'htt', 'Ġspace', 'Ġretrieved', 'Ġmay', 'Ġhill', 'Ġje', 'ff', 'Ġmay', 'int', 'els', 'Ġwarns', 'Ġgalaxy', 'Ġmay', 'Ġdrift', 'Ġorbit', 'web', 'arch', 'iv', 'Ġsatell', 'et', 'oday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġapr', 'il', 'gal', 'axy', 'Ġstill', 'Ġad', 'rift', 'Ġposes', 'Ġthreat', 'Ġorbital', 'Ġneighbors', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'http', 'sp', 'ac', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'os', 'Ġj', 'athan', 'Ġmay', 'z', 'ombie', 'Ġsatellite', 'Ġprompts', 'Ġorbital', 'Ġw', 'alt', 'z', 'Ġnews', 'Ġretrieved', 'Ġmay', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġj', 'une', 'int', 'els', 'es', 'Ġsafely', 'Ġnegotiate', 'Ġpassage', 'Ġway', 'ward', 'Ġcraft', 'ht', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'http', 'sp', 'ac', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġj', 'uly', 'int', 'els', 'Ġaver', 'ts', 'Ġgalaxy', 'Ġinterference', 'archive', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'uly', 'Ġgalaxy', 'Ġint', 'els', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'z', 'ombies', 'Ġthreatens', 'Ġar', 'ctic', 'Ġtelecommunications', 'Ġoct', 'ober', 'Ġfallout', 'Ġgalaxy']</t>
+          <t>['Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġhal', 'v', 'ors', 'en', 'Ġtodd', 'Ġse', 'pt', 'ember', 'las', 'Ġro', 'ars', 'Ġlife', 'Ġair', 'Ġforce', 'Ġsatellite', 'Ġonboard', 'htt', 'board', 'Ġfl', 'ida', 'Ġtoday', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġlaunch', 'Ġarchived', 'Ġoct', 'ober', 'Ġway', 'back', 'Ġmachine', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaccessed', '09', 'protected', 'Ġmilitary', 'Ġsatellite', 'Ġcommunication', 'Ġproject', 'Ġmarks', 'Ġsuccessful', 'Ġlaunch', 'Ġcape', 'aver', 'al', 'Ġmaple', 'Ġleaf', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'las', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġu', 'la', 'Ġretrieved', 'Ġj', 'une', 'Ġstep', 'hen', 'Ġcl', 'ark', 'Ġmarch', 'space', 'Ġforce', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġscheduled', 'Ġth', 'ursday', 'sp', 'ac', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġk', 'el', 'becca', 'Ġmarch', 'space', 'Ġforce', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġhill', 'Ġretrieved', 'Ġmarch', 'Ġdun', 'n', 'Ġmar', 'cia', 'Ġmarch', 'space', 'Ġforce', 'Ġlaunches', 'st', 'Ġmission', 'Ġvirus', 'Ġprecautions', 'http', 'Ġassociated', 'Ġpress', 'Ġretrieved', 'Ġmarch', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġmarch', 'ula', "'s", 'las', 'Ġlaunches', 'Ġcommunications', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġu', 'Ġspace', 'Ġforce', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġbr', 'ad', 'Ġber', 'gan', 'Ġmarch', 'Ġfirst', 'Ġtime', 'Ġus', 'Ġspace', 'Ġforce', 'Ġlaunching', 'Ġorbit', 'las', 'Ġrocket', 'Ġinteresting', 'Ġengineering', 'Ġretrieved', 'Ġapr', 'il', 'Ġedit', 'old', 'id', 'Ġarticle', 'Ġuses', 'Ġcontent', 'adv', 'anced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'atellite', ')"', 'Ġlicensed', 'Ġway', 'Ġpermits', 'Ġreuse', 'Ġcreative', 'Ġcommons', 'Ġun', 'ported', 'Ġlicense', 'Ġrelevant', 'Ġterms', 'Ġmust', 'Ġfollowed', 'Ġlaunch', 'Ġcc', 'af', 'Ġaug', 'ust', '07', 'Ġed', 'Ġlaunch', 'Ġcc', 'af', 'Ġ04', 'Ġmay', 'Ġed', 'Ġage', 'html', 'Ġlaunch', 'Ġcc', 'af', 'Ġse', 'pt', 'ember', 'Ġed']</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -555,7 +555,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['Ġdou', 'g', 'Ġlung', 'Ġtv', 'technology', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġapr', 'il', 'Ġnational', 'Ġweather', 'Ġservice', 'c', 'data', 'Ġmanagement', 'Ġchange', 'Ġnotices', 'Ġn', 'ws', 'aa', 'gov', 'Ġn', 'ws', 'ï', '¬', 'ģ', 'ce', 'Ġchief', 'Ġinformation', 'ï', '¬', 'ģ', 'cer', 'Ġtelecommunications', 'Ġoperations', 'Ġcenter', 'Ġsilver', 'Ġspring', 'Ġjan', 'Ġ04', 'Ġrich', 'ard', 'Ġrob', 'inson', 'national', 'Ġweather', 'Ġservice', 'c', 'data', 'Ġmanagement', 'Ġchange', 'Ġnotices', 'n', 'ws', 'aa', 'gov', 'Ġretrieved', 'Ġapr', 'il', 'z', 'ombies', 'Ġthree', 'Ġsatellites', 'Ġcross', 'h', 'airs', 'gal', 'axy', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'z', 'ombie', 'Ġsatellite', 'Ġanother', 'Ġï', '¬', 'Ĥ', 'Ġl', 'ite', 'ï', '¬', 'Ĥ', 'html', 'Ġnews', 'mber', 'run', 'away', 'Ġzombie', 'Ġsatellite', 'Ġgalaxy', 'Ġcontinues', 'Ġpose', 'Ġinterference', 'Ġthreat', 'http', 'space', 'c', 'Ġspace', 'Ġoct', 'ober', 'Ġretrieved', 'Ġapr', 'il', 'Ġturned', 'Ġsatellite', 'Ġzombie', 'Ġstatic', 'Ġshock', 'Ġnews', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'Ġnews', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġretrieved', 'Ġaug', 'ust', 'Ġretrieved']</t>
+          <t>['Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -568,7 +568,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>['Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġlist', 'Ġtypes', 'Ġu', 'Ġreconnaissance', 'Ġsatellites', 'Ġdeployed', 'Ġonward', 'Ġaerial', 'Ġview', 'Ġos', 'ama', 'Ġbin', 'Ġlad', 'en', "'s", 'Ġcompound', 'Ġp', 'ak', 'istani', 'Ġcity', 'Ġab', 'bott', 'abad', 'Ġmade', 'Ġc', 'ia', 'Ġcor', 'ona', 'Ġsatellite', 'Ġreconnaissance', 'Ġsatellite', 'Ġreconnaissance', 'Ġsatellite', 'Ġintelligence', 'Ġsatellite', 'common', 'ly', 'Ġalthough', 'Ġun', 'offic', 'ially', 'Ġreferred', 'Ġsatellite', 'Ġearth', 'Ġobservation', 'Ġsatellite', 'Ġcommunications', 'Ġsatellite', 'Ġdeployed', 'Ġmilitary', 'Ġintelligence', 'Ġapplications', 'Ġfirst', 'Ġgeneration', 'Ġtype', 'e', '.,', 'Ġcor', 'ona', 'Ġz', 'en', 'Ġtook', 'Ġphotographs', 'Ġejected', 'isters', 'Ġphotographic', 'Ġfilm', 'Ġwould', 'Ġdescend', 'Ġback', 'Ġearth', "'s", 'Ġatmosphere', 'Ġcor', 'ona', 'Ġcapsules', 'Ġretrieved', 'Ġmid', 'air', 'Ġfloated', 'Ġparach', 'utes', 'Ġlater', 'Ġspacecraft', 'Ġdigital', 'Ġimaging', 'Ġsystems', 'Ġdownloaded', 'Ġimages', 'Ġvia', 'Ġencrypted', 'Ġradio', 'Ġlinks', 'Ġunited', 'Ġstates', 'Ġinformation', 'Ġavailable', 'Ġreconnaissance', 'Ġsatellites', 'Ġprograms', 'Ġexisted', 'Ġinformation', 'Ġdeclass', 'ified', 'Ġdue', 'Ġage', 'Ġinformation', 'Ġprograms', 'Ġtime', 'Ġstill', 'Ġclassified', 'Ġinformation', 'Ġsmall', 'Ġamount', 'Ġinformation', 'Ġavailable', 'Ġsubsequent', 'Ġmissions', 'date', 'Ġreconnaissance', 'Ġsatellite', 'Ġimages', 'Ġdeclass', 'ified', 'Ġoccasion', 'Ġleaked', 'Ġcase', 'Ġphotographs', 'Ġsent', 'Ġj', 'ane', "'s", 'Ġdefence', 'Ġweekly', 'Ġmarch', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġofficially', 'Ġordered', 'Ġdevelopment', 'Ġadvanced', 'Ġreconnaissance', 'Ġsatellite', 'Ġprovide', 'Ġcontinuous', 'Ġsurveillance', 'pre', 'selected', 'Ġareas', 'Ġearth', 'Ġorder', 'Ġdetermine', 'Ġstatus', 'Ġpotential', 'Ġenemy', 'âĢ', 'Ļ', 'Ġwar', 'making', 'Ġcapability', '".[', 'Ġseveral', 'Ġmajor', 'Ġtypes', 'Ġreconnaissance', 'Ġsatellite', 'Ġmissile', 'Ġearly', 'Ġwarning', 'Ġprovides', 'Ġwarning', 'Ġattack', 'Ġdetecting', 'Ġballistic', 'Ġmissile', 'Ġlaunches', 'Ġearliest', 'Ġknown', 'Ġmissile', 'Ġdefense', 'Ġalarm', 'Ġsystem', 'Ġnuclear', 'Ġexplosion', 'Ġdetection', 'Ġdetects', 'Ġnuclear', 'Ġdeton', 'ation', 'Ġspace', 'Ġvel', 'Ġearliest', 'Ġknown', 'Ġhistory', 'Ġtypes', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġu', 'Ġlac', 'rosse', 'Ġradar', 'Ġsatellite', 'Ġconstruction', 'Ġmodel', 'Ġg', 'erman', 'Ġsar', 'lu', 'pe', 'Ġreconnaissance', 'Ġsatellite', 'Ġinside', 'Ġcosmos', 'Ġrocket', 'Ġmicrowave', 'Ġinterception', 'r', 'hy', 'ol', 'ite', 'Ġelectronic', 'Ġreconnaissance', 'Ġsignals', 'Ġintelligence', 'Ġintercept', 'Ġstray', 'Ġradio', 'Ġwaves', 'Ġsol', 'rad', 'Ġearliest', 'Ġoptical', 'Ġimaging', 'Ġsurveillance', 'Ġearth', 'Ġimaging', 'Ġsatellites', 'Ġsatellite', 'Ġimages', 'Ġsurvey', 'Ġclose']</t>
+          <t>['las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'las', 'Ġfamily', 'las', 'Ġcomparison', 'Ġrole', 'Ġexpend', 'able', 'Ġlaunch', 'Ġsystem', 'Ġvarious', 'Ġapplications', 'Ġmanufacturer', 'Ġconv', 'air', 'Ġgeneral', 'Ġdynamics', 'Ġlock', 'heed', 'Ġmart', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'Ġintroduction', 'Ġstatus', 'las', 'current', 'Ġprimary', 'Ġusers', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġnational', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġadministration', 'Ġproduced', 'âĢĵ', 'dec', 'ade', 'Ġvariants', 'las', 'las', 'las', 'las', 'las', 'las', 'rocket', 'Ġfamily', 'las', 'Ġfamily', 'Ġus', 'Ġmissiles', 'Ġspace', 'Ġlaunch', 'Ġvehicles', 'Ġoriginated', 'las', 'las', 'Ġinter', 'continental', 'Ġballistic', 'Ġmissile', 'Ġprogram', 'Ġinitiated', 'Ġlate', 'Ġconv', 'air', 'Ġdivision', 'Ġgeneral', 'las', 'Ġliquid', 'Ġpropell', 'ant', 'Ġrocket', 'Ġburning', 'Ġk', 'eros', 'ene', 'Ġfuel', 'Ġliquid', 'Ġthree', 'Ġengines', 'Ġconfigured', 'Ġunusual', 'stage', 'half', 'par', 'allel', 'Ġstaging', 'Ġdesign', 'Ġtwo', 'board', 'Ġbooster', 'Ġengines', 'Ġj', 'ett', 'ison', 'ed', 'Ġalong', 'Ġsupporting', 'Ġstructures', 'Ġascent', 'Ġcenter', 'Ġsustain', 'er', 'Ġengine', 'Ġpropell', 'ant', 'Ġtanks', 'Ġstructural', 'Ġelements', 'Ġremained', 'Ġconnected', 'Ġpropell', 'ant', 'Ġdepletion', 'Ġengine', 'Ġshutdown', 'las', 'Ġname', 'Ġoriginally', 'Ġproposed', 'Ġk', 'arel', 'Ġboss', 'art', 'Ġdesign', 'Ġteam', 'Ġworking', 'Ġconv', 'air', 'Ġproject', 'Ġusing', 'Ġname', 'Ġmighty', 'Ġtitan', 'Ġg', 'reek', 'Ġmythology', 'Ġreflected', 'Ġmissile', "'s", 'Ġplace', 'Ġbiggest', 'Ġpowerful', 'Ġtime', 'Ġalso', 'Ġreflected', 'Ġparent', 'Ġcompany', 'Ġconv', 'air', 'las', 'Ġcorporation', 'Ġmissiles', 'Ġsaw', 'Ġbrief', 'Ġservice', 'Ġlast', 'Ġsquadron', 'Ġtaken', 'Ġoperational', 'Ġalert', 'Ġhowever', 'las', 'Ġboosters', 'Ġlaunched', 'Ġfirst', 'Ġfour', 'Ġus', 'Ġastronauts', 'Ġorbit', 'Ġearth', 'Ġcontrast', 'Ġpreceding', 'Ġtwo', 'Ġred', 'stone', 'Ġsub', 'orb', 'ital', 'Ġlaunches', 'las', 'ag', 'ena', 'las', 'cent', 'aur', 'Ġsatellite', 'Ġlaunch', 'Ġvehicles', 'Ġalso', 'Ġderived', 'Ġdirectly', 'Ġoriginal', 'las', 'las', 'cent', 'aur', 'Ġevolved', 'las', 'Ġvarious', 'Ġmodels', 'Ġlaunched', 'Ġtimes', 'Ġlaunches', 'Ġsucceeding', 'las', 'las', 'Ġstill', 'Ġservice', 'Ġlaunches', 'Ġplanned', 'Ġmid', 'las', 'Ġlaunches', 'Ġconducted', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'Ġv']</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>['look', 'Ġtele', 'photo', 'Ġcor', 'ona', 'Ġearliest', 'Ġknown', 'Ġspectral', 'Ġimaging', 'Ġcommonplace', 'Ġradar', 'Ġimaging', 'Ġsurveillance', 'Ġspace', 'based', 'Ġrad', 'ars', 'Ġuse', 'Ġsynthetic', 'ap', 'ert', 'ure', 'Ġradar', 'Ġused', 'Ġnight', 'Ġcloud', 'Ġcover', 'Ġearliest', 'Ġknown', 'v', 'iet', 'Ġus', 'Ġseries', 'Ġexamples', 'Ġreconnaissance', 'Ġsatellite', 'Ġmissions', 'Ġhigh', 'Ġresolution', 'Ġphotography', 'im', 'int', 'Ġmeasurement', 'Ġsignature', 'Ġintelligence', 'mas', 'int', 'Ġcommunications', 'Ġeaves', 'dropping', 'ig', 'int', 'Ġcovert', 'Ġcommunications', 'Ġmonitoring', 'Ġnuclear', 'Ġtest', 'Ġban', 'Ġcompliance', 'see', 'Ġnational', 'Ġtechnical', 'Ġmeans', 'Ġdetection', 'Ġmissile', 'Ġlaunches', 'Ġaug', 'ust', 'Ġthought', 'billion', 'Ġhigh', 'powered', 'Ġsatellite', 'Ġcapable', 'Ġsnapping', 'Ġpictures', 'Ġdetailed', 'Ġenough', 'Ġdistinguish', 'Ġmake', 'Ġmodel', 'Ġautomobile', 'Ġhundreds', 'Ġmiles', '"[', 'Ġlaunched', 'Ġcal', 'ornia', "'s", 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġusing', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlauncher', 'Ġameric', "'s", 'Ġhighest', 'pay', 'load', 'Ġspace', 'Ġlaunch', 'Ġvehicle', 'Ġtime', 'Ġfe', 'b', 'ruary', 'Ġr', 'ussian', 'Ġk', 'os', 'mos', 'Ġoriginally', 'Ġlaunched', 'Ġused', 'Ġnaval', 'Ġmissile', 'Ġtargeting', 'Ġmade', 'Ġuncontrolled', 'Ġatmospheric', 'Ġentry', 'v', 'iet', 'Ġled', 'Ġameric', 'Ġfears', 'Ġbomber', 'Ġgap', 'Ġgaining', 'Ġsatellite', 'Ġphotography', 'Ġunited', 'Ġstates', 'Ġintelligence', 'Ġagencies', 'Ġable', 'Ġstate', 'Ġcertainty', 'Ġnew', 'Ġcomplexes', 'Ġestablished', 'Ġus', 'sr', 'Ġpast', 'Ġyear', '".', 'Ġpresident', 'Ġly', 'nd', 'Ġb', 'Ġjohn', 'son', 'Ġtold', 'Ġgathering', ':[', "'t", 'Ġwant', 'Ġquoted', 'Ġ...', "'ve", 'Ġspent', 'Ġbillion', 'Ġspace', 'Ġprogram', 'Ġnothing', 'Ġelse', 'Ġcome', 'Ġexcept', 'Ġknowledge', 'Ġgained', 'Ġspace', 'Ġphotography', 'Ġwould', 'Ġworth', 'Ġten', 'Ġtimes', 'Ġwhole', 'Ġprogram', 'Ġcost', 'Ġmissions', 'Ġbenefits', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġtonight', 'Ġknow', 'Ġmany', 'Ġmissiles', 'Ġenemy', 'Ġturned', 'Ġguesses', 'Ġway', 'Ġthings', "'t", 'Ġneed', 'Ġbuilding', 'Ġthings', "'t", 'Ġneed', 'Ġbuild', 'Ġharbor', 'ing', 'Ġfears', "'t", 'Ġneed', 'Ġharbor', 'Ġstate', 'Ġunion', 'Ġaddress', 'Ġpresident', 'Ġj', 'im', 'Ġcar', 'ter', 'Ġexplained', 'Ġhumanity', 'Ġbenefited', 'Ġpresence', 'Ġameric', 'Ġsatellites', ':[', 'Ġsatellites']</t>
+          <t>['enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġcal', 'ornia', 'las', 'Ġused', 'Ġexpend', 'able', 'Ġlaunch', 'Ġsystem', 'Ġag', 'ena', 'Ġcent', 'aur', 'Ġupper', 'Ġstages', 'Ġmar', 'iner', 'Ġspace', 'Ġprobes', 'Ġused', 'Ġexplore', 'Ġmercury', 'Ġven', 'us', 'Ġmars', 'âĢĵ', ');', 'Ġlaunch', 'Ġten', 'Ġmercury', 'Ġprogram', 'Ġmissions', 'âĢĵ', 'Ġfirst', 'Ġsuccessful', 'Ġtest', 'Ġlaunch', 'las', 'Ġmissile', 'Ġde', 'cember', 'Ġapproximately', 'las', 'Ġmissiles', 'las', 'Ġboosters', 'Ġwould', 'Ġcollapse', 'Ġweight', 'Ġkept', 'Ġpress', 'urized', 'Ġnitrogen', 'Ġgas', 'Ġtanks', 'Ġdevoid', 'Ġpropell', 'ants', 'las', 'Ġbooster', 'Ġunusual', 'Ġuse', 'ball', 'oon', 'Ġtanks', 'Ġrockets', 'Ġmade', 'Ġthin', 'Ġstainless', 'Ġsteel', 'Ġoffered', 'Ġminimal', 'Ġrigid', 'Ġsupport', 'Ġpressure', 'Ġtanks', 'Ġgave', 'Ġrig', 'idity', 'Ġrequired', 'Ġspace', 'Ġflight', 'Ġorder', 'Ġsave', 'Ġweight', 'Ġpainted', 'Ġneeded', 'Ġspecially', 'Ġdesigned', 'Ġoil', 'Ġprevent', 'Ġrust', 'Ġoriginal', 'Ġuse', 'Ġwater', 'Ġdisplacement', 'Ġlaunch', 'Ġvehicles', 'Ġbased', 'Ġoriginal', 'las', 'las', 'Ġmissile', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'las', 'Ġmissile', 'las', 'b', 'Ġscore', 'Ġpayload', 'Ġmercury', 'las', 'Ġlaunch', 'Ġcomplex', 'las', 'Ġused', 'Ġfirst', 'Ġstage', 'Ġsatellite', 'Ġlaunch', 'Ġvehicles', 'Ġhalf', 'Ġcentury', 'Ġmany', 'Ġeventually', 'Ġconverted', 'Ġorbital', 'Ġlaunch', 'Ġvehicles', 'Ġremoved', 'Ġservice', 'Ġmissiles', 'Ġmissiles', 'Ġconverted', 'las', 'Ġe', 'f', 'space', 'Ġboosters', 'Ġused', 'Ġlaunch', 'Ġearly', 'block', 'Ġsatellites', 'Ġearly', 'las', 'Ġrockets', 'Ġalso', 'Ġbuilt', 'Ġspecifically', 'Ġnon', 'military', 'Ġuses', 'Ġde', 'cember', 'las', 'Ġused', 'Ġlaunch', 'Ġsignal', 'Ġcommunication', 'Ġorbiting', 'Ġrelay', 'Ġequipment', 'score', 'Ġsatellite', 'Ġfirst', 'Ġprototype', 'Ġcommunications', 'Ġsatellite', 'Ġfirst', 'Ġtest', 'Ġsatellite', 'Ġdirect', 'Ġpractical', 'Ġcommunications', 'Ġpayload', 'Ġplaced', 'Ġlow', 'Ġearth', 'Ġorbit', 'las', 'Ġserial', 'Ġnumber', 'Ġwithout', 'Ġupper', 'Ġstage', 'las', 'b', 'score', 'Ġheaviest', 'Ġartificial', 'Ġobject', 'Ġorbit', 'Ġfirst', 'Ġvoice', 'Ġrelay', 'Ġsatellite', 'Ġfirst', 'Ġhuman', 'made', 'Ġobject', 'Ġspace', 'Ġeasily', 'Ġvisible', 'Ġnaked', 'Ġeye', 'Ġdue', 'Ġlarge', 'Ġmirror', 'pol', 'ished', 'Ġstainless', 'Ġsteel', 'Ġtank', 'Ġfirst', 'Ġflight']</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -594,7 +594,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['Ġexample', 'Ġenormously', 'Ġimportant', 'Ġstabil', 'izing', 'Ġworld', 'Ġaffairs', 'Ġthereby', 'Ġmake', 'Ġsignificant', 'Ġcontribution', 'Ġsecurity', 'Ġnations', 'Ġreconnaissance', 'Ġsatellites', 'Ġused', 'Ġenforce', 'Ġhuman', 'Ġrights', 'Ġsatellite', 'Ġsent', 'inel', 'Ġproject', 'Ġmonitors', 'Ġatrocities', 'Ġsu', 'dan', 'Ġsouth', 'Ġsu', 'dan', 'Ġadditionally', 'Ġcompanies', 'Ġge', 'oe', 'ye', 'Ġdigital', 'gl', 'obe', 'Ġprovided', 'Ġcommercial', 'Ġsatellite', 'Ġimagery', 'Ġsupport', 'Ġnatural', 'Ġdisaster', 'Ġresponse', 'Ġhumanitarian', 'Ġmissions', 'Ġsatellites', 'Ġcommonly', 'Ġseen', 'Ġfiction', 'Ġmilitary', 'Ġfiction', 'Ġworks', 'Ġfiction', 'Ġfocus', 'Ġspecifically', 'Ġsatellites', 'Ġinclude', 'mac', 'Ġproject', 'Ġenemy', 'Ġstate', 'Ġbody', 'Ġlies', 'Ġice', 'Ġstation', 'Ġz', 'ebra', 'Ġpar', 'man', 'u', 'Ġstory', 'Ġp', 'ok', 'hran', 'Ġpatriot', 'Ġgames', 'Ġaerial', 'Ġreconnaissance', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'u', '.)', 'Ġeuro', 'pe', 'Ġunion', 'Ġsatellite', 'Ġcentre', 'Ġlist', 'Ġintelligence', 'Ġgathering', 'Ġdisciplines', 'Ġlist', 'Ġk', 'os', 'mos', 'Ġsatellites', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'u', '.)', 'Ġsat', 'Ġmove', 'cor', 'ona', 'Ġhistory', 'Ġr', 'ona', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', '].', 'Ġarchived', 'Ġoriginal', 'Ġr', 'cor', 'ona', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'cor', 'ona', 'Ġprogram', 'Ġmission', 'Ġspacecraft', 'Ġlibrary', 'Ġarchived', 'Ġoriginal', 'http', 'space', 'j', 'pl', 'n', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfiction', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġwr', 'ight', 'ichael', 'ron', 'Ġcar', 'oline', 'Ġrand', 'Ġde', 'cember', 'two', 'Ġyears', 'Ġmor', 'ison', 'Ġnew', 'ork', 'Ġtimes', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġer', 'ickson', 'Ġmark', 'Ġunknown', 'Ġtogether', 'Ġdod', 'Ġn', 'asa', 'Ġearly', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'http', 'Ġair', 'Ġuniversity', 'Ġpress', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġreconnaissance', 'Ġsatellite', 'Ġinf', 'ople', 'ase', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġnavy', "'s", 'Ġmissions', 'Ġspace', 'Ġu', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'nn', 'igan', 'Ġaug', 'ust']</t>
+          <t>['Ġwould', 'Ġlong', 'Ġcareer', 'las', 'Ġsatellite', 'Ġlauncher', 'las', 'Ġmissile', 'derived', 'Ġused', 'Ġorbital', 'Ġlaunches', 'Ġag', 'ena', 'Ġcent', 'aur', 'Ġupper', 'Ġstages', 'Ġmodified', 'las', 'Ġused', 'Ġorbital', 'Ġelement', 'Ġproject', 'Ġmercury', 'Ġlaunching', 'Ġfour', 'Ġcrew', 'ed', 'Ġmercury', 'Ġspacecraft', 'Ġlow', 'Ġearth', 'Ġorbit', 'las', 'Ġlaunches', 'Ġconducted', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġlaunch', 'Ġcomplexes', 'Ġv', 'enberg', 'Ġlaunch', 'Ġcomplex', 'Ġtwo', 'Ġsub', 'orb', 'ital', 'Ġstage', 'Ġhalf', 'Ġvehicles', 'Ġused', 'Ġproject', 'Ġfire', 'Ġsounding', 'Ġrockets', 'las', 'Ġspace', 'Ġlauncher', 'Ġvariants', 'Ġwh', 'itt', 'led', 'las', 'cent', 'aur', 'Ġrefurb', 'ished', 'Ġlaunch', 'Ġrate', 'l', 'ases', 'Ġdecreased', 'Ġdue', 'Ġadvent', 'Ġspace', 'Ġshuttle', 'las', 'Ġlaunches', 'Ġcontinued', 'Ġlast', 'classic', 'las', 'Ġballoon', 'Ġtanks', 'Ġj', 'ett', 'ison', 'able', 'Ġbooster', 'Ġsection', 'Ġlaunched', 'sat', 'Ġair', 'Ġforce', 'las', 'Ġboosters', 'Ġalso', 'Ġused', 'Ġlast', 'Ġfour', 'Ġcrew', 'ed', 'Ġproject', 'Ġmercury', 'Ġmissions', 'Ġfirst', 'Ġunited', 'Ġstates', 'Ġcrew', 'ed', 'Ġspace', 'Ġprogram', 'Ġfe', 'b', 'ruary', 'Ġlaunched', 'Ġfriendship', 'Ġmade', 'Ġthree', 'Ġearth', 'Ġorbits', 'Ġcarrying', 'Ġjohn', 'Ġgl', 'enn', 'Ġfirst', 'Ġunited', 'Ġstates', 'Ġastronaut', 'Ġorbit', 'Ġearth', 'Ġidentical', 'las', 'Ġboosters', 'Ġsuccessfully', 'Ġlaunched', 'Ġthree', 'Ġcrew', 'ed', 'Ġmercury', 'Ġorbital', 'Ġmissions', 'las', 'Ġsaw', 'Ġbeginnings', 'work', 'horse', 'Ġstatus', 'Ġmercury', 'las', 'Ġmissions', 'Ġresulted', 'Ġl', 'Ġcol', 'Ġjohn', 'Ġh', 'Ġgl', 'enn', 'Ġbecoming', 'Ġfirst', 'Ġameric', 'Ġorbit', 'Ġearth', 'major', 'uri', 'Ġgag', 'arin', 'v', 'iet', 'Ġcos', 'mon', 'aut', 'Ġfirst', 'Ġhuman', 'Ġorbit', '.)', 'las', 'Ġalso', 'Ġused', 'Ġthroughout', 'Ġmid', 'Ġlaunch', 'Ġag', 'ena', 'Ġtarget', 'Ġvehicles', 'Ġused', 'Ġgem', 'ini', 'Ġprogram', 'Ġbeginning', 'Ġag', 'ena', 'Ġupper', 'Ġstage', 'Ġpowered', 'Ġhyper', 'g', 'olic', 'Ġpropell', 'ant', 'Ġused', 'Ġextensively', 'las', 'Ġlaunch', 'Ġvehicles', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġn', 'ro', 'Ġc', 'ia', 'Ġused', 'Ġlaunch', 'Ġsig', 'int', 'Ġsatellites', 'Ġn', 'asa', 'Ġused', 'Ġranger', 'Ġprogram', 'Ġobtain', 'las', 'Ġscore', 'Ġlaunch', 'las', 'Ġbased', 'Ġlaunchers', 'Ġmercury', 'Ġprogram', 'las', 'ag', 'ena']</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['monster', 'Ġrocket', 'Ġblast', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġcoast', 'Ġr', 'attle', 'Ġsouth', 'land', 'story', 'Ġlos', 'Ġangel', 'es', 'Ġtimes', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmel', 'issa', 'Ġgold', 'Ġfe', 'b', 'ruary', 'fr', 'ag', 'ments', 'v', 'iet', 'era', 'Ġsatellite', 'Ġburn', 'Ġearth', "'s", 'Ġatmosphere', 'Ġmash', 'able', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'pp', 'en', 'heimer', 'Ġspace', 'Ġshuttle', 'Ġdecision', 'Ġts', 'htm', 'Ġn', 'asa', 'Ġpp', 'Ġstate', 'Ġunion', 'Ġannual', 'Ġmessage', 'Ġcongress', 'Ġstate', 'Ġunion', 'Ġaddress', 'Ġameric', 'Ġpresidency', 'Ġproject', 'Ġretrieved', 'Ġapr', 'il', 'commercial', 'Ġsatellite', 'Ġimagery', 'Ġcompanies', 'Ġpartner', 'Ġu', 'Ġgeological', 'Ġsurvey', 'Ġsupport', 'Ġinternational', 'Ġcharter', 'space', 'Ġmajor', 'Ġdisasters', 'Ġus', 'gs', 'Ġnews', 'room', 'Ġunited', 'Ġstates', 'Ġgeological', 'Ġsurvey', 'Ġretrieved', 'Ġapr', 'il', 'Ġk', 'upper', 'berg', 'Ġp', 'aul', 'Ġsatellites', 'Ġro', 'sen', 'Ġpublishing', 'Ġgroup', 'Ġric', 'hel', 'son', 'Ġje', 'ff', 'rey', 'Ġameric', "'s", 'Ġsecret', 'Ġeyes', 'Ġspace', 'Ġu', 'Ġkey', 'hole', 'Ġsatellite', 'Ġprogram', 'Ġhar', 'per', 'Ġrow', 'ris', 'Ġpat', 'Ġspies', 'Ġsurveillance', 'Ġsatellites', 'Ġwar', 'Ġpeace', 'Ġber', 'lin', 'Ġnew', 'ork', 'Ġspring', 'er', 'Ġch', 'iche', 'ster', 'Ġassociation', 'Ġpra', 'x', 'Ġpublishing', 'http', 'cl', 'c', 'Ġcl', 'c', 'Ġf', 'Ġintelligence', 'Ġresource', 'Ġprogram', 'Ġimagery', 'Ġintelligence', 'im', 'int', 'Ġir', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsatellite', 'Ġarchived', 'Ġh', 'tm', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'mis', 'rs', 'Ġreading', 'Ġexternal', 'Ġlinks', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġspac', 'ep', 'orts', 'Ġaround', 'Ġworld', 'Ġal', 'bar', 'Ġspace', 'Ġresearch', 'Ġcenter', 'Ġmilitary', 'Ġintelligence', 'Ġsatellites', 'Ġv', 'n', 'asa', 'Ġremote', 'Ġsensing', 'Ġtutorial', 'Ġretrieved']</t>
+          <t>['las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'Ġfirst', 'Ġclose', 'Ġimages', 'Ġsurface', 'Ġmoon', 'Ġmar', 'iner', 'Ġfirst', 'Ġspacecraft', 'Ġfly', 'Ġanother', 'Ġplanet', 'Ġag', 'ena', 'Ġtarget', 'Ġvehicles', 'Ġused', 'Ġlater', 'Ġspace', 'Ġrend', 'ezvous', 'Ġpractice', 'Ġmissions', 'Ġgem', 'ini', 'Ġlaunched', 'las', 'Ġrocket', 'las', 'cent', 'aur', 'Ġexpend', 'able', 'Ġlaunch', 'Ġsystem', 'Ġderived', 'las', 'Ġmissile', 'Ġlaunches', 'Ġconducted', 'Ġtwo', 'Ġpads', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'las', 'Ġengines', 'Ġupgraded', 'Ġstructure', 'Ġreinforced', 'Ġlarge', 'Ġupper', 'Ġstage', 'Ġalong', 'Ġelong', 'ated', 'Ġpropell', 'ant', 'Ġtanks', 'Ġfirst', 'Ġlaunch', 'Ġattempt', 'las', 'cent', 'aur', 'Ġmay', 'Ġfailed', 'Ġrocket', 'Ġexploding', 'Ġtake', 'Ġfootage', 'Ġshown', 'Ġpen', 'ultimate', 'Ġshot', 'Ġart', 'Ġfilm', 'Ġk', 'oya', 'q', 'ats', 'Ġdirected', 'Ġgod', 'frey', 'Ġreg', 'gio', 'Ġbeginning', 'Ġliquid', 'Ġhydrogen', 'fuel', 'ed', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġalso', 'Ġused', 'Ġdozens', 'las', 'Ġlaunches', 'Ġn', 'asa', 'Ġlaunched', 'Ġsurvey', 'Ġprogram', 'Ġlunar', 'Ġland', 'er', 'Ġspacecraft', 'Ġmars', 'bound', 'Ġmar', 'iner', 'Ġprogram', 'Ġspacecraft', 'las', 'cent', 'aur', 'Ġlaunch', 'Ġvehicles', 'Ġfollowing', 'Ġretirement', 'las', 'e', 'Ġalong', 'las', 'f', 'Ġrefurb', 'ished', 'Ġorbital', 'Ġlaunches', 'Ġlast', 'las', 'Ġe', 'f', 'Ġspacecraft', 'Ġlaunch', 'Ġconducted', 'Ġmarch', 'Ġusing', 'Ġrocket', 'Ġoriginally', 'Ġbuilt', 'las', 'e', 'Ġlast', 'las', 'Ġe', 'f', 'Ġlaunch', 'Ġuse', 'Ġrocket', 'Ġoriginally', 'Ġbuilt', 'las', 'f', 'Ġconducted', 'Ġj', 'une', 'las', 'Ġe', 'f', 'Ġused', 'Ġlaunch', 'Ġblock', 'Ġseries', 'Ġsatellites', 'Ġlast', 'Ġrefurb', 'ished', 'las', 'f', 'Ġvehicle', 'Ġlaunched', 'Ġv', 'enberg', 'Ġcarrying', 'Ġsatellite', 'Ġdefense', 'Ġmeteor', 'ological', 'Ġsatellite', 'Ġprogram', 'Ġmodel', 'Ġname', 'Ġfirst', 'Ġlaunch', 'Ġlast', 'Ġlaunch', 'Ġtotal', 'Ġlaunches', 'Ġsuccesses', 'Ġbase', 'Ġupper', 'Ġstage', 'Ġnotable', 'Ġpayload', 'Ġremarks', 'las', 'ga', 'las', 'Ġst', 'orable', 'Ġpropell', 'ant', 'Ġstage', 'Ġnone', 'Ġdevelopment', 'Ġessentially', 'Ġidentical', 'las', 'ag', 'ena', 'Ġcancelled', 'Ġaccordingly', 'las', 'able', 'Ġalt', 'air', 'Ġpioneer', 'Ġpioneer', 'Ġpioneer', 'Ġrockets', 'Ġfailed', 'Ġstatic', 'Ġï', '¬', 'ģ', 'ring', 'Ġattempts']</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -620,7 +620,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'ipedia', 'Ġillustration', 'Ġsatellites', 'Ġtwo', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġknown', 'Ġblock', 'left', 'Ġblock', 'right', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġsystem', 'Ġhigh', 'Ġcapacity', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'Ġplanned', 'Ġuse', 'Ġpartnership', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'od', 'adian', 'Ġdepartment', 'Ġnational', 'Ġdefence', 'nd', 'Ġaust', 'ral', 'ian', 'Ġdepartment', 'Ġdefence', 'Ġsystem', 'Ġcomposed', 'Ġspace', 'Ġsegment', 'Ġsatellites', 'Ġterminal', 'Ġsegment', 'Ġusers', 'Ġcontrol', 'Ġsegment', 'Ġoperators', 'Ġdod', 'Ġwide', 'band', 'Ġsatellite', 'Ġcommunication', 'Ġservices', 'Ġcurrently', 'Ġprovided', 'Ġcombination', 'Ġexisting', 'Ġdefense', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'sc', 'Ġglobal', 'Ġbroadcast', 'Ġservice', 'g', 'bs', 'Ġsatellites', 'Ġaccording', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġquoted', 'Ġspace', 'flight', 'Ġsingle', 'Ġspacecraft', 'Ġmuch', 'Ġbandwidth', 'Ġentire', 'Ġexisting', 'sc', 'Ġconstellation', '."[', 'Ġoperations', 'Ġcurrently', 'Ġrun', 'th', 'Ġspace', 'Ġoperations', 'Ġsquadron', 'Ġsch', 'ri', 'ever', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġwell', 'rd', 'Ġspace', 'Ġoperations', 'Ġsquadron', 'Ġconstellation', 'Ġsatellites', 'Ġincreases', 'Ġcommunications', 'Ġcapabilities', 'Ġmilit', 'aries', 'Ġunited', 'Ġstates', 'ada', 'Ġaust', 'ral', 'ia', 'Ġproviding', 'Ġadditional', 'Ġbandwidth', 'Ġcommunications', 'Ġcapabilities', 'Ġtactical', 'Ġcommand', 'Ġcontrol', 'Ġcommunications', 'Ġcomputers', 'Ġintelligence', 'Ġsurveillance', 'Ġreconnaissance', 'Ġbattle', 'Ġmanagement', 'Ġcombat', 'Ġsupport', 'Ġinformation', 'ada', 'Ġalso', 'Ġsigned', 'Ġbecome', 'Ġpartner', 'Ġalso', 'Ġaug', 'ments', 'Ġcurrent', 'Ġka', 'band', 'Ġglobal', 'Ġbroadcast', 'Ġservice', 'Ġf', 'Ġsatellites', 'Ġproviding', 'Ġadditional', 'Ġinformation', 'Ġbroadcast', 'Ġcapabilities', 'Ġwell', 'Ġproviding', 'Ġnew', 'Ġtwo', 'way', 'Ġcapability', 'Ġband', 'Ġprovides', 'Ġservices', 'Ġus', 'Ġdod', 'Ġaust', 'ral', 'ian', 'Ġdepartment', 'Ġdefence', 'Ġsystem', 'Ġsupports', 'Ġcontinuous', 'hour', 'per', 'day', 'Ġwide', 'band', 'Ġsatellite', 'Ġservices', 'Ġtactical', 'Ġusers', 'Ġfixed', 'Ġinfrastructure', 'Ġusers', 'Ġlimited', 'Ġprotected', 'Ġservices', 'Ġprovided', 'Ġconditions', 'Ġstress', 'Ġselected', 'Ġusers', 'Ġemploying', 'Ġterrestrial', 'Ġmod', 'ems', 'Ġcapable', 'Ġproviding', 'Ġprotection', 'Ġjam', 'ming', 'Ġmission', 'Ġcapabilities', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'ipedia', 'Ġsatellites', 'Ġcomplement', 'sc', 'Ġservice', 'Ġlife', 'Ġenhancement', 'Ġprogram', 'sle', 'p', 'Ġg', 'bs', 'Ġpayload', 'Ġoffset', 'Ġeventual', 'Ġdecline', 'sc', 'Ġcapability', 'Ġoffer']</t>
+          <t>['Ġlaunch', 'Ġpioneer', 'Ġspacecraft', 'Ġmoon', 'las', 'las', 'Ġag', 'ena', 'Ġmar', 'iner', 'Ġranger', 'Ġprogram', 'Ġmissile', 'Ġdefense', 'Ġalarm', 'Ġsystem', 'las', 'cent', 'aur', 'las', 'Ġe', 'f', 'Ġtab', 'ulated', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'Ġmodel', 'Ġname', 'Ġfirst', 'Ġlaunch', 'Ġlast', 'Ġlaunch', 'Ġtotal', 'Ġlaunches', 'Ġsuccesses', 'Ġbase', 'Ġupper', 'Ġstage', 'Ġnotable', 'Ġpayload', 'Ġremarks', 'Ġbaseline', 'las', 'ag', 'ena', 'Ġsub', 'family', 'Ġvehicle', 'las', 'las', 'Ġnone', 'Ġfriendship', 'Ġaur', 'ora', 'igma', 'Ġfaith', 'Ġhuman', 'rated', 'las', 'las', 'las', 'Ġag', 'ena', 'Ġcor', 'ona', 'Ġgam', 'bit', 'Ġexcept', 'Ġreliability', 'Ġimprovements', 'las', 'las', 'Ġag', 'ena', 'Ġcanyon', 'Ġexcept', 'Ġstretched', 'las', 'las', 'Ġag', 'ena', 'Ġorbiting', 'Ġastronomical', 'Ġobserv', 'atory', 'las', 'las', 'Ġcent', 'aur', 'Ġsurvey', 'Ġbaseline', 'las', 'cent', 'aur', 'Ġsub', 'family', 'Ġvehicle', 'las', 'las', 'Ġcent', 'aur', 'Ġstretched', 'las', 'las', 'Ġcent', 'aur', 'Ġmar', 'iner', 'Ġexcept', 'Ġcent', 'aur', 'rated', 'las', 'Ġelectronics', 'Ġintegrated', 'Ġcent', 'aur', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'Ġmodel', 'Ġname', 'Ġfirst', 'Ġlaunch', 'Ġlast', 'Ġlaunch', 'Ġtotal', 'Ġlaunches', 'Ġsuccesses', 'Ġbase', 'Ġupper', 'Ġstage', 'Ġnotable', 'Ġpayload', 'Ġremarks', 'las', 'las', 'Ġcent', 'aur', 'las', 'Ġlonger', '06', 'las', 'las', 'Ġderived', 'Ġcent', 'aur', 'Ġderived', 'Ġcr', 'res', 'las', 'Ġexcept', 'Ġstrengthened', 'Ġpayload', 'Ġfair', 'ing', 'Ġring', 'Ġlaser', 'Ġgy', 'ro', 'Ġadded', 'las', 'las', 'Ġderived', 'Ġcent', 'aur', 'Ġderived', 'Ġe', 'ut', 'els', 'las', 'Ġexcept', 'las', 'Ġstretched', 'Ġengines', 'rated', 'Ġadded', 'Ġhyd', 'raz', 'ine', 'Ġroll', 'Ġcontrol', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġfoam', 'Ġinsulation', 'Ġdeleted', 'Ġ', 'vern', 'iers', 'Ġcent', 'aur', 'Ġstretched', 'Ġdevelopment', 'Ġdone', 'Ġgeneral', 'Ġdynamics', 'Ġpart', 'Ġlock', 'heed', 'Ġmart', 'las', 'las', 'Ġderived', 'Ġcent', 'aur', 'Ġderived', 'las', 'Ġexcept', 'Ġcent', 'aur', 'Ġengines', 'rated', 'Ġkn', 'Ġthrust', 'p', 'Ġincrease', 'Ġextend', 'ible', 'zz', 'les', 'las', 'las', 'Ġderived', 'Ġcent', 'aur', 'Ġderived', 'las', 'Ġexcept', 'Ġcast']</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -633,7 +633,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['Ġinstantaneous', 'Ġswitch', 'able', 'Ġbandwidth', 'Ġthus', 'Ġsupply', 'Ġtimes', 'Ġcapacity', 'sc', 'Ġservice', 'Ġlife', 'Ġenhancement', 'Ġprogram', 'sle', 'p', 'Ġsatellite', 'Ġfull', 'Ġconstellation', 'Ġsatellites', 'Ġoperational', 'Ġreplace', 'sc', 'Ġsystem', 'Ġg', 'bit', 'Ġwide', 'band', 'Ġcapacity', 'Ġprovided', 'Ġgreater', 'Ġcapability', 'Ġbandwidth', 'sc', 'Ġsatellites', 'Ġcombined', 'Ġoperation', 'Ġusage', 'Ġsystem', 'Ġbroken', 'Ġsegments', 'Ġend', 'Ġusers', 'Ġcommunication', 'Ġservices', 'Ġprovided', 'Ġdescribed', 'Ġdod', 'Ġterminal', 'Ġsegment', 'Ġusers', 'Ġinclude', 'Ġaust', 'ral', 'ian', 'Ġdefence', 'Ġforce', 'Ġu', 'Ġarmy', 'Ġground', 'Ġmobile', 'Ġterminals', 'Ġu', 'Ġnavy', 'Ġships', 'Ġsubmarines', 'Ġnational', 'Ġcommand', 'Ġauthorities', 'Ġnuclear', 'Ġforces', 'Ġvarious', 'Ġnational', 'Ġsecurity', 'ied', 'Ġnational', 'Ġforces', 'Ġadditionally', 'Ġsatellite', 'Ġcontrol', 'Ġnetwork', 'Ġalso', 'Ġuse', 'Ġsimilar', 'Ġmanner', 'sc', 'Ġconstellation', 'Ġused', 'Ġroute', 'Ġpackets', 'Ġdefense', 'Ġinformation', 'Ġsystems', 'Ġagency', 'dis', 'cloud', 'Ġestablish', 'Ġcommand', 'Ġcontrol', 'Ġstreams', 'Ġvarious', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'Ġone', 'Ġemerging', 'Ġapplications', 'Ġsat', 'move', 'Ġextensively', 'Ġused', 'Ġmilitary', 'Ġtactical', 'Ġvehicles', 'Ġblue', 'Ġforce', 'Ġtracking', 'Ġmissions', 'Ġsatellite', 'Ġoperators', 'Ġcharge', 'Ġcommanding', 'Ġmonitoring', 'Ġsatellite', "'s", 'Ġbus', 'Ġpayload', 'Ġsystems', 'Ġwell', 'Ġmanaging', 'Ġnetwork', 'Ġoperating', 'Ġsatellite', 'Ġcontrol', 'Ġsegment', 'Ġlike', 'sc', 'Ġconstellation', 'Ġreplace', 'Ġspacecraft', 'Ġbus', 'Ġcommanded', 'th', 'Ġspace', 'Ġoperations', 'Ġsquadron', 'Ġsch', 'ri', 'ever', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġcolor', 'ado', 'Ġpayload', 'Ġcommanding', 'Ġnetwork', 'Ġcontrol', 'Ġhandled', 'Ġarmy', 'rd', 'Ġsignal', 'Ġbattalion', 'Ġheadquartered', 'Ġnearby', 'Ġpet', 'erson', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġcolor', 'ado', 'Ġsubordinate', 'Ġelements', 'Ġcompany', 'Ġfort', 'Ġdet', 'rick', 'ary', 'land', 'Ġcompany', 'Ġfort', 'ade', 'ary', 'land', 'Ġcompany', 'Ġland', 'st', 'uh', 'l', 'Ġg', 'erman', 'Ġcompany', 'Ġw', 'ah', 'ia', 'wa', 'Ġhaw', 'aii', 'Ġcompany', 'Ġfort', 'Ġbuck', 'ner', 'kin', 'awa', 'Ġj', 'apan', 'Ġprimary', 'Ġcontractor', 'Ġsatellites', 'Ġbo', 'e', 'ing', 'Ġsatellite', 'Ġdevelopment', 'Ġcenter', 'Ġbuilding', 'Ġaround', 'Ġbo', 'e', 'ing', 'Ġsatellite', 'Ġbus', 'Ġoriginally', 'Ġfive', 'Ġsatellites', 'Ġplanned', 'Ġoct', 'ober', 'Ġaust', 'ral', 'ia', "'s", 'Ġdepartment', 'Ġdefence', 'Ġannounced', 'Ġcountry', 'Ġwould', 'Ġfund', 'Ġsixth', 'Ġsatellite', 'Ġconstellation', 'Ġorbits']</t>
+          <t>['Ġ', 'iva', 'Ġstrap', 'Ġboosters', 'Ġadded', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'Ġmodel', 'Ġname', 'Ġfirst', 'Ġlaunch', 'Ġlast', 'Ġlaunch', 'Ġtotal', 'Ġlaunches', 'Ġsuccesses', 'Ġbase', 'Ġupper', 'Ġstage', 'Ġnotable', 'Ġpayload', 'Ġremarks', 'las', 'las', 'Ġnone', 'Ġov', 'orb', 'iting', 'Ġvehicle', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġrefurb', 'ished', 'Ġorbital', 'Ġlaunch', 'las', 'las', 'Ġnone', 'Ġrefurb', 'ished', 'Ġorbital', 'Ġlaunch', 'las', 'las', 'Ġnone', 'Ġrefurb', 'ished', 'Ġorbital', 'Ġlaunch', 'las', 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'las', 'Ġcent', 'aur', 'Ġstage', 'Ġremoved', 'Ġn', 'oss', 'Ġsatellites', 'las', 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġwest', 'Ġcoast', 'Ġav', 'ionics', 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġspace', 'Ġbooster', 'Ġhold', 'Ġsystem', 'Ġversus', 'Ġweapon', 'Ġsystem', 'Ġï', '¬', 'Ĥ', 'away', 'Ġfirst', 'Ġstage', 'las', 'Ġdiscontinued', 'Ġuse', 'Ġthree', 'Ġengines', 'Ġstaging', 'Ġfavor', 'Ġsingle', 'Ġr', 'ussian', 'built', 'Ġener', 'gom', 'ash', 'Ġr', 'Ġengine', 'Ġretaining', 'Ġstage', "'s", 'Ġballoon', 'Ġtank', 'Ġconstruction', 'las', 'Ġcontinued', 'Ġuse', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġavailable', 'Ġsingle', 'Ġdual', 'Ġengines', 'las', 'Ġv', 'Ġcurrently', 'Ġservice', 'Ġdeveloped', 'Ġlock', 'heed', 'Ġmart', 'Ġpart', 'Ġus', 'Ġair', 'Ġforce', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'e', 'el', 'v', 'Ġprogram', 'Ġfirst', 'Ġlaunched', 'Ġaug', 'ust', 'Ġoperation', 'Ġtransferred', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġjoint', 'Ġventure', 'Ġlock', 'heed', 'Ġmart', 'Ġbo', 'e', 'ing', 'Ġlock', 'heed', 'Ġmart', 'Ġcontinued', 'Ġmarket', 'Ġr', 'Ġera', 'las', 'las', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'Ġlaunch', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġlaunch', 'las', 'Ġcarrying', 'Ġl', 'ro', 'Ġl', 'cross', 'las', 'Ġcommercial', 'Ġcustomers', 'Ġse', 'pt', 'ember', 'Ġannounced', 'Ġrocket', 'Ġretired', 'Ġfulfilling', 'Ġremaining', 'Ġlaunch', 'Ġcontracts', 'las', 'Ġbuilt', 'Ġdec', 'atur', 'Ġal', 'abama', 'Ġmaintains', 'Ġtwo', 'Ġlaunch', 'Ġsites', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'las', 'Ġfirst', 'Ġstage', 'Ġcalled', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġcontinues', 'Ġuse', 'Ġener', 'gom', 'ash', 'Ġr', 'Ġintroduced', 'las', 'Ġemploys', 'Ġrigid', 'Ġframework', 'Ġinstead', 'Ġballoon', 'Ġtanks']</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -646,7 +646,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['Ġaltitude', 'Ġmi', 'Ġweigh', 'Ġapproximately', 'Ġprogram', 'Ġintends', 'Ġuse', 'Ġdelta', 'Ġiv', 'las', 'Ġlaunch', 'Ġvehicles', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġestimates', 'Ġsatellite', 'Ġcost', 'Ġapproximately', 'Ġus', 'Ġmillion', 'Ġfirst', 'Ġthree', 'Ġsatellites', 'Ġform', 'Ġblock', 'Ġspace', 'Ġsegment', 'Ġnext', 'Ġthree', 'Ġsatellites', 'Ġmake', 'Ġblock', 'Ġnext', 'Ġfour', 'Ġmake', 'Ġblock', 'Ġfollow', 'Ġfirst', 'Ġlaunch', 'Ġconducted', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġoct', 'ober', 'Ġ00', 'Ġut', 'c', 'Ġsatellite', 'Ġcarried', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġlifting', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġlaunch', 'Ġsatellite', 'Ġgiven', 'Ġu', 'Ġmilitary', 'Ġsegments', 'Ġlaunches', 'Ġblock', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'ipedia', 'Ġdesignation', 'Ġus', 'Ġcoverage', 'Ġarea', 'Ġstretches', 'Ġwest', 'Ġcoast', 'Ġunited', 'Ġstates', 'Ġsoutheast', 'Ġlaunch', 'Ġsecond', 'Ġsatellite', 'usa', 'Ġalso', 'Ġconducted', 'Ġu', 'la', 'Ġapr', 'il', 'Ġ01', '00', 'Ġut', 'c', 'Ġusing', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġsatellite', 'Ġpositioned', 'Ġequ', 'ator', 'Ġaround', 'Â°', 'Ġeast', 'Ġlong', 'itude', 'Ġind', 'ian', 'Ġocean', 'Ġuse', 'Ġunited', 'Ġstates', 'Ġcentral', 'Ġcommand', 'Ġaf', 'ghan', 'istan', 'Ġparts', 'Ġsouthwest', 'ia', 'Ġoriginally', 'Ġsecond', 'Ġspacecraft', 'Ġfly', 'Ġdelta', 'Ġiv', 'Ġthird', 'las', 'Ġswitched', 'Ġundisclosed', 'Ġreason', 'usa', 'Ġlaunched', 'Ġde', 'cember', 'Ġ01', '00', 'Ġut', 'c', 'Ġcovers', 'l', 'antic', 'Ġocean', 'Ġsatellite', 'Ġlaunched', 'Ġdelta', 'Ġiv', 'Ġlaunch', 'Ġvehicle', 'Ġoriginally', 'las', 'Ġreplaced', 'usa', 'Ġfirst', 'Ġsatellite', 'Ġblock', 'Ġlaunched', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġdelta', 'Ġiv', 'Ġjan', 'uary', 'Ġ00', '00', 'usa']</t>
+          <t>['Ġrigid', 'Ġfu', 'selage', 'Ġheavier', 'Ġeasier', 'Ġhandle', 'Ġtransport', 'Ġeliminating', 'Ġneed', 'Ġconstant', 'Ġinternal', 'Ġpressure', 'Ġfive', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġstrap', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġused', 'Ġaugment', 'Ġfirst', 'Ġstage', 'Ġthrust', 'Ġupper', 'Ġstage', 'Ġremains', 'Ġcent', 'aur', 'Ġpowered', 'Ġsingle', 'Ġdual', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġengines', 'Ġmodel', 'Ġname', 'Ġfirst', 'Ġlaunch', 'Ġlast', 'Ġlaunch', 'Ġtotal', 'Ġlaunches', 'Ġsuccesses', 'st', 'stage', 'Ġengines', 'Ġupper', 'stage', 'Ġengines', 'Ġnotable', 'Ġpayload', 'Ġremarks', 'las', 'Ġe', 'ut', 'els', 'Ġmajor', 'Ġrevision', 'las', 'Ġnew', 'Ġr', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġengine', 'Ġnormal', 'Ġstaging', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġstretched', 'Ġstrengthened', 'Ġfirst', 'Ġsingle', 'Ġengine', 'Ġcent', 'aur', 'las', 'las', 'Ġexcept', 'Ġcent', 'aur', 'Ġstretched', 'Ġoptional', 'Ġdual', 'Ġengine', 'Ġcent', 'aur', 'las', 'Ġlunar', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġl', 'cross', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġmajor', 'Ġrevision', 'las', 'Ġnew', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġstructure', 'Ġoptional', 'Ġsolid', 'Ġstrap', 'Ġboosters', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'Ġmodel', 'Ġname', 'Ġfirst', 'Ġlaunch', 'Ġlast', 'Ġlaunch', 'Ġtotal', 'Ġlaunches', 'Ġsuccesses', 'st', 'stage', 'Ġengines', 'Ġupper', 'stage', 'Ġengines', 'Ġnotable', 'Ġpayload', 'Ġremarks', 'las', 'Ġnew', 'Ġhor', 'izons', 'Ġmars', 'Ġscience', 'Ġlaboratory', 'Ġrevision', 'las', 'Ġoptional', 'Ġsolid', 'Ġstrap', 'Ġboosters', 'Ġcent', 'aur', 'Ġstage', 'Ġencaps', 'ulated', 'Ġinside', 'Ġpayload', 'Ġfair', 'ing', 'las', 'Ġstar', 'liner', 'Ġbo', 'e', 'ing', 'Ġoft', 'Ġrevision', 'las', 'Ġoptional', 'Ġtwo', 'Ġsolid', 'Ġstrap', 'Ġboosters', 'Ġcent', 'aur', 'Ġpayload', 'Ġfair', 'ing', 'Ġstar', 'liner', 'Ġspacecraft', 'Ġus', 'Ġcongress', 'Ġpassed', 'Ġlegislation', 'Ġrestricting', 'Ġpurchase', 'Ġuse', 'Ġr', 'ussian', 'supp', 'lied', 'Ġr', 'Ġengine', 'Ġused', 'Ġfirst', 'Ġstage', 'Ġbooster', 'las', 'Ġformal', 'Ġstudy', 'Ġcontracts', 'Ġissued', 'Ġj', 'une', 'Ġnumber', 'Ġus', 'Ġrocket', 'Ġengine', 'Ġsuppliers', 'Ġse', 'pt', 'ember', 'Ġu', 'la', 'Ġannounced', 'Ġentered', 'Ġpartnership', 'Ġblue', 'Ġorigin', 'Ġdevelop', 'Ġl', 'ox', 'eth', 'ane', 'Ġengine', 'Ġreplace', 'Ġr', 'Ġnew', 'Ġvul', 'Ġrocket', 'Ġengine', 'Ġdevelopment', 'Ġyears', 'Ġblue', 'Ġorigin', 'Ġu', 'la', 'Ġexpects', 'Ġnew', 'Ġstage', 'Ġengine', 'Ġstart', 'Ġflying', 'Ġearlier', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -659,7 +659,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>['Ġsuccessfully', 'Ġlaunched', 'Ġdelta', 'Ġiv', 'Ġlaunch', 'Ġvehicle', 'Ġflying', 'Ġmedium', 'Ġconfiguration', 'Ġlift', 'Ġtaking', 'Ġplace', 'Ġfl', 'ida', 'Ġmay', 'Ġ00', 'usa', 'Ġlaunched', 'Ġdelta', 'Ġiv', 'Ġlaunch', 'Ġvehicle', 'Ġaug', 'ust', 'Ġ00', 'Ġut', 'c', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġaug', 'ust', 'Ġbo', 'e', 'ing', 'Ġawarded', 'Ġair', 'Ġforce', 'Ġcontract', 'Ġworth', 'Ġus', 'Ġmillion', 'Ġbegin', 'Ġwork', 'Ġseventh', 'Ġsatellite', 'Ġnew', 'Ġsatellite', 'Ġproc', 'ured', 'Ġblock', 'Ġfollow', 'Ġcontract', 'Ġincluded', 'Ġoptions', 'Ġproduction', 'Ġsatellites', 'usa', 'Ġsuccessfully', 'Ġlaunched', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġlaunch', 'Ġvehicle', 'Ġlif', 'ff', 'Ġtaking', 'Ġplace', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġfl', 'ida', 'Ġj', 'uly', 'Ġ00', 'usa', 'Ġsuccessfully', 'Ġlaunched', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġlaunch', 'Ġvehicle', 'Ġde', 'cember', 'Ġut', 'c', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'Ġdelta', 'Ġiv', "'s", 'Ġdelta', 'Ġcry', 'ogenic', 'Ġsecond', 'Ġstage', 'Ġdeployed', 'Ġsatellite', 'Ġplanned', 'Ġde', 'cember', 'Ġ00', 'Ġut', 'c', 'usa', 'Ġlaunched', 'Ġmarch', 'Ġ00', '00', 'Ġut', 'c', 'Ġlaunched', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġlaunch', 'Ġvehicle', 'Ġsatellite', 'Ġpartially', 'funded', 'Ġallied', 'Ġnations', 'Ġincluding', 'ada', 'Ġden', 'mark', 'Ġnet', 'lands', 'Ġlux', 'em', 'bourg', 'Ġnew', 'Ġzeal', 'Ġunited', 'Ġstates', 'Ġmilitary', 'Ġaccess', 'Ġentire', 'Ġconstellation', 'usa', 'Ġlaunched', 'Ġatop', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġlaunch', 'Ġvehicle', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġmarch', 'Ġ02', 'Ġlatest', 'Ġpart', 'Ġconstellation', 'Ġhighly', 'cap', 'able', 'Ġcommunications', 'Ġsatellites', 'Ġserve', 'Ġarmed', 'Ġforces', 'Ġunited', 'Ġblock', 'Ġblock', 'Ġfollow', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'ipedia', 'Ġstates', 'Ġallies', 'Ġcarries', 'Ġka', 'band', 'Ġx', 'band', 'Ġtrans', 'p', 'ond', 'ers', '088', 'Ġgig', 'tz', 'Ġbandwidth', 'Ġoffering', 'link', 'Ġspeeds', 'Ġgig', 'ab', 'Ġper', 'Ġsecond']</t>
+          <t>['Ġlegislation', 'Ġprevent', 'Ġaward', 'Ġmilitary', 'Ġlaunch', 'Ġcontracts', 'Ġvehicles', 'Ġuse', 'Ġr', 'ussian', 'made', 'Ġengines', 'Ġapproved', 'Ġus', 'Ġcongress', 'Ġbill', 'Ġallows', 'Ġu', 'la', 'Ġcontinue', 'Ġuse', 'Ġr', 'Ġengines', 'Ġalready', 'Ġorder', 'Ġtime', 'Ġse', 'pt', 'ember', 'Ġu', 'la', 'Ġannounced', 'las', 'Ġretired', 'Ġfulfill', 'Ġremaining', 'Ġlaunch', 'Ġcontracts', 'Ġremaining', 'Ġr', 'Ġremaining', 'Ġrockets', 'Ġdelivered', 'Ġprior', 'Ġapr', 'il', 'Ġannouncement', 'Ġvul', 'Ġlaunch', 'Ġvehicle', 'Ġfirst', 'Ġdecade', 'Ġsince', 'Ġu', 'la', 'Ġformed', 'Ġlock', 'heed', 'Ġmart', 'Ġbo', 'e', 'ing', 'Ġnumber', 'Ġproposals', 'Ġconcept', 'Ġstudies', 'Ġfuture', 'Ġlaunch', 'Ġvehicles', 'Ġnone', 'Ġsubsequently', 'Ġfunded', 'Ġfull', 'Ġdevelopment', 'Ġtwo', 'Ġconcepts', 'las', 'Ġheavy', 'las', 'Ġphase', 'Ġr', 'Ġphase', 'Ġformerly', 'prop', 'osed', 'Ġlaunch', 'Ġvehicles', 'las', 'Ġheavy', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'las', 'Ġheavy', 'Ġu', 'la', 'Ġconcept', 'Ġproposal', 'Ġwould', 'Ġused', 'Ġthree', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġstages', 'Ġstrapped', 'Ġtogether', 'Ġprovide', 'Ġcapability', 'Ġnecessary', 'Ġlift', 'Ġton', 'ne', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġu', 'la', 'Ġstated', 'Ġapproximately', 'Ġhardware', 'Ġrequired', 'las', 'Ġalready', 'Ġflown', 'las', 'Ġsingle', 'core', 'Ġvehicles', 'Ġreport', 'Ġprepared', 'Ġrand', 'Ġcorporation', 'Ġoffice', 'Ġsecretary', 'Ġdefense', 'Ġstated', 'Ġlock', 'heed', 'Ġmart', 'Ġdecided', 'Ġdevelop', 'las', 'Ġheavy', 'lift', 'Ġvehicle', 'Ġreport', 'Ġrecommended', 'Ġair', 'Ġforce', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'eter', 'mine', 'Ġnecessity', 'Ġe', 'el', 'v', 'Ġheavy', 'lift', 'Ġvariant', 'Ġincluding', 'Ġdevelopment', 'las', 'Ġheavy', '",', 'res', 'olve', 'Ġr', 'Ġissue', 'Ġincluding', 'Ġcop', 'rodu', 'ction', 'Ġstockpile', 'Ġu', 'Ġdevelopment', 'Ġr', 'Ġreplacement', '."[', 'Ġlifting', 'Ġcapability', 'las', 'Ġroughly', 'Ġequivalent', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlatter', 'Ġutilizes', 'Ġengines', 'Ġdeveloped', 'Ġproduced', 'Ġdomestically', 'Ġpr', 'att', 'Ġwhit', 'ney', 'Ġrocket', 'dy', 'ne', 'Ġde', 'cember', 'Ġmerger', 'Ġbo', 'e', 'ing', 'Ġlock', 'heed', 'mart', 'Ġspace', 'Ġoperations', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'las', 'Ġprogram', 'Ġgained', 'Ġaccess', 'Ġtool', 'ing', 'Ġprocesses']</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -672,7 +672,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['Ġbo', 'e', 'ing', 'Ġreceived', 'Ġcontract', 'Ġbuild', 'th', 'Ġsatellite', 'Ġcompleted', 'Ġbo', 'e', 'ing', 'Ġmillion', 'Ġcontract', 'Ġu', 'Ġspace', 'Ġforce', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġlaunch', 'Ġpatches', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġmil', 'star', 'Ġdefense', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'sc', 'ust', 'ral', 'ia', 'Ġgets', 'Ġaccess', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġsystem', 'Ġde', 'ag', 'el', 'mber', 'Ġretrieved', 'Ġaug', 'ust', 'wide', 'band', 'Ġglobal', 'Ġsat', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'environment', 'al', 'Ġassessment', 'Ġu', 'Ġair', 'Ġforce', 'Ġwide', 'band', 'Ġgap', 'ï', '¬', 'ģ', 'ller', 'Ġsatellite', 'Ġprogram', 'web', 'ar', 'Ġdefense', 'Ġtechnical', 'Ġinformation', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'pre', 'launch', 'Ġops', 'Ġkeep', 'Ġcrews', 'Ġbusy', 'Ġcape', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'ada', "'s", 'Ġparticipation', 'Ġwide', 'band', 'Ġglobal', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'http', 'Ġforces', 'gc', 'ca', 'Ġgovernment', 'ada', 'Ġjan', 'uary', 'Ġretrieved', 'Ġoct', 'ober', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'ipedia', 'wide', 'band', 'Ġgap', 'ï', '¬', 'ģ', 'ller', 'Ġsystem', 'Ġglobal', 'security', 'org', 'ust', 'ral', 'ia', 'Ġfund', 'Ġsixth', 'Ġsatellite', 'Ġsatellite', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'bo', 'e', 'ing', 'Ġawarded', 'Ġfollow', 'Ġcontract', 'Ġseventh', 'Ġsatellite', 'block', 'ii', 'Ġfollow', 'Ġlaunched', 'Ġj', 'uly', 'Ġadvant', 'ec', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'elta', 'Ġassigned', 'Ġdeliver', 'Ġmilitary', 'Ġsatellite', 'Ġorbit', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'las', 'Ġrocket', 'Ġsuccessfully', 'Ġlaunches', 'Ġmilitary', 'Ġsatellite', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'air', 'men', 'Ġhelp', 'Ġlaunch', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay']</t>
+          <t>['Ġdiameter', 'Ġstages', 'Ġused', 'Ġdelta', 'Ġiv', 'Ġdiameter', 'Ġstage', 'Ġcould', 'Ġconce', 'ivably', 'Ġaccepted', 'Ġdual', 'Ġr', 'Ġengines', 'Ġresulting', 'Ġconceptual', 'Ġheavy', 'lift', 'Ġvehicle', 'Ġcalled', 'las', 'Ġphase', 'Ġaug', 'ust', 'ine', 'Ġreport', 'las', 'three', 'Ġstages', 'Ġparallel', 'Ġr', 'Ġalong', 'Ġshuttle', 'derived', 'Ġl', 'ite', 'Ġconsidered', 'Ġpossible', 'Ġheavy', 'Ġlif', 'ter', 'Ġconcept', 'Ġuse', 'Ġfuture', 'Ġspace', 'Ġmissions', 'Ġaug', 'ust', 'ine', 'Ġreport', 'las', 'Ġconcept', 'Ġvehicle', 'Ġwould', 'Ġnotion', 'ally', 'Ġable', 'Ġlaunch', 'Ġpayload', 'Ġmass', 'Ġapproximately', 'Ġmetric', 'Ġtons', 'Ġorbit', 'Ġconcept', 'Ġproceed', 'Ġonto', 'Ġfull', 'Ġdevelopment', 'Ġnever', 'Ġbuilt', 'Ġcomparison', 'Ġorbital', 'Ġlauncher', 'Ġfamilies', 'Ġdelta', 'rocket', 'Ġfamily', 'Ġlist', 'las', 'Ġlaunches', 'Ġrusty', 'Ġbart', 'las', 'Ġchron', 'ology', 'Ġarchived', 'Ġoriginal', '04', 'Ġdeny', 'Ġrocket', 'Ġlag', 'las', 'Ġfiring', 'Ġkey', 'notes', 'Ġu', 'Ġmissile', 'Ġbuild', '01', 'den', 'rocket', 'lag', 'Ġuniversal', 'Ġnews', 'el', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhel', 'en', 'Ġwells', 'Ġsus', 'Ġh', 'Ġwhite', 'ley', 'Ġcar', 'rie', 'Ġe', 'Ġk', 'ge', 'ann', 'es', 'Ġorigin', 'Ġn', 'asa', 'Ġnames', 'Ġn', 'asa', 'Ġscience', 'Ġtechnical', 'Ġinformation', 'ï', '¬', 'ģ', 'ce', 'Ġpp', 'âĢĵ', 'Ġweek', 'Ġhistory', 'Ġfe', 'b', 'Ġair', 'Ġforce', 'Ġawards', 'Ġcontract', 'las', 'Ġpropulsion', 'Ġsystem', 'Ġro', 'pu', 'Ġu', 'Ġair', 'Ġforce', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmarch', 'Ġhistory', 'Ġlearn', 'Ġstories', 'Ġbehind', 'Ġbrand', 'Ġretrieved', '06', 'las', 'Ġe', 'Ġencyclopedia', 'Ġastronaut', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'project', 'Ġscore', 'Ġpat', 'terson', 'Ġarmy', 'Ġhealth', 'Ġclinic', 'Ġarchived', 'Ġoriginal', '06', 'score', 'sign', 'al', 'Ġcommunication', 'Ġorbiting', 'Ġrelay', 'Ġequipment', ')"', 'Ġglobal', 'security', 'org', 'Ġretrieved', 'Ġoct', 'ober', 'Ġvideo', 'las', 'Ġorbit', 'Ġradios', 'Ġ', 'ike', "'s", 'Ġmessage', 'Ġpeace', 'Ġworld', 'Ġuniversal']</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>['Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ill', 'ustration', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'ula', 'Ġdelta', 'Ġiv', 'Ġsuccessfully', 'Ġlo', 'fts', 'Ġsatellite', 'Ġmay', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecond', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġmission', 'Ġu', 'Ġair', 'Ġforce', 'Ġless', 'Ġthree', 'Ġmonths', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaug', 'ust', 'Ġretrieved', 'Ġmay', 'se', 'venth', 'Ġsatellite', 'Ġair', 'Ġforce', "'s", 'Ġseries', 'Ġlaunched', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'Ġwall', 'ike', 'Ġde', 'cember', 'us', 'Ġair', 'Ġforce', 'Ġlaunches', 'Ġadvanced', 'Ġmilitary', 'Ġcommunications', 'Ġsatellite', 'Ġspace', 'Ġretrieved', 'Ġde', 'cember', 'ula', 'Ġdelta', 'Ġiv', 'Ġlaunches', 'Ġsatellite', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'Ġhunt', 'Ġke', 'vin', 'fall', 'wide', 'band', 'Ġglobal', 'Ġsat', 'Ġintegration', 'Ġroyal', 'adian', 'Ġnavy', 'Ġmaritime', 'Ġengineering', 'Ġjournal', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'http', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'Ġse', 'Ġk', 'imm', 'ons', 'Ġarmy', 'Ġnews', 'Ġservice', 'Ġmarch', 'Ġsatellite', 'Ġlaunch', 'Ġenhances', 'Ġcomm', 'Ġarmy', 'Ġmissions', 'contract', 'Ġapr', 'il', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'bo', 'e', 'ing', 'Ġreceives', 'Ġmillion', 'Ġair', 'Ġforce', 'Ġcontract', 'Ġcommunications', 'Ġsatellite', 'Ġe', 'Ġspac', 'en', 'ews', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġmedia', 'Ġrelated', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'imedia', 'Ġcommons', 'Ġexternal', 'Ġlinks', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġwik', 'ipedia', 'Ġretrieved']</t>
+          <t>['Ġnews', 'els', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ency', 'cl', 'op', 'edia', 'Ġastronaut', 'ica', 'las', 'htm', 'Ġastronaut', 'ix', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'uly', 'las', 'Ġphase', 'Ġsee', 'Ġalso', 'Ġreferences', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'ari', 'q', 'Ġmal', 'ik', 'aug', 'ust', 'final', 'las', 'Ġrocket', 'Ġorbits', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġu', 'Ġsatellite', 'Ġspace', 'Ġretrieved', 'Ġmarch', 'Ġmark', 'Ġw', 'ade', 'las', 'ag', 'ena', 'Ġh', 'tm', 'Ġastronaut', 'ix', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġoct', 'ober', 'las', 'Ġf', 'Ġspac', 'el', 'aun', 'chn', 'ow', 'Ġretrieved', 'Ġmarch', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġapr', 'il', 'las', 'ga', 'Ġastronaut', 'ix', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġoct', 'ober', 'elta', 'Ġastronaut', 'ix', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'las', 'sl', 'v', 'b', 'Ġag', 'ena', 'Ġspace', 'sky', 'rocket', 'de', 'Ġretrieved', 'Ġoct', 'ober', 'las', 'Ġencyclopedia', 'Ġastronaut', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġoct', 'ober', 'space', 'Ġlaunch', 'Ġreport', 'las', 'Ġdata', 'Ġsheet', 'Ġdec', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'lock', 'heed', 'Ġmart', 'Ġready', 'Ġlaunch', 'Ġint', 'els', 'Ġspacecraft', 'Ġlock', 'heed', 'Ġmart', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġaug', 'ust', 'ula', 'Ġstops', 'Ġselling', 'Ġcenterpiece', 'las', 'Ġv', 'Ġsetting', 'Ġpath', 'Ġrocket', "'s", 'Ġretirement', 'htt', 'Ġverge', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ev', 'olved', 'Ġexpend', 'able']</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -698,7 +698,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['Ġswarm', 'Ġtechnologies', 'Ġwik', 'ipedia', 'Ġswarm', 'Ġtechnologies', 'Ġinc', 'Ġtype', 'Ġprivate', 'Ġindustry', 'Ġtelecommunications', 'Ġfounded', 'Ġfounders', 'ara', 'Ġsp', 'angelo', 'ce', 'Ġben', 'Ġlong', 'ier', 'Ġheadquarters', 'Ġpal', 'Ġal', 'Ġcal', 'ornia', 'Ġu', 'Ġnumber', 'Ġemployees', ')[', 'Ġparent', 'Ġspace', 'x', 'Ġwebsite', 'sw', 'arm', 'space', 'http', 'sw', 'arm', 'Ġpace', 'Ġswarm', 'Ġtechnologies', 'Ġswarm', 'Ġtechnologies', 'Ġinc', 'Ġprivate', 'Ġcompany', 'Ġbuilding', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġconstellation', 'Ġcommunications', 'Ġinternet', 'Ġthings', 'iot', 'Ġdevices', 'Ġusing', 'Ġstore', 'Ġforward', 'Ġdesign', 'Ġsocial', 'Ġcapital', 'Ġincub', 'ated', 'Ġswarm', 'Ġcraft', 'Ġventures', 'Ġearly', 'Ġinvestor', 'Ġj', 'uly', 'Ġswarm', 'Ġentered', 'Ġagreement', 'Ġbecome', 'Ġdirect', 'Ġwholly', 'owned', 'Ġsubsidiary', 'Ġspace', 'x', 'q', 'tel', 'Ġventure', 'Ġcapital', 'Ġarm', 'Ġc', 'ia', 'Ġlists', 'Ġswarm', 'Ġtechnologies', 'Ġone', 'Ġstartups', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġlicence', 'Ġlow', 'Ġbandwidth', 'Ġcommunications', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġswarm', 'Ġbecame', 'Ġfirst', 'Ġu', 'Ġcompany', 'Ġfound', 'Ġdeployed', 'Ġsatellites', 'Ġwithout', 'Ġregulatory', 'Ġapproval', 'Ġinvestigation', 'Ġstartup', "'s", 'Ġlaunch', 'Ġfirst', 'Ġfour', 'Ġpic', 'os', 'atell', 'ites', 'Ġind', 'ian', 'Ġrocket', 'Ġjan', 'uary', 'Ġde', 'cember', 'Ġswarm', 'Ġlaunched', 'Ġtest', 'Ġsatellites', 'Ġplanned', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellites', 'Ġprovide', 'Ġcommunication', 'ot', 'Ġdevices', 'Ġfe', 'b', 'ruary', 'Ġswarm', 'Ġannounced', 'Ġcommercial', 'Ġservices', 'Ġlive', 'Ġusing', 'Ġcommercial', 'Ġsatellites', 'Ġproviding', 'Ġglobal', 'Ġlow', 'Ġcost', 'Ġdata', 'Ġservice', 'Ġcustomers', 'Ġswarm', 'Ġtile', 'Ġdedicated', 'Ġtwo', 'way', 'Ġsatellite', 'Ġdata', 'Ġmodem', 'Ġdesigned', 'Ġlow', 'Ġenergy', 'Ġembedded', 'Ġthird', 'party', 'Ġproducts', 'Ġproducts', 'Ġinclude', 'Ġdata', 'Ġplan', 'Ġdevelopment', 'Ġswarm', 'Ġtechnologies', 'Ġfounded', 'ara', 'Ġsp', 'angelo', 'Ġben', 'jamin', 'Ġlong', 'ier', 'Ġformer', 'Ġemployees', 'Ġgoogle', 'Ġapple', 'Ġrespectively', 'Ġcompany', 'Ġbecame', 'Ġwidely', 'Ġknown', 'Ġindustry', 'Ġcircles', 'Ġillegally', 'Ġlaunching', 'Ġfirst', 'Ġfour', 'Ġtest', 'Ġsatellites', 'Ġresponsible', 'Ġus', 'Ġregulatory', 'Ġauthority', 'Ġrefused', 'Ġlicense', 'Ġstart', 'Ġfeared', 'Ġsatellites', 'Ġcould', 'Ġsmall', 'Ġrecognized', 'Ġspace', 'Ġsurveillance', 'Ġsystems', 'Ġcould', 'Ġbecome', 'Ġparticularly', 'Ġdangerous', 'Ġturning', 'visible', 'Ġspace', 'Ġdebris', 'Ġdespite', 'Ġsatellites', 'Ġalong', 'Ġaround', 'Ġpayload', 'Ġlaunched', 'Ġind', 'ian', 'Ġrocket']</t>
+          <t>['Ġlaunch', 'Ġvehicle', 'Ġaf', 'sp', 'c', 'af', 'mil', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġoct', 'ober', 'ula', 'Ġcould', 'Ġmany', 'Ġr', 'ussian', 'made', 'Ġr', 'Ġengines', 'Ġspac', 'en', 'ews', '01', 'Ġretrieved', '04', 'Ġfer', 'ster', 'Ġwar', 'ren', '09', 'ula', 'Ġinvest', 'Ġblue', 'Ġorigin', 'Ġengine', 'Ġr', 'Ġreplacement', 'Ġace', 'ment', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', '09', 'Ġpet', 'ersen', 'Ġmelody', 'cong', 'ress', 'ks', 'Ġbill', 'Ġbanning', 'Ġpurchases', 'Ġr', 'ussian', 'made', 'Ġrocket', 'Ġengines', 'Ġla', 'Ġtimes', 'Ġretrieved', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġrand', 'Ġcorporation', 'Ġp', 'Ġretrieved', 'Ġoct', 'ober', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġrand', 'Ġcorporation', 'Ġp', 'Ġretrieved', 'Ġoct', 'ober', 'las', 'Ġe', 'el', 'v', 'Ġlock', 'heed', 'mart', 'Ġretrieved', '02', '08', 'Ġglobal', 'security', 'org', 'Ġretrieved', 'Ġfinal', 'Ġreport', 'Ġseeking', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġprogram', 'Ġworthy', 'Ġgreat', 'Ġnation', 'Ġoct', 'ober', 'Ġp', 'Ġretrieved', '02', '07', 'review', 'Ġu', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġplans', 'Ġcommittee', 'Ġgain', 'Ġchrist', 'opher', 'las', 'Ġair', 'Ġforce', 'Ġreass', 'essing', 'Ġbeginnings', 'Ġameric', "'s", 'Ġfirst', 'Ġinter', 'continental', 'Ġreading', 'las', 'rocket', 'Ġfamily', 'Ġwik', 'ipedia', 'Ġballistic', 'Ġmissile', 'Ġtechnology', 'Ġculture', 'ap', 'ril', 'âĢĵ', 'las', 'Ġencyclopedia', 'Ġastronaut', 'ica', 'htm', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>['Ġimposed', '000', 'Ġfine', 'Ġhousing', 'Ġnext', 'Ġtest', 'Ġsatellites', 'Ġenlarged', 'Ġtogether', 'Ġcorrespond', 'ingly', 'Ġenlarged', 'Ġradar', 'Ġreflect', 'ors', 'Ġg', 'ps', 'based', 'Ġposition', 'Ġtransmitter', 'Ġincreased', 'Ġtrace', 'ability', 'Ġpermitted', 'Ġlicensing', 'Ġconstruction', 'Ġactual', 'Ġconstellation', 'Ġbegan', 'Ġlaunch', 'Ġtwelve', 'Ġthird', 'generation', 'Ġspace', 'bees', 'Ġse', 'pt', 'ember', 'Ġeuro', 'pe', 'ga', 'Ġrocket', 'Ġadditional', 'Ġspace', 'bee', 'Ġsatellites', 'Ġlaunched', 'Ġend', 'Ġjan', 'uary', 'Ġcommercial', 'Ġoperations', 'Ġconstellation', 'Ġbegan', 'Ġj', 'uly', 'Ġspace', 'x', 'Ġacquired', 'Ġswarm', 'Ġmillion', 'Ġthird', 'generation', 'Ġspace', 'bee', 'Ġsatellites', 'Ġweigh', 'Ġaround', 'Ġgrams', 'Ġlike', 'Ġfirst', 'Ġgeneration', 'u', 'Ġcubes', 'Ġformat', 'Ġaccording', 'Ġmanufacturer', 'Ġcentimeters', 'Ġsize', 'Ġsecond', 'Ġgeneration', 'Ġcubes', 'ats', 'Ġsolar', 'Ġcells', 'Ġpower', 'Ġsupply', 'Ġlocated', 'Ġtop', 'Ġbottom', 'Ġantenna', 'Ġcommunication', 'Ġground', 'Ġstations', 'Ġwrapped', 'Ġaround', 'Ġsatellite', 'Ġlaunched', 'Ġunfolds', 'Ġhistory', 'Ġtechnology', 'Ġuse', 'Ġswarm', 'Ġtechnologies', 'Ġwik', 'ipedia', 'Ġrelease', 'Ġspace', 'Ġdata', 'Ġexchange', 'Ġperformed', 'Ġrelatively', 'Ġsmall', 'Ġbandwidth', 'Ġone', 'Ġhand', 'Ġend', 'Ġdevices', 'Ġhand', 'Ġground', 'Ġstations', 'Ġconnected', 'Ġinternet', 'Ġcompletion', 'Ġconstellation', 'Ġleast', 'Ġthree', 'Ġsatellites', 'Ġalways', 'Ġreach', 'able', 'Ġpoint', 'Ġearth', 'Ġswarm', 'Ġtechnologies', 'Ġoffers', 'Ġdata', 'Ġtransfer', 'Ġplans', 'Ġstarting', 'Ġper', 'Ġyear', 'Ġper', 'Ġconnected', 'Ġdevice', 'Ġprice', 'Ġdata', 'Ġpackets', 'Ġbytes', 'Ġtransmitted', 'Ġmonthly', 'Ġus', 'Ġcorporation', 'Ġswarm', 'Ġfollow', 'Ġus', 'Ġspace', 'Ġregulatory', 'Ġprocedures', 'Ġapr', 'il', 'Ġswarm', 'Ġapplied', 'Ġpermission', 'Ġexperimental', 'Ġradio', 'Ġservice', 'Ġlicense', 'Ġinitial', 'Ġpic', 'os', 'atell', 'ites', 'Ġrejected', 'Ġapplication', 'Ġde', 'cember', 'Ġdue', 'Ġconcerns', 'Ġtracking', 'Ġsmall', 'Ġsize', 'Ġsatellites', 'asuring', 'u', 'Ġcubes', 'Ġsize', 'Ġlaunched', 'Ġind', 'ia', 'Ġfollowing', 'Ġmonth', 'Ġlaunch', 'Ġreported', 'Ġauthorized', 'Ġapr', 'il', 'Ġlaunch', 'Ġsatellites', 'Ġimmediately', 'Ġdelayed', 'Ġpermission', 'Ġwithdrawn', 'Ġinvestigation', 'Ġfound', 'Ġswarm', 'Ġlaunched', 'Ġfour', 'Ġunauthorized', 'Ġsatellites', 'Ġalso', 'Ġunlawfully']</t>
+          <t>['las', 'Ġwik', 'ipedia', 'las', 'Ġlaunch', 'las', 'Ġcarrying', 'Ġlunar', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġl', 'cross', 'Ġspace', 'Ġprobes', 'Ġj', 'une', 'Ġfunction', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġsize', 'Ġheight', 'Ġft', 'Ġpayload', 'Ġfair', 'ing', 'Ġft', 'Ġstar', 'liner', 'Ġdiameter', 'Ġft', 'Ġmass', '000', '000', 'Ġstages', 'Ġstar', 'Ġupper', 'Ġstage', 'Ġcapacity', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', 'âĢĵ', 'âĢĵ', 'Ġpayload', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġmass', 'âĢĵ', 'âĢĵ', 'Ġassociated', 'Ġrockets', 'Ġfamily', 'las', 'Ġbased', 'las', 'Ġcomparable', 'Ġdelta', 'Ġiv', 'Ġfal', 'con', 'Ġlong', 'Ġmarch', 'Ġpro', 'ton', 'Ġsat', 'urn', 'Ġlaunch', 'Ġhistory', 'las', 'las', 'Ġv', 'Ġexpend', 'able', 'Ġlaunch', 'Ġsystem', 'Ġfifth', 'Ġmajor', 'Ġversion', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġfamily', 'Ġoriginally', 'Ġdesigned', 'Ġlock', 'heed', 'Ġmart', 'Ġoperated', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġjoint', 'Ġventure', 'Ġlock', 'heed', 'Ġmart', 'Ġbo', 'e', 'ing', 'las', 'Ġalso', 'Ġmajor', 'Ġn', 'asa', 'Ġlaunch', 'Ġvehicle', 'Ġameric', "'s", 'Ġlongest', 'serving', 'Ġactive', 'Ġrocket', 'Ġaug', 'ust', 'Ġu', 'la', 'Ġannounced', 'las', 'Ġwould', 'Ġretired', 'Ġremaining', 'Ġlaunches', 'Ġsold', 'mber', 'Ġlaunches', 'Ġremain', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġconsists', 'Ġtwo', 'Ġmain', 'Ġstages', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġr', 'ussian', 'Ġr', 'Ġengine', 'Ġmanufactured', 'Ġener', 'gom', 'ash', 'Ġburning', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġpowered', 'Ġone', 'Ġtwo', 'Ġameric', 'Ġengine', 'Ġmanufactured', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġburns', 'Ġliquid', 'Ġhydrogen', 'Ġliquid', 'Ġstar', 'Ġupper', 'Ġstage', 'Ġused', 'Ġnew', 'Ġhor', 'izons', 'Ġmission', 'Ġthird', 'Ġstage', 'Ġstrap', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġused', 'Ġconfigurations', 'Ġused', 'Ġoriginally', 'Ġreplaced', 'mber', 'Ġgraph', 'ite', 'ep', 'oxy', 'Ġmotor', 'gem', 'Ġstandard', 'Ġpayload', 'Ġfair', 'ings']</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -724,7 +724,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['Ġtransmitted', 'Ġsignals', 'Ġearth', 'Ġstations', 'Ġge', 'org', 'ia', 'Ġinvestigation', 'Ġalso', 'Ġdiscovered', 'Ġswarm', 'Ġperformed', 'Ġvarious', 'Ġequipment', 'Ġtests', 'Ġlaunch', 'Ġwithout', 'Ġrequired', 'Ġauthor', 'izations', 'Ġincluding', 'Ġweather', 'Ġballoons', 'Ġground', 'Ġstations', 'Ġindustry', 'Ġreaction', 'Ġalso', 'Ġhighly', 'Ġnegative', 'Ġfearing', 'Ġdisruption', 'Ġun', 'coord', 'inated', 'Ġactivity', 'Ġalso', 'Ġenhanced', 'Ġfuture', 'Ġregulation', 'Ġspace', 'flight', 'Ġinc', '.,', 'Ġarranged', 'Ġind', 'ian', 'Ġlaunch', 'Ġrides', 'hare', 'Ġchanged', 'Ġprocesses', 'Ġcheck', 'Ġcustomers', 'Ġproper', 'Ġlicenses', 'Ġsettlement', 'Ġrequired', 'Ġswarm', 'Ġpay', 'Ġpenalty', '000', 'Ġfollow', 'Ġstrict', 'Ġcompliance', 'Ġplan', 'Ġprevent', 'Ġfuture', 'Ġviolations', 'Ġincluded', 'Ġsubmitting', 'Ġadditional', 'Ġdetails', 'Ġleast', 'Ġdays', 'Ġplanned', 'Ġlaunch', 'Ġnext', 'Ġthree', 'Ġyears', 'Ġnoted', 'Ġfine', 'Ġrelatively', 'Ġsmall', 'Ġincreased', 'Ġinitial', 'Ġamount', 'Ġagreed', 'Ġcompany', 'Ġenforcement', 'Ġbureau', 'Ġcommissioner', 'Ġobserved', 'Ġnegative', 'Ġpublicity', 'Ġwould', 'Ġprobably', 'Ġprevent', 'Ġrepet', 'itions', 'Ġswarm', 'Ġspace', 'bee', 'Ġconstellation', 'Ġpic', 'os', 'atell', 'ites', 'Ġpredominantly', 'Ġcubes', 'u', 'Ġform', 'Ġfactor', 'Ġintended', 'Ġreach', 'Ġquantity', 'Ġspace', 'bee', 'Ġtest', 'Ġmodels', 'Ġlarger', 'Ġass', 'u', 'age', 'Ġconcerns', 'Ġradar', 'Ġtracking', 'Ġswarm', "'s", 'Ġwebsite', 'Ġlists', 'Ġsatellites', 'Ġmass', 'Ġsize', 'Ġmm', 'Ġcontroversy', 'Ġfine', 'Ġsatellite', 'Ġconstellation', 'Ġswarm', 'Ġtechnologies', 'Ġwik', 'ipedia', 'Ġspace', 'bee', 'Ġlaunches', 'Ġflight', 'Ġmission', 'Ġcos', 'par', 'Ġid', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġlaunch', 'Ġsite', 'Ġlaunch', 'Ġvehicle', 'Ġorbit', 'Ġaltitude', 'Ġinclination', 'Ġnumber', 'Ġdeployed', 'Ġde', 'orb', 'ited', 'Ġoutcome', 'Ġspace', 'bee', 'âĢĵ', '004', 'Ġjan', 'uary', 'Ġ03', '00', 'Ġsat', 'ish', 'haw', 'Ġspace', 'Ġcentre', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġfour', 'Ġexperimental', 'Ġsatellites', 'Ġspace', 'bee', 'Ġbuilt', 'u', 'Ġcubes', 'Ġdemonstrate', 'Ġtwo', 'way', 'Ġsatellite', 'Ġcommunications', 'Ġdata', 'Ġrelay', 'Ġswarm', 'Ġtechnologies', 'Ġinc', 'Ġspace', 'bee', 'âĢĵ', 'Ġde', 'cember', '05', 'Ġv', 'enberg', 'Ġfal', 'con', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġthree', 'Ġexperimental', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'âĢĵ', 'Ġj', 'une', 'Ġ04', '00', 'Ġmah', 'ia', 'Ġelectron', 'Ġmi', 'Â°']</t>
+          <t>['Ġft', 'Ġdiameter', 'Ġvarious', 'Ġlengths', 'las', 'Ġdeveloped', 'Ġlock', 'heed', 'Ġmart', 'Ġcommercial', 'Ġlaunch', 'Ġservices', 'Ġpart', 'Ġu', 'Ġair', 'Ġforce', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'e', 'el', 'v', 'Ġprogram', 'Ġmade', 'Ġinaugural', 'Ġflight', 'Ġaug', 'ust', 'Ġvehicle', 'Ġoperates', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġv', 'enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġcontinued', 'Ġmarket', 'las', 'Ġcommercial', 'Ġcustomers', 'Ġworldwide', 'Ġjan', 'uary', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġassumed', 'Ġcontrol', 'Ġcommercial', 'Ġmarketing', 'Ġsales', 'las', 'Ġfirst', 'Ġstage', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġconfused', 'Ġdelta', 'Ġiv', "'s", 'Ġcommon', 'Ġbooster', 'Ġcore', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġlength', 'Ġpowered', 'Ġone', 'Ġn', 'po', 'Ġener', 'gom', 'ash', 'Ġr', 'Ġmain', 'Ġengine', 'Ġburning', 'Ġliquid', 'Ġbooster', 'Ġoperates', 'Ġfour', 'Ġminutes', 'Ġproviding', '000', 'Ġthrust', 'Ġthrust', 'Ġaugmented', 'Ġfive', 'ero', 'jet', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġgem', 'Ġstrap', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġproviding', 'Ġadditional', '000', 'Ġthrust', 'Ġseconds', 'Ġmain', 'Ġdifferences', 'las', 'Ġearlier', 'las', 'Ġfamily', 'Ġlaunch', 'Ġvehicles', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġtanks', 'Ġlonger', 'Ġuse', 'Ġstainless', 'Ġsteel', 'Ġmon', 'oco', 'que', 'Ġpressure', 'Ġstabilized', 'ball', 'oon', 'Ġconstruction', 'Ġtanks', 'og', 'rid', 'Ġaluminum', 'Ġstruct', 'urally', 'Ġstable', 'Ġun', 'press', 'urized', 'Ġaccommodation', 'Ġpoints', 'Ġparallel', 'Ġstages', 'Ġsmaller', 'Ġsol', 'ids', 'Ġidentical', 'Ġliquids', 'Ġbuilt', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġstructures', 'Ġstaging', 'Ġtechnique', 'Ġlonger', 'Ġused', 'Ġdiscontinued', 'las', 'Ġintroduction', 'Ġr', 'ussian', 'Ġr', 'Ġengine', 'Ġmain', 'stage', 'Ġdiameter', 'Ġincreased', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġuses', 'Ġpressure', 'st', 'abil', 'ized', 'Ġpropell', 'ant', 'tank', 'Ġdesign', 'Ġcry', 'ogenic', 'Ġpropell', 'ants', 'Ġcent', 'aur', 'Ġstage', 'las', 'Ġstretched', 'Ġft', 'Ġrelative', 'las', 'Ġcent', 'aur', 'Ġpowered', 'Ġeither', 'Ġone', 'Ġtwo', 'ero']</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -737,7 +737,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['Ġsuccess', 'Ġtwo', 'Ġexperimental', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'âĢĵ', 'Ġse', 'pt', 'ember', 'Ġ01', 'Ġk', 'ou', 'ga', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġtwelve', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'âĢĵ', 'Ġspace', 'bee', 'mber', 'Ġ02', '01', 'Ġmah', 'ia', 'Ġelectron', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġeighteen', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'âĢĵ', '006', 'Ġjan', 'uary', '00', '00', 'Ġfal', 'con', 'Ġsuccess', 'Ġthirty', 'six', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'âĢĵ', '015', 'Ġfe', 'b', 'ruary', 'Ġ04', '00', 'Ġsd', 'sc', 'Ġsuccess', 'Ġtwelve', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'âĢĵ', 'Ġspace', 'bee', 'Ġj', 'une', '00', 'Ġfal', 'con', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġtwenty', 'four', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġfour', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'Ġspace', 'bee', 'Ġmarch', '00', 'Ġk', 'odi', 'ak', 'Ġrocket', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', 'Ġmay', 'Ġmah', 'ia', 'Ġelectron', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġswarm', 'Ġtechnologies', 'Ġwik', 'ipedia', 'Ġspace', 'bee', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'bee', '001', 'Ġjan', 'uary', '00', 'Ġfal', 'con', 'Ġmi', 'Â°', 'Ġsuccess', 'Ġcommercial', 'Ġsatellites', 'Ġspace', 'bee', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġstory', 'Ġswarm', 'Ġtechnologies', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust']</t>
+          <t>['jet', 'Ġrocket', 'dy', 'ne', 'Ġengines', 'Ġengine', 'Ġdeveloping', 'Ġthrust', 'Ġkn', 'Ġinert', 'ial', 'Ġnavigation', 'Ġunit', 'u', 'Ġlocated', 'Ġcent', 'aur', 'Ġprovides', 'Ġguidance', 'Ġnavigation', 'las', 'Ġcent', 'aur', 'Ġcontrols', 'las', 'Ġcent', 'aur', 'Ġtank', 'Ġpressures', 'Ġpropell', 'ant', 'Ġuse', 'Ġcent', 'aur', 'Ġengines', 'Ġcapable', 'Ġmultiple', 'Ġins', 'pace', 'Ġstarts', 'Ġmaking', 'Ġpossible', 'Ġinsertion', 'Ġlow', 'Ġearth', 'Ġparking', 'Ġorbit', 'Ġfollowed', 'Ġcoast', 'Ġperiod', 'Ġinsertion', 'Ġg', 'Ġsubsequent', 'Ġthird', 'Ġburn', 'Ġfollowing', 'Ġmulti', 'hour', 'Ġcoast', 'Ġpermit', 'Ġdirect', 'Ġinjection', 'Ġpayload', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcent', 'aur', 'Ġvehicle', 'Ġhighest', 'Ġproportion', 'Ġburn', 'able', 'Ġpropell', 'ant', 'Ġrelative', 'Ġtotal', 'Ġmass', 'Ġmodern', 'Ġhydrogen', 'Ġupper', 'Ġstage', 'Ġhence', 'Ġdeliver', 'Ġsubstantial', 'Ġpayload', 'Ġhigh', 'energy', 'Ġstate', 'las', 'Ġpayload', 'Ġfair', 'ings', 'Ġavailable', 'Ġtwo', 'Ġdiam', 'eters', 'Ġdepending', 'Ġsatellite', 'Ġrequirements', 'Ġft', 'Ġdiameter', 'Ġfair', 'ing', 'Ġoriginally', 'Ġdesigned', 'las', 'Ġbooster', 'Ġcomes', 'Ġthree', 'Ġdifferent', 'Ġlengths', 'Ġoriginal', 'Ġft', 'Ġversion', 'Ġextended', 'Ġft', 'Ġversions', 'Ġfirst', 'Ġflown', 'Ġrespectively', 'Ġav', '008', 'ast', 'ra', 'Ġav', '004', 'ars', 'Ġmissions', 'Ġfair', 'ings', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġlength', 'Ġconsidered', 'Ġnever', 'Ġimplemented', 'Ġft', 'Ġdiameter', 'Ġfair', 'ing', 'Ġinternally', 'Ġusable', 'Ġdiameter', 'Ġft', 'Ġdeveloped', 'Ġbuilt', 'Ġru', 'ag', 'Ġspace', 'Ġsw', 'itzerland', 'Ġru', 'ag', 'Ġfair', 'ing', 'Ġuses', 'Ġcarbon', 'Ġfiber', 'Ġcomposite', 'Ġconstruction', 'Ġbased', 'Ġsimilar', 'Ġflight', 'proven', 'Ġfair', 'ing', 'ri', 'ane', 'Ġthree', 'Ġconfigurations', 'Ġmanufactured', 'Ġsupport', 'las', 'Ġv', 'Ġvehicle', 'Ġdescription', 'las', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġfair', 'ing', 'las', 'Ġwik', 'ipedia', 'show', 'show', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġv', 'af', 'b', 'Ġtotal', 'Ġlaunches', 'Ġsuccess']</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -750,7 +750,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['space', 'x', 'Ġacquire', 'Ġswarm', 'Ġtechnologies', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'q', 'tel', 'Ġwebsite', 'q', 'tel', 'Ġportfolio', 'Ġcold', 'ew', 'ey', 'Ġdev', 'Ġoct', 'ober', 'sw', 'arm', 'Ġgets', 'Ġgreen', 'Ġlight', 'atellite', 'Ġconstellation', 'Ġtech', 'cr', 'unch', 'Ġretrieved', 'Ġaug', 'ust', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġoct', 'ober', 'company', 'Ġlaunched', 'Ġsatellites', 'Ġwithout', 'Ġpermission', 'Ġgets', 'Ġnew', 'Ġlicense', 'Ġlaunch', 'Ġprobes', 'Ġverge', 'Ġretrieved', 'Ġaug', 'ust', 'Ġsp', 'angelo', 'ara', 'Ġse', 'pt', 'ember', 'sw', 'arm', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcommercial', 'Ġsatellites', 'Ġswarm', 'Ġtechnologies', 'Ġretrieved', 'Ġjan', 'uary', 'Ġsp', 'angelo', 'ara', 'Ġfe', 'b', 'ruary', 'sw', 'arm', 'Ġcommercially', 'Ġlive', '!"', 'Ġe', 'Ġswarm', 'Ġtechnologies', 'Ġretrieved', 'Ġaug', 'ust', 'products', 'Ġswarm', 'Ġtechnologies', 'Ġretrieved', 'Ġaug', 'ust', 'ichael', 'Ġsheet', 'z', 'Ġformer', 'Ġgoogle', 'Ġengineer', "'s", 'Ġstart', 'Ġslammed', 'Ġunauthorized', 'Ġsatellite', 'Ġlaunch', 'w', 'Ġmarch', '000', 'Ġdollar', 'Ġstra', 'fe', 'Ġf', 'Ã¼r', 'Ġn', 'icht', 'Ġgene', 'hm', 'ig', 'te', 'Ġsatell', 'en', 'ise', 'Ġonline', 'Ġde', 'cember', 'Ġswarm', 'Ġgets', 'Ġgreen', 'Ġlight', 'atellite', 'Ġconstellation', 'Ġtech', 'cr', 'unch', 'Ġoct', 'ober', 'Ġspace', 'bee', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġde', 'cember', 'Ġtrack', 'ability', 'Ġdetect', 'ability', 'Ġspace', 'bee', 'Ġsatellites', 'Ġn', 'key', 'Ġle', 'ol', 'abs', 'Ġoct', 'ober', 'Ġsatellite', 'Ġstartup', 'Ġswarm', 'Ġkicks', 'Ġspace', 'based', 'Ġinternet', 'Ġservice', 'Ġfortune', 'Ġfe', 'b', 'ruary', 'Ġmaiden', 'berg', 'Ġmic', 'ah', 'Ġdri', 'ebus', 'ch', 'Ġcor', 'rie', 'Ġj', 'Ġber', 'ber', 'Ġaug', 'ust', 'Ġrare', 'Ġlook', 'Ġfinances', 'Ġel', 'Ġmus', 'k', "'s", 'Ġsecretive', 'Ġspace', 'x', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġtechnology', 'Ġretrieved', 'Ġde', 'cember', 'Ġproducts', 'Ġder', 'st', 'eller', 'bsite', 'Ġretrieved', 'mber', 'Ġhar', 'ris', 'Ġmark', 'Ġmarch', 'Ġaccuses', 'Ġstealth', 'Ġstartup', 'Ġlaunching', 'Ġrogue', 'Ġsatellites']</t>
+          <t>['es', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġhot', 'Ġbird', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'mber', 'Ġtype', 'Ġpassengers', 'c', 'argo', 'Ġspace', 'Ġprobes', 'Ġpersever', 'ance', 'Ġcuriosity', 'Ġinsight', 'Ġjun', 'Ġl', 'ro', 'Ġl', 'cross', 'ms', 'aven', 'Ġnew', 'Ġhor', 'izons', 'Ġos', 'iris', 'rex', 'Ġsolar', 'Ġdynamics', 'Ġobserv', 'atory', 'Ġvan', 'en', 'Ġprobes', 'Ġbo', 'e', 'ing', 'Ġcy', 'gn', 'us', 'Ġsolo', 'Ġstar', 'liner', 'Ġgoes', 'Ġtd', 'rs', 'Ġn', 'ro', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġpayload', 'Ġintruder', 'Ġqu', 'asar', 'b', 'irs', 'Ġft', 'Ġft', 'Ġft', 'Ġlong', 'Ġclassic', 'Ġft', 'Ġfair', 'ing', 'Ġcovers', 'Ġpayload', 'Ġru', 'ag', 'Ġfair', 'ing', 'Ġmuch', 'Ġlonger', 'Ġfully', 'Ġencl', 'oses', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġmany', 'Ġsystems', 'las', 'Ġsubject', 'Ġupgrade', 'Ġenhancement', 'Ġprior', 'Ġfirst', 'las', 'Ġflight', 'Ġsince', 'Ġtime', 'Ġwork', 'Ġnew', 'Ġfault', 'Ġtolerant', 'Ġinert', 'ial', 'Ġnavigation', 'Ġunit', 'ft', 'u', 'Ġstarted', 'Ġenhance', 'Ġmission', 'Ġreliability', 'las', 'Ġvehicles', 'Ġreplacing', 'Ġexisting', 'Ġnon', 'red', 'und', 'ant', 'Ġnavigation', 'Ġcomputing', 'Ġequipment', 'Ġfault', 'oler', 'ant', 'Ġunit', 'Ġupgraded', 'Ġft', 'u', 'Ġfirst', 'Ġflew', 'Ġfollow', 'Ġorder', 'Ġft', 'u', 'Ġunits', 'Ġawarded', 'Ġu', 'la', 'Ġannounced', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'produced', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġuse', 'las', 'Ġwould', 'Ġsupers', 'eded', 'Ġnew', 'Ġgem', 'Ġboosters', 'Ġproduced', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'Ġextended', 'Ġgem', 'Ġboosters', 'Ġalso', 'Ġused', 'Ġvul', 'Ġcent', 'aur', 'Ġlaunch', 'Ġvehicle', 'Ġreplace', 'las', 'Ġfirst', 'las', 'Ġlaunch', 'Ġgem', 'Ġboosters', 'Ġhappened', 'mber', 'Ġproposals', 'Ġdesign', 'Ġwork', 'Ġhuman', 'rate', 'las', 'Ġbegan', 'Ġearly', 'Ġu', 'la', "'s", 'Ġparent', 'Ġcompany', 'Ġlock', 'heed', 'Ġmart', 'Ġreporting', 'Ġagreement', 'Ġbig', 'el', 'ow', 'Ġaerospace', 'Ġintended', 'Ġlead', 'Ġcommercial', 'Ġprivate', 'Ġtrips', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġhuman', 'rating', 'Ġdesign', 'Ġsimulation', 'Ġwork', 'Ġbegan', 'Ġearnest', 'Ġaward', 'Ġmillion', 'Ġfirst', 'Ġphase', 'Ġn', 'asa', 'Ġcommercial', 'Ġcrew']</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -763,7 +763,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>['Ġie', 'ee', 'Ġspectrum', 'Ġretrieved', 'Ġaug', 'ust', 'ism', 'iss', 'ed', 'without', 'Ġprejudice', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġreaches', '000', 'Ġsettlement', 'Ġunauthorized', 'Ġsatellite', 'Ġlaunch', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġreferences', 'Ġswarm', 'Ġtechnologies', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'indust', 'ry', 'Ġworried', 'Ġregulatory', 'Ġbacklash', 'Ġunauthorized', 'Ġcubes', 'Ġlaunch', 'htt', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġaug', 'ust', 'later', 'Ġyear', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġrocket', 'Ġlaunch', 'Ġbiggest', 'Ġbatch', 'Ġsatellites', 'Ġyet', 'Ġe', 'r', 'ides', 'hare', 'Ġverge', 'Ġretrieved', 'Ġaug', 'ust', 'statement', 'Ġcommissioner', 'ichael', 'ri', 'elly', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', 'space', 'bee', 'Ġ...', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġaug', 'ust', 'display', 'Ġspace', 'bee', 'Ġn', 'ss', 'ca', 'Ġid', 'Ġspace', 'bee', 'Ġcos', 'par', 'Ġid', '004', 'ah', 'Ġn', 'asa', 'Ġmay', 'Ġretrieved', 'Ġjan', 'uary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'display', 'Ġspace', 'bee', 'Ġcos', 'par', 'Ġid', 'bm', 'bm', 'Ġn', 'asa', 'Ġmay', 'Ġretrieved', 'Ġjan', 'uary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'display', 'Ġspace', 'bee', 'Ġn', 'asa', 'Ġmay', 'Ġretrieved', 'Ġjan', 'uary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'cd', 'owell', 'Ġj', 'athan', 'space', 'bee', '06', 'ak', 'Ġj', 'athan', "'s", 'Ġlaunch', 'Ġlog', 'Ġretrieved', 'Ġjan', 'uary', 'cd', 'owell', 'Ġj', 'athan', 'space', 'bee', '08', 'aa', 'Ġj', 'athan', "'s", 'Ġlaunch', 'Ġlog', 'Ġretrieved', 'Ġjan', 'uary', 'Ġch', 'atur', 'ved']</t>
+          <t>['Ġprogram', 'Ġdevelop', 'Ġemergency', 'Ġdetection', 'Ġsystem', 'eds', ').[', 'Ġfe', 'b', 'ruary', 'Ġu', 'la', 'Ġreceived', 'Ġextension', 'Ġapr', 'il', 'Ġn', 'asa', 'Ġfinishing', 'Ġwork', 'Ġed', 'Ġn', 'asa', 'Ġsolic', 'ited', 'Ġproposals', 'Ġphase', 'Ġoct', 'ober', 'Ġu', 'la', 'Ġproposed', 'Ġcomplete', 'Ġdesign', 'Ġwork', 'Ġed', 'Ġtime', 'Ġn', 'asa', "'s", 'Ġgoal', 'Ġget', 'Ġastronauts', 'Ġorbit', 'ula', 'Ġpresident', 'Ġce', 'ichael', 'Ġg', 'ass', 'Ġstated', 'Ġschedule', 'Ġacceleration', 'Ġpossible', 'Ġfunded', 'Ġaddition', 'Ġemergency', 'Ġdetection', 'Ġsystem', 'Ġmajor', 'Ġchanges', 'Ġexpected', 'las', 'Ġrocket', 'Ġground', 'Ġinfrastructure', 'Ġmodifications', 'Ġplanned', 'Ġlikely', 'Ġcandidate', 'Ġhuman', 'rating', 'Ġconfiguration', 'Ġfair', 'ing', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġdual', 'Ġengines', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġu', 'la', 'Ġannounced', 'Ġagreement', 'Ġpossibility', 'Ġcert', 'ifying', 'las', 'Ġn', 'asa', "'s", 'Ġstandards', 'Ġhuman', 'Ġspace', 'flight', 'Ġu', 'la', 'Ġagreed', 'Ġprovide', 'Ġn', 'asa', 'Ġdata', 'las', 'Ġv', 'Ġn', 'asa', 'Ġwould', 'Ġprovide', 'Ġu', 'la', 'Ġdraft', 'Ġhuman', 'Ġcertification', 'Ġrequirements', 'Ġhuman', 'rated', 'las', 'Ġalso', 'Ġstill', 'Ġconsideration', 'Ġcarry', 'Ġspace', 'flight', 'Ġparticipants', 'Ġproposed', 'Ġbig', 'el', 'ow', 'Ġcommercial', 'Ġspace', 'Ġstation', 'ierra', 'Ġne', 'v', 'ada', 'Ġcorporation', 'nc', 'Ġpicked', 'las', 'Ġbooster', 'Ġdream', 'Ġch', 'aser', 'Ġcrew', 'ed', 'Ġspace', 'plane', 'Ġdream', 'Ġch', 'aser', 'Ġintended', 'Ġlaunch', 'las', 'Ġv', 'Ġfly', 'Ġcrew', 'Ġiss', 'Ġlanding', 'Ġhorizontally', 'Ġfollowing', 'Ġlifting', 'body', 'entry', 'Ġhowever', 'Ġlate', 'Ġn', 'asa', 'Ġselect', 'Ġdream', 'Ġch', 'aser', 'Ġone', 'Ġtwo', 'Ġvehicles', 'Ġselected', 'Ġcommercial', 'Ġcrew', 'Ġcompetition', 'Ġaug', 'ust', 'Ġbo', 'e', 'ing', 'Ġannounced', 'Ġwould', 'Ġuse', 'las', 'Ġinitial', 'Ġlaunch', 'Ġvehicle', 'Ġc', 'st', 'Ġcrew', 'Ġcapsule', 'Ġc', 'st', 'Ġtake', 'Ġn', 'asa', 'Ġastronauts', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġalso', 'Ġintended', 'Ġservice', 'Ġproposed', 'Ġbig', 'el', 'ow', 'Ġcommercial', 'Ġspace', 'Ġstation', 'Ġthree', 'flight', 'Ġtest', 'Ġprogram', 'Ġprojected', 'Ġcompleted', 'Ġcert', 'ifying', 'las', 'Ġcombination', 'Ġhuman', 'Ġspace']</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>['Ġfe', 'b', 'ruary', 'Ġlifts', 'azon', 'ia', 'Ġsatellites', 'ro', 'Ġsays', 'Ġlaunch', 'Ġsuccessful', 'Ġhind', 'ust', 'Ġtimes', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġlent', 'z', 'anny', 'Ġj', 'une', 'space', 'x', 'Ġsuccessfully', 'Ġlaunches', 'Ġtransporter', 'Ġmission', 'Ġsatellites', 'w', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġj', 'une', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'sw', 'arm', 'Ġlaunched', 'Ġsatellites', 'Ġast', 'ra', 'Ġmission', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'cd', 'owell', 'Ġj', 'athan', 'planet', 'Ġapr', 'il', "'s", 'Ġclear', 'Ġast', 'ra', 'Ġl', 'v', '000', 'Ġmission', 'Ġlaunched', 'Ġspace', 'bees', 'Ġnamely', 'Ġspace', 'bee', 'Ġnew', 'Ġzeal', 'Ġï', '¬', 'Ĥ', 'agged', 'Ġspace', 'bee', 'Ġtwo', 'Ġid', "'d", 'Ġ', 'ids', 'Ġyet', 'Ġspace', 'bees', 'Ġlaunched', 'Ġtransporter', 'weet', 'Ġretrieved', 'Ġapr', 'il', 'Ġvia', 'Ġtwitter', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'fort', 'Ġpayload', 'Ġride', 'Ġorbit', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġrocket', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'em', 'ole', 'Ġanth', 'ony', 'Ġmay', 'rocket', 'Ġlab', 'Ġmakes', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġbooster', 'Ġcatch', 'Ġattempt', 'Ġsuccessful', 'Ġback', 'Ġmission', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġmay', 'Ġlent', 'z', 'anny', 'Ġjan', 'uary', 'space', 'x', 'Ġrings', 'Ġtransporter', 'Ġrides', 'hare', 'Ġmission', 'nas', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġjan', 'uary', 'ï', '¬', 'ģ', 'cial', 'Ġwebsite', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['flight', 'Ġoperations', 'Ġfirst', 'Ġflight', 'Ġexpected', 'Ġinclude', 'las', 'Ġrocket', 'Ġintegrated', 'Ġunc', 'rew', 'ed', 'Ġc', 'st', 'Ġcapsule', 'Ġsecond', 'Ġflight', 'flight', 'Ġlaunch', 'Ġabort', 'Ġsystem', 'Ġdemonstration', 'Ġmiddle', 'Ġyear', 'Ġthird', 'Ġflight', 'Ġcrew', 'ed', 'Ġmission', 'Ġcarrying', 'Ġtwo', 'Ġbo', 'e', 'ing', 'Ġtest', 'p', 'ilot', 'Ġastronauts', 'Ġle', 'Ġreturning', 'Ġsafely', 'Ġend', 'Ġplans', 'Ġmaterial', 'ize', 'Ġn', 'asa', 'Ġselected', 'Ġbo', 'e', 'ing', 'Ġc', 'st', 'Ġspace', 'Ġcapsule', 'Ġpart', 'Ġprogram', 'Ġextensive', 'Ġdelays', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġc', 'st', 'Ġfirst', 'Ġlaunch', 'Ġunc', 'rew', 'ed', 'Ġc', 'st', 'Ġcapsule', 'Ġbo', 'e', 'ing', 'Ġoft', 'Ġoccurred', 'Ġatop', 'Ġhuman', 'rated', 'las', 'Ġmorning', 'Ġde', 'cember', 'Ġmission', 'Ġfailed', 'Ġmeet', 'Ġgoals', 'Ġdue', 'Ġspacecraft', 'Ġfailure', 'Ġthough', 'las', 'Ġlauncher', 'Ġperformed', 'Ġwell', 'las', 'Ġlaunched', 'Ġstar', 'liner', 'Ġcapsule', 'Ġsecond', 'Ġtime', 'Ġending', 'Ġmission', 'Ġsuccess', 'azon', 'Ġselected', 'las', 'Ġlaunch', 'Ġsatellites', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġoffer', 'Ġhigh', 'speed', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'Ġservice', 'Ġcontract', 'Ġsigned', 'azon', 'Ġnine', 'Ġlaunches', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġaims', 'Ġput', 'Ġthousands', 'Ġsatellites', 'Ġorbit', 'Ġu', 'la', 'azon', "'s", 'Ġfirst', 'Ġlaunch', 'Ġprovider', 'las', 'Ġbooster', 'Ġconfiguration', 'Ġthree', 'digit', 'Ġdesignation', 'Ġfirst', 'Ġdigit', 'Ġshows', 'Ġdiameter', 'Ġmeters', 'Ġpayload', 'Ġfair', 'ing', 'Ġvalue', 'Ġfair', 'ing', 'Ġlaunches', 'n', 'Ġcrew', 'Ġcapsule', 'Ġlaunches', 'Ġpayload', 'Ġfair', 'ing', 'Ġused', 'Ġcrew', 'Ġcapsule', 'Ġlaunched', 'Ġsecond', 'Ġdigit', 'Ġindicates', 'Ġnumber', 'Ġsolid', 'Ġrocket', 'Ġupgrades', 'Ġhuman', 'rating', 'Ġcertification', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġversions', 'las', 'Ġwik', 'ipedia', 'Ġtop', 'az', 'Ġboosters', 'Ġboosters', 'Ġheight', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġmaximum', 'Ġthrust', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġboosters', 'Ġgem']</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -789,7 +789,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġf', 'en', 'gy', 'un', 'Ġâ', '»', 'Ľ', 'äº', 'ĳ', 'åį', '«', 'æĺ', 'Ł', 'Ġmodel', 'Ġsh', 'ghai', 'Ġmuseum', 'Ġprogram', 'Ġoverview', 'Ġcountry', 'Ġpeople', "'s", 'Ġrepublic', 'Ġch', 'ina', 'Ġpurpose', 'Ġmeteor', 'ology', 'Ġstatus', 'Ġactive', 'Ġprogram', 'Ġhistory', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġse', 'pt', 'ember', 'Ġvehicle', 'Ġinformation', 'Ġlaunch', 'Ġvehicle', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġf', 'en', 'gy', 'un', 'Ġsimplified', 'Ġch', 'inese', 'Ġé', '£', 'İ', 'äº', 'ĳ', 'Ġtraditional', 'Ġch', 'inese', 'Ġé', '¢', '¨', 'éĽ', '²', 'Ġlit', 'wind', 'Ġcloud', "')", 'Ġch', 'ina', "'s", 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'Ġpolar', 'Ġsun', 'syn', 'chron', 'ous', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġthree', 'axis', 'Ġstabilized', 'Ġf', 'en', 'gy', 'un', 'Ġsatellite', 'Ġbuilt', 'Ġsh', 'ghai', 'Ġacademy', 'Ġspace', 'flight', 'Ġtechnology', 'ast', 'Ġoperated', 'Ġch', 'ina', 'Ġmeteor', 'ological', 'Ġadministration', 'Ġdate', 'Ġch', 'ina', 'Ġlaunched', 'Ġtwenty', 'one', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġfour', 'Ġclasses', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġpolar', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġf', 'en', 'gy', 'un', 'Ġge', 'os', 'ynchronous', 'Ġjan', 'uary', 'Ġch', 'ina', 'Ġdestroyed', 'Ġone', 'Ġsatellites', 'Ġcos', 'par', '025', 'Ġtest', 'Ġantis', 'atellite', 'Ġmissile', 'Ġaccording', 'Ġn', 'asa', 'Ġintentional', 'Ġdestruction', 'Ġcreated', '000', 'Ġhigh', 'vel', 'ocity', 'Ġdebris', 'Ġitems', 'Ġlarger', 'Ġamount', 'Ġdangerous', 'Ġspace', 'Ġjunk', 'Ġspace', 'Ġmission', 'Ġhistory', 'Ġfour', 'Ġsatellites', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġch', 'ina', "'s", 'Ġfirst', 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġplaced', 'Ġpolar', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġsatellites', 'Ġorb', 'ited', 'Ġearth', 'Ġlow', 'Ġaltitude', 'app', 'rox', 'imate', 'Ġearth', "'s", 'Ġsurface', 'Ġhigh', 'Ġinclination', 'Â°', 'Â°', 'Ġtravers', 'ing', 'Ġnorth', 'Ġpole', 'Ġevery', 'Ġminutes', 'Ġgiving', 'Ġf', 'class', 'Ġsatellites', 'Ġglobal', 'Ġmeteor', 'ological', 'Ġcoverage', 'Ġrapid', 'Ġrevisit', 'Ġtime', 'Ġcloser', 'Ġproximity', 'Ġclouds', 'Ġimage', 'Ġlaunched', 'Ġse', 'pt', 'ember', 'Ġlasted', 'Ġdays', 'Ġsuffered', 'Ġattitude', 'Ġcontrol', 'Ġproblems', 'Ġlaunched', 'Ġse', 'pt', 'ember', 'Ġalong', 'Ġfirst', 'Ġtwo', 'Ġqui', 'ix', 'ing', 'Ġballoon', 'Ġsatellites', 'Ġlasted', 'Ġlate', 'Ġattitude', 'Ġcontrol', 'Ġsystem', 'Ġalso', 'Ġfailed', 'Ġlaunched']</t>
+          <t>['Ġboosters', 'Ġheight', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfirst', 'Ġstage', 'las', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', '05', 'Ġpropell', 'ant', 'Ġmass', '089', 'Ġpowered', 'Ġr', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'sea', 'Ġlevel', 'Ġkn', '000', 'v', 'ac', 'uum', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', '05', 'sea', 'Ġlevel', 'v', 'ac', 'uum', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'Ġcent', 'aur', 'Ġheight', 'Ġft', 'Ġdiameter', '05', 'Ġft', 'Ġempty', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġpowered', 'sec', 'dec', 'las', 'Ġfamily', 'Ġasymm', 'etric', 'Ġdeveloped', 'Ġboosters', 'Ġattached', 'Ġbase', 'Ġlaunch', 'Ġvehicle', 'Ġrange', 'Ġft', 'Ġfair', 'ing', 'Ġft', 'Ġfair', 'ing', 'Ġseen', 'Ġfirst', 'Ġimage', 'Ġlayouts', 'Ġasymm', 'etrical', 'Ġthird', 'Ġdigit', 'Ġrepresents', 'Ġnumber', 'Ġengines', 'Ġcent', 'aur', 'Ġstage', 'Ġeither', '".', 'Ġexample', 'las', 'meter', 'Ġfair', 'ing', 'Ġcent', 'aur', 'Ġengine', 'Ġwhereas', 'las', 'meter', 'Ġfair', 'ing', 'Ġcent', 'aur', 'Ġengine', 'las', 'Ġfair', 'ing', 'Ġtwo', 'Ġcent', 'aur', 'Ġengines', 'Ġfirst', 'Ġlaunched', 'Ġflight', 'Ġcarried', 'Ġstar', 'liner', 'Ġvehicle', 'Ġfirst', 'Ġorbital', 'Ġtest', 'Ġflight', 'Ġj', 'une', 'Ġversions', 'las', 'Ġv', 'Ġdesign', 'Ġproduction', 'Ġrights', 'Ġintellectual', 'Ġproperty', 'Ġrights', 'Ġowned', 'Ġu', 'la', 'Ġlock', 'heed', 'Ġmart', 'Ġlist', 'Ġdate', 'Ġaug', 'ust', 'Ġmass', 'Ġle', 'Ġnumbers', 'Ġinclination']</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -802,7 +802,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['Ġmay', 'Ġalong', 'Ġalso', 'Ġcompleted', 'Ġtwo', 'year', 'Ġdesign', 'Ġlife', 'Ġoperating', 'Ġjan', 'uary', 'Ġlast', 'Ġsatellite', 'Ġclass', 'Ġlaunched', 'Ġmay', 'Ġoperated', 'Ġcontinuously', 'Ġnine', 'Ġyears', 'Ġmay', 'Ġoperations', 'Ġtemporarily', 'Ġlost', 'Ġdespite', 'Ġresusc', 'itation', 'Ġfailed', 'Ġapr', 'il', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġlaunched', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'Ġsh', 'xi', 'Ġprovince', 'Ġlong', 'Ġmarch', 'Ġrockets', 'Ġweighed', 'Ġrespectively', 'Ġaboard', 'Ġsatellite', 'Ġtwo', 'Ġmult', 'ich', 'annel', 'Ġvisible', 'Ġinfrared', 'Ġscanning', 'Ġradi', 'ometers', 'vis', 'r', 'Ġbuilt', 'Ġsh', 'ghai', 'Ġinstitute', 'Ġtechnical', 'Ġphysics', 'sit', 'p', 'Ġbearing', 'Ġoptical', 'Ġscanner', 'Ġimage', 'Ġprocessor', 'Ġradiant', 'Ġcooler', 'Ġcontroller', 'Ġradiant', 'Ġcooler', 'Ġsatellites', 'Ġalso', 'Ġcarried', 'Ġboard', 'Ġhigh', 'energy', 'Ġparticle', 'Ġdetector', 'pd', 'Ġstudy', 'Ġspace', 'Ġenvironment', 'Ġcontributing', 'Ġincreased', 'Ġmass', 'Ġsatellites', 'Ġpowered', 'Ġtwo', 'Ġdeploy', 'able', 'Ġsolar', 'Ġarrays', 'Ġinternal', 'Ġbatteries', 'Ġjan', 'uary', 'Ġch', 'ina', 'Ġconducted', 'Ġfirst', 'Ġanti', 'atellite', 'Ġmissile', 'Ġtest', 'Ġdestroying', 'Ġkinetic', 'Ġkill', 'Ġvehicle', 'Ġidentified', 'Ġunited', 'Ġstates', 'Ġdefense', 'Ġintelligence', 'Ġagency', 'ia', 'Ġsc', 'Ġmodified', 'Ġballistic', 'Ġmissile', 'Ġmounted', 'Ġkill', 'Ġvehicle', 'Ġshoot', 'Ġsubsequent', 'Ġcreation', 'Ġrecord', 'setting', 'Ġamount', 'orbit', 'Ġdebris', 'Ġdrew', 'Ġserious', 'Ġinternational', 'Ġsatellites', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġbased', 'Ġspin', 'st', 'abil', 'ized', 'ong', 'Ġf', 'ang', 'Ġh', 'ong', 'Ġplatform', 'Ġch', 'ina', "'s", 'Ġfirst', 'Ġclass', 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġunlike', 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġpolar', 'Ġorbit', 'like', 'Ġclasses', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġremain', 'Ġfixed', 'Ġposition', 'Ġrelative', 'Ġearth', '000', 'Ġsurface', 'Ġmaintain', 'Ġconstant', 'Ġwatch', 'Ġassigned', 'Ġarea', 'Ġunlike', 'Ġpolar', 'Ġorbiting', 'Ġsatellites', 'Ġview', 'Ġarea', 'Ġtwice', 'Ġday', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġimage', 'Ġlocation', 'Ġfast', 'Ġminute', 'Ġshow', 'Ġlong', 'Ġterm', 'Ġmeteor', 'ological', 'Ġtrends', 'Ġcost', 'Ġresolution', 'Ġbuilt', 'Ġsh', 'ghai', 'Ġinstitute', 'Ġsatellite', 'Ġengineering', 'Ġoperated', 'Ġch', 'inese', 'Ġmeteor', 'ological', 'Ġadministration', 'Ġsatellites', 'Ġtall', 'Ġspin', 'st', 'abil', 'ized', 'Ġrotating', 'Ġrot', 'ations']</t>
+          <t>['Â°', 'Ġupper', 'Ġstages', 'Ġsec', 'Ġsingle', 'Ġengine', 'Ġcent', 'aur', 'Ġdec', 'Ġdual', 'Ġengine', 'Ġcent', 'aur', 'Ġlaunch', 'Ġsystem', 'Ġstatus', 'Ġactive', 'Ġretired', 'Ġnever', 'Ġlaunched', 'Ġplanned', 'Ġcapabilities', 'las', 'Ġwik', 'ipedia', 'Ġmaximum', 'Ġthrust', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'las', 'Ġversion', 'Ġfair', 'ing', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġle', 'Ġpayload', 'Ġg', 'Ġlaunches', 'Ġdate', 'Ġbase', 'Ġprice', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġheavy', 'Ġsec', 'Ġheavy', 'Ġdec', 'Ġdec', 'las', 'Ġwik', 'ipedia', 'Ġversion', 'Ġfair', 'ing', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġle', 'Ġpayload', 'Ġg', 'Ġlaunches', 'Ġdate', 'Ġbase', 'Ġprice', 'Ġc', 'st', 'Ġstar', 'liner', 'Ġnone', 'Ġdec', '000', 'Ġiss', 'Ġpricing', 'Ġinformation', 'las', 'Ġlaunches', 'Ġlimited', 'Ġn', 'asa', 'Ġcontracted']</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -815,7 +815,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>['Ġper', 'Ġminute', 'Ġf', 'class', 'Ġsatellites', 'Ġmarketed', 'Ġopenly', 'Ġavailable', 'Ġdata', 'Ġwhereby', 'Ġuser', 'Ġreceiver', 'Ġcould', 'Ġview', 'Ġderived', 'Ġsensory', 'Ġdata', 'Ġsatellites', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġmass', 'Ġkilograms', 'Ġuse', 'Ġsolar', 'Ġcells', 'Ġbatteries', 'Ġpower', 'Ġap', 'gee', 'Ġmotor', 'Ġj', 'ett', 'ison', 'ed', 'Ġatt', 'aining', 'Ġorbit', 'Ġapr', 'il', 'Ġch', 'ina', 'Ġattempted', 'Ġlaunch', 'Ġf', 'en', 'gy', 'un', 'Ġx', 'ich', 'ang', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'Ġprior', 'Ġmating', 'Ġlong', 'Ġmarch', 'Ġfire', 'Ġcaused', 'Ġexplosion', 'Ġdestroying', 'Ġsatellite', 'Ġkilling', 'Ġtechnician', 'Ġinjuring', 'Ġothers', 'Ġofficials', 'Ġch', 'inese', 'Ġspace', 'Ġagency', 'Ġdescribed', 'Ġmillion', 'Ġus', 'Ġloss', 'Ġsatellite', 'major', 'Ġsetback', 'Ġch', 'inese', 'Ġspace', 'Ġprogram', 'Ġdespite', 'Ġch', 'ina', 'Ġlaunched', 'Ġeight', 'Ġsuccessive', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġwithout', 'Ġincident', 'Ġclasses', 'Ġf', 'en', 'gy', 'un', 'Ġdestruction', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġmodel', 'Ġsh', 'ghai', 'Ġmuseum', 'Ġmock', 'Ġsatellite', 'Ġch', 'inese', 'Ġparticipation', 'Ġmonitoring', 'Ġaur', 'oras', 'Ġscientific', 'Ġspace', 'Ġweather', 'Ġinvestigation', 'Ġinitiated', 'Ġlaunch', 'Ġsatellite', 'Ġcarries', 'Ġwide', 'field', 'Ġaur', 'oral', 'Ġim', 'ager', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġch', 'ina', 'Ġlaunched', 'Ġtwo', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġsatellites', 'Ġsatellite', 'Ġlaunch', 'Ġorbit', 'Ġorbital', 'ps', 'Ġinclination', 'Ġperiod', 'min', 'Ġcos', 'par', 'Ġlaun', 'c', 'Ġsite', 'Ġf', 'eny', 'un', 'Ġse', 'pt', 'ember', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '080', 'Ġf', 'en', 'gy', 'un', 'Ġse', 'pt', 'ember', 'Ġsun', 'syn', 'chron', 'ous', '02', 'Â°', '08', 'Ġf', 'en', 'gy', 'un', '01', 'Ġapr', 'il', 'Ġexploded', 'Ġlaunch', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '029', 'Ġf', 'en', 'gy', 'un', 'Ġmay', 'Ġsun', 'syn', 'chron', 'ous', 'Â°']</t>
+          <t>['Ġu', 'la', 'Ġlaunch', 'aven', 'Ġmission', 'las', 'Ġapproximately', 'Ġus', 'Ġmillion', 'Ġcost', 'Ġconfiguration', 'Ġu', 'Ġair', 'Ġforce', 'Ġblock', 'Ġlaunch', 'Ġvehicles', 'Ġus', 'Ġmillion', 'Ġtd', 'rs', 'Ġlaunch', 'las', 'Ġcost', 'Ġn', 'asa', 'Ġus', 'Ġmillion', 'Ġstarting', 'Ġu', 'la', 'Ġprovided', 'Ġpricing', 'las', 'Ġrocket', 'builder', 'Ġwebsite', 'Ġadvertising', 'Ġbase', 'Ġprice', 'Ġlaunch', 'Ġvehicle', 'Ġconfiguration', 'Ġranges', 'Ġus', 'Ġmillion', 'Ġus', 'Ġmillion', 'Ġadditional', 'Ġadds', 'Ġaverage', 'Ġmillion', 'Ġcost', 'Ġlaunch', 'Ġvehicle', 'Ġcustomers', 'Ġalso', 'Ġchoose', 'Ġpurchase', 'Ġlarger', 'Ġpayload', 'Ġfair', 'ings', 'Ġadditional', 'Ġlaunch', 'Ġservice', 'Ġoptions', 'Ġn', 'asa', 'Ġair', 'Ġforce', 'Ġlaunch', 'Ġcosts', 'Ġoften', 'Ġhigher', 'Ġequivalent', 'Ġcommercial', 'Ġmissions', 'Ġdue', 'Ġadditional', 'Ġgovernment', 'Ġaccounting', 'Ġanalysis', 'Ġprocessing', 'Ġmission', 'Ġassurance', 'Ġrequirements', 'Ġadd', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġcost', 'Ġlaunch', 'Ġlaunch', 'Ġcosts', 'Ġcommercial', 'Ġsatellites', 'Ġg', 'Ġaveraged', 'Ġus', 'Ġmillion', 'Ġsignificantly', 'Ġlower', 'Ġhistoric', 'las', 'Ġpricing', 'Ġhowever', 'Ġrecent', 'Ġyears', 'Ġprice', 'las', 'Ġdropped', 'Ġapproximately', 'Ġus', 'Ġmillion', 'Ġus', 'Ġmillion', 'Ġlarge', 'Ġpart', 'Ġdue', 'Ġcompetitive', 'Ġpressure', 'Ġemerged', 'Ġlaunch', 'Ġservices', 'Ġmarketplace', 'Ġearly', 'Ġu', 'la', 'Ġce', 'ory', 'Ġbr', 'uno', 'Ġstated', 'Ġu', 'la', 'Ġneeds', 'Ġleast', 'Ġtwo', 'Ġcommercial', 'Ġmissions', 'Ġyear', 'Ġorder', 'Ġstay', 'Ġprofitable', 'Ġgoing', 'Ġforward', 'Ġu', 'la', 'Ġattempting', 'Ġwin', 'Ġmissions', 'Ġpurely', 'Ġlowest', 'Ġpurchase', 'Ġprice', 'Ġstating', 'would', 'Ġrather', 'Ġbest', 'Ġvalue', 'Ġprovider', '".[', 'Ġu', 'la', 'Ġsuggested', 'Ġcustomers', 'Ġwould', 'Ġmuch', 'Ġlower', 'Ġinsurance', 'Ġdelay', 'Ġcosts', 'Ġhigh', 'las', 'Ġreliability', 'Ġschedule', 'Ġcertainty', 'Ġmaking', 'Ġoverall', 'Ġcustomer', 'Ġcosts', 'Ġclose', 'Ġusing', 'Ġcompetitors', 'Ġlike', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġu', 'la', 'Ġoffered', 'las', 'Ġheavy', 'Ġoption', 'Ġwould', 'Ġuse', 'Ġthree', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġstages', 'Ġstrapped', 'Ġtogether', 'Ġlift', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġu', 'la', 'Ġstated', 'Ġtime', 'Ġhardware', 'Ġrequired', 'las', 'Ġheavy', 'Ġalready', 'Ġflown', 'las', 'Ġsingle']</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -828,7 +828,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>['025', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '032', 'Ġf', 'en', 'gy', 'un', 'Ġmay', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '024', 'b', 'Ġf', 'en', 'gy', 'un', 'Ġoct', 'ober', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '04', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '05', 'Ġf', 'en', 'gy', 'un', 'Ġmay', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '026', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', 'Ġf', 'en', 'gy', 'un', 'mber', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '059', 'Ġf', 'en', 'gy', 'un', 'Ġjan', 'uary', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '002', 'Ġf', 'en', 'gy', 'un', 'Ġse', 'pt', 'ember', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '052', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '090', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '07', 'Ġf', 'en', 'gy', 'un', 'mber', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '010', '07', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary']</t>
+          <t>['core', 'Ġvehicles', 'Ġlifting', 'Ġcapability', 'Ġproposed', 'Ġlaunch', 'Ġvehicle', 'Ġroughly', 'Ġequivalent', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġuses', 'Ġengines', 'Ġdeveloped', 'Ġproduced', 'Ġdomestically', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġreport', 'Ġprepared', 'Ġrand', 'Ġcorporation', 'Ġoffice', 'Ġsecretary', 'Ġdefense', 'Ġstated', 'Ġlock', 'heed', 'Ġmart', 'Ġdecided', 'Ġdevelop', 'las', 'Ġheavy', 'lift', 'Ġvehicle', 'Ġreport', 'Ġrecommended', 'Ġu', 'Ġair', 'Ġforce', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'n', 'ro', 'eter', 'mine', 'Ġnecessity', 'Ġe', 'el', 'v', 'Ġheavy', 'lift', 'Ġvariant', 'Ġincluding', 'Ġdevelopment', 'las', 'Ġheavy', '",', 'res', 'olve', 'Ġr', 'Ġissue', 'Ġincluding', 'Ġcop', 'rodu', 'ction', 'Ġstockpile', 'Ġunited', 'Ġstates', 'Ġdevelopment', 'Ġr', 'Ġreplacement', '".[', 'Ġu', 'la', 'Ġstated', 'las', 'Ġheavy', 'Ġvariant', 'Ġcould', 'Ġavailable', 'Ġcustomers', 'Ġmonths', 'Ġdate', 'Ġorder', 'las', 'Ġlate', 'las', 'Ġprogram', 'Ġgained', 'Ġaccess', 'Ġtool', 'ing', 'Ġprocesses', 'meter', 'iameter', 'Ġstages', 'Ġused', 'Ġdelta', 'Ġiv', 'Ġbo', 'e', 'ing', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'Ġoperations', 'Ġmerged', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġled', 'Ġproposal', 'Ġcombine', 'meter', 'iameter', 'Ġdelta', 'Ġiv', 'Ġtank', 'age', 'Ġproduction', 'Ġprocesses', 'Ġdual', 'Ġr', 'Ġengines', 'Ġresulting', 'las', 'Ġphase', 'las', 'Ġconsisting', 'Ġthree', 'meter', 'Ġstages', 'Ġparallel', 'Ġr', 'Ġconsidered', 'Ġaug', 'ust', 'ine', 'Ġreport', 'Ġpossible', 'Ġheavy', 'Ġlif', 'ter', 'Ġuse', 'Ġfuture', 'Ġspace', 'Ġmissions', 'Ġwell', 'Ġshuttle', 'derived', 'Ġl', 'ite', 'Ġbuilt', 'las', 'Ġprojected', 'Ġable', 'Ġlaunch', 'Ġpayload', 'Ġmass', 'Ġapproximately', 'Ġlong', 'Ġtons', 'Ġshort', 'Ġtons', 'Ġorbit', 'Â°', 'Ġinclination', 'Ġbooster', 'Ġrocket', 'las', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġused', 'Ġfirst', 'Ġstage', 'Ġjoint', 'Ġus', 'j', 'apan', 'ese', 'Ġrocket', 'Ġscheduled', 'Ġmake', 'Ġfirst', 'Ġflight', 'Ġlaunches', 'Ġwould', 'las', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġhowever', 'Ġj', 'apan', 'ese', 'Ġgovernment', 'Ġdecided', 'Ġcancel', 'Ġproject', 'Ġde', 'cember', 'lic', 'ensing', 'Ġrejected', 'Ġu', 'la', 'Ġmay', 'Ġconsortium']</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>['Â°', '050', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '047', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'uly', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '008', '06', 'Ġf', 'en', 'gy', 'un', 'Ġapr', 'il', 'Ġlow', 'Ġearth', 'km', 'Â°', '055', 'Ġf', 'en', 'gy', 'un', 'Ġaug', 'ust', 'Ġsun', 'syn', 'chron', 'ous', 'km', 'Â°', 'Ġsources', 'Ġus', 'space', 'Ġn', 'asa', 'Ġw', 'mo', 'Ġcel', 'est', 'rak', 'Ġlist', 'Ġsatellites', 'Ġsee', 'Ġalso', 'Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġch', 'ina', 'Ġmeteor', 'ological', 'Ġadministration', 'Ġch', 'inese', 'Ġanti', 'atellite', 'Ġmissile', 'Ġtest', 'Ġya', 'ogan', 'Ġga', 'en', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġj', 'uly', 'ch', 'ina', 'Ġlo', 'fts', 'Ġf', 'en', 'gy', 'un', 'Ġpolar', 'Ġweather', 'Ġsatellite', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġx', 'ian', 'Ġdi', 'Ġz', 'hang', 'Ġp', 'eng', 'Ġf', 'ang', 'Ġmen', 'g', 'Ġchang', 'Ġjan', 'uary', 'Ġfirst', 'Ġf', 'en', 'gy', 'un', 'Ġsatellite', 'Ġinternational', 'Ġuser', 'Ġconference', 'http', 'Ġadvances', 'Ġatmospheric', 'Ġsciences', 'ijing', 'Ġch', 'ina', 'Ġspring', 'er', 'Ġpublishing', 'aug', 'ust', '):', 'âĢĵ', 'Ġdavid', 'Ġle', 'ard', 'Ġfe', 'b', 'ruary', 'ch', 'ina', "'s", 'Ġanti', 'atellite', 'Ġtest', 'Ġworrisome', 'Ġdebris', 'Ġcloud', 'Ġcircles', 'Ġearth', 'Ġspace', 'Ġk', 'est', 'en', 'baum', 'Ġdavid', 'Ġjan', 'uary', 'ch', 'inese', 'Ġmissile', 'Ġdestroys', 'Ġsatellite', 'mile', 'Ġorbit', 'Ġn', 'pr', 'Ġn', 'asa', 'Ġident', 'ï', '¬', 'ģ', 'es', 'Ġtop', 'Ġten', 'Ġspace', 'Ġjunk', 'Ġmissions', 'ichael', 'Ġco', 'oney', 'Ġnetwork', 'world', 'Ġj', 'uly', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', 'space', 'sk', 'yr', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'two', 'Ġorbits', 'Ġone', 'Ġmission', 'Ġsatellites', 'Ġwork', 'Ġtogether', 'Ġprovide', 'Ġcritical']</t>
+          <t>['Ġcompanies', 'Ġincluding', 'ero', 'jet', 'Ġdyn', 'etics', 'Ġsought', 'Ġlicense', 'Ġproduction', 'Ġmanufacturing', 'Ġrights', 'las', 'Ġusing', 'Ġengine', 'Ġplace', 'Ġr', 'Ġproposal', 'Ġrejected', 'Ġlaunch', 'Ġcost', 'Ġhistorically', 'Ġproposed', 'Ġversions', 'las', 'Ġlaunches', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġaug', 'ust', '05', 'Ġcc', 'af', 'Ġhot', 'Ġbird', 'Ġcommercial', 'Ġcommunications', 'Ġsatellite', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġmay', 'Ġcc', 'af', 'Ġhell', 'Ġsat', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'Ġsatellite', 'Ġg', 'ree', 'ce', 'Ġcy', 'prus', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġrainbow', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġfirst', 'las', 'Ġlaunch', 'Ġde', 'cember', '07', 'Ġcc', 'af', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġmarch', 'Ġcc', 'af', 'ars', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġmars', 'Ġorbit', 'er', 'Ġhel', 'oc', 'entric', 'oc', 'entric', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġn', 'asa', 'Ġjan', 'uary', '00', 'Ġcc', 'af', 'Ġnew', 'Ġhor', 'izons', 'Ġpl', 'uto', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġprobe', 'Ġhyper', 'b', 'olic', 'Ġsuccess', 'Ġbo', 'e', 'ing', 'Ġstar', 'Ġth', 'ir', 'Ġstage', 'Ġused', 'Ġï', '¬', 'ģ', 'r', 'st', 'la', 'Ġlaunch', 'Ġthird', 'Ġstage', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġast', 'ra', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġmarch', 'Ġ03', 'Ġcc', 'af', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġmilitary', 'Ġresearch', 'Ġsatellites', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġu', 'la', 'las', 'Ġlaunch', 'Ġfirst', 'las', 'Ġn', 'igh', 'Ġlaunch', 'Ġfirst', 'Ġthree', 'burn', 'las', 'Ġmission', 'Ġorbital', 'Ġexpress', 'Ġfal', 'cons', 'Ġj', 'une', 'Ġcc', 'af', 'Ġus', 'b', 'Ġtwo', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellites', 'Ġle', 'Ġsuccess']</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -854,7 +854,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>['Ġdata', 'Ġweather', 'Ġforecasts', 'aa', 'âĢĵ', 'n', 'asa', 'Ġgoes', 'r', 'Ġj', 'une', 'Ġhill', 'ger', 'ald', 'Ġw', 'compl', 'iment', 'ing', 'Ġge', 'ost', 'ation', 'ary', 'Ġweather', 'Ġsatellites', 'Ġtopical', 'Ġtime', 'j', 'uly', 'âĢĵ', 'aug', 'ust', '):', 'âĢĵ', 'Ġvia', 'Ġcolor', 'ado', 'Ġstate', 'Ġuniversity', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', ')"', 'space', 'sk', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'atellite', 'Ġunited', 'Ġnations', 'Ġworld', 'Ġmeteor', 'ological', 'Ġorganization', 'Ġde', 'cember', 'Ġl', 'ui', '.,', 'Ġimaging', 'Ġglobal', 'Ġaur', 'oras', 'Ġspace', 'Ġlight', 'Ġscience', 'Ġapplications', 'Ġz', 'hang', 'Ġx', 'iao', 'x', 'Ġc', 'hen', 'Ġbo', 'Ġfe', 'Ġsong', 'Ġke', 'fe', 'Ġling', 'ping', 'Ġqu', 'f', 'eng', 'Ġli', 'Ġj', 'ia', 'wei', 'Ġw', 'ang', 'Ġx', 'iao', 'ong', 'Ġz', 'hang', 'Ġh', 'ong', 'ji', 'Ġw', 'ang', 'Ġha', 'f', 'eng', 'Ġh', 'Ġz', 'hen', 'wei', 'Ġsun', 'Ġli', 'ang', 'Ġz', 'hang', 'ai', 'Ġsh', 'u', 'ang', 'wide', 'ï', '¬', 'ģ', 'e', 'ld', 'Ġaur', 'oral', 'Ġim', 'ager', 'Ġonboard', 'Ġf', 'en', 'gy', 'un', 'Ġsatellite', 'Ġlight', 'Ġscience', 'Ġapplications', '):', 'h', '01', 'Ġc', 'Ġpm', 'id', 'sen', 'ator', 'Ġcl', 'inton', 'Ġquestions', 'Ġvice', 'Ġadm', 'iral', 'Ġjohn', 'cc', 'nell', 'Ġus', 'n', 'ret', 'Ġdirector', 'Ġnational', 'Ġintelligence', 'Ġlieutenant', 'Ġgeneral', 'ichael', 'ples', 'Ġus', 'Ġdirector', 'Ġdefense', 'Ġintelligence', 'Ġagency', 'Ġsenate', 'Ġarmed', 'Ġservices', 'Ġcommittee', 'Ġhearing', 'Ġworldwide', 'Ġthreats', 'http', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'htm', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ch', 'inese', 'Ġtest', 'Ġarchived', 'h', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'iss', 'Ġcrew', 'Ġtake', 'Ġescape', 'Ġcapsules', 'Ġspace', 'Ġjunk', 'Ġalert', 'Ġmarch']</t>
+          <t>['Ġfirst', 'las', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfo', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'las', 'Ġachieve', 'Ġintended', 'Ġorbit', 'Ġpayload', 'Ġcompensated', 'Ġshortfall', 'Ġn', 'ro', 'Ġdeclared', 'Ġmission', 'Ġoct', 'ober', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġvalve', 'Ġreplacement', 'Ġdelayed', 'Ġlaunch', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġde', 'cember', '05', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġmarch', '02', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġv', 'enberg', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġ', 'ico', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlock', 'heed', 'Ġmart', 'Ġcommercial', 'Ġlaunch', 'Ġservices', 'Ġlaunch', 'Ġheaviest', 'Ġpayload', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġlargest', 'sat', 'Ġworld', 'Ġtime', 'Ġlaunch', 'Ġth', 'Ġlaunch', 'Ġter', 'rest', 'ar', 'ri', 'ane', 'Ġtel', 'star', 'v', 'Ġj', 'uly', 'Ġfal', 'con', 'Ġapr', 'il', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġj', 'une', 'Ġcc', 'af', 'Ġl', 'ro', 'l', 'cross', 'Ġlunar', 'Ġexploration', 'Ġlunar', 'Ġsuccess', 'Ġfirst', 'Ġcent', 'aur', 'Ġstage', 'Ġimpact', 'Ġmoon', 'Ġse', 'pt', 'ember', 'Ġcc', 'af', 'Ġus', 'p', 'adium', 'Ġnight', 'Ġpan', 'Ġmilitary', 'sat', 'Ġsuccess', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġfragmented', 'Ġorbit', 'Ġmarch', 'Ġoct', 'ober', 'Ġv', 'af', 'b', 'Ġus', 'ms', 'p', 'Ġmilitary', 'Ġweather', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'mber', 'Ġ06', 'Ġcc', 'af', 'Ġint', 'els', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlaunch', 'Ġfe', 'b', 'ruary', 'Ġcc', 'af', 'Ġsolar', 'Ġtelescope', 'Ġg', 'Ġsuccess']</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġnews', 'Ġconcern', 'Ġch', 'ina', "'s", 'Ġmissile', 'Ġtest', 'Ġretrieved', 'Ġjan', 'uary', 'Ġarchived', 'Ġmay', 'Ġway', 'back', 'Ġmachine', 'Ġag', 'ence', 'Ġfr', 'ance', 'pres', 'se', 'jan', 'uary', 'b', 'rit', 'Ġconcerned', 'Ġch', 'inese', 'Ġsatellite', 'Ġshoot', 'Ġspaced', 'aily', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġk', 'est', 'en', 'baum', 'Ġdavid', 'jan', 'uary', 'ch', 'inese', 'Ġmissile', 'Ġdestroys', 'Ġsatellite', 'mile', 'Ġorbit', 'Ġp', 'story', 'id', 'Ġnational', 'Ġpublic', 'Ġradio', 'Ġarchived', 'web', 'arch', 'iv', 'Ġp', 'story', 'id', 'Ġoriginal', 'mber', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', 'h', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'weather', 'Ġsatellites', 'Ġnational', 'Ġweather', 'Ġservice', 'Ġh', 'anson', 'Ġde', 'rek', 'Ġper', 'onto', 'Ġj', 'ames', 'Ġh', 'ild', 'er', 'brand', 'Ġdou', 'glas', 'aa', "'s", 'Ġeyes', 'Ġfive', 'Ġdecades', 'Ġweather', 'Ġforecasting', 'Ġenvironmental', 'Ġsatellites', 'Ġfuture', 'Ġsatellites', 'Ġpromise', 'Ġmeteor', 'ologists', 'Ġsociety', '?"', 'Ġg', 'environment', 'al', 'Ġworld', 'Ġmeteor', 'ological', 'Ġorganization', 'Ġty', 'ler', 'Ġpat', 'rick', 'Ġe', 'Ġapr', 'il', 'ch', 'ina', 'Ġsays', 'Ġblast', "'t", 'Ġslow', 'Ġsatellite', 'Ġlaunch', 'ings', 'Ġnew', 'ork', 'Ġtimes', 'Ġp', 'con', 'cern', 'Ġch', 'ina', "'s", 'Ġmissile', 'Ġtest', 'Ġic', 'st', 'Ġnews', '01', 'Ġsatellite', 'Ġprogramme', 'Ġretrieved', 'Ġreferences', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġapr', 'il', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'Ġpiece', 'Ġex', 'tern', 'Ġfair', 'ing', 'Ġbreak', 'Ġimpact', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġwashed', 'Ġh', 'ilton', 'Ġhead', 'Ġisland', 'Ġaug', 'ust', '07', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ04', '03', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġmarch', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'Ġapr', 'il', 'Ġ04', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġjun', 'Ġj', 'upiter', 'Ġorbit', 'er', 'Ġhyper', 'b', 'olic', 'Ġj', 'ovic', 'entric', 'Ġsuccess', 'mber', '02', 'Ġcc', 'af', 'Ġmars', 'Ġscience', 'Ġlaboratory', 'ms', 'l', 'Ġmars', 'Ġrover', 'Ġhyper', 'b', 'olic', 'ars', 'Ġlanding', 'Ġsuccess', 'Ġfirst', 'Ġlaunch', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uation', 'Ġcent', 'aur', 'Ġentered', 'Ġorb', 'Ġaround', 'Ġfe', 'b', 'ruary', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'th', 'Ġcent', 'aur', 'Ġlaunch', 'Ġheaviest', 'Ġpayload', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġj', 'une', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'th', 'Ġe', 'el', 'v', 'Ġlaunch', 'Ġaug', 'ust', 'Ġ08', '05', 'Ġcc', 'af', 'Ġvan', 'en', 'Ġprobes', 'r', 'bsp', 'Ġvan', 'en', 'Ġbelts', 'Ġexploration', 'Ġsuccess', 'Ġse', 'pt', 'ember']</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -880,7 +880,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>['Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġartist', "'s", 'Ġimpression', 'Ġsatellite', 'Ġmanufacturer', 'Ġlock', 'heed', 'Ġmart', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġoperator', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġapplications', 'Ġmilitary', 'Ġcommunications', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġbus', '00', 'Ġlaunch', 'Ġmass', 'Ġregime', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġdesign', 'Ġlife', 'Ġyears', 'planned', 'Ġdimensions', 'Ġproduction', 'Ġstatus', 'Ġoperational', 'Ġactive', 'Ġorder', 'Ġbuilt', 'Ġlaunched', 'Ġoperational', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġconstellation', 'Ġcommunications', 'Ġsatellites', 'Ġoperated', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġused', 'Ġrelay', 'Ġsecure', 'Ġcommunications', 'Ġunited', 'Ġstates', 'Ġarmed', 'Ġforces', 'Ġb', 'rit', 'ish', 'Ġarmed', 'Ġforces', 'adian', 'Ġarmed', 'Ġforces', 'Ġnet', 'lands', 'Ġarmed', 'Ġforces', 'Ġaust', 'ral', 'ian', 'Ġdefence', 'Ġforce', 'Ġsystem', 'Ġconsists', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġfinal', 'Ġsatellite', 'Ġlaunched', 'Ġmarch', 'Ġbackward', 'Ġcompatible', 'Ġreplaces', 'Ġolder', 'Ġmil', 'star', 'Ġsystem', 'Ġoperate', 'Ġupl', 'ink', 'extremely', 'Ġhigh', 'Ġfrequency', 'Ġband', 'link', 'super', 'Ġhigh', 'Ġfrequency', 'Ġband', ').[', 'Ġsystem', 'Ġjoint', 'Ġservice', 'Ġcommunications', 'Ġsystem', 'Ġprovides', 'Ġsurviv', 'able', 'Ġglobal', 'Ġsecure', 'Ġprotected', 'Ġjam', 'resistant', 'Ġcommunications', 'Ġhigh', 'priority', 'Ġmilitary', 'Ġground', 'Ġsea', 'Ġair', 'Ġassets', 'Ġsatellites', 'Ġuse', 'Ġmany', 'Ġnarrow', 'Ġspot', 'Ġbeams', 'Ġdirected', 'Ġtowards', 'Ġearth', 'Ġrelay', 'Ġcommunications', 'Ġusers', 'Ġcross', 'links', 'Ġsatellites', 'Ġallow', 'Ġrelay', 'Ġcommunications', 'Ġdirectly', 'Ġrather', 'Ġvia', 'Ġground', 'Ġstation', 'Ġsatellites', 'Ġdesigned', 'Ġprovide', 'Ġjam', 'resistant', 'Ġcommunications', 'Ġlow', 'Ġprobability', 'Ġinterception', 'Ġincorporate', 'Ġfrequency', 'ho', 'pping', 'Ġradio', 'Ġtechnology', 'Ġwell', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġadapt', 'Ġradiation', 'Ġpatterns', 'Ġorder', 'Ġblock', 'Ġpotential', 'Ġsources', 'Ġjam', 'ming', 'Ġincorporates', 'Ġexisting', 'Ġmil', 'star', 'Ġlow', 'Ġdata', 'rate', 'Ġmedium', 'Ġdata', 'rate', 'Ġsignals', 'Ġproviding', 'âĢĵ', '00', 'Ġbit', 'Ġk', 'bit', 'âĢĵ', 'bit', 'Ġrespectively', 'Ġalso', 'Ġincorporates', 'Ġnew', 'Ġsignal', 'Ġallowing', 'Ġdata', 'Ġrates', 'bit', 'Ġcomplete', 'Ġspace', 'Ġsegment', 'Ġsystem', 'Ġconsist', 'Ġsatellites', 'Ġprovides', 'Ġcoverage', 'Ġsurface', 'Ġearth', 'Ġlat', 'itudes', 'Â°', 'Ġnorth', 'Â°', 'Ġsouth', 'Ġnorthern', 'Ġpolar', 'Ġregions']</t>
+          <t>['Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellites', 'Ġle', 'Ġsuccess', 'Ġde', 'cember', '03', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġjan', 'uary', 'Ġ01', 'Ġcc', 'af', 'Ġtd', 'rs', 'k', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġfe', 'b', 'ruary', '02', 'Ġv', 'af', 'b', 'Ġlands', 'Ġearth', 'Ġobservation', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġwest', 'Ġcoast', 'la', 'Ġlaunch', 'Ġn', 'asa', 'Ġmarch', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġgeo', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġfirst', 'Ġsatellite', 'Ġlaunched', 'las', 'Ġj', 'uly', '00', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ08', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'mber', 'Ġcc', 'af', 'aven', 'Ġmars', 'Ġorbit', 'er', 'Ġhyper', 'b', 'olic', 'oc', 'entric', 'Ġsuccess', 'Ġde', 'cember', 'Ġ07', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsuccess', 'Ġjan', 'uary', 'Ġ02', 'Ġcc', 'af', 'Ġtd', 'rs', 'l', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġapr', 'il', 'Ġv', 'af', 'b', 'Ġus', 'Ġmilitary', 'Ġweather', 'Ġsatellite', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsuccess', 'th', 'Ġr', 'Ġlaunch', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmay', '09', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġaug', 'ust', 'Ġ03']</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>['Ġenhanced', 'Ġpolar', 'Ġsystem', 'Ġacts', 'Ġadjunct', 'Ġprovide', 'Ġcoverage', 'Ġinitial', 'Ġcontract', 'Ġdesign', 'Ġdevelopment', 'Ġsatellites', 'Ġawarded', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'Ġsystems', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġtechnology', 'mber', 'Ġcovered', 'Ġsystem', 'Ġdevelopment', 'Ġdemonstration', 'Ġphase', 'Ġprogram', 'Ġcontract', 'Ġcovered', 'Ġoverview', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġmaiden', 'Ġlaunch', 'Ġaug', 'ust', 'usa', 'Ġlast', 'Ġlaunch', 'Ġmarch', 'usa', 'Ġconstruction', 'Ġlaunch', 'Ġthree', 'Ġsatellites', 'Ġconstruction', 'Ġmission', 'Ġcontrol', 'Ġsegment', 'Ġcontract', 'Ġmanaged', 'Ġmil', 'sat', 'Ġprogram', 'Ġoffice', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'Ġlike', 'Ġmil', 'star', 'Ġsystem', 'Ġoperated', 'th', 'Ġspace', 'Ġoperations', 'Ġsquadron', 'Ġlocated', 'Ġsch', 'ri', 'ever', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġextends', 'cross', 'links', 'Ġamong', 'Ġearlier', 'Ġmil', 'star', 'Ġsatellites', 'Ġmakes', 'Ġmuch', 'Ġless', 'Ġvulnerable', 'Ġattacks', 'Ġground', 'Ġstations', 'Ġge', 'os', 'ynchronous', 'Ġsatellite', 'Ġequ', 'ator', 'Ġstill', 'Ġneeds', 'Ġsupplemented', 'Ġadditional', 'Ġsystems', 'Ġoptimized', 'Ġpolar', 'Ġcoverage', 'Ġhigh', 'Ġlat', 'itudes', 'Ġapr', 'il', 'Ġdefense', 'Ġdepartment', 'Ġbudget', 'Ġrequest', 'Ġsecretary', 'Ġdefense', 'Ġro', 'bert', 'Ġgates', 'Ġsaid', 'Ġplanned', 'Ġcancel', 'Ġtransform', 'ational', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'Ġstill', 'Ġdesign', 'Ġphase', 'Ġfavor', 'Ġadditional', 'Ġcapacity', 'Ġindividual', 'Ġsatellites', 'Ġexclusive', 'Ġlaunch', 'Ġexpenses', 'Ġcost', 'Ġmillion', 'Ġprior', 'Ġunited', 'Ġstates', 'Ġallied', 'Ġmilitary', 'Ġsatellite', 'Ġcommunications', 'Ġsystems', 'Ġfell', 'Ġone', 'Ġthree', 'Ġcategories', ':[', 'Ġwide', 'band', 'Ġmaximum', 'Ġbandwidth', 'Ġamong', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġsemi', 'ï', '¬', 'ģ', 'x', 'ed', 'Ġearth', 'Ġstations', 'Ġprotected', 'Ġsurviv', 'able', 'Ġelectronic', 'Ġwarfare', 'Ġattacks', 'Ġeven', 'Ġbandwidth', 'Ġsac', 'ri', 'ï', '¬', 'ģ', 'ced', 'Ġnarrow', 'band', 'Ġprincipally', 'Ġtactical', 'Ġuse', 'Ġsac', 'ri', 'ï', '¬', 'ģ', 'cing', 'Ġbandwidth', 'Ġsimplicity', 'Ġreliability', 'Ġlight', 'Ġweight', 'Ġterrestrial', 'Ġequipment', 'Ġhowever', 'Ġconver', 'ges', 'Ġrole', 'Ġwide', 'band', 'Ġdefense', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'sc', 'Ġprotected', 'Ġmil', 'star', 'Ġpredecessors', 'Ġincreasing', 'Ġbandwidth', 'Ġstill', 'Ġneed', 'Ġspecialized', 'Ġsatellite', 'Ġcommunications', 'Ġextremely', 'Ġhigh', 'Ġdata', 'Ġrate', 'Ġspace', 'Ġsensors', 'Ġge', 'osp', 'atial', 'Ġsignals', 'Ġintelligence', 'Ġsatellites', 'linked', 'Ġdata', 'Ġtypically', 'Ġgo', 'Ġspecialized', 'Ġreceiver', 'Ġprocessed', 'Ġsmaller', 'Ġamounts', 'Ġprocessed', 'Ġdata', 'Ġflow', 'Ġsatellites', 'Ġsent', 'Ġspace', 'Ġusing', 'Ġevolved']</t>
+          <t>['Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġaug', 'ust', 'Ġv', 'af', 'b', 'Ġworldview', 'Ġearth', 'Ġimaging', 'Ġsatellite', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'cl', 'io', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġfragmented', 'Ġaug', 'ust', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġoct', 'ober', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'th', 'las', 'Ġlaunch', 'Ġde', 'cember', 'Ġ03', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġfirst', 'Ġuse', 'Ġengine', 'Ġcent', 'aur', 'Ġstage', 'Ġjan', 'uary', 'Ġ01', '04', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġmarch', 'Ġ02', 'Ġcc', 'af', 'ms', 'Ġmagnet', 'osphere', 'Ġresearch', 'Ġsatellites', 'Ġsuccess', 'Ġmay', '05', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġoct', 'ober', 'Ġcc', 'af', 'los', 'sat', 'Ġg', 'Ġsuccess', 'Ġoct', 'ober', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellites', 'Ġle', 'Ġsuccess', 'Ġoct', 'ober', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġcy', 'gn', 'us', 'Ġcr', 'Ġiss', 'Ġlogistics', 'Ġspacecraft', 'Ġle', 'Ġsuccess', 'Ġfirst', 'las', 'Ġrocket', 'Ġuse', 'Ġdirectly', 'Ġsupport', 'Ġth', 'Ġiss', 'Ġprogram', 'Ġfe']</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>['Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'e', 'el', 'v', 'Ġpayload', 'Ġweight', 'Ġlaunch', 'Ġapproximately', '000', '000', 'Ġtime', 'Ġexp', 'ends', 'Ġpropell', 'ants', 'Ġachieve', 'Ġproper', 'Ġorbit', 'Ġweight', 'Ġapproximately', 'Ġsatellites', 'Ġoperate', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'ge', 'Ġorbit', 'Ġtakes', 'Ġdays', 'Ġorbital', 'Ġadjustments', 'Ġreach', 'Ġstable', 'Ġgeo', 'position', 'Ġlaunch', 'Ġupl', 'inks', 'Ġcross', 'links', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'links', 'Ġuse', 'Ġsuper', 'Ġhigh', 'Ġfrequency', 'Ġvariety', 'Ġfrequencies', 'Ġused', 'Ġwell', 'Ġdesire', 'Ġtightly', 'Ġfocused', 'links', 'Ġsecurity', 'Ġrequire', 'Ġrange', 'Ġantennas', 'Ġseen', 'Ġpicture', 'link', 'Ġphased', 'Ġarrays', 'Ġcross', 'links', 'Ġupl', 'ink', 'link', 'Ġnull', 'ing', 'Ġantennas', 'Ġbands', 'Ġlaunch', 'Ġpositioning', 'Ġelectronics', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġupl', 'ink', 'Ġphased', 'Ġarray', 'Ġupl', 'ink', 'link', 'Ġg', 'imb', 'aled', 'Ġdish', 'Ġantenna', 'Ġupl', 'ink', 'link', 'Ġearth', 'Ġcoverage', 'Ġhorns', 'Ġphased', 'Ġarray', 'Ġtechnology', 'Ġnew', 'Ġcommunications', 'Ġsatellites', 'Ġincreases', 'Ġreliability', 'Ġremoving', 'Ġmechanical', 'Ġmovement', 'Ġrequired', 'Ġg', 'imb', 'aled', 'Ġmotor', 'driven', 'Ġantennas', 'Ġlow', 'Ġgain', 'Ġearth', 'Ġcoverage', 'Ġantennas', 'Ġsend', 'Ġinformation', 'Ġanywhere', 'Ġthird', 'Ġearth', 'Ġcovered', 'Ġsatellite', "'s", 'Ġfootprint', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġprovide', 'Ġsuper', 'Ġhigh', 'gain', 'Ġearth', 'Ġcover', 'ages', 'Ġenabling', 'Ġworldwide', 'Ġunsc', 'hed', 'uled', 'Ġaccess', 'Ġusers', 'Ġincluding', 'Ġsmall', 'Ġportable', 'Ġterminals', 'Ġsubmarines', 'Ġmedium', 'Ġresolution', 'Ġcoverage', 'Ġantennas', 'rc', 'Ġhighly', 'Ġdirectional', 'spot', 'Ġcoverage', 'Ġtime', 'shared', 'Ġcover', 'Ġtargets', 'Ġtwo', 'Ġhigh', 'resolution', 'Ġcoverage', 'Ġarea', 'Ġantennas', 'Ġenable', 'Ġoperations', 'Ġpresence', 'beam', 'Ġjam', 'ming', 'Ġnull', 'ing', 'Ġantennas', 'Ġpart', 'Ġelectronic', 'Ġdefense', 'Ġhelps', 'Ġdiscriminate', 'Ġtrue', 'Ġsignals', 'Ġelectronic', 'Ġattack', 'Ġanother', 'Ġchange', 'Ġexisting', 'Ġsatellites', 'Ġusing', 'Ġsolid', 'state', 'Ġtransmit', 'ters', 'Ġrather', 'Ġtraveling', 'Ġwave', 'Ġtubes', 'Ġused', 'Ġhigh', 'power', 'Ġmilitary', 'Ġapplications', 'Ġtw', 'ts', 'Ġfixed', 'Ġpower', 'Ġoutput', 'Ġnewer', 'Ġdevices', 'Ġallow', 'Ġvarying', 'Ġtransmitted', 'Ġpower', 'Ġlowering', 'Ġprobability', 'Ġintercept', 'Ġoverall', 'Ġpower', 'Ġefficiency', 'Ġpayload', 'Ġflight', 'Ġsoftware', 'Ġcontains', 'Ġapproximately', '000', 'Ġlines', 'Ġreal', 'time', 'Ġdistributed', 'Ġembedded', 'Ġcode', 'Ġexecuting', 'Ġsimultaneously', 'board', 'Ġprocessors', 'Ġprovides', 'Ġindividual', 'Ġdigital', 'Ġdata', 'Ġstreams', 'Ġrates', 'Ġbits', 'second', 'Ġmeg', 'ab', 'second', 'Ġinclude']</t>
+          <t>['b', 'ruary', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġmarch', 'Ġ03', '05', 'Ġcc', 'af', 'Ġcy', 'gn', 'us', 'Ġcr', 'Ġiss', 'Ġlogistics', 'Ġspacecraft', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġstage', 'Ġshut', 'Ġdow', 'Ġearly', 'Ġaff', 'e', 'Ġmission', 'Ġoutcome', 'Ġj', 'une', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', '05', 'Ġcc', 'af', 'Ġos', 'iris', 'rex', 'Ġasteroid', 'Ġsample', 'Ġreturn', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'mber', 'Ġv', 'af', 'b', 'Ġworldview', 'Ġn', 'ro', 'Ġcubes', 'ats', 'Ġearth', 'Ġimaging', 'Ġcubes', 'ats', 'Ġsuccess', 'Ġlaunch', 'mber', 'Ġcc', 'af', 'Ġgoes', 'r', 'go', 'es', 'Ġmeteor', 'ology', 'Ġg', 'Ġsuccess', 'th', 'Ġe', 'el', 'v', 'Ġlaunch', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġe', 'ch', 'ost', 'ar', 'j', 'upiter', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlaunch', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġjan', 'uary', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmarch', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġcy', 'gn', 'us', 'Ġcr', 'Ġiss', 'Ġlogistics', 'Ġspacecraft', 'Ġle', 'Ġsuccess', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġtd', 'rs', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ05', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġoct', 'ober', 'Ġ07', 'Ġcc', 'af', 'Ġus']</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -919,7 +919,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>['Ġgo', 'Ġbeyond', 'Ġmil', 'star', "'s", 'Ġlow', 'Ġdata', 'Ġrate', 'ld', 'r', 'Ġmedium', 'Ġdata', 'Ġrate', 'Ġwell', 'Ġactually', 'Ġfairly', 'Ġslow', 'Ġhigh', 'Ġdata', 'Ġrate', 'Ġsubmarines', 'Ġfaster', 'Ġlinks', 'Ġdesignated', 'Ġextended', 'Ġdata', 'Ġrates', 'Ġnumber', 'Ġground', 'Ġterminals', 'Ġairborne', 'Ġterminal', 'Ġpart', 'Ġfamily', 'Ġadvanced', 'Ġbeyond', 'fab', 'Ġproject', 'Ġground', 'Ġstations', 'Ġinclude', 'Ġsingle', 'channel', 'Ġant', 'ij', 'Ġman', 'port', 'able', 'Ġterminal', 'sc', 'amp', 'Ġsecure', 'Ġmobile', 'Ġanti', 'jam', 'Ġreliable', 'Ġtactical', 'Ġterminal', 'smart', 'Ġsubmarine', 'Ġhigh', 'Ġdata', 'Ġrate', 'sub', 'Ġsystem', 'Ġbo', 'e', 'ing', 'Ġprime', 'Ġcontractor', 'Ġcommunications', 'Ġrock', 'well', 'Ġmajor', 'Ġsubcontract', 'ors', 'Ġfirst', 'Ġfab', 'incre', 'ment', 'Ġdelivered', 'Ġuse', 'Ġspirit', 'Ġaircraft', 'Ġfe', 'b', 'ruary', 'Ġplanned', 'Ġaircraft', 'Ġincluding', 'Ġaircraft', 'Ġinstallations', 'Ġgo', 'Ġfixed', 'Ġtransport', 'able', 'Ġcommand', 'Ġposts', 'Ġsuccessfully', 'Ġinter', 'operated', 'Ġlegacy', 'Ġcommunications', 'Ġusing', 'Ġcommand', 'Ġpost', 'Ġterminal', 'Ġarmy', 'Ġsingle', 'Ġchannel', 'Ġanti', 'jam', 'Ġman', 'Ġportable', 'Ġterminal', 'Ġfirst', 'Ġsatellite', 'Ġus', 'Ġsuccessfully', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġaug', 'ust', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġoccurred', 'Ġfour', 'Ġyears', 'Ġbehind', 'Ġschedule', 'Ġcontract', 'Ġawarded', 'Ġfirst', 'Ġlaunch', 'Ġexpected', 'Ġservices', 'Ġsatellites', 'usa', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġtaken', 'Ġplace', 'Ġprogram', 'Ġrestruct', 'ured', 'Ġoct', 'ober', 'Ġnational', 'Ġsecurity', 'Ġagency', 'ns', 'Ġdeliver', 'Ġkey', 'Ġcryptographic', 'Ġequipment', 'Ġpayload', 'Ġcontractor', 'Ġtime', 'Ġmeet', 'Ġlaunch', 'Ġschedule', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġsuccessfully', 'Ġplaced', 'Ġsatellite', 'Ġtransfer', 'Ġorbit', 'Ġper', 'ig', 'ee', 'Ġap', 'gee', '000', 'Ġinclination', 'Â°', 'Ġsatellite', 'Ġvehicle', "'s", 'Ġliquid', 'Ġap', 'gee', 'Ġengine', 'Ġprovided', 'Ġfailed', 'Ġraise', 'Ġorbit', 'Ġtwo', 'Ġattempts', 'Ġsolve', 'Ġproblem', 'Ġper', 'ig', 'ee', 'Ġaltitude', 'Ġraised', '00', 'Ġtwelve', 'Ġfir', 'ings', 'Ġsmaller', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'provided', 'Ġreaction', 'Ġengine', 'Ġassembly', 'Ġthr', 'usters', 'Ġoriginally', 'Ġintended', 'Ġattitude', 'Ġcontrol', 'Ġengine', 'Ġburns', 'Ġaltitude', 'Ġsolar', 'Ġpanels']</t>
+          <t>['Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġjan', 'uary', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmarch', '02', 'Ġcc', 'af', 'Ġgoes', 'go', 'es', 'Ġmeteor', 'ology', 'Ġg', 'Ġsuccess', 'Ġexpended', 'th', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġgeo', 'Ġsuccess', 'Ġmay', '05', 'Ġv', 'af', 'b', 'Ġinsight', 'Ġmar', 'co', 'Ġmars', 'Ġland', 'er', 'Ġcubes', 'ats', 'Ġhyper', 'b', 'olic', 'ars', 'Ġlanding', 'Ġsuccess', 'Ġfirst', 'Ġinter', 'plan', 'etary', 'Ġmission', 'Ġv', 'af', 'b', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġinter', 'plan', 'etary', 'Ġcubes', 'ats', 'Ġoct', 'ober', 'Ġ04', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'th', 'Ġcent', 'aur', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġfragmented', 'Ġorbit', 'Ġapr', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġstar', 'liner', 'Ġbo', 'e', 'ing', 'Ġoft', 'Ġunc', 'rew', 'ed', 'Ġorbital', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġle', 'iss', 'Ġsuccess', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġdual', 'engine', 'Ġcent', 'aur', 'las', 'Ġv', 'Ġfirst', 'Ġorbital', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġstar', 'liner', 'Ġplanned', 'Ġvisit', 'Ġiss', 'Ġanomaly', 'Ġstar', 'liner', 'Ġvehicle', 'Ġleft', 'Ġspacecraft', 'Ġlow', 'Ġorbit', 'las', 'Ġrock', 'Ġperformed', 'Ġexpected', 'Ġthus', 'Ġth', 'Ġmission', 'Ġlisted', 'Ġsuccessful', 'Ġfe', 'b', 'ruary', 'Ġ04', '03', 'Ġcc', 'af', 'Ġsolar', 'Ġorbit', 'er', 'Ġsolar', 'Ġhel', 'oph', 'ysics', 'Ġorbit', 'er', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'Ġlast', 'Ġflight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġmarch', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'Ġever', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġth', 'Ġu']</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -932,7 +932,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>['Ġdeployed', 'Ġorbit', 'Ġraised', 'Ġtoward', 'Ġoperational', 'Ġorbit', 'Ġcourse', 'Ġnine', 'Ġmonths', 'Ġusing', 'Ġnew', 'ton', 'Ġhall', 'Ġthr', 'usters', 'Ġalso', 'Ġprovided', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġform', 'Ġelectric', 'Ġpropulsion', 'Ġhighly', 'Ġefficient', 'Ġlow', 'Ġthrust', 'Ġtook', 'Ġmuch', 'Ġlonger', 'Ġinitially', 'Ġintended', 'Ġdue', 'Ġlower', 'Ġstarting', 'Ġaltitude', 'Ġmaneuvers', 'Ġled', 'Ġprogram', 'Ġdelays', 'Ġsecond', 'Ġthird', 'Ġsatellite', 'Ġvehicle', 'Ġla', 'es', 'Ġanalyzed', 'Ġgovernment', 'Ġaccountability', 'Ġoffice', 'Ġreport', 'Ġreleased', 'Ġj', 'uly', 'Ġstated', 'Ġblocked', 'Ġfuel', 'Ġline', 'Ġliquid', 'Ġap', 'gee', 'Ġengine', 'Ġlikely', 'Ġcaused', 'Ġpiece', 'Ġcloth', 'Ġinadvertently', 'Ġleft', 'Ġline', 'Ġmanufacturing', 'Ġprocess', 'Ġbelieved', 'Ġprimary', 'Ġcause', 'Ġfailure', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġselected', 'Ġacquisition', 'Ġreport', 'Ġadds', 'Ġfuel', 'Ġloading', 'Ġprocedures', 'Ġun', 'met', 'Ġthermal', 'Ġcontrol', 'Ġrequirements', 'Ġcould', 'Ġalso', 'Ġcontributed', 'Ġremaining', 'Ġsatellites', 'Ġdeclared', 'Ġflight', 'ready', 'Ġmonth', 'Ġprior', 'Ġrelease', 'Ġreport', 'Ġlike', 'Ġfirst', 'Ġsatellite', 'Ġsecond', 'Ġlaunched', 'las', 'Ġflying', 'Ġconfiguration', 'Ġlaunch', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġtook', 'Ġplace', 'Ġmay', 'Ġthree', 'Ġmonths', 'Ġmaneuver', 'ing', 'Ġreached', 'Ġproper', 'Ġposition', 'Ġtesting', 'Ġprocedures', 'Ġstarted', 'Ġcompletion', 'Ġcheckout', 'Ġannounced', 'mber', 'Ġcontrol', 'Ġturned', 'th', 'Ġair', 'Ġforce', 'Ġoperations', 'Ġexpected', 'year', 'Ġservice', 'Ġlife', 'Ġthird', 'Ġsatellite', 'Ġlaunched', 'Ġcape', 'aver', 'al', 'Ġse', 'pt', 'ember', 'Ġ08', 'Ġtwo', 'hour', 'Ġwindow', 'Ġlaunch', 'Ġsatellite', 'Ġopened', 'Ġ07', '04', 'Ġut', 'c', 'Ġlaunch', 'Ġoccurred', 'Ġsoon', 'Ġweather', 'related', 'Ġclouds', 'Ġhigh', 'alt', 'itude', 'Ġwinds', 'Ġcleared', 'Ġsufficiently', 'Ġmeet', 'Ġlaunch', 'Ġcriteria', 'Ġsuccessful', 'Ġlaunch', 'Ġfailure', 'Ġkick', 'Ġmotor', 'Ġrecovery', 'Ġusing', 'Ġhall', 'effect', 'Ġthr', 'usters', 'usa', 'usa', 'usa', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġfourth', 'Ġsatellite', 'Ġlaunched', 'Ġoct', 'ober', 'Ġcape', 'aver', 'al', 'Ġ04', 'Ġut', 'c', 'Ġusing', 'las', 'Ġrocket', 'Ġoperated', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', ').[', 'Ġfifth', 'Ġsatellite']</t>
+          <t>['Ġspace', 'Ġforce', 'th', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġengine', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'Ġfal', 'cons', '))', 'Ġmilitary', 'Ġspace', 'plane', 'Ġus', 'afa', 'Ġsat', 'Ġle', 'Ġsuccess', 'Ġsixth', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'cons', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġmars', 'Ġmars', 'Ġrover', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'Ġlaunch', 'Ġpersever', 'ance', 'Ġrover', 'mber', 'Ġcc', 'af', 'Ġus', 'n', 'rol', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġusage', 'Ġnew', 'Ġgem', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'ge', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġfirst', 'Ġusage', 'Ġupper', 'Ġstage', 'Ġengine', 'Ġmission', 'Ġsuccessful', 'Ġunexpected', 'Ġvibration', 'Ġobserved', 'Ġnew', 'Ġengine', 'Ġuse', 'Ġengine', 'Ġvariant', 'Ġhold', 'Ġpending', 'Ġbetter', 'Ġunderstanding', 'Ġse', 'pt', 'ember', 'Ġlands', 'Ġearth', 'Ġobservation', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġoct', 'ober', 'Ġ09', 'Ġcc', 'af', 'Ġl', 'u', 'cy', 'Ġspace', 'Ġprobe', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġtechnology', 'Ġdemonstration', 'Ġgeo', 'Ġsuccess', 'Ġlongest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġever', 'las', 'Ġrocket', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġjan', 'uary', '00', 'g', 'ss', 'ap', 'Ġspace', 'Ġsurveillance', 'Ġgeo', 'Ġsuccess', 'Ġfirst', 'Ġplan', 'ne', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġmarch', 'Ġgoes', 'Ġmeteor', 'ology', 'Ġgeo', 'Ġsuccess', 'Ġmay', 'Ġbo', 'e', 'Ġunc', 'rew', 'ed', 'Ġorbital', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġle', 'iss', 'Ġsuccess', 'Ġj', 'uly', 'Ġus', 'sf', 'w', 'f', 'ov', 'Ġearly', 'Ġwarning', 'Ġgeo', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ']</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -945,7 +945,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>['Ġlaunched', 'Ġaug', 'ust', 'Ġcape', 'aver', 'al', 'Ġut', 'c', 'Ġusing', 'las', 'Ġrocket', 'Ġsecondary', 'Ġpayload', 'Ġnamed', 'Ġaccompanied', 'Ġsatellite', 'Ġorbit', 'Ġsixth', 'Ġsatellite', 'Ġlaunched', 'Ġmarch', 'Ġut', 'c', 'las', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġfirst', 'Ġlaunch', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmission', 'Ġsince', 'Ġestablishment', 'Ġnew', 'Ġmilitary', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'Ġsystem', 'Ġachieves', 'Ġinitial', 'Ġoperational', 'Ġcapability', 'Ġlos', 'Ġangel', 'es', 'Ġair', 'Ġforce', 'Ġbase', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'two', 'Ġu', 'Ġmilitary', 'Ġsatellite', 'Ġlaunches', 'Ġdelayed', 'Ġnext', 'Ġyear', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġretrieved', 'Ġjan', 'uary', 'Ġready', 'Ġlaunch', 'Ġlos', 'Ġangel', 'es', 'Ġair', 'Ġforce', 'Ġbase', 'Ġretrieved', 'Ġaug', 'ust', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġretrieved', 'Ġj', 'une', 'adv', 'anced', 'Ġpayload', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġarchived', 'Ġoriginal', 'ht', 'Ġmarch', 'Ġretrieved', 'mber', 'Ġwhite', 'rew', 'us', 'mc', 'Ġeyes', 'Ġimproved', 'Ġar', 'ctic', 'Ġcommunications', 'Ġsystems', 'Ġprocedures', 'Ġj', 'ane', "'s", 'Ġinformation', 'Ġgroup', 'Ġcapt', 'Ġhill', 'Ġwarned', 'Ġus', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', "'s", 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġsat', 'Ġconstellation', 'Ġineffective', 'th', 'Ġparallel', 'Ġnorth', 'Ġ[...]', 'lock', 'heed', 'Ġmart', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'enh', 'anced', 'Ġpolar', 'Ġsystem', 'usa', 'usa', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġlore', 'ike', 'jan', 'uary', 'extreme', 'Ġcost', 'Ġgrowth', 'Ġthemes', 'Ġus', 'Ġair', 'Ġforce', 'Ġmajor', 'Ġdefense', 'Ġacquisition', 'Ġprograms', 'Ġresearch', 'Ġgate', 'Ġretrieved', 'Ġapr', 'il', 'Ġelf', 'ers', 'Ġg', 'Ġmill', 'er', 'winter', 'future', 'Ġu', 'Ġmilitary', 'Ġsatellite', 'Ġcommunication', 'Ġsystems', 'Ġaerospace', 'Ġcorporation', 'Ġcross', 'link', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġaug', 'ust', 'ag', 'ile', 'Ġantennas', 'Ġaid', 'Ġwarriors', 'Ġaf', 'ce', 'Ġsignal', 'Ġj', 'uly']</t>
+          <t>['g', 'uration', 'th', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġengine', 'Ġaug', 'ust', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġgeo', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġoct', 'ober', 'es', 'es', 'Ġcommunication', 'Ġsatellites', 'Ġgeo', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'mber', 'Ġ09', 'Ġloft', 'id', 'Ġenvironmental', 'Ġsatellites', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġlas', 'las', 'Ġlaunch', 'Ġfinal', 'Ġï', '¬', 'Ĥ', 'ight', 'las', 'meter', 'Ġfair', 'ing', 'th', 'Ġuse', 'Ġsingle', 'Ġengine', 'Ġcent', 'aur', 'Ġu', 'la', 'Ġstopped', 'Ġselling', 'las', 'Ġv', 'Ġfly', 'Ġlaunches', 'Ġplanned', 'Ġlaunches', 'Ġsee', 'Ġlist', 'las', 'Ġlaunches', 'âĢĵ', 'Ġfirst', 'Ġpayload', 'Ġhot', 'Ġbird', 'Ġcommunications', 'Ġsatellite', 'Ġlaunched', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġaug', 'ust', 'las', 'Ġaug', 'ust', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġlaunched', 'Ġaboard', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġlaunch', 'Ġvehicle', 'Ġcompleted', 'Ġburns', 'minute', 'Ġperiod', 'Ġplaced', 'Ġinter', 'plan', 'etary', 'Ġtransfer', 'Ġorbit', 'Ġtowards', 'Ġmars', 'Ġjan', 'uary', 'Ġnew', 'Ġhor', 'izons', 'Ġlaunched', 'Ġlock', 'heed', 'Ġmart', 'las', 'Ġrocket', 'Ġthird', 'Ġstage', 'Ġadded', 'Ġincrease', 'Ġhel', 'oc', 'entric', 'escape', 'Ġspeed', 'Ġfirst', 'Ġlaunch', 'las', 'Ġconfiguration', 'Ġfive', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġfirst', 'las', 'Ġthird', 'Ġstage', 'Ġde', 'cember', 'las', 'Ġlifted', 'Ġheaviest', 'Ġpayload', 'Ġdate', 'Ġorbit', 'Ġcy', 'gn', 'us', 'Ġres', 'upp', 'ly', 'Ġcraft', 'Ġse', 'pt', 'ember', 'Ġos', 'iris', 'rex', 'Ġasteroid', 'Ġsample', 'Ġreturn', 'Ġmission', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġarrived', 'Ġasteroid', 'Ġb', 'enn', 'u', 'Ġde', 'cember', 'Ġdeparted', 'Ġback', 'Ġearth', 'Ġmay', 'Ġarrive', 'Ġse', 'pt', 'ember', 'Ġsample', 'Ġranging', 'Ġgrams', 'Ġkilograms']</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -958,7 +958,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>['north', 'rop', 'Ġgr', 'um', 'man', 'Ġqual', 'ï', '¬', 'ģ', 'es', 'Ġextended', 'Ġdata', 'Ġrate', 'Ġsoftware', 'Ġadvanced', 'Ġmilitary', 'Ġcommunications', 'Ġsatellite', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġtechnology', 'mber', 'Ġarchived', 'Ġoriginal', 'es', 'html', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġbomber', 'Ġreceives', 'Ġfirst', 'Ġfab', 'Ġsatellite', 'Ġcommunication', 'Ġterminal', 'Ġde', 'ag', 'el', 'Ġfe', 'b', 'ruary', 'Ġro', 'bert', 'ud', 'ney', 'oct', 'ober', 'game', 'Ġchang', 'ers', 'Ġspace', 'Ġair', 'Ġforce', 'Ġmagazine', 'Ġretrieved', 'Ġapr', 'il', 'Ġdefense', 'Ġacquisitions', 'Ġassessments', 'Ġselected', 'Ġweapon', 'Ġprograms', 'web', 'ar', 'Ġunited', 'Ġstates', 'Ġgovernment', 'Ġaccountability', 'ï', '¬', 'ģ', 'ce', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġray', 'Ġspace', 'flight', 'Ġair', 'Ġforce', 'Ġsatellite', "'s", 'Ġepic', 'Ġascent', 'Ġï', '¬', 'ģ', 'n', 'ish', 'Ġsoon', 'http', 'space', 'ï', '¬', 'Ĥ', 'Ġoct', 'ober', 'access', 'ed', 'Ġde', 'cember', 'main', 'Ġengine', 'Ġprobably', 'Ġblame', 'Ġtrouble', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġray', 'Ġoct', 'ober', 'air', 'Ġforce', 'Ġsatellite', "'s", 'Ġepic', 'Ġascent', 'Ġï', '¬', 'ģ', 'n', 'ish', 'Ġsoon', 'space', 'ï', '¬', 'Ĥ', 'ig', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'dep', 'artment', 'Ġdefense', 'Ġselected', 'Ġacquisition', 'Ġreport', 'Ġde', 'cember', 'web', 'arch', 'es', 'wh', 'mil', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'air', 'Ġforce', 'Ġrec', 'ou', 'ps', 'Ġcosts', 'Ġsave', 'Ġstranded', 'Ġsatellite', 'http', 'Ġretrieved', 'Ġj', 'une', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġmission', 'Ġstatus', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġmission', 'Ġstatus', 'Ġcenter', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'mber', 'Ġadvanced']</t>
+          <t>['Ġfirst', 'Ġfour', 'Ġbo', 'e', 'ing', 'Ġspace', 'plane', 'Ġmissions', 'Ġsuccessfully', 'Ġlaunched', 'las', 'Ġv', 'Ġalso', 'Ġknown', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġreusable', 'Ġrobotic', 'Ġspacecraft', 'Ġoperated', 'Ġus', 'af', 'Ġautonom', 'ously', 'Ġconduct', 'Ġland', 'ings', 'Ġorbit', 'Ġrunway', 'Ġflights', 'Ġlaunched', 'las', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'Ġfirst', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġlanding', 'Ġspace', 'Ġshuttle', '000', 'Ġft', 'Ġrunway', 'Ġoccurred', 'Ġde', 'cember', 'Ġland', 'ings', 'Ġoccur', 'Ġv', 'enberg', 'Ġcape', 'aver', 'al', 'Ġdepending', 'Ġmission', 'Ġrequirements', 'Ġnotable', 'Ġmissions', 'las', 'Ġwik', 'ipedia', 'Ġde', 'cember', 'Ġfirst', 'Ġstar', 'liner', 'Ġcrew', 'Ġcapsule', 'Ġlaunched', 'Ġbo', 'e', 'oft', 'Ġun', 'crew', 'ed', 'Ġtest', 'Ġflight', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġperformed', 'Ġflaw', 'lessly', 'Ġanomaly', 'Ġspacecraft', 'Ġleft', 'Ġwrong', 'Ġorbit', 'Ġorbit', 'Ġlow', 'Ġreach', 'Ġflight', "'s", 'Ġdestination', 'Ġiss', 'Ġmission', 'Ġsubsequently', 'Ġcut', 'Ġshort', 'Ġlaunches', 'Ġj', 'uly', 'Ġstarting', 'Ġfirst', 'Ġlaunch', 'Ġaug', 'ust', 'las', 'Ġachieved', 'Ġmission', 'Ġsuccess', 'Ġrate', 'Ġvehicle', 'Ġsuccess', 'Ġrate', 'Ġcontrast', 'Ġindustry', 'Ġsuccess', 'Ġrate', 'âĢĵ', 'Ġfirst', 'Ġanomal', 'ous', 'Ġevent', 'Ġuse', 'las', 'Ġlaunch', 'Ġsystem', 'Ġoccurred', 'Ġj', 'une', 'Ġengine', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'las', 'Ġshut', 'Ġearly', 'Ġleaving', 'Ġpayload', 'Ġpair', 'Ġocean', 'Ġsurveillance', 'Ġsatellites', 'Ġlower', 'Ġintended', 'Ġorbit', 'Ġcause', 'Ġanomaly', 'Ġtraced', 'Ġleak', 'Ġvalve', 'Ġallowed', 'Ġfuel', 'Ġleak', 'Ġcoast', 'Ġfirst', 'Ġsecond', 'Ġburns', 'Ġresulting', 'Ġlack', 'Ġfuel', 'Ġcaused', 'Ġsecond', 'Ġburn', 'Ġterminate', 'Ġseconds', 'Ġearly', 'Ġreplacing', 'Ġvalve', 'Ġled', 'Ġdelay', 'Ġnext', 'las', 'Ġlaunch', 'Ġhowever', 'Ġcustomer', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'Ġcategorized', 'Ġmission', 'Ġsuccess', 'Ġflight', 'Ġmarch', 'Ġsuffered', 'performance', 'Ġanomaly', 'Ġfirst', 'stage', 'Ġburn', 'Ġshut', 'Ġseconds', 'Ġearly', 'Ġcent', 'aur', 'Ġproceeded', 'Ġboost', 'Ġorbital', 'Ġcy', 'gn', 'us', 'Ġpayload', 'Ġheaviest', 'las', 'Ġdate', 'Ġintended', 'Ġorbit']</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>['Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġwik', 'ipedia', 'Ġhal', 'v', 'ors', 'en', 'Ġtodd', 'Ġse', 'pt', 'ember', 'las', 'Ġro', 'ars', 'Ġlife', 'Ġair', 'Ġforce', 'Ġsatellite', 'Ġonboard', 'htt', 'board', 'Ġfl', 'ida', 'Ġtoday', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġlaunch', 'Ġarchived', 'Ġoct', 'ober', 'Ġway', 'back', 'Ġmachine', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaccessed', '09', 'protected', 'Ġmilitary', 'Ġsatellite', 'Ġcommunication', 'Ġproject', 'Ġmarks', 'Ġsuccessful', 'Ġlaunch', 'Ġcape', 'aver', 'al', 'Ġmaple', 'Ġleaf', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'las', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġu', 'la', 'Ġretrieved', 'Ġj', 'une', 'Ġstep', 'hen', 'Ġcl', 'ark', 'Ġmarch', 'space', 'Ġforce', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġscheduled', 'Ġth', 'ursday', 'sp', 'ac', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġk', 'el', 'becca', 'Ġmarch', 'space', 'Ġforce', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġhill', 'Ġretrieved', 'Ġmarch', 'Ġdun', 'n', 'Ġmar', 'cia', 'Ġmarch', 'space', 'Ġforce', 'Ġlaunches', 'st', 'Ġmission', 'Ġvirus', 'Ġprecautions', 'http', 'Ġassociated', 'Ġpress', 'Ġretrieved', 'Ġmarch', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġmarch', 'ula', "'s", 'las', 'Ġlaunches', 'Ġcommunications', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġu', 'Ġspace', 'Ġforce', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġbr', 'ad', 'Ġber', 'gan', 'Ġmarch', 'Ġfirst', 'Ġtime', 'Ġus', 'Ġspace', 'Ġforce', 'Ġlaunching', 'Ġorbit', 'las', 'Ġrocket', 'Ġinteresting', 'Ġengineering', 'Ġretrieved', 'Ġapr', 'il', 'Ġedit', 'old', 'id', 'Ġarticle', 'Ġuses', 'Ġcontent', 'adv', 'anced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'atellite', ')"', 'Ġlicensed', 'Ġway', 'Ġpermits', 'Ġreuse', 'Ġcreative', 'Ġcommons', 'Ġun', 'ported', 'Ġlicense', 'Ġrelevant', 'Ġterms', 'Ġmust', 'Ġfollowed', 'Ġlaunch', 'Ġcc', 'af', 'Ġaug', 'ust', '07', 'Ġed', 'Ġlaunch', 'Ġcc', 'af', 'Ġ04', 'Ġmay', 'Ġed', 'Ġage', 'html', 'Ġlaunch', 'Ġcc', 'af', 'Ġse', 'pt', 'ember', 'Ġed']</t>
+          <t>['Ġusing', 'Ġfuel', 'Ġreserves', 'Ġmake', 'Ġshortfall', 'Ġfirst', 'Ġstage', 'Ġlonger', 'Ġburn', 'Ġcut', 'Ġshort', 'Ġlater', 'Ġcent', 'aur', 'Ġdisposal', 'Ġburn', 'Ġinvestigation', 'Ġincident', 'Ġrevealed', 'Ġanomaly', 'Ġdue', 'Ġfault', 'Ġmain', 'Ġengine', 'Ġmixture', 'rat', 'io', 'Ġsupply', 'Ġvalve', 'Ġrestricted', 'Ġflow', 'Ġfuel', 'Ġengine', 'Ġinvestigation', 'Ġsubsequent', 'Ġexamination', 'Ġvalves', 'Ġupcoming', 'Ġmissions', 'Ġled', 'Ġdelay', 'Ġnext', 'Ġseveral', 'Ġlaunches', 'Ġbo', 'e', 'ing', 'Ġstar', 'liner', 'Ġbo', 'e', 'ing', 'Ġel', 'ana', 'Ġge', 'ost', 'ation', 'ary', 'Ġoperational', 'Ġenvironmental', 'Ġsatellite', 'ars', 'Ġinsight', 'Ġjun', 'Ġl', 'u', 'cy', 'Ġlunar', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġlunar', 'Ġcrater', 'Ġobservation', 'Ġsensing', 'Ġsatellite', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġcuriosity', 'Ġpersever', 'ance', 'Ġingenuity', 'aven', 'th', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġlaunch', 'Ġnew', 'Ġhor', 'izons', 'Ġn', 'rol', 'Ġlaunches', 'Ġos', 'iris', 'rex', 'Ġsolar', 'Ġdynamics', 'Ġobserv', 'atory', 'Ġsolar', 'Ġorbit', 'er', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġus', 'Ġgeopolitical', 'Ġu', 'Ġpolitical', 'Ġconsiderations', 'Ġr', 'ussian', 'Ġwar', 'Ġcrime', 'Ġled', 'Ġeffort', 'Ġreplace', 'Ġr', 'ussian', 'supp', 'lied', 'Ġr', 'Ġengine', 'Ġused', 'Ġfirst', 'stage', 'Ġbooster', 'las', 'Ġv', 'Ġformal', 'Ġstudy', 'Ġcontracts', 'Ġissued', 'Ġj', 'une', 'Ġnumber', 'Ġu', 'Ġrocket', 'engine', 'Ġsuppliers', 'Ġresults', 'Ġstudies', 'Ġled', 'Ġdecision', 'Ġu', 'la', 'Ġdevelop', 'Ġnew', 'Ġvul', 'Ġcent', 'aur', 'Ġlaunch', 'Ġvehicle', 'Ġreplace', 'Ġexisting', 'las', 'Ġdelta', 'Ġse', 'pt', 'ember', 'Ġu', 'la', 'Ġannounced', 'Ġpartnership', 'Ġblue', 'Ġorigin', 'Ġdevelop', 'Ġl', 'ox', 'eth', 'ane', 'Ġengine', 'Ġreplace', 'Ġr', 'Ġnew', 'Ġfirst', 'stage', 'Ġbooster', 'las', 'Ġcore', 'Ġdesigned', 'Ġaround', 'Ġfuel', 'Ġcannot', 'Ġretro', 'fitted', 'Ġuse', 'Ġmethane', 'fuel', 'ed', 'Ġengine', 'Ġnew', 'Ġfirst', 'Ġstage', 'Ġdeveloped', 'Ġbooster', 'Ġfirst', 'stage', 'Ġtank', 'age', 'Ġdiameter', 'Ġdelta', 'Ġiv', 'Ġpowered', 'Ġtwo', 'Ġkn', '000', 'Ġthrust', 'Ġengine', 'Ġalready', 'Ġthird', 'Ġyear', 'Ġdevelopment', 'Ġblue', 'Ġorigin', 'Ġu', 'la', 'Ġexpected', 'Ġnew', 'Ġstage', 'Ġengine', 'Ġstart', 'Ġflying', 'Ġearlier', 'Ġvul', 'Ġinitially', 'Ġplanned', 'Ġuse', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'las', 'Ġv', 'Ġlater', 'Ġupgrade', 'ces', 'Ġhowever', 'ces', 'Ġlonger', 'Ġpursued', 'Ġcent', 'aur', 'Ġused', 'Ġinstead', 'Ġalso', 'Ġuse', 'Ġvariable', 'Ġnumber', 'Ġoptional', 'Ġsolid']</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -984,7 +984,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġrocket', 'Ġboosters', 'Ġcalled', 'Ġgem', 'Ġderived', 'Ġnew', 'Ġsolid', 'Ġboosters', 'Ġplanned', 'las', 'ero', 'jet', 'Ġrocket', 'Ġengine', 'Ġdevelopment', 'Ġbackup', 'Ġplan', 'Ġvul', 'Ġaug', 'ust', 'Ġfirst', 'Ġvul', 'Ġflight', 'Ġplanned', 'Ġlate', 'Ġmission', 'Ġsuccess', 'Ġrecord', 'Ġnotable', 'Ġpayload', 'Ġreplacement', 'Ġvul', 'Ġretirement', 'las', 'Ġwik', 'ipedia', 'Ġaug', 'ust', 'Ġu', 'la', 'Ġannounced', 'Ġlonger', 'Ġselling', 'Ġlaunches', 'las', 'Ġwould', 'Ġfulfill', 'Ġexisting', 'Ġlaunch', 'Ġcontracts', 'Ġmade', 'Ġfinal', 'Ġpurchase', 'Ġr', 'Ġmotors', 'Ġneeded', 'Ġlast', 'Ġmotors', 'Ġdelivered', 'Ġapr', 'il', 'Ġlast', 'Ġlaunch', 'Ġoccur', 'Ġtime', 'Ġmid', '".[', 'Ġoct', 'ober', 'Ġlaunches', 'Ġremain', 'Ġcore', 'Ġstage', 'las', 'Ġraised', 'Ġvertical', 'Ġposition', 'orb', 'ital', 'Ġtest', 'Ġvehicle', 'Ġenc', 'ased', 'Ġpayload', 'Ġfair', 'ing', 'Ġapr', 'il', 'Ġlaunch', 'las', 'Ġmoved', 'Ġlaunch', 'Ġpad', 'las', 'Ġlaunch', 'Ġpad', 'las', 'Ġignition', 'las', 'Ġnew', 'Ġhor', 'izons', 'Ġprobe', 'Ġlaunches', 'Ġlaunch', 'Ġpad', 'Ġcape', 'aver', 'al', 'Ġcomparable', 'Ġrockets', 'Ġang', 'ara', 'ri', 'ane', 'Ġdelta', 'Ġiv', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlong', 'Ġmarch', 'Ġpro', 'ton', 'Ġvul', 'Ġcent', 'aur', 'Ġz', 'en', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcomparison', 'Ġorbital', 'Ġlaunchers', 'Ġfamilies', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġpronounced', 'las', 'Ġï', '¬', 'ģ', '".', 'v', 'Ġr', 'oman', 'Ġnum', 'eral', 'rocket', 'builder', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'las', 'Ġv', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġde', 'cember', 'Ġfrank', 'le', 'Ġj', 'ared', 'Ġj', 'uly', 'ula', 'Ġdelays', 'Ġfocused', 'Ġprotecting', 'Ġpercent', 'Ġmission', 'Ġsuccess', 'Ġrate', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġde', 'cember', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'n', 'ro', 'g', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'ula', 'Ġread', 'ies', 'las', 'Ġlaunch']</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -997,7 +997,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>['Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġlifting', 'Ġcarrying', 'Ġfunction', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġmillion', ')[', 'Ġsize', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġmass', 'Ġft', '000', '000', '000', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', 'Ġft', '000', 'Ġexpended', 'Ġfal', 'con', 'Ġrocket', 'Ġfamily', 'Ġleft', 'Ġright', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġblock', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġpartially', 'Ġreusable', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcarry', 'Ġcargo', 'Ġcrew', 'Ġearth', 'Ġorbit', 'Ġdesigned', 'Ġmanufactured', 'Ġlaunched', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġspace', 'x', 'Ġalso', 'Ġused', 'Ġexpend', 'able', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġfirst', 'Ġfal', 'con', 'Ġlaunch', 'Ġj', 'une', 'Ġfirst', 'Ġfal', 'con', 'Ġiss', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġmission', 'Ġiss', 'Ġlaunched', 'Ġoct', 'ober', 'Ġbecame', 'Ġfirst', 'Ġcommercial', 'Ġrocket', 'Ġever', 'Ġlaunch', 'Ġhumans', 'Ġorbit', 'Ġcurrently', 'Ġvehicle', 'Ġcapable', 'Ġu', 'Ġrocket', 'Ġcurrently', 'Ġcertified', 'Ġtransporting', 'Ġhumans', 'Ġinternational', 'Ġspace', 'Ġbecame', 'Ġu', 'Ġrocket', 'Ġlaunches', 'Ġhistory', 'Ġbest', 'Ġsafety', 'Ġrecord', 'Ġsuffered', 'Ġone', 'Ġflight', 'Ġfailure', 'Ġrocket', 'Ġtwo', 'Ġstages', 'Ġfirst', 'bo', 'oster', 'Ġstage', 'Ġcarries', 'Ġsecond', 'Ġstage', 'Ġpayload', 'Ġpredetermined', 'Ġaltitude', 'Ġsecond', 'Ġstage', 'Ġlifts', 'Ġpayload', 'Ġultimate', 'Ġdestination', 'Ġbooster', 'Ġcapable', 'Ġlanding', 'Ġvertically', 'Ġfacilitate', 'Ġreuse', 'Ġfeat', 'Ġfirst', 'Ġachieved', 'Ġflight', 'Ġde', 'cember', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġsuccessfully', 'Ġlanded', 'Ġboosters', 'Ġtimes', 'Ġindividual', 'Ġboosters', 'Ġflown', 'Ġmany', 'Ġflights', 'Ġstages', 'Ġpowered', 'Ġspace', 'x', 'Ġmer', 'lin', 'Ġengines', 'Ġusing', 'Ġcry', 'ogenic', 'Ġliquid', 'Ġrocket', 'grade', 'Ġk', 'eros', 'ene', 'Ġheaviest', 'Ġpayload', 'Ġflown', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġint', 'els', 'Ġcarrying', 'Ġtel', 'star', 'v']</t>
+          <t>['Ġreconnaissance', 'Ġsatellite', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'las', 'Ġsolid', 'Ġrocket', 'Ġmotor', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġarchived', 'Ġoriginal', 'Ġol', 'id', 'rocket', 'otor', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'space', 'Ġlaunch', 'Ġreport', 'las', 'Ġdata', 'Ġsheet', 'las', 'html', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġoct', 'ober', 'Ġarchived', 'http', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'gem', 'gem', 'Ġfact', 'Ġsheet', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġphoto', 'Ġgallery', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġreferences', 'las', 'Ġwik', 'ipedia', 'develop', 'ing', 'Ġvul', 'Ġcent', 'aur', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġaug', 'ust', 'ula', 'Ġstops', 'Ġselling', 'Ġcenterpiece', 'las', 'Ġv', 'Ġsetting', 'Ġpath', 'Ġrocket', "'s", 'Ġretirement', 'Ġverge', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġcent', 'ennial', 'Ġcolor', 'ado', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'lock', 'heed', 'Ġmart', 'Ġready', 'Ġlaunch', 'Ġint', 'els', 'Ġspacecraft', 'Ġlock', 'heed', 'Ġmart', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġassumes', 'Ġmarketing', 'Ġsales', 'las', 'Ġlock', 'heed', 'Ġmart', 'Ġpar', 'abolic', 'arc', 'Ġpar', 'abolic', 'Ġarc', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'las', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġpp', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'las', 'Ġstar', 'liner', 'Ġoft', 'Ġnumbers', 'Ġarchived', 'Ġoriginal', 'http', 'n', 'umbers', 'Ġj', 'uly', 'ev', 'olved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'Ġmarch', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1010,7 +1010,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>['075', 'Ġformer', 'Ġlaunched', 'Ġadvantageous', 'Ġsuper', 'syn', 'chron', 'ous', 'Ġtransfer', 'Ġorbit', 'Ġlatter', 'Ġwent', 'Ġlower', 'energy', 'Ġg', 'Ġap', 'gee', 'Ġwell', 'Ġge', 'ost', 'ation', 'ary', 'Ġaltitude', 'Ġjan', 'uary', 'Ġfal', 'con', 'Ġset', 'Ġrecord', 'Ġsatellites', 'Ġlaunched', 'Ġsingle', 'Ġrocket', 'Ġcarrying', 'Ġorbit', 'Ġfal', 'con', 'Ġhuman', 'rated', 'Ġtransporting', 'Ġn', 'asa', 'Ġastronauts', 'Ġiss', 'Ġfal', 'con', 'Ġcertified', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġprogram', 'Ġn', 'asa', 'Ġlaunch', 'Ġservices', 'Ġprogram', 'category', '",', 'Ġlaunch', 'Ġexpensive', 'Ġimportant', 'Ġcomplex', 'Ġn', 'asa', 'Ġmissions', 'Ġrocket', 'Ġevolved', 'Ġseveral', 'Ġversions', 'Ġflew', 'âĢĵ', 'Ġflew', 'âĢĵ', 'Ġfull', 'Ġthrust', 'Ġfirst', 'Ġlaunched', 'Ġencomp', 'assing', 'Ġblock', 'Ġvariant', 'Ġoperation', 'Ġsince', 'Ġmay', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġannounced', 'Ġplans', 'Ġlaunch', 'Ġfal', 'con', 'Ġfirst', 'Ġhalf', 'Ġinitial', 'Ġlaunch', 'Ġwould', 'Ġoccur', 'Ġspace', 'x', 'Ġspent', 'Ġcapital', 'Ġdevelop', 'Ġprevious', 'Ġlauncher', 'Ġfal', 'con', 'Ġdevelopment', 'Ġfal', 'con', 'Ġaccelerated', 'Ġpartial', 'Ġn', 'asa', 'Ġfunding', 'Ġcommitments', 'Ġpurchase', 'Ġflights', 'Ġspecific', 'Ġcapabilities', 'Ġdemonstrated', 'Ġfunding', 'Ġstarted', 'Ġseed', 'Ġmoney', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'c', 'ots', 'Ġprogram', 'Ġcontract', 'Ġstructured', 'Ġspace', 'Ġact', 'Ġagreement', 'Ġdevelop', 'Ġdemonstrate', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservice', '",', 'Ġincluding', 'Ġpurchase', 'Ġthree', 'Ġdemonstration', 'Ġflights', 'Ġoverall', 'Ġcontract', 'Ġaward', 'Ġus', 'Ġmillion', 'Ġprovide', 'Ġthree', 'Ġdemonstration', 'Ġlaunches', 'Ġfal', 'con', 'Ġspace', 'x', 'Ġdragon', 'Ġcargo', 'Ġspacecraft', 'Ġadditional', 'Ġmilestones', 'Ġadded', 'Ġlater', 'Ġraising', 'Ġtotal', 'Ġcontract', 'Ġvalue', 'Ġus', 'Ġmillion', 'Ġspace', 'x', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'c', 'rs', 'Ġcontract', 'Ġn', 'asa', "'s", 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'c', 'ots', 'Ġprogram', 'Ġdeliver', 'Ġcargo', 'Ġiss', 'Ġusing', 'Ġfal', 'con', 'dragon', 'Ġfunds', 'Ġwould', 'Ġdis', 'b', 'ursed', 'Ġdemonstration', 'Ġmissions', 'Ġsuccessfully', 'Ġthoroughly', 'Ġcompleted', 'Ġcontract', 'Ġtotaled', 'Ġus', 'Ġbillion', 'Ġminimum', 'Ġmissions', 'Ġferry', 'Ġsupplies', 'Ġiss', 'Ġspace', 'x', 'Ġestimated', 'Ġfal', 'con', 'Ġdevelopment', 'Ġcosts', 'Ġorder']</t>
+          <t>['Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbon', 'nie', 'Ġbir', 'ck', 'en', 'st', 'aed', 'Ġb', 'ern', 'ard', 'Ġf', 'Ġk', 'utter', 'Ġfrank', 'Ġz', 'eg', 'ler', 'cent', 'aur', 'Ġapplication', 'Ġrobotic', 'Ġcrew', 'ed', 'Ġlunar', 'Ġland', 'er', 'Ġevolution', 'web', 'Ġol', 'ution', 'pdf', 'Ġameric', 'Ġinstitute', 'Ġphysics', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'las', 'Ġrockets', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'laun', 'cher', 'Ġfair', 'ings', 'Ġstructures', 'Ġru', 'ag', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'las', 'las', 'v', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġaug', 'ust', 'h', 'oney', 'well', 'Ġawarded', 'Ġmillion', 'las', 'Ġcontract', 'Ġmilitary', 'Ġaerospace', 'Ġelectronics', 'Ġapr', 'il', 'Ġretrieved', 'mber', 'las', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'h', 'oney', 'well', 'Ġprovides', 'Ġguidance', 'Ġsystem', 'las', 'Ġrocket', 'ww', 'Ġspace', 'travel', 'Ġaug', 'ust', 'Ġretrieved', 'mber', 'Ġj', 'ason', 'Ġrh', 'ian', 'Ġse', 'pt', 'ember', 'ula', 'Ġselects', 'Ġorbital', 'k', "'s", 'Ġgem', 'las', 'Ġvul', 'Ġboosters', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġinsider', 'Ġarchived', 'w', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġrocket', 'Ġboosters', 'Ġhelp', 'Ġsuccessfully', 'Ġlaunch', 'Ġunited', 'Ġlaunch', 'Ġalliance', "'s", 'las', 'Ġv', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġnews', 'room', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġg', 'ask', 'ill', 'Ġbr', 'addock', 'Ġjan', 'uary', 'human', 'Ġrated', 'las', 'Ġbig', 'el', 'ow', 'Ġspace', 'Ġstation', 'Ġdetails', 'Ġemerge', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'n', 'asa', 'Ġselects', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġcommercial', 'Ġcrew', 'Ġdevelopment', 'Ġprogram', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary']</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1023,7 +1023,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>['Ġus', 'Ġmillion', 'Ġn', 'asa', 'Ġestimated', 'Ġdevelopment', 'Ġcosts', 'Ġbillion', 'Ġtraditional', 'Ġcost', 'plus', 'Ġcontract', 'Ġapproach', 'Ġused', 'Ġn', 'asa', 'Ġreport', 'est', 'imated', 'Ġwould', 'Ġcost', 'Ġagency', 'Ġdevelopment', 'Ġhistory', 'Ġconception', 'Ġfunding', 'Ġfal', 'con', 'Ġwik', 'ipedia', '000', 'Ġlanding', 'ds', '000', '000', 'Ġpayload', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', 'Ġft', '000', 'Ġexpended', '000', 'Ġlanding', '000', 'Ġpayload', 'Ġmars', 'Ġtransfer', 'Ġorbit', 'Ġmass', 'Ġft', 'Ġassociated', 'Ġrockets', 'Ġderivative', 'Ġwork', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġft', 'Ġblock', 'Ġactive', 'Ġft', 'Ġblock', 'Ġretired', 'Ġft', 'Ġblock', 'Ġretired', 'Ġretired', 'Ġretired', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġv', 'enberg', 'Ġv', 'enberg', 'future', 'Ġtotal', 'Ġlaunches', 'ft', 'Ġsuccess', 'es', 'ft', 'Ġfailure', 'ï', '¬', 'Ĥ', 'ight', 'Ġpartial', 'Ġfailure', 'Ġcr', ')[', 'Ġnotable', 'Ġoutcome', 'ft', 'Ġpre', 'ï', '¬', 'Ĥ', 'ight', 'Ġdestruction', 'Ġland', 'ings', 'Ġattempts', 'Ġbillion', 'Ġdevelop', 'Ġrocket', 'Ġlike', 'Ġfal', 'con', 'Ġbooster', 'Ġbased', 'Ġupon', 'Ġn', 'asa', "'s", 'Ġtraditional', 'Ġcontracting', 'Ġprocesses', 'Ġcommercial', 'Ġdevelopment', 'Ġapproach', 'Ġmight', 'Ġallowed', 'Ġagency', 'Ġpay', 'Ġus', 'Ġbillion', '".[', 'Ġspace', 'x', 'Ġreleased', 'Ġcombined', 'Ġdevelopment', 'Ġcosts', 'Ġfal', 'con', 'Ġdragon', 'Ġn', 'asa', 'Ġprovided', 'Ġus', 'Ġmillion', 'Ġspace', 'x', 'Ġprovided', 'Ġus', 'Ġmillion', 'Ġcongressional', 'Ġtestimony', 'Ġspace', 'x', 'Ġsuggested', 'Ġunusual', 'Ġn', 'asa', 'Ġprocess', 'setting', 'Ġhigh', 'level', 'Ġrequirement', 'Ġcargo', 'Ġtransport', 'Ġspace', 'Ġstation', 'Ġleaving', 'Ġdetails', 'Ġindustry', 'Ġallowed', 'Ġspace', 'x', 'Ġcomplete', 'Ġtask', 'Ġsubstantially', 'Ġlower', 'Ġcost', 'according', 'Ġn', 'asa', "'s", 'Ġindependently', 'Ġverified', 'Ġnumbers', 'Ġspace', 'x', "'s", 'Ġdevelopment', 'Ġcosts', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġrockets', 'Ġestimated', 'Ġapproximately', 'Ġmillion', 'Ġtotal', '."[', 'Ġspace', 'x', 'Ġoriginally', 'Ġintended', 'Ġfollow']</t>
+          <t>['Ġaward', 'ees', 'Ġone', 'Ġyear', 'Ġlater', '?"', 'web', 'arc', 'Ġnewsp', 'ace', 'Ġjournal', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'http', 'new', 'sp', 'Ġhey', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'safety', 'Ġsystem', 'Ġtested', 'las', 'Ġdelta', 'Ġrockets', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'ul', 'acc', 'dev', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġbegins', 'Ġcommercial', 'Ġpartnership', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ht', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġboy', 'le', 'Ġal', 'Ġj', 'uly', 'rocket', 'Ġventure', 'Ġwork', 'Ġn', 'asa', 'Ġcosmic', 'Ġlog', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'uly', 'Ġke', 'lly', 'Ġjohn', 'Ġaug', 'ust', 'las', 'Ġrising', 'Ġoccasion', 'Ġspace', 'blog', 'Ġfl', 'ida', 'Ġtoday', 'Ġmel', 'bourne', 'Ġfl', 'ida', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġaug', 'ust', 'bo', 'e', 'ing', 'Ġselects', 'las', 'Ġrocket', 'Ġinitial', 'Ġcommercial', 'Ġcrew', 'Ġlaunches', 'h', 'press', 'Ġrelease', 'Ġh', 'ouston', 'Ġbo', 'e', 'ing', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'http', 'bo', 'e', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġmal', 'ik', 'ari', 'q', 'Ġaug', 'ust', 'bo', 'e', 'ing', 'Ġneeds', 'Ġspace', 'Ġpilots', 'Ġspaceship', 'Ġrocket', 'Ġtest', 'Ġflights', 'Ġspace', 'Ġarchived', 'web', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġp', 'app', 'al', 'ardo', 'Ġjo', 'e', 'bo', 'e', 'ing', "'s", 'Ġstar', 'liner', 'Ġfalls', 'Ġshort', 'Ġbig', 'Ġblow', 'Ġn', 'asa', "'s", 'Ġcrew', 'ed', 'Ġprogram', 'Ġpopular', 'Ġmechanics', 'Ġretrieved', 'Ġde', 'cember', 'las', 'Ġwik', 'ipedia', 'Ġsheet', 'z', 'ichael', 'Ġde', 'cember', 'bo', 'e', 'ing', 'Ġstar', 'liner', 'Ġfails', 'Ġkey', 'Ġn', 'asa', 'Ġmission', 'Ġautonomous', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsystem', 'Ġmalf', 'unctions']</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>['Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġintermediate', 'Ġcapacity', 'Ġvehicle', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġline', 'Ġvehicles', 'Ġnamed', 'Ġfictional', 'Ġstarship', 'mill', 'enn', 'ium', 'Ġfal', 'con', 'Ġstar', 'Ġwars', 'Ġfilm', 'Ġseries', 'Ġspace', 'x', 'Ġannounced', 'Ġinstead', 'Ġproceeding', 'Ġfal', 'con', 'fully', 'Ġreusable', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', '",', 'Ġalready', 'Ġsecured', 'Ġgovernment', 'Ġcustomer', 'Ġfal', 'con', 'Ġdescribed', 'Ġcapable', 'Ġlaunching', 'Ġapproximately', 'Ġkilograms', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġprojected', 'Ġpriced', '000', '000', 'Ġus', 'Ġper', 'Ġflight', 'Ġft', 'Ġpayload', 'Ġfair', 'ing', 'Ġmillion', 'Ġft', 'Ġfair', 'ing', 'Ġspace', 'x', 'Ġalso', 'Ġannounced', 'Ġheavy', 'Ġversion', 'Ġfal', 'con', 'Ġpayload', 'Ġcapacity', 'Ġapproximately', '000', 'Ġkilograms', '000', 'Ġfal', 'con', 'Ġintended', 'Ġsupport', 'Ġle', 'Ġg', 'Ġmissions', 'Ġwell', 'Ġcrew', 'Ġcargo', 'Ġmissions', 'Ġiss', 'Ġoriginal', 'Ġn', 'asa', 'Ġc', 'ots', 'Ġcontract', 'Ġcalled', 'Ġfirst', 'Ġdemonstration', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġcompletion', 'Ġthree', 'Ġdemonstration', 'Ġmissions', 'Ġse', 'pt', 'ember', 'Ġfe', 'b', 'ruary', 'Ġdate', 'Ġslipped', 'Ġfirst', 'Ġquarter', 'Ġaccording', 'Ġmus', 'k', 'Ġcomplexity', 'Ġcape', 'aver', 'al', 'Ġregulatory', 'Ġrequirements', 'Ġcontributed', 'Ġdelay', 'Ġfirst', 'Ġmulti', 'engine', 'Ġtest', 'two', 'Ġengines', 'Ġfiring', 'Ġsimultaneously', 'Ġconnected', 'Ġfirst', 'Ġstage', 'Ġcompleted', 'Ġjan', 'uary', 'Ġsuccessive', 'Ġtests', 'Ġled', 'Ġsecond', 'mission', 'Ġlength', 'Ġnine', 'Ġengine', 'Ġtest', 'fire', 'mber', 'Ġoct', 'ober', 'Ġfirst', 'Ġflight', 'ready', 'engine', 'Ġtest', 'Ġfire', 'Ġtest', 'Ġfacility', 'Ġmc', 'greg', 'Ġtex', 'mber', 'Ġspace', 'x', 'Ġconducted', 'Ġinitial', 'Ġsecond', 'Ġstage', 'Ġtest', 'Ġfiring', 'Ġlasting', 'Ġforty', 'Ġseconds', 'Ġjan', 'uary', 'Ġsecond', 'mission', 'Ġlength', 'Ġorbit', 'insert', 'ion', 'Ġfiring', 'Ġsecond', 'Ġstage', 'Ġconducted', 'Ġelements', 'Ġstack', 'Ġarrived', 'Ġlaunch', 'Ġsite', 'Ġintegration', 'Ġbeginning', 'Ġfe', 'b', 'ruary', 'Ġflight', 'Ġstack', 'Ġwent', 'Ġvertical', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġmarch', 'Ġspace', 'x', 'Ġperformed', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġfirst', 'Ġstage', 'Ġfired', 'Ġwithout', 'Ġlaunch', 'Ġtest', 'Ġaborted', 'Ġdue', 'Ġfailure', 'Ġhigh']</t>
+          <t>['Ġretrieved', 'Ġj', 'une', 'bo', 'e', 'ing', 'Ġstar', 'liner', 'Ġcapsule', 'Ġlifts', 'Ġspace', 'Ġstation', 'Ġsecond', 'Ġorbital', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtest', 'oft', 'launch', 'html', 'Ġcollect', 'space', 'Ġretrieved', 'Ġj', 'une', 'star', 'liner', 'Ġconcludes', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlanding', 'Ġnew', 'x', 'ico', 'http', 'Ġe', 'w', 'ex', 'ico', 'Ġspac', 'en', 'ews', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġsheet', 'z', 'ichael', 'Ġapr', 'il', 'amazon', 'Ġsigns', 'Ġu', 'la', 'Ġrockets', 'Ġlaunch', 'Ġje', 'ff', 'zos', 'Ġk', 'ui', 'per', 'Ġinternet', 'Ġsatellites', 'es', 'html', 'Ġretrieved', 'Ġj', 'uly', 'las', 'Ġv', 'Ġu', 'la', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġmarch', 'ike', 'Ġgr', 'uss', 'Ġj', 'une', 'air', 'Ġforce', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġu', 'la', 'Ġposition', 'las', 'Ġproduction', 'Ġrights', 'Ġspac', 'en', 'ews', 'jon', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġlaunch', 'Ġvehicle', 'Ġdatabase', 'web', 'arch', 'iv', 'Ġh', 'las', 'Ġj', 'athan', 'cd', 'owell', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'las', 'Ġmission', 'Ġplanner', "'s", 'Ġguide', 'Ġmarch', 'Ġarchived', 'htt', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġretrieved', 'Ġu', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġdevelopments', 'Ġconcepts', 'Ġvehicles', 'Ġtechnologies', 'Ġspac', 'ep', 'orts', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġe', 'gan', 'Ġbar', 'bara', 'bar', 'gan', 'Ġoct', 'ober', 'Ġcalling', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'Ġpayload', 'Ġfair', 'ing', 'Ġstar', 'liner', 'Ġboard', 'tw', 'itte', 'weet', 'Ġvia', 'Ġtwitter', 'Ġk', 'bs', 'Ġgun', 'ter', 'star', 'liner', 'c', 'st', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract']</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>['pressure', 'Ġhelium', 'Ġpump', 'Ġsystems', 'Ġabort', 'Ġperformed', 'Ġexpected', 'Ġadditional', 'Ġissues', 'Ġneeded', 'Ġaddressing', 'Ġsubsequent', 'Ġtest', 'Ġmarch', 'Ġfired', 'Ġfirst', 'stage', 'Ġengines', 'Ġseconds', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġproduction', 'Ġline', 'Ġmanufactured', 'Ġfal', 'con', 'Ġdragon', 'Ġspacecraft', 'Ġevery', 'Ġthree', 'Ġmonths', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', "'s", 'Ġtotal', 'Ġmanufacturing', 'Ġspace', 'Ġincreased', 'Ġnearly', '000', '000', '000', 'Ġft', 'Ġorder', 'Ġachieve', 'Ġproduction', 'Ġrate', 'Ġrocket', 'Ġcores', 'Ġannually', 'Ġfactory', 'Ġproducing', 'Ġone', 'Ġfal', 'con', 'Ġper', 'Ġmonth', 'mber', 'Ġfe', 'b', 'ruary', 'Ġproduction', 'Ġrate', 'Ġfal', 'con', 'Ġcores', 'Ġincreased', 'Ġper', 'Ġyear', 'Ġnumber', 'Ġfirst', 'Ġstage', 'Ġcores', 'Ġcould', 'Ġassembled', 'Ġone', 'Ġtime', 'Ġreached', 'Ġsince', 'Ġspace', 'x', 'Ġroutinely', 'Ġreused', 'Ġfirst', 'Ġstages', 'Ġreducing', 'Ġdemand', 'Ġnew', 'Ġcores', 'Ġspace', 'x', 'Ġperformed', 'Ġlaunches', 'Ġusing', 'Ġtwo', 'Ġnew', 'Ġboosters', 'Ġsuccessfully', 'Ġrecovered', 'Ġbooster', 'Ġone', 'Ġflight', 'Ġhaw', 'th', 'orne', 'Ġfactory', 'Ġproduces', 'Ġone', 'exp', 'end', 'able', 'Ġsecond', 'Ġstage', 'Ġlaunch', 'Ġdevelopment', 'Ġtesting', 'Ġproduction', 'Ġlaunch', 'Ġhistory', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġft', 'Ġblock', 'Ġmay', 'bang', 'aband', 'hu', 'Ġsatellite', 'Ġft', 'Ġde', 'cember', 'Ġflight', ')[', 'Ġse', 'pt', 'ember', 'Ġcass', 'ope', 'Ġj', 'une', 'dragon', 'Ġc', 'ots', 'Ġdemo', ')[', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġft', 'Ġblock', 'Ġj', 'une', 'space', 'x', 'Ġjan', 'uary', 'j', 'ason', 'Ġmarch', 'space', 'x', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġft', 'Ġblock', 'Ġmer', 'lin', 'maximum', 'Ġthrust', 'Ġft', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġmaximum', 'Ġthrust', 'Ġft', 'late', '):', '000', 'Ġft', '000', '000', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '05', 'Ġsea', 'Ġlevel', 'Ġvacuum', 'Ġburn', 'Ġtime', 'Ġft', 'Ġseconds', 'Ġseconds', 'Ġseconds']</t>
+          <t>['aven', 'Ġmission', 'http', 'mar', 'Ġmars', 'n', 'asa', 'gov', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ula', 'Ġfrequently', 'Ġasked', 'Ġquestions', 'Ġlaunch', 'Ġcosts', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'Ġnorth', 'Ġk', 'Ġoct', 'ober', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġtd', 'rs', 'Ġsatellite', 'Ġn', 'asa', 'gov', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgr', 'ush', 'Ġlore', 'n', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġunve', 'ils', 'Ġwebsite', 'Ġlets', 'Ġprice', 'Ġrocket', 'like', 'Ġbuilding', 'Ġcar', 'ww', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġstep', 'hen', 'Ġcl', 'ark', 'mber', 'izing', 'Ġameric', "'s", 'Ġplace', 'Ġglobal', 'Ġlaunch', 'Ġindustry', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'commercial', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġth', 'om', 'pson', 'Ġlore', 'n', 'ce', 'ory', 'Ġbr', 'uno', 'Ġexplains', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġstay', 'Ġahead', 'Ġcompetitors', 'Ġforb', 'es', 'Ġretrieved', 'Ġde', 'cember', 'Ġgreat', 'Ġrocket', 'Ġrace', 'Ġg', 'rocket', 'race', 'Ġfortune', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'iam', 'Ġhar', 'wood', 'mber', 'ula', 'Ġunve', 'ils', 'rocket', 'builder', 'Ġwebsite', 'bsite', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġder', 'bsite', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'las', 'Ġproduct', 'Ġcard', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġrand', 'Ġcorporation', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġdf', 'Ġoct', 'ober', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġrand', 'Ġcorporation', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġdf', 'Ġoct', 'ober', 'Ġfinal', 'Ġreport', 'Ġseeking', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġprogram', 'Ġworthy', 'Ġgreat', 'Ġnation', 'Ġe', 'port', 'pdf', 'Ġarchived', 'Ġway', 'back', 'Ġmachine', 'Ġoct', 'ober']</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>['Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'Ġrockets', 'Ġfal', 'con', 'Ġfamily', 'Ġlaunched', 'Ġtimes', 'Ġyears', 'Ġresulting', 'Ġfull', 'Ġmission', 'Ġsuccesses', '%),', 'Ġone', 'Ġpartial', 'Ġsuccess', 'space', 'x', 'Ġdelivered', 'Ġcargo', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġsecondary', 'Ġpayload', 'Ġstranded', 'Ġlower', 'planned', 'Ġorbit', 'Ġone', 'Ġfull', 'Ġfailure', 'Ġspace', 'x', 'Ġspacecraft', 'Ġlost', 'Ġflight', 'Ġexplosion', 'Ġadditionally', 'Ġone', 'Ġrocket', 'Ġpayload', 'Ġdestroyed', 'Ġlaunch', 'Ġpreparation', 'pad', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġactive', 'Ġversion', 'Ġfal', 'con', 'Ġblock', 'Ġflown', 'Ġmissions', 'Ġfull', 'Ġsuccesses', 'Ġfal', 'con', 'Ġset', 'Ġnew', 'Ġrecord', 'Ġlaunches', 'Ġsuccessful', 'Ġlaunch', 'Ġvehicle', 'Ġtype', 'Ġcalendar', 'Ġyear', 'Ġprevious', 'Ġrecord', 'Ġheld', 'Ġlaunches', 'Ġsuccessful', 'Ġfirst', 'Ġrocket', 'Ġversion', 'Ġfal', 'con', 'Ġlaunched', 'Ġfive', 'Ġtimes', 'Ġj', 'une', 'Ġmarch', 'Ġsuccessor', 'Ġfal', 'con', 'Ġtimes', 'Ġse', 'pt', 'ember', 'Ġjan', 'uary', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġtimes', 'Ġde', 'cember', 'Ġpresent', 'Ġlatest', 'Ġfull', 'Ġthrust', 'Ġvariant', 'Ġblock', 'Ġintroduced', 'Ġmay', 'Ġblock', 'Ġboosters', 'Ġflown', 'Ġtwice', 'Ġrequired', 'Ġseveral', 'Ġmonths', 'Ġrefurb', 'ishment', 'Ġblock', 'Ġversions', 'Ġdesigned', 'Ġsustain', 'Ġflights', 'Ġinspections', 'Ġfal', 'con', 'Ġheavy', 'Ġderivative', 'Ġconsists', 'Ġstrengthened', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġcenter', 'Ġcore', 'Ġtwo', 'Ġadditional', 'Ġfal', 'con', 'Ġfirst', 'Ġstages', 'Ġattached', 'Ġused', 'Ġboosters', 'Ġfitted', 'Ġaer', 'odynamic', 'Ġnose', 'cone', 'Ġinstead', 'Ġusual', 'Ġfal', 'con', 'Ġinter', 'stage', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġpowered', 'Ġft', 'Ġregular', 'Ġmer', 'lin', 'Ġvacuum', 'Ġregular', 'Ġnozzle', 'Ġft', 'Ġshort', 'Ġmer', 'lin', 'Ġvacuum', 'Ġshort', 'Ġnozzle', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmaximum', 'Ġthrust', 'Ġft', 'Ġregular', 'Ġkn', '000', 'Ġft', 'Ġshort', 'Ġkn', '000', '01', 'Ġkn', '000', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġft', 'Ġregular', 'Ġft', 'Ġshort', 'Ġburn', 'Ġtime', 'Ġft', 'Ġregular', 'Ġseconds', 'Ġft', 'Ġshort', 'Ġseconds']</t>
+          <t>['Ġreview', 'Ġu', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġplans', 'Ġcommittee', 'Ġgraphic', 'Ġp', 'Ġretrieved', '02', '07', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'development', 'Ġlaunch', 'Ġvehicle', 'Ġnew', 'Ġmedium', 'Ġclass', 'Ġlaunch', 'Ġvehicle', 'Ġj', 'apan', 'Ġengineering', 'Ġreview', 'Ġretrieved', 'mber', 'j', 'apan', 'Ġscraps', 'Ġrocket', 'Ġdevelopment', 'Ġproject', 'ock', 'alyst', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġr', 'icle', 'id', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'ike', 'Ġgr', 'uss', 'Ġmay', 'ero', 'jet', 'Ġteam', 'Ġseeking', 'las', 'Ġproduction', 'Ġrights', 'Ġspac', 'en', 'ews', 'aug', 'ural', 'las', 'Ġscores', 'Ġsuccess', 'Ġil', 'Ġlock', 'heed', 'Ġmart', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ils', 'Ġlaunches', 'Ġhell', 'sat', 'las', 'Ġv', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ils', 'Ġlaunches', 'Ġrainbow', 'Ġsatellite', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ils', 'Ġlaunches', 'Ġwraps', 'Ġyear', 'Ġmission', 'Ġsuccesses', 'ht', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'las', 'Ġwik', 'ipedia', 'ils', 'las', 'Ġvehicle', 'Ġlifts', 'Ġmassive', 'Ġsatellite', 'ars', 'http', 'ils', 'l', 'Ġell', 'ite', 'ars', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġmarch', 'Ġarchived', 'Ġsat', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'asa', "'s", 'Ġmultip', 'ur', 'pose', 'Ġmars', 'Ġmission', 'Ġsuccessfully', 'Ġlaunched', 'Ġn', 'asa', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'html', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', "'s", 'Ġpl', 'uto', 'Ġmission', 'Ġlaunched', 'Ġtoward', 'Ġnew', 'Ġhor', 'izons']</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>['Ġseconds', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfal', 'con', 'Ġfirst', 'stage', 'Ġboosters', 'Ġlanded', 'Ġsuccessfully', 'Ġattempts', '%),', '%)', 'Ġfal', 'con', 'Ġblock', 'Ġversion', 'Ġtotal', 'fl', 'ights', 'Ġfirst', 'Ġstage', 'Ġboosters', 'Ġsuccessfully', 'Ġlaunched', 'Ġpayload', 'Ġrocket', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġlaunch', 'Ġsites', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlaunch', 'Ġc', 'ots', 'Ġdemo', 'Ġflight', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġfal', 'con', 'Ġft', 'used', 'Ġfal', 'con', 'Ġblock', 'new', 'Ġfal', 'con', 'Ġblock', 'used', 'Ġfal', 'con', 'Ġheavy', 'Ġk', 'sc', 'Ġloss', 'Ġlaunch', 'Ġloss', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġpartial', 'Ġfailure', 'Ġsuccess', 'commercial', 'Ġgovernment', 'Ġsuccess', 'st', 'arl', 'ink', 'Ġplanned', 'commercial', 'Ġgovernment', 'Ġplanned', 'st', 'arl', 'ink', 'Ġground', 'pad', 'Ġfailure', 'Ġdrone', 'ship', 'Ġfailure', 'Ġocean', 'Ġtest', 'Ġfailure', 'Ġparachute', 'Ġtest', 'Ġfailure', 'ii', 'Ġground', 'pad', 'Ġsuccess', 'Ġdrone', 'ship', 'Ġsuccess', 'Ġocean', 'Ġtest', 'Ġsuccess', 'iii', 'Ġattempt', 'Ġcontrolled', 'Ġdescent', 'Ġocean', 'Ġtouchdown', 'Ġcontrol', 'Ġfailed', 'Ġrecovery', 'Ġpassive', 'entry', 'Ġfailed', 'Ġparachute', 'Ġdeployment', 'Ġcontrolled', 'Ġdescent', 'Ġsoft', 'Ġvertical', 'Ġocean', 'Ġtouchdown', 'Ġrecovery', 'Ġflight', 'Ġdragon', 'Ġspacecraft', 'Ġqual', 'ï', '¬', 'ģ', 'cation', 'Ġunit', 'Ġj', 'une', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtest', 'Ġdragon', 'Ġflight', 'Ġdragon', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcargo', 'Ġdelivery', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġoperational', 'Ġcargo', 'Ġmission', 'Ġiss', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdemonstration', 'Ġrocket', "'s", 'Ġengine', 'Ġcapability', 'Ġdue', 'Ġfailure', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġmer', 'lin', 'Ġengine', 'Ġflight', 'Ġcass', 'ope', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrocket', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġv', 'enberg', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġattempt', 'Ġprop', 'ulsive', 'Ġreturn', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġge', 'os', 'ynchronous']</t>
+          <t>['web', 'ar', 'Ġn', 'asa', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ils', 'Ġlaunches', 'Ġast', 'ra', 'Ġsatellite', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'news', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfirst', 'Ġus', 'af', 'las', 'Ġv', 'htt', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'mission', 'Ġstatus', 'Ġcenter', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'web', 'arch', 'iv', 'Ġn', 'ro', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'n', 'ro', 'g', 'n', 'ro', 'gov', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'ula', 'Ġread', 'ies', 'las', 'Ġlaunch', 'Ġreconnaissance', 'Ġsatellite', 'h', 'Ġspace', 'flight', 'Ġinsider', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'atellite', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġpet', 'erson', 'Ġpat', 'rick', 'Ġse', 'pt', 'ember', 'f', 'ault', 'Ġvalve', 'Ġpushes', 'Ġback', 'las', 'Ġlaunch', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'http', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'ro', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'ell', 'ite', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'united', 'Ġlaunch', 'Ġalliance', 'Ġinaugural', 'las', 'Ġwest', 'Ġcoast', 'Ġlaunch', 'Ġsuccess', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'Ġheaviest', 'Ġcommercial', 'Ġsatellite', 'las']</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>['Ġtransfer', 'Ġorbit', 'g', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġn', 'ongo', 'vernment', 'al', 'Ġpayload', 'Ġflight', 'Ġadded', 'Ġlanding', 'Ġlegs', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfully', 'Ġcontrolled', 'Ġdescent', 'Ġvertical', 'Ġocean', 'Ġtouchdown', 'Ġflight', 'Ġdeep', 'Ġspace', 'Ġclimate', 'Ġobserv', 'atory', 'sc', 'ov', 'r', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġhyper', 'b', 'olic', 'Ġmission', 'Ġinjecting', 'Ġspacecraft', 'Ġpoint', 'Ġflight', 'Ġtotal', 'Ġloss', 'Ġmission', 'Ġdue', 'Ġstructural', 'Ġfailure', 'Ġhelium', 'pressure', 'Ġsecond', 'Ġstage', 'Ġflight', 'Ġorb', 'comm', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġvertical', 'Ġlanding', 'Ġorbital', 'class', 'Ġrocket', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanding', 'Ġvertically', 'Ġachieved', 'Ġautonomous', 'Ġspac', 'eport', 'Ġdrone', 'Ġship', 'Ġsea', 'Ġtotal', 'Ġvehicle', 'Ġpayload', 'Ġloss', 'Ġprior', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'would', 'Ġflight', 'Ġflight', 'Ġcr', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġflight', 'es', 'Ġï', '¬', 'ģ', 'r', 'st', 'ï', '¬', 'Ĥ', 'ight', 'Ġpreviously', 'Ġï', '¬', 'Ĥ', 'Ġorbital', 'Ġclass', 'Ġbooster', 'Ġpreviously', 'Ġused', 'Ġspace', 'x', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrecovery', 'Ġfair', 'ing', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġspace', 'plane', 'Ġflight', 'Ġbang', 'aband', 'hu', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġblock', 'Ġversion', 'Ġlaunch', 'Ġoutcomes', 'Ġbooster', 'Ġland', 'ings', 'Ġnotable', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġhistoric', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġlanding', 'Ġcape', 'aver', 'al', 'Ġlanding', 'Ġzone', 'Ġde', 'cember', 'Ġflight', 'Ġtel', 'star', 'v', 'Ġheaviest', 'Ġcommunications', 'Ġsatellite', 'Ġever', 'Ġdelivered', 'Ġflight', 'Ġcrew', 'Ġdragon', 'Ġdemo', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġcrew', 'Ġdragon', 'Ġcarry', 'Ġastronauts', 'Ġflight', 'Ġrad', 'ars', 'Ġconstellation', 'Ġvaluable', 'Ġcommercial', 'Ġpayload', 'Ġput', 'Ġorbit', 'Ġflight', 'Ġstar', 'link', 'Ġlaunch', 'Ġsuccessful', 'Ġï', '¬', 'Ĥ']</t>
+          <t>['Ġv', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmoon', 'Ġmission', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'cl', 'ues', 'Ġmystery', 'Ġpayload', 'Ġemerge', 'Ġsoon', 'Ġlaunch', 'web', 'ar', 'Ġ01', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'h', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpan', 'Ġsatellite', 'w', 'Ġes', 'news', 'sh', 'tml', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'rocket', 'Ġstage', 'Ġlaunched', 'Ġyears', 'Ġago', 'Ġdisinteg', 'rates', 'Ġtrail', 'Ġspace', 'Ġjunk', 'video', ')"', 'Ġspace', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'th', 'las', 'Ġmission', 'Ġsuccessfully', 'Ġlaunches', 'ms', 'p', 'Ġf', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'th', 'Ġcommercial', 'Ġmission', 'Ġint', 'els', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'Ġsolar', 'Ġobserv', 'atory', 'Ġmission', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmission', 'w', 'Ġes', 'news', 'sh', 'tml', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġexperts', 'Ġweigh', 'Ġrocket', 'Ġdebris', 'Ġfound', 'Ġh', 'ilton', 'Ġhead', 'http', 'w', 'ist', 'Ġw', 'ist', 'v', 'Ġretrieved', 'Ġarchived', 'Ġmarch', 'Ġway', 'back', 'Ġmachine', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfirst', 'Ġmission', 'htt', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġnational', 'Ġdefense', 'Ġmission', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>['ight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrecovery', 'Ġfailure', 'Ġpreviously', 'Ġï', '¬', 'Ĥ', 'Ġrecovered', 'Ġbooster', 'Ġflight', 'Ġsuccessful', 'Ġstar', 'link', 'Ġlaunch', 'Ġsaw', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfailure', 'Ġmer', 'lin', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġengine', 'Ġascent', 'Ġsecond', 'Ġascent', 'Ġengine', 'Ġfailure', 'Ġrocket', 'Ġfollowing', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġflight', 'Ġcrew', 'Ġdragon', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcrew', 'ed', 'Ġlaunch', 'Ġcrew', 'Ġdragon', 'Ġcarrying', 'Ġtwo', 'Ġastronauts', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcrew', 'ed', 'Ġoperational', 'Ġlaunch', 'Ġcrew', 'Ġdragon', 'Ġholding', 'Ġrecord', 'Ġlongest', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġu', 'Ġcrew', 'Ġvehicle', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġcargo', 'Ġdragon', 'Ġunc', 'rew', 'ed', 'Ġvariant', 'Ġcrew', 'Ġdragon', 'Ġflight', 'Ġtransporter', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdedicated', 'Ġsmall', 'sat', 'Ġrides', 'hare', 'Ġlaunch', 'Ġset', 'Ġrecord', 'Ġsatellites', 'Ġlaunched', 'Ġsingle', 'Ġlaunch', 'Ġsatellites', 'Ġsurpass', 'ing', 'Ġprevious', 'Ġrecord', 'Ġsatellites', 'Ġheld', 'mber', 'Ġlaunch', 'Ġant', 'ares', 'Ġflight', 'Ġroutine', 'Ġstar', 'link', 'Ġlaunch', 'Ġexperienced', 'Ġearly', 'Ġshut', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġmer', 'lin', 'Ġengine', 'Ġascent', 'Ġdue', 'Ġdamage', 'Ġstill', 'Ġdelivered', 'Ġpayload', 'Ġtarget', 'Ġorbit', 'Ġflight', 'Ġinspiration', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġorbital', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'private', 'Ġcrew', 'Ġflight', 'Ġdart', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġplanetary', 'Ġdefenses', 'Ġmission', 'Ġnear', 'earth', 'Ġobjects', 'Ġflight', 'th', 'Ġsuccessful', 'Ġvertical', 'Ġlanding', 'Ġorbital', 'class', 'Ġrocket', 'Ġsixth', 'Ġanniversary', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanding', 'Ġflight', 'Ġheaviest', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġblock', 'Ġpayload', 'Ġstar', 'link', 'Ġsatellites', 'Ġflight', 'th', 'Ġconsecutive', 'Ġsuccessful', 'Ġfal', 'con', 'Ġmission', 'Ġflight', 'th', 'Ġoverall', 'Ġsuccessful', 'Ġbooster', 'Ġlanding', 'Ġtwo', 'stage', 'Ġl', 'ox', 'r', 'p', 'powered', 'Ġlaunch', 'Ġvehicle', 'Ġfirst', 'Ġstage', 'Ġheight', 'Ġft', 'Ġheight', 'Ġinter', 'stage', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'Ġlithium', 'Ġskin']</t>
+          <t>['united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecond', 'Ġmission', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'las', 'Ġwik', 'ipedia', 'ula', 'Ġsuccessfully', 'Ġlaunches', 'Ġfifth', 'Ġn', 'ro', 'Ġmission', 'Ġseven', 'Ġmonths', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'sb', 'irs', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġjun', 'Ġspacecraft', 'Ġfive', 'year', 'Ġjourney', 'Ġstudy', 'Ġj', 'upiter', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġhar', 'wood', 'iam', 'mber', 'ars', 'Ġscience', 'Ġlaboratory', 'Ġbegins', 'Ġcruise', 'Ġred', 'Ġplanet', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'chall', 'enge', 'Ġgetting', 'Ġmars', 'Ġchapter', 'Ġlaunching', 'Ġcuriosity', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġr', 'ik', 'sle', 'ws', 'ki', 'mber', 'us', 'Ġmart', 'ian', 'Ġn', 'uke', 'ruck', 'Ġlaunches', 'Ġwithout', 'Ġhitch', '..."', 'Ġregister', 'Ġarchived', 'Ġoriginal', 'ms', 'l', 'launch', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'th', 'Ġcent', 'aur', 'Ġsuccessfully', 'Ġlaunches', 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġmission', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġray', 'Ġfe', 'b', 'ruary', 'land', 'mark', 'Ġlaunch', 'Ġrocket', 'ry', 'Ġcent', 'aur', 'Ġset', 'Ġflight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġent', 'aur', 'Ġapr', 'il', 'Ġgra', 'ham', 'iam', 'Ġber', 'gin', 'Ġch', 'ris', 'mber', 'Ġhanded', 'Ġus', 'af', 'Ġcompleting', 'orbit', 'Ġtesting', 'nas', 'asp', 'Ġing', 'Ġnas', 'asp', 'ace', 'ï', '¬']</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>['Ġaluminum', 'Ġdom', 'es', 'Ġlanding', 'Ġlegs', 'Ġnumber', 'Ġmaterial', 'Ġcarbon', 'Ġï', '¬', 'ģ', 'ber', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġnumber', 'Ġmer', 'lin', 'Ġengines', 'Ġsea', 'Ġlevel', 'Ġpropell', 'ant', 'Ġthrust', 'Ġsea', 'Ġlevel', 'Ġkn', '000', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'sea', 'level', 'Ġsec', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'v', 'ac', 'uum', 'Ġsec', 'Ġsec', 'Ġburn', 'Ġtime', 'Ġsec', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġsecond', 'Ġstage', 'Ġdesign', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġinteractive', 'Ġmodel', 'Ġfal', 'con', 'Ġfully', 'Ġintegrated', 'Ġleft', 'Ġexploded', 'Ġview', 'Ġright', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'Ġlithium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġnumber', 'Ġmer', 'lin', 'Ġengines', 'Ġvacuum', 'Ġpropell', 'ant', 'Ġthrust', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'v', 'ac', 'uum', 'Ġsec', 'Ġburn', 'Ġtime', 'Ġsec', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengine', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġstages', 'Ġequipped', 'Ġmer', 'lin', 'Ġrocket', 'Ġengines', 'Ġevery', 'Ġmer', 'lin', 'Ġengine', 'Ġproduces', 'Ġkn', '000', 'Ġthrust', 'Ġuse', 'Ġpy', 'roph', 'oric', 'Ġmixture', 'te', 'te', 'b', 'Ġengine', 'Ġign', 'iter', 'Ġbooster', 'Ġstage', 'Ġengines', 'Ġarranged', 'Ġcon', 'g', 'uration', 'Ġspace', 'x', 'Ġcalls', 'Ġoct', 'aw', 'eb', 'Ġsecond', 'Ġstage', 'Ġfal', 'con', 'Ġshort', 'Ġregular', 'Ġnozzle', 'Ġmer', 'lin', 'Ġvacuum', 'Ġengine', 'Ġversion', 'Ġfal', 'con', 'Ġcapable', 'Ġlosing', 'Ġengines', 'Ġstill', 'Ġcomplete', 'Ġmission', 'Ġburning', 'Ġremaining', 'Ġengines', 'Ġlonger', 'Ġmer', 'lin', 'Ġrocket', 'Ġengine', 'Ġcontrolled', 'Ġthree', 'Ġvoting', 'Ġcomputers', 'Ġcp', 'us', 'Ġconstantly', 'Ġcheck', 'Ġtrio', 'Ġmer', 'lin', 'Ġengines', 'Ġvector', 'Ġthrust', 'Ġadjust', 'Ġtrajectory', 'Ġpropell', 'ant', 'Ġtank', 'Ġwalls', 'Ġdom', 'es']</t>
+          <t>['Ĥ', 'ight', 'Ġretrieved', 'mber', 'Ġarchived', 'htt', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġgra', 'ham', 'iam', 'Ġse', 'pt', 'ember', 'ula', 'las', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġlaunches', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġthird', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'ala', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġtracking', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġray', 'las', 'Ġrocket', 'Ġlaunch', 'Ġcontinues', 'Ġlegacy', 'Ġlands', 'http', 'sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'web', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecond', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'b', 'irs', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'w', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'ula', 'Ġlaunches', 'th', 'Ġsuccessful', 'Ġmission', 'Ġmonths', 'Ġlaunch', 'Ġsatellite', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'Ġsuccessfully', 'Ġlaunches', 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġmission', 'Ġu', 'Ġnavy', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'Ġsuccessfully', 'Ġlaunches', 'aven', 'Ġmission', 'Ġjourney', 'Ġred', 'Ġplanet', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1127,7 +1127,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>['Ġmade', 'Ġaluminium', 'âĢĵ', 'l', 'ith', 'ium', 'Ġalloy', 'Ġspace', 'x', 'Ġuses', 'Ġfriction', 'st', 'ir', 'Ġweld', 'ed', 'Ġtank', 'Ġstrength', 'Ġreliability', 'Ġsecond', 'Ġstage', 'Ġtank', 'Ġshorter', 'Ġversion', 'Ġfirst', 'Ġstage', 'Ġtank', 'Ġuses', 'Ġtool', 'ing', 'Ġmaterial', 'Ġmanufacturing', 'Ġtechniques', 'Ġinter', 'stage', 'Ġconnects', 'Ġupper', 'Ġlower', 'Ġstages', 'Ġcarbon', 'f', 'ib', 'Ġaluminium', 'core', 'Ġcomposite', 'Ġstructure', 'Ġholds', 'Ġreusable', 'Ġseparation', 'Ġcol', 'lets', 'Ġp', 'ne', 'umatic', 'Ġpus', 'Ġsystem', 'Ġoriginal', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġtwelve', 'Ġattachment', 'Ġpoints', 'Ġreduced', 'Ġthree', 'Ġfal', 'con', 'Ġuses', 'Ġpayload', 'Ġfair', 'ing', 'n', 'ose', 'Ġcone', 'Ġprotect', 'non', 'dragon', 'Ġsatellites', 'Ġlaunch', 'Ġfair', 'ing', 'Ġft', 'Ġlong', 'Ġft', 'Ġdiameter', 'Ġweighs', 'Ġapproximately', 'Ġconstructed', 'Ġcarbon', 'Ġfiber', 'Ġskin', 'Ġoverl', 'aid', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġcore', 'Ġspace', 'x', 'Ġdesigned', 'Ġfabric', 'ates', 'Ġfair', 'ings', 'Ġhaw', 'th', 'orne', 'Ġtesting', 'Ġcompleted', 'Ġn', 'asa', "'s", 'Ġplum', 'Ġbro', 'ok', 'Ġstation', 'Ġfacility', 'Ġspring', 'Ġacoustic', 'Ġshock', 'Ġmechanical', 'Ġvibration', 'Ġlaunch', 'Ġplus', 'Ġelectromagnetic', 'Ġstatic', 'Ġdischarge', 'Ġconditions', 'Ġsimulated', 'Ġfull', 'size', 'Ġtest', 'Ġarticle', 'Ġvacuum', 'Ġchamber', 'Ġsince', 'Ġfair', 'ings', 'Ġdesigned', 'enter', 'Ġearth', "'s", 'Ġatmosphere', 'Ġreused', 'Ġfuture', 'Ġmissions', 'Ġengine', 'Ġtanks', 'Ġfair', 'ing', 'Ġcontrol', 'Ġsystems', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġlaunched', 'Ġdragon', 'Ġspacecraft', 'Ġdeliver', 'Ġcargo', 'Ġiss', 'Ġfal', 'con', 'left', 'right', 'Ġengine', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġv', 'enberg', 'fal', 'con', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġuses', 'Ġmultiple', 'Ġredundant', 'Ġflight', 'Ġcomputers', 'Ġfault', 'oler', 'ant', 'Ġdesign', 'Ġsoftware', 'Ġruns', 'Ġlinux', 'Ġwritten', 'Ġflexibility', 'Ġcommercial', 'lf', 'Ġparts', 'Ġsystem', 'wide', 'Ġradiation', 'oler', 'ant', 'Ġdesign', 'Ġused', 'Ġinstead', 'Ġrad', 'hard', 'ened', 'Ġparts', 'Ġstage', 'Ġstage', 'level', 'Ġflight', 'Ġcomputers', 'Ġaddition', 'Ġmer', 'lin', 'specific', 'Ġengine', 'Ġcontrollers', 'Ġfault', 'oler', 'ant', 'Ġtri', 'ad', 'Ġdesign', 'Ġhandle', 'Ġstage', 'Ġcontrol', 'Ġfunctions', 'Ġengine', 'Ġmicro', 'controller', 'Ġruns', 'Ġpower', 'pc', 'Ġarchitecture', 'Ġboosters', 'Ġdeliberately', 'Ġexpended', 'Ġlegs']</t>
+          <t>['Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġu', 'la', 'Ġarchived', 'Ġoriginal', 'Ġe', 'ws', 'sh', 'tml', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġtracking', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġpayload', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġair', 'Ġforce', "'s", 'Ġweather', 'Ġsatellite', 'Ġorbit', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecond', 'Ġmission', 'Ġseven', 'Ġdays', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfour', 'Ġmissions', 'Ġseven', 'Ġweeks', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġtwo', 'Ġrockets', 'Ġfour', 'Ġdays', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġlaunches', 'Ġworldview', 'Ġsatellite', 'Ġdigital', 'gl', 'obe', 'Ġg', 'ital', 'gl', 'obe', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġig', 'ital', 'gl', 'obe', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'ula', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecretive', 'Ġcl', 'io', 'Ġmission', 'Ġse', 'pt', 'ember', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġwik', 'ipedia', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'th', 'Ġmission', 'Ġcape', 'aver', 'al', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'orb', 'ital', 'Ġdebris', 'Ġquarterly', 'Ġnews', 'Ġn', 'asa', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'th', 'las', 'Ġrocket', 'ht', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober']</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>['Ġfins', 'Ġrecover', 'able', 'Ġboosters', 'Ġinclude', 'Ġfour', 'Ġext', 'ensible', 'Ġlanding', 'Ġlegs', 'Ġattached', 'Ġaround', 'Ġbase', 'Ġcontrol', 'Ġcore', "'s", 'Ġdescent', 'Ġatmosphere', 'Ġspace', 'x', 'Ġuses', 'Ġgrid', 'Ġfins', 'Ġdeploy', 'Ġvehicle', 'Ġmoments', 'Ġstage', 'Ġseparation', 'Ġflew', 'Ġfive', 'Ġsuccessful', 'Ġorbital', 'Ġlaunches', 'âĢĵ', 'Ġmuch', 'Ġlarger', 'Ġmade', 'Ġfirst', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġdemonstration', 'Ġmission', 'Ġcarried', 'Ġsmall', 'Ġprimary', 'Ġpayload', 'Ġcass', 'ope', 'Ġsatellite', 'Ġlarger', 'Ġpayload', 'Ġfollowed', 'Ġstarting', 'Ġlaunch', 'Ġgeo', 'Ġcommunications', 'Ġsatellite', 'Ġused', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicles', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmade', 'Ġfirst', 'Ġflight', 'Ġde', 'cember', 'Ġfirst', 'Ġstage', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġreusable', 'Ġcurrent', 'Ġversion', 'Ġknown', 'Ġfal', 'con', 'Ġblock', 'Ġmade', 'Ġfirst', 'Ġflight', 'Ġmay', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'Ġdeveloped', 'âĢĵ', 'Ġflew', 'Ġfirst', 'Ġtime', 'Ġmade', 'Ġfive', 'Ġflights', 'Ġretired', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġnine', 'Ġmer', 'lin', 'Ġengines', 'Ġarranged', 'Ġgrid', 'Ġsea', 'level', 'Ġthrust', 'Ġkn', '000', 'Ġtotal', 'Ġlif', 'ff', 'Ġthrust', '000', 'Ġkn', '000', 'Ġsecond', 'Ġstage', 'Ġpowered', 'Ġsingle', 'Ġmer', 'lin', 'Ġengine', 'Ġmodified', 'Ġvacuum', 'Ġoperation', 'Ġexpansion', 'Ġratio', 'Ġnominal', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġg', 'ase', 'ous', 'Ġthr', 'usters', 'Ġused', 'Ġsecond', 'stage', 'Ġreaction', 'Ġcontrol', 'Ġsystem', 'Ġearly', 'Ġattempts', 'Ġadd', 'Ġlightweight', 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġbooster', 'Ġstage', 'Ġparachute', 'Ġrecovery', 'Ġsuccessful', 'Ġspace', 'x', 'Ġbegan', 'Ġformal', 'Ġdevelopment', 'Ġprogram', 'Ġreusable', 'Ġfal', 'con', 'Ġinitially', 'Ġfocusing', 'Ġfirst', 'Ġstage', 'Ġheavier', 'Ġthrust', 'Ġnine', 'Ġpowerful', 'Ġmer', 'lin', 'Ġengines', 'Ġrearr', 'anged', 'oct', 'agonal', 'Ġpattern', 'Ġspace', 'x', 'Ġcalled', 'Ġoct', 'aw', 'eb', 'Ġdesigned', 'Ġsimplify', 'Ġstream', 'line', 'Ġfuel', 'Ġtanks', 'Ġlonger', 'Ġmaking', 'Ġrocket', 'Ġsusceptible', 'Ġbending', 'Ġflight', 'Ġfirst', 'Ġstage', 'Ġoffered', 'Ġtotal', 'Ġsea', 'level', 'Ġthrust', 'Ġlif', 'ff', 'Ġkil', 'onew', 'tons', '000', 'Ġengines', 'Ġburning', 'Ġnominal', 'Ġseconds', 'Ġstage', 'Ġthrust', 'Ġrises', 'Ġkn', '000']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġu', 'Ġnavy', "'s", 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġx', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsolar', 'Ġprobes', 'Ġstudy', 'Ġspace', 'Ġweather', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġglobal', 'Ġpositioning', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġx', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġu', 'Ġnavy', "'s", 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'h', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġreaches', 'Ġsuccessful', 'Ġmissions', 'los', 'Ġsatellite', 'ite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġsatellite', 'Ġoct', 'ober', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'air', 'force', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġcy', 'gn', 'us', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>['Ġbooster', 'Ġclimbs', 'Ġatmosphere', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġredesigned', 'Ġreduce', 'Ġnumber', 'Ġattachment', 'Ġpoints', 'Ġtwelve', 'Ġthree', 'Ġvehicle', 'Ġupgraded', 'Ġav', 'ionics', 'Ġsoftware', 'Ġimprovements', 'Ġincreased', 'Ġpayload', 'Ġcapability', '000', '000', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġstated', 'Ġpayload', 'Ġcapacity', 'Ġpublished', 'Ġprice', 'Ġlist', 'Ġextra', 'Ġmargin', 'Ġreserved', 'Ġreturning', 'Ġstages', 'Ġvia', 'Ġpowered', 'entry', 'Ġdevelopment', 'Ġtesting', 'Ġfirst', 'Ġstage', 'Ġcompleted', 'Ġj', 'uly', 'Ġfirst', 'Ġlaunch', 'Ġcame', 'Ġse', 'pt', 'ember', 'Ġsecond', 'Ġstage', 'Ġign', 'iter', 'Ġpropell', 'ant', 'Ġlines', 'Ġlater', 'Ġinsulated', 'Ġbetter', 'Ġsupport', 'space', 'Ġrestart', 'Ġfollowing', 'Ġlong', 'Ġcoast', 'Ġphases', 'Ġorbital', 'Ġtrajectory', 'Ġmaneuvers', 'Ġfour', 'Ġext', 'ensible', 'Ġcarbon', 'Ġfiber', 'al', 'uminum', 'Ġhoney', 'comb', 'Ġlanding', 'Ġlegs', 'Ġincluded', 'Ġlater', 'Ġflights', 'Ġland', 'ings', 'Ġlegs', 'ï', '¬', 'ģ', 'ns', 'Ġversions', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġclose', 'Ġnewer', 'Ġtitanium', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'Ġsecond', 'Ġir', 'idium', 'Ġnext', 'Ġmission', 'Ġj', 'une', 'Ġspace', 'x', 'Ġpricing', 'Ġpayload', 'Ġspecifications', 'Ġpublished', 'Ġmarch', 'Ġincluded', 'Ġperformance', 'Ġpublished', 'Ġprice', 'Ġlist', 'Ġindicated', 'Ġspace', 'x', 'Ġreserved', 'Ġadditional', 'Ġperformance', 'Ġperform', 'us', 'ability', 'Ġtesting', 'Ġmany', 'Ġengineering', 'Ġchanges', 'Ġsupport', 'us', 'ability', 'Ġrecovery', 'Ġfirst', 'Ġstage', 'Ġmade', 'Ġupgrade', 'Ġalso', 'Ġknown', 'Ġfull', 'Ġthrust', 'Ġmade', 'Ġmajor', 'Ġchanges', 'Ġadded', 'Ġcry', 'ogenic', 'Ġpropell', 'ant', 'Ġcooling', 'Ġincrease', 'Ġdensity', 'Ġallowing', 'Ġhigher', 'Ġthrust', 'Ġimproved', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġstretched', 'Ġsecond', 'Ġstage', 'Ġhold', 'Ġadditional', 'Ġpropell', 'ant', 'Ġstrengthened', 'Ġstr', 'uts', 'Ġholding', 'Ġhelium', 'Ġbottles', 'Ġbelieved', 'Ġinvolved', 'Ġfailure', 'Ġflight', 'Ġoffered', 'Ġreusable', 'Ġfirst', 'Ġstage', 'Ġplans', 'Ġreuse', 'Ġsecond', 'stage', 'Ġabandoned', 'Ġweight', 'Ġheat', 'Ġshield', 'Ġequipment', 'Ġwould', 'Ġreduce', 'Ġpayload', 'Ġreusable', 'Ġbooster', 'Ġdeveloped', 'Ġusing', 'Ġsystems', 'Ġsoftware', 'Ġtested', 'Ġfal', 'con', 'Ġprototypes', 'Ġautonomous', 'Ġflight', 'Ġsafety', 'Ġsystem', 'af', 'ss', 'Ġreplaced', 'Ġground', 'based', 'Ġmission', 'Ġflight', 'Ġcontrol', 'Ġpersonnel', 'Ġequipment', 'Ġaf', 'ss', 'Ġoffered', 'board', 'Ġpositioning', 'Ġnavigation', 'Ġtiming', 'Ġsources', 'Ġdecision', 'Ġlogic', 'Ġbenefits', 'Ġaf', 'ss', 'Ġincluded', 'Ġincreased', 'Ġpublic', 'Ġsafety', 'Ġreduced', 'Ġreliance', 'Ġrange', 'Ġinfrastructure']</t>
+          <t>['Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpounds', 'Ġcargo', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġu', 'Ġnavy', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġos', 'iris', 'rex', 'Ġspacecraft', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'n', 'asa', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġworldview', 'Ġdigital', 'gl', 'obe', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġarchived', 'Ġobe', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġgoes', 'r', 'Ġsatellite', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'las', 'Ġwik', 'ipedia', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġe', 'ch', 'ost', 'ar', 'Ġsatellite', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'http', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'Ġu', 'air', 'force', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload']</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>['Ġreduced', 'Ġrange', 'Ġspac', 'el', 'ift', 'Ġcost', 'Ġincreased', 'Ġschedule', 'Ġpredict', 'ability', 'Ġavailability', 'Ġoperational', 'Ġflexibility', 'Ġlaunch', 'Ġslot', 'Ġflexibility', '".[', 'Ġft', "'s", 'Ġcapacity', 'Ġallowed', 'Ġspace', 'x', 'Ġchoose', 'Ġincreasing', 'Ġpayload', 'Ġdecreasing', 'Ġlaunch', 'Ġprice', 'Ġfirst', 'Ġsuccessful', 'Ġlanding', 'Ġcame', 'Ġde', 'cember', 'Ġfirst', 'Ġref', 'light', 'Ġmarch', 'Ġfe', 'b', 'ruary', 'Ġcr', 'Ġlaunch', 'Ġfirst', 'Ġoperational', 'Ġlaunch', 'Ġutilizing', 'Ġaf', 'ss', 'Ġspace', 'x', 'Ġlaunches', 'Ġmarch', 'Ġused', 'Ġaf', 'ss', 'Ġj', 'une', 'Ġmission', 'Ġcarried', 'Ġsecond', 'Ġbatch', 'Ġten', 'Ġir', 'idium', 'Ġnext', 'Ġsatellites', 'Ġaluminium', 'Ġgrid', 'Ġfins', 'Ġreplaced', 'Ġlarger', 'Ġtitanium', 'Ġversions', 'Ġimprove', 'Ġcontrol', 'Ġauthority', 'Ġheat', 'Ġtolerance', 'entry', 'Ġspace', 'x', 'Ġstarted', 'Ġincluding', 'Ġincremental', 'Ġchanges', 'Ġinternally', 'Ġdubbed', 'Ġblock', 'Ġinitially', 'Ġsecond', 'Ġstage', 'Ġmodified', 'Ġblock', 'Ġstandards', 'Ġflying', 'Ġtop', 'Ġblock', 'Ġfirst', 'Ġstage', 'Ġthree', 'Ġmissions', 'ars', 'Ġmay', 'Ġint', 'els', 'Ġj', 'uly', 'Ġblock', 'Ġdescribed', 'Ġtransition', 'Ġfull', 'Ġthrust', 'Ġblock', 'Ġblock', 'Ġincludes', 'Ġincremental', 'Ġengine', 'Ġthrust', 'Ġupgrades', 'Ġleading', 'Ġblock', 'Ġmaiden', 'Ġflight', 'Ġfull', 'Ġblock', 'Ġdesign', 'first', 'Ġsecond', 'Ġstages', 'Ġspace', 'x', 'Ġcr', 'Ġmission', 'Ġaug', 'ust', 'Ġv', 'full', 'Ġthrust', 'Ġblock', 'Ġblock', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġoct', 'ober', 'Ġmus', 'k', 'Ġdescribed', 'Ġblock', 'Ġcoming', 'Ġlot', 'Ġminor', 'Ġrefin', 'ements', 'Ġcollectively', 'Ġimportant', 'rated', 'Ġthrust', 'Ġimproved', 'Ġlegs', 'Ġsignificant', '".[', 'Ġjan', 'uary', 'Ġmus', 'k', 'Ġadded', 'Ġblock', 'sign', 'ificantly', 'Ġimproves', 'Ġperformance', 'Ġease', 'us', 'ability', '".[', 'Ġmaiden', 'Ġflight', 'Ġtook', 'Ġplace', 'Ġmay', 'Ġbang', 'aband', 'hu', 'Ġsatellite', 'Ġsatellite', 'Ġblock', 'Ġsecond', 'Ġstage', 'Ġincluded', 'Ġupgrades', 'Ġenable', 'Ġlinger', 'Ġorbit', 'Ġreign', 'ite', 'Ġengine', 'Ġthree', 'Ġtimes', 'Ġversion', 'ret', 'ired', 'ret', 'ired', 'Ġfull', 'Ġthrust', 'Ġblock', 'Ġblock', 'ret', 'ired', 'Ġblock', 'active', ')[', 'Ġstage', 'Ġengines', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġmer', 'lin', 'graded', ')[', 'Ġmer', 'lin', 'graded', 'Ġstage']</t>
+          <t>['Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġul', 'al', 'aunch', 'Ġarchived', 'web', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġire', 'ne', 'Ġapr', 'il', 'las', 'Ġrocket', 'Ġlaunches', 'Ġprivate', 'Ġcy', 'gn', 'us', 'Ġcargo', 'Ġship', 'Ġspace', 'Ġstation', 'Ġspace', 'Ġarchived', 'http', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġtd', 'rs', 'Ġsatellite', 'Ġul', 'al', 'aunch', 'Ġarchived', 'Ġr', 'sm', 'aspx', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'http', 'ul', 'al', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġgra', 'ham', 'iam', 'Ġoct', 'ober', 'las', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġlaunches', 'Ġarchived', 'web', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġmission', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġgoes', 'Ġweather', 'Ġsatellite', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġn', 'aa', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmission', 'Ġu', 'Ġair', 'Ġforce', '.-', 'air', 'force', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġwest', 'Ġcoast', "'s", 'Ġfirst', 'Ġinter', 'plan', 'etary', 'Ġmission', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmission', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmaple', 'Ġleaf', 'Ġse', 'pt', 'ember']</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>['Ġmass', 'Ġdry', 'Ġmass', '000', 'Ġstage', 'Ġengines', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmer', 'lin', 'Ġvacuum', 'graded', ')[', 'Ġmer', 'lin', 'Ġvacuum', 'graded', 'short', 'Ġregular', 'Ġnozzle', 'Ġstage', 'Ġmass', 'Ġdry', 'Ġmass', 'Ġheight', 'Ġdiameter', 'Ġinitial', 'Ġthrust', 'Ġtf', ')[', 'Ġtakeoff', 'Ġmass', '000', '000', '000', '000', 'Ġfair', 'ing', 'Ġdiameter', 'ĠâĢĶ', 'Ġfair', 'ing', 'Ġmass', 'Ġpayload', 'Ġle', 'Ġcape', 'aver', 'al', 'âĢĵ', '000', 'exp', 'end', 'able', ')[', 'b', 'exp', 'end', 'able', 'usable', ')[', 'c', 'Ġpayload', 'Ġg', 'exp', 'end', 'able', 'usable', 'exp', 'end', 'able', 'usable', ')[', 'Ġsuccess', 'Ġratio', 'Ġpre', 'cluded', ')[', 'f', 'Ġfal', 'con', 'Ġlaunched', 'Ġdragon', 'Ġspacecraft', 'Ġnever', 'Ġlaunched', 'Ġclam', 'shell', 'Ġpayload', 'Ġfair', 'ing', 'Ġb', 'Ġpayload', 'Ġrestricted', '000', 'Ġdue', 'Ġstructural', 'Ġlimit', 'Ġpayload', 'Ġadapter', 'Ġï', '¬', 'ģ', 'ting', 'p', 'af', ').[', 'Ġc', 'Ġheaviest', 'Ġexplicitly', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġpayload', 'Ġspace', 'x', 'Ġprimary', 'Ġpayload', 'Ġdragon', 'Ġsuccessful', 'Ġsecondary', 'Ġpayload', 'Ġplaced', 'Ġincorrect', 'Ġorbit', 'Ġchanged', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġpro', 'ï', '¬', 'ģ', 'le', 'Ġdue', 'Ġmalfunction', 'Ġshut', 'Ġsingle', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġengine', 'Ġlikely', 'Ġenough', 'Ġfuel', 'Ġoxid', 'izer', 'Ġremained', 'Ġsecond', 'Ġstage']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'z', 'ador', 'Ġph', 'ill', 'ip', 'aug', 'ust', 'orb', 'ital', 'Ġdebris', 'Ġquarterly', 'Ġnews', 'Ġn', 'asa', 'Ġorbital', 'Ġn', 'asa', 'break', 'las', 'Ġcent', 'aur', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġcommunications', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'star', 'liner', 'Ġsuffers', 'Ġmission', 'short', 'ening', 'Ġfailure', 'Ġsuccessful', 'Ġlaunch', 'htt', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsolar', 'Ġorbit', 'er', 'Ġstudy', 'Ġsun', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfirst', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġmission', 'Ġu', 'Ġspace', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsixth', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġspace', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġstr', 'ick', 'land', 'Ġash', 'ley', 'Ġj', 'uly', 'ars', 'Ġlaunch', 'Ġn', 'asa', 'Ġsends', 'Ġpersever', 'ance', 'Ġrover', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'rol', 'Ġmission', 'Ġsupport', 'Ġnational', 'Ġsecurity', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġmission', 'Ġsupport', 'Ġnational', 'Ġsecurity', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ula', 'Ġdelays', 'Ġuse', 'Ġenhanced', 'Ġupper', 'stage', 'Ġengine', 'Ġpending', 'Ġstudies', 'Ġspac', 'en', 'ews', 'Ġj', 'une', 'Ġne', 'al', 'Ġle', 'e', 'Ġkan', 'ay', 'ama', 'Ġse', 'pt', 'ember', 'n', 'asa', "'s", 'Ġlands', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'enberg', 'Ġarchived', 'Ġch', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġwik', 'ipedia']</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>['Ġorbital', 'Ġinsertion', 'Ġenough', 'Ġwithin', 'Ġn', 'asa', 'Ġsafety', 'Ġmargins', 'Ġprotection', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġe', 'Ġfailed', 'Ġmission', 'Ġfal', 'con', 'Ġspace', 'x', 'Ġlost', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġoperation', 'Ġdue', 'pressure', 'Ġevent', 'Ġsecond', 'Ġstage', 'Ġtank', 'Ġf', 'Ġone', 'Ġrocket', 'Ġpayload', 'Ġdestroyed', 'Ġlaunch', 'Ġpreparation', 'Ġroutine', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġachieved', 'Ġfull', 'Ġmission', 'Ġsuccesses', '%).', 'Ġspace', 'x', 'Ġsucceeded', 'Ġprimary', 'Ġmission', 'Ġleft', 'Ġsecondary', 'Ġpayload', 'Ġwrong', 'Ġorbit', 'Ġspace', 'x', 'Ġdestroyed', 'Ġflight', 'Ġaddition', 'Ġdisinteg', 'rated', 'Ġlaunch', 'Ġpad', 'Ġfueling', 'Ġengine', 'Ġtest', 'Ġbased', 'Ġpoint', 'Ġestimation', 'Ġestimate', 'Ġreliability', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġbecome', 'Ġreliable', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġoperation', 'Ġblock', 'Ġsuccess', 'Ġrate', 'Ġcomparison', 'Ġindustry', 'Ġbenchmark', 'Ġseries', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', 'Ġlatest', 'Ġsuccess', 'Ġrate', '%),', 'Ġr', 'ussian', 'Ġpro', 'ton', 'Ġseries', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', 'Ġlatest', 'Ġpro', 'ton', "'s", 'Ġsuccess', 'Ġrate', '%),', 'Ġeuro', 'pe', 'ri', 'ane', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', '%,', 'Ġch', 'inese', 'Ġlong', 'Ġmarch', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', '%.', 'Ġlaunch', 'Ġsequence', 'Ġincludes', 'Ġhold', 'Ġfeature', 'Ġallows', 'Ġfull', 'Ġengine', 'Ġignition', 'Ġsystems', 'Ġcheck', 'Ġlif', 'ff', 'Ġfirst', 'stage', 'Ġengine', 'Ġstarts', 'Ġlauncher', 'Ġheld', 'Ġreleased', 'Ġflight', 'Ġpropulsion', 'Ġvehicle', 'Ġsystems', 'Ġconfirmed', 'Ġoperating', 'Ġnormally', 'Ġsimilar', 'Ġhold', 'Ġsystems', 'Ġused', 'Ġlaunch', 'Ġvehicles', 'Ġsat', 'urn', 'Ġspace', 'Ġshuttle', 'Ġautomatic', 'Ġsafe', 'Ġshut', 'cap', 'abilities', 'Ġperformance', 'Ġreliability', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġun', 'loading', 'Ġpropell', 'ant', 'Ġoccur', 'Ġabnormal', 'Ġconditions', 'Ġdetected', 'Ġprior', 'Ġlaunch', 'Ġdate', 'Ġspace', 'x', 'Ġtypically', 'Ġcompletes', 'Ġtest', 'Ġcycle', 'Ġculminating', 'Ġthree', 'half', 'Ġsecond', 'Ġfirst', 'Ġstage', 'Ġengine', 'Ġstatic', 'Ġfiring', 'Ġtriple', 'red', 'und', 'ant', 'Ġflight', 'Ġcomputers', 'Ġinert', 'ial', 'Ġnavigation', 'Ġoverlay', 'Ġadditional']</t>
+          <t>['Ġwar', 'ren', 'Ġhay', 'gen', 'Ġoct', 'ober', 'n', 'asa', 'Ġu', 'la', 'Ġlaunch', 'Ġhistoric', 'Ġl', 'u', 'cy', 'Ġmission', 'Ġretrieved', 'Ġoct', 'ober', 'Ġf', 'letcher', 'Ġcol', 'Ġde', 'cember', 'ula', 'Ġlaunches', 'las', 'Ġlong', 'Ġduration', 'Ġmission', 'Ġspace', 'Ġforce', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġde', 'cember', 'Ġgra', 'ham', 'iam', 'Ġjan', 'uary', 'ula', "'s", 'las', 'Ġlaunches', 'Ġsatellite', 'ins', 'pection', 'Ġmission', 'Ġspace', 'Ġforce', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġkan', 'ay', 'ama', 'Ġle', 'e', 'Ġmarch', 'Ġn', 'asa', "'s", 'Ġgoes', 'Ġweather', 'Ġsatellite', 'Ġlaunches', 'Ġu', 'la', 'las', 'Ġv', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġmarch', 'Ġgra', 'ham', 'iam', 'Ġmay', 'star', 'liner', 'Ġlaunch', 'Ġmakes', 'Ġorbit', 'Ġheading', 'Ġiss', 'Ġr', 'oft', 'launch', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġmay', 'Ġgra', 'ham', 'iam', 'Ġj', 'uly', 'las', 'Ġlaunches', 'Ġtwo', 'Ġexperimental', 'Ġmilitary', 'Ġsatellites', 'Ġus', 'sf', 'Ġmission', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġj', 'uly', 'Ġgra', 'ham', 'iam', 'Ġaug', 'ust', 'ula', "'s", 'las', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'n', 'al', 'b', 'irs', 'Ġgeo', 'Ġmissile', 'Ġdetection', 'Ġsatellite', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġaug', 'ust', 'Ġkan', 'ay', 'ama', 'Ġle', 'e', 'Ġoct', 'ober', 'final', 'las', 'Ġlaunches', 'Ġdual', 'es', 'es', 'Ġsatellites', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'mber', 'las', 'Ġrocket', 'Ġbids', 'Ġfarewell', 'Ġcal', 'ornia', 'Ġu', 'la', 'Ġread', 'ies', 'Ġvul', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'mber', 'ula', 'las', 'Ġretire', 'Ġmissions', 'Ġbo', 'e', 'ing', 'lock', 'heed', "'s", 'Ġventure', 'Ġstops', 'Ġsale', 'Ġrocket', 'Ġh', 'tm', 'Ġaug', 'ust', 'status', 'Ġhot', 'bird', 'Ġretrieved', 'mber', 'new', 'Ġhor', 'izons', 'Ġpl', 'uto', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġfly', 'Ġhor', 'izons', 'htm', 'Ġsolar', 'views', 'Ġretrieved', 'mber', 'Ġray', 'las', 'Ġrocket', 'Ġsends']</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>['Ġaccuracy', 'Ġlike', 'Ġsat', 'urn', 'Ġfamily', 'Ġrockets', 'Ġmultiple', 'Ġengines', 'Ġallow', 'Ġmission', 'Ġcompletion', 'Ġeven', 'Ġone', 'Ġfails', 'Ġdetailed', 'Ġdescriptions', 'Ġdestructive', 'Ġengine', 'Ġfailure', 'Ġmodes', 'Ġdesigned', 'Ġengine', 'Ġcapabilities', 'Ġmade', 'Ġpublic', 'Ġspace', 'x', 'Ġemphasized', 'Ġfirst', 'Ġstage', 'Ġdesigned', 'engine', 'Ġcapability', 'Ġoct', 'ober', 'Ġpartial', 'Ġsuccess', 'Ġengine', 'Ġlost', 'Ġpressure', 'Ġseconds', 'Ġshut', 'Ġcompensate', 'Ġresulting', 'Ġloss', 'Ġacceleration', 'Ġfirst', 'Ġstage', 'Ġburn', 'Ġseconds', 'Ġlonger', 'Ġplanned', 'Ġsecond', 'Ġstage', 'Ġburn', 'Ġextra', 'Ġseconds', 'Ġextra', 'Ġburn', 'Ġtime', 'Ġreduced', 'Ġfuel', 'Ġreserves', 'Ġlikelihood', 'Ġsufficient', 'Ġfuel', 'Ġexecute', 'Ġmission', 'Ġdropped', '%.', 'Ġn', 'asa', 'Ġpurchased', 'Ġlaunch', 'Ġtherefore', 'Ġcontract', 'ually', 'Ġcontrolled', 'Ġseveral', 'Ġmission', 'Ġdecision', 'Ġpoints', 'Ġn', 'asa', 'Ġdeclined', 'Ġspace', 'x', "'s", 'Ġrequest', 'Ġrestart', 'Ġsecond', 'Ġstage', 'Ġattempt', 'Ġdeliver', 'Ġsecondary', 'Ġpayload', 'Ġcorrect', 'Ġorbit', 'Ġresult', 'Ġsecondary', 'Ġpayload', 'ent', 'ered', 'Ġatmosphere', 'Ġmer', 'lin', 'Ġengines', 'Ġsuffered', 'Ġtwo', 'Ġpremature', 'Ġshutdown', 'Ġascent', 'Ġneither', 'Ġaffected', 'Ġprimary', 'Ġmission', 'Ġlanding', 'Ġattempts', 'Ġfailed', 'Ġmarch', 'Ġstar', 'link', 'Ġmission', 'Ġone', 'Ġfirst', 'Ġstage', 'Ġengines', 'Ġfailed', 'Ġseconds', 'Ġcut', 'Ġdue', 'Ġignition', 'op', 'rop', 'yl', 'Ġalcohol', 'Ġproperly', 'Ġpur', 'ged', 'Ġcleaning', 'Ġanother', 'Ġstar', 'link', 'Ġmission', 'Ġfe', 'b', 'ruary', 'Ġhot', 'Ġexhaust', 'Ġg', 'asses', 'Ġentered', 'Ġengine', 'Ġdue', 'Ġfatigue', 'related', 'Ġhole', 'Ġcover', 'Ġspace', 'x', 'Ġstated', 'Ġfailed', 'Ġcover', 'highest', '...', 'Ġnumber', 'Ġflights', 'Ġparticular', 'Ġboot', 'cover', 'Ġdesign', 'Ġseen', '."[', 'Ġspace', 'x', 'Ġplanned', 'Ġbeginning', 'Ġmake', 'Ġstages', 'Ġreusable', 'Ġfirst', 'Ġstages', 'Ġearly', 'Ġfal', 'con', 'Ġflights', 'Ġequipped', 'Ġparach', 'utes', 'Ġcovered', 'Ġlayer', 'Ġabl', 'ative', 'Ġc', 'ork', 'Ġallow', 'Ġsurvive', 'Ġatmospheric', 'entry', 'Ġdefeated', 'Ġaccompanying', 'Ġaer', 'odynamic', 'Ġstress', 'Ġheating', 'Ġstages', 'Ġsalt', 'water', 'Ġlate', 'Ġspace', 'x', 'Ġeliminated', 'Ġparach', 'utes', 'Ġfavor', 'Ġpowered', 'Ġdescent', 'Ġdesign', 'Ġcomplete', 'Ġfe', 'b', 'ruary', 'Ġpowered', 'Ġland', 'ings', 'Ġfirst', 'Ġflight', 'tested', 'Ġsub', 'orb', 'ital', 'Ġgrass', 'ho', 'pper', 'Ġrocket']</t>
+          <t>['Ġcy', 'gn', 'us', 'Ġhot', 'Ġpursuit', 'Ġspace', 'Ġstation', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'os', 'iris', 'rex', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġoct', 'ober', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġretrieved', 'mber', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġlands', 'Ġv', 'enberg', 'af', 'Ġu', 'Ġair', 'Ġforce', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'ula', 'Ġdelays', 'Ġfocused', 'Ġprotecting', 'Ġpercent', 'Ġmission', 'Ġsuccess', 'Ġrate', 'Ġr', 'cent', 'success', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfa', 'hey', 'Ġmark', 'Ġse', 'pt', 'ember', 'Ġrocket', 'Ġblows', 'Ġspace', 'Ġinsurers', 'Ġpay', 'Ġarchived', 'http', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'air', 'Ġforce', 'Ġissues', 'Ġsecond', 'Ġupdate', 'Ġregarding', 'las', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġanomaly', 'Ġreview', 'Ġu', 'Ġair', 'Ġforce', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'web', 'arch', 'iv', 'press', 'Ġrelease', 'Ġn', 'ro', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġlaunch', 'Ġupdate', 'press', 'Ġrelease', 'Ġn', 'ro', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'las', 'Ġforced', 'Ġimprov', 'ise', 'uesday', "'s", 'Ġclimb', 'Ġorbit', 'http', 'space', 'press', 'Ġrelease', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġmarch', 'Ġarchived', 'cl', 'imb', 'orbit', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġray', 'new', 'Ġlineup', 'Ġspelled', 'Ġupcoming', 'las', 'Ġrocket', 'Ġlaunches', 'Ġcape', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġfer', 'ster', 'Ġwar', 'ren']</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1218,7 +1218,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>['Ġlow', 'alt', 'itude', 'Ġlow', 'speed', 'Ġdemonstration', 'Ġtest', 'Ġvehicle', 'Ġmade', 'Ġeight', 'Ġvertical', 'Ġland', 'ings', 'Ġincluding', 'second', 'Ġround', 'trip', 'Ġflight', 'Ġaltitude', 'Ġft', 'Ġmarch', 'Ġspace', 'x', 'Ġannounced', 'Ġfirst', 'Ġflight', 'Ġevery', 'Ġbooster', 'Ġwould', 'Ġequipped', 'Ġpowered', 'Ġdescent', 'Ġexplanatory', 'Ġgraphic', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġb', 'arge', 'Ġlanding', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġstage', 'Ġseparation', 'Ġflight', 'Ġplan', 'Ġcalled', 'Ġfirst', 'Ġstage', 'Ġconduct', 'Ġburn', 'Ġreduce', 'entry', 'Ġvelocity', 'Ġsecond', 'Ġburn', 'Ġreaching', 'Ġwater', 'Ġalthough', 'Ġcomplete', 'Ġsuccess', 'Ġstage', 'Ġable', 'Ġchange', 'Ġdirection', 'Ġmake', 'Ġcontrolled', 'Ġentry', 'Ġatmosphere', 'Ġfinal', 'Ġlanding', 'Ġburn', 'Ġthr', 'usters', 'Ġcould', 'Ġovercome', 'Ġaer', 'odynam', 'ically', 'Ġinduced', 'Ġspin', 'Ġcentrif', 'ugal', 'Ġforce', 'Ġdeprived', 'Ġengine', 'Ġfuel', 'Ġleading', 'Ġearly', 'Ġengine', 'Ġshutdown', 'Ġhard', 'Ġsplash', 'Ġfour', 'Ġocean', 'Ġlanding', 'Ġtests', 'Ġbooster', 'Ġattempted', 'Ġlanding', 'ds', 'Ġfloating', 'Ġplatform', 'Ġjan', 'uary', 'Ġrocket', 'Ġincorporated', 'Ġfirst', 'Ġtime', 'Ġorbital', 'Ġmission', 'Ġgrid', 'Ġfin', 'Ġaer', 'odynamic', 'Ġcontrol', 'Ġsurfaces', 'Ġsuccessfully', 'Ġguided', 'Ġship', 'Ġrunning', 'Ġhydraulic', 'Ġfluid', 'Ġcrashing', 'Ġplatform', 'Ġsecond', 'Ġattempt', 'Ġoccurred', 'Ġapr', 'il', 'Ġengine', 'Ġcapability', 'us', 'ability', 'Ġpost', 'mission', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtests', 'Ġlanding', 'Ġattempts', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġsuccessfully', 'Ġlanding', 'ds', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtime', 'Ġfollowing', 'Ġlaunch', 'Ġspace', 'x', 'Ġiss', 'Ġï', '¬', 'ģ', 'r', 'st', 'ï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġmarch', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġrocket', 'Ġdelivered', 'Ġe', 'ut', 'els', 'Ġwest', 'Ġsatellites', 'Ġsupers', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'Ġlaunching', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'Ġmarch', 'Ġlaunch', 'Ġbip', 'ro', 'pell', 'ant', 'Ġvalve', 'Ġbecame', 'Ġstuck', 'Ġpreventing', 'Ġcontrol', 'Ġsystem', 'Ġreacting', 'Ġrapidly', 'Ġenough', 'Ġsuccessful', 'Ġlanding', 'Ġfirst', 'Ġattempt', 'Ġland', 'Ġbooster', 'Ġground', 'Ġpad', 'Ġnear', 'Ġlaunch', 'Ġsite', 'Ġoccurred', 'Ġflight', 'Ġde', 'cember', 'Ġlanding', 'Ġsuccessful', 'Ġbooster', 'Ġfirst', 'Ġtime', 'Ġhistory']</t>
+          <t>['Ġse', 'pt', 'ember', 'ula', 'Ġinvest', 'Ġblue', 'Ġorigin', 'Ġengine', 'Ġr', 'Ġreplacement', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ike', 'Ġgr', 'uss', 'Ġapr', 'il', 'ula', "'s", 'Ġnext', 'Ġrocket', 'Ġnamed', 'Ġvul', 'Ġspac', 'en', 'ews', 'ike', 'Ġgr', 'uss', 'Ġapr', 'il', 'ula', "'s", 'Ġvul', 'Ġrocket', 'Ġrolled', 'Ġstages', 'Ġg', 'es', 'Ġspac', 'en', 'ews', 'ler', 'Ġamy', 'Ġmay', 'indust', 'ry', 'Ġteam', 'Ġhopes', 'Ġresurrect', 'las', 'Ġpost', 'Ġr', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'ula', 'Ġstudying', 'Ġlong', 'term', 'Ġupgrades', 'Ġvul', 'Ġamy', 'ler', 'Ġapr', 'il', 'ula', 'Ġce', 'Ġcalls', 'Ġavailability', 'Ġdate', 'Ġengine', 'rid', 'ic', 'ulous', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'une', 'expl', 'os', 'ive', 'Ġtest', 'Ġpushes', 'st', 'Ġu', 'la', 'Ġvul', 'Ġrocket', 'Ġlaunch', 'Ġleast', 'Ġj', 'une', 'Ġce', 'Ġsays', 'Ġms', 'n', 'Ġretrieved', 'Ġapr', 'il', 'Ġu', 'la', 'las', 'Ġdata', 'Ġsheets', 'las', 'Ġseries', 'Ġcut', 'away', 'las', 'Ġseries', 'Ġcut', 'away', 'Ġu', 'la', 'las', 'Ġrocket', 'builder', 'Ġlock', 'heed', 'Ġmart', 'las', 'Ġlaunch', 'Ġvehicles', 'Ġencyclopedia', 'Ġastronaut', 'ica', 'las', 'Ġexternal', 'Ġlinks', 'las', 'Ġwik', 'ipedia', 'Ġspace', 'Ġlaunch', 'Ġreport', 'las', 'Ġdata', 'Ġsheet', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>['Ġlaunching', 'Ġorbital', 'Ġmission', 'Ġfirst', 'Ġstage', 'Ġachieved', 'Ġcontrolled', 'Ġvertical', 'Ġlanding', 'Ġfirst', 'Ġsuccessful', 'Ġbooster', 'Ġlanding', 'ds', 'Ġoccurred', 'Ġapr', 'il', 'Ġdrone', 'Ġship', 'Ġcourse', 'Ġstill', 'Ġlove', 'Ġsixteen', 'Ġtest', 'Ġflights', 'Ġconducted', 'Ġachieved', 'Ġsoft', 'Ġlanding', 'Ġbooster', 'Ġrecovery', 'Ġsince', 'Ġjan', 'uary', 'Ġexceptions', 'Ġcentre', 'Ġcore', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġflight', 'Ġfal', 'con', 'Ġheavy', 'Ġus', 'af', 'Ġmission', 'Ġfal', 'con', 'Ġres', 'upp', 'ly', 'Ġmission', 'Ġstar', 'link', 'Ġmissions', 'Ġevery', 'Ġlanding', 'Ġattempt', 'Ġsuccessful', 'Ġpost', 'land', 'ing', 'Ġloss', 'Ġfirst', 'Ġstage', 'Ġoccurred', 'Ġfal', 'con', 'Ġheavy', 'Ġar', 'abs', 'Ġcentre', 'Ġcore', 'Ġfell', 'Ġoverboard', 'Ġrough', 'Ġseas', 'Ġvoyage', 'Ġland', 'Ġfirst', 'Ġoperational', 'Ġrel', 'aunch', 'Ġpreviously', 'Ġflown', 'Ġbooster', 'Ġaccomplished', 'Ġmarch', 'es', 'Ġmission', 'Ġapr', 'il', 'Ġlanding', 'Ġsecond', 'Ġtime', 'Ġretired', 'Ġj', 'une', 'Ġbooster', 'Ġhelped', 'Ġcarry', 'Ġbul', 'g', 'ari', 'Ġtowards', 'Ġg', 'Ġir', 'idium', 'Ġnext', 'Ġle', 'Ġmission', 'Ġjan', 'uary', 'Ġachieving', 'Ġreuse', 'Ġlanding', 'Ġrecovered', 'Ġbooster', 'Ġthird', 'Ġreuse', 'Ġflight', 'Ġcame', 'mber', 'Ġmission', 'Ġcore', 'Ġmission', 'Ġfal', 'con', 'Ġfirst', 'Ġblock', 'Ġbooster', 'Ġproduced', 'Ġflown', 'Ġinitially', 'Ġbang', 'aband', 'hu', 'Ġsatellite', 'Ġmission', 'Ġmay', 'Ġfirst', 'Ġbooster', 'Ġreached', 'Ġmissions', 'Ġmus', 'k', 'Ġindicated', 'Ġspace', 'x', 'Ġintends', 'Ġfly', 'Ġboosters', 'Ġsee', 'Ġfailure', 'Ġstar', 'link', 'Ġmissions', 'Ġde', 'cember', 'Ġrecord', 'Ġflights', 'Ġbooster', 'Ġdespite', 'Ġpublic', 'Ġstatements', 'Ġwould', 'Ġendeavor', 'Ġmake', 'Ġsecond', 'stage', 'Ġreusable', 'Ġwell', 'Ġlate', 'Ġspace', 'x', 'Ġdetermined', 'Ġmass', 'Ġneeded', 'Ġheat', 'Ġshield', 'Ġlanding', 'Ġengines', 'Ġequipment', 'Ġsupport', 'Ġrecovery', 'Ġsecond', 'Ġstage', 'Ġprohib', 'itive', 'Ġabandoned', 'Ġsecond', 'stage', 'us', 'ability', 'Ġefforts', 'Ġspace', 'x', 'Ġdeveloped', 'Ġpayload', 'Ġfair', 'ings', 'Ġequipped', 'Ġsteer', 'able', 'Ġparachute', 'Ġwell', 'Ġthr', 'usters', 'Ġrecovered', 'Ġreused', 'Ġpayload', 'Ġfair', 'ing', 'Ġhalf', 'Ġrecovered', 'Ġfollowing', 'Ġsoft', 'land', 'ing', 'Ġocean', 'Ġfirst', 'Ġtime', 'Ġmarch', 'Ġfollowing', 'es', 'Ġsubsequently', 'Ġdevelopment', 'Ġbegan', 'Ġship', 'based', 'Ġsystem']</t>
+          <t>['Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'Ġwik', 'ipedia', 'Ġangels', 'Ġmission', 'Ġtype', 'Ġtechnology', 'Ġdemonstr', 'ator', 'Ġoperator', 'Ġaf', 'rl', 'Ġcos', 'par', 'Ġid', '043', 'c', 'Ġsat', 'cat', '01', 'Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'ang', 'els', 'Ġproject', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'Ġproject', 'Ġdevelop', 'Ġsmall', 'Ġsatellite', 'Ġorbit', 'Ġclose', 'Ġlarger', 'Ġspacecraft', 'Ġmonitor', 'Ġlocal', 'Ġspace', 'Ġenvironment', 'Ġangels', 'Ġdesigned', 'Ġevaluate', 'sa', 'Ġtechniques', 'Ġlimited', 'Ġregion', 'Ġaround', 'Ġdelta', 'Ġlaunch', 'Ġvehicle', 'Ġupper', 'Ġstage', 'Ġseveral', 'Ġhundred', 'Ġkilometers', 'Ġgeo', 'Ġtesting', 'Ġmaneuver', 'ing', 'Ġconcepts', 'Ġaround', 'Ġrocket', 'Ġbody', 'Ġvehicle', 'Ġbegan', 'Ġexperiments', 'Ġapproximately', 'Ġaway', 'Ġupper', 'Ġstage', 'Ġcautiously', 'Ġprogressed', 'Ġseveral', 'Ġmonths', 'Ġtests', 'Ġwithin', 'Ġseveral', 'Ġkilometers', 'Ġpart', 'Ġresearch', 'Ġeffort', 'Ġangels', 'Ġexplored', 'Ġincreased', 'Ġlevels', 'Ġautomation', 'Ġmission', 'Ġplanning', 'Ġexecution', 'Ġenable', 'Ġtimely', 'Ġsafe', 'Ġcomplex', 'Ġoperations', 'Ġreduced', 'Ġoperations', 'Ġfootprint', 'Ġangels', 'Ġlaunched', 'Ġrocket', 'Ġsecondary', 'Ġpayload', 'g', 'ss', 'ap', 'Ġmission', 'Ġdelivered', 'Ġdirectly', 'Ġgeo', 'Ġplanned', 'Ġoperating', 'Ġduration', 'Ġone', 'Ġyear', 'Ġsatellite', 'Ġmet', 'Ġvarious', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġmission', 'Ġobjectives', 'Ġeventually', 'Ġdecom', 'mission', 'ed', 'mber', 'Ġsinger', 'Ġj', 'ere', 'air', 'Ġforce', 'Ġangels', 'Ġsatellite', 'Ġesc', 'orts', 'Ġtake', 'Ġflight', 'http', 'sp', 'Ġspace', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', '07', 'fact', 'Ġsheet', 'Ġautomated', 'Ġnavigation', 'Ġguidance', 'Ġexperiment', 'Ġlocal', 'Ġspace', 'ang', 'els', ')"', 'http', 'Ġaf', 'rl', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdelta', 'iv', 'Ġmission', 'Ġoverview', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġreferences', 'Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġk', 'bs', 'Ġgun', 'ter', 'ang', 'els', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1244,7 +1244,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>['Ġinvolving', 'Ġmassive', 'Ġnet', 'Ġorder', 'Ġcatch', 'Ġreturning', 'Ġfair', 'ings', 'Ġtwo', 'Ġdedicated', 'Ġships', 'fitted', 'Ġrole', 'Ġmaking', 'Ġfirst', 'Ġcatches', 'Ġhowever', 'Ġfollowing', 'Ġmixed', 'Ġsuccess', 'Ġspace', 'x', 'Ġreturned', 'Ġwater', 'Ġland', 'ings', 'Ġwet', 'Ġrecovery', 'Ġearly', 'Ġregularly', 'Ġlaunching', 'Ġthree', 'Ġorbital', 'Ġlaunch', 'Ġsites', 'Ġlaunch', 'Ġcomplex', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġlatter', 'Ġdamaged', 'Ġaccident', 'Ġse', 'pt', 'ember', 'Ġoperational', 'Ġde', 'cember', 'Ġapr', 'il', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġspace', 'Ġlaunch', 'Ġdelta', 'Ġgranted', 'Ġspace', 'x', 'Ġpermission', 'Ġlease', 'Ġv', 'enberg', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġlikely', 'Ġbecome', 'Ġfourth', 'Ġlaunch', 'Ġsite', 'Ġfal', 'con', 'Ġtime', 'Ġmaiden', 'Ġflight', 'Ġprice', 'Ġlaunch', 'Ġlisted', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġlist', 'Ġprice', 'Ġincreased', 'Ġthereafter', 'Ġus', 'âĢĵ', 'Ġmillion', ').[', 'Ġmillion', 'Ġaug', 'ust', 'Ġmillion', 'j', 'une', 'Ġmillion', 'full', 'Ġthrust', 'Ġmay', 'Ġmillion', ').[', 'Ġdragon', 'Ġcargo', 'Ġmissions', 'Ġiss', 'Ġaverage', 'Ġcost', 'Ġmillion', 'Ġfixed', 'price', 'Ġcontract', 'Ġn', 'asa', 'Ġincluding', 'Ġcost', 'Ġspacecraft', 'sc', 'ov', 'r', 'Ġmission', 'Ġlaunched', 'Ġfal', 'con', 'Ġnational', 'Ġocean', 'ic', 'Ġatmospheric', 'Ġadministration', 'Ġcost', 'Ġmillion', 'Ġrel', 'aunch', 'Ġrecovery', 'Ġsecond', 'Ġstages', 'Ġfair', 'ings', 'Ġlaunch', 'Ġsites', 'Ġpricing', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġel', 'Ġmus', 'k', 'Ġstated', 'ult', 'imately', 'Ġbelieve', 'Ġper', 'Ġpound', 'kg', 'Ġpayload', 'Ġdelivered', 'Ġorbit', 'Ġless', 'Ġachievable', '".[', 'Ġlaunch', 'Ġprice', 'Ġfull', 'Ġle', 'Ġpayload', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġcosts', 'Ġreached', 'Ġus', 'lb', 'Ġ($', 'kg', 'Ġmus', 'k', 'Ġestimated', 'Ġfuel', 'Ġoxid', 'izer', 'Ġcost', '000', 'Ġfirst', 'Ġstage', 'Ġuses']</t>
+          <t>['Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġsixth', 'Ġservice', 'Ġmodule', 'Ġplaced', 'Ġinside', 'Ġpayload', 'Ġfair', 'ing', 'Ġrole', 'Ġunc', 'rew', 'ed', 'Ġspace', 'plane', 'Ġnational', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġmanufacturer', 'Ġbo', 'e', 'ing', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġapr', 'il', 'ï', '¬', 'ģ', 'r', 'st', 'Ġdrop', 'Ġtest', 'Ġintroduction', 'Ġapr', 'il', 'ï', '¬', 'ģ', 'r', 'st', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġbo', 'e', 'ing', 'Ġbo', 'e', 'ing', 'Ġalso', 'Ġknown', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġreusable', 'Ġrobotic', 'Ġspacecraft', 'Ġboosted', 'Ġspace', 'Ġlaunch', 'Ġvehicle', 'ent', 'ers', 'Ġearth', "'s", 'Ġatmosphere', 'Ġlands', 'Ġspace', 'plane', 'Ġoperated', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġorbital', 'Ġspace', 'flight', 'Ġmissions', 'Ġintended', 'Ġdemonstrate', 'Ġreusable', 'Ġspace', 'Ġtechnologies', 'percent', 'sc', 'aled', 'Ġderivative', 'Ġearlier', 'Ġbo', 'e', 'ing', 'Ġbegan', 'Ġn', 'asa', 'Ġproject', 'Ġtransferred', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġprogram', 'Ġmanaged', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġfirst', 'Ġflew', 'Ġdrop', 'Ġtest', 'Ġfirst', 'Ġorbital', 'Ġmission', 'Ġlaunched', 'Ġapr', 'il', 'las', 'Ġrocket', 'Ġreturned', 'Ġearth', 'Ġde', 'cember', 'Ġsubsequent', 'Ġflights', 'Ġgradually', 'Ġextended', 'Ġmission', 'Ġduration', 'Ġreaching', 'Ġdays', 'Ġorbit', 'Ġfifth', 'Ġmission', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'Ġrocket', 'Ġlatest', 'Ġmission', 'Ġsixth', 'Ġlaunched', 'las', 'Ġmay', 'Ġconcluded', 'mber', 'Ġreaching', 'Ġtotal', '08', 'Ġdays', 'Ġn', 'asa', 'Ġselected', 'Ġbo', 'e', 'ing', 'Ġintegrated', 'Ġdefense', 'Ġsystems', 'Ġdesign', 'Ġdevelop', 'Ġorbital', 'Ġvehicle', 'Ġbuilt', 'Ġcal', 'ornia', 'Ġbranch', 'Ġbo', 'e', 'ing', "'s", 'Ġphantom', 'Ġworks', 'Ġfour', 'year', 'Ġperiod', 'Ġtotal', 'Ġus', 'Ġmillion', 'Ġspent', 'Ġproject', 'Ġn', 'asa', 'Ġcontributing', 'Ġus', 'Ġmillion', 'Ġu', 'Ġair', 'Ġforce', 'Ġus', 'Ġmillion', 'Ġbo', 'e', 'ing', 'Ġmillion', 'Ġlate', 'Ġnew', 'Ġus', 'Ġmillion', 'Ġcontract', 'Ġawarded', 'Ġbo', 'e', 'ing', 'Ġpart', 'Ġn', 'asa', "'s", 'Ġspace', 'Ġlaunch', 'Ġinitiative', 'Ġframework', 'Ġaer', 'odynamic', 'Ġdesign', 'Ġderived', 'Ġlarger', 'Ġspace', 'Ġshuttle', 'Ġorbit', 'er', 'Ġhence', 'Ġsimilar', 'Ġlift', 'dr', 'ag', 'Ġratio', 'Ġlower', 'Ġcross', 'Ġrange', 'Ġhigher', 'Ġalt', 'itudes', 'Ġmach', 'Ġnumbers', 'Ġcompared', 'arp', "'s", 'Ġhyp', 'erson', 'ic', 'Ġtechnology', 'Ġvehicle', 'Ġearly', 'Ġrequirement']</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>['030', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġliquid', '020', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġfuel', 'Ġsecond', 'Ġstage', 'Ġuses', '000', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġliquid', '000', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġdecreased', 'Ġlaunch', 'Ġcosts', 'Ġdrew', 'Ġcompetitors', 'rian', 'esp', 'ace', 'Ġbegan', 'Ġworking', 'ri', 'ane', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġvul', 'Ġcent', 'aur', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'ils', 'Ġpro', 'ton', 'Ġmedium', 'Ġj', 'une', 'Ġj', 'athan', 'Ġh', 'eller', 'space', 'x', 'Ġvice', 'Ġpresident', 'Ġcommercial', 'Ġsales', 'Ġsaid', 'Ġprice', 'Ġdiscounts', 'Ġgiven', 'Ġearly', 'Ġcustomers', 'Ġmission', 'Ġreused', 'Ġboosters', 'Ġbecome', 'Ġstandard', 'Ġprice', 'Ġoct', 'ober', 'Ġfal', 'con', 'base', 'Ġprice', 'Ġmillion', 'Ġper', 'Ġlaunch', 'Ġlowered', 'Ġmillion', 'Ġflights', 'Ġscheduled', 'Ġbeyond', 'Ġapr', 'il', 'Ġro', 'sc', 'os', 'mos', 'Ġadministrator', 'mit', 'ry', 'Ġro', 'go', 'zin', 'Ġsaid', 'Ġoutfit', 'Ġcutting', 'Ġprices', '%,', 'Ġalleging', 'Ġspace', 'x', 'Ġprice', 'Ġdumping', 'Ġcharging', 'Ġcommercial', 'Ġcustomers', 'Ġmillion', 'Ġper', 'Ġflight', 'Ġcharging', 'Ġn', 'asa', 'Ġmuch', 'Ġflight', 'Ġmus', 'k', 'Ġdenied', 'Ġclaim', 'Ġreplied', 'Ġprice', 'Ġdifference', 'Ġreflected', 'Ġreusable', 'Ġr', 'ussian', 'Ġrockets', 'Ġsingle', 'Ġuse', 'Ġu', 'la', 'Ġce', 'ory', 'Ġbr', 'uno', 'Ġstated', 'Ġestimate', 'Ġremains', 'Ġaround', 'Ġflights', 'Ġfleet', 'Ġaverage', 'Ġachieve', 'Ġconsistent', 'Ġbre', 'ake', 'ven', 'Ġpoint', 'Ġ...', 'Ġone', 'Ġcome', 'Ġanywhere', 'Ġclose', '".[', 'Ġhowever', 'Ġel', 'Ġmus', 'k', 'Ġresponded', 'pay', 'load', 'Ġreduction', 'Ġdue', 'us', 'ability', 'Ġbooster', 'Ġfair', 'ing', 'Ġfal', 'con', 'Ġrecovery', 'Ġrefurb', '%,', "'re", 'Ġroughly', 'Ġeven', 'Ġflights', 'Ġdefinitely', 'Ġahead', '".[', 'Ġreported', 'Ġapr', 'il', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', "'s", 'Ġlaunches', 'Ġcosting', 'Ġmillion', 'Ġdue', 'Ġneeded', 'Ġextra', 'Ġsecurity', 'Ġspace', 'x', 'Ġexecutive', 'Ġchrist', 'opher', 'Ġcou', 'l', 'ur', 'Ġstated', 'using', 'Ġrockets', 'Ġcould', 'Ġbring', 'Ġprices', 'Ġeven', 'Ġlower', 'cost', 'Ġmillion', 'Ġlaunch', "'s", 'Ġeverything', '".[', 'Ġpayload', 'Ġservices', 'Ġinclude', 'Ġsecondary', 'Ġtert', 'iary', 'Ġpayload', 'Ġmounted', 'Ġvia', 'Ġe', 'el', 'v', 'Ġsecondary', 'Ġpayload', 'Ġadapter']</t>
+          <t>['Ġspacecraft', 'Ġcalled', 'Ġtotal', 'Ġmission', 'Ġdelta', 'v', '000', 'Ġmiles', 'Ġper', 'Ġhour', 'Ġorbital', 'Ġmaneuvers', 'Ġearly', 'Ġgoal', 'Ġprogram', 'Ġrend', 'ezvous', 'Ġsatellites', 'Ġperform', 'Ġrepairs', 'Ġoriginally', 'Ġdevelopment', 'Ġorigins', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġstatus', 'Ġservice', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġcompleted', 'th', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'ba', 'Ġprimary', 'Ġuser', 'Ġn', 'asa', 'arp', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġnumber', 'Ġbuilt', 'Ġdeveloped', 'Ġbo', 'e', 'ing', 'Ġartist', "'s", 'Ġrendering', 'Ġspacecraft', 'Ġscaled', 'Ġcompos', 'ites', 'Ġwhite', 'Ġknight', 'Ġused', 'Ġlaunch', 'Ġglide', 'Ġtests', 'Ġdesigned', 'Ġcarried', 'Ġorbit', 'Ġcargo', 'Ġbay', 'Ġspace', 'Ġshuttle', 'Ġunderwent', 'Ġredesign', 'Ġlaunch', 'Ġdelta', 'Ġiv', 'Ġcomparable', 'Ġrocket', 'Ġdetermined', 'Ġshuttle', 'Ġflight', 'Ġwould', 'Ġun', 'econom', 'ical', 'Ġtransferred', 'Ġn', 'asa', 'Ġdefense', 'Ġadvanced', 'Ġresearch', 'Ġprojects', 'Ġagency', 'arp', 'Ġse', 'pt', 'ember', 'Ġthereafter', 'Ġprogram', 'Ġbecame', 'Ġclassified', 'Ġproject', 'arp', 'Ġpromoted', 'Ġpart', 'Ġindependent', 'Ġspace', 'Ġpolicy', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġpursued', 'Ġsince', 'Ġchallenger', 'Ġdisaster', 'Ġvehicle', 'Ġused', 'Ġatmospheric', 'Ġdrop', 'Ġtest', 'Ġgl', 'ider', 'Ġpropulsion', 'Ġsystem', 'Ġinstead', 'Ġoperational', 'Ġvehicle', "'s", 'Ġpayload', 'Ġbay', 'Ġdoors', 'Ġenclosed', 'Ġreinforced', 'Ġupper', 'Ġfu', 'selage', 'Ġstructure', 'Ġallow', 'ated', 'Ġmother', 'ship', 'Ġse', 'pt', 'ember', 'arp', 'Ġannounced', 'Ġinitial', 'Ġatmospheric', 'Ġdrop', 'Ġtests', 'Ġwould', 'Ġlaunched', 'Ġscaled', 'Ġcompos', 'ites', 'Ġwhite', 'Ġknight', 'Ġhigh', 'alt', 'itude', 'Ġresearch', 'Ġj', 'une', 'Ġcompleted', 'Ġcaptive', 'carry', 'Ġflight', 'Ġunderneath', 'Ġwhite', 'Ġknight', 'Ġmo', 'j', 'ave', 'Ġspac', 'eport', 'Ġmo', 'j', 'ave', 'Ġcal', 'ornia', 'Ġsecond', 'Ġhalf', 'Ġunderwent', 'Ġstructural', 'Ġupgrades', 'Ġincluding', 'Ġreinforcement', 'Ġnose', 'Ġwheel', 'Ġsupports', 'Ġx', "'s", 'Ġpublic', 'Ġdebut', 'Ġfirst', 'Ġfree', 'Ġflight', 'Ġscheduled', 'Ġmarch', 'Ġcanceled', 'Ġdue', 'Ġar', 'ctic', 'Ġstorm', 'Ġnext', 'Ġflight', 'Ġattempt', 'Ġmarch', 'Ġcanceled', 'Ġdue', 'Ġhigh', 'Ġwinds', 'Ġmarch', 'Ġflew', 'Ġdat', 'al', 'ink', 'Ġfailure', 'Ġprevented', 'Ġfree', 'Ġflight', 'Ġvehicle', 'Ġreturned', 'Ġground', 'Ġstill', 'Ġattached', 'Ġwhite']</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>['es', 'pa', 'Ġring', 'Ġinter', 'stage', 'Ġadapter', 'Ġfirst', 'Ġused', 'Ġlaunching', 'Ġsecondary', 'Ġpayload', 'Ġus', 'Ġdod', 'Ġmissions', 'Ġuse', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicles', 'e', 'el', 'v', 'las', 'Ġdelta', 'Ġiv', 'Ġenables', 'Ġsecondary', 'Ġeven', 'Ġtert', 'iary', 'Ġmissions', 'Ġminimal', 'Ġimpact', 'Ġoriginal', 'Ġmission', 'Ġspace', 'x', 'Ġannounced', 'Ġpricing', 'Ġes', 'pa', 'compatible', 'Ġpayload', 'Ġspace', 'x', 'Ġfirst', 'Ġput', 'Ġfal', 'con', 'Ġpublic', 'Ġdisplay', 'Ġheadquarters', 'Ġhaw', 'th', 'orne', 'Ġcal', 'ornia', 'Ġspace', 'x', 'Ġdonated', 'Ġfal', 'con', 'Ġspace', 'Ġcenter', 'Ġh', 'ouston', 'Ġh', 'ouston', 'Ġtex', 'Ġbooster', 'Ġflew', 'Ġtwo', 'Ġmissions', 'th', 'th', 'Ġsupply', 'Ġmissions', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġfirst', 'Ġfal', 'con', 'Ġrocket', 'Ġn', 'asa', 'Ġagreed', 'Ġfly', 'Ġsecond', 'Ġtime', '".[', 'Ġspace', 'x', 'Ġdonated', 'Ġfal', 'con', 'Ġheavy', 'Ġside', 'Ġbooster', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġvisitor', 'Ġcomplex', 'os', 'Ġbang', 'aband', 'hu', 'Ġsatellite', 'res', 'heet', 'Ġlunar', 'Ġland', 'er', 'Ġbo', 'e', 'ing', 'Ġcrew', 'Ġcargo', 'Ġdragon', 'Ġdouble', 'Ġasteroid', 'Ġred', 'irection', 'Ġtest', 'art', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunches', 'Ġir', 'idium', 'Ġnext', 'Ġconstellation', 'Ġlaunches', 'Ġus', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġn', 'rol', 'Ġorb', 'comm', 'Ġrad', 'ars', 'Ġconstellation', 'es', 'Ġsir', 'ius', 'Ġlaunches', 'Ġspace', 'x', 'Ġstar', 'link', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'et', 'Ġsurvey', 'Ġsatellite', 'ess', 'Ġsecondary', 'Ġpayload', 'Ġhistorical', 'Ġartifacts', 'Ġmuseum', 'Ġfal', 'con', 'Ġnotable', 'Ġpayload', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġz', 'uma', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġlist', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġboosters', 'Ġspace', 'x', 'Ġlaunch', 'Ġvehicles', 'Ġlanding', 'Ġsuccess', 'Ġdetails', 'Ġlist', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'fal', 'con', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'fal', 'con', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'fal', 'con', 'Ġoverview', ')"', 'Ġspace', 'x', 'Ġarchived']</t>
+          <t>['Ġknight', 'Ġcarrier', 'Ġaircraft', 'Ġapr', 'il', 'Ġmade', 'Ġfirst', 'Ġfree', 'Ġglide', 'Ġflight', 'Ġlanding', 'Ġvehicle', 'ran', 'Ġrunway', 'Ġsustained', 'Ġminor', 'Ġdamage', 'Ġfollowing', 'Ġvehicle', "'s", 'Ġextended', 'Ġdowntime', 'Ġrepairs', 'Ġprogram', 'Ġmoved', 'Ġmo', 'j', 'ave', 'Ġair', 'Ġforce', 'Ġplant', 'Ġpal', 'md', 'ale', 'Ġcal', 'ornia', 'Ġremainder', 'Ġflight', 'Ġtest', 'Ġprogram', 'Ġwhite', 'Ġknight', 'Ġcontinued', 'Ġbased', 'Ġmo', 'j', 'ave', 'Ġthough', 'Ġfer', 'ried', 'Ġplant', 'Ġtest', 'Ġflights', 'Ġscheduled', 'Ġfive', 'Ġadditional', 'Ġflights', 'Ġperformed', 'n', 'Ġtwo', 'Ġresulted', 'Ġreleases', 'Ġsuccessful', 'Ġland', 'ings', 'Ġtwo', 'Ġfree', 'Ġflights', 'Ġoccurred', 'Ġaug', 'ust', 'Ġse', 'pt', 'ember', 'mber', 'Ġu', 'Ġair', 'Ġforce', 'Ġannounced', 'Ġwould', 'Ġdevelop', 'Ġvariant', 'Ġn', 'asa', "'s", 'Ġair', 'Ġforce', 'Ġversion', 'Ġdesignated', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġprogram', 'Ġbuilt', 'Ġearlier', 'Ġindustry', 'Ġgovernment', 'Ġefforts', 'arp', 'Ġn', 'asa', 'Ġair', 'Ġforce', 'Ġleadership', 'Ġair', 'Ġforce', 'Ġrapid', 'Ġcapabilities', 'Ġoffice', 'Ġpartnership', 'Ġn', 'asa', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'Ġbo', 'e', 'ing', 'Ġprime', 'Ġcontractor', 'Ġprogram', 'Ġdesigned', 'Ġglide', 'Ġtesting', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġremain', 'Ġorbit', 'Ġdays', 'Ġtime', 'Ġsecretary', 'Ġair', 'Ġforce', 'Ġstated', 'Ġprogram', 'Ġwould', 'Ġfocus', 'risk', 'Ġreduction', 'Ġexperimentation', 'Ġoperational', 'Ġconcept', 'Ġdevelopment', 'Ġreusable', 'Ġspace', 'Ġvehicle', 'Ġtechnologies', 'Ġsupport', 'Ġlong', 'term', 'Ġdevelopmental', 'Ġspace', 'Ġobjectives', '".[', 'Ġoriginally', 'Ġscheduled', 'Ġlaunch', 'Ġpayload', 'Ġbay', 'Ġspace', 'Ġshuttle', 'Ġfollowing', 'Ġspace', 'Ġshuttle', 'Ġcol', 'umb', 'ia', 'Ġdisaster', 'Ġtransferred', 'Ġdelta', 'Ġsubsequently', 'Ġtransferred', 'Ġshrouded', 'Ġconfiguration', 'las', 'Ġrocket', 'Ġfollowing', 'Ġconcerns', 'Ġun', 'sh', 'roud', 'ed', 'Ġspacecraft', "'s", 'Ġaer', 'odynamic', 'Ġproperties', 'Ġlaunch', 'Ġfollowing', 'Ġmissions', 'Ġspacecraft', 'Ġprimarily', 'Ġland', 'Ġrunway', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġcal', 'ornia', 'Ġed', 'wards', 'Ġair', 'Ġforce', 'Ġbase', 'Ġsecondary', 'Ġsite', 'Ġmanufacturing', 'Ġwork', 'Ġbegan', 'Ġsecond', 'Ġconducted', 'Ġmaiden', 'Ġmission', 'Ġmarch', 'Ġoct', 'ober', 'Ġn', 'asa', 'Ġconfirmed', 'Ġvehicles', 'Ġwould', 'Ġhoused', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter']</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'aven', 'port', 'Ġjan', 'uary', 'space', 'x', 'Ġlaunches', 'Ġstar', 'link', 'Ġgroup', 'Ġmission', 'Ġfl', 'ida', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'air', 'Ġforce', 'Ġrequirements', 'Ġkeep', 'Ġspace', 'x', 'Ġlanding', 'Ġfal', 'con', 'Ġbooster', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġseem', 'ang', 'al', 'Ġrob', 'Ġmay', 'space', 'x', 'Ġtest', 'fires', 'Ġnew', 'Ġfal', 'con', 'Ġblock', 'Ġrocket', 'Ġahead', 'Ġmaiden', 'Ġflight', 'updated', ')"', 'htt', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġoct', 'ober', 'orb', 'comm', 'Ġcraft', 'Ġlaunched', 'Ġfal', 'con', 'Ġfalls', 'Ġorbit', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġr', 'bit', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'orb', 'comm', 'Ġrequested', 'Ġspace', 'x', 'Ġcarry', 'Ġone', 'Ġsmall', 'Ġsatellites', 'igh', 'ing', 'Ġhundred', 'Ġpounds', 'Ġversus', 'Ġdragon', '000', 'Ġpounds', ')...', 'Ġhigher', 'Ġorbit', 'Ġtest', 'Ġdata', 'orb', 'comm', 'Ġgather', 'Ġrequested', 'Ġattempt', 'Ġrestart', 'Ġraise', 'Ġaltitude', 'Ġn', 'asa', 'Ġagreed', 'Ġallow', 'Ġcondition', 'Ġsubstantial', 'Ġpropell', 'ant', 'Ġreserves', 'Ġsince', 'Ġorbit', 'Ġwould', 'Ġclose', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġimportant', 'Ġappreciate', 'Ġorb', 'comm', 'Ġunderstood', 'Ġbeginning', 'Ġorbit', 'raising', 'Ġmaneuver', 'Ġtentative', 'Ġaccepted', 'Ġhigh', 'Ġrisk', 'Ġsatellite', 'Ġremaining', 'Ġdragon', 'Ġinsertion', 'Ġorbit', '..."', 'Ġgra', 'ham', 'iam', 'Ġde', 'cember', 'space', 'x', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġnails', 'Ġhistoric', 'Ġcore', 'Ġreturn', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġlaunch', 'Ġalso', 'Ġmarked', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġinternally', 'Ġknown', 'graded', 'Ġfal', 'con', 'Ġgra', 'ham', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġsuccessfully']</t>
+          <t>['Ġorbit', 'er', 'Ġprocessing', 'Ġfacilities', 'Ġhang', 'ars', 'Ġpreviously', 'Ġoccupied', 'Ġspace', 'Ġshuttle', 'Ġbo', 'e', 'ing', 'Ġsaid', 'Ġspace', 'Ġplanes', 'Ġwould', 'Ġuse', 'Ġjan', 'uary', 'Ġair', 'Ġforce', 'Ġpreviously', 'Ġsaid', 'Ġconsidering', 'Ġconsolid', 'ating', 'Ġoperations', 'Ġhoused', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġcal', 'ornia', 'Ġnearer', 'Ġlaunch', 'Ġsite', 'Ġcape', 'aver', 'al', 'Ġn', 'asa', 'Ġalso', 'Ġstated', 'Ġprogram', 'Ġcompleted', 'Ġtests', 'Ġdetermine', 'Ġwhether', 'Ġone', 'fourth', 'Ġsize', 'Ġspace', 'Ġshuttle', 'Ġcould', 'Ġland', 'Ġformer', 'Ġshuttle', 'Ġrun', 'ways', 'Ġn', 'asa', 'Ġfurthermore', 'Ġstated', 'Ġrenovations', 'Ġtwo', 'Ġhang', 'ars', 'Ġwould', 'Ġcompleted', 'Ġend', 'Ġmain', 'Ġdoors', 'Ġmarked', 'Ġmessage', 'home', 'Ġpoint', 'Ġactivities', 'Ġproject', 'Ġsecret', 'Ġofficial', 'Ġu', 'Ġair', 'Ġforce', 'Ġstatement', 'Ġproject', 'Ġexperimental', 'Ġtest', 'Ġprogram', 'Ġdemonstrate', 'Ġtechnologies', 'Ġreliable', 'Ġreusable', 'Ġunc', 'rew', 'ed', 'Ġspace', 'Ġtest', 'Ġplatform', 'Ġu', 'Ġair', 'Ġforce', '".[', 'Ġprimary', 'Ġobjectives', 'Ġtwo', 'fold', 'Ġreusable', 'Ġspacecraft', 'Ġtechnology', 'Ġoperating', 'Ġexperiments', 'Ġreturned', 'Ġearth', 'Ġair', 'Ġforce', 'Ġstates', 'Ġincludes', 'Ġtesting', 'Ġav', 'ionics', 'Ġflight', 'Ġsystems', 'Ġguidance', 'Ġnavigation', 'Ġthermal', 'Ġprotection', 'Ġinsulation', 'Ġpropulsion', 'entry', 'Ġsystems', 'Ġmay', 'Ġtom', 'Ġbur', 'gh', 'ard', 'Ġspeculated', 'Ġspace', 'Ġdaily', 'Ġcould', 'Ġused', 'Ġsatellite', 'Ġdeliver', 'Ġweapons', 'Ġspace', 'Ġpent', 'agon', 'Ġsubsequently', 'Ġdenied', 'Ġclaims', 'Ġtest', 'Ġmissions', 'Ġsupported', 'Ġdevelopment', 'Ġspace', 'based', 'Ġweapons', 'Ġjan', 'uary', 'Ġallegations', 'Ġmade', 'Ġused', 'Ġch', 'ina', "'s", 'iang', 'ong', 'Ġspace', 'Ġstation', 'Ġmodule', 'Ġformer', 'Ġu', 'Ġair', 'Ġforce', 'Ġorbital', 'Ġanalyst', 'Ġb', 'rian', 'Ġweed', 'en', 'Ġlater', 'Ġrefuted', 'Ġclaim', 'Ġemphasizing', 'Ġdifferent', 'Ġorbits', 'Ġtwo', 'Ġspacecraft', 'Ġpre', 'cluded', 'Ġpractical', 'Ġsurveillance', 'Ġfly', 'bys', 'Ġoct', 'ober', 'Ġguardian', 'Ġreported', 'Ġclaims', 'Ġsecurity', 'Ġexperts', 'Ġused', 'Ġtest', 'Ġreconnaissance', 'Ġsensors', 'Ġparticularly', 'Ġhold', 'Ġradiation', 'Ġhazards', 'Ġorbit', '".[', 'mber', 'Ġinternational', 'Ġbusiness', 'Ġtimes', 'Ġspeculated', 'Ġu', 'Ġgovernment', 'Ġtesting', 'Ġversion', 'Ġem', 'drive', 'Ġelectromagnetic', 'Ġmicrowave', 'Ġthr', 'uster', 'Ġfourth', 'Ġflight', 'Ġem', 'drive', 'Ġtechnology']</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>['Ġlaunches', 'Ġdebut', 'Ġfal', 'con', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'det', 'ailed', 'Ġmission', 'Ġdata', 'Ġfal', 'con', 'Ġfirst', 'Ġflight', 'Ġdemonstration', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġn', 'stration', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'fal', 'con', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġreferences', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'space', 'x', 'Ġfal', 'con', 'Ġupper', 'Ġstage', 'Ġengine', 'Ġsuccessfully', 'Ġcompletes', 'Ġfull', 'Ġmission', 'Ġduration', 'Ġfiring', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'os', 'Ġj', 'athan', 'Ġoct', 'ober', 'space', 'x', 'Ġlifts', 'Ġiss', 'Ġcargo', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'n', 'asa', 'Ġspace', 'x', 'Ġlaunch', 'Ġastronauts', 'Ġnew', 'Ġera', 'Ġprivate', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġh', 'Ġmay', 'Ġarchived', 'Ġh', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġc', 'aw', 'ley', 'Ġj', 'ames', 'mber', 'n', 'asa', 'Ġspace', 'x', 'Ġcomplete', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġfirst', 'Ġhuman', 'rated', 'Ġcommercial', 'Ġspace', 'Ġsystem', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'mber', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġbecame', 'Ġameric', "'s", 'Ġwork', 'horse', 'Ġrocket', 'Ġar', 'ste', 'chn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġwall', 'ike', 'Ġj', 'une', 'happy', 'Ġbirthday', 'Ġfal', 'con', 'Ġspace', 'x', "'s", 'Ġwork', 'horse', 'Ġrocket', 'Ġdebuted', 'Ġyears', 'Ġago', 'Ġtoday', 'sp', 'Ġspace', 'Ġarchived', 'years']</t>
+          <t>['Ġtransfer', 'Ġcontract', 'Ġbo', 'e', 'ing', 'Ġundertaken', 'Ġvia', 'Ġstate', 'Ġdepartment', 'Ġexport', 'Ġlicense', 'Ġapproved', 'Ġministry', 'Ġdefence', 'Ġbo', 'e', 'ing', 'Ġsince', 'Ġstated', 'Ġlonger', 'Ġpursuing', 'Ġarea', 'Ġresearch', 'Ġu', 'Ġair', 'Ġforce', 'Ġstated', 'Ġtesting', 'Ġh', 'alle', 'ffect', 'Ġthr', 'uster', 'Ġsystem', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġj', 'uly', 'Ġformer', 'Ġunited', 'Ġstates', 'Ġsecretary', 'Ġair', 'Ġforce', 'ather', 'Ġwil', 'son', 'Ġexplained', 'Ġellipt', 'ic', 'Ġorbit', 'Ġcould', 'Ġper', 'ig', 'ee', 'Ġuse', 'Ġthin', 'Ġatmosphere', 'Ġmake', 'Ġorbit', 'Ġchange', 'Ġpreventing', 'Ġobservers', 'Ġdiscovering', 'Ġnew', 'Ġorbit', 'Ġpermitting', 'Ġsecret', 'Ġactivities', 'Ġspeculation', 'Ġregarding', 'Ġpurpose', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'far', 'Ġright', 'Ġsmallest', 'Ġlight', 'est', 'Ġorbital', 'Ġspace', 'plane', 'Ġyet', 'Ġï', '¬', 'Ĥ', 'Ġnorth', 'Ġameric', 'Ġspaceship', 'one', 'Ġsub', 'orb', 'ital', 'Ġspace', 'planes', 'Ġshown', 'Ġbur', 'Ġconducted', 'Ġunc', 'rew', 'ed', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġastronomer', 'Ġj', 'athan', 'cd', 'owell', 'Ġeditor', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġstated', 'Ġsatellites', 'Ġlaunched', 'Ġreported', 'Ġrequired', 'Ġregistration', 'Ġconvention', 'Ġunited', 'Ġnations', 'Ġoffice', 'Ġouter', 'Ġspace', 'Ġaffairs', 'Ġparties', 'Ġconvention', 'Ġwould', 'Ġknow', 'Ġprocessing', 'Ġcarried', 'Ġinside', 'Ġb', 'ays', 'Ġorbit', 'er', 'Ġprocessing', 'Ġfacility', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġfl', 'ida', 'Ġvehicle', 'Ġloaded', 'Ġtop', 'secret', 'Ġpayload', 'Ġplaced', 'Ġinside', 'Ġfair', 'ing', 'Ġalong', 'Ġstage', 'Ġadapter', 'Ġtransported', 'Ġlaunch', 'Ġsite', 'Ġprevious', 'Ġlaunch', 'Ġsites', 'Ġincluded', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġlanding', 'Ġdone', 'Ġone', 'Ġthree', 'Ġsites', 'Ġacross', 'Ġus', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġv', 'enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġed', 'wards', 'Ġair', 'Ġforce', 'Ġbase', 'Ġreturn', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġplaced', 'Ġpayload', 'ister', 'Ġloaded', 'Ġbo', 'e', 'ing', 'Ġcargo', 'Ġplane', 'Ġk', 'enn', 'edy', 'Ġunloaded', 'Ġtowed', 'Ġprepared', 'Ġnext', 'Ġflight', 'Ġtechnicians', 'Ġmust', 'Ġwear', 'Ġprotective', 'Ġsuits', 'Ġdue', 'Ġtoxic', 'Ġhyper', 'g', 'olic', 'Ġgases', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġreusable', 'Ġrobotic', 'Ġspace', 'plane', 'Ġapproximately', 'percent']</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>['html', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġmay', 'Ġsafest', 'Ġrocket', 'Ġever', 'Ġlaunched', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'web', 'arch', 'iv', 'Ġcut', 'ive', 'success', 'es', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġev', 'ans', 'Ġben', 'Ġj', 'uly', 'space', 'x', "'s", 'sweet', 'Ġsixteen', 'Ġlaunches', 'Ġstar', 'links', 'Ġenters', 'us', 'ability', 'Ġrecord', 'Ġbooks', 'w', 'Ġameric', 'asp', 'ace', 'Ġmal', 'ik', 'ari', 'q', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġrocket', 'Ġlanding', 'Ġphotos', 'Ġsimply', 'Ġjaw', 'dropping', 'Ġspace', 'Ġarchived', 'Ġos', 'html', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġth', 'omas', 'Ġr', 'ach', 'ael', 'Ġl', 'space', 'x', "'s", 'Ġrockets', 'Ġspacecraft', 'Ġreally', 'Ġcool', 'Ġnames', 'Ġmean', '?"', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġtodd', 'Ġdavid', 'Ġj', 'uly', 'int', 'els', 'Ġlaunched', 'Ġadvantageous', 'Ġsuper', 'syn', 'chron', 'ous', 'Ġtransfer', 'Ġorbit', 'Ġfal', 'con', 'htt', 'Ġser', 'adata', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġk', 'yle', 'Ġed', 'Ġj', 'uly', 'Ġspace', 'Ġlaunch', 'Ġreport', 'w', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', '07', 'Ġfal', 'con', 'Ġtel', 'star', 'v', '075', 'Ġcc', 'Ġg', '-"', 'Ġwatt', 'les', 'Ġjack', 'ie', 'Ġjan', 'uary', 'space', 'x', 'Ġlaunches', 'Ġsatellites', 'Ġone', 'Ġrocket', 'Ġrecord', 'setting', 'Ġmission', 'Ġc', 'n', 'index', 'html', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'uc', 'inski', 'iam', 'Ġfour', 'Ġn', 'ssl', 'Ġlaunch', 'Ġvehicle', 'Ġdevelopers', 'Ġsay', "'ll", 'Ġready', 'Ġmobil', 'us', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'mber', 'space', 'x', "'s", 'Ġfal']</t>
+          <t>['scale', 'Ġderivative', 'Ġbo', 'e', 'ing', 'Ġx', 'Ġmeasuring', 'Ġfeet', 'Ġlength', 'Ġfeatures', 'Ġtwo', 'Ġangled', 'Ġtail', 'Ġfins', 'Ġlaunches', 'Ġatop', 'las', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġrocket', 'Ġspace', 'plane', 'Ġdesigned', 'Ġoperate', 'Ġspeed', 'Ġrange', 'Ġmach', 'entry', 'Ġtechnologies', 'Ġdemonstrated', 'Ġinclude', 'Ġimproved', 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġenhanced', 'Ġav', 'ionics', 'Ġautonomous', 'Ġguidance', 'Ġsystem', 'Ġadvanced', 'Ġair', 'frame', 'Ġspace', 'plane', "'s", 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġbuilt', 'Ġupon', 'Ġprevious', 'Ġgenerations', 'Ġatmospheric', 'entry', 'Ġspacecraft', 'Ġincorporating', 'Ġsil', 'ica', 'Ġceramic', 'Ġtiles', 'Ġav', 'ionics', 'Ġsuite', 'Ġused', 'Ġbo', 'e', 'ing', 'Ġdevelop', 'Ġc', 'st', 'Ġcrew', 'ed', 'Ġspacecraft', 'Ġdevelopment', 'aid', 'Ġdesign', 'Ġdevelopment', 'Ġn', 'asa', "'s", 'Ġorbital', 'Ġspace', 'Ġplane', 'Ġdesigned', 'Ġprovide', 'Ġcrew', 'Ġrescue', 'Ġcrew', 'Ġtransport', 'Ġcapability', 'Ġinternational', 'Ġspace', 'Ġstation', '",', 'Ġaccording', 'Ġn', 'asa', 'Ġfact', 'Ġsheet', 'Ġn', 'asa', 'Ġpowered', 'Ġone', 'ero', 'jet', 'Ġengine', 'Ġusing', 'Ġst', 'orable', 'Ġpropell', 'ants', 'Ġproviding', 'Ġthrust', 'Ġpounds', 'force', 'Ġhuman', 'rated', 'Ġengine', 'Ġused', 'Ġdual', 'power', 'Ġastronaut', 'Ġtraining', 'Ġvehicle', 'Ġgiven', 'Ġnew', 'Ġflight', 'Ġcertification', 'Ġuse', 'Ġhydrogen', 'Ġpropell', 'ants', 'Ġreportedly', 'Ġchanged', 'Ġhyper', 'g', 'olic', 'Ġpropulsion', 'Ġsystem', 'Ġlands', 'Ġautomatically', 'Ġupon', 'Ġreturning', 'Ġorbit', 'Ġthird', 'Ġreusable', 'Ġspacecraft', 'Ġcapability', 'v', 'iet', 'Ġbur', 'Ġshuttle', 'Ġu', 'Ġspace', 'Ġshuttle', 'Ġautomatic', 'Ġlanding', 'Ġcapability', 'Ġmid', 'Ġnever', 'Ġtested', 'Ġsmallest', 'Ġlight', 'est', 'Ġorbital', 'Ġspace', 'plane', 'Ġflown', 'Ġdate', 'Ġlaunch', 'Ġmass', 'Ġaround', '000', 'Ġpounds', '000', 'Ġapproximately', 'Ġone', 'Ġquarter', 'Ġsize', 'Ġspace', 'Ġshuttle', 'Ġorbit', 'er', 'Ġprocessing', 'Ġdesign', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġapr', 'il', 'Ġspace', 'Ġfoundation', 'Ġawarded', 'Ġteam', 'Ġspace', 'Ġachievement', 'Ġaward', 'Ġsignificantly', 'Ġadvancing', 'Ġstate', 'Ġart', 'Ġreusable', 'Ġspacecraft', 'orbit', 'Ġoperations', 'Ġdesign', 'Ġdevelopment', 'Ġtest']</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1322,7 +1322,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>['con', 'Ġrocket', 'Ġcert', 'ï', '¬', 'ģ', 'ed', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġprecious', 'Ġscience', 'Ġmissions', 'h', 'Ġc', 'ation', 'html', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'space', 'x', 'Ġreveals', 'Ġfal', 'con', 'Ġhall', 'ow', 'een', 'Ġdate', 'nas', 'asp', 'Ġe', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġoct', 'ober', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġadministration', 'Ġnational', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'Ġnew', 'Ġera', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġgovernment', 'Ġprinting', 'ï', '¬', 'ģ', 'ce', '09', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdavid', 'Ġj', 'Ġfr', 'kel', 'Ġapr', 'il', 'min', 'utes', 'Ġn', 'ac', 'Ġcommercial', 'Ġspace', 'Ġcommittee', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'c', 'ots', 'Ġdemo', 'Ġcompetition', 'na', 'Ġn', 'asa', 'Ġjan', 'uary', 'Ġarchived', 'Ġcompetition', 'html', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'space', 'Ġexploration', 'Ġtechnologies', 'space', 'x', ')"', 'http', 'Ġn', 'asa', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'statement', 'iam', 'Ġh', 'Ġger', 'sten', 'ier', 'Ġassociate', 'Ġadministrator', 'Ġspace', 'Ġoperations', 'Ġcommittee', 'Ġscience', 'Ġspace', 'Ġtechnology', 'Ġsubcommittee', 'Ġspace', 'Ġaer', 'aut', 'ics', 'Ġu', 'Ġhouse', 'Ġrepresentatives', 'http', 'science', 'hou', 'Ġu', 'Ġhouse', 'Ġrepresentatives', 'Ġmay', 'Ġarchived', 'web', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġde', 'cember', 'space', 'x', "'s", 'Ġdragon', 'Ġspacecraft', 'Ġsuccessfully']</t>
+          <t>['Ġorbital', 'Ġoperation', 'Ġspace', 'Ġflight', 'Ġvehicle', 'Ġthree', 'Ġmissions', 'Ġtotaling', 'Ġdays', 'Ġspace', '".[', 'Ġtwo', 'Ġoperational', 'Ġcompleted', 'Ġorbital', 'Ġmissions', 'Ġspent', 'Ġcombined', 'Ġdays', 'Ġyears', 'Ġspace', 'Ġoperational', 'Ġhistory', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġflight', 'Ġvehicle', 'Ġlaunch', 'Ġdate', 'Ġlanding', 'Ġdate', 'Ġlauncher', 'Ġmission', 'Ġduration', 'Ġnotes', 'Ġstatus', 'Ġapr', 'il', 'Ġut', 'c', 'Ġde', 'cember', 'Ġ09', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġfirst', 'Ġlaunch', 'las', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġfirst', 'Ġameric', 'Ġautonomous', 'Ġorbital', 'Ġrunway', 'Ġlanding', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlanded', 'Ġv', 'enberg', 'Ġsuccess', 'Ġmarch', 'Ġut', 'c', 'Ġj', 'une', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsecond', 'Ġlanded', 'Ġv', 'enberg', 'Ġsuccess', 'Ġde', 'cember', '03', 'Ġut', 'c', 'Ġoct', 'ober', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġsecond', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanded', 'Ġv', 'enberg', 'Ġsuccess', 'Ġmay', '05', 'Ġut', 'c', 'Ġmay', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġsecond', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsecond', 'Ġfirst', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġsuccess', 'Ġse', 'pt', 'ember', '00', 'Ġut', 'c', 'Ġoct', 'ober', 'Ġ07', 'Ġut', 'c', 'Ġfal', 'con', 'Ġblock', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġfirst', 'Ġlaunch', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġvehicle', 'Ġsuccess', 'Ġmay', 'Ġut', 'c', 'mber', 'Ġut', 'c', 'las', 'Ġus', '08', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġcarried', 'Ġexperiments', 'Ġdate', 'Ġfirst', 'Ġlaunch', 'Ġus', 'sf', 'Ġlongest', 'Ġmission', 'Ġlanded', 'Ġk', 'enn', 'edy', 'Ġsuccess', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġsits', 'Ġrunway', 'Ġlanding', 'Ġv', 'enberg', 'Ġend', 'usa', 'Ġmission', 'Ġde', 'cember', 'Ġflight', 'Ġvehicle', 'Ġlaunch', 'Ġdate', 'Ġlanding', 'Ġdate', 'Ġlauncher', 'Ġmission', 'Ġduration', 'Ġnotes', 'Ġstatus', 'Ġspace', 'Ġcenter', 'Ġde', 'cember', 'Ġfal', 'con']</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1335,7 +1335,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>['ent', 'ers', 'Ġorbit', 'Ġr', 'bit', 'press', 'Ġrelease', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmoney', 'Ġstew', 'art', 'Ġmarch', 'comp', 'etition', 'Ġfuture', 'Ġe', 'el', 'v', 'Ġprogram', 'part', ')"', 'Ġcle', 'Ġspace', 'Ġreview', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgovernment', 'Ġnecessary', 'Ġanchor', 'Ġtenant', 'Ġcommercial', 'Ġcargo', "'s", 'Ġsu', 'f', 'ï', '¬', 'ģ', 'cient', 'Ġbuild', 'Ġnew', 'Ġeconomic', 'Ġecosystem', '",', 'Ġsays', 'Ġsc', 'ott', 'Ġhub', 'bard', 'Ġaer', 'aut', 'ics', 'Ġresearcher', 'Ġst', 'ford', 'Ġuniversity', 'Ġcal', 'ornia', 'Ġformer', 'Ġdirector', 'Ġn', 'asa', "'s", 'es', 'Ġresearch', 'Ġcenter', 'ett', 'Ġfield', 'Ġcal', 'ornia', '."', 'Ġspace', 'x', 'Ġde', 'cember', 'n', 'asa', 'Ġselects', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġbooster', 'Ġdragon', 'Ġspacecraft', 'Ġcargo', 'Ġres', 'upp', 'ly', 'press', 'Ġrelease', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġfacts', 'Ġspace', 'x', 'Ġcosts', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġspace', 'x', 'usa', 'php', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġn', 'af', 'Ġcost', 'Ġestimates', 'Ġn', 'asa', 'gov', 'Ġaug', 'ust', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġgoes', 'âĢĶ', 'se', 'eks', 'Ġgovernment', 'Ġfunds', 'Ġdeep', 'Ġspace', 'Ġar', 'Ġtechn', 'ica', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġpl', 'oration', 'Ġj', 'uly', 'Ġshot', 'well', 'Ġj', 'une', 'Ġdiscussion', 'Ġshot', 'well', 'Ġpresident', 'Ġco', 'Ġspace', 'x', 'l', 'antic', 'Ġcouncil', 'Ġevent', 'Ġoccurs', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'une', 'n', 'asa', 'Ġultimately', 'Ġgave', 'Ġus', 'Ġmillion', 'Ġspace', 'x', 'Ġput', 'Ġmillion', 'Ġ...', 'Ġe', 'el', 'v', 'class', 'Ġlaunch', 'Ġvehicle', 'Ġ...', 'Ġwell', 'Ġcapsule', '."', 'Ġdavid', 'Ġle', 'ard', 'space', 'x', 'Ġtackles', 'Ġreusable', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġnews', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['Ġheavy', 'uss', 'f', 'Ġfirst', 'Ġlaunch', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġplanned', 'Ġfirst', 'Ġlaunched', 'Ġfirst', 'Ġmission', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġapr', 'il', 'Ġut', 'c', 'Ġspacecraft', 'Ġplaced', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġtesting', 'Ġu', 'Ġair', 'Ġforce', 'Ġrevealed', 'Ġorbital', 'Ġdetails', 'Ġmission', 'Ġworldwide', 'Ġnetwork', 'Ġamateur', 'Ġastronomers', 'Ġclaimed', 'Ġidentified', 'Ġspacecraft', 'Ġorbit', 'Ġmay', 'Ġspacecraft', 'Ġinclination', 'Â°', 'Ġcircling', 'Ġearth', 'Ġevery', 'Ġminutes', 'Ġorbit', 'Ġmiles', 'Ġrep', 'uted', 'ly', 'Ġpassed', 'Ġgiven', 'Ġspot', 'Ġearth', 'Ġevery', 'Ġfour', 'Ġdays', 'Ġoperated', 'Ġaltitude', 'Ġtypical', 'Ġmilitary', 'Ġsurveillance', 'Ġsatellites', 'Ġorbit', 'Ġalso', 'Ġcommon', 'Ġamong', 'Ġcivilian', 'Ġle', 'Ġsatellites', 'Ġspace', 'plane', "'s", 'Ġaltitude', 'Ġiss', 'Ġcrew', 'ed', 'Ġspacecraft', 'Ġu', 'Ġair', 'Ġforce', 'Ġannounced', 'âĢĵ', 'Ġde', 'cember', 'Ġlanding', 'mber', 'Ġscheduled', 'Ġde', 'orb', 'ited', 'ent', 'ered', 'Ġearth', "'s", 'Ġatmosphere', 'Ġlanded', 'Ġsuccessfully', 'Ġv', 'enberg', 'Ġde', 'cember', 'Ġ09', 'Ġut', 'c', 'Ġconducting', 'Ġfirst', 'Ġus', 'Ġautonomous', 'Ġorbital', 'Ġlanding', 'Ġonto', 'Ġrunway', 'Ġfirst', 'Ġlanding', 'Ġsince', 'v', 'iet', 'Ġbur', 'Ġshuttle', 'Ġspent', 'Ġdays', 'Ġhours', 'Ġspace', 'Ġsuffered', 'Ġtire', 'Ġblow', 'Ġlanding', 'Ġsustained', 'Ġminor', 'Ġdamage', 'Ġunderside', 'Ġsecond', 'Ġlaunched', 'Ġinaugural', 'Ġmission', 'Ġdesignated', 'Ġaboard', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġmarch', 'Ġmission', 'Ġclassified', 'Ġdescribed', 'Ġu', 'Ġmilitary', 'Ġeffort', 'Ġtest', 'Ġnew', 'Ġspace', 'Ġtechnologies', 'mber', 'Ġu', 'Ġair', 'Ġforce', 'Ġannounced', 'Ġwould', 'Ġextend', 'Ġus', 'Ġbeyond', 'day', 'Ġbaseline', 'Ġduration', 'Ġapr', 'il', 'Ġgeneral', 'iam', 'Ġl', 'Ġshel', 'ton', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġdeclared', 'Ġongoing', 'Ġmission', 'spect', 'acular', 'Ġsuccess', '".[', 'Ġmay', 'Ġair', 'Ġforce', 'Ġstated', 'Ġwould', 'Ġland', 'Ġv', 'enberg', 'Ġj', 'une']</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>['Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġmal', 'ik', 'ari', 'q', 'Ġmay', "'s", 'Ġstar', 'Ġwars', 'Ġday', 'Ġspace', 'x', 'Ġlaunched', 'fal', 'con', 'Ġspace', 'Ġspace', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġannounces', 'Ġfal', 'con', 'Ġfully', 'Ġreusable', 'Ġheavy', 'Ġlift', 'Ġlaunch', 'Ġvehicle', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'space', 'Ġact', 'Ġagreement', 'Ġn', 'asa', 'Ġspace', 'Ġexploration', 'Ġtechnologies', 'Ġinc', '.,', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'Ġdemonstration', 'Ġn', 'asa', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġco', 'pping', 'er', 'Ġrob', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġfal', 'con', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġdelayed', 'Ġmonths', 'Ġlate', 'http', 'ï', '¬', 'Ĥ', 'ight', 'gl', 'Ġflight', 'Ġglobal', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġconducts', 'Ġfirst', 'Ġmulti', 'engine', 'Ġfiring', 'Ġfal', 'con', 'Ġrocket', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmarch', 'space', 'x', 'Ġsuccessfully', 'Ġconducts', 'Ġfull', 'Ġmission', 'length', 'Ġï', '¬', 'ģ', 'ring', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'press', 'Ġrelease', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'mber', 'mer', 'lin', 'Ġvacuum', 'Ġengine', 'Ġtest', 'Ġyoutube', 'mber', 'Ġarchived', 'http', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'space', 'x', 'Ġannounces', 'Ġfal', 'con', 'Ġassembly', 'Ġunderway', 'Ġcap', 'Ġpe', 'html', 'lando', 'Ġsent', 'inel', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'dates', 'Ġspace', 'x', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġk', 'mer', 'Ġk', 'en', 'Ġmarch']</t>
+          <t>['Ġspacecraft', 'Ġlanded', 'Ġautonom', 'ously', 'Ġj', 'une', 'Ġspent', 'Ġdays', 'Ġhours', 'Ġspace', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġsits', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġmission', 'Ġsits', 'Ġrunway', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'mber', '09', 'th', 'Ġday', 'usa', 'Ġmission', 'Ġthird', 'Ġmission', 'Ġsecond', 'Ġflight', 'Ġfirst', 'Ġoriginally', 'Ġscheduled', 'Ġlaunch', 'Ġoct', 'ober', 'Ġpostponed', 'Ġengine', 'Ġissue', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġsuccessfully', 'Ġlaunched', 'Ġcape', 'aver', 'al', 'Ġde', 'cember', '03', 'Ġut', 'c', 'Ġorbit', 'Ġspacecraft', 'Ġdesignated', 'Ġus', 'Ġlanding', 'Ġoccurred', 'Ġv', 'enberg', 'Ġoct', 'ober', 'Ġut', 'c', 'Ġtotal', 'Ġtime', 'Ġorbit', 'Ġdays', 'Ġfourth', 'Ġmission', 'Ġcod', 'en', 'amed', 'Ġdesignated', 'Ġus', 'Ġorbit', 'Ġsecond', 'Ġflight', 'Ġsecond', 'Ġvehicle', 'Ġlaunched', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġmay', '05', 'Ġobjectives', 'Ġincluded', 'Ġtest', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', "'s", 'Ġhall', 'effect', 'Ġthr', 'uster', 'Ġsupport', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġcommunications', 'Ġsatellite', 'Ġprogram', 'Ġn', 'asa', 'Ġinvestigation', 'Ġperformance', 'Ġvarious', 'Ġmaterials', 'Ġspace', 'Ġleast', 'Ġdays', 'Ġvehicle', 'Ġspent', 'Ġrecord', 'breaking', 'Ġdays', 'Ġhours', 'Ġorbit', 'Ġlanding', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', "'s", 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġmay', 'Ġfifth', 'Ġmission', 'Ġdesignated', 'Ġus', 'Ġlaunched', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġlaunch', 'Ġcomplex', 'Ġse', 'pt', 'ember', '00', 'Ġut', 'c', 'Ġarrival', 'Ġhurricane', 'Ġ', 'irm', 'Ġlaunch', 'Ġvehicle', 'Ġfal', 'con', 'Ġrocket', 'Ġnumber', 'Ġsmall', 'Ġsatellites', 'Ġalso', 'Ġshared', 'Ġspacecraft', 'Ġinserted', 'Ġhigher', 'Ġinclination', 'Ġorbit', 'Ġprevious', 'Ġmissions', 'Ġexpanding', 'Ġenvelope', 'Ġflight', 'Ġspacecraft', 'Ġmodified', 'Ġorbit', 'Ġusing', 'board', 'Ġpropulsion', 'Ġsystem']</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>['successful', 'Ġengine', 'Ġtest', 'Ġfiring', 'Ġspace', 'x', 'Ġinaugural', 'Ġfal', 'con', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġden', 'ise', 'Ġch', 'ow', 'Ġde', 'cember', 'q', 'Ġspace', 'x', 'Ġce', 'Ġel', 'Ġmus', 'k', 'Ġmaster', 'Ġprivate', 'Ġspace', 'Ġdragons', 'sp', 'ac', 'html', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'production', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'space', 'x', 'Ġsays', 'Ġfal', 'con', 'Ġcompete', 'Ġe', 'el', 'v', 'Ġyear', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'within', 'Ġyear', 'Ġneed', 'Ġget', 'Ġright', 'Ġrocket', 'Ġcore', 'Ġevery', 'Ġfour', 'Ġweeks', 'Ġrocket', 'Ġcore', 'Ġevery', 'Ġtwo', 'Ġweeks', '...', 'Ġend', 'Ġsays', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġcompany', 'Ġplans', 'Ġrat', 'chet', 'Ġproduction', 'Ġcores', 'Ġper', 'Ġyear', '."', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġseeks', 'Ġaccelerate', 'Ġfal', 'con', 'Ġproduction', 'Ġlaunch', 'Ġrates', 'Ġyear', 'http', 'sp', 'ac', 'en', 'ew', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġoct', 'ober', 'cong', 'rats', 'space', 'x', 'Ġteam', 'th', 'Ġlaunch', 'Ġyear', 'Ġfal', 'con', 'Ġholds', 'Ġrecord', 'Ġlaunches', 'Ġsingle', 'Ġvehicle', 'Ġtype', 'Ġyear', 'http', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġdeb', 'uts', 'Ġnew', 'Ġmodel', 'Ġfal', 'con', 'Ġrocket', 'Ġdesigned', 'Ġastronauts', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġb', 'aylor', 'ichael', 'Ġmay', 'Ġblock', 'Ġspace', 'x', 'Ġincrease', 'Ġlaunch', 'Ġcad', 'ence', 'Ġlower', 'Ġprices', 'nas', 'asp', 'lower', 'pr', 'ices', 'Ġretrieved', 'Ġj', 'uly', 'Ġje', 'ff', 'Ġf', 'oust', 'Ġse', 'pt']</t>
+          <t>['Ġcomplete', 'Ġpayload', 'Ġclassified', 'Ġair', 'Ġforce', 'Ġannounced', 'Ġone', 'Ġexperiment', 'Ġflying', 'Ġadvanced', 'Ġstruct', 'urally', 'Ġembedded', 'Ġthermal', 'Ġspread', 'er', 'ets', 'ii', 'Ġmeasures', 'Ġperformance', 'Ġoscill', 'ating', 'Ġheat', 'Ġmission', 'Ġcompleted', 'Ġvehicle', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġoct', 'ober', 'Ġ07', 'Ġsixth', 'Ġmission', 'Ġu', 'Ġspace', 'Ġforce', 'formerly', 'Ġknown', 'Ġlaunched', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġmay', '00', 'Ġmission', 'Ġfirst', 'Ġtime', 'Ġspace', 'plane', 'Ġcarried', 'Ġservice', 'Ġmodule', 'Ġring', 'Ġattached', 'Ġrear', 'Ġvehicle', 'Ġhosting', 'Ġmultiple', 'Ġexperiments', 'Ġmission', 'Ġhosts', 'Ġexperiments', 'Ġprior', 'Ġflights', 'Ġincluding', 'Ġtwo', 'Ġn', 'asa', 'Ġexperiments', 'Ġone', 'Ġsample', 'Ġplate', 'Ġevaluating', 'Ġreaction', 'Ġselect', 'Ġmaterials', 'Ġconditions', 'Ġspace', 'Ġsecond', 'Ġstudies', 'Ġeffect', 'Ġambient', 'Ġspace', 'Ġradiation', 'Ġseeds', 'Ġthird', 'Ġexperiment', 'Ġdesigned', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġtransforms', 'Ġsolar', 'Ġpower', 'Ġradio', 'Ġfrequency', 'Ġmicrowave', 'Ġenergy', 'Ġstudies', 'Ġtransmitting', 'Ġenergy', 'Ġearth', 'Ġremains', 'Ġdepartment', 'Ġair', 'Ġforce', 'Ġasset', 'Ġnewly', 'Ġestablished', 'Ġu', 'Ġspace', 'Ġforce', 'Ġresponsible', 'Ġlaunch', 'orbit', 'Ġoperations', 'Ġlanding', 'uss', 'f', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġreleased', 'Ġsmall', 'Ġsatellite', 'Ġnamed', 'Ġfal', 'cons', 'usa', 'Ġaround', 'Ġmay', 'Ġdeveloped', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġacademy', 'Ġcad', 'ets', 'Ġpartnership', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'af', 'rl', 'Ġsmall', 'Ġsatellite', 'Ġcarries', 'Ġfive', 'Ġexperimental', 'Ġpayload', 'Ġspacecraft', 'Ġtest', 'Ġnovel', 'Ġelectromagnetic', 'Ġpropulsion', 'Ġsystem', 'Ġlow', 'weight', 'Ġantenna', 'Ġtechnology', 'Ġcommercial', 'Ġreaction', 'Ġwheel', 'Ġprovide', 'Ġattitude', 'Ġcontrol', 'Ġorbit', 'Ġaccording', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġacademy', 'Ġfal', 'cons', "'s", 'Ġexperiments', 'Ġinclude', ':[', 'Ġmagnet', 'og', 'rad', 'ient', 'Ġelectro', 'static', 'Ġplasma', 'Ġthr', 'uster', 'ep', 'Ġnovel', 'Ġelectromagnetic', 'Ġpropulsion', 'Ġsystem', 'Ġmet', 'aterial', 'Ġantenna', 'mma', 'Ġlow', 'Ġsize', 'Ġweight', 'Ġpower', 'Ġantenna', 'Ġphased', 'Ġarray', 'like', 'Ġperformance', 'Ġcarbon', 'Ġnan', 'ot', 'ube', 'Ġexperiment', 'oe', 'Ġc', 'abling', 'Ġcarbon', 'Ġnan', 'ot', 'ube', 'Ġbra', 'iding', 'Ġï', '¬', 'Ĥ', 'ex', 'ed', 'Ġusing', 'Ġshape', 'memory', 'Ġalloy', 'Ġattitude', 'Ġcontrol', 'Ġenergy', 'Ġstorage', 'aces', 'Ġcommercial', 'Ġreaction', 'Ġwheel', 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġï', '¬', 'Ĥ', 'wheel', 'Ġenergy', 'Ġstorage', 'Ġrelease', 'Ġsk', 'yp', 'ad']</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>['ember', 'mus', 'k', 'Ġunve', 'ils', 'Ġrevised', 'Ġversion', 'Ġgiant', 'Ġinter', 'plan', 'etary', 'Ġlaunch', 'Ġsystem', 'Ġarchived', 'Ġoct', 'ober', 'Ġarchive', '".', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġmarch', 'space', 'x', 'Ġmakes', 'Ġaerospace', 'Ġhistory', 'Ġsuccessful', 'Ġlaunch', 'Ġlanding', 'Ġused', 'Ġrocket', 'htt', 'Ġverge', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'Ġl', 'op', 'atto', 'Ġel', 'izabeth', 'Ġmarch', 'space', 'x', 'Ġeven', 'Ġlanded', 'Ġnose', 'Ġcone', 'Ġhistoric', 'Ġused', 'Ġfal', 'con', 'Ġrocket', 'Ġlaunch', 'Ġverge', 'Ġarchived', 'http', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmarch', 'space', 'x', 'Ġfal', 'con', 'Ġsets', 'Ġnew', 'Ġrecord', 'Ġtel', 'star', 'v', 'Ġlaunch', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġj', 'uly', 'Ġarchived', 'unch', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġbids', 'Ġtemporary', 'Ġgoodbye', 'Ġwest', 'Ġcoast', 'Ġlaunch', 'Ġlanding', 'Ġphotos', 'w', 'Ġhot', 'os', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġsticks', 'Ġbooster', 'Ġrecovery', 'Ġcal', 'ornia', 'Ġlanding', 'Ġzone', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'launch', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġblock', 'Ġrad', 'ars', 'Ġconstellation', 'Ġsp', 'acet', 'v', 'Ġarchived', 'h', 'Ġell', 'ation', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġlaunches', 'Ġorbit', 'Ġstar', 'link', 'Ġsatellites', 'âĢĶ', 'igh', 'ing', 'Ġtotal', 'Ġmetric', 'Ġtons', 'âĢĶ', 'mark', 'ing', 'Ġheaviest', 'Ġpayload', 'Ġever', 'Ġï', '¬', 'Ĥ', 'Ġfal', 'con', 'Ġtwitter', 'Ġretrieved', 'Ġjan', 'uary', 'fal', 'con', 'Ġuser', "'s", 'Ġguide', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'h', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia']</t>
+          <t>['lf', 'Ġcameras', 'Ġgp', 'us', 'Ġintegrated', 'Ġlow', 'sw', 'ap', 'size', 'Ġweight', 'Ġpower', 'Ġpackage', 'Ġmission', 'Ġcompleted', 'Ġvehicle', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'mber', 'Ġfirst', 'Ġlaunched', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġfirst', 'Ġgo', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġinstead', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġapproach', 'Ġlanding', 'Ġtest', 'Ġvehicle', 'Ġinitial', 'Ġn', 'asa', 'Ġversion', 'Ġspacecraft', 'Ġused', 'Ġdrop', 'Ġglide', 'Ġtests', 'Ġmodified', 'Ġversion', 'Ġn', 'asa', 'Ġbuilt', 'Ġu', 'Ġair', 'Ġforce', 'Ġtwo', 'Ġbuilt', 'Ġused', 'Ġmultiple', 'Ġorbital', 'Ġmissions', 'uss', 'f', 'Ġvariants', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġthree', 'view', 'Ġplans', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġbo', 'e', 'ing', 'Ġannounced', 'Ġplans', 'Ġscaled', 'Ġvariant', 'Ġreferring', 'Ġspacecraft', 'Ġplanned', 'Ġsize', 'Ġallowing', 'Ġtransport', 'Ġastronauts', 'Ġinside', 'Ġpress', 'urized', 'Ġcompartment', 'Ġhoused', 'Ġcargo', 'Ġbay', 'las', 'Ġvariant', "'s", 'Ġproposed', 'Ġlaunch', 'Ġvehicle', 'Ġrole', 'Ġbo', 'e', 'ing', "'s", 'Ġcould', 'Ġpotentially', 'Ġcompete', 'Ġcorporation', "'s", 'Ġc', 'st', 'Ġstar', 'liner', 'Ġcommercial', 'Ġspace', 'Ġcapsule', 'Ġdata', 'Ġus', 'af', 'Ġbo', 'e', 'ing', 'Ġair', 'Ġspace', 'Ġmagazine', 'Ġphys', 'org', 'Ġgeneral', 'Ġcharacteristics', 'Ġcrew', 'Ġnone', 'Ġcapacity', 'Ġlength', 'Ġft', 'Ġwings', 'pan', 'Ġft', 'Ġheight', 'Ġft', 'Ġtakeoff', 'Ġweight', '000', 'Ġelectrical', 'Ġpower', 'Ġgall', 'ium', 'Ġarsen', 'ide', 'Ġsolar', 'Ġcells', 'Ġlithium', 'ion', 'Ġbatteries', 'Ġpayload', 'Ġbay', 'Ġft', ')[', 'Ġperformance', 'Ġorbital', 'Ġspeed', 'Ġmph', '044', 'Ġorbit', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġorbital', 'Ġtime', 'Ġdays', 'design', ')[', 'n', '08', 'Ġdays', 'demon', 'str', 'ated', ')[', 'Ġbo', 'e', 'ing', 'Ġdyn', 'ar', 'Ġu', 'Ġair', 'Ġforce', "'s", 'Ġoriginal', 'âĢĵ', 'Ġspace', 'plane', 'Ġprogram', 'Ġcancelled', 'Ġcraft']</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>['Ġmission', 'Ġstatus', 'Ġcenter', 'Ġj', 'une', '05', 'Ġut', 'c', 'Ġarchived', 'web', 'Ġmay', 'Ġway', 'back', 'Ġmachine', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaccessed', '06', '02', 'Ġquotation', 'Ġï', '¬', 'Ĥ', 'anges', 'Ġlink', 'Ġrocket', 'Ġground', 'Ġstorage', 'Ġtanks', 'Ġcontaining', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġfuel', 'Ġhelium', 'Ġgas', 'erous', 'Ġnitrogen', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġign', 'itor', 'Ġsource', 'Ġcalled', 'Ġbetter', 'Ġknown', 'Ġtea', 'tab', '".', 'oct', 'aw', 'eb', 'Ġv', 'oct', 'aw', 'eb', 'Ġspace', 'x', 'Ġnews', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġire', 'ne', 'Ġse', 'pt', 'ember', 'mus', 'k', 'Ġsays', 'Ġspace', 'x', 'extremely', 'Ġparanoid', 'Ġread', 'ies', 'Ġfal', 'con', 'Ġcal', 'ornia', 'Ġdebut', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġinformation', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmang', 'els', 'Ġjohn', 'Ġmay', 'n', 'asa', "'s", 'Ġplum', 'Ġbro', 'ok', 'Ġstation', 'Ġtests', 'Ġrocket', 'Ġfair', 'ing', 'Ġspace', 'x', 'Ġcle', 'veland', 'Ġplain', 'Ġdealer', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'Ġsv', 'ak', 'Ġamy', 'mber', 'dragon', "'s", 'rad', 'iation', 'oler', 'ant', 'Ġdesign', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'sche', 'dule', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'land', 'ing', 'Ġlegs', 'Ġspace', 'x', 'Ġnews', 'Ġapr', 'il', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġheavy', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcenter', 'Ġcore', 'Ġboosters', 'Ġcarry', 'Ġlanding', 'Ġlegs', 'Ġland', 'Ġcore', 'Ġsafely', 'Ġearth', 'Ġtakeoff', '."', 'Ġk', 'mer', 'Ġk', 'en', 'Ġjan', 'uary', 'fal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġbooster', 'Ġrecovery', 'Ġfeatured', 'Ġcool', 'Ġnew', 'Ġspace', 'x', 'Ġanimation', 'Ġx', 'anim', 'ation', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary']</t>
+          <t>['Ġconstructed', 'Ġdream', 'Ġch', 'aser', 'Ġlifting', 'body', 'Ġspace', 'plane', 'Ġdeveloped', 'ierra', 'Ġne', 'v', 'ada', 'Ġcorporation', 'Ġorbital', 'Ġsciences', 'Ġproposed', 'Ġunc', 'rew', 'ed', 'Ġsub', 'orb', 'ital', 'Ġreusable', 'rocket', 'Ġtechnology', 'Ġtest', 'bed', 'Ġtechnology', 'Ġdemonstration', 'Ġprogramme', 'Ġind', 'ian', 'Ġreusable', 'Ġspace', 'plane', 'Ġdevelopment', 'Ġproject', 'mes', 'space', 'craft', 'Ġproposed', 'Ġes', 'Ġspacecraft', 'Ġdesign', 'Ġhope', 'x', 'Ġsimilar', 'sized', 'Ġvehicle', 'Ġcomparable', 'Ġrole', 'Ġj', 'ax', 'c', 'ance', 'lled', 'Ġhy', 'flex', 'Ġj', 'apan', 'ese', 'Ġlifting', 'Ġbody', 'Ġspace', 'plane', 'Ġprecursor', 'Ġhope', 'x', 'Ġintermediate', 'Ġexperimental', 'Ġvehicle', 'Ġes', 'Ġdesigned', 'Ġexperimental', 'entry', 'Ġvehicle', 'n', 'long', 'space', 'craft', 'Ġch', 'inese', 'Ġreusable', 'Ġrobotic', 'Ġspace', 'plane', 'Ġdevelopment', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtested', 'sub', 'orb', 'ital', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġch', 'inese', 'Ġreusable', 'Ġexperimental', 'Ġspacecraft', 'Ġch', 'inese', 'Ġreusable', 'Ġspacecraft', 'Ġsk', 'ylon', 'space', 'craft', 'Ġb', 'rit', 'ish', 'Ġreusable', 'Ġunc', 'rew', 'ed', 'Ġspace', 'plane', 'Ġdevelopment', 'Ġspace', 'Ġrider', 'Ġplanned', 'Ġrobotic', 'Ġspace', 'plane', 'Ġfollow', 'Ġes', 'Ġspecifications', 'Ġsee', 'Ġalso', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġlist', 'Ġus', 'Ġsatellites', 'Ġlist', 'Ġx', 'planes', 'Ġcoll', 'ier', 'Ġtrophy', 'Ġsource', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġmission', 'Ġmarkings', 'Ġposted', 'Ġside', 'Ġwhite', 'Ġknight', 'Ġaircraft', 'Ġï', '¬', 'ģ', 'g', 'ure', 'Ġbased', 'Ġpre', 'launch', 'Ġdesign', 'Ġestimates', 'ï', '¬', 'Ĥ', 'ect', 'Ġspacecraft', "'s", 'Ġactual', 'Ġperformance', 'Ġcapacity', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġaug', 'ust', 'pent', 'agon', 'Ġplans', 'Ġkeep', 'Ġspace', 'plane', 'Ġair', 'Ġforce', 'Ġmanagement', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġe', 'ment', 'Ġoriginal', 'Ġmarch', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġconcludes', 'Ġsixth', 'Ġsuccessful', 'Ġmission', 'press', 'Ġrelease', 'Ġu', 'Ġspace', 'Ġforce', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'mber', 'Ġtechnology', 'Ġdemonstr', 'ator', 'Ġblazing', 'Ġtrail', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtransportation', 'Ġsystems', 'Ġn', 'asa', 'Ġfacts', 'Ġn', 'asa', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'air', 'Ġforce', 'Ġbloggers', 'Ġround', 'table', 'Ġair', 'Ġforce', 'Ġset', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġapr', 'il', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>['Ġsim', 'berg', 'Ġrand', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', 'Ġspace', 'x', "'s", 'Ġreusable', 'Ġrocket', 'Ġplans', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġch', 'ris', 'ster', 'Ġbeyond', 'Ġfront', 'iers', 'Ġbroad', 'gate', 'Ġpublications', 'Ġp', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġdf', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'mus', 'k', 'Ġambition', 'Ġspace', 'x', 'Ġaim', 'Ġfully', 'Ġreusable', 'Ġfal', 'con', 'http', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'Ġfal', 'con', "'s", 'Ġfourth', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġgot', 'Ġcooked', "'re", 'Ġgoing', 'Ġbeef', 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġthink', "'s", 'Ġhighly', 'Ġlikely', "'ll", 'Ġrecover', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġget', 'Ġback', "'ll", 'Ġsee', 'Ġsurvived', 'entry', 'Ġgot', 'Ġfried', 'Ġcarry', 'Ġprocess', "'s", 'Ġmake', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġreusable', "'ll", 'Ġeven', 'Ġharder', 'Ġsecond', 'Ġstage', 'Ġgot', 'Ġfull', 'Ġheats', 'h', 'ield', "'ll", 'Ġde', 'orbit', 'Ġpropulsion', 'Ġcommunication', '."', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġannual', 'Ġcomp', 'endium', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'Ġspace', 'x', 'Ġfounder', 'Ġchief', 'Ġdesigner', 'Ġel', 'Ġmus', 'k', 'Ġ03', '05', 'mus', 'k', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'web', 'arch', 'iv', 'Ġ03', '05', 'mus', 'k', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'une', 'oct', 'aw', 'eb', 'Ġspace', 'x', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġcommercial', 'Ġpromise', 'Ġtested']</t>
+          <t>['Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'air', 'Ġforce', 'Ġspace', 'plane', 'Ġodd', 'Ġbird', 'Ġtwisted', 'Ġpast', 'http', 'sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'n', 'asa', 'Ġbo', 'e', 'ing', 'Ġenter', 'Ġcooperative', 'Ġagreement', 'Ġdevelop', 'Ġfly', 'Ġtechnology', 'Ġdemonstr', 'ator', 'htt', 'press', 'Ġrelease', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġpress', 'Ġrelease', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġyen', 'ne', 'Ġp', 'Ġber', 'ger', 'Ġb', 'rian', 'Ġse', 'pt', 'ember', 'n', 'asa', 'Ġtransfers', 'Ġproject', 'arp', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġber', 'ger', 'Ġb', 'rian', 'Ġse', 'pt', 'ember', 'arp', 'Ġtakes', 'Ġspace', 'Ġplane', 'Ġproject', 'Ġnews', 'Ġarchived', 'id', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġexplanatory', 'Ġnotes', 'Ġreferences', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġdavid', 'Ġle', 'ard', 'Ġj', 'une', 'white', 'Ġknight', 'Ġcarries', 'Ġal', 'oft', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġpars', 'ch', 'n', 'ovember', 'bo', 'e', 'ing', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġaug', 'ust', 'mo', 'j', 'ave', 'Ġweb', 'Ġlog', 'Ġentries', 'Ġmo', 'j', 'ave', 'blog', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġoct', 'ober', 'Ġdavid', 'Ġle', 'ard', 'Ġapr', 'il', 'Ġflies', 'Ġmo', 'j', 'ave', 'Ġencounters', 'Ġlanding', 'Ġproblems', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'Ġtest', 'Ġflight', 'Ġb', 'roll', 'Ġaudio', ')"', 'Ġyoutube', 'Ġu', 'Ġair', 'Ġforce', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj']</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>['sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġmarch', 'space', 'x', 'Ġsays', 'Ġrequirements', 'Ġmarkup', 'Ġmake', 'Ġgovernment', 'Ġmissions', 'Ġcostly', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'une', 'Ġdan', 'Ġle', 'one', 'Ġj', 'uly', 'space', 'x', 'Ġtest', 'ï', '¬', 'ģ', 'res', 'Ġupgraded', 'Ġfal', 'con', 'Ġcore', 'Ġthree', 'Ġminutes', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġr', 'three', 'min', 'utes', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġj', 'une', 'red', 'ucing', 'Ġrisk', 'Ġvia', 'Ġground', 'Ġtesting', 'Ġrecipe', 'Ġspace', 'x', 'Ġsuccess', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġsv', 'ak', 'Ġamy', 'mber', 'mus', 'k', 'Ġfal', 'con', 'Ġcapture', 'Ġmarket', 'Ġshare', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', 'Ġcurrently', 'Ġproducing', 'Ġone', 'Ġvehicle', 'Ġper', 'Ġmonth', 'Ġnumber', 'Ġexpected', 'Ġincrease', 'Ġper', 'Ġyear', 'Ġnext', 'Ġcouple', 'Ġquarters', "'.", 'Ġend', 'Ġsays', 'Ġspace', 'x', 'Ġproduce', 'Ġlaunch', 'Ġvehicles', 'Ġper', 'Ġyear', '."', 'land', 'ing', 'Ġlegs', 'Ġg', 'leg', 'Ġspace', 'x', 'Ġj', 'uly', 'Ġarchived', 'land', 'ing', 'leg', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġl', 'ind', 'sey', 'Ġcl', 'ark', 'Ġmarch', 'space', 'x', 'Ġmoving', 'Ġquickly', 'Ġtowards', 'Ġï', '¬', 'Ĥ', 'back', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġnewsp', 'ace', 'Ġwatch', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'Ġmess', 'ier', 'Ġdou', 'g', 'Ġmarch', 'dragon', 'Ġpost', 'mission', 'Ġpress', 'Ġconference', 'Ġnotes', 'Ġpar', 'abolic', 'Ġarc', 'Ġarchived', 'Ġn', 'ference', 'notes', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmarch', 'Ġshot', 'well', 'Ġfe', 'b', 'ruary', 'Ġshot', 'well', 'Ġcomments', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġconference', 'htt', 'Ġcommercial', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġevent', 'Ġoccurs']</t>
+          <t>['une', 'Ġretrieved', 'mber', 'Ġdavid', 'Ġle', 'ard', 'mber', 'u', 'Ġair', 'Ġforce', 'Ġpushes', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'http', 'sp', 'ac', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'las', 'Ġrocket', 'Ġdelivers', 'Ġair', 'Ġforce', 'Ġspace', 'plane', 'Ġorbit', 'http', 'space', 'ï', '¬', 'Ĥ', 'ight', 'n', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'air', 'Ġforce', 'Ġspace', 'plane', 'Ġarrives', 'Ġfl', 'ida', 'Ġlaunch', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġcov', 'ault', 'Ġcra', 'ig', 'Ġaug', 'ust', 'us', 'af', 'Ġlaunch', 'Ġfirst', 'Ġspace', 'plane', 'Ġdemonstr', 'ator', 'web', 'arch', 'iv', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġh', 'annel', 'aw', 'st', 'Ġaug', 'ust', 'ris', 'Ġde', 'cember', 'second', 'Ġprepared', 'Ġlaunch', 'Ġaviation', 'Ġweek', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmarch', 'air', 'Ġforce', "'s", 'Ġsecond', 'Ġrobotic', 'Ġspace', 'Ġshuttle', 'Ġcircling', 'Ġearth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġdean', 'Ġj', 'ames', 'Ġoct', 'ober', 'n', 'asa', 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġuse', 'Ġshuttle', 'Ġhang', 'ars', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġoct', 'ober', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'fact', 'Ġsheet', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġsm', 'ith', 'str', 'ick', 'land', 'Ġk', 'iona', 'Ġmay', 'Ġknow', 'Ġleast', 'Ġtwo', 'Ġpayload', 'Ġair', 'Ġspace']</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>['âĢĵ', '05', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġrev', 'http', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'http', 'space', 'x', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġje', 'ff', 'Ġf', 'oust', 'Ġde', 'cember', 'space', 'x', 'Ġpreparing', 'Ġlaunch', 'sign', 'ï', '¬', 'ģ', 'c', 'antly', 'Ġimproved', 'Ġfal', 'con', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'anian', 'Ġc', 'Ġsc', 'ott', 'Ġoct', 'ober', 'Ġel', 'Ġmus', 'k', 'Ġmit', 'Ġinterview', 'Ġevent', 'Ġoccurs', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'uly', 'Ġvia', 'Ġyoutube', 'th', 'Ġsw', 'Ġsupports', 'Ġsuccessful', 'Ġfal', 'con', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunch', 'th', 'Ġspace', 'Ġwing', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġshot', 'well', 'Ġmarch', 'Ġbroadcast', 'Ġspecial', 'Ġedition', 'Ġinterview', 'Ġshot', 'well', 'audio', 'Ġï', '¬', 'ģ', 'le', 'Ġspace', 'Ġshow', 'Ġevent', 'Ġoccurs', 'Ġ08', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'h', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġde', 'cember', 'space', 'x', 'Ġsuccessfully', 'Ġlanded', 'Ġfal', 'con', 'Ġrocket', 'Ġlaunching', 'Ġspace', 'ww', 'land', 'ing', 'success', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġj', 'ames', 'Ġdean', 'Ġmarch', 'usable', 'Ġfal', 'con', 'Ġrocket', 'Ġtriumph', 'Ġspace', 'x', 'Ġel', 'Ġmus', 'k', 'Ġus', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'el', 'mus', 'k', 'Ġj', 'une', 'flying', 'Ġlarger', 'Ġsign', 'ï', '¬', 'ģ', 'c', 'antly', 'Ġupgraded', 'Ġhyp', 'erson', 'ic', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġsingle', 'Ġpiece', 'Ġcast', 'Ġcut', 'Ġtitanium', 'Ġtake', 'entry', 'Ġheat', 'Ġshielding', 'twitter', 'weet', 'Ġretrieved', 'Ġj']</t>
+          <t>['smith', 'sonian', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġbur', 'gh', 'ard', 'Ġtom', 'Ġmay', 'Ġmilitar', 'ization', 'Ġouter', 'Ġspace', 'Ġpent', 'agon', "'s", 'Ġspace', 'Ġwarriors', 'ht', 'Ġspace', 'Ġdaily', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġp', 'arn', 'ell', 'Ġbrid', 'aine', 'Ġjan', 'uary', 'us', 'space', 'Ġwar', 'plane', 'Ġmay', 'Ġspying', 'Ġch', 'inese', 'Ġspac', 'el', 'ab', 'http', 'Ġregister', 'Ġarchived', 'web', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcor', 'oc', 'oto', 'Ġgen', 'al', 'yn', 'Ġjan', 'uary', 'ex', 'pert', 'Ġu', 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġlikely', 'sp', 'ying', 'Ġch', 'ina', 'Ġmodule', 'Ġinternational', 'Ġbusiness', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'uh', 'Ġal', 'Ġoct', 'ober', 'Ġsecret', 'Ġspace', 'Ġplane', "'s", 'Ġmission', 'Ġremains', 'Ġmystery', 'Ġoutside', 'Ġus', 'Ġmilitary', 'Ġguardian', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġr', 'uss', 'ary', 'ann', 'mber', 'space', 'Ġrace', 'Ġrevealed', 'Ġus', 'Ġch', 'ina', 'Ġtest', 'Ġfuturistic', 'Ġem', 'drive', 'iang', 'ong', 'Ġmysterious', 'Ġplane', 'Ġinternational', 'Ġbusiness', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġsh', 'aw', 'yer', 'Ġro', 'ger', 'n', 'ovember', 'âĢĵ', 'de', 'cember', 'second', 'Ġgeneration', 'Ġem', 'drive', 'Ġpropulsion', 'Ġapplied', 'st', 'Ġlauncher', 'Ġinterstellar', 'Ġprobe', 'Ġact', 'Ġastronaut', 'ica', 'âĢĵ', '07', '002', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġdepartment', 'Ġtrade', 'Ġindustry', 'bo', 'e', 'ing', 'Ġend', 'Ġuser', 'Ġundertaking', 'Ġretrieved', 'Ġde', 'cember', 'Ġh', 'ambling', 'Ġdavid', 'mber', 'pro', 'pell', 'ent', 'less', 'Ġspace', 'Ġpropulsion', 'Ġresearch', 'Ġcontinues', 'http', 'av', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġretrieved', 'Ġde', 'cember', 'Ġray', 'Ġapr', 'il', 'Ġlaunch', 'Ġdate', 'Ġï', '¬', 'ģ', 'r', 'ms', 'Ġnew', 'Ġdetails', 'Ġemerge', 'Ġexperiment', 'htt', 'Ġn', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>['une', 'Ġvia', 'Ġtwitter', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġj', 'une', 'space', 'x', "'s", 'Ġfinal', 'Ġfal', 'con', 'Ġdesign', 'Ġcoming', 'Ġyear', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'w', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġaug', 'ust', 'home', 'Ġforums', 'Ġsign', 'Ġiss', 'Ġcommercial', 'Ġshuttle', 'Ġsl', 'ion', 'Ġr', 'ussian', 'Ġeuro', 'pe', 'Ġch', 'inese', 'Ġunmanned', 'Ġfal', 'con', 'Ġblock', 'Ġdebut', 'Ġsuccess', 'Ġdragon', 'Ġarrives', 'Ġstation', 'Ġber', 'thing', 'Ġg', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġgra', 'ham', 'iam', 'Ġaug', 'ust', 'space', 'x', 'Ġfal', 'con', 'Ġlaunches', 'Ġcr', 'Ġdragon', 'Ġmission', 'Ġiss', 'Ġretrieved', 'Ġj', 'uly', 'Ġboy', 'le', 'Ġal', 'Ġoct', 'ober', 'space', 'x', "'s", 'Ġel', 'Ġmus', 'k', 'Ġg', 'eeks', 'Ġmars', 'Ġinter', 'plan', 'etary', 'Ġtransport', 'Ġplan', 'Ġreddit', 'Ġgeek', 'wire', 'Ġarchived', 'Ġut', 'ars', 'reddit', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary', 'space', 'x', 'Ġmay', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'n', 'al', 'Ġexpend', 'able', 'Ġrocket', 'Ġe', 'rocket', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'Ġcooper', 'Ġben', 'Ġapr', 'il', 'rocket', 'Ġlaunch', 'Ġviewing', 'Ġguide', 'Ġcape', 'aver', 'al', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', 'Ġset', 'Ġdebut', 'Ġfal', 'con', 'Ġrocket', 'Ġupgrades', 'Ġlaunch', 'Ġnext', 'Ġweek', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'web', 'Ġunch', 'next', 'week', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj']</t>
+          <t>['Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġpaw', 'ly', 'k', 'Ġori', 'ana', 'Ġj', 'uly', 'former', 'Ġsec', 'af', 'Ġexplains', 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġthrows', 'Ġenemies', 'Ġmilitary', 'Ġarchived', 'Ġow', 'en', 'emies', 'html', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġz', 'hen', 'Ġoct', 'ober', 'Ġus', 'Ġspace', 'Ġplane', 'Ġmark', 'Ġstart', 'Ġnew', 'Ġmilitary', 'Ġfrontier', '?"', 'front', 'ier', 'Ġsouth', 'Ġch', 'ina', 'Ġmorning', 'Ġpost', 'Ġarchived', 'front', 'ier', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'space', 'ï', '¬', 'Ĥ', 'ight', 'las', 'Ġlaunch', 'Ġreport', 'las', 'Ġrocket', 'Ġdelivers', 'Ġair', 'Ġforce', 'Ġspace', 'plane', 'Ġorbit', 'sp', "'s", 'Ġknow', 'Ġshadowy', 'Ġrecord', 'Ġdays', 'Ġspace', 'Ġoct', 'ober', 'Ġmill', 'er', 'Ġp', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġj', 'une', 'space', 'x', 'Ġscores', 'Ġcontract', 'Ġlaunch', 'Ġair', 'Ġforce', "'s", 'Ġsecretive', 'Ġspace', 'plane', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'mother', 'ship', 'Ġadop', 'ts', 'Ġnew', 'Ġspace', 'Ġplane', 'Ġ00', 'Ġnews', 'Ġarchived', 'id', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġdemonstr', 'ator', 'Ġtest', 'Ġfuture', 'Ġlaunch', 'Ġtechnologies', 'Ġorbit', 'entry', 'Ġenvironments', 'Ġn', 'asa', 'Ġmay', 'Ġfs', '05', 'ms', 'fc', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġaust', 'ap', 'ril', 'Ġspace', 'Ġvehicle', 'Ġstarting', 'Ġnew', 'Ġage', 'Ġspace', 'Ġcontrol', 'http', 'app', 'report', 'Ġdefense', 'Ġtechnical', 'Ġinformation', 'Ġcenter', 'Ġad', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġg', 'ary', 'Ġpay', 'ton', 'Ġsecretary', 'Ġair', 'Ġforce', 'Ġspace', 'Ġprograms', 'Ġmedia']</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>['une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġblock', 'Ġrockets', 'Ġtargets', 'mber', 'Ġlaunch', 'Ġdebut', 'es', 'lar', 'ati', 'Ġarchived', 'Ġove', 'mber', 'launch', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġk', 'yle', 'Ġed', 'space', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'http', 'sp', 'ac', 'el', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'f', 'iche', 'Ġtechnique', 'Ġfal', 'con', 'technical', 'Ġdata', 'Ġsheet', 'Ġfal', 'con', '].', 'Ġes', 'pace', 'Ġexploration', 'Ġfrench', 'Ġmay', 'Ġpp', 'âĢĵ', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'space', 'x', 'Ġdebut', 'Ġupgraded', 'Ġfal', 'con', 'Ġreturn', 'Ġflight', 'Ġmission', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'space', 'Ġlaunch', 'Ġreport', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġspace', 'flight', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġoverview', 'http', 'space', 'ï', '¬', 'Ĥ', 'ig', 'Ġspace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġspace', 'x', 'bang', 'aband', 'hu', 'Ġsatellite', 'Ġmission', 'yout', 'ub', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'web', 'ar', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'mber', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġprepares', 'Ġmission', 'Ġdragon', "'s", 'Ġreturn', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġaforementioned', 'Ġsecond', 'Ġstage', 'Ġtasked', 'Ġbusy', 'Ġrole', 'Ġmission', 'Ġloft', 'ing', 'Ġspacecraft']</t>
+          <t>['Ġtele', 'conference', 'pent', 'agon', 'Ġlaunch', 'Ġdefense', 'gov', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'Ġapr', 'il', 'bo', 'e', 'ing', "'s", 'Ġnew', 'Ġcrew', 'carry', 'ing', 'Ġspaceship', 'Ġtaking', 'Ġshape', 'http', 'sp', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'p', 'ilot', 'less', 'Ġus', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġdays', 'Ġorbit', 'Ġspace', 'Ġdaily', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'erson', 'iam', 'Ġe', '.;', 'ler', 'Ġk', 'athy', 'Ġcro', 'ck', 'et', 'ave', 'Ġle', 'w', 'Ġtim', 'Ġcur', 'tis', 'Ġper', 'oxide', 'Ġpropulsion', 'Ġturn', 'Ġcentury', 'th', 'Ġinternational', 'Ġsym', 'posium', 'Ġliquid', 'Ġspace', 'Ġpropulsion', 'Ġmarch', 'il', 'b', 'ron', 'n', 'Ġg', 'erman', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'uly', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'bert', 'Ġbart', 'Ġj', 'uly', 'per', 'oxide', 'Ġtest', 'Ġprograms', 'Ġflight', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'web', 'p', 'Ġn', 'asa', 'Ġengineering', 'Ġtest', 'Ġdirector', 'ate', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġsm', 'ith', 'str', 'ick', 'land', 'Ġk', 'iona', 'f', 'eb', 'ruary', "'s", '?"', 'Ġair', 'Ġspace', 'smith', 'sonian', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcher', 'ok', 'Ġb', 'oris', 'Ġe', 'ed', '.).', 'Ġrockets', 'Ġpeople', 'Ġ', 'ÑĢ', 'Ð°', 'Ðº', 'Ðµ', 'ÑĤ', 'Ñĭ', 'ĠÐ', '»', 'Ñ', 'İ', 'Ð´', 'Ð¸', 'Ġn', 'asa', 'Ġhistory', 'Ġseries', 'Ġvol', 'Ġn', 'asa', 'Ġp', 'Ġsp', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'Ġway', 'ne', 'Ġh', 'ale', 'Ġoral', 'Ġhistory', 'Ġn', 'asa', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une']</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1465,7 +1465,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>['Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', '."', 'Ġbar', 'bara', 'Ġop', 'rome', 'Ġoct', 'ober', 'ia', 'Ġdevelops', 'Ġsmall', 'Ġelectric', 'powered', 'sat', 'Ġdef', 'ensen', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'Ġtons', 'Ġlargest', 'Ġcommunications', 'Ġsatellite', 'Ġever', 'Ġbuilt', 'Ġ', 'ia', 'Ġscheduled', 'Ġlaunch', 'Ġearly', 'Ġcape', 'aver', 'al', 'Ġaboard', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlauncher', 'Ġreplace', 'Ġnearing', 'Ġend', 'year', 'Ġlife', '."', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġgun', 'ter', 'Ġarchived', 'w', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'orb', 'comm', 'Ġcraft', 'Ġfalls', 'Ġearth', 'Ġcompany', 'Ġclaims', 'Ġtotal', 'Ġloss', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'active', 'Ġlaunch', 'Ġvehicle', 'Ġreliability', 'Ġstatistics', 'http', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġarchived', 'Ġoriginal', 'g', 'html', 'rate', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'list', 'e', 'Ġde', 'ous', 'Ġles', 'Ġl', 'ance', 'ments', 'z', 'Ġk', 'os', 'mon', 'av', 'ika', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'est', 'imating', 'Ġreliability', 'Ġspacecraft', 'Ġmission', 'Ġ01', '0001', 'pdf', 'Ġn', 'asa', 'Ġjan', 'uary', 'Ġfigure', 'Ġhistorical', 'Ġrocket', 'Ġlaunch', 'Ġdata', 'Ġrocket', 'Ġfamily', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'hold', 'Ġarms', 'Ġtail', 'Ġservice', 'asts', 'http', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'fal', 'con', 'Ġcompletes', 'Ġfull', 'duration', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġe', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay']</t>
+          <t>['Ġalways', 'Ġconcern', 'Ġparticularly', 'Ġgot', 'Ġlonger', 'Ġlonger', 'Ġï', '¬', 'Ĥ', 'ights', "'s", 'Ġvest', 'ib', 'ular', 'Ġthings', 'Ġhappen', 'Ġvision', 'Ġchanges', 'Ġhappen', 'Ġpeople', 'Ġconcerned', 'Ġlanding', 'Ġwanted', 'Ġmake', 'Ġsure', 'Ġviable', 'Ġauto', 'land', 'Ġsystem', 'Ġprogram', 'Ġmanager', 'Ġgave', 'Ġus', 'Ġdirection', 'Ġtest', 'Ġsts', 'Ġworked', 'Ġhard', 'Ġdot', "'s", 'Ġcross', "'s", 'Ġcould', 'Ġauto', 'land', 'Ġtest', 'Ġauto', 'land', 'Ġtest', 'âĢĶ', "'re", 'Ġusing', 'Ġreal', 'Ġorbit', 'er', 'Ġlive', 'Ġcrew', "'ve", 'Ġgot', 'Ġkidding', 'Ġright', 'Ġmark', 'Ġcould', 'Ġreally', 'Ġbad', 'Ġ...', 'j', 'ed', 'j', 'ere', 'miah', 'Ġw', '.]', 'Ġpear', 'son', 'Ġassociate', 'Ġadministrator', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġformer', 'Ġmarine', 'Ġcorps', 'Ġgeneral', 'Ġrecall', 'Ġreviewed', 'Ġsaid', "'re", 'Ġgoing', 'Ġï', '¬', 'Ĥ', 'ying', 'Ġlong', 'duration', 'Ġï', '¬', 'Ĥ', 'ights', "'t", 'Ġneed', "'re", 'Ġgoing', 'Ġknock', '."', 'Ġdevastating', 'Ġteam', 'Ġset', 'Ġready', 'Ġexcited', 'Ġthought', 'Ġwould', 'Ġgood', 'Ġcapability', '."', 'Ġhal', 'v', 'ors', 'Ġtodd', 'Ġde', 'cember', 'Ġmini', 'shut', 'tle', 'Ġshrouded', 'Ġsecrecy', 'Ġcre', 'cy', '09', 'Ġair', 'Ġforce', 'Ġtimes', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'inside', 'Ġus', 'Ġair', 'Ġforce', "'s", 'Ġnext', 'Ġspace', 'Ġplane', 'Ġmystery', 'Ġmission', 'ht', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'secret', 'Ġspace', 'Ġplane', 'Ġspotted', 'Ġamateur', 'Ġsky', 'wat', 'chers', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'ateur', 'Ġastronomers', 'Ġunravel']</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1478,7 +1478,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>['space', 'x', 'Ġconducts', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'Ġtypically', 'Ġends', 'second', 'Ġengine', 'Ġï', '¬', 'ģ', 'ring', 'Ġevery', 'Ġlaunch', 'Ġwr', 'ing', 'Ġissues', 'Ġrocket', 'Ġground', 'Ġsystems', 'Ġexercise', 'Ġalso', 'Ġhelps', 'Ġengineers', 'Ġrehe', 'arse', 'Ġreal', 'Ġlaunch', 'Ġday', '."', 'Ġcl', 'ark', 'Ġstep', 'hen', 'st', 'arl', 'ink', 'Ġsatellite', 'Ġdeployments', 'Ġcontinue', 'Ġsuccessful', 'Ġfal', 'con', 'Ġlaunch', 'launch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'uly', 'ichael', 'Ġbel', 'ï', '¬', 'ģ', 'ore', 'Ġse', 'pt', 'ember', 'behind', 'Ġscenes', 'Ġworld', "'s", 'Ġambitious', 'Ġrocket', 'Ġmakers', 'http', 'popular', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'dates', 'Ġde', 'cember', '007', 'Ġupdates', 'Ġarchive', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'ht', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġnine', 'Ġengines', 'Ġstage', 'Ġworking', 'Ġwell', 'Ġsystem', 'Ġextensively', 'Ġtest', 'engine', 'Ġcapability', 'Ġincludes', 'Ġexplosive', 'Ġï', '¬', 'ģ', 'Ġtesting', 'Ġbarriers', 'Ġseparate', 'Ġengines', 'Ġvehicle', 'Ġ...', 'Ġsaid', 'Ġfailure', 'Ġmodes', "'ve", 'Ġseen', 'Ġdate', 'Ġtest', 'Ġstand', 'Ġmer', 'lin', 'Ġrelatively', 'Ġbenign', 'Ġturbo', 'Ġpump', 'Ġcombustion', 'Ġchamber', 'Ġnozzle', 'Ġrupture', 'Ġexplos', 'ively', 'Ġeven', 'Ġsubjected', 'Ġextreme', 'Ġcircumstances', 'Ġseen', 'Ġgas', 'Ġgenerator', 'Ġdrives', 'Ġturbo', 'Ġpump', 'Ġassembly', 'Ġblow', 'Ġapart', 'Ġstart', 'Ġsequence', 'Ġchecks', 'Ġplace', 'Ġprevent', 'Ġhappening', 'Ġsmall', 'Ġdevice', 'Ġunlikely', 'Ġcause', 'Ġmajor', 'Ġdamage', 'Ġengine', 'Ġlet', 'Ġalone', 'Ġneighbouring', 'Ġones', 'Ġeven', 'Ġengine', 'Ġn', 'ace', 'es', 'Ġcommercial', 'Ġjets', 'Ġï', '¬', 'ģ', 'expl', 'os', 'ive', 'Ġbarriers', 'Ġassume', 'Ġentire', 'Ġchamber', 'Ġblows', 'Ġapart', 'Ġworst', 'Ġpossible', 'Ġway', 'Ġbottom', 'Ġclose', 'Ġpanels', 'Ġdesigned', 'Ġdirect', 'Ġforce', 'Ġï', '¬', 'Ĥ', 'ame', 'Ġdownward', 'Ġaway', 'Ġneighbouring', 'Ġengines', 'Ġstage', 'Ġ...', "'ve", 'Ġfound', 'Ġfal', 'con', 'Ġability', 'Ġwithstand', 'Ġone', 'Ġeven', 'Ġmultiple', 'Ġengine', 'Ġfailures', 'Ġcommercial', 'Ġair', 'liners', 'Ġstill', 'Ġcomplete', 'Ġmission', 'Ġcompelling', 'Ġselling', 'Ġpoint', 'Ġcustomers', 'Ġapart']</t>
+          <t>['Ġorbit', 'Ġsay', 'Ġlikely', 'Ġuse', 'Ġdeploying', 'Ġsatellites', 'http', 'new', 'Ġnews', 'au', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġbroad', 'iam', 'Ġj', 'Ġmay', 'sur', 'illance', 'Ġsuspected', 'Ġspacecraft', "'s", 'Ġmain', 'Ġrole', 'n', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'pre', 'par', 'ations', 'Ġunderway', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanding', 'Ġu', 'Ġair', 'Ġforce', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'us', 'af', 'Ġlanding', 'Ġslated', 'Ġdec', 'âĢĵ', 'Ġaviation', 'Ġweek', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'home', 'Ġu', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġreturns', 'Ġearth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġwar', 'wic', 'j', 'Ġgra', 'ham', 'Ġde', 'cember', 'us', 'af', "'s", 'Ġspace', 'plane', 'Ġreturns', 'Ġearth', 'web', 'arch', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġr', 'con', 'Ġp', 'aul', 'Ġde', 'cember', 'Ġus', 'Ġmilitary', 'Ġspace', 'plane', 'Ġreturns', 'Ġearth', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'cc', 'ants', 'ike', 'usa', 'Ġsatellite', 'Ġdetails', '010', 'ad', 'ell', 'ite', '/?', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġwall', 'ike', 'Ġmarch', 'secret', 'ive', 'Ġspace', 'Ġplane', 'Ġlaunches', 'Ġnew', 'Ġmystery', 'Ġmission', 'Ġspace', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'mber', 'military', 'Ġspace', 'Ġshuttle', 'Ġreceives', 'Ġmission', 'Ġextension', 'Ġspace', 'ï', '¬']</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>['Ġspace', 'Ġshuttle', 'Ġnone', 'Ġexisting', 'Ġlaunch', 'Ġvehicles', 'Ġafford', 'Ġlose', 'Ġeven', 'Ġsingle', 'Ġthrust', 'Ġchamber', 'Ġwithout', 'Ġcausing', 'Ġloss', 'Ġmission', '."', 'space', 'x', 'Ġengine', 'Ġissue', 'Ġlast', 'Ġstar', 'link', 'Ġmission', 'Ġcaused', 'Ġcleaning', 'Ġï', '¬', 'Ĥ', 'uid', 'Ġaccording', 'Ġel', 'Ġmus', 'k', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'component', 'Ġfatigue', 'Ġcaused', 'Ġearly', 'Ġshutdown', 'Ġmer', 'lin', 'Ġengine', 'Ġlast', 'Ġspace', 'x', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'http', 'Ġretrieved', 'Ġjan', 'uary', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġmarch', 'ch', 'ris', 'Ġber', 'gin', 'Ġn', 'sf', 'Ġtwitter', 'Ġfal', 'con', 'Ġlanding', 'Ġfailure', 'Ġupdate', 'Ġmer', 'lin', 'Ġengine', 'Ġboot', 'Ġlife', 'Ġleader', 'Ġdeveloped', 'Ġhole', 'Ġsent', 'Ġhot', 'Ġgas', "'t", 'Ġsupposed', 'Ġshut', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġenough', 'Ġthrust', 'Ġlanding', 'Ġtwitter', 'Ġretrieved', 'Ġjan', 'uary', 'Ġl', 'ind', 'sey', 'Ġcl', 'ark', 'inter', 'view', 'Ġel', 'Ġmus', 'k', 'http', 'h', 'obby', 'Ġh', 'obb', 'ys', 'pace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'x', 'Ġattempt', 'Ġdevelop', 'Ġfully', 'Ġreusable', 'Ġspace', 'Ġlaunch', 'Ġvehicle', 'Ġwashing', 'ton', 'Ġpost', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġrocket', "'s", 'Ġstages', 'Ġwould', 'Ġreturn', 'Ġlaunch', 'Ġsite', 'Ġtouch', 'Ġvertically', 'Ġrocket', 'Ġpower', 'Ġlanding', 'Ġgear', 'Ġdelivering', 'Ġspacecraft', 'Ġorbit', '."', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġwall', 'ike', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġunve', 'ils', 'Ġplan', 'Ġworld', "'s", 'Ġfirst', 'Ġfully', 'Ġreusable', 'Ġrocket', 'Ġspace', 'Ġarchived', 'Ġket', 'el', 'mus', 'k', 'html', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġboy', 'le', 'Ġal', 'Ġde', 'cember', 'space', 'x', 'Ġlaunches', 'Ġgrass', 'ho', 'pper', 'Ġrocket', 'story', 'high', 'Ġhop', 'Ġtex', 'http', 'cos', 'mi', 'Ġcosmic', 'Ġlog', 'Ġarchived', 'Ġoriginal', 'Ġmarch']</t>
+          <t>['Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'air', 'Ġforce', "'s", 'Ġsecret', 'spect', 'acular', 'Ġsuccess', 'id', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'pre', 'par', 'ations', 'Ġunderway', 'Ġlanding', 'Ġu', 'Ġair', 'Ġforce', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'air', 'Ġforce', "'s", 'Ġsecretive', 'Ġspace', 'Ġplane', 'Ġland', 'Ġsoon', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġlands', 'Ġmorning', 'Ġv', 'enberg', 'Ġl', 'anta', 'Ġmar', 'ia', 'Ġtimes', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġwall', 'ike', 'Ġj', 'une', 'air', 'Ġforce', "'s", 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġcal', 'Ġmystery', 'Ġmission', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġray', 'Ġse', 'pt', 'ember', 'another', 'las', 'Ġread', 'ied', 'Ġlaunch', 'Ġmini', 'Ġspace', 'Ġshuttle', 'http', 'space', 'ï', '¬', 'Ĥ', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġoct', 'ober', 'cc', 'ull', 'ough', 'Ġamy', 'Ġoct', 'ober', 'Ġlaunch', 'Ġdelayed', 'Ġair', 'Ġforce', 'Ġmagazine', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġde', 'cember', 'kinson', 'Ġn', 'ancy', 'Ġde', 'cember', 'air', 'Ġforce', "'s", 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġlaunches', 'Ġthird', 'Ġmission', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'mber', 'new', 'Ġdelay', 'Ġmysterious', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġlaunch', 'http', 'Ġspace', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'n', 'ss', 'dc', 'Ġid']</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġde', 'cember', 'Ġgra', 'ham', 'iam', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġsuccessfully', 'Ġlaunches', 'Ġdebut', 'Ġfal', 'con', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'dragon', 'Ġsuccessfully', 'Ġlaunched', 'Ġrocket', 'Ġrecovery', 'Ġdemo', 'Ġcrash', 'Ġlands', 'http', 'space', 'ï', '¬', 'Ĥ', 'ight', 'n', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'ris', 'Ġapr', 'il', 'space', 'x', 'Ġchecks', 'Ġthrottle', 'Ġvalve', 'Ġflawed', 'Ġfal', 'con', 'Ġrecovery', 'Ġattempt', 'att', 'empt', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'Ġwall', 'ike', 'Ġde', 'cember', 'wow', 'Ġspace', 'x', 'Ġlands', 'Ġorbital', 'Ġrocket', 'Ġsuccessfully', 'Ġhistoric', 'Ġfirst', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'space', 'x', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġlanding', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġsecond', 'Ġstage', 'Ġcontinuing', 'Ġnom', 'inally', 'http', 'weet', 'Ġretrieved', 'Ġmay', 'Ġvia', 'Ġtwitter', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'launch', 'Ġschedule', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmark', 'us', 'Ġpay', 'er', 'Ġmarch', 'ses', 'Ġlaunched', 'Ġsuccessfully', 'Ġspace', 'x', "'s", 'Ġï', '¬', 'Ĥ', 'ight', 'proven', 'Ġfal', 'con', 'Ġrocket', 'ses', 'co', 'press', 'Ġrelease', 'es', 'Ġarchived', 'http', 'Ġen', 'fal', 'con', 'rocket', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'une', 'Ġbart', 'Ġle', 'ah', 'Ġapr', 'il', 'tw', 'ice', 'laun', 'ched', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġreturned', 'Ġport', 'aver', 'al', 'Ġspace', 'flight', 'Ġinsider', 'Ġarchived', 'Ġ', 'eral', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'bul', 'gar', 'ia', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcommunications', 'Ġsatellite', 'Ġride', 'Ġspace', 'x', "'s", 'Ġsecond', 'Ġreused', 'Ġrocket', 'space', 'ï']</t>
+          <t>['07', 'Ġnational', 'Ġspace', 'Ġscience', 'Ġdata', 'Ġcenter', 'Ġn', 'asa', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbad', 'ger', 'Ġer', 'ic', 'Ġde', 'cember', 'air', 'Ġforce', 'Ġlaunches', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġpars', 'ons', 'Ġdan', 'Ġoct', 'ober', 'us', 'Ġair', 'Ġforce', "'s", 'Ġshadowy', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġdays', 'Ġorbit', 'Ġn', '04', 'Ġflight', 'Ġglobal', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'secret', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġus', 'Ġair', 'Ġforce', 'Ġbase', 'Ġunknown', 'Ġtwo', 'year', 'Ġmission', 'Ġguardian', 'Ġassociated', 'Ġpress', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'Ġoct', 'ober', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġrecord', 'sh', 'attering', 'Ġsecret', 'Ġmission', 'Ġspace', 'Ġarchived', 'Ġe', 'land', 'ing', 'html', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġray', 'Ġmay', 'rec', 'ap', 'Ġstory', 'Ġspace', 'plane', 'Ġemb', 'arks', 'Ġfourth', 'Ġvoyage', 'Ġorbit', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', "'s", 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġhall', 'Ġthr', 'uster', 'Ġdemonstrates', 'Ġsuccessful', 'orbit', 'Ġoperation', 'htt', 'press', 'Ġrelease', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġj', 'uly', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'Ġmay', 'us', 'Ġair', 'Ġforce', 'Ġlaunches', 'Ġspace', 'Ġplane', 'th', 'Ġmystery', 'Ġmission', 'http', 'Ġspace', 'Ġarchived', 'Ġh', 'mission', 'html', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġray', 'Ġmay', 'Ġspace', 'plane', 'Ġreturns', 'Ġearth', 'Ġmakes', 'Ġautop', 'ilot', 'Ġlanding', 'Ġfl', 'ida', 'Ġlot', 'land', 'ing', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight']</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>['¬', 'Ĥ', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'p', 'rel', 'aunch', 'Ġpreview', 'Ġspace', 'x', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'every', 'Ġeveryday', 'Ġastronaut', 'mber', 'Ġarchived', 'w', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'space', 'x', 'Ġresume', 'Ġstar', 'link', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġstretching', 'Ġreused', 'Ġfal', 'con', 'Ġrockets', 'Ġlimits', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġlaunches', 'Ġstar', 'link', 'Ġsatellites', 'Ġrecord', 'th', 'Ġlif', 'ff', 'Ġlanding', 'Ġreused', 'Ġrocket', 'Ġspace', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġr', 'us', 'sell', 'Ġb', 'og', 'ove', 'Ġj', 'uly', 'use', 'Ġspace', 'x', 'Ġplan', 'Ġachieve', 'us', 'ability', 'Ġfal', 'con', 'second', 'Ġstage', '?"', 'htt', 'Ġst', 'ac', 'ke', 'x', 'change', 'Ġarchived', 'stage', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġjan', 'uary', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', 'Ġsuccessfully', 'Ġcatches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġfair', 'ing', 'Ġste', 'ven', "'s", 'ms', 'Ġtree', "'s", 'Ġnet', 'ww', 'Ġeven', 'ms', 'tree', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġapr', 'il', 'rocket', 'Ġreport', 'Ġspace', 'x', 'Ġab', 'ons', 'Ġcatching', 'Ġfair', 'ings', '..."', 'Ġer', 'st', 'ages', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'space', 'x', 'Ġpoised', 'Ġlaunch', 'Ġhistoric', 'Ġpad', 'http', '09', 'Ġsm', 'ith', 'sonian', 'Ġair', 'Ġspace', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsim', 'burg', 'Ġrand', 'space', 'x', 'Ġpress']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġjack', 'son', 'anda', 'Ġmay', 'air', 'Ġforce', "'s", 'Ġmysterious', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġwakes', 'Ġfl', 'ida', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġlaunches', 'Ġair', 'Ġforce', "'s", 'Ġspace', 'plane', 'Ġhurricane', 'Ġ', 'irm', 'Ġreaches', 'Ġfl', 'ida', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġgra', 'ham', 'iam', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġfal', 'con', 'w', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'air', 'Ġforce', 'Ġpreparing', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'f', 'th', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġmission', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġair', 'Ġforce', 'Ġnews', 'Ġservice', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdavid', 'Ġle', 'ard', 'Ġaug', 'ust', 'ster', 'ious', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġnear', 'Ġyear', 'Ġorbit', 'http', 'Ġspace', 'Ġarchived', 'http', 'year', 'orbit', 'html', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'adv', 'anced', 'Ġstruct', 'urally', 'Ġembedded', 'Ġthermal', 'Ġspread', 'er', 'ets', 'ii', ')"', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'u', 'Ġmilitary', "'s", 'Ġspace', 'plane', 'Ġlands', 'Ġfl', 'ida', 'space', 'ï', '¬', 'Ĥ', 'ig', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgall', 'op', 'Ġj', 'Ġoct', 'ober', 'u', 'Ġair', 'force', "'s", 'Ġreturns', 'Ġearth', 'bo', 'om', 'Ġnew', 'Ġrecord', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġus', 'Ġtoday', 'Ġfl', 'ida', 'Ġtoday', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgra', 'ham', 'iam', 'Ġmay', 'ula', 'las', 'Ġlaunches', 'Ġsixth', 'Ġmission', 'Ġspace', 'plane', 'w', 'space', 'Ġforce']</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1530,7 +1530,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>['Ġconference', 'http', 'tr', 'ste', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', '..', 'Ġmus', 'k', 'Ġquote', 'Ġnever', 'Ġgive', 'Ġnever', 'us', 'ability', 'Ġone', 'Ġimportant', 'Ġgoals', 'Ġbecome', 'Ġbiggest', 'Ġlaunch', 'Ġcompany', 'Ġworld', 'Ġmaking', 'Ġmoney', 'Ġhand', 'Ġï', '¬', 'ģ', 'st', "'re", 'Ġstill', 'Ġreusable', 'Ġconsider', 'Ġus', 'Ġfailed', '".', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġmarch', 'space', 'x', 'Ġprepares', 'Ġfal', 'con', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunch', 'Ġtargets', 'Ġreturn', 'n', 'asa', 'Ġ', 'urn', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġch', 'ris', 'Ġg', 'eb', 'hardt', 'Ġapr', 'il', 'fal', 'con', 'Ġheavy', 'Ġbuild', 'Ġbegins', 'Ġpad', 'Ġrebuild', 'Ġprogressing', 'Ġwell', 'Ġess', 'ing', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'space', 'Ġlaunch', 'Ġdelta', 'Ġlease', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġspace', 'Ġx', 'Ġv', 'enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġoverview', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġus', 'Ġbeat', 'Ġch', 'ina', 'Ġfacts', 'Ġspace', 'x', 'Ġcosts', 'htt', 'Ġom', 'usa', 'php', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'space', 'x', 'Ġbooks', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtwo', 'Ġlaunches', 'Ġu', 'Ġmilitary', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġtestimony', 'Ġel', 'Ġmus', 'k', 'Ġmay', 'space', 'Ġshuttle', 'Ġfuture', 'Ġspace', 'Ġlaunch', 'Ġvehicles', 'Ġu', 'Ġsenate']</t>
+          <t>["'s", 'Ġsecretive', 'Ġplane', 'Ġspent', 'Ġdays', 'Ġorbit', 'mber', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'pay', 'loads', 'Ġrevealed', 'Ġnext', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġmilitary', 'Ġspace', 'plane', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġmay', 'next', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġscheduled', 'Ġlaunch', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'cd', 'owell', 'Ġj', 'athan', 'Ġj', 'une', 'jon', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'graded', 'Ġspace', 'plane', 'Ġrockets', 'Ġorbit', 'Ġaboard', 'las', 'Ġlauncher', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġk', 'les', 'ius', 'ichael', 'jan', 'uary', 'space', 'Ġshuttle', 'j', 'r', '/?', 'Ġair', 'Ġspace', 'Ġmagazine', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġdavid', 'Ġle', 'ard', 'Ġoct', 'ober', 'secret', 'ive', 'Ġus', 'Ġspace', 'Ġplane', 'Ġcould', 'Ġevolve', 'Ġcarry', 'Ġastronauts', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'bo', 'e', 'ing', 'Ġbo', 'e', 'ing', 'Ġcitizens', 'Ġspace', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġbo', 'e', 'ing', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġjohn', 'Ġapr', 'il', 'air', 'Ġforce', 'Ġlaunch', 'Ġrobotic', 'Ġwing', 'ed', 'Ġspace', 'Ġplane', 'Ġphys', 'org', 'Ġassociated', 'Ġpress', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġle', 'ard', 'Ġdavid', 'mber', 'secret', 'ive', 'Ġair', 'Ġforce', 'Ġrobotic', 'Ġspace', 'Ġplane', 'Ġmay', 'Ġnearing', 'Ġmission', "'s", 'Ġend', 'html', 'Ġspace', 'Ġretrieved', 'Ġapr', 'il', 'Ġmol', 'c', 'zan', 'Ġted', 'Ġmay', 'Ġsearch', 'Ġelements']</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmarch', 'national', 'Ġpress', 'Ġclub', 'Ġfuture', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'press', 'Ġrelease', 'Ġc', 'span', 'org', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'environment', 'al', 'Ġassessment', 'Ġboost', 'back', 'Ġlanding', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġwest', 'web', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġmarch', 'space', 'x', 'Ġï', '¬', 'Ĥ', 'Ġreused', 'Ġrockets', 'Ġhalf', 'Ġlaunches', 'Ġcompetition', 'Ġl', 'ags', 'Ġfar', 'Ġbehind', 'laun', 'ches', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġtargets', 'Ġcommercial', 'Ġstarship', 'Ġlaunch', 'sp', 'ac', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'ster', 'Ġch', 'ris', 'Ġoct', 'ober', 'space', 'x', 'Ġreduces', 'Ġlaunch', 'Ġcosts', 'Ġc', 'es', 'launch', 'cost', 'Ġadvanced', 'Ġtelevision', 'Ġarchived', 'web', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'r', 'ussia', 'Ġcut', 'Ġspace', 'Ġlaunch', 'Ġprices', 'Ġpercent', 'Ġresponse', 'Ġspace', 'x', 'Ġpredatory', 'Ġpricing', 'Ġarchived', 'http', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'el', 'mus', 'k', 'Ġapr', 'il', 'space', 'x', 'Ġrockets', 'Ġreusable', '%.', 'Ġactual', 'Ġproblem', 'weet', 'Ġretrieved', 'Ġmay', 'Ġvia', 'Ġtwitter', 'ula', 'Ġce', 'ory', 'Ġbr', 'uno', "'s", 'Ġview', 'Ġeconomics', 'using', 'Ġrockets', 'Ġprop', 'ulsive', 'Ġï', '¬', 'Ĥ', 'back', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġel', 'Ġmus', 'k', 'Ġbreaks', 'Ġcosts', 'Ġreusable', 'Ġrockets', 'econom', 'ics', 'Ġarchived', 'econom', 'ics', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved']</t>
+          <t>['html', 'Ġsat', 'obs', 'org', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'une', 'Ġev', 'ans', 'ichael', 'Ġapr', 'il', 'launch', 'Ġsecret', 'Ġus', 'Ġspace', 'Ġship', 'Ġmasks', 'Ġeven', 'Ġsecret', 'Ġlaunch', 'Ġnew', 'Ġweapon', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'plane', 'Ġcompletes', 'Ġsixth', 'Ġmission', 'Ġlands', 'Ġnearly', 'Ġmonths', 'Ġorbit', 'sp', 'ac', 'en', 'ew', 'mber', 'Ġbent', 'ley', 'Ġmatt', 'hew', 'Ġspace', 'planes', 'Ġairport', 'Ġspac', 'eport', 'Ġnew', 'ork', 'Ġspring', 'er', 'Ġreading', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġg', 'ump', 'Ġdavid', 'Ġp', 'Ġspace', 'Ġenterprise', 'Ġbeyond', 'Ġn', 'asa', 'Ġwest', 'port', 'Ġconnect', 'icut', 'Ġpra', 'eger', 'Ġmill', 'er', 'Ġj', 'ay', 'Ġx', 'planes', 'Ġh', 'ck', 'ley', 'Ġmid', 'land', 'Ġyen', 'ne', 'Ġbill', 'Ġstory', 'Ġbo', 'e', 'ing', 'Ġcompany', 'Ġmin', 'neapolis', 'Ġmin', 'n', '.:', 'Ġz', 'en', 'ith', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġfact', 'Ġsheet', 'Ġarchived', 'Ġj', 'une', 'Ġway', 'back', 'Ġmachine', 'Ġu', 'Ġair', 'Ġforce', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġpage', 'Ġbo', 'e', 'ing', 'Ġfact', 'Ġsheet', 'Ġarchived', 'Ġoct', 'ober', 'Ġway', 'back', 'Ġmachine', 'Ġn', 'asa', 'gov', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>['Ġse', 'pt', 'ember', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'new', 'Ġopportunities', 'Ġsmall', 'sat', 'Ġlaunches', 'Ġspace', 'Ġreview', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġ...', 'Ġdeveloped', 'Ġprices', 'Ġï', '¬', 'Ĥ', 'ying', 'Ġsecondary', 'Ġpayload', 'Ġ...', 'Ġp', 'pod', 'Ġwould', 'Ġcost', '000', '000', 'Ġmissions', 'Ġle', '000', '000', 'Ġmissions', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', 'Ġesp', 'ac', 'lass', 'Ġsatellite', 'Ġweighing', 'Ġkilograms', 'Ġwould', 'Ġcost', 'âĢĵ', 'Ġmillion', 'Ġle', 'Ġmissions', 'âĢĵ', 'Ġmillion', 'Ġg', 'Ġmissions', 'Ġsaid', '."', 'space', 'x', 'Ġputs', 'Ġhistoric', 'Ġï', '¬', 'Ĥ', 'Ġrocket', 'Ġpermanent', 'Ġdisplay', 'http', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġmay', 'old', 'Ġfal', 'con', 'Ġrockets', 'Ġdone', 'Ġï', '¬', 'ģ', 'ring', 'Ġengines', 'ï', '¬', 'Ĥ', 'ame', 'Ġimag', 'inations', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'web', 'ar', 'h', 'ouston', 'Ġoriginal', 'Ġmay', 'space', 'x', 'Ġfal', 'con', 'Ġbooster', 'Ġexhibit', 'Ġopen', 'space', 'ce', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġloc', 'ke', 'Ġj', 'ared', 'Ġoct', 'ober', 'Ġ"[', 'update', 'Ġnew', 'Ġarrival', 'Ġfootage', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġbooster', 'Ġarrives', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġvisitor', 'Ġcomplex', 'Ġpermanent', 'Ġdisplay', 'space', 'exp', 'Ġspace', 'Ġexplored', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'ï', '¬', 'ģ', 'cial', 'Ġpage', 'Ġsa', 'ocom', 'Ġlaunch', 'Ġlanding', 'Ġtest', 'Ġï', '¬', 'ģ', 'ring', 'Ġtwo', 'Ġmer', 'lin', 'Ġengines', 'Ġconnected', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġmovie', 'Ġmovie', 'Ġjan', 'uary', 'Ġpress', 'Ġrelease', 'Ġannouncing', 'Ġdesign', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġhopes', 'Ġsupply', 'Ġiss', 'Ġnew', 'Ġfal', 'con', 'Ġheavy', 'Ġlauncher', 'flight', 'Ġinternational', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġlaunches', 'Ġfal', 'con', 'Ġcustomer', 'Ġr', 'index', 'php', 'Ġarchived', 'Ġj', 'une', 'Ġway', 'back', 'Ġmachine', 'defense', 'Ġindustry', 'Ġdaily', 'Ġse']</t>
+          <t>['Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġreplica', 'Ġsp', 'ut', 'nik', 'Ġcommunications', 'Ġsatellite', 'Ġcommunications', 'Ġsatellite', 'Ġartificial', 'Ġsatellite', 'Ġrel', 'ays', 'Ġampl', 'ifies', 'Ġradio', 'Ġtele', 'communication', 'Ġsignals', 'Ġvia', 'Ġtrans', 'p', 'onder', 'Ġcreates', 'Ġcommunication', 'Ġchannel', 'Ġsource', 'Ġtransmitter', 'Ġreceiver', 'Ġdifferent', 'Ġlocations', 'Ġearth', 'Ġcommunications', 'Ġsatellites', 'Ġused', 'Ġtelevision', 'Ġtelephone', 'Ġradio', 'Ġinternet', 'Ġmilitary', 'Ġapplications', 'Ġmany', 'Ġcommunications', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġmiles', 'Ġequ', 'ator', 'Ġsatellite', 'Ġappears', 'Ġstationary', 'Ġpoint', 'Ġtherefore', 'Ġsatellite', 'Ġdish', 'Ġantennas', 'Ġground', 'Ġstations', 'Ġaimed', 'Ġpermanently', 'Ġspot', 'Ġmove', 'Ġtrack', 'Ġsatellite', 'Ġothers', 'Ġform', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġantennas', 'Ġground', 'Ġfollow', 'Ġposition', 'Ġsatellites', 'Ġswitch', 'Ġsatellites', 'Ġfrequently', 'Ġhigh', 'Ġfrequency', 'Ġradio', 'Ġwaves', 'Ġused', 'Ġtelecommunications', 'Ġlinks', 'Ġtravel', 'Ġline', 'Ġsight', 'Ġob', 'structed', 'Ġcurve', 'Ġearth', 'Ġpurpose', 'Ġcommunications', 'Ġsatellites', 'Ġrelay', 'Ġsignal', 'Ġaround', 'Ġcurve', 'Ġearth', 'Ġallowing', 'Ġcommunication', 'Ġwidely', 'Ġseparated', 'Ġgeographical', 'Ġpoints', 'Ġcommunications', 'Ġsatellites', 'Ġuse', 'Ġwide', 'Ġrange', 'Ġradio', 'Ġmicrowave', 'Ġfrequencies', 'Ġavoid', 'Ġsignal', 'Ġinterference', 'Ġinternational', 'Ġorganizations', 'Ġregulations', 'Ġfrequency', 'Ġranges', 'bands', 'Ġcertain', 'Ġorganizations', 'Ġallowed', 'Ġuse', 'Ġallocation', 'Ġbands', 'Ġminim', 'izes', 'Ġrisk', 'Ġsignal', 'Ġinterference', 'Ġoct', 'ober', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'Ġpublished', 'Ġarticle', 'Ġtitled', 'ext', 'r', 'ater', 'restrial', 'Ġrel', 'ays', 'Ġb', 'rit', 'ish', 'Ġmagazine', 'Ġwireless', 'Ġarticle', 'Ġdescribed', 'Ġfundamentals', 'Ġbehind', 'Ġdeployment', 'Ġartificial', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġrelay', 'Ġradio', 'Ġsignals', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'Ġoften', 'Ġquoted', 'Ġinventor', 'Ġconcept', 'Ġcommunications', 'Ġsatellite', 'Ġterm', 'cl', 'ar', 'ke', 'Ġbelt', 'Ġemployed', 'Ġdescription', 'Ġfirst', 'Ġartificial', 'Ġearth', 'Ġsatellite', 'Ġsp', 'ut', 'nik', 'Ġput', 'Ġorbit', 'v', 'iet', 'Ġunion', 'Ġoct', 'ober', 'Ġdeveloped', 'ikhail', 'ikh', 'rav', 'ov', 'Ġser', 'gey', 'Ġk', 'ole', 'v', 'Ġbuilding', 'Ġwork', 'Ġk', 'stant', 'Ġsp', 'ut', 'nik', 'Ġequipped', 'Ġonboard', 'Ġradio', 'Ġtransmitter', 'Ġworked', 'Ġtwo', 'Ġfrequencies', '005', '002', 'Ġmeters', 'Ġwavelength', 'Ġsatellite', 'Ġplaced']</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>['pt', 'ember', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġorbit', 'Ġsend', 'Ġdata', 'Ġone', 'Ġpoint', 'Ġearth', 'Ġanother', 'Ġradio', 'Ġtransmitter', 'Ġmeant', 'Ġstudy', 'Ġproperties', 'Ġradio', 'Ġwave', 'Ġdistribution', 'Ġthroughout', 'Ġion', 'osphere', 'Ġhistory', 'Ġorigins', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'las', 'b', 'Ġscore', 'Ġlaunch', 'Ġpad', 'Ġrocket', 'without', 'Ġbooster', 'Ġengines', 'Ġconstituted', 'Ġsatellite', 'Ġlaunch', 'Ġsp', 'ut', 'nik', 'Ġmajor', 'Ġstep', 'Ġexploration', 'Ġspace', 'Ġrocket', 'Ġdevelopment', 'Ġmarks', 'Ġbeginning', 'Ġspace', 'Ġtwo', 'Ġmajor', 'Ġclasses', 'Ġcommunications', 'Ġsatellites', 'Ġpassive', 'Ġactive', 'Ġpassive', 'Ġsatellites', 'Ġreflect', 'Ġsignal', 'Ġcoming', 'Ġsource', 'Ġtoward', 'Ġdirection', 'Ġreceiver', 'Ġpassive', 'Ġsatellites', 'Ġreflected', 'Ġsignal', 'Ġamplified', 'Ġsatellite', 'Ġsmall', 'Ġamount', 'Ġtransmitted', 'Ġenergy', 'Ġactually', 'Ġreaches', 'Ġreceiver', 'Ġsince', 'Ġsatellite', 'Ġfar', 'Ġearth', 'Ġradio', 'Ġsignal', 'Ġatten', 'uated', 'Ġdue', 'Ġfree', 'space', 'Ġpath', 'Ġloss', 'Ġsignal', 'Ġreceived', 'Ġearth', 'Ġweak', 'Ġactive', 'Ġsatellites', 'Ġhand', 'Ġamplify', 'Ġreceived', 'Ġsignal', 'Ġret', 'rans', 'mitting', 'Ġreceiver', 'Ġground', 'Ġpassive', 'Ġsatellites', 'Ġfirst', 'Ġcommunications', 'Ġsatellites', 'Ġlittle', 'Ġused', 'Ġwork', 'Ġbegun', 'Ġfield', 'Ġelectrical', 'Ġintelligence', 'Ġgathering', 'Ġunited', 'Ġstates', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġled', 'Ġproject', 'Ġnamed', 'Ġcommunication', 'Ġmoon', 'Ġrelay', 'Ġmilitary', 'Ġplanners', 'Ġlong', 'Ġshown', 'Ġconsiderable', 'Ġinterest', 'Ġsecure', 'Ġreliable', 'Ġcommunications', 'Ġlines', 'Ġtactical', 'Ġnecessity', 'Ġultimate', 'Ġgoal', 'Ġproject', 'Ġcreation', 'Ġlongest', 'Ġcommunications', 'Ġcircuit', 'Ġhuman', 'Ġhistory', 'Ġmoon', 'Ġearth', "'s", 'Ġnatural', 'Ġsatellite', 'Ġacting', 'Ġpassive', 'Ġrelay', 'Ġachieving', 'Ġfirst', 'Ġtrans', 'cean', 'ic', 'Ġcommunication', 'Ġwashing', 'ton', 'Ġhaw', 'aii', 'Ġjan', 'uary', 'Ġsystem', 'Ġpublicly', 'Ġinaug', 'urated', 'Ġput', 'Ġformal', 'Ġproduction', 'Ġjan', 'uary', 'Ġfirst', 'Ġsatellite', 'Ġpurpose', 'built', 'Ġactively', 'Ġrelay', 'Ġcommunications', 'Ġproject', 'Ġscore', 'Ġled', 'Ġadvanced', 'Ġresearch', 'Ġprojects', 'Ġagency', 'arp', 'Ġlaunched', 'Ġde', 'cember', 'Ġused', 'Ġtape', 'Ġrecorder', 'Ġcarry', 'Ġstored', 'Ġvoice', 'Ġmessage', 'Ġwell', 'Ġreceive', 'Ġstore', 'Ġret', 'rans', 'mit', 'Ġmessages', 'Ġused', 'Ġsend', 'Ġchrist', 'mas', 'Ġgreeting', 'Ġworld', 'Ġu', 'Ġpresident', 'Ġdw', 'ight', 'Ġe', 'isen', 'hower', 'Ġsatellite', 'Ġalso', 'Ġexecuted', 'Ġseveral', 'Ġreal', 'time', 'Ġtransmissions', 'Ġnon', 'charge', 'able', 'Ġbatteries', 'Ġfailed', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>['09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġelectron', 'Ġelectron', 'Ġlaunching', 'Ġtrop', 'ics', 'Ġmanufacturer', 'Ġrocket', 'Ġlab', 'Ġcountry', 'Ġorigin', 'Ġnew', 'Ġzeal', 'Ġunited', 'Ġstates', 'Ġproject', 'Ġcost', 'Ġus', 'Ġmillion', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġmillion', 'Ġsize', 'Ġheight', 'Ġdiameter', 'Ġft', 'Ġmass', '000', 'Ġstages', 'âĢĵ', 'Ġcapacity', 'Ġpayload', 'Ġle', 'Ġmass', 'Ġoriginal', 'Ġupdated', 'Ġpayload', 'Ġmass', 'Ġoriginal', 'Ġupdated', 'Ġassociated', 'Ġrockets', 'Ġcomparable', 'Ġsh', 'av', 'Ġun', 'ha', 'Ġprime', 'Ġmi', 'ura', 'Ġrocket', 'Ġlab', 'Ġelectron', 'red', 'irect', 'ed', 'Ġelectron', 'rocket', '))', 'Ġelectron', 'Ġtwo', 'stage', 'Ġpartially', 'Ġrecover', 'able', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġdeveloped', 'Ġrocket', 'Ġlab', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġwholly', 'Ġowned', 'Ġnew', 'Ġzeal', 'Ġsubsidiary', 'Ġelectron', 'Ġdeveloped', 'Ġservice', 'Ġcommercial', 'Ġsmall', 'Ġsatellite', 'Ġlaunch', 'Ġmarket', 'Ġr', 'utherford', 'Ġengines', 'Ġfirst', 'Ġelectric', 'p', 'ump', 'fed', 'Ġengine', 'Ġpower', 'Ġorbital', 'class', 'Ġrocket', 'Ġelectron', 'Ġoften', 'Ġflown', 'Ġkick', 'stage', 'Ġrocket', 'Ġlab', "'s", 'Ġphoton', 'Ġspacecraft', 'Ġalthough', 'Ġrocket', 'Ġdesigned', 'Ġexpend', 'able', 'Ġrocket', 'Ġlab', 'Ġrecovered', 'Ġfirst', 'Ġstage', 'Ġtwice', 'Ġworking', 'Ġtowards', 'Ġcapability', 'using', 'Ġbooster', 'Ġflight', 'Ġbooster', 'Ġfeatured', 'Ġfirst', 'Ġhelicopter', 'Ġcatch', 'Ġrecovery', 'Ġattempt', 'Ġde', 'cember', 'Ġelectron', 'Ġcompleted', 'Ġflight', 'Ġqualification', 'Ġfirst', 'Ġrocket', 'Ġlaunched', 'Ġmay', 'Ġflight', 'Ġcalled', "'s", 'Ġtest', '",', 'Ġreaching', 'Ġspace', 'Ġachieving', 'Ġorbit', 'Ġdue', 'Ġglitch', 'Ġcommunication', 'Ġequipment', 'Ġground', 'Ġsecond', 'Ġflight', 'Ġjan', 'uary', 'Ġelectron', 'Ġreached', 'Ġorbit', 'Ġdeployed', 'Ġthree', 'Ġcubes', 'ats', 'Ġmission', 'Ġcalled', 'still', 'Ġtesting', '".[', 'Ġfirst', 'Ġcommercial', 'Ġlaunch', 'Ġelectron', 'Ġthird', 'Ġlaunch', 'Ġoverall', 'Ġoccurred', 'mber', 'Ġmission', 'Ġcalled', "'s", 'Ġbusiness', 'Ġtime', '".[', 'Ġsince', 'Ġelectron', 'Ġlaunched', 'Ġsuccessfully', 'Ġthirty', 'Ġtimes', 'Ġelectron', 'Ġuses', 'Ġtwo', 'Ġstages', 'Ġdiameter', 'Ġft', '))', 'Ġfilled', 'Ġpropell', 'ant', 'Ġmain', 'Ġbody', 'Ġrocket', 'Ġconstructed', 'Ġusing', 'Ġlightweight', 'Ġcarbon', 'Ġcomposite', 'Ġmaterial', 'Ġstages', 'Ġuse', 'Ġr', 'utherford', 'Ġrocket']</t>
+          <t>['Ġeight', 'Ġhours', 'Ġactual', 'Ġoperation', 'Ġdirect', 'Ġsuccessor', 'Ġscore', 'Ġanother', 'Ġar', 'pa', 'led', 'Ġproject', 'Ġcalled', 'Ġcourier', 'Ġcourier', 'Ġlaunched', 'Ġoct', 'ober', 'Ġexplore', 'Ġwhether', 'Ġwould', 'Ġpossible', 'Ġestablish', 'Ġglobal', 'Ġmilitary', 'Ġcommunications', 'Ġnetwork', 'Ġusing', 'del', 'ayed', 'Ġrepe', 'ater', 'Ġsatellites', 'Ġreceive', 'Ġstore', 'Ġinformation', 'Ġcommanded', 'Ġreb', 'road', 'cast', 'Ġdays', 'Ġcommand', 'Ġsystem', 'Ġfailure', 'Ġended', 'Ġcommunications', 'Ġsatellite', 'Ġn', 'asa', "'s", 'Ġsatellite', 'Ġapplications', 'Ġprogram', 'Ġlaunched', 'Ġfirst', 'Ġartificial', 'Ġsatellite', 'Ġused', 'Ġpassive', 'Ġrelay', 'Ġcommunications', 'Ġecho', 'Ġaug', 'ust', 'Ġecho', 'Ġal', 'umin', 'ized', 'Ġballoon', 'Ġsatellite', 'Ġacting', 'Ġpassive', 'Ġreflect', 'Ġmicrowave', 'Ġsignals', 'Ġcommunication', 'Ġsignals', 'Ġbounced', 'Ġsatellite', 'Ġone', 'Ġpoint', 'Ġearth', 'Ġanother', 'Ġexperiment', 'Ġsought', 'Ġestablish', 'Ġfeasibility', 'Ġworldwide', 'Ġbroadcasts', 'Ġtelephone', 'Ġradio', 'Ġtelevision', 'Ġsignals', 'Ġearly', 'Ġactive', 'Ġpassive', 'Ġsatellite', 'Ġexperiments', 'Ġï', '¬', 'ģ', 'r', 'sts', 'Ġexperiments', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġtel', 'star', 'Ġfirst', 'Ġactive', 'Ġdirect', 'Ġrelay', 'Ġcommunications', 'Ġcommercial', 'Ġsatellite', 'Ġmarked', 'Ġfirst', 'Ġtrans', 'atlantic', 'Ġtransmission', 'Ġtelevision', 'Ġsignals', 'Ġbelonging', 'Ġpart', 'Ġmulti', 'national', 'Ġagreement', 'Ġbell', 'Ġtelephone', 'Ġlaboratories', 'Ġn', 'asa', 'Ġb', 'rit', 'ish', 'Ġgeneral', 'Ġpost', 'Ġoffice', 'Ġfrench', 'Ġnational', 'Ġp', 'tt', 'post', 'Ġoffice', 'Ġdevelop', 'Ġsatellite', 'Ġcommunications', 'Ġlaunched', 'Ġn', 'asa', 'Ġcape', 'aver', 'al', 'Ġj', 'uly', 'Ġfirst', 'Ġprivately', 'Ġsponsored', 'Ġspace', 'Ġlaunch', 'Ġanother', 'Ġpassive', 'Ġrelay', 'Ġexperiment', 'Ġprimarily', 'Ġintended', 'Ġmilitary', 'Ġcommunications', 'Ġpurposes', 'Ġproject', 'Ġwest', 'Ġled', 'Ġmass', 'achusetts', 'Ġinstitute', 'Ġtechnology', "'s", 'Ġl', 'incoln', 'Ġlaboratory', 'Ġinitial', 'Ġfailure', 'Ġlaunch', 'Ġmay', 'Ġdispersed', 'Ġmillion', 'Ġcopper', 'Ġneedle', 'Ġdip', 'oles', 'Ġcreate', 'Ġpassive', 'Ġreflecting', 'Ġbelt', 'Ġeven', 'Ġthough', 'Ġhalf', 'Ġdip', 'oles', 'Ġproperly', 'Ġseparated', 'Ġproject', 'Ġable', 'Ġsuccessfully', 'Ġexperiment', 'Ġcommunicate', 'Ġusing', 'Ġfrequencies', 'Ġband', 'Ġspectrum', 'Ġimmediate', 'Ġante', 'ced', 'ent', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġhug', 'hes', 'Ġaircraft', 'Ġcompany', "'s", 'Ġsyn', 'Ġlaunched', 'Ġj', 'uly', 'Ġsyn', 'Ġfirst', 'Ġcommunications', 'Ġsatellite', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġrev', 'olved', 'Ġaround', 'Ġearth', 'Ġper', 'Ġday', 'Ġconstant', 'Ġspeed', 'Ġstill', 'Ġnorth', 'âĢĵ', 'Ġsouth']</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>['Ġengine', 'Ġfirst', 'Ġelectric', 'p', 'ump', 'fed', 'Ġengine', 'Ġpower', 'Ġorbital', 'Ġrocket', 'Ġelectric', 'Ġpumps', 'Ġpowered', 'Ġlithium', 'poly', 'mer', 'Ġbatteries', 'Ġsecond', 'Ġstage', 'Ġuses', 'Ġthree', 'Ġbatteries', 'hot', 'Ġswapped', '",', 'Ġtwo', 'Ġbatteries', 'Ġj', 'ett', 'ison', 'ed', 'Ġdepleted', 'Ġshed', 'Ġmass', 'Ġnine', 'Ġr', 'utherford', 'Ġengines', 'Ġfirst', 'Ġstage', 'Ġone', 'Ġvacuum', 'optim', 'ized', 'Ġversion', 'Ġsecond', 'Ġstage', 'Ġfirst', 'Ġstage', 'Ġengines', 'Ġdeliver', 'Ġkn', '000', 'Ġthrust', 'Ġsecond', 'Ġstage', 'Ġdelivers', 'Ġkn', 'Ġthrust', 'Ġalmost', 'Ġengines', 'Ġparts', 'Ġprinted', 'Ġsave', 'Ġtime', 'Ġmoney', 'Ġmanufacturing', 'Ġprocess', 'Ġrocket', 'Ġlab', 'Ġalso', 'Ġdeveloped', 'Ġoptional', 'Ġthird', 'Ġstage', 'Ġknown', 'kick', 'Ġstage', '",', 'Ġdesigned', 'Ġcircular', 'ize', 'Ġorbits', 'Ġsatellite', 'Ġpayload', 'Ġstage', 'Ġalso', 'Ġputs', 'Ġsatellites', 'Ġaccurate', 'Ġorbit', 'Ġless', 'Ġtime', 'Ġelectron', 'Ġkick', 'Ġstage', 'Ġequipped', 'Ġsingle', 'Ġcur', 'ie', 'Ġengine', 'Ġcapable', 'Ġperforming', 'Ġmultiple', 'Ġburns', 'Ġuses', 'Ġunspecified', 'green', 'Ġbip', 'ro', 'pell', 'ant', 'Ġprinted', 'Ġfirst', 'Ġused', 'Ġelectron', "'s", 'Ġsecond', 'Ġflight', 'Ġkick', 'Ġstage', 'Ġtransport', 'Ġpayload', 'Ġrocket', 'Ġlab', 'Ġalso', 'Ġdeveloped', 'Ġderivative', 'Ġspacecraft', 'Ġkick', 'Ġstage', 'Ġphoton', 'Ġintended', 'Ġuse', 'Ġlunar', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'Ġphoton', 'Ġcapable', 'Ġdelivering', 'Ġsmall', 'Ġpayload', 'Ġlunar', 'Ġorbit', 'Ġdesign', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Äģ', 'h', 'ia', 'active', 'Ġmars', 'active', 'Ġsax', 'av', 'ord', 'prop', 'osed', 'utherland', 'prop', 'osed', ')[', 'Ġtotal', 'Ġlaunches', 'Ġsuccess', 'es', 'Ġfailure', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġmay', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġse', 'pt', 'ember', 'active', 'Ġfirst', 'Ġstage', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġpowered', 'Ġr', 'utherford', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', 'Ġkn', 'Ġvacuum', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', '05', 'Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'Ġheight', 'Ġft', 'Ġdiameter']</t>
+          <t>['Ġmotion', 'Ġspecial', 'Ġequipment', 'Ġneeded', 'Ġtrack', 'Ġsuccessor', 'Ġsyn', 'Ġlaunched', 'Ġj', 'uly', 'Ġfirst', 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġsatellite', 'Ġsyn', 'Ġobtained', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġwithout', 'Ġnorth', 'âĢĵ', 'south', 'Ġmotion', 'Ġmaking', 'Ġappear', 'Ġground', 'Ġstationary', 'Ġobject', 'Ġdirect', 'Ġextension', 'Ġpassive', 'Ġexperiments', 'Ġproject', 'Ġwest', 'Ġl', 'incoln', 'Ġexperimental', 'Ġsatellite', 'Ġprogram', 'Ġalso', 'Ġconducted', 'Ġl', 'incoln', 'Ġlaboratory', 'Ġbehalf', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġles', 'Ġactive', 'Ġcommunications', 'Ġsatellite', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġexplore', 'Ġfeasibility', 'Ġactive', 'Ġsolid', 'state', 'Ġband', 'Ġlong', 'range', 'Ġmilitary', 'Ġcommunications', 'Ġtotal', 'Ġnine', 'Ġsatellites', 'Ġlaunched', 'Ġpart', 'Ġseries', 'Ġunited', 'Ġstates', 'Ġsaw', 'Ġcreation', 'Ġcommunications', 'Ġsatellite', 'Ġcorporation', 'sat', 'Ġprivate', 'Ġcorporation', 'Ġsubject', 'Ġinstruction', 'Ġus', 'Ġgovernment', 'Ġmatters', 'Ġnational', 'Ġpolicy', 'Ġnext', 'Ġtwo', 'Ġyears', 'Ġinternational', 'Ġnegotiations', 'Ġled', 'Ġint', 'els', 'Ġagreements', 'Ġturn', 'Ġled', 'Ġlaunch', 'Ġint', 'els', 'Ġalso', 'Ġknown', 'Ġearly', 'Ġbird', 'Ġapr', 'il', 'Ġfirst', 'Ġcommercial', 'Ġcommunications', 'Ġsatellite', 'Ġplaced', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġsubsequent', 'Ġint', 'els', 'Ġlaunches', 'Ġprovided', 'Ġmulti', 'dest', 'ination', 'Ġservice', 'Ġvideo', 'Ġaudio', 'Ġdata', 'Ġservice', 'Ġships', 'Ġsea', 'int', 'els', 'âĢĵ', 'Ġcompletion', 'Ġfully', 'Ġglobal', 'Ġnetwork', 'Ġint', 'els', 'âĢĵ', 'Ġsignificant', 'Ġexpansions', 'Ġcommercial', 'Ġsatellite', 'Ġcapacity', 'Ġint', 'els', 'Ġway', 'Ġbecome', 'Ġpart', 'Ġcompetitive', 'Ġprivate', 'Ġtelecommunications', 'Ġindustry', 'Ġstarted', 'Ġget', 'Ġcompetition', 'Ġlikes', 'Ġpan', 'ams', 'Ġunited', 'Ġstates', 'Ġironically', 'Ġbought', 'Ġarch', 'rival', 'Ġint', 'els', 'Ġlaunched', 'Ġunited', 'Ġstates', 'Ġlaunch', 'Ġsource', 'Ġoutside', 'v', 'iet', 'Ġunion', 'Ġparticipate', 'Ġint', 'els', 'Ġagreements', 'v', 'iet', 'Ġunion', 'Ġlaunched', 'Ġfirst', 'Ġcommunications', 'Ġsatellite', 'Ġapr', 'il', 'Ġpart', 'Ġprogram', 'Ġprogram', 'Ġalso', 'Ġunique', 'Ġtime', 'Ġuse', 'Ġbecame', 'Ġknown', 'Ġorbit', 'Ġdescribes', 'Ġinternational', 'Ġcommercial', 'Ġsatellite', 'Ġprojects']</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>['Ġft', 'Ġpowered', 'Ġr', 'utherford', 'Ġmaximum', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġpropell', 'ant', 'Ġkick', 'Ġstage', 'optional', 'Ġphoton', 'Ġpowered', 'Ġcur', 'ie', 'Ġmaximum', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġpropell', 'ant', 'Ġvisc', 'ous', 'Ġliquid', 'Ġmonop', 'ro', 'pell', 'ant', 'ap', 'Ġal', 'Ġkick', 'Ġstage', 'optional', 'Ġphoton', 'mod', 'ï', '¬', 'ģ', 'ed', 'Ġpowered', 'Ġhyper', 'cur', 'ie', 'Ġrocket', 'Ġlab', "'s", 'Ġelectron', 'Ġreturn', 'Ġphases', 'Ġelectron', 'Ġpayload', 'Ġfair', 'ing', 'Ġfeet', 'Ġinches', 'Ġlength', 'Ġfeet', 'Ġinches', 'Ġdiameter', 'Ġtotal', 'Ġmass', 'Ġmanufacturing', 'Ġcarbon', 'Ġcomposite', 'Ġcomponents', 'Ġmain', 'Ġflight', 'Ġstructure', 'Ġtraditionally', 'Ġrequired', 'Ġhours', 'Ġextensive', 'Ġhand', 'Ġlabor', 'Ġprocess', 'Ġlate', 'Ġrocket', 'Ġlab', 'Ġbrought', 'Ġnew', 'Ġrobotic', 'Ġmanufacturing', 'Ġcapability', 'Ġonline', 'Ġproduce', 'Ġcomposite', 'Ġparts', 'Ġelectron', 'Ġhours', 'Ġrobot', 'Ġnicknamed', 'ros', 'ie', 'Ġrobot', '",', 'Ġjets', 'ons', 'Ġcharacter', 'Ġprocess', 'Ġmake', 'Ġcarbon', 'Ġfiber', 'Ġstructures', 'Ġwell', 'Ġhandle', 'Ġcutting', 'Ġdrilling', 'Ġsand', 'ing', 'Ġparts', 'Ġready', 'Ġfinal', 'Ġassembly', 'Ġcompany', 'Ġobjective', 'mber', 'Ġreduce', 'Ġoverall', 'Ġelectron', 'Ġmanufacturing', 'Ġcycle', 'Ġseven', 'Ġdays', 'Ġr', 'utherford', 'Ġengine', 'Ġproduction', 'Ġmakes', 'Ġextensive', 'Ġuse', 'Ġadditive', 'Ġmanufacturing', 'Ġsince', 'Ġearliest', 'Ġflights', 'Ġelectron', 'Ġallows', 'Ġcapability', 'Ġscale', 'Ġproduction', 'Ġrelatively', 'Ġstraightforward', 'Ġmanner', 'Ġincreasing', 'Ġnumber', 'Ġcapability', 'Ġprinters', 'Ġaug', 'ust', 'Ġrocket', 'Ġlab', 'Ġannounced', 'Ġrecovery', 'Ġref', 'light', 'Ġplans', 'Ġfirst', 'Ġstage', 'Ġelectron', 'Ġalthough', 'Ġplans', 'Ġstarted', 'Ġinternally', 'Ġlate', 'Ġelectron', 'Ġoriginally', 'Ġdesigned', 'Ġreusable', 'Ġlaunch', 'Ġvehicle', 'Ġsmall', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġpursued', 'Ġdue', 'Ġincreased', 'Ġunderstanding', 'Ġelectron', "'s", 'Ġperformance', 'Ġbased', 'Ġanalysis', 'Ġprevious', 'Ġflights', 'Ġthough', 'Ġsensors', 'Ġvehicle', 'Ġaddition', 'us', 'ability', 'Ġpursued', 'Ġmeet', 'Ġlaunch', 'Ġdemands', 'Ġcounteract', 'Ġdecreased', 'Ġpayload', 'Ġcapacity', 'Ġcaused', 'Ġadded', 'Ġmass', 'Ġrecovery', 'Ġhardware', 'Ġperformance', 'Ġimprovements', 'Ġelectrons', 'Ġexpected', 'Ġearly', 'Ġphases', 'Ġrecovery', 'Ġincluded', 'Ġdata', 'Ġgathering', 'Ġsurviving', 'Ġatmospheric', 'entry', 'Ġalso', 'Ġknown', 'Ġwall', '".[', 'Ġnext', 'Ġphase', 'Ġrequire', 'Ġsuccessful', 'Ġdeployment']</t>
+          <t>['Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġorbit', 'Ġsize', 'Ġcomparison', 'Ġgl', 'ass', 'Ġgal', 'ile', 'id', 'ou', 'Ġir', 'idium', 'Ġconst', 'ell', 'ations', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġgraveyard', 'Ġorbit', 'Ġvan', 'en', 'Ġradiation', 'Ġbelts', 'Ġearth', 'Ġscale', 'Ġmoon', "'s", 'Ġorbit', 'Ġaround', 'Ġtimes', 'Ġlarge', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'b', 'Ġï', '¬', 'ģ', 'le', 'Ġhover', 'Ġorbit', 'Ġlabel', 'Ġhighlight', 'Ġclick', 'Ġload', 'Ġarticle', '.)', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'Ġtwo', 'Ġhigh', 'Ġap', 'ge', 'es', 'Ġdaily', 'Ġnorthern', 'Ġhemisphere', 'Ġorbit', 'Ġprovides', 'Ġlong', 'Ġdwell', 'Ġtime', 'Ġr', 'ussian', 'Ġterritory', 'Ġwell', 'ada', 'Ġhigher', 'Ġlat', 'itudes', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġequ', 'ator', 'Ġcommunications', 'Ġsatellites', 'Ġusually', 'Ġone', 'Ġthree', 'Ġprimary', 'Ġtypes', 'Ġorbit', 'Ġorbital', 'Ġclass', 'ifications', 'Ġused', 'Ġspecify', 'Ġorbital', 'Ġdetails', 'Ġle', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'ng', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'ge', 'Ġmiles', 'Ġearth', "'s", 'Ġsurface', 'Ġorbit', 'Ġspecial', 'Ġcharacteristic', 'Ġapparent', 'Ġposition', 'Ġsatellite', 'Ġviewed', 'Ġground', 'Ġobserver', 'Ġchange', 'Ġsatellite', 'Ġappears', 'stand', 'Ġstill', 'Ġsatellite', "'s", 'Ġorbital', 'Ġperiod', 'Ġrotation', 'Ġrate', 'Ġearth', 'Ġadvantage', 'Ġorbit', 'Ġground', 'Ġantennas', 'Ġtrack', 'Ġsatellite', 'Ġacross', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġpoint', 'Ġlocation', 'Ġsatellite', 'Ġappears', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellites', 'Ġcloser', 'Ġearth', 'Ġorbital', 'Ġalt', 'itudes', 'Ġrange', '000', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', 'Ġregion', 'Ġmedium', 'Ġorbits', 'Ġreferred', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', 'Ġsatellites', 'Ġle', 'Ġorbit', 'Ġearth', 'Ġfaster', 'Ġremain', 'Ġvisible', 'Ġfixed', 'Ġpoint', 'Ġearth', 'Ġcontinually', 'Ġlike', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġappear', 'Ġground', 'Ġobserver', 'Ġcross', 'set']</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>['Ġaer', 'odynamic', 'Ġde', 'celer', 'ator', 'Ġball', 'ute', 'Ġslow', 'Ġbooster', 'Ġfollowed', 'Ġdeployment', 'Ġpar', 'af', 'oil', 'Ġconcluded', 'Ġtouchdown', 'Ġocean', 'Ġsuccessful', 'Ġtouchdown', 'Ġocean', 'Ġstage', 'Ġwould', 'Ġmoved', 'Ġonto', 'Ġship', 'Ġrefurb', 'ishment', 'Ġref', 'light', 'Ġrocket', 'Ġlab', 'Ġreleased', 'Ġinformation', 'Ġaer', 'odynamic', 'Ġde', 'celer', 'ator', 'Ġwould', 'Ġrequired', 'Ġslow', 'Ġbooster', 'Ġatmospheric', 'entry', 'Ġlate', 'Ġphases', 'Ġelectron', 'Ġreuse', 'Ġinvolve', 'Ġusing', 'Ġpar', 'af', 'oil', 'Ġmid', 'air', 'Ġretrieval', 'Ġhelicopter', 'Ġsuccessful', 'Ġmid', 'air', 'Ġretrieval', 'Ġhelicopter', 'Ġwould', 'Ġbring', 'Ġelectron', 'Ġship', 'Ġwould', 'Ġbring', 'Ġstage', 'Ġlaunch', 'Ġsite', 'Ġrefurb', 'ishment', 'Ġlaunch', 'Ġlater', 'Ġrocket', 'Ġlab', 'Ġabandoned', 'Ġplan', 'Ġcatch', 'Ġstage', 'Ġhelicopter', 'Ġuse', 'Ġocean', 'Ġlanding', 'Ġinstead', 'Ġone', 'Ġrecovered', 'Ġr', 'utherford', 'Ġengine', 'Ġpassed', 'Ġfive', 'Ġfull', 'duration', 'Ġhot', 'Ġfire', 'Ġtests', 'Ġdeclared', 'Ġready', 'Ġfly', 'Ġrocket', 'Ġlab', "'s", 'th', 'Ġelectron', 'Ġmission', 'Ġreused', 'Ġrefurb', 'ished', 'Ġr', 'utherford', 'Ġengine', 'Ġprevious', 'Ġflight', 'Ġproduction', 'us', 'ability', 'Ġaer', 'othermal', 'Ġde', 'celer', 'ator', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġmaximum', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġpropell', 'ant', 'Ġun', 'spe', 'ci', 'ï', '¬', 'ģ', 'ed', 'Ġhyper', 'g', 'olic', 'Ġbip', 'ro', 'pell', 'ant', 'Ġrocket', 'Ġlab', 'Ġinvestigating', 'us', 'ability', 'Ġdecided', 'Ġpursue', 'Ġprop', 'ulsive', 'Ġrecovery', 'Ġlike', 'Ġspace', 'x', 'Ġinstead', 'Ġuse', 'Ġatmosphere', 'Ġslow', 'Ġbooster', 'Ġknown', 'aer', 'othermal', 'Ġde', 'celer', 'ator', 'Ġtechnology', 'Ġexact', 'Ġmethods', 'Ġused', 'Ġproprietary', 'Ġmay', 'Ġinclude', 'Ġkeeping', 'Ġproper', 'Ġorientation', 'ent', 'ering', 'Ġatmosphere', 'Ġelectron', 'Ġinitially', 'Ġpayload', 'Ġcapacity', 'âĢĵ', 'âĢĵ', 'Ġmi', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġpursuit', 'us', 'ability', 'Ġrocket', 'Ġlab', 'Ġmade', 'Ġchanges', 'Ġelectron', 'Ġflight', 'Ġ("', "'s", 'Ġfunny', 'Ġlooking', 'Ġc', 'actus', 'make', 'Ġrain', '")', 'Ġinstruments', 'Ġfirst', 'Ġstage', 'Ġneeded', 'Ġgather', 'Ġdata', 'Ġhelp', 'Ġref', 'light', 'Ġprogram', 'Ġflight', 'Ġ("', 'look', 'Ġhands', '")', 'Ġbrut', 'us', 'Ġinstrument', 'Ġcollected', 'Ġdata', 'Ġfirst', 'Ġstage', 'Ġstudy', 'entry', 'Ġdesigned', 'Ġable', 'Ġsurvive', 'Ġsplash', 'Ġocean', 'Ġflight', 'Ġ("']</t>
+          <t>['Ġgo', 'Ġbehind', 'Ġearth', 'Ġbeyond', 'Ġvisible', 'Ġhorizon', 'Ġtherefore', 'Ġprovide', 'Ġcontinuous', 'Ġcommunications', 'Ġcapability', 'Ġlower', 'Ġorbits', 'Ġrequires', 'Ġlarger', 'Ġnumber', 'Ġsatellites', 'Ġone', 'Ġsatellites', 'Ġalways', 'Ġvisible', 'Ġtransmission', 'Ġcommunication', 'Ġsignals', 'Ġhowever', 'Ġdue', 'Ġcloser', 'Ġdistance', 'Ġearth', 'Ġle', 'Ġsatellites', 'Ġcommunicate', 'Ġground', 'Ġreduced', 'Ġlatency', 'Ġlower', 'Ġpower', 'Ġwould', 'Ġrequired', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġtypically', 'Ġcircular', 'Ġorbit', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', "'s", 'Ġsurface', 'Ġcorrespond', 'ingly', 'Ġperiod', 'time', 'Ġrev', 'olve', 'Ġaround', 'Ġearth', 'Ġminutes', 'Ġlow', 'Ġaltitude', 'Ġsatellites', 'Ġvisible', 'Ġwithin', 'Ġradius', 'Ġroughly', '000', 'Ġkilometres', 'Ġmi', 'Ġsub', 'atellite', 'Ġpoint', 'Ġaddition', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġchange', 'Ġposition', 'Ġrelative', 'Ġground', 'Ġposition', 'Ġquickly', 'Ġeven', 'Ġlocal', 'Ġapplications', 'Ġmany', 'Ġsatellites', 'Ġneeded', 'Ġmission', 'Ġrequires', 'Ġuninterrupted', 'Ġconnectivity', 'Ġsatellite', 'Ġorbits', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġlow', 'earth', 'orb', 'iting', 'Ġsatellites', 'Ġless', 'Ġexpensive', 'Ġlaunch', 'Ġorbit', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġdue', 'Ġproximity', 'Ġground', 'Ġrequire', 'Ġhigh', 'Ġsignal', 'Ġstrength', 'sign', 'al', 'Ġstrength', 'Ġfalls', 'Ġsquare', 'Ġdistance', 'Ġsource', 'Ġeffect', 'Ġconsiderable', 'Ġthus', 'Ġtrade', 'Ġnumber', 'Ġsatellites', 'Ġcost', 'Ġaddition', 'Ġimportant', 'Ġdifferences', 'Ġonboard', 'Ġground', 'Ġequipment', 'Ġneeded', 'Ġsupport', 'Ġtwo', 'Ġtypes', 'Ġmissions', 'Ġgroup', 'Ġsatellites', 'Ġworking', 'Ġconcert', 'Ġknown', 'Ġsatellite', 'Ġconstellation', 'Ġtwo', 'Ġconst', 'ell', 'ations', 'Ġintended', 'Ġprovide', 'Ġsatellite', 'Ġphone', 'Ġlow', 'speed', 'Ġdata', 'Ġservices', 'Ġprimarily', 'Ġremote', 'Ġareas', 'Ġir', 'idium', 'Ġglobal', 'star', 'Ġsystems', 'Ġir', 'idium', 'Ġsystem', 'Ġsatellites', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġinter', 'atellite', 'Ġlinks', 'Ġprovide', 'Ġservice', 'Ġavailability', 'Ġentire', 'Ġsurface', 'Ġearth', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'Ġoperated', 'Ġspace', 'x', 'Ġaims', 'Ġglobal', 'Ġsatellite', 'Ġinternet', 'Ġaccess', 'Ġcoverage', 'Ġalso', 'Ġpossible', 'Ġoffer', 'Ġdiscontin', 'uous', 'Ġcoverage', 'Ġusing', 'Ġlow', 'earth', 'orbit', 'Ġsatellite', 'Ġcapable', 'Ġstoring', 'Ġdata', 'Ġreceived', 'Ġpassing', 'Ġone', 'Ġpart']</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1634,7 +1634,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>['running', 'Ġfingers', '")', 'Ġblock', 'Ġupdate', 'Ġfirst', 'Ġstage', 'Ġelectron', 'Ġallow', 'Ġfirst', 'Ġguided', 'entry', 'Ġfirst', 'Ġstage', 'Ġbooster', 'Ġupdates', 'Ġincluded', 'Ġadditional', 'Ġhardware', 'Ġguidance', 'Ġnavigation', 'Ġonboard', 'Ġflight', 'Ġcomputers', 'band', 'Ġtele', 'metry', 'Ġgather', 'Ġlivestream', 'Ġdata', 'Ġgathered', 'entry', 'Ġfirst', 'Ġstage', 'Ġalso', 'Ġreaction', 'Ġcontrol', 'Ġsystem', 'Ġorient', 'Ġbooster', 'Ġstage', 'Ġseparation', 'Ġfirst', 'Ġstage', 'Ġusing', 'Ġnew', 'Ġhardware', 'Ġinstalled', 'Ġflipped', 'Â°', 'Ġprepare', 'entry', 'Ġthroughout', 'entry', 'Ġstage', 'Ġguided', 'Ġthough', 'Ġatmosphere', 'Ġright', 'Ġorientation', 'Ġangle', 'Ġattack', 'Ġbase', 'Ġheat', 'Ġshield', 'Ġprotect', 'Ġbooster', 'Ġdestruction', 'Ġusing', 'Ġonboard', 'Ġcomputers', 'Ġbooster', 'Ġsuccessfully', 'Ġsurvived', 'Ġguided', 'entry', 'Ġdespite', 'Ġde', 'celer', 'ation', 'Ġhardware', 'Ġonboard', 'Ġdestruct', 'ively', 'Ġspl', 'ashed', 'Ġocean', 'Ġmph', 'Ġplanned', 'entry', 'Ġsuccessful', 'Ġrocket', 'Ġlab', 'Ġplans', 'Ġrecover', 'Ġstage', 'Ġinstead', 'Ġwanted', 'Ġdemonstrate', 'Ġability', 'Ġsuccessfully', 'enter', 'Ġflight', 'Ġ("', 'birds', 'Ġfeather', '")', 'Ġdemonstrated', 'Ġsimilar', 'Ġsuccess', 'Ġatmospheric', 'entry', 'Ġtests', 'Ġsimilar', 'Ġflight', 'Ġexpected', 'Ġfollowing', 'Ġflight', 'Ġ("', 'birds', 'Ġfeather', '"),', 'Ġmid', 'f', 'eb', 'ruary', 'Ġlow', 'Ġaltitude', 'Ġtests', 'Ġdone', 'Ġtest', 'Ġparach', 'utes', 'Ġapr', 'il', 'Ġrocket', 'Ġlab', 'Ġshared', 'Ġsuccessful', 'Ġdemonstration', 'Ġmid', 'air', 'Ġretrieval', 'Ġdone', 'Ġmarch', 'Ġelectron', 'Ġtest', 'Ġarticle', 'Ġdropped', 'Ġhelicopter', 'Ġdeployed', 'Ġparach', 'utes', 'Ġhelicopter', 'Ġcarrying', 'Ġlong', 'bo', 'om', 'Ġsn', 'agged', 'Ġdro', 'gue', 'Ġline', 'Ġparachute', 'Ġft', 'Ġdemonstrating', 'Ġsuccessful', 'Ġretrieval', 'Ġfollowing', 'Ġcatch', 'Ġtest', 'Ġarticle', 'Ġbrought', 'Ġback', 'Ġland', 'Ġflight', 'Ġ("', 'return', 'Ġsender', '"),', 'Ġfirst', 'Ġrecover', 'Ġfirst', 'Ġstage', 'Ġbooster', 'Ġsplash', 'Ġpac', 'ific', 'Ġocean', 'Ġrocket', 'Ġalso', 'Ġloft', 'ed', 'Ġthirty', 'Ġpayload', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġincluding', 'Ġtitanium', 'Ġmass', 'Ġsimulator', 'Ġshape', 'Ġgarden', 'Ġgn', 'ome', 'gn', 'ome', 'Ġch', 'om', 'ps', 'ki', 'Ġvideo', 'Ġgame', 'Ġhalf', 'life', 'Ġaug', 'ust', 'Ġrocket', 'Ġlab', 'Ġannounced', 'Ġincreased', 'Ġpayload', 'Ġelectron', 'âĢĵ', 'âĢĵ', 'Ġpayload', 'Ġcapacity', 'Ġincrease']</t>
+          <t>['Ġearth', 'Ġtransmitting', 'Ġlater', 'Ġpassing', 'Ġanother', 'Ġpart', 'Ġcase', 'Ġcascade', 'Ġsystem', 'ada', "'s", 'Ġcass', 'ope', 'Ġcommunications', 'Ġsatellite', 'Ġanother', 'Ġsystem', 'Ġusing', 'Ġstore', 'Ġforward', 'Ġmethod', 'Ġorb', 'comm', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġorbit', 'Ġsomewhere', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', "'s", 'Ġsurface', 'Ġsatellites', 'Ġsimilar', 'Ġle', 'Ġsatellites', 'Ġfunctionality', 'Ġsatellites', 'Ġvisible', 'Ġmuch', 'Ġlonger', 'Ġperiods', 'Ġtime', 'Ġle', 'Ġsatellites', 'Ġusually', 'Ġhours', 'Ġsatellites', 'Ġlarger', 'Ġcoverage', 'Ġarea', 'Ġle', 'Ġsatellites', 'Ġsatellite', "'s", 'Ġlonger', 'Ġduration', 'Ġvisibility', 'Ġwider', 'Ġfootprint', 'Ġmeans', 'Ġfewer', 'Ġsatellites', 'Ġneeded', 'Ġnetwork', 'Ġle', 'Ġnetwork', 'Ġone', 'Ġdisadvantage', 'Ġsatellite', "'s", 'Ġdistance', 'Ġgives', 'Ġlonger', 'Ġtime', 'Ġdelay', 'Ġweaker', 'Ġsignal', 'Ġle', 'Ġsatellite', 'Ġalthough', 'Ġlimitations', 'Ġsevere', 'Ġgeo', 'Ġsatellite', 'Ġlike', 'Ġle', 'os', 'Ġsatellites', 'Ġmaintain', 'Ġstationary', 'Ġdistance', 'Ġearth', 'Ġcontrast', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġsatellites', 'Ġalways', 'Ġkilometres', 'Ġmi', 'Ġearth', 'Ġtypically', 'Ġorbit', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellite', '000', 'Ġkilometres', '000', 'Ġmi', 'Ġearth', 'Ġvarious', 'Ġpatterns', 'Ġsatellites', 'Ġmake', 'Ġtrip', 'Ġaround', 'Ġearth', 'Ġanywhere', 'Ġhours', 'Ġcommunications', 'Ġsatellite', 'Ġtel', 'star', 'Ġlaunched', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġdesigned', 'Ġhelp', 'Ġfacilitate', 'Ġhigh', 'speed', 'Ġtelephone', 'Ġsignals', 'Ġalthough', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġpractical', 'Ġway', 'Ġtransmit', 'Ġsignals', 'Ġhorizon', 'Ġmajor', 'Ġdrawback', 'Ġsoon', 'Ġrealised', 'Ġorbital', 'Ġperiod', 'Ġhours', 'Ġmatch', 'Ġearth', "'s", 'Ġrot', 'ational', 'Ġperiod', 'Ġhours', 'Ġcontinuous', 'Ġcoverage', 'Ġimpossible', 'Ġapparent', 'Ġmultiple', 'os', 'Ġneeded', 'Ġused', 'Ġorder', 'Ġprovide', 'Ġcontinuous', 'Ġcoverage', 'Ġsatellite', 'Ġconstellation', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġexamples', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfour', 'Ġconstellation', 'Ġsatellites', 'Ġlaunched', 'Ġsatellites', 'Ġprovide', 'Ġbroadband', 'Ġinternet', 'Ġservices', 'Ġparticular', 'Ġremote', 'Ġlocations', 'Ġmaritime', 'ï', '¬', 'Ĥ', 'ight', 'Ġuse', 'Ġorbit', 'Ġaltitude']</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1647,7 +1647,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>['Ġmainly', 'Ġdue', 'Ġbattery', 'Ġadvancements', 'Ġincreased', 'Ġpayload', 'Ġcapacity', 'Ġallows', 'Ġoffset', 'Ġmass', 'Ġadded', 'Ġrecovery', 'Ġtechnology', 'Ġaddition', 'Ġpayload', 'Ġmass', 'Ġcould', 'Ġflown', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'Ġothers', 'Ġelectron', 'Ġexpended', 'Ġrocket', 'Ġlab', 'Ġalso', 'Ġannounced', 'Ġexpanded', 'Ġfair', 'ings', 'Ġft', 'Ġdiameter', 'Ġlarger', 'Ġstandard', 'Ġft', 'Ġlong', 'Ġft', 'Ġdiameter', 'Ġfair', 'ings', 'Ġstri', 'x', 'Î±', 'Ġmission', 'Ġsyn', 'spective', 'Ġde', 'cember', 'Ġused', 'Ġextended', 'Ġfair', 'ing', 'Ġrocket', 'Ġlab', 'Ġdeveloped', 'fts', 'Ġlaunches', 'Ġnew', 'Ġzeal', 'Ġdec', 'Ġfirst', 'Ġlaunch', 'Ġus', 'Ġused', 'Ġn', 'asa', 'Ġautonomous', 'Ġflight', 'Ġtermination', 'Ġunit', 'Ġvehicle', 'Ġmod', 'ï', '¬', 'ģ', 'cation', 'Ġhistory', 'Ġfair', 'ings', 'Ġautonomous', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtermination', 'Ġsystems', 'Ġapplications', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Äģ', 'h', 'ia', 'Ġlaunch', 'Ġsite', 'Ġconstruction', 'Ġelectron', 'Ġdesigned', 'Ġlaunch', 'âĢĵ', 'âĢĵ', 'Ġpayload', 'Ġmi', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġsuitable', 'Ġcubes', 'ats', 'Ġsmall', 'Ġpayload', 'Ġoct', 'ober', 'Ġrocket', 'Ġlab', 'Ġopened', 'Ġfactory', 'Ġlarge', 'Ġenough', 'Ġproduce', 'Ġrockets', 'Ġper', 'Ġyear', 'Ġaccording', 'Ġcompany', 'Ġcustomers', 'Ġmay', 'Ġchoose', 'Ġencaps', 'ulate', 'Ġspacecraft', 'Ġpayload', 'Ġfair', 'ings', 'Ġprovided', 'Ġcompany', 'Ġeasily', 'Ġattached', 'Ġrocket', 'Ġshortly', 'Ġlaunch', 'Ġstarting', 'Ġprice', 'Ġdelivering', 'Ġpayload', 'Ġorbit', 'Ġmillion', 'Ġper', 'Ġlaunch', 'Ġoffers', 'Ġdedicated', 'Ġservice', 'Ġprice', 'Ġpoint', 'Ġmoon', 'Ġexpress', 'Ġcontracted', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġlunar', 'Ġland', 'ers', 'multiple', 'Ġlaunches', 'Ġcontracted', 'Ġplanned', 'Ġmoon', 'Ġexpress', 'Ġoperations', 'Ġelectron', 'Ġcompete', 'Ġgoogle', 'Ġlunar', 'Ġprize', 'Ġnone', 'Ġcontenders', 'Ġmet', 'Ġprize', 'Ġdeadline', 'Ġcompetition', 'Ġclosed', 'Ġwithout', 'Ġwinner', 'Ġsometime', 'Ġclosure', 'Ġmoon', 'Ġexpress', 'Ġelectron', 'Ġlaunches', 'Ġremained', 'Ġscheduled', 'Ġfe', 'b', 'ruary', 'Ġlaunches', 'Ġmoon', 'Ġexpress', 'Ġusing', 'Ġelectron', 'Ġcanceled', 'Ġapr', 'il', 'Ġrocket', 'Ġlab', 'Ġannounced', 'Ġelectron', 'Ġderivative', 'Ġvehicle', 'Ġnamed', 'Ġhaste', 'hyp', 'erson', 'ic', 'Ġaccelerator', 'Ġsub', 'orb', 'ital', 'Ġtest', 'Ġelectron', 'Ġcapable', 'Ġdelivering', 'Ġsub', 'orb', 'ital', 'Ġtrajectory', 'Ġcustomers', 'Ġinclude', 'Ġdyn', 'etics']</t>
+          <t>['06', 'Ġkilometres', '010', 'Ġobserver', 'Ġearth', 'Ġsatellite', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġappears', 'Ġmotion', 'less', 'Ġfixed', 'Ġposition', 'Ġrevolves', 'Ġaround', 'Ġearth', 'Ġearth', "'s", 'Ġangular', 'Ġvelocity', 'one', 'Ġrevolution', 'Ġper', 'Ġside', 'real', 'Ġday', 'Ġequ', 'atorial', 'Ġorbit', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġuseful', 'Ġcommunications', 'Ġground', 'Ġantennas', 'Ġaimed', 'Ġsatellite', 'Ġwithout', 'Ġtrack', 'Ġsatellite', "'s", 'Ġmotion', 'Ġrelatively', 'Ġinexpensive', 'Ġapplications', 'Ġrequire', 'Ġmany', 'Ġground', 'Ġantennas', 'Ġdirect', 'v', 'Ġdistribution', 'Ġsavings', 'Ġground', 'Ġequipment', 'Ġoutweigh', 'Ġcost', 'Ġcomplexity', 'Ġplacing', 'Ġsatellite', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġsyn', 'Ġlaunched', 'Ġaug', 'ust', 'Ġused', 'Ġcommunication', 'Ġacross', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġstarting', 'Ġtelevision', 'Ġcoverage', 'Ġsummer', 'lymp', 'ics', 'Ġshortly', 'Ġsyn', 'Ġint', 'els', 'Ġaka', 'Ġearly', 'Ġbird', 'Ġlaunched', 'Ġapr', 'il', 'Ġplaced', 'Ġorbit', 'Â°', 'Ġwest', 'Ġlong', 'itude', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġtelecommunications', 'l', 'antic', 'Ġocean', 'mber', 'ada', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġserving', 'Ġcontinent', 'ik', 'Ġlaunched', 'Ġtel', 'es', 'ada', 'Ġunited', 'Ġstates', 'Ġfollowing', 'Ġsuit', 'Ġlaunch', 'Ġwest', 'ar', 'Ġwestern', 'Ġunion', 'Ġapr', 'il', 'Ġmay', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġsatellite', 'Ġworld', 'Ġthree', 'axis', 'Ġstabilized', 'Ġlaunched', 'Ġexperimental', 'Ġsatellite', 'Ġbuilt', 'Ġn', 'asa', 'Ġlaunches', 'Ġtel', 'star', 'Ġwest', 'ar', 'Ġsatellites', 'Ġr', 'ca', 'Ġameric', 'om', 'later', 'Ġge', 'Ġameric', 'om', 'es', 'Ġlaunched', 'Ġsat', 'Ġsat', 'Ġinstrumental', 'Ġhelping', 'Ġearly', 'Ġcable', 'Ġchannels', 'Ġfree', 'form', 'Ġweather', 'Ġchannel', 'Ġbecome', 'Ġsuccessful', 'Ġchannels', 'Ġdistributed', 'Ġprogramming', 'Ġlocal', 'Ġcable', 'Ġhead', 'ends', 'Ġusing', 'Ġsatellite', 'Ġadditionally', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsatellite', 'Ġused', 'Ġbroadcast', 'Ġtelevision', 'Ġnetworks', 'Ġunited', 'Ġstates', 'Ġlike', 'Ġdistribute', 'Ġprogramming', 'Ġlocal', 'Ġaf', 'ï', '¬', 'ģ', 'li', 'ate', 'Ġstations', 'Ġsat', 'Ġwidely', 'Ġused', 'Ġtwice', 'Ġcommunications', 'Ġcapacity', 'Ġcompeting', 'Ġwest', 'ar', 'Ġameric']</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>['Ġusing', 'Ġrocket', 'Ġlaunch', 'Ġtest', 'Ġvehicles', 'Ġmach', 'b', 'Ġprogram', 'Ġfirst', 'Ġlaunch', 'Ġdynam', 'Ġoccurred', 'Ġj', 'une', 'Ġlaunch', 'Ġcomplex', 'Ġmid', 'atlantic', 'Ġregional', 'Ġspac', 'eport', 'Ġrocket', 'Ġlaunched', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġcomplex', 'Äģ', 'h', 'ia', 'Ġpeninsula', 'Ġnew', 'Ġzeal', 'Ġlaunch', 'Ġpad', "'s", 'Ġremote', 'Ġsparse', 'ly', 'Ġpopulated', 'Ġlocation', 'Ġintended', 'Ġenable', 'Ġhigh', 'Ġfrequency', 'Ġlaunches', 'Ġrocket', 'Ġlaunch', 'Ġpad', 'Ġprivately', 'Ġfunded', 'Ġfirst', 'Ġtime', 'Ġparts', 'Ġorbital', 'Ġlaunch', 'Ġoperation', 'Ġentirely', 'Ġrun', 'Ġprivate', 'Ġsector', 'Ġprivate', 'Ġspace', 'flight', 'Ġcompanies', 'Ġlease', 'Ġlaunch', 'Ġfacilities', 'Ġgovernment', 'Ġagencies', 'Ġlaunch', 'Ġsub', 'orb', 'ital', 'Ġrockets', ').[', 'Ġoct', 'ober', 'Ġrocket', 'Ġlab', 'Ġselected', 'Ġvirgin', 'ia', 'Ġspace', "'s", 'Ġmid', 'atlantic', 'Ġregional', 'Ġspac', 'eport', 'ars', 'Ġwall', 'ops', 'Ġflight', 'Ġfacility', 'Ġvirgin', 'ia', 'Ġfuture', 'Ġsecondary', 'Ġlaunch', 'Ġsite', 'Ġunited', 'Ġstates', 'Ġcalled', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġcomplex', 'Ġlaunch', 'Ġcomplex', 'Ġexpected', 'Ġserve', 'Ġgovernment', 'Ġcustomers', 'Ġfirst', 'Ġlaunch', 'Ġhappened', 'Ġjan', 'uary', 'Ġelectron', 'Ġrocket', 'Ġsuccessfully', 'Ġorb', 'ited', 'Ġsatellites', 'Ġadditionally', 'Ġspace', 'Ġagency', 'Ġgiving', 'Ġhigh', 'lands', 'Ġislands', 'Ġenterprise', 'Ġopportunity', 'Ġdevelop', 'Ġelectron', 'Ġlaunch', 'Ġpad', 'h', 'Ã', '²', 'ine', 'Ġpeninsula', 'utherland', 'Ġsc', 'ot', 'land', 'Ġlocation', 'Ġwould', 'Ġnamed', 'utherland', 'Ġspac', 'eport', 'Ġelectron', 'Ġflown', 'Ġtimes', 'Ġsince', 'Ġmay', 'Ġtotal', 'Ġsuccesses', 'Ġfailures', 'Ġinitial', 'Ġtest', 'Ġflight', 'Ġcalled', "'s", 'Ġtest', '",', 'Ġfailed', 'Ġdue', 'Ġglitch', 'Ġcommunication', 'Ġequipment', 'Ġground', 'Ġfollow', 'Ġmissions', 'Ġcalled', 'still', 'Ġtesting', '",', "'s", 'Ġbusiness', 'Ġtime', 'Ġone', "'s", 'Ġpick', 'ering', '",', 'Ġdelivered', 'Ġmultiple', 'Ġsmall', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġaug', 'ust', 'Ġmission', 'Ġnamed', 'look', 'Ġhands', 'Ġsuccessfully', 'Ġdelivered', 'Ġfour', 'Ġsatellites', 'Ġoct', 'ober', 'Ġmission', 'Ġnamed', 'Ġcrow', 'Ġflies', 'Ġsuccessfully', 'Ġlaunched', 'Äģ', 'h', 'ia', 'Ġdeploying', 'Ġsmall', 'Ġsatellite', 'Ġkick', 'Ġstage', 'Ġparking', 'Ġj', 'uly', 'Ġth', 'ir', 'teenth', 'Ġelectron', 'Ġrocket', 'Ġlaunch', 'Ġfailed', 'Ġcustomer', 'Ġpayload', 'Ġboard', 'Ġfirst', 'Ġfailure', 'Ġmaiden', 'Ġflight', 'Ġmay']</t>
+          <t>['Ġtrans', 'p', 'ond', 'ers', 'Ġopposed', 'Ġwest', 'ar', 'Ġresulting', 'Ġlower', 'Ġtrans', 'p', 'onder', 'usage', 'Ġcosts', 'Ġsatellites', 'Ġlater', 'Ġdecades', 'Ġtended', 'Ġeven', 'Ġhigher', 'Ġtrans', 'p', 'onder', 'Ġnumbers', 'Ġhug', 'hes', 'Ġspace', 'Ġcommunications', 'Ġbo', 'e', 'ing', 'Ġsatellite', 'Ġdevelopment', 'Ġcenter', 'Ġbuilt', 'Ġnearly', 'Ġpercent', 'Ġone', 'Ġhundred', 'Ġsatellites', 'Ġservice', 'Ġworldwide', 'Ġmajor', 'Ġsatellite', 'Ġmanufacturers', 'Ġinclude', 'Ġspace', 'Ġsystems', 'lor', 'al', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'Ġstar', 'Ġbus', 'Ġseries', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'ge', 'Ġexamples', 'Ġgeo', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġind', 'ian', 'Ġspace', 'Ġresearch', 'Ġorganisation', 'Ġlock', 'heed', 'Ġmart', 'Ġformer', 'Ġr', 'ca', 'Ġast', 'ro', 'Ġelectronics', 'ge', 'Ġast', 'ro', 'Ġspace', 'Ġbusiness', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġal', 'c', 'atel', 'Ġspace', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġspace', 'bus', 'Ġseries', 'Ġast', 'rium', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġmust', 'Ġoperate', 'Ġequ', 'ator', 'Ġtherefore', 'Ġappear', 'Ġlower', 'Ġhorizon', 'Ġreceiver', 'Ġgets', 'Ġfarther', 'Ġequ', 'ator', 'Ġcause', 'Ġproblems', 'Ġextreme', 'Ġnort', 'ly', 'Ġlat', 'itudes', 'Ġaffecting', 'Ġconnectivity', 'Ġcausing', 'Ġmultip', 'ath', 'Ġinterference', 'ca', 'used', 'Ġsignals', 'Ġreflecting', 'Ġground', 'Ġground', 'Ġantenna', 'Ġthus', 'Ġareas', 'Ġclose', 'Ġnorth', 'Ġsouth', 'Ġpole', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġmay', 'Ġappear', 'Ġhorizon', 'Ġtherefore', 'Ġorbit', 'Ġsatellites', 'Ġlaunched', 'Ġmainly', 'Ġr', 'ussia', 'Ġalleviate', 'Ġproblem', 'Ġorbits', 'Ġappealing', 'Ġalternative', 'Ġcases', 'Ġorbit', 'Ġhighly', 'Ġinclined', 'Ġguaranteeing', 'Ġgood', 'Ġelevation', 'Ġselected', 'Ġpositions', 'Ġnorthern', 'Ġportion', 'Ġorbit', 'e', 'lev', 'ation', 'Ġextent', 'Ġsatellite', "'s", 'Ġposition', 'Ġhorizon', 'Ġthus', 'Ġsatellite', 'Ġhorizon', 'Ġzero', 'Ġelevation', 'Ġsatellite', 'Ġdirectly', 'Ġoverhead', 'Ġelevation', 'Ġdegrees', '.)', 'Ġorbit', 'Ġdesigned', 'Ġsatellite', 'Ġspends', 'Ġgreat', 'Ġmajority', 'Ġtime', 'Ġfar', 'Ġnorthern', 'Ġlat', 'itudes', 'Ġground', 'Ġfootprint', 'Ġmoves', 'Ġslightly', 'Ġperiod', 'Ġone', 'Ġhalf', 'Ġday', 'Ġsatellite', 'Ġavailable', 'Ġoperation', 'Ġtargeted', 'Ġregion', 'Ġnine', 'Ġhours', 'Ġevery', 'Ġsecond', 'Ġrevolution', 'Ġway', 'Ġconstellation', 'Ġthree', 'Ġsatellites', 'plus', 'orbit', 'Ġsp', 'ares', 'Ġprovide', 'Ġuninterrupted', 'Ġcoverage', 'Ġfirst', 'Ġsatellite', 'Ġseries', 'Ġlaunched', 'Ġapr', 'il', 'Ġused', 'Ġexperimental', 'Ġtransmission', 'Ġsignals', 'Ġmos', 'cow']</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>['Ġtwentieth', 'Ġlaunch', 'Ġalso', 'Ġfailed', 'still', 'Ġtesting', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsuccessful', 'Ġlaunch', 'Ġel', 'ana', 'Ġone', "'s", 'Ġpick', 'ering', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġn', 'asa', 'sponsored', 'Ġlaunch', 'Ġn', 'rol', 'birds', 'Ġfeather', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġn', 'ro', 'sponsored', 'Ġlaunch', 'Ġsub', 'orb', 'ital', 'Ġlaunches', 'Ġlaunch', 'Ġsites', 'Ġlaunch', 'Ġhistory', 'Ġnotable', 'Ġlaunches', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'n', 'ro', 'Ġpayload', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġrocket', 'Ġlaunch', 'Ġcomplex', 'return', 'Ġsender', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġocean', 'Ġrecovery', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', "'s", 'Ġlittle', 'Ġch', 'ile', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġcap', 'stone', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġmoon', 'Ġhaw', 'keye', 'Ġcluster', 'v', 'irgin', 'ia', 'Ġlaunch', 'Ġlovers', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġlaunch', 'Ġcomplex', 'Ġmid', 'atlantic', 'Ġregional', 'Ġspac', 'eport', 'Ġorbital', 'Ġlaunch', 'Ġfailure', 'Ġorbital', 'Ġlaunch', 'Ġsuccess', 'Ġsub', 'orb', 'ital', 'Ġlaunch', 'Ġfailure', 'Ġsub', 'orb', 'ital', 'Ġlaunch', 'Ġsuccess', 'Ġscheduled', 'Ġorbital', 'Ġmissions', 'Ġmah', 'ia', 'Ġmah', 'ia', 'Ġmars', 'Ġlaunch', 'Ġstatistics', 'Ġlaunch', 'Ġoutcomes', 'Ġlaunch', 'Ġsites', 'Ġbooster', 'Ġtests', 'Ġrecover', 'ies', 'Ġrocket', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġattempt', 'Ġatmospheric', 'Ġtest', 'Ġsuccess', 'Ġocean', 'Ġrecovery', 'Ġsuccess', 'Ġaerial', 'Ġcapture', 'Ġpartial', 'Ġfailure', 'Ġblock', 'Ġblock', 'Ġupgrade', 'th', 'rust', 'ers', 'Ġblock', 'Ġupgrade', 'par', 'ach', 'ute', 'Ġblock', 'Ġupgrade', 'par', 'af', 'oil', 'Ġhaste', 'sub', 'orb', 'ital', 'Ġsmall', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcomparison', 'Ġorbital', 'Ġlauncher', 'Ġfamilies', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġfal', 'con', 'Ġfire', 'ï', '¬', 'Ĥ', 'Ġalpha', 'Ġmi', 'ura', 'Ġvector', 'r', 'rocket', 'Ġlab', 'Ġcelebrates', 'Ġrich', 'Ġten', 'year', 'Ġhistory', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'Ġgets', 'Ġsecond', 'Ġlaunch', 'Ġsite', 'Ġgears', 'Ġrapid', 'Ġflight', 'Ġcad', 'ence', 'ar', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġoct', 'ober', 'Ġbots', 'ford']</t>
+          <t>['Ġupl', 'ink', 'Ġstation', 'link', 'Ġstations', 'Ġlocated', 'iber', 'ia', 'Ġr', 'ussian', 'Ġfar', 'Ġeast', 'ils', 'k', 'Ġk', 'hab', 'arov', 'sk', 'Ġmag', 'adan', 'Ġv', 'lad', 'iv', 'ost', 'ok', 'mber', 'v', 'iet', 'Ġengineers', 'Ġcreated', 'Ġunique', 'Ġsystem', 'Ġnational', 'Ġnetwork', 'Ġsatellite', 'Ġtelevision', 'Ġcalled', 'Ġorbit', 'Ġbased', 'Ġsatellites', 'Ġunited', 'Ġstates', 'Ġnational', 'Ġpolar', 'orb', 'iting', 'Ġoperational', 'Ġenvironmental', 'Ġsatellite', 'Ġsystem', 'n', 'po', 'ess', 'Ġestablished', 'Ġconsolidate', 'Ġpolar', 'Ġsatellite', 'Ġoperations', 'Ġn', 'asa', 'national', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġadministration', 'national', 'Ġocean', 'ic', 'Ġatmospheric', 'Ġadministration', 'Ġn', 'po', 'ess', 'Ġmanages', 'Ġnumber', 'Ġsatellites', 'Ġvarious', 'Ġpurposes', 'Ġexample', 'ets', 'Ġmeteor', 'ological', 'Ġsatellite', 'Ġe', 'um', 'ets', 'Ġeuro', 'pe', 'Ġbranch', 'Ġprogram', 'Ġmet', 'op', 'Ġmeteor', 'ological', 'Ġoperations', 'Ġorbits', 'Ġsun', 'Ġsynchron', 'ous', 'Ġmeaning', 'Ġcross', 'Ġequ', 'ator', 'Ġlocal', 'Ġtime', 'Ġday', 'Ġexample', 'Ġsatellites', 'Ġn', 'po', 'ess', 'civil', 'ian', 'Ġorbit', 'Ġcross', 'Ġequ', 'ator', 'Ġgoing', 'Ġsouth', 'Ġnorth', 'Ġtimes', 'Ġorbit', 'Ġpolar', 'Ġorbit', 'Ġbeyond', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġplans', 'Ġinitiatives', 'Ġbring', 'Ġdedicated', 'Ġcommunications', 'Ġsatellite', 'Ġbeyond', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġn', 'asa', 'Ġproposed', 'Ġlun', 'et', 'Ġdata', 'Ġnetwork', 'Ġaiming', 'Ġprovide', 'ĠâĢ', 'ŀ', 'l', 'un', 'ar', 'Ġinternet', 'Ġcis', 'l', 'un', 'ar', 'Ġspacecraft', 'Ġinstallations', 'Ġmoon', 'light', 'Ġinitiative', 'Ġequivalent', 'Ġes', 'Ġproject', 'Ġstated', 'Ġcompatible', 'Ġproviding', 'Ġnavig', 'ational', 'Ġservices', 'Ġlunar', 'Ġsurface', 'Ġprogrammes', 'Ġsatellite', 'Ġconst', 'ell', 'st', 'ions', 'Ġseveral', 'Ġsatellites', 'Ġvarious', 'Ġorbits', 'Ġaround', 'Ġmoon', 'Ġorbits', 'Ġalso', 'Ġplanned', 'Ġused', 'Ġpositions', 'Ġpoints', 'Ġalso', 'Ġproposed', 'Ġcommunication', 'Ġsatellites', 'Ġcovering', 'Ġmoon', 'Ġalike', 'Ġcommunication', 'Ġsatellites', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġcover', 'Ġearth', 'Ġalso', 'Ġdedicated', 'Ġcommunication', 'Ġsatellites', 'Ġorbits', 'Ġaround', 'Ġmars', 'Ġsupporting', 'Ġdifferent', 'Ġmissions', 'Ġsurface', 'Ġorbits', 'Ġconsidered', 'Ġmars', 'Ġtelecommunications', 'Ġorbit', 'er', 'Ġcommunications', 'Ġsatellites', 'Ġusually', 'Ġcomposed', 'Ġfollowing', 'Ġsubsystem', 'Ġcommunication', 'Ġpayload', 'Ġnormally', 'Ġcomposed', 'Ġtrans', 'p', 'ond', 'ers', 'Ġantennas', 'Ġswitching', 'Ġsystems', 'Ġengines', 'Ġused', 'Ġbring', 'Ġsatellite', 'Ġdesired', 'Ġorbit', 'Ġstation', 'Ġkeeping', 'Ġtracking', 'Ġstabilization']</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>['Ġend', 'Ġmay', 'rocket', 'Ġlab', 'Ġelectron', 'Ġr', 'utherford', 'Ġp', 'eter', 'Ġbeck', 'Ġstarted', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġplace', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġinsider', 'Ġretrieved', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'Ġelectron', "'s", 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsuccessfully', 'Ġmakes', 'Ġspace', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġbeck', 'Ġp', 'eter', 'ye', 'Ġtook', 'Ġus', 'Ġget', 'Ġorbit', 'Ġbelieve', 'Ġmuch', '!"', 'Ġtwitter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ye', 'Ġtook', 'Ġus', 'Ġmillion', 'Ġget', 'Ġorbit', 'Ġbelieve', 'Ġmuch', '!"', 'Ġv', 'ance', 'Ġash', 'lee', 'Ġfe', 'b', 'ruary', 'Ġsmall', 'Ġrocket', 'Ġmaker', 'Ġrunning', 'Ġdifferent', 'Ġkind', 'Ġspace', 'Ġrace', 'bl', 'Ġbloom', 'berg', 'Ġretrieved', 'Ġoct', 'ober', 'aven', 'port', 'Ġchrist', 'ian', 'Ġoct', 'ober', 'v', 'irgin', 'ia', 'Ġrocket', 'Ġlaunch', 'Ġsite', "'s", 'Ġgrow', 'Ġsuccessful', 'Ġstartup', 'Ġsince', 'Ġspace', 'x', 'Ġwashing', 'ton', 'Ġpost', 'Ġretrieved', 'Ġoct', 'ober', 'elect', 'ron', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġelectron', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'mber', 'Ġretrieved', 'mber', 'Ġb', 'ennett', 'Ġj', 'ay', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġreveals', 'Ġsecret', 'Ġengine', 'kick', 'Ġstage', 'Ġelectron', 'Ġrocket', 'http', 'Ġpopular', 'Ġmechanics', 'Ġretrieved', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġincreases', 'Ġelectron', 'Ġpayload', 'Ġcapacity', 'Ġenabling', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'us', 'ability', 'roc', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġmay', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'uly', 'sc', 'ot', 'land', 'Ġsite', 'Ġselected', 'Ġlaunch', 'Ġbase', 'Ġlock', 'heed', 'Ġmart', 'Ġorb', 'ex', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġsee', 'Ġalso', 'Ġreferences', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġether', 'ington', 'arrell']</t>
+          <t>['Ġsubsystem', 'Ġused', 'Ġkeep', 'Ġsatellite', 'Ġright', 'Ġorbit', 'Ġantennas', 'Ġpointed', 'Ġright', 'Ġdirection', 'Ġpower', 'Ġsystem', 'Ġpointed', 'Ġtowards', 'Ġsun', 'Ġpower', 'Ġsubsystem', 'Ġused', 'Ġpower', 'Ġsatellite', 'Ġsystems', 'Ġnormally', 'Ġcomposed', 'Ġsolar', 'Ġcells', 'Ġbatteries', 'Ġmaintain', 'Ġpower', 'Ġsolar', 'Ġeclipse', 'Ġcommand', 'Ġcontrol', 'Ġsubsystem', 'Ġmaintains', 'Ġcommunications', 'Ġground', 'Ġcontrol', 'Ġstations', 'Ġground', 'Ġcontrol', 'Ġearth', 'Ġstations', 'Ġmonitor', 'Ġsatellite', 'Ġperformance', 'Ġcontrol', 'Ġfunctionality', 'Ġvarious', 'Ġphases', 'Ġlife', 'cycle', 'Ġbandwidth', 'Ġavailable', 'Ġsatellite', 'Ġdepends', 'Ġupon', 'Ġnumber', 'Ġtrans', 'p', 'ond', 'ers', 'Ġprovided', 'Ġsatellite', 'Ġservice', 'Ġvoice', 'Ġinternet', 'Ġradio', 'Ġrequires', 'Ġdifferent', 'Ġamount', 'Ġbandwidth', 'Ġtransmission', 'Ġtypically', 'Ġknown', 'Ġlink', 'Ġbudget', 'ing', 'Ġnetwork', 'Ġsimulator', 'Ġused', 'Ġarrive', 'Ġexact', 'Ġvalue', 'ocating', 'Ġfrequencies', 'Ġsatellite', 'Ġservices', 'Ġcomplicated', 'Ġprocess', 'Ġrequires', 'Ġinternational', 'Ġcoordination', 'Ġplanning', 'Ġcarried', 'Ġausp', 'ices', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', 'Ġfacilitate', 'Ġfrequency', 'Ġplanning', 'Ġworld', 'Ġdivided', 'Ġthree', 'Ġregions', 'Ġregion', 'Ġeuro', 'pe', 'Ġaf', 'rica', 'Ġmiddle', 'Ġeast', 'Ġformerly', 'v', 'iet', 'Ġunion', 'ong', 'olia', 'Ġregion', 'Ġnorth', 'Ġsouth', 'Ġameric', 'Ġgreen', 'land', 'Ġregion', 'ia', 'excluding', 'Ġregion', 'Ġareas', 'Ġaust', 'ral', 'ia', 'Ġsouthwest', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġwithin', 'Ġregions', 'Ġfrequency', 'Ġbands', 'Ġallocated', 'Ġvarious', 'Ġsatellite', 'Ġservices', 'Ġalthough', 'Ġgiven', 'Ġservice', 'Ġmay', 'Ġallocated', 'Ġdifferent', 'Ġfrequency', 'Ġbands', 'Ġdifferent', 'Ġregions', 'Ġservices', 'Ġprovided', 'Ġsatellites', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'f', 'ss', 'Ġbroadcasting', 'Ġsatellite', 'Ġservice', 'b', 'ss', 'Ġmobile', 'atellite', 'Ġservice', 'Ġstructure', 'Ġfrequency', 'Ġallocation', 'Ġsatellite', 'Ġsystems', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġir', 'idium', 'Ġsatellite', 'Ġservice', 'Ġservice', 'Ġfirst', 'Ġhistorically', 'Ġimportant', 'Ġapplication', 'Ġcommunication', 'Ġsatellites', 'Ġinter', 'continental', 'Ġlong', 'Ġdistance', 'Ġtele', 'phony', 'Ġfixed', 'Ġpublic', 'Ġswitched', 'Ġtelephone', 'Ġnetwork', 'Ġrel', 'ays', 'Ġtelephone', 'Ġcalls', 'Ġland', 'Ġline', 'Ġtele', 'phones', 'Ġearth', 'Ġstation', 'Ġtransmitted', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'link', 'Ġfollows', 'Ġanalogous', 'Ġpath', 'Ġimprovements', 'Ġsubmarine', 'Ġcommunications', 'Ġcables', 'Ġuse', 'Ġfiber', 'opt', 'ics', 'Ġcaused', 'Ġdecline', 'Ġuse', 'Ġsatellites', 'Ġfixed', 'Ġtele', 'phony', 'Ġlate', 'th', 'Ġcentury', 'Ġsatellite', 'Ġcommunications', 'Ġstill', 'Ġused', 'Ġmany', 'Ġapplications', 'Ġtoday', 'Ġremote', 'Ġislands', 'Ġasc', 'ension', 'Ġisland', 'Ġsaint', 'Ġhel', 'ena', 'Ġdie', 'go', 'Ġgar', 'cia']</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1699,7 +1699,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>['Ġmay', 'rocket', 'Ġlab', 'Ġtests', 'Ġnew', 'Ġhyper', 'cur', 'ie', 'Ġengine', 'Ġpower', 'Ġdeep', 'Ġspace', 'Ġdelivery', 'Ġvehicle', 'Ġl', 'ivery', 'veh', 'icle', 'Ġtech', 'cr', 'unch', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'rocket', 'Ġlab', 'Ġp', 'eter', 'Ġbeck', 'Ġsmall', 'sat', 'Ġkeynote', 'Ġyoutube', 'Ġrocket', 'Ġlab', 'rocket', 'Ġlab', 'Ġcelebrates', 'Ġrich', 'Ġten', 'year', 'Ġhistory', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', 'view', 'Ġdetails', 'Ġretrieved', 'mber', 'elect', 'ron', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġapr', 'il', 'printed', 'Ġbattery', 'powered', 'Ġrocket', 'Ġengine', 'Ġpopular', 'Ġscience', 'Ġretrieved', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġmakes', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġbooster', 'Ġrecovery', 'Ġsuccessful', 'Ġlaunch', 'Ġtech', 'cr', 'unch', 'mber', 'Ġretrieved', 'mber', 'new', 'Ġzeal', 'Ġspace', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġprivate', 'Ġsite', 'Ġnews', 'Ġmay', 'Ġretrieved', 'Ġmay', 'new', 'Ġzeal', 'Ġtest', 'Ġrocket', 'Ġmakes', 'Ġspace', 'Ġorbit', 'Ġindependent', 'ie', 'Ġassociated', 'Ġpress', 'Ġmay', 'Ġretrieved', 'Ġmay', 'rocket', 'Ġlab', 'Ġcompletes', 'Ġpost', 'flight', 'Ġanalysis', 'Ġelectron', 'Ġtest', 'Ġrocket', 'Ġlab', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġr', 'yan', 'Ġh', 'olly', 'Ġjan', 'uary', 'blast', 'Ġrocket', 'Ġlab', 'Ġsuccessfully', 'Ġreaches', 'Ġorbit', 'Ġnew', 'Ġzeal', 'Ġherald', 'Ġretrieved', 'Ġjan', 'uary', 'Ġrocket', 'Ġlab', 'Ġus', 'mber', "'s", 'Ġbusiness', 'Ġtime', 'Ġlaunch', 'Ġretrieved', 'mber', 'Ġsm', 'yth', 'Ġjam', 'ie', 'Ġjan', 'uary', 'private', 'Ġgroup', 'world', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcheap', 'Ġrocket', 'Ġlaunch', 'Ġfinancial', 'Ġtimes', 'Ġretrieved', 'Ġjan', 'uary', 'launch', 'Ġweek', 'Ġarrives', 'Ġrocket', 'Ġlab', "'s", 'Ġelectron', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġbr', 'Ã¼', 'g', 'ge', 'bert', 'elect', 'ron', 'Ġb', 'de', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġbr']</t>
+          <t>['Ġeas', 'ter', 'Ġisland', 'Ġsubmarine', 'Ġcables', 'Ġservice', 'Ġneed', 'Ġsatellite', 'Ġtele', 'phones', 'Ġalso', 'Ġregions', 'Ġcontinents', 'Ġcountries', 'Ġland', 'line', 'Ġtelecommunications', 'Ġrare', 'Ġnon', 'Ġexist', 'ent', 'Ġexample', 'Ġlarge', 'Ġregions', 'Ġsouth', 'Ġameric', 'Ġaf', 'rica', 'ada', 'Ġch', 'ina', 'Ġr', 'ussia', 'Ġaust', 'ral', 'ia', 'Ġsatellite', 'Ġcommunications', 'Ġalso', 'Ġprovide', 'Ġconnection', 'Ġedges', 'Ġant', 'ar', 'ctica', 'Ġgreen', 'land', 'Ġland', 'Ġuse', 'Ġsatellite', 'Ġphones', 'Ġrigs', 'Ġsea', 'Ġbackup', 'Ġhospitals', 'Ġmilitary', 'Ġrecreation', 'Ġships', 'Ġsea', 'Ġwell', 'Ġplanes', 'Ġoften', 'Ġuse', 'Ġsatellite', 'Ġphones', 'Ġsatellite', 'Ġphone', 'Ġsystems', 'Ġaccomplished', 'Ġnumber', 'Ġmeans', 'Ġlarge', 'Ġscale', 'Ġoften', 'Ġlocal', 'Ġtelephone', 'Ġsystem', 'Ġisolated', 'Ġarea', 'Ġlink', 'Ġtelephone', 'Ġsystem', 'Ġmain', 'Ġland', 'Ġarea', 'Ġalso', 'Ġservices', 'Ġpatch', 'Ġradio', 'Ġsignal', 'Ġtelephone', 'Ġsystem', 'Ġexample', 'Ġalmost', 'Ġtype', 'Ġsatellite', 'Ġused', 'Ġsatellite', 'Ġphones', 'Ġconnect', 'Ġdirectly', 'Ġconstellation', 'Ġeither', 'Ġge', 'ost', 'ation', 'ary', 'Ġlow', 'earth', 'orbit', 'Ġsatellites', 'Ġcalls', 'Ġforwarded', 'Ġsatellite', 'Ġteleport', 'Ġconnected', 'Ġpublic', 'Ġswitched', 'Ġtelephone', 'Ġnetwork', 'Ġtelevision', 'Ġbecame', 'Ġmain', 'Ġmarket', 'Ġdemand', 'Ġsimultaneous', 'Ġdelivery', 'Ġrelatively', 'Ġsignals', 'Ġlarge', 'Ġbandwidth', 'Ġmany', 'Ġreceivers', 'Ġprecise', 'Ġmatch', 'Ġcapabilities', 'Ġge', 'os', 'ynchronous', 'ats', 'Ġtwo', 'Ġsatellite', 'Ġtypes', 'Ġused', 'Ġnorth', 'Ġameric', 'Ġtelevision', 'Ġradio', 'Ġdirect', 'Ġbroadcast', 'Ġsatellite', 'bs', 'Ġfixed', 'Ġservice', 'Ġsatellite', 'f', 'ss', 'Ġdefinitions', 'Ġf', 'ss', 'bs', 'Ġsatellites', 'Ġoutside', 'Ġnorth', 'Ġameric', 'Ġespecially', 'Ġeuro', 'pe', 'Ġbit', 'Ġambiguous', 'Ġsatellites', 'Ġused', 'Ġdirect', 'home', 'Ġtelevision', 'Ġeuro', 'pe', 'Ġhigh', 'Ġpower', 'Ġoutput', 'bs', 'class', 'Ġsatellites', 'Ġnorth', 'Ġameric', 'Ġuse', 'Ġlinear', 'Ġpolarization', 'Ġf', 'ss', 'class', 'Ġsatellites', 'Ġexamples', 'Ġast', 'ra', 'Ġe', 'ut', 'els', 'Ġhot', 'bird', 'Ġspacecraft', 'Ġorbit', 'Ġeuro', 'pe', 'Ġcontinent', 'Ġterms', 'Ġf', 'ss', 'bs', 'Ġused', 'Ġthroughout', 'Ġnorth', 'Ġameric', 'Ġcontinent', 'Ġuncommon', 'Ġeuro', 'pe', 'Ġfixed', 'Ġservice', 'Ġsatellites', 'Ġuse', 'Ġband', 'Ġlower', 'Ġportions', 'Ġband', 'Ġnormally', 'Ġused', 'Ġbroadcast', 'Ġfeeds', 'Ġtelevision', 'Ġnetworks', 'Ġlocal', 'Ġaffiliate', 'Ġstations', 'Ġprogram', 'Ġfeeds', 'Ġnetwork', 'Ġsynd', 'icated', 'Ġprogramming', 'Ġlive', 'Ġshots', 'Ġback', 'haul']</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>['Ã¼', 'g', 'ge', 'bert', 'elect', 'ron', 'Ġpropulsion', 'Ġb', 'de', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'prop', 'ulsion', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġlaunch', 'Ġalso', 'Ġtested', 'Ġnew', 'Ġkick', 'Ġstage', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġcircular', 'izes', 'Ġorbit', 'Ġnew', 'Ġelectron', 'Ġkick', 'Ġstage', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'rocket', 'Ġlab', 'Ġincreases', 'Ġelectron', 'Ġpayload', 'Ġcapacity', 'Ġenabling', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'us', 'ability', 'roc', 'Ġusability', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'ep', 'Ġrocket', 'Ġlab', 'Ġplan', 'Ġdeliver', 'Ġsatellites', 'Ġmoon', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġf', 'oust', 'Ġje', 'ff', 'mber', 'rocket', 'Ġlab', 'Ġintroduces', 'Ġrobotic', 'Ġmanufacturing', 'Ġsystem', 'Ġincrease', 'Ġelectron', 'Ġproduction', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġel', 'izabeth', 'ell', 'mber', 'space', 'x', 'Ġcompetitor', "'s", 'ros', 'ie', 'Ġrobot', 'Ġpump', 'Ġrocket', 'Ġparts', 'Ġevery', 'Ġhours', 'Ġforb', 'es', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġannounces', 'us', 'ability', 'Ġplans', 'Ġelectron', 'Ġrocket', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġj', 'uly', 'Ġbeck', 'Ġp', 'eter', 'Ġaug', 'ust', "'s", 'Ġrocket', 'Ġlab', 'Ġchanged', 'Ġmind', 'Ġreusable', 'Ġlaunch', 'inter', 'view', 'Ġinterviewed', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġattempt', 'Ġreuse', 'Ġelectron', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'uly', 'Ġsheet', 'z', 'ichael', 'Ġde', 'cember', 'rocket', 'Ġlab', 'pun', 'ched', 'Ġwall', '",', 'Ġce', 'Ġsays', 'Ġpassing', 'Ġkey', 'Ġmilestone', 'Ġeffort', 'Ġreuse', 'Ġrockets', 'Ġace', 'x', 'html', 'Ġretrieved', 'Ġj', 'uly', 'kinson']</t>
+          <t>['Ġwell', 'Ġused', 'Ġapplications', 'Ġtele', 'phony', 'Ġtelevision', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġdistance', 'Ġlearning', 'Ġschools', 'Ġuniversities', 'Ġbusiness', 'Ġtelevision', 'Ġvide', 'ocon', 'f', 'eren', 'cing', 'Ġgeneral', 'Ġcommercial', 'Ġtelecommunications', 'Ġf', 'ss', 'Ġsatellites', 'Ġalso', 'Ġused', 'Ġdistribute', 'Ġnational', 'Ġcable', 'Ġchannels', 'Ġcable', 'Ġtelevision', 'Ġhead', 'ends', 'Ġfree', 'air', 'Ġsatellite', 'Ġchannels', 'Ġalso', 'Ġusually', 'Ġdistributed', 'Ġf', 'ss', 'Ġsatellites', 'Ġband', 'Ġint', 'els', 'Ġameric', 'Ġgalaxy', 'r', 'Ġsatellites', 'Ġnorth', 'Ġameric', 'Ġprovide', 'Ġquite', 'Ġlarge', 'Ġamount', 'Ġf', 'ta', 'Ġchannels', 'Ġband', 'Ġtrans', 'p', 'ond', 'ers', 'Ġameric', 'Ġdish', 'Ġnetwork', 'bs', 'Ġservice', 'Ġalso', 'Ġrecently', 'Ġused', 'Ġf', 'ss', 'Ġtechnology', 'Ġwell', 'Ġprogramming', 'Ġpackages', 'Ġrequiring', 'Ġsuper', 'ish', 'Ġantenna', 'Ġdue', 'Ġdish', 'Ġnetwork', 'Ġneeding', 'Ġcapacity', 'Ġcarry', 'Ġlocal', 'Ġtelevision', 'Ġstations', 'Ġper', 'must', 'carry', 'Ġregulations', 'Ġbandwidth', 'Ġcarry', 'Ġchannels', 'Ġdirect', 'Ġbroadcast', 'Ġsatellite', 'Ġcommunications', 'Ġsatellite', 'Ġtransm', 'Ġsmall', 'bs', 'Ġsatellite', 'Ġdishes', 'usually', 'Ġinches', 'Ġdiameter', 'Ġdirect', 'Ġbroadcast', 'Ġsatellites', 'Ġgenerally', 'Ġoperate', 'Ġupper', 'Ġportion', 'Ġmicrowave', 'Ġband', 'bs', 'Ġtechnology', 'Ġused', 'th', 'oriented', 'direct', 'oh', 'ome', 'Ġsatellite', 'Ġservices', 'Ġdirect', 'v', 'Ġdish', 'Ġnetwork', 'Ġunited', 'Ġstates', 'Ġbell', 'Ġsatellite', 'Ġsh', 'aw', 'Ġdirect', 'ada', 'Ġfre', 'es', 'Ġire', 'land', 'Ġnew', 'Ġzeal', 'Ġdst', 'v', 'Ġsouth', 'Ġaf', 'rica', 'Ġoperating', 'Ġlower', 'Ġfrequency', 'Ġlower', 'Ġpower', 'bs', 'Ġf', 'ss', 'Ġsatellites', 'Ġrequire', 'Ġmuch', 'Ġlarger', 'Ġdish', 'Ġreception', 'Ġfeet', 'Ġdiameter', 'Ġband', 'Ġfeet', 'Ġlarger', 'Ġband', 'Ġuse', 'Ġlinear', 'Ġpolarization', 'Ġtrans', 'p', 'ond', 'ers', 'Ġinput', 'Ġoutput', 'Ġopposed', 'Ġcircular', 'Ġpolarization', 'Ġused', 'bs', 'Ġsatellites', 'Ġminor', 'Ġtechnical', 'Ġdifference', 'Ġusers', 'Ġnotice', 'Ġf', 'ss', 'Ġsatellite', 'Ġtechnology', 'Ġalso', 'Ġoriginally', 'Ġused', 'th', 'Ġsatellite', 'Ġlate', 'Ġearly', 'Ġunited', 'Ġstates', 'Ġform', 'te', 'levision', 'Ġreceive', 'Ġreceivers', 'Ġdishes', 'Ġalso', 'Ġused', 'Ġband', 'Ġform', 'def', 'unct', 'Ġprim', 'est', 'ar', 'Ġsatellite', 'Ġservice', 'Ġsatellites', 'Ġlaunched', 'Ġtrans', 'p', 'ond', 'ers', 'Ġka', 'Ġband', 'Ġdirect']</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>['Ġ', 'ian', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġelectron', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcompany', 'Ġpreviews', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġrecovery', 'http', 'Ġretrieved', 'Ġj', 'uly', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġaug', 'ust', 'small', 'Ġsatellite', 'Ġlauncher', 'Ġrocket', 'Ġlab', 'Ġunve', 'ils', 'Ġplans', 'Ġrecover', 'Ġrockets', 'Ġmid', 'air', 'Ġhelicopters', 'Ġverge', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġattempt', 'Ġfirst', 'Ġlaunch', 'printed', 'Ġengine', "'s", 'Ġalready', 'Ġflown', 'Ġspace', 'g', 'iz', 'mod', 'co', 'Ġg', 'iz', 'mod', 'Ġsheet', 'z', 'ichael', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġunve', 'ils', 'Ġplan', 'Ġland', 'Ġsmall', 'Ġrockets', 'Ġcatching', 'Ġhelicopter', 'Ġretrieved', 'Ġj', 'uly', 'Ġco', 'ï', '¬', 'ģ', 'e', 'ld', 'Ġcall', 'Ġse', 'pt', 'ember', 'rocket', 'Ġlab', 'Ġopens', 'Ġprivate', 'Ġorbital', 'Ġlaunch', 'Ġsite', 'Ġnew', 'Ġzeal', 'sp', 'Ġspace', 'Ġretrieved', 'Ġjan', 'uary', 'next', 'Ġgeneration', 'Ġelectron', 'Ġbooster', 'Ġpad', 'Ġrocket', 'Ġlab', "'s", 'th', 'Ġmission', 'Ġrocket', 'Ġlab', 'Ġus', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'elect', 'ron', 'Ġlaunches', 'Ġsmall', 'ats', 'Ġtest', 'Ġrocket', 'us', 'ability', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'uly', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'rocket', 'Ġlab', "'s", 'th', 'Ġlaunch', 'Ġtests', 'Ġbooster', 'Ġrecovery', 'Ġtechnology', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'amp', 'son', 'Ġben', 'Ġde', 'cember', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtests', 'entry', 'Ġrocket', 'Ġbooster', 'ero', 'Ġaerospace', 'Ġtesting', 'Ġinternational', 'Ġretrieved', 'Ġde', 'cember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'ro', 'Ġsatellite', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġdeploy', 'Ġn', 'ro', 'Ġsatellite', 'th', 'Ġelectron', 'Ġmission', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'letcher', 'Ġcol', 'Ġj', 'une', 'rocket', 'Ġlab', 'Ġlaunches', 'th', 'Ġelectron']</t>
+          <t>['v', "'s", 'Ġspac', 'eway', 'Ġsatellite', 'ik', 'Ġn', 'asa', 'ro', 'Ġalso', 'Ġlaunched', 'Ġexperimental', 'Ġsatellites', 'Ġcarrying', 'Ġka', 'Ġband', 'acons', 'Ġrecently', 'Ġmanufacturers', 'Ġalso', 'Ġintroduced', 'Ġspecial', 'Ġantennas', 'Ġmobile', 'Ġreception', 'bs', 'Ġtelevision', 'Ġusing', 'Ġglobal', 'Ġpositioning', 'Ġsystem', 'Ġtechnology', 'Ġreference', 'Ġantennas', 'Ġautomatically', 'aim', 'Ġsatellite', 'Ġmatter', 'Ġvehicle', 'Ġantenna', 'Ġmounted', 'Ġsituated', 'Ġmobile', 'Ġsatellite', 'Ġantennas', 'Ġpopular', 'Ġrecreational', 'Ġvehicle', 'Ġowners', 'Ġmobile', 'bs', 'Ġantennas', 'Ġalso', 'Ġused', 'Ġjet', 'blue', 'Ġair', 'ways', 'Ġdirect', 'v', 'supp', 'lied', 'Ġlive', 'tv', 'Ġsubsidiary', 'Ġjet', 'blue', 'Ġpassengers', 'Ġview', 'board', 'Ġscreens', 'Ġmounted', 'Ġseats', 'Ġsatellite', 'Ġradio', 'Ġoffers', 'Ġaudio', 'Ġbroadcast', 'Ġservices', 'Ġcountries', 'Ġnotably', 'Ġunited', 'Ġstates', 'Ġmobile', 'Ġservices', 'Ġallow', 'Ġlisteners', 'Ġroam', 'Ġcontinent', 'Ġlistening', 'Ġaudio', 'Ġprogramming', 'Ġanywhere', 'Ġradio', 'Ġbroadcasting', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġsatellite', 'Ġradio', 'Ġsubscription', 'Ġradio', 'Ġdigital', 'Ġradio', 'Ġsignal', 'Ġbroadcast', 'Ġcommunications', 'Ġsatellite', 'Ġcovers', 'Ġmuch', 'Ġwider', 'Ġgeographical', 'Ġrange', 'Ġterrestrial', 'Ġradio', 'Ġsignals', 'Ġamateur', 'Ġradio', 'Ġoperators', 'Ġaccess', 'Ġamateur', 'Ġsatellites', 'Ġdesigned', 'Ġspecifically', 'Ġcarry', 'Ġamateur', 'Ġradio', 'Ġtraffic', 'Ġsatellites', 'Ġoperate', 'Ġspace', 'borne', 'Ġrepe', 'aters', 'Ġgenerally', 'Ġaccessed', 'ateurs', 'Ġequipped', 'Ġradio', 'Ġequipment', 'Ġhighly', 'Ġdirectional', 'Ġantennas', 'ag', 'Ġdish', 'Ġantennas', 'Ġdue', 'Ġlaunch', 'Ġcosts', 'Ġcurrent', 'Ġamateur', 'Ġsatellites', 'Ġlaunched', 'Ġfairly', 'Ġlow', 'Ġearth', 'Ġorbits', 'Ġdesigned', 'Ġdeal', 'Ġlimited', 'Ġnumber', 'Ġbrief', 'Ġcontacts', 'Ġgiven', 'Ġtime', 'Ġsatellites', 'Ġalso', 'Ġprovide', 'Ġdata', 'forward', 'ing', 'Ġservices', 'Ġusing', 'Ġsimilar', 'Ġprotocols', 'Ġsatellite', 'Ġcommunication', 'Ġtechnology', 'Ġused', 'Ġmeans', 'Ġconnect', 'Ġinternet', 'Ġvia', 'Ġbroadband', 'Ġdata', 'Ġconnections', 'Ġuseful', 'Ġusers', 'Ġlocated', 'Ġremote', 'Ġareas', 'Ġcannot', 'Ġaccess', 'Ġbroadband', 'Ġconnection', 'Ġrequire', 'Ġhigh', 'Ġavailability', 'Ġservices', 'Ġcommunications', 'Ġsatellites', 'Ġused', 'Ġmilitary', 'Ġcommunications', 'Ġapplications', 'Ġglobal', 'Ġcommand', 'Ġcontrol', 'Ġsystems', 'Ġexamples', 'Ġmilitary', 'Ġsystems', 'Ġuse', 'Ġcommunication', 'Ġsatellites', 'Ġmil', 'star', 'sc', 'Ġfl', 'ts', 'Ġunited', 'Ġstates', 'Ġn', 'ato', 'Ġsatellites', 'Ġunited', 'Ġkingdom', 'Ġsatellites', 'Ġinstance', 'Ġsk', 'yn', 'et', 'Ġsatellites', 'Ġformer', 'v', 'iet', 'Ġunion', 'Ġind', 'ia', 'Ġlaunched', 'Ġfirst', 'Ġmilitary', 'Ġcommunication', 'Ġsatellite', 'Ġtrans', 'p']</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>['Ġcontinues', 'Ġwork', 'Ġfuture', 'Ġplans', 'nas', 'Ġretrieved', 'Ġj', 'uly', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'rocket', 'Ġlab', 'Ġreports', 'Ġrecovery', 'Ġtest', 'Ġsuccess', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġelectron', 'Ġtest', 'Ġbooster', 'Ġrecovery', 'Ġspac', 'en', 'ews', 'mber', 'Ġretrieved', 'mber', 'rocket', 'Ġlab', 'Ġattempt', 'Ġelectron', 'Ġstage', 'Ġrecovery', 'Ġnext', 'Ġlaunch', 'Ġspac', 'en', 'ews', 'mber', 'Ġretrieved', 'mber', 'Ġr', 'yan', 'Ġjack', 'son', 'mber', 'half', 'life', 'Ġgarden', 'Ġgn', 'ome', 'Ġreaches', 'Ġspace', 'Ġaboard', 'Ġrocket', 'Ġlab', "'s", 'Ġelectron', 'http', 'Ġretrieved', 'mber', 'rocket', 'Ġlab', 'Ġlaunch', 'Ġpayload', 'Ġusers', 'Ġguide', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġready', 'Ġattempt', 'Ġelectron', 'Ġbooster', 'Ġrecovery', 'Ġspac', 'en', 'ews', 'cal', 'end', 'ario', 'Ġde', 'Ġlan', 'z', 'ient', 'os', 'Ġcosmos', 'Ġsp', 'anish', 'oci', 'aci', 'Ã³n', 'Ġaer', 'oes', 'p', 'acial', 'Ġcosmos', 'Ġjan', 'uary', 'Ġp', 'Ġretrieved', 'Ġde', 'cember', 'Ġowl', "'s", 'Ġnight', 'Ġbegins', 'Ġ[...]', 'Ġlan', 'z', 'ient', 'Ġdel', 'Ġsat', 'Ã©', 'lite', 'Ġstri', 'x', 'Î±', 'Ġsu', 'ama', 'Ã±o', 'Ġoblig', 'Ã³', 'Ġutil', 'iz', 'ar', 'Ġun', 'Ġco', 'ï', '¬', 'ģ', 'Ġextend', 'ida', 'rocket', 'Ġlab', 'Ġdeb', 'uts', 'Ġfully', 'Ġautonomous', 'Ġflight', 'Ġtermination', 'Ġsystem', 'Ġspace', 'ref', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġn', 'asa', 'Ġsafety', 'Ġsystem', 'Ġenables', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġwall', 'ops', 'Ġjan', 'odd', 'Ġtim', 'Ġoct', 'ober', 'exclusive', 'Ġinside', 'Ġlook', 'Ġrocket', 'Ġlab', "'s", 'Ġsecret', 'Ġnew', 'Ġmega', 'Ġfactory', '!"', 'Ġeveryday', 'Ġastronaut', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'pay', 'load', 'Ġuser', "'s", 'Ġguide', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'roc', 'ke', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġjan']</t>
+          <t>['ond', 'ers', 'Ġoperate', 'Ġf', 'Ġband', 'Ġbands', 'Ġtypically', 'Ġmilitary', 'Ġsatellites', 'Ġoperate', 'also', 'Ġknown', 'Ġx', 'band', 'also', 'Ġknown', 'Ġka', 'Ġband', 'Ġfrequency', 'Ġbands', 'Ġnear', 'ground', 'Ġsitu', 'Ġenvironmental', 'Ġmonitoring', 'Ġequipment', 'Ġtide', 'Ġgau', 'ges', 'Ġweather', 'Ġstations', 'Ġweather', 'Ġbu', 'oys', 'Ġradios', 'ond', 'es', 'Ġmay', 'Ġuse', 'Ġsatellites', 'Ġone', 'way', 'Ġdata', 'Ġtransmission', 'Ġtwo', 'way', 'Ġtele', 'metry', 'Ġmay', 'Ġbased', 'Ġsecondary', 'Ġpayload', 'Ġweather', 'Ġsatellite', 'Ġcase', 'Ġgoes', 'Ġmete', 'os', 'Ġothers', 'Ġarg', 'os', 'Ġsystem', 'Ġdedicated', 'Ġsatellites', 'Ġdata', 'Ġrate', 'Ġtypically', 'Ġmuch', 'Ġlower', 'Ġsatellite', 'Ġinternet', 'Ġaccess', 'Ġcommercial', 'ization', 'Ġspace', 'Ġhistory', 'Ġtele', 'communication', 'Ġinter', 'atellite', 'Ġcommunications', 'Ġsatellite', 'Ġlist', 'Ġcommunication', 'Ġsatellite', 'Ġcompanies', 'Ġlist', 'Ġcommunications', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'sts', 'Ġnewsp', 'ace', 'Ġreconnaissance', 'Ġsatellite', 'Ġamateur', 'Ġradio', 'Ġinternet', 'Ġaccess', 'Ġmilitary', 'Ġdata', 'Ġcollection', 'Ġsee', 'Ġalso', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġrelay', 'dis', 'amb', 'ig', 'uation', 'Ġsat', 'Ġmove', 'Ġsatellite', 'Ġdata', 'Ġunit', 'Ġsatellite', 'Ġdelay', 'Ġsatellite', 'Ġmodem', 'Ġsatellite', 'Ġspace', 'Ġsegment', 'Ġspace', 'Ġpollution', 'Ġorbital', 'Ġperiods', 'Ġspeeds', 'Ġcalculated', 'Ġusing', 'Ġrelations', 'Ġradius', 'Ġorbit', 'Ġmetres', 'Ġorbital', 'Ġperiod', 'Ġseconds', 'Ġorbital', 'Ġspeed', 'Ġgravitational', 'Ġconstant', 'Ġapproximately', 'ĠÃĹ', 'âĪĴ', 'Ġmass', 'Ġearth', 'Ġapproximately', 'ĠÃĹ', 'ĠÃĹ', 'Ġb', 'Ġapproximately', 'Ġtimes', 'Ġradius', 'Ġlength', 'Ġmoon', 'Ġnearest', 'Ġtimes', 'Ġmoon', 'Ġfart', 'hest', 'Ġlab', 'rador', 'Ġvir', 'gil', '02', 'atellite', 'Ġcommunication', 'Ġb', 'rit', 'ann', 'ica', 'Ġretrieved', '02', 'atell', 'ites', 'Ġcommunication', 'Ġsatellites', 'Ġdex', 'html', 'Ġretrieved', '02', 'military', 'Ġsatellite', 'Ġcommunications', 'Ġfundamentals', 'Ġaerospace', 'Ġcorporation', 'web', 'arch', 'iv', 'fund', 'ament', 'als', 'Ġaerospace', '04', '01', 'Ġarchived', 'Ġoriginal', '09', '05', 'Ġretrieved', '02', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'oct', 'ober', 'ext', 'r']</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>['uary', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġstartup', 'Ġrocket', 'Ġlab', 'Ġsends', 'Ġelectron', 'Ġrocket', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtime', 'h', 'Ġverge', 'Ġretrieved', 'Ġjan', 'uary', 'Ġwall', 'ike', 'Ġjan', 'uary', 'ex', 'pri', 'ze', 'Ġgoogle', "'s", 'Ġmillion', 'Ġmoon', 'Ġrace', 'Ġends', 'Ġwinner', 'sp', 'Ġspace', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmoon', 'Ġexpress', 'mo', 'one', 'x', 'Ġfe', 'b', 'ruary', 'Ġupcoming', 'Ġlaunch', 'Ġrocket', 'lab', 'Ġcontracted', 'Ġrocket', 'lab', 'Ġback', 'Ġattempt', 'Ġcurrently', 'Ġfocused', 'Ġefforts', 'Ġsupporting', 'Ġn', 'asa', 'Ġcommercial', 'Ġlunar', 'Ġpayload', 'Ġservices', 'cl', 'ps', 'Ġcontract', 'weet', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'rocket', 'Ġlab', 'Ġintroduces', 'Ġsub', 'orb', 'ital', 'Ġtest', 'bed', 'Ġrocket', 'Ġselected', 'Ġhyp', 'erson', 'ic', 'Ġtest', 'Ġflights', 'fl', 'ights', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'es', 'nic', 'Ġtre', 'vor', 'Ġj', 'une', 'launch', 'Ġroundup', 'Ġrocket', 'Ġlab', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġhaste', 'Ġmission', 'Ġspace', 'x', 'Ġlaunch', 'Ġsat', 'ria', 'Ġretrieved', 'Ġj', 'une', 'rocket', 'Ġlab', 'Ġselects', 'Ġwall', 'ops', 'Ġu', 'Ġlaunch', 'Ġsite', 'u', 'launch', 'site', 'Ġspac', 'en', 'ews', 'Ġoct', 'ober', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'rocket', 'Ġlab', 'Ġï', '¬', 'Ĥ', 'ies', 'Ġnew', 'Ġzeal', 'Ġwork', 'Ġprogresses', 'Ġvirgin', 'ia', 'Ġlaunch', 'Ġpad', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'Ġhar', 'wood', 'iam', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġsatellites', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġu', 'Ġsoil', 'Ġnews', 'Ġretrieved', 'Ġjan', 'uary', 'os', 'Ġj', 'athan', 'Ġj', 'uly', 'sc', 'ot', 'land', 'Ġhost', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġspac', 'eport', 'Ġent', 'Ġnews', 'Ġretrieved', 'Ġj', 'uly', 'utherland', 'Ġspac', 'eport', 'Ġsc', 'ot', 'land', 'Ġsp', 'acet', 'v', 'Ġretrieved', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġcompletes', 'Ġpost', 'flight', 'Ġanalysis', 'ly', 'sis', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġaug']</t>
+          <t>['ater', 'restrial', 'Ġrel', 'ays', 'Ġrocket', 'Ġstations', 'Ġgive', 'Ġworld', 'wide', 'Ġradio', 'Ġcoverage', '?"', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'Ġinstitute', 'Ġspace', 'Ġeducation', 'Ġretrieved', 'Ġjan', 'uary', 'ike', 'Ġmills', 'Ġaug', 'ust', 'orbit', 'Ġwars', 'Ġwashing', 'ton', 'Ġpost', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'ovember', 'Ġman', 'Ġbehind', 'Ġcurtain', 'Ġair', 'Ġspace', 'Ġmagazine', 'Ġretrieved', 'Ġjan', 'uary', 'Ġanat', 'oly', 'Ġz', 'ak', 'design', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġart', 'ï', '¬', 'ģ', 'cial', 'Ġsatellite', 'Ġearth', 'Ġretrieved', 'Ġjan', 'uary', 'Ġvan', 'Ġke', 'uren', 'Ġdavid', 'Ġk', 'chapter', 'Ġmoon', 'Ġeyes', 'Ġmoon', 'Ġcommunication', 'Ġrelay', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', '".', 'rica', 'rew', 'ed', '.).', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'Ġn', 'asa', 'Ġhistory', 'ï', '¬', 'ģ', 'ce', 'Ġreferences', 'Ġnotes', 'Ġcitations', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġmart', 'ald', 'erson', 'Ġp', 'aul', 'Ġbart', 'ian', 'Ġl', 'u', 'cy', 'arch', 'Ġcommunications', 'Ġsatellites', 'Ġproject', 'Ġscore', 'th', 'Ġed', '.).', 'united', 'Ġstates', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġactivities', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġannual', 'Ġreport', 'Ġcongress', 'history', 'Ġpublished', 'Ġhouse', 'Ġdocument', 'Ġnumber', 'th', 'Ġcongress', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsession', 'Ġwhite', 'Ġhouse', 'Ġfe', 'b', 'ruary', 'Ġpp', 'âĢĵ', 'Ġretrieved', 'Ġjan', 'uary', 'c', 'ou', 'rier', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġstates', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġactivities', 'Ġwhite', 'Ġhouse', 'Ġjan', 'uary', 'Ġpp', 'âĢĵ', 'Ġretrieved', 'Ġjan', 'uary', 'echo', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmart', 'ald', 'erson', 'Ġp', 'aul', 'Ġbart', 'ian', 'Ġl', 'u', 'cy', 'arch', 'Ġcommunications', 'Ġsatellites', 'Ġtel', 'star', 'th', 'Ġed', '.).', 'united', 'Ġstates', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġactivities', 'Ġwhite', 'Ġhouse', 'Ġjan', 'uary', 'Ġpp', 'Ġretrieved', 'Ġjan']</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1764,7 +1764,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>['ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'tele', 'metry', 'Ġglitch', 'Ġkept', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġelectron', 'Ġrocket', 'Ġreaching', 'Ġorbit', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'ell', 'Ġel', 'izabeth', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġelectron', 'Ġbooster', 'Ġlaunches', 'Ġsatellites', 'Ġorbit', 'sp', 'ac', 'Ġspace', 'Ġretrieved', 'Ġaug', 'ust', 'Ġether', 'ington', 'arrell', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'f', 'th', 'Ġelectron', 'Ġrocket', 'Ġyear', 'tech', 'Ġtech', 'cr', 'unch', 'Ġretrieved', 'mber', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġelectron', 'Ġlaunch', 'Ġfails', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', "'s", 'th', 'Ġelectron', 'Ġlaunch', 'Ġends', 'Ġfailure', 'Ġloss', 'Ġpayload', 'Ġtech', 'cr', 'unch', 'Ġmay', 'Ġretrieved', 'Ġmay', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġdelivers', 'Ġnan', 'os', 'atell', 'ites', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsuccessful', 'Ġtest', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'n', 'asa', 'Ġrocket', 'Ġlab', 'Ġpartner', 'Ġsuccessful', 'Ġsatellite', 'Ġlaunch', 'Ġnew', 'Ġzeal', 'h', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġwall', 'ike', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġsp', 'ys', 'Ġagency', 'Ġguides', 'Ġbooster', 'Ġback', 'Ġearth', 'Ġspace', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'return', 'Ġsender', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġde', 'cember', 'Ġelectron', 'Ġwebsite', 'Ġrocket', 'lab', 'usa', 'Ġelectron', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġrocket', 'lab', 'usa', 'Ġcomputer', 'Ġsimulation', 'Ġelectron', 'Ġlaunch', 'Ġyoutube', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['uary', 'Ġward', 'iam', 'Ġw', '.;', 'Ġfl', 'oyd', 'Ġfrank', 'lin', 'Ġw', 'chapter', 'Ġthirty', 'Ġyears', 'Ġspace', 'Ġcommunications', 'Ġresearch', 'Ġdevelopment', 'Ġl', 'incoln', 'Ġlaboratory', '".', 'rica', 'rew', 'ed', '.).', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'Ġn', 'asa', 'Ġhistory', 'ï', '¬', 'ģ', 'ce', 'project', 'Ġwest', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġcomp', 'endium', 'Ġsatellite', 'Ġcommunications', 'Ġprograms', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġpp', 'Ġretrieved', 'Ġjan', 'uary', 'syn', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'syn', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'les', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġcomp', 'endium', 'Ġsatellite', 'Ġcommunications', 'Ġprograms', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġpp', 'Ġretrieved', 'Ġjan', 'uary', 'Ġpel', 'ton', 'Ġj', 'ose', 'ph', 'Ġn', 'history', 'Ġsatellite', 'Ġcommunications', '".', 'Ġpel', 'ton', 'Ġj', '.;', 'Ġmad', 'ry', '.;', 'Ġcam', 'ach', 'ol', 'ara', 'eds', '.).', 'Ġhand', 'book', 'Ġsatellite', 'Ġapplications', 'Ġnew', 'ork', 'Ġspring', 'er', 'early', 'Ġbird', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġcomp', 'endium', 'Ġsatellite', 'Ġcommunications', 'Ġprograms', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġpp', 'Ġretrieved', 'Ġjan', 'uary', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġal', 'ts', 'h', 'uler', 'Ġj', 'os', 'Ã©', 'chapter', 'Ġshort', 'wave', 'Ġscatter', 'Ġsatellite', 'Ġcub', "'s", 'Ġinternational', 'Ġcommunications', '".', 'rica', 'rew', 'ed', '.).', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'Ġn', 'asa', 'Ġhistory', 'ï', '¬', 'ģ', 'ce', 'Ġman', 'n', 'uben', 'ap', 'ril', 'sky', 'tr', 'ac', 'sat', 'series', 'Ġdifferences', 'Ġstrengths', 'Ġweaknesses', 'Ġle', 'Ġgeo', 'Ġsatellites', 'Ġretrieved', 'mber', 'ad', 'c', 'Ġspace', 'Ġdebris', 'Ġmitigation', 'Ġguidelines', 'Ġinter', 'agency', 'Ġspace', 'Ġdebris', 'Ġcoordination', 'Ġcommittee', 'Ġissued', 'Ġsteering']</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1777,7 +1777,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>['Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġng', 'Ġartists', 'Ġimpression', 'Ġextended', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġtype', 'Ġused', 'Ġmission', 'Ġmission', 'Ġtype', 'Ġiss', 'Ġlogistics', 'Ġoperator', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġcos', 'par', 'Ġid', 'Ġsat', 'cat', 'Ġmission', 'Ġduration', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġprogress', 'Ġspacecraft', 'Ġproperties', 'Ġspacecraft', 'Ġlaure', 'l', 'Ġcl', 'ark', 'Ġspacecraft', 'Ġtype', 'Ġenhanced', 'Ġcy', 'gn', 'us', 'Ġmanufacturer', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġaug', 'ust', 'Ġ00', 'Ġrocket', 'Ġant', 'ares', 'Ġlaunch', 'Ġsite', 'Ġwall', 'ops', 'Ġpad', 'Ġcontractor', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġend', 'Ġmission', 'Ġdisposal', 'Ġde', 'orb', 'ited', 'Ġdecay', 'Ġdate', 'planned', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġge', 'oc', 'entric', 'Ġorbit', 'Ġregime', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġinclination', 'Â°', 'Ġber', 'thing', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġber', 'thing', 'Ġport', 'Ġunity', 'Ġn', 'ad', 'ir', 'Ġr', 'ms', 'Ġcapture', 'Ġaug', 'ust', 'Ġ09', 'Ġut', 'c', 'Ġber', 'thing', 'Ġdate', 'Ġaug', 'ust', 'Ġut', 'c', 'Ġtime', 'Ġb', 'ert', 'hed', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġprogress', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġmission', 'Ġpatch', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġcy', 'gn', 'us', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġng', 'Ġnineteenth', 'Ġflight', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġrobotic', 'Ġres', 'upp', 'ly', 'Ġspacecraft', 'Ġcy', 'gn', 'us', 'Ġeighteenth', 'Ġflight', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġcontract', 'Ġn', 'asa', 'Ġmission', 'Ġlaunched', 'Ġaug', 'ust', 'Ġ00', 'Ġeighth', 'Ġlaunch', 'Ġcy', 'gn', 'us', 'Ġcontract', 'Ġorbital', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'Ġn', 'asa', 'Ġjointly', 'Ġdeveloped', 'Ġnew', 'Ġspace', 'Ġtransportation', 'Ġsystem', 'Ġprovide', 'Ġcommercial', 'Ġcargo', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'c', 'ots', 'Ġprogram', 'Ġorbital', 'Ġdesigned', 'Ġacquired', 'Ġbuilt', 'Ġassembled', 'Ġcomponents', 'Ġant', 'ares', 'Ġmedium', 'class', 'Ġlaunch', 'Ġvehicle', 'Ġcy', 'gn', 'us', 'Ġadvanced', 'Ġspacecraft', 'Ġusing', 'Ġpress', 'urized', 'Ġcargo', 'Ġmodule', 'Ġprovided', 'Ġindustrial', 'Ġpartner', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġservice', 'Ġmodule', 'Ġbased', 'Ġorbital', 'Ġge', 'ost']</t>
+          <t>['Ġgroup', 'Ġworking', 'Ġgroup', 'Ġse', 'pt', 'ember', 'region', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġle', 'Ġregion', 'Ġspherical', 'Ġregion', 'Ġextends', 'Ġearth', "'s", 'Ġsurface', 'Ġaltitude', 'z', '000', 'Ġflight', 'Ġlaunch', 'Ġkit', 'rian', 'esp', 'ace', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'project', 'Ġmoon', 'light', 'Ġoct', 'moon', 'light', 'Ġweb', 'inar', 'Ġmar', 'Ġhorn', 'ig', '05', '01', 'ty', 'cho', 'Ġsupporting', 'Ġpermanently', 'Ġcrew', 'ed', 'Ġlunar', 'Ġexploration', 'Ġhigh', 'speed', 'Ġoptical', 'Ġcommunication', 'Ġeverywhere', 'Ġes', 'Ġhorn', 'ig', '06', 'ty', 'cho', 'Ġmission', 'Ġearth', 'moon', 'Ġlib', 'ration', 'Ġpoint', 'ac', 'ac', 'Ġir', 'idium', 'Ġarchived', 'Ġoriginal', '08', 'Ġretrieved', '09', 'united', 'Ġstates', ')"', 'Ġretrieved', 'Ġapr', 'il', 'gs', 'ro', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'ind', 'ian', 'Ġsuccessfully', 'Ġlo', 'fts', 'Ġg', 'sat', 'Ġsatellite', 'Ġn', 'asa', 'Ġspace', 'Ġflight', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'direct', 'v', "'s", 'Ġspac', 'eway', 'Ġsatellite', 'Ġlaunches', 'Ġnew', 'Ġera', 'Ġhigh', 'de', 'ï', '¬', 'ģ', 'n', 'ition', 'Ġprogramming', 'Ġnext', 'Ġgeneration', 'Ġsatellite', 'Ġinitiate', 'Ġhistoric', 'Ġexpansion', 'Ġdirect', 'v', 'Ġspace', 'ref', 'Ġapr', 'il', 'Ġretrieved', '05', 'ind', 'ia', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'military', 'Ġsatellite', 'Ġput', 'Ġearth', "'s", 'Ġorbit', 'Ġn', 'tv', '09', '04', 'Ġretrieved', '09', 'Ġk', 'ramer', 'bert', 'Ġj', 'data', 'Ġcollection', 'mess', 'aging', 'Ġsystems', '".', 'Ġobservation', 'Ġearth', 'Ġenvironment', 'Ġber', 'lin', 'idel', 'berg', 'Ġspring', 'er', 'Ġber', 'lin', 'idel', 'berg', 'Ġpp', 'âĢĵ', 'atellite', 'Ġdata', 'Ġtele', 'communication', 'Ġhand', 'book', 'Ġlibrary', 'w', 'mo', 'int', 'Ġretrieved', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġinter', 'governmental', 'Ġocean', 'ographic']</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>['ar', 'Ġsatellite', 'Ġbus', 'Ġflight', 'Ġused', 'Ġlast', 'Ġremaining', 'Ġant', 'ares', 'Ġseries', 'Ġconstructed', 'Ġu', 'k', 'raine', 'Ġuses', 'Ġr', 'ussian', 'Ġmotors', 'Ġnext', 'Ġthree', 'Ġcy', 'gn', 'us', 'Ġmissions', 'Ġuse', 'Ġfal', 'con', 'Ġsubsequent', 'Ġmission', 'Ġuse', 'Ġnext', 'generation', 'Ġant', 'ares', 'Ġseries', 'Ġdepend', 'Ġu', 'k', 'rain', 'ian', 'Ġr', 'ussian', 'Ġparts', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġeighth', 'Ġcy', 'gn', 'us', 'Ġmission', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġcontract', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'Ġconfirmed', 'Ġfe', 'b', 'ruary', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġtur', 'aly', 'Ġfabric', 'ate', 'Ġtwo', 'Ġadditional', 'Ġpress', 'urized', 'Ġcargo', 'Ġmodules', 'Ġpair', 'Ġforthcoming', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġmissions', 'Ġcurrent', 'Ġplans', 'Ġtwo', 'Ġadditional', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġdesignated', 'Ġng', 'Ġng', 'Ġhistory', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġproduction', 'Ġintegration', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġperformed', 'Ġdull', 'es', 'Ġvirgin', 'ia', 'Ġcy', 'gn', 'us', 'Ġservice', 'Ġmodule', 'ated', 'Ġpress', 'urized', 'Ġcargo', 'Ġmodule', 'Ġlaunch', 'Ġsite', 'Ġmission', 'Ġoperations', 'Ġconducted', 'Ġcontrol', 'Ġcenters', 'Ġdull', 'es', 'Ġvirgin', 'ia', 'Ġh', 'ouston', 'Ġtex', 'Ġfour', 'teenth', 'Ġflight', 'Ġenhanced', 'sized', 'Ġcy', 'gn', 'us', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġloaded', 'Ġcargo', 'Ġnew', 'Ġexperiments', 'Ġarriving', 'Ġorbiting', 'Ġlaboratory', 'Ġinspire', 'Ġfuture', 'Ġscientists', 'Ġexplorers', 'Ġprovide', 'Ġvaluable', 'Ġinsight', 'Ġresearchers', 'Ġn', 'asa', 'Ġscientific', 'Ġresearch', 'Ġstudies', 'Ġinnovative', 'Ġparalysis', 'Ġtherapy', 'Ġenabling', 'Ġneuro', 'reg', 'ener', 'ation', 'ne', 'uron', 'ix', 'Ġsponsored', 'Ġiss', 'Ġnational', 'Ġlab', 'Ġdemonstrates', 'Ġformation', 'Ġneuron', 'Ġcell', 'Ġcultures', 'Ġmicro', 'gravity', 'Ġtests', 'Ġneuron', 'spe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġgene', 'Ġtherapy', 'Ġgene', 'Ġtherapy', 'Ġshows', 'Ġpromise', 'Ġpotential', 'Ġtreatment', 'Ġpeople', 'Ġparalysis', 'Ġneurological', 'Ġdiseases', 'Ġal', 'z', 'heimer', 'âĢ', 'Ļ', 'Ġpark', 'inson', 'âĢ', 'Ļ', 'Ġmodels', 'Ġneeded', 'Ġtest', 'Ġtherapies', 'Ġcannot', 'Ġgrown', 'Ġearth', 'âĢ', 'Ļ', 'Ġgravity', 'Ġcreating', 'Ġcell', 'Ġcultures', 'Ġmicro', 'gravity', 'Ġcould', 'Ġprovide', 'Ġplatform', 'Ġdrug', 'Ġdiscovery', 'Ġgene', 'Ġtherapy', 'Ġtesting', 'Ġspacecraft', 'Ġfire', 'Ġexperiments', 'saf', 'ï', '¬', 'ģ', 'vi', 'Ġunderstanding', 'Ġï', '¬', 'ģ', 'Ġbehaves']</t>
+          <t>['Ġcommission', 'equ', 'ipment', 'Ġneeded', 'Ġtele', 'metry', 'Ġdata', '".', 'Ġmanual', 'Ġsea', 'Ġlevel', 'Ġmeasurement', 'Ġinterpretation', 'Ġvolume', 'Ġv', 'Ġradar', 'Ġgau', 'ges', 'unes', 'doc', 'u', 'Ġretrieved', '08', 'Ġsl', 'otten', 'Ġh', 'ugh', 'Ġr', 'Ġbeyond', 'Ġsp', 'ut', 'nik', 'Ġspace', 'Ġrace', 'Ġorigins', 'Ġglobal', 'Ġsatellite', 'Ġcommunications', 'john', 'Ġhop', 'kins', 'Ġuniversity', 'Ġpress', ');', 'Ġonline', 'Ġreview', 'Ġsatellite', 'Ġindustry', 'Ġassociation', 'ia', 'org', 'Ġcommunications', 'Ġsatellites', 'Ġshort', 'Ġhistory', 'Ġarchived', '05', 'Ġway', 'back', 'Ġmachine', 'Ġdavid', 'Ġj', 'Ġwh', 'al', 'en', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'n', 'asa', 'Ġsp', 'Ġretrieved', 'Ġreading', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>['Ġspace', 'Ġvital', 'Ġdeveloping', 'Ġï', '¬', 'ģ', 'Ġprevention', 'Ġï', '¬', 'ģ', 'Ġsuppression', 'Ġmethods', 'Ġï', '¬', 'Ĥ', 'ame', 'related', 'Ġexperiments', 'ï', '¬', 'ģ', 'cult', 'Ġconduct', 'Ġaboard', 'Ġoccupied', 'Ġspacecraft', 'Ġspacecraft', 'Ġfire', 'Ġexperiments', 'saf', 'ï', '¬', 'ģ', 'Ġuse', 'Ġcy', 'gn', 'us', 'Ġres', 'upp', 'ly', 'Ġcraft', 'Ġleaves', 'Ġspace', 'Ġstation', 'Ġremove', 'Ġrisk', 'Ġcrew', 'Ġspacecraft', 'Ġsaf', 'ï', '¬', 'ģ', 'vi', 'Ġlast', 'Ġseries', 'Ġbuilding', 'Ġprevious', 'Ġresults', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'amm', 'ability', 'Ġdifferent', 'Ġlevels', 'Ġdemonstrate', 'Ġï', '¬', 'ģ', 'Ġdetection', 'Ġmonitoring', 'Ġwell', 'Ġpost', 'ï', '¬', 'ģ', 'Ġcleanup', 'Ġcapabilities', 'Ġexploration', 'Ġpot', 'able', 'Ġwater', 'Ġdispens', 'er', 'expl', 'oration', 'Ġuses', 'Ġadvanced', 'Ġwater', 'Ġsan', 'ization', 'Ġmicrobial', 'Ġgrowth', 'Ġreduction', 'Ġmethods', 'Ġdisp', 'enses', 'Ġhot', 'Ġwater', 'Ġimproved', 'Ġversion', 'Ġsystem', 'Ġlaunched', 'Ġfall', 'Ġsponsored', 'Ġn', 'asa', 'Ġbiological', 'Ġphysical', 'Ġsciences', 'Ġdivision', 'Ġstudy', 'Ġaimed', 'Ġunderstanding', 'Ġorganisms', 'Ġevolve', 'Ġadapt', 'Ġspace', 'Ġenvironment', 'Ġexperiment', 'Ġb', 'ac', 'illus', 'Ġsubt', 'il', 'Ġbacteria', 'Ġgrown', 'Ġspecially', 'Ġdesigned', 'Ġenvironmental', 'Ġhardware', 'Ġrange', 'Ġconditions', 'Ġallowing', 'Ġresearchers', 'Ġinvestigate', 'Ġwhether', 'Ġadaptation', 'Ġprocess', 'Ġoccurs', 'Ġdifferently', 'Ġmicro', 'gravity', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġenvironment', 'Ġwhole', 'Ġrepeat', 'Ġunc', 'rew', 'ed', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġspacecraft', 'Ġmanifest', 'Ġresearch', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'launch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġj', 'une', 'orb', 'ital', 'Ġlooks', 'Ġahead', 'Ġcy', 'gn', 'us', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġant', 'ares', 'Ġcommercial', 'Ġmarket', 'Ġres', 'commercial', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'north', 'rop', 'Ġgr', 'um', 'man', 'optim', 'istic', 'Ġreceive', 'Ġn', 'asa', 'Ġcargo', 'Ġmission', 'Ġorders', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'cy', 'gn', 'us', 'Ġspacecraft', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġfire']</t>
+          <t>['Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġng', 'Ġartists', 'Ġimpression', 'Ġextended', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġtype', 'Ġused', 'Ġmission', 'Ġmission', 'Ġtype', 'Ġiss', 'Ġlogistics', 'Ġoperator', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġcos', 'par', 'Ġid', 'Ġsat', 'cat', 'Ġmission', 'Ġduration', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġprogress', 'Ġspacecraft', 'Ġproperties', 'Ġspacecraft', 'Ġlaure', 'l', 'Ġcl', 'ark', 'Ġspacecraft', 'Ġtype', 'Ġenhanced', 'Ġcy', 'gn', 'us', 'Ġmanufacturer', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġaug', 'ust', 'Ġ00', 'Ġrocket', 'Ġant', 'ares', 'Ġlaunch', 'Ġsite', 'Ġwall', 'ops', 'Ġpad', 'Ġcontractor', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġend', 'Ġmission', 'Ġdisposal', 'Ġde', 'orb', 'ited', 'Ġdecay', 'Ġdate', 'planned', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġge', 'oc', 'entric', 'Ġorbit', 'Ġregime', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġinclination', 'Â°', 'Ġber', 'thing', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġber', 'thing', 'Ġport', 'Ġunity', 'Ġn', 'ad', 'ir', 'Ġr', 'ms', 'Ġcapture', 'Ġaug', 'ust', 'Ġ09', 'Ġut', 'c', 'Ġber', 'thing', 'Ġdate', 'Ġaug', 'ust', 'Ġut', 'c', 'Ġtime', 'Ġb', 'ert', 'hed', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġprogress', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġmission', 'Ġpatch', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġcy', 'gn', 'us', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġng', 'Ġnineteenth', 'Ġflight', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġrobotic', 'Ġres', 'upp', 'ly', 'Ġspacecraft', 'Ġcy', 'gn', 'us', 'Ġeighteenth', 'Ġflight', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġcontract', 'Ġn', 'asa', 'Ġmission', 'Ġlaunched', 'Ġaug', 'ust', 'Ġ00', 'Ġeighth', 'Ġlaunch', 'Ġcy', 'gn', 'us', 'Ġcontract', 'Ġorbital', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'Ġn', 'asa', 'Ġjointly', 'Ġdeveloped', 'Ġnew', 'Ġspace', 'Ġtransportation', 'Ġsystem', 'Ġprovide', 'Ġcommercial', 'Ġcargo', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'c', 'ots', 'Ġprogram', 'Ġorbital', 'Ġdesigned', 'Ġacquired', 'Ġbuilt', 'Ġassembled', 'Ġcomponents', 'Ġant', 'ares', 'Ġmedium', 'class', 'Ġlaunch', 'Ġvehicle', 'Ġcy', 'gn', 'us', 'Ġadvanced', 'Ġspacecraft', 'Ġusing', 'Ġpress', 'urized', 'Ġcargo', 'Ġmodule', 'Ġprovided', 'Ġindustrial', 'Ġpartner', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġservice', 'Ġmodule', 'Ġbased', 'Ġorbital', 'Ġge', 'ost']</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>['ï', '¬', 'Ĥ', 'Ġpartner', 'Ġupgraded', 'Ġant', 'ares', 'Ġspac', 'en', 'ews', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġev', 'ans', 'Ġben', 'Ġfe', 'b', 'ruary', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġgreen', 'lights', 'Ġtwo', 'Ġcy', 'gn', 'us', 'Ġmissions', 'Ġng', 'Ġarrives', 'Ġspace', 'Ġstation', 'Ġameric', 'asp', 'ace', 'Ġretrieved', 'Ġapr', 'il', 'Ġle', 'one', 'Ġdan', 'Ġaug', 'ust', 'n', 'asa', 'Ġorders', 'Ġtwo', 'Ġiss', 'Ġcargo', 'Ġmissions', 'Ġorbital', 'ht', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġapr', 'il', 'ng', 'Ġmission', 'Ġe', 'hand', 'pdf', 'press', 'Ġrelease', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġretrieved', 'Ġj', 'uly', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġiss', 'Ġprogram', 'ï', '¬', 'ģ', 'ce', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġmars', 'Ġke', 'lli', 'Ġj', 'uly', 'view', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', "'s", 'th', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġmission', 'mission', 'Ġn', 'asa', 'Ġretrieved', 'Ġaug', 'ust', 'exper', 'iment', 'Ġdetails', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'fac', 'ility', 'Ġdetails', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'Ġk', 'ovo', 'ael', 'Ġj', 'uly', 'Ġcell', '02', 'space', 'x', ')"', 'Ġn', 'asa', 'Ġretrieved', 'Ġaug', 'ust', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġn', 'asa', 'Ġpage', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['ar', 'Ġsatellite', 'Ġbus', 'Ġflight', 'Ġused', 'Ġlast', 'Ġremaining', 'Ġant', 'ares', 'Ġseries', 'Ġconstructed', 'Ġu', 'k', 'raine', 'Ġuses', 'Ġr', 'ussian', 'Ġmotors', 'Ġnext', 'Ġthree', 'Ġcy', 'gn', 'us', 'Ġmissions', 'Ġuse', 'Ġfal', 'con', 'Ġsubsequent', 'Ġmission', 'Ġuse', 'Ġnext', 'generation', 'Ġant', 'ares', 'Ġseries', 'Ġdepend', 'Ġu', 'k', 'rain', 'ian', 'Ġr', 'ussian', 'Ġparts', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġeighth', 'Ġcy', 'gn', 'us', 'Ġmission', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġcontract', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'Ġconfirmed', 'Ġfe', 'b', 'ruary', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġtur', 'aly', 'Ġfabric', 'ate', 'Ġtwo', 'Ġadditional', 'Ġpress', 'urized', 'Ġcargo', 'Ġmodules', 'Ġpair', 'Ġforthcoming', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'Ġmissions', 'Ġcurrent', 'Ġplans', 'Ġtwo', 'Ġadditional', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġdesignated', 'Ġng', 'Ġng', 'Ġhistory', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġproduction', 'Ġintegration', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġperformed', 'Ġdull', 'es', 'Ġvirgin', 'ia', 'Ġcy', 'gn', 'us', 'Ġservice', 'Ġmodule', 'ated', 'Ġpress', 'urized', 'Ġcargo', 'Ġmodule', 'Ġlaunch', 'Ġsite', 'Ġmission', 'Ġoperations', 'Ġconducted', 'Ġcontrol', 'Ġcenters', 'Ġdull', 'es', 'Ġvirgin', 'ia', 'Ġh', 'ouston', 'Ġtex', 'Ġfour', 'teenth', 'Ġflight', 'Ġenhanced', 'sized', 'Ġcy', 'gn', 'us', 'Ġcy', 'gn', 'us', 'Ġspacecraft', 'Ġloaded', 'Ġcargo', 'Ġnew', 'Ġexperiments', 'Ġarriving', 'Ġorbiting', 'Ġlaboratory', 'Ġinspire', 'Ġfuture', 'Ġscientists', 'Ġexplorers', 'Ġprovide', 'Ġvaluable', 'Ġinsight', 'Ġresearchers', 'Ġn', 'asa', 'Ġscientific', 'Ġresearch', 'Ġstudies', 'Ġinnovative', 'Ġparalysis', 'Ġtherapy', 'Ġenabling', 'Ġneuro', 'reg', 'ener', 'ation', 'ne', 'uron', 'ix', 'Ġsponsored', 'Ġiss', 'Ġnational', 'Ġlab', 'Ġdemonstrates', 'Ġformation', 'Ġneuron', 'Ġcell', 'Ġcultures', 'Ġmicro', 'gravity', 'Ġtests', 'Ġneuron', 'spe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġgene', 'Ġtherapy', 'Ġgene', 'Ġtherapy', 'Ġshows', 'Ġpromise', 'Ġpotential', 'Ġtreatment', 'Ġpeople', 'Ġparalysis', 'Ġneurological', 'Ġdiseases', 'Ġal', 'z', 'heimer', 'âĢ', 'Ļ', 'Ġpark', 'inson', 'âĢ', 'Ļ', 'Ġmodels', 'Ġneeded', 'Ġtest', 'Ġtherapies', 'Ġcannot', 'Ġgrown', 'Ġearth', 'âĢ', 'Ļ', 'Ġgravity', 'Ġcreating', 'Ġcell', 'Ġcultures', 'Ġmicro', 'gravity', 'Ġcould', 'Ġprovide', 'Ġplatform', 'Ġdrug', 'Ġdiscovery', 'Ġgene', 'Ġtherapy', 'Ġtesting', 'Ġspacecraft', 'Ġfire', 'Ġexperiments', 'saf', 'ï', '¬', 'ģ', 'vi', 'Ġunderstanding', 'Ġï', '¬', 'ģ', 'Ġbehaves']</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>['Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġflight', 'Ġcarrying', 'Ġorb', 'comm', 'Ġsatellites', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġrecovered', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfollowing', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsuccessful', 'Ġfal', 'con', 'Ġlanding', 'Ġfunction', 'Ġpartially', 'Ġreusable', 'Ġorbital', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'usable', ')[', 'Ġsize', 'Ġheight', 'Ġft', 'Ġpayload', 'Ġfair', 'ing', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'also', 'Ġknown', 'Ġfal', 'con', 'Ġvariants', 'Ġblock', 'Ġblock', 'Ġpartially', 'Ġreusable', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġdesigned', 'Ġmanufactured', 'Ġspace', 'x', 'Ġfirst', 'Ġdesigned', 'âĢĵ', 'Ġfirst', 'Ġlaunch', 'Ġoperations', 'Ġde', 'cember', 'mber', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġperformed', 'Ġlaunches', 'Ġwithout', 'Ġfailures', 'Ġbased', 'Ġle', 'w', 'Ġpoint', 'Ġestimate', 'Ġreliability', 'Ġrocket', 'Ġreliable', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġcurrently', 'Ġoperation', 'Ġde', 'cember', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġfal', 'con', 'Ġfamily', 'Ġfirst', 'Ġlaunch', 'Ġvehicle', 'Ġorbital', 'Ġtrajectory', 'Ġsuccessfully', 'Ġvertically', 'Ġland', 'Ġfirst', 'Ġstage', 'Ġlanding', 'Ġfollowed', 'Ġtechnology', 'Ġdevelopment', 'Ġprogram', 'Ġconducted', 'Ġrequired', 'Ġtechnology', 'Ġadvances', 'Ġlanding', 'Ġlegs', 'Ġpioneered', 'Ġfal', 'con', 'Ġversion', 'Ġversion', 'Ġnever', 'Ġlanded', 'Ġintact', 'Ġstarting', 'Ġpreviously', 'Ġflown', 'Ġfirst', 'stage', 'Ġboosters', 'Ġreused', 'Ġlaunch', 'Ġnew', 'Ġpayload', 'Ġorbit', 'Ġquickly', 'Ġbecame', 'Ġroutine', 'Ġhalf', 'Ġfal', 'con', 'Ġflights', 'Ġreused', 'Ġbooster', 'Ġfraction', 'Ġreused', 'Ġboosters', 'Ġincreased', '%.', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġsubstantial', 'Ġupgrade', 'Ġprevious', 'Ġfal', 'con', 'Ġrocket', 'Ġflew', 'Ġlast', 'Ġmission', 'Ġjan', 'uary', 'rated', 'Ġfirst', 'Ġsecond', 'stage', 'Ġengines', 'Ġlarger', 'Ġsecond', 'stage', 'Ġpropell', 'ant', 'Ġtank', 'Ġpropell', 'ant', 'Ġdens', 'ification', 'Ġvehicle', 'Ġcarry', 'Ġsubstantial', 'Ġpayload', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġperform', 'Ġprop', 'ulsive', 'Ġlanding', 'Ġrecovery', 'Ġprincipal', 'Ġobjective', 'Ġnew', 'Ġdesign', 'Ġfacilitate', 'Ġbooster', 'us', 'ability', 'Ġlarger', 'Ġrange']</t>
+          <t>['Ġspace', 'Ġvital', 'Ġdeveloping', 'Ġï', '¬', 'ģ', 'Ġprevention', 'Ġï', '¬', 'ģ', 'Ġsuppression', 'Ġmethods', 'Ġï', '¬', 'Ĥ', 'ame', 'related', 'Ġexperiments', 'ï', '¬', 'ģ', 'cult', 'Ġconduct', 'Ġaboard', 'Ġoccupied', 'Ġspacecraft', 'Ġspacecraft', 'Ġfire', 'Ġexperiments', 'saf', 'ï', '¬', 'ģ', 'Ġuse', 'Ġcy', 'gn', 'us', 'Ġres', 'upp', 'ly', 'Ġcraft', 'Ġleaves', 'Ġspace', 'Ġstation', 'Ġremove', 'Ġrisk', 'Ġcrew', 'Ġspacecraft', 'Ġsaf', 'ï', '¬', 'ģ', 'vi', 'Ġlast', 'Ġseries', 'Ġbuilding', 'Ġprevious', 'Ġresults', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'amm', 'ability', 'Ġdifferent', 'Ġlevels', 'Ġdemonstrate', 'Ġï', '¬', 'ģ', 'Ġdetection', 'Ġmonitoring', 'Ġwell', 'Ġpost', 'ï', '¬', 'ģ', 'Ġcleanup', 'Ġcapabilities', 'Ġexploration', 'Ġpot', 'able', 'Ġwater', 'Ġdispens', 'er', 'expl', 'oration', 'Ġuses', 'Ġadvanced', 'Ġwater', 'Ġsan', 'ization', 'Ġmicrobial', 'Ġgrowth', 'Ġreduction', 'Ġmethods', 'Ġdisp', 'enses', 'Ġhot', 'Ġwater', 'Ġimproved', 'Ġversion', 'Ġsystem', 'Ġlaunched', 'Ġfall', 'Ġsponsored', 'Ġn', 'asa', 'Ġbiological', 'Ġphysical', 'Ġsciences', 'Ġdivision', 'Ġstudy', 'Ġaimed', 'Ġunderstanding', 'Ġorganisms', 'Ġevolve', 'Ġadapt', 'Ġspace', 'Ġenvironment', 'Ġexperiment', 'Ġb', 'ac', 'illus', 'Ġsubt', 'il', 'Ġbacteria', 'Ġgrown', 'Ġspecially', 'Ġdesigned', 'Ġenvironmental', 'Ġhardware', 'Ġrange', 'Ġconditions', 'Ġallowing', 'Ġresearchers', 'Ġinvestigate', 'Ġwhether', 'Ġadaptation', 'Ġprocess', 'Ġoccurs', 'Ġdifferently', 'Ġmicro', 'gravity', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġenvironment', 'Ġwhole', 'Ġrepeat', 'Ġunc', 'rew', 'ed', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġspacecraft', 'Ġmanifest', 'Ġresearch', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġcy', 'gn', 'us', 'Ġng', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'launch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġj', 'une', 'orb', 'ital', 'Ġlooks', 'Ġahead', 'Ġcy', 'gn', 'us', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġant', 'ares', 'Ġcommercial', 'Ġmarket', 'Ġres', 'commercial', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'north', 'rop', 'Ġgr', 'um', 'man', 'optim', 'istic', 'Ġreceive', 'Ġn', 'asa', 'Ġcargo', 'Ġmission', 'Ġorders', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'cy', 'gn', 'us', 'Ġspacecraft', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġfire']</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>['Ġmissions', 'Ġincluding', 'Ġdelivery', 'Ġlarge', 'Ġcomm', 'ats', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġlike', 'Ġearlier', 'Ġversions', 'Ġfal', 'con', 'Ġlike', 'Ġsat', 'urn', 'Ġseries', 'Ġap', 'ollo', 'Ġprogram', 'Ġpresence', 'Ġmultiple', 'Ġfirst', 'stage', 'Ġengines', 'Ġallow', 'Ġmission', 'Ġcompletion', 'Ġeven', 'Ġone', 'Ġfirst', 'stage', 'Ġengines', 'Ġfails', 'Ġmid', 'flight', 'Ġdesign', 'Ġmod', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġdiameter', 'Ġmass', '000', '000', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġle', 'Â°', 'Ġmass', 'Ġexpend', 'able', 'Ġreusable', 'Ġpayload', 'Ġg', 'Â°', 'Ġmass', 'Ġexpend', 'able', 'Ġreusable', '000', '000', 'Ġpayload', 'Ġmars', 'Ġmass', '020', 'Ġassociated', 'Ġrockets', 'Ġfamily', 'Ġfal', 'con', 'Ġderivative', 'Ġwork', 'Ġfal', 'con', 'Ġheavy', 'Ġcomparable', 'las', 'Ġlong', 'Ġmarch', 'b', 'e', 'Ġpro', 'ton', 'ri', 'ane', 'Ġes', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġv', 'enberg', 'Ġk', 'enn', 'edy', 'Ġtotal', 'Ġlaunches', 'Ġleft', 'Ġright', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġthree', 'Ġlaunch', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġfal', 'con', 'Ġthree', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġfal', 'con', 'full', 'Ġthrust', 'Ġtwo', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġfal', 'con', 'Ġblock', 'Ġfal', 'con', 'Ġheavy', 'Ġthird', 'Ġversion', 'Ġfal', 'con', 'Ġdeveloped', 'âĢĵ', 'Ġmade', 'Ġmaiden', 'Ġflight', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmodified', 'Ġreusable', 'Ġvariant', 'Ġfal', 'con', 'Ġfamily', 'Ġcapabilities', 'Ġexceed', 'Ġfal', 'con', 'Ġincluding', 'Ġability', 'land', 'Ġfirst', 'Ġstage', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġmissions', 'Ġdrone', 'Ġship', '"[', 'Ġrocket', 'Ġdesigned', 'Ġusing', 'Ġsystems', 'Ġsoftware', 'Ġtechnology', 'Ġdeveloped', 'Ġpart', 'Ġspace', 'x', 'Ġreusable', 'Ġlaunch', 'Ġsystem', 'Ġdevelopment', 'Ġprogram', 'Ġprivate', 'Ġinitiative', 'Ġspace', 'x', 'Ġfacilitate', 'Ġrapid', 'us', 'ability', 'Ġfirst', 'âĢĵ', 'Ġlong', 'Ġterm', 'Ġsecond', 'âĢĶ', 'st', 'ages', 'Ġspace', 'x', 'Ġlaunch', 'Ġvehicles', 'Ġvarious', 'Ġtechnologies', 'Ġtested', 'Ġgrass', 'ho', 'pper', 'Ġtechnology', 'Ġdemonstr', 'ator', 'Ġwell', 'Ġseveral', 'Ġflights', 'Ġfal', 'con', 'Ġpost', 'mission', 'Ġbooster', 'Ġcontrolled']</t>
+          <t>['ï', '¬', 'Ĥ', 'Ġpartner', 'Ġupgraded', 'Ġant', 'ares', 'Ġspac', 'en', 'ews', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġev', 'ans', 'Ġben', 'Ġfe', 'b', 'ruary', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġgreen', 'lights', 'Ġtwo', 'Ġcy', 'gn', 'us', 'Ġmissions', 'Ġng', 'Ġarrives', 'Ġspace', 'Ġstation', 'Ġameric', 'asp', 'ace', 'Ġretrieved', 'Ġapr', 'il', 'Ġle', 'one', 'Ġdan', 'Ġaug', 'ust', 'n', 'asa', 'Ġorders', 'Ġtwo', 'Ġiss', 'Ġcargo', 'Ġmissions', 'Ġorbital', 'ht', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġapr', 'il', 'ng', 'Ġmission', 'Ġe', 'hand', 'pdf', 'press', 'Ġrelease', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġretrieved', 'Ġj', 'uly', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġiss', 'Ġprogram', 'ï', '¬', 'ģ', 'ce', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġmars', 'Ġke', 'lli', 'Ġj', 'uly', 'view', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', "'s", 'th', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġmission', 'mission', 'Ġn', 'asa', 'Ġretrieved', 'Ġaug', 'ust', 'exper', 'iment', 'Ġdetails', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'fac', 'ility', 'Ġdetails', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'Ġk', 'ovo', 'ael', 'Ġj', 'uly', 'Ġcell', '02', 'space', 'x', ')"', 'Ġn', 'asa', 'Ġretrieved', 'Ġaug', 'ust', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġn', 'asa', 'Ġpage', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>['des', 'cent', 'Ġtests', 'Ġconducted', 'Ġspace', 'x', 'Ġmade', 'Ġnumber', 'Ġmodifications', 'Ġexisting', 'Ġfal', 'con', 'Ġnew', 'Ġrocket', 'Ġknown', 'Ġinternally', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġalso', 'Ġknown', 'Ġfal', 'con', 'Ġenhanced', 'Ġfal', 'con', 'Ġfull', 'performance', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġupgrade', 'Ġprincipal', 'Ġobjective', 'Ġnew', 'Ġdesign', 'Ġfacilitate', 'Ġbooster', 'us', 'ability', 'Ġlarger', 'Ġrange', 'Ġmissions', 'Ġincluding', 'Ġdelivery', 'Ġlarge', 'Ġcomm', 'ats', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġmodifications', 'Ġupgraded', 'Ġversion', 'Ġinclude', 'Ġliquid', 'Ġsub', 'cool', 'ed', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠÂ°', 'r', 'ĠâĪĴ', 'ĠÂ°', 'f', 'Ġcooled', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠÂ°', 'r', 'Ġdensity', 'owing', 'Ġfuel', 'Ġoxid', 'izer', 'Ġstored', 'Ġgiven', 'Ġtank', 'Ġvolume', 'Ġwell', 'Ġincreasing', 'Ġpropell', 'ant', 'Ġmass', 'Ġï', '¬', 'Ĥ', 'ow', 'Ġturb', 'op', 'umps', 'Ġincreasing', 'Ġthrust', 'Ġupgraded', 'Ġstructure', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġlonger', 'Ġsecond', 'Ġstage', 'Ġpropell', 'ant', 'Ġtanks', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġsuccess', 'es', 'Ġnotable', 'Ġoutcome', 'destroy', 'ed', 'Ġlaunch', 'Ġland', 'ings', 'Ġattempts', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġactive', 'Ġtype', 'Ġpassengers', 'c', 'argo', 'Ġdragon', 'Ġcapsule', 'Ġdragon', 'Ġcrew', 'Ġcapsule', 'Ġir', 'idium', 'Ġnext', 'Ġï', '¬', 'Ĥ', 'e', 'et', 'Ġz', 'uma', 'Ġbo', 'e', 'ing', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'ess', 'res', 'heet', 'Ġland', 'er', 'Ġstar', 'link', 'Ġrad', 'ars', 'Ġconstellation', 'Ġsent', 'inel', 'ichael', 'Ġfre', 'il', 'ich', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', 'Ġkn', '000', 'Ġvacuum', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġseconds', 'Ġvacuum', 'Ġseconds', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġchilled', 'Ġsecond', 'large', 'Ġnozzle', ')[', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġlonger', 'Ġstronger', 'Ġinter', 'stage', 'Ġhousing', 'Ġsecond', 'Ġstage', 'Ġengine', 'Ġnozzle', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġattitude', 'Ġthr', 'usters', 'Ġcenter', 'Ġpus', 'Ġadded', 'Ġstage', 'Ġseparation']</t>
+          <t>['Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlaunches', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġfunction', 'Ġorbital', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġus', 'Ġmillion', 'Ġn', 'ro', 'Ġus', 'Ġmillion', 'Ġsize', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġwidth', 'Ġft', 'Ġmass', '000', '000', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġdelta', 'Ġiv', 'Ġheavy', 'elta', 'h', 'Ġexpend', 'able', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġlargest', 'Ġtype', 'Ġdelta', 'Ġiv', 'Ġfamily', 'Ġworld', "'s", 'Ġthird', 'Ġhighest', 'capacity', 'Ġlaunch', 'Ġvehicle', 'Ġoperation', 'Ġbehind', 'Ġn', 'asa', "'s", 'Ġspace', 'Ġlaunch', 'Ġsystem', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġclosely', 'Ġfollowed', 'Ġcasc', "'s", 'Ġlong', 'Ġmarch', 'Ġmanufactured', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġfirst', 'Ġlaunched', 'Ġu', 'la', 'Ġretire', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġj', 'une', 'Ġone', 'Ġflight', 'Ġremains', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġconsists', 'Ġcentral', 'Ġcommon', 'Ġbooster', 'Ġcore', 'Ġtwo', 'Ġadditional', 'Ġliquid', 'Ġrocket', 'Ġboosters', 'Ġinstead', 'Ġsolid', 'Ġrocket', 'Ġmotors', 'Ġused', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġversions', 'Ġlift', 'Ġthree', 'Ġcores', 'Ġoperate', 'Ġfull', 'Ġthrust', 'Ġseconds', 'Ġlater', 'Ġcenter', 'Ġcore', 'Ġthrott', 'les', 'Ġconserve', 'Ġfuel', 'Ġbooster', 'Ġseparation', 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġburn', 'Ġseconds', 'Ġlaunch', 'Ġseparated', 'Ġcore', 'Ġbooster', 'Ġthrott', 'les', 'Ġback', 'Ġfull', 'Ġthrust', 'Ġcore', 'Ġburns', 'Ġseconds', 'Ġlater', 'Ġsecond', 'Ġstage', 'Ġcompletes', 'Ġascent', 'Ġlaunch', 'Ġvehicle', 'Ġuses', 'Ġthree', 'Ġengines', 'Ġone', 'Ġcentral', 'Ġcore', 'Ġone', 'Ġbooster', 'Ġlast', 'Ġseconds', 'Ġcountdown', 'Ġhydrogen', 'Ġfuel', 'Ġflows', 'Ġengines', 'Ġupwards', 'Ġalong', 'Ġbooster', 'Ġbody', 'Ġignition', 'Ġhydrogen', 'Ġinfl', 'ames', 'Ġmaking', 'Ġcharacteristic', 'Ġfireball', 'Ġcharred', 'Ġlook', 'Ġbooster', 'Ġdelta', 'Ġiv', 'Ġline', 'Ġrockets', 'Ġdeveloped', 'Ġmc', 'nell', 'Ġdou', 'glas', 'Ġprogram', 'Ġlater', 'Ġtransferred', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġpowerful', 'Ġmember', 'Ġline', 'Ġalso', 'Ġincludes', 'Ġsmaller', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlift', 'Ġlow', 'Ġearth', 'Ġorbit']</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -1868,7 +1868,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>['Ġdesign', 'Ġevolution', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġoct', 'aw', 'eb', 'Ġupgraded', 'Ġlanding', 'Ġlegs', 'Ġmer', 'lin', 'Ġengine', 'Ġthrust', 'Ġincreased', 'Ġfull', 'th', 'rust', 'Ġvariant', 'Ġmer', 'lin', 'Ġtaking', 'Ġadvantage', 'Ġdens', 'er', 'Ġpropell', 'ants', 'Ġachieved', 'Ġsub', 'cool', 'ing', 'Ġmer', 'lin', 'Ġvacuum', 'Ġthrust', 'Ġincreased', 'Ġsub', 'cool', 'ing', 'Ġpropell', 'ants', 'Ġseveral', 'Ġsmall', 'Ġmass', 'red', 'uction', 'Ġefforts', 'Ġmodified', 'Ġdesign', 'Ġgained', 'Ġadditional', 'Ġmetres', 'Ġft', 'Ġheight', 'Ġstretching', 'Ġexactly', 'Ġmetres', 'Ġft', 'Ġincluding', 'Ġpayload', 'Ġfair', 'ing', 'Ġgaining', 'Ġoverall', 'Ġperformance', 'Ġincrease', 'Ġpercent', 'Ġnew', 'Ġfirst', 'stage', 'Ġengine', 'Ġmuch', 'Ġincreased', 'Ġthrust', 'weight', 'Ġratio', 'Ġfull', 'th', 'rust', 'Ġfirst', 'Ġstage', 'Ġbooster', 'Ġcould', 'Ġreach', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcarrying', 'Ġupper', 'Ġstage', 'Ġheavy', 'Ġsatellite', 'Ġversions', 'Ġlaunched', 'Ġincluded', 'Ġexperimental', 'Ġrecovery', 'Ġsystem', 'Ġpayload', 'Ġfair', 'ing', 'Ġhalves', 'Ġmarch', 'Ġspace', 'x', 'Ġfirst', 'Ġtime', 'Ġrecovered', 'Ġfair', 'ing', 'es', 'Ġmission', 'Ġthanks', 'Ġthr', 'usters', 'Ġsteer', 'able', 'Ġparachute', 'Ġhelping', 'Ġglide', 'Ġtowards', 'Ġgentle', 'Ġtouchdown', 'Ġwater', 'Ġj', 'une', 'Ġflight', 'ir', 'idium', 'Ġnext', 'âĢĵ', 'Ġaluminum', 'Ġgrid', 'Ġfins', 'Ġreplaced', 'Ġtitanium', 'Ġversions', 'Ġimprove', 'Ġcontrol', 'Ġauthority', 'Ġbetter', 'Ġcope', 'Ġheat', 'entry', 'Ġfollowing', 'Ġpost', 'flight', 'Ġinspections', 'Ġel', 'Ġmus', 'k', 'Ġannounced', 'Ġnew', 'Ġgrid', 'Ġfins', 'Ġlikely', 'Ġrequire', 'Ġservice', 'Ġflights', 'Ġspace', 'x', 'Ġdeveloping', 'Ġtime', 'Ġalternative', 'Ġautonomous', 'Ġsystem', 'Ġreplace', 'Ġtraditional', 'Ġground', 'based', 'Ġsystems', 'Ġuse', 'Ġus', 'Ġlaunches', 'Ġdecades', 'Ġautonomous', 'Ġsystem', 'Ġuse', 'Ġspace', 'x', 'Ġsub', 'orb', 'ital', 'Ġtest', 'Ġflights', 'Ġtex', 'Ġflown', 'Ġparallel', 'Ġnumber', 'Ġorbital', 'Ġlaunches', 'Ġpart', 'Ġsystem', 'Ġtest', 'Ġprocess', 'Ġgain', 'Ġapproval', 'Ġuse', 'Ġoperational', 'Ġflights', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', "'s", 'Ġcr', 'Ġlaunch', 'Ġfirst', 'Ġoperational', 'Ġlaunch', 'Ġutilizing', 'Ġnew', 'Ġautonomous', 'Ġflight', 'Ġsafety', 'Ġsystem', 'af', 'ss', 'either', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', "'s", 'Ġeastern', 'Ġwestern', 'Ġranges', '."', 'Ġfollowing', 'Ġspace', 'x', 'Ġflight', 'Ġautonomous', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtermination', 'Ġsystem']</t>
+          <t>['Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', ').[', 'Ġliquid', 'fuel', 'ed', 'Ġlaunch', 'Ġvehicle', 'Ġconsisting', 'Ġupper', 'Ġstage', 'Ġone', 'Ġmain', 'Ġbooster', 'Ġtwo', 'Ġstrap', 'Ġboosters', 'Ġfirst', 'Ġlaunch', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġcarried', 'Ġboiler', 'plate', 'Ġpayload', 'Ġpartial', 'Ġfailure', 'Ġcav', 'itation', 'Ġliquid', 'oxy', 'gen', 'Ġpropell', 'ant', 'Ġlines', 'Ġcaused', 'Ġshutdown', 'Ġhistory', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġle', 'Ġmass', 'Ġpayload', 'Ġg', 'Ġmass', 'Ġassociated', 'Ġrockets', 'Ġfamily', 'Ġdelta', 'Ġcomparable', 'Ġlong', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġpro', 'ton', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġproduction', 'Ġended', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġv', 'enberg', 'Ġtotal', 'Ġlaunches', 'Ġsuccess', 'es', 'Ġpartial', 'Ġfailure', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'usa', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġj', 'une', 'Ġtype', 'Ġpassengers', 'c', 'argo', 'Ġn', 'ro', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġpayload', 'k', 'enn', 'en', 'ion', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'Ġboosters', 'Ġboosters', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', '000', '000', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġboosters', 'Ġeight', 'Ġseconds', 'Ġearly', 'Ġcore', 'Ġengine', 'Ġnine', 'Ġseconds', 'Ġearly', 'Ġresulted', 'Ġlower', 'Ġstaging', 'Ġvelocity', 'Ġsecond', 'Ġstage', 'Ġunable', 'Ġcompensate', 'Ġpayload', 'Ġleft', 'Ġlower', 'Ġintended', 'Ġorbit', 'Ġfirst', 'Ġoperational', 'Ġpayload', 'sp', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġused', 'Ġlaunch', 'Ġfive', 'Ġvisual', 'Ġelectronic', 'Ġreconnaissance', 'Ġsatellites', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'n', 'ro', 'Ġde', 'cember', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġused', 'Ġlaunch', 'Ġun', 'crew', 'ed', 'Ġtest', 'Ġflight', 'ion', 'Ġspacecraft', 'Ġdesignated', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġseveral', 'Ġdelays', 'Ġmission', 'Ġsuccessfully', 'Ġlaunched', '05', 'Ġut', 'c', 'Ġde', 'cember', 'Ġaug', 'ust', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġadditional', 'Ġstar', 'Ġthird', 'Ġstage', 'Ġused', 'Ġlaunch', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'Ġellipt', 'ical', 'Ġhel', 'oc', 'entric', 'Ġorbit']</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>['Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġseconds', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsecond', 'short', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġseconds', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġmarch', 'Ġdiscarded', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġlower', 'Ġright', 'Ġsecond', 'Ġstage', 'Ġupper', 'Ġleft', 'Ġtwo', 'Ġparts', 'Ġj', 'ett', 'ison', 'ed', 'Ġpayload', 'Ġfair', 'ing', 'Ġe', 'ch', 'ost', 'ar', 'Ġmarch', 'Ġlast', 'Ġspace', 'x', 'Ġlaunch', 'Ġutilizing', 'Ġhistoric', 'Ġsystem', 'Ġground', 'Ġrad', 'ars', 'Ġtracking', 'Ġcomputers', 'Ġpersonnel', 'Ġlaunch', 'Ġbunk', 'ers', 'Ġused', 'Ġsixty', 'Ġyears', 'Ġlaunches', 'Ġeastern', 'Ġrange', 'Ġfuture', 'Ġspace', 'x', 'Ġlaunches', 'Ġaf', 'ss', 'Ġreplaced', 'Ġground', 'based', 'Ġmission', 'Ġflight', 'Ġcontrol', 'Ġpersonnel', 'Ġequipment', 'board', 'Ġpositioning', 'Ġnavigation', 'Ġtiming', 'Ġsources', 'Ġdecision', 'Ġlogic', 'Ġbenefits', 'Ġaf', 'ss', 'Ġinclude', 'Ġincreased', 'Ġpublic', 'Ġsafety', 'Ġreduced', 'Ġreliance', 'Ġrange', 'Ġinfrastructure', 'Ġreduced', 'Ġrange', 'Ġspac', 'el', 'ift', 'Ġcost', 'Ġincreased', 'Ġschedule', 'Ġpredict', 'ability', 'Ġavailability', 'Ġoperational', 'Ġflexibility', 'Ġlaunch', 'Ġslot', 'Ġspace', 'x', 'Ġstarted', 'Ġflying', 'Ġincremental', 'Ġchanges', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġcalling', 'block', '".[', 'Ġfirst', 'Ġsecond', 'Ġstage', 'Ġmodified', 'Ġblock', 'Ġstandards', 'Ġflying', 'Ġtop', 'block', 'Ġfirst', 'Ġstage', 'Ġthree', 'Ġmissions', 'ars', 'Ġmay', 'Ġint', 'els', 'Ġj', 'uly', 'Ġblock', 'Ġdescribed', 'Ġtransition', 'Ġfull', 'Ġthrust', 'block', 'Ġfollowing', 'Ġfal', 'con', 'Ġblock', 'Ġincludes', 'Ġincremental', 'Ġengine', 'Ġthrust', 'Ġupgrades', 'Ġleading', 'Ġfinal', 'Ġthrust', 'Ġblock', 'Ġmaiden', 'Ġflight', 'Ġfull', 'Ġblock', 'Ġdesign', 'first', 'Ġsecond', 'Ġstages', 'Ġn', 'asa', 'Ġcr', 'Ġmission', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġannounced', 'Ġanother', 'Ġseries', 'Ġincremental', 'Ġimprovements', 'Ġdevelopment', 'Ġfal', 'con', 'Ġblock', 'Ġversion', 'Ġsucceeded', 'Ġtransitional', 'Ġblock', 'Ġlargest', 'Ġchanges', 'Ġblock', 'Ġblock', 'Ġhigher', 'Ġthrust', 'Ġengines', 'Ġimprovements', 'Ġlanding', 'Ġlegs', 'Ġadditionally', 'Ġnumerous', 'Ġsmall', 'Ġchanges', 'Ġhelp', 'Ġstream', 'line', 'Ġrecovery', 'us', 'ability']</t>
+          <t>['Ġmay', 'Ġfinal', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġcore', 'Ġboosters', 'Ġfinished', 'Ġconstruction', 'Ġofficially', 'Ġending', 'Ġdelta', 'Ġiv', 'Ġproduction', 'Ġmaking', 'Ġway', 'Ġvul', 'Ġlaunch', 'Ġvehicle', 'Ġcapacity', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Â°', 'Ġlow', 'Ġearth', 'Ġorbit', 'iss', 'Â°', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', '):', 'Ġcapabilities', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġpowered', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġtotal', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '04', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfirst', 'Ġstage', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġpowered', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '04', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'dc', 'ss', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', '010', 'Ġpowered', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'ge', '):', 'Ġlunar', 'Ġtransfer', 'Ġorbit', 'l', '):', '000', '000', 'Ġmars', 'Ġtransfer', 'Ġorbit', '000', '000', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdelta', 'Ġiv', 'Ġheavy', "'s", 'Ġtotal', 'Ġmass', 'Ġlaunch', 'Ġapproximately', '000', '000', 'Ġproduce', 'Ġaround', '000', '000', 'Ġthrust', 'Ġpower', 'Ġrocket', 'Ġsky', 'ward', 'Ġlif', 'ff', 'hide', 'Ġflight', 'Ġdate', 'Ġpayload', 'Ġmass']</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>['Ġfirst', 'stage', 'Ġboosters', 'Ġalterations', 'Ġfocused', 'Ġincreasing', 'Ġspeed', 'Ġproduction', 'Ġefficiency', 'us', 'ability', 'Ġspace', 'x', 'Ġaims', 'Ġfly', 'Ġblock', 'Ġbooster', 'Ġten', 'Ġtimes', 'Ġinspections', 'Ġtimes', 'Ġblock', 'Ġsecond', 'Ġstages', 'Ġbuilt', 'Ġmission', 'Ġextension', 'Ġkit', 'Ġallow', 'Ġlonger', 'Ġduration', 'Ġengine', 'Ġstarts', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġspecifications', 'Ġcharacteristics', 'Ġblock', 'Ġblock', 'Ġrocket', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġcharacteristic', 'Ġfirst', 'Ġstage', 'Ġsecond', 'Ġstage', 'Ġpayload', 'Ġfair', 'ing', 'Ġheight', 'Ġft', 'Ġft', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġft', 'Ġft', 'Ġmass', 'without', 'Ġpropell', 'ant', ')[', '000', 'Ġmass', 'Ġpropell', 'ant', 'Ġn', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġmon', 'oco', 'que', 'Ġhalves', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'Ġlithium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġaluminum', 'Ġlithium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġcarbon', 'Ġï', '¬', 'ģ', 'ber', 'Ġengines', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġvacuum', 'Ġn', 'Ġengine', 'Ġtype', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġtank', 'Ġcapacity', 'Ġk', 'eros', 'ene', 'Ġtank', 'Ġcapacity', 'Ġengine', 'Ġnozzle', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġengine', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġthrust', 'stage', 'Ġtotal', ')[', 'Ġkn', '000', 'sea', 'Ġlevel', 'Ġkn', '000', 'v', 'ac', 'uum', 'Ġpropell', 'ant', 'Ġfeed', 'Ġsystem', 'Ġturb', 'op', 'ump', 'Ġturb', 'op', 'ump', 'Ġthrottle', 'Ġcapability', 'Ġyes', 'Ġkn', 'Ġkn', '000', 'sea', 'Ġlevel', 'ï', '¼', 'ī', 'Ġyes', 'âĢĵ', 'Ġkn']</t>
+          <t>['Ġlaunch', 'Ġsite', 'Ġoutcome', 'Ġde', 'cember', 'Ġdemos', 'Ġspark', 'ie', 'Ġr', 'alph', 'ie', 'Ġpounds', 'Ġkilograms', 'Ġcape', 'aver', 'al', 'Ġpartial', 'Ġfailure', 'mber', 'sp', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'Ġpounds', 'Ġkilograms', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġjan', 'uary', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'mber', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġjan', 'uary', 'Ġk', 'enn', 'en', 'usa', 'Ġpounds', '000', 'Ġkilograms', 'Ġv', 'enberg', 'Ġsuccess', 'Ġj', 'une', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġaug', 'ust', 'Ġk', 'enn', 'en', 'usa', 'Ġpounds', '000', 'Ġkilograms', 'Ġv', 'enberg', 'Ġsuccess', 'Ġde', 'cember', 'ion', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġpounds', '000', 'Ġkilograms', 'b', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġj', 'une', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġaug', 'ust', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'c', 'Ġpounds', 'Ġkilograms', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġjan', 'uary', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġv', 'enberg', 'Ġsuccess', 'Ġde', 'cember', 'ion', 'Ġmentor', 'usa', 'Ġn', 'rol', ')[', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġapr', 'il', 'Ġk', 'enn', 'en', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġv', 'enberg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġk', 'enn', 'en', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġv', 'enberg', 'Ġsuccess', 'Ġj', 'une', 'ion', 'Ġmentor', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġmissions', 'Ġthirteen', 'Ġsixteen', 'Ġannounced', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'Ġfinal', 'Ġfive', 'Ġmissions', 'Ġincluding', 'Ġmodifications', 'Ġu', 'la', 'Ġawarded', 'Ġbillion', 'Ġus', 'Ġmillion', 'Ġper', 'Ġlaunch', 'Ġcompared', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġprice', 'Ġj', 'une']</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -1907,7 +1907,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>['000', 'âĢĵ', '000', 'v', 'ac', 'uum', 'Ġrestart', 'Ġcapability', 'Ġyes', 'Ġengines', 'Ġburns', 'Ġyes', 'Ġdual', 'Ġredundant', 'Ġte', 'ate', 'b', 'Ġpy', 'roph', 'oric', 'Ġign', 'ers', 'Ġtank', 'Ġpress', 'ur', 'ization', 'Ġheated', 'Ġhelium', 'Ġheated', 'Ġhelium', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġg', 'imb', 'aled', 'Ġengine', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġshutdown', 'Ġprocess', 'Ġcommanded', 'Ġcommanded', 'Ġn', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġp', 'ne', 'umatic', 'Ġn', 'Ġp', 'ne', 'umatic', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġrocket', 'Ġspace', 'x', 'Ġdragon', 'Ġspacecraft', 'Ġlaunch', 'Ġpad', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġuses', 'Ġmeter', 'Ġlong', 'Ġinter', 'stage', 'Ġlonger', 'Ġstronger', 'Ġfal', 'con', 'Ġinter', 'stage', 'pos', 'ite', 'Ġstructure', 'Ġconsisting', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġcore', 'Ġsurrounded', 'Ġcarbon', 'Ġfiber', 'Ġface', 'Ġsheet', 'Ġpl', 'ies', '".[', 'Ġoverall', 'Ġlength', 'Ġvehicle', 'Ġlaunch', 'Ġmeters', 'Ġtotal', 'Ġfueled', 'Ġmass', '000', 'Ġaluminium', 'l', 'ith', 'ium', 'Ġalloy', 'Ġused', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġupgraded', 'Ġvehicle', 'includes', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġsystems', 'Ġallow', 'Ġspace', 'x', 'Ġreturn', 'Ġfirst', 'Ġstage', 'Ġlaunch', 'Ġsite', 'Ġcompletion', 'Ġprimary', 'Ġmission', 'Ġrequirements', 'Ġsystems', 'Ġinclude', 'Ġfour', 'Ġdeploy', 'able', 'Ġlanding', 'Ġlegs', 'Ġlocked', 'Ġfirst', 'stage', 'Ġtank', 'Ġascent', 'Ġexcess', 'Ġpropell', 'ant', 'Ġreserved', 'Ġfal', 'con', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġoperations', 'Ġdiverted', 'Ġuse', 'Ġprimary', 'Ġmission', 'Ġobjective', 'Ġrequired', 'Ġensuring', 'Ġsufficient', 'Ġperformance', 'Ġmargins', 'Ġsuccessful', 'Ġmissions', '".[', 'Ġnominal', 'Ġpayload', 'Ġcapacity', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġkilograms', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġprice', 'Ġper', 'Ġlaunch', 'Ġmillion', 'Ġversus', 'Ġkilograms', 'Ġexpend', 'able', 'Ġfirst', 'stage', 'Ġearly', 'Ġmarch', 'Ġspace', 'x', 'Ġpricing', 'Ġpayload', 'Ġspecifications', 'Ġpublished', 'Ġexpend', 'able', 'Ġfal', 'con', 'Ġrocket', 'Ġactually', 'Ġincluded', 'Ġpercent', 'Ġperformance', 'Ġpublished', 'Ġprice', 'Ġlist', 'Ġindicated', 'Ġtime', 'Ġadditional', 'Ġperformance', 'Ġreserved', 'Ġspace', 'x', 'Ġconduct', 'us', 'ability', 'Ġtesting', 'Ġfal', 'con', 'Ġstill', 'Ġachieving']</t>
+          <t>['Ġone', 'Ġremains', 'Ġu', 'la', 'Ġret', 'ires', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlaunch', 'Ġhistory', 'Ġfuture', 'Ġlaunches', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġflight', 'Ġdate', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġmass', 'Ġorbit', 'Ġcustomer', 'Ġlaunch', 'Ġoutcome', 'Ġmarch', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġgeo', 'Ġus', 'Ġn', 'ro', 'Ġplanned', 'Ġreconnaissance', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'n', 'al', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġdelta', 'Ġrocket', 'Ġfamily', 'per', 'formed', 'Ġlower', 'Ġorbit', 'Ġplanned', 'Ġb', 'ï', '¬', 'ģ', 'cially', 'Ġreported', 'Ġmass', '000', 'Ġincludes', 'Ġlaunch', 'Ġabort', 'Ġsystem', 'las', 'Ġreach', 'Ġorbit', 'Ġexcludes', 'Ġresidual', 'Ġmass', 'Ġupper', 'Ġstage', 'Ġreach', 'Ġorbit', 'Ġlikely', 'Ġoffset', 'ting', 'Ġmass', 'Ġlas', 'Ġc', 'Ġstar', 'Ġupper', 'Ġstage', 'Ġcurrent', 'Ġlong', 'Ġmarch', 'ge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġlong', 'Ġmarch', 'low', 'Ġearth', 'Ġorbit', 'Ġlong', 'Ġmarch', 'ge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġfal', 'con', 'Ġheavy', 'Ġpro', 'ton', 'Ġdevelopment', 'Ġang', 'ara', 'ri', 'ane', 'Ġnew', 'Ġgl', 'enn', 'Ġvul', 'Ġcent', 'aur', 'Ġretired', 'Ġcancelled', 'ri', 'ane', 'ret', 'ired', 'las', 'Ġheavy', 'prop', 'osed', 'Ġnever', 'Ġdeveloped', 'Ġsat', 'urn', 'ret', 'ired', 'Ġtitan', 'ret', 'ired', 'Ġtitan', 'Ġiv', 'ret', 'ired', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġcomparison', 'Ġorbital', 'Ġrocket', 'Ġengines', 'Ġcomparison', 'Ġspace', 'Ġstation', 'Ġcargo', 'Ġvehicles', 'Ġcomparable', 'Ġvehicles', 'Ġsee', 'Ġalso', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġnational', 'Ġlaunch', 'Ġsystem', 'âĢĵ', 'Ġstudy', 'ula', 'Ġce', 'ory', 'Ġbr', 'uno', 'Ġtwitter', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'elta', 'Ġiv', 'Ġheavy', 'Ġgoes', 'Ġus', "'s", 'Ġcurrent', 'Ġfuture', 'Ġretirement', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġdelta', 'elta', 'Ġiv', 'Ġheavy', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'elta', 'Ġiv', 'Ġpayload', 'Ġplanner', "'s", 'Ġguide', 'Ġj', 'une', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'mission', 'Ġstatus', 'Ġcenter', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'Ġu', 'la', 'Ġdelta', 'heavy', 'Ġcurrently', 'Ġworld', "'s", 'Ġlargest', 'Ġrocket', 'Ġproviding', 'Ġnation', 'Ġreliable', 'Ġproven', 'Ġheavy', 'Ġlift']</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -1920,7 +1920,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>['Ġspecified', 'Ġpayload', 'Ġcustomers', 'Ġmany', 'Ġengineering', 'Ġchanges', 'Ġsupport', 'us', 'ability', 'Ġrecovery', 'Ġfirst', 'Ġstage', 'Ġmade', 'Ġearlier', 'Ġversion', 'Ġspace', 'x', 'Ġindicated', 'Ġroom', 'Ġincrease', 'Ġpayload', 'Ġperformance', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġdecrease', 'Ġlaunch', 'Ġprice', 'Ġspace', 'x', 'Ġannounced', 'Ġnumber', 'Ġmodifications', 'Ġprevious', 'Ġversion', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġnew', 'Ġrocket', 'Ġknown', 'Ġinternally', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġalso', 'Ġknown', 'Ġvariety', 'Ġnames', 'Ġincluding', 'Ġfal', 'con', 'Ġenhanced', 'Ġfal', 'con', 'Ġfull', 'performance', 'Ġfal', 'con', 'Ġupgraded', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġupgrade', 'Ġsince', 'Ġfirst', 'Ġflight', 'full', 'Ġthrust', 'Ġupgrade', '",', 'Ġspace', 'x', 'Ġreferring', 'Ġversion', 'Ġfal', 'con', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġexplained', 'Ġmarch', 'Ġnew', 'Ġdesign', 'Ġwould', 'Ġresult', 'Ġstreamlined', 'Ġproduction', 'Ġwell', 'Ġimproved', 'Ġperformance', ':[', 'Ġgot', 'Ġhigher', 'Ġthrust', 'Ġengines', 'Ġfinished', 'Ġdevelopment', "'re", 'qual', 'ification', 'Ġtesting', '].', "'re", 'Ġalso', 'Ġmodifying', 'Ġstructure', 'Ġlittle', 'Ġbit', 'Ġwant', 'Ġbuilding', 'Ġtwo', 'Ġversions', 'Ġtwo', 'Ġcores', 'Ġfactory', 'Ġwould', 'Ġgreat', 'Ġcustomer', 'Ġperspective', "'s", 'Ġincrease', 'Ġperformance', 'Ġmaybe', 'Ġlittle', 'Ġallows', 'Ġus', 'Ġland', 'Ġfirst', 'Ġstage', 'Ġg', 'Ġmissions', 'Ġdrone', 'Ġship', 'Ġdevelopment', 'Ġhistory', 'Ġdevelopment', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġaccording', 'Ġspace', 'x', 'Ġstatement', 'Ġmay', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwould', 'Ġlikely', 'Ġrequire', 'Ġrec', 'ert', 'ification', 'Ġlaunch', 'Ġunited', 'Ġstates', 'Ġgovernment', 'Ġcontracts', 'Ġshot', 'well', 'Ġstated', 'Ġiter', 'ative', 'Ġprocess', 'Ġagencies', ']"', 'Ġbecome', 'Ġquicker', 'Ġquicker', 'Ġcertify', 'Ġnew', 'Ġversions', 'Ġvehicle', '."[', 'Ġus', 'Ġair', 'Ġforce', 'Ġcertified', 'Ġupgraded', 'Ġversion', 'Ġlaunch', 'Ġvehicle', 'Ġused', 'Ġus', 'Ġmilitary', 'Ġlaunches', 'Ġjan', 'uary', 'Ġbased', 'Ġone', 'Ġsuccessful', 'Ġlaunch', 'Ġdate', 'Ġdemonstrated', 'cap', 'ability', 'Ġdesign', 'Ġproduce', 'Ġqualify', 'Ġdeliver', 'Ġnew', 'Ġlaunch', 'Ġsystem', 'Ġprovide', 'Ġmission', 'Ġassurance', 'Ġsupport', 'Ġrequired', 'Ġdeliver', 'Ġn', 'ss', 'national', 'Ġsecurity', 'Ġspace', 'Ġsatellites', 'Ġupgraded', 'Ġfirst', 'Ġstage', 'Ġbegan', 'Ġacceptance', 'Ġtesting', 'Ġspace', 'x', "'s", 'Ġmc', 'greg', 'Ġfacility']</t>
+          <t>['Ġcapability', 'Ġcountry', "'s", 'Ġnational', 'Ġsecurity', 'Ġpayload', 'Ġeast', 'Ġwest', 'Ġcoasts', '."', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġspace', 'x', "'s", 'Ġbig', 'Ġnew', 'Ġrocket', 'Ġsucceeds', 'Ġfirst', 'Ġtest', 'Ġlaunch', 'Ġl', 'Ġnew', 'ork', 'Ġtimes', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġheavy', 'Ġcapable', 'Ġlifting', '000', 'Ġpounds', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġrocket', 'Ġtoday', '."', 'bo', 'e', 'ing', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġachieves', 'Ġmajor', 'Ġtest', 'Ġobjectives', 'Ġfirst', 'Ġflight', 'Ġarchived', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġbo', 'e', 'ing', 'Ġaccessed', 'Ġmarch', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġaug', 'ust', 'ula', 'Ġlaunch', 'Ġdelta', 'Ġheavy', 'th', 'Ġmission', 'Ġfour', 'Ġgo', 'Ġrocket', 'Ġretired', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'elta', 'heavy', 'Ġlikely', 'Ġheading', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġtop', 'Ġsecret', 'Ġpayload', 'space', 'ï', '¬', 'Ĥ', 'igh', 'Ġad', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġer', 'ic', 'Ġber', 'ger', 'Ġjan', 'uary', 'Ġmassive', 'Ġrocket', 'Ġcreates', 'Ġï', '¬', 'ģ', 'ball', 'Ġlaunches', "'s", 'Ġdesign', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġapr', 'il', 'elta', 'Ġiv', 'Ġheavy', 'Ġpowerful', 'Ġlaunch', 'Ġvehicle', 'Ġspace', 'Ġretrieved', 'Ġj', 'uly', 'elta', 'heavy', 'Ġinvestigation', 'Ġident', 'ï', '¬', 'ģ', 'es', 'Ġrocket', "'s", 'Ġproblem', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'second', 'Ġstage', 'Ġign', 'ites', 'Ġfirst', 'Ġstage', 'Ġfalls', 'Ġaway', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'elta', 'Ġiv', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'Ġker', 'olar', 'pro', 'Ġul', 'al', 'aunch', 'Ġretrieved', 'Ġde', 'cember', 'ula', "'s", 'Ġdelta', 'Ġrocket', 'Ġassembly', 'Ġline', 'Ġfalls', 'Ġsilent', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġreferences', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'elta', 'Ġiv', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġj', 'une', 'j', 'une', 'pdf', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'une', 'Ġpp']</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>['Ġse', 'pt', 'ember', 'Ġfirst', 'Ġtwo', 'Ġstatic', 'Ġfire', 'Ġtests', 'Ġcompleted', 'Ġse', 'pt', 'ember', 'Ġincluded', 'Ġsub', 'cool', 'ed', 'Ġpropell', 'ant', 'Ġimproved', 'Ġmer', 'lin', 'Ġengines', 'Ġrocket', 'Ġreached', 'Ġfull', 'Ġthrottle', 'Ġstatic', 'Ġfire', 'Ġscheduled', 'Ġlaunch', 'Ġearlier', 'mber', 'es', '.,', 'Ġsatellite', 'Ġowner', 'Ġoperator', 'Ġannounced', 'Ġplans', 'Ġfe', 'b', 'ruary', 'Ġlaunch', 'Ġsatellite', 'Ġfirst', 'Ġflight', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġevent', 'Ġspace', 'x', 'Ġelected', 'Ġlaunch', 'Ġsecond', 'Ġflight', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġorb', 'comm', 'Ġsecond', 'Ġconstellation', 'Ġfirst', 'Ġflight', 'Ġch', 'ris', 'Ġber', 'gin', 'Ġnas', 'asp', 'ace', 'flight', 'Ġexplained', 'Ġrequired', 'Ġcomplicated', 'Ġsecond', 'stage', 'Ġburn', 'Ġprofile', 'Ġinvolving', 'Ġone', 'Ġrestart', 'Ġsecond', 'stage', 'Ġengine', 'Ġorb', 'comm', 'Ġmission', 'Ġwould', 'allow', 'Ġsecond', 'Ġstage', 'Ġconduct', 'Ġadditional', 'Ġtesting', 'Ġahead', 'Ġtaxing', 'Ġmission', '."[', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġcompleted', 'Ġmaiden', 'Ġflight', 'Ġde', 'cember', 'Ġcarrying', 'Ġorb', 'comm', 'atellite', 'Ġpayload', 'Ġorbit', 'Ġlanding', 'Ġrocket', "'s", 'Ġfirst', 'Ġstage', 'Ġintact', 'Ġspace', 'x', "'s", 'Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġsecond', 'Ġmission', 'Ġoccurred', 'Ġmarch', 'mber', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġflown', 'Ġmissions', 'Ġsuccess', 'Ġrate', '%.', 'Ġfirst', 'Ġstage', 'Ġrecovered', 'Ġone', 'Ġrocket', 'Ġdestroyed', 'Ġpre', 'launch', 'Ġtests', 'Ġcounted', 'Ġone', 'Ġflown', 'Ġmissions', 'Ġse', 'pt', 'ember', 'Ġrocket', 'Ġcarrying', 'Ġspace', "'s", 'Ġexploded', 'Ġlaunch', 'pad', 'launch', 'Ġcomplex', 'Ġfueling', 'Ġpreparation', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġtest', 'Ġconducted', 'Ġpreparation', 'Ġlaunch', 'th', 'Ġfal', 'con', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġvehicle', 'Ġpayload', 'Ġdestroyed', 'Ġexplosion', 'Ġsubsequent', 'Ġinvestigation', 'Ġshowed', 'Ġroot', 'Ġcause', 'Ġignition', 'Ġsolid', 'Ġliquid', 'Ġcompressed', 'Ġlayers', 'Ġimmersed', 'Ġhelium', 'Ġtanks', 'Ġcarbon', 'f', 'iber', 'Ġwra', 'ppings', 'Ġresolve', 'Ġissue', 'Ġflights', 'Ġspace', 'x', 'Ġmade', 'Ġdesign', 'Ġchanges', 'Ġtanks', 'Ġchanges', 'Ġfueling', 'Ġprocedure', 'Ġtesting', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlaunch', 'Ġhistory', 'Ġlaunch', 'Ġlanding', 'Ġsites', 'Ġlaunch', 'Ġsites', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia']</t>
+          <t>['âĢĵ', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'elta', 'Ġiv', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġretrieved', 'Ġj', 'uly', 'Ġray', 'Ġde', 'cember', 'Ġheavy', 'Ġtriple', 'sized', 'Ġdelta', 'Ġrocket', 'Ġdebut', 'web', 'arc', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġview', 'html', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'live', 'Ġcoverage', 'Ġlaunch', 'Ġdelta', 'heavy', 'Ġrocket', 'Ġset', 'Ġearly', 'aturday', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġk', 'bs', 'Ġgun', 'ter', 'elta', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġmarch', 'n', 'asa', 'ion', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġpress', 'Ġkit', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġp', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'launch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'launch', 'Ġmission', 'Ġexecution', 'Ġforecast', 'th', 'Ġweather', 'Ġsquadron', 'Ġpat', 'rick', 'Ġair', 'Ġforce', 'Ġbase', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'elta', 'heavy', 'Ġrocket', 'Ġlifts', 'Ġn', 'ro', 'Ġsatellite', 'sp', 'ac', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġray', 'Ġj', 'une', 'sur', 'illance', 'Ġsatellite', 'Ġlaunching', 'Ġth', 'ursday', 'Ġatop', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġrocket', 'rocket', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'air', 'Ġforce', 'Ġawards', 'Ġu', 'la', 'Ġus', 'Ġbillion', 'Ġcontract', 'Ġcomplete', 'Ġï', '¬', 'ģ', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġn', 'ro', 'Ġmissions', 'h', 'missions', 'Ġspac', 'en', 'ews', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'n', 'ssl', 'Ġphase', 'Ġindustry', 'Ġday', 'Ġspace', 'Ġsystems', 'Ġcommand', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġdelta', 'Ġiv', 'Ġbooster', 'Ġintegration', 'Ġanother', 'Ġstep', 'Ġtoward', 'Ġfirst', 'ion', 'Ġflight', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>['Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġspace', 'x', 'Ġfirst', 'Ġused', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġrockets', 'Ġlike', 'Ġpredecessor', 'Ġfal', 'con', 'Ġfollowing', 'Ġaccident', 'Ġlaunches', 'Ġeast', 'Ġcoast', 'Ġswitched', 'Ġrefurb', 'ished', 'Ġpad', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġleased', 'Ġarchitectural', 'Ġengineering', 'Ġdesign', 'Ġwork', 'Ġchanges', 'Ġbegun', 'Ġcontract', 'Ġlease', 'Ġpad', 'Ġn', 'asa', 'Ġsigned', 'Ġapr', 'il', 'Ġconstruction', 'Ġcomm', 'encing', 'Ġlater', 'Ġincluding', 'Ġbuilding', 'Ġlarge', 'Ġhorizontal', 'Ġintegration', 'Ġfacility', 'h', 'Ġorder', 'Ġhouse', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicles', 'Ġassociated', 'Ġhardware', 'Ġpayload', 'Ġprocessing', 'Ġfirst', 'Ġlaunch', 'Ġoccurred', 'Ġfe', 'b', 'ruary', 'Ġcr', 'Ġmission', 'Ġcrew', 'Ġaccess', 'Ġarm', 'Ġwhite', 'Ġroom', 'Ġwork', 'Ġstill', 'Ġneed', 'Ġcompleted', 'Ġcrew', 'ed', 'Ġlaunches', 'Ġspace', 'x', 'Ġdragon', 'Ġcapsule', 'Ġscheduled', 'Ġadditional', 'Ġprivate', 'Ġlaunch', 'Ġsite', 'Ġintended', 'Ġsolely', 'Ġcommercial', 'Ġlaunches', 'Ġplanned', 'Ġb', 'oca', 'Ġch', 'ica', 'Ġvillage', 'Ġnear', 'Ġbrown', 'ville', 'Ġtex', 'Ġfollowing', 'Ġmulti', 'state', 'Ġevaluation', 'Ġprocess', 'âĢĵ', 'mid', 'Ġlooking', 'Ġfl', 'ida', 'Ġge', 'org', 'ia', 'Ġpu', 'erto', 'Ġr', 'ico', 'Ġhowever', 'Ġfocus', 'Ġsite', 'Ġchanged', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġv', 'ol', 'Ġtest', 'Ġflights', 'Ġsubsc', 'ale', 'Ġstarship', 'Ġho', 'pper', 'Ġtest', 'Ġvehicle', 'Ġunlikely', 'Ġever', 'Ġused', 'Ġfal', 'con', 'Ġheavy', 'Ġflights', 'Ġcurrent', 'Ġlaunch', 'Ġpads', 'Ġprovide', 'Ġenough', 'Ġlaunch', 'Ġcapability', 'Ġspace', 'x', 'Ġcompleted', 'Ġconstruction', 'Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġknown', 'Ġzone', 'Ġconsisting', 'Ġpad', 'Ġfeet', 'Ġdiameter', 'Ġfirst', 'Ġused', 'Ġde', 'cember', 'Ġsuccessful', 'Ġlanding', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlanding', 'Ġfirst', 'Ġoverall', 'Ġsuccessful', 'Ġfal', 'con', 'Ġthird', 'Ġlanding', 'Ġattempt', 'Ġhard', 'Ġsurface', 'Ġj', 'une', 'Ġone', 'Ġlanding', 'Ġattempt', 'Ġfailed', 'Ġbooster', 'Ġlanded', 'Ġoffshore', 'Ġfollowing', 'Ġdays', 'Ġtowed', 'Ġback', 'Ġport', 'aver', 'al', 'Ġraised', 'Ġwater', 'Ġusing', 'Ġtwo', 'Ġcr', 'anes', 'Ġbrought', 'Ġback', 'Ġspace', 'x', 'Ġhangar', 'Ġdirectly', 'Ġnext', 'Ġspace', 'x', 'Ġconstructed', 'Ġallow']</t>
+          <t>['Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġlifting', 'Ġcarrying', 'Ġfunction', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġmillion', ')[', 'Ġsize', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġmass', 'Ġft', '000', '000', '000', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', 'Ġft', '000', 'Ġexpended', 'Ġfal', 'con', 'Ġrocket', 'Ġfamily', 'Ġleft', 'Ġright', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġblock', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġpartially', 'Ġreusable', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcarry', 'Ġcargo', 'Ġcrew', 'Ġearth', 'Ġorbit', 'Ġdesigned', 'Ġmanufactured', 'Ġlaunched', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġspace', 'x', 'Ġalso', 'Ġused', 'Ġexpend', 'able', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġfirst', 'Ġfal', 'con', 'Ġlaunch', 'Ġj', 'une', 'Ġfirst', 'Ġfal', 'con', 'Ġiss', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġmission', 'Ġiss', 'Ġlaunched', 'Ġoct', 'ober', 'Ġbecame', 'Ġfirst', 'Ġcommercial', 'Ġrocket', 'Ġever', 'Ġlaunch', 'Ġhumans', 'Ġorbit', 'Ġcurrently', 'Ġvehicle', 'Ġcapable', 'Ġu', 'Ġrocket', 'Ġcurrently', 'Ġcertified', 'Ġtransporting', 'Ġhumans', 'Ġinternational', 'Ġspace', 'Ġbecame', 'Ġu', 'Ġrocket', 'Ġlaunches', 'Ġhistory', 'Ġbest', 'Ġsafety', 'Ġrecord', 'Ġsuffered', 'Ġone', 'Ġflight', 'Ġfailure', 'Ġrocket', 'Ġtwo', 'Ġstages', 'Ġfirst', 'bo', 'oster', 'Ġstage', 'Ġcarries', 'Ġsecond', 'Ġstage', 'Ġpayload', 'Ġpredetermined', 'Ġaltitude', 'Ġsecond', 'Ġstage', 'Ġlifts', 'Ġpayload', 'Ġultimate', 'Ġdestination', 'Ġbooster', 'Ġcapable', 'Ġlanding', 'Ġvertically', 'Ġfacilitate', 'Ġreuse', 'Ġfeat', 'Ġfirst', 'Ġachieved', 'Ġflight', 'Ġde', 'cember', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġsuccessfully', 'Ġlanded', 'Ġboosters', 'Ġtimes', 'Ġindividual', 'Ġboosters', 'Ġflown', 'Ġmany', 'Ġflights', 'Ġstages', 'Ġpowered', 'Ġspace', 'x', 'Ġmer', 'lin', 'Ġengines', 'Ġusing', 'Ġcry', 'ogenic', 'Ġliquid', 'Ġrocket', 'grade', 'Ġk', 'eros', 'ene', 'Ġheaviest', 'Ġpayload', 'Ġflown', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġint', 'els', 'Ġcarrying', 'Ġtel', 'star', 'v']</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>['Ġsimultaneous', 'Ġbooster', 'Ġland', 'ings', 'Ġfal', 'con', 'Ġheavy', 'Ġflights', 'mber', 'Ġfour', 'Ġboosters', 'Ġlanded', 'Ġspace', 'x', 'Ġalso', 'Ġcreated', 'Ġlanding', 'Ġsite', 'Ġformer', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġlaunch', 'Ġsite', 'Ġdemolished', 'Ġreconstruction', 'Ġlanding', 'Ġsite', 'Ġoct', 'ober', 'Ġfal', 'con', 'Ġrocket', 'Ġbooster', 'Ġsuccessfully', 'Ġlanded', 'Ġnew', 'Ġground', 'Ġpad', 'Ġknown', 'Ġfirst', 'Ġtime', 'Ġstarting', 'Ġspace', 'x', 'Ġcommissioned', 'Ġconstruction', 'Ġautonomous', 'Ġspac', 'eport', 'Ġdrone', 'Ġships', 'ds', 'Ġdeck', 'Ġbarg', 'es', 'fitted', 'Ġstation', 'keeping', 'Ġengines', 'Ġlarge', 'Ġlanding', 'Ġplatform', 'Ġships', 'Ġstationed', 'Ġhundreds', 'Ġkilometers', 'range', 'Ġallow', 'Ġfirst', 'Ġstage', 'Ġrecovery', 'Ġhigh', 'vel', 'ocity', 'Ġmissions', 'Ġcannot', 'Ġreturn', 'Ġlaunch', 'Ġsite', 'Ġlanding', 'Ġsites', 'Ġdrone', 'Ġships', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġthree', 'Ġoperational', 'Ġdrone', 'Ġships', 'Ġread', 'Ġinstructions', 'Ġcourse', 'Ġstill', 'Ġlove', 'Ġshortfall', 'Ġgrav', 'itas', 'Ġshortfall', 'Ġgrav', 'itas', 'Ġread', 'Ġinstructions', 'Ġused', 'l', 'antic', 'Ġlaunches', 'Ġcape', 'aver', 'al', 'Ġcourse', 'Ġstill', 'Ġlove', 'Ġoperated', 'Ġpac', 'ific', 'Ġport', 'Ġv', 'enberg', 'Ġtransporter', 'Ġmission', 'Ġlaunch', 'Ġdebuted', 'Ġnew', 'Ġnozzle', 'Ġextension', 'Ġdesign', 'Ġaimed', 'Ġincreasing', 'Ġcad', 'ence', 'Ġreducing', 'Ġcosts', 'Ġnew', 'Ġnozzle', 'Ġextension', 'Ġshorter', 'Ġresult', 'Ġengine', 'Ġlower', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġtherefore', 'Ġperformance', 'Ġdue', 'Ġï', '¬', 'Ĥ', 'Ġmissions', "'t", 'Ġneed', 'Ġfal', 'con', 'Ġfull', 'Ġperformance', 'Ġcapability', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'http', 'space', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'Ġb', 'aylor', 'ichael', 'Ġmay', 'Ġblock', 'Ġspace', 'x', 'Ġincrease', 'Ġlaunch', 'Ġcad', 'ence', 'Ġlower', 'Ġprices', 'pr', 'ices', 'Ġretrieved', 'Ġmay', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'mber', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['075', 'Ġformer', 'Ġlaunched', 'Ġadvantageous', 'Ġsuper', 'syn', 'chron', 'ous', 'Ġtransfer', 'Ġorbit', 'Ġlatter', 'Ġwent', 'Ġlower', 'energy', 'Ġg', 'Ġap', 'gee', 'Ġwell', 'Ġge', 'ost', 'ation', 'ary', 'Ġaltitude', 'Ġjan', 'uary', 'Ġfal', 'con', 'Ġset', 'Ġrecord', 'Ġsatellites', 'Ġlaunched', 'Ġsingle', 'Ġrocket', 'Ġcarrying', 'Ġorbit', 'Ġfal', 'con', 'Ġhuman', 'rated', 'Ġtransporting', 'Ġn', 'asa', 'Ġastronauts', 'Ġiss', 'Ġfal', 'con', 'Ġcertified', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġprogram', 'Ġn', 'asa', 'Ġlaunch', 'Ġservices', 'Ġprogram', 'category', '",', 'Ġlaunch', 'Ġexpensive', 'Ġimportant', 'Ġcomplex', 'Ġn', 'asa', 'Ġmissions', 'Ġrocket', 'Ġevolved', 'Ġseveral', 'Ġversions', 'Ġflew', 'âĢĵ', 'Ġflew', 'âĢĵ', 'Ġfull', 'Ġthrust', 'Ġfirst', 'Ġlaunched', 'Ġencomp', 'assing', 'Ġblock', 'Ġvariant', 'Ġoperation', 'Ġsince', 'Ġmay', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġannounced', 'Ġplans', 'Ġlaunch', 'Ġfal', 'con', 'Ġfirst', 'Ġhalf', 'Ġinitial', 'Ġlaunch', 'Ġwould', 'Ġoccur', 'Ġspace', 'x', 'Ġspent', 'Ġcapital', 'Ġdevelop', 'Ġprevious', 'Ġlauncher', 'Ġfal', 'con', 'Ġdevelopment', 'Ġfal', 'con', 'Ġaccelerated', 'Ġpartial', 'Ġn', 'asa', 'Ġfunding', 'Ġcommitments', 'Ġpurchase', 'Ġflights', 'Ġspecific', 'Ġcapabilities', 'Ġdemonstrated', 'Ġfunding', 'Ġstarted', 'Ġseed', 'Ġmoney', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'c', 'ots', 'Ġprogram', 'Ġcontract', 'Ġstructured', 'Ġspace', 'Ġact', 'Ġagreement', 'Ġdevelop', 'Ġdemonstrate', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservice', '",', 'Ġincluding', 'Ġpurchase', 'Ġthree', 'Ġdemonstration', 'Ġflights', 'Ġoverall', 'Ġcontract', 'Ġaward', 'Ġus', 'Ġmillion', 'Ġprovide', 'Ġthree', 'Ġdemonstration', 'Ġlaunches', 'Ġfal', 'con', 'Ġspace', 'x', 'Ġdragon', 'Ġcargo', 'Ġspacecraft', 'Ġadditional', 'Ġmilestones', 'Ġadded', 'Ġlater', 'Ġraising', 'Ġtotal', 'Ġcontract', 'Ġvalue', 'Ġus', 'Ġmillion', 'Ġspace', 'x', 'Ġcommercial', 'Ġres', 'upp', 'ly', 'Ġservices', 'c', 'rs', 'Ġcontract', 'Ġn', 'asa', "'s", 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'c', 'ots', 'Ġprogram', 'Ġdeliver', 'Ġcargo', 'Ġiss', 'Ġusing', 'Ġfal', 'con', 'dragon', 'Ġfunds', 'Ġwould', 'Ġdis', 'b', 'ursed', 'Ġdemonstration', 'Ġmissions', 'Ġsuccessfully', 'Ġthoroughly', 'Ġcompleted', 'Ġcontract', 'Ġtotaled', 'Ġus', 'Ġbillion', 'Ġminimum', 'Ġmissions', 'Ġferry', 'Ġsupplies', 'Ġiss', 'Ġspace', 'x', 'Ġestimated', 'Ġfal', 'con', 'Ġdevelopment', 'Ġcosts', 'Ġorder']</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>['Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'es', 'nic', 'Ġtre', 'vor', 'Ġoct', 'ober', 'st', 'arl', 'ink', 'Ġgroup', 'Ġfal', 'con', 'Ġblock', 'Ġeveryday', 'Ġastronaut', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'mber', 'fal', 'con', 'Ġblock', 'Ġnext', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġk', 'bs', 'Ġgun', 'ter', 'fal', 'con', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'mber', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'el', 'mus', 'k', 'Ġde', 'cember', 'Ġ"-', 'Ġcase', 'Ġdeep', 'Ġcry', 'Ġincreases', 'Ġdensity', 'Ġampl', 'ï', '¬', 'ģ', 'es', 'Ġrocket', 'Ġperformance', 'Ġfirst', 'Ġtime', 'Ġanyone', 'Ġgone', 'Ġlow', 'Ġchilled', 'f', 'Ġf', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'trans', 'porter', 'Ġretrieved', 'Ġmarch', 'es', 'nic', 'Ġtre', 'vor', 'Ġj', 'uly', 'ech', 'ost', 'ar', 'Ġfal', 'con', 'Ġheavy', 'Ġeveryday', 'Ġastronaut', 'Ġretrieved', 'Ġj', 'uly', 'Ġnotes', 'Ġreferences', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'active', 'Ġlaunch', 'Ġvehicle', 'Ġreliability', 'Ġstatistics', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġlaunches', 'Ġretrie', 'ves', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrecycled', 'Ġrocket', 'Ġwashing', 'ton', 'Ġpost', 'Ġassociated', 'Ġpress', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġmarch', 'space', 'x', 'Ġlaunches', 'Ġsatellite', 'Ġpartly', 'Ġused', 'Ġrocket', 'http', 'Ġnew', 'ork', 'Ġtimes', 'Ġretrieved', 'Ġapr', 'il', 'Ġvia', 'Ġn', 'yt', 'imes', 'Ġb', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġoct', 'ober', 'space', 'x', 'Ġchanges', 'Ġfal', 'con', 'Ġreturn', 'ï', '¬', 'Ĥ', 'ight', 'Ġplans', 'htt', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmarch', 'space', 'x', 'Ġaims', 'Ġdebut', 'Ġnew', 'Ġversion', 'Ġfal']</t>
+          <t>['Ġus', 'Ġmillion', 'Ġn', 'asa', 'Ġestimated', 'Ġdevelopment', 'Ġcosts', 'Ġbillion', 'Ġtraditional', 'Ġcost', 'plus', 'Ġcontract', 'Ġapproach', 'Ġused', 'Ġn', 'asa', 'Ġreport', 'est', 'imated', 'Ġwould', 'Ġcost', 'Ġagency', 'Ġdevelopment', 'Ġhistory', 'Ġconception', 'Ġfunding', 'Ġfal', 'con', 'Ġwik', 'ipedia', '000', 'Ġlanding', 'ds', '000', '000', 'Ġpayload', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', 'Ġft', '000', 'Ġexpended', '000', 'Ġlanding', '000', 'Ġpayload', 'Ġmars', 'Ġtransfer', 'Ġorbit', 'Ġmass', 'Ġft', 'Ġassociated', 'Ġrockets', 'Ġderivative', 'Ġwork', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġft', 'Ġblock', 'Ġactive', 'Ġft', 'Ġblock', 'Ġretired', 'Ġft', 'Ġblock', 'Ġretired', 'Ġretired', 'Ġretired', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġv', 'enberg', 'Ġv', 'enberg', 'future', 'Ġtotal', 'Ġlaunches', 'ft', 'Ġsuccess', 'es', 'ft', 'Ġfailure', 'ï', '¬', 'Ĥ', 'ight', 'Ġpartial', 'Ġfailure', 'Ġcr', ')[', 'Ġnotable', 'Ġoutcome', 'ft', 'Ġpre', 'ï', '¬', 'Ĥ', 'ight', 'Ġdestruction', 'Ġland', 'ings', 'Ġattempts', 'Ġbillion', 'Ġdevelop', 'Ġrocket', 'Ġlike', 'Ġfal', 'con', 'Ġbooster', 'Ġbased', 'Ġupon', 'Ġn', 'asa', "'s", 'Ġtraditional', 'Ġcontracting', 'Ġprocesses', 'Ġcommercial', 'Ġdevelopment', 'Ġapproach', 'Ġmight', 'Ġallowed', 'Ġagency', 'Ġpay', 'Ġus', 'Ġbillion', '".[', 'Ġspace', 'x', 'Ġreleased', 'Ġcombined', 'Ġdevelopment', 'Ġcosts', 'Ġfal', 'con', 'Ġdragon', 'Ġn', 'asa', 'Ġprovided', 'Ġus', 'Ġmillion', 'Ġspace', 'x', 'Ġprovided', 'Ġus', 'Ġmillion', 'Ġcongressional', 'Ġtestimony', 'Ġspace', 'x', 'Ġsuggested', 'Ġunusual', 'Ġn', 'asa', 'Ġprocess', 'setting', 'Ġhigh', 'level', 'Ġrequirement', 'Ġcargo', 'Ġtransport', 'Ġspace', 'Ġstation', 'Ġleaving', 'Ġdetails', 'Ġindustry', 'Ġallowed', 'Ġspace', 'x', 'Ġcomplete', 'Ġtask', 'Ġsubstantially', 'Ġlower', 'Ġcost', 'according', 'Ġn', 'asa', "'s", 'Ġindependently', 'Ġverified', 'Ġnumbers', 'Ġspace', 'x', "'s", 'Ġdevelopment', 'Ġcosts', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġrockets', 'Ġestimated', 'Ġapproximately', 'Ġmillion', 'Ġtotal', '."[', 'Ġspace', 'x', 'Ġoriginally', 'Ġintended', 'Ġfollow']</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -1985,7 +1985,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>['con', 'Ġsummer', 'Ġspace', 'Ġnews', 'Ġretrieved', 'Ġmarch', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġrev', 'Ġspace', 'x', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'space', 'x', "'s", 'Ġnew', 'Ġspin', 'Ġfal', 'con', 'Ġaviation', 'Ġweek', 'Ġaviation', 'Ġweek', 'Ġnetwork', 'Ġretrieved', 'Ġoct', 'ober', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'space', 'x', "'s", 'Ġshot', 'well', 'Ġtalks', 'Ġrapt', 'Ġfal', 'con', 'Ġsatellite', 'Ġinternet', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġp', 'enton', 'Ġretrieved', 'Ġmay', 'Ġab', 'bott', 'Ġj', 'ose', 'ph', 'Ġmay', 'space', 'x', "'s", 'Ġgrass', 'ho', 'pper', 'Ġleaping', 'Ġspac', 'eport', 'w', 'ac', 'Ġw', 'aco', 'Ġtrib', 'une', 'Ġretrieved', 'Ġapr', 'il', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġapr', 'il', 'space', 'x', 'Ġpreparing', 'Ġbusy', 'Ġseason', 'Ġmissions', 'Ġtest', 'Ġmilestones', 'Ġest', 'mil', 'estones', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġse', 'pt', 'ember', 'full', 'Ġthrust', 'Ġfal', 'con', 'Ġstage', 'Ġundergoing', 'Ġtesting', 'Ġmc', 'greg', 'h', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġse', 'pt', 'ember', 'fal', 'con', 'Ġupgrades', 'current', 'Ġvehicle', 'Ġupgrade', 'Ġspac', 'en', 'ews', 'Ġjournalist', 'Ġtwitter', 'Ġfeed', 'Ġspace', 'x', 'Ġslide', 'Ġrep', 'ublished', 'Ġtwitter', 'Ġretrieved', 'Ġjan', 'uary', 'Ġel', 'Ġmus', 'k', 'Ġtwitter', 'el', 'mus', 'k', 'Ġde', 'cember', 'Ġ"-', 'Ġcase', 'Ġdeep', 'Ġcry', 'Ġincreases', 'Ġdensity', 'Ġampl', 'ï', '¬', 'ģ', 'es', 'Ġrocket', 'Ġperformance', 'Ġfirst', 'Ġtime', 'Ġanyone', 'Ġgone', 'Ġlow', 'Ġchilled', 'f', 'Ġf', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'ses', 'Ġbetting', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġupgrade', 'Ġdebut', 'Ġapproaches', 'Ġspace', 'Ġnews', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'fal', 'con', 'Ġperformance', 'Ġmid', 'size', 'Ġgeo', '?"', 'Ġaviation', 'Ġweek', 'Ġarchived']</t>
+          <t>['Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġintermediate', 'Ġcapacity', 'Ġvehicle', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġline', 'Ġvehicles', 'Ġnamed', 'Ġfictional', 'Ġstarship', 'mill', 'enn', 'ium', 'Ġfal', 'con', 'Ġstar', 'Ġwars', 'Ġfilm', 'Ġseries', 'Ġspace', 'x', 'Ġannounced', 'Ġinstead', 'Ġproceeding', 'Ġfal', 'con', 'fully', 'Ġreusable', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', '",', 'Ġalready', 'Ġsecured', 'Ġgovernment', 'Ġcustomer', 'Ġfal', 'con', 'Ġdescribed', 'Ġcapable', 'Ġlaunching', 'Ġapproximately', 'Ġkilograms', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġprojected', 'Ġpriced', '000', '000', 'Ġus', 'Ġper', 'Ġflight', 'Ġft', 'Ġpayload', 'Ġfair', 'ing', 'Ġmillion', 'Ġft', 'Ġfair', 'ing', 'Ġspace', 'x', 'Ġalso', 'Ġannounced', 'Ġheavy', 'Ġversion', 'Ġfal', 'con', 'Ġpayload', 'Ġcapacity', 'Ġapproximately', '000', 'Ġkilograms', '000', 'Ġfal', 'con', 'Ġintended', 'Ġsupport', 'Ġle', 'Ġg', 'Ġmissions', 'Ġwell', 'Ġcrew', 'Ġcargo', 'Ġmissions', 'Ġiss', 'Ġoriginal', 'Ġn', 'asa', 'Ġc', 'ots', 'Ġcontract', 'Ġcalled', 'Ġfirst', 'Ġdemonstration', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġcompletion', 'Ġthree', 'Ġdemonstration', 'Ġmissions', 'Ġse', 'pt', 'ember', 'Ġfe', 'b', 'ruary', 'Ġdate', 'Ġslipped', 'Ġfirst', 'Ġquarter', 'Ġaccording', 'Ġmus', 'k', 'Ġcomplexity', 'Ġcape', 'aver', 'al', 'Ġregulatory', 'Ġrequirements', 'Ġcontributed', 'Ġdelay', 'Ġfirst', 'Ġmulti', 'engine', 'Ġtest', 'two', 'Ġengines', 'Ġfiring', 'Ġsimultaneously', 'Ġconnected', 'Ġfirst', 'Ġstage', 'Ġcompleted', 'Ġjan', 'uary', 'Ġsuccessive', 'Ġtests', 'Ġled', 'Ġsecond', 'mission', 'Ġlength', 'Ġnine', 'Ġengine', 'Ġtest', 'fire', 'mber', 'Ġoct', 'ober', 'Ġfirst', 'Ġflight', 'ready', 'engine', 'Ġtest', 'Ġfire', 'Ġtest', 'Ġfacility', 'Ġmc', 'greg', 'Ġtex', 'mber', 'Ġspace', 'x', 'Ġconducted', 'Ġinitial', 'Ġsecond', 'Ġstage', 'Ġtest', 'Ġfiring', 'Ġlasting', 'Ġforty', 'Ġseconds', 'Ġjan', 'uary', 'Ġsecond', 'mission', 'Ġlength', 'Ġorbit', 'insert', 'ion', 'Ġfiring', 'Ġsecond', 'Ġstage', 'Ġconducted', 'Ġelements', 'Ġstack', 'Ġarrived', 'Ġlaunch', 'Ġsite', 'Ġintegration', 'Ġbeginning', 'Ġfe', 'b', 'ruary', 'Ġflight', 'Ġstack', 'Ġwent', 'Ġvertical', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġmarch', 'Ġspace', 'x', 'Ġperformed', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġfirst', 'Ġstage', 'Ġfired', 'Ġwithout', 'Ġlaunch', 'Ġtest', 'Ġaborted', 'Ġdue', 'Ġfailure', 'Ġhigh']</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -1998,7 +1998,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'el', 'Ġmus', 'k', 'Ġtwitter', 'Ġtwitter', 'Ġretrieved', 'Ġapr', 'il', 'Ġl', 'op', 'atto', 'Ġel', 'izabeth', 'Ġmarch', 'space', 'x', 'Ġeven', 'Ġlanded', 'Ġnose', 'Ġcone', 'Ġhistoric', 'Ġused', 'Ġfal', 'con', 'Ġrocket', 'Ġlaunch', 'Ġverge', 'Ġretrieved', 'Ġapr', 'il', 'el', 'mus', 'k', 'Ġj', 'une', 'flying', 'Ġlarger', 'Ġsign', 'ï', '¬', 'ģ', 'c', 'antly', 'Ġupgraded', 'Ġhyp', 'erson', 'ic', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġsingle', 'Ġpiece', 'Ġcast', 'Ġcut', 'Ġtitanium', 'Ġtake', 'entry', 'Ġheat', 'Ġshielding', 'weet', 'Ġretrieved', 'Ġapr', 'il', 'Ġvia', 'Ġtwitter', 'el', 'mus', 'k', 'Ġj', 'une', 'new', 'Ġtitanium', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġworked', 'Ġeven', 'Ġbetter', 'Ġexpected', 'Ġcapable', 'Ġind', 'e', 'ï', '¬', 'ģ', 'n', 'ite', 'Ġnumber', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġservice', 'weet', 'Ġretrieved', 'Ġapr', 'il', 'Ġvia', 'Ġtwitter', 'th', 'Ġsw', 'Ġsupports', 'Ġsuccessful', 'Ġfal', 'con', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunch', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġmarch', 'air', 'Ġforce', 'Ġreveals', 'Ġplan', 'Ġlaunches', 'Ġper', 'Ġyear', 'Ġcape', 'aver', 'al', 'Ġape', 'Ġretrieved', 'Ġapr', 'il', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġj', 'une', 'space', 'x', "'s", 'Ġfinal', 'Ġfal', 'con', 'Ġdesign', 'Ġcoming', 'Ġyear', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġspace', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġaug', 'ust', 'home', 'Ġforums', 'Ġsign', 'Ġiss', 'Ġcommercial', 'Ġshuttle', 'Ġsl', 'ion', 'Ġr', 'ussian', 'Ġeuro', 'pe', 'Ġch', 'inese', 'Ġunmanned', 'Ġfal', 'con', 'Ġblock', 'Ġdebut', 'Ġsuccess', 'Ġdragon', 'Ġarrives', 'Ġstation', 'Ġber', 'thing', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlaunches', 'Ġcr', 'Ġdragon', 'Ġmission', 'Ġiss', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il']</t>
+          <t>['pressure', 'Ġhelium', 'Ġpump', 'Ġsystems', 'Ġabort', 'Ġperformed', 'Ġexpected', 'Ġadditional', 'Ġissues', 'Ġneeded', 'Ġaddressing', 'Ġsubsequent', 'Ġtest', 'Ġmarch', 'Ġfired', 'Ġfirst', 'stage', 'Ġengines', 'Ġseconds', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġproduction', 'Ġline', 'Ġmanufactured', 'Ġfal', 'con', 'Ġdragon', 'Ġspacecraft', 'Ġevery', 'Ġthree', 'Ġmonths', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', "'s", 'Ġtotal', 'Ġmanufacturing', 'Ġspace', 'Ġincreased', 'Ġnearly', '000', '000', '000', 'Ġft', 'Ġorder', 'Ġachieve', 'Ġproduction', 'Ġrate', 'Ġrocket', 'Ġcores', 'Ġannually', 'Ġfactory', 'Ġproducing', 'Ġone', 'Ġfal', 'con', 'Ġper', 'Ġmonth', 'mber', 'Ġfe', 'b', 'ruary', 'Ġproduction', 'Ġrate', 'Ġfal', 'con', 'Ġcores', 'Ġincreased', 'Ġper', 'Ġyear', 'Ġnumber', 'Ġfirst', 'Ġstage', 'Ġcores', 'Ġcould', 'Ġassembled', 'Ġone', 'Ġtime', 'Ġreached', 'Ġsince', 'Ġspace', 'x', 'Ġroutinely', 'Ġreused', 'Ġfirst', 'Ġstages', 'Ġreducing', 'Ġdemand', 'Ġnew', 'Ġcores', 'Ġspace', 'x', 'Ġperformed', 'Ġlaunches', 'Ġusing', 'Ġtwo', 'Ġnew', 'Ġboosters', 'Ġsuccessfully', 'Ġrecovered', 'Ġbooster', 'Ġone', 'Ġflight', 'Ġhaw', 'th', 'orne', 'Ġfactory', 'Ġproduces', 'Ġone', 'exp', 'end', 'able', 'Ġsecond', 'Ġstage', 'Ġlaunch', 'Ġdevelopment', 'Ġtesting', 'Ġproduction', 'Ġlaunch', 'Ġhistory', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġft', 'Ġblock', 'Ġmay', 'bang', 'aband', 'hu', 'Ġsatellite', 'Ġft', 'Ġde', 'cember', 'Ġflight', ')[', 'Ġse', 'pt', 'ember', 'Ġcass', 'ope', 'Ġj', 'une', 'dragon', 'Ġc', 'ots', 'Ġdemo', ')[', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġft', 'Ġblock', 'Ġj', 'une', 'space', 'x', 'Ġjan', 'uary', 'j', 'ason', 'Ġmarch', 'space', 'x', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġft', 'Ġblock', 'Ġmer', 'lin', 'maximum', 'Ġthrust', 'Ġft', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġmaximum', 'Ġthrust', 'Ġft', 'late', '):', '000', 'Ġft', '000', '000', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '05', 'Ġsea', 'Ġlevel', 'Ġvacuum', 'Ġburn', 'Ġtime', 'Ġft', 'Ġseconds', 'Ġseconds', 'Ġseconds']</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>['mus', 'k', 'Ġpreviews', 'Ġbusy', 'Ġyear', 'Ġahead', 'Ġspace', 'x', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġholds', 'Ġpre', 'launch', 'Ġb', 'rie', 'ï', '¬', 'ģ', 'ng', 'Ġhistoric', 'Ġpad', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġyoutube', 'f', 'iche', 'Ġtechnique', 'Ġfal', 'con', 'technical', 'Ġdata', 'Ġsheet', 'Ġfal', 'con', '].', 'Ġes', 'pace', 'Ġexploration', 'Ġfrench', 'Ġmay', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġusers', 'Ġguide', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġlight', 'Ġmetals', 'Ġhelp', 'Ġspace', 'x', 'Ġland', 'Ġfal', 'con', 'Ġrockets', 'Ġastonishing', 'Ġaccuracy', 'li', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġshot', 'well', 'Ġmarch', 'Ġbroadcast', 'Ġspecial', 'Ġedition', 'Ġinterview', 'Ġshot', 'well', 'audio', 'Ġï', '¬', 'ģ', 'le', 'Ġspace', 'Ġshow', 'Ġevent', 'Ġoccurs', 'Ġ08', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'license', 'Ġorder', '090', 'Ġrev', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġgra', 'ham', 'iam', 'Ġde', 'cember', 'space', 'x', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġnails', 'Ġhistoric', 'Ġcore', 'Ġreturn', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġde', 'cember', 'Ġgr', 'uss', 'ike', 'Ġjan', 'uary', 'fal', 'con', 'Ġupgrade', 'Ġgets', 'Ġair', 'Ġforce', 'Ġlaunch', 'Ġmilitary', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'Ġshot', 'well', 'Ġfe', 'b', 'ruary', 'Ġshot', 'well', 'Ġcomments', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġconference', 'Ġcommercial', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġevent', 'Ġoccurs', 'âĢĵ', '05', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmarch', 'space', 'x', 'Ġsays', 'Ġfal', 'con', 'Ġupgrade', "'t", 'Ġrequire', 'Ġnew', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġspace', 'Ġnews']</t>
+          <t>['Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'Ġrockets', 'Ġfal', 'con', 'Ġfamily', 'Ġlaunched', 'Ġtimes', 'Ġyears', 'Ġresulting', 'Ġfull', 'Ġmission', 'Ġsuccesses', '%),', 'Ġone', 'Ġpartial', 'Ġsuccess', 'space', 'x', 'Ġdelivered', 'Ġcargo', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġsecondary', 'Ġpayload', 'Ġstranded', 'Ġlower', 'planned', 'Ġorbit', 'Ġone', 'Ġfull', 'Ġfailure', 'Ġspace', 'x', 'Ġspacecraft', 'Ġlost', 'Ġflight', 'Ġexplosion', 'Ġadditionally', 'Ġone', 'Ġrocket', 'Ġpayload', 'Ġdestroyed', 'Ġlaunch', 'Ġpreparation', 'pad', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġactive', 'Ġversion', 'Ġfal', 'con', 'Ġblock', 'Ġflown', 'Ġmissions', 'Ġfull', 'Ġsuccesses', 'Ġfal', 'con', 'Ġset', 'Ġnew', 'Ġrecord', 'Ġlaunches', 'Ġsuccessful', 'Ġlaunch', 'Ġvehicle', 'Ġtype', 'Ġcalendar', 'Ġyear', 'Ġprevious', 'Ġrecord', 'Ġheld', 'Ġlaunches', 'Ġsuccessful', 'Ġfirst', 'Ġrocket', 'Ġversion', 'Ġfal', 'con', 'Ġlaunched', 'Ġfive', 'Ġtimes', 'Ġj', 'une', 'Ġmarch', 'Ġsuccessor', 'Ġfal', 'con', 'Ġtimes', 'Ġse', 'pt', 'ember', 'Ġjan', 'uary', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġtimes', 'Ġde', 'cember', 'Ġpresent', 'Ġlatest', 'Ġfull', 'Ġthrust', 'Ġvariant', 'Ġblock', 'Ġintroduced', 'Ġmay', 'Ġblock', 'Ġboosters', 'Ġflown', 'Ġtwice', 'Ġrequired', 'Ġseveral', 'Ġmonths', 'Ġrefurb', 'ishment', 'Ġblock', 'Ġversions', 'Ġdesigned', 'Ġsustain', 'Ġflights', 'Ġinspections', 'Ġfal', 'con', 'Ġheavy', 'Ġderivative', 'Ġconsists', 'Ġstrengthened', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġcenter', 'Ġcore', 'Ġtwo', 'Ġadditional', 'Ġfal', 'con', 'Ġfirst', 'Ġstages', 'Ġattached', 'Ġused', 'Ġboosters', 'Ġfitted', 'Ġaer', 'odynamic', 'Ġnose', 'cone', 'Ġinstead', 'Ġusual', 'Ġfal', 'con', 'Ġinter', 'stage', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġpowered', 'Ġft', 'Ġregular', 'Ġmer', 'lin', 'Ġvacuum', 'Ġregular', 'Ġnozzle', 'Ġft', 'Ġshort', 'Ġmer', 'lin', 'Ġvacuum', 'Ġshort', 'Ġnozzle', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmaximum', 'Ġthrust', 'Ġft', 'Ġregular', 'Ġkn', '000', 'Ġft', 'Ġshort', 'Ġkn', '000', '01', 'Ġkn', '000', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġft', 'Ġregular', 'Ġft', 'Ġshort', 'Ġburn', 'Ġtime', 'Ġft', 'Ġregular', 'Ġseconds', 'Ġft', 'Ġshort', 'Ġseconds']</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2024,7 +2024,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġmay', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'fal', 'con', 'Ġupgrade', 'Ġreceives', 'Ġblessing', 'Ġu', 'Ġair', 'Ġforce', 'htt', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġjan', 'uary', 'graded', 'Ġfal', 'con', 'Ġfirst', 'stage', 'Ġstatic', 'Ġfire', 'Ġu', 'eu', 'Ġyoutube', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġse', 'pt', 'ember', 'first', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġcompleted', 'Ġupgraded', 'Ġfal', 'con', 'http', 'sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'ses', 'Ġsigns', 'Ġlaunch', 'Ġpowerful', 'Ġfal', 'con', 'Ġengines', 'Ġn', 'eng', 'ines', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġmay', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġoct', 'ober', 'space', 'x', 'Ġselects', 'Ġmission', 'Ġfal', 'con', 'Ġreturn', 'Ġflight', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġoct', 'ober', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġlaunch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmal', 'ik', 'ari', 'q', 'Ġse', 'pt', 'ember', 'launch', 'pad', 'Ġexplosion', 'Ġdestroys', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġrocket', 'Ġsatellite', 'Ġfl', 'ida', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġse', 'pt', 'ember', 'omaly', 'Ġupdates', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'space', 'x', 'Ġseeks', 'Ġaccelerate', 'Ġfal', 'con', 'Ġproduction', 'Ġlaunch', 'Ġrates', 'Ġyear', 'Ġspac', 'en', 'ews', 'h', 'Ġspac', 'en', 'ews', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'n', 'asa', 'Ġsigns', 'Ġhistoric', 'Ġlaunch', 'Ġpad', 'Ġspace', 'x', 'Ġcollect', 'space', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġj', 'uly', 'pad', 'Ġspace', 'x', 'Ġlaying', 'Ġgroundwork', 'Ġfal', 'con', 'Ġheavy', 'Ġdebut', 'h', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il']</t>
+          <t>['Ġseconds', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfal', 'con', 'Ġfirst', 'stage', 'Ġboosters', 'Ġlanded', 'Ġsuccessfully', 'Ġattempts', '%),', '%)', 'Ġfal', 'con', 'Ġblock', 'Ġversion', 'Ġtotal', 'fl', 'ights', 'Ġfirst', 'Ġstage', 'Ġboosters', 'Ġsuccessfully', 'Ġlaunched', 'Ġpayload', 'Ġrocket', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġlaunch', 'Ġsites', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlaunch', 'Ġc', 'ots', 'Ġdemo', 'Ġflight', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġfal', 'con', 'Ġft', 'used', 'Ġfal', 'con', 'Ġblock', 'new', 'Ġfal', 'con', 'Ġblock', 'used', 'Ġfal', 'con', 'Ġheavy', 'Ġk', 'sc', 'Ġloss', 'Ġlaunch', 'Ġloss', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġpartial', 'Ġfailure', 'Ġsuccess', 'commercial', 'Ġgovernment', 'Ġsuccess', 'st', 'arl', 'ink', 'Ġplanned', 'commercial', 'Ġgovernment', 'Ġplanned', 'st', 'arl', 'ink', 'Ġground', 'pad', 'Ġfailure', 'Ġdrone', 'ship', 'Ġfailure', 'Ġocean', 'Ġtest', 'Ġfailure', 'Ġparachute', 'Ġtest', 'Ġfailure', 'ii', 'Ġground', 'pad', 'Ġsuccess', 'Ġdrone', 'ship', 'Ġsuccess', 'Ġocean', 'Ġtest', 'Ġsuccess', 'iii', 'Ġattempt', 'Ġcontrolled', 'Ġdescent', 'Ġocean', 'Ġtouchdown', 'Ġcontrol', 'Ġfailed', 'Ġrecovery', 'Ġpassive', 'entry', 'Ġfailed', 'Ġparachute', 'Ġdeployment', 'Ġcontrolled', 'Ġdescent', 'Ġsoft', 'Ġvertical', 'Ġocean', 'Ġtouchdown', 'Ġrecovery', 'Ġflight', 'Ġdragon', 'Ġspacecraft', 'Ġqual', 'ï', '¬', 'ģ', 'cation', 'Ġunit', 'Ġj', 'une', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtest', 'Ġdragon', 'Ġflight', 'Ġdragon', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcargo', 'Ġdelivery', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġoperational', 'Ġcargo', 'Ġmission', 'Ġiss', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdemonstration', 'Ġrocket', "'s", 'Ġengine', 'Ġcapability', 'Ġdue', 'Ġfailure', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġmer', 'lin', 'Ġengine', 'Ġflight', 'Ġcass', 'ope', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrocket', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġv', 'enberg', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġattempt', 'Ġprop', 'ulsive', 'Ġreturn', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġge', 'os', 'ynchronous']</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2037,7 +2037,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>['space', 'x', 'Ġbreaks', 'Ġground', 'Ġb', 'oca', 'Ġch', 'ica', 'Ġbeach', 'Ġl', 'Ġbrown', 'ville', 'Ġherald', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'tex', 'Ġfl', 'ida', 'Ġbattle', 'Ġspace', 'x', 'Ġspac', 'eport', 'Ġpar', 'abolic', 'Ġarc', 'Ġretrieved', 'mber', 'Ġdean', 'Ġj', 'ames', 'Ġmay', 'Ġstates', 'Ġv', 'ie', 'Ġspace', 'x', "'s", 'Ġcommercial', 'Ġrocket', 'Ġlaunches', 'Ġus', 'Ġtoday', 'Ġretrieved', 'Ġapr', 'il', 'aven', 'port', 'Ġchrist', 'ian', 'Ġde', 'cember', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġpulls', 'Ġdramatic', 'Ġhistoric', 'Ġlanding', 'Ġwashing', 'ton', 'Ġpost', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġdemol', 'ishes', 'Ġtitan', 'Ġpad', 'Ġyoutube', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'sa', 'ocom', 'Ġmission', 'Ġspace', 'x', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'el', 'mus', 'k', 'Ġjan', 'uary', 'aim', 'ing', 'Ġlaunch', 'Ġweekend', 'hop', 'efully', 'Ġland', 'Ġdrones', 'hip', 'Ġship', 'Ġland', 'ings', 'Ġneeded', 'Ġhigh', 'Ġvelocity', 'Ġmissions', 'weet', 'Ġvia', 'Ġtwitter', 'el', 'mus', 'k', 'Ġjan', 'uary', 'Ġspeed', 'Ġstage', 'Ġseparation', 'Ġship', 'Ġneed', 'Ġzero', 'Ġlateral', 'Ġvelocity', 'Ġstage', '000', '01', 'weet', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġel', 'Ġmus', 'k', 'Ġshares', 'Ġphoto', 'Ġdrone', 'Ġship', 'Ġenables', 'Ġmissions', 'Ġretrieved']</t>
+          <t>['Ġtransfer', 'Ġorbit', 'g', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġn', 'ongo', 'vernment', 'al', 'Ġpayload', 'Ġflight', 'Ġadded', 'Ġlanding', 'Ġlegs', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfully', 'Ġcontrolled', 'Ġdescent', 'Ġvertical', 'Ġocean', 'Ġtouchdown', 'Ġflight', 'Ġdeep', 'Ġspace', 'Ġclimate', 'Ġobserv', 'atory', 'sc', 'ov', 'r', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġhyper', 'b', 'olic', 'Ġmission', 'Ġinjecting', 'Ġspacecraft', 'Ġpoint', 'Ġflight', 'Ġtotal', 'Ġloss', 'Ġmission', 'Ġdue', 'Ġstructural', 'Ġfailure', 'Ġhelium', 'pressure', 'Ġsecond', 'Ġstage', 'Ġflight', 'Ġorb', 'comm', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġvertical', 'Ġlanding', 'Ġorbital', 'class', 'Ġrocket', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanding', 'Ġvertically', 'Ġachieved', 'Ġautonomous', 'Ġspac', 'eport', 'Ġdrone', 'Ġship', 'Ġsea', 'Ġtotal', 'Ġvehicle', 'Ġpayload', 'Ġloss', 'Ġprior', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'would', 'Ġflight', 'Ġflight', 'Ġcr', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġflight', 'es', 'Ġï', '¬', 'ģ', 'r', 'st', 'ï', '¬', 'Ĥ', 'ight', 'Ġpreviously', 'Ġï', '¬', 'Ĥ', 'Ġorbital', 'Ġclass', 'Ġbooster', 'Ġpreviously', 'Ġused', 'Ġspace', 'x', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrecovery', 'Ġfair', 'ing', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġspace', 'plane', 'Ġflight', 'Ġbang', 'aband', 'hu', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġblock', 'Ġversion', 'Ġlaunch', 'Ġoutcomes', 'Ġbooster', 'Ġland', 'ings', 'Ġnotable', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġhistoric', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġlanding', 'Ġcape', 'aver', 'al', 'Ġlanding', 'Ġzone', 'Ġde', 'cember', 'Ġflight', 'Ġtel', 'star', 'v', 'Ġheaviest', 'Ġcommunications', 'Ġsatellite', 'Ġever', 'Ġdelivered', 'Ġflight', 'Ġcrew', 'Ġdragon', 'Ġdemo', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġcrew', 'Ġdragon', 'Ġcarry', 'Ġastronauts', 'Ġflight', 'Ġrad', 'ars', 'Ġconstellation', 'Ġvaluable', 'Ġcommercial', 'Ġpayload', 'Ġput', 'Ġorbit', 'Ġflight', 'Ġstar', 'link', 'Ġlaunch', 'Ġsuccessful', 'Ġï', '¬', 'Ĥ']</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>['las', 'Ġwik', 'ipedia', 'las', 'Ġlaunch', 'las', 'Ġcarrying', 'Ġlunar', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġl', 'cross', 'Ġspace', 'Ġprobes', 'Ġj', 'une', 'Ġfunction', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġsize', 'Ġheight', 'Ġft', 'Ġpayload', 'Ġfair', 'ing', 'Ġft', 'Ġstar', 'liner', 'Ġdiameter', 'Ġft', 'Ġmass', '000', '000', 'Ġstages', 'Ġstar', 'Ġupper', 'Ġstage', 'Ġcapacity', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', 'âĢĵ', 'âĢĵ', 'Ġpayload', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġmass', 'âĢĵ', 'âĢĵ', 'Ġassociated', 'Ġrockets', 'Ġfamily', 'las', 'Ġbased', 'las', 'Ġcomparable', 'Ġdelta', 'Ġiv', 'Ġfal', 'con', 'Ġlong', 'Ġmarch', 'Ġpro', 'ton', 'Ġsat', 'urn', 'Ġlaunch', 'Ġhistory', 'las', 'las', 'Ġv', 'Ġexpend', 'able', 'Ġlaunch', 'Ġsystem', 'Ġfifth', 'Ġmajor', 'Ġversion', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġfamily', 'Ġoriginally', 'Ġdesigned', 'Ġlock', 'heed', 'Ġmart', 'Ġoperated', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġjoint', 'Ġventure', 'Ġlock', 'heed', 'Ġmart', 'Ġbo', 'e', 'ing', 'las', 'Ġalso', 'Ġmajor', 'Ġn', 'asa', 'Ġlaunch', 'Ġvehicle', 'Ġameric', "'s", 'Ġlongest', 'serving', 'Ġactive', 'Ġrocket', 'Ġaug', 'ust', 'Ġu', 'la', 'Ġannounced', 'las', 'Ġwould', 'Ġretired', 'Ġremaining', 'Ġlaunches', 'Ġsold', 'mber', 'Ġlaunches', 'Ġremain', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġconsists', 'Ġtwo', 'Ġmain', 'Ġstages', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġr', 'ussian', 'Ġr', 'Ġengine', 'Ġmanufactured', 'Ġener', 'gom', 'ash', 'Ġburning', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġpowered', 'Ġone', 'Ġtwo', 'Ġameric', 'Ġengine', 'Ġmanufactured', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġburns', 'Ġliquid', 'Ġhydrogen', 'Ġliquid', 'Ġstar', 'Ġupper', 'Ġstage', 'Ġused', 'Ġnew', 'Ġhor', 'izons', 'Ġmission', 'Ġthird', 'Ġstage', 'Ġstrap', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġused', 'Ġconfigurations', 'Ġused', 'Ġoriginally', 'Ġreplaced', 'mber', 'Ġgraph', 'ite', 'ep', 'oxy', 'Ġmotor', 'gem', 'Ġstandard', 'Ġpayload', 'Ġfair', 'ings']</t>
+          <t>['ight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrecovery', 'Ġfailure', 'Ġpreviously', 'Ġï', '¬', 'Ĥ', 'Ġrecovered', 'Ġbooster', 'Ġflight', 'Ġsuccessful', 'Ġstar', 'link', 'Ġlaunch', 'Ġsaw', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfailure', 'Ġmer', 'lin', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġengine', 'Ġascent', 'Ġsecond', 'Ġascent', 'Ġengine', 'Ġfailure', 'Ġrocket', 'Ġfollowing', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġflight', 'Ġcrew', 'Ġdragon', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcrew', 'ed', 'Ġlaunch', 'Ġcrew', 'Ġdragon', 'Ġcarrying', 'Ġtwo', 'Ġastronauts', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcrew', 'ed', 'Ġoperational', 'Ġlaunch', 'Ġcrew', 'Ġdragon', 'Ġholding', 'Ġrecord', 'Ġlongest', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġu', 'Ġcrew', 'Ġvehicle', 'Ġflight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġcargo', 'Ġdragon', 'Ġunc', 'rew', 'ed', 'Ġvariant', 'Ġcrew', 'Ġdragon', 'Ġflight', 'Ġtransporter', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdedicated', 'Ġsmall', 'sat', 'Ġrides', 'hare', 'Ġlaunch', 'Ġset', 'Ġrecord', 'Ġsatellites', 'Ġlaunched', 'Ġsingle', 'Ġlaunch', 'Ġsatellites', 'Ġsurpass', 'ing', 'Ġprevious', 'Ġrecord', 'Ġsatellites', 'Ġheld', 'mber', 'Ġlaunch', 'Ġant', 'ares', 'Ġflight', 'Ġroutine', 'Ġstar', 'link', 'Ġlaunch', 'Ġexperienced', 'Ġearly', 'Ġshut', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġmer', 'lin', 'Ġengine', 'Ġascent', 'Ġdue', 'Ġdamage', 'Ġstill', 'Ġdelivered', 'Ġpayload', 'Ġtarget', 'Ġorbit', 'Ġflight', 'Ġinspiration', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġorbital', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'private', 'Ġcrew', 'Ġflight', 'Ġdart', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġplanetary', 'Ġdefenses', 'Ġmission', 'Ġnear', 'earth', 'Ġobjects', 'Ġflight', 'th', 'Ġsuccessful', 'Ġvertical', 'Ġlanding', 'Ġorbital', 'class', 'Ġrocket', 'Ġsixth', 'Ġanniversary', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanding', 'Ġflight', 'Ġheaviest', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġblock', 'Ġpayload', 'Ġstar', 'link', 'Ġsatellites', 'Ġflight', 'th', 'Ġconsecutive', 'Ġsuccessful', 'Ġfal', 'con', 'Ġmission', 'Ġflight', 'th', 'Ġoverall', 'Ġsuccessful', 'Ġbooster', 'Ġlanding', 'Ġtwo', 'stage', 'Ġl', 'ox', 'r', 'p', 'powered', 'Ġlaunch', 'Ġvehicle', 'Ġfirst', 'Ġstage', 'Ġheight', 'Ġft', 'Ġheight', 'Ġinter', 'stage', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'Ġlithium', 'Ġskin']</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>['Ġft', 'Ġdiameter', 'Ġvarious', 'Ġlengths', 'las', 'Ġdeveloped', 'Ġlock', 'heed', 'Ġmart', 'Ġcommercial', 'Ġlaunch', 'Ġservices', 'Ġpart', 'Ġu', 'Ġair', 'Ġforce', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'e', 'el', 'v', 'Ġprogram', 'Ġmade', 'Ġinaugural', 'Ġflight', 'Ġaug', 'ust', 'Ġvehicle', 'Ġoperates', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġv', 'enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġcontinued', 'Ġmarket', 'las', 'Ġcommercial', 'Ġcustomers', 'Ġworldwide', 'Ġjan', 'uary', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġassumed', 'Ġcontrol', 'Ġcommercial', 'Ġmarketing', 'Ġsales', 'las', 'Ġfirst', 'Ġstage', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġconfused', 'Ġdelta', 'Ġiv', "'s", 'Ġcommon', 'Ġbooster', 'Ġcore', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġlength', 'Ġpowered', 'Ġone', 'Ġn', 'po', 'Ġener', 'gom', 'ash', 'Ġr', 'Ġmain', 'Ġengine', 'Ġburning', 'Ġliquid', 'Ġbooster', 'Ġoperates', 'Ġfour', 'Ġminutes', 'Ġproviding', '000', 'Ġthrust', 'Ġthrust', 'Ġaugmented', 'Ġfive', 'ero', 'jet', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġgem', 'Ġstrap', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġproviding', 'Ġadditional', '000', 'Ġthrust', 'Ġseconds', 'Ġmain', 'Ġdifferences', 'las', 'Ġearlier', 'las', 'Ġfamily', 'Ġlaunch', 'Ġvehicles', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġtanks', 'Ġlonger', 'Ġuse', 'Ġstainless', 'Ġsteel', 'Ġmon', 'oco', 'que', 'Ġpressure', 'Ġstabilized', 'ball', 'oon', 'Ġconstruction', 'Ġtanks', 'og', 'rid', 'Ġaluminum', 'Ġstruct', 'urally', 'Ġstable', 'Ġun', 'press', 'urized', 'Ġaccommodation', 'Ġpoints', 'Ġparallel', 'Ġstages', 'Ġsmaller', 'Ġsol', 'ids', 'Ġidentical', 'Ġliquids', 'Ġbuilt', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġstructures', 'Ġstaging', 'Ġtechnique', 'Ġlonger', 'Ġused', 'Ġdiscontinued', 'las', 'Ġintroduction', 'Ġr', 'ussian', 'Ġr', 'Ġengine', 'Ġmain', 'stage', 'Ġdiameter', 'Ġincreased', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġuses', 'Ġpressure', 'st', 'abil', 'ized', 'Ġpropell', 'ant', 'tank', 'Ġdesign', 'Ġcry', 'ogenic', 'Ġpropell', 'ants', 'Ġcent', 'aur', 'Ġstage', 'las', 'Ġstretched', 'Ġft', 'Ġrelative', 'las', 'Ġcent', 'aur', 'Ġpowered', 'Ġeither', 'Ġone', 'Ġtwo', 'ero']</t>
+          <t>['Ġaluminum', 'Ġdom', 'es', 'Ġlanding', 'Ġlegs', 'Ġnumber', 'Ġmaterial', 'Ġcarbon', 'Ġï', '¬', 'ģ', 'ber', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġnumber', 'Ġmer', 'lin', 'Ġengines', 'Ġsea', 'Ġlevel', 'Ġpropell', 'ant', 'Ġthrust', 'Ġsea', 'Ġlevel', 'Ġkn', '000', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'sea', 'level', 'Ġsec', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'v', 'ac', 'uum', 'Ġsec', 'Ġsec', 'Ġburn', 'Ġtime', 'Ġsec', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġsecond', 'Ġstage', 'Ġdesign', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġinteractive', 'Ġmodel', 'Ġfal', 'con', 'Ġfully', 'Ġintegrated', 'Ġleft', 'Ġexploded', 'Ġview', 'Ġright', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'Ġlithium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġnumber', 'Ġmer', 'lin', 'Ġengines', 'Ġvacuum', 'Ġpropell', 'ant', 'Ġthrust', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'v', 'ac', 'uum', 'Ġsec', 'Ġburn', 'Ġtime', 'Ġsec', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengine', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġstages', 'Ġequipped', 'Ġmer', 'lin', 'Ġrocket', 'Ġengines', 'Ġevery', 'Ġmer', 'lin', 'Ġengine', 'Ġproduces', 'Ġkn', '000', 'Ġthrust', 'Ġuse', 'Ġpy', 'roph', 'oric', 'Ġmixture', 'te', 'te', 'b', 'Ġengine', 'Ġign', 'iter', 'Ġbooster', 'Ġstage', 'Ġengines', 'Ġarranged', 'Ġcon', 'g', 'uration', 'Ġspace', 'x', 'Ġcalls', 'Ġoct', 'aw', 'eb', 'Ġsecond', 'Ġstage', 'Ġfal', 'con', 'Ġshort', 'Ġregular', 'Ġnozzle', 'Ġmer', 'lin', 'Ġvacuum', 'Ġengine', 'Ġversion', 'Ġfal', 'con', 'Ġcapable', 'Ġlosing', 'Ġengines', 'Ġstill', 'Ġcomplete', 'Ġmission', 'Ġburning', 'Ġremaining', 'Ġengines', 'Ġlonger', 'Ġmer', 'lin', 'Ġrocket', 'Ġengine', 'Ġcontrolled', 'Ġthree', 'Ġvoting', 'Ġcomputers', 'Ġcp', 'us', 'Ġconstantly', 'Ġcheck', 'Ġtrio', 'Ġmer', 'lin', 'Ġengines', 'Ġvector', 'Ġthrust', 'Ġadjust', 'Ġtrajectory', 'Ġpropell', 'ant', 'Ġtank', 'Ġwalls', 'Ġdom', 'es']</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2076,7 +2076,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>['jet', 'Ġrocket', 'dy', 'ne', 'Ġengines', 'Ġengine', 'Ġdeveloping', 'Ġthrust', 'Ġkn', 'Ġinert', 'ial', 'Ġnavigation', 'Ġunit', 'u', 'Ġlocated', 'Ġcent', 'aur', 'Ġprovides', 'Ġguidance', 'Ġnavigation', 'las', 'Ġcent', 'aur', 'Ġcontrols', 'las', 'Ġcent', 'aur', 'Ġtank', 'Ġpressures', 'Ġpropell', 'ant', 'Ġuse', 'Ġcent', 'aur', 'Ġengines', 'Ġcapable', 'Ġmultiple', 'Ġins', 'pace', 'Ġstarts', 'Ġmaking', 'Ġpossible', 'Ġinsertion', 'Ġlow', 'Ġearth', 'Ġparking', 'Ġorbit', 'Ġfollowed', 'Ġcoast', 'Ġperiod', 'Ġinsertion', 'Ġg', 'Ġsubsequent', 'Ġthird', 'Ġburn', 'Ġfollowing', 'Ġmulti', 'hour', 'Ġcoast', 'Ġpermit', 'Ġdirect', 'Ġinjection', 'Ġpayload', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcent', 'aur', 'Ġvehicle', 'Ġhighest', 'Ġproportion', 'Ġburn', 'able', 'Ġpropell', 'ant', 'Ġrelative', 'Ġtotal', 'Ġmass', 'Ġmodern', 'Ġhydrogen', 'Ġupper', 'Ġstage', 'Ġhence', 'Ġdeliver', 'Ġsubstantial', 'Ġpayload', 'Ġhigh', 'energy', 'Ġstate', 'las', 'Ġpayload', 'Ġfair', 'ings', 'Ġavailable', 'Ġtwo', 'Ġdiam', 'eters', 'Ġdepending', 'Ġsatellite', 'Ġrequirements', 'Ġft', 'Ġdiameter', 'Ġfair', 'ing', 'Ġoriginally', 'Ġdesigned', 'las', 'Ġbooster', 'Ġcomes', 'Ġthree', 'Ġdifferent', 'Ġlengths', 'Ġoriginal', 'Ġft', 'Ġversion', 'Ġextended', 'Ġft', 'Ġversions', 'Ġfirst', 'Ġflown', 'Ġrespectively', 'Ġav', '008', 'ast', 'ra', 'Ġav', '004', 'ars', 'Ġmissions', 'Ġfair', 'ings', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġlength', 'Ġconsidered', 'Ġnever', 'Ġimplemented', 'Ġft', 'Ġdiameter', 'Ġfair', 'ing', 'Ġinternally', 'Ġusable', 'Ġdiameter', 'Ġft', 'Ġdeveloped', 'Ġbuilt', 'Ġru', 'ag', 'Ġspace', 'Ġsw', 'itzerland', 'Ġru', 'ag', 'Ġfair', 'ing', 'Ġuses', 'Ġcarbon', 'Ġfiber', 'Ġcomposite', 'Ġconstruction', 'Ġbased', 'Ġsimilar', 'Ġflight', 'proven', 'Ġfair', 'ing', 'ri', 'ane', 'Ġthree', 'Ġconfigurations', 'Ġmanufactured', 'Ġsupport', 'las', 'Ġv', 'Ġvehicle', 'Ġdescription', 'las', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġfair', 'ing', 'las', 'Ġwik', 'ipedia', 'show', 'show', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġv', 'af', 'b', 'Ġtotal', 'Ġlaunches', 'Ġsuccess']</t>
+          <t>['Ġmade', 'Ġaluminium', 'âĢĵ', 'l', 'ith', 'ium', 'Ġalloy', 'Ġspace', 'x', 'Ġuses', 'Ġfriction', 'st', 'ir', 'Ġweld', 'ed', 'Ġtank', 'Ġstrength', 'Ġreliability', 'Ġsecond', 'Ġstage', 'Ġtank', 'Ġshorter', 'Ġversion', 'Ġfirst', 'Ġstage', 'Ġtank', 'Ġuses', 'Ġtool', 'ing', 'Ġmaterial', 'Ġmanufacturing', 'Ġtechniques', 'Ġinter', 'stage', 'Ġconnects', 'Ġupper', 'Ġlower', 'Ġstages', 'Ġcarbon', 'f', 'ib', 'Ġaluminium', 'core', 'Ġcomposite', 'Ġstructure', 'Ġholds', 'Ġreusable', 'Ġseparation', 'Ġcol', 'lets', 'Ġp', 'ne', 'umatic', 'Ġpus', 'Ġsystem', 'Ġoriginal', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġtwelve', 'Ġattachment', 'Ġpoints', 'Ġreduced', 'Ġthree', 'Ġfal', 'con', 'Ġuses', 'Ġpayload', 'Ġfair', 'ing', 'n', 'ose', 'Ġcone', 'Ġprotect', 'non', 'dragon', 'Ġsatellites', 'Ġlaunch', 'Ġfair', 'ing', 'Ġft', 'Ġlong', 'Ġft', 'Ġdiameter', 'Ġweighs', 'Ġapproximately', 'Ġconstructed', 'Ġcarbon', 'Ġfiber', 'Ġskin', 'Ġoverl', 'aid', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġcore', 'Ġspace', 'x', 'Ġdesigned', 'Ġfabric', 'ates', 'Ġfair', 'ings', 'Ġhaw', 'th', 'orne', 'Ġtesting', 'Ġcompleted', 'Ġn', 'asa', "'s", 'Ġplum', 'Ġbro', 'ok', 'Ġstation', 'Ġfacility', 'Ġspring', 'Ġacoustic', 'Ġshock', 'Ġmechanical', 'Ġvibration', 'Ġlaunch', 'Ġplus', 'Ġelectromagnetic', 'Ġstatic', 'Ġdischarge', 'Ġconditions', 'Ġsimulated', 'Ġfull', 'size', 'Ġtest', 'Ġarticle', 'Ġvacuum', 'Ġchamber', 'Ġsince', 'Ġfair', 'ings', 'Ġdesigned', 'enter', 'Ġearth', "'s", 'Ġatmosphere', 'Ġreused', 'Ġfuture', 'Ġmissions', 'Ġengine', 'Ġtanks', 'Ġfair', 'ing', 'Ġcontrol', 'Ġsystems', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġlaunched', 'Ġdragon', 'Ġspacecraft', 'Ġdeliver', 'Ġcargo', 'Ġiss', 'Ġfal', 'con', 'left', 'right', 'Ġengine', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġv', 'enberg', 'fal', 'con', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġuses', 'Ġmultiple', 'Ġredundant', 'Ġflight', 'Ġcomputers', 'Ġfault', 'oler', 'ant', 'Ġdesign', 'Ġsoftware', 'Ġruns', 'Ġlinux', 'Ġwritten', 'Ġflexibility', 'Ġcommercial', 'lf', 'Ġparts', 'Ġsystem', 'wide', 'Ġradiation', 'oler', 'ant', 'Ġdesign', 'Ġused', 'Ġinstead', 'Ġrad', 'hard', 'ened', 'Ġparts', 'Ġstage', 'Ġstage', 'level', 'Ġflight', 'Ġcomputers', 'Ġaddition', 'Ġmer', 'lin', 'specific', 'Ġengine', 'Ġcontrollers', 'Ġfault', 'oler', 'ant', 'Ġtri', 'ad', 'Ġdesign', 'Ġhandle', 'Ġstage', 'Ġcontrol', 'Ġfunctions', 'Ġengine', 'Ġmicro', 'controller', 'Ġruns', 'Ġpower', 'pc', 'Ġarchitecture', 'Ġboosters', 'Ġdeliberately', 'Ġexpended', 'Ġlegs']</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>['es', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġhot', 'Ġbird', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'mber', 'Ġtype', 'Ġpassengers', 'c', 'argo', 'Ġspace', 'Ġprobes', 'Ġpersever', 'ance', 'Ġcuriosity', 'Ġinsight', 'Ġjun', 'Ġl', 'ro', 'Ġl', 'cross', 'ms', 'aven', 'Ġnew', 'Ġhor', 'izons', 'Ġos', 'iris', 'rex', 'Ġsolar', 'Ġdynamics', 'Ġobserv', 'atory', 'Ġvan', 'en', 'Ġprobes', 'Ġbo', 'e', 'ing', 'Ġcy', 'gn', 'us', 'Ġsolo', 'Ġstar', 'liner', 'Ġgoes', 'Ġtd', 'rs', 'Ġn', 'ro', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġpayload', 'Ġintruder', 'Ġqu', 'asar', 'b', 'irs', 'Ġft', 'Ġft', 'Ġft', 'Ġlong', 'Ġclassic', 'Ġft', 'Ġfair', 'ing', 'Ġcovers', 'Ġpayload', 'Ġru', 'ag', 'Ġfair', 'ing', 'Ġmuch', 'Ġlonger', 'Ġfully', 'Ġencl', 'oses', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġmany', 'Ġsystems', 'las', 'Ġsubject', 'Ġupgrade', 'Ġenhancement', 'Ġprior', 'Ġfirst', 'las', 'Ġflight', 'Ġsince', 'Ġtime', 'Ġwork', 'Ġnew', 'Ġfault', 'Ġtolerant', 'Ġinert', 'ial', 'Ġnavigation', 'Ġunit', 'ft', 'u', 'Ġstarted', 'Ġenhance', 'Ġmission', 'Ġreliability', 'las', 'Ġvehicles', 'Ġreplacing', 'Ġexisting', 'Ġnon', 'red', 'und', 'ant', 'Ġnavigation', 'Ġcomputing', 'Ġequipment', 'Ġfault', 'oler', 'ant', 'Ġunit', 'Ġupgraded', 'Ġft', 'u', 'Ġfirst', 'Ġflew', 'Ġfollow', 'Ġorder', 'Ġft', 'u', 'Ġunits', 'Ġawarded', 'Ġu', 'la', 'Ġannounced', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'produced', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġuse', 'las', 'Ġwould', 'Ġsupers', 'eded', 'Ġnew', 'Ġgem', 'Ġboosters', 'Ġproduced', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'Ġextended', 'Ġgem', 'Ġboosters', 'Ġalso', 'Ġused', 'Ġvul', 'Ġcent', 'aur', 'Ġlaunch', 'Ġvehicle', 'Ġreplace', 'las', 'Ġfirst', 'las', 'Ġlaunch', 'Ġgem', 'Ġboosters', 'Ġhappened', 'mber', 'Ġproposals', 'Ġdesign', 'Ġwork', 'Ġhuman', 'rate', 'las', 'Ġbegan', 'Ġearly', 'Ġu', 'la', "'s", 'Ġparent', 'Ġcompany', 'Ġlock', 'heed', 'Ġmart', 'Ġreporting', 'Ġagreement', 'Ġbig', 'el', 'ow', 'Ġaerospace', 'Ġintended', 'Ġlead', 'Ġcommercial', 'Ġprivate', 'Ġtrips', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġhuman', 'rating', 'Ġdesign', 'Ġsimulation', 'Ġwork', 'Ġbegan', 'Ġearnest', 'Ġaward', 'Ġmillion', 'Ġfirst', 'Ġphase', 'Ġn', 'asa', 'Ġcommercial', 'Ġcrew']</t>
+          <t>['Ġfins', 'Ġrecover', 'able', 'Ġboosters', 'Ġinclude', 'Ġfour', 'Ġext', 'ensible', 'Ġlanding', 'Ġlegs', 'Ġattached', 'Ġaround', 'Ġbase', 'Ġcontrol', 'Ġcore', "'s", 'Ġdescent', 'Ġatmosphere', 'Ġspace', 'x', 'Ġuses', 'Ġgrid', 'Ġfins', 'Ġdeploy', 'Ġvehicle', 'Ġmoments', 'Ġstage', 'Ġseparation', 'Ġflew', 'Ġfive', 'Ġsuccessful', 'Ġorbital', 'Ġlaunches', 'âĢĵ', 'Ġmuch', 'Ġlarger', 'Ġmade', 'Ġfirst', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġdemonstration', 'Ġmission', 'Ġcarried', 'Ġsmall', 'Ġprimary', 'Ġpayload', 'Ġcass', 'ope', 'Ġsatellite', 'Ġlarger', 'Ġpayload', 'Ġfollowed', 'Ġstarting', 'Ġlaunch', 'Ġgeo', 'Ġcommunications', 'Ġsatellite', 'Ġused', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicles', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmade', 'Ġfirst', 'Ġflight', 'Ġde', 'cember', 'Ġfirst', 'Ġstage', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġreusable', 'Ġcurrent', 'Ġversion', 'Ġknown', 'Ġfal', 'con', 'Ġblock', 'Ġmade', 'Ġfirst', 'Ġflight', 'Ġmay', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'Ġdeveloped', 'âĢĵ', 'Ġflew', 'Ġfirst', 'Ġtime', 'Ġmade', 'Ġfive', 'Ġflights', 'Ġretired', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġnine', 'Ġmer', 'lin', 'Ġengines', 'Ġarranged', 'Ġgrid', 'Ġsea', 'level', 'Ġthrust', 'Ġkn', '000', 'Ġtotal', 'Ġlif', 'ff', 'Ġthrust', '000', 'Ġkn', '000', 'Ġsecond', 'Ġstage', 'Ġpowered', 'Ġsingle', 'Ġmer', 'lin', 'Ġengine', 'Ġmodified', 'Ġvacuum', 'Ġoperation', 'Ġexpansion', 'Ġratio', 'Ġnominal', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġg', 'ase', 'ous', 'Ġthr', 'usters', 'Ġused', 'Ġsecond', 'stage', 'Ġreaction', 'Ġcontrol', 'Ġsystem', 'Ġearly', 'Ġattempts', 'Ġadd', 'Ġlightweight', 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġbooster', 'Ġstage', 'Ġparachute', 'Ġrecovery', 'Ġsuccessful', 'Ġspace', 'x', 'Ġbegan', 'Ġformal', 'Ġdevelopment', 'Ġprogram', 'Ġreusable', 'Ġfal', 'con', 'Ġinitially', 'Ġfocusing', 'Ġfirst', 'Ġstage', 'Ġheavier', 'Ġthrust', 'Ġnine', 'Ġpowerful', 'Ġmer', 'lin', 'Ġengines', 'Ġrearr', 'anged', 'oct', 'agonal', 'Ġpattern', 'Ġspace', 'x', 'Ġcalled', 'Ġoct', 'aw', 'eb', 'Ġdesigned', 'Ġsimplify', 'Ġstream', 'line', 'Ġfuel', 'Ġtanks', 'Ġlonger', 'Ġmaking', 'Ġrocket', 'Ġsusceptible', 'Ġbending', 'Ġflight', 'Ġfirst', 'Ġstage', 'Ġoffered', 'Ġtotal', 'Ġsea', 'level', 'Ġthrust', 'Ġlif', 'ff', 'Ġkil', 'onew', 'tons', '000', 'Ġengines', 'Ġburning', 'Ġnominal', 'Ġseconds', 'Ġstage', 'Ġthrust', 'Ġrises', 'Ġkn', '000']</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2102,7 +2102,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>['Ġprogram', 'Ġdevelop', 'Ġemergency', 'Ġdetection', 'Ġsystem', 'eds', ').[', 'Ġfe', 'b', 'ruary', 'Ġu', 'la', 'Ġreceived', 'Ġextension', 'Ġapr', 'il', 'Ġn', 'asa', 'Ġfinishing', 'Ġwork', 'Ġed', 'Ġn', 'asa', 'Ġsolic', 'ited', 'Ġproposals', 'Ġphase', 'Ġoct', 'ober', 'Ġu', 'la', 'Ġproposed', 'Ġcomplete', 'Ġdesign', 'Ġwork', 'Ġed', 'Ġtime', 'Ġn', 'asa', "'s", 'Ġgoal', 'Ġget', 'Ġastronauts', 'Ġorbit', 'ula', 'Ġpresident', 'Ġce', 'ichael', 'Ġg', 'ass', 'Ġstated', 'Ġschedule', 'Ġacceleration', 'Ġpossible', 'Ġfunded', 'Ġaddition', 'Ġemergency', 'Ġdetection', 'Ġsystem', 'Ġmajor', 'Ġchanges', 'Ġexpected', 'las', 'Ġrocket', 'Ġground', 'Ġinfrastructure', 'Ġmodifications', 'Ġplanned', 'Ġlikely', 'Ġcandidate', 'Ġhuman', 'rating', 'Ġconfiguration', 'Ġfair', 'ing', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġdual', 'Ġengines', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġu', 'la', 'Ġannounced', 'Ġagreement', 'Ġpossibility', 'Ġcert', 'ifying', 'las', 'Ġn', 'asa', "'s", 'Ġstandards', 'Ġhuman', 'Ġspace', 'flight', 'Ġu', 'la', 'Ġagreed', 'Ġprovide', 'Ġn', 'asa', 'Ġdata', 'las', 'Ġv', 'Ġn', 'asa', 'Ġwould', 'Ġprovide', 'Ġu', 'la', 'Ġdraft', 'Ġhuman', 'Ġcertification', 'Ġrequirements', 'Ġhuman', 'rated', 'las', 'Ġalso', 'Ġstill', 'Ġconsideration', 'Ġcarry', 'Ġspace', 'flight', 'Ġparticipants', 'Ġproposed', 'Ġbig', 'el', 'ow', 'Ġcommercial', 'Ġspace', 'Ġstation', 'ierra', 'Ġne', 'v', 'ada', 'Ġcorporation', 'nc', 'Ġpicked', 'las', 'Ġbooster', 'Ġdream', 'Ġch', 'aser', 'Ġcrew', 'ed', 'Ġspace', 'plane', 'Ġdream', 'Ġch', 'aser', 'Ġintended', 'Ġlaunch', 'las', 'Ġv', 'Ġfly', 'Ġcrew', 'Ġiss', 'Ġlanding', 'Ġhorizontally', 'Ġfollowing', 'Ġlifting', 'body', 'entry', 'Ġhowever', 'Ġlate', 'Ġn', 'asa', 'Ġselect', 'Ġdream', 'Ġch', 'aser', 'Ġone', 'Ġtwo', 'Ġvehicles', 'Ġselected', 'Ġcommercial', 'Ġcrew', 'Ġcompetition', 'Ġaug', 'ust', 'Ġbo', 'e', 'ing', 'Ġannounced', 'Ġwould', 'Ġuse', 'las', 'Ġinitial', 'Ġlaunch', 'Ġvehicle', 'Ġc', 'st', 'Ġcrew', 'Ġcapsule', 'Ġc', 'st', 'Ġtake', 'Ġn', 'asa', 'Ġastronauts', 'Ġinternational', 'Ġspace', 'Ġstation', 'iss', 'Ġalso', 'Ġintended', 'Ġservice', 'Ġproposed', 'Ġbig', 'el', 'ow', 'Ġcommercial', 'Ġspace', 'Ġstation', 'Ġthree', 'flight', 'Ġtest', 'Ġprogram', 'Ġprojected', 'Ġcompleted', 'Ġcert', 'ifying', 'las', 'Ġcombination', 'Ġhuman', 'Ġspace']</t>
+          <t>['Ġbooster', 'Ġclimbs', 'Ġatmosphere', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġredesigned', 'Ġreduce', 'Ġnumber', 'Ġattachment', 'Ġpoints', 'Ġtwelve', 'Ġthree', 'Ġvehicle', 'Ġupgraded', 'Ġav', 'ionics', 'Ġsoftware', 'Ġimprovements', 'Ġincreased', 'Ġpayload', 'Ġcapability', '000', '000', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġstated', 'Ġpayload', 'Ġcapacity', 'Ġpublished', 'Ġprice', 'Ġlist', 'Ġextra', 'Ġmargin', 'Ġreserved', 'Ġreturning', 'Ġstages', 'Ġvia', 'Ġpowered', 'entry', 'Ġdevelopment', 'Ġtesting', 'Ġfirst', 'Ġstage', 'Ġcompleted', 'Ġj', 'uly', 'Ġfirst', 'Ġlaunch', 'Ġcame', 'Ġse', 'pt', 'ember', 'Ġsecond', 'Ġstage', 'Ġign', 'iter', 'Ġpropell', 'ant', 'Ġlines', 'Ġlater', 'Ġinsulated', 'Ġbetter', 'Ġsupport', 'space', 'Ġrestart', 'Ġfollowing', 'Ġlong', 'Ġcoast', 'Ġphases', 'Ġorbital', 'Ġtrajectory', 'Ġmaneuvers', 'Ġfour', 'Ġext', 'ensible', 'Ġcarbon', 'Ġfiber', 'al', 'uminum', 'Ġhoney', 'comb', 'Ġlanding', 'Ġlegs', 'Ġincluded', 'Ġlater', 'Ġflights', 'Ġland', 'ings', 'Ġlegs', 'ï', '¬', 'ģ', 'ns', 'Ġversions', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġclose', 'Ġnewer', 'Ġtitanium', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'Ġsecond', 'Ġir', 'idium', 'Ġnext', 'Ġmission', 'Ġj', 'une', 'Ġspace', 'x', 'Ġpricing', 'Ġpayload', 'Ġspecifications', 'Ġpublished', 'Ġmarch', 'Ġincluded', 'Ġperformance', 'Ġpublished', 'Ġprice', 'Ġlist', 'Ġindicated', 'Ġspace', 'x', 'Ġreserved', 'Ġadditional', 'Ġperformance', 'Ġperform', 'us', 'ability', 'Ġtesting', 'Ġmany', 'Ġengineering', 'Ġchanges', 'Ġsupport', 'us', 'ability', 'Ġrecovery', 'Ġfirst', 'Ġstage', 'Ġmade', 'Ġupgrade', 'Ġalso', 'Ġknown', 'Ġfull', 'Ġthrust', 'Ġmade', 'Ġmajor', 'Ġchanges', 'Ġadded', 'Ġcry', 'ogenic', 'Ġpropell', 'ant', 'Ġcooling', 'Ġincrease', 'Ġdensity', 'Ġallowing', 'Ġhigher', 'Ġthrust', 'Ġimproved', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġstretched', 'Ġsecond', 'Ġstage', 'Ġhold', 'Ġadditional', 'Ġpropell', 'ant', 'Ġstrengthened', 'Ġstr', 'uts', 'Ġholding', 'Ġhelium', 'Ġbottles', 'Ġbelieved', 'Ġinvolved', 'Ġfailure', 'Ġflight', 'Ġoffered', 'Ġreusable', 'Ġfirst', 'Ġstage', 'Ġplans', 'Ġreuse', 'Ġsecond', 'stage', 'Ġabandoned', 'Ġweight', 'Ġheat', 'Ġshield', 'Ġequipment', 'Ġwould', 'Ġreduce', 'Ġpayload', 'Ġreusable', 'Ġbooster', 'Ġdeveloped', 'Ġusing', 'Ġsystems', 'Ġsoftware', 'Ġtested', 'Ġfal', 'con', 'Ġprototypes', 'Ġautonomous', 'Ġflight', 'Ġsafety', 'Ġsystem', 'af', 'ss', 'Ġreplaced', 'Ġground', 'based', 'Ġmission', 'Ġflight', 'Ġcontrol', 'Ġpersonnel', 'Ġequipment', 'Ġaf', 'ss', 'Ġoffered', 'board', 'Ġpositioning', 'Ġnavigation', 'Ġtiming', 'Ġsources', 'Ġdecision', 'Ġlogic', 'Ġbenefits', 'Ġaf', 'ss', 'Ġincluded', 'Ġincreased', 'Ġpublic', 'Ġsafety', 'Ġreduced', 'Ġreliance', 'Ġrange', 'Ġinfrastructure']</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2115,7 +2115,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>['flight', 'Ġoperations', 'Ġfirst', 'Ġflight', 'Ġexpected', 'Ġinclude', 'las', 'Ġrocket', 'Ġintegrated', 'Ġunc', 'rew', 'ed', 'Ġc', 'st', 'Ġcapsule', 'Ġsecond', 'Ġflight', 'flight', 'Ġlaunch', 'Ġabort', 'Ġsystem', 'Ġdemonstration', 'Ġmiddle', 'Ġyear', 'Ġthird', 'Ġflight', 'Ġcrew', 'ed', 'Ġmission', 'Ġcarrying', 'Ġtwo', 'Ġbo', 'e', 'ing', 'Ġtest', 'p', 'ilot', 'Ġastronauts', 'Ġle', 'Ġreturning', 'Ġsafely', 'Ġend', 'Ġplans', 'Ġmaterial', 'ize', 'Ġn', 'asa', 'Ġselected', 'Ġbo', 'e', 'ing', 'Ġc', 'st', 'Ġspace', 'Ġcapsule', 'Ġpart', 'Ġprogram', 'Ġextensive', 'Ġdelays', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġc', 'st', 'Ġfirst', 'Ġlaunch', 'Ġunc', 'rew', 'ed', 'Ġc', 'st', 'Ġcapsule', 'Ġbo', 'e', 'ing', 'Ġoft', 'Ġoccurred', 'Ġatop', 'Ġhuman', 'rated', 'las', 'Ġmorning', 'Ġde', 'cember', 'Ġmission', 'Ġfailed', 'Ġmeet', 'Ġgoals', 'Ġdue', 'Ġspacecraft', 'Ġfailure', 'Ġthough', 'las', 'Ġlauncher', 'Ġperformed', 'Ġwell', 'las', 'Ġlaunched', 'Ġstar', 'liner', 'Ġcapsule', 'Ġsecond', 'Ġtime', 'Ġending', 'Ġmission', 'Ġsuccess', 'azon', 'Ġselected', 'las', 'Ġlaunch', 'Ġsatellites', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġoffer', 'Ġhigh', 'speed', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'Ġservice', 'Ġcontract', 'Ġsigned', 'azon', 'Ġnine', 'Ġlaunches', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġaims', 'Ġput', 'Ġthousands', 'Ġsatellites', 'Ġorbit', 'Ġu', 'la', 'azon', "'s", 'Ġfirst', 'Ġlaunch', 'Ġprovider', 'las', 'Ġbooster', 'Ġconfiguration', 'Ġthree', 'digit', 'Ġdesignation', 'Ġfirst', 'Ġdigit', 'Ġshows', 'Ġdiameter', 'Ġmeters', 'Ġpayload', 'Ġfair', 'ing', 'Ġvalue', 'Ġfair', 'ing', 'Ġlaunches', 'n', 'Ġcrew', 'Ġcapsule', 'Ġlaunches', 'Ġpayload', 'Ġfair', 'ing', 'Ġused', 'Ġcrew', 'Ġcapsule', 'Ġlaunched', 'Ġsecond', 'Ġdigit', 'Ġindicates', 'Ġnumber', 'Ġsolid', 'Ġrocket', 'Ġupgrades', 'Ġhuman', 'rating', 'Ġcertification', 'Ġproject', 'Ġk', 'ui', 'per', 'Ġversions', 'las', 'Ġwik', 'ipedia', 'Ġtop', 'az', 'Ġboosters', 'Ġboosters', 'Ġheight', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġmaximum', 'Ġthrust', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġboosters', 'Ġgem']</t>
+          <t>['Ġreduced', 'Ġrange', 'Ġspac', 'el', 'ift', 'Ġcost', 'Ġincreased', 'Ġschedule', 'Ġpredict', 'ability', 'Ġavailability', 'Ġoperational', 'Ġflexibility', 'Ġlaunch', 'Ġslot', 'Ġflexibility', '".[', 'Ġft', "'s", 'Ġcapacity', 'Ġallowed', 'Ġspace', 'x', 'Ġchoose', 'Ġincreasing', 'Ġpayload', 'Ġdecreasing', 'Ġlaunch', 'Ġprice', 'Ġfirst', 'Ġsuccessful', 'Ġlanding', 'Ġcame', 'Ġde', 'cember', 'Ġfirst', 'Ġref', 'light', 'Ġmarch', 'Ġfe', 'b', 'ruary', 'Ġcr', 'Ġlaunch', 'Ġfirst', 'Ġoperational', 'Ġlaunch', 'Ġutilizing', 'Ġaf', 'ss', 'Ġspace', 'x', 'Ġlaunches', 'Ġmarch', 'Ġused', 'Ġaf', 'ss', 'Ġj', 'une', 'Ġmission', 'Ġcarried', 'Ġsecond', 'Ġbatch', 'Ġten', 'Ġir', 'idium', 'Ġnext', 'Ġsatellites', 'Ġaluminium', 'Ġgrid', 'Ġfins', 'Ġreplaced', 'Ġlarger', 'Ġtitanium', 'Ġversions', 'Ġimprove', 'Ġcontrol', 'Ġauthority', 'Ġheat', 'Ġtolerance', 'entry', 'Ġspace', 'x', 'Ġstarted', 'Ġincluding', 'Ġincremental', 'Ġchanges', 'Ġinternally', 'Ġdubbed', 'Ġblock', 'Ġinitially', 'Ġsecond', 'Ġstage', 'Ġmodified', 'Ġblock', 'Ġstandards', 'Ġflying', 'Ġtop', 'Ġblock', 'Ġfirst', 'Ġstage', 'Ġthree', 'Ġmissions', 'ars', 'Ġmay', 'Ġint', 'els', 'Ġj', 'uly', 'Ġblock', 'Ġdescribed', 'Ġtransition', 'Ġfull', 'Ġthrust', 'Ġblock', 'Ġblock', 'Ġincludes', 'Ġincremental', 'Ġengine', 'Ġthrust', 'Ġupgrades', 'Ġleading', 'Ġblock', 'Ġmaiden', 'Ġflight', 'Ġfull', 'Ġblock', 'Ġdesign', 'first', 'Ġsecond', 'Ġstages', 'Ġspace', 'x', 'Ġcr', 'Ġmission', 'Ġaug', 'ust', 'Ġv', 'full', 'Ġthrust', 'Ġblock', 'Ġblock', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġoct', 'ober', 'Ġmus', 'k', 'Ġdescribed', 'Ġblock', 'Ġcoming', 'Ġlot', 'Ġminor', 'Ġrefin', 'ements', 'Ġcollectively', 'Ġimportant', 'rated', 'Ġthrust', 'Ġimproved', 'Ġlegs', 'Ġsignificant', '".[', 'Ġjan', 'uary', 'Ġmus', 'k', 'Ġadded', 'Ġblock', 'sign', 'ificantly', 'Ġimproves', 'Ġperformance', 'Ġease', 'us', 'ability', '".[', 'Ġmaiden', 'Ġflight', 'Ġtook', 'Ġplace', 'Ġmay', 'Ġbang', 'aband', 'hu', 'Ġsatellite', 'Ġsatellite', 'Ġblock', 'Ġsecond', 'Ġstage', 'Ġincluded', 'Ġupgrades', 'Ġenable', 'Ġlinger', 'Ġorbit', 'Ġreign', 'ite', 'Ġengine', 'Ġthree', 'Ġtimes', 'Ġversion', 'ret', 'ired', 'ret', 'ired', 'Ġfull', 'Ġthrust', 'Ġblock', 'Ġblock', 'ret', 'ired', 'Ġblock', 'active', ')[', 'Ġstage', 'Ġengines', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġmer', 'lin', 'graded', ')[', 'Ġmer', 'lin', 'graded', 'Ġstage']</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2128,7 +2128,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>['Ġboosters', 'Ġheight', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfirst', 'Ġstage', 'las', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', '05', 'Ġpropell', 'ant', 'Ġmass', '089', 'Ġpowered', 'Ġr', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'sea', 'Ġlevel', 'Ġkn', '000', 'v', 'ac', 'uum', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', '05', 'sea', 'Ġlevel', 'v', 'ac', 'uum', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'Ġcent', 'aur', 'Ġheight', 'Ġft', 'Ġdiameter', '05', 'Ġft', 'Ġempty', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġpowered', 'sec', 'dec', 'las', 'Ġfamily', 'Ġasymm', 'etric', 'Ġdeveloped', 'Ġboosters', 'Ġattached', 'Ġbase', 'Ġlaunch', 'Ġvehicle', 'Ġrange', 'Ġft', 'Ġfair', 'ing', 'Ġft', 'Ġfair', 'ing', 'Ġseen', 'Ġfirst', 'Ġimage', 'Ġlayouts', 'Ġasymm', 'etrical', 'Ġthird', 'Ġdigit', 'Ġrepresents', 'Ġnumber', 'Ġengines', 'Ġcent', 'aur', 'Ġstage', 'Ġeither', '".', 'Ġexample', 'las', 'meter', 'Ġfair', 'ing', 'Ġcent', 'aur', 'Ġengine', 'Ġwhereas', 'las', 'meter', 'Ġfair', 'ing', 'Ġcent', 'aur', 'Ġengine', 'las', 'Ġfair', 'ing', 'Ġtwo', 'Ġcent', 'aur', 'Ġengines', 'Ġfirst', 'Ġlaunched', 'Ġflight', 'Ġcarried', 'Ġstar', 'liner', 'Ġvehicle', 'Ġfirst', 'Ġorbital', 'Ġtest', 'Ġflight', 'Ġj', 'une', 'Ġversions', 'las', 'Ġv', 'Ġdesign', 'Ġproduction', 'Ġrights', 'Ġintellectual', 'Ġproperty', 'Ġrights', 'Ġowned', 'Ġu', 'la', 'Ġlock', 'heed', 'Ġmart', 'Ġlist', 'Ġdate', 'Ġaug', 'ust', 'Ġmass', 'Ġle', 'Ġnumbers', 'Ġinclination']</t>
+          <t>['Ġmass', 'Ġdry', 'Ġmass', '000', 'Ġstage', 'Ġengines', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmer', 'lin', 'Ġvacuum', 'graded', ')[', 'Ġmer', 'lin', 'Ġvacuum', 'graded', 'short', 'Ġregular', 'Ġnozzle', 'Ġstage', 'Ġmass', 'Ġdry', 'Ġmass', 'Ġheight', 'Ġdiameter', 'Ġinitial', 'Ġthrust', 'Ġtf', ')[', 'Ġtakeoff', 'Ġmass', '000', '000', '000', '000', 'Ġfair', 'ing', 'Ġdiameter', 'ĠâĢĶ', 'Ġfair', 'ing', 'Ġmass', 'Ġpayload', 'Ġle', 'Ġcape', 'aver', 'al', 'âĢĵ', '000', 'exp', 'end', 'able', ')[', 'b', 'exp', 'end', 'able', 'usable', ')[', 'c', 'Ġpayload', 'Ġg', 'exp', 'end', 'able', 'usable', 'exp', 'end', 'able', 'usable', ')[', 'Ġsuccess', 'Ġratio', 'Ġpre', 'cluded', ')[', 'f', 'Ġfal', 'con', 'Ġlaunched', 'Ġdragon', 'Ġspacecraft', 'Ġnever', 'Ġlaunched', 'Ġclam', 'shell', 'Ġpayload', 'Ġfair', 'ing', 'Ġb', 'Ġpayload', 'Ġrestricted', '000', 'Ġdue', 'Ġstructural', 'Ġlimit', 'Ġpayload', 'Ġadapter', 'Ġï', '¬', 'ģ', 'ting', 'p', 'af', ').[', 'Ġc', 'Ġheaviest', 'Ġexplicitly', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġpayload', 'Ġspace', 'x', 'Ġprimary', 'Ġpayload', 'Ġdragon', 'Ġsuccessful', 'Ġsecondary', 'Ġpayload', 'Ġplaced', 'Ġincorrect', 'Ġorbit', 'Ġchanged', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġpro', 'ï', '¬', 'ģ', 'le', 'Ġdue', 'Ġmalfunction', 'Ġshut', 'Ġsingle', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġengine', 'Ġlikely', 'Ġenough', 'Ġfuel', 'Ġoxid', 'izer', 'Ġremained', 'Ġsecond', 'Ġstage']</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>['Â°', 'Ġupper', 'Ġstages', 'Ġsec', 'Ġsingle', 'Ġengine', 'Ġcent', 'aur', 'Ġdec', 'Ġdual', 'Ġengine', 'Ġcent', 'aur', 'Ġlaunch', 'Ġsystem', 'Ġstatus', 'Ġactive', 'Ġretired', 'Ġnever', 'Ġlaunched', 'Ġplanned', 'Ġcapabilities', 'las', 'Ġwik', 'ipedia', 'Ġmaximum', 'Ġthrust', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'las', 'Ġversion', 'Ġfair', 'ing', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġle', 'Ġpayload', 'Ġg', 'Ġlaunches', 'Ġdate', 'Ġbase', 'Ġprice', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġsec', 'Ġus', 'Ġmillion', 'Ġdec', 'Ġheavy', 'Ġsec', 'Ġheavy', 'Ġdec', 'Ġdec', 'las', 'Ġwik', 'ipedia', 'Ġversion', 'Ġfair', 'ing', 'Ġupper', 'Ġstage', 'Ġpayload', 'Ġle', 'Ġpayload', 'Ġg', 'Ġlaunches', 'Ġdate', 'Ġbase', 'Ġprice', 'Ġc', 'st', 'Ġstar', 'liner', 'Ġnone', 'Ġdec', '000', 'Ġiss', 'Ġpricing', 'Ġinformation', 'las', 'Ġlaunches', 'Ġlimited', 'Ġn', 'asa', 'Ġcontracted']</t>
+          <t>['Ġorbital', 'Ġinsertion', 'Ġenough', 'Ġwithin', 'Ġn', 'asa', 'Ġsafety', 'Ġmargins', 'Ġprotection', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġe', 'Ġfailed', 'Ġmission', 'Ġfal', 'con', 'Ġspace', 'x', 'Ġlost', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġoperation', 'Ġdue', 'pressure', 'Ġevent', 'Ġsecond', 'Ġstage', 'Ġtank', 'Ġf', 'Ġone', 'Ġrocket', 'Ġpayload', 'Ġdestroyed', 'Ġlaunch', 'Ġpreparation', 'Ġroutine', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġachieved', 'Ġfull', 'Ġmission', 'Ġsuccesses', '%).', 'Ġspace', 'x', 'Ġsucceeded', 'Ġprimary', 'Ġmission', 'Ġleft', 'Ġsecondary', 'Ġpayload', 'Ġwrong', 'Ġorbit', 'Ġspace', 'x', 'Ġdestroyed', 'Ġflight', 'Ġaddition', 'Ġdisinteg', 'rated', 'Ġlaunch', 'Ġpad', 'Ġfueling', 'Ġengine', 'Ġtest', 'Ġbased', 'Ġpoint', 'Ġestimation', 'Ġestimate', 'Ġreliability', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġbecome', 'Ġreliable', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġoperation', 'Ġblock', 'Ġsuccess', 'Ġrate', 'Ġcomparison', 'Ġindustry', 'Ġbenchmark', 'Ġseries', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', 'Ġlatest', 'Ġsuccess', 'Ġrate', '%),', 'Ġr', 'ussian', 'Ġpro', 'ton', 'Ġseries', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', 'Ġlatest', 'Ġpro', 'ton', "'s", 'Ġsuccess', 'Ġrate', '%),', 'Ġeuro', 'pe', 'ri', 'ane', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', '%,', 'Ġch', 'inese', 'Ġlong', 'Ġmarch', 'Ġperformed', 'Ġlaunches', 'Ġsuccess', 'Ġrate', '%.', 'Ġlaunch', 'Ġsequence', 'Ġincludes', 'Ġhold', 'Ġfeature', 'Ġallows', 'Ġfull', 'Ġengine', 'Ġignition', 'Ġsystems', 'Ġcheck', 'Ġlif', 'ff', 'Ġfirst', 'stage', 'Ġengine', 'Ġstarts', 'Ġlauncher', 'Ġheld', 'Ġreleased', 'Ġflight', 'Ġpropulsion', 'Ġvehicle', 'Ġsystems', 'Ġconfirmed', 'Ġoperating', 'Ġnormally', 'Ġsimilar', 'Ġhold', 'Ġsystems', 'Ġused', 'Ġlaunch', 'Ġvehicles', 'Ġsat', 'urn', 'Ġspace', 'Ġshuttle', 'Ġautomatic', 'Ġsafe', 'Ġshut', 'cap', 'abilities', 'Ġperformance', 'Ġreliability', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġun', 'loading', 'Ġpropell', 'ant', 'Ġoccur', 'Ġabnormal', 'Ġconditions', 'Ġdetected', 'Ġprior', 'Ġlaunch', 'Ġdate', 'Ġspace', 'x', 'Ġtypically', 'Ġcompletes', 'Ġtest', 'Ġcycle', 'Ġculminating', 'Ġthree', 'half', 'Ġsecond', 'Ġfirst', 'Ġstage', 'Ġengine', 'Ġstatic', 'Ġfiring', 'Ġtriple', 'red', 'und', 'ant', 'Ġflight', 'Ġcomputers', 'Ġinert', 'ial', 'Ġnavigation', 'Ġoverlay', 'Ġadditional']</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>['Ġu', 'la', 'Ġlaunch', 'aven', 'Ġmission', 'las', 'Ġapproximately', 'Ġus', 'Ġmillion', 'Ġcost', 'Ġconfiguration', 'Ġu', 'Ġair', 'Ġforce', 'Ġblock', 'Ġlaunch', 'Ġvehicles', 'Ġus', 'Ġmillion', 'Ġtd', 'rs', 'Ġlaunch', 'las', 'Ġcost', 'Ġn', 'asa', 'Ġus', 'Ġmillion', 'Ġstarting', 'Ġu', 'la', 'Ġprovided', 'Ġpricing', 'las', 'Ġrocket', 'builder', 'Ġwebsite', 'Ġadvertising', 'Ġbase', 'Ġprice', 'Ġlaunch', 'Ġvehicle', 'Ġconfiguration', 'Ġranges', 'Ġus', 'Ġmillion', 'Ġus', 'Ġmillion', 'Ġadditional', 'Ġadds', 'Ġaverage', 'Ġmillion', 'Ġcost', 'Ġlaunch', 'Ġvehicle', 'Ġcustomers', 'Ġalso', 'Ġchoose', 'Ġpurchase', 'Ġlarger', 'Ġpayload', 'Ġfair', 'ings', 'Ġadditional', 'Ġlaunch', 'Ġservice', 'Ġoptions', 'Ġn', 'asa', 'Ġair', 'Ġforce', 'Ġlaunch', 'Ġcosts', 'Ġoften', 'Ġhigher', 'Ġequivalent', 'Ġcommercial', 'Ġmissions', 'Ġdue', 'Ġadditional', 'Ġgovernment', 'Ġaccounting', 'Ġanalysis', 'Ġprocessing', 'Ġmission', 'Ġassurance', 'Ġrequirements', 'Ġadd', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġcost', 'Ġlaunch', 'Ġlaunch', 'Ġcosts', 'Ġcommercial', 'Ġsatellites', 'Ġg', 'Ġaveraged', 'Ġus', 'Ġmillion', 'Ġsignificantly', 'Ġlower', 'Ġhistoric', 'las', 'Ġpricing', 'Ġhowever', 'Ġrecent', 'Ġyears', 'Ġprice', 'las', 'Ġdropped', 'Ġapproximately', 'Ġus', 'Ġmillion', 'Ġus', 'Ġmillion', 'Ġlarge', 'Ġpart', 'Ġdue', 'Ġcompetitive', 'Ġpressure', 'Ġemerged', 'Ġlaunch', 'Ġservices', 'Ġmarketplace', 'Ġearly', 'Ġu', 'la', 'Ġce', 'ory', 'Ġbr', 'uno', 'Ġstated', 'Ġu', 'la', 'Ġneeds', 'Ġleast', 'Ġtwo', 'Ġcommercial', 'Ġmissions', 'Ġyear', 'Ġorder', 'Ġstay', 'Ġprofitable', 'Ġgoing', 'Ġforward', 'Ġu', 'la', 'Ġattempting', 'Ġwin', 'Ġmissions', 'Ġpurely', 'Ġlowest', 'Ġpurchase', 'Ġprice', 'Ġstating', 'would', 'Ġrather', 'Ġbest', 'Ġvalue', 'Ġprovider', '".[', 'Ġu', 'la', 'Ġsuggested', 'Ġcustomers', 'Ġwould', 'Ġmuch', 'Ġlower', 'Ġinsurance', 'Ġdelay', 'Ġcosts', 'Ġhigh', 'las', 'Ġreliability', 'Ġschedule', 'Ġcertainty', 'Ġmaking', 'Ġoverall', 'Ġcustomer', 'Ġcosts', 'Ġclose', 'Ġusing', 'Ġcompetitors', 'Ġlike', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġu', 'la', 'Ġoffered', 'las', 'Ġheavy', 'Ġoption', 'Ġwould', 'Ġuse', 'Ġthree', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġstages', 'Ġstrapped', 'Ġtogether', 'Ġlift', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġu', 'la', 'Ġstated', 'Ġtime', 'Ġhardware', 'Ġrequired', 'las', 'Ġheavy', 'Ġalready', 'Ġflown', 'las', 'Ġsingle']</t>
+          <t>['Ġaccuracy', 'Ġlike', 'Ġsat', 'urn', 'Ġfamily', 'Ġrockets', 'Ġmultiple', 'Ġengines', 'Ġallow', 'Ġmission', 'Ġcompletion', 'Ġeven', 'Ġone', 'Ġfails', 'Ġdetailed', 'Ġdescriptions', 'Ġdestructive', 'Ġengine', 'Ġfailure', 'Ġmodes', 'Ġdesigned', 'Ġengine', 'Ġcapabilities', 'Ġmade', 'Ġpublic', 'Ġspace', 'x', 'Ġemphasized', 'Ġfirst', 'Ġstage', 'Ġdesigned', 'engine', 'Ġcapability', 'Ġoct', 'ober', 'Ġpartial', 'Ġsuccess', 'Ġengine', 'Ġlost', 'Ġpressure', 'Ġseconds', 'Ġshut', 'Ġcompensate', 'Ġresulting', 'Ġloss', 'Ġacceleration', 'Ġfirst', 'Ġstage', 'Ġburn', 'Ġseconds', 'Ġlonger', 'Ġplanned', 'Ġsecond', 'Ġstage', 'Ġburn', 'Ġextra', 'Ġseconds', 'Ġextra', 'Ġburn', 'Ġtime', 'Ġreduced', 'Ġfuel', 'Ġreserves', 'Ġlikelihood', 'Ġsufficient', 'Ġfuel', 'Ġexecute', 'Ġmission', 'Ġdropped', '%.', 'Ġn', 'asa', 'Ġpurchased', 'Ġlaunch', 'Ġtherefore', 'Ġcontract', 'ually', 'Ġcontrolled', 'Ġseveral', 'Ġmission', 'Ġdecision', 'Ġpoints', 'Ġn', 'asa', 'Ġdeclined', 'Ġspace', 'x', "'s", 'Ġrequest', 'Ġrestart', 'Ġsecond', 'Ġstage', 'Ġattempt', 'Ġdeliver', 'Ġsecondary', 'Ġpayload', 'Ġcorrect', 'Ġorbit', 'Ġresult', 'Ġsecondary', 'Ġpayload', 'ent', 'ered', 'Ġatmosphere', 'Ġmer', 'lin', 'Ġengines', 'Ġsuffered', 'Ġtwo', 'Ġpremature', 'Ġshutdown', 'Ġascent', 'Ġneither', 'Ġaffected', 'Ġprimary', 'Ġmission', 'Ġlanding', 'Ġattempts', 'Ġfailed', 'Ġmarch', 'Ġstar', 'link', 'Ġmission', 'Ġone', 'Ġfirst', 'Ġstage', 'Ġengines', 'Ġfailed', 'Ġseconds', 'Ġcut', 'Ġdue', 'Ġignition', 'op', 'rop', 'yl', 'Ġalcohol', 'Ġproperly', 'Ġpur', 'ged', 'Ġcleaning', 'Ġanother', 'Ġstar', 'link', 'Ġmission', 'Ġfe', 'b', 'ruary', 'Ġhot', 'Ġexhaust', 'Ġg', 'asses', 'Ġentered', 'Ġengine', 'Ġdue', 'Ġfatigue', 'related', 'Ġhole', 'Ġcover', 'Ġspace', 'x', 'Ġstated', 'Ġfailed', 'Ġcover', 'highest', '...', 'Ġnumber', 'Ġflights', 'Ġparticular', 'Ġboot', 'cover', 'Ġdesign', 'Ġseen', '."[', 'Ġspace', 'x', 'Ġplanned', 'Ġbeginning', 'Ġmake', 'Ġstages', 'Ġreusable', 'Ġfirst', 'Ġstages', 'Ġearly', 'Ġfal', 'con', 'Ġflights', 'Ġequipped', 'Ġparach', 'utes', 'Ġcovered', 'Ġlayer', 'Ġabl', 'ative', 'Ġc', 'ork', 'Ġallow', 'Ġsurvive', 'Ġatmospheric', 'entry', 'Ġdefeated', 'Ġaccompanying', 'Ġaer', 'odynamic', 'Ġstress', 'Ġheating', 'Ġstages', 'Ġsalt', 'water', 'Ġlate', 'Ġspace', 'x', 'Ġeliminated', 'Ġparach', 'utes', 'Ġfavor', 'Ġpowered', 'Ġdescent', 'Ġdesign', 'Ġcomplete', 'Ġfe', 'b', 'ruary', 'Ġpowered', 'Ġland', 'ings', 'Ġfirst', 'Ġflight', 'tested', 'Ġsub', 'orb', 'ital', 'Ġgrass', 'ho', 'pper', 'Ġrocket']</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2167,7 +2167,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>['core', 'Ġvehicles', 'Ġlifting', 'Ġcapability', 'Ġproposed', 'Ġlaunch', 'Ġvehicle', 'Ġroughly', 'Ġequivalent', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġuses', 'Ġengines', 'Ġdeveloped', 'Ġproduced', 'Ġdomestically', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġreport', 'Ġprepared', 'Ġrand', 'Ġcorporation', 'Ġoffice', 'Ġsecretary', 'Ġdefense', 'Ġstated', 'Ġlock', 'heed', 'Ġmart', 'Ġdecided', 'Ġdevelop', 'las', 'Ġheavy', 'lift', 'Ġvehicle', 'Ġreport', 'Ġrecommended', 'Ġu', 'Ġair', 'Ġforce', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'n', 'ro', 'eter', 'mine', 'Ġnecessity', 'Ġe', 'el', 'v', 'Ġheavy', 'lift', 'Ġvariant', 'Ġincluding', 'Ġdevelopment', 'las', 'Ġheavy', '",', 'res', 'olve', 'Ġr', 'Ġissue', 'Ġincluding', 'Ġcop', 'rodu', 'ction', 'Ġstockpile', 'Ġunited', 'Ġstates', 'Ġdevelopment', 'Ġr', 'Ġreplacement', '".[', 'Ġu', 'la', 'Ġstated', 'las', 'Ġheavy', 'Ġvariant', 'Ġcould', 'Ġavailable', 'Ġcustomers', 'Ġmonths', 'Ġdate', 'Ġorder', 'las', 'Ġlate', 'las', 'Ġprogram', 'Ġgained', 'Ġaccess', 'Ġtool', 'ing', 'Ġprocesses', 'meter', 'iameter', 'Ġstages', 'Ġused', 'Ġdelta', 'Ġiv', 'Ġbo', 'e', 'ing', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'Ġoperations', 'Ġmerged', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġled', 'Ġproposal', 'Ġcombine', 'meter', 'iameter', 'Ġdelta', 'Ġiv', 'Ġtank', 'age', 'Ġproduction', 'Ġprocesses', 'Ġdual', 'Ġr', 'Ġengines', 'Ġresulting', 'las', 'Ġphase', 'las', 'Ġconsisting', 'Ġthree', 'meter', 'Ġstages', 'Ġparallel', 'Ġr', 'Ġconsidered', 'Ġaug', 'ust', 'ine', 'Ġreport', 'Ġpossible', 'Ġheavy', 'Ġlif', 'ter', 'Ġuse', 'Ġfuture', 'Ġspace', 'Ġmissions', 'Ġwell', 'Ġshuttle', 'derived', 'Ġl', 'ite', 'Ġbuilt', 'las', 'Ġprojected', 'Ġable', 'Ġlaunch', 'Ġpayload', 'Ġmass', 'Ġapproximately', 'Ġlong', 'Ġtons', 'Ġshort', 'Ġtons', 'Ġorbit', 'Â°', 'Ġinclination', 'Ġbooster', 'Ġrocket', 'las', 'Ġcommon', 'Ġcore', 'Ġbooster', 'Ġused', 'Ġfirst', 'Ġstage', 'Ġjoint', 'Ġus', 'j', 'apan', 'ese', 'Ġrocket', 'Ġscheduled', 'Ġmake', 'Ġfirst', 'Ġflight', 'Ġlaunches', 'Ġwould', 'las', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġhowever', 'Ġj', 'apan', 'ese', 'Ġgovernment', 'Ġdecided', 'Ġcancel', 'Ġproject', 'Ġde', 'cember', 'lic', 'ensing', 'Ġrejected', 'Ġu', 'la', 'Ġmay', 'Ġconsortium']</t>
+          <t>['Ġlow', 'alt', 'itude', 'Ġlow', 'speed', 'Ġdemonstration', 'Ġtest', 'Ġvehicle', 'Ġmade', 'Ġeight', 'Ġvertical', 'Ġland', 'ings', 'Ġincluding', 'second', 'Ġround', 'trip', 'Ġflight', 'Ġaltitude', 'Ġft', 'Ġmarch', 'Ġspace', 'x', 'Ġannounced', 'Ġfirst', 'Ġflight', 'Ġevery', 'Ġbooster', 'Ġwould', 'Ġequipped', 'Ġpowered', 'Ġdescent', 'Ġexplanatory', 'Ġgraphic', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġb', 'arge', 'Ġlanding', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġstage', 'Ġseparation', 'Ġflight', 'Ġplan', 'Ġcalled', 'Ġfirst', 'Ġstage', 'Ġconduct', 'Ġburn', 'Ġreduce', 'entry', 'Ġvelocity', 'Ġsecond', 'Ġburn', 'Ġreaching', 'Ġwater', 'Ġalthough', 'Ġcomplete', 'Ġsuccess', 'Ġstage', 'Ġable', 'Ġchange', 'Ġdirection', 'Ġmake', 'Ġcontrolled', 'Ġentry', 'Ġatmosphere', 'Ġfinal', 'Ġlanding', 'Ġburn', 'Ġthr', 'usters', 'Ġcould', 'Ġovercome', 'Ġaer', 'odynam', 'ically', 'Ġinduced', 'Ġspin', 'Ġcentrif', 'ugal', 'Ġforce', 'Ġdeprived', 'Ġengine', 'Ġfuel', 'Ġleading', 'Ġearly', 'Ġengine', 'Ġshutdown', 'Ġhard', 'Ġsplash', 'Ġfour', 'Ġocean', 'Ġlanding', 'Ġtests', 'Ġbooster', 'Ġattempted', 'Ġlanding', 'ds', 'Ġfloating', 'Ġplatform', 'Ġjan', 'uary', 'Ġrocket', 'Ġincorporated', 'Ġfirst', 'Ġtime', 'Ġorbital', 'Ġmission', 'Ġgrid', 'Ġfin', 'Ġaer', 'odynamic', 'Ġcontrol', 'Ġsurfaces', 'Ġsuccessfully', 'Ġguided', 'Ġship', 'Ġrunning', 'Ġhydraulic', 'Ġfluid', 'Ġcrashing', 'Ġplatform', 'Ġsecond', 'Ġattempt', 'Ġoccurred', 'Ġapr', 'il', 'Ġengine', 'Ġcapability', 'us', 'ability', 'Ġpost', 'mission', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtests', 'Ġlanding', 'Ġattempts', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġsuccessfully', 'Ġlanding', 'ds', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtime', 'Ġfollowing', 'Ġlaunch', 'Ġspace', 'x', 'Ġiss', 'Ġï', '¬', 'ģ', 'r', 'st', 'ï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġmarch', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġrocket', 'Ġdelivered', 'Ġe', 'ut', 'els', 'Ġwest', 'Ġsatellites', 'Ġsupers', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'Ġlaunching', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'Ġmarch', 'Ġlaunch', 'Ġbip', 'ro', 'pell', 'ant', 'Ġvalve', 'Ġbecame', 'Ġstuck', 'Ġpreventing', 'Ġcontrol', 'Ġsystem', 'Ġreacting', 'Ġrapidly', 'Ġenough', 'Ġsuccessful', 'Ġlanding', 'Ġfirst', 'Ġattempt', 'Ġland', 'Ġbooster', 'Ġground', 'Ġpad', 'Ġnear', 'Ġlaunch', 'Ġsite', 'Ġoccurred', 'Ġflight', 'Ġde', 'cember', 'Ġlanding', 'Ġsuccessful', 'Ġbooster', 'Ġfirst', 'Ġtime', 'Ġhistory']</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>['Ġcompanies', 'Ġincluding', 'ero', 'jet', 'Ġdyn', 'etics', 'Ġsought', 'Ġlicense', 'Ġproduction', 'Ġmanufacturing', 'Ġrights', 'las', 'Ġusing', 'Ġengine', 'Ġplace', 'Ġr', 'Ġproposal', 'Ġrejected', 'Ġlaunch', 'Ġcost', 'Ġhistorically', 'Ġproposed', 'Ġversions', 'las', 'Ġlaunches', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġaug', 'ust', '05', 'Ġcc', 'af', 'Ġhot', 'Ġbird', 'Ġcommercial', 'Ġcommunications', 'Ġsatellite', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġmay', 'Ġcc', 'af', 'Ġhell', 'Ġsat', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'Ġsatellite', 'Ġg', 'ree', 'ce', 'Ġcy', 'prus', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġrainbow', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġfirst', 'las', 'Ġlaunch', 'Ġde', 'cember', '07', 'Ġcc', 'af', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġmarch', 'Ġcc', 'af', 'ars', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġmars', 'Ġorbit', 'er', 'Ġhel', 'oc', 'entric', 'oc', 'entric', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġn', 'asa', 'Ġjan', 'uary', '00', 'Ġcc', 'af', 'Ġnew', 'Ġhor', 'izons', 'Ġpl', 'uto', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġprobe', 'Ġhyper', 'b', 'olic', 'Ġsuccess', 'Ġbo', 'e', 'ing', 'Ġstar', 'Ġth', 'ir', 'Ġstage', 'Ġused', 'Ġï', '¬', 'ģ', 'r', 'st', 'la', 'Ġlaunch', 'Ġthird', 'Ġstage', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġast', 'ra', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġmarch', 'Ġ03', 'Ġcc', 'af', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġmilitary', 'Ġresearch', 'Ġsatellites', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġu', 'la', 'las', 'Ġlaunch', 'Ġfirst', 'las', 'Ġn', 'igh', 'Ġlaunch', 'Ġfirst', 'Ġthree', 'burn', 'las', 'Ġmission', 'Ġorbital', 'Ġexpress', 'Ġfal', 'cons', 'Ġj', 'une', 'Ġcc', 'af', 'Ġus', 'b', 'Ġtwo', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellites', 'Ġle', 'Ġsuccess']</t>
+          <t>['Ġlaunching', 'Ġorbital', 'Ġmission', 'Ġfirst', 'Ġstage', 'Ġachieved', 'Ġcontrolled', 'Ġvertical', 'Ġlanding', 'Ġfirst', 'Ġsuccessful', 'Ġbooster', 'Ġlanding', 'ds', 'Ġoccurred', 'Ġapr', 'il', 'Ġdrone', 'Ġship', 'Ġcourse', 'Ġstill', 'Ġlove', 'Ġsixteen', 'Ġtest', 'Ġflights', 'Ġconducted', 'Ġachieved', 'Ġsoft', 'Ġlanding', 'Ġbooster', 'Ġrecovery', 'Ġsince', 'Ġjan', 'uary', 'Ġexceptions', 'Ġcentre', 'Ġcore', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġflight', 'Ġfal', 'con', 'Ġheavy', 'Ġus', 'af', 'Ġmission', 'Ġfal', 'con', 'Ġres', 'upp', 'ly', 'Ġmission', 'Ġstar', 'link', 'Ġmissions', 'Ġevery', 'Ġlanding', 'Ġattempt', 'Ġsuccessful', 'Ġpost', 'land', 'ing', 'Ġloss', 'Ġfirst', 'Ġstage', 'Ġoccurred', 'Ġfal', 'con', 'Ġheavy', 'Ġar', 'abs', 'Ġcentre', 'Ġcore', 'Ġfell', 'Ġoverboard', 'Ġrough', 'Ġseas', 'Ġvoyage', 'Ġland', 'Ġfirst', 'Ġoperational', 'Ġrel', 'aunch', 'Ġpreviously', 'Ġflown', 'Ġbooster', 'Ġaccomplished', 'Ġmarch', 'es', 'Ġmission', 'Ġapr', 'il', 'Ġlanding', 'Ġsecond', 'Ġtime', 'Ġretired', 'Ġj', 'une', 'Ġbooster', 'Ġhelped', 'Ġcarry', 'Ġbul', 'g', 'ari', 'Ġtowards', 'Ġg', 'Ġir', 'idium', 'Ġnext', 'Ġle', 'Ġmission', 'Ġjan', 'uary', 'Ġachieving', 'Ġreuse', 'Ġlanding', 'Ġrecovered', 'Ġbooster', 'Ġthird', 'Ġreuse', 'Ġflight', 'Ġcame', 'mber', 'Ġmission', 'Ġcore', 'Ġmission', 'Ġfal', 'con', 'Ġfirst', 'Ġblock', 'Ġbooster', 'Ġproduced', 'Ġflown', 'Ġinitially', 'Ġbang', 'aband', 'hu', 'Ġsatellite', 'Ġmission', 'Ġmay', 'Ġfirst', 'Ġbooster', 'Ġreached', 'Ġmissions', 'Ġmus', 'k', 'Ġindicated', 'Ġspace', 'x', 'Ġintends', 'Ġfly', 'Ġboosters', 'Ġsee', 'Ġfailure', 'Ġstar', 'link', 'Ġmissions', 'Ġde', 'cember', 'Ġrecord', 'Ġflights', 'Ġbooster', 'Ġdespite', 'Ġpublic', 'Ġstatements', 'Ġwould', 'Ġendeavor', 'Ġmake', 'Ġsecond', 'stage', 'Ġreusable', 'Ġwell', 'Ġlate', 'Ġspace', 'x', 'Ġdetermined', 'Ġmass', 'Ġneeded', 'Ġheat', 'Ġshield', 'Ġlanding', 'Ġengines', 'Ġequipment', 'Ġsupport', 'Ġrecovery', 'Ġsecond', 'Ġstage', 'Ġprohib', 'itive', 'Ġabandoned', 'Ġsecond', 'stage', 'us', 'ability', 'Ġefforts', 'Ġspace', 'x', 'Ġdeveloped', 'Ġpayload', 'Ġfair', 'ings', 'Ġequipped', 'Ġsteer', 'able', 'Ġparachute', 'Ġwell', 'Ġthr', 'usters', 'Ġrecovered', 'Ġreused', 'Ġpayload', 'Ġfair', 'ing', 'Ġhalf', 'Ġrecovered', 'Ġfollowing', 'Ġsoft', 'land', 'ing', 'Ġocean', 'Ġfirst', 'Ġtime', 'Ġmarch', 'Ġfollowing', 'es', 'Ġsubsequently', 'Ġdevelopment', 'Ġbegan', 'Ġship', 'based', 'Ġsystem']</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2193,7 +2193,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>['Ġfirst', 'las', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfo', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'las', 'Ġachieve', 'Ġintended', 'Ġorbit', 'Ġpayload', 'Ġcompensated', 'Ġshortfall', 'Ġn', 'ro', 'Ġdeclared', 'Ġmission', 'Ġoct', 'ober', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġvalve', 'Ġreplacement', 'Ġdelayed', 'Ġlaunch', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġde', 'cember', '05', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġmarch', '02', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġfirst', 'las', 'Ġlaunch', 'Ġv', 'enberg', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġ', 'ico', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlock', 'heed', 'Ġmart', 'Ġcommercial', 'Ġlaunch', 'Ġservices', 'Ġlaunch', 'Ġheaviest', 'Ġpayload', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġlargest', 'sat', 'Ġworld', 'Ġtime', 'Ġlaunch', 'Ġth', 'Ġlaunch', 'Ġter', 'rest', 'ar', 'ri', 'ane', 'Ġtel', 'star', 'v', 'Ġj', 'uly', 'Ġfal', 'con', 'Ġapr', 'il', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġj', 'une', 'Ġcc', 'af', 'Ġl', 'ro', 'l', 'cross', 'Ġlunar', 'Ġexploration', 'Ġlunar', 'Ġsuccess', 'Ġfirst', 'Ġcent', 'aur', 'Ġstage', 'Ġimpact', 'Ġmoon', 'Ġse', 'pt', 'ember', 'Ġcc', 'af', 'Ġus', 'p', 'adium', 'Ġnight', 'Ġpan', 'Ġmilitary', 'sat', 'Ġsuccess', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġfragmented', 'Ġorbit', 'Ġmarch', 'Ġoct', 'ober', 'Ġv', 'af', 'b', 'Ġus', 'ms', 'p', 'Ġmilitary', 'Ġweather', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'mber', 'Ġ06', 'Ġcc', 'af', 'Ġint', 'els', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlaunch', 'Ġfe', 'b', 'ruary', 'Ġcc', 'af', 'Ġsolar', 'Ġtelescope', 'Ġg', 'Ġsuccess']</t>
+          <t>['Ġinvolving', 'Ġmassive', 'Ġnet', 'Ġorder', 'Ġcatch', 'Ġreturning', 'Ġfair', 'ings', 'Ġtwo', 'Ġdedicated', 'Ġships', 'fitted', 'Ġrole', 'Ġmaking', 'Ġfirst', 'Ġcatches', 'Ġhowever', 'Ġfollowing', 'Ġmixed', 'Ġsuccess', 'Ġspace', 'x', 'Ġreturned', 'Ġwater', 'Ġland', 'ings', 'Ġwet', 'Ġrecovery', 'Ġearly', 'Ġregularly', 'Ġlaunching', 'Ġthree', 'Ġorbital', 'Ġlaunch', 'Ġsites', 'Ġlaunch', 'Ġcomplex', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġlatter', 'Ġdamaged', 'Ġaccident', 'Ġse', 'pt', 'ember', 'Ġoperational', 'Ġde', 'cember', 'Ġapr', 'il', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġspace', 'Ġlaunch', 'Ġdelta', 'Ġgranted', 'Ġspace', 'x', 'Ġpermission', 'Ġlease', 'Ġv', 'enberg', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġlikely', 'Ġbecome', 'Ġfourth', 'Ġlaunch', 'Ġsite', 'Ġfal', 'con', 'Ġtime', 'Ġmaiden', 'Ġflight', 'Ġprice', 'Ġlaunch', 'Ġlisted', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġlist', 'Ġprice', 'Ġincreased', 'Ġthereafter', 'Ġus', 'âĢĵ', 'Ġmillion', ').[', 'Ġmillion', 'Ġaug', 'ust', 'Ġmillion', 'j', 'une', 'Ġmillion', 'full', 'Ġthrust', 'Ġmay', 'Ġmillion', ').[', 'Ġdragon', 'Ġcargo', 'Ġmissions', 'Ġiss', 'Ġaverage', 'Ġcost', 'Ġmillion', 'Ġfixed', 'price', 'Ġcontract', 'Ġn', 'asa', 'Ġincluding', 'Ġcost', 'Ġspacecraft', 'sc', 'ov', 'r', 'Ġmission', 'Ġlaunched', 'Ġfal', 'con', 'Ġnational', 'Ġocean', 'ic', 'Ġatmospheric', 'Ġadministration', 'Ġcost', 'Ġmillion', 'Ġrel', 'aunch', 'Ġrecovery', 'Ġsecond', 'Ġstages', 'Ġfair', 'ings', 'Ġlaunch', 'Ġsites', 'Ġpricing', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġel', 'Ġmus', 'k', 'Ġstated', 'ult', 'imately', 'Ġbelieve', 'Ġper', 'Ġpound', 'kg', 'Ġpayload', 'Ġdelivered', 'Ġorbit', 'Ġless', 'Ġachievable', '".[', 'Ġlaunch', 'Ġprice', 'Ġfull', 'Ġle', 'Ġpayload', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġcosts', 'Ġreached', 'Ġus', 'lb', 'Ġ($', 'kg', 'Ġmus', 'k', 'Ġestimated', 'Ġfuel', 'Ġoxid', 'izer', 'Ġcost', '000', 'Ġfirst', 'Ġstage', 'Ġuses']</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2206,7 +2206,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>['Ġapr', 'il', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'Ġpiece', 'Ġex', 'tern', 'Ġfair', 'ing', 'Ġbreak', 'Ġimpact', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġwashed', 'Ġh', 'ilton', 'Ġhead', 'Ġisland', 'Ġaug', 'ust', '07', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ04', '03', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġmarch', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'Ġapr', 'il', 'Ġ04', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġjun', 'Ġj', 'upiter', 'Ġorbit', 'er', 'Ġhyper', 'b', 'olic', 'Ġj', 'ovic', 'entric', 'Ġsuccess', 'mber', '02', 'Ġcc', 'af', 'Ġmars', 'Ġscience', 'Ġlaboratory', 'ms', 'l', 'Ġmars', 'Ġrover', 'Ġhyper', 'b', 'olic', 'ars', 'Ġlanding', 'Ġsuccess', 'Ġfirst', 'Ġlaunch', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uation', 'Ġcent', 'aur', 'Ġentered', 'Ġorb', 'Ġaround', 'Ġfe', 'b', 'ruary', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'th', 'Ġcent', 'aur', 'Ġlaunch', 'Ġheaviest', 'Ġpayload', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġj', 'une', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'th', 'Ġe', 'el', 'v', 'Ġlaunch', 'Ġaug', 'ust', 'Ġ08', '05', 'Ġcc', 'af', 'Ġvan', 'en', 'Ġprobes', 'r', 'bsp', 'Ġvan', 'en', 'Ġbelts', 'Ġexploration', 'Ġsuccess', 'Ġse', 'pt', 'ember']</t>
+          <t>['030', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġliquid', '020', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġfuel', 'Ġsecond', 'Ġstage', 'Ġuses', '000', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġliquid', '000', 'Ġimp', 'Ġgal', 'Ġus', 'Ġgal', 'Ġdecreased', 'Ġlaunch', 'Ġcosts', 'Ġdrew', 'Ġcompetitors', 'rian', 'esp', 'ace', 'Ġbegan', 'Ġworking', 'ri', 'ane', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġvul', 'Ġcent', 'aur', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'ils', 'Ġpro', 'ton', 'Ġmedium', 'Ġj', 'une', 'Ġj', 'athan', 'Ġh', 'eller', 'space', 'x', 'Ġvice', 'Ġpresident', 'Ġcommercial', 'Ġsales', 'Ġsaid', 'Ġprice', 'Ġdiscounts', 'Ġgiven', 'Ġearly', 'Ġcustomers', 'Ġmission', 'Ġreused', 'Ġboosters', 'Ġbecome', 'Ġstandard', 'Ġprice', 'Ġoct', 'ober', 'Ġfal', 'con', 'base', 'Ġprice', 'Ġmillion', 'Ġper', 'Ġlaunch', 'Ġlowered', 'Ġmillion', 'Ġflights', 'Ġscheduled', 'Ġbeyond', 'Ġapr', 'il', 'Ġro', 'sc', 'os', 'mos', 'Ġadministrator', 'mit', 'ry', 'Ġro', 'go', 'zin', 'Ġsaid', 'Ġoutfit', 'Ġcutting', 'Ġprices', '%,', 'Ġalleging', 'Ġspace', 'x', 'Ġprice', 'Ġdumping', 'Ġcharging', 'Ġcommercial', 'Ġcustomers', 'Ġmillion', 'Ġper', 'Ġflight', 'Ġcharging', 'Ġn', 'asa', 'Ġmuch', 'Ġflight', 'Ġmus', 'k', 'Ġdenied', 'Ġclaim', 'Ġreplied', 'Ġprice', 'Ġdifference', 'Ġreflected', 'Ġreusable', 'Ġr', 'ussian', 'Ġrockets', 'Ġsingle', 'Ġuse', 'Ġu', 'la', 'Ġce', 'ory', 'Ġbr', 'uno', 'Ġstated', 'Ġestimate', 'Ġremains', 'Ġaround', 'Ġflights', 'Ġfleet', 'Ġaverage', 'Ġachieve', 'Ġconsistent', 'Ġbre', 'ake', 'ven', 'Ġpoint', 'Ġ...', 'Ġone', 'Ġcome', 'Ġanywhere', 'Ġclose', '".[', 'Ġhowever', 'Ġel', 'Ġmus', 'k', 'Ġresponded', 'pay', 'load', 'Ġreduction', 'Ġdue', 'us', 'ability', 'Ġbooster', 'Ġfair', 'ing', 'Ġfal', 'con', 'Ġrecovery', 'Ġrefurb', '%,', "'re", 'Ġroughly', 'Ġeven', 'Ġflights', 'Ġdefinitely', 'Ġahead', '".[', 'Ġreported', 'Ġapr', 'il', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', "'s", 'Ġlaunches', 'Ġcosting', 'Ġmillion', 'Ġdue', 'Ġneeded', 'Ġextra', 'Ġsecurity', 'Ġspace', 'x', 'Ġexecutive', 'Ġchrist', 'opher', 'Ġcou', 'l', 'ur', 'Ġstated', 'using', 'Ġrockets', 'Ġcould', 'Ġbring', 'Ġprices', 'Ġeven', 'Ġlower', 'cost', 'Ġmillion', 'Ġlaunch', "'s", 'Ġeverything', '".[', 'Ġpayload', 'Ġservices', 'Ġinclude', 'Ġsecondary', 'Ġtert', 'iary', 'Ġpayload', 'Ġmounted', 'Ġvia', 'Ġe', 'el', 'v', 'Ġsecondary', 'Ġpayload', 'Ġadapter']</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2219,7 +2219,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>['Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellites', 'Ġle', 'Ġsuccess', 'Ġde', 'cember', '03', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġjan', 'uary', 'Ġ01', 'Ġcc', 'af', 'Ġtd', 'rs', 'k', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġfe', 'b', 'ruary', '02', 'Ġv', 'af', 'b', 'Ġlands', 'Ġearth', 'Ġobservation', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġwest', 'Ġcoast', 'la', 'Ġlaunch', 'Ġn', 'asa', 'Ġmarch', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġgeo', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġfirst', 'Ġsatellite', 'Ġlaunched', 'las', 'Ġj', 'uly', '00', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ08', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'mber', 'Ġcc', 'af', 'aven', 'Ġmars', 'Ġorbit', 'er', 'Ġhyper', 'b', 'olic', 'oc', 'entric', 'Ġsuccess', 'Ġde', 'cember', 'Ġ07', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsuccess', 'Ġjan', 'uary', 'Ġ02', 'Ġcc', 'af', 'Ġtd', 'rs', 'l', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġapr', 'il', 'Ġv', 'af', 'b', 'Ġus', 'Ġmilitary', 'Ġweather', 'Ġsatellite', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsuccess', 'th', 'Ġr', 'Ġlaunch', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmay', '09', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġaug', 'ust', 'Ġ03']</t>
+          <t>['es', 'pa', 'Ġring', 'Ġinter', 'stage', 'Ġadapter', 'Ġfirst', 'Ġused', 'Ġlaunching', 'Ġsecondary', 'Ġpayload', 'Ġus', 'Ġdod', 'Ġmissions', 'Ġuse', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicles', 'e', 'el', 'v', 'las', 'Ġdelta', 'Ġiv', 'Ġenables', 'Ġsecondary', 'Ġeven', 'Ġtert', 'iary', 'Ġmissions', 'Ġminimal', 'Ġimpact', 'Ġoriginal', 'Ġmission', 'Ġspace', 'x', 'Ġannounced', 'Ġpricing', 'Ġes', 'pa', 'compatible', 'Ġpayload', 'Ġspace', 'x', 'Ġfirst', 'Ġput', 'Ġfal', 'con', 'Ġpublic', 'Ġdisplay', 'Ġheadquarters', 'Ġhaw', 'th', 'orne', 'Ġcal', 'ornia', 'Ġspace', 'x', 'Ġdonated', 'Ġfal', 'con', 'Ġspace', 'Ġcenter', 'Ġh', 'ouston', 'Ġh', 'ouston', 'Ġtex', 'Ġbooster', 'Ġflew', 'Ġtwo', 'Ġmissions', 'th', 'th', 'Ġsupply', 'Ġmissions', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġfirst', 'Ġfal', 'con', 'Ġrocket', 'Ġn', 'asa', 'Ġagreed', 'Ġfly', 'Ġsecond', 'Ġtime', '".[', 'Ġspace', 'x', 'Ġdonated', 'Ġfal', 'con', 'Ġheavy', 'Ġside', 'Ġbooster', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġvisitor', 'Ġcomplex', 'os', 'Ġbang', 'aband', 'hu', 'Ġsatellite', 'res', 'heet', 'Ġlunar', 'Ġland', 'er', 'Ġbo', 'e', 'ing', 'Ġcrew', 'Ġcargo', 'Ġdragon', 'Ġdouble', 'Ġasteroid', 'Ġred', 'irection', 'Ġtest', 'art', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunches', 'Ġir', 'idium', 'Ġnext', 'Ġconstellation', 'Ġlaunches', 'Ġus', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġn', 'rol', 'Ġorb', 'comm', 'Ġrad', 'ars', 'Ġconstellation', 'es', 'Ġsir', 'ius', 'Ġlaunches', 'Ġspace', 'x', 'Ġstar', 'link', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'et', 'Ġsurvey', 'Ġsatellite', 'ess', 'Ġsecondary', 'Ġpayload', 'Ġhistorical', 'Ġartifacts', 'Ġmuseum', 'Ġfal', 'con', 'Ġnotable', 'Ġpayload', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġz', 'uma', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġlist', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'stage', 'Ġboosters', 'Ġspace', 'x', 'Ġlaunch', 'Ġvehicles', 'Ġlanding', 'Ġsuccess', 'Ġdetails', 'Ġlist', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'fal', 'con', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'fal', 'con', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'fal', 'con', 'Ġoverview', ')"', 'Ġspace', 'x', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>['Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġaug', 'ust', 'Ġv', 'af', 'b', 'Ġworldview', 'Ġearth', 'Ġimaging', 'Ġsatellite', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'cl', 'io', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġfragmented', 'Ġaug', 'ust', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġoct', 'ober', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'th', 'las', 'Ġlaunch', 'Ġde', 'cember', 'Ġ03', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġfirst', 'Ġuse', 'Ġengine', 'Ġcent', 'aur', 'Ġstage', 'Ġjan', 'uary', 'Ġ01', '04', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġmarch', 'Ġ02', 'Ġcc', 'af', 'ms', 'Ġmagnet', 'osphere', 'Ġresearch', 'Ġsatellites', 'Ġsuccess', 'Ġmay', '05', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġle', 'Ġsuccess', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġoct', 'ober', 'Ġcc', 'af', 'los', 'sat', 'Ġg', 'Ġsuccess', 'Ġoct', 'ober', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellites', 'Ġle', 'Ġsuccess', 'Ġoct', 'ober', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġcy', 'gn', 'us', 'Ġcr', 'Ġiss', 'Ġlogistics', 'Ġspacecraft', 'Ġle', 'Ġsuccess', 'Ġfirst', 'las', 'Ġrocket', 'Ġuse', 'Ġdirectly', 'Ġsupport', 'Ġth', 'Ġiss', 'Ġprogram', 'Ġfe']</t>
+          <t>['Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'aven', 'port', 'Ġjan', 'uary', 'space', 'x', 'Ġlaunches', 'Ġstar', 'link', 'Ġgroup', 'Ġmission', 'Ġfl', 'ida', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'air', 'Ġforce', 'Ġrequirements', 'Ġkeep', 'Ġspace', 'x', 'Ġlanding', 'Ġfal', 'con', 'Ġbooster', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġseem', 'ang', 'al', 'Ġrob', 'Ġmay', 'space', 'x', 'Ġtest', 'fires', 'Ġnew', 'Ġfal', 'con', 'Ġblock', 'Ġrocket', 'Ġahead', 'Ġmaiden', 'Ġflight', 'updated', ')"', 'htt', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġoct', 'ober', 'orb', 'comm', 'Ġcraft', 'Ġlaunched', 'Ġfal', 'con', 'Ġfalls', 'Ġorbit', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġr', 'bit', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'orb', 'comm', 'Ġrequested', 'Ġspace', 'x', 'Ġcarry', 'Ġone', 'Ġsmall', 'Ġsatellites', 'igh', 'ing', 'Ġhundred', 'Ġpounds', 'Ġversus', 'Ġdragon', '000', 'Ġpounds', ')...', 'Ġhigher', 'Ġorbit', 'Ġtest', 'Ġdata', 'orb', 'comm', 'Ġgather', 'Ġrequested', 'Ġattempt', 'Ġrestart', 'Ġraise', 'Ġaltitude', 'Ġn', 'asa', 'Ġagreed', 'Ġallow', 'Ġcondition', 'Ġsubstantial', 'Ġpropell', 'ant', 'Ġreserves', 'Ġsince', 'Ġorbit', 'Ġwould', 'Ġclose', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġimportant', 'Ġappreciate', 'Ġorb', 'comm', 'Ġunderstood', 'Ġbeginning', 'Ġorbit', 'raising', 'Ġmaneuver', 'Ġtentative', 'Ġaccepted', 'Ġhigh', 'Ġrisk', 'Ġsatellite', 'Ġremaining', 'Ġdragon', 'Ġinsertion', 'Ġorbit', '..."', 'Ġgra', 'ham', 'iam', 'Ġde', 'cember', 'space', 'x', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġnails', 'Ġhistoric', 'Ġcore', 'Ġreturn', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġlaunch', 'Ġalso', 'Ġmarked', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġinternally', 'Ġknown', 'graded', 'Ġfal', 'con', 'Ġgra', 'ham', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġsuccessfully']</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2245,7 +2245,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>['b', 'ruary', 'Ġcc', 'af', 'Ġus', 'Ġnavigation', 'Ġsatellite', 'Ġsuccess', 'Ġmarch', 'Ġ03', '05', 'Ġcc', 'af', 'Ġcy', 'gn', 'us', 'Ġcr', 'Ġiss', 'Ġlogistics', 'Ġspacecraft', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġstage', 'Ġshut', 'Ġdow', 'Ġearly', 'Ġaff', 'e', 'Ġmission', 'Ġoutcome', 'Ġj', 'une', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', '05', 'Ġcc', 'af', 'Ġos', 'iris', 'rex', 'Ġasteroid', 'Ġsample', 'Ġreturn', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'mber', 'Ġv', 'af', 'b', 'Ġworldview', 'Ġn', 'ro', 'Ġcubes', 'ats', 'Ġearth', 'Ġimaging', 'Ġcubes', 'ats', 'Ġsuccess', 'Ġlaunch', 'mber', 'Ġcc', 'af', 'Ġgoes', 'r', 'go', 'es', 'Ġmeteor', 'ology', 'Ġg', 'Ġsuccess', 'th', 'Ġe', 'el', 'v', 'Ġlaunch', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġe', 'ch', 'ost', 'ar', 'j', 'upiter', 'Ġcommercial', 'sat', 'Ġg', 'Ġsuccess', 'Ġlaunch', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġjan', 'uary', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmarch', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġcy', 'gn', 'us', 'Ġcr', 'Ġiss', 'Ġlogistics', 'Ġspacecraft', 'Ġle', 'Ġsuccess', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġtd', 'rs', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġ05', 'Ġv', 'af', 'b', 'Ġus', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġsuccess', 'Ġoct', 'ober', 'Ġ07', 'Ġcc', 'af', 'Ġus']</t>
+          <t>['Ġlaunches', 'Ġdebut', 'Ġfal', 'con', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'det', 'ailed', 'Ġmission', 'Ġdata', 'Ġfal', 'con', 'Ġfirst', 'Ġflight', 'Ġdemonstration', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġn', 'stration', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'fal', 'con', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġreferences', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'space', 'x', 'Ġfal', 'con', 'Ġupper', 'Ġstage', 'Ġengine', 'Ġsuccessfully', 'Ġcompletes', 'Ġfull', 'Ġmission', 'Ġduration', 'Ġfiring', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'os', 'Ġj', 'athan', 'Ġoct', 'ober', 'space', 'x', 'Ġlifts', 'Ġiss', 'Ġcargo', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'n', 'asa', 'Ġspace', 'x', 'Ġlaunch', 'Ġastronauts', 'Ġnew', 'Ġera', 'Ġprivate', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġh', 'Ġmay', 'Ġarchived', 'Ġh', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġc', 'aw', 'ley', 'Ġj', 'ames', 'mber', 'n', 'asa', 'Ġspace', 'x', 'Ġcomplete', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġfirst', 'Ġhuman', 'rated', 'Ġcommercial', 'Ġspace', 'Ġsystem', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'mber', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġbecame', 'Ġameric', "'s", 'Ġwork', 'horse', 'Ġrocket', 'Ġar', 'ste', 'chn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġwall', 'ike', 'Ġj', 'une', 'happy', 'Ġbirthday', 'Ġfal', 'con', 'Ġspace', 'x', "'s", 'Ġwork', 'horse', 'Ġrocket', 'Ġdebuted', 'Ġyears', 'Ġago', 'Ġtoday', 'sp', 'Ġspace', 'Ġarchived', 'years']</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>['Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġjan', 'uary', 'Ġ00', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġmarch', '02', 'Ġcc', 'af', 'Ġgoes', 'go', 'es', 'Ġmeteor', 'ology', 'Ġg', 'Ġsuccess', 'Ġexpended', 'th', 'Ġapr', 'il', 'Ġcc', 'af', 'Ġmilitary', 'sat', 'Ġgeo', 'Ġsuccess', 'Ġmay', '05', 'Ġv', 'af', 'b', 'Ġinsight', 'Ġmar', 'co', 'Ġmars', 'Ġland', 'er', 'Ġcubes', 'ats', 'Ġhyper', 'b', 'olic', 'ars', 'Ġlanding', 'Ġsuccess', 'Ġfirst', 'Ġinter', 'plan', 'etary', 'Ġmission', 'Ġv', 'af', 'b', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġinter', 'plan', 'etary', 'Ġcubes', 'ats', 'Ġoct', 'ober', 'Ġ04', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'th', 'Ġcent', 'aur', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġfragmented', 'Ġorbit', 'Ġapr', 'Ġaug', 'ust', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġstar', 'liner', 'Ġbo', 'e', 'ing', 'Ġoft', 'Ġunc', 'rew', 'ed', 'Ġorbital', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġle', 'iss', 'Ġsuccess', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġdual', 'engine', 'Ġcent', 'aur', 'las', 'Ġv', 'Ġfirst', 'Ġorbital', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġstar', 'liner', 'Ġplanned', 'Ġvisit', 'Ġiss', 'Ġanomaly', 'Ġstar', 'liner', 'Ġvehicle', 'Ġleft', 'Ġspacecraft', 'Ġlow', 'Ġorbit', 'las', 'Ġrock', 'Ġperformed', 'Ġexpected', 'Ġthus', 'Ġth', 'Ġmission', 'Ġlisted', 'Ġsuccessful', 'Ġfe', 'b', 'ruary', 'Ġ04', '03', 'Ġcc', 'af', 'Ġsolar', 'Ġorbit', 'er', 'Ġsolar', 'Ġhel', 'oph', 'ysics', 'Ġorbit', 'er', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'Ġlast', 'Ġflight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġmarch', 'Ġcc', 'af', 'Ġus', 'Ġmilitary', 'sat', 'Ġg', 'Ġsuccess', 'Ġfirst', 'Ġever', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġth', 'Ġu']</t>
+          <t>['html', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġmay', 'Ġsafest', 'Ġrocket', 'Ġever', 'Ġlaunched', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'web', 'arch', 'iv', 'Ġcut', 'ive', 'success', 'es', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġev', 'ans', 'Ġben', 'Ġj', 'uly', 'space', 'x', "'s", 'sweet', 'Ġsixteen', 'Ġlaunches', 'Ġstar', 'links', 'Ġenters', 'us', 'ability', 'Ġrecord', 'Ġbooks', 'w', 'Ġameric', 'asp', 'ace', 'Ġmal', 'ik', 'ari', 'q', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġrocket', 'Ġlanding', 'Ġphotos', 'Ġsimply', 'Ġjaw', 'dropping', 'Ġspace', 'Ġarchived', 'Ġos', 'html', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġth', 'omas', 'Ġr', 'ach', 'ael', 'Ġl', 'space', 'x', "'s", 'Ġrockets', 'Ġspacecraft', 'Ġreally', 'Ġcool', 'Ġnames', 'Ġmean', '?"', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġtodd', 'Ġdavid', 'Ġj', 'uly', 'int', 'els', 'Ġlaunched', 'Ġadvantageous', 'Ġsuper', 'syn', 'chron', 'ous', 'Ġtransfer', 'Ġorbit', 'Ġfal', 'con', 'htt', 'Ġser', 'adata', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġk', 'yle', 'Ġed', 'Ġj', 'uly', 'Ġspace', 'Ġlaunch', 'Ġreport', 'w', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', '07', 'Ġfal', 'con', 'Ġtel', 'star', 'v', '075', 'Ġcc', 'Ġg', '-"', 'Ġwatt', 'les', 'Ġjack', 'ie', 'Ġjan', 'uary', 'space', 'x', 'Ġlaunches', 'Ġsatellites', 'Ġone', 'Ġrocket', 'Ġrecord', 'setting', 'Ġmission', 'Ġc', 'n', 'index', 'html', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'uc', 'inski', 'iam', 'Ġfour', 'Ġn', 'ssl', 'Ġlaunch', 'Ġvehicle', 'Ġdevelopers', 'Ġsay', "'ll", 'Ġready', 'Ġmobil', 'us', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'mber', 'space', 'x', "'s", 'Ġfal']</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>['Ġspace', 'Ġforce', 'th', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġengine', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'Ġfal', 'cons', '))', 'Ġmilitary', 'Ġspace', 'plane', 'Ġus', 'afa', 'Ġsat', 'Ġle', 'Ġsuccess', 'Ġsixth', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'cons', 'Ġj', 'uly', 'Ġcc', 'af', 'Ġmars', 'Ġmars', 'Ġrover', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'Ġlaunch', 'Ġpersever', 'ance', 'Ġrover', 'mber', 'Ġcc', 'af', 'Ġus', 'n', 'rol', 'Ġn', 'ro', 'Ġreconnaissance', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġfirst', 'Ġusage', 'Ġnew', 'Ġgem', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġmay', 'Ġcc', 'af', 'Ġus', 'sb', 'irs', 'ge', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġg', 'Ġsuccess', 'Ġfirst', 'Ġusage', 'Ġupper', 'Ġstage', 'Ġengine', 'Ġmission', 'Ġsuccessful', 'Ġunexpected', 'Ġvibration', 'Ġobserved', 'Ġnew', 'Ġengine', 'Ġuse', 'Ġengine', 'Ġvariant', 'Ġhold', 'Ġpending', 'Ġbetter', 'Ġunderstanding', 'Ġse', 'pt', 'ember', 'Ġlands', 'Ġearth', 'Ġobservation', 'Ġsatellite', 'Ġle', 'Ġsuccess', 'Ġoct', 'ober', 'Ġ09', 'Ġcc', 'af', 'Ġl', 'u', 'cy', 'Ġspace', 'Ġprobe', 'Ġhel', 'oc', 'entric', 'Ġsuccess', 'Ġde', 'cember', 'Ġcc', 'af', 'Ġtechnology', 'Ġdemonstration', 'Ġgeo', 'Ġsuccess', 'Ġlongest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġever', 'las', 'Ġrocket', 'las', 'Ġwik', 'ipedia', 'Ġflight', 'Ġdate', 'Ġtime', 'ut', 'c', 'Ġtype', 'Ġserial', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġtype', 'Ġpayload', 'Ġorbit', 'Ġoutcome', 'Ġremarks', 'Ġjan', 'uary', '00', 'g', 'ss', 'ap', 'Ġspace', 'Ġsurveillance', 'Ġgeo', 'Ġsuccess', 'Ġfirst', 'Ġplan', 'ne', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġmarch', 'Ġgoes', 'Ġmeteor', 'ology', 'Ġgeo', 'Ġsuccess', 'Ġmay', 'Ġbo', 'e', 'Ġunc', 'rew', 'ed', 'Ġorbital', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġle', 'iss', 'Ġsuccess', 'Ġj', 'uly', 'Ġus', 'sf', 'w', 'f', 'ov', 'Ġearly', 'Ġwarning', 'Ġgeo', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ']</t>
+          <t>['con', 'Ġrocket', 'Ġcert', 'ï', '¬', 'ģ', 'ed', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġprecious', 'Ġscience', 'Ġmissions', 'h', 'Ġc', 'ation', 'html', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'space', 'x', 'Ġreveals', 'Ġfal', 'con', 'Ġhall', 'ow', 'een', 'Ġdate', 'nas', 'asp', 'Ġe', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġoct', 'ober', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġadministration', 'Ġnational', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'Ġnew', 'Ġera', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġgovernment', 'Ġprinting', 'ï', '¬', 'ģ', 'ce', '09', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdavid', 'Ġj', 'Ġfr', 'kel', 'Ġapr', 'il', 'min', 'utes', 'Ġn', 'ac', 'Ġcommercial', 'Ġspace', 'Ġcommittee', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'c', 'ots', 'Ġdemo', 'Ġcompetition', 'na', 'Ġn', 'asa', 'Ġjan', 'uary', 'Ġarchived', 'Ġcompetition', 'html', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'space', 'Ġexploration', 'Ġtechnologies', 'space', 'x', ')"', 'http', 'Ġn', 'asa', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'statement', 'iam', 'Ġh', 'Ġger', 'sten', 'ier', 'Ġassociate', 'Ġadministrator', 'Ġspace', 'Ġoperations', 'Ġcommittee', 'Ġscience', 'Ġspace', 'Ġtechnology', 'Ġsubcommittee', 'Ġspace', 'Ġaer', 'aut', 'ics', 'Ġu', 'Ġhouse', 'Ġrepresentatives', 'http', 'science', 'hou', 'Ġu', 'Ġhouse', 'Ġrepresentatives', 'Ġmay', 'Ġarchived', 'web', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġde', 'cember', 'space', 'x', "'s", 'Ġdragon', 'Ġspacecraft', 'Ġsuccessfully']</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>['g', 'uration', 'th', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġengine', 'Ġaug', 'ust', 'Ġus', 'sb', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġgeo', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġoct', 'ober', 'es', 'es', 'Ġcommunication', 'Ġsatellites', 'Ġgeo', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'mber', 'Ġ09', 'Ġloft', 'id', 'Ġenvironmental', 'Ġsatellites', 'Ġsuccess', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġlas', 'las', 'Ġlaunch', 'Ġfinal', 'Ġï', '¬', 'Ĥ', 'ight', 'las', 'meter', 'Ġfair', 'ing', 'th', 'Ġuse', 'Ġsingle', 'Ġengine', 'Ġcent', 'aur', 'Ġu', 'la', 'Ġstopped', 'Ġselling', 'las', 'Ġv', 'Ġfly', 'Ġlaunches', 'Ġplanned', 'Ġlaunches', 'Ġsee', 'Ġlist', 'las', 'Ġlaunches', 'âĢĵ', 'Ġfirst', 'Ġpayload', 'Ġhot', 'Ġbird', 'Ġcommunications', 'Ġsatellite', 'Ġlaunched', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġaug', 'ust', 'las', 'Ġaug', 'ust', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġlaunched', 'Ġaboard', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġlaunch', 'Ġvehicle', 'Ġcompleted', 'Ġburns', 'minute', 'Ġperiod', 'Ġplaced', 'Ġinter', 'plan', 'etary', 'Ġtransfer', 'Ġorbit', 'Ġtowards', 'Ġmars', 'Ġjan', 'uary', 'Ġnew', 'Ġhor', 'izons', 'Ġlaunched', 'Ġlock', 'heed', 'Ġmart', 'las', 'Ġrocket', 'Ġthird', 'Ġstage', 'Ġadded', 'Ġincrease', 'Ġhel', 'oc', 'entric', 'escape', 'Ġspeed', 'Ġfirst', 'Ġlaunch', 'las', 'Ġconfiguration', 'Ġfive', 'Ġsolid', 'Ġrocket', 'Ġboosters', 'Ġfirst', 'las', 'Ġthird', 'Ġstage', 'Ġde', 'cember', 'las', 'Ġlifted', 'Ġheaviest', 'Ġpayload', 'Ġdate', 'Ġorbit', 'Ġcy', 'gn', 'us', 'Ġres', 'upp', 'ly', 'Ġcraft', 'Ġse', 'pt', 'ember', 'Ġos', 'iris', 'rex', 'Ġasteroid', 'Ġsample', 'Ġreturn', 'Ġmission', 'Ġlaunched', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġarrived', 'Ġasteroid', 'Ġb', 'enn', 'u', 'Ġde', 'cember', 'Ġdeparted', 'Ġback', 'Ġearth', 'Ġmay', 'Ġarrive', 'Ġse', 'pt', 'ember', 'Ġsample', 'Ġranging', 'Ġgrams', 'Ġkilograms']</t>
+          <t>['ent', 'ers', 'Ġorbit', 'Ġr', 'bit', 'press', 'Ġrelease', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmoney', 'Ġstew', 'art', 'Ġmarch', 'comp', 'etition', 'Ġfuture', 'Ġe', 'el', 'v', 'Ġprogram', 'part', ')"', 'Ġcle', 'Ġspace', 'Ġreview', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgovernment', 'Ġnecessary', 'Ġanchor', 'Ġtenant', 'Ġcommercial', 'Ġcargo', "'s", 'Ġsu', 'f', 'ï', '¬', 'ģ', 'cient', 'Ġbuild', 'Ġnew', 'Ġeconomic', 'Ġecosystem', '",', 'Ġsays', 'Ġsc', 'ott', 'Ġhub', 'bard', 'Ġaer', 'aut', 'ics', 'Ġresearcher', 'Ġst', 'ford', 'Ġuniversity', 'Ġcal', 'ornia', 'Ġformer', 'Ġdirector', 'Ġn', 'asa', "'s", 'es', 'Ġresearch', 'Ġcenter', 'ett', 'Ġfield', 'Ġcal', 'ornia', '."', 'Ġspace', 'x', 'Ġde', 'cember', 'n', 'asa', 'Ġselects', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġbooster', 'Ġdragon', 'Ġspacecraft', 'Ġcargo', 'Ġres', 'upp', 'ly', 'press', 'Ġrelease', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġfacts', 'Ġspace', 'x', 'Ġcosts', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġspace', 'x', 'usa', 'php', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġn', 'af', 'Ġcost', 'Ġestimates', 'Ġn', 'asa', 'gov', 'Ġaug', 'ust', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġgoes', 'âĢĶ', 'se', 'eks', 'Ġgovernment', 'Ġfunds', 'Ġdeep', 'Ġspace', 'Ġar', 'Ġtechn', 'ica', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġpl', 'oration', 'Ġj', 'uly', 'Ġshot', 'well', 'Ġj', 'une', 'Ġdiscussion', 'Ġshot', 'well', 'Ġpresident', 'Ġco', 'Ġspace', 'x', 'l', 'antic', 'Ġcouncil', 'Ġevent', 'Ġoccurs', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'une', 'n', 'asa', 'Ġultimately', 'Ġgave', 'Ġus', 'Ġmillion', 'Ġspace', 'x', 'Ġput', 'Ġmillion', 'Ġ...', 'Ġe', 'el', 'v', 'class', 'Ġlaunch', 'Ġvehicle', 'Ġ...', 'Ġwell', 'Ġcapsule', '."', 'Ġdavid', 'Ġle', 'ard', 'space', 'x', 'Ġtackles', 'Ġreusable', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġnews', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>['Ġfirst', 'Ġfour', 'Ġbo', 'e', 'ing', 'Ġspace', 'plane', 'Ġmissions', 'Ġsuccessfully', 'Ġlaunched', 'las', 'Ġv', 'Ġalso', 'Ġknown', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġreusable', 'Ġrobotic', 'Ġspacecraft', 'Ġoperated', 'Ġus', 'af', 'Ġautonom', 'ously', 'Ġconduct', 'Ġland', 'ings', 'Ġorbit', 'Ġrunway', 'Ġflights', 'Ġlaunched', 'las', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'Ġfirst', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġlanding', 'Ġspace', 'Ġshuttle', '000', 'Ġft', 'Ġrunway', 'Ġoccurred', 'Ġde', 'cember', 'Ġland', 'ings', 'Ġoccur', 'Ġv', 'enberg', 'Ġcape', 'aver', 'al', 'Ġdepending', 'Ġmission', 'Ġrequirements', 'Ġnotable', 'Ġmissions', 'las', 'Ġwik', 'ipedia', 'Ġde', 'cember', 'Ġfirst', 'Ġstar', 'liner', 'Ġcrew', 'Ġcapsule', 'Ġlaunched', 'Ġbo', 'e', 'oft', 'Ġun', 'crew', 'ed', 'Ġtest', 'Ġflight', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġperformed', 'Ġflaw', 'lessly', 'Ġanomaly', 'Ġspacecraft', 'Ġleft', 'Ġwrong', 'Ġorbit', 'Ġorbit', 'Ġlow', 'Ġreach', 'Ġflight', "'s", 'Ġdestination', 'Ġiss', 'Ġmission', 'Ġsubsequently', 'Ġcut', 'Ġshort', 'Ġlaunches', 'Ġj', 'uly', 'Ġstarting', 'Ġfirst', 'Ġlaunch', 'Ġaug', 'ust', 'las', 'Ġachieved', 'Ġmission', 'Ġsuccess', 'Ġrate', 'Ġvehicle', 'Ġsuccess', 'Ġrate', 'Ġcontrast', 'Ġindustry', 'Ġsuccess', 'Ġrate', 'âĢĵ', 'Ġfirst', 'Ġanomal', 'ous', 'Ġevent', 'Ġuse', 'las', 'Ġlaunch', 'Ġsystem', 'Ġoccurred', 'Ġj', 'une', 'Ġengine', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'las', 'Ġshut', 'Ġearly', 'Ġleaving', 'Ġpayload', 'Ġpair', 'Ġocean', 'Ġsurveillance', 'Ġsatellites', 'Ġlower', 'Ġintended', 'Ġorbit', 'Ġcause', 'Ġanomaly', 'Ġtraced', 'Ġleak', 'Ġvalve', 'Ġallowed', 'Ġfuel', 'Ġleak', 'Ġcoast', 'Ġfirst', 'Ġsecond', 'Ġburns', 'Ġresulting', 'Ġlack', 'Ġfuel', 'Ġcaused', 'Ġsecond', 'Ġburn', 'Ġterminate', 'Ġseconds', 'Ġearly', 'Ġreplacing', 'Ġvalve', 'Ġled', 'Ġdelay', 'Ġnext', 'las', 'Ġlaunch', 'Ġhowever', 'Ġcustomer', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'Ġcategorized', 'Ġmission', 'Ġsuccess', 'Ġflight', 'Ġmarch', 'Ġsuffered', 'performance', 'Ġanomaly', 'Ġfirst', 'stage', 'Ġburn', 'Ġshut', 'Ġseconds', 'Ġearly', 'Ġcent', 'aur', 'Ġproceeded', 'Ġboost', 'Ġorbital', 'Ġcy', 'gn', 'us', 'Ġpayload', 'Ġheaviest', 'las', 'Ġdate', 'Ġintended', 'Ġorbit']</t>
+          <t>['Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġmal', 'ik', 'ari', 'q', 'Ġmay', "'s", 'Ġstar', 'Ġwars', 'Ġday', 'Ġspace', 'x', 'Ġlaunched', 'fal', 'con', 'Ġspace', 'Ġspace', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġannounces', 'Ġfal', 'con', 'Ġfully', 'Ġreusable', 'Ġheavy', 'Ġlift', 'Ġlaunch', 'Ġvehicle', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'space', 'Ġact', 'Ġagreement', 'Ġn', 'asa', 'Ġspace', 'Ġexploration', 'Ġtechnologies', 'Ġinc', '.,', 'Ġcommercial', 'Ġorbital', 'Ġtransportation', 'Ġservices', 'Ġdemonstration', 'Ġn', 'asa', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġco', 'pping', 'er', 'Ġrob', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġfal', 'con', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġdelayed', 'Ġmonths', 'Ġlate', 'http', 'ï', '¬', 'Ĥ', 'ight', 'gl', 'Ġflight', 'Ġglobal', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġconducts', 'Ġfirst', 'Ġmulti', 'engine', 'Ġfiring', 'Ġfal', 'con', 'Ġrocket', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmarch', 'space', 'x', 'Ġsuccessfully', 'Ġconducts', 'Ġfull', 'Ġmission', 'length', 'Ġï', '¬', 'ģ', 'ring', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'press', 'Ġrelease', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'mber', 'mer', 'lin', 'Ġvacuum', 'Ġengine', 'Ġtest', 'Ġyoutube', 'mber', 'Ġarchived', 'http', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'space', 'x', 'Ġannounces', 'Ġfal', 'con', 'Ġassembly', 'Ġunderway', 'Ġcap', 'Ġpe', 'html', 'lando', 'Ġsent', 'inel', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'dates', 'Ġspace', 'x', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġk', 'mer', 'Ġk', 'en', 'Ġmarch']</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>['Ġusing', 'Ġfuel', 'Ġreserves', 'Ġmake', 'Ġshortfall', 'Ġfirst', 'Ġstage', 'Ġlonger', 'Ġburn', 'Ġcut', 'Ġshort', 'Ġlater', 'Ġcent', 'aur', 'Ġdisposal', 'Ġburn', 'Ġinvestigation', 'Ġincident', 'Ġrevealed', 'Ġanomaly', 'Ġdue', 'Ġfault', 'Ġmain', 'Ġengine', 'Ġmixture', 'rat', 'io', 'Ġsupply', 'Ġvalve', 'Ġrestricted', 'Ġflow', 'Ġfuel', 'Ġengine', 'Ġinvestigation', 'Ġsubsequent', 'Ġexamination', 'Ġvalves', 'Ġupcoming', 'Ġmissions', 'Ġled', 'Ġdelay', 'Ġnext', 'Ġseveral', 'Ġlaunches', 'Ġbo', 'e', 'ing', 'Ġstar', 'liner', 'Ġbo', 'e', 'ing', 'Ġel', 'ana', 'Ġge', 'ost', 'ation', 'ary', 'Ġoperational', 'Ġenvironmental', 'Ġsatellite', 'ars', 'Ġinsight', 'Ġjun', 'Ġl', 'u', 'cy', 'Ġlunar', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġlunar', 'Ġcrater', 'Ġobservation', 'Ġsensing', 'Ġsatellite', 'Ġmars', 'Ġreconnaissance', 'Ġorbit', 'er', 'Ġcuriosity', 'Ġpersever', 'ance', 'Ġingenuity', 'aven', 'th', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġlaunch', 'Ġnew', 'Ġhor', 'izons', 'Ġn', 'rol', 'Ġlaunches', 'Ġos', 'iris', 'rex', 'Ġsolar', 'Ġdynamics', 'Ġobserv', 'atory', 'Ġsolar', 'Ġorbit', 'er', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġus', 'Ġgeopolitical', 'Ġu', 'Ġpolitical', 'Ġconsiderations', 'Ġr', 'ussian', 'Ġwar', 'Ġcrime', 'Ġled', 'Ġeffort', 'Ġreplace', 'Ġr', 'ussian', 'supp', 'lied', 'Ġr', 'Ġengine', 'Ġused', 'Ġfirst', 'stage', 'Ġbooster', 'las', 'Ġv', 'Ġformal', 'Ġstudy', 'Ġcontracts', 'Ġissued', 'Ġj', 'une', 'Ġnumber', 'Ġu', 'Ġrocket', 'engine', 'Ġsuppliers', 'Ġresults', 'Ġstudies', 'Ġled', 'Ġdecision', 'Ġu', 'la', 'Ġdevelop', 'Ġnew', 'Ġvul', 'Ġcent', 'aur', 'Ġlaunch', 'Ġvehicle', 'Ġreplace', 'Ġexisting', 'las', 'Ġdelta', 'Ġse', 'pt', 'ember', 'Ġu', 'la', 'Ġannounced', 'Ġpartnership', 'Ġblue', 'Ġorigin', 'Ġdevelop', 'Ġl', 'ox', 'eth', 'ane', 'Ġengine', 'Ġreplace', 'Ġr', 'Ġnew', 'Ġfirst', 'stage', 'Ġbooster', 'las', 'Ġcore', 'Ġdesigned', 'Ġaround', 'Ġfuel', 'Ġcannot', 'Ġretro', 'fitted', 'Ġuse', 'Ġmethane', 'fuel', 'ed', 'Ġengine', 'Ġnew', 'Ġfirst', 'Ġstage', 'Ġdeveloped', 'Ġbooster', 'Ġfirst', 'stage', 'Ġtank', 'age', 'Ġdiameter', 'Ġdelta', 'Ġiv', 'Ġpowered', 'Ġtwo', 'Ġkn', '000', 'Ġthrust', 'Ġengine', 'Ġalready', 'Ġthird', 'Ġyear', 'Ġdevelopment', 'Ġblue', 'Ġorigin', 'Ġu', 'la', 'Ġexpected', 'Ġnew', 'Ġstage', 'Ġengine', 'Ġstart', 'Ġflying', 'Ġearlier', 'Ġvul', 'Ġinitially', 'Ġplanned', 'Ġuse', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'las', 'Ġv', 'Ġlater', 'Ġupgrade', 'ces', 'Ġhowever', 'ces', 'Ġlonger', 'Ġpursued', 'Ġcent', 'aur', 'Ġused', 'Ġinstead', 'Ġalso', 'Ġuse', 'Ġvariable', 'Ġnumber', 'Ġoptional', 'Ġsolid']</t>
+          <t>['successful', 'Ġengine', 'Ġtest', 'Ġfiring', 'Ġspace', 'x', 'Ġinaugural', 'Ġfal', 'con', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġden', 'ise', 'Ġch', 'ow', 'Ġde', 'cember', 'q', 'Ġspace', 'x', 'Ġce', 'Ġel', 'Ġmus', 'k', 'Ġmaster', 'Ġprivate', 'Ġspace', 'Ġdragons', 'sp', 'ac', 'html', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'production', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'space', 'x', 'Ġsays', 'Ġfal', 'con', 'Ġcompete', 'Ġe', 'el', 'v', 'Ġyear', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'within', 'Ġyear', 'Ġneed', 'Ġget', 'Ġright', 'Ġrocket', 'Ġcore', 'Ġevery', 'Ġfour', 'Ġweeks', 'Ġrocket', 'Ġcore', 'Ġevery', 'Ġtwo', 'Ġweeks', '...', 'Ġend', 'Ġsays', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġcompany', 'Ġplans', 'Ġrat', 'chet', 'Ġproduction', 'Ġcores', 'Ġper', 'Ġyear', '."', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġseeks', 'Ġaccelerate', 'Ġfal', 'con', 'Ġproduction', 'Ġlaunch', 'Ġrates', 'Ġyear', 'http', 'sp', 'ac', 'en', 'ew', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġoct', 'ober', 'cong', 'rats', 'space', 'x', 'Ġteam', 'th', 'Ġlaunch', 'Ġyear', 'Ġfal', 'con', 'Ġholds', 'Ġrecord', 'Ġlaunches', 'Ġsingle', 'Ġvehicle', 'Ġtype', 'Ġyear', 'http', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġdeb', 'uts', 'Ġnew', 'Ġmodel', 'Ġfal', 'con', 'Ġrocket', 'Ġdesigned', 'Ġastronauts', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġb', 'aylor', 'ichael', 'Ġmay', 'Ġblock', 'Ġspace', 'x', 'Ġincrease', 'Ġlaunch', 'Ġcad', 'ence', 'Ġlower', 'Ġprices', 'nas', 'asp', 'lower', 'pr', 'ices', 'Ġretrieved', 'Ġj', 'uly', 'Ġje', 'ff', 'Ġf', 'oust', 'Ġse', 'pt']</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>['Ġrocket', 'Ġboosters', 'Ġcalled', 'Ġgem', 'Ġderived', 'Ġnew', 'Ġsolid', 'Ġboosters', 'Ġplanned', 'las', 'ero', 'jet', 'Ġrocket', 'Ġengine', 'Ġdevelopment', 'Ġbackup', 'Ġplan', 'Ġvul', 'Ġaug', 'ust', 'Ġfirst', 'Ġvul', 'Ġflight', 'Ġplanned', 'Ġlate', 'Ġmission', 'Ġsuccess', 'Ġrecord', 'Ġnotable', 'Ġpayload', 'Ġreplacement', 'Ġvul', 'Ġretirement', 'las', 'Ġwik', 'ipedia', 'Ġaug', 'ust', 'Ġu', 'la', 'Ġannounced', 'Ġlonger', 'Ġselling', 'Ġlaunches', 'las', 'Ġwould', 'Ġfulfill', 'Ġexisting', 'Ġlaunch', 'Ġcontracts', 'Ġmade', 'Ġfinal', 'Ġpurchase', 'Ġr', 'Ġmotors', 'Ġneeded', 'Ġlast', 'Ġmotors', 'Ġdelivered', 'Ġapr', 'il', 'Ġlast', 'Ġlaunch', 'Ġoccur', 'Ġtime', 'Ġmid', '".[', 'Ġoct', 'ober', 'Ġlaunches', 'Ġremain', 'Ġcore', 'Ġstage', 'las', 'Ġraised', 'Ġvertical', 'Ġposition', 'orb', 'ital', 'Ġtest', 'Ġvehicle', 'Ġenc', 'ased', 'Ġpayload', 'Ġfair', 'ing', 'Ġapr', 'il', 'Ġlaunch', 'las', 'Ġmoved', 'Ġlaunch', 'Ġpad', 'las', 'Ġlaunch', 'Ġpad', 'las', 'Ġignition', 'las', 'Ġnew', 'Ġhor', 'izons', 'Ġprobe', 'Ġlaunches', 'Ġlaunch', 'Ġpad', 'Ġcape', 'aver', 'al', 'Ġcomparable', 'Ġrockets', 'Ġang', 'ara', 'ri', 'ane', 'Ġdelta', 'Ġiv', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlong', 'Ġmarch', 'Ġpro', 'ton', 'Ġvul', 'Ġcent', 'aur', 'Ġz', 'en', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcomparison', 'Ġorbital', 'Ġlaunchers', 'Ġfamilies', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġpronounced', 'las', 'Ġï', '¬', 'ģ', '".', 'v', 'Ġr', 'oman', 'Ġnum', 'eral', 'rocket', 'builder', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'las', 'Ġv', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġde', 'cember', 'Ġfrank', 'le', 'Ġj', 'ared', 'Ġj', 'uly', 'ula', 'Ġdelays', 'Ġfocused', 'Ġprotecting', 'Ġpercent', 'Ġmission', 'Ġsuccess', 'Ġrate', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġde', 'cember', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'n', 'ro', 'g', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'ula', 'Ġread', 'ies', 'las', 'Ġlaunch']</t>
+          <t>['ember', 'mus', 'k', 'Ġunve', 'ils', 'Ġrevised', 'Ġversion', 'Ġgiant', 'Ġinter', 'plan', 'etary', 'Ġlaunch', 'Ġsystem', 'Ġarchived', 'Ġoct', 'ober', 'Ġarchive', '".', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġmarch', 'space', 'x', 'Ġmakes', 'Ġaerospace', 'Ġhistory', 'Ġsuccessful', 'Ġlaunch', 'Ġlanding', 'Ġused', 'Ġrocket', 'htt', 'Ġverge', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'Ġl', 'op', 'atto', 'Ġel', 'izabeth', 'Ġmarch', 'space', 'x', 'Ġeven', 'Ġlanded', 'Ġnose', 'Ġcone', 'Ġhistoric', 'Ġused', 'Ġfal', 'con', 'Ġrocket', 'Ġlaunch', 'Ġverge', 'Ġarchived', 'http', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmarch', 'space', 'x', 'Ġfal', 'con', 'Ġsets', 'Ġnew', 'Ġrecord', 'Ġtel', 'star', 'v', 'Ġlaunch', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġj', 'uly', 'Ġarchived', 'unch', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġbids', 'Ġtemporary', 'Ġgoodbye', 'Ġwest', 'Ġcoast', 'Ġlaunch', 'Ġlanding', 'Ġphotos', 'w', 'Ġhot', 'os', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġsticks', 'Ġbooster', 'Ġrecovery', 'Ġcal', 'ornia', 'Ġlanding', 'Ġzone', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'launch', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġblock', 'Ġrad', 'ars', 'Ġconstellation', 'Ġsp', 'acet', 'v', 'Ġarchived', 'h', 'Ġell', 'ation', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġlaunches', 'Ġorbit', 'Ġstar', 'link', 'Ġsatellites', 'âĢĶ', 'igh', 'ing', 'Ġtotal', 'Ġmetric', 'Ġtons', 'âĢĶ', 'mark', 'ing', 'Ġheaviest', 'Ġpayload', 'Ġever', 'Ġï', '¬', 'Ĥ', 'Ġfal', 'con', 'Ġtwitter', 'Ġretrieved', 'Ġjan', 'uary', 'fal', 'con', 'Ġuser', "'s", 'Ġguide', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'h', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia']</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>['Ġreconnaissance', 'Ġsatellite', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'las', 'Ġsolid', 'Ġrocket', 'Ġmotor', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġarchived', 'Ġoriginal', 'Ġol', 'id', 'rocket', 'otor', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'space', 'Ġlaunch', 'Ġreport', 'las', 'Ġdata', 'Ġsheet', 'las', 'html', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġoct', 'ober', 'Ġarchived', 'http', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'gem', 'gem', 'Ġfact', 'Ġsheet', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġphoto', 'Ġgallery', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġreferences', 'las', 'Ġwik', 'ipedia', 'develop', 'ing', 'Ġvul', 'Ġcent', 'aur', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġaug', 'ust', 'ula', 'Ġstops', 'Ġselling', 'Ġcenterpiece', 'las', 'Ġv', 'Ġsetting', 'Ġpath', 'Ġrocket', "'s", 'Ġretirement', 'Ġverge', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġcent', 'ennial', 'Ġcolor', 'ado', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'lock', 'heed', 'Ġmart', 'Ġready', 'Ġlaunch', 'Ġint', 'els', 'Ġspacecraft', 'Ġlock', 'heed', 'Ġmart', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġassumes', 'Ġmarketing', 'Ġsales', 'las', 'Ġlock', 'heed', 'Ġmart', 'Ġpar', 'abolic', 'arc', 'Ġpar', 'abolic', 'Ġarc', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'las', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġpp', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'las', 'Ġstar', 'liner', 'Ġoft', 'Ġnumbers', 'Ġarchived', 'Ġoriginal', 'http', 'n', 'umbers', 'Ġj', 'uly', 'ev', 'olved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'Ġmarch', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['Ġmission', 'Ġstatus', 'Ġcenter', 'Ġj', 'une', '05', 'Ġut', 'c', 'Ġarchived', 'web', 'Ġmay', 'Ġway', 'back', 'Ġmachine', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaccessed', '06', '02', 'Ġquotation', 'Ġï', '¬', 'Ĥ', 'anges', 'Ġlink', 'Ġrocket', 'Ġground', 'Ġstorage', 'Ġtanks', 'Ġcontaining', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġfuel', 'Ġhelium', 'Ġgas', 'erous', 'Ġnitrogen', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġign', 'itor', 'Ġsource', 'Ġcalled', 'Ġbetter', 'Ġknown', 'Ġtea', 'tab', '".', 'oct', 'aw', 'eb', 'Ġv', 'oct', 'aw', 'eb', 'Ġspace', 'x', 'Ġnews', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġire', 'ne', 'Ġse', 'pt', 'ember', 'mus', 'k', 'Ġsays', 'Ġspace', 'x', 'extremely', 'Ġparanoid', 'Ġread', 'ies', 'Ġfal', 'con', 'Ġcal', 'ornia', 'Ġdebut', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġinformation', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmang', 'els', 'Ġjohn', 'Ġmay', 'n', 'asa', "'s", 'Ġplum', 'Ġbro', 'ok', 'Ġstation', 'Ġtests', 'Ġrocket', 'Ġfair', 'ing', 'Ġspace', 'x', 'Ġcle', 'veland', 'Ġplain', 'Ġdealer', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'Ġsv', 'ak', 'Ġamy', 'mber', 'dragon', "'s", 'rad', 'iation', 'oler', 'ant', 'Ġdesign', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'sche', 'dule', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'land', 'ing', 'Ġlegs', 'Ġspace', 'x', 'Ġnews', 'Ġapr', 'il', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġheavy', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcenter', 'Ġcore', 'Ġboosters', 'Ġcarry', 'Ġlanding', 'Ġlegs', 'Ġland', 'Ġcore', 'Ġsafely', 'Ġearth', 'Ġtakeoff', '."', 'Ġk', 'mer', 'Ġk', 'en', 'Ġjan', 'uary', 'fal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġbooster', 'Ġrecovery', 'Ġfeatured', 'Ġcool', 'Ġnew', 'Ġspace', 'x', 'Ġanimation', 'Ġx', 'anim', 'ation', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary']</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>['Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbon', 'nie', 'Ġbir', 'ck', 'en', 'st', 'aed', 'Ġb', 'ern', 'ard', 'Ġf', 'Ġk', 'utter', 'Ġfrank', 'Ġz', 'eg', 'ler', 'cent', 'aur', 'Ġapplication', 'Ġrobotic', 'Ġcrew', 'ed', 'Ġlunar', 'Ġland', 'er', 'Ġevolution', 'web', 'Ġol', 'ution', 'pdf', 'Ġameric', 'Ġinstitute', 'Ġphysics', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'las', 'Ġrockets', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'laun', 'cher', 'Ġfair', 'ings', 'Ġstructures', 'Ġru', 'ag', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'las', 'las', 'v', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġaug', 'ust', 'h', 'oney', 'well', 'Ġawarded', 'Ġmillion', 'las', 'Ġcontract', 'Ġmilitary', 'Ġaerospace', 'Ġelectronics', 'Ġapr', 'il', 'Ġretrieved', 'mber', 'las', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'h', 'oney', 'well', 'Ġprovides', 'Ġguidance', 'Ġsystem', 'las', 'Ġrocket', 'ww', 'Ġspace', 'travel', 'Ġaug', 'ust', 'Ġretrieved', 'mber', 'Ġj', 'ason', 'Ġrh', 'ian', 'Ġse', 'pt', 'ember', 'ula', 'Ġselects', 'Ġorbital', 'k', "'s", 'Ġgem', 'las', 'Ġvul', 'Ġboosters', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġinsider', 'Ġarchived', 'w', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġrocket', 'Ġboosters', 'Ġhelp', 'Ġsuccessfully', 'Ġlaunch', 'Ġunited', 'Ġlaunch', 'Ġalliance', "'s", 'las', 'Ġv', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġnews', 'room', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġg', 'ask', 'ill', 'Ġbr', 'addock', 'Ġjan', 'uary', 'human', 'Ġrated', 'las', 'Ġbig', 'el', 'ow', 'Ġspace', 'Ġstation', 'Ġdetails', 'Ġemerge', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'n', 'asa', 'Ġselects', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġcommercial', 'Ġcrew', 'Ġdevelopment', 'Ġprogram', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary']</t>
+          <t>['Ġsim', 'berg', 'Ġrand', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', 'Ġspace', 'x', "'s", 'Ġreusable', 'Ġrocket', 'Ġplans', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġch', 'ris', 'ster', 'Ġbeyond', 'Ġfront', 'iers', 'Ġbroad', 'gate', 'Ġpublications', 'Ġp', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġdf', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'mus', 'k', 'Ġambition', 'Ġspace', 'x', 'Ġaim', 'Ġfully', 'Ġreusable', 'Ġfal', 'con', 'http', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'Ġfal', 'con', "'s", 'Ġfourth', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġgot', 'Ġcooked', "'re", 'Ġgoing', 'Ġbeef', 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġthink', "'s", 'Ġhighly', 'Ġlikely', "'ll", 'Ġrecover', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġget', 'Ġback', "'ll", 'Ġsee', 'Ġsurvived', 'entry', 'Ġgot', 'Ġfried', 'Ġcarry', 'Ġprocess', "'s", 'Ġmake', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġreusable', "'ll", 'Ġeven', 'Ġharder', 'Ġsecond', 'Ġstage', 'Ġgot', 'Ġfull', 'Ġheats', 'h', 'ield', "'ll", 'Ġde', 'orbit', 'Ġpropulsion', 'Ġcommunication', '."', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġannual', 'Ġcomp', 'endium', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'Ġspace', 'x', 'Ġfounder', 'Ġchief', 'Ġdesigner', 'Ġel', 'Ġmus', 'k', 'Ġ03', '05', 'mus', 'k', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'web', 'arch', 'iv', 'Ġ03', '05', 'mus', 'k', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'une', 'oct', 'aw', 'eb', 'Ġspace', 'x', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġcommercial', 'Ġpromise', 'Ġtested']</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2362,7 +2362,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>['Ġaward', 'ees', 'Ġone', 'Ġyear', 'Ġlater', '?"', 'web', 'arc', 'Ġnewsp', 'ace', 'Ġjournal', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'http', 'new', 'sp', 'Ġhey', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'safety', 'Ġsystem', 'Ġtested', 'las', 'Ġdelta', 'Ġrockets', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'ul', 'acc', 'dev', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġbegins', 'Ġcommercial', 'Ġpartnership', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ht', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġboy', 'le', 'Ġal', 'Ġj', 'uly', 'rocket', 'Ġventure', 'Ġwork', 'Ġn', 'asa', 'Ġcosmic', 'Ġlog', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'uly', 'Ġke', 'lly', 'Ġjohn', 'Ġaug', 'ust', 'las', 'Ġrising', 'Ġoccasion', 'Ġspace', 'blog', 'Ġfl', 'ida', 'Ġtoday', 'Ġmel', 'bourne', 'Ġfl', 'ida', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġaug', 'ust', 'bo', 'e', 'ing', 'Ġselects', 'las', 'Ġrocket', 'Ġinitial', 'Ġcommercial', 'Ġcrew', 'Ġlaunches', 'h', 'press', 'Ġrelease', 'Ġh', 'ouston', 'Ġbo', 'e', 'ing', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'http', 'bo', 'e', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġmal', 'ik', 'ari', 'q', 'Ġaug', 'ust', 'bo', 'e', 'ing', 'Ġneeds', 'Ġspace', 'Ġpilots', 'Ġspaceship', 'Ġrocket', 'Ġtest', 'Ġflights', 'Ġspace', 'Ġarchived', 'web', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġp', 'app', 'al', 'ardo', 'Ġjo', 'e', 'bo', 'e', 'ing', "'s", 'Ġstar', 'liner', 'Ġfalls', 'Ġshort', 'Ġbig', 'Ġblow', 'Ġn', 'asa', "'s", 'Ġcrew', 'ed', 'Ġprogram', 'Ġpopular', 'Ġmechanics', 'Ġretrieved', 'Ġde', 'cember', 'las', 'Ġwik', 'ipedia', 'Ġsheet', 'z', 'ichael', 'Ġde', 'cember', 'bo', 'e', 'ing', 'Ġstar', 'liner', 'Ġfails', 'Ġkey', 'Ġn', 'asa', 'Ġmission', 'Ġautonomous', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsystem', 'Ġmalf', 'unctions']</t>
+          <t>['sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġmarch', 'space', 'x', 'Ġsays', 'Ġrequirements', 'Ġmarkup', 'Ġmake', 'Ġgovernment', 'Ġmissions', 'Ġcostly', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'une', 'Ġdan', 'Ġle', 'one', 'Ġj', 'uly', 'space', 'x', 'Ġtest', 'ï', '¬', 'ģ', 'res', 'Ġupgraded', 'Ġfal', 'con', 'Ġcore', 'Ġthree', 'Ġminutes', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġr', 'three', 'min', 'utes', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġj', 'une', 'red', 'ucing', 'Ġrisk', 'Ġvia', 'Ġground', 'Ġtesting', 'Ġrecipe', 'Ġspace', 'x', 'Ġsuccess', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġsv', 'ak', 'Ġamy', 'mber', 'mus', 'k', 'Ġfal', 'con', 'Ġcapture', 'Ġmarket', 'Ġshare', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', 'Ġcurrently', 'Ġproducing', 'Ġone', 'Ġvehicle', 'Ġper', 'Ġmonth', 'Ġnumber', 'Ġexpected', 'Ġincrease', 'Ġper', 'Ġyear', 'Ġnext', 'Ġcouple', 'Ġquarters', "'.", 'Ġend', 'Ġsays', 'Ġspace', 'x', 'Ġproduce', 'Ġlaunch', 'Ġvehicles', 'Ġper', 'Ġyear', '."', 'land', 'ing', 'Ġlegs', 'Ġg', 'leg', 'Ġspace', 'x', 'Ġj', 'uly', 'Ġarchived', 'land', 'ing', 'leg', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġl', 'ind', 'sey', 'Ġcl', 'ark', 'Ġmarch', 'space', 'x', 'Ġmoving', 'Ġquickly', 'Ġtowards', 'Ġï', '¬', 'Ĥ', 'back', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġnewsp', 'ace', 'Ġwatch', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'Ġmess', 'ier', 'Ġdou', 'g', 'Ġmarch', 'dragon', 'Ġpost', 'mission', 'Ġpress', 'Ġconference', 'Ġnotes', 'Ġpar', 'abolic', 'Ġarc', 'Ġarchived', 'Ġn', 'ference', 'notes', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmarch', 'Ġshot', 'well', 'Ġfe', 'b', 'ruary', 'Ġshot', 'well', 'Ġcomments', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġconference', 'htt', 'Ġcommercial', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġevent', 'Ġoccurs']</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2375,7 +2375,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġj', 'une', 'bo', 'e', 'ing', 'Ġstar', 'liner', 'Ġcapsule', 'Ġlifts', 'Ġspace', 'Ġstation', 'Ġsecond', 'Ġorbital', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtest', 'oft', 'launch', 'html', 'Ġcollect', 'space', 'Ġretrieved', 'Ġj', 'une', 'star', 'liner', 'Ġconcludes', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlanding', 'Ġnew', 'x', 'ico', 'http', 'Ġe', 'w', 'ex', 'ico', 'Ġspac', 'en', 'ews', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġsheet', 'z', 'ichael', 'Ġapr', 'il', 'amazon', 'Ġsigns', 'Ġu', 'la', 'Ġrockets', 'Ġlaunch', 'Ġje', 'ff', 'zos', 'Ġk', 'ui', 'per', 'Ġinternet', 'Ġsatellites', 'es', 'html', 'Ġretrieved', 'Ġj', 'uly', 'las', 'Ġv', 'Ġu', 'la', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġmarch', 'ike', 'Ġgr', 'uss', 'Ġj', 'une', 'air', 'Ġforce', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġu', 'la', 'Ġposition', 'las', 'Ġproduction', 'Ġrights', 'Ġspac', 'en', 'ews', 'jon', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġlaunch', 'Ġvehicle', 'Ġdatabase', 'web', 'arch', 'iv', 'Ġh', 'las', 'Ġj', 'athan', 'cd', 'owell', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'las', 'Ġmission', 'Ġplanner', "'s", 'Ġguide', 'Ġmarch', 'Ġarchived', 'htt', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġretrieved', 'Ġu', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġdevelopments', 'Ġconcepts', 'Ġvehicles', 'Ġtechnologies', 'Ġspac', 'ep', 'orts', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġe', 'gan', 'Ġbar', 'bara', 'bar', 'gan', 'Ġoct', 'ober', 'Ġcalling', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'Ġpayload', 'Ġfair', 'ing', 'Ġstar', 'liner', 'Ġboard', 'tw', 'itte', 'weet', 'Ġvia', 'Ġtwitter', 'Ġk', 'bs', 'Ġgun', 'ter', 'star', 'liner', 'c', 'st', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract']</t>
+          <t>['âĢĵ', '05', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġrev', 'http', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'http', 'space', 'x', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġje', 'ff', 'Ġf', 'oust', 'Ġde', 'cember', 'space', 'x', 'Ġpreparing', 'Ġlaunch', 'sign', 'ï', '¬', 'ģ', 'c', 'antly', 'Ġimproved', 'Ġfal', 'con', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'anian', 'Ġc', 'Ġsc', 'ott', 'Ġoct', 'ober', 'Ġel', 'Ġmus', 'k', 'Ġmit', 'Ġinterview', 'Ġevent', 'Ġoccurs', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'uly', 'Ġvia', 'Ġyoutube', 'th', 'Ġsw', 'Ġsupports', 'Ġsuccessful', 'Ġfal', 'con', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunch', 'th', 'Ġspace', 'Ġwing', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġshot', 'well', 'Ġmarch', 'Ġbroadcast', 'Ġspecial', 'Ġedition', 'Ġinterview', 'Ġshot', 'well', 'audio', 'Ġï', '¬', 'ģ', 'le', 'Ġspace', 'Ġshow', 'Ġevent', 'Ġoccurs', 'Ġ08', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'h', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġde', 'cember', 'space', 'x', 'Ġsuccessfully', 'Ġlanded', 'Ġfal', 'con', 'Ġrocket', 'Ġlaunching', 'Ġspace', 'ww', 'land', 'ing', 'success', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġj', 'ames', 'Ġdean', 'Ġmarch', 'usable', 'Ġfal', 'con', 'Ġrocket', 'Ġtriumph', 'Ġspace', 'x', 'Ġel', 'Ġmus', 'k', 'Ġus', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'el', 'mus', 'k', 'Ġj', 'une', 'flying', 'Ġlarger', 'Ġsign', 'ï', '¬', 'ģ', 'c', 'antly', 'Ġupgraded', 'Ġhyp', 'erson', 'ic', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġsingle', 'Ġpiece', 'Ġcast', 'Ġcut', 'Ġtitanium', 'Ġtake', 'entry', 'Ġheat', 'Ġshielding', 'twitter', 'weet', 'Ġretrieved', 'Ġj']</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>['aven', 'Ġmission', 'http', 'mar', 'Ġmars', 'n', 'asa', 'gov', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ula', 'Ġfrequently', 'Ġasked', 'Ġquestions', 'Ġlaunch', 'Ġcosts', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'Ġnorth', 'Ġk', 'Ġoct', 'ober', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġtd', 'rs', 'Ġsatellite', 'Ġn', 'asa', 'gov', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgr', 'ush', 'Ġlore', 'n', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġunve', 'ils', 'Ġwebsite', 'Ġlets', 'Ġprice', 'Ġrocket', 'like', 'Ġbuilding', 'Ġcar', 'ww', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġstep', 'hen', 'Ġcl', 'ark', 'mber', 'izing', 'Ġameric', "'s", 'Ġplace', 'Ġglobal', 'Ġlaunch', 'Ġindustry', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'commercial', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġth', 'om', 'pson', 'Ġlore', 'n', 'ce', 'ory', 'Ġbr', 'uno', 'Ġexplains', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġstay', 'Ġahead', 'Ġcompetitors', 'Ġforb', 'es', 'Ġretrieved', 'Ġde', 'cember', 'Ġgreat', 'Ġrocket', 'Ġrace', 'Ġg', 'rocket', 'race', 'Ġfortune', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'iam', 'Ġhar', 'wood', 'mber', 'ula', 'Ġunve', 'ils', 'rocket', 'builder', 'Ġwebsite', 'bsite', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġder', 'bsite', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'las', 'Ġproduct', 'Ġcard', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġrand', 'Ġcorporation', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġdf', 'Ġoct', 'ober', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġrand', 'Ġcorporation', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġdf', 'Ġoct', 'ober', 'Ġfinal', 'Ġreport', 'Ġseeking', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġprogram', 'Ġworthy', 'Ġgreat', 'Ġnation', 'Ġe', 'port', 'pdf', 'Ġarchived', 'Ġway', 'back', 'Ġmachine', 'Ġoct', 'ober']</t>
+          <t>['une', 'Ġvia', 'Ġtwitter', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġj', 'une', 'space', 'x', "'s", 'Ġfinal', 'Ġfal', 'con', 'Ġdesign', 'Ġcoming', 'Ġyear', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'w', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġaug', 'ust', 'home', 'Ġforums', 'Ġsign', 'Ġiss', 'Ġcommercial', 'Ġshuttle', 'Ġsl', 'ion', 'Ġr', 'ussian', 'Ġeuro', 'pe', 'Ġch', 'inese', 'Ġunmanned', 'Ġfal', 'con', 'Ġblock', 'Ġdebut', 'Ġsuccess', 'Ġdragon', 'Ġarrives', 'Ġstation', 'Ġber', 'thing', 'Ġg', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġgra', 'ham', 'iam', 'Ġaug', 'ust', 'space', 'x', 'Ġfal', 'con', 'Ġlaunches', 'Ġcr', 'Ġdragon', 'Ġmission', 'Ġiss', 'Ġretrieved', 'Ġj', 'uly', 'Ġboy', 'le', 'Ġal', 'Ġoct', 'ober', 'space', 'x', "'s", 'Ġel', 'Ġmus', 'k', 'Ġg', 'eeks', 'Ġmars', 'Ġinter', 'plan', 'etary', 'Ġtransport', 'Ġplan', 'Ġreddit', 'Ġgeek', 'wire', 'Ġarchived', 'Ġut', 'ars', 'reddit', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary', 'space', 'x', 'Ġmay', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'n', 'al', 'Ġexpend', 'able', 'Ġrocket', 'Ġe', 'rocket', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'Ġcooper', 'Ġben', 'Ġapr', 'il', 'rocket', 'Ġlaunch', 'Ġviewing', 'Ġguide', 'Ġcape', 'aver', 'al', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', 'Ġset', 'Ġdebut', 'Ġfal', 'con', 'Ġrocket', 'Ġupgrades', 'Ġlaunch', 'Ġnext', 'Ġweek', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'web', 'Ġunch', 'next', 'week', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj']</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>['Ġreview', 'Ġu', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġplans', 'Ġcommittee', 'Ġgraphic', 'Ġp', 'Ġretrieved', '02', '07', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'development', 'Ġlaunch', 'Ġvehicle', 'Ġnew', 'Ġmedium', 'Ġclass', 'Ġlaunch', 'Ġvehicle', 'Ġj', 'apan', 'Ġengineering', 'Ġreview', 'Ġretrieved', 'mber', 'j', 'apan', 'Ġscraps', 'Ġrocket', 'Ġdevelopment', 'Ġproject', 'ock', 'alyst', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġr', 'icle', 'id', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'ike', 'Ġgr', 'uss', 'Ġmay', 'ero', 'jet', 'Ġteam', 'Ġseeking', 'las', 'Ġproduction', 'Ġrights', 'Ġspac', 'en', 'ews', 'aug', 'ural', 'las', 'Ġscores', 'Ġsuccess', 'Ġil', 'Ġlock', 'heed', 'Ġmart', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ils', 'Ġlaunches', 'Ġhell', 'sat', 'las', 'Ġv', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ils', 'Ġlaunches', 'Ġrainbow', 'Ġsatellite', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ils', 'Ġlaunches', 'Ġwraps', 'Ġyear', 'Ġmission', 'Ġsuccesses', 'ht', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'las', 'Ġwik', 'ipedia', 'ils', 'las', 'Ġvehicle', 'Ġlifts', 'Ġmassive', 'Ġsatellite', 'ars', 'http', 'ils', 'l', 'Ġell', 'ite', 'ars', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġmarch', 'Ġarchived', 'Ġsat', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'asa', "'s", 'Ġmultip', 'ur', 'pose', 'Ġmars', 'Ġmission', 'Ġsuccessfully', 'Ġlaunched', 'Ġn', 'asa', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'html', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', "'s", 'Ġpl', 'uto', 'Ġmission', 'Ġlaunched', 'Ġtoward', 'Ġnew', 'Ġhor', 'izons']</t>
+          <t>['une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġblock', 'Ġrockets', 'Ġtargets', 'mber', 'Ġlaunch', 'Ġdebut', 'es', 'lar', 'ati', 'Ġarchived', 'Ġove', 'mber', 'launch', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġk', 'yle', 'Ġed', 'space', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'http', 'sp', 'ac', 'el', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'f', 'iche', 'Ġtechnique', 'Ġfal', 'con', 'technical', 'Ġdata', 'Ġsheet', 'Ġfal', 'con', '].', 'Ġes', 'pace', 'Ġexploration', 'Ġfrench', 'Ġmay', 'Ġpp', 'âĢĵ', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'space', 'x', 'Ġdebut', 'Ġupgraded', 'Ġfal', 'con', 'Ġreturn', 'Ġflight', 'Ġmission', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'space', 'Ġlaunch', 'Ġreport', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġspace', 'flight', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġoverview', 'http', 'space', 'ï', '¬', 'Ĥ', 'ig', 'Ġspace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġspace', 'x', 'bang', 'aband', 'hu', 'Ġsatellite', 'Ġmission', 'yout', 'ub', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'web', 'ar', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'mber', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġprepares', 'Ġmission', 'Ġdragon', "'s", 'Ġreturn', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġaforementioned', 'Ġsecond', 'Ġstage', 'Ġtasked', 'Ġbusy', 'Ġrole', 'Ġmission', 'Ġloft', 'ing', 'Ġspacecraft']</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>['web', 'ar', 'Ġn', 'asa', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ils', 'Ġlaunches', 'Ġast', 'ra', 'Ġsatellite', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'news', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfirst', 'Ġus', 'af', 'las', 'Ġv', 'htt', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'mission', 'Ġstatus', 'Ġcenter', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'web', 'arch', 'iv', 'Ġn', 'ro', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'n', 'ro', 'g', 'n', 'ro', 'gov', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'ula', 'Ġread', 'ies', 'las', 'Ġlaunch', 'Ġreconnaissance', 'Ġsatellite', 'h', 'Ġspace', 'flight', 'Ġinsider', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'atellite', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġpet', 'erson', 'Ġpat', 'rick', 'Ġse', 'pt', 'ember', 'f', 'ault', 'Ġvalve', 'Ġpushes', 'Ġback', 'las', 'Ġlaunch', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'http', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'ro', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'ell', 'ite', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'united', 'Ġlaunch', 'Ġalliance', 'Ġinaugural', 'las', 'Ġwest', 'Ġcoast', 'Ġlaunch', 'Ġsuccess', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'Ġheaviest', 'Ġcommercial', 'Ġsatellite', 'las']</t>
+          <t>['Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', '."', 'Ġbar', 'bara', 'Ġop', 'rome', 'Ġoct', 'ober', 'ia', 'Ġdevelops', 'Ġsmall', 'Ġelectric', 'powered', 'sat', 'Ġdef', 'ensen', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'Ġtons', 'Ġlargest', 'Ġcommunications', 'Ġsatellite', 'Ġever', 'Ġbuilt', 'Ġ', 'ia', 'Ġscheduled', 'Ġlaunch', 'Ġearly', 'Ġcape', 'aver', 'al', 'Ġaboard', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlauncher', 'Ġreplace', 'Ġnearing', 'Ġend', 'year', 'Ġlife', '."', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġgun', 'ter', 'Ġarchived', 'w', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'orb', 'comm', 'Ġcraft', 'Ġfalls', 'Ġearth', 'Ġcompany', 'Ġclaims', 'Ġtotal', 'Ġloss', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'active', 'Ġlaunch', 'Ġvehicle', 'Ġreliability', 'Ġstatistics', 'http', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġarchived', 'Ġoriginal', 'g', 'html', 'rate', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'list', 'e', 'Ġde', 'ous', 'Ġles', 'Ġl', 'ance', 'ments', 'z', 'Ġk', 'os', 'mon', 'av', 'ika', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'est', 'imating', 'Ġreliability', 'Ġspacecraft', 'Ġmission', 'Ġ01', '0001', 'pdf', 'Ġn', 'asa', 'Ġjan', 'uary', 'Ġfigure', 'Ġhistorical', 'Ġrocket', 'Ġlaunch', 'Ġdata', 'Ġrocket', 'Ġfamily', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'hold', 'Ġarms', 'Ġtail', 'Ġservice', 'asts', 'http', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'fal', 'con', 'Ġcompletes', 'Ġfull', 'duration', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġe', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay']</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2427,7 +2427,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>['Ġv', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmoon', 'Ġmission', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'cl', 'ues', 'Ġmystery', 'Ġpayload', 'Ġemerge', 'Ġsoon', 'Ġlaunch', 'web', 'ar', 'Ġ01', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'h', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpan', 'Ġsatellite', 'w', 'Ġes', 'news', 'sh', 'tml', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'rocket', 'Ġstage', 'Ġlaunched', 'Ġyears', 'Ġago', 'Ġdisinteg', 'rates', 'Ġtrail', 'Ġspace', 'Ġjunk', 'video', ')"', 'Ġspace', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'th', 'las', 'Ġmission', 'Ġsuccessfully', 'Ġlaunches', 'ms', 'p', 'Ġf', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'th', 'Ġcommercial', 'Ġmission', 'Ġint', 'els', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'Ġsolar', 'Ġobserv', 'atory', 'Ġmission', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmission', 'w', 'Ġes', 'news', 'sh', 'tml', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġexperts', 'Ġweigh', 'Ġrocket', 'Ġdebris', 'Ġfound', 'Ġh', 'ilton', 'Ġhead', 'http', 'w', 'ist', 'Ġw', 'ist', 'v', 'Ġretrieved', 'Ġarchived', 'Ġmarch', 'Ġway', 'back', 'Ġmachine', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfirst', 'Ġmission', 'htt', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġnational', 'Ġdefense', 'Ġmission', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember']</t>
+          <t>['space', 'x', 'Ġconducts', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'Ġtypically', 'Ġends', 'second', 'Ġengine', 'Ġï', '¬', 'ģ', 'ring', 'Ġevery', 'Ġlaunch', 'Ġwr', 'ing', 'Ġissues', 'Ġrocket', 'Ġground', 'Ġsystems', 'Ġexercise', 'Ġalso', 'Ġhelps', 'Ġengineers', 'Ġrehe', 'arse', 'Ġreal', 'Ġlaunch', 'Ġday', '."', 'Ġcl', 'ark', 'Ġstep', 'hen', 'st', 'arl', 'ink', 'Ġsatellite', 'Ġdeployments', 'Ġcontinue', 'Ġsuccessful', 'Ġfal', 'con', 'Ġlaunch', 'launch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'uly', 'ichael', 'Ġbel', 'ï', '¬', 'ģ', 'ore', 'Ġse', 'pt', 'ember', 'behind', 'Ġscenes', 'Ġworld', "'s", 'Ġambitious', 'Ġrocket', 'Ġmakers', 'http', 'popular', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'dates', 'Ġde', 'cember', '007', 'Ġupdates', 'Ġarchive', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'ht', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġnine', 'Ġengines', 'Ġstage', 'Ġworking', 'Ġwell', 'Ġsystem', 'Ġextensively', 'Ġtest', 'engine', 'Ġcapability', 'Ġincludes', 'Ġexplosive', 'Ġï', '¬', 'ģ', 'Ġtesting', 'Ġbarriers', 'Ġseparate', 'Ġengines', 'Ġvehicle', 'Ġ...', 'Ġsaid', 'Ġfailure', 'Ġmodes', "'ve", 'Ġseen', 'Ġdate', 'Ġtest', 'Ġstand', 'Ġmer', 'lin', 'Ġrelatively', 'Ġbenign', 'Ġturbo', 'Ġpump', 'Ġcombustion', 'Ġchamber', 'Ġnozzle', 'Ġrupture', 'Ġexplos', 'ively', 'Ġeven', 'Ġsubjected', 'Ġextreme', 'Ġcircumstances', 'Ġseen', 'Ġgas', 'Ġgenerator', 'Ġdrives', 'Ġturbo', 'Ġpump', 'Ġassembly', 'Ġblow', 'Ġapart', 'Ġstart', 'Ġsequence', 'Ġchecks', 'Ġplace', 'Ġprevent', 'Ġhappening', 'Ġsmall', 'Ġdevice', 'Ġunlikely', 'Ġcause', 'Ġmajor', 'Ġdamage', 'Ġengine', 'Ġlet', 'Ġalone', 'Ġneighbouring', 'Ġones', 'Ġeven', 'Ġengine', 'Ġn', 'ace', 'es', 'Ġcommercial', 'Ġjets', 'Ġï', '¬', 'ģ', 'expl', 'os', 'ive', 'Ġbarriers', 'Ġassume', 'Ġentire', 'Ġchamber', 'Ġblows', 'Ġapart', 'Ġworst', 'Ġpossible', 'Ġway', 'Ġbottom', 'Ġclose', 'Ġpanels', 'Ġdesigned', 'Ġdirect', 'Ġforce', 'Ġï', '¬', 'Ĥ', 'ame', 'Ġdownward', 'Ġaway', 'Ġneighbouring', 'Ġengines', 'Ġstage', 'Ġ...', "'ve", 'Ġfound', 'Ġfal', 'con', 'Ġability', 'Ġwithstand', 'Ġone', 'Ġeven', 'Ġmultiple', 'Ġengine', 'Ġfailures', 'Ġcommercial', 'Ġair', 'liners', 'Ġstill', 'Ġcomplete', 'Ġmission', 'Ġcompelling', 'Ġselling', 'Ġpoint', 'Ġcustomers', 'Ġapart']</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>['united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecond', 'Ġmission', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'las', 'Ġwik', 'ipedia', 'ula', 'Ġsuccessfully', 'Ġlaunches', 'Ġfifth', 'Ġn', 'ro', 'Ġmission', 'Ġseven', 'Ġmonths', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'sb', 'irs', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġjun', 'Ġspacecraft', 'Ġfive', 'year', 'Ġjourney', 'Ġstudy', 'Ġj', 'upiter', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġhar', 'wood', 'iam', 'mber', 'ars', 'Ġscience', 'Ġlaboratory', 'Ġbegins', 'Ġcruise', 'Ġred', 'Ġplanet', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'chall', 'enge', 'Ġgetting', 'Ġmars', 'Ġchapter', 'Ġlaunching', 'Ġcuriosity', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġr', 'ik', 'sle', 'ws', 'ki', 'mber', 'us', 'Ġmart', 'ian', 'Ġn', 'uke', 'ruck', 'Ġlaunches', 'Ġwithout', 'Ġhitch', '..."', 'Ġregister', 'Ġarchived', 'Ġoriginal', 'ms', 'l', 'launch', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'th', 'Ġcent', 'aur', 'Ġsuccessfully', 'Ġlaunches', 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġmission', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġray', 'Ġfe', 'b', 'ruary', 'land', 'mark', 'Ġlaunch', 'Ġrocket', 'ry', 'Ġcent', 'aur', 'Ġset', 'Ġflight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġent', 'aur', 'Ġapr', 'il', 'Ġgra', 'ham', 'iam', 'Ġber', 'gin', 'Ġch', 'ris', 'mber', 'Ġhanded', 'Ġus', 'af', 'Ġcompleting', 'orbit', 'Ġtesting', 'nas', 'asp', 'Ġing', 'Ġnas', 'asp', 'ace', 'ï', '¬']</t>
+          <t>['Ġspace', 'Ġshuttle', 'Ġnone', 'Ġexisting', 'Ġlaunch', 'Ġvehicles', 'Ġafford', 'Ġlose', 'Ġeven', 'Ġsingle', 'Ġthrust', 'Ġchamber', 'Ġwithout', 'Ġcausing', 'Ġloss', 'Ġmission', '."', 'space', 'x', 'Ġengine', 'Ġissue', 'Ġlast', 'Ġstar', 'link', 'Ġmission', 'Ġcaused', 'Ġcleaning', 'Ġï', '¬', 'Ĥ', 'uid', 'Ġaccording', 'Ġel', 'Ġmus', 'k', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'component', 'Ġfatigue', 'Ġcaused', 'Ġearly', 'Ġshutdown', 'Ġmer', 'lin', 'Ġengine', 'Ġlast', 'Ġspace', 'x', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'http', 'Ġretrieved', 'Ġjan', 'uary', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġmarch', 'ch', 'ris', 'Ġber', 'gin', 'Ġn', 'sf', 'Ġtwitter', 'Ġfal', 'con', 'Ġlanding', 'Ġfailure', 'Ġupdate', 'Ġmer', 'lin', 'Ġengine', 'Ġboot', 'Ġlife', 'Ġleader', 'Ġdeveloped', 'Ġhole', 'Ġsent', 'Ġhot', 'Ġgas', "'t", 'Ġsupposed', 'Ġshut', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġenough', 'Ġthrust', 'Ġlanding', 'Ġtwitter', 'Ġretrieved', 'Ġjan', 'uary', 'Ġl', 'ind', 'sey', 'Ġcl', 'ark', 'inter', 'view', 'Ġel', 'Ġmus', 'k', 'http', 'h', 'obby', 'Ġh', 'obb', 'ys', 'pace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'x', 'Ġattempt', 'Ġdevelop', 'Ġfully', 'Ġreusable', 'Ġspace', 'Ġlaunch', 'Ġvehicle', 'Ġwashing', 'ton', 'Ġpost', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġrocket', "'s", 'Ġstages', 'Ġwould', 'Ġreturn', 'Ġlaunch', 'Ġsite', 'Ġtouch', 'Ġvertically', 'Ġrocket', 'Ġpower', 'Ġlanding', 'Ġgear', 'Ġdelivering', 'Ġspacecraft', 'Ġorbit', '."', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġwall', 'ike', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġunve', 'ils', 'Ġplan', 'Ġworld', "'s", 'Ġfirst', 'Ġfully', 'Ġreusable', 'Ġrocket', 'Ġspace', 'Ġarchived', 'Ġket', 'el', 'mus', 'k', 'html', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġboy', 'le', 'Ġal', 'Ġde', 'cember', 'space', 'x', 'Ġlaunches', 'Ġgrass', 'ho', 'pper', 'Ġrocket', 'story', 'high', 'Ġhop', 'Ġtex', 'http', 'cos', 'mi', 'Ġcosmic', 'Ġlog', 'Ġarchived', 'Ġoriginal', 'Ġmarch']</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>['Ĥ', 'ight', 'Ġretrieved', 'mber', 'Ġarchived', 'htt', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġgra', 'ham', 'iam', 'Ġse', 'pt', 'ember', 'ula', 'las', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġlaunches', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġthird', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'ala', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġtracking', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġray', 'las', 'Ġrocket', 'Ġlaunch', 'Ġcontinues', 'Ġlegacy', 'Ġlands', 'http', 'sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'web', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecond', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'b', 'irs', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'w', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'ula', 'Ġlaunches', 'th', 'Ġsuccessful', 'Ġmission', 'Ġmonths', 'Ġlaunch', 'Ġsatellite', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'Ġsuccessfully', 'Ġlaunches', 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġmission', 'Ġu', 'Ġnavy', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'Ġsuccessfully', 'Ġlaunches', 'aven', 'Ġmission', 'Ġjourney', 'Ġred', 'Ġplanet', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember']</t>
+          <t>['Ġretrieved', 'Ġde', 'cember', 'Ġgra', 'ham', 'iam', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġsuccessfully', 'Ġlaunches', 'Ġdebut', 'Ġfal', 'con', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'dragon', 'Ġsuccessfully', 'Ġlaunched', 'Ġrocket', 'Ġrecovery', 'Ġdemo', 'Ġcrash', 'Ġlands', 'http', 'space', 'ï', '¬', 'Ĥ', 'ight', 'n', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'ris', 'Ġapr', 'il', 'space', 'x', 'Ġchecks', 'Ġthrottle', 'Ġvalve', 'Ġflawed', 'Ġfal', 'con', 'Ġrecovery', 'Ġattempt', 'att', 'empt', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'Ġwall', 'ike', 'Ġde', 'cember', 'wow', 'Ġspace', 'x', 'Ġlands', 'Ġorbital', 'Ġrocket', 'Ġsuccessfully', 'Ġhistoric', 'Ġfirst', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'space', 'x', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġlanding', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġsecond', 'Ġstage', 'Ġcontinuing', 'Ġnom', 'inally', 'http', 'weet', 'Ġretrieved', 'Ġmay', 'Ġvia', 'Ġtwitter', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'launch', 'Ġschedule', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmark', 'us', 'Ġpay', 'er', 'Ġmarch', 'ses', 'Ġlaunched', 'Ġsuccessfully', 'Ġspace', 'x', "'s", 'Ġï', '¬', 'Ĥ', 'ight', 'proven', 'Ġfal', 'con', 'Ġrocket', 'ses', 'co', 'press', 'Ġrelease', 'es', 'Ġarchived', 'http', 'Ġen', 'fal', 'con', 'rocket', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'une', 'Ġbart', 'Ġle', 'ah', 'Ġapr', 'il', 'tw', 'ice', 'laun', 'ched', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġreturned', 'Ġport', 'aver', 'al', 'Ġspace', 'flight', 'Ġinsider', 'Ġarchived', 'Ġ', 'eral', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'bul', 'gar', 'ia', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcommunications', 'Ġsatellite', 'Ġride', 'Ġspace', 'x', "'s", 'Ġsecond', 'Ġreused', 'Ġrocket', 'space', 'ï']</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġrocket', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġu', 'la', 'Ġarchived', 'Ġoriginal', 'Ġe', 'ws', 'sh', 'tml', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġtracking', 'Ġdata', 'Ġrelay', 'Ġsatellite', 'Ġpayload', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġair', 'Ġforce', "'s", 'Ġweather', 'Ġsatellite', 'Ġorbit', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecond', 'Ġmission', 'Ġseven', 'Ġdays', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfour', 'Ġmissions', 'Ġseven', 'Ġweeks', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġtwo', 'Ġrockets', 'Ġfour', 'Ġdays', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġlaunches', 'Ġworldview', 'Ġsatellite', 'Ġdigital', 'gl', 'obe', 'Ġg', 'ital', 'gl', 'obe', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġig', 'ital', 'gl', 'obe', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'ula', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġsecretive', 'Ġcl', 'io', 'Ġmission', 'Ġse', 'pt', 'ember', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġwik', 'ipedia', 'united', 'Ġlaunch', 'Ġalliance', 'Ġlaunches', 'th', 'Ġmission', 'Ġcape', 'aver', 'al', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'orb', 'ital', 'Ġdebris', 'Ġquarterly', 'Ġnews', 'Ġn', 'asa', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'th', 'las', 'Ġrocket', 'ht', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober']</t>
+          <t>['¬', 'Ĥ', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'p', 'rel', 'aunch', 'Ġpreview', 'Ġspace', 'x', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'every', 'Ġeveryday', 'Ġastronaut', 'mber', 'Ġarchived', 'w', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'space', 'x', 'Ġresume', 'Ġstar', 'link', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġstretching', 'Ġreused', 'Ġfal', 'con', 'Ġrockets', 'Ġlimits', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġlaunches', 'Ġstar', 'link', 'Ġsatellites', 'Ġrecord', 'th', 'Ġlif', 'ff', 'Ġlanding', 'Ġreused', 'Ġrocket', 'Ġspace', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġr', 'us', 'sell', 'Ġb', 'og', 'ove', 'Ġj', 'uly', 'use', 'Ġspace', 'x', 'Ġplan', 'Ġachieve', 'us', 'ability', 'Ġfal', 'con', 'second', 'Ġstage', '?"', 'htt', 'Ġst', 'ac', 'ke', 'x', 'change', 'Ġarchived', 'stage', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġjan', 'uary', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', 'Ġsuccessfully', 'Ġcatches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġfair', 'ing', 'Ġste', 'ven', "'s", 'ms', 'Ġtree', "'s", 'Ġnet', 'ww', 'Ġeven', 'ms', 'tree', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġapr', 'il', 'rocket', 'Ġreport', 'Ġspace', 'x', 'Ġab', 'ons', 'Ġcatching', 'Ġfair', 'ings', '..."', 'Ġer', 'st', 'ages', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'space', 'x', 'Ġpoised', 'Ġlaunch', 'Ġhistoric', 'Ġpad', 'http', '09', 'Ġsm', 'ith', 'sonian', 'Ġair', 'Ġspace', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsim', 'burg', 'Ġrand', 'space', 'x', 'Ġpress']</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2479,7 +2479,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'las', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġu', 'Ġnavy', "'s", 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġx', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsolar', 'Ġprobes', 'Ġstudy', 'Ġspace', 'Ġweather', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġglobal', 'Ġpositioning', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġx', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġu', 'Ġnavy', "'s", 'Ġmobile', 'Ġuser', 'Ġobjective', 'Ġsystem', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'h', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġreaches', 'Ġsuccessful', 'Ġmissions', 'los', 'Ġsatellite', 'ite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġsatellite', 'Ġoct', 'ober', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'air', 'force', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġcy', 'gn', 'us', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['Ġconference', 'http', 'tr', 'ste', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', '..', 'Ġmus', 'k', 'Ġquote', 'Ġnever', 'Ġgive', 'Ġnever', 'us', 'ability', 'Ġone', 'Ġimportant', 'Ġgoals', 'Ġbecome', 'Ġbiggest', 'Ġlaunch', 'Ġcompany', 'Ġworld', 'Ġmaking', 'Ġmoney', 'Ġhand', 'Ġï', '¬', 'ģ', 'st', "'re", 'Ġstill', 'Ġreusable', 'Ġconsider', 'Ġus', 'Ġfailed', '".', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġmarch', 'space', 'x', 'Ġprepares', 'Ġfal', 'con', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunch', 'Ġtargets', 'Ġreturn', 'n', 'asa', 'Ġ', 'urn', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġch', 'ris', 'Ġg', 'eb', 'hardt', 'Ġapr', 'il', 'fal', 'con', 'Ġheavy', 'Ġbuild', 'Ġbegins', 'Ġpad', 'Ġrebuild', 'Ġprogressing', 'Ġwell', 'Ġess', 'ing', 'Ġnas', 'asp', 'ace', 'flight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'space', 'Ġlaunch', 'Ġdelta', 'Ġlease', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġspace', 'Ġx', 'Ġv', 'enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġoverview', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġus', 'Ġbeat', 'Ġch', 'ina', 'Ġfacts', 'Ġspace', 'x', 'Ġcosts', 'htt', 'Ġom', 'usa', 'php', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'space', 'x', 'Ġbooks', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtwo', 'Ġlaunches', 'Ġu', 'Ġmilitary', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġtestimony', 'Ġel', 'Ġmus', 'k', 'Ġmay', 'space', 'Ġshuttle', 'Ġfuture', 'Ġspace', 'Ġlaunch', 'Ġvehicles', 'Ġu', 'Ġsenate']</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2492,7 +2492,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>['Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpounds', 'Ġcargo', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġu', 'Ġnavy', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġos', 'iris', 'rex', 'Ġspacecraft', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'n', 'asa', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġworldview', 'Ġdigital', 'gl', 'obe', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġarchived', 'Ġobe', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġgoes', 'r', 'Ġsatellite', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'las', 'Ġwik', 'ipedia', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġe', 'ch', 'ost', 'ar', 'Ġsatellite', 'Ġsatellite', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġde', 'cember', 'Ġarchived', 'http', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'Ġu', 'air', 'force', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġpayload']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmarch', 'national', 'Ġpress', 'Ġclub', 'Ġfuture', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'press', 'Ġrelease', 'Ġc', 'span', 'org', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'environment', 'al', 'Ġassessment', 'Ġboost', 'back', 'Ġlanding', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġwest', 'web', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġmarch', 'space', 'x', 'Ġï', '¬', 'Ĥ', 'Ġreused', 'Ġrockets', 'Ġhalf', 'Ġlaunches', 'Ġcompetition', 'Ġl', 'ags', 'Ġfar', 'Ġbehind', 'laun', 'ches', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġtargets', 'Ġcommercial', 'Ġstarship', 'Ġlaunch', 'sp', 'ac', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'ster', 'Ġch', 'ris', 'Ġoct', 'ober', 'space', 'x', 'Ġreduces', 'Ġlaunch', 'Ġcosts', 'Ġc', 'es', 'launch', 'cost', 'Ġadvanced', 'Ġtelevision', 'Ġarchived', 'web', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'r', 'ussia', 'Ġcut', 'Ġspace', 'Ġlaunch', 'Ġprices', 'Ġpercent', 'Ġresponse', 'Ġspace', 'x', 'Ġpredatory', 'Ġpricing', 'Ġarchived', 'http', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'el', 'mus', 'k', 'Ġapr', 'il', 'space', 'x', 'Ġrockets', 'Ġreusable', '%.', 'Ġactual', 'Ġproblem', 'weet', 'Ġretrieved', 'Ġmay', 'Ġvia', 'Ġtwitter', 'ula', 'Ġce', 'ory', 'Ġbr', 'uno', "'s", 'Ġview', 'Ġeconomics', 'using', 'Ġrockets', 'Ġprop', 'ulsive', 'Ġï', '¬', 'Ĥ', 'back', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġel', 'Ġmus', 'k', 'Ġbreaks', 'Ġcosts', 'Ġreusable', 'Ġrockets', 'econom', 'ics', 'Ġarchived', 'econom', 'ics', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>['Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'Ġul', 'al', 'aunch', 'Ġarchived', 'web', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġire', 'ne', 'Ġapr', 'il', 'las', 'Ġrocket', 'Ġlaunches', 'Ġprivate', 'Ġcy', 'gn', 'us', 'Ġcargo', 'Ġship', 'Ġspace', 'Ġstation', 'Ġspace', 'Ġarchived', 'http', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġtd', 'rs', 'Ġsatellite', 'Ġul', 'al', 'aunch', 'Ġarchived', 'Ġr', 'sm', 'aspx', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'http', 'ul', 'al', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġgra', 'ham', 'iam', 'Ġoct', 'ober', 'las', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġlaunches', 'Ġarchived', 'web', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġmission', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'http', 'ul', 'al', 'au', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġgoes', 'Ġweather', 'Ġsatellite', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġarchived', 'Ġn', 'aa', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmission', 'Ġu', 'Ġair', 'Ġforce', '.-', 'air', 'force', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġwest', 'Ġcoast', "'s", 'Ġfirst', 'Ġinter', 'plan', 'etary', 'Ġmission', 'Ġn', 'asa', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmission', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmaple', 'Ġleaf', 'Ġse', 'pt', 'ember']</t>
+          <t>['Ġse', 'pt', 'ember', 'Ġfal', 'con', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'new', 'Ġopportunities', 'Ġsmall', 'sat', 'Ġlaunches', 'Ġspace', 'Ġreview', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġ...', 'Ġdeveloped', 'Ġprices', 'Ġï', '¬', 'Ĥ', 'ying', 'Ġsecondary', 'Ġpayload', 'Ġ...', 'Ġp', 'pod', 'Ġwould', 'Ġcost', '000', '000', 'Ġmissions', 'Ġle', '000', '000', 'Ġmissions', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', 'Ġesp', 'ac', 'lass', 'Ġsatellite', 'Ġweighing', 'Ġkilograms', 'Ġwould', 'Ġcost', 'âĢĵ', 'Ġmillion', 'Ġle', 'Ġmissions', 'âĢĵ', 'Ġmillion', 'Ġg', 'Ġmissions', 'Ġsaid', '."', 'space', 'x', 'Ġputs', 'Ġhistoric', 'Ġï', '¬', 'Ĥ', 'Ġrocket', 'Ġpermanent', 'Ġdisplay', 'http', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmay', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġmay', 'old', 'Ġfal', 'con', 'Ġrockets', 'Ġdone', 'Ġï', '¬', 'ģ', 'ring', 'Ġengines', 'ï', '¬', 'Ĥ', 'ame', 'Ġimag', 'inations', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'web', 'ar', 'h', 'ouston', 'Ġoriginal', 'Ġmay', 'space', 'x', 'Ġfal', 'con', 'Ġbooster', 'Ġexhibit', 'Ġopen', 'space', 'ce', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġloc', 'ke', 'Ġj', 'ared', 'Ġoct', 'ober', 'Ġ"[', 'update', 'Ġnew', 'Ġarrival', 'Ġfootage', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġbooster', 'Ġarrives', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġvisitor', 'Ġcomplex', 'Ġpermanent', 'Ġdisplay', 'space', 'exp', 'Ġspace', 'Ġexplored', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'ï', '¬', 'ģ', 'cial', 'Ġpage', 'Ġsa', 'ocom', 'Ġlaunch', 'Ġlanding', 'Ġtest', 'Ġï', '¬', 'ģ', 'ring', 'Ġtwo', 'Ġmer', 'lin', 'Ġengines', 'Ġconnected', 'Ġfal', 'con', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġmovie', 'Ġmovie', 'Ġjan', 'uary', 'Ġpress', 'Ġrelease', 'Ġannouncing', 'Ġdesign', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġhopes', 'Ġsupply', 'Ġiss', 'Ġnew', 'Ġfal', 'con', 'Ġheavy', 'Ġlauncher', 'flight', 'Ġinternational', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġlaunches', 'Ġfal', 'con', 'Ġcustomer', 'Ġr', 'index', 'php', 'Ġarchived', 'Ġj', 'une', 'Ġway', 'back', 'Ġmachine', 'defense', 'Ġindustry', 'Ġdaily', 'Ġse']</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'z', 'ador', 'Ġph', 'ill', 'ip', 'aug', 'ust', 'orb', 'ital', 'Ġdebris', 'Ġquarterly', 'Ġnews', 'Ġn', 'asa', 'Ġorbital', 'Ġn', 'asa', 'break', 'las', 'Ġcent', 'aur', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġcommunications', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'http', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'star', 'liner', 'Ġsuffers', 'Ġmission', 'short', 'ening', 'Ġfailure', 'Ġsuccessful', 'Ġlaunch', 'htt', 'Ġde', 'cember', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsolar', 'Ġorbit', 'er', 'Ġstudy', 'Ġsun', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġfirst', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġmission', 'Ġu', 'Ġspace', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġsixth', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġspace', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġstr', 'ick', 'land', 'Ġash', 'ley', 'Ġj', 'uly', 'ars', 'Ġlaunch', 'Ġn', 'asa', 'Ġsends', 'Ġpersever', 'ance', 'Ġrover', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'rol', 'Ġmission', 'Ġsupport', 'Ġnational', 'Ġsecurity', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'mber', 'Ġretrieved', 'mber', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġmission', 'Ġsupport', 'Ġnational', 'Ġsecurity', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ula', 'Ġdelays', 'Ġuse', 'Ġenhanced', 'Ġupper', 'stage', 'Ġengine', 'Ġpending', 'Ġstudies', 'Ġspac', 'en', 'ews', 'Ġj', 'une', 'Ġne', 'al', 'Ġle', 'e', 'Ġkan', 'ay', 'ama', 'Ġse', 'pt', 'ember', 'n', 'asa', "'s", 'Ġlands', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'enberg', 'Ġarchived', 'Ġch', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'las', 'Ġwik', 'ipedia']</t>
+          <t>['pt', 'ember', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>['Ġwar', 'ren', 'Ġhay', 'gen', 'Ġoct', 'ober', 'n', 'asa', 'Ġu', 'la', 'Ġlaunch', 'Ġhistoric', 'Ġl', 'u', 'cy', 'Ġmission', 'Ġretrieved', 'Ġoct', 'ober', 'Ġf', 'letcher', 'Ġcol', 'Ġde', 'cember', 'ula', 'Ġlaunches', 'las', 'Ġlong', 'Ġduration', 'Ġmission', 'Ġspace', 'Ġforce', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġde', 'cember', 'Ġgra', 'ham', 'iam', 'Ġjan', 'uary', 'ula', "'s", 'las', 'Ġlaunches', 'Ġsatellite', 'ins', 'pection', 'Ġmission', 'Ġspace', 'Ġforce', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġkan', 'ay', 'ama', 'Ġle', 'e', 'Ġmarch', 'Ġn', 'asa', "'s", 'Ġgoes', 'Ġweather', 'Ġsatellite', 'Ġlaunches', 'Ġu', 'la', 'las', 'Ġv', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġmarch', 'Ġgra', 'ham', 'iam', 'Ġmay', 'star', 'liner', 'Ġlaunch', 'Ġmakes', 'Ġorbit', 'Ġheading', 'Ġiss', 'Ġr', 'oft', 'launch', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġmay', 'Ġgra', 'ham', 'iam', 'Ġj', 'uly', 'las', 'Ġlaunches', 'Ġtwo', 'Ġexperimental', 'Ġmilitary', 'Ġsatellites', 'Ġus', 'sf', 'Ġmission', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġj', 'uly', 'Ġgra', 'ham', 'iam', 'Ġaug', 'ust', 'ula', "'s", 'las', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'n', 'al', 'b', 'irs', 'Ġgeo', 'Ġmissile', 'Ġdetection', 'Ġsatellite', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġaug', 'ust', 'Ġkan', 'ay', 'ama', 'Ġle', 'e', 'Ġoct', 'ober', 'final', 'las', 'Ġlaunches', 'Ġdual', 'es', 'es', 'Ġsatellites', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'mber', 'las', 'Ġrocket', 'Ġbids', 'Ġfarewell', 'Ġcal', 'ornia', 'Ġu', 'la', 'Ġread', 'ies', 'Ġvul', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'mber', 'ula', 'las', 'Ġretire', 'Ġmissions', 'Ġbo', 'e', 'ing', 'lock', 'heed', "'s", 'Ġventure', 'Ġstops', 'Ġsale', 'Ġrocket', 'Ġh', 'tm', 'Ġaug', 'ust', 'status', 'Ġhot', 'bird', 'Ġretrieved', 'mber', 'new', 'Ġhor', 'izons', 'Ġpl', 'uto', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġfly', 'Ġhor', 'izons', 'htm', 'Ġsolar', 'views', 'Ġretrieved', 'mber', 'Ġray', 'las', 'Ġrocket', 'Ġsends']</t>
+          <t>['Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġflight', 'Ġcarrying', 'Ġorb', 'comm', 'Ġsatellites', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġrecovered', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfollowing', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsuccessful', 'Ġfal', 'con', 'Ġlanding', 'Ġfunction', 'Ġpartially', 'Ġreusable', 'Ġorbital', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'usable', ')[', 'Ġsize', 'Ġheight', 'Ġft', 'Ġpayload', 'Ġfair', 'ing', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'also', 'Ġknown', 'Ġfal', 'con', 'Ġvariants', 'Ġblock', 'Ġblock', 'Ġpartially', 'Ġreusable', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġdesigned', 'Ġmanufactured', 'Ġspace', 'x', 'Ġfirst', 'Ġdesigned', 'âĢĵ', 'Ġfirst', 'Ġlaunch', 'Ġoperations', 'Ġde', 'cember', 'mber', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġperformed', 'Ġlaunches', 'Ġwithout', 'Ġfailures', 'Ġbased', 'Ġle', 'w', 'Ġpoint', 'Ġestimate', 'Ġreliability', 'Ġrocket', 'Ġreliable', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġcurrently', 'Ġoperation', 'Ġde', 'cember', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġfal', 'con', 'Ġfamily', 'Ġfirst', 'Ġlaunch', 'Ġvehicle', 'Ġorbital', 'Ġtrajectory', 'Ġsuccessfully', 'Ġvertically', 'Ġland', 'Ġfirst', 'Ġstage', 'Ġlanding', 'Ġfollowed', 'Ġtechnology', 'Ġdevelopment', 'Ġprogram', 'Ġconducted', 'Ġrequired', 'Ġtechnology', 'Ġadvances', 'Ġlanding', 'Ġlegs', 'Ġpioneered', 'Ġfal', 'con', 'Ġversion', 'Ġversion', 'Ġnever', 'Ġlanded', 'Ġintact', 'Ġstarting', 'Ġpreviously', 'Ġflown', 'Ġfirst', 'stage', 'Ġboosters', 'Ġreused', 'Ġlaunch', 'Ġnew', 'Ġpayload', 'Ġorbit', 'Ġquickly', 'Ġbecame', 'Ġroutine', 'Ġhalf', 'Ġfal', 'con', 'Ġflights', 'Ġreused', 'Ġbooster', 'Ġfraction', 'Ġreused', 'Ġboosters', 'Ġincreased', '%.', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġsubstantial', 'Ġupgrade', 'Ġprevious', 'Ġfal', 'con', 'Ġrocket', 'Ġflew', 'Ġlast', 'Ġmission', 'Ġjan', 'uary', 'rated', 'Ġfirst', 'Ġsecond', 'stage', 'Ġengines', 'Ġlarger', 'Ġsecond', 'stage', 'Ġpropell', 'ant', 'Ġtank', 'Ġpropell', 'ant', 'Ġdens', 'ification', 'Ġvehicle', 'Ġcarry', 'Ġsubstantial', 'Ġpayload', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġperform', 'Ġprop', 'ulsive', 'Ġlanding', 'Ġrecovery', 'Ġprincipal', 'Ġobjective', 'Ġnew', 'Ġdesign', 'Ġfacilitate', 'Ġbooster', 'us', 'ability', 'Ġlarger', 'Ġrange']</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2544,7 +2544,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>['Ġcy', 'gn', 'us', 'Ġhot', 'Ġpursuit', 'Ġspace', 'Ġstation', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'os', 'iris', 'rex', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġoct', 'ober', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġretrieved', 'mber', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġlands', 'Ġv', 'enberg', 'af', 'Ġu', 'Ġair', 'Ġforce', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'ula', 'Ġdelays', 'Ġfocused', 'Ġprotecting', 'Ġpercent', 'Ġmission', 'Ġsuccess', 'Ġrate', 'Ġr', 'cent', 'success', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfa', 'hey', 'Ġmark', 'Ġse', 'pt', 'ember', 'Ġrocket', 'Ġblows', 'Ġspace', 'Ġinsurers', 'Ġpay', 'Ġarchived', 'http', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'air', 'Ġforce', 'Ġissues', 'Ġsecond', 'Ġupdate', 'Ġregarding', 'las', 'Ġcent', 'aur', 'Ġupper', 'Ġstage', 'Ġanomaly', 'Ġreview', 'Ġu', 'Ġair', 'Ġforce', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'ro', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'las', 'Ġv', 'web', 'arch', 'iv', 'press', 'Ġrelease', 'Ġn', 'ro', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġlaunch', 'Ġupdate', 'press', 'Ġrelease', 'Ġn', 'ro', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'las', 'Ġforced', 'Ġimprov', 'ise', 'uesday', "'s", 'Ġclimb', 'Ġorbit', 'http', 'space', 'press', 'Ġrelease', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġmarch', 'Ġarchived', 'cl', 'imb', 'orbit', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġray', 'new', 'Ġlineup', 'Ġspelled', 'Ġupcoming', 'las', 'Ġrocket', 'Ġlaunches', 'Ġcape', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġfer', 'ster', 'Ġwar', 'ren']</t>
+          <t>['Ġmissions', 'Ġincluding', 'Ġdelivery', 'Ġlarge', 'Ġcomm', 'ats', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġlike', 'Ġearlier', 'Ġversions', 'Ġfal', 'con', 'Ġlike', 'Ġsat', 'urn', 'Ġseries', 'Ġap', 'ollo', 'Ġprogram', 'Ġpresence', 'Ġmultiple', 'Ġfirst', 'stage', 'Ġengines', 'Ġallow', 'Ġmission', 'Ġcompletion', 'Ġeven', 'Ġone', 'Ġfirst', 'stage', 'Ġengines', 'Ġfails', 'Ġmid', 'flight', 'Ġdesign', 'Ġmod', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġdiameter', 'Ġmass', '000', '000', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġle', 'Â°', 'Ġmass', 'Ġexpend', 'able', 'Ġreusable', 'Ġpayload', 'Ġg', 'Â°', 'Ġmass', 'Ġexpend', 'able', 'Ġreusable', '000', '000', 'Ġpayload', 'Ġmars', 'Ġmass', '020', 'Ġassociated', 'Ġrockets', 'Ġfamily', 'Ġfal', 'con', 'Ġderivative', 'Ġwork', 'Ġfal', 'con', 'Ġheavy', 'Ġcomparable', 'las', 'Ġlong', 'Ġmarch', 'b', 'e', 'Ġpro', 'ton', 'ri', 'ane', 'Ġes', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġv', 'enberg', 'Ġk', 'enn', 'edy', 'Ġtotal', 'Ġlaunches', 'Ġleft', 'Ġright', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġthree', 'Ġlaunch', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġfal', 'con', 'Ġthree', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġfal', 'con', 'full', 'Ġthrust', 'Ġtwo', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġfal', 'con', 'Ġblock', 'Ġfal', 'con', 'Ġheavy', 'Ġthird', 'Ġversion', 'Ġfal', 'con', 'Ġdeveloped', 'âĢĵ', 'Ġmade', 'Ġmaiden', 'Ġflight', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmodified', 'Ġreusable', 'Ġvariant', 'Ġfal', 'con', 'Ġfamily', 'Ġcapabilities', 'Ġexceed', 'Ġfal', 'con', 'Ġincluding', 'Ġability', 'land', 'Ġfirst', 'Ġstage', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġmissions', 'Ġdrone', 'Ġship', '"[', 'Ġrocket', 'Ġdesigned', 'Ġusing', 'Ġsystems', 'Ġsoftware', 'Ġtechnology', 'Ġdeveloped', 'Ġpart', 'Ġspace', 'x', 'Ġreusable', 'Ġlaunch', 'Ġsystem', 'Ġdevelopment', 'Ġprogram', 'Ġprivate', 'Ġinitiative', 'Ġspace', 'x', 'Ġfacilitate', 'Ġrapid', 'us', 'ability', 'Ġfirst', 'âĢĵ', 'Ġlong', 'Ġterm', 'Ġsecond', 'âĢĶ', 'st', 'ages', 'Ġspace', 'x', 'Ġlaunch', 'Ġvehicles', 'Ġvarious', 'Ġtechnologies', 'Ġtested', 'Ġgrass', 'ho', 'pper', 'Ġtechnology', 'Ġdemonstr', 'ator', 'Ġwell', 'Ġseveral', 'Ġflights', 'Ġfal', 'con', 'Ġpost', 'mission', 'Ġbooster', 'Ġcontrolled']</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>['Ġse', 'pt', 'ember', 'ula', 'Ġinvest', 'Ġblue', 'Ġorigin', 'Ġengine', 'Ġr', 'Ġreplacement', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ike', 'Ġgr', 'uss', 'Ġapr', 'il', 'ula', "'s", 'Ġnext', 'Ġrocket', 'Ġnamed', 'Ġvul', 'Ġspac', 'en', 'ews', 'ike', 'Ġgr', 'uss', 'Ġapr', 'il', 'ula', "'s", 'Ġvul', 'Ġrocket', 'Ġrolled', 'Ġstages', 'Ġg', 'es', 'Ġspac', 'en', 'ews', 'ler', 'Ġamy', 'Ġmay', 'indust', 'ry', 'Ġteam', 'Ġhopes', 'Ġresurrect', 'las', 'Ġpost', 'Ġr', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'ula', 'Ġstudying', 'Ġlong', 'term', 'Ġupgrades', 'Ġvul', 'Ġamy', 'ler', 'Ġapr', 'il', 'ula', 'Ġce', 'Ġcalls', 'Ġavailability', 'Ġdate', 'Ġengine', 'rid', 'ic', 'ulous', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'une', 'expl', 'os', 'ive', 'Ġtest', 'Ġpushes', 'st', 'Ġu', 'la', 'Ġvul', 'Ġrocket', 'Ġlaunch', 'Ġleast', 'Ġj', 'une', 'Ġce', 'Ġsays', 'Ġms', 'n', 'Ġretrieved', 'Ġapr', 'il', 'Ġu', 'la', 'las', 'Ġdata', 'Ġsheets', 'las', 'Ġseries', 'Ġcut', 'away', 'las', 'Ġseries', 'Ġcut', 'away', 'Ġu', 'la', 'las', 'Ġrocket', 'builder', 'Ġlock', 'heed', 'Ġmart', 'las', 'Ġlaunch', 'Ġvehicles', 'Ġencyclopedia', 'Ġastronaut', 'ica', 'las', 'Ġexternal', 'Ġlinks', 'las', 'Ġwik', 'ipedia', 'Ġspace', 'Ġlaunch', 'Ġreport', 'las', 'Ġdata', 'Ġsheet', 'Ġretrieved']</t>
+          <t>['des', 'cent', 'Ġtests', 'Ġconducted', 'Ġspace', 'x', 'Ġmade', 'Ġnumber', 'Ġmodifications', 'Ġexisting', 'Ġfal', 'con', 'Ġnew', 'Ġrocket', 'Ġknown', 'Ġinternally', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġalso', 'Ġknown', 'Ġfal', 'con', 'Ġenhanced', 'Ġfal', 'con', 'Ġfull', 'performance', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġupgrade', 'Ġprincipal', 'Ġobjective', 'Ġnew', 'Ġdesign', 'Ġfacilitate', 'Ġbooster', 'us', 'ability', 'Ġlarger', 'Ġrange', 'Ġmissions', 'Ġincluding', 'Ġdelivery', 'Ġlarge', 'Ġcomm', 'ats', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġmodifications', 'Ġupgraded', 'Ġversion', 'Ġinclude', 'Ġliquid', 'Ġsub', 'cool', 'ed', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠÂ°', 'r', 'ĠâĪĴ', 'ĠÂ°', 'f', 'Ġcooled', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠÂ°', 'r', 'Ġdensity', 'owing', 'Ġfuel', 'Ġoxid', 'izer', 'Ġstored', 'Ġgiven', 'Ġtank', 'Ġvolume', 'Ġwell', 'Ġincreasing', 'Ġpropell', 'ant', 'Ġmass', 'Ġï', '¬', 'Ĥ', 'ow', 'Ġturb', 'op', 'umps', 'Ġincreasing', 'Ġthrust', 'Ġupgraded', 'Ġstructure', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġlonger', 'Ġsecond', 'Ġstage', 'Ġpropell', 'ant', 'Ġtanks', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġsuccess', 'es', 'Ġnotable', 'Ġoutcome', 'destroy', 'ed', 'Ġlaunch', 'Ġland', 'ings', 'Ġattempts', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġactive', 'Ġtype', 'Ġpassengers', 'c', 'argo', 'Ġdragon', 'Ġcapsule', 'Ġdragon', 'Ġcrew', 'Ġcapsule', 'Ġir', 'idium', 'Ġnext', 'Ġï', '¬', 'Ĥ', 'e', 'et', 'Ġz', 'uma', 'Ġbo', 'e', 'ing', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'ess', 'res', 'heet', 'Ġland', 'er', 'Ġstar', 'link', 'Ġrad', 'ars', 'Ġconstellation', 'Ġsent', 'inel', 'ichael', 'Ġfre', 'il', 'ich', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', 'Ġkn', '000', 'Ġvacuum', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġseconds', 'Ġvacuum', 'Ġseconds', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġchilled', 'Ġsecond', 'large', 'Ġnozzle', ')[', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġlonger', 'Ġstronger', 'Ġinter', 'stage', 'Ġhousing', 'Ġsecond', 'Ġstage', 'Ġengine', 'Ġnozzle', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġattitude', 'Ġthr', 'usters', 'Ġcenter', 'Ġpus', 'Ġadded', 'Ġstage', 'Ġseparation']</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2570,7 +2570,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>['Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġsixth', 'Ġservice', 'Ġmodule', 'Ġplaced', 'Ġinside', 'Ġpayload', 'Ġfair', 'ing', 'Ġrole', 'Ġunc', 'rew', 'ed', 'Ġspace', 'plane', 'Ġnational', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġmanufacturer', 'Ġbo', 'e', 'ing', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġapr', 'il', 'ï', '¬', 'ģ', 'r', 'st', 'Ġdrop', 'Ġtest', 'Ġintroduction', 'Ġapr', 'il', 'ï', '¬', 'ģ', 'r', 'st', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġbo', 'e', 'ing', 'Ġbo', 'e', 'ing', 'Ġalso', 'Ġknown', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġreusable', 'Ġrobotic', 'Ġspacecraft', 'Ġboosted', 'Ġspace', 'Ġlaunch', 'Ġvehicle', 'ent', 'ers', 'Ġearth', "'s", 'Ġatmosphere', 'Ġlands', 'Ġspace', 'plane', 'Ġoperated', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġorbital', 'Ġspace', 'flight', 'Ġmissions', 'Ġintended', 'Ġdemonstrate', 'Ġreusable', 'Ġspace', 'Ġtechnologies', 'percent', 'sc', 'aled', 'Ġderivative', 'Ġearlier', 'Ġbo', 'e', 'ing', 'Ġbegan', 'Ġn', 'asa', 'Ġproject', 'Ġtransferred', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġprogram', 'Ġmanaged', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġfirst', 'Ġflew', 'Ġdrop', 'Ġtest', 'Ġfirst', 'Ġorbital', 'Ġmission', 'Ġlaunched', 'Ġapr', 'il', 'las', 'Ġrocket', 'Ġreturned', 'Ġearth', 'Ġde', 'cember', 'Ġsubsequent', 'Ġflights', 'Ġgradually', 'Ġextended', 'Ġmission', 'Ġduration', 'Ġreaching', 'Ġdays', 'Ġorbit', 'Ġfifth', 'Ġmission', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'Ġrocket', 'Ġlatest', 'Ġmission', 'Ġsixth', 'Ġlaunched', 'las', 'Ġmay', 'Ġconcluded', 'mber', 'Ġreaching', 'Ġtotal', '08', 'Ġdays', 'Ġn', 'asa', 'Ġselected', 'Ġbo', 'e', 'ing', 'Ġintegrated', 'Ġdefense', 'Ġsystems', 'Ġdesign', 'Ġdevelop', 'Ġorbital', 'Ġvehicle', 'Ġbuilt', 'Ġcal', 'ornia', 'Ġbranch', 'Ġbo', 'e', 'ing', "'s", 'Ġphantom', 'Ġworks', 'Ġfour', 'year', 'Ġperiod', 'Ġtotal', 'Ġus', 'Ġmillion', 'Ġspent', 'Ġproject', 'Ġn', 'asa', 'Ġcontributing', 'Ġus', 'Ġmillion', 'Ġu', 'Ġair', 'Ġforce', 'Ġus', 'Ġmillion', 'Ġbo', 'e', 'ing', 'Ġmillion', 'Ġlate', 'Ġnew', 'Ġus', 'Ġmillion', 'Ġcontract', 'Ġawarded', 'Ġbo', 'e', 'ing', 'Ġpart', 'Ġn', 'asa', "'s", 'Ġspace', 'Ġlaunch', 'Ġinitiative', 'Ġframework', 'Ġaer', 'odynamic', 'Ġdesign', 'Ġderived', 'Ġlarger', 'Ġspace', 'Ġshuttle', 'Ġorbit', 'er', 'Ġhence', 'Ġsimilar', 'Ġlift', 'dr', 'ag', 'Ġratio', 'Ġlower', 'Ġcross', 'Ġrange', 'Ġhigher', 'Ġalt', 'itudes', 'Ġmach', 'Ġnumbers', 'Ġcompared', 'arp', "'s", 'Ġhyp', 'erson', 'ic', 'Ġtechnology', 'Ġvehicle', 'Ġearly', 'Ġrequirement']</t>
+          <t>['Ġdesign', 'Ġevolution', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġoct', 'aw', 'eb', 'Ġupgraded', 'Ġlanding', 'Ġlegs', 'Ġmer', 'lin', 'Ġengine', 'Ġthrust', 'Ġincreased', 'Ġfull', 'th', 'rust', 'Ġvariant', 'Ġmer', 'lin', 'Ġtaking', 'Ġadvantage', 'Ġdens', 'er', 'Ġpropell', 'ants', 'Ġachieved', 'Ġsub', 'cool', 'ing', 'Ġmer', 'lin', 'Ġvacuum', 'Ġthrust', 'Ġincreased', 'Ġsub', 'cool', 'ing', 'Ġpropell', 'ants', 'Ġseveral', 'Ġsmall', 'Ġmass', 'red', 'uction', 'Ġefforts', 'Ġmodified', 'Ġdesign', 'Ġgained', 'Ġadditional', 'Ġmetres', 'Ġft', 'Ġheight', 'Ġstretching', 'Ġexactly', 'Ġmetres', 'Ġft', 'Ġincluding', 'Ġpayload', 'Ġfair', 'ing', 'Ġgaining', 'Ġoverall', 'Ġperformance', 'Ġincrease', 'Ġpercent', 'Ġnew', 'Ġfirst', 'stage', 'Ġengine', 'Ġmuch', 'Ġincreased', 'Ġthrust', 'weight', 'Ġratio', 'Ġfull', 'th', 'rust', 'Ġfirst', 'Ġstage', 'Ġbooster', 'Ġcould', 'Ġreach', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcarrying', 'Ġupper', 'Ġstage', 'Ġheavy', 'Ġsatellite', 'Ġversions', 'Ġlaunched', 'Ġincluded', 'Ġexperimental', 'Ġrecovery', 'Ġsystem', 'Ġpayload', 'Ġfair', 'ing', 'Ġhalves', 'Ġmarch', 'Ġspace', 'x', 'Ġfirst', 'Ġtime', 'Ġrecovered', 'Ġfair', 'ing', 'es', 'Ġmission', 'Ġthanks', 'Ġthr', 'usters', 'Ġsteer', 'able', 'Ġparachute', 'Ġhelping', 'Ġglide', 'Ġtowards', 'Ġgentle', 'Ġtouchdown', 'Ġwater', 'Ġj', 'une', 'Ġflight', 'ir', 'idium', 'Ġnext', 'âĢĵ', 'Ġaluminum', 'Ġgrid', 'Ġfins', 'Ġreplaced', 'Ġtitanium', 'Ġversions', 'Ġimprove', 'Ġcontrol', 'Ġauthority', 'Ġbetter', 'Ġcope', 'Ġheat', 'entry', 'Ġfollowing', 'Ġpost', 'flight', 'Ġinspections', 'Ġel', 'Ġmus', 'k', 'Ġannounced', 'Ġnew', 'Ġgrid', 'Ġfins', 'Ġlikely', 'Ġrequire', 'Ġservice', 'Ġflights', 'Ġspace', 'x', 'Ġdeveloping', 'Ġtime', 'Ġalternative', 'Ġautonomous', 'Ġsystem', 'Ġreplace', 'Ġtraditional', 'Ġground', 'based', 'Ġsystems', 'Ġuse', 'Ġus', 'Ġlaunches', 'Ġdecades', 'Ġautonomous', 'Ġsystem', 'Ġuse', 'Ġspace', 'x', 'Ġsub', 'orb', 'ital', 'Ġtest', 'Ġflights', 'Ġtex', 'Ġflown', 'Ġparallel', 'Ġnumber', 'Ġorbital', 'Ġlaunches', 'Ġpart', 'Ġsystem', 'Ġtest', 'Ġprocess', 'Ġgain', 'Ġapproval', 'Ġuse', 'Ġoperational', 'Ġflights', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', "'s", 'Ġcr', 'Ġlaunch', 'Ġfirst', 'Ġoperational', 'Ġlaunch', 'Ġutilizing', 'Ġnew', 'Ġautonomous', 'Ġflight', 'Ġsafety', 'Ġsystem', 'af', 'ss', 'either', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', "'s", 'Ġeastern', 'Ġwestern', 'Ġranges', '."', 'Ġfollowing', 'Ġspace', 'x', 'Ġflight', 'Ġautonomous', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtermination', 'Ġsystem']</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2583,7 +2583,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>['Ġspacecraft', 'Ġcalled', 'Ġtotal', 'Ġmission', 'Ġdelta', 'v', '000', 'Ġmiles', 'Ġper', 'Ġhour', 'Ġorbital', 'Ġmaneuvers', 'Ġearly', 'Ġgoal', 'Ġprogram', 'Ġrend', 'ezvous', 'Ġsatellites', 'Ġperform', 'Ġrepairs', 'Ġoriginally', 'Ġdevelopment', 'Ġorigins', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġstatus', 'Ġservice', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġcompleted', 'th', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'ba', 'Ġprimary', 'Ġuser', 'Ġn', 'asa', 'arp', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġnumber', 'Ġbuilt', 'Ġdeveloped', 'Ġbo', 'e', 'ing', 'Ġartist', "'s", 'Ġrendering', 'Ġspacecraft', 'Ġscaled', 'Ġcompos', 'ites', 'Ġwhite', 'Ġknight', 'Ġused', 'Ġlaunch', 'Ġglide', 'Ġtests', 'Ġdesigned', 'Ġcarried', 'Ġorbit', 'Ġcargo', 'Ġbay', 'Ġspace', 'Ġshuttle', 'Ġunderwent', 'Ġredesign', 'Ġlaunch', 'Ġdelta', 'Ġiv', 'Ġcomparable', 'Ġrocket', 'Ġdetermined', 'Ġshuttle', 'Ġflight', 'Ġwould', 'Ġun', 'econom', 'ical', 'Ġtransferred', 'Ġn', 'asa', 'Ġdefense', 'Ġadvanced', 'Ġresearch', 'Ġprojects', 'Ġagency', 'arp', 'Ġse', 'pt', 'ember', 'Ġthereafter', 'Ġprogram', 'Ġbecame', 'Ġclassified', 'Ġproject', 'arp', 'Ġpromoted', 'Ġpart', 'Ġindependent', 'Ġspace', 'Ġpolicy', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġpursued', 'Ġsince', 'Ġchallenger', 'Ġdisaster', 'Ġvehicle', 'Ġused', 'Ġatmospheric', 'Ġdrop', 'Ġtest', 'Ġgl', 'ider', 'Ġpropulsion', 'Ġsystem', 'Ġinstead', 'Ġoperational', 'Ġvehicle', "'s", 'Ġpayload', 'Ġbay', 'Ġdoors', 'Ġenclosed', 'Ġreinforced', 'Ġupper', 'Ġfu', 'selage', 'Ġstructure', 'Ġallow', 'ated', 'Ġmother', 'ship', 'Ġse', 'pt', 'ember', 'arp', 'Ġannounced', 'Ġinitial', 'Ġatmospheric', 'Ġdrop', 'Ġtests', 'Ġwould', 'Ġlaunched', 'Ġscaled', 'Ġcompos', 'ites', 'Ġwhite', 'Ġknight', 'Ġhigh', 'alt', 'itude', 'Ġresearch', 'Ġj', 'une', 'Ġcompleted', 'Ġcaptive', 'carry', 'Ġflight', 'Ġunderneath', 'Ġwhite', 'Ġknight', 'Ġmo', 'j', 'ave', 'Ġspac', 'eport', 'Ġmo', 'j', 'ave', 'Ġcal', 'ornia', 'Ġsecond', 'Ġhalf', 'Ġunderwent', 'Ġstructural', 'Ġupgrades', 'Ġincluding', 'Ġreinforcement', 'Ġnose', 'Ġwheel', 'Ġsupports', 'Ġx', "'s", 'Ġpublic', 'Ġdebut', 'Ġfirst', 'Ġfree', 'Ġflight', 'Ġscheduled', 'Ġmarch', 'Ġcanceled', 'Ġdue', 'Ġar', 'ctic', 'Ġstorm', 'Ġnext', 'Ġflight', 'Ġattempt', 'Ġmarch', 'Ġcanceled', 'Ġdue', 'Ġhigh', 'Ġwinds', 'Ġmarch', 'Ġflew', 'Ġdat', 'al', 'ink', 'Ġfailure', 'Ġprevented', 'Ġfree', 'Ġflight', 'Ġvehicle', 'Ġreturned', 'Ġground', 'Ġstill', 'Ġattached', 'Ġwhite']</t>
+          <t>['Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġseconds', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsecond', 'short', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġvacuum', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġseconds', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġmarch', 'Ġdiscarded', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġlower', 'Ġright', 'Ġsecond', 'Ġstage', 'Ġupper', 'Ġleft', 'Ġtwo', 'Ġparts', 'Ġj', 'ett', 'ison', 'ed', 'Ġpayload', 'Ġfair', 'ing', 'Ġe', 'ch', 'ost', 'ar', 'Ġmarch', 'Ġlast', 'Ġspace', 'x', 'Ġlaunch', 'Ġutilizing', 'Ġhistoric', 'Ġsystem', 'Ġground', 'Ġrad', 'ars', 'Ġtracking', 'Ġcomputers', 'Ġpersonnel', 'Ġlaunch', 'Ġbunk', 'ers', 'Ġused', 'Ġsixty', 'Ġyears', 'Ġlaunches', 'Ġeastern', 'Ġrange', 'Ġfuture', 'Ġspace', 'x', 'Ġlaunches', 'Ġaf', 'ss', 'Ġreplaced', 'Ġground', 'based', 'Ġmission', 'Ġflight', 'Ġcontrol', 'Ġpersonnel', 'Ġequipment', 'board', 'Ġpositioning', 'Ġnavigation', 'Ġtiming', 'Ġsources', 'Ġdecision', 'Ġlogic', 'Ġbenefits', 'Ġaf', 'ss', 'Ġinclude', 'Ġincreased', 'Ġpublic', 'Ġsafety', 'Ġreduced', 'Ġreliance', 'Ġrange', 'Ġinfrastructure', 'Ġreduced', 'Ġrange', 'Ġspac', 'el', 'ift', 'Ġcost', 'Ġincreased', 'Ġschedule', 'Ġpredict', 'ability', 'Ġavailability', 'Ġoperational', 'Ġflexibility', 'Ġlaunch', 'Ġslot', 'Ġspace', 'x', 'Ġstarted', 'Ġflying', 'Ġincremental', 'Ġchanges', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġcalling', 'block', '".[', 'Ġfirst', 'Ġsecond', 'Ġstage', 'Ġmodified', 'Ġblock', 'Ġstandards', 'Ġflying', 'Ġtop', 'block', 'Ġfirst', 'Ġstage', 'Ġthree', 'Ġmissions', 'ars', 'Ġmay', 'Ġint', 'els', 'Ġj', 'uly', 'Ġblock', 'Ġdescribed', 'Ġtransition', 'Ġfull', 'Ġthrust', 'block', 'Ġfollowing', 'Ġfal', 'con', 'Ġblock', 'Ġincludes', 'Ġincremental', 'Ġengine', 'Ġthrust', 'Ġupgrades', 'Ġleading', 'Ġfinal', 'Ġthrust', 'Ġblock', 'Ġmaiden', 'Ġflight', 'Ġfull', 'Ġblock', 'Ġdesign', 'first', 'Ġsecond', 'Ġstages', 'Ġn', 'asa', 'Ġcr', 'Ġmission', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġannounced', 'Ġanother', 'Ġseries', 'Ġincremental', 'Ġimprovements', 'Ġdevelopment', 'Ġfal', 'con', 'Ġblock', 'Ġversion', 'Ġsucceeded', 'Ġtransitional', 'Ġblock', 'Ġlargest', 'Ġchanges', 'Ġblock', 'Ġblock', 'Ġhigher', 'Ġthrust', 'Ġengines', 'Ġimprovements', 'Ġlanding', 'Ġlegs', 'Ġadditionally', 'Ġnumerous', 'Ġsmall', 'Ġchanges', 'Ġhelp', 'Ġstream', 'line', 'Ġrecovery', 'us', 'ability']</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>['Ġknight', 'Ġcarrier', 'Ġaircraft', 'Ġapr', 'il', 'Ġmade', 'Ġfirst', 'Ġfree', 'Ġglide', 'Ġflight', 'Ġlanding', 'Ġvehicle', 'ran', 'Ġrunway', 'Ġsustained', 'Ġminor', 'Ġdamage', 'Ġfollowing', 'Ġvehicle', "'s", 'Ġextended', 'Ġdowntime', 'Ġrepairs', 'Ġprogram', 'Ġmoved', 'Ġmo', 'j', 'ave', 'Ġair', 'Ġforce', 'Ġplant', 'Ġpal', 'md', 'ale', 'Ġcal', 'ornia', 'Ġremainder', 'Ġflight', 'Ġtest', 'Ġprogram', 'Ġwhite', 'Ġknight', 'Ġcontinued', 'Ġbased', 'Ġmo', 'j', 'ave', 'Ġthough', 'Ġfer', 'ried', 'Ġplant', 'Ġtest', 'Ġflights', 'Ġscheduled', 'Ġfive', 'Ġadditional', 'Ġflights', 'Ġperformed', 'n', 'Ġtwo', 'Ġresulted', 'Ġreleases', 'Ġsuccessful', 'Ġland', 'ings', 'Ġtwo', 'Ġfree', 'Ġflights', 'Ġoccurred', 'Ġaug', 'ust', 'Ġse', 'pt', 'ember', 'mber', 'Ġu', 'Ġair', 'Ġforce', 'Ġannounced', 'Ġwould', 'Ġdevelop', 'Ġvariant', 'Ġn', 'asa', "'s", 'Ġair', 'Ġforce', 'Ġversion', 'Ġdesignated', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġprogram', 'Ġbuilt', 'Ġearlier', 'Ġindustry', 'Ġgovernment', 'Ġefforts', 'arp', 'Ġn', 'asa', 'Ġair', 'Ġforce', 'Ġleadership', 'Ġair', 'Ġforce', 'Ġrapid', 'Ġcapabilities', 'Ġoffice', 'Ġpartnership', 'Ġn', 'asa', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'Ġbo', 'e', 'ing', 'Ġprime', 'Ġcontractor', 'Ġprogram', 'Ġdesigned', 'Ġglide', 'Ġtesting', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġremain', 'Ġorbit', 'Ġdays', 'Ġtime', 'Ġsecretary', 'Ġair', 'Ġforce', 'Ġstated', 'Ġprogram', 'Ġwould', 'Ġfocus', 'risk', 'Ġreduction', 'Ġexperimentation', 'Ġoperational', 'Ġconcept', 'Ġdevelopment', 'Ġreusable', 'Ġspace', 'Ġvehicle', 'Ġtechnologies', 'Ġsupport', 'Ġlong', 'term', 'Ġdevelopmental', 'Ġspace', 'Ġobjectives', '".[', 'Ġoriginally', 'Ġscheduled', 'Ġlaunch', 'Ġpayload', 'Ġbay', 'Ġspace', 'Ġshuttle', 'Ġfollowing', 'Ġspace', 'Ġshuttle', 'Ġcol', 'umb', 'ia', 'Ġdisaster', 'Ġtransferred', 'Ġdelta', 'Ġsubsequently', 'Ġtransferred', 'Ġshrouded', 'Ġconfiguration', 'las', 'Ġrocket', 'Ġfollowing', 'Ġconcerns', 'Ġun', 'sh', 'roud', 'ed', 'Ġspacecraft', "'s", 'Ġaer', 'odynamic', 'Ġproperties', 'Ġlaunch', 'Ġfollowing', 'Ġmissions', 'Ġspacecraft', 'Ġprimarily', 'Ġland', 'Ġrunway', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġcal', 'ornia', 'Ġed', 'wards', 'Ġair', 'Ġforce', 'Ġbase', 'Ġsecondary', 'Ġsite', 'Ġmanufacturing', 'Ġwork', 'Ġbegan', 'Ġsecond', 'Ġconducted', 'Ġmaiden', 'Ġmission', 'Ġmarch', 'Ġoct', 'ober', 'Ġn', 'asa', 'Ġconfirmed', 'Ġvehicles', 'Ġwould', 'Ġhoused', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter']</t>
+          <t>['Ġfirst', 'stage', 'Ġboosters', 'Ġalterations', 'Ġfocused', 'Ġincreasing', 'Ġspeed', 'Ġproduction', 'Ġefficiency', 'us', 'ability', 'Ġspace', 'x', 'Ġaims', 'Ġfly', 'Ġblock', 'Ġbooster', 'Ġten', 'Ġtimes', 'Ġinspections', 'Ġtimes', 'Ġblock', 'Ġsecond', 'Ġstages', 'Ġbuilt', 'Ġmission', 'Ġextension', 'Ġkit', 'Ġallow', 'Ġlonger', 'Ġduration', 'Ġengine', 'Ġstarts', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġspecifications', 'Ġcharacteristics', 'Ġblock', 'Ġblock', 'Ġrocket', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġcharacteristic', 'Ġfirst', 'Ġstage', 'Ġsecond', 'Ġstage', 'Ġpayload', 'Ġfair', 'ing', 'Ġheight', 'Ġft', 'Ġft', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġft', 'Ġft', 'Ġmass', 'without', 'Ġpropell', 'ant', ')[', '000', 'Ġmass', 'Ġpropell', 'ant', 'Ġn', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġmon', 'oco', 'que', 'Ġhalves', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'Ġlithium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġaluminum', 'Ġlithium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġcarbon', 'Ġï', '¬', 'ģ', 'ber', 'Ġengines', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġvacuum', 'Ġn', 'Ġengine', 'Ġtype', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġtank', 'Ġcapacity', 'Ġk', 'eros', 'ene', 'Ġtank', 'Ġcapacity', 'Ġengine', 'Ġnozzle', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġengine', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġthrust', 'stage', 'Ġtotal', ')[', 'Ġkn', '000', 'sea', 'Ġlevel', 'Ġkn', '000', 'v', 'ac', 'uum', 'Ġpropell', 'ant', 'Ġfeed', 'Ġsystem', 'Ġturb', 'op', 'ump', 'Ġturb', 'op', 'ump', 'Ġthrottle', 'Ġcapability', 'Ġyes', 'Ġkn', 'Ġkn', '000', 'sea', 'Ġlevel', 'ï', '¼', 'ī', 'Ġyes', 'âĢĵ', 'Ġkn']</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>['Ġorbit', 'er', 'Ġprocessing', 'Ġfacilities', 'Ġhang', 'ars', 'Ġpreviously', 'Ġoccupied', 'Ġspace', 'Ġshuttle', 'Ġbo', 'e', 'ing', 'Ġsaid', 'Ġspace', 'Ġplanes', 'Ġwould', 'Ġuse', 'Ġjan', 'uary', 'Ġair', 'Ġforce', 'Ġpreviously', 'Ġsaid', 'Ġconsidering', 'Ġconsolid', 'ating', 'Ġoperations', 'Ġhoused', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġcal', 'ornia', 'Ġnearer', 'Ġlaunch', 'Ġsite', 'Ġcape', 'aver', 'al', 'Ġn', 'asa', 'Ġalso', 'Ġstated', 'Ġprogram', 'Ġcompleted', 'Ġtests', 'Ġdetermine', 'Ġwhether', 'Ġone', 'fourth', 'Ġsize', 'Ġspace', 'Ġshuttle', 'Ġcould', 'Ġland', 'Ġformer', 'Ġshuttle', 'Ġrun', 'ways', 'Ġn', 'asa', 'Ġfurthermore', 'Ġstated', 'Ġrenovations', 'Ġtwo', 'Ġhang', 'ars', 'Ġwould', 'Ġcompleted', 'Ġend', 'Ġmain', 'Ġdoors', 'Ġmarked', 'Ġmessage', 'home', 'Ġpoint', 'Ġactivities', 'Ġproject', 'Ġsecret', 'Ġofficial', 'Ġu', 'Ġair', 'Ġforce', 'Ġstatement', 'Ġproject', 'Ġexperimental', 'Ġtest', 'Ġprogram', 'Ġdemonstrate', 'Ġtechnologies', 'Ġreliable', 'Ġreusable', 'Ġunc', 'rew', 'ed', 'Ġspace', 'Ġtest', 'Ġplatform', 'Ġu', 'Ġair', 'Ġforce', '".[', 'Ġprimary', 'Ġobjectives', 'Ġtwo', 'fold', 'Ġreusable', 'Ġspacecraft', 'Ġtechnology', 'Ġoperating', 'Ġexperiments', 'Ġreturned', 'Ġearth', 'Ġair', 'Ġforce', 'Ġstates', 'Ġincludes', 'Ġtesting', 'Ġav', 'ionics', 'Ġflight', 'Ġsystems', 'Ġguidance', 'Ġnavigation', 'Ġthermal', 'Ġprotection', 'Ġinsulation', 'Ġpropulsion', 'entry', 'Ġsystems', 'Ġmay', 'Ġtom', 'Ġbur', 'gh', 'ard', 'Ġspeculated', 'Ġspace', 'Ġdaily', 'Ġcould', 'Ġused', 'Ġsatellite', 'Ġdeliver', 'Ġweapons', 'Ġspace', 'Ġpent', 'agon', 'Ġsubsequently', 'Ġdenied', 'Ġclaims', 'Ġtest', 'Ġmissions', 'Ġsupported', 'Ġdevelopment', 'Ġspace', 'based', 'Ġweapons', 'Ġjan', 'uary', 'Ġallegations', 'Ġmade', 'Ġused', 'Ġch', 'ina', "'s", 'iang', 'ong', 'Ġspace', 'Ġstation', 'Ġmodule', 'Ġformer', 'Ġu', 'Ġair', 'Ġforce', 'Ġorbital', 'Ġanalyst', 'Ġb', 'rian', 'Ġweed', 'en', 'Ġlater', 'Ġrefuted', 'Ġclaim', 'Ġemphasizing', 'Ġdifferent', 'Ġorbits', 'Ġtwo', 'Ġspacecraft', 'Ġpre', 'cluded', 'Ġpractical', 'Ġsurveillance', 'Ġfly', 'bys', 'Ġoct', 'ober', 'Ġguardian', 'Ġreported', 'Ġclaims', 'Ġsecurity', 'Ġexperts', 'Ġused', 'Ġtest', 'Ġreconnaissance', 'Ġsensors', 'Ġparticularly', 'Ġhold', 'Ġradiation', 'Ġhazards', 'Ġorbit', '".[', 'mber', 'Ġinternational', 'Ġbusiness', 'Ġtimes', 'Ġspeculated', 'Ġu', 'Ġgovernment', 'Ġtesting', 'Ġversion', 'Ġem', 'drive', 'Ġelectromagnetic', 'Ġmicrowave', 'Ġthr', 'uster', 'Ġfourth', 'Ġflight', 'Ġem', 'drive', 'Ġtechnology']</t>
+          <t>['000', 'âĢĵ', '000', 'v', 'ac', 'uum', 'Ġrestart', 'Ġcapability', 'Ġyes', 'Ġengines', 'Ġburns', 'Ġyes', 'Ġdual', 'Ġredundant', 'Ġte', 'ate', 'b', 'Ġpy', 'roph', 'oric', 'Ġign', 'ers', 'Ġtank', 'Ġpress', 'ur', 'ization', 'Ġheated', 'Ġhelium', 'Ġheated', 'Ġhelium', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġg', 'imb', 'aled', 'Ġengine', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġshutdown', 'Ġprocess', 'Ġcommanded', 'Ġcommanded', 'Ġn', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġp', 'ne', 'umatic', 'Ġn', 'Ġp', 'ne', 'umatic', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġrocket', 'Ġspace', 'x', 'Ġdragon', 'Ġspacecraft', 'Ġlaunch', 'Ġpad', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġuses', 'Ġmeter', 'Ġlong', 'Ġinter', 'stage', 'Ġlonger', 'Ġstronger', 'Ġfal', 'con', 'Ġinter', 'stage', 'pos', 'ite', 'Ġstructure', 'Ġconsisting', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġcore', 'Ġsurrounded', 'Ġcarbon', 'Ġfiber', 'Ġface', 'Ġsheet', 'Ġpl', 'ies', '".[', 'Ġoverall', 'Ġlength', 'Ġvehicle', 'Ġlaunch', 'Ġmeters', 'Ġtotal', 'Ġfueled', 'Ġmass', '000', 'Ġaluminium', 'l', 'ith', 'ium', 'Ġalloy', 'Ġused', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġupgraded', 'Ġvehicle', 'includes', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġsystems', 'Ġallow', 'Ġspace', 'x', 'Ġreturn', 'Ġfirst', 'Ġstage', 'Ġlaunch', 'Ġsite', 'Ġcompletion', 'Ġprimary', 'Ġmission', 'Ġrequirements', 'Ġsystems', 'Ġinclude', 'Ġfour', 'Ġdeploy', 'able', 'Ġlanding', 'Ġlegs', 'Ġlocked', 'Ġfirst', 'stage', 'Ġtank', 'Ġascent', 'Ġexcess', 'Ġpropell', 'ant', 'Ġreserved', 'Ġfal', 'con', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġoperations', 'Ġdiverted', 'Ġuse', 'Ġprimary', 'Ġmission', 'Ġobjective', 'Ġrequired', 'Ġensuring', 'Ġsufficient', 'Ġperformance', 'Ġmargins', 'Ġsuccessful', 'Ġmissions', '".[', 'Ġnominal', 'Ġpayload', 'Ġcapacity', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġkilograms', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġprice', 'Ġper', 'Ġlaunch', 'Ġmillion', 'Ġversus', 'Ġkilograms', 'Ġexpend', 'able', 'Ġfirst', 'stage', 'Ġearly', 'Ġmarch', 'Ġspace', 'x', 'Ġpricing', 'Ġpayload', 'Ġspecifications', 'Ġpublished', 'Ġexpend', 'able', 'Ġfal', 'con', 'Ġrocket', 'Ġactually', 'Ġincluded', 'Ġpercent', 'Ġperformance', 'Ġpublished', 'Ġprice', 'Ġlist', 'Ġindicated', 'Ġtime', 'Ġadditional', 'Ġperformance', 'Ġreserved', 'Ġspace', 'x', 'Ġconduct', 'us', 'ability', 'Ġtesting', 'Ġfal', 'con', 'Ġstill', 'Ġachieving']</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>['Ġtransfer', 'Ġcontract', 'Ġbo', 'e', 'ing', 'Ġundertaken', 'Ġvia', 'Ġstate', 'Ġdepartment', 'Ġexport', 'Ġlicense', 'Ġapproved', 'Ġministry', 'Ġdefence', 'Ġbo', 'e', 'ing', 'Ġsince', 'Ġstated', 'Ġlonger', 'Ġpursuing', 'Ġarea', 'Ġresearch', 'Ġu', 'Ġair', 'Ġforce', 'Ġstated', 'Ġtesting', 'Ġh', 'alle', 'ffect', 'Ġthr', 'uster', 'Ġsystem', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġj', 'uly', 'Ġformer', 'Ġunited', 'Ġstates', 'Ġsecretary', 'Ġair', 'Ġforce', 'ather', 'Ġwil', 'son', 'Ġexplained', 'Ġellipt', 'ic', 'Ġorbit', 'Ġcould', 'Ġper', 'ig', 'ee', 'Ġuse', 'Ġthin', 'Ġatmosphere', 'Ġmake', 'Ġorbit', 'Ġchange', 'Ġpreventing', 'Ġobservers', 'Ġdiscovering', 'Ġnew', 'Ġorbit', 'Ġpermitting', 'Ġsecret', 'Ġactivities', 'Ġspeculation', 'Ġregarding', 'Ġpurpose', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'far', 'Ġright', 'Ġsmallest', 'Ġlight', 'est', 'Ġorbital', 'Ġspace', 'plane', 'Ġyet', 'Ġï', '¬', 'Ĥ', 'Ġnorth', 'Ġameric', 'Ġspaceship', 'one', 'Ġsub', 'orb', 'ital', 'Ġspace', 'planes', 'Ġshown', 'Ġbur', 'Ġconducted', 'Ġunc', 'rew', 'ed', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġastronomer', 'Ġj', 'athan', 'cd', 'owell', 'Ġeditor', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġstated', 'Ġsatellites', 'Ġlaunched', 'Ġreported', 'Ġrequired', 'Ġregistration', 'Ġconvention', 'Ġunited', 'Ġnations', 'Ġoffice', 'Ġouter', 'Ġspace', 'Ġaffairs', 'Ġparties', 'Ġconvention', 'Ġwould', 'Ġknow', 'Ġprocessing', 'Ġcarried', 'Ġinside', 'Ġb', 'ays', 'Ġorbit', 'er', 'Ġprocessing', 'Ġfacility', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġfl', 'ida', 'Ġvehicle', 'Ġloaded', 'Ġtop', 'secret', 'Ġpayload', 'Ġplaced', 'Ġinside', 'Ġfair', 'ing', 'Ġalong', 'Ġstage', 'Ġadapter', 'Ġtransported', 'Ġlaunch', 'Ġsite', 'Ġprevious', 'Ġlaunch', 'Ġsites', 'Ġincluded', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġlanding', 'Ġdone', 'Ġone', 'Ġthree', 'Ġsites', 'Ġacross', 'Ġus', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġv', 'enberg', 'Ġspace', 'Ġforce', 'Ġbase', 'Ġed', 'wards', 'Ġair', 'Ġforce', 'Ġbase', 'Ġreturn', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġplaced', 'Ġpayload', 'ister', 'Ġloaded', 'Ġbo', 'e', 'ing', 'Ġcargo', 'Ġplane', 'Ġk', 'enn', 'edy', 'Ġunloaded', 'Ġtowed', 'Ġprepared', 'Ġnext', 'Ġflight', 'Ġtechnicians', 'Ġmust', 'Ġwear', 'Ġprotective', 'Ġsuits', 'Ġdue', 'Ġtoxic', 'Ġhyper', 'g', 'olic', 'Ġgases', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġreusable', 'Ġrobotic', 'Ġspace', 'plane', 'Ġapproximately', 'percent']</t>
+          <t>['Ġspecified', 'Ġpayload', 'Ġcustomers', 'Ġmany', 'Ġengineering', 'Ġchanges', 'Ġsupport', 'us', 'ability', 'Ġrecovery', 'Ġfirst', 'Ġstage', 'Ġmade', 'Ġearlier', 'Ġversion', 'Ġspace', 'x', 'Ġindicated', 'Ġroom', 'Ġincrease', 'Ġpayload', 'Ġperformance', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġdecrease', 'Ġlaunch', 'Ġprice', 'Ġspace', 'x', 'Ġannounced', 'Ġnumber', 'Ġmodifications', 'Ġprevious', 'Ġversion', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġnew', 'Ġrocket', 'Ġknown', 'Ġinternally', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġalso', 'Ġknown', 'Ġvariety', 'Ġnames', 'Ġincluding', 'Ġfal', 'con', 'Ġenhanced', 'Ġfal', 'con', 'Ġfull', 'performance', 'Ġfal', 'con', 'Ġupgraded', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġupgrade', 'Ġsince', 'Ġfirst', 'Ġflight', 'full', 'Ġthrust', 'Ġupgrade', '",', 'Ġspace', 'x', 'Ġreferring', 'Ġversion', 'Ġfal', 'con', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġexplained', 'Ġmarch', 'Ġnew', 'Ġdesign', 'Ġwould', 'Ġresult', 'Ġstreamlined', 'Ġproduction', 'Ġwell', 'Ġimproved', 'Ġperformance', ':[', 'Ġgot', 'Ġhigher', 'Ġthrust', 'Ġengines', 'Ġfinished', 'Ġdevelopment', "'re", 'qual', 'ification', 'Ġtesting', '].', "'re", 'Ġalso', 'Ġmodifying', 'Ġstructure', 'Ġlittle', 'Ġbit', 'Ġwant', 'Ġbuilding', 'Ġtwo', 'Ġversions', 'Ġtwo', 'Ġcores', 'Ġfactory', 'Ġwould', 'Ġgreat', 'Ġcustomer', 'Ġperspective', "'s", 'Ġincrease', 'Ġperformance', 'Ġmaybe', 'Ġlittle', 'Ġallows', 'Ġus', 'Ġland', 'Ġfirst', 'Ġstage', 'Ġg', 'Ġmissions', 'Ġdrone', 'Ġship', 'Ġdevelopment', 'Ġhistory', 'Ġdevelopment', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġaccording', 'Ġspace', 'x', 'Ġstatement', 'Ġmay', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwould', 'Ġlikely', 'Ġrequire', 'Ġrec', 'ert', 'ification', 'Ġlaunch', 'Ġunited', 'Ġstates', 'Ġgovernment', 'Ġcontracts', 'Ġshot', 'well', 'Ġstated', 'Ġiter', 'ative', 'Ġprocess', 'Ġagencies', ']"', 'Ġbecome', 'Ġquicker', 'Ġquicker', 'Ġcertify', 'Ġnew', 'Ġversions', 'Ġvehicle', '."[', 'Ġus', 'Ġair', 'Ġforce', 'Ġcertified', 'Ġupgraded', 'Ġversion', 'Ġlaunch', 'Ġvehicle', 'Ġused', 'Ġus', 'Ġmilitary', 'Ġlaunches', 'Ġjan', 'uary', 'Ġbased', 'Ġone', 'Ġsuccessful', 'Ġlaunch', 'Ġdate', 'Ġdemonstrated', 'cap', 'ability', 'Ġdesign', 'Ġproduce', 'Ġqualify', 'Ġdeliver', 'Ġnew', 'Ġlaunch', 'Ġsystem', 'Ġprovide', 'Ġmission', 'Ġassurance', 'Ġsupport', 'Ġrequired', 'Ġdeliver', 'Ġn', 'ss', 'national', 'Ġsecurity', 'Ġspace', 'Ġsatellites', 'Ġupgraded', 'Ġfirst', 'Ġstage', 'Ġbegan', 'Ġacceptance', 'Ġtesting', 'Ġspace', 'x', "'s", 'Ġmc', 'greg', 'Ġfacility']</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2635,7 +2635,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>['scale', 'Ġderivative', 'Ġbo', 'e', 'ing', 'Ġx', 'Ġmeasuring', 'Ġfeet', 'Ġlength', 'Ġfeatures', 'Ġtwo', 'Ġangled', 'Ġtail', 'Ġfins', 'Ġlaunches', 'Ġatop', 'las', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġrocket', 'Ġspace', 'plane', 'Ġdesigned', 'Ġoperate', 'Ġspeed', 'Ġrange', 'Ġmach', 'entry', 'Ġtechnologies', 'Ġdemonstrated', 'Ġinclude', 'Ġimproved', 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġenhanced', 'Ġav', 'ionics', 'Ġautonomous', 'Ġguidance', 'Ġsystem', 'Ġadvanced', 'Ġair', 'frame', 'Ġspace', 'plane', "'s", 'Ġthermal', 'Ġprotection', 'Ġsystem', 'Ġbuilt', 'Ġupon', 'Ġprevious', 'Ġgenerations', 'Ġatmospheric', 'entry', 'Ġspacecraft', 'Ġincorporating', 'Ġsil', 'ica', 'Ġceramic', 'Ġtiles', 'Ġav', 'ionics', 'Ġsuite', 'Ġused', 'Ġbo', 'e', 'ing', 'Ġdevelop', 'Ġc', 'st', 'Ġcrew', 'ed', 'Ġspacecraft', 'Ġdevelopment', 'aid', 'Ġdesign', 'Ġdevelopment', 'Ġn', 'asa', "'s", 'Ġorbital', 'Ġspace', 'Ġplane', 'Ġdesigned', 'Ġprovide', 'Ġcrew', 'Ġrescue', 'Ġcrew', 'Ġtransport', 'Ġcapability', 'Ġinternational', 'Ġspace', 'Ġstation', '",', 'Ġaccording', 'Ġn', 'asa', 'Ġfact', 'Ġsheet', 'Ġn', 'asa', 'Ġpowered', 'Ġone', 'ero', 'jet', 'Ġengine', 'Ġusing', 'Ġst', 'orable', 'Ġpropell', 'ants', 'Ġproviding', 'Ġthrust', 'Ġpounds', 'force', 'Ġhuman', 'rated', 'Ġengine', 'Ġused', 'Ġdual', 'power', 'Ġastronaut', 'Ġtraining', 'Ġvehicle', 'Ġgiven', 'Ġnew', 'Ġflight', 'Ġcertification', 'Ġuse', 'Ġhydrogen', 'Ġpropell', 'ants', 'Ġreportedly', 'Ġchanged', 'Ġhyper', 'g', 'olic', 'Ġpropulsion', 'Ġsystem', 'Ġlands', 'Ġautomatically', 'Ġupon', 'Ġreturning', 'Ġorbit', 'Ġthird', 'Ġreusable', 'Ġspacecraft', 'Ġcapability', 'v', 'iet', 'Ġbur', 'Ġshuttle', 'Ġu', 'Ġspace', 'Ġshuttle', 'Ġautomatic', 'Ġlanding', 'Ġcapability', 'Ġmid', 'Ġnever', 'Ġtested', 'Ġsmallest', 'Ġlight', 'est', 'Ġorbital', 'Ġspace', 'plane', 'Ġflown', 'Ġdate', 'Ġlaunch', 'Ġmass', 'Ġaround', '000', 'Ġpounds', '000', 'Ġapproximately', 'Ġone', 'Ġquarter', 'Ġsize', 'Ġspace', 'Ġshuttle', 'Ġorbit', 'er', 'Ġprocessing', 'Ġdesign', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġapr', 'il', 'Ġspace', 'Ġfoundation', 'Ġawarded', 'Ġteam', 'Ġspace', 'Ġachievement', 'Ġaward', 'Ġsignificantly', 'Ġadvancing', 'Ġstate', 'Ġart', 'Ġreusable', 'Ġspacecraft', 'orbit', 'Ġoperations', 'Ġdesign', 'Ġdevelopment', 'Ġtest']</t>
+          <t>['Ġse', 'pt', 'ember', 'Ġfirst', 'Ġtwo', 'Ġstatic', 'Ġfire', 'Ġtests', 'Ġcompleted', 'Ġse', 'pt', 'ember', 'Ġincluded', 'Ġsub', 'cool', 'ed', 'Ġpropell', 'ant', 'Ġimproved', 'Ġmer', 'lin', 'Ġengines', 'Ġrocket', 'Ġreached', 'Ġfull', 'Ġthrottle', 'Ġstatic', 'Ġfire', 'Ġscheduled', 'Ġlaunch', 'Ġearlier', 'mber', 'es', '.,', 'Ġsatellite', 'Ġowner', 'Ġoperator', 'Ġannounced', 'Ġplans', 'Ġfe', 'b', 'ruary', 'Ġlaunch', 'Ġsatellite', 'Ġfirst', 'Ġflight', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġevent', 'Ġspace', 'x', 'Ġelected', 'Ġlaunch', 'Ġsecond', 'Ġflight', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlaunch', 'Ġorb', 'comm', 'Ġsecond', 'Ġconstellation', 'Ġfirst', 'Ġflight', 'Ġch', 'ris', 'Ġber', 'gin', 'Ġnas', 'asp', 'ace', 'flight', 'Ġexplained', 'Ġrequired', 'Ġcomplicated', 'Ġsecond', 'stage', 'Ġburn', 'Ġprofile', 'Ġinvolving', 'Ġone', 'Ġrestart', 'Ġsecond', 'stage', 'Ġengine', 'Ġorb', 'comm', 'Ġmission', 'Ġwould', 'allow', 'Ġsecond', 'Ġstage', 'Ġconduct', 'Ġadditional', 'Ġtesting', 'Ġahead', 'Ġtaxing', 'Ġmission', '."[', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġcompleted', 'Ġmaiden', 'Ġflight', 'Ġde', 'cember', 'Ġcarrying', 'Ġorb', 'comm', 'atellite', 'Ġpayload', 'Ġorbit', 'Ġlanding', 'Ġrocket', "'s", 'Ġfirst', 'Ġstage', 'Ġintact', 'Ġspace', 'x', "'s", 'Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġsecond', 'Ġmission', 'Ġoccurred', 'Ġmarch', 'mber', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġversion', 'Ġflown', 'Ġmissions', 'Ġsuccess', 'Ġrate', '%.', 'Ġfirst', 'Ġstage', 'Ġrecovered', 'Ġone', 'Ġrocket', 'Ġdestroyed', 'Ġpre', 'launch', 'Ġtests', 'Ġcounted', 'Ġone', 'Ġflown', 'Ġmissions', 'Ġse', 'pt', 'ember', 'Ġrocket', 'Ġcarrying', 'Ġspace', "'s", 'Ġexploded', 'Ġlaunch', 'pad', 'launch', 'Ġcomplex', 'Ġfueling', 'Ġpreparation', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġtest', 'Ġconducted', 'Ġpreparation', 'Ġlaunch', 'th', 'Ġfal', 'con', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġvehicle', 'Ġpayload', 'Ġdestroyed', 'Ġexplosion', 'Ġsubsequent', 'Ġinvestigation', 'Ġshowed', 'Ġroot', 'Ġcause', 'Ġignition', 'Ġsolid', 'Ġliquid', 'Ġcompressed', 'Ġlayers', 'Ġimmersed', 'Ġhelium', 'Ġtanks', 'Ġcarbon', 'f', 'iber', 'Ġwra', 'ppings', 'Ġresolve', 'Ġissue', 'Ġflights', 'Ġspace', 'x', 'Ġmade', 'Ġdesign', 'Ġchanges', 'Ġtanks', 'Ġchanges', 'Ġfueling', 'Ġprocedure', 'Ġtesting', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlaunch', 'Ġhistory', 'Ġlaunch', 'Ġlanding', 'Ġsites', 'Ġlaunch', 'Ġsites', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia']</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2648,7 +2648,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>['Ġorbital', 'Ġoperation', 'Ġspace', 'Ġflight', 'Ġvehicle', 'Ġthree', 'Ġmissions', 'Ġtotaling', 'Ġdays', 'Ġspace', '".[', 'Ġtwo', 'Ġoperational', 'Ġcompleted', 'Ġorbital', 'Ġmissions', 'Ġspent', 'Ġcombined', 'Ġdays', 'Ġyears', 'Ġspace', 'Ġoperational', 'Ġhistory', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġflight', 'Ġvehicle', 'Ġlaunch', 'Ġdate', 'Ġlanding', 'Ġdate', 'Ġlauncher', 'Ġmission', 'Ġduration', 'Ġnotes', 'Ġstatus', 'Ġapr', 'il', 'Ġut', 'c', 'Ġde', 'cember', 'Ġ09', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġfirst', 'Ġlaunch', 'las', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġfirst', 'Ġameric', 'Ġautonomous', 'Ġorbital', 'Ġrunway', 'Ġlanding', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlanded', 'Ġv', 'enberg', 'Ġsuccess', 'Ġmarch', 'Ġut', 'c', 'Ġj', 'une', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsecond', 'Ġlanded', 'Ġv', 'enberg', 'Ġsuccess', 'Ġde', 'cember', '03', 'Ġut', 'c', 'Ġoct', 'ober', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġsecond', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanded', 'Ġv', 'enberg', 'Ġsuccess', 'Ġmay', '05', 'Ġut', 'c', 'Ġmay', 'Ġut', 'c', 'las', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġsecond', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsecond', 'Ġfirst', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġsuccess', 'Ġse', 'pt', 'ember', '00', 'Ġut', 'c', 'Ġoct', 'ober', 'Ġ07', 'Ġut', 'c', 'Ġfal', 'con', 'Ġblock', 'Ġus', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġfirst', 'Ġlaunch', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġvehicle', 'Ġsuccess', 'Ġmay', 'Ġut', 'c', 'mber', 'Ġut', 'c', 'las', 'Ġus', '08', 'Ġdays', 'Ġhours', 'Ġminutes', 'Ġcarried', 'Ġexperiments', 'Ġdate', 'Ġfirst', 'Ġlaunch', 'Ġus', 'sf', 'Ġlongest', 'Ġmission', 'Ġlanded', 'Ġk', 'enn', 'edy', 'Ġsuccess', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġsits', 'Ġrunway', 'Ġlanding', 'Ġv', 'enberg', 'Ġend', 'usa', 'Ġmission', 'Ġde', 'cember', 'Ġflight', 'Ġvehicle', 'Ġlaunch', 'Ġdate', 'Ġlanding', 'Ġdate', 'Ġlauncher', 'Ġmission', 'Ġduration', 'Ġnotes', 'Ġstatus', 'Ġspace', 'Ġcenter', 'Ġde', 'cember', 'Ġfal', 'con']</t>
+          <t>['Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġspace', 'x', 'Ġfirst', 'Ġused', 'Ġlaunch', 'Ġcomplex', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġspace', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġrockets', 'Ġlike', 'Ġpredecessor', 'Ġfal', 'con', 'Ġfollowing', 'Ġaccident', 'Ġlaunches', 'Ġeast', 'Ġcoast', 'Ġswitched', 'Ġrefurb', 'ished', 'Ġpad', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġleased', 'Ġarchitectural', 'Ġengineering', 'Ġdesign', 'Ġwork', 'Ġchanges', 'Ġbegun', 'Ġcontract', 'Ġlease', 'Ġpad', 'Ġn', 'asa', 'Ġsigned', 'Ġapr', 'il', 'Ġconstruction', 'Ġcomm', 'encing', 'Ġlater', 'Ġincluding', 'Ġbuilding', 'Ġlarge', 'Ġhorizontal', 'Ġintegration', 'Ġfacility', 'h', 'Ġorder', 'Ġhouse', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicles', 'Ġassociated', 'Ġhardware', 'Ġpayload', 'Ġprocessing', 'Ġfirst', 'Ġlaunch', 'Ġoccurred', 'Ġfe', 'b', 'ruary', 'Ġcr', 'Ġmission', 'Ġcrew', 'Ġaccess', 'Ġarm', 'Ġwhite', 'Ġroom', 'Ġwork', 'Ġstill', 'Ġneed', 'Ġcompleted', 'Ġcrew', 'ed', 'Ġlaunches', 'Ġspace', 'x', 'Ġdragon', 'Ġcapsule', 'Ġscheduled', 'Ġadditional', 'Ġprivate', 'Ġlaunch', 'Ġsite', 'Ġintended', 'Ġsolely', 'Ġcommercial', 'Ġlaunches', 'Ġplanned', 'Ġb', 'oca', 'Ġch', 'ica', 'Ġvillage', 'Ġnear', 'Ġbrown', 'ville', 'Ġtex', 'Ġfollowing', 'Ġmulti', 'state', 'Ġevaluation', 'Ġprocess', 'âĢĵ', 'mid', 'Ġlooking', 'Ġfl', 'ida', 'Ġge', 'org', 'ia', 'Ġpu', 'erto', 'Ġr', 'ico', 'Ġhowever', 'Ġfocus', 'Ġsite', 'Ġchanged', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġv', 'ol', 'Ġtest', 'Ġflights', 'Ġsubsc', 'ale', 'Ġstarship', 'Ġho', 'pper', 'Ġtest', 'Ġvehicle', 'Ġunlikely', 'Ġever', 'Ġused', 'Ġfal', 'con', 'Ġheavy', 'Ġflights', 'Ġcurrent', 'Ġlaunch', 'Ġpads', 'Ġprovide', 'Ġenough', 'Ġlaunch', 'Ġcapability', 'Ġspace', 'x', 'Ġcompleted', 'Ġconstruction', 'Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġknown', 'Ġzone', 'Ġconsisting', 'Ġpad', 'Ġfeet', 'Ġdiameter', 'Ġfirst', 'Ġused', 'Ġde', 'cember', 'Ġsuccessful', 'Ġlanding', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġlanding', 'Ġfirst', 'Ġoverall', 'Ġsuccessful', 'Ġfal', 'con', 'Ġthird', 'Ġlanding', 'Ġattempt', 'Ġhard', 'Ġsurface', 'Ġj', 'une', 'Ġone', 'Ġlanding', 'Ġattempt', 'Ġfailed', 'Ġbooster', 'Ġlanded', 'Ġoffshore', 'Ġfollowing', 'Ġdays', 'Ġtowed', 'Ġback', 'Ġport', 'aver', 'al', 'Ġraised', 'Ġwater', 'Ġusing', 'Ġtwo', 'Ġcr', 'anes', 'Ġbrought', 'Ġback', 'Ġspace', 'x', 'Ġhangar', 'Ġdirectly', 'Ġnext', 'Ġspace', 'x', 'Ġconstructed', 'Ġallow']</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>['Ġheavy', 'uss', 'f', 'Ġfirst', 'Ġlaunch', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġplanned', 'Ġfirst', 'Ġlaunched', 'Ġfirst', 'Ġmission', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġapr', 'il', 'Ġut', 'c', 'Ġspacecraft', 'Ġplaced', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġtesting', 'Ġu', 'Ġair', 'Ġforce', 'Ġrevealed', 'Ġorbital', 'Ġdetails', 'Ġmission', 'Ġworldwide', 'Ġnetwork', 'Ġamateur', 'Ġastronomers', 'Ġclaimed', 'Ġidentified', 'Ġspacecraft', 'Ġorbit', 'Ġmay', 'Ġspacecraft', 'Ġinclination', 'Â°', 'Ġcircling', 'Ġearth', 'Ġevery', 'Ġminutes', 'Ġorbit', 'Ġmiles', 'Ġrep', 'uted', 'ly', 'Ġpassed', 'Ġgiven', 'Ġspot', 'Ġearth', 'Ġevery', 'Ġfour', 'Ġdays', 'Ġoperated', 'Ġaltitude', 'Ġtypical', 'Ġmilitary', 'Ġsurveillance', 'Ġsatellites', 'Ġorbit', 'Ġalso', 'Ġcommon', 'Ġamong', 'Ġcivilian', 'Ġle', 'Ġsatellites', 'Ġspace', 'plane', "'s", 'Ġaltitude', 'Ġiss', 'Ġcrew', 'ed', 'Ġspacecraft', 'Ġu', 'Ġair', 'Ġforce', 'Ġannounced', 'âĢĵ', 'Ġde', 'cember', 'Ġlanding', 'mber', 'Ġscheduled', 'Ġde', 'orb', 'ited', 'ent', 'ered', 'Ġearth', "'s", 'Ġatmosphere', 'Ġlanded', 'Ġsuccessfully', 'Ġv', 'enberg', 'Ġde', 'cember', 'Ġ09', 'Ġut', 'c', 'Ġconducting', 'Ġfirst', 'Ġus', 'Ġautonomous', 'Ġorbital', 'Ġlanding', 'Ġonto', 'Ġrunway', 'Ġfirst', 'Ġlanding', 'Ġsince', 'v', 'iet', 'Ġbur', 'Ġshuttle', 'Ġspent', 'Ġdays', 'Ġhours', 'Ġspace', 'Ġsuffered', 'Ġtire', 'Ġblow', 'Ġlanding', 'Ġsustained', 'Ġminor', 'Ġdamage', 'Ġunderside', 'Ġsecond', 'Ġlaunched', 'Ġinaugural', 'Ġmission', 'Ġdesignated', 'Ġaboard', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġmarch', 'Ġmission', 'Ġclassified', 'Ġdescribed', 'Ġu', 'Ġmilitary', 'Ġeffort', 'Ġtest', 'Ġnew', 'Ġspace', 'Ġtechnologies', 'mber', 'Ġu', 'Ġair', 'Ġforce', 'Ġannounced', 'Ġwould', 'Ġextend', 'Ġus', 'Ġbeyond', 'day', 'Ġbaseline', 'Ġduration', 'Ġapr', 'il', 'Ġgeneral', 'iam', 'Ġl', 'Ġshel', 'ton', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġdeclared', 'Ġongoing', 'Ġmission', 'spect', 'acular', 'Ġsuccess', '".[', 'Ġmay', 'Ġair', 'Ġforce', 'Ġstated', 'Ġwould', 'Ġland', 'Ġv', 'enberg', 'Ġj', 'une']</t>
+          <t>['Ġsimultaneous', 'Ġbooster', 'Ġland', 'ings', 'Ġfal', 'con', 'Ġheavy', 'Ġflights', 'mber', 'Ġfour', 'Ġboosters', 'Ġlanded', 'Ġspace', 'x', 'Ġalso', 'Ġcreated', 'Ġlanding', 'Ġsite', 'Ġformer', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġlaunch', 'Ġsite', 'Ġdemolished', 'Ġreconstruction', 'Ġlanding', 'Ġsite', 'Ġoct', 'ober', 'Ġfal', 'con', 'Ġrocket', 'Ġbooster', 'Ġsuccessfully', 'Ġlanded', 'Ġnew', 'Ġground', 'Ġpad', 'Ġknown', 'Ġfirst', 'Ġtime', 'Ġstarting', 'Ġspace', 'x', 'Ġcommissioned', 'Ġconstruction', 'Ġautonomous', 'Ġspac', 'eport', 'Ġdrone', 'Ġships', 'ds', 'Ġdeck', 'Ġbarg', 'es', 'fitted', 'Ġstation', 'keeping', 'Ġengines', 'Ġlarge', 'Ġlanding', 'Ġplatform', 'Ġships', 'Ġstationed', 'Ġhundreds', 'Ġkilometers', 'range', 'Ġallow', 'Ġfirst', 'Ġstage', 'Ġrecovery', 'Ġhigh', 'vel', 'ocity', 'Ġmissions', 'Ġcannot', 'Ġreturn', 'Ġlaunch', 'Ġsite', 'Ġlanding', 'Ġsites', 'Ġdrone', 'Ġships', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġthree', 'Ġoperational', 'Ġdrone', 'Ġships', 'Ġread', 'Ġinstructions', 'Ġcourse', 'Ġstill', 'Ġlove', 'Ġshortfall', 'Ġgrav', 'itas', 'Ġshortfall', 'Ġgrav', 'itas', 'Ġread', 'Ġinstructions', 'Ġused', 'l', 'antic', 'Ġlaunches', 'Ġcape', 'aver', 'al', 'Ġcourse', 'Ġstill', 'Ġlove', 'Ġoperated', 'Ġpac', 'ific', 'Ġport', 'Ġv', 'enberg', 'Ġtransporter', 'Ġmission', 'Ġlaunch', 'Ġdebuted', 'Ġnew', 'Ġnozzle', 'Ġextension', 'Ġdesign', 'Ġaimed', 'Ġincreasing', 'Ġcad', 'ence', 'Ġreducing', 'Ġcosts', 'Ġnew', 'Ġnozzle', 'Ġextension', 'Ġshorter', 'Ġresult', 'Ġengine', 'Ġlower', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġtherefore', 'Ġperformance', 'Ġdue', 'Ġï', '¬', 'Ĥ', 'Ġmissions', "'t", 'Ġneed', 'Ġfal', 'con', 'Ġfull', 'Ġperformance', 'Ġcapability', 'cap', 'abilities', 'Ġservices', ')"', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'http', 'space', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'Ġb', 'aylor', 'ichael', 'Ġmay', 'Ġblock', 'Ġspace', 'x', 'Ġincrease', 'Ġlaunch', 'Ġcad', 'ence', 'Ġlower', 'Ġprices', 'pr', 'ices', 'Ġretrieved', 'Ġmay', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'mber', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>['Ġspacecraft', 'Ġlanded', 'Ġautonom', 'ously', 'Ġj', 'une', 'Ġspent', 'Ġdays', 'Ġhours', 'Ġspace', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġsits', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġmission', 'Ġsits', 'Ġrunway', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'mber', '09', 'th', 'Ġday', 'usa', 'Ġmission', 'Ġthird', 'Ġmission', 'Ġsecond', 'Ġflight', 'Ġfirst', 'Ġoriginally', 'Ġscheduled', 'Ġlaunch', 'Ġoct', 'ober', 'Ġpostponed', 'Ġengine', 'Ġissue', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġsuccessfully', 'Ġlaunched', 'Ġcape', 'aver', 'al', 'Ġde', 'cember', '03', 'Ġut', 'c', 'Ġorbit', 'Ġspacecraft', 'Ġdesignated', 'Ġus', 'Ġlanding', 'Ġoccurred', 'Ġv', 'enberg', 'Ġoct', 'ober', 'Ġut', 'c', 'Ġtotal', 'Ġtime', 'Ġorbit', 'Ġdays', 'Ġfourth', 'Ġmission', 'Ġcod', 'en', 'amed', 'Ġdesignated', 'Ġus', 'Ġorbit', 'Ġsecond', 'Ġflight', 'Ġsecond', 'Ġvehicle', 'Ġlaunched', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġmay', '05', 'Ġobjectives', 'Ġincluded', 'Ġtest', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', "'s", 'Ġhall', 'effect', 'Ġthr', 'uster', 'Ġsupport', 'Ġadvanced', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġcommunications', 'Ġsatellite', 'Ġprogram', 'Ġn', 'asa', 'Ġinvestigation', 'Ġperformance', 'Ġvarious', 'Ġmaterials', 'Ġspace', 'Ġleast', 'Ġdays', 'Ġvehicle', 'Ġspent', 'Ġrecord', 'breaking', 'Ġdays', 'Ġhours', 'Ġorbit', 'Ġlanding', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', "'s", 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġmay', 'Ġfifth', 'Ġmission', 'Ġdesignated', 'Ġus', 'Ġlaunched', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġlaunch', 'Ġcomplex', 'Ġse', 'pt', 'ember', '00', 'Ġut', 'c', 'Ġarrival', 'Ġhurricane', 'Ġ', 'irm', 'Ġlaunch', 'Ġvehicle', 'Ġfal', 'con', 'Ġrocket', 'Ġnumber', 'Ġsmall', 'Ġsatellites', 'Ġalso', 'Ġshared', 'Ġspacecraft', 'Ġinserted', 'Ġhigher', 'Ġinclination', 'Ġorbit', 'Ġprevious', 'Ġmissions', 'Ġexpanding', 'Ġenvelope', 'Ġflight', 'Ġspacecraft', 'Ġmodified', 'Ġorbit', 'Ġusing', 'board', 'Ġpropulsion', 'Ġsystem']</t>
+          <t>['Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'es', 'nic', 'Ġtre', 'vor', 'Ġoct', 'ober', 'st', 'arl', 'ink', 'Ġgroup', 'Ġfal', 'con', 'Ġblock', 'Ġeveryday', 'Ġastronaut', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'mber', 'fal', 'con', 'Ġblock', 'Ġnext', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġk', 'bs', 'Ġgun', 'ter', 'fal', 'con', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'mber', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'el', 'mus', 'k', 'Ġde', 'cember', 'Ġ"-', 'Ġcase', 'Ġdeep', 'Ġcry', 'Ġincreases', 'Ġdensity', 'Ġampl', 'ï', '¬', 'ģ', 'es', 'Ġrocket', 'Ġperformance', 'Ġfirst', 'Ġtime', 'Ġanyone', 'Ġgone', 'Ġlow', 'Ġchilled', 'f', 'Ġf', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'trans', 'porter', 'Ġretrieved', 'Ġmarch', 'es', 'nic', 'Ġtre', 'vor', 'Ġj', 'uly', 'ech', 'ost', 'ar', 'Ġfal', 'con', 'Ġheavy', 'Ġeveryday', 'Ġastronaut', 'Ġretrieved', 'Ġj', 'uly', 'Ġnotes', 'Ġreferences', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'active', 'Ġlaunch', 'Ġvehicle', 'Ġreliability', 'Ġstatistics', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġlaunches', 'Ġretrie', 'ves', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġrecycled', 'Ġrocket', 'Ġwashing', 'ton', 'Ġpost', 'Ġassociated', 'Ġpress', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġmarch', 'space', 'x', 'Ġlaunches', 'Ġsatellite', 'Ġpartly', 'Ġused', 'Ġrocket', 'http', 'Ġnew', 'ork', 'Ġtimes', 'Ġretrieved', 'Ġapr', 'il', 'Ġvia', 'Ġn', 'yt', 'imes', 'Ġb', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġoct', 'ober', 'space', 'x', 'Ġchanges', 'Ġfal', 'con', 'Ġreturn', 'ï', '¬', 'Ĥ', 'ight', 'Ġplans', 'htt', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmarch', 'space', 'x', 'Ġaims', 'Ġdebut', 'Ġnew', 'Ġversion', 'Ġfal']</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>['Ġcomplete', 'Ġpayload', 'Ġclassified', 'Ġair', 'Ġforce', 'Ġannounced', 'Ġone', 'Ġexperiment', 'Ġflying', 'Ġadvanced', 'Ġstruct', 'urally', 'Ġembedded', 'Ġthermal', 'Ġspread', 'er', 'ets', 'ii', 'Ġmeasures', 'Ġperformance', 'Ġoscill', 'ating', 'Ġheat', 'Ġmission', 'Ġcompleted', 'Ġvehicle', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'Ġoct', 'ober', 'Ġ07', 'Ġsixth', 'Ġmission', 'Ġu', 'Ġspace', 'Ġforce', 'formerly', 'Ġknown', 'Ġlaunched', 'las', 'Ġrocket', 'Ġcape', 'aver', 'al', 'Ġmay', '00', 'Ġmission', 'Ġfirst', 'Ġtime', 'Ġspace', 'plane', 'Ġcarried', 'Ġservice', 'Ġmodule', 'Ġring', 'Ġattached', 'Ġrear', 'Ġvehicle', 'Ġhosting', 'Ġmultiple', 'Ġexperiments', 'Ġmission', 'Ġhosts', 'Ġexperiments', 'Ġprior', 'Ġflights', 'Ġincluding', 'Ġtwo', 'Ġn', 'asa', 'Ġexperiments', 'Ġone', 'Ġsample', 'Ġplate', 'Ġevaluating', 'Ġreaction', 'Ġselect', 'Ġmaterials', 'Ġconditions', 'Ġspace', 'Ġsecond', 'Ġstudies', 'Ġeffect', 'Ġambient', 'Ġspace', 'Ġradiation', 'Ġseeds', 'Ġthird', 'Ġexperiment', 'Ġdesigned', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġtransforms', 'Ġsolar', 'Ġpower', 'Ġradio', 'Ġfrequency', 'Ġmicrowave', 'Ġenergy', 'Ġstudies', 'Ġtransmitting', 'Ġenergy', 'Ġearth', 'Ġremains', 'Ġdepartment', 'Ġair', 'Ġforce', 'Ġasset', 'Ġnewly', 'Ġestablished', 'Ġu', 'Ġspace', 'Ġforce', 'Ġresponsible', 'Ġlaunch', 'orbit', 'Ġoperations', 'Ġlanding', 'uss', 'f', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġreleased', 'Ġsmall', 'Ġsatellite', 'Ġnamed', 'Ġfal', 'cons', 'usa', 'Ġaround', 'Ġmay', 'Ġdeveloped', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġacademy', 'Ġcad', 'ets', 'Ġpartnership', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'af', 'rl', 'Ġsmall', 'Ġsatellite', 'Ġcarries', 'Ġfive', 'Ġexperimental', 'Ġpayload', 'Ġspacecraft', 'Ġtest', 'Ġnovel', 'Ġelectromagnetic', 'Ġpropulsion', 'Ġsystem', 'Ġlow', 'weight', 'Ġantenna', 'Ġtechnology', 'Ġcommercial', 'Ġreaction', 'Ġwheel', 'Ġprovide', 'Ġattitude', 'Ġcontrol', 'Ġorbit', 'Ġaccording', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġacademy', 'Ġfal', 'cons', "'s", 'Ġexperiments', 'Ġinclude', ':[', 'Ġmagnet', 'og', 'rad', 'ient', 'Ġelectro', 'static', 'Ġplasma', 'Ġthr', 'uster', 'ep', 'Ġnovel', 'Ġelectromagnetic', 'Ġpropulsion', 'Ġsystem', 'Ġmet', 'aterial', 'Ġantenna', 'mma', 'Ġlow', 'Ġsize', 'Ġweight', 'Ġpower', 'Ġantenna', 'Ġphased', 'Ġarray', 'like', 'Ġperformance', 'Ġcarbon', 'Ġnan', 'ot', 'ube', 'Ġexperiment', 'oe', 'Ġc', 'abling', 'Ġcarbon', 'Ġnan', 'ot', 'ube', 'Ġbra', 'iding', 'Ġï', '¬', 'Ĥ', 'ex', 'ed', 'Ġusing', 'Ġshape', 'memory', 'Ġalloy', 'Ġattitude', 'Ġcontrol', 'Ġenergy', 'Ġstorage', 'aces', 'Ġcommercial', 'Ġreaction', 'Ġwheel', 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġï', '¬', 'Ĥ', 'wheel', 'Ġenergy', 'Ġstorage', 'Ġrelease', 'Ġsk', 'yp', 'ad']</t>
+          <t>['con', 'Ġsummer', 'Ġspace', 'Ġnews', 'Ġretrieved', 'Ġmarch', 'fal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġrev', 'Ġspace', 'x', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'space', 'x', "'s", 'Ġnew', 'Ġspin', 'Ġfal', 'con', 'Ġaviation', 'Ġweek', 'Ġaviation', 'Ġweek', 'Ġnetwork', 'Ġretrieved', 'Ġoct', 'ober', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'space', 'x', "'s", 'Ġshot', 'well', 'Ġtalks', 'Ġrapt', 'Ġfal', 'con', 'Ġsatellite', 'Ġinternet', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġp', 'enton', 'Ġretrieved', 'Ġmay', 'Ġab', 'bott', 'Ġj', 'ose', 'ph', 'Ġmay', 'space', 'x', "'s", 'Ġgrass', 'ho', 'pper', 'Ġleaping', 'Ġspac', 'eport', 'w', 'ac', 'Ġw', 'aco', 'Ġtrib', 'une', 'Ġretrieved', 'Ġapr', 'il', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġapr', 'il', 'space', 'x', 'Ġpreparing', 'Ġbusy', 'Ġseason', 'Ġmissions', 'Ġtest', 'Ġmilestones', 'Ġest', 'mil', 'estones', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġse', 'pt', 'ember', 'full', 'Ġthrust', 'Ġfal', 'con', 'Ġstage', 'Ġundergoing', 'Ġtesting', 'Ġmc', 'greg', 'h', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġse', 'pt', 'ember', 'fal', 'con', 'Ġupgrades', 'current', 'Ġvehicle', 'Ġupgrade', 'Ġspac', 'en', 'ews', 'Ġjournalist', 'Ġtwitter', 'Ġfeed', 'Ġspace', 'x', 'Ġslide', 'Ġrep', 'ublished', 'Ġtwitter', 'Ġretrieved', 'Ġjan', 'uary', 'Ġel', 'Ġmus', 'k', 'Ġtwitter', 'el', 'mus', 'k', 'Ġde', 'cember', 'Ġ"-', 'Ġcase', 'Ġdeep', 'Ġcry', 'Ġincreases', 'Ġdensity', 'Ġampl', 'ï', '¬', 'ģ', 'es', 'Ġrocket', 'Ġperformance', 'Ġfirst', 'Ġtime', 'Ġanyone', 'Ġgone', 'Ġlow', 'Ġchilled', 'f', 'Ġf', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'ses', 'Ġbetting', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġupgrade', 'Ġdebut', 'Ġapproaches', 'Ġspace', 'Ġnews', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġsv', 'ak', 'Ġamy', 'Ġmarch', 'fal', 'con', 'Ġperformance', 'Ġmid', 'size', 'Ġgeo', '?"', 'Ġaviation', 'Ġweek', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -2700,7 +2700,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>['lf', 'Ġcameras', 'Ġgp', 'us', 'Ġintegrated', 'Ġlow', 'sw', 'ap', 'size', 'Ġweight', 'Ġpower', 'Ġpackage', 'Ġmission', 'Ġcompleted', 'Ġvehicle', 'Ġlanding', 'Ġshuttle', 'Ġlanding', 'Ġfacility', 'mber', 'Ġfirst', 'Ġlaunched', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġfirst', 'Ġgo', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġinstead', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġapproach', 'Ġlanding', 'Ġtest', 'Ġvehicle', 'Ġinitial', 'Ġn', 'asa', 'Ġversion', 'Ġspacecraft', 'Ġused', 'Ġdrop', 'Ġglide', 'Ġtests', 'Ġmodified', 'Ġversion', 'Ġn', 'asa', 'Ġbuilt', 'Ġu', 'Ġair', 'Ġforce', 'Ġtwo', 'Ġbuilt', 'Ġused', 'Ġmultiple', 'Ġorbital', 'Ġmissions', 'uss', 'f', 'Ġvariants', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġthree', 'view', 'Ġplans', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġbo', 'e', 'ing', 'Ġannounced', 'Ġplans', 'Ġscaled', 'Ġvariant', 'Ġreferring', 'Ġspacecraft', 'Ġplanned', 'Ġsize', 'Ġallowing', 'Ġtransport', 'Ġastronauts', 'Ġinside', 'Ġpress', 'urized', 'Ġcompartment', 'Ġhoused', 'Ġcargo', 'Ġbay', 'las', 'Ġvariant', "'s", 'Ġproposed', 'Ġlaunch', 'Ġvehicle', 'Ġrole', 'Ġbo', 'e', 'ing', "'s", 'Ġcould', 'Ġpotentially', 'Ġcompete', 'Ġcorporation', "'s", 'Ġc', 'st', 'Ġstar', 'liner', 'Ġcommercial', 'Ġspace', 'Ġcapsule', 'Ġdata', 'Ġus', 'af', 'Ġbo', 'e', 'ing', 'Ġair', 'Ġspace', 'Ġmagazine', 'Ġphys', 'org', 'Ġgeneral', 'Ġcharacteristics', 'Ġcrew', 'Ġnone', 'Ġcapacity', 'Ġlength', 'Ġft', 'Ġwings', 'pan', 'Ġft', 'Ġheight', 'Ġft', 'Ġtakeoff', 'Ġweight', '000', 'Ġelectrical', 'Ġpower', 'Ġgall', 'ium', 'Ġarsen', 'ide', 'Ġsolar', 'Ġcells', 'Ġlithium', 'ion', 'Ġbatteries', 'Ġpayload', 'Ġbay', 'Ġft', ')[', 'Ġperformance', 'Ġorbital', 'Ġspeed', 'Ġmph', '044', 'Ġorbit', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġorbital', 'Ġtime', 'Ġdays', 'design', ')[', 'n', '08', 'Ġdays', 'demon', 'str', 'ated', ')[', 'Ġbo', 'e', 'ing', 'Ġdyn', 'ar', 'Ġu', 'Ġair', 'Ġforce', "'s", 'Ġoriginal', 'âĢĵ', 'Ġspace', 'plane', 'Ġprogram', 'Ġcancelled', 'Ġcraft']</t>
+          <t>['Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'el', 'Ġmus', 'k', 'Ġtwitter', 'Ġtwitter', 'Ġretrieved', 'Ġapr', 'il', 'Ġl', 'op', 'atto', 'Ġel', 'izabeth', 'Ġmarch', 'space', 'x', 'Ġeven', 'Ġlanded', 'Ġnose', 'Ġcone', 'Ġhistoric', 'Ġused', 'Ġfal', 'con', 'Ġrocket', 'Ġlaunch', 'Ġverge', 'Ġretrieved', 'Ġapr', 'il', 'el', 'mus', 'k', 'Ġj', 'une', 'flying', 'Ġlarger', 'Ġsign', 'ï', '¬', 'ģ', 'c', 'antly', 'Ġupgraded', 'Ġhyp', 'erson', 'ic', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġsingle', 'Ġpiece', 'Ġcast', 'Ġcut', 'Ġtitanium', 'Ġtake', 'entry', 'Ġheat', 'Ġshielding', 'weet', 'Ġretrieved', 'Ġapr', 'il', 'Ġvia', 'Ġtwitter', 'el', 'mus', 'k', 'Ġj', 'une', 'new', 'Ġtitanium', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġworked', 'Ġeven', 'Ġbetter', 'Ġexpected', 'Ġcapable', 'Ġind', 'e', 'ï', '¬', 'ģ', 'n', 'ite', 'Ġnumber', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġservice', 'weet', 'Ġretrieved', 'Ġapr', 'il', 'Ġvia', 'Ġtwitter', 'th', 'Ġsw', 'Ġsupports', 'Ġsuccessful', 'Ġfal', 'con', 'Ġe', 'ch', 'ost', 'ar', 'Ġlaunch', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġmarch', 'air', 'Ġforce', 'Ġreveals', 'Ġplan', 'Ġlaunches', 'Ġper', 'Ġyear', 'Ġcape', 'aver', 'al', 'Ġape', 'Ġretrieved', 'Ġapr', 'il', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġj', 'une', 'space', 'x', "'s", 'Ġfinal', 'Ġfal', 'con', 'Ġdesign', 'Ġcoming', 'Ġyear', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġspace', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġfal', 'con', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġaug', 'ust', 'home', 'Ġforums', 'Ġsign', 'Ġiss', 'Ġcommercial', 'Ġshuttle', 'Ġsl', 'ion', 'Ġr', 'ussian', 'Ġeuro', 'pe', 'Ġch', 'inese', 'Ġunmanned', 'Ġfal', 'con', 'Ġblock', 'Ġdebut', 'Ġsuccess', 'Ġdragon', 'Ġarrives', 'Ġstation', 'Ġber', 'thing', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlaunches', 'Ġcr', 'Ġdragon', 'Ġmission', 'Ġiss', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il']</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>['Ġconstructed', 'Ġdream', 'Ġch', 'aser', 'Ġlifting', 'body', 'Ġspace', 'plane', 'Ġdeveloped', 'ierra', 'Ġne', 'v', 'ada', 'Ġcorporation', 'Ġorbital', 'Ġsciences', 'Ġproposed', 'Ġunc', 'rew', 'ed', 'Ġsub', 'orb', 'ital', 'Ġreusable', 'rocket', 'Ġtechnology', 'Ġtest', 'bed', 'Ġtechnology', 'Ġdemonstration', 'Ġprogramme', 'Ġind', 'ian', 'Ġreusable', 'Ġspace', 'plane', 'Ġdevelopment', 'Ġproject', 'mes', 'space', 'craft', 'Ġproposed', 'Ġes', 'Ġspacecraft', 'Ġdesign', 'Ġhope', 'x', 'Ġsimilar', 'sized', 'Ġvehicle', 'Ġcomparable', 'Ġrole', 'Ġj', 'ax', 'c', 'ance', 'lled', 'Ġhy', 'flex', 'Ġj', 'apan', 'ese', 'Ġlifting', 'Ġbody', 'Ġspace', 'plane', 'Ġprecursor', 'Ġhope', 'x', 'Ġintermediate', 'Ġexperimental', 'Ġvehicle', 'Ġes', 'Ġdesigned', 'Ġexperimental', 'entry', 'Ġvehicle', 'n', 'long', 'space', 'craft', 'Ġch', 'inese', 'Ġreusable', 'Ġrobotic', 'Ġspace', 'plane', 'Ġdevelopment', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtested', 'sub', 'orb', 'ital', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġch', 'inese', 'Ġreusable', 'Ġexperimental', 'Ġspacecraft', 'Ġch', 'inese', 'Ġreusable', 'Ġspacecraft', 'Ġsk', 'ylon', 'space', 'craft', 'Ġb', 'rit', 'ish', 'Ġreusable', 'Ġunc', 'rew', 'ed', 'Ġspace', 'plane', 'Ġdevelopment', 'Ġspace', 'Ġrider', 'Ġplanned', 'Ġrobotic', 'Ġspace', 'plane', 'Ġfollow', 'Ġes', 'Ġspecifications', 'Ġsee', 'Ġalso', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġlist', 'Ġus', 'Ġsatellites', 'Ġlist', 'Ġx', 'planes', 'Ġcoll', 'ier', 'Ġtrophy', 'Ġsource', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġmission', 'Ġmarkings', 'Ġposted', 'Ġside', 'Ġwhite', 'Ġknight', 'Ġaircraft', 'Ġï', '¬', 'ģ', 'g', 'ure', 'Ġbased', 'Ġpre', 'launch', 'Ġdesign', 'Ġestimates', 'ï', '¬', 'Ĥ', 'ect', 'Ġspacecraft', "'s", 'Ġactual', 'Ġperformance', 'Ġcapacity', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġaug', 'ust', 'pent', 'agon', 'Ġplans', 'Ġkeep', 'Ġspace', 'plane', 'Ġair', 'Ġforce', 'Ġmanagement', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġe', 'ment', 'Ġoriginal', 'Ġmarch', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġconcludes', 'Ġsixth', 'Ġsuccessful', 'Ġmission', 'press', 'Ġrelease', 'Ġu', 'Ġspace', 'Ġforce', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'mber', 'Ġtechnology', 'Ġdemonstr', 'ator', 'Ġblazing', 'Ġtrail', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtransportation', 'Ġsystems', 'Ġn', 'asa', 'Ġfacts', 'Ġn', 'asa', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'air', 'Ġforce', 'Ġbloggers', 'Ġround', 'table', 'Ġair', 'Ġforce', 'Ġset', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġapr', 'il', 'Ġarchived']</t>
+          <t>['mus', 'k', 'Ġpreviews', 'Ġbusy', 'Ġyear', 'Ġahead', 'Ġspace', 'x', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġholds', 'Ġpre', 'launch', 'Ġb', 'rie', 'ï', '¬', 'ģ', 'ng', 'Ġhistoric', 'Ġpad', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġyoutube', 'f', 'iche', 'Ġtechnique', 'Ġfal', 'con', 'technical', 'Ġdata', 'Ġsheet', 'Ġfal', 'con', '].', 'Ġes', 'pace', 'Ġexploration', 'Ġfrench', 'Ġmay', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġusers', 'Ġguide', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġlight', 'Ġmetals', 'Ġhelp', 'Ġspace', 'x', 'Ġland', 'Ġfal', 'con', 'Ġrockets', 'Ġastonishing', 'Ġaccuracy', 'li', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'Ġshot', 'well', 'Ġmarch', 'Ġbroadcast', 'Ġspecial', 'Ġedition', 'Ġinterview', 'Ġshot', 'well', 'audio', 'Ġï', '¬', 'ģ', 'le', 'Ġspace', 'Ġshow', 'Ġevent', 'Ġoccurs', 'Ġ08', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'license', 'Ġorder', '090', 'Ġrev', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġgra', 'ham', 'iam', 'Ġde', 'cember', 'space', 'x', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġnails', 'Ġhistoric', 'Ġcore', 'Ġreturn', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġde', 'cember', 'Ġgr', 'uss', 'ike', 'Ġjan', 'uary', 'fal', 'con', 'Ġupgrade', 'Ġgets', 'Ġair', 'Ġforce', 'Ġlaunch', 'Ġmilitary', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'Ġshot', 'well', 'Ġfe', 'b', 'ruary', 'Ġshot', 'well', 'Ġcomments', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġconference', 'Ġcommercial', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġevent', 'Ġoccurs', 'âĢĵ', '05', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmarch', 'space', 'x', 'Ġsays', 'Ġfal', 'con', 'Ġupgrade', "'t", 'Ġrequire', 'Ġnew', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġspace', 'Ġnews']</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'air', 'Ġforce', 'Ġspace', 'plane', 'Ġodd', 'Ġbird', 'Ġtwisted', 'Ġpast', 'http', 'sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'n', 'asa', 'Ġbo', 'e', 'ing', 'Ġenter', 'Ġcooperative', 'Ġagreement', 'Ġdevelop', 'Ġfly', 'Ġtechnology', 'Ġdemonstr', 'ator', 'htt', 'press', 'Ġrelease', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġpress', 'Ġrelease', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġyen', 'ne', 'Ġp', 'Ġber', 'ger', 'Ġb', 'rian', 'Ġse', 'pt', 'ember', 'n', 'asa', 'Ġtransfers', 'Ġproject', 'arp', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġber', 'ger', 'Ġb', 'rian', 'Ġse', 'pt', 'ember', 'arp', 'Ġtakes', 'Ġspace', 'Ġplane', 'Ġproject', 'Ġnews', 'Ġarchived', 'id', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġexplanatory', 'Ġnotes', 'Ġreferences', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġdavid', 'Ġle', 'ard', 'Ġj', 'une', 'white', 'Ġknight', 'Ġcarries', 'Ġal', 'oft', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġpars', 'ch', 'n', 'ovember', 'bo', 'e', 'ing', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġaug', 'ust', 'mo', 'j', 'ave', 'Ġweb', 'Ġlog', 'Ġentries', 'Ġmo', 'j', 'ave', 'blog', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġoct', 'ober', 'Ġdavid', 'Ġle', 'ard', 'Ġapr', 'il', 'Ġflies', 'Ġmo', 'j', 'ave', 'Ġencounters', 'Ġlanding', 'Ġproblems', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'Ġtest', 'Ġflight', 'Ġb', 'roll', 'Ġaudio', ')"', 'Ġyoutube', 'Ġu', 'Ġair', 'Ġforce', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj']</t>
+          <t>['Ġretrieved', 'Ġmay', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'fal', 'con', 'Ġupgrade', 'Ġreceives', 'Ġblessing', 'Ġu', 'Ġair', 'Ġforce', 'htt', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġjan', 'uary', 'graded', 'Ġfal', 'con', 'Ġfirst', 'stage', 'Ġstatic', 'Ġfire', 'Ġu', 'eu', 'Ġyoutube', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġse', 'pt', 'ember', 'first', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġcompleted', 'Ġupgraded', 'Ġfal', 'con', 'http', 'sp', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'ses', 'Ġsigns', 'Ġlaunch', 'Ġpowerful', 'Ġfal', 'con', 'Ġengines', 'Ġn', 'eng', 'ines', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġmay', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġoct', 'ober', 'space', 'x', 'Ġselects', 'Ġmission', 'Ġfal', 'con', 'Ġreturn', 'Ġflight', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġoct', 'ober', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġlaunch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmal', 'ik', 'ari', 'q', 'Ġse', 'pt', 'ember', 'launch', 'pad', 'Ġexplosion', 'Ġdestroys', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġrocket', 'Ġsatellite', 'Ġfl', 'ida', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġse', 'pt', 'ember', 'omaly', 'Ġupdates', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġwik', 'ipedia', 'space', 'x', 'Ġseeks', 'Ġaccelerate', 'Ġfal', 'con', 'Ġproduction', 'Ġlaunch', 'Ġrates', 'Ġyear', 'Ġspac', 'en', 'ews', 'h', 'Ġspac', 'en', 'ews', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'n', 'asa', 'Ġsigns', 'Ġhistoric', 'Ġlaunch', 'Ġpad', 'Ġspace', 'x', 'Ġcollect', 'space', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġj', 'uly', 'pad', 'Ġspace', 'x', 'Ġlaying', 'Ġgroundwork', 'Ġfal', 'con', 'Ġheavy', 'Ġdebut', 'h', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġapr', 'il']</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -2739,7 +2739,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>['une', 'Ġretrieved', 'mber', 'Ġdavid', 'Ġle', 'ard', 'mber', 'u', 'Ġair', 'Ġforce', 'Ġpushes', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'http', 'sp', 'ac', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'las', 'Ġrocket', 'Ġdelivers', 'Ġair', 'Ġforce', 'Ġspace', 'plane', 'Ġorbit', 'http', 'space', 'ï', '¬', 'Ĥ', 'ight', 'n', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġfe', 'b', 'ruary', 'air', 'Ġforce', 'Ġspace', 'plane', 'Ġarrives', 'Ġfl', 'ida', 'Ġlaunch', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġcov', 'ault', 'Ġcra', 'ig', 'Ġaug', 'ust', 'us', 'af', 'Ġlaunch', 'Ġfirst', 'Ġspace', 'plane', 'Ġdemonstr', 'ator', 'web', 'arch', 'iv', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġh', 'annel', 'aw', 'st', 'Ġaug', 'ust', 'ris', 'Ġde', 'cember', 'second', 'Ġprepared', 'Ġlaunch', 'Ġaviation', 'Ġweek', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmarch', 'air', 'Ġforce', "'s", 'Ġsecond', 'Ġrobotic', 'Ġspace', 'Ġshuttle', 'Ġcircling', 'Ġearth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġdean', 'Ġj', 'ames', 'Ġoct', 'ober', 'n', 'asa', 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġuse', 'Ġshuttle', 'Ġhang', 'ars', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġoct', 'ober', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'fact', 'Ġsheet', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġsm', 'ith', 'str', 'ick', 'land', 'Ġk', 'iona', 'Ġmay', 'Ġknow', 'Ġleast', 'Ġtwo', 'Ġpayload', 'Ġair', 'Ġspace']</t>
+          <t>['space', 'x', 'Ġbreaks', 'Ġground', 'Ġb', 'oca', 'Ġch', 'ica', 'Ġbeach', 'Ġl', 'Ġbrown', 'ville', 'Ġherald', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'tex', 'Ġfl', 'ida', 'Ġbattle', 'Ġspace', 'x', 'Ġspac', 'eport', 'Ġpar', 'abolic', 'Ġarc', 'Ġretrieved', 'mber', 'Ġdean', 'Ġj', 'ames', 'Ġmay', 'Ġstates', 'Ġv', 'ie', 'Ġspace', 'x', "'s", 'Ġcommercial', 'Ġrocket', 'Ġlaunches', 'Ġus', 'Ġtoday', 'Ġretrieved', 'Ġapr', 'il', 'aven', 'port', 'Ġchrist', 'ian', 'Ġde', 'cember', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġpulls', 'Ġdramatic', 'Ġhistoric', 'Ġlanding', 'Ġwashing', 'ton', 'Ġpost', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġdemol', 'ishes', 'Ġtitan', 'Ġpad', 'Ġyoutube', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'sa', 'ocom', 'Ġmission', 'Ġspace', 'x', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'el', 'mus', 'k', 'Ġjan', 'uary', 'aim', 'ing', 'Ġlaunch', 'Ġweekend', 'hop', 'efully', 'Ġland', 'Ġdrones', 'hip', 'Ġship', 'Ġland', 'ings', 'Ġneeded', 'Ġhigh', 'Ġvelocity', 'Ġmissions', 'weet', 'Ġvia', 'Ġtwitter', 'el', 'mus', 'k', 'Ġjan', 'uary', 'Ġspeed', 'Ġstage', 'Ġseparation', 'Ġship', 'Ġneed', 'Ġzero', 'Ġlateral', 'Ġvelocity', 'Ġstage', '000', '01', 'weet', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġel', 'Ġmus', 'k', 'Ġshares', 'Ġphoto', 'Ġdrone', 'Ġship', 'Ġenables', 'Ġmissions', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -2752,7 +2752,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>['smith', 'sonian', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġbur', 'gh', 'ard', 'Ġtom', 'Ġmay', 'Ġmilitar', 'ization', 'Ġouter', 'Ġspace', 'Ġpent', 'agon', "'s", 'Ġspace', 'Ġwarriors', 'ht', 'Ġspace', 'Ġdaily', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġp', 'arn', 'ell', 'Ġbrid', 'aine', 'Ġjan', 'uary', 'us', 'space', 'Ġwar', 'plane', 'Ġmay', 'Ġspying', 'Ġch', 'inese', 'Ġspac', 'el', 'ab', 'http', 'Ġregister', 'Ġarchived', 'web', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcor', 'oc', 'oto', 'Ġgen', 'al', 'yn', 'Ġjan', 'uary', 'ex', 'pert', 'Ġu', 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġlikely', 'sp', 'ying', 'Ġch', 'ina', 'Ġmodule', 'Ġinternational', 'Ġbusiness', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'uh', 'Ġal', 'Ġoct', 'ober', 'Ġsecret', 'Ġspace', 'Ġplane', "'s", 'Ġmission', 'Ġremains', 'Ġmystery', 'Ġoutside', 'Ġus', 'Ġmilitary', 'Ġguardian', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġr', 'uss', 'ary', 'ann', 'mber', 'space', 'Ġrace', 'Ġrevealed', 'Ġus', 'Ġch', 'ina', 'Ġtest', 'Ġfuturistic', 'Ġem', 'drive', 'iang', 'ong', 'Ġmysterious', 'Ġplane', 'Ġinternational', 'Ġbusiness', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġsh', 'aw', 'yer', 'Ġro', 'ger', 'n', 'ovember', 'âĢĵ', 'de', 'cember', 'second', 'Ġgeneration', 'Ġem', 'drive', 'Ġpropulsion', 'Ġapplied', 'st', 'Ġlauncher', 'Ġinterstellar', 'Ġprobe', 'Ġact', 'Ġastronaut', 'ica', 'âĢĵ', '07', '002', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġdepartment', 'Ġtrade', 'Ġindustry', 'bo', 'e', 'ing', 'Ġend', 'Ġuser', 'Ġundertaking', 'Ġretrieved', 'Ġde', 'cember', 'Ġh', 'ambling', 'Ġdavid', 'mber', 'pro', 'pell', 'ent', 'less', 'Ġspace', 'Ġpropulsion', 'Ġresearch', 'Ġcontinues', 'http', 'av', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġretrieved', 'Ġde', 'cember', 'Ġray', 'Ġapr', 'il', 'Ġlaunch', 'Ġdate', 'Ġï', '¬', 'ģ', 'r', 'ms', 'Ġnew', 'Ġdetails', 'Ġemerge', 'Ġexperiment', 'htt', 'Ġn', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived']</t>
+          <t>['Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlaunch', 'Ġfunction', 'Ġpartially', 'Ġreusable', 'Ġheav', 'yl', 'ift', 'Ġsuper', 'Ġheavy', 'âĢĳ', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġreusable', 'Ġmillion', ')[', 'Ġexpend', 'able', 'Ġus', 'Ġmillion', ')[', 'Ġsize', 'Ġheight', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġheavy', 'Ġpartially', 'Ġreusable', 'Ġsuper', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcarry', 'Ġcargo', 'Ġearth', 'Ġorbit', 'Ġbeyond', 'Ġdesigned', 'Ġmanufactured', 'Ġlaunched', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġspace', 'x', 'Ġrocket', 'Ġconsists', 'Ġcenter', 'Ġcore', 'Ġtwo', 'Ġfal', 'con', 'Ġboosters', 'Ġattached', 'Ġsecond', 'Ġstage', 'Ġtop', 'Ġcenter', 'Ġcore', 'Ġfal', 'con', 'Ġheavy', 'Ġsecond', 'Ġhighest', 'Ġpayload', 'Ġcapacity', 'Ġcurrently', 'Ġoperational', 'Ġlaunch', 'Ġvehicle', 'Ġbehind', 'Ġn', 'asa', "'s", 'Ġspace', 'Ġlaunch', 'Ġsystem', 'sl', 'Ġfourth', 'highest', 'Ġcapacity', 'Ġrocket', 'Ġreach', 'Ġorbit', 'Ġtrailing', 'Ġbehind', 'Ġsl', 'Ġenerg', 'ia', 'Ġsat', 'urn', 'Ġv', 'Ġspace', 'x', 'Ġconducted', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġmaiden', 'Ġlaunch', 'Ġfe', 'b', 'ruary', 'Ġdummy', 'Ġpayload', 'Ġrocket', 'Ġcarried', 'es', 'la', 'Ġroad', 'ster', 'Ġbelonging', 'Ġspace', 'x', 'Ġfounder', 'Ġel', 'Ġmus', 'k', 'Ġman', 'ne', 'quin', 'Ġdubbed', 'star', 'man', 'Ġdriver', "'s", 'Ġsecond', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġoccurred', 'Ġapr', 'il', 'Ġthree', 'Ġbooster', 'Ġrockets', 'Ġsuccessfully', 'Ġreturned', 'Ġearth', 'Ġthird', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġsuccessfully', 'Ġoccurred', 'Ġj', 'une', 'Ġsince', 'Ġfal', 'con', 'Ġheavy', 'Ġcertified', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'n', 'ssl', 'Ġprogram', 'Ġfal', 'con', 'Ġheavy', 'Ġdesigned', 'Ġable', 'Ġcarry', 'Ġhumans', 'Ġspace', 'Ġbeyond', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġalthough', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġintend', 'Ġtransport', 'Ġpeople', 'Ġfal', 'con', 'Ġheavy', 'Ġpursue', 'Ġhuman', 'rating', 'Ġcertification', 'Ġprocess', 'Ġtransport', 'Ġn', 'asa', 'Ġastronauts', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġexpected', 'Ġeventually', 'Ġsupers', 'eded', 'Ġstarship', 'Ġlaunch', 'Ġsystem', 'Ġcurrently', 'Ġdeveloped', 'Ġconcepts', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġusing', 'Ġthree', 'Ġfal', 'con', 'Ġcore', 'Ġboosters', 'Ġapproximate', 'Ġpayload', 'le', 'Ġcapacity', 'Ġtwo', 'Ġtons', 'Ġinitially', 'Ġdiscussed', 'Ġearly', 'Ġconcept', 'Ġthree', 'Ġcore', 'Ġbooster', 'Ġstages', 'Ġcompany', "'s"]</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġpaw', 'ly', 'k', 'Ġori', 'ana', 'Ġj', 'uly', 'former', 'Ġsec', 'af', 'Ġexplains', 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġthrows', 'Ġenemies', 'Ġmilitary', 'Ġarchived', 'Ġow', 'en', 'emies', 'html', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġz', 'hen', 'Ġoct', 'ober', 'Ġus', 'Ġspace', 'Ġplane', 'Ġmark', 'Ġstart', 'Ġnew', 'Ġmilitary', 'Ġfrontier', '?"', 'front', 'ier', 'Ġsouth', 'Ġch', 'ina', 'Ġmorning', 'Ġpost', 'Ġarchived', 'front', 'ier', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'space', 'ï', '¬', 'Ĥ', 'ight', 'las', 'Ġlaunch', 'Ġreport', 'las', 'Ġrocket', 'Ġdelivers', 'Ġair', 'Ġforce', 'Ġspace', 'plane', 'Ġorbit', 'sp', "'s", 'Ġknow', 'Ġshadowy', 'Ġrecord', 'Ġdays', 'Ġspace', 'Ġoct', 'ober', 'Ġmill', 'er', 'Ġp', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġj', 'une', 'space', 'x', 'Ġscores', 'Ġcontract', 'Ġlaunch', 'Ġair', 'Ġforce', "'s", 'Ġsecretive', 'Ġspace', 'plane', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'mother', 'ship', 'Ġadop', 'ts', 'Ġnew', 'Ġspace', 'Ġplane', 'Ġ00', 'Ġnews', 'Ġarchived', 'id', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġdemonstr', 'ator', 'Ġtest', 'Ġfuture', 'Ġlaunch', 'Ġtechnologies', 'Ġorbit', 'entry', 'Ġenvironments', 'Ġn', 'asa', 'Ġmay', 'Ġfs', '05', 'ms', 'fc', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġaust', 'ap', 'ril', 'Ġspace', 'Ġvehicle', 'Ġstarting', 'Ġnew', 'Ġage', 'Ġspace', 'Ġcontrol', 'http', 'app', 'report', 'Ġdefense', 'Ġtechnical', 'Ġinformation', 'Ġcenter', 'Ġad', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġg', 'ary', 'Ġpay', 'ton', 'Ġsecretary', 'Ġair', 'Ġforce', 'Ġspace', 'Ġprograms', 'Ġmedia']</t>
+          <t>['yet', 'un', 'fl', 'Ġfal', 'con', 'Ġreferred', 'Ġfal', 'con', 'Ġheavy', 'Ġhistory', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdiameter', 'Ġft', 'Ġbooster', 'Ġwidth', 'Ġft', 'Ġmass', '000', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', '000', 'Ġpayload', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', '000', 'Ġpayload', 'Ġmars', 'Ġtransfer', 'Ġorbit', 'Ġmass', '000', 'Ġpayload', 'Ġpl', 'uto', 'Ġmass', 'Ġassociated', 'Ġrockets', 'Ġbased', 'Ġfal', 'con', 'Ġcomparable', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġnew', 'Ġgl', 'enn', 'Ġsat', 'urn', 'Ġspace', 'Ġlaunch', 'Ġsystem', 'Ġvul', 'Ġcent', 'aur', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġv', 'enberg', 'future', 'Ġtotal', 'Ġlaunches', 'Ġsuccess', 'es', 'Ġland', 'ings', 'Ġcenter', 'Ġcore', 'Ġlanded', 'lost', 'Ġsea', 'Ġattempted', 'Ġside', 'Ġboosters', 'Ġlanded', 'Ġattempted', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġbreaking', 'Ġground', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġpad', 'Ġspace', 'x', 'Ġunveiled', 'Ġplan', 'Ġfal', 'con', 'Ġheavy', 'Ġpublic', 'Ġwashing', 'ton', 'Ġnews', 'Ġconference', 'Ġapr', 'il', 'Ġinitial', 'Ġtest', 'Ġflight', 'Ġexpected', 'Ġnumber', 'Ġfactors', 'Ġdelayed', 'Ġplanned', 'Ġmaiden', 'Ġflight', 'Ġincluding', 'Ġtwo', 'Ġanomalies', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicles', 'Ġrequired', 'Ġengineering', 'Ġresources', 'Ġdedicated', 'Ġfailure', 'Ġanalysis', 'Ġhalting', 'Ġflight', 'Ġoperations', 'Ġmany', 'Ġmonths', 'Ġintegration', 'Ġstructural', 'Ġchallenges', 'Ġcombining', 'Ġthree', 'Ġfal', 'con', 'Ġcores', 'Ġmuch', 'Ġdifficult', 'Ġexpected', 'Ġj', 'uly', 'Ġel', 'Ġmus', 'k', 'Ġsaid', 'Ġactually', 'Ġended', 'Ġway', 'Ġharder', 'Ġfal', 'con', 'Ġheavy', 'Ġthought', 'Ġ...', 'Ġpretty', 'Ġnaive', '".[', 'Ġinitial', 'Ġtest', 'Ġflight', 'Ġfirst', 'Ġfal', 'con', 'Ġheavy', 'Ġlifted', 'Ġfe', 'b', 'ruary', 'Ġut', 'c', 'Ġcarrying', 'Ġdummy', 'Ġpayload', 'Ġel', 'Ġmus', 'k', "'s", 'Ġpersonal', 'es', 'la', 'Ġroad', 'ster', 'Ġbeyond', 'Ġmars', 'Ġmus', 'k', 'Ġfirst', 'Ġmentioned', 'Ġfal', 'con', 'Ġheavy', 'Ġse', 'pt', 'ember', 'Ġnews', 'Ġupdate', 'Ġreferring', 'Ġcustomer', 'Ġrequest', 'Ġmonths', 'Ġprior', 'Ġvarious', 'Ġsolutions', 'Ġusing', 'Ġplanned', 'Ġfal', 'con']</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>['Ġtele', 'conference', 'pent', 'agon', 'Ġlaunch', 'Ġdefense', 'gov', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'htt', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'Ġapr', 'il', 'bo', 'e', 'ing', "'s", 'Ġnew', 'Ġcrew', 'carry', 'ing', 'Ġspaceship', 'Ġtaking', 'Ġshape', 'http', 'sp', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'p', 'ilot', 'less', 'Ġus', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġdays', 'Ġorbit', 'Ġspace', 'Ġdaily', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'erson', 'iam', 'Ġe', '.;', 'ler', 'Ġk', 'athy', 'Ġcro', 'ck', 'et', 'ave', 'Ġle', 'w', 'Ġtim', 'Ġcur', 'tis', 'Ġper', 'oxide', 'Ġpropulsion', 'Ġturn', 'Ġcentury', 'th', 'Ġinternational', 'Ġsym', 'posium', 'Ġliquid', 'Ġspace', 'Ġpropulsion', 'Ġmarch', 'il', 'b', 'ron', 'n', 'Ġg', 'erman', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'uly', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'bert', 'Ġbart', 'Ġj', 'uly', 'per', 'oxide', 'Ġtest', 'Ġprograms', 'Ġflight', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'web', 'p', 'Ġn', 'asa', 'Ġengineering', 'Ġtest', 'Ġdirector', 'ate', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġsm', 'ith', 'str', 'ick', 'land', 'Ġk', 'iona', 'f', 'eb', 'ruary', "'s", '?"', 'Ġair', 'Ġspace', 'smith', 'sonian', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcher', 'ok', 'Ġb', 'oris', 'Ġe', 'ed', '.).', 'Ġrockets', 'Ġpeople', 'Ġ', 'ÑĢ', 'Ð°', 'Ðº', 'Ðµ', 'ÑĤ', 'Ñĭ', 'ĠÐ', '»', 'Ñ', 'İ', 'Ð´', 'Ð¸', 'Ġn', 'asa', 'Ġhistory', 'Ġseries', 'Ġvol', 'Ġn', 'asa', 'Ġp', 'Ġsp', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'Ġway', 'ne', 'Ġh', 'ale', 'Ġoral', 'Ġhistory', 'Ġn', 'asa', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une']</t>
+          <t>['Ġnever', 'Ġflown', 'Ġexplored', 'Ġcost', 'effective', 'Ġreliable', 'Ġiteration', 'Ġone', 'Ġused', 'engine', 'Ġfirst', 'Ġstage', 'âĢĶ', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġdeveloped', 'Ġprivate', 'Ġcapital', 'Ġmus', 'k', 'Ġstating', 'Ġcost', 'Ġus', 'Ġmillion', 'Ġgovernment', 'Ġfinancing', 'Ġprovided', 'Ġdevelopment', 'Ġfal', 'con', 'Ġheavy', 'Ġdesign', 'Ġbased', 'Ġfal', 'con', 'Ġfu', 'selage', 'Ġengines', 'Ġspace', 'x', 'Ġaiming', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'fal', 'con', 'Ġheavy', 'Ġwould', 'Ġcouple', 'Ġyears', '".', 'Ġspeaking', 'Ġmars', 'Ġsociety', 'Ġconference', 'Ġmus', 'k', 'Ġalso', 'Ġindicated', 'Ġexpected', 'Ġhydrogen', 'fuel', 'ed', 'Ġupper', 'Ġstage', 'Ġwould', 'Ġfollow', 'Ġtwo', 'Ġthree', 'Ġyears', 'Ġlater', 'Ġwould', 'Ġaround', ').[', 'Ġconception', 'Ġfunding', 'Ġdesign', 'Ġdevelopment', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġoct', 'ober', 'Ġboosters', 'Ġboosters', 'Ġpowered', 'Ġtotal', 'Ġmer', 'lin', 'Ġper', 'Ġbooster', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', '000', 'Ġvacuum', '000', 'Ġtotal', 'Ġthrust', 'Ġsea', 'Ġlevel', '000', 'Ġvacuum', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '05', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġchilled', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', '000', 'Ġvacuum', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '05', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġchilled', 'Ġsecond', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġleft', 'Ġright', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġthree', 'Ġversions', 'Ġfal', 'con', 'Ġthree', 'Ġversions', 'Ġfal', 'con', 'full', 'Ġthrust', 'Ġthree', 'Ġversions', 'Ġfal', 'con', 'Ġblock', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġheavy', 'Ġblock', 'Ġapr', 'il', 'Ġcapabilities', 'Ġperformance', 'Ġfal', 'con', 'Ġvehicle', 'Ġbetter', 'Ġunderstood', 'Ġspace', 'x', 'Ġcompleted', 'Ġtwo', 'Ġsuccessful', 'Ġdemonstration', 'Ġmissions', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġone', 'Ġincluded', 'Ġreign', 'ition']</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -2791,7 +2791,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>['Ġalways', 'Ġconcern', 'Ġparticularly', 'Ġgot', 'Ġlonger', 'Ġlonger', 'Ġï', '¬', 'Ĥ', 'ights', "'s", 'Ġvest', 'ib', 'ular', 'Ġthings', 'Ġhappen', 'Ġvision', 'Ġchanges', 'Ġhappen', 'Ġpeople', 'Ġconcerned', 'Ġlanding', 'Ġwanted', 'Ġmake', 'Ġsure', 'Ġviable', 'Ġauto', 'land', 'Ġsystem', 'Ġprogram', 'Ġmanager', 'Ġgave', 'Ġus', 'Ġdirection', 'Ġtest', 'Ġsts', 'Ġworked', 'Ġhard', 'Ġdot', "'s", 'Ġcross', "'s", 'Ġcould', 'Ġauto', 'land', 'Ġtest', 'Ġauto', 'land', 'Ġtest', 'âĢĶ', "'re", 'Ġusing', 'Ġreal', 'Ġorbit', 'er', 'Ġlive', 'Ġcrew', "'ve", 'Ġgot', 'Ġkidding', 'Ġright', 'Ġmark', 'Ġcould', 'Ġreally', 'Ġbad', 'Ġ...', 'j', 'ed', 'j', 'ere', 'miah', 'Ġw', '.]', 'Ġpear', 'son', 'Ġassociate', 'Ġadministrator', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġformer', 'Ġmarine', 'Ġcorps', 'Ġgeneral', 'Ġrecall', 'Ġreviewed', 'Ġsaid', "'re", 'Ġgoing', 'Ġï', '¬', 'Ĥ', 'ying', 'Ġlong', 'duration', 'Ġï', '¬', 'Ĥ', 'ights', "'t", 'Ġneed', "'re", 'Ġgoing', 'Ġknock', '."', 'Ġdevastating', 'Ġteam', 'Ġset', 'Ġready', 'Ġexcited', 'Ġthought', 'Ġwould', 'Ġgood', 'Ġcapability', '."', 'Ġhal', 'v', 'ors', 'Ġtodd', 'Ġde', 'cember', 'Ġmini', 'shut', 'tle', 'Ġshrouded', 'Ġsecrecy', 'Ġcre', 'cy', '09', 'Ġair', 'Ġforce', 'Ġtimes', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'inside', 'Ġus', 'Ġair', 'Ġforce', "'s", 'Ġnext', 'Ġspace', 'Ġplane', 'Ġmystery', 'Ġmission', 'ht', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'secret', 'Ġspace', 'Ġplane', 'Ġspotted', 'Ġamateur', 'Ġsky', 'wat', 'chers', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'ateur', 'Ġastronomers', 'Ġunravel']</t>
+          <t>['Ġsecond', 'stage', 'Ġengine', 'Ġpress', 'Ġconference', 'Ġnational', 'Ġpress', 'Ġclub', 'Ġwashing', 'ton', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġstated', 'Ġfal', 'con', 'Ġheavy', 'Ġwould', 'carry', 'Ġpayload', 'Ġorbit', 'Ġescape', 'Ġvelocity', 'Ġvehicle', 'Ġhistory', 'Ġapart', 'Ġsat', 'urn', 'Ġmoon', 'Ġrocket', 'Ġ...', 'v', 'iet', 'Ġenerg', 'ia', 'Ġrocket', '".[', 'Ġyear', 'Ġexpected', 'Ġincrease', 'Ġdemand', 'Ġvariants', 'Ġspace', 'x', 'Ġannounced', 'Ġplans', 'Ġexpand', 'Ġmanufacturing', 'Ġcapacity', 'Ġbuild', 'Ġtowards', 'Ġcapability', 'Ġproducing', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġfal', 'con', 'Ġheavy', 'Ġside', 'Ġbooster', 'Ġevery', 'Ġweek', 'Ġupper', 'Ġstage', 'Ġevery', 'Ġtwo', 'Ġspace', 'x', 'Ġannounced', 'Ġnumber', 'Ġchanges', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġworked', 'Ġparallel', 'Ġupgrade', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġreleased', 'Ġphoto', 'Ġshowing', 'Ġfal', 'con', 'Ġheavy', 'Ġinter', 'stage', 'Ġcompany', 'Ġheadquarters', 'Ġhaw', 'th', 'orne', 'Ġcal', 'ornia', 'Ġmay', 'Ġnew', 'Ġpartly', 'Ġunderground', 'Ġtest', 'Ġstand', 'Ġbuilt', 'Ġspace', 'x', 'Ġrocket', 'Ġdevelopment', 'Ġtest', 'Ġfacility', 'Ġmc', 'greg', 'Ġtex', 'Ġspecifically', 'Ġtest', 'Ġtriple', 'Ġcores', 'Ġtwenty', 'seven', 'Ġrocket', 'Ġengines', 'Ġfal', 'con', 'Ġheavy', 'Ġmay', 'Ġspace', 'x', 'Ġconducted', 'Ġfirst', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġflight', 'design', 'Ġfal', 'con', 'Ġheavy', 'Ġcenter', 'Ġcore', 'Ġmc', 'greg', 'Ġfacility', 'Ġj', 'uly', 'Ġmus', 'k', 'Ġdiscussed', 'Ġpublicly', 'Ġchallenges', 'Ġtesting', 'Ġcomplex', 'Ġlaunch', 'Ġvehicle', 'Ġlike', 'Ġthree', 'core', 'Ġfal', 'con', 'Ġheavy', 'Ġindicating', 'Ġlarge', 'Ġextent', 'Ġnew', 'Ġdesign', 'Ġreally', 'Ġimpossible', 'Ġtest', 'Ġground', 'Ġcould', 'Ġeffectively', 'Ġtested', 'Ġindependent', 'Ġactual', 'Ġflight', 'Ġtests', 'Ġtesting', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġmaiden', 'Ġlaunch', 'Ġfal', 'con', 'Ġheavy', 'Ġse', 'pt', 'ember', 'Ġthree', 'Ġfirst', 'Ġstage', 'Ġcores', 'Ġcompleted', 'Ġstatic', 'Ġfire', 'Ġtests', 'Ġground', 'Ġtest', 'Ġstand', 'Ġfirst', 'Ġfal', 'con', 'Ġheavy', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġconducted', 'Ġjan', 'uary', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġplanning', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'Ġheavy', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġcal', 'ornia', 'Ġunited', 'Ġstates', 'Ġwest', 'Ġcoast']</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>['Ġorbit', 'Ġsay', 'Ġlikely', 'Ġuse', 'Ġdeploying', 'Ġsatellites', 'http', 'new', 'Ġnews', 'au', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġbroad', 'iam', 'Ġj', 'Ġmay', 'sur', 'illance', 'Ġsuspected', 'Ġspacecraft', "'s", 'Ġmain', 'Ġrole', 'n', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'pre', 'par', 'ations', 'Ġunderway', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlanding', 'Ġu', 'Ġair', 'Ġforce', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'us', 'af', 'Ġlanding', 'Ġslated', 'Ġdec', 'âĢĵ', 'Ġaviation', 'Ġweek', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'home', 'Ġu', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġreturns', 'Ġearth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġwar', 'wic', 'j', 'Ġgra', 'ham', 'Ġde', 'cember', 'us', 'af', "'s", 'Ġspace', 'plane', 'Ġreturns', 'Ġearth', 'web', 'arch', 'Ġaviation', 'Ġweek', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġr', 'con', 'Ġp', 'aul', 'Ġde', 'cember', 'Ġus', 'Ġmilitary', 'Ġspace', 'plane', 'Ġreturns', 'Ġearth', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'cc', 'ants', 'ike', 'usa', 'Ġsatellite', 'Ġdetails', '010', 'ad', 'ell', 'ite', '/?', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġwall', 'ike', 'Ġmarch', 'secret', 'ive', 'Ġspace', 'Ġplane', 'Ġlaunches', 'Ġnew', 'Ġmystery', 'Ġmission', 'Ġspace', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'mber', 'military', 'Ġspace', 'Ġshuttle', 'Ġreceives', 'Ġmission', 'Ġextension', 'Ġspace', 'ï', '¬']</t>
+          <t>['Ġspace', 'x', 'Ġrefurb', 'ished', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġaccommodate', 'Ġfal', 'con', 'Ġheavy', 'Ġfirst', 'Ġlaunch', 'Ġcape', 'aver', 'al', 'Ġfl', 'ida', 'Ġeast', 'Ġcoast', 'Ġlaunch', 'Ġcomplex', 'Ġplanned', 'Ġlate', 'Ġdue', 'Ġpartly', 'Ġfailure', 'Ġspace', 'x', 'Ġj', 'une', 'Ġspace', 'x', 'Ġres', 'ched', 'uled', 'Ġmaiden', 'Ġfal', 'con', 'Ġheavy', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġoccur', 'Ġearlier', 'Ġapr', 'il', 'Ġflight', 'Ġlaunched', 'Ġrefurb', 'ished', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġlaunch', 'Ġcomplex', 'Ġflight', 'Ġpostponed', 'Ġlate', 'Ġearly', 'Ġsummer', 'Ġlate', 'Ġfinally', 'Ġfe', 'b', 'ruary', 'Ġj', 'uly', 'Ġmeeting', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġresearch', 'Ġdevelopment', 'Ġmeeting', 'Ġwashing', 'ton', 'Ġmus', 'k', 'played', 'Ġexpectations', 'Ġsuccess', 'Ġmaiden', 'Ġflight', "'s", 'Ġreal', 'Ġgood', 'Ġchance', 'Ġvehicle', "'t", 'Ġmake', 'Ġorbit', 'Ġ...', 'Ġhope', 'Ġmakes', 'Ġfar', 'Ġenough', 'Ġaway', 'Ġpad', 'Ġcause', 'Ġpad', 'Ġdamage', 'Ġwould', 'Ġconsider', 'Ġeven', 'Ġwin', 'Ġhonest', 'Ġde', 'cember', 'Ġmus', 'k', 'Ġtweeted', 'Ġdummy', 'Ġpayload', 'Ġmaiden', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġwould', 'Ġpersonal', 'es', 'la', 'Ġroad', 'ster', 'Ġplaying', 'Ġdavid', 'Ġbow', 'ie', "'s", 'space', 'Ġodd', 'ity', 'though', 'Ġsong', 'Ġactually', 'Ġused', 'Ġlaunch', 'life', 'Ġmars', '"),', 'Ġwould', 'Ġlaunched', 'Ġorbit', 'Ġaround', 'Ġsun', 'Ġreach', 'Ġorbit', 'Ġmars', 'Ġreleased', 'Ġpictures', 'Ġfollowing', 'Ġdays', 'Ġcar', 'Ġthree', 'Ġcameras', 'Ġattached', 'Ġprovide', 'ep', 'ic', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġheavy', 'Ġmoved', 'Ġlaunch', 'Ġpad', 'Ġpreparation', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġengines', 'Ġexpected', 'Ġjan', 'uary', 'Ġhowever', 'Ġdue', 'Ġu', 'Ġgovernment', 'Ġshutdown', 'Ġbegan', 'Ġjan', 'uary', 'Ġtesting', 'Ġlaunch', 'Ġdelayed', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġconducted', 'Ġjan', 'uary', 'Ġmus', 'k', 'Ġconfirmed', 'Ġvia', 'Ġtwitter', 'Ġtest', 'Ġgood', 'Ġlater', 'Ġannounced', 'Ġrocket', 'Ġwould', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġfe', 'b', 'ruary', 'Ġdelay', 'Ġtwo', 'Ġhours', 'Ġdue', 'Ġhigh', 'Ġwinds']</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -2817,7 +2817,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>['Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'air', 'Ġforce', "'s", 'Ġsecret', 'spect', 'acular', 'Ġsuccess', 'id', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'pre', 'par', 'ations', 'Ġunderway', 'Ġlanding', 'Ġu', 'Ġair', 'Ġforce', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġdavid', 'Ġle', 'ard', 'Ġmay', 'air', 'Ġforce', "'s", 'Ġsecretive', 'Ġspace', 'Ġplane', 'Ġland', 'Ġsoon', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġlands', 'Ġmorning', 'Ġv', 'enberg', 'Ġl', 'anta', 'Ġmar', 'ia', 'Ġtimes', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġwall', 'ike', 'Ġj', 'une', 'air', 'Ġforce', "'s", 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġcal', 'Ġmystery', 'Ġmission', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġray', 'Ġse', 'pt', 'ember', 'another', 'las', 'Ġread', 'ied', 'Ġlaunch', 'Ġmini', 'Ġspace', 'Ġshuttle', 'http', 'space', 'ï', '¬', 'Ĥ', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġoct', 'ober', 'cc', 'ull', 'ough', 'Ġamy', 'Ġoct', 'ober', 'Ġlaunch', 'Ġdelayed', 'Ġair', 'Ġforce', 'Ġmagazine', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġde', 'cember', 'kinson', 'Ġn', 'ancy', 'Ġde', 'cember', 'air', 'Ġforce', "'s", 'Ġsecret', 'Ġspace', 'Ġplane', 'Ġlaunches', 'Ġthird', 'Ġmission', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġdavid', 'Ġle', 'ard', 'mber', 'new', 'Ġdelay', 'Ġmysterious', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġlaunch', 'http', 'Ġspace', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'n', 'ss', 'dc', 'Ġid']</t>
+          <t>['Ġfal', 'con', 'Ġheavy', 'Ġlifted', 'Ġside', 'Ġboosters', 'Ġlanded', 'Ġsafely', 'Ġlanding', 'Ġzones', 'Ġminutes', 'Ġlater', 'Ġhowever', 'Ġone', 'Ġthree', 'Ġengines', 'Ġcenter', 'Ġbooster', 'Ġintended', 'Ġrestart', 'Ġignited', 'Ġdescent', 'Ġcausing', 'Ġbooster', 'Ġdestroyed', 'Ġupon', 'Ġimpacting', 'Ġocean', 'Ġspeed', 'Ġmph', ').[', 'Ġinitially', 'Ġel', 'Ġmus', 'k', 'Ġtweeted', 'Ġroad', 'ster', 'shot', 'Ġplanned', 'Ġhel', 'oc', 'entric', 'Ġorbit', 'Ġwould', 'Ġreach', 'Ġasteroid', 'Ġbelt', 'Ġlater', 'Ġobservations', 'Ġtelescopes', 'Ġshowed', 'Ġroad', 'ster', 'Ġwould', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġbuilt', 'Ġfal', 'con', 'Ġblock', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġlaunch', 'Ġpad', 'Ġj', 'une', 'Ġslightly', 'Ġexceed', 'Ġorbit', 'Ġmars', 'Ġap', 'hel', 'ion', 'Ġyear', 'Ġsuccessful', 'Ġdemo', 'Ġflight', 'Ġspace', 'x', 'Ġsigned', 'Ġfive', 'Ġcommercial', 'Ġcontracts', 'Ġworth', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġmeaning', 'Ġmanaged', 'Ġcover', 'Ġdevelopment', 'Ġcost', 'Ġrocket', 'Ġsecond', 'Ġflight', 'Ġfirst', 'Ġcommercial', 'Ġone', 'Ġoccurred', 'Ġapr', 'il', 'Ġlaunching', 'Ġar', 'abs', 'Ġthree', 'Ġboosters', 'Ġlanding', 'Ġsuccessfully', 'Ġfirst', 'Ġtime', 'Ġthird', 'Ġflight', 'Ġoccurred', 'Ġj', 'une', 'Ġlaunching', 'od', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġpayload', 'Ġpayload', 'Ġcomposed', 'Ġsmall', 'Ġspacecraft', 'Ġoperational', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġmissions', 'Ġint', 'els', 'ars', 'Ġplanned', 'Ġlate', 'Ġmoved', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġrocket', 'Ġversion', 'Ġbecome', 'Ġpowerful', 'Ġenough', 'Ġlift', 'Ġheavy', 'Ġpayload', 'Ġexpend', 'able', 'Ġj', 'une', 'Ġu', 'Ġspace', 'Ġforce', 'Ġcertified', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunching', 'Ġtop', 'Ġsecret', 'Ġsatellites', 'Ġfirst', 'Ġlaunch', 'Ġus', 'sf', 'Ġhappened', 'mber', 'Ġsecond', 'Ġus', 'sf', 'Ġlaunched', 'Ġweeks', 'Ġus', 'sf', 'Ġv', 'ias', 'Ġselected', 'Ġfal', 'con', 'Ġheavy', 'Ġlate', 'Ġlaunching', 'Ġv', 'ias', 'Ġsatellite', 'Ġscheduled', 'Ġlaunch', 'âĢĵ', 'Ġtimeframe', 'Ġhowever', 'Ġwould', 'Ġlaunch', 'Ġmay']</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>['07', 'Ġnational', 'Ġspace', 'Ġscience', 'Ġdata', 'Ġcenter', 'Ġn', 'asa', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbad', 'ger', 'Ġer', 'ic', 'Ġde', 'cember', 'air', 'Ġforce', 'Ġlaunches', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġu', 'Ġair', 'Ġforce', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġpars', 'ons', 'Ġdan', 'Ġoct', 'ober', 'us', 'Ġair', 'Ġforce', "'s", 'Ġshadowy', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġdays', 'Ġorbit', 'Ġn', '04', 'Ġflight', 'Ġglobal', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'secret', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġus', 'Ġair', 'Ġforce', 'Ġbase', 'Ġunknown', 'Ġtwo', 'year', 'Ġmission', 'Ġguardian', 'Ġassociated', 'Ġpress', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'Ġoct', 'ober', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġrecord', 'sh', 'attering', 'Ġsecret', 'Ġmission', 'Ġspace', 'Ġarchived', 'Ġe', 'land', 'ing', 'html', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġray', 'Ġmay', 'rec', 'ap', 'Ġstory', 'Ġspace', 'plane', 'Ġemb', 'arks', 'Ġfourth', 'Ġvoyage', 'Ġorbit', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', "'s", 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġhall', 'Ġthr', 'uster', 'Ġdemonstrates', 'Ġsuccessful', 'orbit', 'Ġoperation', 'htt', 'press', 'Ġrelease', 'ero', 'jet', 'Ġrocket', 'dy', 'ne', 'Ġj', 'uly', 'Ġarchived', 'web', 'arc', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'Ġmay', 'us', 'Ġair', 'Ġforce', 'Ġlaunches', 'Ġspace', 'Ġplane', 'th', 'Ġmystery', 'Ġmission', 'http', 'Ġspace', 'Ġarchived', 'Ġh', 'mission', 'html', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġray', 'Ġmay', 'Ġspace', 'plane', 'Ġreturns', 'Ġearth', 'Ġmakes', 'Ġautop', 'ilot', 'Ġlanding', 'Ġfl', 'ida', 'Ġlot', 'land', 'ing', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight']</t>
+          <t>['Ġoct', 'ober', 'Ġfal', 'con', 'Ġheavy', 'Ġembarked', 'th', 'Ġflight', 'Ġcarrying', 'Ġn', 'asa', 'Ġsatellite', 'Ġps', 'cy', 'Ġasteroid', 'Ġmission', 'Ġside', 'Ġboosters', 'Ġreturn', 'Ġearth', 'Ġcenter', 'Ġcore', 'Ġexpended', 'Ġdecision', 'Ġmade', 'Ġcreate', 'Ġtoler', 'able', 'Ġmargins', 'Ġmission', 'Ġfollowing', 'Ġannouncement', 'Ġn', 'asa', "'s", 'Ġart', 'emis', 'Ġprogram', 'Ġreturning', 'Ġhumans', 'Ġmoon', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġmentioned', 'Ġseveral', 'Ġtimes', 'Ġalternative', 'Ġexpensive', 'Ġspace', 'Ġlaunch', 'Ġsystem', 'sl', 'Ġprogram', 'Ġn', 'asa', 'Ġdecided', 'Ġexclusively', 'Ġuse', 'Ġsl', 'Ġlaunch', 'ion', 'Ġcapsule', 'Ġhowever', 'Ġfal', 'con', 'Ġheavy', 'Ġsupport', 'Ġcommercial', 'Ġmissions', 'Ġart', 'emis', 'Ġprogram', 'Ġsince', 'Ġused', 'Ġtransport', 'Ġdragon', 'Ġspacecraft', 'Ġlunar', 'Ġgateway', 'Ġalso', 'Ġselected', 'Ġlaunch', 'Ġfirst', 'Ġtwo', 'Ġelements', 'Ġlunar', 'Ġgateway', 'Ġpower', 'Ġpropulsion', 'Ġelement', 'ppe', 'Ġhabit', 'ation', 'Ġlogistics', 'Ġoutpost', 'h', 'alo', 'Ġsingle', 'Ġlaunch', 'mber', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġrover', 'Ġaboard', 'Ġast', 'rob', 'otic', 'Ġtechnology', "'s", 'Ġgr', 'iffin', 'Ġland', 'er', 'Ġpart', 'Ġart', 'emis', 'Ġprogram', "'s", 'Ġcommercial', 'Ġlunar', 'Ġpayload', 'Ġservices', 'cl', 'ps', 'Ġinitiative', 'Ġfal', 'con', 'Ġheavy', 'Ġconsists', 'Ġstruct', 'urally', 'Ġstrengthened', 'Ġfal', 'con', 'core', 'Ġcomponent', 'Ġtwo', 'Ġadditional', 'Ġfal', 'con', 'Ġfirst', 'Ġstages', 'Ġaer', 'odynamic', 'Ġnose', 'âĢĵ', 'con', 'es', 'Ġmounted', 'board', 'Ġserving', 'Ġstrap', 'Ġboosters', 'Ġconcept', 'ually', 'Ġsimilar', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlauncher', 'Ġproposals', 'las', 'Ġheavy', 'Ġr', 'ussian', 'Ġang', 'ara', 'Ġtriple', 'Ġfirst', 'Ġstage', 'Ġcarries', 'Ġstandard', 'Ġfal', 'con', 'Ġsecond', 'Ġstage', 'Ġturn', 'Ġcarries', 'Ġpayload', 'Ġfair', 'ing', 'Ġfal', 'con', 'Ġheavy', 'Ġsecond', 'Ġhighest', 'Ġlift', 'Ġcapability', 'Ġoperational', 'Ġrocket', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', '000', 'Ġtrans', 'ars', 'Ġinjection', 'Ġrocket', 'Ġdesigned', 'Ġmeet', 'Ġexceed', 'Ġcurrent', 'Ġrequirements', 'Ġhuman', 'Ġrating', 'Ġstructural', 'Ġsafety', 'Ġmargins', 'Ġlater', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġdesign', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġpad', 'Ġmer', 'lin', 'Ġengine', 'Ġflight', 'Ġloads', 'Ġhigher', 'Ġmargins', 'Ġrockets', 'Ġfal', 'con']</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġjack', 'son', 'anda', 'Ġmay', 'air', 'Ġforce', "'s", 'Ġmysterious', 'Ġspace', 'Ġplane', 'Ġlands', 'Ġwakes', 'Ġfl', 'ida', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġlaunches', 'Ġair', 'Ġforce', "'s", 'Ġspace', 'plane', 'Ġhurricane', 'Ġ', 'irm', 'Ġreaches', 'Ġfl', 'ida', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġgra', 'ham', 'iam', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġfal', 'con', 'w', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'air', 'Ġforce', 'Ġpreparing', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'f', 'th', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġmission', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġair', 'Ġforce', 'Ġnews', 'Ġservice', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdavid', 'Ġle', 'ard', 'Ġaug', 'ust', 'ster', 'ious', 'Ġmilitary', 'Ġspace', 'Ġplane', 'Ġnear', 'Ġyear', 'Ġorbit', 'http', 'Ġspace', 'Ġarchived', 'http', 'year', 'orbit', 'html', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'adv', 'anced', 'Ġstruct', 'urally', 'Ġembedded', 'Ġthermal', 'Ġspread', 'er', 'ets', 'ii', ')"', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'u', 'Ġmilitary', "'s", 'Ġspace', 'plane', 'Ġlands', 'Ġfl', 'ida', 'space', 'ï', '¬', 'Ĥ', 'ig', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgall', 'op', 'Ġj', 'Ġoct', 'ober', 'u', 'Ġair', 'force', "'s", 'Ġreturns', 'Ġearth', 'bo', 'om', 'Ġnew', 'Ġrecord', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġus', 'Ġtoday', 'Ġfl', 'ida', 'Ġtoday', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgra', 'ham', 'iam', 'Ġmay', 'ula', 'las', 'Ġlaunches', 'Ġsixth', 'Ġmission', 'Ġspace', 'plane', 'w', 'space', 'Ġforce']</t>
+          <t>['Ġheavy', 'Ġdesigned', 'Ġoutset', 'Ġcarry', 'Ġhumans', 'Ġspace', 'Ġwould', 'Ġrestore', 'Ġpossibility', 'Ġflying', 'Ġcrew', 'ed', 'Ġmissions', 'Ġmoon', 'Ġmars', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġthree', 'Ġfal', 'con', 'Ġderived', 'Ġcores', 'Ġequipped', 'Ġnine', 'Ġmer', 'lin', 'Ġengines', 'Ġfal', 'con', 'Ġheavy', 'Ġtotal', 'Ġsea', 'level', 'Ġthrust', 'Ġlif', 'ff', '000', 'Ġmer', 'lin', 'Ġengines', 'Ġthrust', 'Ġrises', '000', 'Ġcraft', 'Ġclimbs', 'Ġatmosphere', 'Ġupper', 'Ġstage', 'Ġpowered', 'Ġsingle', 'Ġmer', 'lin', 'Ġengine', 'Ġmodified', 'Ġvacuum', 'Ġoperation', 'Ġthrust', 'Ġkn', '000', 'Ġexpansion', 'Ġratio', 'Ġnominal', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġlaunch', 'Ġcenter', 'Ġcore', 'Ġthrott', 'les', 'Ġfull', 'Ġpower', 'Ġseconds', 'Ġadditional', 'Ġthrust', 'Ġthrott', 'les', 'Ġallows', 'Ġlonger', 'Ġburn', 'Ġtime', 'Ġside', 'Ġboosters', 'Ġseparate', 'Ġcenter', 'Ġcore', 'Ġthrott', 'les', 'Ġback', 'Ġmaximum', 'Ġthrust', 'Ġadded', 'Ġreliability', 'Ġrestart', 'Ġengine', 'Ġdual', 'Ġredundant', 'Ġpy', 'roph', 'oric', 'Ġign', 'ers', 'te', 'te', 'b', ').[', 'Ġinter', 'stage', 'Ġconnects', 'Ġupper', 'Ġlower', 'Ġstage', 'Ġfal', 'con', 'Ġcarbon', 'Ġfiber', 'Ġaluminum', 'Ġcore', 'Ġcomposite', 'Ġstructure', 'Ġstage', 'Ġseparation', 'Ġoccurs', 'Ġvia', 'Ġreusable', 'Ġseparation', 'Ġcol', 'lets', 'Ġp', 'ne', 'umatic', 'Ġpus', 'Ġsystem', 'Ġfal', 'con', 'Ġtank', 'Ġwalls', 'Ġdom', 'es', 'Ġmade', 'Ġaluminium', 'âĢĵ', 'l', 'ith', 'ium', 'Ġalloy', 'Ġspace', 'x', 'Ġuses', 'f', 'riction', 'Ġstir', 'Ġweld', 'ed', 'Ġtank', 'Ġsecond', 'Ġstage', 'Ġtank', 'Ġfal', 'con', 'Ġsimply', 'Ġshorter', 'Ġversion', 'Ġfirst', 'Ġstage', 'Ġtank', 'Ġuses', 'Ġtool', 'ing', 'Ġmaterial', 'Ġmanufacturing', 'Ġtechniques', 'Ġapproach', 'Ġreduces', 'Ġmanufacturing', 'Ġcosts', 'Ġvehicle', 'Ġproduction', 'Ġthree', 'Ġcores', 'Ġfal', 'con', 'Ġheavy', 'Ġarrange', 'Ġengines', 'Ġstructural', 'Ġform', 'Ġspace', 'x', 'Ġcalls', 'Ġoct', 'aw', 'eb', 'Ġaimed', 'Ġstream', 'lining', 'Ġmanufacturing', 'Ġprocess', 'Ġcore', 'Ġincludes', 'Ġfour', 'Ġext', 'ensible', 'Ġlanding', 'Ġcontrol', 'Ġdescent', 'Ġboosters', 'Ġcenter', 'Ġcore', 'Ġatmosphere', 'Ġspace', 'x', 'Ġuses', 'Ġfour', 'Ġretract', 'able', 'Ġgrid', 'Ġfins', 'Ġtop', 'Ġthree', 'Ġfal', 'con', 'Ġboosters', 'Ġextend', 'Ġseparation', 'Ġimmediately', 'Ġside', 'Ġboosters', 'Ġseparate', 'Ġcenter', 'Ġengine', 'Ġburns', 'Ġseconds', 'Ġorder', 'Ġcontrol', 'Ġbooster', "'s", 'Ġtrajectory', 'Ġsafely', 'Ġaway', 'Ġrocket', 'Ġgrid', 'Ġfins', 'Ġdeploy']</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -2856,7 +2856,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>["'s", 'Ġsecretive', 'Ġplane', 'Ġspent', 'Ġdays', 'Ġorbit', 'mber', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'pay', 'loads', 'Ġrevealed', 'Ġnext', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġmilitary', 'Ġspace', 'plane', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġmay', 'next', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġscheduled', 'Ġlaunch', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'cd', 'owell', 'Ġj', 'athan', 'Ġj', 'une', 'jon', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġreport', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'graded', 'Ġspace', 'plane', 'Ġrockets', 'Ġorbit', 'Ġaboard', 'las', 'Ġlauncher', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġk', 'les', 'ius', 'ichael', 'jan', 'uary', 'space', 'Ġshuttle', 'j', 'r', '/?', 'Ġair', 'Ġspace', 'Ġmagazine', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġdavid', 'Ġle', 'ard', 'Ġoct', 'ober', 'secret', 'ive', 'Ġus', 'Ġspace', 'Ġplane', 'Ġcould', 'Ġevolve', 'Ġcarry', 'Ġastronauts', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'bo', 'e', 'ing', 'Ġbo', 'e', 'ing', 'Ġcitizens', 'Ġspace', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġbo', 'e', 'ing', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġjohn', 'Ġapr', 'il', 'air', 'Ġforce', 'Ġlaunch', 'Ġrobotic', 'Ġwing', 'ed', 'Ġspace', 'Ġplane', 'Ġphys', 'org', 'Ġassociated', 'Ġpress', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġle', 'ard', 'Ġdavid', 'mber', 'secret', 'ive', 'Ġair', 'Ġforce', 'Ġrobotic', 'Ġspace', 'Ġplane', 'Ġmay', 'Ġnearing', 'Ġmission', "'s", 'Ġend', 'html', 'Ġspace', 'Ġretrieved', 'Ġapr', 'il', 'Ġmol', 'c', 'zan', 'Ġted', 'Ġmay', 'Ġsearch', 'Ġelements']</t>
+          <t>['Ġboosters', 'Ġturn', 'Ġback', 'Ġearth', 'Ġfollowed', 'Ġlanding', 'Ġlegs', 'Ġbooster', 'Ġlands', 'Ġsoftly', 'Ġground', 'Ġfully', 'Ġreusable', 'Ġlaunch', 'Ġconfiguration', 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġland', 'Ġdifferent', 'Ġdrone', 'Ġships', 'Ġpartial', 'Ġreusable', 'Ġconfiguration', 'Ġcenter', 'Ġcore', 'Ġcontinues', 'Ġfire', 'Ġstage', 'Ġseparation', 'Ġfully', 'Ġreusable', 'Ġlaunches', 'Ġgrid', 'Ġfins', 'Ġlegs', 'Ġdeploy', 'Ġcenter', 'Ġcore', 'Ġtouches', 'Ġeither', 'Ġback', 'Ġland', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdrone', 'Ġship', 'Ġstages', 'Ġexpended', 'Ġlanding', 'Ġlegs', 'Ġgrid', 'Ġfins', 'Ġomitted', 'Ġvehicle', 'Ġlanding', 'Ġlegs', 'Ġmade', 'Ġcarbon', 'Ġfiber', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġstructure', 'Ġfour', 'Ġlegs', 'Ġst', 'ow', 'Ġalong', 'Ġsides', 'Ġcore', 'Ġlif', 'ff', 'Ġextend', 'Ġoutward', 'Ġlanding', 'Ġfal', 'con', 'Ġheavy', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġcharacteristics', 'hide', 'Ġcharacteristic', 'Ġfirst', 'Ġstage', 'Ġcore', 'Ġunit', 'Ġcenter', 'Ġbooster', 'Ġsecond', 'Ġstage', 'Ġpayload', 'Ġfair', 'ing', 'Ġheight', 'Ġft', 'Ġft', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġft', 'Ġft', 'Ġdry', 'Ġmass', '000', 'Ġfueled', 'Ġmass', '000', '000', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġmon', 'oco', 'que', 'Ġhalves', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'âĢĵ', 'l', 'ith', 'ium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġaluminum', 'âĢĵ', 'l', 'ith', 'ium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġcarbon', 'Ġï', '¬', 'ģ', 'ber', 'Ġengines', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġvacuum', 'Ġengine', 'Ġtype', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġtank', 'Ġcapacity', '000', '000', 'Ġk', 'eros', 'ene', 'Ġtank', 'Ġcapacity', '000', '000', 'Ġengine', 'Ġnozzle', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġengine', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġthrust', 'Ġstage', 'Ġtotal', '000', 'Ġsea', 'Ġlevel']</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>['html', 'Ġsat', 'obs', 'org', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'une', 'Ġev', 'ans', 'ichael', 'Ġapr', 'il', 'launch', 'Ġsecret', 'Ġus', 'Ġspace', 'Ġship', 'Ġmasks', 'Ġeven', 'Ġsecret', 'Ġlaunch', 'Ġnew', 'Ġweapon', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'plane', 'Ġcompletes', 'Ġsixth', 'Ġmission', 'Ġlands', 'Ġnearly', 'Ġmonths', 'Ġorbit', 'sp', 'ac', 'en', 'ew', 'mber', 'Ġbent', 'ley', 'Ġmatt', 'hew', 'Ġspace', 'planes', 'Ġairport', 'Ġspac', 'eport', 'Ġnew', 'ork', 'Ġspring', 'er', 'Ġreading', 'Ġbo', 'e', 'ing', 'Ġwik', 'ipedia', 'Ġg', 'ump', 'Ġdavid', 'Ġp', 'Ġspace', 'Ġenterprise', 'Ġbeyond', 'Ġn', 'asa', 'Ġwest', 'port', 'Ġconnect', 'icut', 'Ġpra', 'eger', 'Ġmill', 'er', 'Ġj', 'ay', 'Ġx', 'planes', 'Ġh', 'ck', 'ley', 'Ġmid', 'land', 'Ġyen', 'ne', 'Ġbill', 'Ġstory', 'Ġbo', 'e', 'ing', 'Ġcompany', 'Ġmin', 'neapolis', 'Ġmin', 'n', '.:', 'Ġz', 'en', 'ith', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġfact', 'Ġsheet', 'Ġarchived', 'Ġj', 'une', 'Ġway', 'back', 'Ġmachine', 'Ġu', 'Ġair', 'Ġforce', 'Ġorbital', 'Ġtest', 'Ġvehicle', 'Ġpage', 'Ġbo', 'e', 'ing', 'Ġfact', 'Ġsheet', 'Ġarchived', 'Ġoct', 'ober', 'Ġway', 'back', 'Ġmachine', 'Ġn', 'asa', 'gov', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġkn', '000', 'Ġvacuum', 'Ġpropell', 'ant', 'Ġfeed', 'Ġsystem', 'Ġturb', 'op', 'ump', 'Ġturb', 'op', 'ump', 'Ġthrottle', 'Ġcapability', 'Ġyes', 'âĢĵ', 'Ġkn', '000', 'âĢĵ', '000', 'Ġsea', 'Ġlevel', 'Ġyes', 'âĢĵ', 'Ġkn', '000', 'âĢĵ', '000', 'Ġvacuum', 'Ġrestart', 'Ġcapability', 'Ġyes', 'Ġengines', 'Ġboost', 'back', 'entry', 'Ġlanding', 'Ġyes', 'Ġdual', 'Ġredundant', 'Ġtea', 'te', 'b', 'Ġpy', 'roph', 'oric', 'Ġign', 'ers', 'Ġtank', 'Ġpress', 'ur', 'ization', 'Ġheated', 'Ġhelium', 'Ġheated', 'Ġhelium', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġg', 'imb', 'aled', 'Ġengine', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġshutdown', 'Ġprocess', 'Ġcommanded', 'Ġcommanded', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġp', 'ne', 'umatic', 'Ġp', 'ne', 'umatic', 'Ġrocket', 'Ġspecifications', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġtwenty', 'seven', 'Ġmer', 'lin', 'Ġengines', 'Ġï', '¬', 'ģ', 'ring', 'Ġlaunch', 'Ġar', 'abs', 'Ġfal', 'con', 'Ġheavy', 'Ġuses', 'Ġft', 'Ġinter', 'stage', 'Ġattached', 'Ġfirst', 'Ġstage', 'Ġcore', 'Ġcomposite', 'Ġstructure', 'Ġconsisting', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġcore', 'Ġsurrounded', 'Ġcarbon', 'Ġfiber', 'Ġface', 'Ġsheet', 'Ġpl', 'ies', 'Ġunlike', 'Ġfal', 'con', 'Ġblack', 'Ġthermal', 'Ġprotection', 'Ġlayer', 'Ġinter', 'stage', 'Ġblock', 'Ġcenter', 'Ġcore', 'Ġboosters', 'Ġlater', 'Ġpainted', 'Ġwhite', 'Ġseen', 'Ġfal', 'con', 'Ġheavy', 'Ġflights', 'Ġfar', 'Ġprobably', 'Ġdue', 'Ġast', 'hetics', 'Ġfal', 'con', 'Ġheavy', 'Ġlogo', 'Ġproviding', 'Ġgrey', 'ish', 'Ġoverall', 'Ġlength', 'Ġvehicle', 'Ġlaunch', 'Ġft', 'Ġtotal', 'Ġfueled', 'Ġmass', '000', 'Ġwithout', 'Ġrecovery', 'Ġstage', 'Ġfal', 'con', 'Ġheavy', 'Ġinject', '000', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', '000', 'Ġven', 'us', 'Ġmars', 'Ġfal', 'con', 'Ġheavy', 'Ġincludes', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġsystems', 'Ġallow', 'Ġspace', 'x', 'Ġreturn', 'Ġfirst', 'Ġstage', 'Ġboosters', 'Ġlaunch', 'Ġsite', 'Ġwell', 'Ġrecover', 'Ġfirst', 'Ġstage', 'Ġcore', 'Ġfollowing', 'Ġlanding', 'Ġautonomous', 'Ġspac', 'eport', 'Ġdrone', 'Ġship', 'Ġb', 'arge', 'Ġcompletion', 'Ġprimary', 'Ġmission', 'Ġrequirements', 'Ġsystems', 'Ġinclude', 'Ġfour', 'Ġdeploy', 'able', 'Ġlanding', 'Ġlegs', 'Ġlocked', 'Ġfirst', 'stage', 'Ġtank', 'Ġcore', 'Ġascent', 'Ġdeploy', 'Ġprior', 'Ġtouchdown', 'Ġexcess', 'Ġpropell', 'ant', 'Ġreserved', 'Ġfal', 'con', 'Ġheavy']</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>['ars', 'Ġwik', 'ipedia', 'ars', 'Ġglobal', 'Ġtype', 'Ġsubsidiary', 'Ġindustry', 'Ġsatellite', 'Ġcommunication', 'Ġfounded', 'Ġheadquarters', 'Ġl', 'ondon', 'Ġeng', 'land', 'Ġkey', 'Ġpeople', 'rew', 'Ġsu', 'k', 'aw', 'chair', 'Ġperson', 'Ġr', 'aj', 'ee', 'v', 'Ġsur', 'ce', 'Ġrevenue', 'Ġus', 'Ġmillion', ')[', 'Ġoperating', 'Ġincome', 'Ġus', 'Ġmillion', ')[', 'Ġnet', 'Ġincome', 'Ġus', 'Ġmillion', ')[', 'Ġnumber', 'Ġemployees', ')[', 'Ġparent', 'Ġv', 'ias', 'Ġwebsite', 'ars', 'ars', 'ars', 'Ġsatellite', 'ars', 'ars', 'Ġb', 'rit', 'ish', 'Ġsatellite', 'Ġtelecommunications', 'Ġcompany', 'Ġoffering', 'Ġglobal', 'Ġmobile', 'Ġservices', 'Ġprovides', 'Ġtelephone', 'Ġdata', 'Ġservices', 'Ġusers', 'Ġworldwide', 'Ġvia', 'Ġportable', 'Ġmobile', 'Ġterminals', 'Ġcommunicate', 'Ġground', 'Ġstations', 'Ġfourteen', 'Ġge', 'ost', 'ation', 'ary', 'Ġtelecommunications', 'Ġsatellites', 'ars', "'s", 'Ġnetwork', 'Ġprovides', 'Ġcommunications', 'Ġservices', 'Ġrange', 'Ġgovernments', 'Ġaid', 'Ġagencies', 'Ġmedia', 'Ġoutlets', 'Ġbusinesses', 'especially', 'Ġshipping', 'Ġairline', 'Ġmining', 'Ġindustries', 'Ġneed', 'Ġcommunicate', 'Ġremote', 'Ġregions', 'Ġreliable', 'Ġterrestrial', 'Ġnetwork', 'Ġcompany', 'Ġlisted', 'Ġl', 'ondon', 'Ġstock', 'Ġexchange', 'Ġacquired', 'Ġconnect', 'Ġbid', 'co', 'Ġconsortium', 'Ġconsisting', 'Ġpartners', 'Ġwar', 'burg', 'Ġp', 'inc', 'us', 'Ġinvestment', 'Ġboard', 'Ġont', 'ario', 'Ġteachers', 'Ġpension', 'Ġplan', 'Ġde', 'cember', 'mber', 'Ġdeal', 'Ġannounced', 'ars', "'s", 'Ġowners', 'Ġv', 'ias', 'Ġv', 'ias', 'Ġpurchase', 'ars', 'Ġacquisition', 'Ġcompleted', 'Ġmay', 'Ġpresent', 'Ġcompany', 'Ġorigin', 'ates', 'Ġinternational', 'Ġmaritime', 'Ġsatellite', 'Ġorganization', 'ars', 'Ġnon', 'profit', 'Ġinter', 'governmental', 'Ġorganisation', 'Ġestablished', 'Ġbehest', 'Ġinternational', 'Ġmaritime', 'Ġorganization', 'imo', ')âĢĶ', 'Ġunited', 'Ġnations', 'Ġmaritime', 'Ġbody', 'âĢĶ', 'Ġpursuant', 'Ġconvention', 'Ġinternational', 'Ġmaritime', 'Ġsatellite', 'Ġorganization', 'Ġsigned', 'Ġcountries', 'Ġorganisation', 'Ġcreated', 'Ġestablish', 'Ġoperate', 'Ġsatellite', 'Ġcommunications', 'Ġnetwork', 'Ġmaritime', 'Ġcommunity', 'Ġcoordination', 'Ġinternational', 'Ġcivil', 'Ġaviation', 'Ġorganization', 'Ġconvention', 'Ġgoverning', 'ars', 'Ġamended', 'Ġinclude', 'Ġimprovements', 'Ġaer', 'autical', 'Ġcommunications']</t>
+          <t>['Ġfirst', 'stage', 'Ġrecovery', 'Ġoperations', 'Ġdiverted', 'Ġuse', 'Ġprimary', 'Ġmission', 'Ġobjective', 'Ġrequired', 'Ġensuring', 'Ġsufficient', 'Ġperformance', 'Ġmargins', 'Ġsuccessful', 'Ġmissions', 'Ġnominal', 'Ġpayload', 'Ġcapacity', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', '000', 'Ġrecovery', 'Ġthree', 'Ġfirst', 'stage', 'Ġcores', 'Ġprice', 'Ġper', 'Ġlaunch', 'Ġmillion', 'Ġversus', '000', 'Ġfully', 'Ġexpend', 'able', 'Ġmode', 'Ġfal', 'con', 'Ġheavy', 'Ġalso', 'Ġinject', '000', 'Ġpayload', 'Ġg', 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġrecovered', 'Ġpartially', 'Ġreusable', 'Ġfal', 'con', 'Ġheavy', 'Ġfalls', 'Ġheavy', 'lift', 'Ġrange', 'Ġlaunch', 'Ġsystems', 'Ġcapable', 'Ġlifting', 'âĢĵ', '000', 'âĢĵ', '000', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġclassification', 'Ġsystem', 'Ġused', 'Ġn', 'asa', 'Ġhuman', 'Ġspace', 'flight', 'Ġreview', 'Ġpanel', 'Ġfully', 'Ġexpend', 'able', 'Ġfal', 'con', 'Ġheavy', 'Ġsuper', 'Ġheavy', 'lift', 'Ġcategory', 'Ġmaximum', 'Ġpayload', '000', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġinitial', 'Ġconcept', 'fal', 'con', 'Ġenvisioned', 'Ġpayload', 'Ġle', 'Ġapr', 'il', 'Ġprojected', '000', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġpayload', '000', 'Ġlater', 'Ġreports', 'Ġprojected', 'Ġhigher', 'Ġpayload', 'Ġbeyond', 'Ġle', 'Ġincluding', '000', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', '000', 'Ġtransl', 'un', 'ar', 'Ġtrajectory', '000', 'Ġtrans', 'mart', 'ian', 'Ġorbit', 'Ġmars', 'Ġlate', 'Ġspace', 'x', 'Ġraised', 'Ġprojected', 'Ġg', 'Ġpayload', 'Ġfal', 'con', 'Ġheavy', '000', 'Ġapr', 'il', 'Ġprojected', 'Ġle', 'Ġpayload', 'Ġfal', 'con', 'Ġheavy', 'Ġraised', '000', '000', 'Ġmaximum', 'Ġpayload', 'Ġachieved', 'Ġrocket', 'Ġflies', 'Ġfully', 'Ġexpend', 'able', 'Ġlaunch', 'Ġprofile', 'Ġrecovering', 'Ġthree', 'Ġfirst', 'stage', 'Ġboosters', 'Ġcore', 'Ġbooster', 'Ġexpended', 'Ġtwo', 'Ġside', 'boost', 'ers', 'Ġrecovered', 'Ġmus', 'k', 'Ġestimates', 'Ġpayload', 'Ġpenalty', 'Ġaround', '%,', 'Ġwould', 'Ġstill', 'Ġyield', '000', 'Ġlift', 'Ġcapability', 'Ġreturning', 'Ġthree', 'Ġboosters', 'Ġlaunch', 'Ġsite', 'Ġrather', 'Ġlanding', 'Ġdrone', 'Ġships', 'Ġwould', 'Ġyield', 'Ġpayload']</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -2895,7 +2895,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>['Ġnotably', 'Ġpublic', 'Ġmember', 'Ġstates', 'Ġowned', 'Ġvarying', 'Ġshares', 'Ġoperational', 'Ġbusiness', 'Ġmain', 'Ġoffices', 'Ġoriginally', 'Ġlocated', 'Ġe', 'ust', 'Ġtower', 'Ġe', 'ust', 'Ġroad', 'Ġl', 'ondon', 'Ġhistory', 'Ġorigins', 'Ġprivatization', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġsatellite', 'Ġtelephone', 'Ġuse', 'Ġnatural', 'Ġdisaster', 'Ġn', 'ias', 'Ġind', 'ones', 'ia', 'Ġunit', 'Ġdepicted', 'Ġmanufactured', 'Ġthr', 'ane', 'Ġthr', 'ane', 'Ġden', 'mark', 'ap', 'ril', 'Ġmid', 'Ġmany', 'Ġmember', 'Ġstates', 'Ġunwilling', 'Ġinvest', 'Ġimprovements', 'ars', "'s", 'Ġnetwork', 'Ġespecially', 'Ġowing', 'Ġcompetitive', 'Ġnature', 'Ġsatellite', 'Ġcommunications', 'Ġindustry', 'Ġmany', 'Ġrecognised', 'Ġneed', 'Ġmaintain', 'Ġorganisation', "'s", 'Ġolder', 'Ġsystems', 'Ġneed', 'Ġinter', 'governmental', 'Ġorganisation', 'Ġoversee', 'Ġpublic', 'Ġsafety', 'Ġaspects', 'Ġsatellite', 'Ġcommunication', 'Ġnetworks', 'Ġagreement', 'Ġreached', 'Ġmodify', 'ars', "'s", 'Ġmission', 'Ġinter', 'governmental', 'Ġorganisation', 'Ġseparate', 'Ġprivat', 'ise', 'Ġorganisation', "'s", 'Ġoperational', 'Ġbusiness', 'Ġpublic', 'Ġsafety', 'Ġobligations', 'Ġattached', 'Ġapr', 'il', 'ars', 'Ġsucceeded', 'Ġinternational', 'Ġmobile', 'Ġsatellite', 'Ġorganization', 'im', 'Ġinter', 'governmental', 'Ġregulatory', 'Ġbody', 'Ġsatellite', 'Ġcommunications', 'ars', "'s", 'Ġoperational', 'Ġunit', 'Ġseparated', 'Ġbecame', 'Ġu', 'k', 'based', 'Ġcompany', 'ars', 'Ġim', 'ars', 'Ġsigned', 'Ġagreement', 'Ġimposing', 'Ġpublic', 'Ġsafety', 'Ġobligations', 'Ġnew', 'Ġcompany', 'ars', 'Ġfirst', 'Ġinternational', 'Ġsatellite', 'Ġorganisation', 'Ġprivat', 'ised', 'Ġpartners', 'Ġperm', 'ira', 'Ġbought', 'Ġshares', 'Ġcompany', 'Ġcompany', 'Ġalso', 'Ġfirst', 'Ġlisted', 'Ġl', 'ondon', 'Ġstock', 'Ġexchange', 'Ġyear', 'Ġmarch', 'Ġdisclosed', 'Ġu', 'Ġhedge', 'Ġfund', 'Ġharb', 'inger', 'Ġcapital', 'Ġowned', 'Ġcompany', 'ars', 'Ġcompleted', 'Ġacquisition', 'Ġsatellite', 'Ġcommunications', 'Ġprovider', 'Ġstrat', 'os', 'Ġglobal', 'Ġcorporation', 'str', 'atos', ')[', 'Ġacquired', 'per', 'Ġcent', 'Ġstake', 'Ġsky', 'wave', 'Ġmobile', 'Ġcommunications', 'Ġinc', '.,', 'Ġprovider', 'ars', 'Ġnetwork', 'Ġservices', 'Ġturn', 'Ġpurchased', 'Ġglobal', 'wave', 'Ġbusiness', 'Ġtrans', 'core', 'ars', 'Ġmacro', 'bert', 'Ġaward', 'Ġbroadband', 'Ġglobal', 'Ġarea', 'Ġnetwork', 'Ġservice', 'ars']</t>
+          <t>['Ġcapabilities', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġlong', 'Ġexposure', 'Ġnight', 'Ġlaunch', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġreusable', 'Ġside', 'Ġboosters', 'Ġland', 'Ġunison', 'Ġcape', 'aver', 'al', 'Ġlanding', 'Ġzones', 'Ġfollowing', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfe', 'b', 'ruary', 'Ġmaximum', 'Ġtheoretical', 'Ġpayload', 'Ġcapacity', 'Ġdestination', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġaug', 'ust', 'Ġapr', 'il', 'Ġmay', 'Ġmarch', 'Ġsince', 'Ġapr', 'il', 'Ġle', 'Â°', 'Ġexpend', 'able', 'Ġg', 'Â°', 'Ġexpend', 'able', 'Ġg', 'Â°', 'Ġreusable', 'Ġmars', 'Ġpl', 'uto', 'Ġspace', 'x', 'Ġconducted', 'Ġparallel', 'Ġdevelopment', 'Ġreusable', 'Ġrocket', 'Ġarchitecture', 'Ġfal', 'con', 'Ġapplies', 'Ġparts', 'Ġfal', 'con', 'Ġheavy', 'Ġwell', 'Ġearly', 'Ġspace', 'x', 'Ġexpressed', 'Ġhopes', 'Ġrocket', 'Ġstages', 'Ġwould', 'Ġeventually', 'Ġreusable', 'Ġspace', 'x', 'Ġsince', 'Ġdemonstrated', 'Ġroutine', 'Ġland', 'Ġsea', 'Ġrecovery', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġsuccessfully', 'Ġrecovered', 'Ġmultiple', 'Ġpayload', 'Ġfair', 'ings', 'Ġcase', 'Ġfal', 'con', 'Ġheavy', 'Ġtwo', 'Ġouter', 'Ġcores', 'Ġseparate', 'Ġrocket', 'Ġearlier', 'Ġflight', 'Ġthus', 'Ġmoving', 'Ġlower', 'Ġvelocity', 'Ġfal', 'con', 'Ġlaunch', 'Ġprofile', 'Ġfirst', 'Ġflight', 'Ġfal', 'con', 'Ġheavy', 'Ġspace', 'x', 'Ġconsidered', 'Ġattempting', 'Ġrecover', 'Ġsecond', 'Ġstage', 'Ġexecute', 'Ġplan', 'Ġfal', 'con', 'Ġheavy', 'Ġpayload', 'Ġperformance', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', 'Ġreduced', 'Ġreusable', 'Ġtechnology', 'Ġmuch', 'Ġlower', 'Ġprice', 'Ġrecovering', 'Ġthree', 'Ġbooster', 'Ġcores', 'Ġg', 'Ġpayload', '000', 'Ġtwo', 'Ġoutside', 'Ġcores', 'Ġrecovered', 'Ġcenter', 'Ġcore', 'Ġexpended', 'Ġg', 'Ġpayload', 'Ġwould', 'Ġapproximately', '000', 'Ġcomparison', 'Ġnext', 'av', 'iest', 'Ġcontemporary', 'Ġrocket', 'Ġfully', 'Ġexpend', 'able', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġdeliver', '000', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginally', 'Ġdesigned', 'Ġunique', 'pro', 'pell', 'ant', 'Ġcross', 'feed', 'Ġcapability', 'Ġwhereby', 'Ġcenter', 'Ġcore', 'Ġengines', 'Ġwould', 'Ġsupplied', 'Ġfuel', 'Ġoxid', 'izer', 'Ġtwo', 'Ġside', 'Ġcores', 'Ġseparation', 'Ġoperating', 'Ġengines', 'Ġfull']</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -2908,7 +2908,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>['Ġfirst', 'Ġprovided', 'Ġservices', 'Ġusing', 'Ġmar', 'cs', 'Ġlaunched', 'Ġus', 'Ġnavy', 'Ġes', 'Ġrespectively', 'Ġearly', 'ars', 'Ġlaunched', 'Ġfirst', 'Ġdedicated', 'Ġsatellite', 'Ġconstellation', 'ars', 'Ġsatellites', 'Ġprovided', 'ars', 'Ġservice', 'Ġmaritime', 'Ġuses', 'ars', "'s", 'Ġsecond', 'Ġconstellation', 'ars', 'Ġlaunched', 'Ġconsisting', 'Ġfive', 'Ġge', 'ost', 'ation', 'ary', 'Ġl', 'band', 'Ġsatellites', 'Ġconstellation', 'Ġprovides', 'ars', 'b', 'ars', 'c', 'Ġservices', 'Ġprimarily', 'Ġproviding', 'Ġlow', 'Ġbandwidth', 'Ġcommunications', 'Ġsafety', 'Ġservices', 'Ġglobal', 'Ġshipping', 'Ġfollowing', 'Ġprivat', 'isation', 'ars', 'Ġdeveloped', 'Ġlaunched', 'Ġfirst', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'Ġoffering', 'Ġglobal', 'Ġcoverage', 'Ġservice', 'Ġprovided', 'Ġinitially', 'Ġthree', 'ars', 'Ġsatellite', 'Ġlaunched', 'Ġextended', 'Ġaddition', 'Ġal', 'phas', 'ars', 'Ġbegan', 'Ġdevelopment', 'Ġhigh', 'Ġthroughput', 'Ġsatellite', 'h', 'ts', 'Ġconstellation', 'Ġglobal', 'Ġx', 'press', 'Ġoperating', 'Ġka', 'band', 'Ġportion', 'Ġspectrum', 'Ġglobal', 'Ġx', 'press', 'Ġlaunched', 'Ġoffers', 'Ġglobal', 'Ġsatellite', 'Ġcapacity', 'Ġvarious', 'Ġmarkets', 'Ġincluding', 'Ġshipping', 'Ġaviation', 'Ġglobal', 'Ġx', 'press', 'Ġalso', 'Ġmarks', 'Ġsignificant', 'Ġexpansion', 'ars', "'s", 'Ġcommercial', 'Ġoperations', 'Ġaviation', 'Ġmarkets', 'ars', 'Ġlaunched', 'Ġfirst', 'band', 'Ġsatellite', 'Ġintended', 'Ġprovide', 'Ġassociation', 'Ġl', 'te', 'Ġground', 'Ġnetwork', 'Ġinf', 'light', 'Ġinternet', 'Ġaccess', 'Ġacross', 'Ġeuro', 'pe', 'Ġmarch', 'ars', 'Ġpartnered', 'Ġisot', 'rop', 'ic', 'Ġsystems', 'Ġdevelop', 'Ġstate', 'art', 'Ġelectronic', 'Ġscanning', 'Ġantenna', 'Ġintended', 'Ġused', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'ars', 'Ġwik', 'ipedia', 'Ġse', 'pt', 'ember', 'ars', 'Ġannounced', 'Ġstrategic', 'Ġcollaboration', 'Ġpan', 'asonic', 'Ġav', 'ionics', 'Ġcorporation', 'Ġinitial', 'Ġten', 'year', 'Ġperiod', 'Ġprovide', 'flight', 'Ġbroadband', 'Ġcommercial', 'Ġairlines', 'ars', 'Ġexclusive', 'Ġprovider', 'Ġpan', 'asonic', 'Ġconnectivity', 'Ġusing', 'Ġka', 'band', 'Ġsatellite', 'Ġsignal', 'ars', 'Ġoffering', 'Ġpan', 'asonic', "'s", 'Ġportfolio', 'Ġservices']</t>
+          <t>['Ġthrust', 'Ġlaunch', 'Ġfuel', 'Ġsupplied', 'Ġmainly', 'Ġside', 'Ġboosters', 'Ġwould', 'Ġde', 'plete', 'Ġside', 'Ġboosters', 'Ġsooner', 'Ġallowing', 'Ġearlier', 'Ġseparation', 'Ġreduce', 'Ġmass', 'Ġaccelerated', 'Ġwould', 'Ġleave', 'Ġcenter', 'Ġcore', 'Ġpropell', 'ant', 'Ġavailable', 'Ġbooster', 'Ġseparation', 'us', 'ability', 'Ġpropell', 'ant', 'Ġcross', 'feed', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġmus', 'k', 'Ġstated', 'Ġcross', 'feed', 'Ġwould', 'Ġimplemented', 'Ġinstead', 'Ġcenter', 'Ġbooster', 'Ġthrott', 'les', 'Ġshortly', 'Ġlif', 'ff', 'Ġconserve', 'Ġfuel', 'Ġresumes', 'Ġfull', 'Ġthrust', 'Ġside', 'Ġboosters', 'Ġseparated', 'Ġscience', 'Ġfocus', 'Ġfe', 'b', 'ruary', 'Ġpublished', 'Ġarticle', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġenvironmental', 'Ġimpact', 'Ġstated', 'Ġconcerns', 'Ġfrequent', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġcontribute', 'Ġpollution', 'Ġatmosphere', 'Ġplanetary', 'Ġsociety', 'Ġconcerned', 'Ġlaunching', 'Ġnon', 'ster', 'ile', 'Ġobject', 'Ġdone', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġflight', 'Ġinter', 'plan', 'etary', 'Ġspace', 'Ġmay', 'Ġrisk', 'Ġbiological', 'Ġcontamination', 'Ġforeign', 'Ġscientists', 'Ġpur', 'due', 'Ġuniversity', 'Ġthought', 'irt', 'iest', 'Ġman', 'made', 'Ġobject', 'Ġever', 'Ġsent', 'Ġspace', 'Ġterms', 'Ġbacteria', 'Ġamount', 'Ġnoting', 'Ġcar', 'Ġpreviously', 'Ġdriven', 'Ġlos', 'Ġangel', 'es', 'Ġfre', 'eways', 'Ġalthough', 'Ġvehicle', 'Ġsteril', 'ized', 'Ġsolar', 'Ġradiation', 'Ġtime', 'Ġbacteria', 'Ġmight', 'Ġsurvive', 'Ġpieces', 'Ġplastic', 'Ġcould', 'Ġcontam', 'inate', 'Ġmars', 'Ġdistant', 'Ġfuture', 'Ġstudy', 'Ġconducted', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġfound', 'Ġboost', 'back', 'Ġlanding', 'Ġfal', 'con', 'Ġheavy', 'Ġboosters', 'would', 'Ġsignificantly', 'Ġaffect', 'Ġquality', 'Ġhuman', 'Ġenvironment', '".[', 'Ġappearance', 'Ġmay', 'Ġunited', 'Ġstates', 'Ġsenate', 'Ġcommittee', 'Ġcommerce', 'Ġscience', 'Ġtransportation', 'Ġmus', 'k', 'Ġtestified', 'long', 'Ġterm', 'Ġplans', 'Ġcall', 'Ġdevelopment', 'Ġheavy', 'Ġlift', 'Ġproduct', 'Ġeven', 'Ġsuper', 'heavy', 'Ġcustomer', 'Ġdemand', 'Ġexpect', 'Ġsize', 'Ġincrease', 'Ġwould', 'Ġresult', 'Ġmeaningful', 'Ġdecrease', 'Ġcost', 'Ġper', 'Ġpound', 'Ġorbit', 'Ġ...', 'Ġultimately', 'Ġbelieve', 'Ġus', 'Ġper', 'Ġpound', 'Ġless', 'Ġachievable', '".[', 'kg', 'Ġ($', 'lb', 'Ġgoal', 'Ġstated', 'Ġmus', 'k', 'Ġcost', 'Ġle', 'cap', 'able', 'Ġlaunch', 'Ġsystem', 'Ġstudy', 'Ġz', 'en', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcould', 'Ġcarry', '000', 'Ġle', 'Ġus', 'âĢĵ']</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>['Ġcommercial', 'Ġaviation', 'Ġcustomers', 'Ġmarch', 'Ġmal', 'ays', 'ia', 'Ġairlines', 'Ġflight', 'Ġdisappeared', 'Ġpassengers', 'Ġcrew', 'Ġen', 'Ġroute', 'Ġk', 'uala', 'Ġlump', 'ur', 'ijing', 'Ġturning', 'Ġaway', 'Ġplanned', 'Ġpath', 'Ġdisappearing', 'Ġradar', 'Ġcoverage', 'Ġaircraft', "'s", 'Ġsatellite', 'Ġdata', 'Ġunit', 'Ġremained', 'Ġcontact', 'ars', "'s", 'Ġground', 'Ġstation', 'Ġper', 'th', 'Ġvia', 'Ġsatellite', 'ind', 'ian', 'Ġocean', 'Ġregion', 'Â°', 'Ġeast', 'Ġaircraft', 'Ġused', 'ars', "'s", 'Ġclassic', 'ero', 'Ġsatellite', 'Ġphone', 'Ġservice', 'Ġanalysis', 'Ġcommunications', 'ars', 'Ġindependently', 'Ġagencies', 'Ġdetermined', 'Ġaircraft', 'Ġflew', 'Ġsouthern', 'Ġind', 'ian', 'Ġocean', 'Ġused', 'Ġguide', 'Ġsearch', 'Ġaircraft', 'Ġmarch', 'Ġcompany', "'s", 'Ġboard', 'Ġagreed', 'Ġrecommend', 'Ġtakeover', 'Ġoffer', 'Ġbillion', 'Ġconnect', 'Ġbid', 'co', 'Ġconsortium', 'Ġconsisting', 'Ġpartners', 'Ġwar', 'burg', 'Ġp', 'inc', 'us', 'Ġinvestment', 'Ġboard', 'Ġont', 'ario', 'Ġteachers', 'Ġpension', 'Ġplan', 'Ġoct', 'ober', 'Ġbloom', 'berg', 'Ġreported', 'Ġgovernment', 'Ġset', 'Ġapprove', 'Ġtakeover', 'Ġfinal', 'Ġconsultation', 'Ġdeal', 'Ġset', 'Ġconclude', 'Ġoct', 'ober', 'mber', 'ars', 'Ġrejected', 'Ġele', 'venth', 'hour', 'Ġeffort', 'Ġderail', 'Ġbillion', 'Ġsale', 'Ġaccused', 'Ġignoring', 'Ġpotential', 'Ġboost', 'Ġcompany', "'s", 'Ġvalue', 'Ġoak', 'tree', 'Ġargued', 'Ġrecommended', 'Ġoffer', 'ars', 'Ġfailed', 'Ġtake', 'Ġaccount', 'Ġpotential', 'Ġvalue', 'Ġspectrum', 'Ġassets', 'Ġused', 'ars', "'s", 'Ġu', 'Ġpartner', 'Ġlig', 'ado', 'ars', 'Ġdel', 'isted', 'Ġl', 'ondon', 'Ġstock', 'Ġexchange', 'Ġprivate', 'Ġequity', 'Ġfunds', 'Ġtook', 'Ġcontrol', 'Ġcompany', 'Ġde', 'cember', 'Ġtime', 'ars', 'Ġoperating', 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġsatellites', 'mber', 'Ġdeal', 'Ġannounced', 'ars', "'s", 'Ġowners', 'Ġled', 'Ġwar', 'burg', 'Ġp', 'inc', 'us', 'Ġv', 'ias', 'Ġv', 'ias', 'Ġwould', 'Ġpurchase', 'ars', 'Ġcash', 'Ġissuing', 'Ġapproximately', 'Ġmillion', 'Ġshares', 'Ġv', 'ias', 'Ġstock', 'Ġtaking', 'Ġv', 'ias', 'Ġpromised', 'Ġhonour', 'Ġpledge', 'Ġmade', 'Ġprevious', 'Ġowners', 'Ġtaken', 'Ġprivate', 'ars', 'Ġwould', 'Ġremain', 'Ġu', 'k', 'based', 'Ġcompany', 'Ġplanned', 'Ġinvestments', 'Ġprovisional']</t>
+          <t>['Ġmillion', 'Ġspace', 'x', 'Ġstated', 'Ġcost', 'Ġreaching', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcould', 'Ġlow', 'kg', 'Ġ($', '000', 'lb', 'Ġannual', 'Ġrate', 'Ġfour', 'Ġlaunches', 'Ġsustained', 'Ġplanned', 'Ġeventually', 'Ġlaunch', 'Ġmany', 'Ġfal', 'con', 'Ġheav', 'ies', 'Ġfal', 'con', 'Ġannually', 'Ġpublished', 'Ġprices', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġchanged', 'Ġdevelopment', 'Ġprogressed', 'Ġannounced', 'Ġprices', 'Ġvarious', 'Ġversions', 'Ġfal', 'con', 'Ġheavy', 'Ġpriced', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġmillion', '000', 'Ġg', 'Ġmillion', '000', 'Ġg', 'Ġearly', 'Ġprice', 'Ġstated', 'Ġus', 'Ġmillion', '000', 'Ġle', '000', 'Ġg', 'fully', 'Ġexpend', 'able', ').[', 'Ġequ', 'ates', 'Ġprice', 'Ġus', 'Ġper', 'Ġle', 'Ġus', 'Ġper', 'Ġg', 'Ġpublished', 'Ġprice', 'Ġreusable', 'Ġlaunch', 'Ġmillion', 'Ġhowever', 'Ġn', 'asa', 'Ġcontracted', 'Ġspace', 'x', 'Ġlaunch', 'Ġn', 'ancy', 'Ġgrace', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġfal', 'con', 'Ġheavy', 'Ġapproximately', 'Ġmillion', 'Ġincluding', 'Ġlaunch', 'Ġservice', 'Ġmission', 'Ġrelated', 'Ġcosts', 'Ġnearest', 'Ġcompeting', 'Ġu', 'Ġrocket', 'Ġu', 'la', "'s", 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġle', 'Ġpayload', 'Ġcapacity', '000', 'Ġcosts', 'Ġus', 'Ġper', 'Ġle', 'Ġus', 'Ġper', 'Ġg', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġretired', 'Ġone', 'Ġflight', 'Ġremaining', 'Ġj', 'une', 'Ġenvironmental', 'Ġimpact', 'Ġlaunch', 'Ġprices', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġcompetitors', 'Ġonwards', 'Ġmay', 'Ġinclude', 'Ġspace', 'x', 'Ġstarship', 'Ġle', 'Ġblue', 'Ġorigin', "'s", 'Ġnew', 'Ġgl', 'enn', 'Ġle', 'Ġrelativity', 'Ġspace', "'s", 'Ġter', 'ran', 'Ġle', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġvul', 'Ġcent', 'aur', 'Ġle', 'Ġdue', 'Ġimprovements', 'Ġperformance', 'Ġfal', 'con']</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>['Ġapproval', 'Ġmerger', 'Ġgiven', 'Ġcompetition', 'Ġmarkets', 'Ġauthority', 'Ġmarch', 'Ġmay', 'Ġset', 'Ġdate', 'Ġformal', 'Ġdecision', 'Ġmay', 'Ġacquisition', 'Ġclosed', 'ars', 'Ġhead', 'Ġoffice', 'Ġold', 'Ġstreet', 'Ġround', 'Ġl', 'ondon', 'Ġborough', 'lington', 'Ġaside', 'Ġcommercial', 'Ġservices', 'ars', 'Ġprovides', 'Ġglobal', 'Ġmaritime', 'Ġdistress', 'Ġsafety', 'Ġsystem', 'g', 'md', 'ss', 'Ġships', 'Ġaircraft', 'Ġcharge', 'Ġpublic', 'Ġservice', 'Ġmal', 'ays', 'ia', 'Ġairlines', 'Ġflight', 'Ġtakeover', 'Ġconnect', 'Ġbid', 'co', 'Ġprivat', 'isation', 'Ġacquisition', 'Ġv', 'ias', 'Ġoperations', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġglobal', 'Ġcity', 'Ġroad', 'Ġl', 'ondon', 'jan', 'uary', 'Ġservices', 'Ġinclude', 'Ġtraditional', 'Ġvoice', 'Ġcalls', 'Ġlow', 'level', 'Ġdata', 'Ġtracking', 'Ġsystems', 'Ġhigh', 'speed', 'Ġinternet', 'Ġdata', 'Ġservices', 'Ġwell', 'Ġdistress', 'Ġsafety', 'Ġservices', 'Ġbroadband', 'Ġglobal', 'Ġarea', 'Ġnetwork', 'Ġnetwork', 'Ġprovides', 'Ġgeneral', 'Ġpacket', 'Ġradio', 'Ġservice', 'g', 'pr', 'Ġtype', 'Ġservices', 'Ġk', 'bit', 'Ġlatency', 'Ġvia', 'Ġinternet', 'Ġprotocol', 'Ġsatellite', 'Ġmodem', 'Ġsize', 'Ġnotebook', 'Ġcomputer', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġoffers', 'bit', 'Ġlatency', 'Ġvia', 'Ġantennas', 'Ġsmall', 'Ġservices', 'Ġprovide', 'Ġmobile', 'Ġintegrated', 'Ġservices', 'Ġdigital', 'Ġnetwork', 'isd', 'n', 'Ġservices', 'Ġused', 'Ġmedia', 'Ġlive', 'Ġreporting', 'Ġworld', 'Ġevents', 'Ġvia', 'Ġvide', 'ophone', 'Ġinf', 'light', 'Ġinternet', 'Ġaccess', 'Ġvia', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġprice', 'Ġcall', 'Ġvia', 'ars', 'Ġdropped', 'Ġlevel', 'Ġcomparable', 'Ġmany', 'Ġcases', 'Ġlower', 'Ġinternational', 'Ġroaming', 'Ġcosts', 'Ġhotel', 'Ġphone', 'Ġcalls', 'Ġvoice', 'Ġcall', 'Ġcharges', 'Ġlocation', 'Ġworld', 'Ġservice', 'Ġused', 'Ġtariffs', 'Ġcalls', 'ars', 'Ġcountry', 'Ġcodes', 'Ġvary', 'Ġdepending', 'Ġcountry', 'Ġplaced', 'ars', 'Ġprimarily', 'Ġuses', 'Ġcountry', 'Ġcode', 'see', ').[', 'Ġnewer', 'ars', 'Ġservices', 'Ġuse', 'Ġtechnology', 'Ġfeatures', 'Ġalways', 'Ġcapability', 'Ġusers', 'Ġcharged', 'Ġamount', 'Ġdata', 'Ġsend', 'Ġreceive', 'Ġrather', 'Ġlength', 'Ġtime', 'Ġconnected', 'Ġaddition']</t>
+          <t>['Ġheavier', 'Ġsatellites', 'Ġflown', 'Ġg', 'Ġint', 'els', 'ars', 'Ġf', 'Ġended', 'Ġlaunched', 'Ġdebut', 'Ġfal', 'con', 'Ġheavy', 'Ġspace', 'x', 'Ġanticipated', 'Ġfirst', 'Ġcommercial', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġwould', 'Ġthree', 'Ġmonths', 'Ġsuccessful', 'Ġmaiden', 'Ġflight', 'Ġdue', 'Ġdelays', 'Ġfirst', 'Ġcommercial', 'Ġpayload', 'Ġar', 'abs', 'Ġsuccessfully', 'Ġlaunched', 'Ġapr', 'il', 'Ġyear', 'Ġtwo', 'Ġmonths', 'Ġfirst', 'Ġflight', 'Ġspace', 'x', 'Ġhoped', 'Ġlaunches', 'Ġevery', 'Ġyear', 'Ġlaunches', 'Ġlaunches', 'Ġpayload', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġflight', 'Ġlaunch', 'Ġdate', 'Ġpayload', 'Ġmass', 'Ġcustomer', 'Ġprice', 'Ġoutcome', 'Ġfe', 'b', 'ruary', 'Ġel', 'Ġmus', 'k', "'s", 'es', 'la', 'Ġroad', 'ster', 'Ġspace', 'x', 'Ġinternal', 'Ġsuccess', 'Ġdemonstration', 'Ġï', '¬', 'Ĥ', 'ight', 'es', 'la', 'Ġroad', 'ster', 'Ġsent', 'Ġtrans', 'ars', 'Ġinjection', 'Ġhel', 'oc', 'entric', 'Ġorbit', 'Ġside', 'Ġboosters', 'Ġlanded', 'Ġsuccessfully', 'Ġcenter', 'Ġbooster', 'Ġstruck', 'Ġocean', 'Ġdestroyed', 'Ġtwo', 'Ġengines', 'Ġfailed', 'Ġrel', 'ight', 'Ġlanding', 'Ġburn', 'Ġdamaging', 'Ġtwo', 'Ġdrone', 'Ġship', "'s", 'Ġengines', 'Ġapr', 'il', 'Ġar', 'abs', 'Ġar', 'abs', 'Ġundisclosed', 'Ġsuccess', 'Ġheavy', 'Ġcommunications', 'Ġsatellite', 'Ġpurchased', 'Ġar', 'ab', 'Ġleague', 'Ġthree', 'Ġboosters', 'Ġlanded', 'Ġsuccessfully', 'Ġcenter', 'Ġcore', 'Ġsubsequently', 'Ġfell', 'Ġlost', 'Ġtransport', 'Ġdue', 'Ġheavy', 'Ġseas', 'Ġtwo', 'Ġside', 'boost', 'ers', 'Ġreused', 'Ġlaunch', 'Ġj', 'une', 'Ġ06', 'Ġus', 'af', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġus', 'Ġmillion', 'Ġsuccess', 'Ġmission', 'Ġsupported', 'Ġu', 'Ġair', 'Ġforce', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'formerly', 'Ġe', 'el', 'v', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġprocess', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginal', 'Ġcontract', 'Ġprice', 'Ġus', 'Ġmillion', 'Ġlater', 'Ġreduced', 'Ġbig', 'Ġpart', 'Ġdue', 'Ġmilitary', "'s", 'Ġagreement', 'Ġï', '¬', 'Ĥ', 'Ġmission', 'Ġreused', 'Ġside']</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -2947,7 +2947,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>['Ġsatellites', 'ars', 'Ġcollaboration', 'Ġagreement', 'ces', 'Ġregarding', 'Ġhandheld', 'Ġvoice', 'Ġservices', 'Ġthree', 'Ġtypes', 'Ġcoverage', 'Ġrelated', 'ars', 'Ġsatellite', 'Ġsatellite', 'Ġequipped', 'Ġsingle', 'Ġglobal', 'Ġbeam', 'Ġcovers', 'Ġone', 'third', 'Ġearth', "'s", 'Ġsurface', 'Ġapart', 'Ġpoles', 'Ġoverall', 'Ġglobal', 'Ġbeam', 'Ġcoverage', 'Ġextends', 'Ġlat', 'itudes', 'ĠâĪĴ', 'Â°', 'Ġregardless', 'Ġlong', 'itude', 'Ġregional', 'Ġbeam', 'Ġcovers', 'Ġfraction', 'Ġarea', 'Ġcovered', 'Ġglobal', 'Ġbeam', 'Ġcollectively', 'Ġregional', 'Ġbeams', 'Ġoffer', 'Ġvirtually', 'Ġcoverage', 'Ġglobal', 'Ġbeams', 'Ġuse', 'Ġregional', 'Ġbeams', 'Ġallow', 'Ġuser', 'Ġterminals', 'also', 'Ġcalled', 'Ġmobile', 'Ġearth', 'Ġstations', 'Ġoperate', 'Ġsignificantly', 'Ġsmaller', 'Ġantennas', 'Ġregional', 'Ġbeams', 'Ġintroduced', 'Ġsatellites', 'Ġsatellite', 'Ġprovides', 'Ġfour', 'Ġspot', 'Ġbeams', 'Ġsatellite', 'Ġprovides', 'Ġregional', 'Ġbeams', 'Ġnarrow', 'Ġbeams', 'Ġoffered', 'Ġthree', 'ars', 'Ġsatellites', 'Ġnarrow', 'Ġbeams', 'Ġvary', 'Ġsize', 'Ġtend', 'Ġseveral', 'Ġhundred', 'Ġkilometres', 'Ġacross', 'Ġnarrow', 'Ġbeams', 'Ġmuch', 'Ġsmaller', 'Ġglobal', 'Ġregional', 'Ġbeams', 'Ġfar', 'Ġnumerous', 'Ġhence', 'Ġoffer', 'Ġglobal', 'Ġcoverage', 'Ġnarrow', 'Ġspot', 'Ġbeams', 'Ġallow', 'Ġyet', 'Ġcoverage', 'Ġglobal', 'Ġbeam', 'Ġcoverage', 'Ġregional', 'Ġspot', 'Ġbeam', 'Ġcoverage', 'Ġnarrow', 'Ġspot', 'Ġbeam', 'Ġcoverage', 'ars', 'Ġwik', 'ipedia', 'Ġsmaller', 'Ġantennas', 'Ġmuch', 'Ġhigher', 'Ġdata', 'Ġrates', 'Ġform', 'Ġbackbone', 'ars', "'s", 'Ġhandheld', 'gs', 'ps', 'Ġbroadband', 'Ġservices', 'Ġcoverage', 'Ġintroduced', 'Ġsatellites', 'Ġsatellite', 'Ġprovides', 'Ġaround', 'Ġnarrow', 'Ġspot', 'Ġbeams', 'ars', 'Ġsatellites', 'Ġprovide', 'Ġglobal', 'Ġcoverage', 'Ġusing', 'Ġfour', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġsatellite', 'Ġsupports', 'Ġbeams', 'Ġgiving', 'Ġtotal', 'Ġcoverage', 'Ġapproximately', 'Ġone', 'third', 'Ġearth', "'s", 'Ġsurface', 'Ġper', 'Ġsatellite', 'Ġaddition', 'Ġsteer', 'able', 'Ġbeams', 'Ġavailable', 'Ġper', 'Ġsatellite', 'Ġmay', 'Ġmoved', 'Ġprovide', 'Ġhigher', 'Ġcapacity', 'Ġselected', 'Ġlocations', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġwik', 'ipedia', 'Ġsatellite', 'mber', 'Ġfirst', 'Ġsatellite', 'Ġextend', 'Ġoriginal', 'Ġsatellite', 'Ġfirst', 'Ġgeneration', 'Ġglobal', 'Ġx', 'press', 'Ġconstellation', 'Ġlaunched', 'Ġcentre', 'Ġspatial', 'Ġguy', 'ana', 'ri', 'ane', 'Ġlaunch', 'Ġvehicle', 'Ġsatellite', 'Ġcoverage', 'Ġlong', 'itude', 'Ġvehicles', 'Ġlaunch', 'Ġdate', 'ut', 'c', 'Ġservices', 'Ġnotes', 'Ġmar', 'Ġseries', 'Ġmar', 'Ġdelta', 'Ġfe', 'b', 'ruary', 'Ġdecom', 'mission', 'ed', 'Ġmar']</t>
+          <t>['Ġboosters', 'Ġsecondary', 'Ġpayload', 'Ġinclude', 'Ġorbit', 'ers', 'Ġlights', 'ail', 'Ġot', 'b', 'host', 'ing', 'Ġdeep', 'Ġspace', 'Ġatomic', 'Ġclock', '])', 'Ġcosmic', 'culus', 'r', 'Ġprox', 'Ġsuccessfully', 'Ġreused', 'Ġboosters', 'Ġsecond', 'Ġfal', 'con', 'Ġheavy', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcenter', 'Ġcore', 'Ġbooster', 'Ġland', 'Ġsuccessfully', 'Ġdestroyed', 'Ġupon', 'Ġimpact', 'l', 'antic', 'Ġocean', 'mber', 'Ġus', 'sf', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmillennium', 'Ġspace', 'Ġsystems', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'us', 'Ġmillion', 'Ġus', 'Ġmillion', 'Ġcontract', 'Ġincluding', 'Ġtwo', 'Ġfal', 'con', '])', 'Ġsuccess', 'Ġfirst', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġcontract', 'Ġawarded', 'Ġspace', 'x', 'Ġprice', 'Ġtypical', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlaunch', 'us', 'Ġmillion', 'Ġpayload', 'Ġincludes', 'Ġtwo', 'Ġseparate', 'Ġsatellites', 'Ġleast', 'Ġthree', 'Ġadditional', 'Ġrides', 'hare', 'Ġpayload', 'including', 'Ġtet', 'ra', ')[', 'Ġweighs', 'Ġroughly', 'Ġlaunch', 'Ġlaunched', 'Ġdirect', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġnecess', 'itating', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtime', 'Ġplanned', 'Ġpartially', 'Ġexpend', 'able', 'Ġlaunch', 'Ġdeliberately', 'Ġexpend', 'Ġcenter', 'Ġcore', 'Ġlacks', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġlanding', 'Ġgear', 'Ġneeded', 'Ġlanding', 'Ġtwo', 'Ġside', 'boost', 'ers', 'Ġlanded', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġoriginally', 'Ġscheduled', 'Ġdelayed', 'Ġdue', 'Ġpayload', 'Ġissues', 'mber', 'Ġsecond', 'Ġstage', 'Ġfeatured', 'Ġgray', 'Ġband', 'Ġdue', 'Ġlong', 'Ġcoast', 'Ġphase', 'Ġsubsequent', 'Ġburns', 'Ġallow', 'Ġheat', 'Ġsunlight', 'Ġabsorbed', 'Ġwarm', 'Ġk', 'eros', 'ene', 'Ġtank', 'Ġlonger', 'Ġcoast', 'ing', 'Ġperiod', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġf', 'h', 'Ġthird', 'Ġfal', 'con', 'Ġrocket', 'Ġgets', 'Ġcold', 'Ġk', 'eros', 'ene', 'Ġfreezes', 'Ġmuch', 'Ġhigher', 'Ġtemperature', 'Ġfal', 'con', 'âĢ', 'Ļ', 'Ġliquid', 'Ġoxid', 'izer', 'Ġbecomes', 'Ġvisc', 'ous', 'Ġsl', 'ush', 'like', 'Ġfreezes', 'Ġsolid', 'Ġingested', 'Ġsl', 'ush', 'Ġfuel', 'Ġwould', 'Ġlikely', 'Ġprevent', 'Ġignition', 'Ġdestroy', 'Ġupper', 'Ġstage', 'âĢ', 'Ļ', 'Ġmer', 'lin', 'Ġengine', 'Ġjan', 'uary']</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -2960,7 +2960,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>['Ġdelta', 'Ġoct', 'ober', 'Ġtransferred', 'Ġint', 'els', 'Ġdecom', 'mission', 'ed', 'Ġmar', 'Ġdelta', 'Ġj', 'une', 'Ġdecom', 'mission', 'ed', 'cs', 'Ġseries', 'cs', 'ri', 'ane', 'Ġde', 'cember', 'Ġde', 'activated', 'Ġaug', 'ust', 'cs', 'b', 'ri', 'ane', 'Ġse', 'pt', 'ember', 'Ġlaunch', 'Ġfailure', 'cs', 'c', 'ri', 'ane', 'mber', 'Ġalso', 'Ġknown', 'cs', 'b', 'Ġde', 'activated', 'ars', 'Ġseries', 'ars', 'Ġdelta', 'Ġoct', 'ober', 'Ġdecom', 'mission', 'ed', 'Ġapr', 'il', 'Ġprevious', 'Ġrecord', 'Ġholder', 'Ġmission', 'Ġlifespan', 'ars', 'Ġdelta', 'Ġmarch', 'Ġdecom', 'mission', 'ed', 'Ġde', 'cember', 'Ġsatellites', 'ars', 'Ġwik', 'ipedia', 'Ġworld', 'Ġrecord', 'Ġmission', 'Ġlifespan', 'ars', 'ri', 'ane', 'Ġde', 'cember', 'Ġdecom', 'mission', 'ed', 'ars', 'ri', 'ane', 'Ġapr', 'il', 'Ġdecom', 'mission', 'ed', 'ars', 'Ġseries', 'ars', 'las', 'Ġapr', 'il', 'Ġreass', 'igned', 'Ġmaritime', 'Ġsafety', 'Ġbackup', 'Ġservice', 'ars', 'Ġpro', 'ton', 'k', 'dm', 'Ġse', 'pt', 'ember', 'Ġreass', 'igned', 'Ġmaritime', 'Ġsafety', 'Ġbackup', 'Ġservice', 'ars', 'Â°', 'Ġeast', 'las', 'Ġde', 'cember', 'Ġexisting', 'Ġevolved', 'Ġservices', 'ars', 'ri', 'ane', 'Ġj', 'une', 'Ġdecom', 'mission', 'ed', 'ars', 'Â°', 'Ġwest', 'ri', 'ane', 'Ġfe', 'b', 'ruary', 'Ġvarious', 'Ġleases', 'ars', 'Ġseries', 'ars', 'Ġap', 'ac', 'Â°', 'Ġeast', 'las', 'Ġmarch', 'Ġfamily', 'Ġsp', 'Ġlease', 'Ġservices', 'ars', 'Â°', 'Ġeast', 'Ġz', 'en', 'sl', 'mber', 'Ġfamily', 'Ġsp', 'Ġlease', 'Ġservices', 'Ġfleet', 'broad', 'band', 'Ġswift', 'broad', 'band', 'Ġtransferred', 'Â°', 'Ġeast', 'Â°', 'Ġeast', 'Ġmid', 'ars', 'mer', 'Â°', 'Ġwest', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġaug', 'ust', 'Ġfamily', 'Ġlease', 'Ġservices', 'ars', 'al', 'phas', ')[', 'Ġem', 'ea', 'Â°', 'Ġeast', 'ri', 'ane']</t>
+          <t>['Ġu', 'Ġspace', 'Ġforce', 'Ġus', 'Ġmillion', 'includes', 'Ġnew', 'Ġsuccess', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġused', 'Ġnew', 'Ġcenter', 'Ġcore', 'Ġexpend', 'able', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġlanding', 'Ġgear', 'Ġtwo', 'Ġreused', 'Ġside', 'boost', 'ers', 'Ġlanded', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġsecond', 'Ġstage', 'Ġgray', 'Ġband', 'Ġthermal', 'Ġpurposes', 'Ġmission', 'Ġrequirements', 'Ġsimilar', 'Ġus', 'sf', 'Ġmission', 'Ġmay', 'Ġ00', 'Ġv', 'ias', 'Ġameric', 'Ġar', 'ct', 'urus', 'aur', 'ora', ')[', 'Ġg', 'space', 'aka', 'Ġn', 'us', 'ant', 'ara', 'h', 'Ġv', 'ias', 'str', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġdat', 'ap', 'ort', 'Ġpt', 'Ġp', 'asi', 'ï', '¬', 'ģ', 'k', 'ate', 'lit', 'Ġn', 'us', 'ant', 'ara', 'Ġsuccess', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginally', 'Ġslated', 'Ġlaunch', 'Ġv', 'ias', 'Ġsatellite', 'Ġdue', 'Ġdelays', 'ri', 'ane', 'Ġlaunch', 'Ġvehicle', 'Ġused', 'Ġinstead', 'Ġv', 'ias', 'Ġmaintained', 'Ġlaunch', 'Ġoption', 'Ġdelivered', 'Ġnext', 'Ġka', 'band', 'Ġsatellite', 'Ġaboard', 'Ġfal', 'con', 'Ġheavy', 'Ġone', 'Ġintended', 'Ġprovide', 'Ġservice', 'Ġameric', 'Ġregion', 'str', 'Ġmicro', 'ge', 'Ġsatellite', 'Ġar', 'ct', 'urus', 'Ġadded', 'Ġindependent', 'Ġsecondary', 'Ġpayload', 'Ġlate', 'Ġse', 'pt', 'ember', 'Ġfollowing', 'Ġseries', 'Ġengine', 'Ġburns', 'Ġlong', 'Ġperiods', 'Ġcoast', 'ing', 'Ġupper', 'Ġstage', 'Ġfal', 'con', 'Ġheavy', 'Ġdeployed', 'Ġsatellite', 'Ġnear', 'ge', 'os', 'ynchronous', 'Ġorbit', 'Ġapproximately', 'Ġupper', 'Ġstage', 'Ġwent', 'Ġsuccessfully', 'Ġdeploy', 'Ġadditional', 'Ġpayload', 'Ġg', 'space', 'Ġar', 'ct', 'urus', 'Ġsecond', 'Ġstage', 'Ġgray', 'Ġband', 'Ġreason', 'Ġus', 'sf', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġexpend', 'Ġthree', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcores', 'Ġj', 'uly', 'Ġ03', '04', 'Ġj', 'upiter', 'ech', 'ost', 'ar', ')[', 'Ġe', 'ch', 'ost', 'ar', 'Ġsuccess', 'Ġheaviest', 'Ġcommercial', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġweighing', 'Ġlaunch', 'Ġsecond', 'Ġstage', 'Ġgray', 'Ġband', 'Ġreason', 'Ġus', 'sf', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtime', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'ured', 'Ġmedium', 'Ġcoast']</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>['eca', 'Ġj', 'uly', 'Ġfamily', 'Ġsp', 'Ġlease', 'Ġservices', 'ars', 'Ġseries', 'ars', 'Ġeuro', 'pe', 'Ġmiddle', 'Ġeast', 'Ġaf', 'rica', 'Â°', 'Ġeast', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġde', 'cember', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġameric', 'Â°', 'Ġwest', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġfe', 'b', 'ruary', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'ia', 'Ġwest', 'Ġameric', 'Â°', 'Ġeast', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġaug', 'ust', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġeuro', 'pe', 'orbit', 'Ġspare', 'Â°', 'Ġeast', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmay', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġeuro', 'pe', 'Ġmiddle', 'Ġeast', 'Â°', 'Ġeast', 'ri', 'ane', 'eca', 'mber', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġhigher', 'Ġcapacity', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġgeneration', 'Ġsatellites', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'ars', 'Ġe', 'hell', 'Ġsat', ')[', 'Ġeuro', 'pe', 'Â°', 'Ġeast', 'ri', 'ane', 'Ġj', 'une', 'band', 'Ġservices', 'Ġeuro', 'pe', 'Ġaviation', 'ars', 'Ġseries', 'ars', 'Ġf', 'Ġde', 'cember', 'ars', 'Ġfal', 'con', 'Ġblock', 'Ġfe', 'b', 'ruary', 'Ġpermanent', 'Ġtelephone', 'Ġcountry', 'Ġcode', 'Ġcalling', 'ars', 'Ġdestinations', 'Ġsn', 'ac', 'single', 'Ġnetwork', 'Ġaccess', 'Ġcode', 'Ġnumber', 'Ġautomatic', 'Ġloc', 'ator', 'Ġnecessary', 'Ġknow', 'Ġsatellite', 'Ġdestination', 'ars', 'Ġterminal', 'Ġlogged', 'Ġsn', 'ac', 'Ġusable', 'ars', 'Ġservices', 'Ġcountry', 'Ġcodes', 'Ġphased', 'Ġde', 'cember', 'l', 'antic', 'Ġocean', 'Ġregion', 'Ġeast', 'e', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġocean', 'Ġregion', 'por', 'Ġind', 'ian', 'Ġocean', 'Ġregion', 'ior', 'l', 'antic', 'Ġocean', 'Ġregion', 'Ġwest', 'Ġcountry', 'Ġcodes']</t>
+          <t>['Ġphase', 'Ġcore', 'Ġexpended', 'Ġtwo', 'Ġboosters', 'Ġrecovered', 'Ġland', 'Ġpayload', 'Ġfair', 'ing', 'Ġrecovery', 'Ġattempted', 'Ġoct', 'ober', 'Ġpsyche', 'Ġn', 'asa', 'iscovery', 'Ġus', 'Ġmillion', 'Ġsuccess', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunched', 'Ġpsyche', 'Ġorbit', 'er', 'Ġmission', 'Ġhel', 'oc', 'entric', 'Ġorbit', 'Ġpsyche', 'Ġspacecraft', 'Ġvisit', 'Ġpsyche', 'Ġasteroid', 'Ġmain', 'Ġasteroid', 'Ġbelt', 'Ġcore', 'Ġexpended', 'Ġtwo', 'Ġboosters', 'Ġrecovered', 'Ġland', 'Ġnet', 'Ġde', 'cember', 'Ġus', 'sf', 'Ġu', 'Ġspace', 'Ġforce', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġsecond', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġawarded', 'Ġj', 'une', 'Ġnet', 'Ġapr', 'il', 'Ġgoes', 'u', 'Ġn', 'asa', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġse', 'pt', 'ember', 'Ġn', 'asa', 'Ġawarded', 'Ġspace', 'x', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġge', 'ost', 'ation', 'ary', 'Ġgoes', 'u', 'Ġweather', 'Ġsatellite', 'Ġnet', 'Ġoct', 'ober', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġn', 'asa', 'plan', 'etary', 'Ġmissions', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġconduct', 'Ġdetailed', 'Ġsurvey', 'Ġeuro', 'pa', 'Ġuse', 'Ġsophisticated', 'Ġsuite', 'Ġscience', 'Ġinstruments', 'Ġinvestigate', 'Ġwhether', 'Ġicy', 'Ġmoon', 'Ġconditions', 'Ġsuitable', 'Ġlife', 'Ġkey', 'Ġmission', 'Ġobjectives', 'Ġproduce', 'Ġhigh', 'resolution', 'Ġimages', 'Ġeuro', 'pa', "'s", 'Ġsurface', 'Ġdetermine', 'Ġcomposition', 'Ġlook', 'Ġsigns', 'Ġrecent', 'Ġongoing', 'Ġgeological', 'Ġactivity', 'Ġmeasure', 'Ġthickness', 'Ġmoon', "'s", 'Ġicy', 'Ġshell', 'Ġsearch', 'Ġsubs', 'ur', 'face', 'Ġlakes', 'Ġdetermine', 'Ġdepth', 'Ġsal', 'inity', 'Ġeuro', 'pa', "'s", 'Ġocean', 'Ġmission', 'Ġï', '¬', 'Ĥ', 'Ġpast', 'Ġmars', 'Ġearth', 'Ġarriving', 'Ġj', 'upiter', 'Ġapr', 'il', 'Ġnet', 'mber', 'Ġv', 'iper', 'gr', 'ï', '¬', 'ģ', 'n', 'Ġmission', 'Ġast', 'rob', 'otic', 'n', 'asa', 'art', 'emis', 'Ġundisclosed', 'list', 'Ġprice', 'Ġmillion', 'Ġplanned', 'Ġast', 'rob', 'otic', "'s", 'Ġgr', 'ï', '¬', 'ģ', 'n', 'Ġlunar', 'Ġland', 'er', 'Ġdeliver', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġspacecraft', 'Ġlunar', 'Ġsouth', 'Ġpole', 'Ġexpected', 'Ġrecover', 'Ġboosters', 'Ġnet', 'Ġde', 'cember', 'Ġpower', 'Ġpropulsion', 'Ġelement', 'ppe', 'Ġn', 'asa', 'art', 'emis', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia']</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -2986,7 +2986,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>['ars', 'Ġwik', 'ipedia', 'ars', 'Ġsatellite', 'Ġlocations', 'Ġsince', 'Ġj', 'uly', 'ars', 'Ġusers', 'Ġusing', 'Ġservice', 'Ġprovided', 'Ġch', 'ina', 'Ġtransport', 'Ġtele', 'communication', 'Ġinformation', 'Ġcenter', 'Ġmay', 'Ġapply', 'Ġdigits', 'Ġch', 'inese', 'Ġmobile', 'Ġphone', 'Ġnumbers', 'Ġstarting', 'Ġinternational', 'Ġcall', 'Ġfunction', 'Ġrequired', 'Ġmaking', 'Ġphone', 'Ġcalls', 'Ġnumbers', 'Ġmainland', 'Ġch', 'ina', 'ars', 'Ġnetworks', 'Ġprovide', 'Ġexisting', 'Ġevolved', 'Ġadvanced', 'Ġservices', 'Ġexisting', 'Ġevolved', 'Ġservices', 'Ġoffered', 'Ġland', 'Ġearth', 'Ġstations', 'Ġowned', 'Ġoperated', 'ars', 'Ġcompanies', 'Ġcommercial', 'Ġagreement', 'ars', 'Ġadvanced', 'Ġservices', 'Ġprovided', 'Ġvia', 'Ġdistribution', 'Ġpartners', 'Ġsatellite', 'Ġgate', 'ways', 'Ġowned', 'Ġoperated', 'ars', 'Ġdirectly', 'Ġglobal', 'Ġx', 'press', 'Ġsince', 'ars', 'Ġoffered', 'Ġhigh', 'Ġthroughput', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġservice', 'Ġprovides', 'Ġbased', 'Ġglobal', 'Ġservice', 'bit', 'link', 'bit', 'Ġupl', 'ink', 'Ġlatency', 'Ġservices', 'Ġprovided', 'Ġmaritime', 'Ġaviation', 'Ġgovernment', 'Ġenterprise', 'Ġmarkets', 'Ġglobal', 'Ġx', 'press', 'Ġsupported', 'Ġexisting', 'Ġl', 'band', 'Ġnetwork', 'Ġservices', 'Ġoffered', 'Ġusing', 'Ġcombination', 'Ġtwo', 'Ġnetworks', 'Ġincrease', 'Ġavailability', 'Ġreliability', 'Ġmarch', 'ars', 'Ġpartnered', 'Ġisot', 'rop', 'ic', 'Ġsystems', 'Ġdevelop', 'elect', 'ronic', 'Ġscanning', 'Ġantenna', 'Ġintended', 'Ġused', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'ars', 'Ġoffers', 'Ġaviation', 'Ġservices', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġdeveloped', 'Ġpartnership', 'Ġde', 'utsche', 'Ġtele', 'k', 'om', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġuses', 'Ġground', 'based', 'Ġl', 'te', 'Ġnetwork', 'ars', 'band', 'Ġsatellite', 'Ġprovide', 'g', 'bit', 'Ġcapacity', 'Ġaircraft', 'Ġeuro', 'pe', 'Ġairspace', 'Ġproject', 'Ġfaced', 'Ġnumber', 'Ġlegal', 'Ġregulatory', 'Ġchallenges', 'Ġoct', 'ober', 'ars', 'Ġstated', 'Ġcommercial', 'Ġservice', 'Ġwould', 'Ġbegin', 'Ġconstruction', 'Ġground', 'Ġnetwork', 'Ġcompleted', 'Ġfe', 'b', 'ruary', 'Ġmid', 'Ġservice', 'Ġoffered', 'Ġroutes', 'Ġkey', 'Ġdestinations', 'Ġl', 'ondon', 'Ġmad', 'rid', 'Ġbar', 'celona', 'hens', 'Ġl', 'bon', 'Ġpr', 'ague', 'Ġr', 'ome', 'Ġvi', 'enna', 'Ġearly']</t>
+          <t>['Ġhabit', 'ation', 'Ġlogistics', 'Ġoutpost', 'h', 'alo', 'Ġfirst', 'Ġelements', 'Ġgateway', 'Ġmini', 'station', 'Ġpart', 'Ġart', 'emis', 'Ġprogram', 'Ġawarded', 'Ġfe', 'b', 'ruary', 'Ġmax', 'ar', 'Ġalready', 'Ġmade', 'Ġmillion', 'Ġpayments', 'Ġspace', 'x', 'Ġcontract', 'Ġlaunch', 'Ġp', 'pe', 'Ġlater', 'Ġn', 'asa', 'Ġdecided', 'Ġlaunch', 'Ġp', 'pe', 'Ġh', 'alo', 'Ġtogether', 'Ġnet', 'Ġoct', 'ober', 'Ġn', 'ancy', 'Ġgrace', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'launch', 'Ġservices', 'Ġprogram', 'Ġmillion', 'Ġplanned', 'Ġinfrared', 'Ġspace', 'Ġtelescope', 'Ġstationed', 'Ġsun', 'earth', 'Ġl', 'ba', 'Ġast', 'rob', 'otic', 'ba', 'dragon', 'Ġn', 'asa', 'gate', 'way', 'Ġlogistics', 'Ġservices', 'Ġplanned', 'Ġmarch', 'Ġn', 'asa', 'Ġannounced', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcontract', 'Ġgateway', 'Ġlogistics', 'Ġservices', 'Ġguarantees', 'Ġleast', 'Ġtwo', 'Ġlaunches', 'Ġnew', 'Ġdragon', 'Ġres', 'upp', 'ly', 'Ġspacecraft', 'Ġtop', 'Ġfal', 'con', 'Ġheavy', 'Ġcarry', '000', 'Ġcargo', 'Ġlunar', 'Ġorbit', 'âĢĵ', 'Ġmonths', 'Ġlong', 'Ġmissions', 'dragon', 'Ġn', 'asa', 'gate', 'way', 'Ġlogistics', 'Ġservices', 'Ġplanned', 'Ġsecond', 'Ġdragon', 'Ġï', '¬', 'Ĥ', 'ight', 'ba', 'ba', 'Ġint', 'els', 'ba', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcommercial', 'Ġagreement', 'Ġfal', 'con', 'Ġheavy', 'Ġsigned', 'Ġmay', 'Ġoption', 'Ġstill', 'Ġmaintained', 'Ġsatellite', 'Ġchosen', 'Ġmay', 'Ġspace', 'x', 'Ġannounced', 'Ġint', 'els', 'Ġsigned', 'Ġfirst', 'Ġcommercial', 'Ġcontract', 'Ġfal', 'con', 'Ġheavy', 'Ġflight', 'Ġconfirmed', 'Ġtime', 'Ġfirst', 'Ġint', 'els', 'Ġlaunch', 'Ġwould', 'Ġoccur', 'Ġagreement', 'Ġspace', 'x', 'Ġdelivering', 'Ġsatellites', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', ').[', 'Ġaug', 'ust', 'Ġemerged', 'Ġint', 'els', 'Ġcontract', 'Ġreass', 'igned', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmission', 'Ġdeliver', 'Ġint', 'els', 'Ġorbit', 'Ġthird', 'Ġquarter', 'Ġperformance', 'Ġimprovements', 'Ġfal', 'con', 'Ġvehicle', 'Ġfamily', 'Ġsince', 'Ġannouncement', 'Ġadvertising', '000', 'Ġg', 'Ġexpend', 'able', 'Ġflight', 'Ġprofile', 'Ġenable', 'Ġlaunch', 'Ġsatellite', 'Ġwithout', 'Ġupgrading', 'Ġfal', 'con', 'Ġheavy', 'Ġvariant', 'ars', 'Ġbooked', 'Ġthree']</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>['Ġservice', 'Ġused', '000', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġthroughout', 'Ġeuro', 'pe', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġaircraft', 'Ġoperated', 'Ġb', 'rit', 'ish', 'Ġair', 'ways', 'ber', 'ia', 'Ġv', 'uel', 'ing', 'Ġfamily', 'Ġset', 'Ġip', 'based', 'Ġshared', 'car', 'rier', 'Ġservices', ':[', 'Ġbroadband', 'Ġglobal', 'Ġarea', 'Ġnetwork', 'Ġuse', 'Ġland', 'Ġuses', 'Ġsatellites', 'Ġoffer', 'Ġshared', 'channel', 'Ġpacket', 'sw', 'itched', 'Ġservice', 'Ġk', 'bit', 'u', 'pl', 'ink', 'link', 'Ġspeeds', 'Ġmay', 'Ġdiffer', 'Ġdepend', 'Ġterminal', 'Ġmodel', 'Ġstreaming', 'ip', 'Ġservice', 'Ġk', 'bit', 'Ġx', 'stream', 'Ġdata', 'Ġrate', 'services', 'Ġdepend', 'Ġterminal', 'Ġmodel', 'Ġterminals', 'Ġalso', 'Ġoffer', 'Ġcircuit', 'sw', 'itched', 'Ġmobile', 'Ġintegrated', 'Ġservices', 'Ġdigital', 'Ġnetwork', 'isd', 'n', 'Ġservices', 'Ġk', 'bit', 'Ġeven', 'Ġlow', 'Ġspeed', 'Ġk', 'bit', 'Ġvoice', 'Ġetc', 'Ġservices', 'Ġservice', 'Ġavailable', 'Ġglobally', 'Ġsatellites', 'Ġfleet', 'broad', 'band', 'Ġmaritime', 'Ġservice', 'Ġfleet', 'broad', 'band', 'Ġbased', 'Ġtechnology', 'Ġoffering', 'Ġsimilar', 'Ġservices', 'Ġusing', 'Ġinfrastructure', 'Ġrange', 'Ġfleet', 'Ġbroadband', 'Ġuser', 'Ġterminals', 'Ġavailable', 'Ġdesigned', 'Ġships', 'Ġnetworks', 'Ġhigh', 'Ġthroughput', 'Ġservices', 'Ġadvanced', 'Ġservices', 'ars', 'Ġwik', 'ipedia', 'Ġswift', 'broad', 'band', 'Ġaer', 'autical', 'Ġservice', 'Ġswift', 'broad', 'band', 'Ġbased', 'Ġtechnology', 'Ġoffers', 'Ġsimilar', 'Ġservices', 'Ġterminals', 'Ġdesigned', 'Ġcommercial', 'Ġprivate', 'Ġmilitary', 'Ġaircraft', 'Ġfamily', 'Ġset', 'Ġip', 'based', 'Ġservices', 'Ġdesigned', 'Ġlong', 'term', 'Ġmachine', 'machine', 'Ġmanagement', 'Ġfixed', 'Ġassets', ':[', 'Ġlaunched', 'Ġjan', 'uary', 'Ġglobal', 'Ġip', 'based', 'Ġlow', 'data', 'Ġrate', 'Ġservice', 'Ġdesigned', 'Ġhigh', 'Ġdata', 'Ġavailability', 'Ġperformance', 'Ġpermanently', 'Ġunmanned', 'Ġenvironments', 'Ġhigh', 'frequency', 'Ġlow', 'lat', 'ency', 'Ġdata', 'Ġreporting', 'Ġintended', 'Ġmonitoring', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġassets', 'Ġpipelines', 'Ġoil', 'Ġwell', 'Ġheads', 'Ġback', 'haul', 'ing', 'Ġelectricity', 'Ġconsumption', 'Ġdata', 'Ġwithin', 'Ġutility', 'Ġglobal', 'Ġshort', 'Ġburst', 'Ġdata', 'Ġstore', 'Ġforward', 'Ġservice', 'Ġintended', 'Ġdeliver', 'Ġmessages', 'Ġbytes', 'Ġsend', 'Ġdirection', 'Ġbytes', 'Ġreceive', 'Ġdirection', 'Ġservice', 'Ġdelivered', 'Ġmarket', 'Ġvia', 'Ġsky', 'wave', 'Ġmobile', 'Ġcommunications', 'Ġhoney', 'well', 'Ġglobal', 'Ġtracking', 'data', 'Ġpro', 'data', 'Ġpro', 'Ġglobal', 'Ġsatellite', 'Ġdata', 'Ġservice', 'Ġdesigned', 'Ġtwo', 'way', 'Ġtext', 'Ġdata', 'Ġcommunications', 'Ġremote', 'Ġassets']</t>
+          <t>['Ġlaunches', 'Ġfal', 'con', 'Ġheavy', 'Ġdue', 'Ġdelays', 'Ġswitched', 'Ġpayload', 'ri', 'ane', 'Ġsimilarly', 'Ġint', 'els', 'Ġcase', 'Ġanother', 'Ġsatellite', 'Ġcontract', 'ars', 'Ġswitched', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġdue', 'Ġincreased', 'Ġlif', 'ff', 'Ġcapacity', 'Ġremaining', 'Ġcontract', 'Ġcovered', 'Ġlaunch', 'ars', 'Ġfal', 'con', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġannounced', 'Ġfirst', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġcontract', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'od', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'Ġawarded', 'Ġspace', 'x', 'Ġtwo', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'e', 'el', 'v', ')-', 'class', 'Ġmissions', 'Ġincluding', 'Ġspace', 'Ġfirst', 'Ġcommercial', 'Ġcontracts', 'Ġdepartment', 'Ġdefense', 'Ġcontracts', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġtest', 'Ġprogram', 'Ġmission', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginally', 'Ġscheduled', 'Ġlaunched', 'Ġmarch', 'Ġplaced', 'Ġnear', 'Ġcircular', 'Ġorbit', 'Ġaltitude', 'Ġmi', 'Ġinclination', 'Â°', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġsent', 'Ġu', 'Ġair', 'Ġforce', 'Ġupdated', 'Ġletter', 'Ġintent', 'Ġoutlining', 'Ġcertification', 'Ġprocess', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġnational', 'Ġsecurity', 'Ġsatellites', 'Ġprocess', 'Ġincludes', 'Ġthree', 'Ġsuccessful', 'Ġflights', 'Ġfal', 'con', 'Ġheavy', 'Ġincluding', 'Ġtwo', 'Ġconsecutive', 'Ġsuccessful', 'Ġflights', 'Ġletter', 'Ġstated', 'Ġfal', 'con', 'Ġheavy', 'Ġready', 'Ġfly', 'Ġnational', 'Ġsecurity', 'Ġpayload', 'Ġj', 'uly', 'Ġspace', 'x', 'Ġannounced', 'Ġfirst', 'Ġtest', 'Ġflight', 'Ġwould', 'Ġtake', 'Ġplace', 'Ġde', 'cember', 'Ġpushing', 'Ġlaunch', 'Ġsecond', 'Ġlaunch', 'space', 'Ġtest', 'Ġprogram', 'Ġj', 'une', 'Ġmay', 'Ġoccasion', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'Ġblock', 'Ġvariant', 'Ġdelay', 'Ġoct', 'ober', 'Ġannounced', 'Ġlaunch', 'Ġeventually', 'Ġpushed', 'Ġj', 'une', 'Ġmission', 'Ġused', 'Ġthree', 'Ġblock', 'Ġcores', 'Ġspace', 'x', 'Ġawarded', 'Ġlaunches', 'Ġphase', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'n', 'ssl', 'Ġcontracts', 'Ġincludes', 'Ġseveral', 'Ġlaunches', 'Ġvertical', 'Ġintegration', 'Ġfacility', 'Ġdevelopment', 'Ġlarger', 'Ġfair', 'ing', 'Ġpayload', 'Ġmission', 'Ġdepartment', 'Ġdefense', 'Ġincluded', 'Ġsmall', 'Ġspacecraft', 'Ġu', 'Ġmilitary', 'Ġn', 'asa', 'Ġresearch', 'Ġinstitutions']</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>['Ġmessage', 'Ġsize', 'Ġmobile', 'Ġk', 'bytes', 'Ġmobile', 'Ġk', 'bytes', 'Ġtypical', 'Ġdelivery', 'Ġtime', 'Ġseconds', 'Ġservice', 'Ġintended', 'Ġmission', 'critical', 'Ġapplications', 'Ġmanaging', 'Ġtrucks', 'Ġï', '¬', 'ģ', 'hing', 'Ġvessels', 'Ġoil', 'Ġgas', 'Ġheavy', 'Ġequipment', 'Ġtext', 'Ġmessage', 'Ġremote', 'Ġworkers', 'Ġsecurity', 'Ġapplications', 'Ġprovided', 'Ġsky', 'wave', 'Ġmobile', 'Ġcommunications', 'Ġinc', 'Ġpart', 'Ġorb', 'comm', 'Ġcompany', 'Ġoffers', 'Ġportable', 'Ġfixed', 'Ġphone', 'Ġservices', ':[', 'phone', 'phone', 'Ġmobile', 'Ġsatellite', 'Ġphone', 'Ġoffering', 'Ġvoice', 'Ġtele', 'phony', 'Ġvariety', 'Ġdata', 'Ġcapabilities', 'Ġincluding', 'Ġsm', 'Ġshort', 'Ġmessage', 'Ġemail', 'ing', 'Ġlook', 'send', 'Ġwell', 'Ġsupporting', 'Ġdata', 'Ġservice', 'phone', 'Ġlink', 'phone', 'Ġlink', 'Ġlow', 'cost', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġglobal', 'Ġsatellite', 'Ġphone', 'Ġservice', 'Ġprovides', 'Ġvoice', 'Ġconnectivity', 'Ġworking', 'Ġliving', 'Ġareas', 'Ġwithout', 'Ġcellular', 'Ġcoverage', 'Ġincludes', 'Ġdata', 'Ġcapabilities', 'Ġfleet', 'phone', 'ars', "'s", 'Ġfleet', 'phone', 'Ġservice', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġphone', 'Ġservice', 'Ġuse', 'Ġsmaller', 'Ġvessels', 'Ġvoice', 'Ġcommunications', 'Ġprimary', 'Ġrequirement', 'Ġvessels', 'Ġadditional', 'Ġvoice', 'Ġlines', 'Ġneeded', 'Ġprovides', 'Ġlow', 'cost', 'Ġglobal', 'Ġsatellite', 'Ġphone', 'Ġservice', 'Ġoption', 'Ġworking', 'Ġsailing', 'Ġoutside', 'Ġcellular', 'Ġcoverage', 'Ġbased', 'Ġolder', 'Ġtechnologies', ':[', 'Ġaer', 'autical', 'classic', 'ero', '):', 'Ġprovides', 'Ġanalogue', 'Ġvoice', 'fax', 'data', 'Ġservices', 'Ġaircraft', 'Ġthree', 'Ġlevels', 'Ġterminals', 'ero', 'l', 'low', 'Ġgain', 'Ġantenna', 'Ġprimarily', 'Ġpacket', 'Ġdata', 'Ġincluding', 'Ġac', 'ars', 'Ġads', 'ero', 'h', 'high', 'Ġgain', 'Ġantenna', 'Ġmedium', 'Ġquality', 'Ġvoice', 'Ġfax', 'data', 'Ġbit', 'ero', 'inter', 'mediate', 'Ġgain', 'Ġantenna', 'Ġlow', 'Ġquality', 'Ġvoice', 'Ġfax', 'data', 'Ġbit', 'Ġnote', 'Ġalso', 'Ġaircraft', 'Ġrated', 'Ġversions', 'ars', 'c', 'Ġmini', 'Ġaircraft', 'Ġversion', 'Ġg', 'Ġcalled', 'Ġswift', 'see', 'Ġcommunications', 'Ġglobal', 'Ġvoice', 'Ġservices', 'Ġexisting', 'Ġevolved', 'Ġservices', 'ars', 'Ġwik', 'ipedia', 'ars', 'b', 'Ġservice', 'Ġretired', 'Ġde', 'cember', 'Ġprovided', 'Ġdigital', 'Ġvoice', 'Ġservices', 'Ġte', 'lex', 'Ġservices', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit']</t>
+          <t>[':[', 'Ġgreen', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', 'Ġpayload', 'Ġproject', 'Ġpartly', 'Ġdeveloped', 'Ġu', 'Ġair', 'Ġforce', 'Ġdemonstrate', 'Ġless', 'oxic', 'Ġanother', 'Ġsecondary', 'Ġpayload', 'Ġmini', 'atur', 'ized', 'Ġdeep', 'Ġspace', 'Ġatomic', 'Ġclock', 'Ġexpected', 'Ġfacilitate', 'Ġautonomous', 'Ġnavigation', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', "'s", 'Ġdemonstration', 'Ġscience', 'Ġexperiments', 'Ġmass', 'Ġmeasure', 'Ġeffects', 'Ġlow', 'Ġfrequency', 'Ġradio', 'Ġwaves', 'Ġspace', 'Ġradiation', 'Ġb', 'rit', 'ish', 'orb', 'ital', 'Ġtest', 'Ġbed', 'Ġpayload', 'Ġhosting', 'Ġseveral', 'Ġcommercial', 'Ġmilitary', 'Ġexperiments', 'Ġsmall', 'Ġsatellites', 'Ġincluded', 'Ġprox', 'Ġbuilt', 'Ġge', 'org', 'ia', 'Ġtech', 'Ġstudents', 'Ġtest', 'printed', 'Ġthr', 'uster', 'Ġmini', 'atur', 'ized', 'Ġgy', 'ro', 'scope', 'Ġlights', 'ail', 'Ġplanetary', 'Ġsociety', 'culus', 'r', 'Ġnan', 'os', 'atellite', 'ich', 'igan', 'Ġtech', 'Ġcubes', 'ats', 'Ġu', 'Ġair', 'Ġforce', 'Ġacademy', 'Ġnaval', 'Ġpost', 'graduate', 'Ġschool', 'Ġunited', 'Ġstates', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġuniversity', 'Ġtex', 'Ġaust', 'Ġcal', 'ornia', 'Ġpoly', 'techn', 'ic', 'Ġstate', 'Ġuniversity', 'Ġcubes', 'Ġassembled', 'Ġstudents', 'Ġmer', 'r', 'itt', 'Ġisland', 'Ġhigh', 'Ġschool', 'Ġfl', 'ida', 'Ġblock', 'second', 'Ġstage', 'Ġallowed', 'Ġmultiple', 'Ġreign', 'itions', 'Ġplace', 'Ġmany', 'Ġpayload', 'Ġmultiple', 'Ġorbits', 'Ġlaunch', 'Ġplanned', 'Ġinclude', '000', 'Ġball', 'ast', 'Ġmass', 'Ġball', 'ast', 'Ġmass', 'Ġlater', 'Ġomitted', 'Ġtotal', 'Ġmass', 'Ġpayload', 'Ġstack', 'Ġn', 'asa', 'es', 'Ġresearch', 'Ġcenter', 'Ġproposed', 'Ġmars', 'Ġmission', 'Ġcalled', 'Ġred', 'Ġdragon', 'Ġwould', 'Ġuse', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġtrans', 'mart', 'ian', 'Ġinjection', 'Ġvehicle', 'Ġvariant', 'Ġdragon', 'Ġcapsule', 'Ġenter', 'Ġmart', 'ian', 'Ġatmosphere', 'Ġproposed', 'Ġscience', 'Ġobjectives', 'Ġdetect', 'Ġbios', 'ign', 'atures', 'Ġdrill', 'Ġft', 'Ġunderground', 'Ġeffort', 'Ġsample', 'Ġreservoirs', 'Ġwater', 'Ġice', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġmission', 'Ġn', 'asa', 'Ġcontracts', 'Ġsolar', 'Ġsystem', 'Ġtransport', 'Ġmissions', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġunited', 'Ġstates', 'Ġportal', 'Ġcompanies', 'Ġportal', 'Ġknown', 'Ġexist', 'Ġsurface', 'Ġmission', 'Ġcost', 'Ġprojected', 'Ġless', 'Ġus', 'Ġmillion', 'Ġincluding', 'Ġlaunch', 'Ġcost', 'Ġspace', 'x', 'Ġestimation', '000', 'âĢĵ']</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>['Ġhigh', 'Ġspeed', 'Ġdata', 'Ġservices', 'Ġk', 'bit', 'Ġalso', 'leased', 'Ġmode', 'ars', 'b', 'Ġavailable', 'Ġspare', 'ars', 'Ġsatellites', 'ars', 'c', 'Ġeffectively', 'atellite', 'Ġte', 'lex', 'Ġterminal', 'Ġlow', 'speed', 'digital', 'trans', 'mission', 'Ġbit', 'Ġrate', 'Ġbit', 'Ġinformation', 'Ġbit', 'Ġrate', 'Ġbit', 'Ġstore', 'forward', 'Ġpolling', 'Ġetc', 'Ġcapabilities', 'Ġcertain', 'Ġmodels', 'ars', 'c', 'Ġterminals', 'Ġapproved', 'Ġglobal', 'Ġmaritime', 'Ġdistress', 'Ġsafety', 'Ġsystem', 'g', 'md', 'ss', 'Ġsystem', 'Ġequipped', 'ars', 'Ġprovides', 'Ġvoice', 'Ġservices', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit', 'Ġpaved', 'Ġway', 'Ġtowards', 'ars', 'mini', 'Ġservice', 'Ġended', 'Ġmini', 'Ġprovides', 'Ġvoice', 'Ġservices', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit', 'Ġone', 'Ġk', 'bit', 'Ġchannel', 'Ġtakes', 'Ġk', 'bit', 'Ġsatellite', 'Ġservice', 'Ġclosed', 'Ġearly', 'Ġjan', 'uary', 'Ġg', 'global', 'Ġarea', 'Ġnetwork', '):', 'Ġprovides', 'Ġselection', 'Ġlow', 'Ġspeed', 'Ġservices', 'Ġlike', 'Ġvoice', 'Ġk', 'bit', 'Ġdata', 'Ġk', 'bit', 'dn', 'Ġlike', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'dn', 'Ġshared', 'channel', 'Ġpacket', 'sw', 'itched', 'Ġdata', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'Ġpacket', 'Ġdata', 'Ġservice', 'Ġformerly', 'ars', 'Ġpacket', 'Ġdata', 'Ġservice', 'Ġg', 'Ġalso', 'Ġknown', 'Ġservice', 'Ġclosed', 'Ġearly', 'Ġjan', 'uary', 'Ġfleet', 'Ġfamily', 'Ġnetworks', 'Ġincludes', 'ars', 'fleet', 'ars', 'fleet', 'ars', 'fleet', 'Ġmembers', 'Ġnumbers', 'Ġcome', 'Ġdiameter', 'Ġantenna', 'Ġcent', 'imet', 'res', 'Ġmuch', 'Ġlike', 'Ġg', 'Ġprovides', 'Ġselection', 'Ġlow', 'Ġspeed', 'Ġservices', 'Ġlike', 'Ġvoice', 'Ġk', 'bit', 'Ġfax', 'data', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġservices', 'Ġlike', 'Ġfax', 'data', 'Ġk', 'bit', 'dn', 'Ġlike', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'dn']</t>
+          <t>['000', 'âĢĵ', 'Ġsurface', 'Ġmars', 'Ġsoft', 'Ġretro', 'prop', 'ulsive', 'Ġlanding', 'Ġfollowing', 'Ġlimited', 'Ġatmospheric', 'Ġde', 'celer', 'ation', 'Ġusing', 'Ġparachute', 'Ġheat', 'Ġshield', 'Ġbeyond', 'Ġred', 'Ġdragon', 'Ġconcept', 'Ġspace', 'x', 'Ġseeing', 'Ġpotential', 'Ġfal', 'con', 'Ġheavy', 'Ġdragon', 'Ġcarry', 'Ġscience', 'Ġpayload', 'Ġacross', 'Ġmuch', 'Ġsolar', 'Ġsystem', 'Ġparticularly', 'Ġj', 'upiter', "'s", 'Ġmoon', 'Ġeuro', 'pa', 'Ġspace', 'x', 'Ġannounced', 'Ġprop', 'ulsive', 'Ġlanding', 'Ġdragon', 'Ġwould', 'Ġdeveloped', 'Ġcapsule', 'Ġwould', 'Ġreceive', 'Ġlanding', 'Ġlegs', 'Ġconsequently', 'Ġred', 'Ġdragon', 'Ġmissions', 'Ġmars', 'Ġcanceled', 'Ġfavor', 'Ġstarship', 'Ġlarger', 'Ġvehicle', 'Ġusing', 'Ġdifferent', 'Ġlanding', 'Ġtechnology', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġinitial', 'Ġmodules', 'Ġlunar', 'Ġgateway', 'Ġpower', 'Ġpropulsion', 'Ġelement', 'ppe', 'Ġhabit', 'ation', 'Ġlogistics', 'Ġoutpost', 'h', 'alo', ').[', 'Ġdecrease', 'Ġcomplexity', 'Ġn', 'asa', 'Ġannounced', 'Ġfe', 'b', 'ruary', 'Ġlaunching', 'Ġfirst', 'Ġtwo', 'Ġelements', 'Ġsingle', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġtargeting', 'Ġlaunch', 'Ġdate', 'Ġearlier', 'mber', 'Ġswitching', 'Ġmerged', 'Ġlaunch', 'Ġn', 'asa', 'Ġlisted', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġp', 'pe', 'Ġlone', 'Ġlaunch', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġfirst', 'Ġaward', 'Ġres', 'upp', 'ly', 'Ġmission', 'Ġlunar', 'Ġgateway', 'Ġplacing', 'Ġnew', 'Ġdragon', 'Ġspacecraft', 'Ġtransl', 'un', 'ar', 'Ġinjection', 'Ġorbit', 'Ġn', 'asa', 'Ġchose', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġpsyche', 'Ġmission', 'Ġmetallic', 'Ġasteroid', 'Ġlaunched', 'Ġoct', 'ober', 'Ġcontract', 'Ġworth', 'Ġus', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġinitially', 'Ġtargeted', 'Ġlaunched', 'Ġsl', 'Ġrocket', 'Ġhowever', 'Ġdue', 'Ġextensive', 'Ġdelays', 'Ġn', 'asa', 'Ġawarded', 'Ġlaunch', 'Ġcontract', 'Ġspace', 'x', 'Ġfully', 'Ġexpend', 'able', 'Ġfal', 'con', 'Ġheavy', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġcomparison', 'Ġorbital', 'Ġlaunchers', 'Ġfamilies', 'Ġspace', 'x', 'Ġmars', 'Ġtransportation', 'Ġinfrastructure', 'Ġsat', 'urn', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġreused', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġheavy', 'Ġlift', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġarchived', 'Ġlunar', 'Ġmissions', 'Ġpsyche', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġreferences', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġsheet', 'z', 'ichael']</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -3038,7 +3038,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>['Ġshared', 'channel', 'Ġpacket', 'sw', 'itched', 'Ġdata', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'Ġpacket', 'Ġdata', 'Ġservice', 'Ġsee', 'Ġhowever', 'Ġservices', 'Ġavailable', 'Ġmembers', 'Ġfamily', 'Ġlatest', 'Ġservice', 'Ġsupported', 'Ġmobile', 'dn', 'Ġk', 'bit', 'ars', 'fleet', 'Ġterminals', 'Ġswift', 'Ġsimilar', 'Ġg', 'Ġproviding', 'Ġvoice', 'Ġlow', 'Ġrate', 'Ġfax', 'data', 'k', 'bit', 'dn', 'Ġservices', 'Ġprivate', 'Ġbusiness', 'Ġcommercial', 'Ġaircraft', 'Ġswift', 'Ġoften', 'Ġsold', 'Ġmulti', 'channel', 'Ġversion', 'Ġsupport', 'Ġseveral', 'Ġtimes', 'k', 'bit', 'ars', 'ars', "'s", 'Ġp', 'ager', 'Ġalthough', 'Ġmuch', 'Ġlarger', 'Ġterrestrial', 'Ġversions', 'Ġunits', 'Ġequipped', 'Ġoriginal', 'ars', 'Ġterminals', 'Ġone', 'way', 'Ġmobile', 'Ġp', 'agers', 'Ġnewer', 'ars', 'Ġterminals', 'Ġequivalent', 'Ġtwo', 'way', 'Ġp', 'ager', 'Ġmain', 'Ġuse', 'Ġtechnology', 'Ġnowadays', 'Ġtracking', 'Ġtrucks', 'Ġbu', 'oys', 'Ġsc', 'ada', 'Ġapplications', 'mobile', 'Ġpacket', 'Ġdata', 'Ġservice', '):', 'Ġpreviously', 'Ġknown', 'Ġip', 'based', 'Ġdata', 'Ġservice', 'Ġseveral', 'Ġusers', 'Ġshare', 'k', 'bit', 'Ġcarrier', 'Ġmanner', 'Ġsimilar', 'Ġad', 'sl', 'Ġmp', 'ds', 'spe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġterminals', 'Ġsold', 'Ġrather', 'Ġservice', 'Ġcomes', 'Ġterminals', 'Ġdesigned', 'Ġg', 'Ġfleet', 'Ġswift', 'phone', 'Ġprovides', 'Ġvoice', 'Ġservices', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit', 'Ġservice', 'Ġemerged', 'Ġcollaboration', 'Ġagreement', 'ces', 'Ġavailable', 'Ġem', 'ea', 'Ġap', 'ac', 'Ġsatellite', 'Ġregions', 'Ġcoverage', 'Ġavailable', 'Ġaf', 'rica', 'Ġmiddle', 'east', 'ia', 'Ġeuro', 'pe', 'Ġwell', 'Ġmaritime', 'Ġareas', 'Ġem', 'ea', 'Ġap', 'ac', 'Ġcoverage', 'Ġj', 'une', 'Ġeuro', 'pe', 'Ġparliament', 'Ġeuro', 'pe', 'Ġcouncil', 'Ġadopted', 'Ġeuro', 'pe', "'s", 'Ġdecision', 'Ġestablish', 'Ġsingle', 'Ġselection', 'Ġauthor', 'isation', 'Ġprocess', 'es', 'ap', 'Ġeuro', 'pe', 'band', 'Ġapplication', 'Ġprocess', 'Ġensure', 'Ġcoordinated', 'Ġintroduction', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'ss', 'Ġprojects', 'Ġsince', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork']</t>
+          <t>['Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', 'Ġsays', 'Ġnew', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġcr', 'ushes', 'Ġcompetition', 'Ġcost', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'fal', 'con', 'Ġheavy', 'Ġspace', 'x', 'Ġretrieved', 'Ġapr', 'il', 'Ġhar', 'wood', 'iam', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġputs', 'Ġspectacular', 'Ġshow', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġ', 'ight', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġah', 'mad', 'ase', 'er', 'mar', 'Ġah', 'med', 'Ġk', 'amara', 'Ġah', 'med', 'Ġlim', 'Ġg', 'ab', 'riel', 'Ġmag', 'owan', 'Ġca', 'lin', 'dor', 'ova', 'Ġbl', 'aga', 'se', 'ee', 'Ġche', 'ung', 'Ġwhite', 'Ġtom', 'Ġmars', 'Ġsociety', 'Ġinspiration', 'Ġmars', 'Ġinternational', 'Ġstudent', 'Ġdesign', 'Ġcompetition', 'Ġmars', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġde', 'cember', 'Ġ"-', 'ĠÂ°', 'f', 'Ġcase', 'Ġdeep', 'Ġcry', 'Ġincreases', 'Ġdensity', 'Ġampl', 'ï', '¬', 'ģ', 'es', 'Ġrocket', 'Ġperformance', 'Ġfirst', 'Ġtime', 'Ġanyone', 'Ġgone', 'Ġlow', 'Ġchilled', 'ĠÂ°', 'f', 'ĠÂ°', 'f', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'fal', 'con', 'Ġoverview', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'el', 'Ġmus', 'k', "'s", 'Ġhuge', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġset', 'Ġlaunch', 'ment', 'Ġnews', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġaug', 'ust', 'Ġar', 'abs', 'Ġmission', 'Ġg', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġse', 'pt', 'ember', 'air', 'Ġforce', 'Ġcert', 'ï', '¬', 'ģ', 'ed', 'Ġfal', 'con', 'Ġheavy', 'Ġnational', 'Ġsecurity', 'Ġlaunch', 'Ġwork', 'Ġneeded', 'Ġmeet', 'Ġrequired', 'Ġorbits', 'Ġspac', 'en', 'ews', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -3051,7 +3051,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>['ars', 'Ġwik', 'ipedia', 'Ġeuro', 'pe', 'Ġlate', 'Ġselection', 'Ġprocess', 'Ġattracted', 'Ġfour', 'Ġapplications', 'Ġprospective', 'Ġoperators', 'ico', 'Ġglobal', 'Ġcommunications', 'ico', 'ars', 'Ġsolar', 'Ġmobile', 'ech', 'ost', 'ar', 'Ġmobile', 'Ġter', 'rest', 'ar', ').[', 'Ġmay', 'Ġeuro', 'pe', 'Ġcommission', 'Ġselected', 'Ġtwo', 'Ġoperators', 'ars', 'Ġventures', 'Ġsolar', 'Ġmobile', 'Ġgiving', 'Ġoperators', 'Ġright', 'Ġuse', 'Ġspecific', 'Ġradio', 'Ġfrequencies', 'Ġidentified', 'Ġcommission', "'s", 'Ġdecision', 'Ġright', 'Ġoperate', 'Ġrespective', 'Ġmobile', 'Ġsatellite', 'Ġsystems', '".', 'Ġmember', 'Ġstates', 'Ġensure', 'Ġtwo', 'Ġoperators', 'Ġright', 'Ġuse', 'Ġspecific', 'Ġradio', 'Ġfrequencies', 'Ġidentified', 'Ġcommission', "'s", 'Ġdecision', 'Ġright', 'Ġoperate', 'Ġrespective', 'Ġmobile', 'Ġsatellite', 'Ġsystems', 'Ġyears', 'Ġselection', 'Ġdecision', 'Ġoperators', 'Ġcompelled', 'Ġstart', 'Ġoperations', 'Ġwithin', 'Ġmonths', 'may', 'Ġselection', 'ars', "'s", 'band', 'Ġsatellite', 'Ġprogramme', 'Ġprovides', 'Ġmobile', 'Ġmultimedia', 'Ġbroadcast', 'Ġmobile', 'Ġtwo', 'way', 'Ġbroadband', 'Ġtelecommunications', 'Ġnext', 'generation', 'ss', 'Ġservices', 'Ġacross', 'Ġmember', 'Ġstates', 'Ġeuro', 'pe', 'Ġunion', 'Ġfar', 'Ġeast', 'Ġmos', 'cow', 'Ġank', 'ara', 'Ġmeans', 'Ġhybrid', 'Ġnetwork', 'Ġbuilt', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġlaunched', 'Ġcomplementary', 'Ġground', 'Ġnetwork', 'Ġconsists', 'Ġaround', 'Ġl', 'te', 'Ġbase', 'Ġstations', 'Ġconstructed', 'Ġde', 'utsche', 'Ġtele', 'k', 'om', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġfaced', 'Ġlegal', 'Ġchallenges', 'Ġincluding', 'Ġone', 'Ġv', 'ias', 'Ġalleging', 'Ġunfair', 'Ġbidding', 'Ġpractices', 'Ġmisuse', 'Ġspectrum', 'Ġruling', 'Ġbel', 'gian', 'Ġtelecommunications', 'Ġregulator', 'Ġrev', 'oking', 'Ġpermission', 'Ġuse', 'Ġground', 'Ġnetwork', 'ars', 'Ġordered', 'Ġfifth', 'Ġglobal', 'Ġx', 'press', 'Ġsatellite', 'Ġth', 'ales', 'Ġgroup', 'Ġsatellite', 'Ġlaunched', 'mber', 'Ġcentre', 'Ġspatial', 'Ġguy', 'ana', 'Ġaboard', 'ri', 'ane', 'Ġlaunch', 'Ġvehicle', 'Ġsatellite', 'Ġdescribed', 'Ġhigh', 'Ġthroughput', 'Ġsatellite', "',", 'Ġprovides', 'Ġservices', 'Ġmiddle', 'Ġeast', 'Ġind', 'ia', 'Ġeuro', 'pe', 'Ġformer', 'Ġce', 'Ġru', 'pert', 'Ġpear', 'ce', 'new', 'Ġce', 'Ġr', 'aj', 'ee', 'v', 'Ġsur', 'Ġindicated', 'ars', 'Ġplanned', 'Ġexpansion', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġtrials', 'Ġnew', 'Ġtechnologies', 'Ġdemonstrated', 'Ġbandwidth', 'bit', 'Ġexisting', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġfar', 'Ġexcess', 'Ġexisting', 'Ġpolar', 'Ġcoverage', 'Ġprovide', 'Ġcoverage', 'Ġusers', 'Ġar', 'ctic']</t>
+          <t>['Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġpas', 'z', 'tor', 'el', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'x', "'s", 'Ġnew', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġunlikely', 'Ġcarry', 'Ġastronauts', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'mus', 'k', 'Ġunve', 'ils', 'Ġrevised', 'Ġversion', 'Ġgiant', 'Ġinter', 'plan', 'etary', 'Ġlaunch', 'Ġsystem', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġinterview', 'Ġel', 'Ġmus', 'k', 'Ġmus', 'k', 'html', 'Ġh', 'obb', 'ys', 'pace', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġel', 'Ġk', 'oen', 'igs', 'mann', 'Ġh', 'ans', 'Ġg', 'ure', 'vich', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġattempt', 'Ġmaking', 'Ġaccess', 'Ġspace', 'Ġaffordable', 'Ġreliable', 'Ġpleasant', 'di', 'th', 'Ġannual', 'ia', 'us', 'u', 'Ġconference', 'Ġsmall', 'Ġsatellites', 'Ġlog', 'Ġut', 'ah', 'Ġut', 'ah', 'Ġstate', 'Ġuniversity', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġg', 'ask', 'ill', 'Ġbr', 'addock', 'Ġoct', 'ober', 'space', 'x', 'Ġreveals', 'Ġfal', 'con', 'Ġhall', 'ow', 'een', 'Ġdate', 'nas', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', 'Ġenters', 'Ġrealm', 'Ġheavy', 'lift', 'Ġrocket', 'ry', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġwall', 'ike', 'Ġj', 'uly', 'space', 'x', "'s", 'Ġbig', 'Ġnew', 'Ġrocket', 'Ġmay', 'Ġcrash', 'st', 'Ġflight', 'Ġel', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġmus', 'k', 'Ġel', 'Ġj', 'uly', 'Ġel', 'Ġmus', 'k', 'Ġiss', 'Ġr', 'Ġconference', 'video', 'Ġiss', 'Ġr', 'Ġconference', 'Ġwashing']</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -3064,7 +3064,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>['Ġregion', 'ars', 'Ġplans', 'Ġimprove', 'Ġglobal', 'x', 'press', 'Ġconnectivity', 'Â°', 'Ġnorth', 'Ġtwo', 'Ġhigh', 'capacity', 'Ġmulti', 'beam', 'Ġpayload', 'Ġplanned', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbits', 'Ġreliable', 'Ġcoverage', 'ars', 'Ġworked', 'Ġpartnership', 'Ġspace', 'way', 'os', 'Ġar', 'ctic', 'Ġsatellite', 'Ġbroadband', 'Ġmission', 'Ġsatellites', 'Ġcarrying', 'ars', 'Ġpayload', 'Ġmanufactured', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'ng', 'Ġlaunch', 'Ġscheduled', 'Ġglobal', 'Ġx', 'press', 'Ġexpansion', 'ars', 'ars', 'Ġwik', 'ipedia', 'Ġend', 'ars', 'Ġordered', 'Ġtwo', 'Ġsixth', 'Ġgeneration', 'Ġsatellites', 'Ġair', 'bus', 'Ġsatellites', 'Ġplanned', 'Ġoffer', 'Ġka', 'Ġl', 'band', 'Ġpayload', 'Ġadditional', 'Ġcapacity', 'Ġexisting', 'Ġglobal', 'Ġx', 'press', 'Ġnetworks', 'Ġannounced', 'Ġfirst', 'Ġsatellites', 'Ġwould', 'Ġlaunched', 'hi', 'Ġde', 'cember', 'ars', 'Ġparticipating', 'Ġtwo', 'Ġes', 'Ġart', 'es', 'Ġprograms', 'Ġir', 'Ġice', 'Ġir', 'Ġproject', 'Ġimprove', 'Ġtracking', 'Ġaircraft', 'Ġimprove', 'Ġcommunications', 'Ġaircraft', 'Ġair', 'Ġtra', 'f', 'ï', '¬', 'ģ', 'c', 'Ġcontrollers', 'ars', 'Ġprovide', 'Ġhigh', 'Ġcapacity', 'Ġsatellite', 'Ġcommunications', 'Ġlinks', 'Ġaircraft', 'Ġimprove', 'Ġdetection', 'Ġaircraft', 'Ġlocations', 'Ġtime', 'Ġspace', 'Ġice', 'ars', 'Ġcommunications', 'Ġevolution', 'Ġpartnership', 'Ġindustrial', 'Ġpartners', 'Ġintended', 'Ġidentify', 'Ġinnovative', 'Ġtechnologies', 'Ġexpand', 'Ġenhance', 'Ġcapabilities', 'Ġnext', 'Ġgeneration', 'Ġsatellite', 'ars', 'Ġir', 'idium', 'Ġfrequency', 'Ġbands', 'Ġab', 'ut', 'Ġthus', 'Ġsat', 'Ġradio', 'Ġability', 'Ġinterfere', 'Ġusually', 'Ġfar', 'Ġpowerful', 'ars', 'Ġradio', 'Ġdisrupt', 'Ġir', 'idium', 'Ġradio', 'âĢĵ', 'âĢĵ', 'Ġft', 'Ġaway', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġmobile', 'atellite', 'Ġservice', 'Ġsatellite', 'Ġphone', 'Ġaer', 'om', 'obile', 'Ġglobal', 'star', 'Ġglob', 'als', 'Ġgroup', 'Ġinter', 'put', 'nik', 'Ġir', 'idium', 'Ġcommunications', 'Ġlib', 'rest', 'ream', 'Ġmaritime', 'Ġsafety', 'Ġinformation', 'Ġnetworks', 'air', 'Ġorb', 'comm', 'Ġradi', 'ote', 'le', 'phone', 'es', 'Ġbroadband', 'Ġmaritime', 'Ġspace', 'Ġglobal', 'Ġth', 'ur', 'aya', 'Ġir', 'Ġice', 'Ġissues', 'Ġsee', 'Ġalso', 'ars']</t>
+          <t>['ton', 'Ġu', 'Ġevent', 'Ġoccurs', '00', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'Ġlot', 'Ġrisk', 'Ġassociated', 'Ġfal', 'con', 'Ġheavy', 'Ġreal', 'Ġgood', 'Ġchance', 'Ġvehicle', 'Ġmake', 'Ġorbit', 'Ġ...', 'Ġhope', 'Ġmakes', 'Ġfar', 'Ġenough', 'Ġaway', 'Ġpad', 'Ġcause', 'Ġpad', 'Ġdamage', 'Ġwould', 'Ġconsider', 'Ġeven', 'Ġwin', 'Ġhonest', 'Ġ...', 'Ġthink', 'Ġfal', 'con', 'Ġheavy', 'Ġgoing', 'Ġgreat', 'Ġvehicle', 'Ġmuch', 'Ġreally', 'Ġimpossible', 'Ġtest', 'Ġground', "'ll", 'Ġbest', 'Ġ...', 'Ġactually', 'Ġended', 'Ġway', 'Ġharder', 'Ġfal', 'con', 'Ġheavy', 'Ġthought', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsounds', 'Ġreal', 'Ġeasy', 'Ġstick', 'Ġtwo', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstages', 'Ġstrap', 'Ġboosters', 'Ġhard', 'Ġeverything', 'Ġchanges', 'Ġloads', 'Ġchange', 'Ġaer', 'odynamics', 'Ġtotally', 'Ġchange', 'Ġtripled', 'Ġvibration', 'Ġac', 'oust', 'ics', 'Ġbreak', 'Ġqual', 'ï', '¬', 'ģ', 'cation', 'Ġlevels', 'Ġhardware', 'Ġredesign', 'Ġcenter', 'Ġcore', 'Ġair', 'frame', 'Ġseparation', 'Ġsystems', 'Ġ...', 'Ġreally', 'Ġway', 'Ġway', 'ï', '¬', 'ģ', 'cult', 'Ġoriginally', 'Ġthought', 'Ġpretty', 'Ġnaive', 'Ġ...', 'Ġoptimized', "'s", 'Ġtimes', 'Ġpayload', 'Ġcapability', 'Ġfal', 'con', '."', 'Ġmus', 'k', 'Ġel', 'Ġde', 'cember', 'j', 'une', 'Ġse', 'pt', 'ember', 'Ġupdate', 'http', 'space', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġbo', 'oz', 'er', 'Ġr', 'Ġmarch', 'rocket', 'us', 'ability', 'Ġdriver', 'Ġeconomic', 'Ġgrowth', 'http', 'hes', 'p', 'Ġspace', 'Ġreview', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'Ġmus', 'k', 'Ġel', 'Ġaug', 'ust', 'trans', 'cript', 'Ġel', 'Ġmus', 'k', 'Ġfuture', 'Ġspace', 'x', 'web', 'arch', 'iv', 'Ġshit', 'el', 'ons', 'ays', 'Ġmars', 'Ġsociety', 'Ġconference', 'Ġboulder', 'Ġcolor', 'ado', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'f']</t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -3077,7 +3077,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>['Ġwik', 'ipedia', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'p', 'rel', 'iminary', 'Ġfull', 'Ġyear', 'Ġresults', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'ï', '¬', 'ģ', 'ces', 'ars', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġus', 'ars', 'v', 'ias', 'Ġcompletes', 'Ġacquisition', 'ars', 'Ġv', 'ias', 'Ġmay', 'Ġretrieved', 'Ġj', 'uly', 'prop', 'osed', 'Ġamendments', 'Ġconvention', 'Ġinternational', 'Ġmobile', 'Ġsatellite', 'Ġorganization', 'im', ')"', 'Ġinternational', 'Ġcivil', 'Ġaviation', 'Ġorganization', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'agar', 'Ġdavid', 'Ġhar', 'ris', 'Ġr', 'ed', '.).', 'Ġprivat', 'isation', 'ars', 'Ġspecial', 'Ġproblems', '".', 'Ġinternational', 'Ġorganisations', 'Ġspace', 'Ġlaw', 'Ġproceedings', 'Ġthird', 'Ġcoll', 'oqu', 'ium', 'Ġper', 'ug', 'ia', 'aly', 'âĢĵ', 'Ġmay', 'âĢĵ', 'Ġj', 'athan', 'Ġhig', 'gins', 'Ġsatellite', 'Ġnews', 'g', 'athering', 'Ġfocal', 'Ġpress', 'Ġp', 'Ġgod', 'win', 'Ġmatt', 'hew', 'Ġde', 'cember', 'inter', 'view', 'Ġroy', 'Ġgib', 'son', 'Ġoral', 'Ġhistory', 'Ġeuro', 'pe', 'Ġspace', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġp', 'Ġretrieved', 'Ġj', 'une', 'Ġj', 'athan', 'Ġhig', 'gins', 'Ġp', 'oll', 'ars', 'Ġsense', 'Ġsat', 'Ġsatell', 'et', 'oday', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'private', 'Ġequity', 'Ġorbits', 'ars', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġbuys', 'Ġstrat', 'os', 'Ġglobal', 'Ġwashing', 'ton', 'Ġbusiness', 'Ġjournal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'Ġsand', 'le', 'Ġp', 'aul', 'Ġapr', 'il', 'ars', 'Ġtake', 'Ġstake', 'Ġtracking', 'Ġco', 'Ġsky', 'wave', 'uters', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ars', 'Ġgrabs', 'Ġmacro', 'bert', 'Ġengineering', 'Ġprize', 'Ġmars', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['dragon', 'Ġpreparing', 'Ġiss', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmarch', 'space', 'x', 'Ġaims', 'Ġdebut', 'Ġnew', 'Ġversion', 'Ġfal', 'con', 'Ġsummer', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġspace', 'x', 'Ġde', 'cember', 'fal', 'con', 'Ġheavy', 'Ġinter', 'stage', 'Ġpre', 'pped', 'Ġrocket', 'Ġfactory', 'Ġf', 'h', 'Ġï', '¬', 'Ĥ', 'ies', 'Ġnext', 'Ġyear', 'Ġpowerful', 'Ġoperational', 'Ġrocket', 'Ġworld', 'Ġfactor', 'Ġtwo', 'ht', 'Ġinst', 'agram', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġheavy', 'Ġtest', 'Ġstand', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġmay', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġmay', 'space', 'x', 'Ġproves', 'Ġfal', 'con', 'Ġheavy', 'Ġindeed', 'Ġreal', 'Ġrocket', 'Ġtest', 'Ġï', '¬', 'ģ', 'ring', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'space', 'x', 'Ġmay', 'first', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'Ġfal', 'con', 'Ġheavy', 'Ġcenter', 'Ġcore', 'Ġcompleted', 'Ġmc', 'greg', 'Ġrocket', 'Ġdevelopment', 'Ġfacility', 'Ġlast', 'Ġweek', 'weet', 'Ġretrieved', 'Ġmay', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġse', 'pt', 'ember', 'fal', 'con', 'Ġheavy', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcores', 'Ġcompleted', 'Ġtesting', 'Ġrocket', 'Ġdevelopment', 'Ġfacility', 'Ġmc', 'greg', 'Ġtex', 'Ġ01', 'weet', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġperforms', 'Ġcrucial', 'Ġtest', 'Ġï', '¬', 'ģ', 'Ġfal', 'con', 'Ġheavy', 'Ġpotentially', 'Ġpaving', 'Ġway', 'Ġlaunch', 'ww', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'u', 'Ġspace', 'x', 'Ġbuild', 'Ġheavy', 'lift', 'Ġlow', 'cost', 'Ġrocket', 'uters', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'x', 'Ġannounces', 'Ġlaunch', 'Ġdate', 'Ġworld', "'s", 'Ġpowerful']</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -3090,7 +3090,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>['Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'making', 'Ġthings', 'Ġbetter', 'Ġï', '¬', 'ģ', 'n', 'al', 'ists', 'Ġannounced', 'Ġb', 'rit', "'s", 'Ġtop', 'Ġengineering', 'Ġaward', 'Ġnews', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġreferences', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġends', 'Ġservice', 'Ġyears', 'ara', 'org', 'Ġarchived', 'Ġoriginal', 'Ġris', 'htm', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmarch', 'Ġlaunch', 'cs', 'Ġes', 'ars', 'Ġspace', 'sky', 'rocket', 'de', 'ars', 'Ġprovides', 'Ġtwo', 'way', 'Ġdata', 'Ġmessaging', 'Ġcommunication', 'Ġservices', 'ars', 'esa', 'ars', 'Ġagreement', 'Ġimprove', 'Ġsatellite', 'Ġmobile', 'Ġphone', 'Ġdata', 'Ġservices', 'http', 'esa', 'Ġes', 'int', 'ars', 'Ġarchived', 'Ġoriginal', 'ww', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'global', 'Ġx', 'press', 'ars', 'Ġaviation', 'ars', 'euro', 'pe', 'Ġaviation', 'Ġnetwork', 'ars', 'ars', 'Ġpartners', 'Ġisot', 'rop', 'ic', 'Ġsystems', 'Ġdevelop', 'Ġnext', 'gen', 'Ġka', 'band', 'Ġmobility', 'Ġantenna', 'http', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'ars', 'Ġpan', 'asonic', 'Ġpartner', 'ï', '¬', 'Ĥ', 'ight', 'Ġconnectivity', 'uters', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ars', 'Ġpan', 'asonic', 'Ġannounce', 'Ġstrategic', 'Ġcollaboration', 'Ġquick', 'Ġfacts', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġï', '¬', 'ģ', 'rm', 'Ġbehind', 'Ġmal', 'ays', 'ia', 'Ġairlines', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġbreakthrough', 'Ġnews', 'Ġmarch', 'Ġash', 'ton', 'Ġch', 'ris', 'Ġbru', 'ce', 'Ġal', 'Ġsh', 'uster', 'Ġcoll', 'edge', 'Ġg', 'ary', 'Ġdick', 'inson', 'Ġmark', 'Ġse', 'pt', 'ember', 'Ġsearch', 'Ġjournal', 'Ġnavigation', 'Ġroyal', 'Ġinstitute', 'Ġnavigation', 'âĢĵ', 'Ġsatellite', 'Ġoperator', 'ars', 'Ġagrees', 'Ġbillion', 'Ġtakeover', 'Ġguardian', 'Ġmarch', 'Ġretrieved']</t>
+          <t>['Ġrocket', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'first', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġscheduled', 'Ġspring', 'http', 'sp', 'ac', 'ene', 'Ġspac', 'en', 'ews', 'Ġarchived', 'http', 'web', 'archive', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'launch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'http', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġseeks', 'Ġaccelerate', 'Ġfal', 'con', 'Ġproduction', 'Ġlaunch', 'Ġrates', 'Ġyear', 'year', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġaug', 'ust', 'pad', 'Ġhardware', 'Ġchanges', 'Ġpreview', 'Ġnew', 'Ġera', 'Ġspace', 'Ġcoast', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'space', 'x', 'Ġpushing', 'Ġback', 'Ġtarget', 'Ġlaunch', 'Ġdate', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmars', 'Ġmission', 'Ġverge', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'launch', 'Ġschedule', 'Ġe', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'deb', 'ut', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġplanned', 'Ġearly', 'Ġnext', 'Ġyear', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġpl', 'ait', 'Ġphil', 'Ġde', 'cember', 'el', 'Ġmus', 'k', 'Ġroad', 'ster', 'Ġmars', 'Ġwire', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'mus', 'k', 'Ġsays', 'es', 'la', 'Ġcar', 'Ġï', '¬', 'Ĥ', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġspac', 'en', 'ews', 'Ġde', 'cember', 'Ġarchived', 'w', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde']</t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -3103,7 +3103,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>['Ġaug', 'ust', 'Ġgovernment', 'Ġset', 'Ġapprove', 'Ġbillion', 'ars', 'Ġbuy', 'Ġbloom', 'berg', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġf', 'ild', 'es', 'Ġnic', 'mber', 'ars', 'Ġrejects', 'Ġactivist', 'Ġeffort', 'Ġthwart', 'Ġbillion', 'Ġtakeover', 'htt', 'Ġfinancial', 'Ġtimes', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'ars', 'Ġdel', 'ists', 'Ġstock', 'Ġexchange', 'Ġbuy', 'Ġspac', 'en', 'ews', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'ars', 'Ġwik', 'ipedia', 'private', 'Ġequity', 'Ġgiants', 'Ġtake', 'Ġcontrol', 'ars', 'Ġhedge', 'Ġfunds', 'Ġfold', 'Ġte', 'legraph', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ason', 'Ġrainbow', 'mber', 'v', 'ias', 'Ġbuying', 'ars', 'Ġbillion', 'Ġdeal', 'sp', 'ac', 'ene', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', 'Ġsim', 'Ġshar', 'wood', 'mber', 'space', 'Ġbroadband', 'ï', '¬', 'ģ', 'Ġv', 'ias', 'Ġacqu', 'ires', 'Ġrival', 'ars', 'ht', 'Ġregister', 'Ġretrieved', 'mber', 'Ġprovision', 'ally', 'Ġclears', 'Ġsatellite', 'Ġcomm', 'Ġdeal', 'Ġfollowing', 'depth', 'Ġreview', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'administ', 'rative', 'Ġtimetable', 'Ġgovernment', 'Ġpublishing', 'Ġservice', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'Ġmay', 'Ġrevised', 'Ġstatutory', 'Ġdeadline', 'Ġfollowing', 'Ġextension', 'Ġfre', 'eman', 'ike', 'Ġmay', 'c', 'arl', 'bad', "'s", 'Ġv', 'ias', 'Ġboosts', 'Ġsatellite', 'Ġinternet', 'Ġfootprint', 'Ġglobally', 'Ġcompletion', 'ars', 'Ġacquisition', 'ition', 'Ġsan', 'Ġdie', 'go', 'Ġunion', 'ribune', 'Ġrainbow', 'Ġj', 'ason', 'Ġmay', 'atellite', 'Ġoperators', 'Ġv', 'ias', 'ars', 'Ġcomplete', 'Ġmerger', 'Ġdeal', 'h', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'une', 'priv', 'acy', 'Ġpolicy', 'ars', 'Ġretrieved', 'Ġmarch', 'Ġcity', 'Ġroad', 'Ġl', 'ondon', 'Ġunited', 'Ġkingdom', 'g', 'md', 'ss', 'Ġweather', 'Ġweather', 'g', 'md', 'ss', 'org', 'Ġretrieved', 'Ġapr', 'il']</t>
+          <t>['cember', 'Ġkn', 'app', 'lex', 'Ġde', 'cember', 'el', 'Ġmus', 'k', 'Ġshows', 'Ġphotos', 'es', 'la', 'Ġroad', 'ster', 'Ġgetting', 'Ġpre', 'pped', 'Ġgo', 'Ġmars', 'Ġforb', 'es', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġke', 'lly', 'Ġem', 'Ġjan', 'uary', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġstatus', 'Ġupdates', 'Ġtargeting', 'Ġfr', 'iday', 'Ġtest', 'Ġï', '¬', 'ģ', 'Ġk', 'sc', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', '001', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġjan', 'uary', 'Ġshutdown', 'Ġmeans', 'Ġspace', 'x', "'t", 'Ġtest', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġcreating', 'Ġdelays', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'ap', 'atos', 'ennis', 'Ġjan', 'uary', 'Ġ01', 'Ġhistoric', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġfire', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'el', 'mus', 'k', 'Ġjan', 'uary', 'aim', 'ing', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġfe', 'b', 'ruary', 'Ġap', 'ollo', 'Ġlaunch', 'pad', 'Ġcape', 'Ġk', 'enn', 'edy', 'Ġeasy', 'Ġviewing', 'Ġpublic', 'Ġcause', 'way', 'weet', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġfe', 'b', 'ruary', 'continue', 'Ġmonitor', 'Ġupper', 'Ġlevel', 'Ġwind', 'ar', 'Ġnew', 'Ġest', 'Ġut', 'c', 'weet', 'Ġvia', 'Ġtwitter', 'el', 'mus', 'k', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġside', 'Ġcores', 'Ġlanded', 'Ġspace', 'x', "'s", 'Ġlanding', 'Ġzones', 'weet', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġlanded', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġtwo', 'Ġboosters', 'Ġcore', 'Ġclipped', 'Ġdrone', 'Ġship', 'Ġmph', 'Ġg', 'iz', 'mod', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmiddle', 'Ġbooster', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġfailed', 'Ġland', 'Ġdrone', 'Ġship']</t>
         </is>
       </c>
       <c r="C206" t="n">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>['ars', 'Ġretrieved', 'Ġoct', 'ober', 'ars', 'enter', 'prise', 'Ġservices', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġf', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'global', 'Ġmobile', 'Ġbroadband', 'ars', 'Ġretrieved', 'Ġmarch', 'trans', 'forming', 'Ġsatellite', 'Ġnews', 'g', 'athering', 'Ġtext', 'false', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'one', 'Ġworld', 'Ġone', 'Ġnumber', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġwik', 'ipedia', 'Ġprovides', 'eyes', 'Ġears', 'Ġoil', 'Ġrigs', 'en', 'text', 'false', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'low', 'cost', 'Ġhand', 'held', 'Ġfixed', 'Ġvoice', 'Ġservices', 'ars', 'ces', 'aces', 'ars', 'Ġsatellite', 'Ġsystem', 'Ġworks', 'Ġw', 'cc', 'lp', 'Ġarchived', 'Ġoriginal', 'Ġn', 'ex', 'asp', 'pg', 'id', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġglobal', 'Ġx', 'press', 'Ġcoverage', 'low', 'res', 'pdf', 'ars', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'mar', 'itime', 'Ġsolution', 'Ġoverview', 'sh', 'ane', 'Ġro', 'ss', 'b', 'acher', 'dig', 'itals', 'hip', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġhen', 'ry', 'Ġc', 'aleb', 'mber', 'arian', 'e', 'Ġlaunches', 'Ġsatellites', 'ars', 'sp', 'ac', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', 'air', 'bus', 'built', 'ars', 'Ġsatellite', 'Ġbreaks', 'Ġworld', 'Ġrecord', 'Ġmission', 'Ġlifespan', 'ion', 'lif', 'es', 'pan', 'Ġvia', 'Ġsatellite', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'ars', 'Ġnational', 'Ġspace', 'Ġscience', 'Ġdata', 'Ġcenter', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgo', 'Ġgiant', 'Ġcomm']</t>
+          <t>['ww', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', "'s", 'es', 'la', 'shot', 'Ġmars', 'Ġorbit', "'t", 'Ġreach', 'Ġasteroid', 'Ġbelt', 'Ġclaimed', 'ww', 'Ġus', 'k', 'ars', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġyear', 'Ġcolossal', 'Ġspace', 'x', 'Ġrocket', "'s", 'Ġdebut', 'Ġfal', 'con', 'Ġheavy', 'high', 'Ġvalue', 'Ġuses', 'Ġdespite', 'Ġskepticism', 'case', 'html', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġar', 'abs', 'Ġreset', 'uesday', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmarch', 'r', 'ides', 'hare', 'Ġmission', 'Ġu', 'Ġmilitary', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġsecond', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġaug', 'ust', 'ses', 'Ġagrees', 'Ġlaunch', 'Ġsatellite', 'ï', '¬', 'Ĥ', 'ight', 'proven', 'Ġfal', 'con', 'Ġrocket', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'mber', 'ars', 'Ġjuggling', 'Ġtwo', 'Ġlaunches', 'Ġsays', 'Ġspace', 'x', 'Ġreturn', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġwatt', 'les', 'Ġjack', 'ie', 'mber', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġthree', 'Ġyears', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunches', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġmission', 'Ġus', 'Ġspace', 'Ġforce', 'sp', 'Ġspace', 'Ġjan', 'uary', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -3129,7 +3129,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>['Ġsatellite', 'Ġnews', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'Ġc', 'aleb', 'Ġhen', 'ry', 'Ġj', 'une', 'ars', 'Ġsatellite', 'Ġrel', 'ocating', 'Ġcover', 'Ġmiddle', 'Ġeast', 'ia', 'Ġvia', 'Ġsatellite', 'Ġretrieved', 'Ġde', 'cember', 'ils', 'Ġpro', 'ton', 'Ġsuccessfully', 'Ġlaunches', 'ars', 'Ġsatellite', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'fl', 'aw', 'less', 'Ġlaunch', 'Ġal', 'phas', 'Ġtelecom', 'atellite', 'Ġes', 'Ġj', 'uly', 'Ġsatellites', 'ars', 'Ġretrieved', 'Ġjan', 'uary', 'ars', ')"', 'Ġspace', 'sky', 'rocket', 'de', 'Ġretrieved', 'Ġjan', 'uary', 'ars', 'Ġbegins', 'Ġglobal', 'Ġx', 'press', 'Ġroll', '09', 'Ġnews', 'Ġde', 'cember', 'ars', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġde', 'cember', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġlaunches', 'Ġsecond', 'Ġglobal', 'Ġx', 'press', 'Ġsatellite', 'Ġment', 'Ġnews', 'Ġfe', 'b', 'ruary', 'Ġmission', 'mission', 'ars', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ars', 'Ġpurchase', 'Ġfourth', 'ars', 'Ġsatellite', 'Ġbo', 'e', 'ing', 'press', 'Ġrelease', 'ars', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġmission', 'Ġspace', 'Ġx', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ars', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġsuccessful', 'Ġlaunch', 'ars', 'atell', 'ites', 'ars', 'Ġretrieved', 'Ġde', 'cember', 'Ġï', '¬', 'ģ', 'r', 'st', 'ars', 'Ġspacecraft', 'Ġscheduled', 'Ġlaunch', 'ub', 'ishi', 'Ġheavy', 'Ġindustries', 'hi', 'Ġend', 'Ġsecond', 'Ġfollow', '."', 'ars', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġsuccessful', 'Ġlaunch', 'Ġworld']</t>
+          <t>['h', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'v', 'ias', 'Ġameric', 'Ġsuccessfully', 'Ġlaunched', 'Ġv', 'ias', 'Ġmay', 'n', 'asa', 'Ġhead', 'Ġrules', 'Ġspace', 'x', 'Ġrockets', 'Ġmoon', 'Ġmission', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġj', 'uly', 'n', 'asa', "'s", 'Ġdaunting', 'Ġlist', 'Ġsending', 'Ġpeople', 'Ġback', 'Ġmoon', 'htt', 'Ġverge', 'Ġarchived', 'ary', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġn', 'asa', 'Ġtries', 'Ġland', 'Ġmoon', 'Ġplenty', 'Ġrockets', 'Ġchoose', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'n', 'asa', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġfinal', 'ize', 'Ġmoon', 'Ġoutpost', 'Ġliving', 'Ġquarters', 'Ġcontract', 'n', 'asa', 'g', 'Ġn', 'asa', 'press', 'Ġrelease', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġselects', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġlunar', 'Ġrover', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'fal', 'con', 'Ġheavy', 'Ġoverview', 'Ġspace', 'x', 'Ġarchived', 'Ġe', 'avy', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'space', 'x', 'Ġannounces', 'Ġlaunch', 'Ġdate', 'Ġworld', "'s", 'Ġpowerful', 'Ġrocket', 'Ġspace', 'ref', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'oct', 'aw', 'eb', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'land', 'ing', 'Ġlegs', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġk', 'mer', 'Ġk', 'en', 'Ġjan', 'uary', 'fal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġbooster', 'Ġrecovery', 'Ġfeatured', 'Ġcool', 'Ġnew', 'Ġspace', 'x', 'Ġanimation', 'Ġuniverse', 'Ġtoday', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -3142,7 +3142,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>["'s", 'Ġadvanced', 'Ġsatellite', 'ars', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġsuccessfully', 'Ġlaunched', 'ars', "'s", 'Ġlatest', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġlast', 'Ġnight', 'Ġlaunch', 'Ġpad', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', '."', 'æµ', '·', 'äº', 'ĭ', 'åį', '«', 'æĺ', 'Ł', 'çĶ', 'µ', 'è¯', 'Ŀ', 'åı', '·', 'æ', '®', 'µ', 'æ', 'Ĭ', 'ķ', 'â', '¼', 'Ĭ', 'ä½¿', 'â', '½', '¤', 'Ġch', 'inese', 'hu', 'Ġnews', 'Ġj', 'uly', 'global', 'Ġx', 'press', 'Ġseamless', 'Ġsatellite', 'Ġbroadband', 'ars', 'Ġal', 'x', 'press', 'ars', 'global', 'Ġexpress', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'bel', 'gian', 'Ġcourt', 'Ġpunches', 'Ġhole', 'ars', "'s", 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġspac', 'en', 'ews', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'successful', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġshows', 'Ġe', 'Ġtrack', 'Ġlaunch', 'ars', 'Ġaviation', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġde', 'utsche', 'Ġtele', 'k', 'om', 'Ġcomplete', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġspac', 'en', 'ews', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'euro', 'pe', 'Ġaviation', 'Ġnetwork', 'ean', 'ï', '¬', 'Ĥ', 'ight', 'Ġbroadband', 'Ġavailable', 'Ġthousands', 'Ġairline', 'Ġpassengers', 'ars', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ã¶', 'Ġjan', 'uary', 'euro', 'pe', "'s", 'Ġfastest', 'ï', '¬', 'Ĥ', 'ight', 'Ġwi', 'fi', 'Ġservice', 'Ġexpands', 'Ġcoverage', 'http', 'Ġft', 'n', 'news', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ars', 'Ġservices', 'ars', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġretrieved', 'Ġmarch', 'voice', 'ars', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġwik', 'ipedia', 'phone', 'Ġoverview', 'ars', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmarch', 'Ġservices', 'Ġglance', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġse']</t>
+          <t>['Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġn', 'ield', 'Ġge', 'orge', 'Ġc', 'ap', 'ril', 'Ġdraft', 'Ġenvironmental', 'Ġimpact', 'Ġstatement', 'Ġspace', 'x', 'Ġtex', 'Ġlaunch', 'Ġsite', 'report', 'Ġvol', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'ï', '¬', 'ģ', 'ce', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġsim', 'berg', 'Ġrand', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', 'Ġspace', 'x', "'s", 'Ġreusable', 'Ġrocket', 'Ġplans', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'f', 'iche', 'Ġtechnique', 'Ġfal', 'con', 'Ġheavy', 'technical', 'Ġdata', 'Ġsheet', 'Ġfal', 'con', 'Ġheavy', '].', 'Ġes', 'pace', 'Ġexploration', 'Ġfrench', 'Ġj', 'une', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġk', 'sc', 'Ġjan', 'uary', 'Ġut', 'c', ')"', 'forum', 'n', 'Ġretrieved', 'Ġjan', 'uary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'seeking', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġprogram', 'Ġworthy', 'Ġgreat', 'Ġnation', 'na', 'Ġn', 'asa', 'Ġoct', 'ober', 'Ġarchived', 'http', 'Ġreport', 'pdf', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', 'Ġenters', 'Ġrealm', 'Ġheavy', 'lift', 'Ġrocket', 'ry', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'Ġexploration', 'Ġtechnologies', 'Ġcorporation', 'Ġfal', 'con', 'Ġheavy', 'Ġal', 'con', 'heavy', 'Ġspace', 'x', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġbroch', 'ure', 'Ġarchived', 'Ġoriginal', 'Ġace', 'x', 'bro', 'ch', 'ure', 'pdf', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġpress', 'Ġconference', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch']</t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -3155,7 +3155,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>['Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġb', 'ars', 'Ġretrieved', 'Ġj', 'une', 'mission', 'Ġboost', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'Ġp', 'aves', 'Ġway', 'Ġwide', 'Ġhigh', 'Ġspeed', 'Ġdata', 'Ġcommunications', 'Ġeuro', 'pa', 'web', 'Ġportal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'new', 'Ġsatellites', 'Ġeuro', 'pe', 'Ġcommission', 'Ġstarts', 'Ġselection', 'Ġprocedure', 'Ġoperators', 'Ġpan', 'euro', 'pe', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'Ġeuro', 'pa', 'web', 'Ġportal', 'Ġretrieved', 'Ġapr', 'il', 'euro', 'pe', 'Ġcommission', 'Ġp', 'aves', 'Ġway', 'Ġeuro', 'pe', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'press', 'Ġrelease', 'Ġeuro', 'pe', 'Ġcommission', 'Ġmay', 'mobile', 'Ġsatellite', 'Ġservices', 'Ġeuro', 'pe', 'Ġfrequently', 'Ġasked', 'Ġquestions', 'Ġeuro', 'pa', 'web', 'Ġportal', 'Ġretrieved', 'Ġapr', 'il', 'Ġfel', 'ix', 'Ġb', 'ate', 'Ġmay', 'ars', 'Ġsolar', 'Ġwin', 'Ġspectrum', 'Ġrights', 'uters', 'Ġretrieved', 'Ġapr', 'il', 'pan', 'euro', 'pe', 'Ġnumbers', 'Ġservices', 'Ġeuro', 'pe', 'Ġcommission', 'Ġretrieved', 'Ġapr', 'il', 'euro', 'pas', 'Ġhell', 'ass', 'Ġskyrocket', 'de', 'Ġretrieved', 'Ġmay', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġone', 'Ġgiant', 'Ġstep', 'Ġcloser', 'ars', 'Ġaviation', 'Ġretrieved', 'Ġmarch', 'ï', '¬', 'Ĥ', 'ight', 'Ġwifi', 'Ġbattle', 'Ġeuro', 'pe', 'Ġtakes', 'Ġfinancial', 'Ġtimes', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'bel', 'gian', 'Ġcourt', 'Ġpunches', 'Ġhole', 'ars', "'s", 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġspac', 'en', 'ews', 'Ġmarch', 'ars', 'Ġorders', 'Ġï', '¬', 'ģ', 'f', 'th', 'Ġglobal', 'Ġx', 'press', 'Ġsatellite', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġspac', 'en', 'ews', 'Ġj', 'une', 'ars', 'Ġce', 'Ġhints', 'Ġadvanced', 'Ġglobal', 'Ġx', 'press', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġmarch', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġbuild', 'Ġtwo', 'Ġtriple', 'pay', 'load', 'Ġsatellites', 'Ġspace', 'way', 'Ġspace', 'x', 'Ġlaunch', 'htt', 'Ġace', 'x', 'launch', 'Ġspac', 'en', 'ews', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'ars']</t>
+          <t>['Ġretrieved', 'Ġapr', 'il', 'fe', 'ibility', 'Ġdragon', 'derived', 'Ġmars', 'Ġland', 'er', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġhuman', 'pre', 'c', 'ursor', 'Ġinvestigations', 'htt', 'net', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'cap', 'abilities', 'Ġservices', 'Ġbout', 'cap', 'abilities', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġties', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmarch', 'el', 'mus', 'k', 'Ġfe', 'b', 'ruary', 'side', 'Ġboosters', 'Ġlanding', 'Ġdrones', 'hips', 'Ġcenter', 'Ġexpended', 'Ġperformance', 'Ġpenalty', 'Ġfully', 'Ġexpended', 'Ġcost', 'Ġslightly', 'Ġhigher', 'Ġexpended', 'Ġaround', 'Ġmillion', 'weet', 'Ġvia', 'Ġtwitter', 'Ġmus', 'k', 'Ġel', 'Ġse', 'pt', 'ember', 'Ġbecoming', 'Ġmulti', 'planet', 'Ġspecies', 'video', 'Ġad', 'elaide', 'Ġaust', 'ral', 'ia', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġyoutube', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġjan', 'uary', 'mus', 'k', 'Ġambition', 'Ġspace', 'x', 'Ġaim', 'Ġfully', 'Ġreusable', 'Ġfal', 'con', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'fair', 'ing', 'Ġrecovery', 'Ġattempts', 'Ġspace', 'xf', 'le', 'et', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmarch', 'space', 'x', 'Ġï', '¬', 'Ĥ', 'ies', 'Ġrocket', 'Ġsecond', 'Ġtime', 'Ġhistoric', 'Ġtest', 'Ġcost', 'cutting', 'Ġtechnology', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'mus', 'k', 'Ġmarch', 'consider', 'ing', 'Ġtrying', 'Ġbring', 'Ġupper', 'Ġstage', 'Ġback', 'Ġfal', 'con', 'Ġheavy', 'Ġdemo', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfull', 'us', 'ability', 'Ġodds', 'Ġsuccess', 'Ġlow', 'Ġmaybe', 'Ġworth', 'Ġshot', 'weet', 'Ġretrieved', 'Ġj', 'une', 'Ġvia', 'Ġtwitter', 'ula', 'Ġdelta', 'Ġiv', 'Ġreference', 'Ġpage', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġe', 'ts', 'elta', 'iv', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġstr', 'ick', 'land', 'Ġjohn', 'Ġk', 'se', 'pt', 'ember', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġbooster', 'http']</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>['Ġawards', 'Ġcontract', 'Ġair', 'bus', 'ars', 'hi', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'ars', 'Ġsatellite', 'ars', 'ars', 'Ġwik', 'ipedia', 'atellite', 'Ġcommunication', 'Ġair', 'Ġtra', 'f', 'ï', '¬', 'ģ', 'c', 'Ġmanagement', 'iris', ')"', 'Ġes', 'int', 'esa', 'Ġusing', 'ars', 'Ġir', 'Ġopen', 'Ġskies', 'Ġav', 'ionics', 'Ġaviation', 'today', 'Ġmarch', 'ice', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġinterference', 'Ġinformation', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmarch', 'ï', '¬', 'ģ', 'cial', 'Ġwebsite', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['n', 'ss', 'Ġnational', 'Ġspace', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'x', 'Ġannounces', 'Ġlaunch', 'Ġdate', 'Ġworld', "'s", 'Ġpowerful', 'Ġrocket', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'el', 'mus', 'k', 'Ġmay', 'Ġf', 'h', 'Ġexpend', 'able', 'Ġperformance', 'Ġinclude', 'Ġcross', 'feed', '?"', 'Ġcross', 'Ġfeed', 'Ġwould', 'Ġhelp', 'Ġperformance', 'Ġneeded', 'Ġnumbers', 'weet', 'Ġretrieved', 'Ġj', 'une', 'Ġvia', 'Ġtwitter', 'Ġenvironmental', 'Ġimpact', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', '?"', 'Ġscience', 'Ġfocus', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'avis', 'Ġj', 'ason', 'let', "'s", 'Ġtalk', 'Ġel', 'Ġmus', 'k', 'Ġlaunching', 'es', 'la', 'Ġspace', 'Ġplanetary', 'Ġsociety', 'Ġretrieved', 'Ġoct', 'ober', 'Ġpur', 'due', 'Ġuniversity', 'Ġfe', 'b', 'ruary', 'tes', 'la', 'Ġspace', 'Ġcould', 'Ġcarry', 'Ġbacteria', 'Ġearth', 'phy', 'Ġphys', 'org', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'z', 'ond', 'Ġdavid', 'Ġfe', 'b', 'ruary', 'es', 'la', 'Ġroad', 'ster', 'Ġcould', 'Ġdirt', 'iest', 'Ġman', 'made', 'Ġobject', 'Ġspace', 'Ġnew', 'las', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ad', 'option', 'Ġenvironmental', 'Ġassessment', 'Ġfinding', 'Ġsign', 'ï', '¬', 'ģ', 'c', 'ant', 'Ġimpact', 'Ġboost', 'back', 'Ġlanding', 'Ġfal', 'con', 'Ġheavy', 'Ġboosters', 'Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġtestimony', 'Ġel', 'Ġmus', 'k', 'Ġmay', 'space', 'Ġshuttle', 'Ġfuture', 'Ġspace', 'Ġlaunch', 'Ġvehicles', 'Ġspace', 'ref', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une']</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>['Ġke', 'pler', 'Ġwik', 'ipedia', 'Ġke', 'pler', 'Ġartist', "'s", 'Ġconception', 'Ġsimultaneous', 'Ġtransit', 'Ġthree', 'Ġplanets', 'Ġke', 'pler', 'Ġobserved', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġspacecraft', 'Ġaug', 'Ġobservation', 'Ġdata', 'Ġepoch', 'Ġj', 'Ġequ', 'ox', 'Ġj', 'Ġconstellation', 'Ġcy', 'gn', 'us', 'Ġright', 'Ġasc', 'ension', 'h', 'Ġdecl', 'ination', 'Â°', 'âĢ²', '03', 'âĢ³', 'Ġapparent', 'Ġmagnitude', 'v', 'Ġcharacteristics', 'Ġspectral', 'Ġtype', 'Ġast', 'rom', 'etry', 'Ġproper', 'Ġmotion', 'Î¼', 'Ġra', 'ĠâĪĴ', '025', 'Ġmas', 'yr', 'Ġdec', '.:', 'ĠâĪĴ', '06', '029', 'Ġmas', 'yr', 'Ġpar', 'ax', 'ÏĢ', '01', 'Ġmas', 'Ġdistance', 'Ġly', 'Ġabsolute', 'Ġmagnitude', 'Ġdetails', 'Ġmass', '04', '005', 'âĺ', 'ī', 'Ġradius', '021', '025', 'Ġr', 'âĺ', 'ī', 'Ġsurface', 'Ġgravity', 'log', 'Ġg', '02', 'Ġtemperature', 'Ġmet', 'icity', 'fe', 'h', '06', '007', 'Ġdex', 'Ġrot', 'ational', 'Ġvelocity', 'v', 'Ġsin', 'Ġage', 'Ġdesign', 'ations', 'Ġk', 'ic', 'mass', 'Ġdatabase', 'Ġreferences', 'Ġsim', 'bad', 'Ġdata', 'Ġk', 'ic', 'Ġdata', 'Ġid', 'Ġke', 'pler', 'Ġcoordinates', 'h', 'Â°', 'âĢ²', 'âĢ³', 'Ġke', 'pler', 'Ġalso', 'Ġdesignated', 'mass', 'Ġsun', 'like', 'Ġstar', 'Ġslightly', 'Ġlarger', 'Ġsun', 'Ġconstellation', 'Ġcy', 'gn', 'us', 'Ġlocated', 'Ġlight', 'Ġyears', 'Ġearth', 'Ġlocated', 'Ġwithin', 'Ġfield', 'Ġvision', 'Ġke', 'pler', 'Ġspacecraft', 'Ġsatellite', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġmission', 'Ġuses', 'Ġdetect', 'Ġplanets', 'Ġmay', 'Ġtrans', 'iting', 'Ġstars', 'Ġannounced', 'Ġfe', 'b', 'ruary', 'Ġstar', 'Ġsystem', 'Ġamong', 'Ġcompact', 'Ġflatt', 'est', 'Ġsystems', 'Ġyet', 'Ġdiscovered', 'Ġfirst', 'Ġdiscovered', 'Ġcase', 'Ġstar', 'Ġsystem', 'Ġtrans', 'iting', 'Ġplanets', 'Ġdiscovered', 'Ġplanets', 'Ġlarger', 'Ġearth', 'Ġlarger', 'Ġones', 'Ġne', 'pt', 'une', "'s", 'Ġsize', 'Ġke', 'pler', 'Ġplanets', 'Ġdiscovered', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġmission']</t>
+          <t>['iet', 'zen', 'Ġfrank', 'Ġmarch', 'sp', 'ac', 'el', 'ift', 'Ġwashing', 'ton', 'Ġinternational', 'Ġspace', 'Ġtransportation', 'Ġassociation', 'Ġfal', 'tering', 'Ġmyth', 'Ġus', '000', 'Ġper', 'Ġpound', 'Ġw', 'html', 'id', 'Ġspace', 'ref', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'cap', 'abilities', 'Ġservices', 'mber', 'Ġarchived', 'Ġoriginal', 'cap', 'abilities', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmarch', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'cap', 'abilities', 'Ġj', 'uly', 'space', 'x', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġdod', 'son', 'Ġg', 'ere', 'l', 'le', 'Ġj', 'uly', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġpace', 'tel', 'esc', 'ope', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'elta', 'Ġiv', 'Ġul', 'al', 'aunch', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġv', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġset', 'Ġlaunch', 'Ġmassive', 'Ġsatellite', 'Ġj', 'uly', 'nd', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġdays', 'es', 'lar', 'ati', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ars', 'Ġjuggling', 'Ġtwo', 'Ġlaunches', 'Ġsays', 'Ġspace', 'x', 'Ġreturn', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'http', 'sp', 'ac', 'en', 'ews', 'c', 'Ġspac', 'en', 'ews', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġde', 'cember', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġset', 'Ġfal', 'con', 'Ġheavy', 'Ġdebut', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary']</t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -3194,7 +3194,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>['Ġmission', 'Ġtasked', 'Ġdiscovering', 'Ġplanets', 'Ġtransit', 'Ġaround', 'Ġstars', 'Ġtransit', 'Ġmethod', 'Ġke', 'pler', 'Ġuses', 'Ġinvolves', 'Ġdetecting', 'Ġdips', 'Ġbrightness', 'Ġstars', 'Ġdips', 'Ġbrightness', 'Ġinterpreted', 'Ġplanets', 'Ġwhose', 'Ġorbits', 'Ġmove', 'Ġfront', 'Ġstars', 'Ġperspective', 'Ġearth', 'Ġke', 'pler', 'Ġfirst', 'Ġdiscovered', 'Ġex', 'oplan', 'etary', 'Ġsystem', 'Ġthree', 'Ġtrans', 'iting', 'Ġplanets', 'Ġke', 'pler', 'Ġnamed', 'Ġke', 'pler', 'Ġmission', 'th', 'Ġstar', 'Ġconfirmed', 'Ġplanets', 'Ġdiscovered', 'Ġke', 'pler', 'Ġfield', 'Ġview', 'Ġplanets', 'Ġnamed', 'Ġalphabet', 'ically', 'Ġstarting', 'Ġinner', 'Ġb', 'Ġc', 'Ġe', 'Ġf', 'Ġg', 'Ġdistingu', 'ishers', 'Ġtagged', 'Ġonto', 'Ġname', 'Ġhome', 'Ġstar', 'Ġke', 'pler', 'Ġg', 'type', 'Ġstar', 'Ġapproximately', 'Ġmass', 'Ġradius', 'Ġsun', 'Ġsurface', 'Ġtemperature', 'Ġestimated', 'Ġage', 'Ġaround', 'Ġbillion', 'Ġyears', 'Ġcomparison', 'Ġsun', 'Ġbillion', 'Ġyears', 'Ġsurface', 'Ġtemperature', 'Ġapparent', 'Ġmagnitude', 'Ġfaint', 'Ġseen', 'Ġnaked', 'Ġknown', 'Ġplanets', 'Ġtransit', 'Ġstar', 'Ġmeans', 'Ġplanets', 'Ġorbits', 'Ġappear', 'Ġcross', 'Ġfront', 'Ġstar', 'Ġviewed', 'Ġearth', "'s", 'Ġperspective', 'Ġincl', 'inations', 'Ġrelative', 'Ġearth', "'s", 'Ġline', 'Ġsight', 'Ġfar', 'Ġplane', 'Ġsight', 'Ġvary', 'Ġlittle', 'Ġdegree', 'Ġallows', 'Ġdirect', 'Ġmeasurements', 'Ġplanets', 'Ġperiods', 'Ġrelative', 'Ġdiam', 'eters', 'comp', 'ared', 'Ġhost', 'Ġstar', 'Ġmonitoring', 'Ġplanet', "'s", 'Ġtransit', 'Ġstar', 'Ġsimulations', 'Ġsuggest', 'Ġmean', 'Ġmutual', 'Ġincl', 'inations', 'Ġplanetary', 'Ġorbits', 'Â°', 'Ġmeaning', 'Ġsystem', 'Ġprobably', 'Ġcop', 'lan', 'ar', 'fl', 'atter', 'Ġsolar', 'Ġsystem', 'Ġcorresponding', 'Ġfigure', 'Â°', 'Ġestimated', 'Ġmasses', 'Ġplanets', 'Ġfall', 'Ġrange', 'Ġearth', 'Ġne', 'pt', 'une', 'Ġestimated', 'Ġdens', 'ities', 'Ġlower', 'Ġearth', 'Ġimply', 'Ġnone', 'Ġearth', 'like', 'Ġcomposition', 'Ġsignificant', 'Ġhydrogen', 'hel', 'ium', 'Ġatmosphere', 'Ġpredicted', 'Ġplanets', 'Ġc', 'Ġe', 'Ġf', 'Ġg', 'Ġplanet', 'Ġmay', 'Ġsurrounded', 'Ġsteam', 'Ġatmosphere', 'Ġperhaps', 'Ġhydrogen', 'Ġatmosphere']</t>
+          <t>['Ġgovernment', 'opened', 'Ġspace', 'x', 'Ġsought', 'Ġtwo', 'Ġfal', 'con', 'Ġheavy', 'Ġpermits', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'two', 'months', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'draft', 'Ġenvironmental', 'Ġassessment', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlaunches', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġoct', 'ober', 'fal', 'con', 'heavy', 'block', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'tes', 'la', 'Ġroad', 'ster', 'aka', 'Ġstar', 'man', '017', ')"', 'sd', 'j', 'pl', 'n', 'asa', 'gov', 'Ġn', 'asa', 'Ġmarch', 'Ġarchived', 'Ġmand', '=-', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġroar', 'Ġthunder', 'Ġcarries', 'Ġspace', 'x', "'s", 'Ġambition', 'Ġorbit', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġde', 'cember', 'pay', 'load', 'Ġmidnight', 'Ġcherry', 'es', 'la', 'Ġroad', 'ster', 'Ġplaying', 'Ġspace', 'Ġodd', 'ity', 'Ġdestination', 'Ġmars', 'Ġorbit', 'Ġdeep', 'Ġspace', 'Ġbillion', 'Ġyears', "'t", 'Ġblow', 'Ġascent', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġde', 'cember', 'Ġred', 'Ġcar', 'Ġred', 'Ġplanet', 'weet', 'Ġretrieved', 'Ġjan', 'uary', 'Ġvia', 'Ġtwitter', 'Ġapr', 'il', 'launch', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġpushed', 'Ġth', 'ursday', 'Ġw', 'l', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'ar', 'abs', 'Ġgun']</t>
         </is>
       </c>
       <c r="C213" t="n">
@@ -3207,7 +3207,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>['Ġlow', 'Ġdens', 'ities', 'Ġlikely', 'Ġresult', 'Ġhigh', 'volume', 'Ġextended', 'Ġatmosp', 'heres', 'Ġsurround', 'Ġcores', 'Ġiron', 'Ġrock', 'Ġpossibly', 'Ġinner', 'Ġconstituents', 'Ġke', 'pler', 'Ġsystem', 'Ġtime', 'Ġdiscoveries', 'Ġcomprehens', 'ively', 'Ġunderstood', 'Ġextras', 'olar', 'Ġplanets', 'Ġsmaller', 'Ġne', 'pt', 'une', 'Ġcurrently', 'Ġobservations', 'Ġplace', 'Ġfirm', 'Ġconstraint', 'Ġmass', 'Ġplanet', 'Ġ(&lt;', 'Ġhowever', 'Ġformation', 'Ġevolution', 'Ġstudies', 'Ġindicate', 'Ġmass', 'Ġplanet', 'Ġmuch', 'Ġgreater', 'Ġke', 'pler', 'Ġplanets', 'Ġmay', 'Ġformed', 'Ġsitu', 'e', '.,', 'Ġobserved', 'Ġorbital', 'Ġlocations', 'Ġsitu', 'Ġmay', 'Ġstarted', 'Ġformation', 'Ġfarther', 'Ġaway', 'Ġstar', 'Ġmigrating', 'Ġinward', 'Ġgravitational', 'Ġinteractions', 'Ġg', 'ase', 'ous', 'Ġprot', 'oplan', 'etary', 'Ġdisk', 'Ġsecond', 'Ġscenario', 'Ġpredicts', 'Ġsubstantial', 'Ġfraction', 'Ġplanets', 'Ġmass', 'Ġregardless', 'Ġformation', 'Ġscenario', 'Ġg', 'ase', 'ous', 'Ġcomponent', 'Ġplanets', 'Ġn', 'omen', 'cl', 'ature', 'Ġhistory', 'Ġcharacteristics', 'Ġplanetary', 'Ġsystem', 'Ġke', 'pler', 'Ġwik', 'ipedia', 'Ġorbit', 'Ġke', 'pler', 'Ġplanets', 'Ġcomparison', 'Ġorbits', 'Ġplanets', 'Ġmercury', 'Ġven', 'us', 'Ġaccounts', 'Ġless', 'Ġmasses', 'Ġâī', 'Ī', 'Ġâī', 'Ī', 'Ġrad', 'ii', 'Ġdynam', 'ical', 'Ġsimulation', 'Ġshown', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġlikely', 'Ġundergone', 'Ġsubstantial', 'Ġinward', 'Ġmigration', 'Ġpast', 'Ġproducing', 'Ġobserved', 'Ġpattern', 'Ġlower', 'mass', 'Ġplanets', 'Ġtight', 'est', 'Ġorbits', 'Ġadditional', 'Ġyet', 'Ġunob', 'served', 'Ġgas', 'Ġgiant', 'Ġplanets', 'Ġwider', 'Ġorbit', 'Ġlikely', 'Ġnecessary', 'Ġmigration', 'Ġsmaller', 'Ġplanets', 'Ġproceed', 'Ġfar', 'Ġinward', 'Ġsystem', 'Ġamong', 'Ġcompact', 'Ġknown', 'Ġorbits', 'Ġplanets', 'Ġwould', 'Ġeasily', 'Ġfit', 'Ġinside', 'Ġorbit', 'Ġmercury', 'Ġslightly', 'Ġoutside', 'Ġdespite', 'Ġclose', 'Ġpacking', 'Ġorbits', 'Ġdynam', 'ical', 'Ġinteg', 'rations', 'Ġindicate', 'Ġke', 'pler', 'Ġsystem', 'Ġpotential', 'Ġstable', 'Ġtime', 'Ġscale', 'Ġbillions', 'Ġyears', 'Ġhowever', 'Ġmay', 'Ġapproaching', 'Ġinstability', 'Ġdue', 'Ġsecular', 'Ġresonance', 'Ġinvolving', 'Ġc', 'Ġhappens', 'Ġlikely', 'Ġbecome', 'Ġeccentric', 'Ġenough', 'Ġcoll', 'ides', 'Ġnone', 'Ġplanets', 'Ġlow', 'rat', 'io', 'Ġorbital', 'Ġreson', 'ances', 'Ġmultiple', 'Ġplanets', 'Ġgrav', 'itation', 'ally', 'Ġtug', 'Ġstabilize', "'s", 'Ġorbits', 'Ġresulting', 'Ġsimple', 'Ġratios', 'Ġorbital', 'Ġperiods']</t>
+          <t>['ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'ar', 'abs', 'Ġce', 'Ġfal', 'con', 'Ġheavy', 'Ġgives', 'Ġsatellite', 'Ġextra', 'Ġlife', 'Ġspac', 'en', 'ews', 'Ġapr', 'il', 'Ġarchived', 'Ġra', 'life', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġsuccessful', 'Ġcommercial', 'Ġdebut', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'n', 'asa', 'Ġlooking', 'Ġlaunch', 'Ġdelayed', 'Ġspace', 'Ġscience', 'Ġmissions', 'Ġearly', 'Ġar', 'ly', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġgra', 'ham', 'iam', 'Ġapr', 'il', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġar', 'abs', 'nas', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġke', 'lly', 'Ġem', 'Ġapr', 'il', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġcore', 'Ġbooster', 'Ġlost', 'Ġrough', 'Ġseas', 'Ġen', 'Ġroute', 'Ġport', 'aver', 'al', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġapr', 'il', 'fal', 'con', 'Ġheavy', 'Ġstar', 'link', 'Ġheadline', 'Ġspace', 'x', "'s", 'Ġupcoming', 'Ġmanifest', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'x', 'Ġlaunch', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'n', 'asa', 'k', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'pm', 'Ġyoutube', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'rocket', 'Ġlaunch', 'Ġviewing', 'Ġcape', 'aver', 'al', 'Ġwatch', 'Ġview', 'Ġsee', 'las', 'Ġdelta', 'Ġfal', 'con', 'Ġlaunches', 'Ġviewing', 'html', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'pre', 'view', 'Ġsucceed', 'Ġfail', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġsure', '..."', 'Ġplanetary']</t>
         </is>
       </c>
       <c r="C214" t="n">
@@ -3220,7 +3220,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>['Ġhowever', 'Ġclose', 'Ġratio', 'Ġcould', 'Ġconce', 'ivably', 'Ġplanets', 'Ġsystem', 'Ġtransit', 'Ġstar', 'Ġwould', 'Ġdetectable', 'Ġeffects', 'Ġgravity', 'Ġmotion', 'Ġvisible', 'Ġplanets', 'much', 'Ġne', 'pt', 'une', 'Ġdiscovered', 'Ġpresence', 'Ġadditional', 'Ġgas', 'Ġgiant', 'Ġplanets', 'Ġcurrently', 'Ġexcluded', 'Ġorbital', 'Ġradius', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġcompanion', 'Ġorder', 'Ġstar', 'Ġmass', 'Ġsem', 'im', 'ajor', 'Ġaxis', 'Ġorbital', 'Ġperiod', 'days', 'Ġeccentric', 'ity', 'Ġinclination', 'Ġradius', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '09', '001', '000', 'ĠâĪĴ', '0010', '045', 'ĠâĪĴ', '04', 'ĠâĪĴ', 'Â°', '07', 'ĠâĪĴ', '04', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '001', '00', 'ĠâĪĴ', '000', '026', '06', 'ĠâĪĴ', '013', 'ĠâĪĴ', 'Â°', '05', 'ĠâĪĴ', '06', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '001', '000', '004', '007', 'ĠâĪĴ', '002', 'ĠâĪĴ', 'Â°', '06', 'ĠâĪĴ', '07', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '002', '000', 'ĠâĪĴ', '00', '012', '006', 'ĠâĪĴ', '006', '02', 'ĠâĪĴ', '02', 'Â°', '07', 'ĠâĪĴ', '09', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '002', '00', 'ĠâĪĴ', '00', '013', '011', 'ĠâĪĴ', '009', '04', 'Â°']</t>
+          <t>['Ġsociety', 'Ġarchived', 'web', 'arch', 'iv', 'Ġe', 'w', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'lights', 'ail', 'Ġplanetary', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgreen', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', ')"', 'Ġages', 'td', 'green', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'green', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', ')"', 'Ġball', 'Ġaerospace', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġgreen', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', ')"', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġcorp', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdeep', 'Ġspace', 'Ġatomic', 'Ġclock', 'ds', 'ac', 'Ġoverview', 'Ġarchived', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġn', 'asa', 'Ġaccessed', 'Ġde', 'cember', 'Ġgeneral', 'Ġatom', 'ics', 'Ġcompletes', 'Ġready', 'launch', 'Ġtesting', 'Ġorbital', 'Ġtest', 'Ġbed', 'Ġsatellite', 'Ġarchived', 'h', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġgeneral', 'Ġatom', 'ics', 'Ġelectromagnetic', 'Ġsystems', 'Ġpress', 'Ġrelease', 'Ġapr', 'il', 'space', 'x', 'Ġawarded', 'Ġtwo', 'Ġe', 'el', 'v', 'class', 'Ġmissions', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'http', 'space', 'Ġspace', 'x', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'form', 'os', 'Ġcosmic', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'oc', 'ulus', 'r', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'r', 'htm', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'fal', 'con', 'Ġoverloaded', 'Ġknowledge', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġscheduled', 'Ġoct', 'ober', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġnews', 'Ġarchived', 'htt']</t>
         </is>
       </c>
       <c r="C215" t="n">
@@ -3233,7 +3233,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>['04', 'ĠâĪĴ', '07', 'Ġr', 'ðŁ', 'ľ', '¨', 'ðŁ', 'ľ', '¨', '004', '0010', 'ĠâĪĴ', '000', '013', '011', 'ĠâĪĴ', '009', '05', 'ĠâĪĴ', '06', 'Â°', '06', 'ĠâĪĴ', '08', 'Ġr', 'ðŁ', 'ľ', '¨', 'Ġrelative', 'Ġsize', 'Ġpositions', 'Ġplanets', 'Ġke', 'pler', 'Ġinner', 'Ġsolar', 'Ġsystem', 'Ġcomparison', 'Ġdiam', 'eters', 'Ġplanets', 'Ġstars', 'Ġscaled', 'Ġfactor', 'Ġlist', 'Ġmulti', 'plan', 'etary', 'Ġsystems', 'Ġke', 'pler', 'Ġmission', 'Ġgl', 'ies', 'e', 'c', 'ri', 'Ġbrown', 'Ġg', '.;', 'Ġet', 'Ġal', 'ga', 'ia', 'Ġcollaboration', 'aug', 'ust', 'ga', 'ia', 'Ġdata', 'Ġrelease', 'Ġsummary', 'Ġcontents', 'Ġsurvey', 'Ġproperties', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġar', 'x', 'iv', '04', '09', 'ui', 'Ġga', 'ia', 'Ġrecord', 'Ġsource', 'Ġviz', 'ier', 'Ġl', 'iss', 'auer', 'Ġjack', 'Ġj', '.;', 'Ġet', 'Ġal', 'Ġclosely', 'Ġpacked', 'Ġsystem', 'Ġlow', 'mass', 'Ġlow', 'density', 'Ġplanets', 'Ġtrans', 'iting', 'Ġke', 'pler', '".', 'Ġnature', '):', 'âĢĵ', 'Ġar', 'x', 'iv', 'f', 'nature', '09', 'Ġpm', 'id', 'Ġn', 'ih', 'gov', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġke', 'pler', 'Ġwik', 'ipedia', 'Ġbed', 'ell', 'gan', 'Ġet', 'Ġal', 'ke', 'pler', 'Ġsolar', 'Ġtwin', 'Ġrev', 'ising', 'Ġmasses', 'Ġrad', 'ii', 'Ġbenchmark', 'Ġplanets', 'Ġvia', 'Ġprecise', 'Ġstellar', 'Ġcharacterization', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġar', 'x', 'iv', '06', 'htt', 'http', 'ke', 'pler', 'Ġpl', 'er', 'Ġsim', 'bad', 'Ġcentre', 'Ġde', 'n', 'Ã©', 'es', 'Ġastron', 'om', 'iques', 'Ġde', 'Ġstr', 'bourg', 'Ġretrieved', '05', '09', 'mass', 'Ġj', 'Ġsim', 'bad', 'Ġcentre', 'Ġde', 'n', 'Ã©', 'es', 'Ġastron', 'om', 'iques', 'Ġde', 'Ġstr']</t>
+          <t>['Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġcenter', 'Ġcore', 'Ġnarrowly', 'Ġmiss', 'Ġinverse', 'Ġj', 'une', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'uss', 'f', 'Ġspace', 'Ġforce', 'Ġsuccessfully', 'Ġcompletes', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'ero', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'air', 'Ġforce', 'Ġawards', 'Ġmillion', 'Ġlaunch', 'Ġservice', 'Ġcontracts', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġwins', 'Ġpotential', 'Ġus', 'Ġmillion', 'Ġcontract', 'Ġus', 'af', 'Ġn', 'ro', 'Ġsatellite', 'Ġlaunch', 'Ġservices', 'http', 'Ġh', 'services', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġr', 'v', 'ices', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'us', 'Ġspace', 'Ġforce', 'Ġtet', 'ra', 'Ġsatellite', 'Ġprepared', 'Ġlaunch', 'month', 'Ġintegration', 'Ġpar', 'abolic', 'Ġarc', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġse', 'pt', 'ember', 'space', 'x', "'s", 'Ġnext', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġslips', 'ww', 'es', 'lar', 'ati', 'Ġarchived', 'web', 'Ġed', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'uss', 'f', 'Ġcentre', 'Ġcore', 'Ġlacks', 'Ġlanding', 'Ġgear', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġtwitter', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġthree', 'year', 'Ġwait', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġcould', 'Ġlaunch', 'Ġlater', 'Ġmonth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġcore', 'Ġstage', 'Ġexpended', 'Ġus', 'sf', 'Ġrocket', "'s", 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġreturned', 'Ġnear', 'sim', 'ultane', 'ous', 'Ġland', 'ings', 'Ġspace', 'x', "'s", 'Ġrecovery', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation']</t>
         </is>
       </c>
       <c r="C216" t="n">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>['bourg', 'ichael', 'ew', 'hin', 'ney', 'Ġrac', 'hel', 'Ġh', 'oo', 'ver', 'rent', 'Ġj', 'Ġper', 'ro', 'tto', 'Ġfe', 'b', 'ruary', 'n', 'asa', "'s", 'Ġke', 'pler', 'Ġspacecraft', 'Ġdiscovers', 'Ġextraordinary', 'Ġnew', 'Ġplanetary', 'Ġsystem', 'Ġn', 'asa', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfr', 'aser', 'Ġc', 'Ġse', 'pt', 'ember', 'Ġold', 'Ġsun', '?"', 'Ġuniverse', 'Ġtoday', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfr', 'aser', 'Ġc', 'se', 'pt', 'ember', 'tem', 'perature', 'Ġsun', 'htt', 'Ġuniverse', 'Ġtoday', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġboy', 'le', 'Ġal', 'Ġfe', 'b', 'ruary', 'plan', 'etary', 'Ġsix', 'pack', 'Ġposes', 'Ġpuzzle', 'Ġcosmic', 'Ġlog', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġl', 'iss', 'auer', 'Ġjack', 'Ġj', '.;', 'Ġet', 'Ġal', 'Ġplanets', 'Ġknown', 'Ġorbit', 'Ġke', 'pler', 'Ġlow', 'Ġdens', 'ities', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġar', 'x', 'iv', 'angelo', 'Ġg', '.;', 'Ġbod', 'en', 'heimer', 'Ġp', 'Ġsitu', 'Ġsitu', 'Ġformation', 'Ġmodels', 'Ġke', 'pler', 'Ġplanets', '".', 'Ġastroph', 'ysical', 'Ġjournal', '):', 'Ġid', 'Ġpp', '.).', 'Ġar', 'x', 'iv', '06', '080', 'ar', 'x', 'iv', 'Ġg', 'abs', '06', '080', 'ui', 'ads', 'ab', 'Ġpus', 'id', 'Ġna', 'eye', 'Ġro', 'bert', 'Ġfe', 'b', 'ruary', 'ke', 'pler', "'s", 'Ġoutrageous', 'Ġsystem', 'Ġplanets', 'Ġtelescope', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġjohn', 'atson', 'Ġfe', 'b', 'ruary', 'Ġwealth', 'Ġworlds', 'Ġke', 'pler', 'Ġspacecraft', 'Ġfinds', 'Ġnew', 'Ġex', 'oplan', 'ets', 'Ġhints', 'htt', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhands', 'Ġr', 'lex', 'ander', 'Ġw', 'Ġde', 'hn', 'en', 'standing', 'Ġassembly', 'Ġke', 'pler', "'s", 'Ġcompact', 'Ġplanetary', 'Ġsystems', '",', 'ac', 'Ġhands', '.;', 'lex', 'ander', 'Ġr', 'Ġmight']</t>
+          <t>['Ġmilitary', 'Ġspokesperson', 'Ġsaid', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġus', 'sf', 'Ġmission', 'Ġwould', 'Ġtarget', 'Ġlanding', 'Ġtwo', 'Ġspace', 'x', 'Ġdrone', 'Ġships', 'Ġï', '¬', 'Ĥ', 'ating', 'range', 'l', 'antic', 'Ġocean', '."', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'launch', 'Ġn', 'asa', "'s", 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġdelayed', 'Ġlate', 'Ġse', 'pt', 'ember', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'se', 'pt', 'ember', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'one', 'Ġmissions', 'Ġus', 'sf', 'Ġtent', 'atively', 'Ġscheduled', 'Ġlate', 'Ġj', 'une', 'Ġpostponed', 'Ġind', 'e', 'ï', '¬', 'ģ', 'n', 'itely', 'Ġ...', 'Ġdelays', 'Ġupcoming', 'Ġfal', 'con', 'Ġheavy', 'Ġmissions', 'Ġcaused', 'Ġpayload', 'Ġissues', '."', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġoct', 'ober', 'space', 'x', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġthree', 'Ġyears', 'Ġeyes', 'Ġlate', 'oct', 'ober', 'Ġlif', 'ff', 'two', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġthree', 'year', 'Ġwait', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġcould', 'Ġlaunch', 'Ġlater', 'Ġmonth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġspace', 'Ġforce', 'Ġsaid', 'Ġmission', 'Ġmilitary', 'Ġsays', 'Ġlaunch', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġlike', 'Ġus', 'sf', 'Ġcurrently', 'Ġscheduled', 'Ġjan', 'uary', '."', 'space', 'Ġnews', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'mber', 'Ġcl', 'ark', 'Ġstep', 'hen', 'fal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġpad', 'Ġone', 'Ġspace', 'x', "'s", 'Ġcomplex', 'Ġmissions', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'Ġnext', 'Ġmilitary', 'Ġmission', 'Ġï', '¬', 'Ĥ', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġnamed', 'Ġlaunch', 'Ġl', 'pe', 'Ġspacecraft', 'Ġspace', 'Ġforce', 'Ġcommunications', 'Ġsatellite', 'Ġtandem', 'Ġlaunch', 'Ġscheduled', 'Ġjan', 'uary', 'Ġuse', 'Ġfal', 'con', 'Ġheavy', 'Ġside', 'Ġboosters', 'Ġï', '¬', 'Ĥ', 'Ġus', 'sf', 'Ġmission']</t>
         </is>
       </c>
       <c r="C217" t="n">
@@ -3259,7 +3259,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>['Ġgiants', 'Ġunseen', 'Ġj', 'upiter', 'mass', 'Ġplanets', 'Ġsculpt', 'ors', 'Ġtightly', 'packed', 'Ġplanetary', 'Ġsystems', '",', 'Ġmonthly', 'Ġnotices', 'Ġroyal', 'Ġastronomical', 'Ġsociety', '):', 'âĢĵ', 'Ġar', 'x', 'iv', '026', 'Ġb', '026', 'Ġcont', 'ras', 'Ġp', 'Ġgran', 'ados', 'Ġbo', 'ley', 'Ġc', 'Ġmarch', 'Ġdynamics', 'Ġtightly', 'packed', 'Ġplanetary', 'Ġsystems', 'Ġpresence', 'Ġouter', 'Ġplanet', 'Ġcase', 'Ġstudies', 'Ġusing', 'Ġke', 'pler', 'Ġke', 'pler', '".', 'Ġastronomical', 'Ġjournal', '):', 'Ġar', 'x', 'iv', '02', '01', 'http', 'Ġbec', 'ker', 'Ġj', 'ul', 'iet', 'te', 'Ġc', '.;', 'Ġad', 'ams', 'Ġf', 'red', 'Ġc', 'effects', 'Ġunseen', 'Ġadditional', 'Ġplanetary', 'Ġpert', 'ur', 'bers', 'Ġcompact', 'Ġextras', 'olar', 'Ġplanetary', 'Ġsystems', '",', 'Ġmonthly', 'Ġnotices', 'Ġroyal', 'Ġastronomical', 'Ġsociety', 'âĢĵ', 'Ġar', 'x', 'iv', '02', '07', '005', 'Ġpus', 'id', '005', 'Ġk', 'ub', 'ys', 'h', 'k', 'ina', '.;', 'Ġfoss', 'ati', 'Ġl', '.;', 'Ġmust', 'ill', 'Ġj', '.;', 'Ġcub', 'ill', 'os', 'Ġp', 'Ġe', '.;', 'av', 'ies', 'Ġb', '.;', 'Ġer', 'ka', 'ev', 'Ġn', 'Ġv', '.;', 'Ġjohn', 'stone', 'Ġc', 'Ġp', '.;', 'Ġk', 'lyak', 'ova', 'Ġk', 'Ġg', '.;', 'Ġlam', 'mer', 'Ġh', '.;', 'Ġlend', 'l', '.;', 'Ġod', 'ert', 'Ġp', 'Ġke', 'pler', 'Ġsystem', 'Ġevolution', 'Ġstellar', 'Ġhigh', 'energy', 'Ġemission', 'Ġinitial', 'Ġplanetary', 'Ġatmospheric', 'Ġmass', 'Ġfractions', '".', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġar', 'x', 'iv', '09', 'http', '003', '003', 'ï', '¬', 'ģ', 'cial', 'Ġrelease', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġspacecraft', 'Ġdiscovers', 'Ġextraordinary', 'Ġnew', 'Ġplanetary', 'Ġsystem', 'Ġyoutube', 'Ġanimation', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġorbits', 'Ġplanet', 'Ġsizes', 'Ġastronomers', 'Ġfind', 'pack', 'Ġplanets', 'Ġalien', 'Ġsolar', 'Ġsystem', 'Ġn', 'asa', 'Ġastronomy', 'Ġpicture', 'Ġday', 'Ġworlds', 'Ġke', 'pler', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġassuming', 'Ġsuccessful', 'Ġrecovery', 'Ġlanding', 'Ġzones', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġspace', 'Ġforce', 'Ġsaid', '."', 'fal', 'con', 'Ġheavy', 'Ġcould', 'Ġlaunch', 'Ġthree', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmissions', 'Ġspac', 'en', 'ews', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġoct', 'ober', 'v', 'ias', 'Ġameric', 'Ġar', 'ct', 'urus', 'Ġnext', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġrainbow', 'Ġj', 'ason', 'Ġse', 'pt', 'ember', 'next', 'Ġcommercial', 'Ġfal', 'con', 'Ġheavy', 'Ġmission', 'Ġlaunch', 'Ġdebut', 'str', 'Ġsatellite', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'application', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'str', 'Ġb', 'erm', 'uda', 'Ġattachment', 'Ġnarrative', 'fc', 'str', 'Ġb', 'erm', 'uda', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'ar', 'abs', 'Ġfal', 'con', 'Ġheavy', 'Ġmission', 'Ġslated', 'Ġde', 'cember', 'âĢĵ', 'jan', 'uary', 'Ġtimeframe', 'Ġspac', 'en', 'ews', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'v', 'ias', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġnext', 'gen', 'Ġbroadband', 'Ġsatellite', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'v', 'ias', 'Ġspace', 'x', 'Ġenter', 'Ġcontract', 'Ġfuture', 'Ġv', 'ias', 'Ġsatellite', 'Ġlaunch', 'Ġv', 'ias', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġb', 'aylor', 'ichael', 'fal', 'con', 'Ġheavy', 'Ġe', 'ch', 'ost', 'ar', 'j', 'upiter', ')"', 'Ġtails', 'Ġarchived', 'Ġn', 'ches', 'details', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġmay', 'j', 'upiter', 'Ġe', 'ch', 'ost', 'ar', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay']</t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -3272,7 +3272,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>['Ġtechnology', 'Ġdemonstration', 'Ġwik', 'ipedia', 'Ġtechnology', 'Ġdemonstration', 'Ġtechnology', 'Ġdemonstration', 'Ġtech', 'Ġdemo', 'Ġalso', 'Ġknown', 'Ġdemonstr', 'ator', 'Ġmodel', 'Ġprototype', 'Ġrough', 'Ġexample', 'Ġotherwise', 'Ġincomplete', 'Ġversion', 'Ġconceivable', 'Ġproduct', 'Ġfuture', 'Ġsystem', 'Ġput', 'Ġtogether', 'Ġproof', 'Ġconcept', 'Ġprimary', 'Ġpurpose', 'Ġshowcasing', 'Ġpossible', 'Ġapplications', 'Ġfeasibility', 'Ġperformance', 'Ġmethod', 'Ġidea', 'Ġnew', 'Ġtechnology', 'Ġused', 'Ġdemonstrations', 'Ġinvestors', 'Ġpartners', 'Ġjournalists', 'Ġeven', 'Ġpotential', 'Ġcustomers', 'Ġorder', 'Ġconvince', 'Ġviability', 'Ġchosen', 'Ġapproach', 'Ġtest', 'Ġordinary', 'Ġusers', 'Ġtechnology', 'Ġdemonstrations', 'Ġoften', 'Ġused', 'Ġcomputer', 'Ġindustry', 'Ġemerging', 'Ġimportant', 'Ġtool', 'Ġresponse', 'Ġshort', 'Ġdevelopment', 'Ġcycles', 'Ġsoftware', 'Ġhardware', 'Ġdevelopment', 'Ġcomputer', 'Ġgame', 'Ġdevelopers', 'Ġuse', 'Ġtech', 'Ġdemos', 'Ġr', 'ouse', 'Ġmaintain', 'Ġinterest', 'Ġtitles', 'Ġstill', 'Ġdevelopment', 'Ġgame', 'Ġengines', 'Ġusually', 'Ġready', 'Ġart', 'Ġï', '¬', 'ģ', 'n', 'ished', 'Ġensure', 'Ġfunctionality', 'Ġearly', 'Ġtesting', 'Ġshort', 'Ġsegments', 'Ġusing', 'Ġï', '¬', 'ģ', 'n', 'ished', 'Ġgame', 'Ġengines', 'Ġmay', 'Ġpresented', 'Ġgame', 'Ġdemos', 'Ġgraphics', 'Ġcards', 'Ġmanufacturers', 'Ġuse', 'Ġtech', 'Ġdemos', 'Ġshowcase', 'Ġperformance', 'Ġcards', 'Ġeven', 'Ġgames', 'Ġdeliver', 'Ġperformance', 'Ġproduct', 'Ġready', 'Ġused', 'Ġoutside', 'Ġdevelopment', 'Ġlabs', 'mber', 'Ġn', 'vidia', 'Ġstarted', 'Ġpractice', 'Ġfeaturing', 'Ġrealistic', 'Ġcharacters', 'Ġgraphics', 'Ġcard', 'Ġtechnology', 'Ġdemos', 'Ġreleasing', 'Ġdawn', 'Ġg', 'ef', 'orce', 'Ġcard', 'Ġdemo', 'Ġfeatured', 'Ġforest', 'Ġfairy', 'Ġsemi', 'real', 'istic', 'Ġshort', 'Ġhair', 'Ġbeautiful', 'Ġwings', 'Ġlater', 'Ġn', 'vidia', 'Ġfollowed', 'Ġsimilar', 'Ġnew', 'Ġdemos', 'Ġtechnologies', 'Ġjoined', 'Ġrace', 'Ġnature', 'Ġmuch', 'Ġless', 'Ġcomplex', 'Ġcomplete', 'Ġgames', 'Ġinclude', 'Ġdynamic', 'Ġphysics', 'Ġmodelling', 'Ġaudio', 'Ġengines', 'Ġetc', '.),', 'Ġtechnology', 'Ġdemos', 'Ġgraphics', 'Ġdeliver', 'Ġsubstantially', 'Ġbetter', 'Ġimage', 'Ġquality', 'Ġmaking', 'Ġgeneral', 'Ġlook', 'Ġgames', 'Ġlag', 'Ġseveral', 'Ġyears', 'Ġbehind', 'Ġvideo', 'Ġcard', 'Ġtechnology', 'Ġdemos', 'Ġexample', 'Ġplay', 'station', 'Ġdemos', 'Ġn', 'co', 'Ġgirl', 'Ġlif', 'el', 'ike', 'Ġfemale', 'Ġcharacter', 'Ġridge', 'Ġracer', 'Ġw', 'inking', 'Ġï', '¬', 'Ĥ', 'irt', 'iously', 'Ġviewers', 'Ġold', 'Ġman', 'Ġused', 'Ġprocessing', 'Ġpower', 'Ġproduce', 'Ġhigh', 'quality', 'Ġsingle', 'Ġcharacter', 'Ġmodel', 'Ġstatic', 'Ġenvironment', 'Ġtrailers', 'Ġalso', 'Ġshowed', 'Ġraven', 'Ġbuff', 'Ġwoman', 'Ġrobot', 'Ġshowing', 'Ġmartial', 'Ġart', 'Ġmoves', 'Ġcomputer', 'Ġtechnology', 'Ġdemos', 'Ġconfused', 'Ġdem', 'osc', 'ene', 'based', 'Ġdemos', 'Ġalthough', 'Ġoften', 'Ġdemonstrating', 'Ġnew', 'Ġsoftware', 'Ġtechniques']</t>
+          <t>['n', 'asa', 'Ġcontinues', 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġn', 'asa', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġpsyche', 'Ġmission', 'nas', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġus', 'sf', 'Ġnext', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'air', 'Ġforce', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġspace', 'x', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'contract', 'Ġaug', 'Ġdefense', 'gov', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'space', 'Ġexploration', 'Ġtechnologies', 'Ġcorp', '.,', 'Ġhaw', 'th', 'orne', 'Ġcal', 'ornia', 'Ġawarded', '07', 'Ġbilateral', 'Ġmod', 'ï', '¬', 'ģ', 'cation', 'p', '0000', 'Ġpreviously', 'Ġawarded', 'Ġspace', 'Ġforce', 'Ġcontract', 'Ġfa', 'c', '000', '...', 'Ġ...', 'Ġtotal', 'Ġcumulative', 'Ġface', 'Ġvalue', 'Ġcontract', '07', '."', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'ms', 'r', 'Ġintegrated', 'Ġmaster', 'Ġschedule', 'ï', '¬', 'ģ', 'ce', 'Ġsafety', 'Ġmission', 'Ġassurance', 'Ġn', 'asa', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'n', 'asa', 'g', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġmarg', 'etta', 'Ġro', 'bert', 'Ġse', 'pt', 'ember', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġgoes', 'u', 'Ġmission', 'Ġss', 'ion', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġmission', 'w', 'press', 'Ġrelease', 'Ġn', 'asa', 'Ġj', 'uly']</t>
         </is>
       </c>
       <c r="C219" t="n">
@@ -3285,7 +3285,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>['Ġregarded', 'Ġstand', 'alone', 'Ġform', 'Ġcomputer', 'Ġart', 'Ġdemo', 'Ġslam', 'Ġwebsite', 'Ġgoogle', 'Ġinc', '.,', 'Ġlaunched', 'Ġslogan', 'bring', 'Ġcreativity', 'Ġbring', 'Ġtech', 'Ġbring', 'Ġgeneral', 'Ġfool', 'Ġdemo', 'Ġslam', '!",', 'Ġlarge', 'Ġcollection', 'Ġtechnology', 'Ġdemonstrations', 'Ġuploaded', 'Ġusers', 'Ġgoogle', 'Ġexecutives', 'Ġwell', 'Ġgo', 'cont', 'ender', "'.", 'Ġcomputers', 'Ġgaming', 'Ġgoogle', 'Ġtech', 'Ġdemo', 'Ġsales', 'Ġengineering', 'Ġtechnology', 'Ġdemonstration', 'Ġtechnology', 'Ġdemonstration', 'Ġwik', 'ipedia', 'Ġsales', 'Ġengineering', 'Ġstaff', 'Ġoften', 'Ġbearing', 'Ġtitle', 'Ġsales', 'Ġengineer', 'Ġpres', 'ales', 'Ġconsultant', 'Ġprepare', 'Ġtechnology', 'Ġdemonstrations', 'Ġbusiness', 'Ġmeetings', 'Ġseminars', 'Ġshow', 'Ġcapabilities', 'Ġbusiness', 'Ġproducts', 'Ġinclude', 'Ġsoftware', 'Ġhardware', 'Ġproducts', 'Ġshow', 'Ġmultiple', 'Ġproducts', 'Ġintegrating', 'Ġtogether', 'Ġusually', 'Ġdemonstration', 'Ġless', 'Ġproof', 'Ġconcept', 'Ġcome', 'Ġway', 'Ġshowing', 'Ġbusiness', 'Ġproject', 'Ġmay', 'Ġjustified', 'Ġlarge', 'Ġcompanies', 'Ġtens', 'Ġhundreds', 'Ġsales', 'Ġengineers', 'Ġoften', 'Ġteam', 'Ġspecialize', 'Ġproduction', 'Ġdemonstration', 'Ġsystems', 'Ġplans', 'Ġdemo', 'Ġmode', 'Ġgame', 'Ġdemo', 'Ġresearch', 'Ġdevelopment', 'Ġmother', 'Ġdemos', 'Ġdou', 'glas', 'Ġeng', 'el', 'bart', "'s", 'Ġdemonstration', 'Ġeasy', 'Ġsteps', 'Ġgreat', 'Ġtech', 'Ġdemo', 'Ġgreat', 'Ġtech', 'Ġdemo', 'Ġretrieved', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġarchived', 'ion', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġflagship', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġinches', 'Ġforward', 'Ġshack', 'led', 'Ġearth', 'Ġsuper', 'cl', 'uster', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'n', 'asa', 'Ġuse', 'Ġcommercial', 'Ġlaunch', 'Ġvehicle', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġspac', 'en', 'ews', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġde', 'cember', 'Ġcol', 'ap', 'rete', 'Ġanth', 'ony', 'Ġaug', 'ust', 'vi', 'per', 'Ġlunar', 'Ġwater', 'Ġreconnaissance', 'Ġmission', 'sc', 'ie', 'Ġac', 'pdf', 'Ġn', 'asa', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'n', 'asa', 'Ġrepl', 'ans', 'Ġcl', 'ps', 'Ġdelivery', 'Ġv', 'iper', 'Ġreduce', 'Ġrisk', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġcol', 'ap', 'rete', 'Ġanth', 'ony', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġselects', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġlunar', 'Ġrover', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġselects', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġlunar', 'Ġrover', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġassessments', 'Ġmajor', 'Ġprojects', 'Ġapr', 'il', 'pdf', 'Ġus', 'Ġgovernment', 'Ġaccountability', 'ï', '¬', 'ģ', 'ce', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'n', 'asa', 'Ġplans', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtwo', 'Ġgateway', 'Ġelements', 'Ġrocket', 'space', 'f', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember']</t>
         </is>
       </c>
       <c r="C220" t="n">
@@ -3298,7 +3298,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>['Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'Ġwik', 'ipedia', 'Ġangels', 'Ġmission', 'Ġtype', 'Ġtechnology', 'Ġdemonstr', 'ator', 'Ġoperator', 'Ġaf', 'rl', 'Ġcos', 'par', 'Ġid', '043', 'c', 'Ġsat', 'cat', '01', 'Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'ang', 'els', 'Ġproject', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'Ġproject', 'Ġdevelop', 'Ġsmall', 'Ġsatellite', 'Ġorbit', 'Ġclose', 'Ġlarger', 'Ġspacecraft', 'Ġmonitor', 'Ġlocal', 'Ġspace', 'Ġenvironment', 'Ġangels', 'Ġdesigned', 'Ġevaluate', 'sa', 'Ġtechniques', 'Ġlimited', 'Ġregion', 'Ġaround', 'Ġdelta', 'Ġlaunch', 'Ġvehicle', 'Ġupper', 'Ġstage', 'Ġseveral', 'Ġhundred', 'Ġkilometers', 'Ġgeo', 'Ġtesting', 'Ġmaneuver', 'ing', 'Ġconcepts', 'Ġaround', 'Ġrocket', 'Ġbody', 'Ġvehicle', 'Ġbegan', 'Ġexperiments', 'Ġapproximately', 'Ġaway', 'Ġupper', 'Ġstage', 'Ġcautiously', 'Ġprogressed', 'Ġseveral', 'Ġmonths', 'Ġtests', 'Ġwithin', 'Ġseveral', 'Ġkilometers', 'Ġpart', 'Ġresearch', 'Ġeffort', 'Ġangels', 'Ġexplored', 'Ġincreased', 'Ġlevels', 'Ġautomation', 'Ġmission', 'Ġplanning', 'Ġexecution', 'Ġenable', 'Ġtimely', 'Ġsafe', 'Ġcomplex', 'Ġoperations', 'Ġreduced', 'Ġoperations', 'Ġfootprint', 'Ġangels', 'Ġlaunched', 'Ġrocket', 'Ġsecondary', 'Ġpayload', 'g', 'ss', 'ap', 'Ġmission', 'Ġdelivered', 'Ġdirectly', 'Ġgeo', 'Ġplanned', 'Ġoperating', 'Ġduration', 'Ġone', 'Ġyear', 'Ġsatellite', 'Ġmet', 'Ġvarious', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġmission', 'Ġobjectives', 'Ġeventually', 'Ġdecom', 'mission', 'ed', 'mber', 'Ġsinger', 'Ġj', 'ere', 'air', 'Ġforce', 'Ġangels', 'Ġsatellite', 'Ġesc', 'orts', 'Ġtake', 'Ġflight', 'http', 'sp', 'Ġspace', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', '07', 'fact', 'Ġsheet', 'Ġautomated', 'Ġnavigation', 'Ġguidance', 'Ġexperiment', 'Ġlocal', 'Ġspace', 'ang', 'els', ')"', 'http', 'Ġaf', 'rl', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdelta', 'iv', 'Ġmission', 'Ġoverview', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġreferences', 'Ġautonomous', 'Ġnan', 'os', 'atellite', 'Ġguardian', 'Ġevaluating', 'Ġlocal', 'Ġspace', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġk', 'bs', 'Ġgun', 'ter', 'ang', 'els', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġretrieved']</t>
+          <t>['Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġpot', 'ter', 'Ġse', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġawards', 'Ġcontract', 'Ġlaunch', 'Ġinitial', 'Ġelements', 'Ġlunar', 'Ġoutpost', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'Ġnews', 'mber', 'Ġarchived', 'eway', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'press', 'Ġrelease', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'uly', 'n', 'asa', 'Ġintroduces', 'Ġnew', 'Ġwider', 'Ġset', 'Ġeyes', 'Ġuniverse', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'web', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'uly', 'Ġobserv', 'atory', 'Ġbegin', 'Ġoperations', 'Ġtravelling', 'Ġgravitational', 'Ġbalance', 'Ġpoint', 'Ġknown', 'Ġearth', 'sun', 'sc', 'ig', 'u', 'ys', 'pace', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġlaunching', 'Ġdebut', 'Ġland', 'er', 'Ġvul', 'Ġsaid', 'Ġtoday', 'Ġpurchasing', 'Ġfal', 'con', 'Ġheavy', 'Ġthird', 'Ġland', 'er', 'Ġmission', 'Ġmoon', 'Ġmission', 'Ġlaunch', 'Ġast', 'rob', 'otic', 'Ġland', 'er', 'Ġmoon', "'s", 'Ġsouth', 'Ġpole', 'weet', 'Ġvia', 'Ġtwitter', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'n', 'asa', 'Ġplanning', 'Ġspend', 'Ġbillion', 'Ġspace', 'Ġstation', 'Ġde', 'orbit', 'Ġmodule', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġplans', 'Ġstart', 'Ġwork', 'Ġyear', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġgateway', 'Ġlogistics', 'Ġmission', 'Ġion', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġcl', 'ark', 'Ġstep', 'hen', 'n', 'asa', 'Ġpicks', 'Ġspace', 'x', 'Ġdeliver', 'Ġcargo', 'Ġgateway', 'Ġstation', 'Ġlunar', 'Ġorbit', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġsheet', 'z', 'ichael', 'Ġmarch', 'space', 'x', "'s", 'Ġpowerful', 'Ġrocket', 'Ġsend', 'Ġn', 'asa', 'Ġcargo']</t>
         </is>
       </c>
       <c r="C221" t="n">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>['Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġreplica', 'Ġsp', 'ut', 'nik', 'Ġcommunications', 'Ġsatellite', 'Ġcommunications', 'Ġsatellite', 'Ġartificial', 'Ġsatellite', 'Ġrel', 'ays', 'Ġampl', 'ifies', 'Ġradio', 'Ġtele', 'communication', 'Ġsignals', 'Ġvia', 'Ġtrans', 'p', 'onder', 'Ġcreates', 'Ġcommunication', 'Ġchannel', 'Ġsource', 'Ġtransmitter', 'Ġreceiver', 'Ġdifferent', 'Ġlocations', 'Ġearth', 'Ġcommunications', 'Ġsatellites', 'Ġused', 'Ġtelevision', 'Ġtelephone', 'Ġradio', 'Ġinternet', 'Ġmilitary', 'Ġapplications', 'Ġmany', 'Ġcommunications', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġmiles', 'Ġequ', 'ator', 'Ġsatellite', 'Ġappears', 'Ġstationary', 'Ġpoint', 'Ġtherefore', 'Ġsatellite', 'Ġdish', 'Ġantennas', 'Ġground', 'Ġstations', 'Ġaimed', 'Ġpermanently', 'Ġspot', 'Ġmove', 'Ġtrack', 'Ġsatellite', 'Ġothers', 'Ġform', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġantennas', 'Ġground', 'Ġfollow', 'Ġposition', 'Ġsatellites', 'Ġswitch', 'Ġsatellites', 'Ġfrequently', 'Ġhigh', 'Ġfrequency', 'Ġradio', 'Ġwaves', 'Ġused', 'Ġtelecommunications', 'Ġlinks', 'Ġtravel', 'Ġline', 'Ġsight', 'Ġob', 'structed', 'Ġcurve', 'Ġearth', 'Ġpurpose', 'Ġcommunications', 'Ġsatellites', 'Ġrelay', 'Ġsignal', 'Ġaround', 'Ġcurve', 'Ġearth', 'Ġallowing', 'Ġcommunication', 'Ġwidely', 'Ġseparated', 'Ġgeographical', 'Ġpoints', 'Ġcommunications', 'Ġsatellites', 'Ġuse', 'Ġwide', 'Ġrange', 'Ġradio', 'Ġmicrowave', 'Ġfrequencies', 'Ġavoid', 'Ġsignal', 'Ġinterference', 'Ġinternational', 'Ġorganizations', 'Ġregulations', 'Ġfrequency', 'Ġranges', 'bands', 'Ġcertain', 'Ġorganizations', 'Ġallowed', 'Ġuse', 'Ġallocation', 'Ġbands', 'Ġminim', 'izes', 'Ġrisk', 'Ġsignal', 'Ġinterference', 'Ġoct', 'ober', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'Ġpublished', 'Ġarticle', 'Ġtitled', 'ext', 'r', 'ater', 'restrial', 'Ġrel', 'ays', 'Ġb', 'rit', 'ish', 'Ġmagazine', 'Ġwireless', 'Ġarticle', 'Ġdescribed', 'Ġfundamentals', 'Ġbehind', 'Ġdeployment', 'Ġartificial', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġrelay', 'Ġradio', 'Ġsignals', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'Ġoften', 'Ġquoted', 'Ġinventor', 'Ġconcept', 'Ġcommunications', 'Ġsatellite', 'Ġterm', 'cl', 'ar', 'ke', 'Ġbelt', 'Ġemployed', 'Ġdescription', 'Ġfirst', 'Ġartificial', 'Ġearth', 'Ġsatellite', 'Ġsp', 'ut', 'nik', 'Ġput', 'Ġorbit', 'v', 'iet', 'Ġunion', 'Ġoct', 'ober', 'Ġdeveloped', 'ikhail', 'ikh', 'rav', 'ov', 'Ġser', 'gey', 'Ġk', 'ole', 'v', 'Ġbuilding', 'Ġwork', 'Ġk', 'stant', 'Ġsp', 'ut', 'nik', 'Ġequipped', 'Ġonboard', 'Ġradio', 'Ġtransmitter', 'Ġworked', 'Ġtwo', 'Ġfrequencies', '005', '002', 'Ġmeters', 'Ġwavelength', 'Ġsatellite', 'Ġplaced']</t>
+          <t>['Ġmoon', "'s", 'Ġorbit', 'Ġsupply', 'Ġastronauts', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'space', 'x', 'Ġwins', 'Ġn', 'asa', 'Ġcommercial', 'Ġcargo', 'Ġcontract', 'Ġlunar', 'Ġgateway', 'Ġspac', 'en', 'ews', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġj', 'une', 'ar', 'abs', 'Ġfal', 'con', 'Ġheavy', 'Ġmission', 'Ġslated', 'Ġde', 'cember', 'âĢĵ', 'jan', 'uary', 'Ġtimeframe', 'Ġe', 'frame', 'Ġspac', 'en', 'ews', 'Ġarchived', 'time', 'frame', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'herty', 'Ġca', 'lin', 'Ġj', 'une', 'first', 'Ġever', 'Ġcommercial', 'Ġlaunch', 'Ġvia', 'Ġel', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġcould', 'Ġhappen', 'Ġend', 'Ġyear', 'Ġexpress', 'co', 'uk', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġannounces', 'Ġfirst', 'Ġcommercial', 'Ġcontract', 'Ġlaunch', 'Ġred', 'Ġorbit', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġde', 'cember', 'int', 'els', 'Ġsigns', 'Ġfirst', 'Ġcommercial', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġagreement', 'Ġspace', 'x', 'http', 'sp', 'ac', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġment', 'space', 'x', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġde', 'cember', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġj', 'uly', 'ars', 'Ġbooks', 'Ġfal', 'con', 'Ġheavy', 'Ġthree', 'Ġlaunches', 'http', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġes', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'ars', 'Ġshifts', 'Ġsatellite', 'Ġspace', 'x', 'rian', 'esp', 'ace', 'http', 'sp', 'ac', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġx', 'arian', 'esp', 'ace', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġde', 'cember', 'Ġk', 'bs', 'Ġgun', 'ter', 'ars', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une']</t>
         </is>
       </c>
       <c r="C222" t="n">
@@ -3324,7 +3324,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>['Ġorbit', 'Ġsend', 'Ġdata', 'Ġone', 'Ġpoint', 'Ġearth', 'Ġanother', 'Ġradio', 'Ġtransmitter', 'Ġmeant', 'Ġstudy', 'Ġproperties', 'Ġradio', 'Ġwave', 'Ġdistribution', 'Ġthroughout', 'Ġion', 'osphere', 'Ġhistory', 'Ġorigins', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'las', 'b', 'Ġscore', 'Ġlaunch', 'Ġpad', 'Ġrocket', 'without', 'Ġbooster', 'Ġengines', 'Ġconstituted', 'Ġsatellite', 'Ġlaunch', 'Ġsp', 'ut', 'nik', 'Ġmajor', 'Ġstep', 'Ġexploration', 'Ġspace', 'Ġrocket', 'Ġdevelopment', 'Ġmarks', 'Ġbeginning', 'Ġspace', 'Ġtwo', 'Ġmajor', 'Ġclasses', 'Ġcommunications', 'Ġsatellites', 'Ġpassive', 'Ġactive', 'Ġpassive', 'Ġsatellites', 'Ġreflect', 'Ġsignal', 'Ġcoming', 'Ġsource', 'Ġtoward', 'Ġdirection', 'Ġreceiver', 'Ġpassive', 'Ġsatellites', 'Ġreflected', 'Ġsignal', 'Ġamplified', 'Ġsatellite', 'Ġsmall', 'Ġamount', 'Ġtransmitted', 'Ġenergy', 'Ġactually', 'Ġreaches', 'Ġreceiver', 'Ġsince', 'Ġsatellite', 'Ġfar', 'Ġearth', 'Ġradio', 'Ġsignal', 'Ġatten', 'uated', 'Ġdue', 'Ġfree', 'space', 'Ġpath', 'Ġloss', 'Ġsignal', 'Ġreceived', 'Ġearth', 'Ġweak', 'Ġactive', 'Ġsatellites', 'Ġhand', 'Ġamplify', 'Ġreceived', 'Ġsignal', 'Ġret', 'rans', 'mitting', 'Ġreceiver', 'Ġground', 'Ġpassive', 'Ġsatellites', 'Ġfirst', 'Ġcommunications', 'Ġsatellites', 'Ġlittle', 'Ġused', 'Ġwork', 'Ġbegun', 'Ġfield', 'Ġelectrical', 'Ġintelligence', 'Ġgathering', 'Ġunited', 'Ġstates', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġled', 'Ġproject', 'Ġnamed', 'Ġcommunication', 'Ġmoon', 'Ġrelay', 'Ġmilitary', 'Ġplanners', 'Ġlong', 'Ġshown', 'Ġconsiderable', 'Ġinterest', 'Ġsecure', 'Ġreliable', 'Ġcommunications', 'Ġlines', 'Ġtactical', 'Ġnecessity', 'Ġultimate', 'Ġgoal', 'Ġproject', 'Ġcreation', 'Ġlongest', 'Ġcommunications', 'Ġcircuit', 'Ġhuman', 'Ġhistory', 'Ġmoon', 'Ġearth', "'s", 'Ġnatural', 'Ġsatellite', 'Ġacting', 'Ġpassive', 'Ġrelay', 'Ġachieving', 'Ġfirst', 'Ġtrans', 'cean', 'ic', 'Ġcommunication', 'Ġwashing', 'ton', 'Ġhaw', 'aii', 'Ġjan', 'uary', 'Ġsystem', 'Ġpublicly', 'Ġinaug', 'urated', 'Ġput', 'Ġformal', 'Ġproduction', 'Ġjan', 'uary', 'Ġfirst', 'Ġsatellite', 'Ġpurpose', 'built', 'Ġactively', 'Ġrelay', 'Ġcommunications', 'Ġproject', 'Ġscore', 'Ġled', 'Ġadvanced', 'Ġresearch', 'Ġprojects', 'Ġagency', 'arp', 'Ġlaunched', 'Ġde', 'cember', 'Ġused', 'Ġtape', 'Ġrecorder', 'Ġcarry', 'Ġstored', 'Ġvoice', 'Ġmessage', 'Ġwell', 'Ġreceive', 'Ġstore', 'Ġret', 'rans', 'mit', 'Ġmessages', 'Ġused', 'Ġsend', 'Ġchrist', 'mas', 'Ġgreeting', 'Ġworld', 'Ġu', 'Ġpresident', 'Ġdw', 'ight', 'Ġe', 'isen', 'hower', 'Ġsatellite', 'Ġalso', 'Ġexecuted', 'Ġseveral', 'Ġreal', 'time', 'Ġtransmissions', 'Ġnon', 'charge', 'able', 'Ġbatteries', 'Ġfailed', 'Ġde', 'cember']</t>
+          <t>['Ġretrieved', 'Ġj', 'une', 'Ġdavid', 'Ġle', 'ard', 'Ġapr', 'il', 'space', 'craft', 'Ġpowered', 'green', 'Ġpropell', 'ant', 'Ġlaunch', 'htt', 'Ġspace', 'Ġarchived', 'http', 'Ġss', 'ion', 'gp', 'im', 'html', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'space', 'x', 'Ġoffers', 'Ġlarge', 'Ġrockets', 'Ġsmall', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'ds', 'ac', 'deep', 'Ġspace', 'Ġatomic', 'Ġclock', ')"', 'Ġn', 'asa', 'Ġearth', 'Ġobservation', 'Ġresources', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgr', 'uss', 'ike', 'Ġapr', 'il', 'space', 'x', 'Ġsends', 'Ġair', 'Ġforce', 'Ġoutline', 'Ġfal', 'con', 'Ġheavy', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'avis', 'Ġj', 'ason', 'Ġmay', 'lights', 'ail', 'Ġlaunch', 'Ġslips', 'Ġfall', 'Ġplanetary', 'Ġsociety', 'Ġarchived', 'web', 'arc', 'launch', 'sl', 'ip', 'html', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'space', 'Ġforce', 'Ġawards', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġphase', 'Ġlaunch', 'Ġservice', 'Ġcontracts', 'Ġu', 'la', 'Ġspace', 'x', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'green', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'Ġproject', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'deep', 'Ġspace', 'Ġatomic', 'Ġclock', 'Ġjet', 'Ġpropulsion', 'Ġlaboratory', 'Ġn', 'asa', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġblock', 'Ġrockets', 'Ġtargets', 'mber']</t>
         </is>
       </c>
       <c r="C223" t="n">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>['Ġeight', 'Ġhours', 'Ġactual', 'Ġoperation', 'Ġdirect', 'Ġsuccessor', 'Ġscore', 'Ġanother', 'Ġar', 'pa', 'led', 'Ġproject', 'Ġcalled', 'Ġcourier', 'Ġcourier', 'Ġlaunched', 'Ġoct', 'ober', 'Ġexplore', 'Ġwhether', 'Ġwould', 'Ġpossible', 'Ġestablish', 'Ġglobal', 'Ġmilitary', 'Ġcommunications', 'Ġnetwork', 'Ġusing', 'del', 'ayed', 'Ġrepe', 'ater', 'Ġsatellites', 'Ġreceive', 'Ġstore', 'Ġinformation', 'Ġcommanded', 'Ġreb', 'road', 'cast', 'Ġdays', 'Ġcommand', 'Ġsystem', 'Ġfailure', 'Ġended', 'Ġcommunications', 'Ġsatellite', 'Ġn', 'asa', "'s", 'Ġsatellite', 'Ġapplications', 'Ġprogram', 'Ġlaunched', 'Ġfirst', 'Ġartificial', 'Ġsatellite', 'Ġused', 'Ġpassive', 'Ġrelay', 'Ġcommunications', 'Ġecho', 'Ġaug', 'ust', 'Ġecho', 'Ġal', 'umin', 'ized', 'Ġballoon', 'Ġsatellite', 'Ġacting', 'Ġpassive', 'Ġreflect', 'Ġmicrowave', 'Ġsignals', 'Ġcommunication', 'Ġsignals', 'Ġbounced', 'Ġsatellite', 'Ġone', 'Ġpoint', 'Ġearth', 'Ġanother', 'Ġexperiment', 'Ġsought', 'Ġestablish', 'Ġfeasibility', 'Ġworldwide', 'Ġbroadcasts', 'Ġtelephone', 'Ġradio', 'Ġtelevision', 'Ġsignals', 'Ġearly', 'Ġactive', 'Ġpassive', 'Ġsatellite', 'Ġexperiments', 'Ġï', '¬', 'ģ', 'r', 'sts', 'Ġexperiments', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġtel', 'star', 'Ġfirst', 'Ġactive', 'Ġdirect', 'Ġrelay', 'Ġcommunications', 'Ġcommercial', 'Ġsatellite', 'Ġmarked', 'Ġfirst', 'Ġtrans', 'atlantic', 'Ġtransmission', 'Ġtelevision', 'Ġsignals', 'Ġbelonging', 'Ġpart', 'Ġmulti', 'national', 'Ġagreement', 'Ġbell', 'Ġtelephone', 'Ġlaboratories', 'Ġn', 'asa', 'Ġb', 'rit', 'ish', 'Ġgeneral', 'Ġpost', 'Ġoffice', 'Ġfrench', 'Ġnational', 'Ġp', 'tt', 'post', 'Ġoffice', 'Ġdevelop', 'Ġsatellite', 'Ġcommunications', 'Ġlaunched', 'Ġn', 'asa', 'Ġcape', 'aver', 'al', 'Ġj', 'uly', 'Ġfirst', 'Ġprivately', 'Ġsponsored', 'Ġspace', 'Ġlaunch', 'Ġanother', 'Ġpassive', 'Ġrelay', 'Ġexperiment', 'Ġprimarily', 'Ġintended', 'Ġmilitary', 'Ġcommunications', 'Ġpurposes', 'Ġproject', 'Ġwest', 'Ġled', 'Ġmass', 'achusetts', 'Ġinstitute', 'Ġtechnology', "'s", 'Ġl', 'incoln', 'Ġlaboratory', 'Ġinitial', 'Ġfailure', 'Ġlaunch', 'Ġmay', 'Ġdispersed', 'Ġmillion', 'Ġcopper', 'Ġneedle', 'Ġdip', 'oles', 'Ġcreate', 'Ġpassive', 'Ġreflecting', 'Ġbelt', 'Ġeven', 'Ġthough', 'Ġhalf', 'Ġdip', 'oles', 'Ġproperly', 'Ġseparated', 'Ġproject', 'Ġable', 'Ġsuccessfully', 'Ġexperiment', 'Ġcommunicate', 'Ġusing', 'Ġfrequencies', 'Ġband', 'Ġspectrum', 'Ġimmediate', 'Ġante', 'ced', 'ent', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġhug', 'hes', 'Ġaircraft', 'Ġcompany', "'s", 'Ġsyn', 'Ġlaunched', 'Ġj', 'uly', 'Ġsyn', 'Ġfirst', 'Ġcommunications', 'Ġsatellite', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġrev', 'olved', 'Ġaround', 'Ġearth', 'Ġper', 'Ġday', 'Ġconstant', 'Ġspeed', 'Ġstill', 'Ġnorth', 'âĢĵ', 'Ġsouth']</t>
+          <t>['Ġlaunch', 'Ġdebut', 'es', 'lar', 'ati', 'Ġretrieved', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġsurprise', 'Ġfal', 'con', 'Ġheavy', 'Ġbooster', 'Ġlanding', 'Ġsmash', 'Ġdistance', 'Ġrecord', 'Ġj', 'une', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġwall', 'ike', 'Ġj', 'uly', 'red', 'Ġdragon', 'Ġmission', 'Ġmull', 'ed', 'Ġcheap', 'Ġsearch', 'Ġmars', 'Ġlife', 'Ġspace', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġmay', 'fal', 'con', 'Ġheavy', 'Ġen', 'ab', 'ler', 'Ġdragon', 'Ġsolar', 'Ġsystem', 'Ġexplorer', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'el', 'Ġmus', 'k', 'Ġsuggests', 'Ġspace', 'x', 'Ġscra', 'pping', 'Ġplans', 'Ġland', 'Ġdragon', 'Ġcapsules', 'Ġmars', 'Ġverge', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'w', 'Ġj', 'uly', 'Ġcl', 'ark', 'Ġstep', 'hen', 'n', 'asa', 'Ġchooses', 'Ġmax', 'ar', 'Ġbuild', 'Ġkey', 'stone', 'Ġmodule', 'Ġlunar', 'Ġgateway', 'Ġstation', 'http', 'Ġway', 'station', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'ion', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġplans', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtwo', 'Ġgateway', 'Ġelements', 'Ġrocket', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ass', 'ess', 'ments', 'Ġmajor', 'Ġprojects', 'Ġg', 'ao', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'psy', 'che', 'Ġspacecraft', 'Ġseparates', 'Ġfal', 'con', 'Ġheavy', 'Ġsecond', 'Ġstage', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsh', 'ie', 'ber', 'Ġj', 'athan', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġwins']</t>
         </is>
       </c>
       <c r="C224" t="n">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>['Ġmotion', 'Ġspecial', 'Ġequipment', 'Ġneeded', 'Ġtrack', 'Ġsuccessor', 'Ġsyn', 'Ġlaunched', 'Ġj', 'uly', 'Ġfirst', 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġsatellite', 'Ġsyn', 'Ġobtained', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġwithout', 'Ġnorth', 'âĢĵ', 'south', 'Ġmotion', 'Ġmaking', 'Ġappear', 'Ġground', 'Ġstationary', 'Ġobject', 'Ġdirect', 'Ġextension', 'Ġpassive', 'Ġexperiments', 'Ġproject', 'Ġwest', 'Ġl', 'incoln', 'Ġexperimental', 'Ġsatellite', 'Ġprogram', 'Ġalso', 'Ġconducted', 'Ġl', 'incoln', 'Ġlaboratory', 'Ġbehalf', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġles', 'Ġactive', 'Ġcommunications', 'Ġsatellite', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġexplore', 'Ġfeasibility', 'Ġactive', 'Ġsolid', 'state', 'Ġband', 'Ġlong', 'range', 'Ġmilitary', 'Ġcommunications', 'Ġtotal', 'Ġnine', 'Ġsatellites', 'Ġlaunched', 'Ġpart', 'Ġseries', 'Ġunited', 'Ġstates', 'Ġsaw', 'Ġcreation', 'Ġcommunications', 'Ġsatellite', 'Ġcorporation', 'sat', 'Ġprivate', 'Ġcorporation', 'Ġsubject', 'Ġinstruction', 'Ġus', 'Ġgovernment', 'Ġmatters', 'Ġnational', 'Ġpolicy', 'Ġnext', 'Ġtwo', 'Ġyears', 'Ġinternational', 'Ġnegotiations', 'Ġled', 'Ġint', 'els', 'Ġagreements', 'Ġturn', 'Ġled', 'Ġlaunch', 'Ġint', 'els', 'Ġalso', 'Ġknown', 'Ġearly', 'Ġbird', 'Ġapr', 'il', 'Ġfirst', 'Ġcommercial', 'Ġcommunications', 'Ġsatellite', 'Ġplaced', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġsubsequent', 'Ġint', 'els', 'Ġlaunches', 'Ġprovided', 'Ġmulti', 'dest', 'ination', 'Ġservice', 'Ġvideo', 'Ġaudio', 'Ġdata', 'Ġservice', 'Ġships', 'Ġsea', 'int', 'els', 'âĢĵ', 'Ġcompletion', 'Ġfully', 'Ġglobal', 'Ġnetwork', 'Ġint', 'els', 'âĢĵ', 'Ġsignificant', 'Ġexpansions', 'Ġcommercial', 'Ġsatellite', 'Ġcapacity', 'Ġint', 'els', 'Ġway', 'Ġbecome', 'Ġpart', 'Ġcompetitive', 'Ġprivate', 'Ġtelecommunications', 'Ġindustry', 'Ġstarted', 'Ġget', 'Ġcompetition', 'Ġlikes', 'Ġpan', 'ams', 'Ġunited', 'Ġstates', 'Ġironically', 'Ġbought', 'Ġarch', 'rival', 'Ġint', 'els', 'Ġlaunched', 'Ġunited', 'Ġstates', 'Ġlaunch', 'Ġsource', 'Ġoutside', 'v', 'iet', 'Ġunion', 'Ġparticipate', 'Ġint', 'els', 'Ġagreements', 'v', 'iet', 'Ġunion', 'Ġlaunched', 'Ġfirst', 'Ġcommunications', 'Ġsatellite', 'Ġapr', 'il', 'Ġpart', 'Ġprogram', 'Ġprogram', 'Ġalso', 'Ġunique', 'Ġtime', 'Ġuse', 'Ġbecame', 'Ġknown', 'Ġorbit', 'Ġdescribes', 'Ġinternational', 'Ġcommercial', 'Ġsatellite', 'Ġprojects']</t>
+          <t>['Ġmillion', 'Ġlaunch', 'Ġcontract', 'Ġexplore', 'Ġpsyche', "'s", 'Ġheavy', 'Ġmetal', 'Ġasteroid', 'Ġtech', 'cr', 'unch', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmoon', 'Ġmar', 'ie', 'lla', 'Ġfe', 'b', 'ruary', 'n', 'asa', "'s", 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġuse', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġeng', 'ad', 'get', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġpot', 'ter', 'Ġse', 'Ġj', 'uly', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġmission', 'Ġion', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'ï', '¬', 'ģ', 'cial', 'Ġpage', 'Ġfal', 'con', 'Ġheavy', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġanimation', 'Ġfe', 'b', 'ruary', 'Ġel', 'Ġmus', 'k', 'Ġfal', 'con', 'Ġheavy', 'Ġchange', 'Ġspace', 'Ġtravel', 'Ġverge', 'Ġyoutube', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C225" t="n">
@@ -3363,7 +3363,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>['Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġorbit', 'Ġsize', 'Ġcomparison', 'Ġgl', 'ass', 'Ġgal', 'ile', 'id', 'ou', 'Ġir', 'idium', 'Ġconst', 'ell', 'ations', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġgraveyard', 'Ġorbit', 'Ġvan', 'en', 'Ġradiation', 'Ġbelts', 'Ġearth', 'Ġscale', 'Ġmoon', "'s", 'Ġorbit', 'Ġaround', 'Ġtimes', 'Ġlarge', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'b', 'Ġï', '¬', 'ģ', 'le', 'Ġhover', 'Ġorbit', 'Ġlabel', 'Ġhighlight', 'Ġclick', 'Ġload', 'Ġarticle', '.)', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'Ġtwo', 'Ġhigh', 'Ġap', 'ge', 'es', 'Ġdaily', 'Ġnorthern', 'Ġhemisphere', 'Ġorbit', 'Ġprovides', 'Ġlong', 'Ġdwell', 'Ġtime', 'Ġr', 'ussian', 'Ġterritory', 'Ġwell', 'ada', 'Ġhigher', 'Ġlat', 'itudes', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġequ', 'ator', 'Ġcommunications', 'Ġsatellites', 'Ġusually', 'Ġone', 'Ġthree', 'Ġprimary', 'Ġtypes', 'Ġorbit', 'Ġorbital', 'Ġclass', 'ifications', 'Ġused', 'Ġspecify', 'Ġorbital', 'Ġdetails', 'Ġle', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'ng', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'ge', 'Ġmiles', 'Ġearth', "'s", 'Ġsurface', 'Ġorbit', 'Ġspecial', 'Ġcharacteristic', 'Ġapparent', 'Ġposition', 'Ġsatellite', 'Ġviewed', 'Ġground', 'Ġobserver', 'Ġchange', 'Ġsatellite', 'Ġappears', 'stand', 'Ġstill', 'Ġsatellite', "'s", 'Ġorbital', 'Ġperiod', 'Ġrotation', 'Ġrate', 'Ġearth', 'Ġadvantage', 'Ġorbit', 'Ġground', 'Ġantennas', 'Ġtrack', 'Ġsatellite', 'Ġacross', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġpoint', 'Ġlocation', 'Ġsatellite', 'Ġappears', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellites', 'Ġcloser', 'Ġearth', 'Ġorbital', 'Ġalt', 'itudes', 'Ġrange', '000', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', 'Ġregion', 'Ġmedium', 'Ġorbits', 'Ġreferred', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', 'Ġsatellites', 'Ġle', 'Ġorbit', 'Ġearth', 'Ġfaster', 'Ġremain', 'Ġvisible', 'Ġfixed', 'Ġpoint', 'Ġearth', 'Ġcontinually', 'Ġlike', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġappear', 'Ġground', 'Ġobserver', 'Ġcross', 'set']</t>
+          <t>['Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġf', 'en', 'gy', 'un', 'Ġâ', '»', 'Ľ', 'äº', 'ĳ', 'åį', '«', 'æĺ', 'Ł', 'Ġmodel', 'Ġsh', 'ghai', 'Ġmuseum', 'Ġprogram', 'Ġoverview', 'Ġcountry', 'Ġpeople', "'s", 'Ġrepublic', 'Ġch', 'ina', 'Ġpurpose', 'Ġmeteor', 'ology', 'Ġstatus', 'Ġactive', 'Ġprogram', 'Ġhistory', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġse', 'pt', 'ember', 'Ġvehicle', 'Ġinformation', 'Ġlaunch', 'Ġvehicle', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġf', 'en', 'gy', 'un', 'Ġsimplified', 'Ġch', 'inese', 'Ġé', '£', 'İ', 'äº', 'ĳ', 'Ġtraditional', 'Ġch', 'inese', 'Ġé', '¢', '¨', 'éĽ', '²', 'Ġlit', 'wind', 'Ġcloud', "')", 'Ġch', 'ina', "'s", 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'Ġpolar', 'Ġsun', 'syn', 'chron', 'ous', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġthree', 'axis', 'Ġstabilized', 'Ġf', 'en', 'gy', 'un', 'Ġsatellite', 'Ġbuilt', 'Ġsh', 'ghai', 'Ġacademy', 'Ġspace', 'flight', 'Ġtechnology', 'ast', 'Ġoperated', 'Ġch', 'ina', 'Ġmeteor', 'ological', 'Ġadministration', 'Ġdate', 'Ġch', 'ina', 'Ġlaunched', 'Ġtwenty', 'one', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġfour', 'Ġclasses', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġpolar', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġf', 'en', 'gy', 'un', 'Ġge', 'os', 'ynchronous', 'Ġjan', 'uary', 'Ġch', 'ina', 'Ġdestroyed', 'Ġone', 'Ġsatellites', 'Ġcos', 'par', '025', 'Ġtest', 'Ġantis', 'atellite', 'Ġmissile', 'Ġaccording', 'Ġn', 'asa', 'Ġintentional', 'Ġdestruction', 'Ġcreated', '000', 'Ġhigh', 'vel', 'ocity', 'Ġdebris', 'Ġitems', 'Ġlarger', 'Ġamount', 'Ġdangerous', 'Ġspace', 'Ġjunk', 'Ġspace', 'Ġmission', 'Ġhistory', 'Ġfour', 'Ġsatellites', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġch', 'ina', "'s", 'Ġfirst', 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġplaced', 'Ġpolar', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġsatellites', 'Ġorb', 'ited', 'Ġearth', 'Ġlow', 'Ġaltitude', 'app', 'rox', 'imate', 'Ġearth', "'s", 'Ġsurface', 'Ġhigh', 'Ġinclination', 'Â°', 'Â°', 'Ġtravers', 'ing', 'Ġnorth', 'Ġpole', 'Ġevery', 'Ġminutes', 'Ġgiving', 'Ġf', 'class', 'Ġsatellites', 'Ġglobal', 'Ġmeteor', 'ological', 'Ġcoverage', 'Ġrapid', 'Ġrevisit', 'Ġtime', 'Ġcloser', 'Ġproximity', 'Ġclouds', 'Ġimage', 'Ġlaunched', 'Ġse', 'pt', 'ember', 'Ġlasted', 'Ġdays', 'Ġsuffered', 'Ġattitude', 'Ġcontrol', 'Ġproblems', 'Ġlaunched', 'Ġse', 'pt', 'ember', 'Ġalong', 'Ġfirst', 'Ġtwo', 'Ġqui', 'ix', 'ing', 'Ġballoon', 'Ġsatellites', 'Ġlasted', 'Ġlate', 'Ġattitude', 'Ġcontrol', 'Ġsystem', 'Ġalso', 'Ġfailed', 'Ġlaunched']</t>
         </is>
       </c>
       <c r="C226" t="n">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>['Ġgo', 'Ġbehind', 'Ġearth', 'Ġbeyond', 'Ġvisible', 'Ġhorizon', 'Ġtherefore', 'Ġprovide', 'Ġcontinuous', 'Ġcommunications', 'Ġcapability', 'Ġlower', 'Ġorbits', 'Ġrequires', 'Ġlarger', 'Ġnumber', 'Ġsatellites', 'Ġone', 'Ġsatellites', 'Ġalways', 'Ġvisible', 'Ġtransmission', 'Ġcommunication', 'Ġsignals', 'Ġhowever', 'Ġdue', 'Ġcloser', 'Ġdistance', 'Ġearth', 'Ġle', 'Ġsatellites', 'Ġcommunicate', 'Ġground', 'Ġreduced', 'Ġlatency', 'Ġlower', 'Ġpower', 'Ġwould', 'Ġrequired', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġtypically', 'Ġcircular', 'Ġorbit', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', "'s", 'Ġsurface', 'Ġcorrespond', 'ingly', 'Ġperiod', 'time', 'Ġrev', 'olve', 'Ġaround', 'Ġearth', 'Ġminutes', 'Ġlow', 'Ġaltitude', 'Ġsatellites', 'Ġvisible', 'Ġwithin', 'Ġradius', 'Ġroughly', '000', 'Ġkilometres', 'Ġmi', 'Ġsub', 'atellite', 'Ġpoint', 'Ġaddition', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġchange', 'Ġposition', 'Ġrelative', 'Ġground', 'Ġposition', 'Ġquickly', 'Ġeven', 'Ġlocal', 'Ġapplications', 'Ġmany', 'Ġsatellites', 'Ġneeded', 'Ġmission', 'Ġrequires', 'Ġuninterrupted', 'Ġconnectivity', 'Ġsatellite', 'Ġorbits', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġlow', 'earth', 'orb', 'iting', 'Ġsatellites', 'Ġless', 'Ġexpensive', 'Ġlaunch', 'Ġorbit', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġdue', 'Ġproximity', 'Ġground', 'Ġrequire', 'Ġhigh', 'Ġsignal', 'Ġstrength', 'sign', 'al', 'Ġstrength', 'Ġfalls', 'Ġsquare', 'Ġdistance', 'Ġsource', 'Ġeffect', 'Ġconsiderable', 'Ġthus', 'Ġtrade', 'Ġnumber', 'Ġsatellites', 'Ġcost', 'Ġaddition', 'Ġimportant', 'Ġdifferences', 'Ġonboard', 'Ġground', 'Ġequipment', 'Ġneeded', 'Ġsupport', 'Ġtwo', 'Ġtypes', 'Ġmissions', 'Ġgroup', 'Ġsatellites', 'Ġworking', 'Ġconcert', 'Ġknown', 'Ġsatellite', 'Ġconstellation', 'Ġtwo', 'Ġconst', 'ell', 'ations', 'Ġintended', 'Ġprovide', 'Ġsatellite', 'Ġphone', 'Ġlow', 'speed', 'Ġdata', 'Ġservices', 'Ġprimarily', 'Ġremote', 'Ġareas', 'Ġir', 'idium', 'Ġglobal', 'star', 'Ġsystems', 'Ġir', 'idium', 'Ġsystem', 'Ġsatellites', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġinter', 'atellite', 'Ġlinks', 'Ġprovide', 'Ġservice', 'Ġavailability', 'Ġentire', 'Ġsurface', 'Ġearth', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'Ġoperated', 'Ġspace', 'x', 'Ġaims', 'Ġglobal', 'Ġsatellite', 'Ġinternet', 'Ġaccess', 'Ġcoverage', 'Ġalso', 'Ġpossible', 'Ġoffer', 'Ġdiscontin', 'uous', 'Ġcoverage', 'Ġusing', 'Ġlow', 'earth', 'orbit', 'Ġsatellite', 'Ġcapable', 'Ġstoring', 'Ġdata', 'Ġreceived', 'Ġpassing', 'Ġone', 'Ġpart']</t>
+          <t>['Ġmay', 'Ġalong', 'Ġalso', 'Ġcompleted', 'Ġtwo', 'year', 'Ġdesign', 'Ġlife', 'Ġoperating', 'Ġjan', 'uary', 'Ġlast', 'Ġsatellite', 'Ġclass', 'Ġlaunched', 'Ġmay', 'Ġoperated', 'Ġcontinuously', 'Ġnine', 'Ġyears', 'Ġmay', 'Ġoperations', 'Ġtemporarily', 'Ġlost', 'Ġdespite', 'Ġresusc', 'itation', 'Ġfailed', 'Ġapr', 'il', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġlaunched', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'Ġsh', 'xi', 'Ġprovince', 'Ġlong', 'Ġmarch', 'Ġrockets', 'Ġweighed', 'Ġrespectively', 'Ġaboard', 'Ġsatellite', 'Ġtwo', 'Ġmult', 'ich', 'annel', 'Ġvisible', 'Ġinfrared', 'Ġscanning', 'Ġradi', 'ometers', 'vis', 'r', 'Ġbuilt', 'Ġsh', 'ghai', 'Ġinstitute', 'Ġtechnical', 'Ġphysics', 'sit', 'p', 'Ġbearing', 'Ġoptical', 'Ġscanner', 'Ġimage', 'Ġprocessor', 'Ġradiant', 'Ġcooler', 'Ġcontroller', 'Ġradiant', 'Ġcooler', 'Ġsatellites', 'Ġalso', 'Ġcarried', 'Ġboard', 'Ġhigh', 'energy', 'Ġparticle', 'Ġdetector', 'pd', 'Ġstudy', 'Ġspace', 'Ġenvironment', 'Ġcontributing', 'Ġincreased', 'Ġmass', 'Ġsatellites', 'Ġpowered', 'Ġtwo', 'Ġdeploy', 'able', 'Ġsolar', 'Ġarrays', 'Ġinternal', 'Ġbatteries', 'Ġjan', 'uary', 'Ġch', 'ina', 'Ġconducted', 'Ġfirst', 'Ġanti', 'atellite', 'Ġmissile', 'Ġtest', 'Ġdestroying', 'Ġkinetic', 'Ġkill', 'Ġvehicle', 'Ġidentified', 'Ġunited', 'Ġstates', 'Ġdefense', 'Ġintelligence', 'Ġagency', 'ia', 'Ġsc', 'Ġmodified', 'Ġballistic', 'Ġmissile', 'Ġmounted', 'Ġkill', 'Ġvehicle', 'Ġshoot', 'Ġsubsequent', 'Ġcreation', 'Ġrecord', 'setting', 'Ġamount', 'orbit', 'Ġdebris', 'Ġdrew', 'Ġserious', 'Ġinternational', 'Ġsatellites', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġbased', 'Ġspin', 'st', 'abil', 'ized', 'ong', 'Ġf', 'ang', 'Ġh', 'ong', 'Ġplatform', 'Ġch', 'ina', "'s", 'Ġfirst', 'Ġclass', 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġunlike', 'Ġmeteor', 'ological', 'Ġsatellites', 'Ġpolar', 'Ġorbit', 'like', 'Ġclasses', 'Ġsatellites', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġremain', 'Ġfixed', 'Ġposition', 'Ġrelative', 'Ġearth', '000', 'Ġsurface', 'Ġmaintain', 'Ġconstant', 'Ġwatch', 'Ġassigned', 'Ġarea', 'Ġunlike', 'Ġpolar', 'Ġorbiting', 'Ġsatellites', 'Ġview', 'Ġarea', 'Ġtwice', 'Ġday', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġimage', 'Ġlocation', 'Ġfast', 'Ġminute', 'Ġshow', 'Ġlong', 'Ġterm', 'Ġmeteor', 'ological', 'Ġtrends', 'Ġcost', 'Ġresolution', 'Ġbuilt', 'Ġsh', 'ghai', 'Ġinstitute', 'Ġsatellite', 'Ġengineering', 'Ġoperated', 'Ġch', 'inese', 'Ġmeteor', 'ological', 'Ġadministration', 'Ġsatellites', 'Ġtall', 'Ġspin', 'st', 'abil', 'ized', 'Ġrotating', 'Ġrot', 'ations']</t>
         </is>
       </c>
       <c r="C227" t="n">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>['Ġearth', 'Ġtransmitting', 'Ġlater', 'Ġpassing', 'Ġanother', 'Ġpart', 'Ġcase', 'Ġcascade', 'Ġsystem', 'ada', "'s", 'Ġcass', 'ope', 'Ġcommunications', 'Ġsatellite', 'Ġanother', 'Ġsystem', 'Ġusing', 'Ġstore', 'Ġforward', 'Ġmethod', 'Ġorb', 'comm', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġorbit', 'Ġsomewhere', '000', 'Ġkilometres', 'Ġmi', 'Ġearth', "'s", 'Ġsurface', 'Ġsatellites', 'Ġsimilar', 'Ġle', 'Ġsatellites', 'Ġfunctionality', 'Ġsatellites', 'Ġvisible', 'Ġmuch', 'Ġlonger', 'Ġperiods', 'Ġtime', 'Ġle', 'Ġsatellites', 'Ġusually', 'Ġhours', 'Ġsatellites', 'Ġlarger', 'Ġcoverage', 'Ġarea', 'Ġle', 'Ġsatellites', 'Ġsatellite', "'s", 'Ġlonger', 'Ġduration', 'Ġvisibility', 'Ġwider', 'Ġfootprint', 'Ġmeans', 'Ġfewer', 'Ġsatellites', 'Ġneeded', 'Ġnetwork', 'Ġle', 'Ġnetwork', 'Ġone', 'Ġdisadvantage', 'Ġsatellite', "'s", 'Ġdistance', 'Ġgives', 'Ġlonger', 'Ġtime', 'Ġdelay', 'Ġweaker', 'Ġsignal', 'Ġle', 'Ġsatellite', 'Ġalthough', 'Ġlimitations', 'Ġsevere', 'Ġgeo', 'Ġsatellite', 'Ġlike', 'Ġle', 'os', 'Ġsatellites', 'Ġmaintain', 'Ġstationary', 'Ġdistance', 'Ġearth', 'Ġcontrast', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġsatellites', 'Ġalways', 'Ġkilometres', 'Ġmi', 'Ġearth', 'Ġtypically', 'Ġorbit', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellite', '000', 'Ġkilometres', '000', 'Ġmi', 'Ġearth', 'Ġvarious', 'Ġpatterns', 'Ġsatellites', 'Ġmake', 'Ġtrip', 'Ġaround', 'Ġearth', 'Ġanywhere', 'Ġhours', 'Ġcommunications', 'Ġsatellite', 'Ġtel', 'star', 'Ġlaunched', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġdesigned', 'Ġhelp', 'Ġfacilitate', 'Ġhigh', 'speed', 'Ġtelephone', 'Ġsignals', 'Ġalthough', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġpractical', 'Ġway', 'Ġtransmit', 'Ġsignals', 'Ġhorizon', 'Ġmajor', 'Ġdrawback', 'Ġsoon', 'Ġrealised', 'Ġorbital', 'Ġperiod', 'Ġhours', 'Ġmatch', 'Ġearth', "'s", 'Ġrot', 'ational', 'Ġperiod', 'Ġhours', 'Ġcontinuous', 'Ġcoverage', 'Ġimpossible', 'Ġapparent', 'Ġmultiple', 'os', 'Ġneeded', 'Ġused', 'Ġorder', 'Ġprovide', 'Ġcontinuous', 'Ġcoverage', 'Ġsatellite', 'Ġconstellation', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġexamples', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfour', 'Ġconstellation', 'Ġsatellites', 'Ġlaunched', 'Ġsatellites', 'Ġprovide', 'Ġbroadband', 'Ġinternet', 'Ġservices', 'Ġparticular', 'Ġremote', 'Ġlocations', 'Ġmaritime', 'ï', '¬', 'Ĥ', 'ight', 'Ġuse', 'Ġorbit', 'Ġaltitude']</t>
+          <t>['Ġper', 'Ġminute', 'Ġf', 'class', 'Ġsatellites', 'Ġmarketed', 'Ġopenly', 'Ġavailable', 'Ġdata', 'Ġwhereby', 'Ġuser', 'Ġreceiver', 'Ġcould', 'Ġview', 'Ġderived', 'Ġsensory', 'Ġdata', 'Ġsatellites', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġmass', 'Ġkilograms', 'Ġuse', 'Ġsolar', 'Ġcells', 'Ġbatteries', 'Ġpower', 'Ġap', 'gee', 'Ġmotor', 'Ġj', 'ett', 'ison', 'ed', 'Ġatt', 'aining', 'Ġorbit', 'Ġapr', 'il', 'Ġch', 'ina', 'Ġattempted', 'Ġlaunch', 'Ġf', 'en', 'gy', 'un', 'Ġx', 'ich', 'ang', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'Ġprior', 'Ġmating', 'Ġlong', 'Ġmarch', 'Ġfire', 'Ġcaused', 'Ġexplosion', 'Ġdestroying', 'Ġsatellite', 'Ġkilling', 'Ġtechnician', 'Ġinjuring', 'Ġothers', 'Ġofficials', 'Ġch', 'inese', 'Ġspace', 'Ġagency', 'Ġdescribed', 'Ġmillion', 'Ġus', 'Ġloss', 'Ġsatellite', 'major', 'Ġsetback', 'Ġch', 'inese', 'Ġspace', 'Ġprogram', 'Ġdespite', 'Ġch', 'ina', 'Ġlaunched', 'Ġeight', 'Ġsuccessive', 'Ġf', 'en', 'gy', 'un', 'Ġsatellites', 'Ġwithout', 'Ġincident', 'Ġclasses', 'Ġf', 'en', 'gy', 'un', 'Ġdestruction', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġmodel', 'Ġsh', 'ghai', 'Ġmuseum', 'Ġmock', 'Ġsatellite', 'Ġch', 'inese', 'Ġparticipation', 'Ġmonitoring', 'Ġaur', 'oras', 'Ġscientific', 'Ġspace', 'Ġweather', 'Ġinvestigation', 'Ġinitiated', 'Ġlaunch', 'Ġsatellite', 'Ġcarries', 'Ġwide', 'field', 'Ġaur', 'oral', 'Ġim', 'ager', 'Ġf', 'en', 'gy', 'un', 'Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġch', 'ina', 'Ġlaunched', 'Ġtwo', 'Ġf', 'en', 'gy', 'un', 'Ġclass', 'Ġsatellites', 'Ġsatellite', 'Ġlaunch', 'Ġorbit', 'Ġorbital', 'ps', 'Ġinclination', 'Ġperiod', 'min', 'Ġcos', 'par', 'Ġlaun', 'c', 'Ġsite', 'Ġf', 'eny', 'un', 'Ġse', 'pt', 'ember', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '080', 'Ġf', 'en', 'gy', 'un', 'Ġse', 'pt', 'ember', 'Ġsun', 'syn', 'chron', 'ous', '02', 'Â°', '08', 'Ġf', 'en', 'gy', 'un', '01', 'Ġapr', 'il', 'Ġexploded', 'Ġlaunch', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '029', 'Ġf', 'en', 'gy', 'un', 'Ġmay', 'Ġsun', 'syn', 'chron', 'ous', 'Â°']</t>
         </is>
       </c>
       <c r="C228" t="n">
@@ -3402,7 +3402,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>['06', 'Ġkilometres', '010', 'Ġobserver', 'Ġearth', 'Ġsatellite', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġappears', 'Ġmotion', 'less', 'Ġfixed', 'Ġposition', 'Ġrevolves', 'Ġaround', 'Ġearth', 'Ġearth', "'s", 'Ġangular', 'Ġvelocity', 'one', 'Ġrevolution', 'Ġper', 'Ġside', 'real', 'Ġday', 'Ġequ', 'atorial', 'Ġorbit', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġuseful', 'Ġcommunications', 'Ġground', 'Ġantennas', 'Ġaimed', 'Ġsatellite', 'Ġwithout', 'Ġtrack', 'Ġsatellite', "'s", 'Ġmotion', 'Ġrelatively', 'Ġinexpensive', 'Ġapplications', 'Ġrequire', 'Ġmany', 'Ġground', 'Ġantennas', 'Ġdirect', 'v', 'Ġdistribution', 'Ġsavings', 'Ġground', 'Ġequipment', 'Ġoutweigh', 'Ġcost', 'Ġcomplexity', 'Ġplacing', 'Ġsatellite', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġsyn', 'Ġlaunched', 'Ġaug', 'ust', 'Ġused', 'Ġcommunication', 'Ġacross', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġstarting', 'Ġtelevision', 'Ġcoverage', 'Ġsummer', 'lymp', 'ics', 'Ġshortly', 'Ġsyn', 'Ġint', 'els', 'Ġaka', 'Ġearly', 'Ġbird', 'Ġlaunched', 'Ġapr', 'il', 'Ġplaced', 'Ġorbit', 'Â°', 'Ġwest', 'Ġlong', 'itude', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġtelecommunications', 'l', 'antic', 'Ġocean', 'mber', 'ada', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġserving', 'Ġcontinent', 'ik', 'Ġlaunched', 'Ġtel', 'es', 'ada', 'Ġunited', 'Ġstates', 'Ġfollowing', 'Ġsuit', 'Ġlaunch', 'Ġwest', 'ar', 'Ġwestern', 'Ġunion', 'Ġapr', 'il', 'Ġmay', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġsatellite', 'Ġworld', 'Ġthree', 'axis', 'Ġstabilized', 'Ġlaunched', 'Ġexperimental', 'Ġsatellite', 'Ġbuilt', 'Ġn', 'asa', 'Ġlaunches', 'Ġtel', 'star', 'Ġwest', 'ar', 'Ġsatellites', 'Ġr', 'ca', 'Ġameric', 'om', 'later', 'Ġge', 'Ġameric', 'om', 'es', 'Ġlaunched', 'Ġsat', 'Ġsat', 'Ġinstrumental', 'Ġhelping', 'Ġearly', 'Ġcable', 'Ġchannels', 'Ġfree', 'form', 'Ġweather', 'Ġchannel', 'Ġbecome', 'Ġsuccessful', 'Ġchannels', 'Ġdistributed', 'Ġprogramming', 'Ġlocal', 'Ġcable', 'Ġhead', 'ends', 'Ġusing', 'Ġsatellite', 'Ġadditionally', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsatellite', 'Ġused', 'Ġbroadcast', 'Ġtelevision', 'Ġnetworks', 'Ġunited', 'Ġstates', 'Ġlike', 'Ġdistribute', 'Ġprogramming', 'Ġlocal', 'Ġaf', 'ï', '¬', 'ģ', 'li', 'ate', 'Ġstations', 'Ġsat', 'Ġwidely', 'Ġused', 'Ġtwice', 'Ġcommunications', 'Ġcapacity', 'Ġcompeting', 'Ġwest', 'ar', 'Ġameric']</t>
+          <t>['025', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '032', 'Ġf', 'en', 'gy', 'un', 'Ġmay', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '024', 'b', 'Ġf', 'en', 'gy', 'un', 'Ġoct', 'ober', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '04', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '05', 'Ġf', 'en', 'gy', 'un', 'Ġmay', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '026', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', 'Ġf', 'en', 'gy', 'un', 'mber', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '059', 'Ġf', 'en', 'gy', 'un', 'Ġjan', 'uary', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '002', 'Ġf', 'en', 'gy', 'un', 'Ġse', 'pt', 'ember', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '052', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '090', 'Ġf', 'en', 'gy', 'un', 'Ġde', 'cember', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '07', 'Ġf', 'en', 'gy', 'un', 'mber', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '010', '07', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary']</t>
         </is>
       </c>
       <c r="C229" t="n">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>['Ġtrans', 'p', 'ond', 'ers', 'Ġopposed', 'Ġwest', 'ar', 'Ġresulting', 'Ġlower', 'Ġtrans', 'p', 'onder', 'usage', 'Ġcosts', 'Ġsatellites', 'Ġlater', 'Ġdecades', 'Ġtended', 'Ġeven', 'Ġhigher', 'Ġtrans', 'p', 'onder', 'Ġnumbers', 'Ġhug', 'hes', 'Ġspace', 'Ġcommunications', 'Ġbo', 'e', 'ing', 'Ġsatellite', 'Ġdevelopment', 'Ġcenter', 'Ġbuilt', 'Ġnearly', 'Ġpercent', 'Ġone', 'Ġhundred', 'Ġsatellites', 'Ġservice', 'Ġworldwide', 'Ġmajor', 'Ġsatellite', 'Ġmanufacturers', 'Ġinclude', 'Ġspace', 'Ġsystems', 'lor', 'al', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'Ġstar', 'Ġbus', 'Ġseries', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'ge', 'Ġexamples', 'Ġgeo', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġind', 'ian', 'Ġspace', 'Ġresearch', 'Ġorganisation', 'Ġlock', 'heed', 'Ġmart', 'Ġformer', 'Ġr', 'ca', 'Ġast', 'ro', 'Ġelectronics', 'ge', 'Ġast', 'ro', 'Ġspace', 'Ġbusiness', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġal', 'c', 'atel', 'Ġspace', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġspace', 'bus', 'Ġseries', 'Ġast', 'rium', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġmust', 'Ġoperate', 'Ġequ', 'ator', 'Ġtherefore', 'Ġappear', 'Ġlower', 'Ġhorizon', 'Ġreceiver', 'Ġgets', 'Ġfarther', 'Ġequ', 'ator', 'Ġcause', 'Ġproblems', 'Ġextreme', 'Ġnort', 'ly', 'Ġlat', 'itudes', 'Ġaffecting', 'Ġconnectivity', 'Ġcausing', 'Ġmultip', 'ath', 'Ġinterference', 'ca', 'used', 'Ġsignals', 'Ġreflecting', 'Ġground', 'Ġground', 'Ġantenna', 'Ġthus', 'Ġareas', 'Ġclose', 'Ġnorth', 'Ġsouth', 'Ġpole', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġmay', 'Ġappear', 'Ġhorizon', 'Ġtherefore', 'Ġorbit', 'Ġsatellites', 'Ġlaunched', 'Ġmainly', 'Ġr', 'ussia', 'Ġalleviate', 'Ġproblem', 'Ġorbits', 'Ġappealing', 'Ġalternative', 'Ġcases', 'Ġorbit', 'Ġhighly', 'Ġinclined', 'Ġguaranteeing', 'Ġgood', 'Ġelevation', 'Ġselected', 'Ġpositions', 'Ġnorthern', 'Ġportion', 'Ġorbit', 'e', 'lev', 'ation', 'Ġextent', 'Ġsatellite', "'s", 'Ġposition', 'Ġhorizon', 'Ġthus', 'Ġsatellite', 'Ġhorizon', 'Ġzero', 'Ġelevation', 'Ġsatellite', 'Ġdirectly', 'Ġoverhead', 'Ġelevation', 'Ġdegrees', '.)', 'Ġorbit', 'Ġdesigned', 'Ġsatellite', 'Ġspends', 'Ġgreat', 'Ġmajority', 'Ġtime', 'Ġfar', 'Ġnorthern', 'Ġlat', 'itudes', 'Ġground', 'Ġfootprint', 'Ġmoves', 'Ġslightly', 'Ġperiod', 'Ġone', 'Ġhalf', 'Ġday', 'Ġsatellite', 'Ġavailable', 'Ġoperation', 'Ġtargeted', 'Ġregion', 'Ġnine', 'Ġhours', 'Ġevery', 'Ġsecond', 'Ġrevolution', 'Ġway', 'Ġconstellation', 'Ġthree', 'Ġsatellites', 'plus', 'orbit', 'Ġsp', 'ares', 'Ġprovide', 'Ġuninterrupted', 'Ġcoverage', 'Ġfirst', 'Ġsatellite', 'Ġseries', 'Ġlaunched', 'Ġapr', 'il', 'Ġused', 'Ġexperimental', 'Ġtransmission', 'Ġsignals', 'Ġmos', 'cow']</t>
+          <t>['Â°', '050', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'une', 'Ġge', 'ost', 'ation', 'ary', 'Â°', '047', 'Ġf', 'en', 'gy', 'un', 'Ġj', 'uly', 'Ġsun', 'syn', 'chron', 'ous', 'Â°', '008', '06', 'Ġf', 'en', 'gy', 'un', 'Ġapr', 'il', 'Ġlow', 'Ġearth', 'km', 'Â°', '055', 'Ġf', 'en', 'gy', 'un', 'Ġaug', 'ust', 'Ġsun', 'syn', 'chron', 'ous', 'km', 'Â°', 'Ġsources', 'Ġus', 'space', 'Ġn', 'asa', 'Ġw', 'mo', 'Ġcel', 'est', 'rak', 'Ġlist', 'Ġsatellites', 'Ġsee', 'Ġalso', 'Ġf', 'en', 'gy', 'un', 'Ġwik', 'ipedia', 'Ġch', 'ina', 'Ġmeteor', 'ological', 'Ġadministration', 'Ġch', 'inese', 'Ġanti', 'atellite', 'Ġmissile', 'Ġtest', 'Ġya', 'ogan', 'Ġga', 'en', 'Ġg', 'eb', 'hardt', 'Ġch', 'ris', 'Ġj', 'uly', 'ch', 'ina', 'Ġlo', 'fts', 'Ġf', 'en', 'gy', 'un', 'Ġpolar', 'Ġweather', 'Ġsatellite', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġx', 'ian', 'Ġdi', 'Ġz', 'hang', 'Ġp', 'eng', 'Ġf', 'ang', 'Ġmen', 'g', 'Ġchang', 'Ġjan', 'uary', 'Ġfirst', 'Ġf', 'en', 'gy', 'un', 'Ġsatellite', 'Ġinternational', 'Ġuser', 'Ġconference', 'http', 'Ġadvances', 'Ġatmospheric', 'Ġsciences', 'ijing', 'Ġch', 'ina', 'Ġspring', 'er', 'Ġpublishing', 'aug', 'ust', '):', 'âĢĵ', 'Ġdavid', 'Ġle', 'ard', 'Ġfe', 'b', 'ruary', 'ch', 'ina', "'s", 'Ġanti', 'atellite', 'Ġtest', 'Ġworrisome', 'Ġdebris', 'Ġcloud', 'Ġcircles', 'Ġearth', 'Ġspace', 'Ġk', 'est', 'en', 'baum', 'Ġdavid', 'Ġjan', 'uary', 'ch', 'inese', 'Ġmissile', 'Ġdestroys', 'Ġsatellite', 'mile', 'Ġorbit', 'Ġn', 'pr', 'Ġn', 'asa', 'Ġident', 'ï', '¬', 'ģ', 'es', 'Ġtop', 'Ġten', 'Ġspace', 'Ġjunk', 'Ġmissions', 'ichael', 'Ġco', 'oney', 'Ġnetwork', 'world', 'Ġj', 'uly', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', 'space', 'sk', 'yr', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'two', 'Ġorbits', 'Ġone', 'Ġmission', 'Ġsatellites', 'Ġwork', 'Ġtogether', 'Ġprovide', 'Ġcritical']</t>
         </is>
       </c>
       <c r="C230" t="n">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>['Ġupl', 'ink', 'Ġstation', 'link', 'Ġstations', 'Ġlocated', 'iber', 'ia', 'Ġr', 'ussian', 'Ġfar', 'Ġeast', 'ils', 'k', 'Ġk', 'hab', 'arov', 'sk', 'Ġmag', 'adan', 'Ġv', 'lad', 'iv', 'ost', 'ok', 'mber', 'v', 'iet', 'Ġengineers', 'Ġcreated', 'Ġunique', 'Ġsystem', 'Ġnational', 'Ġnetwork', 'Ġsatellite', 'Ġtelevision', 'Ġcalled', 'Ġorbit', 'Ġbased', 'Ġsatellites', 'Ġunited', 'Ġstates', 'Ġnational', 'Ġpolar', 'orb', 'iting', 'Ġoperational', 'Ġenvironmental', 'Ġsatellite', 'Ġsystem', 'n', 'po', 'ess', 'Ġestablished', 'Ġconsolidate', 'Ġpolar', 'Ġsatellite', 'Ġoperations', 'Ġn', 'asa', 'national', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġadministration', 'national', 'Ġocean', 'ic', 'Ġatmospheric', 'Ġadministration', 'Ġn', 'po', 'ess', 'Ġmanages', 'Ġnumber', 'Ġsatellites', 'Ġvarious', 'Ġpurposes', 'Ġexample', 'ets', 'Ġmeteor', 'ological', 'Ġsatellite', 'Ġe', 'um', 'ets', 'Ġeuro', 'pe', 'Ġbranch', 'Ġprogram', 'Ġmet', 'op', 'Ġmeteor', 'ological', 'Ġoperations', 'Ġorbits', 'Ġsun', 'Ġsynchron', 'ous', 'Ġmeaning', 'Ġcross', 'Ġequ', 'ator', 'Ġlocal', 'Ġtime', 'Ġday', 'Ġexample', 'Ġsatellites', 'Ġn', 'po', 'ess', 'civil', 'ian', 'Ġorbit', 'Ġcross', 'Ġequ', 'ator', 'Ġgoing', 'Ġsouth', 'Ġnorth', 'Ġtimes', 'Ġorbit', 'Ġpolar', 'Ġorbit', 'Ġbeyond', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġplans', 'Ġinitiatives', 'Ġbring', 'Ġdedicated', 'Ġcommunications', 'Ġsatellite', 'Ġbeyond', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġn', 'asa', 'Ġproposed', 'Ġlun', 'et', 'Ġdata', 'Ġnetwork', 'Ġaiming', 'Ġprovide', 'ĠâĢ', 'ŀ', 'l', 'un', 'ar', 'Ġinternet', 'Ġcis', 'l', 'un', 'ar', 'Ġspacecraft', 'Ġinstallations', 'Ġmoon', 'light', 'Ġinitiative', 'Ġequivalent', 'Ġes', 'Ġproject', 'Ġstated', 'Ġcompatible', 'Ġproviding', 'Ġnavig', 'ational', 'Ġservices', 'Ġlunar', 'Ġsurface', 'Ġprogrammes', 'Ġsatellite', 'Ġconst', 'ell', 'st', 'ions', 'Ġseveral', 'Ġsatellites', 'Ġvarious', 'Ġorbits', 'Ġaround', 'Ġmoon', 'Ġorbits', 'Ġalso', 'Ġplanned', 'Ġused', 'Ġpositions', 'Ġpoints', 'Ġalso', 'Ġproposed', 'Ġcommunication', 'Ġsatellites', 'Ġcovering', 'Ġmoon', 'Ġalike', 'Ġcommunication', 'Ġsatellites', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġcover', 'Ġearth', 'Ġalso', 'Ġdedicated', 'Ġcommunication', 'Ġsatellites', 'Ġorbits', 'Ġaround', 'Ġmars', 'Ġsupporting', 'Ġdifferent', 'Ġmissions', 'Ġsurface', 'Ġorbits', 'Ġconsidered', 'Ġmars', 'Ġtelecommunications', 'Ġorbit', 'er', 'Ġcommunications', 'Ġsatellites', 'Ġusually', 'Ġcomposed', 'Ġfollowing', 'Ġsubsystem', 'Ġcommunication', 'Ġpayload', 'Ġnormally', 'Ġcomposed', 'Ġtrans', 'p', 'ond', 'ers', 'Ġantennas', 'Ġswitching', 'Ġsystems', 'Ġengines', 'Ġused', 'Ġbring', 'Ġsatellite', 'Ġdesired', 'Ġorbit', 'Ġstation', 'Ġkeeping', 'Ġtracking', 'Ġstabilization']</t>
+          <t>['Ġdata', 'Ġweather', 'Ġforecasts', 'aa', 'âĢĵ', 'n', 'asa', 'Ġgoes', 'r', 'Ġj', 'une', 'Ġhill', 'ger', 'ald', 'Ġw', 'compl', 'iment', 'ing', 'Ġge', 'ost', 'ation', 'ary', 'Ġweather', 'Ġsatellites', 'Ġtopical', 'Ġtime', 'j', 'uly', 'âĢĵ', 'aug', 'ust', '):', 'âĢĵ', 'Ġvia', 'Ġcolor', 'ado', 'Ġstate', 'Ġuniversity', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', ')"', 'space', 'sk', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'atellite', 'Ġunited', 'Ġnations', 'Ġworld', 'Ġmeteor', 'ological', 'Ġorganization', 'Ġde', 'cember', 'Ġl', 'ui', '.,', 'Ġimaging', 'Ġglobal', 'Ġaur', 'oras', 'Ġspace', 'Ġlight', 'Ġscience', 'Ġapplications', 'Ġz', 'hang', 'Ġx', 'iao', 'x', 'Ġc', 'hen', 'Ġbo', 'Ġfe', 'Ġsong', 'Ġke', 'fe', 'Ġling', 'ping', 'Ġqu', 'f', 'eng', 'Ġli', 'Ġj', 'ia', 'wei', 'Ġw', 'ang', 'Ġx', 'iao', 'ong', 'Ġz', 'hang', 'Ġh', 'ong', 'ji', 'Ġw', 'ang', 'Ġha', 'f', 'eng', 'Ġh', 'Ġz', 'hen', 'wei', 'Ġsun', 'Ġli', 'ang', 'Ġz', 'hang', 'ai', 'Ġsh', 'u', 'ang', 'wide', 'ï', '¬', 'ģ', 'e', 'ld', 'Ġaur', 'oral', 'Ġim', 'ager', 'Ġonboard', 'Ġf', 'en', 'gy', 'un', 'Ġsatellite', 'Ġlight', 'Ġscience', 'Ġapplications', '):', 'h', '01', 'Ġc', 'Ġpm', 'id', 'sen', 'ator', 'Ġcl', 'inton', 'Ġquestions', 'Ġvice', 'Ġadm', 'iral', 'Ġjohn', 'cc', 'nell', 'Ġus', 'n', 'ret', 'Ġdirector', 'Ġnational', 'Ġintelligence', 'Ġlieutenant', 'Ġgeneral', 'ichael', 'ples', 'Ġus', 'Ġdirector', 'Ġdefense', 'Ġintelligence', 'Ġagency', 'Ġsenate', 'Ġarmed', 'Ġservices', 'Ġcommittee', 'Ġhearing', 'Ġworldwide', 'Ġthreats', 'http', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'htm', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ch', 'inese', 'Ġtest', 'Ġarchived', 'h', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'iss', 'Ġcrew', 'Ġtake', 'Ġescape', 'Ġcapsules', 'Ġspace', 'Ġjunk', 'Ġalert', 'Ġmarch']</t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>['Ġsubsystem', 'Ġused', 'Ġkeep', 'Ġsatellite', 'Ġright', 'Ġorbit', 'Ġantennas', 'Ġpointed', 'Ġright', 'Ġdirection', 'Ġpower', 'Ġsystem', 'Ġpointed', 'Ġtowards', 'Ġsun', 'Ġpower', 'Ġsubsystem', 'Ġused', 'Ġpower', 'Ġsatellite', 'Ġsystems', 'Ġnormally', 'Ġcomposed', 'Ġsolar', 'Ġcells', 'Ġbatteries', 'Ġmaintain', 'Ġpower', 'Ġsolar', 'Ġeclipse', 'Ġcommand', 'Ġcontrol', 'Ġsubsystem', 'Ġmaintains', 'Ġcommunications', 'Ġground', 'Ġcontrol', 'Ġstations', 'Ġground', 'Ġcontrol', 'Ġearth', 'Ġstations', 'Ġmonitor', 'Ġsatellite', 'Ġperformance', 'Ġcontrol', 'Ġfunctionality', 'Ġvarious', 'Ġphases', 'Ġlife', 'cycle', 'Ġbandwidth', 'Ġavailable', 'Ġsatellite', 'Ġdepends', 'Ġupon', 'Ġnumber', 'Ġtrans', 'p', 'ond', 'ers', 'Ġprovided', 'Ġsatellite', 'Ġservice', 'Ġvoice', 'Ġinternet', 'Ġradio', 'Ġrequires', 'Ġdifferent', 'Ġamount', 'Ġbandwidth', 'Ġtransmission', 'Ġtypically', 'Ġknown', 'Ġlink', 'Ġbudget', 'ing', 'Ġnetwork', 'Ġsimulator', 'Ġused', 'Ġarrive', 'Ġexact', 'Ġvalue', 'ocating', 'Ġfrequencies', 'Ġsatellite', 'Ġservices', 'Ġcomplicated', 'Ġprocess', 'Ġrequires', 'Ġinternational', 'Ġcoordination', 'Ġplanning', 'Ġcarried', 'Ġausp', 'ices', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', 'Ġfacilitate', 'Ġfrequency', 'Ġplanning', 'Ġworld', 'Ġdivided', 'Ġthree', 'Ġregions', 'Ġregion', 'Ġeuro', 'pe', 'Ġaf', 'rica', 'Ġmiddle', 'Ġeast', 'Ġformerly', 'v', 'iet', 'Ġunion', 'ong', 'olia', 'Ġregion', 'Ġnorth', 'Ġsouth', 'Ġameric', 'Ġgreen', 'land', 'Ġregion', 'ia', 'excluding', 'Ġregion', 'Ġareas', 'Ġaust', 'ral', 'ia', 'Ġsouthwest', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġwithin', 'Ġregions', 'Ġfrequency', 'Ġbands', 'Ġallocated', 'Ġvarious', 'Ġsatellite', 'Ġservices', 'Ġalthough', 'Ġgiven', 'Ġservice', 'Ġmay', 'Ġallocated', 'Ġdifferent', 'Ġfrequency', 'Ġbands', 'Ġdifferent', 'Ġregions', 'Ġservices', 'Ġprovided', 'Ġsatellites', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'f', 'ss', 'Ġbroadcasting', 'Ġsatellite', 'Ġservice', 'b', 'ss', 'Ġmobile', 'atellite', 'Ġservice', 'Ġstructure', 'Ġfrequency', 'Ġallocation', 'Ġsatellite', 'Ġsystems', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġir', 'idium', 'Ġsatellite', 'Ġservice', 'Ġservice', 'Ġfirst', 'Ġhistorically', 'Ġimportant', 'Ġapplication', 'Ġcommunication', 'Ġsatellites', 'Ġinter', 'continental', 'Ġlong', 'Ġdistance', 'Ġtele', 'phony', 'Ġfixed', 'Ġpublic', 'Ġswitched', 'Ġtelephone', 'Ġnetwork', 'Ġrel', 'ays', 'Ġtelephone', 'Ġcalls', 'Ġland', 'Ġline', 'Ġtele', 'phones', 'Ġearth', 'Ġstation', 'Ġtransmitted', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'link', 'Ġfollows', 'Ġanalogous', 'Ġpath', 'Ġimprovements', 'Ġsubmarine', 'Ġcommunications', 'Ġcables', 'Ġuse', 'Ġfiber', 'opt', 'ics', 'Ġcaused', 'Ġdecline', 'Ġuse', 'Ġsatellites', 'Ġfixed', 'Ġtele', 'phony', 'Ġlate', 'th', 'Ġcentury', 'Ġsatellite', 'Ġcommunications', 'Ġstill', 'Ġused', 'Ġmany', 'Ġapplications', 'Ġtoday', 'Ġremote', 'Ġislands', 'Ġasc', 'ension', 'Ġisland', 'Ġsaint', 'Ġhel', 'ena', 'Ġdie', 'go', 'Ġgar', 'cia']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġnews', 'Ġconcern', 'Ġch', 'ina', "'s", 'Ġmissile', 'Ġtest', 'Ġretrieved', 'Ġjan', 'uary', 'Ġarchived', 'Ġmay', 'Ġway', 'back', 'Ġmachine', 'Ġag', 'ence', 'Ġfr', 'ance', 'pres', 'se', 'jan', 'uary', 'b', 'rit', 'Ġconcerned', 'Ġch', 'inese', 'Ġsatellite', 'Ġshoot', 'Ġspaced', 'aily', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġk', 'est', 'en', 'baum', 'Ġdavid', 'jan', 'uary', 'ch', 'inese', 'Ġmissile', 'Ġdestroys', 'Ġsatellite', 'mile', 'Ġorbit', 'Ġp', 'story', 'id', 'Ġnational', 'Ġpublic', 'Ġradio', 'Ġarchived', 'web', 'arch', 'iv', 'Ġp', 'story', 'id', 'Ġoriginal', 'mber', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', 'h', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'weather', 'Ġsatellites', 'Ġnational', 'Ġweather', 'Ġservice', 'Ġh', 'anson', 'Ġde', 'rek', 'Ġper', 'onto', 'Ġj', 'ames', 'Ġh', 'ild', 'er', 'brand', 'Ġdou', 'glas', 'aa', "'s", 'Ġeyes', 'Ġfive', 'Ġdecades', 'Ġweather', 'Ġforecasting', 'Ġenvironmental', 'Ġsatellites', 'Ġfuture', 'Ġsatellites', 'Ġpromise', 'Ġmeteor', 'ologists', 'Ġsociety', '?"', 'Ġg', 'environment', 'al', 'Ġworld', 'Ġmeteor', 'ological', 'Ġorganization', 'Ġty', 'ler', 'Ġpat', 'rick', 'Ġe', 'Ġapr', 'il', 'ch', 'ina', 'Ġsays', 'Ġblast', "'t", 'Ġslow', 'Ġsatellite', 'Ġlaunch', 'ings', 'Ġnew', 'ork', 'Ġtimes', 'Ġp', 'con', 'cern', 'Ġch', 'ina', "'s", 'Ġmissile', 'Ġtest', 'Ġic', 'st', 'Ġnews', '01', 'Ġsatellite', 'Ġprogramme', 'Ġretrieved', 'Ġreferences', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C232" t="n">
@@ -3454,7 +3454,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>['Ġeas', 'ter', 'Ġisland', 'Ġsubmarine', 'Ġcables', 'Ġservice', 'Ġneed', 'Ġsatellite', 'Ġtele', 'phones', 'Ġalso', 'Ġregions', 'Ġcontinents', 'Ġcountries', 'Ġland', 'line', 'Ġtelecommunications', 'Ġrare', 'Ġnon', 'Ġexist', 'ent', 'Ġexample', 'Ġlarge', 'Ġregions', 'Ġsouth', 'Ġameric', 'Ġaf', 'rica', 'ada', 'Ġch', 'ina', 'Ġr', 'ussia', 'Ġaust', 'ral', 'ia', 'Ġsatellite', 'Ġcommunications', 'Ġalso', 'Ġprovide', 'Ġconnection', 'Ġedges', 'Ġant', 'ar', 'ctica', 'Ġgreen', 'land', 'Ġland', 'Ġuse', 'Ġsatellite', 'Ġphones', 'Ġrigs', 'Ġsea', 'Ġbackup', 'Ġhospitals', 'Ġmilitary', 'Ġrecreation', 'Ġships', 'Ġsea', 'Ġwell', 'Ġplanes', 'Ġoften', 'Ġuse', 'Ġsatellite', 'Ġphones', 'Ġsatellite', 'Ġphone', 'Ġsystems', 'Ġaccomplished', 'Ġnumber', 'Ġmeans', 'Ġlarge', 'Ġscale', 'Ġoften', 'Ġlocal', 'Ġtelephone', 'Ġsystem', 'Ġisolated', 'Ġarea', 'Ġlink', 'Ġtelephone', 'Ġsystem', 'Ġmain', 'Ġland', 'Ġarea', 'Ġalso', 'Ġservices', 'Ġpatch', 'Ġradio', 'Ġsignal', 'Ġtelephone', 'Ġsystem', 'Ġexample', 'Ġalmost', 'Ġtype', 'Ġsatellite', 'Ġused', 'Ġsatellite', 'Ġphones', 'Ġconnect', 'Ġdirectly', 'Ġconstellation', 'Ġeither', 'Ġge', 'ost', 'ation', 'ary', 'Ġlow', 'earth', 'orbit', 'Ġsatellites', 'Ġcalls', 'Ġforwarded', 'Ġsatellite', 'Ġteleport', 'Ġconnected', 'Ġpublic', 'Ġswitched', 'Ġtelephone', 'Ġnetwork', 'Ġtelevision', 'Ġbecame', 'Ġmain', 'Ġmarket', 'Ġdemand', 'Ġsimultaneous', 'Ġdelivery', 'Ġrelatively', 'Ġsignals', 'Ġlarge', 'Ġbandwidth', 'Ġmany', 'Ġreceivers', 'Ġprecise', 'Ġmatch', 'Ġcapabilities', 'Ġge', 'os', 'ynchronous', 'ats', 'Ġtwo', 'Ġsatellite', 'Ġtypes', 'Ġused', 'Ġnorth', 'Ġameric', 'Ġtelevision', 'Ġradio', 'Ġdirect', 'Ġbroadcast', 'Ġsatellite', 'bs', 'Ġfixed', 'Ġservice', 'Ġsatellite', 'f', 'ss', 'Ġdefinitions', 'Ġf', 'ss', 'bs', 'Ġsatellites', 'Ġoutside', 'Ġnorth', 'Ġameric', 'Ġespecially', 'Ġeuro', 'pe', 'Ġbit', 'Ġambiguous', 'Ġsatellites', 'Ġused', 'Ġdirect', 'home', 'Ġtelevision', 'Ġeuro', 'pe', 'Ġhigh', 'Ġpower', 'Ġoutput', 'bs', 'class', 'Ġsatellites', 'Ġnorth', 'Ġameric', 'Ġuse', 'Ġlinear', 'Ġpolarization', 'Ġf', 'ss', 'class', 'Ġsatellites', 'Ġexamples', 'Ġast', 'ra', 'Ġe', 'ut', 'els', 'Ġhot', 'bird', 'Ġspacecraft', 'Ġorbit', 'Ġeuro', 'pe', 'Ġcontinent', 'Ġterms', 'Ġf', 'ss', 'bs', 'Ġused', 'Ġthroughout', 'Ġnorth', 'Ġameric', 'Ġcontinent', 'Ġuncommon', 'Ġeuro', 'pe', 'Ġfixed', 'Ġservice', 'Ġsatellites', 'Ġuse', 'Ġband', 'Ġlower', 'Ġportions', 'Ġband', 'Ġnormally', 'Ġused', 'Ġbroadcast', 'Ġfeeds', 'Ġtelevision', 'Ġnetworks', 'Ġlocal', 'Ġaffiliate', 'Ġstations', 'Ġprogram', 'Ġfeeds', 'Ġnetwork', 'Ġsynd', 'icated', 'Ġprogramming', 'Ġlive', 'Ġshots', 'Ġback', 'haul']</t>
+          <t>['Ġgalaxy', 'Ġwik', 'ipedia', 'Ġgalaxy', 'Ġanimation', 'Ġgalaxy', 'Ġtrajectory', 'Ġoct', 'ober', 'Ġoct', 'ober', 'Ġgalaxy', 'Ġearth', 'Ġmission', 'Ġtype', 'Ġcommunication', 'Ġnavigation', 'Ġoperator', 'Ġpan', 'ams', 'âĢĵ', 'Ġint', 'els', '-)', 'Ġcos', 'par', 'Ġid', '041', 'Ġsat', 'cat', 'Ġmission', 'Ġduration', 'Ġyears', 'planned', 'Ġspacecraft', 'Ġproperties', 'Ġbus', 'Ġge', 'ost', 'ar', 'Ġmanufacturer', 'Ġorbital', 'Ġsciences', 'Ġlaunch', 'Ġmass', '033', 'Ġkilograms', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġoct', 'ober', 'Ġut', 'c', 'Ġrocket', 'ri', 'ane', 'Ġlaunch', 'Ġsite', 'Ġk', 'ou', 'Ġcontractor', 'rian', 'esp', 'ace', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġge', 'oc', 'entric', 'Ġregime', 'Ġge', 'ost', 'ation', 'ary', 'Ġlong', 'itude', 'Â°', 'Ġwest', 'Ġper', 'ig', 'ee', 'Ġaltitude', 'Ġkilometres', 'Ġmi', 'Ġap', 'gee', 'Ġaltitude', 'Ġkilometres', 'Ġmi', 'Ġgalaxy', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġinclination', '06', 'Ġdegrees', 'Ġperiod', 'Ġhours', 'Ġminutes', 'Ġtrans', 'p', 'ond', 'ers', 'Ġband', 'Ġg', 'h', 'Ġband', 'ie', 'ee', 'Ġband', 'Ġband', 'ie', 'ee', 'Ġband', 'Ġgalaxy', 'Ġameric', 'Ġtelecommunications', 'Ġsatellite', 'Ġowned', 'Ġint', 'els', 'Ġlaunched', 'Ġoriginally', 'Ġoperated', 'Ġpan', 'ams', 'Ġsubsequently', 'Ġtransferred', 'Ġint', 'els', 'Ġtwo', 'Ġcompanies', 'Ġmerged', 'Ġoriginally', 'Ġpositioned', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġlong', 'itude', 'Â°', 'Ġwest', 'Ġused', 'Ġprovide', 'Ġcommunication', 'Ġservices', 'Ġnorth', 'Ġameric', 'Ġapr', 'il', 'Ġint', 'els', 'Ġlost', 'Ġcontrol', 'Ġsatellite', 'Ġbegan', 'Ġdrift', 'Ġaway', 'Ġorbital', 'Ġslot', 'Ġpotential', 'Ġcause', 'Ġdisruption', 'Ġsatellites', 'Ġpath', 'Ġde', 'cember', 'Ġint', 'els', 'Ġreported', 'Ġsatellite', 'Ġreboot', 'ed', 'Ġper', 'Ġdesign', 'Ġcommand', 'Ġunit', 'Ġresponding', 'Ġcommands', 'Ġaddition', 'Ġsatellite', 'Ġsecured', 'Ġsafe', 'Ġmode', 'Ġpotential', 'Ġinterference', 'Ġissues', 'Ġgalaxy', 'Ġceased', 'Ġint', 'els', 'Ġrep', 'osition', 'ed', 'Ġgalaxy', 'Ġback', 'Ġoriginal', 'Ġlocation', 'Ġapr', 'il', 'Ġaug', 'ust', 'Ġint', 'els', 'Ġlost', 'Ġcontrol', 'Ġgalaxy', 'Ġattribut', 'ing', 'Ġspace', 'Ġweather', 'Ġevent', 'Ġgalaxy', 'Ġconstructed', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'Ġbased']</t>
         </is>
       </c>
       <c r="C233" t="n">
@@ -3467,7 +3467,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>['Ġwell', 'Ġused', 'Ġapplications', 'Ġtele', 'phony', 'Ġtelevision', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġdistance', 'Ġlearning', 'Ġschools', 'Ġuniversities', 'Ġbusiness', 'Ġtelevision', 'Ġvide', 'ocon', 'f', 'eren', 'cing', 'Ġgeneral', 'Ġcommercial', 'Ġtelecommunications', 'Ġf', 'ss', 'Ġsatellites', 'Ġalso', 'Ġused', 'Ġdistribute', 'Ġnational', 'Ġcable', 'Ġchannels', 'Ġcable', 'Ġtelevision', 'Ġhead', 'ends', 'Ġfree', 'air', 'Ġsatellite', 'Ġchannels', 'Ġalso', 'Ġusually', 'Ġdistributed', 'Ġf', 'ss', 'Ġsatellites', 'Ġband', 'Ġint', 'els', 'Ġameric', 'Ġgalaxy', 'r', 'Ġsatellites', 'Ġnorth', 'Ġameric', 'Ġprovide', 'Ġquite', 'Ġlarge', 'Ġamount', 'Ġf', 'ta', 'Ġchannels', 'Ġband', 'Ġtrans', 'p', 'ond', 'ers', 'Ġameric', 'Ġdish', 'Ġnetwork', 'bs', 'Ġservice', 'Ġalso', 'Ġrecently', 'Ġused', 'Ġf', 'ss', 'Ġtechnology', 'Ġwell', 'Ġprogramming', 'Ġpackages', 'Ġrequiring', 'Ġsuper', 'ish', 'Ġantenna', 'Ġdue', 'Ġdish', 'Ġnetwork', 'Ġneeding', 'Ġcapacity', 'Ġcarry', 'Ġlocal', 'Ġtelevision', 'Ġstations', 'Ġper', 'must', 'carry', 'Ġregulations', 'Ġbandwidth', 'Ġcarry', 'Ġchannels', 'Ġdirect', 'Ġbroadcast', 'Ġsatellite', 'Ġcommunications', 'Ġsatellite', 'Ġtransm', 'Ġsmall', 'bs', 'Ġsatellite', 'Ġdishes', 'usually', 'Ġinches', 'Ġdiameter', 'Ġdirect', 'Ġbroadcast', 'Ġsatellites', 'Ġgenerally', 'Ġoperate', 'Ġupper', 'Ġportion', 'Ġmicrowave', 'Ġband', 'bs', 'Ġtechnology', 'Ġused', 'th', 'oriented', 'direct', 'oh', 'ome', 'Ġsatellite', 'Ġservices', 'Ġdirect', 'v', 'Ġdish', 'Ġnetwork', 'Ġunited', 'Ġstates', 'Ġbell', 'Ġsatellite', 'Ġsh', 'aw', 'Ġdirect', 'ada', 'Ġfre', 'es', 'Ġire', 'land', 'Ġnew', 'Ġzeal', 'Ġdst', 'v', 'Ġsouth', 'Ġaf', 'rica', 'Ġoperating', 'Ġlower', 'Ġfrequency', 'Ġlower', 'Ġpower', 'bs', 'Ġf', 'ss', 'Ġsatellites', 'Ġrequire', 'Ġmuch', 'Ġlarger', 'Ġdish', 'Ġreception', 'Ġfeet', 'Ġdiameter', 'Ġband', 'Ġfeet', 'Ġlarger', 'Ġband', 'Ġuse', 'Ġlinear', 'Ġpolarization', 'Ġtrans', 'p', 'ond', 'ers', 'Ġinput', 'Ġoutput', 'Ġopposed', 'Ġcircular', 'Ġpolarization', 'Ġused', 'bs', 'Ġsatellites', 'Ġminor', 'Ġtechnical', 'Ġdifference', 'Ġusers', 'Ġnotice', 'Ġf', 'ss', 'Ġsatellite', 'Ġtechnology', 'Ġalso', 'Ġoriginally', 'Ġused', 'th', 'Ġsatellite', 'Ġlate', 'Ġearly', 'Ġunited', 'Ġstates', 'Ġform', 'te', 'levision', 'Ġreceive', 'Ġreceivers', 'Ġdishes', 'Ġalso', 'Ġused', 'Ġband', 'Ġform', 'def', 'unct', 'Ġprim', 'est', 'ar', 'Ġsatellite', 'Ġservice', 'Ġsatellites', 'Ġlaunched', 'Ġtrans', 'p', 'ond', 'ers', 'Ġka', 'Ġband', 'Ġdirect']</t>
+          <t>['Ġaround', 'Ġge', 'ost', 'ar', 'Ġsatellite', 'Ġbus', 'Ġcontract', 'Ġmanufacture', 'Ġsigned', 'Ġtime', 'Ġidentical', 'Ġgalaxy', 'Ġgalaxy', 'Ġsatellites', 'Ġalso', 'Ġorder', 'Ġcontract', 'Ġchanged', 'Ġallow', 'Ġaddition', 'Ġtrans', 'p', 'ond', 'ers', 'Ġsupport', 'Ġus', 'Ġgovernment', "'s", 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġcontrol', 'Ġsegment', 'Ġwide', 'Ġarea', 'Ġaug', 'mentation', 'Ġsystem', 'wa', 'Ġus', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġnavigation', 'Ġprogram', 'Ġcommunications', 'Ġpayload', 'Ġaboard', 'Ġgalaxy', 'Ġconsisted', 'Ġtrans', 'p', 'ond', 'ers', 'Ġoperating', 'Ġbands', 'Ġn', 'ato', 'Ġelectromagnetic', 'Ġspectrum', 'Ġband', 'Ġus', 'Ġie', 'ee', 'Ġspectrum', 'Ġalso', 'Ġcarried', 'Ġtwo', 'Ġband', 'ie', 'ee', 'Ġband', 'Ġtrans', 'p', 'ond', 'ers', 'Ġform', 'Ġpart', 'Ġus', 'Ġgovernment', "'s", 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġcontrol', 'Ġsegment', 'Ġused', 'Ġaircraft', 'Ġnavigation', 'Ġlaunch', 'Ġgalaxy', 'Ġsatellite', 'Ġmass', '033', 'Ġkilograms', 'Ġexpected', 'Ġoperational', 'Ġlifespan', 'Ġaround', 'Ġyears', 'Ġlaunch', 'Ġgalaxy', 'Ġconducted', 'rian', 'esp', 'ace', 'Ġusing', 'ri', 'ane', 'Ġcarrier', 'Ġrocket', 'Ġflying', 'Ġgu', 'iana', 'Ġspace', 'Ġcentre', 'Ġk', 'ou', 'Ġfrench', 'Ġlaunch', 'Ġoccurred', 'Ġg', 'mt', 'Ġoct', 'ober', 'Ġopening', 'minute', 'Ġlaunch', 'Ġwindow', 'Ġsuccessfully', 'Ġplaced', 'Ġgalaxy', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'Ġfrench', 'Ġsy', 'racuse', 'Ġmilitary', 'Ġcommunications', 'Ġsatellite', 'Ġlaunched', 'Ġrocket', 'Ġlaunch', 'Ġgalaxy', 'Ġlocated', 'Ġbeneath', 'Ġsy', 'racuse', 'Ġspacecraft', 'Ġmounted', 'Ġatop', 'Ġsy', 'lda', 'Ġadapt', 'Ġsatellite', 'Ġlaunch', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġfollowing', 'Ġseparation', 'Ġcarrier', 'Ġrocket', 'Ġgalaxy', 'Ġraised', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġmeans', 'Ġap', 'gee', 'Ġmotor', 'Ġinsertion', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġoccurred', 'Ġaround', '00', 'Ġoct', 'ober', 'Ġapr', 'il', 'Ġgalaxy', 'Ġceased', 'Ġresponding', 'Ġcommands', 'Ġsent', 'Ġcontrollers', 'Ġground', 'Ġhowever', 'Ġunclear', 'Ġactual', 'Ġinitial', 'Ġfailure', 'Ġdate', 'Ġcommands', 'Ġoften', 'Ġsent', 'Ġsatellite', 'Ġoperators', 'Ġdays', 'Ġeven', 'Ġweeks', 'Ġapart', 'Ġwithout', 'Ġcommands', 'Ġnecessary', 'Ġstation', 'keeping', 'Ġbegan', 'Ġdrift', 'Ġeast', 'Ġaway', 'Ġallotted', 'Ġorbital', 'Ġslot']</t>
         </is>
       </c>
       <c r="C234" t="n">
@@ -3480,7 +3480,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>['v', "'s", 'Ġspac', 'eway', 'Ġsatellite', 'ik', 'Ġn', 'asa', 'ro', 'Ġalso', 'Ġlaunched', 'Ġexperimental', 'Ġsatellites', 'Ġcarrying', 'Ġka', 'Ġband', 'acons', 'Ġrecently', 'Ġmanufacturers', 'Ġalso', 'Ġintroduced', 'Ġspecial', 'Ġantennas', 'Ġmobile', 'Ġreception', 'bs', 'Ġtelevision', 'Ġusing', 'Ġglobal', 'Ġpositioning', 'Ġsystem', 'Ġtechnology', 'Ġreference', 'Ġantennas', 'Ġautomatically', 'aim', 'Ġsatellite', 'Ġmatter', 'Ġvehicle', 'Ġantenna', 'Ġmounted', 'Ġsituated', 'Ġmobile', 'Ġsatellite', 'Ġantennas', 'Ġpopular', 'Ġrecreational', 'Ġvehicle', 'Ġowners', 'Ġmobile', 'bs', 'Ġantennas', 'Ġalso', 'Ġused', 'Ġjet', 'blue', 'Ġair', 'ways', 'Ġdirect', 'v', 'supp', 'lied', 'Ġlive', 'tv', 'Ġsubsidiary', 'Ġjet', 'blue', 'Ġpassengers', 'Ġview', 'board', 'Ġscreens', 'Ġmounted', 'Ġseats', 'Ġsatellite', 'Ġradio', 'Ġoffers', 'Ġaudio', 'Ġbroadcast', 'Ġservices', 'Ġcountries', 'Ġnotably', 'Ġunited', 'Ġstates', 'Ġmobile', 'Ġservices', 'Ġallow', 'Ġlisteners', 'Ġroam', 'Ġcontinent', 'Ġlistening', 'Ġaudio', 'Ġprogramming', 'Ġanywhere', 'Ġradio', 'Ġbroadcasting', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġsatellite', 'Ġradio', 'Ġsubscription', 'Ġradio', 'Ġdigital', 'Ġradio', 'Ġsignal', 'Ġbroadcast', 'Ġcommunications', 'Ġsatellite', 'Ġcovers', 'Ġmuch', 'Ġwider', 'Ġgeographical', 'Ġrange', 'Ġterrestrial', 'Ġradio', 'Ġsignals', 'Ġamateur', 'Ġradio', 'Ġoperators', 'Ġaccess', 'Ġamateur', 'Ġsatellites', 'Ġdesigned', 'Ġspecifically', 'Ġcarry', 'Ġamateur', 'Ġradio', 'Ġtraffic', 'Ġsatellites', 'Ġoperate', 'Ġspace', 'borne', 'Ġrepe', 'aters', 'Ġgenerally', 'Ġaccessed', 'ateurs', 'Ġequipped', 'Ġradio', 'Ġequipment', 'Ġhighly', 'Ġdirectional', 'Ġantennas', 'ag', 'Ġdish', 'Ġantennas', 'Ġdue', 'Ġlaunch', 'Ġcosts', 'Ġcurrent', 'Ġamateur', 'Ġsatellites', 'Ġlaunched', 'Ġfairly', 'Ġlow', 'Ġearth', 'Ġorbits', 'Ġdesigned', 'Ġdeal', 'Ġlimited', 'Ġnumber', 'Ġbrief', 'Ġcontacts', 'Ġgiven', 'Ġtime', 'Ġsatellites', 'Ġalso', 'Ġprovide', 'Ġdata', 'forward', 'ing', 'Ġservices', 'Ġusing', 'Ġsimilar', 'Ġprotocols', 'Ġsatellite', 'Ġcommunication', 'Ġtechnology', 'Ġused', 'Ġmeans', 'Ġconnect', 'Ġinternet', 'Ġvia', 'Ġbroadband', 'Ġdata', 'Ġconnections', 'Ġuseful', 'Ġusers', 'Ġlocated', 'Ġremote', 'Ġareas', 'Ġcannot', 'Ġaccess', 'Ġbroadband', 'Ġconnection', 'Ġrequire', 'Ġhigh', 'Ġavailability', 'Ġservices', 'Ġcommunications', 'Ġsatellites', 'Ġused', 'Ġmilitary', 'Ġcommunications', 'Ġapplications', 'Ġglobal', 'Ġcommand', 'Ġcontrol', 'Ġsystems', 'Ġexamples', 'Ġmilitary', 'Ġsystems', 'Ġuse', 'Ġcommunication', 'Ġsatellites', 'Ġmil', 'star', 'sc', 'Ġfl', 'ts', 'Ġunited', 'Ġstates', 'Ġn', 'ato', 'Ġsatellites', 'Ġunited', 'Ġkingdom', 'Ġsatellites', 'Ġinstance', 'Ġsk', 'yn', 'et', 'Ġsatellites', 'Ġformer', 'v', 'iet', 'Ġunion', 'Ġind', 'ia', 'Ġlaunched', 'Ġfirst', 'Ġmilitary', 'Ġcommunication', 'Ġsatellite', 'Ġtrans', 'p']</t>
+          <t>['Ġtelevision', 'Ġsignals', 'Ġtransferred', 'Ġsatellites', 'Ġintentional', 'Ġtransmissions', 'Ġceased', 'Ġgalaxy', 'Ġsatellite', 'Ġremoved', 'orbit', 'Ġstorage', 'Â°', 'Ġwest', 'Ġreplace', 'Ġgalaxy', 'Â°', 'Ġwest', 'Ġorbital', 'Ġslot', 'Ġgalaxy', 'Ġoriginally', 'Ġslated', 'Ġreplace', 'Ġanother', 'Ġsatellite', 'Ġgalaxy', 'Ġrelocated', 'Â°', 'Ġeast', 'Ġstart', 'Ġmission', 'Ġcritical', 'Ġservice', 'Ġunited', 'Ġstates', 'Ġgovernment', 'Ġdue', 'Ġnecessity', 'Ġrel', 'ocating', 'Ġgalaxy', 'Â°', 'Ġwest', 'Ġint', 'els', 'Ġforced', 'Ġleave', 'Â°', 'Ġwest', 'Ġvacant', 'Ġapr', 'il', 'Ġorbital', 'Ġsciences', 'Ġtheor', 'ized', 'Ġbelieved', 'Ġsolar', 'Ġactivity', 'Ġresponsible', 'Ġsatellite', 'Ġmalfunction', 'ing', 'Ġalthough', 'Ġlater', 'Ġstatement', 'Ġcompany', 'Ġsaid', 'Ġcompany', 'Ġunable', 'Ġactually', 'Ġsettle', 'Ġsingle', 'Ġroot', 'Ġcause', '."[', 'Ġmay', 'Ġattempt', 'Ġmoment', 'ary', 'Ġseries', 'Ġstrong', 'Ġpulses', 'Ġintended', 'Ġcause', 'Ġpower', 'Ġsystem', 'Ġmalfunction', 'Ġsent', 'Ġgalaxy', 'Ġunfortunately', 'Ġdesired', 'Ġeffect', 'Ġcausing', 'Ġpower', 'Ġsystem', 'Ġoverload', 'Ġsubsequent', 'Ġshut', 'Ġactive', 'Ġtrans', 'p', 'ond', 'ers', 'Ġconcern', 'Ġneighboring', 'Ġsatellite', 'Ġoperators', 'Ġtype', 'Ġrecovery', 'Ġattempt', 'Ġwould', 'Ġpotential', 'Ġpermanently', 'Ġdamage', 'Ġsensitive', 'Ġhardware', 'Ġboard', 'Ġsatellite', 'Ġcould', 'Ġcontributed', 'Ġplacing', 'Ġsatellite', 'Ġpermanent', 'Ġunre', 'cover', 'able', 'Ġcontrol', 'Ġstate', 'Ġmay', 'Ġint', 'els', 'es', 'Ġworld', 'Ġskies', 'Ġconfirmed', 'Ġgalaxy', 'Ġwould', 'Ġpass', 'Ġclose', 'Ġlatter', "'s", 'Ġsatellite', 'Ġpotentially', 'Ġcausing', 'Ġinterference', 'Ġcable', 'Ġprogramming', 'Ġunited', 'Ġstates', 'Ġtwo', 'Ġsatellites', 'Ġbroadcast', 'Ġsimilar', 'Ġfrequencies', 'Ġmay', 'Ġj', 'une', 'Ġgalaxy', 'Ġpassed', 'Ġwithin', 'Ġhalf', 'Ġdegree', 'Ġtwo', 'Ġsatellites', 'Ġpassed', 'Ġclose', 'Ġparticularly', 'Ġclosest', 'Ġapproach', 'Ġmay', 'Ġj', 'une', 'Ġsignals', 'Ġgalaxy', 'Ġstill', 'active', 'Ġtrans', 'p', 'ond', 'ers', 'Ġcould', 'Ġinterfered', 'Ġsignals', 'Ġbroadcast', 'es', 'Ġmaneu', 'vered', 'Ġsatellite', 'Ġreduce', 'Ġpossibility', 'Ġinterference', 'es', 'Ġsatellite', 'Ġfollowed', 'Ġbehind', 'Ġgalaxy', 'Ġpass', 'Ġprovide', 'Ġbackup', 'Ġneeded', 'Ġj', 'une', 'Ġint', 'els', 'es', 'Ġreported', 'Ġinterference', 'Ġoccurred', 'Ġclosest', 'Ġapproach', 'Ġsatellites', 'Ġpassing', 'Ġwithin', 'Ġdegrees', 'Ġpassed', 'Ġgalaxy', 'Ġcontinued', 'Ġdrift', 'Ġeast', 'wards', 'Ġj', 'uly']</t>
         </is>
       </c>
       <c r="C235" t="n">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>['ond', 'ers', 'Ġoperate', 'Ġf', 'Ġband', 'Ġbands', 'Ġtypically', 'Ġmilitary', 'Ġsatellites', 'Ġoperate', 'also', 'Ġknown', 'Ġx', 'band', 'also', 'Ġknown', 'Ġka', 'Ġband', 'Ġfrequency', 'Ġbands', 'Ġnear', 'ground', 'Ġsitu', 'Ġenvironmental', 'Ġmonitoring', 'Ġequipment', 'Ġtide', 'Ġgau', 'ges', 'Ġweather', 'Ġstations', 'Ġweather', 'Ġbu', 'oys', 'Ġradios', 'ond', 'es', 'Ġmay', 'Ġuse', 'Ġsatellites', 'Ġone', 'way', 'Ġdata', 'Ġtransmission', 'Ġtwo', 'way', 'Ġtele', 'metry', 'Ġmay', 'Ġbased', 'Ġsecondary', 'Ġpayload', 'Ġweather', 'Ġsatellite', 'Ġcase', 'Ġgoes', 'Ġmete', 'os', 'Ġothers', 'Ġarg', 'os', 'Ġsystem', 'Ġdedicated', 'Ġsatellites', 'Ġdata', 'Ġrate', 'Ġtypically', 'Ġmuch', 'Ġlower', 'Ġsatellite', 'Ġinternet', 'Ġaccess', 'Ġcommercial', 'ization', 'Ġspace', 'Ġhistory', 'Ġtele', 'communication', 'Ġinter', 'atellite', 'Ġcommunications', 'Ġsatellite', 'Ġlist', 'Ġcommunication', 'Ġsatellite', 'Ġcompanies', 'Ġlist', 'Ġcommunications', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'sts', 'Ġnewsp', 'ace', 'Ġreconnaissance', 'Ġsatellite', 'Ġamateur', 'Ġradio', 'Ġinternet', 'Ġaccess', 'Ġmilitary', 'Ġdata', 'Ġcollection', 'Ġsee', 'Ġalso', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġrelay', 'dis', 'amb', 'ig', 'uation', 'Ġsat', 'Ġmove', 'Ġsatellite', 'Ġdata', 'Ġunit', 'Ġsatellite', 'Ġdelay', 'Ġsatellite', 'Ġmodem', 'Ġsatellite', 'Ġspace', 'Ġsegment', 'Ġspace', 'Ġpollution', 'Ġorbital', 'Ġperiods', 'Ġspeeds', 'Ġcalculated', 'Ġusing', 'Ġrelations', 'Ġradius', 'Ġorbit', 'Ġmetres', 'Ġorbital', 'Ġperiod', 'Ġseconds', 'Ġorbital', 'Ġspeed', 'Ġgravitational', 'Ġconstant', 'Ġapproximately', 'ĠÃĹ', 'âĪĴ', 'Ġmass', 'Ġearth', 'Ġapproximately', 'ĠÃĹ', 'ĠÃĹ', 'Ġb', 'Ġapproximately', 'Ġtimes', 'Ġradius', 'Ġlength', 'Ġmoon', 'Ġnearest', 'Ġtimes', 'Ġmoon', 'Ġfart', 'hest', 'Ġlab', 'rador', 'Ġvir', 'gil', '02', 'atellite', 'Ġcommunication', 'Ġb', 'rit', 'ann', 'ica', 'Ġretrieved', '02', 'atell', 'ites', 'Ġcommunication', 'Ġsatellites', 'Ġdex', 'html', 'Ġretrieved', '02', 'military', 'Ġsatellite', 'Ġcommunications', 'Ġfundamentals', 'Ġaerospace', 'Ġcorporation', 'web', 'arch', 'iv', 'fund', 'ament', 'als', 'Ġaerospace', '04', '01', 'Ġarchived', 'Ġoriginal', '09', '05', 'Ġretrieved', '02', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'oct', 'ober', 'ext', 'r']</t>
+          <t>['Ġpassed', 'Ġgalaxy', 'hor', 'izons', 'Ġsatellite', 'Ġlocated', 'Â°', 'Ġwest', 'Ġowned', 'Ġjointly', 'Ġint', 'els', 'Ġperfect', 'Ġjs', 'Ġgroup', 'Ġpass', 'Ġreported', 'Ġcaused', 'Ġdisruption', 'Ġbroadcasts', 'Ġmade', 'Ġgalaxy', 'hor', 'izons', 'Ġj', 'uly', 'Ġgalaxy', 'Ġpassed', 'Ġanother', 'Ġint', 'els', 'Ġspacecraft', 'Ġgalaxy', 'Ġlocated', 'Â°', 'Ġwest', 'Ġclosest', 'Ġapproach', 'Ġoccurred', 'Ġj', 'uly', 'Ġaug', 'ust', 'Ġsatellite', 'Ġdrifted', 'Ġtoward', 'Ġsatellite', 'Ġowned', 'Ġg', 'ci', 'Ġcommunications', 'Ġcompany', 'Ġbroadcasting', 'Ġrural', 'Ġal', 'aska', 'Ġgalaxy', 'Ġpassed', 'ik', 'Ġfailure', 'Ġrecovery', 'Ġfailure', 'Ġreported', 'Ġpasses', 'Ġinterference', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġorbital', 'Ġslot', 'Â°', 'Ġwest', 'Ġnear', 'Ġoct', 'ober', 'Ġsatellite', 'Ġcontinued', 'Ġwatched', 'Ġtelecommunications', 'Ġcompanies', 'Ġdue', 'Ġpotential', 'Ġinterfering', 'Ġc', 'band', 'Ġfrequencies', 'Ġde', 'cember', 'Ġreported', 'Ġgalaxy', 'Ġpotentially', 'Ġcaused', 'Ġoutage', 'Ġnational', 'Ġweather', 'Ġservice', 'ap', 'ort', 'Ġfeed', 'Ġvia', 'es', 'Ġlocated', 'Ġwest', 'Ġde', 'cember', 'Ġfollowing', 'Ġadvisory', 'Ġissued', 'Ġrisk', 'Ġidentified', 'Ġgalaxy', 'Ġrogue', 'Ġsatellite', 'Ġtravers', 'es', 'es', 'Ġorbital', 'Ġposition', 'Ġmay', 'Ġresult', 'Ġpossible', 'Ġloss', 'Ġdata', 'Ġvia', 'Ġaw', 'ips', 'bn', 'ap', 'ort', 'Ġfeed', 'Ġpotential', 'Ġinterference', 'Ġmay', 'Ġtake', 'Ġplace', 'Ġinclusive', 'Ġminimize', 'Ġinterference', 'Ġsignals', 'Ġintended', 'es', 'Ġwest', 'Ġrouted', 'Ġupl', 'ink', 'ed', 'Ġvia', 'meter', 'Ġdish', 'es', 'Ġameric', 'om', 'Ġmaster', 'Ġground', 'Ġstation', 'Ġhaw', 'aii', 'Ġoutside', 'Ġgalaxy', 'Ġupl', 'ink', 'Ġfootprint', 'Ġthroughout', 'Ġfailure', 'Ġdrift', 'Ġperiod', 'Ġgalaxy', 'Ġstatus', 'Ġinformation', 'Ġregarding', 'Ġcontinued', 'Ġoperation', 'Ġtwo', 'Ġl', 'band', 'Ġwide', 'Ġarea', 'Ġaug', 'mentation', 'Ġsystem', 'Ġspace', 'Ġsegment', 'Ġtrans', 'p', 'ond', 'ers', 'Ġutilized', 'Ġaircraft', 'Ġprecision', 'Ġlocation', 'Ġremained', 'Ġunknown', 'Ġprior', 'Ġrecovery', 'Ġgalaxy', 'Ġexpected', 'Ġpass', 'ars', 'Ġdegrees', 'Ġwest', 'Ġlate', 'Ġde', 'cember', 'ars', 'Ġsince', 'Ġperformed', 'Ġwa', 'Ġmission', 'Ġdegrees', 'Ġwest', 'Ġgalaxy']</t>
         </is>
       </c>
       <c r="C236" t="n">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>['ater', 'restrial', 'Ġrel', 'ays', 'Ġrocket', 'Ġstations', 'Ġgive', 'Ġworld', 'wide', 'Ġradio', 'Ġcoverage', '?"', 'Ġar', 'thur', 'Ġc', 'Ġclar', 'ke', 'Ġinstitute', 'Ġspace', 'Ġeducation', 'Ġretrieved', 'Ġjan', 'uary', 'ike', 'Ġmills', 'Ġaug', 'ust', 'orbit', 'Ġwars', 'Ġwashing', 'ton', 'Ġpost', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'ovember', 'Ġman', 'Ġbehind', 'Ġcurtain', 'Ġair', 'Ġspace', 'Ġmagazine', 'Ġretrieved', 'Ġjan', 'uary', 'Ġanat', 'oly', 'Ġz', 'ak', 'design', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġart', 'ï', '¬', 'ģ', 'cial', 'Ġsatellite', 'Ġearth', 'Ġretrieved', 'Ġjan', 'uary', 'Ġvan', 'Ġke', 'uren', 'Ġdavid', 'Ġk', 'chapter', 'Ġmoon', 'Ġeyes', 'Ġmoon', 'Ġcommunication', 'Ġrelay', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', '".', 'rica', 'rew', 'ed', '.).', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'Ġn', 'asa', 'Ġhistory', 'ï', '¬', 'ģ', 'ce', 'Ġreferences', 'Ġnotes', 'Ġcitations', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġmart', 'ald', 'erson', 'Ġp', 'aul', 'Ġbart', 'ian', 'Ġl', 'u', 'cy', 'arch', 'Ġcommunications', 'Ġsatellites', 'Ġproject', 'Ġscore', 'th', 'Ġed', '.).', 'united', 'Ġstates', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġactivities', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġannual', 'Ġreport', 'Ġcongress', 'history', 'Ġpublished', 'Ġhouse', 'Ġdocument', 'Ġnumber', 'th', 'Ġcongress', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsession', 'Ġwhite', 'Ġhouse', 'Ġfe', 'b', 'ruary', 'Ġpp', 'âĢĵ', 'Ġretrieved', 'Ġjan', 'uary', 'c', 'ou', 'rier', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'united', 'Ġstates', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġactivities', 'Ġwhite', 'Ġhouse', 'Ġjan', 'uary', 'Ġpp', 'âĢĵ', 'Ġretrieved', 'Ġjan', 'uary', 'echo', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmart', 'ald', 'erson', 'Ġp', 'aul', 'Ġbart', 'ian', 'Ġl', 'u', 'cy', 'arch', 'Ġcommunications', 'Ġsatellites', 'Ġtel', 'star', 'th', 'Ġed', '.).', 'united', 'Ġstates', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġactivities', 'Ġwhite', 'Ġhouse', 'Ġjan', 'uary', 'Ġpp', 'Ġretrieved', 'Ġjan']</t>
+          <t>['Ġperformed', 'Ġwest', 'Ġgalaxy', 'Ġlike', 'Ġmany', 'Ġcommunications', 'Ġsatellites', 'Ġreb', 'road', 'casts', 'Ġsignals', 'Ġreceives', 'Ġupl', 'ink', 'Ġfrequencies', 'Ġcorresponding', 'Ġc', 'band', 'link', 'Ġfrequencies', 'Ġtherefore', 'Ġpotential', 'Ġinterference', 'Ġexisted', 'Ġgalaxy', 'Ġdrifted', 'Ġline', 'Ġsight', 'Ġground', 'Ġupl', 'ink', 'Ġsegment', 'Ġintended', 'Ġanother', 'Ġcommunications', 'Ġsatellite', 'Ġoperating', 'Ġupl', 'ink', 'Ġfrequency', 'Ġrange', 'Ġpath', 'Ġgalaxy', 'Ġmagnitude', 'Ġinterference', 'Ġrisk', 'Ġdepended', 'Ġlarge', 'Ġnumber', 'Ġvariables', 'Ġincluding', 'Ġsize', 'Ġupl', 'ink', 'Ġantenna', 'Ġused', 'Ġlarger', 'Ġantenna', 'Ġlower', 'Ġrisk', 'Ġhit', 'Ġgalaxy', 'Ġlocation', 'Ġupl', 'ink', 'Ġwhether', 'Ġinside', 'Ġgalaxy', 'Ġfootprint', 'Ġonboard', 'Ġgain', 'Ġcapabilities', 'Ġsatellite', 'Ġprox', 'imate', 'Ġgalaxy', 'Ġsatellite', 'Ġoperators', 'Ġdevised', 'Ġvariety', 'Ġstrategies', 'Ġmitigate', 'Ġpotential', 'Ġinterference', 'Ġbirds', 'link', 'Ġtransmissions', 'Ġincluding', 'Ġtemporarily', 'Ġtransferring', 'Ġupl', 'inks', 'Ġlarger', 'Ġupl', 'ink', 'Ġantenna', 'Ġdeliberately', 'point', 'ing', 'Ġupl', 'ink', 'Ġantennas', 'Ġput', 'Ġgalaxy', 'Ġnull', 'Ġmaneuver', 'ing', 'Ġsatellite', 'Ġpassed', 'Ġmaintain', 'Ġminimum', 'Ġangular', 'Ġseparation', 'Ġincreasing', 'Ġsatellite', "'s", 'Ġgain', 'Ġsensitivity', 'Ġsettings', 'Ġallowing', 'Ġlowering', 'Ġupl', 'ink', 'Ġpower', 'Ġneeded', 'Ġlatter', 'ly', 'Ġmoving', 'Ġupl', 'ink', 'Ġlocation', 'Ġgalaxy', 'Ġupl', 'ink', 'Ġcoverage', 'e', 'Ġhaw', 'aii', 'Ġtechniques', 'Ġsuccessfully', 'Ġable', 'Ġreduce', 'Ġmitigate', 'Ġminimize', 'Ġcommercial', 'Ġsatellite', 'Ġoperations', 'Ġinterference', 'Ġpotential', 'Ġgalaxy', 'Ġfly', 'Ġsmaller', 'Ġsized', 'Ġstationary', 'Ġreceive', 'Ġsites', 'Ġlike', 'Ġused', 'ateurs', 'Ġsm', 'v', 'Ġwider', 'Ġbeam', 'Ġwidth', 'Ġreception', 'Ġpotential', 'Ġmay', 'Ġexperienced', 'Ġinterference', 'Ġpart', 'Ġcommercial', 'Ġoperators', 'Ġexperienced', 'Ġadverse', 'Ġeffects', 'Ġgalaxy', 'Ġfailure', 'Ġperiod', 'Ġthanks', 'Ġexecution', 'Ġmitigation', 'Ġpractices', 'Ġdevised', 'Ġwake', 'Ġcrisis', 'Ġsatellite', 'Ġtheor', 'ized', 'Ġlose', 'Ġattitude', 'Ġcontrol', 'Ġreaction', 'Ġwheels', 'Ġbecame', 'Ġsaturated', 'Ġevent', 'Ġoccurred', 'Ġwould', 'Ġprevent', 'Ġspacecraft', "'s", 'Ġsolar', 'Ġpanels', 'Ġtracking', 'Ġsun', 'Ġwould', 'Ġshut', 'Ġpower', 'Ġreset', 'Ġevent', 'Ġattempts', 'Ġwould', 'Ġmade', 'Ġrecover', 'Ġcontrol', 'Ġsatellite', 'Ġevent', 'Ġoriginally', 'Ġpredicted', 'Ġlate', 'Ġaug', 'ust', 'Ġearly', 'Ġse', 'pt', 'ember', 'Ġupl', 'ink', 'Ġsignal', 'Ġavoidance', 'Ġmitigation', 'Ġpower', 'Ġloss', 'Ġpredictions', 'Ġcriticism', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġint', 'els', 'Ġrevised', 'Ġestimate', 'Ġsometime', 'mber', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C237" t="n">
@@ -3519,7 +3519,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>['uary', 'Ġward', 'iam', 'Ġw', '.;', 'Ġfl', 'oyd', 'Ġfrank', 'lin', 'Ġw', 'chapter', 'Ġthirty', 'Ġyears', 'Ġspace', 'Ġcommunications', 'Ġresearch', 'Ġdevelopment', 'Ġl', 'incoln', 'Ġlaboratory', '".', 'rica', 'rew', 'ed', '.).', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'Ġn', 'asa', 'Ġhistory', 'ï', '¬', 'ģ', 'ce', 'project', 'Ġwest', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġcomp', 'endium', 'Ġsatellite', 'Ġcommunications', 'Ġprograms', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġpp', 'Ġretrieved', 'Ġjan', 'uary', 'syn', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'syn', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'les', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġcomp', 'endium', 'Ġsatellite', 'Ġcommunications', 'Ġprograms', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġpp', 'Ġretrieved', 'Ġjan', 'uary', 'Ġpel', 'ton', 'Ġj', 'ose', 'ph', 'Ġn', 'history', 'Ġsatellite', 'Ġcommunications', '".', 'Ġpel', 'ton', 'Ġj', '.;', 'Ġmad', 'ry', '.;', 'Ġcam', 'ach', 'ol', 'ara', 'eds', '.).', 'Ġhand', 'book', 'Ġsatellite', 'Ġapplications', 'Ġnew', 'ork', 'Ġspring', 'er', 'early', 'Ġbird', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġcomp', 'endium', 'Ġsatellite', 'Ġcommunications', 'Ġprograms', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġpp', 'Ġretrieved', 'Ġjan', 'uary', 'Ġn', 'asa', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġal', 'ts', 'h', 'uler', 'Ġj', 'os', 'Ã©', 'chapter', 'Ġshort', 'wave', 'Ġscatter', 'Ġsatellite', 'Ġcub', "'s", 'Ġinternational', 'Ġcommunications', '".', 'rica', 'rew', 'ed', '.).', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'Ġn', 'asa', 'Ġhistory', 'ï', '¬', 'ģ', 'ce', 'Ġman', 'n', 'uben', 'ap', 'ril', 'sky', 'tr', 'ac', 'sat', 'series', 'Ġdifferences', 'Ġstrengths', 'Ġweaknesses', 'Ġle', 'Ġgeo', 'Ġsatellites', 'Ġretrieved', 'mber', 'ad', 'c', 'Ġspace', 'Ġdebris', 'Ġmitigation', 'Ġguidelines', 'Ġinter', 'agency', 'Ġspace', 'Ġdebris', 'Ġcoordination', 'Ġcommittee', 'Ġissued', 'Ġsteering']</t>
+          <t>['Ġsubsequent', 'Ġcriticism', 'Ġactual', 'Ġscience', 'Ġbehind', 'Ġorbital', 'Ġsciences', 'Ġpredictions', 'Ġint', 'els', 'Ġcompletely', 'Ġabandoned', 'Ġpublished', 'Ġtimeline', 'Ġmethod', 'Ġinstead', 'Ġperiod', 'Ġint', 'els', 'Ġstated', 'Ġbased', 'Ġrevised', 'Ġanalysis', 'Ġestimated', 'Ġwindow', 'Ġgalaxy', 'point', 'Ġloss', 'Ġpower', 'Ġcould', 'Ġoccur', 'Ġearly', 'Ġmonth', 'Ġwithout', 'Ġclar', 'ifying', 'Ġmonth', 'Ġindicated', 'Ġhypothesis', 'Ġused', 'Ġcalculate', 'Ġtimeline', 'Ġpotential', 'Ġoccurrence', 'Ġloss', 'Ġpower', 'Ġimp', 'rec', 'ise', 'Ġdue', 'Ġfact', 'Ġsatellite', 'Ġexperienced', 'Ġerratic', 'Ġloading', 'Ġconditions', 'Ġradio', 'Ġfrequency', 'Ġsignals', 'Ġsince', 'Ġbegan', 'Ġdrift', 'Ġmonths', 'Ġinitial', 'Ġfailure', 'Ġdate', 'Ġpublished', 'Ġtimelines', 'Ġshut', 'Ġproved', 'Ġhopes', 'Ġpublic', 'Ġrelations', 'Ġcampaign', 'Ġbased', 'Ġtheory', 'Ġinterview', 'Ġconducted', 'Ġoct', 'ober', 'Ġsat', 'con', 'Ġconference', 'Ġint', 'els', 'Ġorbital', 'Ġadmitted', 'Ġhoped', 'Ġtimeline', 'Ġscenario', 'Ġtheory', 'Ġunprecedented', 'Ġsituation', 'Ġlearning', 'Ġde', 'cember', 'Ġint', 'els', 'Ġsuccessfully', 'Ġregained', 'Ġcontrol', 'Ġsatellite', 'Ġbase', 'band', 'Ġequipment', 'Ġcommand', 'Ġunit', 'Ġreset', 'Ġfollowing', 'Ġloss', 'Ġlock', 'Ġfull', 'Ġdischarge', 'Ġbatteries', 'Ġreportedly', 'Ġcritical', 'Ġphases', 'Ġrecovery', 'Ġgalaxy', 'Ġcompleted', 'Ġemergency', 'Ġcommand', 'Ġpatch', 'Ġwould', 'Ġallow', 'Ġground', 'Ġcontrollers', 'Ġgain', 'Ġaccess', 'Ġredundant', 'Ġb', 'bes', 'Ġevent', 'Ġsimilar', 'Ġfailure', 'Ġfuture', 'Ġalso', 'Ġsuccessfully', 'Ġapplied', 'Ġgalaxy', 'Ġaccording', 'Ġint', 'els', 'Ġgalaxy', 'Ġrelocated', 'Â°', 'Ġwest', 'Ġorder', 'Ġconduct', 'Ġorbit', 'Ġtesting', 'Ġviability', 'Ġpayload', 'Ġreturn', 'Ġservice', 'Ġsatellite', 'Ġgalaxy', 'Ġfully', 'Ġrecovered', 'Ġmoved', 'Ġback', 'Â°', 'Ġwest', 'Ġgalaxy', 'Ġspacecraft', 'Ġrelocated', 'Ġintended', 'Ġmission', 'Â°', 'Ġwest', 'Ġoct', 'ober', 'Ġint', 'els', 'Ġtransitioned', 'Â°', 'Ġwest', 'Ġcustomers', 'Ġback', 'Ġgalaxy', 'Ġgalaxy', 'Ġaug', 'ust', 'Ġint', 'els', 'Ġsubmitted', 'Ġfiling', 'Ġrequesting', 'Ġpermission', 'Ġsatellite', 'Ġexceed', 'Ġstation', 'Ġkeeping', 'Ġlimits', 'Ġindicating', 'Ġcontrol', 'Ġlost', 'Ġaug', 'ust', 'Ġspacecraft', 'Ġmuted', 'Ġtrans', 'p', 'onder', 'Ġpayload', 'Ġprogrammed', 'Ġautomatically', 'Ġcase', 'Ġloss', 'Ġground', 'Ġcontrol', 'Ġdays', 'Ġlast', 'Ġcommand', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġlist', 'Ġint', 'els', 'Ġsatellites', 'Ġzombie', 'Ġsatellite']</t>
         </is>
       </c>
       <c r="C238" t="n">
@@ -3532,7 +3532,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>['Ġgroup', 'Ġworking', 'Ġgroup', 'Ġse', 'pt', 'ember', 'region', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġle', 'Ġregion', 'Ġspherical', 'Ġregion', 'Ġextends', 'Ġearth', "'s", 'Ġsurface', 'Ġaltitude', 'z', '000', 'Ġflight', 'Ġlaunch', 'Ġkit', 'rian', 'esp', 'ace', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'project', 'Ġmoon', 'light', 'Ġoct', 'moon', 'light', 'Ġweb', 'inar', 'Ġmar', 'Ġhorn', 'ig', '05', '01', 'ty', 'cho', 'Ġsupporting', 'Ġpermanently', 'Ġcrew', 'ed', 'Ġlunar', 'Ġexploration', 'Ġhigh', 'speed', 'Ġoptical', 'Ġcommunication', 'Ġeverywhere', 'Ġes', 'Ġhorn', 'ig', '06', 'ty', 'cho', 'Ġmission', 'Ġearth', 'moon', 'Ġlib', 'ration', 'Ġpoint', 'ac', 'ac', 'Ġir', 'idium', 'Ġarchived', 'Ġoriginal', '08', 'Ġretrieved', '09', 'united', 'Ġstates', ')"', 'Ġretrieved', 'Ġapr', 'il', 'gs', 'ro', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'ind', 'ian', 'Ġsuccessfully', 'Ġlo', 'fts', 'Ġg', 'sat', 'Ġsatellite', 'Ġn', 'asa', 'Ġspace', 'Ġflight', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'direct', 'v', "'s", 'Ġspac', 'eway', 'Ġsatellite', 'Ġlaunches', 'Ġnew', 'Ġera', 'Ġhigh', 'de', 'ï', '¬', 'ģ', 'n', 'ition', 'Ġprogramming', 'Ġnext', 'Ġgeneration', 'Ġsatellite', 'Ġinitiate', 'Ġhistoric', 'Ġexpansion', 'Ġdirect', 'v', 'Ġspace', 'ref', 'Ġapr', 'il', 'Ġretrieved', '05', 'ind', 'ia', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'military', 'Ġsatellite', 'Ġput', 'Ġearth', "'s", 'Ġorbit', 'Ġn', 'tv', '09', '04', 'Ġretrieved', '09', 'Ġk', 'ramer', 'bert', 'Ġj', 'data', 'Ġcollection', 'mess', 'aging', 'Ġsystems', '".', 'Ġobservation', 'Ġearth', 'Ġenvironment', 'Ġber', 'lin', 'idel', 'berg', 'Ġspring', 'er', 'Ġber', 'lin', 'idel', 'berg', 'Ġpp', 'âĢĵ', 'atellite', 'Ġdata', 'Ġtele', 'communication', 'Ġhand', 'book', 'Ġlibrary', 'w', 'mo', 'int', 'Ġretrieved', 'Ġcommunications', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġinter', 'governmental', 'Ġocean', 'ographic']</t>
+          <t>['gal', 'axy', 'Ġint', 'els', 'Ġarchived', 'Ġoriginal', '08', 'Ġretrieved', 'Ġrecovery', 'Ġfailure', 'Ġrecovery', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġgalaxy', 'Ġint', 'els', 'Ġarchived', 'Ġoriginal', '07', 'Ġretrieved', '07', 'wa', 'Ġpr', 'n', 'Ġresumes', 'Ġnormal', 'Ġoperation', 'Ġg', 'Ġge', 'osp', 'atial', 'Ġworld', 'web', 'arch', 'Ġarchived', 'Ġoriginal', '07', 'Ġretrieved', '03', 'Ġrac', 'hel', 'Ġjew', 'ett', '08', 'int', 'els', 'Ġloses', 'Ġcommand', 'Ġgalaxy', 'Ġsatellite', 'Ġvia', 'Ġsatellite', 'ge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġcontrol', 'Ġsegment', 'Ġgoogle', 'Ġsearch', 'google', 'Ġretrieved', 'Ġapr', 'il', 'Ġsatellite', 'Ġdatabase', 'Ġunion', 'Ġconcerned', 'Ġscientists', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'gal', 'axy', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġmay', 'orb', 'ital', 'built', 'Ġgalaxy', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġpan', 'ams', 'Ġcompany', 'Ġlaunches', 'Ġsecond', 'Ġgalaxy', 'Ġsatellite', 'Ġpan', 'ams', 'Ġpast', 'Ġtwo', 'Ġmonths', 'business', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'cd', 'owell', 'Ġj', 'athan', 'launch', 'Ġlog', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġmay', 'Ġboost', 'Ġcivil', 'Ġmilitary', 'Ġcommunications', 'Ġsy', 'racuse', 'Ġgalaxy', 'Ġlaunch', 'Ġkit', 'rian', 'esp', 'ace', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'http', 'arian', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'cd', 'owell', 'Ġj', 'athan', 'index', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcatalog', 'Ġj', 'athan', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġfer', 'ster', 'Ġwar', 'ren', 'Ġapr', 'il', 'int', 'els', 'Ġloses', 'Ġcontact', 'Ġgalaxy', 'Ġsatellite', 'web', 'ci', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'gal', 'axy', 'eb', 'au', 'Ġretrieved', 'Ġapr', 'il', 'Ġgalaxy', 'Ġsaga', 'Ġcontinues']</t>
         </is>
       </c>
       <c r="C239" t="n">
@@ -3545,7 +3545,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>['Ġcommission', 'equ', 'ipment', 'Ġneeded', 'Ġtele', 'metry', 'Ġdata', '".', 'Ġmanual', 'Ġsea', 'Ġlevel', 'Ġmeasurement', 'Ġinterpretation', 'Ġvolume', 'Ġv', 'Ġradar', 'Ġgau', 'ges', 'unes', 'doc', 'u', 'Ġretrieved', '08', 'Ġsl', 'otten', 'Ġh', 'ugh', 'Ġr', 'Ġbeyond', 'Ġsp', 'ut', 'nik', 'Ġspace', 'Ġrace', 'Ġorigins', 'Ġglobal', 'Ġsatellite', 'Ġcommunications', 'john', 'Ġhop', 'kins', 'Ġuniversity', 'Ġpress', ');', 'Ġonline', 'Ġreview', 'Ġsatellite', 'Ġindustry', 'Ġassociation', 'ia', 'org', 'Ġcommunications', 'Ġsatellites', 'Ġshort', 'Ġhistory', 'Ġarchived', '05', 'Ġway', 'back', 'Ġmachine', 'Ġdavid', 'Ġj', 'Ġwh', 'al', 'en', 'Ġbeyond', 'Ġion', 'osphere', 'Ġfifty', 'Ġyears', 'Ġsatellite', 'Ġcommunication', 'n', 'asa', 'Ġsp', 'Ġretrieved', 'Ġreading', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġdou', 'g', 'Ġlung', 'Ġtv', 'technology', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġapr', 'il', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġapr', 'il', 'orb', 'ital', 'Ġblames', 'Ġgalaxy', 'Ġfailure', 'Ġsolar', 'Ġstorm', 'ww', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', '.,', 'Ġspace', 'Ġnews', 'Ġj', 'uly', 'Ġp', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmay', 'att', 'empt', 'Ġshut', 'Ġzombie', 'Ġsatellite', 'Ġgalaxy', 'Ġfails', 'htt', 'Ġspace', 'Ġretrieved', 'Ġmay', 'Ġhill', 'Ġje', 'ff', 'Ġmay', 'int', 'els', 'Ġwarns', 'Ġgalaxy', 'Ġmay', 'Ġdrift', 'Ġorbit', 'web', 'arch', 'iv', 'Ġsatell', 'et', 'oday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġapr', 'il', 'gal', 'axy', 'Ġstill', 'Ġad', 'rift', 'Ġposes', 'Ġthreat', 'Ġorbital', 'Ġneighbors', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'http', 'sp', 'ac', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'os', 'Ġj', 'athan', 'Ġmay', 'z', 'ombie', 'Ġsatellite', 'Ġprompts', 'Ġorbital', 'Ġw', 'alt', 'z', 'Ġnews', 'Ġretrieved', 'Ġmay', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġj', 'une', 'int', 'els', 'es', 'Ġsafely', 'Ġnegotiate', 'Ġpassage', 'Ġway', 'ward', 'Ġcraft', 'ht', 'Ġspace', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'http', 'sp', 'ac', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġj', 'uly', 'int', 'els', 'Ġaver', 'ts', 'Ġgalaxy', 'Ġinterference', 'archive', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'uly', 'Ġgalaxy', 'Ġint', 'els', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'z', 'ombies', 'Ġthreatens', 'Ġar', 'ctic', 'Ġtelecommunications', 'Ġoct', 'ober', 'Ġfallout', 'Ġgalaxy']</t>
         </is>
       </c>
       <c r="C240" t="n">
@@ -3558,7 +3558,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>['Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġlaunch', 'Ġfunction', 'Ġpartially', 'Ġreusable', 'Ġheav', 'yl', 'ift', 'Ġsuper', 'Ġheavy', 'âĢĳ', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġreusable', 'Ġmillion', ')[', 'Ġexpend', 'able', 'Ġus', 'Ġmillion', ')[', 'Ġsize', 'Ġheight', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġheavy', 'Ġpartially', 'Ġreusable', 'Ġsuper', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcarry', 'Ġcargo', 'Ġearth', 'Ġorbit', 'Ġbeyond', 'Ġdesigned', 'Ġmanufactured', 'Ġlaunched', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġspace', 'x', 'Ġrocket', 'Ġconsists', 'Ġcenter', 'Ġcore', 'Ġtwo', 'Ġfal', 'con', 'Ġboosters', 'Ġattached', 'Ġsecond', 'Ġstage', 'Ġtop', 'Ġcenter', 'Ġcore', 'Ġfal', 'con', 'Ġheavy', 'Ġsecond', 'Ġhighest', 'Ġpayload', 'Ġcapacity', 'Ġcurrently', 'Ġoperational', 'Ġlaunch', 'Ġvehicle', 'Ġbehind', 'Ġn', 'asa', "'s", 'Ġspace', 'Ġlaunch', 'Ġsystem', 'sl', 'Ġfourth', 'highest', 'Ġcapacity', 'Ġrocket', 'Ġreach', 'Ġorbit', 'Ġtrailing', 'Ġbehind', 'Ġsl', 'Ġenerg', 'ia', 'Ġsat', 'urn', 'Ġv', 'Ġspace', 'x', 'Ġconducted', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġmaiden', 'Ġlaunch', 'Ġfe', 'b', 'ruary', 'Ġdummy', 'Ġpayload', 'Ġrocket', 'Ġcarried', 'es', 'la', 'Ġroad', 'ster', 'Ġbelonging', 'Ġspace', 'x', 'Ġfounder', 'Ġel', 'Ġmus', 'k', 'Ġman', 'ne', 'quin', 'Ġdubbed', 'star', 'man', 'Ġdriver', "'s", 'Ġsecond', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġoccurred', 'Ġapr', 'il', 'Ġthree', 'Ġbooster', 'Ġrockets', 'Ġsuccessfully', 'Ġreturned', 'Ġearth', 'Ġthird', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġsuccessfully', 'Ġoccurred', 'Ġj', 'une', 'Ġsince', 'Ġfal', 'con', 'Ġheavy', 'Ġcertified', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'n', 'ssl', 'Ġprogram', 'Ġfal', 'con', 'Ġheavy', 'Ġdesigned', 'Ġable', 'Ġcarry', 'Ġhumans', 'Ġspace', 'Ġbeyond', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġalthough', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġintend', 'Ġtransport', 'Ġpeople', 'Ġfal', 'con', 'Ġheavy', 'Ġpursue', 'Ġhuman', 'rating', 'Ġcertification', 'Ġprocess', 'Ġtransport', 'Ġn', 'asa', 'Ġastronauts', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġexpected', 'Ġeventually', 'Ġsupers', 'eded', 'Ġstarship', 'Ġlaunch', 'Ġsystem', 'Ġcurrently', 'Ġdeveloped', 'Ġconcepts', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġusing', 'Ġthree', 'Ġfal', 'con', 'Ġcore', 'Ġboosters', 'Ġapproximate', 'Ġpayload', 'le', 'Ġcapacity', 'Ġtwo', 'Ġtons', 'Ġinitially', 'Ġdiscussed', 'Ġearly', 'Ġconcept', 'Ġthree', 'Ġcore', 'Ġbooster', 'Ġstages', 'Ġcompany', "'s"]</t>
+          <t>['Ġdou', 'g', 'Ġlung', 'Ġtv', 'technology', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġapr', 'il', 'Ġnational', 'Ġweather', 'Ġservice', 'c', 'data', 'Ġmanagement', 'Ġchange', 'Ġnotices', 'Ġn', 'ws', 'aa', 'gov', 'Ġn', 'ws', 'ï', '¬', 'ģ', 'ce', 'Ġchief', 'Ġinformation', 'ï', '¬', 'ģ', 'cer', 'Ġtelecommunications', 'Ġoperations', 'Ġcenter', 'Ġsilver', 'Ġspring', 'Ġjan', 'Ġ04', 'Ġrich', 'ard', 'Ġrob', 'inson', 'national', 'Ġweather', 'Ġservice', 'c', 'data', 'Ġmanagement', 'Ġchange', 'Ġnotices', 'n', 'ws', 'aa', 'gov', 'Ġretrieved', 'Ġapr', 'il', 'z', 'ombies', 'Ġthree', 'Ġsatellites', 'Ġcross', 'h', 'airs', 'gal', 'axy', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'z', 'ombie', 'Ġsatellite', 'Ġanother', 'Ġï', '¬', 'Ĥ', 'Ġl', 'ite', 'ï', '¬', 'Ĥ', 'html', 'Ġnews', 'mber', 'run', 'away', 'Ġzombie', 'Ġsatellite', 'Ġgalaxy', 'Ġcontinues', 'Ġpose', 'Ġinterference', 'Ġthreat', 'http', 'space', 'c', 'Ġspace', 'Ġoct', 'ober', 'Ġretrieved', 'Ġapr', 'il', 'Ġturned', 'Ġsatellite', 'Ġzombie', 'Ġstatic', 'Ġshock', 'Ġnews', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'Ġspace', 'Ġnews', 'Ġgalaxy', 'Ġwik', 'ipedia', 'Ġretrieved', 'Ġaug', 'ust', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C241" t="n">
@@ -3571,7 +3571,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>['yet', 'un', 'fl', 'Ġfal', 'con', 'Ġreferred', 'Ġfal', 'con', 'Ġheavy', 'Ġhistory', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdiameter', 'Ġft', 'Ġbooster', 'Ġwidth', 'Ġft', 'Ġmass', '000', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', '000', 'Ġpayload', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'Ġorbital', 'Ġinclination', 'Â°', 'Ġmass', '000', 'Ġpayload', 'Ġmars', 'Ġtransfer', 'Ġorbit', 'Ġmass', '000', 'Ġpayload', 'Ġpl', 'uto', 'Ġmass', 'Ġassociated', 'Ġrockets', 'Ġbased', 'Ġfal', 'con', 'Ġcomparable', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġnew', 'Ġgl', 'enn', 'Ġsat', 'urn', 'Ġspace', 'Ġlaunch', 'Ġsystem', 'Ġvul', 'Ġcent', 'aur', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġv', 'enberg', 'future', 'Ġtotal', 'Ġlaunches', 'Ġsuccess', 'es', 'Ġland', 'ings', 'Ġcenter', 'Ġcore', 'Ġlanded', 'lost', 'Ġsea', 'Ġattempted', 'Ġside', 'Ġboosters', 'Ġlanded', 'Ġattempted', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġbreaking', 'Ġground', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġpad', 'Ġspace', 'x', 'Ġunveiled', 'Ġplan', 'Ġfal', 'con', 'Ġheavy', 'Ġpublic', 'Ġwashing', 'ton', 'Ġnews', 'Ġconference', 'Ġapr', 'il', 'Ġinitial', 'Ġtest', 'Ġflight', 'Ġexpected', 'Ġnumber', 'Ġfactors', 'Ġdelayed', 'Ġplanned', 'Ġmaiden', 'Ġflight', 'Ġincluding', 'Ġtwo', 'Ġanomalies', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicles', 'Ġrequired', 'Ġengineering', 'Ġresources', 'Ġdedicated', 'Ġfailure', 'Ġanalysis', 'Ġhalting', 'Ġflight', 'Ġoperations', 'Ġmany', 'Ġmonths', 'Ġintegration', 'Ġstructural', 'Ġchallenges', 'Ġcombining', 'Ġthree', 'Ġfal', 'con', 'Ġcores', 'Ġmuch', 'Ġdifficult', 'Ġexpected', 'Ġj', 'uly', 'Ġel', 'Ġmus', 'k', 'Ġsaid', 'Ġactually', 'Ġended', 'Ġway', 'Ġharder', 'Ġfal', 'con', 'Ġheavy', 'Ġthought', 'Ġ...', 'Ġpretty', 'Ġnaive', '".[', 'Ġinitial', 'Ġtest', 'Ġflight', 'Ġfirst', 'Ġfal', 'con', 'Ġheavy', 'Ġlifted', 'Ġfe', 'b', 'ruary', 'Ġut', 'c', 'Ġcarrying', 'Ġdummy', 'Ġpayload', 'Ġel', 'Ġmus', 'k', "'s", 'Ġpersonal', 'es', 'la', 'Ġroad', 'ster', 'Ġbeyond', 'Ġmars', 'Ġmus', 'k', 'Ġfirst', 'Ġmentioned', 'Ġfal', 'con', 'Ġheavy', 'Ġse', 'pt', 'ember', 'Ġnews', 'Ġupdate', 'Ġreferring', 'Ġcustomer', 'Ġrequest', 'Ġmonths', 'Ġprior', 'Ġvarious', 'Ġsolutions', 'Ġusing', 'Ġplanned', 'Ġfal', 'con']</t>
+          <t>['Ġblock', 'Ġwik', 'ipedia', 'Ġblock', 'Ġartist', "'s", 'Ġimpression', 'Ġblock', 'Ġsatellite', 'Ġorbit', 'Ġmanufacturer', 'Ġbo', 'e', 'ing', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġoperator', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġapplications', 'Ġsatellite', 'Ġnavigation', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġlaunch', 'Ġmass', 'Ġpower', 'Ġwatts', 'end', 'Ġlife', 'Ġregime', 'Ġsemi', 'syn', 'chron', 'ous', 'Ġdesign', 'Ġlife', 'Ġyears', 'planned', 'Ġdimensions', 'Ġproduction', 'Ġstatus', 'Ġproduction', 'Ġcompleted', 'Ġorder', 'Ġbuilt', 'Ġlaunched', 'Ġoperational', 'Ġmaiden', 'Ġlaunch', 'Ġmay', 'Ġ03', '00', 'Ġut', 'c', 'Ġblock', 'Ġblock', 'Ġinterim', 'Ġclass', 'atellite', 'Ġused', 'Ġbridge', 'Ġgap', 'Ġprevious', 'Ġnav', 'star', 'Ġglobal', 'Ġpositioning', 'Ġsystem', 'Ġgenerations', 'Ġblock', 'Ġsatellites', 'Ġbecame', 'Ġoperational', 'Ġbuilt', 'Ġbo', 'e', 'ing', 'Ġoperated', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġlaunched', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġusing', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicles', 'Ġfinal', 'Ġcomponent', 'Ġblock', 'Ġconstellation', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġfinal', 'Ġblock', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġcompleting', 'Ġseries', 'Ġspacecraft', 'Ġmass', 'Ġdesign', 'Ġlife', 'Ġyears', 'Ġlike', 'Ġearlier', 'Ġsatellites', 'Ġblock', 'Ġspacecraft', 'Ġoperate', 'Ġsemi', 'syn', 'chron', 'ous', 'Ġmedium', 'Ġearth', 'Ġorbits', 'Ġaltitude', 'Ġapproximately', 'Ġmi', 'Ġorbital', 'Ġperiod', 'Ġtwelve', 'Ġhours', 'Ġsatellites', 'Ġsupplement', 'Ġpartially', 'Ġreplace', 'Ġblock', 'Ġsatellites', 'Ġlaunched', 'Ġdesign', 'Ġlife', 'Ġyears', 'Ġfinal', 'Ġsatellite', 'Ġblock', 'Ġseries', 'Ġdecom', 'mission', 'ed', 'Ġ09', 'Ġoct', 'ober', 'Ġoperational', 'Ġconstellation', 'Ġincludes', 'Ġblock', 'Ġvariants', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicles', 'Ġpowerful', 'Ġdelta', 'Ġused', 'Ġorbit', 'Ġearlier', 'Ġblock', 'Ġsatellites', 'Ġplace', 'Ġsatellites', 'Ġdirectly', 'Ġoperational', 'Ġorbits', 'Ġresult', 'Ġblock', 'Ġsatellites', 'Ġcarry', 'Ġap', 'gee', 'Ġkick', 'Ġmotors', 'Ġoriginal', 'Ġcontract', 'Ġblock', 'Ġsigned', 'Ġcalled', 'Ġspacecraft', 'Ġlater', 'Ġreduced', 'Ġprogram', 'Ġdelays', 'Ġtechnical', 'Ġproblems', 'Ġpushed', 'Ġfirst', 'Ġlaunch', 'Ġbroadcasting', 'safety', 'Ġlife', 'Ġnavigation', 'Ġsignal', 'Ġdemonstrated', 'Ġus', 'Ġbroadcasting', 'Ġnew', 'code', 'Ġsignal', 'Ġdoubling', 'Ġpredicted', 'Ġaccuracy', 'Ġbetter', 'Ġresistance', 'Ġjam', 'ming', 'Ġnew']</t>
         </is>
       </c>
       <c r="C242" t="n">
@@ -3584,7 +3584,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>['Ġnever', 'Ġflown', 'Ġexplored', 'Ġcost', 'effective', 'Ġreliable', 'Ġiteration', 'Ġone', 'Ġused', 'engine', 'Ġfirst', 'Ġstage', 'âĢĶ', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġheavy', 'Ġdeveloped', 'Ġprivate', 'Ġcapital', 'Ġmus', 'k', 'Ġstating', 'Ġcost', 'Ġus', 'Ġmillion', 'Ġgovernment', 'Ġfinancing', 'Ġprovided', 'Ġdevelopment', 'Ġfal', 'con', 'Ġheavy', 'Ġdesign', 'Ġbased', 'Ġfal', 'con', 'Ġfu', 'selage', 'Ġengines', 'Ġspace', 'x', 'Ġaiming', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'fal', 'con', 'Ġheavy', 'Ġwould', 'Ġcouple', 'Ġyears', '".', 'Ġspeaking', 'Ġmars', 'Ġsociety', 'Ġconference', 'Ġmus', 'k', 'Ġalso', 'Ġindicated', 'Ġexpected', 'Ġhydrogen', 'fuel', 'ed', 'Ġupper', 'Ġstage', 'Ġwould', 'Ġfollow', 'Ġtwo', 'Ġthree', 'Ġyears', 'Ġlater', 'Ġwould', 'Ġaround', ').[', 'Ġconception', 'Ġfunding', 'Ġdesign', 'Ġdevelopment', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġoct', 'ober', 'Ġboosters', 'Ġboosters', 'Ġpowered', 'Ġtotal', 'Ġmer', 'lin', 'Ġper', 'Ġbooster', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', '000', 'Ġvacuum', '000', 'Ġtotal', 'Ġthrust', 'Ġsea', 'Ġlevel', '000', 'Ġvacuum', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '05', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġchilled', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', '000', 'Ġvacuum', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '05', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġchilled', 'Ġsecond', 'Ġstage', 'Ġpowered', 'Ġmer', 'lin', 'Ġleft', 'Ġright', 'Ġfal', 'con', 'Ġfal', 'con', 'Ġthree', 'Ġversions', 'Ġfal', 'con', 'Ġthree', 'Ġversions', 'Ġfal', 'con', 'full', 'Ġthrust', 'Ġthree', 'Ġversions', 'Ġfal', 'con', 'Ġblock', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġheavy', 'Ġblock', 'Ġapr', 'il', 'Ġcapabilities', 'Ġperformance', 'Ġfal', 'con', 'Ġvehicle', 'Ġbetter', 'Ġunderstood', 'Ġspace', 'x', 'Ġcompleted', 'Ġtwo', 'Ġsuccessful', 'Ġdemonstration', 'Ġmissions', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġone', 'Ġincluded', 'Ġreign', 'ition']</t>
+          <t>['Ġcharacteristics', 'Ġblock', 'Ġwik', 'ipedia', 'Ġlast', 'Ġlaunch', 'Ġfe', 'b', 'ruary', 'Ġut', 'c', 'Ġblock', 'Ġblock', 'Ġrep', 'rogram', 'mable', 'Ġprocessors', 'Ġreceive', 'Ġsoftware', 'Ġupload', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsatellites', 'Ġselective', 'Ġavailability', 'sa', 'Ġhardware', 'Ġinstalled', 'Ġdegraded', 'Ġcivilian', 'Ġaccuracy', 'Ġturned', 'Ġoriginal', 'Ġsatellite', 'Ġï', '¬', 'Ĥ', 'e', 'et', 'Ġoverall', 'Ġblock', 'Ġsatellites', 'Ġlaunched', 'Ġcurrently', 'Ġoperational', 'Ġlaunch', 'Ġhistory', 'Ġblock', 'Ġwik', 'ipedia', 'Ġblock', 'Ġsatellites', 'Ġsatellite', 'Ġus', 'Ġdesignation', 'Ġlaunch', 'Ġdate', 'ut', 'c', 'Ġrocket', 'Ġlaunch', 'Ġsite', 'Ġstatus', 'Ġnotes', 'Ġref', 'Ġus', 'Ġmay', 'Ġ03', '00', 'Ġdelta', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġj', 'uly', 'Ġ06', 'Ġdelta', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġoct', 'ober', 'Ġdelta', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġlaunch', 'Ġcame', 'Ġshortly', 'th', 'Ġanniversary', 'Ġinaugural', 'Ġdelta', 'Ġiv', 'Ġlaunch', 'Ġus', 'Ġmay', 'las', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġfe', 'b', 'ruary', 'Ġ01', 'Ġdelta', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġmay', 'Ġ00', '03', 'Ġdelta', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġaug', 'ust', 'Ġ03', 'las', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġoct', 'ober', 'las', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġmarch', 'Ġdelta', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġj', 'uly', 'las', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġblock', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġus']</t>
         </is>
       </c>
       <c r="C243" t="n">
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>['Ġsecond', 'stage', 'Ġengine', 'Ġpress', 'Ġconference', 'Ġnational', 'Ġpress', 'Ġclub', 'Ġwashing', 'ton', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġstated', 'Ġfal', 'con', 'Ġheavy', 'Ġwould', 'carry', 'Ġpayload', 'Ġorbit', 'Ġescape', 'Ġvelocity', 'Ġvehicle', 'Ġhistory', 'Ġapart', 'Ġsat', 'urn', 'Ġmoon', 'Ġrocket', 'Ġ...', 'v', 'iet', 'Ġenerg', 'ia', 'Ġrocket', '".[', 'Ġyear', 'Ġexpected', 'Ġincrease', 'Ġdemand', 'Ġvariants', 'Ġspace', 'x', 'Ġannounced', 'Ġplans', 'Ġexpand', 'Ġmanufacturing', 'Ġcapacity', 'Ġbuild', 'Ġtowards', 'Ġcapability', 'Ġproducing', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġfal', 'con', 'Ġheavy', 'Ġside', 'Ġbooster', 'Ġevery', 'Ġweek', 'Ġupper', 'Ġstage', 'Ġevery', 'Ġtwo', 'Ġspace', 'x', 'Ġannounced', 'Ġnumber', 'Ġchanges', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġworked', 'Ġparallel', 'Ġupgrade', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġreleased', 'Ġphoto', 'Ġshowing', 'Ġfal', 'con', 'Ġheavy', 'Ġinter', 'stage', 'Ġcompany', 'Ġheadquarters', 'Ġhaw', 'th', 'orne', 'Ġcal', 'ornia', 'Ġmay', 'Ġnew', 'Ġpartly', 'Ġunderground', 'Ġtest', 'Ġstand', 'Ġbuilt', 'Ġspace', 'x', 'Ġrocket', 'Ġdevelopment', 'Ġtest', 'Ġfacility', 'Ġmc', 'greg', 'Ġtex', 'Ġspecifically', 'Ġtest', 'Ġtriple', 'Ġcores', 'Ġtwenty', 'seven', 'Ġrocket', 'Ġengines', 'Ġfal', 'con', 'Ġheavy', 'Ġmay', 'Ġspace', 'x', 'Ġconducted', 'Ġfirst', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġflight', 'design', 'Ġfal', 'con', 'Ġheavy', 'Ġcenter', 'Ġcore', 'Ġmc', 'greg', 'Ġfacility', 'Ġj', 'uly', 'Ġmus', 'k', 'Ġdiscussed', 'Ġpublicly', 'Ġchallenges', 'Ġtesting', 'Ġcomplex', 'Ġlaunch', 'Ġvehicle', 'Ġlike', 'Ġthree', 'core', 'Ġfal', 'con', 'Ġheavy', 'Ġindicating', 'Ġlarge', 'Ġextent', 'Ġnew', 'Ġdesign', 'Ġreally', 'Ġimpossible', 'Ġtest', 'Ġground', 'Ġcould', 'Ġeffectively', 'Ġtested', 'Ġindependent', 'Ġactual', 'Ġflight', 'Ġtests', 'Ġtesting', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġmaiden', 'Ġlaunch', 'Ġfal', 'con', 'Ġheavy', 'Ġse', 'pt', 'ember', 'Ġthree', 'Ġfirst', 'Ġstage', 'Ġcores', 'Ġcompleted', 'Ġstatic', 'Ġfire', 'Ġtests', 'Ġground', 'Ġtest', 'Ġstand', 'Ġfirst', 'Ġfal', 'con', 'Ġheavy', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġconducted', 'Ġjan', 'uary', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġplanning', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'Ġheavy', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġcal', 'ornia', 'Ġunited', 'Ġstates', 'Ġwest', 'Ġcoast']</t>
+          <t>['Ġoct', 'ober', 'las', 'Ġcape', 'aver', 'al', 'Ġservice', 'Ġus', 'Ġfe', 'b', 'ruary', 'las', 'Ġcape', 'aver', 'al', 'Ġservice', 'id', 'ou', 'Ġnavigation', 'Ġsatellite', 'Ġsystem', 'id', 'ou', 'comp', 'ass', 'Ġnavigation', 'Ġsystem', 'Ġgal', 'ile', 'atellite', 'Ġnavigation', 'Ġgl', 'ass', 'Ġquasi', 'zen', 'ith', 'Ġsatellite', 'Ġsystem', 'global', 'Ġpositioning', 'Ġsystem', 'Ġbo', 'e', 'ing', 'Ġretrieved', 'Ġmay', 'global', 'Ġpositioning', 'Ġsystem', 'Ġbo', 'e', 'ing', 'Ġretrieved', 'Ġmay', 'first', 'Ġblock', 'Ġsatellite', 'Ġlaunched', 'Ġneeded', 'Ġprevent', 'Ġsystem', 'Ġfailure', 'Ġdaily', 'tech', 'Ġarchived', 'Ġoriginal', 'http', 'Ġmay', 'Ġretrieved', 'Ġmay', 'fare', 'well', 'Ġgreat', 'Ġgeneration', 'Ġinside', 'Ġgn', 'ss', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġp', 'ike', 'Ġjohn', 'Ġblock', 'Ġf', 'Ġglobal', 'security', 'org', 'Ġretrieved', 'Ġmay', 'mission', 'Ġoverview', 'Ġdelta', 'Ġiv', 'Ġlaunches', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'ari', 'q', 'Ġmal', 'ik', 'Ġmay', 'air', 'Ġforce', 'Ġlaunches', 'Ġadvanced', 'Ġnew', 'Ġsatellite', 'http', 'space', 'Ġspace', 'ula', 'Ġmarks', 'Ġdelta', 'th', 'Ġanniversary', 'Ġsuccessful', 'Ġdelta', 'Ġiv', 'Ġlaunch', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġair', 'Ġforce', 'Ġdelivery', 'Ġmission', 'Ġorbit', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'uly', 'Ġretrieved', 'Ġoct', 'ober', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġblock', 'Ġwik', 'ipedia', 'united', 'Ġlaunch', 'Ġalliance', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'ula', 'las', 'Ġsets', 'Ġsail', 'Ġnew', 'Ġsatellite', 'Ġmay', 'Ġretrieved', 'Ġmay', 'orbit', 'Ġdata', 'Ġresources', 'Ġactive', 'Ġgn', 'ss', 'Ġsatellites', 'Ġworld', 'Ġretrieved', 'Ġmarch', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'th', 'Ġdelta', 'Ġiv', 'Ġmission', 'Ġcarrying', 'Ġglobal', 'Ġpositioning', 'Ġsystem', 'Ġsatellite', 'Ġu', 'Ġair', 'Ġforce', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmarch']</t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -3610,7 +3610,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>['Ġspace', 'x', 'Ġrefurb', 'ished', 'Ġlaunch', 'Ġcomplex', 'Ġv', 'enberg', 'Ġaccommodate', 'Ġfal', 'con', 'Ġheavy', 'Ġfirst', 'Ġlaunch', 'Ġcape', 'aver', 'al', 'Ġfl', 'ida', 'Ġeast', 'Ġcoast', 'Ġlaunch', 'Ġcomplex', 'Ġplanned', 'Ġlate', 'Ġdue', 'Ġpartly', 'Ġfailure', 'Ġspace', 'x', 'Ġj', 'une', 'Ġspace', 'x', 'Ġres', 'ched', 'uled', 'Ġmaiden', 'Ġfal', 'con', 'Ġheavy', 'Ġflight', 'Ġse', 'pt', 'ember', 'Ġoccur', 'Ġearlier', 'Ġapr', 'il', 'Ġflight', 'Ġlaunched', 'Ġrefurb', 'ished', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġlaunch', 'Ġcomplex', 'Ġflight', 'Ġpostponed', 'Ġlate', 'Ġearly', 'Ġsummer', 'Ġlate', 'Ġfinally', 'Ġfe', 'b', 'ruary', 'Ġj', 'uly', 'Ġmeeting', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġresearch', 'Ġdevelopment', 'Ġmeeting', 'Ġwashing', 'ton', 'Ġmus', 'k', 'played', 'Ġexpectations', 'Ġsuccess', 'Ġmaiden', 'Ġflight', "'s", 'Ġreal', 'Ġgood', 'Ġchance', 'Ġvehicle', "'t", 'Ġmake', 'Ġorbit', 'Ġ...', 'Ġhope', 'Ġmakes', 'Ġfar', 'Ġenough', 'Ġaway', 'Ġpad', 'Ġcause', 'Ġpad', 'Ġdamage', 'Ġwould', 'Ġconsider', 'Ġeven', 'Ġwin', 'Ġhonest', 'Ġde', 'cember', 'Ġmus', 'k', 'Ġtweeted', 'Ġdummy', 'Ġpayload', 'Ġmaiden', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġwould', 'Ġpersonal', 'es', 'la', 'Ġroad', 'ster', 'Ġplaying', 'Ġdavid', 'Ġbow', 'ie', "'s", 'space', 'Ġodd', 'ity', 'though', 'Ġsong', 'Ġactually', 'Ġused', 'Ġlaunch', 'life', 'Ġmars', '"),', 'Ġwould', 'Ġlaunched', 'Ġorbit', 'Ġaround', 'Ġsun', 'Ġreach', 'Ġorbit', 'Ġmars', 'Ġreleased', 'Ġpictures', 'Ġfollowing', 'Ġdays', 'Ġcar', 'Ġthree', 'Ġcameras', 'Ġattached', 'Ġprovide', 'ep', 'ic', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġheavy', 'Ġmoved', 'Ġlaunch', 'Ġpad', 'Ġpreparation', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġengines', 'Ġexpected', 'Ġjan', 'uary', 'Ġhowever', 'Ġdue', 'Ġu', 'Ġgovernment', 'Ġshutdown', 'Ġbegan', 'Ġjan', 'uary', 'Ġtesting', 'Ġlaunch', 'Ġdelayed', 'Ġstatic', 'Ġfire', 'Ġtest', 'Ġconducted', 'Ġjan', 'uary', 'Ġmus', 'k', 'Ġconfirmed', 'Ġvia', 'Ġtwitter', 'Ġtest', 'Ġgood', 'Ġlater', 'Ġannounced', 'Ġrocket', 'Ġwould', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġfe', 'b', 'ruary', 'Ġdelay', 'Ġtwo', 'Ġhours', 'Ġdue', 'Ġhigh', 'Ġwinds']</t>
+          <t>['six', 'th', 'Ġspacecraft', 'Ġlaunches', 'Ġinside', 'Ġgn', 'ss', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'ins', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'bo', 'e', 'ing', 'Ġsatellite', 'Ġlaunch', 'Ġschedule', 'Ġbo', 'e', 'ing', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'las', 'Ġlaunch', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġaug', 'ust', 'las', 'Ġsuccessfully', 'Ġv', 'aults', 'Ġsatellite', 'Ġorbit', 'Ġfl', 'ida', 'Ġtoday', 'Ġaug', 'ust', 'Ġretrieved', 'Ġoct', 'ober', 'notice', 'Ġadvisory', 'Ġnav', 'star', 'Ġusers', 'nan', 'u', 'Ġunited', 'Ġstates', 'Ġcoast', 'Ġguard', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'united', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġmarch', 'las', 'Ġlaunch', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'new', 'Ġsatellite', 'Ġbegins', 'Ġtransmitting', 'Ġusers', 'Ġaround', 'Ġglobe', 'Ġretrieved', 'Ġmarch', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C245" t="n">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>['Ġfal', 'con', 'Ġheavy', 'Ġlifted', 'Ġside', 'Ġboosters', 'Ġlanded', 'Ġsafely', 'Ġlanding', 'Ġzones', 'Ġminutes', 'Ġlater', 'Ġhowever', 'Ġone', 'Ġthree', 'Ġengines', 'Ġcenter', 'Ġbooster', 'Ġintended', 'Ġrestart', 'Ġignited', 'Ġdescent', 'Ġcausing', 'Ġbooster', 'Ġdestroyed', 'Ġupon', 'Ġimpacting', 'Ġocean', 'Ġspeed', 'Ġmph', ').[', 'Ġinitially', 'Ġel', 'Ġmus', 'k', 'Ġtweeted', 'Ġroad', 'ster', 'shot', 'Ġplanned', 'Ġhel', 'oc', 'entric', 'Ġorbit', 'Ġwould', 'Ġreach', 'Ġasteroid', 'Ġbelt', 'Ġlater', 'Ġobservations', 'Ġtelescopes', 'Ġshowed', 'Ġroad', 'ster', 'Ġwould', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġbuilt', 'Ġfal', 'con', 'Ġblock', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġlaunch', 'Ġpad', 'Ġj', 'une', 'Ġslightly', 'Ġexceed', 'Ġorbit', 'Ġmars', 'Ġap', 'hel', 'ion', 'Ġyear', 'Ġsuccessful', 'Ġdemo', 'Ġflight', 'Ġspace', 'x', 'Ġsigned', 'Ġfive', 'Ġcommercial', 'Ġcontracts', 'Ġworth', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġmeaning', 'Ġmanaged', 'Ġcover', 'Ġdevelopment', 'Ġcost', 'Ġrocket', 'Ġsecond', 'Ġflight', 'Ġfirst', 'Ġcommercial', 'Ġone', 'Ġoccurred', 'Ġapr', 'il', 'Ġlaunching', 'Ġar', 'abs', 'Ġthree', 'Ġboosters', 'Ġlanding', 'Ġsuccessfully', 'Ġfirst', 'Ġtime', 'Ġthird', 'Ġflight', 'Ġoccurred', 'Ġj', 'une', 'Ġlaunching', 'od', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġpayload', 'Ġpayload', 'Ġcomposed', 'Ġsmall', 'Ġspacecraft', 'Ġoperational', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġmissions', 'Ġint', 'els', 'ars', 'Ġplanned', 'Ġlate', 'Ġmoved', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġrocket', 'Ġversion', 'Ġbecome', 'Ġpowerful', 'Ġenough', 'Ġlift', 'Ġheavy', 'Ġpayload', 'Ġexpend', 'able', 'Ġj', 'une', 'Ġu', 'Ġspace', 'Ġforce', 'Ġcertified', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunching', 'Ġtop', 'Ġsecret', 'Ġsatellites', 'Ġfirst', 'Ġlaunch', 'Ġus', 'sf', 'Ġhappened', 'mber', 'Ġsecond', 'Ġus', 'sf', 'Ġlaunched', 'Ġweeks', 'Ġus', 'sf', 'Ġv', 'ias', 'Ġselected', 'Ġfal', 'con', 'Ġheavy', 'Ġlate', 'Ġlaunching', 'Ġv', 'ias', 'Ġsatellite', 'Ġscheduled', 'Ġlaunch', 'âĢĵ', 'Ġtimeframe', 'Ġhowever', 'Ġwould', 'Ġlaunch', 'Ġmay']</t>
+          <t>['ars', 'Ġwik', 'ipedia', 'ars', 'Ġglobal', 'Ġtype', 'Ġsubsidiary', 'Ġindustry', 'Ġsatellite', 'Ġcommunication', 'Ġfounded', 'Ġheadquarters', 'Ġl', 'ondon', 'Ġeng', 'land', 'Ġkey', 'Ġpeople', 'rew', 'Ġsu', 'k', 'aw', 'chair', 'Ġperson', 'Ġr', 'aj', 'ee', 'v', 'Ġsur', 'ce', 'Ġrevenue', 'Ġus', 'Ġmillion', ')[', 'Ġoperating', 'Ġincome', 'Ġus', 'Ġmillion', ')[', 'Ġnet', 'Ġincome', 'Ġus', 'Ġmillion', ')[', 'Ġnumber', 'Ġemployees', ')[', 'Ġparent', 'Ġv', 'ias', 'Ġwebsite', 'ars', 'ars', 'ars', 'Ġsatellite', 'ars', 'ars', 'Ġb', 'rit', 'ish', 'Ġsatellite', 'Ġtelecommunications', 'Ġcompany', 'Ġoffering', 'Ġglobal', 'Ġmobile', 'Ġservices', 'Ġprovides', 'Ġtelephone', 'Ġdata', 'Ġservices', 'Ġusers', 'Ġworldwide', 'Ġvia', 'Ġportable', 'Ġmobile', 'Ġterminals', 'Ġcommunicate', 'Ġground', 'Ġstations', 'Ġfourteen', 'Ġge', 'ost', 'ation', 'ary', 'Ġtelecommunications', 'Ġsatellites', 'ars', "'s", 'Ġnetwork', 'Ġprovides', 'Ġcommunications', 'Ġservices', 'Ġrange', 'Ġgovernments', 'Ġaid', 'Ġagencies', 'Ġmedia', 'Ġoutlets', 'Ġbusinesses', 'especially', 'Ġshipping', 'Ġairline', 'Ġmining', 'Ġindustries', 'Ġneed', 'Ġcommunicate', 'Ġremote', 'Ġregions', 'Ġreliable', 'Ġterrestrial', 'Ġnetwork', 'Ġcompany', 'Ġlisted', 'Ġl', 'ondon', 'Ġstock', 'Ġexchange', 'Ġacquired', 'Ġconnect', 'Ġbid', 'co', 'Ġconsortium', 'Ġconsisting', 'Ġpartners', 'Ġwar', 'burg', 'Ġp', 'inc', 'us', 'Ġinvestment', 'Ġboard', 'Ġont', 'ario', 'Ġteachers', 'Ġpension', 'Ġplan', 'Ġde', 'cember', 'mber', 'Ġdeal', 'Ġannounced', 'ars', "'s", 'Ġowners', 'Ġv', 'ias', 'Ġv', 'ias', 'Ġpurchase', 'ars', 'Ġacquisition', 'Ġcompleted', 'Ġmay', 'Ġpresent', 'Ġcompany', 'Ġorigin', 'ates', 'Ġinternational', 'Ġmaritime', 'Ġsatellite', 'Ġorganization', 'ars', 'Ġnon', 'profit', 'Ġinter', 'governmental', 'Ġorganisation', 'Ġestablished', 'Ġbehest', 'Ġinternational', 'Ġmaritime', 'Ġorganization', 'imo', ')âĢĶ', 'Ġunited', 'Ġnations', 'Ġmaritime', 'Ġbody', 'âĢĶ', 'Ġpursuant', 'Ġconvention', 'Ġinternational', 'Ġmaritime', 'Ġsatellite', 'Ġorganization', 'Ġsigned', 'Ġcountries', 'Ġorganisation', 'Ġcreated', 'Ġestablish', 'Ġoperate', 'Ġsatellite', 'Ġcommunications', 'Ġnetwork', 'Ġmaritime', 'Ġcommunity', 'Ġcoordination', 'Ġinternational', 'Ġcivil', 'Ġaviation', 'Ġorganization', 'Ġconvention', 'Ġgoverning', 'ars', 'Ġamended', 'Ġinclude', 'Ġimprovements', 'Ġaer', 'autical', 'Ġcommunications']</t>
         </is>
       </c>
       <c r="C246" t="n">
@@ -3636,7 +3636,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>['Ġoct', 'ober', 'Ġfal', 'con', 'Ġheavy', 'Ġembarked', 'th', 'Ġflight', 'Ġcarrying', 'Ġn', 'asa', 'Ġsatellite', 'Ġps', 'cy', 'Ġasteroid', 'Ġmission', 'Ġside', 'Ġboosters', 'Ġreturn', 'Ġearth', 'Ġcenter', 'Ġcore', 'Ġexpended', 'Ġdecision', 'Ġmade', 'Ġcreate', 'Ġtoler', 'able', 'Ġmargins', 'Ġmission', 'Ġfollowing', 'Ġannouncement', 'Ġn', 'asa', "'s", 'Ġart', 'emis', 'Ġprogram', 'Ġreturning', 'Ġhumans', 'Ġmoon', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġmentioned', 'Ġseveral', 'Ġtimes', 'Ġalternative', 'Ġexpensive', 'Ġspace', 'Ġlaunch', 'Ġsystem', 'sl', 'Ġprogram', 'Ġn', 'asa', 'Ġdecided', 'Ġexclusively', 'Ġuse', 'Ġsl', 'Ġlaunch', 'ion', 'Ġcapsule', 'Ġhowever', 'Ġfal', 'con', 'Ġheavy', 'Ġsupport', 'Ġcommercial', 'Ġmissions', 'Ġart', 'emis', 'Ġprogram', 'Ġsince', 'Ġused', 'Ġtransport', 'Ġdragon', 'Ġspacecraft', 'Ġlunar', 'Ġgateway', 'Ġalso', 'Ġselected', 'Ġlaunch', 'Ġfirst', 'Ġtwo', 'Ġelements', 'Ġlunar', 'Ġgateway', 'Ġpower', 'Ġpropulsion', 'Ġelement', 'ppe', 'Ġhabit', 'ation', 'Ġlogistics', 'Ġoutpost', 'h', 'alo', 'Ġsingle', 'Ġlaunch', 'mber', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġrover', 'Ġaboard', 'Ġast', 'rob', 'otic', 'Ġtechnology', "'s", 'Ġgr', 'iffin', 'Ġland', 'er', 'Ġpart', 'Ġart', 'emis', 'Ġprogram', "'s", 'Ġcommercial', 'Ġlunar', 'Ġpayload', 'Ġservices', 'cl', 'ps', 'Ġinitiative', 'Ġfal', 'con', 'Ġheavy', 'Ġconsists', 'Ġstruct', 'urally', 'Ġstrengthened', 'Ġfal', 'con', 'core', 'Ġcomponent', 'Ġtwo', 'Ġadditional', 'Ġfal', 'con', 'Ġfirst', 'Ġstages', 'Ġaer', 'odynamic', 'Ġnose', 'âĢĵ', 'con', 'es', 'Ġmounted', 'board', 'Ġserving', 'Ġstrap', 'Ġboosters', 'Ġconcept', 'ually', 'Ġsimilar', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlauncher', 'Ġproposals', 'las', 'Ġheavy', 'Ġr', 'ussian', 'Ġang', 'ara', 'Ġtriple', 'Ġfirst', 'Ġstage', 'Ġcarries', 'Ġstandard', 'Ġfal', 'con', 'Ġsecond', 'Ġstage', 'Ġturn', 'Ġcarries', 'Ġpayload', 'Ġfair', 'ing', 'Ġfal', 'con', 'Ġheavy', 'Ġsecond', 'Ġhighest', 'Ġlift', 'Ġcapability', 'Ġoperational', 'Ġrocket', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', '000', 'Ġtrans', 'ars', 'Ġinjection', 'Ġrocket', 'Ġdesigned', 'Ġmeet', 'Ġexceed', 'Ġcurrent', 'Ġrequirements', 'Ġhuman', 'Ġrating', 'Ġstructural', 'Ġsafety', 'Ġmargins', 'Ġlater', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġdesign', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġpad', 'Ġmer', 'lin', 'Ġengine', 'Ġflight', 'Ġloads', 'Ġhigher', 'Ġmargins', 'Ġrockets', 'Ġfal', 'con']</t>
+          <t>['Ġnotably', 'Ġpublic', 'Ġmember', 'Ġstates', 'Ġowned', 'Ġvarying', 'Ġshares', 'Ġoperational', 'Ġbusiness', 'Ġmain', 'Ġoffices', 'Ġoriginally', 'Ġlocated', 'Ġe', 'ust', 'Ġtower', 'Ġe', 'ust', 'Ġroad', 'Ġl', 'ondon', 'Ġhistory', 'Ġorigins', 'Ġprivatization', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġsatellite', 'Ġtelephone', 'Ġuse', 'Ġnatural', 'Ġdisaster', 'Ġn', 'ias', 'Ġind', 'ones', 'ia', 'Ġunit', 'Ġdepicted', 'Ġmanufactured', 'Ġthr', 'ane', 'Ġthr', 'ane', 'Ġden', 'mark', 'ap', 'ril', 'Ġmid', 'Ġmany', 'Ġmember', 'Ġstates', 'Ġunwilling', 'Ġinvest', 'Ġimprovements', 'ars', "'s", 'Ġnetwork', 'Ġespecially', 'Ġowing', 'Ġcompetitive', 'Ġnature', 'Ġsatellite', 'Ġcommunications', 'Ġindustry', 'Ġmany', 'Ġrecognised', 'Ġneed', 'Ġmaintain', 'Ġorganisation', "'s", 'Ġolder', 'Ġsystems', 'Ġneed', 'Ġinter', 'governmental', 'Ġorganisation', 'Ġoversee', 'Ġpublic', 'Ġsafety', 'Ġaspects', 'Ġsatellite', 'Ġcommunication', 'Ġnetworks', 'Ġagreement', 'Ġreached', 'Ġmodify', 'ars', "'s", 'Ġmission', 'Ġinter', 'governmental', 'Ġorganisation', 'Ġseparate', 'Ġprivat', 'ise', 'Ġorganisation', "'s", 'Ġoperational', 'Ġbusiness', 'Ġpublic', 'Ġsafety', 'Ġobligations', 'Ġattached', 'Ġapr', 'il', 'ars', 'Ġsucceeded', 'Ġinternational', 'Ġmobile', 'Ġsatellite', 'Ġorganization', 'im', 'Ġinter', 'governmental', 'Ġregulatory', 'Ġbody', 'Ġsatellite', 'Ġcommunications', 'ars', "'s", 'Ġoperational', 'Ġunit', 'Ġseparated', 'Ġbecame', 'Ġu', 'k', 'based', 'Ġcompany', 'ars', 'Ġim', 'ars', 'Ġsigned', 'Ġagreement', 'Ġimposing', 'Ġpublic', 'Ġsafety', 'Ġobligations', 'Ġnew', 'Ġcompany', 'ars', 'Ġfirst', 'Ġinternational', 'Ġsatellite', 'Ġorganisation', 'Ġprivat', 'ised', 'Ġpartners', 'Ġperm', 'ira', 'Ġbought', 'Ġshares', 'Ġcompany', 'Ġcompany', 'Ġalso', 'Ġfirst', 'Ġlisted', 'Ġl', 'ondon', 'Ġstock', 'Ġexchange', 'Ġyear', 'Ġmarch', 'Ġdisclosed', 'Ġu', 'Ġhedge', 'Ġfund', 'Ġharb', 'inger', 'Ġcapital', 'Ġowned', 'Ġcompany', 'ars', 'Ġcompleted', 'Ġacquisition', 'Ġsatellite', 'Ġcommunications', 'Ġprovider', 'Ġstrat', 'os', 'Ġglobal', 'Ġcorporation', 'str', 'atos', ')[', 'Ġacquired', 'per', 'Ġcent', 'Ġstake', 'Ġsky', 'wave', 'Ġmobile', 'Ġcommunications', 'Ġinc', '.,', 'Ġprovider', 'ars', 'Ġnetwork', 'Ġservices', 'Ġturn', 'Ġpurchased', 'Ġglobal', 'wave', 'Ġbusiness', 'Ġtrans', 'core', 'ars', 'Ġmacro', 'bert', 'Ġaward', 'Ġbroadband', 'Ġglobal', 'Ġarea', 'Ġnetwork', 'Ġservice', 'ars']</t>
         </is>
       </c>
       <c r="C247" t="n">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>['Ġheavy', 'Ġdesigned', 'Ġoutset', 'Ġcarry', 'Ġhumans', 'Ġspace', 'Ġwould', 'Ġrestore', 'Ġpossibility', 'Ġflying', 'Ġcrew', 'ed', 'Ġmissions', 'Ġmoon', 'Ġmars', 'Ġfirst', 'Ġstage', 'Ġpowered', 'Ġthree', 'Ġfal', 'con', 'Ġderived', 'Ġcores', 'Ġequipped', 'Ġnine', 'Ġmer', 'lin', 'Ġengines', 'Ġfal', 'con', 'Ġheavy', 'Ġtotal', 'Ġsea', 'level', 'Ġthrust', 'Ġlif', 'ff', '000', 'Ġmer', 'lin', 'Ġengines', 'Ġthrust', 'Ġrises', '000', 'Ġcraft', 'Ġclimbs', 'Ġatmosphere', 'Ġupper', 'Ġstage', 'Ġpowered', 'Ġsingle', 'Ġmer', 'lin', 'Ġengine', 'Ġmodified', 'Ġvacuum', 'Ġoperation', 'Ġthrust', 'Ġkn', '000', 'Ġexpansion', 'Ġratio', 'Ġnominal', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġlaunch', 'Ġcenter', 'Ġcore', 'Ġthrott', 'les', 'Ġfull', 'Ġpower', 'Ġseconds', 'Ġadditional', 'Ġthrust', 'Ġthrott', 'les', 'Ġallows', 'Ġlonger', 'Ġburn', 'Ġtime', 'Ġside', 'Ġboosters', 'Ġseparate', 'Ġcenter', 'Ġcore', 'Ġthrott', 'les', 'Ġback', 'Ġmaximum', 'Ġthrust', 'Ġadded', 'Ġreliability', 'Ġrestart', 'Ġengine', 'Ġdual', 'Ġredundant', 'Ġpy', 'roph', 'oric', 'Ġign', 'ers', 'te', 'te', 'b', ').[', 'Ġinter', 'stage', 'Ġconnects', 'Ġupper', 'Ġlower', 'Ġstage', 'Ġfal', 'con', 'Ġcarbon', 'Ġfiber', 'Ġaluminum', 'Ġcore', 'Ġcomposite', 'Ġstructure', 'Ġstage', 'Ġseparation', 'Ġoccurs', 'Ġvia', 'Ġreusable', 'Ġseparation', 'Ġcol', 'lets', 'Ġp', 'ne', 'umatic', 'Ġpus', 'Ġsystem', 'Ġfal', 'con', 'Ġtank', 'Ġwalls', 'Ġdom', 'es', 'Ġmade', 'Ġaluminium', 'âĢĵ', 'l', 'ith', 'ium', 'Ġalloy', 'Ġspace', 'x', 'Ġuses', 'f', 'riction', 'Ġstir', 'Ġweld', 'ed', 'Ġtank', 'Ġsecond', 'Ġstage', 'Ġtank', 'Ġfal', 'con', 'Ġsimply', 'Ġshorter', 'Ġversion', 'Ġfirst', 'Ġstage', 'Ġtank', 'Ġuses', 'Ġtool', 'ing', 'Ġmaterial', 'Ġmanufacturing', 'Ġtechniques', 'Ġapproach', 'Ġreduces', 'Ġmanufacturing', 'Ġcosts', 'Ġvehicle', 'Ġproduction', 'Ġthree', 'Ġcores', 'Ġfal', 'con', 'Ġheavy', 'Ġarrange', 'Ġengines', 'Ġstructural', 'Ġform', 'Ġspace', 'x', 'Ġcalls', 'Ġoct', 'aw', 'eb', 'Ġaimed', 'Ġstream', 'lining', 'Ġmanufacturing', 'Ġprocess', 'Ġcore', 'Ġincludes', 'Ġfour', 'Ġext', 'ensible', 'Ġlanding', 'Ġcontrol', 'Ġdescent', 'Ġboosters', 'Ġcenter', 'Ġcore', 'Ġatmosphere', 'Ġspace', 'x', 'Ġuses', 'Ġfour', 'Ġretract', 'able', 'Ġgrid', 'Ġfins', 'Ġtop', 'Ġthree', 'Ġfal', 'con', 'Ġboosters', 'Ġextend', 'Ġseparation', 'Ġimmediately', 'Ġside', 'Ġboosters', 'Ġseparate', 'Ġcenter', 'Ġengine', 'Ġburns', 'Ġseconds', 'Ġorder', 'Ġcontrol', 'Ġbooster', "'s", 'Ġtrajectory', 'Ġsafely', 'Ġaway', 'Ġrocket', 'Ġgrid', 'Ġfins', 'Ġdeploy']</t>
+          <t>['Ġfirst', 'Ġprovided', 'Ġservices', 'Ġusing', 'Ġmar', 'cs', 'Ġlaunched', 'Ġus', 'Ġnavy', 'Ġes', 'Ġrespectively', 'Ġearly', 'ars', 'Ġlaunched', 'Ġfirst', 'Ġdedicated', 'Ġsatellite', 'Ġconstellation', 'ars', 'Ġsatellites', 'Ġprovided', 'ars', 'Ġservice', 'Ġmaritime', 'Ġuses', 'ars', "'s", 'Ġsecond', 'Ġconstellation', 'ars', 'Ġlaunched', 'Ġconsisting', 'Ġfive', 'Ġge', 'ost', 'ation', 'ary', 'Ġl', 'band', 'Ġsatellites', 'Ġconstellation', 'Ġprovides', 'ars', 'b', 'ars', 'c', 'Ġservices', 'Ġprimarily', 'Ġproviding', 'Ġlow', 'Ġbandwidth', 'Ġcommunications', 'Ġsafety', 'Ġservices', 'Ġglobal', 'Ġshipping', 'Ġfollowing', 'Ġprivat', 'isation', 'ars', 'Ġdeveloped', 'Ġlaunched', 'Ġfirst', 'Ġsatellite', 'Ġcommunications', 'Ġsystem', 'Ġoffering', 'Ġglobal', 'Ġcoverage', 'Ġservice', 'Ġprovided', 'Ġinitially', 'Ġthree', 'ars', 'Ġsatellite', 'Ġlaunched', 'Ġextended', 'Ġaddition', 'Ġal', 'phas', 'ars', 'Ġbegan', 'Ġdevelopment', 'Ġhigh', 'Ġthroughput', 'Ġsatellite', 'h', 'ts', 'Ġconstellation', 'Ġglobal', 'Ġx', 'press', 'Ġoperating', 'Ġka', 'band', 'Ġportion', 'Ġspectrum', 'Ġglobal', 'Ġx', 'press', 'Ġlaunched', 'Ġoffers', 'Ġglobal', 'Ġsatellite', 'Ġcapacity', 'Ġvarious', 'Ġmarkets', 'Ġincluding', 'Ġshipping', 'Ġaviation', 'Ġglobal', 'Ġx', 'press', 'Ġalso', 'Ġmarks', 'Ġsignificant', 'Ġexpansion', 'ars', "'s", 'Ġcommercial', 'Ġoperations', 'Ġaviation', 'Ġmarkets', 'ars', 'Ġlaunched', 'Ġfirst', 'band', 'Ġsatellite', 'Ġintended', 'Ġprovide', 'Ġassociation', 'Ġl', 'te', 'Ġground', 'Ġnetwork', 'Ġinf', 'light', 'Ġinternet', 'Ġaccess', 'Ġacross', 'Ġeuro', 'pe', 'Ġmarch', 'ars', 'Ġpartnered', 'Ġisot', 'rop', 'ic', 'Ġsystems', 'Ġdevelop', 'Ġstate', 'art', 'Ġelectronic', 'Ġscanning', 'Ġantenna', 'Ġintended', 'Ġused', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'ars', 'Ġwik', 'ipedia', 'Ġse', 'pt', 'ember', 'ars', 'Ġannounced', 'Ġstrategic', 'Ġcollaboration', 'Ġpan', 'asonic', 'Ġav', 'ionics', 'Ġcorporation', 'Ġinitial', 'Ġten', 'year', 'Ġperiod', 'Ġprovide', 'flight', 'Ġbroadband', 'Ġcommercial', 'Ġairlines', 'ars', 'Ġexclusive', 'Ġprovider', 'Ġpan', 'asonic', 'Ġconnectivity', 'Ġusing', 'Ġka', 'band', 'Ġsatellite', 'Ġsignal', 'ars', 'Ġoffering', 'Ġpan', 'asonic', "'s", 'Ġportfolio', 'Ġservices']</t>
         </is>
       </c>
       <c r="C248" t="n">
@@ -3662,7 +3662,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>['Ġboosters', 'Ġturn', 'Ġback', 'Ġearth', 'Ġfollowed', 'Ġlanding', 'Ġlegs', 'Ġbooster', 'Ġlands', 'Ġsoftly', 'Ġground', 'Ġfully', 'Ġreusable', 'Ġlaunch', 'Ġconfiguration', 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġland', 'Ġdifferent', 'Ġdrone', 'Ġships', 'Ġpartial', 'Ġreusable', 'Ġconfiguration', 'Ġcenter', 'Ġcore', 'Ġcontinues', 'Ġfire', 'Ġstage', 'Ġseparation', 'Ġfully', 'Ġreusable', 'Ġlaunches', 'Ġgrid', 'Ġfins', 'Ġlegs', 'Ġdeploy', 'Ġcenter', 'Ġcore', 'Ġtouches', 'Ġeither', 'Ġback', 'Ġland', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdrone', 'Ġship', 'Ġstages', 'Ġexpended', 'Ġlanding', 'Ġlegs', 'Ġgrid', 'Ġfins', 'Ġomitted', 'Ġvehicle', 'Ġlanding', 'Ġlegs', 'Ġmade', 'Ġcarbon', 'Ġfiber', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġstructure', 'Ġfour', 'Ġlegs', 'Ġst', 'ow', 'Ġalong', 'Ġsides', 'Ġcore', 'Ġlif', 'ff', 'Ġextend', 'Ġoutward', 'Ġlanding', 'Ġfal', 'con', 'Ġheavy', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġcharacteristics', 'hide', 'Ġcharacteristic', 'Ġfirst', 'Ġstage', 'Ġcore', 'Ġunit', 'Ġcenter', 'Ġbooster', 'Ġsecond', 'Ġstage', 'Ġpayload', 'Ġfair', 'ing', 'Ġheight', 'Ġft', 'Ġft', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġft', 'Ġft', 'Ġdry', 'Ġmass', '000', 'Ġfueled', 'Ġmass', '000', '000', 'Ġstructure', 'Ġtype', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġtank', 'Ġmon', 'oco', 'que', 'Ġfuel', 'Ġtank', 'Ġskin', 'Ġstr', 'inger', 'Ġmon', 'oco', 'que', 'Ġhalves', 'Ġstructure', 'Ġmaterial', 'Ġaluminum', 'âĢĵ', 'l', 'ith', 'ium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġaluminum', 'âĢĵ', 'l', 'ith', 'ium', 'Ġskin', 'Ġaluminum', 'Ġdom', 'es', 'Ġcarbon', 'Ġï', '¬', 'ģ', 'ber', 'Ġengines', 'Ġmer', 'lin', 'Ġmer', 'lin', 'Ġvacuum', 'Ġengine', 'Ġtype', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġliquid', 'Ġgas', 'Ġgenerator', 'Ġpropell', 'ant', 'Ġsub', 'cool', 'ed', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġk', 'eros', 'ene', 'Ġliquid', 'Ġtank', 'Ġcapacity', '000', '000', 'Ġk', 'eros', 'ene', 'Ġtank', 'Ġcapacity', '000', '000', 'Ġengine', 'Ġnozzle', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġg', 'imb', 'aled', 'Ġexpansion', 'Ġengine', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġthrust', 'Ġstage', 'Ġtotal', '000', 'Ġsea', 'Ġlevel']</t>
+          <t>['Ġcommercial', 'Ġaviation', 'Ġcustomers', 'Ġmarch', 'Ġmal', 'ays', 'ia', 'Ġairlines', 'Ġflight', 'Ġdisappeared', 'Ġpassengers', 'Ġcrew', 'Ġen', 'Ġroute', 'Ġk', 'uala', 'Ġlump', 'ur', 'ijing', 'Ġturning', 'Ġaway', 'Ġplanned', 'Ġpath', 'Ġdisappearing', 'Ġradar', 'Ġcoverage', 'Ġaircraft', "'s", 'Ġsatellite', 'Ġdata', 'Ġunit', 'Ġremained', 'Ġcontact', 'ars', "'s", 'Ġground', 'Ġstation', 'Ġper', 'th', 'Ġvia', 'Ġsatellite', 'ind', 'ian', 'Ġocean', 'Ġregion', 'Â°', 'Ġeast', 'Ġaircraft', 'Ġused', 'ars', "'s", 'Ġclassic', 'ero', 'Ġsatellite', 'Ġphone', 'Ġservice', 'Ġanalysis', 'Ġcommunications', 'ars', 'Ġindependently', 'Ġagencies', 'Ġdetermined', 'Ġaircraft', 'Ġflew', 'Ġsouthern', 'Ġind', 'ian', 'Ġocean', 'Ġused', 'Ġguide', 'Ġsearch', 'Ġaircraft', 'Ġmarch', 'Ġcompany', "'s", 'Ġboard', 'Ġagreed', 'Ġrecommend', 'Ġtakeover', 'Ġoffer', 'Ġbillion', 'Ġconnect', 'Ġbid', 'co', 'Ġconsortium', 'Ġconsisting', 'Ġpartners', 'Ġwar', 'burg', 'Ġp', 'inc', 'us', 'Ġinvestment', 'Ġboard', 'Ġont', 'ario', 'Ġteachers', 'Ġpension', 'Ġplan', 'Ġoct', 'ober', 'Ġbloom', 'berg', 'Ġreported', 'Ġgovernment', 'Ġset', 'Ġapprove', 'Ġtakeover', 'Ġfinal', 'Ġconsultation', 'Ġdeal', 'Ġset', 'Ġconclude', 'Ġoct', 'ober', 'mber', 'ars', 'Ġrejected', 'Ġele', 'venth', 'hour', 'Ġeffort', 'Ġderail', 'Ġbillion', 'Ġsale', 'Ġaccused', 'Ġignoring', 'Ġpotential', 'Ġboost', 'Ġcompany', "'s", 'Ġvalue', 'Ġoak', 'tree', 'Ġargued', 'Ġrecommended', 'Ġoffer', 'ars', 'Ġfailed', 'Ġtake', 'Ġaccount', 'Ġpotential', 'Ġvalue', 'Ġspectrum', 'Ġassets', 'Ġused', 'ars', "'s", 'Ġu', 'Ġpartner', 'Ġlig', 'ado', 'ars', 'Ġdel', 'isted', 'Ġl', 'ondon', 'Ġstock', 'Ġexchange', 'Ġprivate', 'Ġequity', 'Ġfunds', 'Ġtook', 'Ġcontrol', 'Ġcompany', 'Ġde', 'cember', 'Ġtime', 'ars', 'Ġoperating', 'Ġge', 'ost', 'ation', 'ary', 'Ġcommunications', 'Ġsatellites', 'mber', 'Ġdeal', 'Ġannounced', 'ars', "'s", 'Ġowners', 'Ġled', 'Ġwar', 'burg', 'Ġp', 'inc', 'us', 'Ġv', 'ias', 'Ġv', 'ias', 'Ġwould', 'Ġpurchase', 'ars', 'Ġcash', 'Ġissuing', 'Ġapproximately', 'Ġmillion', 'Ġshares', 'Ġv', 'ias', 'Ġstock', 'Ġtaking', 'Ġv', 'ias', 'Ġpromised', 'Ġhonour', 'Ġpledge', 'Ġmade', 'Ġprevious', 'Ġowners', 'Ġtaken', 'Ġprivate', 'ars', 'Ġwould', 'Ġremain', 'Ġu', 'k', 'based', 'Ġcompany', 'Ġplanned', 'Ġinvestments', 'Ġprovisional']</t>
         </is>
       </c>
       <c r="C249" t="n">
@@ -3675,7 +3675,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>['Ġkn', '000', 'Ġvacuum', 'Ġpropell', 'ant', 'Ġfeed', 'Ġsystem', 'Ġturb', 'op', 'ump', 'Ġturb', 'op', 'ump', 'Ġthrottle', 'Ġcapability', 'Ġyes', 'âĢĵ', 'Ġkn', '000', 'âĢĵ', '000', 'Ġsea', 'Ġlevel', 'Ġyes', 'âĢĵ', 'Ġkn', '000', 'âĢĵ', '000', 'Ġvacuum', 'Ġrestart', 'Ġcapability', 'Ġyes', 'Ġengines', 'Ġboost', 'back', 'entry', 'Ġlanding', 'Ġyes', 'Ġdual', 'Ġredundant', 'Ġtea', 'te', 'b', 'Ġpy', 'roph', 'oric', 'Ġign', 'ers', 'Ġtank', 'Ġpress', 'ur', 'ization', 'Ġheated', 'Ġhelium', 'Ġheated', 'Ġhelium', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġpitch', 'aw', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġg', 'imb', 'aled', 'Ġengine', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġascent', 'Ġattitude', 'Ġcontrol', 'Ġroll', 'Ġg', 'imb', 'aled', 'Ġengines', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġcoast', 'des', 'cent', 'Ġattitude', 'Ġcontrol', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġnitrogen', 'Ġgas', 'Ġthr', 'usters', 'Ġshutdown', 'Ġprocess', 'Ġcommanded', 'Ġcommanded', 'Ġstage', 'Ġseparation', 'Ġsystem', 'Ġp', 'ne', 'umatic', 'Ġp', 'ne', 'umatic', 'Ġrocket', 'Ġspecifications', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġtwenty', 'seven', 'Ġmer', 'lin', 'Ġengines', 'Ġï', '¬', 'ģ', 'ring', 'Ġlaunch', 'Ġar', 'abs', 'Ġfal', 'con', 'Ġheavy', 'Ġuses', 'Ġft', 'Ġinter', 'stage', 'Ġattached', 'Ġfirst', 'Ġstage', 'Ġcore', 'Ġcomposite', 'Ġstructure', 'Ġconsisting', 'Ġaluminum', 'Ġhoney', 'comb', 'Ġcore', 'Ġsurrounded', 'Ġcarbon', 'Ġfiber', 'Ġface', 'Ġsheet', 'Ġpl', 'ies', 'Ġunlike', 'Ġfal', 'con', 'Ġblack', 'Ġthermal', 'Ġprotection', 'Ġlayer', 'Ġinter', 'stage', 'Ġblock', 'Ġcenter', 'Ġcore', 'Ġboosters', 'Ġlater', 'Ġpainted', 'Ġwhite', 'Ġseen', 'Ġfal', 'con', 'Ġheavy', 'Ġflights', 'Ġfar', 'Ġprobably', 'Ġdue', 'Ġast', 'hetics', 'Ġfal', 'con', 'Ġheavy', 'Ġlogo', 'Ġproviding', 'Ġgrey', 'ish', 'Ġoverall', 'Ġlength', 'Ġvehicle', 'Ġlaunch', 'Ġft', 'Ġtotal', 'Ġfueled', 'Ġmass', '000', 'Ġwithout', 'Ġrecovery', 'Ġstage', 'Ġfal', 'con', 'Ġheavy', 'Ġinject', '000', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', '000', 'Ġven', 'us', 'Ġmars', 'Ġfal', 'con', 'Ġheavy', 'Ġincludes', 'Ġfirst', 'stage', 'Ġrecovery', 'Ġsystems', 'Ġallow', 'Ġspace', 'x', 'Ġreturn', 'Ġfirst', 'Ġstage', 'Ġboosters', 'Ġlaunch', 'Ġsite', 'Ġwell', 'Ġrecover', 'Ġfirst', 'Ġstage', 'Ġcore', 'Ġfollowing', 'Ġlanding', 'Ġautonomous', 'Ġspac', 'eport', 'Ġdrone', 'Ġship', 'Ġb', 'arge', 'Ġcompletion', 'Ġprimary', 'Ġmission', 'Ġrequirements', 'Ġsystems', 'Ġinclude', 'Ġfour', 'Ġdeploy', 'able', 'Ġlanding', 'Ġlegs', 'Ġlocked', 'Ġfirst', 'stage', 'Ġtank', 'Ġcore', 'Ġascent', 'Ġdeploy', 'Ġprior', 'Ġtouchdown', 'Ġexcess', 'Ġpropell', 'ant', 'Ġreserved', 'Ġfal', 'con', 'Ġheavy']</t>
+          <t>['Ġapproval', 'Ġmerger', 'Ġgiven', 'Ġcompetition', 'Ġmarkets', 'Ġauthority', 'Ġmarch', 'Ġmay', 'Ġset', 'Ġdate', 'Ġformal', 'Ġdecision', 'Ġmay', 'Ġacquisition', 'Ġclosed', 'ars', 'Ġhead', 'Ġoffice', 'Ġold', 'Ġstreet', 'Ġround', 'Ġl', 'ondon', 'Ġborough', 'lington', 'Ġaside', 'Ġcommercial', 'Ġservices', 'ars', 'Ġprovides', 'Ġglobal', 'Ġmaritime', 'Ġdistress', 'Ġsafety', 'Ġsystem', 'g', 'md', 'ss', 'Ġships', 'Ġaircraft', 'Ġcharge', 'Ġpublic', 'Ġservice', 'Ġmal', 'ays', 'ia', 'Ġairlines', 'Ġflight', 'Ġtakeover', 'Ġconnect', 'Ġbid', 'co', 'Ġprivat', 'isation', 'Ġacquisition', 'Ġv', 'ias', 'Ġoperations', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġglobal', 'Ġcity', 'Ġroad', 'Ġl', 'ondon', 'jan', 'uary', 'Ġservices', 'Ġinclude', 'Ġtraditional', 'Ġvoice', 'Ġcalls', 'Ġlow', 'level', 'Ġdata', 'Ġtracking', 'Ġsystems', 'Ġhigh', 'speed', 'Ġinternet', 'Ġdata', 'Ġservices', 'Ġwell', 'Ġdistress', 'Ġsafety', 'Ġservices', 'Ġbroadband', 'Ġglobal', 'Ġarea', 'Ġnetwork', 'Ġnetwork', 'Ġprovides', 'Ġgeneral', 'Ġpacket', 'Ġradio', 'Ġservice', 'g', 'pr', 'Ġtype', 'Ġservices', 'Ġk', 'bit', 'Ġlatency', 'Ġvia', 'Ġinternet', 'Ġprotocol', 'Ġsatellite', 'Ġmodem', 'Ġsize', 'Ġnotebook', 'Ġcomputer', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġoffers', 'bit', 'Ġlatency', 'Ġvia', 'Ġantennas', 'Ġsmall', 'Ġservices', 'Ġprovide', 'Ġmobile', 'Ġintegrated', 'Ġservices', 'Ġdigital', 'Ġnetwork', 'isd', 'n', 'Ġservices', 'Ġused', 'Ġmedia', 'Ġlive', 'Ġreporting', 'Ġworld', 'Ġevents', 'Ġvia', 'Ġvide', 'ophone', 'Ġinf', 'light', 'Ġinternet', 'Ġaccess', 'Ġvia', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġprice', 'Ġcall', 'Ġvia', 'ars', 'Ġdropped', 'Ġlevel', 'Ġcomparable', 'Ġmany', 'Ġcases', 'Ġlower', 'Ġinternational', 'Ġroaming', 'Ġcosts', 'Ġhotel', 'Ġphone', 'Ġcalls', 'Ġvoice', 'Ġcall', 'Ġcharges', 'Ġlocation', 'Ġworld', 'Ġservice', 'Ġused', 'Ġtariffs', 'Ġcalls', 'ars', 'Ġcountry', 'Ġcodes', 'Ġvary', 'Ġdepending', 'Ġcountry', 'Ġplaced', 'ars', 'Ġprimarily', 'Ġuses', 'Ġcountry', 'Ġcode', 'see', ').[', 'Ġnewer', 'ars', 'Ġservices', 'Ġuse', 'Ġtechnology', 'Ġfeatures', 'Ġalways', 'Ġcapability', 'Ġusers', 'Ġcharged', 'Ġamount', 'Ġdata', 'Ġsend', 'Ġreceive', 'Ġrather', 'Ġlength', 'Ġtime', 'Ġconnected', 'Ġaddition']</t>
         </is>
       </c>
       <c r="C250" t="n">
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>['Ġfirst', 'stage', 'Ġrecovery', 'Ġoperations', 'Ġdiverted', 'Ġuse', 'Ġprimary', 'Ġmission', 'Ġobjective', 'Ġrequired', 'Ġensuring', 'Ġsufficient', 'Ġperformance', 'Ġmargins', 'Ġsuccessful', 'Ġmissions', 'Ġnominal', 'Ġpayload', 'Ġcapacity', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', '000', 'Ġrecovery', 'Ġthree', 'Ġfirst', 'stage', 'Ġcores', 'Ġprice', 'Ġper', 'Ġlaunch', 'Ġmillion', 'Ġversus', '000', 'Ġfully', 'Ġexpend', 'able', 'Ġmode', 'Ġfal', 'con', 'Ġheavy', 'Ġalso', 'Ġinject', '000', 'Ġpayload', 'Ġg', 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġrecovered', 'Ġpartially', 'Ġreusable', 'Ġfal', 'con', 'Ġheavy', 'Ġfalls', 'Ġheavy', 'lift', 'Ġrange', 'Ġlaunch', 'Ġsystems', 'Ġcapable', 'Ġlifting', 'âĢĵ', '000', 'âĢĵ', '000', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġclassification', 'Ġsystem', 'Ġused', 'Ġn', 'asa', 'Ġhuman', 'Ġspace', 'flight', 'Ġreview', 'Ġpanel', 'Ġfully', 'Ġexpend', 'able', 'Ġfal', 'con', 'Ġheavy', 'Ġsuper', 'Ġheavy', 'lift', 'Ġcategory', 'Ġmaximum', 'Ġpayload', '000', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġinitial', 'Ġconcept', 'fal', 'con', 'Ġenvisioned', 'Ġpayload', 'Ġle', 'Ġapr', 'il', 'Ġprojected', '000', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', 'Ġpayload', '000', 'Ġlater', 'Ġreports', 'Ġprojected', 'Ġhigher', 'Ġpayload', 'Ġbeyond', 'Ġle', 'Ġincluding', '000', 'Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', '000', 'Ġtransl', 'un', 'ar', 'Ġtrajectory', '000', 'Ġtrans', 'mart', 'ian', 'Ġorbit', 'Ġmars', 'Ġlate', 'Ġspace', 'x', 'Ġraised', 'Ġprojected', 'Ġg', 'Ġpayload', 'Ġfal', 'con', 'Ġheavy', '000', 'Ġapr', 'il', 'Ġprojected', 'Ġle', 'Ġpayload', 'Ġfal', 'con', 'Ġheavy', 'Ġraised', '000', '000', 'Ġmaximum', 'Ġpayload', 'Ġachieved', 'Ġrocket', 'Ġflies', 'Ġfully', 'Ġexpend', 'able', 'Ġlaunch', 'Ġprofile', 'Ġrecovering', 'Ġthree', 'Ġfirst', 'stage', 'Ġboosters', 'Ġcore', 'Ġbooster', 'Ġexpended', 'Ġtwo', 'Ġside', 'boost', 'ers', 'Ġrecovered', 'Ġmus', 'k', 'Ġestimates', 'Ġpayload', 'Ġpenalty', 'Ġaround', '%,', 'Ġwould', 'Ġstill', 'Ġyield', '000', 'Ġlift', 'Ġcapability', 'Ġreturning', 'Ġthree', 'Ġboosters', 'Ġlaunch', 'Ġsite', 'Ġrather', 'Ġlanding', 'Ġdrone', 'Ġships', 'Ġwould', 'Ġyield', 'Ġpayload']</t>
+          <t>['Ġsatellites', 'ars', 'Ġcollaboration', 'Ġagreement', 'ces', 'Ġregarding', 'Ġhandheld', 'Ġvoice', 'Ġservices', 'Ġthree', 'Ġtypes', 'Ġcoverage', 'Ġrelated', 'ars', 'Ġsatellite', 'Ġsatellite', 'Ġequipped', 'Ġsingle', 'Ġglobal', 'Ġbeam', 'Ġcovers', 'Ġone', 'third', 'Ġearth', "'s", 'Ġsurface', 'Ġapart', 'Ġpoles', 'Ġoverall', 'Ġglobal', 'Ġbeam', 'Ġcoverage', 'Ġextends', 'Ġlat', 'itudes', 'ĠâĪĴ', 'Â°', 'Ġregardless', 'Ġlong', 'itude', 'Ġregional', 'Ġbeam', 'Ġcovers', 'Ġfraction', 'Ġarea', 'Ġcovered', 'Ġglobal', 'Ġbeam', 'Ġcollectively', 'Ġregional', 'Ġbeams', 'Ġoffer', 'Ġvirtually', 'Ġcoverage', 'Ġglobal', 'Ġbeams', 'Ġuse', 'Ġregional', 'Ġbeams', 'Ġallow', 'Ġuser', 'Ġterminals', 'also', 'Ġcalled', 'Ġmobile', 'Ġearth', 'Ġstations', 'Ġoperate', 'Ġsignificantly', 'Ġsmaller', 'Ġantennas', 'Ġregional', 'Ġbeams', 'Ġintroduced', 'Ġsatellites', 'Ġsatellite', 'Ġprovides', 'Ġfour', 'Ġspot', 'Ġbeams', 'Ġsatellite', 'Ġprovides', 'Ġregional', 'Ġbeams', 'Ġnarrow', 'Ġbeams', 'Ġoffered', 'Ġthree', 'ars', 'Ġsatellites', 'Ġnarrow', 'Ġbeams', 'Ġvary', 'Ġsize', 'Ġtend', 'Ġseveral', 'Ġhundred', 'Ġkilometres', 'Ġacross', 'Ġnarrow', 'Ġbeams', 'Ġmuch', 'Ġsmaller', 'Ġglobal', 'Ġregional', 'Ġbeams', 'Ġfar', 'Ġnumerous', 'Ġhence', 'Ġoffer', 'Ġglobal', 'Ġcoverage', 'Ġnarrow', 'Ġspot', 'Ġbeams', 'Ġallow', 'Ġyet', 'Ġcoverage', 'Ġglobal', 'Ġbeam', 'Ġcoverage', 'Ġregional', 'Ġspot', 'Ġbeam', 'Ġcoverage', 'Ġnarrow', 'Ġspot', 'Ġbeam', 'Ġcoverage', 'ars', 'Ġwik', 'ipedia', 'Ġsmaller', 'Ġantennas', 'Ġmuch', 'Ġhigher', 'Ġdata', 'Ġrates', 'Ġform', 'Ġbackbone', 'ars', "'s", 'Ġhandheld', 'gs', 'ps', 'Ġbroadband', 'Ġservices', 'Ġcoverage', 'Ġintroduced', 'Ġsatellites', 'Ġsatellite', 'Ġprovides', 'Ġaround', 'Ġnarrow', 'Ġspot', 'Ġbeams', 'ars', 'Ġsatellites', 'Ġprovide', 'Ġglobal', 'Ġcoverage', 'Ġusing', 'Ġfour', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellites', 'Ġsatellite', 'Ġsupports', 'Ġbeams', 'Ġgiving', 'Ġtotal', 'Ġcoverage', 'Ġapproximately', 'Ġone', 'third', 'Ġearth', "'s", 'Ġsurface', 'Ġper', 'Ġsatellite', 'Ġaddition', 'Ġsteer', 'able', 'Ġbeams', 'Ġavailable', 'Ġper', 'Ġsatellite', 'Ġmay', 'Ġmoved', 'Ġprovide', 'Ġhigher', 'Ġcapacity', 'Ġselected', 'Ġlocations', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġwik', 'ipedia', 'Ġsatellite', 'mber', 'Ġfirst', 'Ġsatellite', 'Ġextend', 'Ġoriginal', 'Ġsatellite', 'Ġfirst', 'Ġgeneration', 'Ġglobal', 'Ġx', 'press', 'Ġconstellation', 'Ġlaunched', 'Ġcentre', 'Ġspatial', 'Ġguy', 'ana', 'ri', 'ane', 'Ġlaunch', 'Ġvehicle', 'Ġsatellite', 'Ġcoverage', 'Ġlong', 'itude', 'Ġvehicles', 'Ġlaunch', 'Ġdate', 'ut', 'c', 'Ġservices', 'Ġnotes', 'Ġmar', 'Ġseries', 'Ġmar', 'Ġdelta', 'Ġfe', 'b', 'ruary', 'Ġdecom', 'mission', 'ed', 'Ġmar']</t>
         </is>
       </c>
       <c r="C251" t="n">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>['Ġcapabilities', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġlong', 'Ġexposure', 'Ġnight', 'Ġlaunch', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġreusable', 'Ġside', 'Ġboosters', 'Ġland', 'Ġunison', 'Ġcape', 'aver', 'al', 'Ġlanding', 'Ġzones', 'Ġfollowing', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfe', 'b', 'ruary', 'Ġmaximum', 'Ġtheoretical', 'Ġpayload', 'Ġcapacity', 'Ġdestination', 'Ġfal', 'con', 'Ġheavy', 'Ġfal', 'con', 'Ġaug', 'ust', 'Ġapr', 'il', 'Ġmay', 'Ġmarch', 'Ġsince', 'Ġapr', 'il', 'Ġle', 'Â°', 'Ġexpend', 'able', 'Ġg', 'Â°', 'Ġexpend', 'able', 'Ġg', 'Â°', 'Ġreusable', 'Ġmars', 'Ġpl', 'uto', 'Ġspace', 'x', 'Ġconducted', 'Ġparallel', 'Ġdevelopment', 'Ġreusable', 'Ġrocket', 'Ġarchitecture', 'Ġfal', 'con', 'Ġapplies', 'Ġparts', 'Ġfal', 'con', 'Ġheavy', 'Ġwell', 'Ġearly', 'Ġspace', 'x', 'Ġexpressed', 'Ġhopes', 'Ġrocket', 'Ġstages', 'Ġwould', 'Ġeventually', 'Ġreusable', 'Ġspace', 'x', 'Ġsince', 'Ġdemonstrated', 'Ġroutine', 'Ġland', 'Ġsea', 'Ġrecovery', 'Ġfal', 'con', 'Ġfirst', 'Ġstage', 'Ġsuccessfully', 'Ġrecovered', 'Ġmultiple', 'Ġpayload', 'Ġfair', 'ings', 'Ġcase', 'Ġfal', 'con', 'Ġheavy', 'Ġtwo', 'Ġouter', 'Ġcores', 'Ġseparate', 'Ġrocket', 'Ġearlier', 'Ġflight', 'Ġthus', 'Ġmoving', 'Ġlower', 'Ġvelocity', 'Ġfal', 'con', 'Ġlaunch', 'Ġprofile', 'Ġfirst', 'Ġflight', 'Ġfal', 'con', 'Ġheavy', 'Ġspace', 'x', 'Ġconsidered', 'Ġattempting', 'Ġrecover', 'Ġsecond', 'Ġstage', 'Ġexecute', 'Ġplan', 'Ġfal', 'con', 'Ġheavy', 'Ġpayload', 'Ġperformance', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', 'Ġreduced', 'Ġreusable', 'Ġtechnology', 'Ġmuch', 'Ġlower', 'Ġprice', 'Ġrecovering', 'Ġthree', 'Ġbooster', 'Ġcores', 'Ġg', 'Ġpayload', '000', 'Ġtwo', 'Ġoutside', 'Ġcores', 'Ġrecovered', 'Ġcenter', 'Ġcore', 'Ġexpended', 'Ġg', 'Ġpayload', 'Ġwould', 'Ġapproximately', '000', 'Ġcomparison', 'Ġnext', 'av', 'iest', 'Ġcontemporary', 'Ġrocket', 'Ġfully', 'Ġexpend', 'able', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġdeliver', '000', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginally', 'Ġdesigned', 'Ġunique', 'pro', 'pell', 'ant', 'Ġcross', 'feed', 'Ġcapability', 'Ġwhereby', 'Ġcenter', 'Ġcore', 'Ġengines', 'Ġwould', 'Ġsupplied', 'Ġfuel', 'Ġoxid', 'izer', 'Ġtwo', 'Ġside', 'Ġcores', 'Ġseparation', 'Ġoperating', 'Ġengines', 'Ġfull']</t>
+          <t>['Ġdelta', 'Ġoct', 'ober', 'Ġtransferred', 'Ġint', 'els', 'Ġdecom', 'mission', 'ed', 'Ġmar', 'Ġdelta', 'Ġj', 'une', 'Ġdecom', 'mission', 'ed', 'cs', 'Ġseries', 'cs', 'ri', 'ane', 'Ġde', 'cember', 'Ġde', 'activated', 'Ġaug', 'ust', 'cs', 'b', 'ri', 'ane', 'Ġse', 'pt', 'ember', 'Ġlaunch', 'Ġfailure', 'cs', 'c', 'ri', 'ane', 'mber', 'Ġalso', 'Ġknown', 'cs', 'b', 'Ġde', 'activated', 'ars', 'Ġseries', 'ars', 'Ġdelta', 'Ġoct', 'ober', 'Ġdecom', 'mission', 'ed', 'Ġapr', 'il', 'Ġprevious', 'Ġrecord', 'Ġholder', 'Ġmission', 'Ġlifespan', 'ars', 'Ġdelta', 'Ġmarch', 'Ġdecom', 'mission', 'ed', 'Ġde', 'cember', 'Ġsatellites', 'ars', 'Ġwik', 'ipedia', 'Ġworld', 'Ġrecord', 'Ġmission', 'Ġlifespan', 'ars', 'ri', 'ane', 'Ġde', 'cember', 'Ġdecom', 'mission', 'ed', 'ars', 'ri', 'ane', 'Ġapr', 'il', 'Ġdecom', 'mission', 'ed', 'ars', 'Ġseries', 'ars', 'las', 'Ġapr', 'il', 'Ġreass', 'igned', 'Ġmaritime', 'Ġsafety', 'Ġbackup', 'Ġservice', 'ars', 'Ġpro', 'ton', 'k', 'dm', 'Ġse', 'pt', 'ember', 'Ġreass', 'igned', 'Ġmaritime', 'Ġsafety', 'Ġbackup', 'Ġservice', 'ars', 'Â°', 'Ġeast', 'las', 'Ġde', 'cember', 'Ġexisting', 'Ġevolved', 'Ġservices', 'ars', 'ri', 'ane', 'Ġj', 'une', 'Ġdecom', 'mission', 'ed', 'ars', 'Â°', 'Ġwest', 'ri', 'ane', 'Ġfe', 'b', 'ruary', 'Ġvarious', 'Ġleases', 'ars', 'Ġseries', 'ars', 'Ġap', 'ac', 'Â°', 'Ġeast', 'las', 'Ġmarch', 'Ġfamily', 'Ġsp', 'Ġlease', 'Ġservices', 'ars', 'Â°', 'Ġeast', 'Ġz', 'en', 'sl', 'mber', 'Ġfamily', 'Ġsp', 'Ġlease', 'Ġservices', 'Ġfleet', 'broad', 'band', 'Ġswift', 'broad', 'band', 'Ġtransferred', 'Â°', 'Ġeast', 'Â°', 'Ġeast', 'Ġmid', 'ars', 'mer', 'Â°', 'Ġwest', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġaug', 'ust', 'Ġfamily', 'Ġlease', 'Ġservices', 'ars', 'al', 'phas', ')[', 'Ġem', 'ea', 'Â°', 'Ġeast', 'ri', 'ane']</t>
         </is>
       </c>
       <c r="C252" t="n">
@@ -3714,7 +3714,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>['Ġthrust', 'Ġlaunch', 'Ġfuel', 'Ġsupplied', 'Ġmainly', 'Ġside', 'Ġboosters', 'Ġwould', 'Ġde', 'plete', 'Ġside', 'Ġboosters', 'Ġsooner', 'Ġallowing', 'Ġearlier', 'Ġseparation', 'Ġreduce', 'Ġmass', 'Ġaccelerated', 'Ġwould', 'Ġleave', 'Ġcenter', 'Ġcore', 'Ġpropell', 'ant', 'Ġavailable', 'Ġbooster', 'Ġseparation', 'us', 'ability', 'Ġpropell', 'ant', 'Ġcross', 'feed', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġmus', 'k', 'Ġstated', 'Ġcross', 'feed', 'Ġwould', 'Ġimplemented', 'Ġinstead', 'Ġcenter', 'Ġbooster', 'Ġthrott', 'les', 'Ġshortly', 'Ġlif', 'ff', 'Ġconserve', 'Ġfuel', 'Ġresumes', 'Ġfull', 'Ġthrust', 'Ġside', 'Ġboosters', 'Ġseparated', 'Ġscience', 'Ġfocus', 'Ġfe', 'b', 'ruary', 'Ġpublished', 'Ġarticle', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġenvironmental', 'Ġimpact', 'Ġstated', 'Ġconcerns', 'Ġfrequent', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġcontribute', 'Ġpollution', 'Ġatmosphere', 'Ġplanetary', 'Ġsociety', 'Ġconcerned', 'Ġlaunching', 'Ġnon', 'ster', 'ile', 'Ġobject', 'Ġdone', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġflight', 'Ġinter', 'plan', 'etary', 'Ġspace', 'Ġmay', 'Ġrisk', 'Ġbiological', 'Ġcontamination', 'Ġforeign', 'Ġscientists', 'Ġpur', 'due', 'Ġuniversity', 'Ġthought', 'irt', 'iest', 'Ġman', 'made', 'Ġobject', 'Ġever', 'Ġsent', 'Ġspace', 'Ġterms', 'Ġbacteria', 'Ġamount', 'Ġnoting', 'Ġcar', 'Ġpreviously', 'Ġdriven', 'Ġlos', 'Ġangel', 'es', 'Ġfre', 'eways', 'Ġalthough', 'Ġvehicle', 'Ġsteril', 'ized', 'Ġsolar', 'Ġradiation', 'Ġtime', 'Ġbacteria', 'Ġmight', 'Ġsurvive', 'Ġpieces', 'Ġplastic', 'Ġcould', 'Ġcontam', 'inate', 'Ġmars', 'Ġdistant', 'Ġfuture', 'Ġstudy', 'Ġconducted', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġfound', 'Ġboost', 'back', 'Ġlanding', 'Ġfal', 'con', 'Ġheavy', 'Ġboosters', 'would', 'Ġsignificantly', 'Ġaffect', 'Ġquality', 'Ġhuman', 'Ġenvironment', '".[', 'Ġappearance', 'Ġmay', 'Ġunited', 'Ġstates', 'Ġsenate', 'Ġcommittee', 'Ġcommerce', 'Ġscience', 'Ġtransportation', 'Ġmus', 'k', 'Ġtestified', 'long', 'Ġterm', 'Ġplans', 'Ġcall', 'Ġdevelopment', 'Ġheavy', 'Ġlift', 'Ġproduct', 'Ġeven', 'Ġsuper', 'heavy', 'Ġcustomer', 'Ġdemand', 'Ġexpect', 'Ġsize', 'Ġincrease', 'Ġwould', 'Ġresult', 'Ġmeaningful', 'Ġdecrease', 'Ġcost', 'Ġper', 'Ġpound', 'Ġorbit', 'Ġ...', 'Ġultimately', 'Ġbelieve', 'Ġus', 'Ġper', 'Ġpound', 'Ġless', 'Ġachievable', '".[', 'kg', 'Ġ($', 'lb', 'Ġgoal', 'Ġstated', 'Ġmus', 'k', 'Ġcost', 'Ġle', 'cap', 'able', 'Ġlaunch', 'Ġsystem', 'Ġstudy', 'Ġz', 'en', 'Ġmedium', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcould', 'Ġcarry', '000', 'Ġle', 'Ġus', 'âĢĵ']</t>
+          <t>['eca', 'Ġj', 'uly', 'Ġfamily', 'Ġsp', 'Ġlease', 'Ġservices', 'ars', 'Ġseries', 'ars', 'Ġeuro', 'pe', 'Ġmiddle', 'Ġeast', 'Ġaf', 'rica', 'Â°', 'Ġeast', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġde', 'cember', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġameric', 'Â°', 'Ġwest', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġfe', 'b', 'ruary', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'ia', 'Ġwest', 'Ġameric', 'Â°', 'Ġeast', 'Ġpro', 'ton', 'Ġbri', 'z', 'Ġaug', 'ust', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġeuro', 'pe', 'orbit', 'Ġspare', 'Â°', 'Ġeast', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmay', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'ars', 'Ġeuro', 'pe', 'Ġmiddle', 'Ġeast', 'Â°', 'Ġeast', 'ri', 'ane', 'eca', 'mber', 'Ġka', 'band', 'Ġglobal', 'Ġdata', 'Ġservices', 'Ġhigher', 'Ġcapacity', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġgeneration', 'Ġsatellites', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'ars', 'Ġe', 'hell', 'Ġsat', ')[', 'Ġeuro', 'pe', 'Â°', 'Ġeast', 'ri', 'ane', 'Ġj', 'une', 'band', 'Ġservices', 'Ġeuro', 'pe', 'Ġaviation', 'ars', 'Ġseries', 'ars', 'Ġf', 'Ġde', 'cember', 'ars', 'Ġfal', 'con', 'Ġblock', 'Ġfe', 'b', 'ruary', 'Ġpermanent', 'Ġtelephone', 'Ġcountry', 'Ġcode', 'Ġcalling', 'ars', 'Ġdestinations', 'Ġsn', 'ac', 'single', 'Ġnetwork', 'Ġaccess', 'Ġcode', 'Ġnumber', 'Ġautomatic', 'Ġloc', 'ator', 'Ġnecessary', 'Ġknow', 'Ġsatellite', 'Ġdestination', 'ars', 'Ġterminal', 'Ġlogged', 'Ġsn', 'ac', 'Ġusable', 'ars', 'Ġservices', 'Ġcountry', 'Ġcodes', 'Ġphased', 'Ġde', 'cember', 'l', 'antic', 'Ġocean', 'Ġregion', 'Ġeast', 'e', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġocean', 'Ġregion', 'por', 'Ġind', 'ian', 'Ġocean', 'Ġregion', 'ior', 'l', 'antic', 'Ġocean', 'Ġregion', 'Ġwest', 'Ġcountry', 'Ġcodes']</t>
         </is>
       </c>
       <c r="C253" t="n">
@@ -3727,7 +3727,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>['Ġmillion', 'Ġspace', 'x', 'Ġstated', 'Ġcost', 'Ġreaching', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcould', 'Ġlow', 'kg', 'Ġ($', '000', 'lb', 'Ġannual', 'Ġrate', 'Ġfour', 'Ġlaunches', 'Ġsustained', 'Ġplanned', 'Ġeventually', 'Ġlaunch', 'Ġmany', 'Ġfal', 'con', 'Ġheav', 'ies', 'Ġfal', 'con', 'Ġannually', 'Ġpublished', 'Ġprices', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġchanged', 'Ġdevelopment', 'Ġprogressed', 'Ġannounced', 'Ġprices', 'Ġvarious', 'Ġversions', 'Ġfal', 'con', 'Ġheavy', 'Ġpriced', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġus', 'âĢĵ', 'Ġmillion', 'Ġmillion', '000', 'Ġg', 'Ġmillion', '000', 'Ġg', 'Ġearly', 'Ġprice', 'Ġstated', 'Ġus', 'Ġmillion', '000', 'Ġle', '000', 'Ġg', 'fully', 'Ġexpend', 'able', ').[', 'Ġequ', 'ates', 'Ġprice', 'Ġus', 'Ġper', 'Ġle', 'Ġus', 'Ġper', 'Ġg', 'Ġpublished', 'Ġprice', 'Ġreusable', 'Ġlaunch', 'Ġmillion', 'Ġhowever', 'Ġn', 'asa', 'Ġcontracted', 'Ġspace', 'x', 'Ġlaunch', 'Ġn', 'ancy', 'Ġgrace', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġfal', 'con', 'Ġheavy', 'Ġapproximately', 'Ġmillion', 'Ġincluding', 'Ġlaunch', 'Ġservice', 'Ġmission', 'Ġrelated', 'Ġcosts', 'Ġnearest', 'Ġcompeting', 'Ġu', 'Ġrocket', 'Ġu', 'la', "'s", 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġle', 'Ġpayload', 'Ġcapacity', '000', 'Ġcosts', 'Ġus', 'Ġper', 'Ġle', 'Ġus', 'Ġper', 'Ġg', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġretired', 'Ġone', 'Ġflight', 'Ġremaining', 'Ġj', 'une', 'Ġenvironmental', 'Ġimpact', 'Ġlaunch', 'Ġprices', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġcompetitors', 'Ġonwards', 'Ġmay', 'Ġinclude', 'Ġspace', 'x', 'Ġstarship', 'Ġle', 'Ġblue', 'Ġorigin', "'s", 'Ġnew', 'Ġgl', 'enn', 'Ġle', 'Ġrelativity', 'Ġspace', "'s", 'Ġter', 'ran', 'Ġle', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġvul', 'Ġcent', 'aur', 'Ġle', 'Ġdue', 'Ġimprovements', 'Ġperformance', 'Ġfal', 'con']</t>
+          <t>['ars', 'Ġwik', 'ipedia', 'ars', 'Ġsatellite', 'Ġlocations', 'Ġsince', 'Ġj', 'uly', 'ars', 'Ġusers', 'Ġusing', 'Ġservice', 'Ġprovided', 'Ġch', 'ina', 'Ġtransport', 'Ġtele', 'communication', 'Ġinformation', 'Ġcenter', 'Ġmay', 'Ġapply', 'Ġdigits', 'Ġch', 'inese', 'Ġmobile', 'Ġphone', 'Ġnumbers', 'Ġstarting', 'Ġinternational', 'Ġcall', 'Ġfunction', 'Ġrequired', 'Ġmaking', 'Ġphone', 'Ġcalls', 'Ġnumbers', 'Ġmainland', 'Ġch', 'ina', 'ars', 'Ġnetworks', 'Ġprovide', 'Ġexisting', 'Ġevolved', 'Ġadvanced', 'Ġservices', 'Ġexisting', 'Ġevolved', 'Ġservices', 'Ġoffered', 'Ġland', 'Ġearth', 'Ġstations', 'Ġowned', 'Ġoperated', 'ars', 'Ġcompanies', 'Ġcommercial', 'Ġagreement', 'ars', 'Ġadvanced', 'Ġservices', 'Ġprovided', 'Ġvia', 'Ġdistribution', 'Ġpartners', 'Ġsatellite', 'Ġgate', 'ways', 'Ġowned', 'Ġoperated', 'ars', 'Ġdirectly', 'Ġglobal', 'Ġx', 'press', 'Ġsince', 'ars', 'Ġoffered', 'Ġhigh', 'Ġthroughput', 'Ġservices', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġservice', 'Ġprovides', 'Ġbased', 'Ġglobal', 'Ġservice', 'bit', 'link', 'bit', 'Ġupl', 'ink', 'Ġlatency', 'Ġservices', 'Ġprovided', 'Ġmaritime', 'Ġaviation', 'Ġgovernment', 'Ġenterprise', 'Ġmarkets', 'Ġglobal', 'Ġx', 'press', 'Ġsupported', 'Ġexisting', 'Ġl', 'band', 'Ġnetwork', 'Ġservices', 'Ġoffered', 'Ġusing', 'Ġcombination', 'Ġtwo', 'Ġnetworks', 'Ġincrease', 'Ġavailability', 'Ġreliability', 'Ġmarch', 'ars', 'Ġpartnered', 'Ġisot', 'rop', 'ic', 'Ġsystems', 'Ġdevelop', 'elect', 'ronic', 'Ġscanning', 'Ġantenna', 'Ġintended', 'Ġused', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'ars', 'Ġoffers', 'Ġaviation', 'Ġservices', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġdeveloped', 'Ġpartnership', 'Ġde', 'utsche', 'Ġtele', 'k', 'om', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġuses', 'Ġground', 'based', 'Ġl', 'te', 'Ġnetwork', 'ars', 'band', 'Ġsatellite', 'Ġprovide', 'g', 'bit', 'Ġcapacity', 'Ġaircraft', 'Ġeuro', 'pe', 'Ġairspace', 'Ġproject', 'Ġfaced', 'Ġnumber', 'Ġlegal', 'Ġregulatory', 'Ġchallenges', 'Ġoct', 'ober', 'ars', 'Ġstated', 'Ġcommercial', 'Ġservice', 'Ġwould', 'Ġbegin', 'Ġconstruction', 'Ġground', 'Ġnetwork', 'Ġcompleted', 'Ġfe', 'b', 'ruary', 'Ġmid', 'Ġservice', 'Ġoffered', 'Ġroutes', 'Ġkey', 'Ġdestinations', 'Ġl', 'ondon', 'Ġmad', 'rid', 'Ġbar', 'celona', 'hens', 'Ġl', 'bon', 'Ġpr', 'ague', 'Ġr', 'ome', 'Ġvi', 'enna', 'Ġearly']</t>
         </is>
       </c>
       <c r="C254" t="n">
@@ -3740,7 +3740,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>['Ġheavier', 'Ġsatellites', 'Ġflown', 'Ġg', 'Ġint', 'els', 'ars', 'Ġf', 'Ġended', 'Ġlaunched', 'Ġdebut', 'Ġfal', 'con', 'Ġheavy', 'Ġspace', 'x', 'Ġanticipated', 'Ġfirst', 'Ġcommercial', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġwould', 'Ġthree', 'Ġmonths', 'Ġsuccessful', 'Ġmaiden', 'Ġflight', 'Ġdue', 'Ġdelays', 'Ġfirst', 'Ġcommercial', 'Ġpayload', 'Ġar', 'abs', 'Ġsuccessfully', 'Ġlaunched', 'Ġapr', 'il', 'Ġyear', 'Ġtwo', 'Ġmonths', 'Ġfirst', 'Ġflight', 'Ġspace', 'x', 'Ġhoped', 'Ġlaunches', 'Ġevery', 'Ġyear', 'Ġlaunches', 'Ġlaunches', 'Ġpayload', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġflight', 'Ġlaunch', 'Ġdate', 'Ġpayload', 'Ġmass', 'Ġcustomer', 'Ġprice', 'Ġoutcome', 'Ġfe', 'b', 'ruary', 'Ġel', 'Ġmus', 'k', "'s", 'es', 'la', 'Ġroad', 'ster', 'Ġspace', 'x', 'Ġinternal', 'Ġsuccess', 'Ġdemonstration', 'Ġï', '¬', 'Ĥ', 'ight', 'es', 'la', 'Ġroad', 'ster', 'Ġsent', 'Ġtrans', 'ars', 'Ġinjection', 'Ġhel', 'oc', 'entric', 'Ġorbit', 'Ġside', 'Ġboosters', 'Ġlanded', 'Ġsuccessfully', 'Ġcenter', 'Ġbooster', 'Ġstruck', 'Ġocean', 'Ġdestroyed', 'Ġtwo', 'Ġengines', 'Ġfailed', 'Ġrel', 'ight', 'Ġlanding', 'Ġburn', 'Ġdamaging', 'Ġtwo', 'Ġdrone', 'Ġship', "'s", 'Ġengines', 'Ġapr', 'il', 'Ġar', 'abs', 'Ġar', 'abs', 'Ġundisclosed', 'Ġsuccess', 'Ġheavy', 'Ġcommunications', 'Ġsatellite', 'Ġpurchased', 'Ġar', 'ab', 'Ġleague', 'Ġthree', 'Ġboosters', 'Ġlanded', 'Ġsuccessfully', 'Ġcenter', 'Ġcore', 'Ġsubsequently', 'Ġfell', 'Ġlost', 'Ġtransport', 'Ġdue', 'Ġheavy', 'Ġseas', 'Ġtwo', 'Ġside', 'boost', 'ers', 'Ġreused', 'Ġlaunch', 'Ġj', 'une', 'Ġ06', 'Ġus', 'af', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġus', 'Ġmillion', 'Ġsuccess', 'Ġmission', 'Ġsupported', 'Ġu', 'Ġair', 'Ġforce', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'formerly', 'Ġe', 'el', 'v', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġprocess', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginal', 'Ġcontract', 'Ġprice', 'Ġus', 'Ġmillion', 'Ġlater', 'Ġreduced', 'Ġbig', 'Ġpart', 'Ġdue', 'Ġmilitary', "'s", 'Ġagreement', 'Ġï', '¬', 'Ĥ', 'Ġmission', 'Ġreused', 'Ġside']</t>
+          <t>['Ġservice', 'Ġused', '000', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġthroughout', 'Ġeuro', 'pe', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġaircraft', 'Ġoperated', 'Ġb', 'rit', 'ish', 'Ġair', 'ways', 'ber', 'ia', 'Ġv', 'uel', 'ing', 'Ġfamily', 'Ġset', 'Ġip', 'based', 'Ġshared', 'car', 'rier', 'Ġservices', ':[', 'Ġbroadband', 'Ġglobal', 'Ġarea', 'Ġnetwork', 'Ġuse', 'Ġland', 'Ġuses', 'Ġsatellites', 'Ġoffer', 'Ġshared', 'channel', 'Ġpacket', 'sw', 'itched', 'Ġservice', 'Ġk', 'bit', 'u', 'pl', 'ink', 'link', 'Ġspeeds', 'Ġmay', 'Ġdiffer', 'Ġdepend', 'Ġterminal', 'Ġmodel', 'Ġstreaming', 'ip', 'Ġservice', 'Ġk', 'bit', 'Ġx', 'stream', 'Ġdata', 'Ġrate', 'services', 'Ġdepend', 'Ġterminal', 'Ġmodel', 'Ġterminals', 'Ġalso', 'Ġoffer', 'Ġcircuit', 'sw', 'itched', 'Ġmobile', 'Ġintegrated', 'Ġservices', 'Ġdigital', 'Ġnetwork', 'isd', 'n', 'Ġservices', 'Ġk', 'bit', 'Ġeven', 'Ġlow', 'Ġspeed', 'Ġk', 'bit', 'Ġvoice', 'Ġetc', 'Ġservices', 'Ġservice', 'Ġavailable', 'Ġglobally', 'Ġsatellites', 'Ġfleet', 'broad', 'band', 'Ġmaritime', 'Ġservice', 'Ġfleet', 'broad', 'band', 'Ġbased', 'Ġtechnology', 'Ġoffering', 'Ġsimilar', 'Ġservices', 'Ġusing', 'Ġinfrastructure', 'Ġrange', 'Ġfleet', 'Ġbroadband', 'Ġuser', 'Ġterminals', 'Ġavailable', 'Ġdesigned', 'Ġships', 'Ġnetworks', 'Ġhigh', 'Ġthroughput', 'Ġservices', 'Ġadvanced', 'Ġservices', 'ars', 'Ġwik', 'ipedia', 'Ġswift', 'broad', 'band', 'Ġaer', 'autical', 'Ġservice', 'Ġswift', 'broad', 'band', 'Ġbased', 'Ġtechnology', 'Ġoffers', 'Ġsimilar', 'Ġservices', 'Ġterminals', 'Ġdesigned', 'Ġcommercial', 'Ġprivate', 'Ġmilitary', 'Ġaircraft', 'Ġfamily', 'Ġset', 'Ġip', 'based', 'Ġservices', 'Ġdesigned', 'Ġlong', 'term', 'Ġmachine', 'machine', 'Ġmanagement', 'Ġfixed', 'Ġassets', ':[', 'Ġlaunched', 'Ġjan', 'uary', 'Ġglobal', 'Ġip', 'based', 'Ġlow', 'data', 'Ġrate', 'Ġservice', 'Ġdesigned', 'Ġhigh', 'Ġdata', 'Ġavailability', 'Ġperformance', 'Ġpermanently', 'Ġunmanned', 'Ġenvironments', 'Ġhigh', 'frequency', 'Ġlow', 'lat', 'ency', 'Ġdata', 'Ġreporting', 'Ġintended', 'Ġmonitoring', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġassets', 'Ġpipelines', 'Ġoil', 'Ġwell', 'Ġheads', 'Ġback', 'haul', 'ing', 'Ġelectricity', 'Ġconsumption', 'Ġdata', 'Ġwithin', 'Ġutility', 'Ġglobal', 'Ġshort', 'Ġburst', 'Ġdata', 'Ġstore', 'Ġforward', 'Ġservice', 'Ġintended', 'Ġdeliver', 'Ġmessages', 'Ġbytes', 'Ġsend', 'Ġdirection', 'Ġbytes', 'Ġreceive', 'Ġdirection', 'Ġservice', 'Ġdelivered', 'Ġmarket', 'Ġvia', 'Ġsky', 'wave', 'Ġmobile', 'Ġcommunications', 'Ġhoney', 'well', 'Ġglobal', 'Ġtracking', 'data', 'Ġpro', 'data', 'Ġpro', 'Ġglobal', 'Ġsatellite', 'Ġdata', 'Ġservice', 'Ġdesigned', 'Ġtwo', 'way', 'Ġtext', 'Ġdata', 'Ġcommunications', 'Ġremote', 'Ġassets']</t>
         </is>
       </c>
       <c r="C255" t="n">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>['Ġboosters', 'Ġsecondary', 'Ġpayload', 'Ġinclude', 'Ġorbit', 'ers', 'Ġlights', 'ail', 'Ġot', 'b', 'host', 'ing', 'Ġdeep', 'Ġspace', 'Ġatomic', 'Ġclock', '])', 'Ġcosmic', 'culus', 'r', 'Ġprox', 'Ġsuccessfully', 'Ġreused', 'Ġboosters', 'Ġsecond', 'Ġfal', 'con', 'Ġheavy', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcenter', 'Ġcore', 'Ġbooster', 'Ġland', 'Ġsuccessfully', 'Ġdestroyed', 'Ġupon', 'Ġimpact', 'l', 'antic', 'Ġocean', 'mber', 'Ġus', 'sf', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmillennium', 'Ġspace', 'Ġsystems', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'us', 'Ġmillion', 'Ġus', 'Ġmillion', 'Ġcontract', 'Ġincluding', 'Ġtwo', 'Ġfal', 'con', '])', 'Ġsuccess', 'Ġfirst', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġcontract', 'Ġawarded', 'Ġspace', 'x', 'Ġprice', 'Ġtypical', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlaunch', 'us', 'Ġmillion', 'Ġpayload', 'Ġincludes', 'Ġtwo', 'Ġseparate', 'Ġsatellites', 'Ġleast', 'Ġthree', 'Ġadditional', 'Ġrides', 'hare', 'Ġpayload', 'including', 'Ġtet', 'ra', ')[', 'Ġweighs', 'Ġroughly', 'Ġlaunch', 'Ġlaunched', 'Ġdirect', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġnecess', 'itating', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtime', 'Ġplanned', 'Ġpartially', 'Ġexpend', 'able', 'Ġlaunch', 'Ġdeliberately', 'Ġexpend', 'Ġcenter', 'Ġcore', 'Ġlacks', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġlanding', 'Ġgear', 'Ġneeded', 'Ġlanding', 'Ġtwo', 'Ġside', 'boost', 'ers', 'Ġlanded', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġoriginally', 'Ġscheduled', 'Ġdelayed', 'Ġdue', 'Ġpayload', 'Ġissues', 'mber', 'Ġsecond', 'Ġstage', 'Ġfeatured', 'Ġgray', 'Ġband', 'Ġdue', 'Ġlong', 'Ġcoast', 'Ġphase', 'Ġsubsequent', 'Ġburns', 'Ġallow', 'Ġheat', 'Ġsunlight', 'Ġabsorbed', 'Ġwarm', 'Ġk', 'eros', 'ene', 'Ġtank', 'Ġlonger', 'Ġcoast', 'ing', 'Ġperiod', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġf', 'h', 'Ġthird', 'Ġfal', 'con', 'Ġrocket', 'Ġgets', 'Ġcold', 'Ġk', 'eros', 'ene', 'Ġfreezes', 'Ġmuch', 'Ġhigher', 'Ġtemperature', 'Ġfal', 'con', 'âĢ', 'Ļ', 'Ġliquid', 'Ġoxid', 'izer', 'Ġbecomes', 'Ġvisc', 'ous', 'Ġsl', 'ush', 'like', 'Ġfreezes', 'Ġsolid', 'Ġingested', 'Ġsl', 'ush', 'Ġfuel', 'Ġwould', 'Ġlikely', 'Ġprevent', 'Ġignition', 'Ġdestroy', 'Ġupper', 'Ġstage', 'âĢ', 'Ļ', 'Ġmer', 'lin', 'Ġengine', 'Ġjan', 'uary']</t>
+          <t>['Ġmessage', 'Ġsize', 'Ġmobile', 'Ġk', 'bytes', 'Ġmobile', 'Ġk', 'bytes', 'Ġtypical', 'Ġdelivery', 'Ġtime', 'Ġseconds', 'Ġservice', 'Ġintended', 'Ġmission', 'critical', 'Ġapplications', 'Ġmanaging', 'Ġtrucks', 'Ġï', '¬', 'ģ', 'hing', 'Ġvessels', 'Ġoil', 'Ġgas', 'Ġheavy', 'Ġequipment', 'Ġtext', 'Ġmessage', 'Ġremote', 'Ġworkers', 'Ġsecurity', 'Ġapplications', 'Ġprovided', 'Ġsky', 'wave', 'Ġmobile', 'Ġcommunications', 'Ġinc', 'Ġpart', 'Ġorb', 'comm', 'Ġcompany', 'Ġoffers', 'Ġportable', 'Ġfixed', 'Ġphone', 'Ġservices', ':[', 'phone', 'phone', 'Ġmobile', 'Ġsatellite', 'Ġphone', 'Ġoffering', 'Ġvoice', 'Ġtele', 'phony', 'Ġvariety', 'Ġdata', 'Ġcapabilities', 'Ġincluding', 'Ġsm', 'Ġshort', 'Ġmessage', 'Ġemail', 'ing', 'Ġlook', 'send', 'Ġwell', 'Ġsupporting', 'Ġdata', 'Ġservice', 'phone', 'Ġlink', 'phone', 'Ġlink', 'Ġlow', 'cost', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġglobal', 'Ġsatellite', 'Ġphone', 'Ġservice', 'Ġprovides', 'Ġvoice', 'Ġconnectivity', 'Ġworking', 'Ġliving', 'Ġareas', 'Ġwithout', 'Ġcellular', 'Ġcoverage', 'Ġincludes', 'Ġdata', 'Ġcapabilities', 'Ġfleet', 'phone', 'ars', "'s", 'Ġfleet', 'phone', 'Ġservice', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġphone', 'Ġservice', 'Ġuse', 'Ġsmaller', 'Ġvessels', 'Ġvoice', 'Ġcommunications', 'Ġprimary', 'Ġrequirement', 'Ġvessels', 'Ġadditional', 'Ġvoice', 'Ġlines', 'Ġneeded', 'Ġprovides', 'Ġlow', 'cost', 'Ġglobal', 'Ġsatellite', 'Ġphone', 'Ġservice', 'Ġoption', 'Ġworking', 'Ġsailing', 'Ġoutside', 'Ġcellular', 'Ġcoverage', 'Ġbased', 'Ġolder', 'Ġtechnologies', ':[', 'Ġaer', 'autical', 'classic', 'ero', '):', 'Ġprovides', 'Ġanalogue', 'Ġvoice', 'fax', 'data', 'Ġservices', 'Ġaircraft', 'Ġthree', 'Ġlevels', 'Ġterminals', 'ero', 'l', 'low', 'Ġgain', 'Ġantenna', 'Ġprimarily', 'Ġpacket', 'Ġdata', 'Ġincluding', 'Ġac', 'ars', 'Ġads', 'ero', 'h', 'high', 'Ġgain', 'Ġantenna', 'Ġmedium', 'Ġquality', 'Ġvoice', 'Ġfax', 'data', 'Ġbit', 'ero', 'inter', 'mediate', 'Ġgain', 'Ġantenna', 'Ġlow', 'Ġquality', 'Ġvoice', 'Ġfax', 'data', 'Ġbit', 'Ġnote', 'Ġalso', 'Ġaircraft', 'Ġrated', 'Ġversions', 'ars', 'c', 'Ġmini', 'Ġaircraft', 'Ġversion', 'Ġg', 'Ġcalled', 'Ġswift', 'see', 'Ġcommunications', 'Ġglobal', 'Ġvoice', 'Ġservices', 'Ġexisting', 'Ġevolved', 'Ġservices', 'ars', 'Ġwik', 'ipedia', 'ars', 'b', 'Ġservice', 'Ġretired', 'Ġde', 'cember', 'Ġprovided', 'Ġdigital', 'Ġvoice', 'Ġservices', 'Ġte', 'lex', 'Ġservices', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit']</t>
         </is>
       </c>
       <c r="C256" t="n">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>['Ġu', 'Ġspace', 'Ġforce', 'Ġus', 'Ġmillion', 'includes', 'Ġnew', 'Ġsuccess', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġused', 'Ġnew', 'Ġcenter', 'Ġcore', 'Ġexpend', 'able', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġlanding', 'Ġgear', 'Ġtwo', 'Ġreused', 'Ġside', 'boost', 'ers', 'Ġlanded', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġsecond', 'Ġstage', 'Ġgray', 'Ġband', 'Ġthermal', 'Ġpurposes', 'Ġmission', 'Ġrequirements', 'Ġsimilar', 'Ġus', 'sf', 'Ġmission', 'Ġmay', 'Ġ00', 'Ġv', 'ias', 'Ġameric', 'Ġar', 'ct', 'urus', 'aur', 'ora', ')[', 'Ġg', 'space', 'aka', 'Ġn', 'us', 'ant', 'ara', 'h', 'Ġv', 'ias', 'str', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġdat', 'ap', 'ort', 'Ġpt', 'Ġp', 'asi', 'ï', '¬', 'ģ', 'k', 'ate', 'lit', 'Ġn', 'us', 'ant', 'ara', 'Ġsuccess', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginally', 'Ġslated', 'Ġlaunch', 'Ġv', 'ias', 'Ġsatellite', 'Ġdue', 'Ġdelays', 'ri', 'ane', 'Ġlaunch', 'Ġvehicle', 'Ġused', 'Ġinstead', 'Ġv', 'ias', 'Ġmaintained', 'Ġlaunch', 'Ġoption', 'Ġdelivered', 'Ġnext', 'Ġka', 'band', 'Ġsatellite', 'Ġaboard', 'Ġfal', 'con', 'Ġheavy', 'Ġone', 'Ġintended', 'Ġprovide', 'Ġservice', 'Ġameric', 'Ġregion', 'str', 'Ġmicro', 'ge', 'Ġsatellite', 'Ġar', 'ct', 'urus', 'Ġadded', 'Ġindependent', 'Ġsecondary', 'Ġpayload', 'Ġlate', 'Ġse', 'pt', 'ember', 'Ġfollowing', 'Ġseries', 'Ġengine', 'Ġburns', 'Ġlong', 'Ġperiods', 'Ġcoast', 'ing', 'Ġupper', 'Ġstage', 'Ġfal', 'con', 'Ġheavy', 'Ġdeployed', 'Ġsatellite', 'Ġnear', 'ge', 'os', 'ynchronous', 'Ġorbit', 'Ġapproximately', 'Ġupper', 'Ġstage', 'Ġwent', 'Ġsuccessfully', 'Ġdeploy', 'Ġadditional', 'Ġpayload', 'Ġg', 'space', 'Ġar', 'ct', 'urus', 'Ġsecond', 'Ġstage', 'Ġgray', 'Ġband', 'Ġreason', 'Ġus', 'sf', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġexpend', 'Ġthree', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcores', 'Ġj', 'uly', 'Ġ03', '04', 'Ġj', 'upiter', 'ech', 'ost', 'ar', ')[', 'Ġe', 'ch', 'ost', 'ar', 'Ġsuccess', 'Ġheaviest', 'Ġcommercial', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġweighing', 'Ġlaunch', 'Ġsecond', 'Ġstage', 'Ġgray', 'Ġband', 'Ġreason', 'Ġus', 'sf', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtime', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'ured', 'Ġmedium', 'Ġcoast']</t>
+          <t>['Ġhigh', 'Ġspeed', 'Ġdata', 'Ġservices', 'Ġk', 'bit', 'Ġalso', 'leased', 'Ġmode', 'ars', 'b', 'Ġavailable', 'Ġspare', 'ars', 'Ġsatellites', 'ars', 'c', 'Ġeffectively', 'atellite', 'Ġte', 'lex', 'Ġterminal', 'Ġlow', 'speed', 'digital', 'trans', 'mission', 'Ġbit', 'Ġrate', 'Ġbit', 'Ġinformation', 'Ġbit', 'Ġrate', 'Ġbit', 'Ġstore', 'forward', 'Ġpolling', 'Ġetc', 'Ġcapabilities', 'Ġcertain', 'Ġmodels', 'ars', 'c', 'Ġterminals', 'Ġapproved', 'Ġglobal', 'Ġmaritime', 'Ġdistress', 'Ġsafety', 'Ġsystem', 'g', 'md', 'ss', 'Ġsystem', 'Ġequipped', 'ars', 'Ġprovides', 'Ġvoice', 'Ġservices', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit', 'Ġpaved', 'Ġway', 'Ġtowards', 'ars', 'mini', 'Ġservice', 'Ġended', 'Ġmini', 'Ġprovides', 'Ġvoice', 'Ġservices', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit', 'Ġone', 'Ġk', 'bit', 'Ġchannel', 'Ġtakes', 'Ġk', 'bit', 'Ġsatellite', 'Ġservice', 'Ġclosed', 'Ġearly', 'Ġjan', 'uary', 'Ġg', 'global', 'Ġarea', 'Ġnetwork', '):', 'Ġprovides', 'Ġselection', 'Ġlow', 'Ġspeed', 'Ġservices', 'Ġlike', 'Ġvoice', 'Ġk', 'bit', 'Ġdata', 'Ġk', 'bit', 'dn', 'Ġlike', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'dn', 'Ġshared', 'channel', 'Ġpacket', 'sw', 'itched', 'Ġdata', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'Ġpacket', 'Ġdata', 'Ġservice', 'Ġformerly', 'ars', 'Ġpacket', 'Ġdata', 'Ġservice', 'Ġg', 'Ġalso', 'Ġknown', 'Ġservice', 'Ġclosed', 'Ġearly', 'Ġjan', 'uary', 'Ġfleet', 'Ġfamily', 'Ġnetworks', 'Ġincludes', 'ars', 'fleet', 'ars', 'fleet', 'ars', 'fleet', 'Ġmembers', 'Ġnumbers', 'Ġcome', 'Ġdiameter', 'Ġantenna', 'Ġcent', 'imet', 'res', 'Ġmuch', 'Ġlike', 'Ġg', 'Ġprovides', 'Ġselection', 'Ġlow', 'Ġspeed', 'Ġservices', 'Ġlike', 'Ġvoice', 'Ġk', 'bit', 'Ġfax', 'data', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġservices', 'Ġlike', 'Ġfax', 'data', 'Ġk', 'bit', 'dn', 'Ġlike', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'dn']</t>
         </is>
       </c>
       <c r="C257" t="n">
@@ -3779,7 +3779,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>['Ġphase', 'Ġcore', 'Ġexpended', 'Ġtwo', 'Ġboosters', 'Ġrecovered', 'Ġland', 'Ġpayload', 'Ġfair', 'ing', 'Ġrecovery', 'Ġattempted', 'Ġoct', 'ober', 'Ġpsyche', 'Ġn', 'asa', 'iscovery', 'Ġus', 'Ġmillion', 'Ġsuccess', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunched', 'Ġpsyche', 'Ġorbit', 'er', 'Ġmission', 'Ġhel', 'oc', 'entric', 'Ġorbit', 'Ġpsyche', 'Ġspacecraft', 'Ġvisit', 'Ġpsyche', 'Ġasteroid', 'Ġmain', 'Ġasteroid', 'Ġbelt', 'Ġcore', 'Ġexpended', 'Ġtwo', 'Ġboosters', 'Ġrecovered', 'Ġland', 'Ġnet', 'Ġde', 'cember', 'Ġus', 'sf', 'Ġu', 'Ġspace', 'Ġforce', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġsecond', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġawarded', 'Ġj', 'une', 'Ġnet', 'Ġapr', 'il', 'Ġgoes', 'u', 'Ġn', 'asa', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġse', 'pt', 'ember', 'Ġn', 'asa', 'Ġawarded', 'Ġspace', 'x', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġge', 'ost', 'ation', 'ary', 'Ġgoes', 'u', 'Ġweather', 'Ġsatellite', 'Ġnet', 'Ġoct', 'ober', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġn', 'asa', 'plan', 'etary', 'Ġmissions', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġconduct', 'Ġdetailed', 'Ġsurvey', 'Ġeuro', 'pa', 'Ġuse', 'Ġsophisticated', 'Ġsuite', 'Ġscience', 'Ġinstruments', 'Ġinvestigate', 'Ġwhether', 'Ġicy', 'Ġmoon', 'Ġconditions', 'Ġsuitable', 'Ġlife', 'Ġkey', 'Ġmission', 'Ġobjectives', 'Ġproduce', 'Ġhigh', 'resolution', 'Ġimages', 'Ġeuro', 'pa', "'s", 'Ġsurface', 'Ġdetermine', 'Ġcomposition', 'Ġlook', 'Ġsigns', 'Ġrecent', 'Ġongoing', 'Ġgeological', 'Ġactivity', 'Ġmeasure', 'Ġthickness', 'Ġmoon', "'s", 'Ġicy', 'Ġshell', 'Ġsearch', 'Ġsubs', 'ur', 'face', 'Ġlakes', 'Ġdetermine', 'Ġdepth', 'Ġsal', 'inity', 'Ġeuro', 'pa', "'s", 'Ġocean', 'Ġmission', 'Ġï', '¬', 'Ĥ', 'Ġpast', 'Ġmars', 'Ġearth', 'Ġarriving', 'Ġj', 'upiter', 'Ġapr', 'il', 'Ġnet', 'mber', 'Ġv', 'iper', 'gr', 'ï', '¬', 'ģ', 'n', 'Ġmission', 'Ġast', 'rob', 'otic', 'n', 'asa', 'art', 'emis', 'Ġundisclosed', 'list', 'Ġprice', 'Ġmillion', 'Ġplanned', 'Ġast', 'rob', 'otic', "'s", 'Ġgr', 'ï', '¬', 'ģ', 'n', 'Ġlunar', 'Ġland', 'er', 'Ġdeliver', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġspacecraft', 'Ġlunar', 'Ġsouth', 'Ġpole', 'Ġexpected', 'Ġrecover', 'Ġboosters', 'Ġnet', 'Ġde', 'cember', 'Ġpower', 'Ġpropulsion', 'Ġelement', 'ppe', 'Ġn', 'asa', 'art', 'emis', 'Ġus', 'Ġmillion', 'Ġplanned', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia']</t>
+          <t>['Ġshared', 'channel', 'Ġpacket', 'sw', 'itched', 'Ġdata', 'Ġservices', 'Ġk', 'bit', 'called', 'Ġmobile', 'Ġpacket', 'Ġdata', 'Ġservice', 'Ġsee', 'Ġhowever', 'Ġservices', 'Ġavailable', 'Ġmembers', 'Ġfamily', 'Ġlatest', 'Ġservice', 'Ġsupported', 'Ġmobile', 'dn', 'Ġk', 'bit', 'ars', 'fleet', 'Ġterminals', 'Ġswift', 'Ġsimilar', 'Ġg', 'Ġproviding', 'Ġvoice', 'Ġlow', 'Ġrate', 'Ġfax', 'data', 'k', 'bit', 'dn', 'Ġservices', 'Ġprivate', 'Ġbusiness', 'Ġcommercial', 'Ġaircraft', 'Ġswift', 'Ġoften', 'Ġsold', 'Ġmulti', 'channel', 'Ġversion', 'Ġsupport', 'Ġseveral', 'Ġtimes', 'k', 'bit', 'ars', 'ars', "'s", 'Ġp', 'ager', 'Ġalthough', 'Ġmuch', 'Ġlarger', 'Ġterrestrial', 'Ġversions', 'Ġunits', 'Ġequipped', 'Ġoriginal', 'ars', 'Ġterminals', 'Ġone', 'way', 'Ġmobile', 'Ġp', 'agers', 'Ġnewer', 'ars', 'Ġterminals', 'Ġequivalent', 'Ġtwo', 'way', 'Ġp', 'ager', 'Ġmain', 'Ġuse', 'Ġtechnology', 'Ġnowadays', 'Ġtracking', 'Ġtrucks', 'Ġbu', 'oys', 'Ġsc', 'ada', 'Ġapplications', 'mobile', 'Ġpacket', 'Ġdata', 'Ġservice', '):', 'Ġpreviously', 'Ġknown', 'Ġip', 'based', 'Ġdata', 'Ġservice', 'Ġseveral', 'Ġusers', 'Ġshare', 'k', 'bit', 'Ġcarrier', 'Ġmanner', 'Ġsimilar', 'Ġad', 'sl', 'Ġmp', 'ds', 'spe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġterminals', 'Ġsold', 'Ġrather', 'Ġservice', 'Ġcomes', 'Ġterminals', 'Ġdesigned', 'Ġg', 'Ġfleet', 'Ġswift', 'phone', 'Ġprovides', 'Ġvoice', 'Ġservices', 'Ġk', 'bit', 'Ġmedium', 'Ġspeed', 'Ġfax', 'data', 'Ġservices', 'Ġk', 'bit', 'Ġservice', 'Ġemerged', 'Ġcollaboration', 'Ġagreement', 'ces', 'Ġavailable', 'Ġem', 'ea', 'Ġap', 'ac', 'Ġsatellite', 'Ġregions', 'Ġcoverage', 'Ġavailable', 'Ġaf', 'rica', 'Ġmiddle', 'east', 'ia', 'Ġeuro', 'pe', 'Ġwell', 'Ġmaritime', 'Ġareas', 'Ġem', 'ea', 'Ġap', 'ac', 'Ġcoverage', 'Ġj', 'une', 'Ġeuro', 'pe', 'Ġparliament', 'Ġeuro', 'pe', 'Ġcouncil', 'Ġadopted', 'Ġeuro', 'pe', "'s", 'Ġdecision', 'Ġestablish', 'Ġsingle', 'Ġselection', 'Ġauthor', 'isation', 'Ġprocess', 'es', 'ap', 'Ġeuro', 'pe', 'band', 'Ġapplication', 'Ġprocess', 'Ġensure', 'Ġcoordinated', 'Ġintroduction', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'ss', 'Ġprojects', 'Ġsince', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork']</t>
         </is>
       </c>
       <c r="C258" t="n">
@@ -3792,7 +3792,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>['Ġhabit', 'ation', 'Ġlogistics', 'Ġoutpost', 'h', 'alo', 'Ġfirst', 'Ġelements', 'Ġgateway', 'Ġmini', 'station', 'Ġpart', 'Ġart', 'emis', 'Ġprogram', 'Ġawarded', 'Ġfe', 'b', 'ruary', 'Ġmax', 'ar', 'Ġalready', 'Ġmade', 'Ġmillion', 'Ġpayments', 'Ġspace', 'x', 'Ġcontract', 'Ġlaunch', 'Ġp', 'pe', 'Ġlater', 'Ġn', 'asa', 'Ġdecided', 'Ġlaunch', 'Ġp', 'pe', 'Ġh', 'alo', 'Ġtogether', 'Ġnet', 'Ġoct', 'ober', 'Ġn', 'ancy', 'Ġgrace', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'launch', 'Ġservices', 'Ġprogram', 'Ġmillion', 'Ġplanned', 'Ġinfrared', 'Ġspace', 'Ġtelescope', 'Ġstationed', 'Ġsun', 'earth', 'Ġl', 'ba', 'Ġast', 'rob', 'otic', 'ba', 'dragon', 'Ġn', 'asa', 'gate', 'way', 'Ġlogistics', 'Ġservices', 'Ġplanned', 'Ġmarch', 'Ġn', 'asa', 'Ġannounced', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcontract', 'Ġgateway', 'Ġlogistics', 'Ġservices', 'Ġguarantees', 'Ġleast', 'Ġtwo', 'Ġlaunches', 'Ġnew', 'Ġdragon', 'Ġres', 'upp', 'ly', 'Ġspacecraft', 'Ġtop', 'Ġfal', 'con', 'Ġheavy', 'Ġcarry', '000', 'Ġcargo', 'Ġlunar', 'Ġorbit', 'âĢĵ', 'Ġmonths', 'Ġlong', 'Ġmissions', 'dragon', 'Ġn', 'asa', 'gate', 'way', 'Ġlogistics', 'Ġservices', 'Ġplanned', 'Ġsecond', 'Ġdragon', 'Ġï', '¬', 'Ĥ', 'ight', 'ba', 'ba', 'Ġint', 'els', 'ba', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcommercial', 'Ġagreement', 'Ġfal', 'con', 'Ġheavy', 'Ġsigned', 'Ġmay', 'Ġoption', 'Ġstill', 'Ġmaintained', 'Ġsatellite', 'Ġchosen', 'Ġmay', 'Ġspace', 'x', 'Ġannounced', 'Ġint', 'els', 'Ġsigned', 'Ġfirst', 'Ġcommercial', 'Ġcontract', 'Ġfal', 'con', 'Ġheavy', 'Ġflight', 'Ġconfirmed', 'Ġtime', 'Ġfirst', 'Ġint', 'els', 'Ġlaunch', 'Ġwould', 'Ġoccur', 'Ġagreement', 'Ġspace', 'x', 'Ġdelivering', 'Ġsatellites', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', ').[', 'Ġaug', 'ust', 'Ġemerged', 'Ġint', 'els', 'Ġcontract', 'Ġreass', 'igned', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġmission', 'Ġdeliver', 'Ġint', 'els', 'Ġorbit', 'Ġthird', 'Ġquarter', 'Ġperformance', 'Ġimprovements', 'Ġfal', 'con', 'Ġvehicle', 'Ġfamily', 'Ġsince', 'Ġannouncement', 'Ġadvertising', '000', 'Ġg', 'Ġexpend', 'able', 'Ġflight', 'Ġprofile', 'Ġenable', 'Ġlaunch', 'Ġsatellite', 'Ġwithout', 'Ġupgrading', 'Ġfal', 'con', 'Ġheavy', 'Ġvariant', 'ars', 'Ġbooked', 'Ġthree']</t>
+          <t>['ars', 'Ġwik', 'ipedia', 'Ġeuro', 'pe', 'Ġlate', 'Ġselection', 'Ġprocess', 'Ġattracted', 'Ġfour', 'Ġapplications', 'Ġprospective', 'Ġoperators', 'ico', 'Ġglobal', 'Ġcommunications', 'ico', 'ars', 'Ġsolar', 'Ġmobile', 'ech', 'ost', 'ar', 'Ġmobile', 'Ġter', 'rest', 'ar', ').[', 'Ġmay', 'Ġeuro', 'pe', 'Ġcommission', 'Ġselected', 'Ġtwo', 'Ġoperators', 'ars', 'Ġventures', 'Ġsolar', 'Ġmobile', 'Ġgiving', 'Ġoperators', 'Ġright', 'Ġuse', 'Ġspecific', 'Ġradio', 'Ġfrequencies', 'Ġidentified', 'Ġcommission', "'s", 'Ġdecision', 'Ġright', 'Ġoperate', 'Ġrespective', 'Ġmobile', 'Ġsatellite', 'Ġsystems', '".', 'Ġmember', 'Ġstates', 'Ġensure', 'Ġtwo', 'Ġoperators', 'Ġright', 'Ġuse', 'Ġspecific', 'Ġradio', 'Ġfrequencies', 'Ġidentified', 'Ġcommission', "'s", 'Ġdecision', 'Ġright', 'Ġoperate', 'Ġrespective', 'Ġmobile', 'Ġsatellite', 'Ġsystems', 'Ġyears', 'Ġselection', 'Ġdecision', 'Ġoperators', 'Ġcompelled', 'Ġstart', 'Ġoperations', 'Ġwithin', 'Ġmonths', 'may', 'Ġselection', 'ars', "'s", 'band', 'Ġsatellite', 'Ġprogramme', 'Ġprovides', 'Ġmobile', 'Ġmultimedia', 'Ġbroadcast', 'Ġmobile', 'Ġtwo', 'way', 'Ġbroadband', 'Ġtelecommunications', 'Ġnext', 'generation', 'ss', 'Ġservices', 'Ġacross', 'Ġmember', 'Ġstates', 'Ġeuro', 'pe', 'Ġunion', 'Ġfar', 'Ġeast', 'Ġmos', 'cow', 'Ġank', 'ara', 'Ġmeans', 'Ġhybrid', 'Ġnetwork', 'Ġbuilt', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġlaunched', 'Ġcomplementary', 'Ġground', 'Ġnetwork', 'Ġconsists', 'Ġaround', 'Ġl', 'te', 'Ġbase', 'Ġstations', 'Ġconstructed', 'Ġde', 'utsche', 'Ġtele', 'k', 'om', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġfaced', 'Ġlegal', 'Ġchallenges', 'Ġincluding', 'Ġone', 'Ġv', 'ias', 'Ġalleging', 'Ġunfair', 'Ġbidding', 'Ġpractices', 'Ġmisuse', 'Ġspectrum', 'Ġruling', 'Ġbel', 'gian', 'Ġtelecommunications', 'Ġregulator', 'Ġrev', 'oking', 'Ġpermission', 'Ġuse', 'Ġground', 'Ġnetwork', 'ars', 'Ġordered', 'Ġfifth', 'Ġglobal', 'Ġx', 'press', 'Ġsatellite', 'Ġth', 'ales', 'Ġgroup', 'Ġsatellite', 'Ġlaunched', 'mber', 'Ġcentre', 'Ġspatial', 'Ġguy', 'ana', 'Ġaboard', 'ri', 'ane', 'Ġlaunch', 'Ġvehicle', 'Ġsatellite', 'Ġdescribed', 'Ġhigh', 'Ġthroughput', 'Ġsatellite', "',", 'Ġprovides', 'Ġservices', 'Ġmiddle', 'Ġeast', 'Ġind', 'ia', 'Ġeuro', 'pe', 'Ġformer', 'Ġce', 'Ġru', 'pert', 'Ġpear', 'ce', 'new', 'Ġce', 'Ġr', 'aj', 'ee', 'v', 'Ġsur', 'Ġindicated', 'ars', 'Ġplanned', 'Ġexpansion', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġtrials', 'Ġnew', 'Ġtechnologies', 'Ġdemonstrated', 'Ġbandwidth', 'bit', 'Ġexisting', 'Ġglobal', 'Ġx', 'press', 'Ġnetwork', 'Ġfar', 'Ġexcess', 'Ġexisting', 'Ġpolar', 'Ġcoverage', 'Ġprovide', 'Ġcoverage', 'Ġusers', 'Ġar', 'ctic']</t>
         </is>
       </c>
       <c r="C259" t="n">
@@ -3805,7 +3805,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>['Ġlaunches', 'Ġfal', 'con', 'Ġheavy', 'Ġdue', 'Ġdelays', 'Ġswitched', 'Ġpayload', 'ri', 'ane', 'Ġsimilarly', 'Ġint', 'els', 'Ġcase', 'Ġanother', 'Ġsatellite', 'Ġcontract', 'ars', 'Ġswitched', 'Ġfal', 'con', 'Ġfull', 'Ġthrust', 'Ġdue', 'Ġincreased', 'Ġlif', 'ff', 'Ġcapacity', 'Ġremaining', 'Ġcontract', 'Ġcovered', 'Ġlaunch', 'ars', 'Ġfal', 'con', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġannounced', 'Ġfirst', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġcontract', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'od', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'Ġawarded', 'Ġspace', 'x', 'Ġtwo', 'Ġevolved', 'Ġexpend', 'able', 'Ġlaunch', 'Ġvehicle', 'e', 'el', 'v', ')-', 'class', 'Ġmissions', 'Ġincluding', 'Ġspace', 'Ġfirst', 'Ġcommercial', 'Ġcontracts', 'Ġdepartment', 'Ġdefense', 'Ġcontracts', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġtest', 'Ġprogram', 'Ġmission', 'Ġfal', 'con', 'Ġheavy', 'Ġoriginally', 'Ġscheduled', 'Ġlaunched', 'Ġmarch', 'Ġplaced', 'Ġnear', 'Ġcircular', 'Ġorbit', 'Ġaltitude', 'Ġmi', 'Ġinclination', 'Â°', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġsent', 'Ġu', 'Ġair', 'Ġforce', 'Ġupdated', 'Ġletter', 'Ġintent', 'Ġoutlining', 'Ġcertification', 'Ġprocess', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġnational', 'Ġsecurity', 'Ġsatellites', 'Ġprocess', 'Ġincludes', 'Ġthree', 'Ġsuccessful', 'Ġflights', 'Ġfal', 'con', 'Ġheavy', 'Ġincluding', 'Ġtwo', 'Ġconsecutive', 'Ġsuccessful', 'Ġflights', 'Ġletter', 'Ġstated', 'Ġfal', 'con', 'Ġheavy', 'Ġready', 'Ġfly', 'Ġnational', 'Ġsecurity', 'Ġpayload', 'Ġj', 'uly', 'Ġspace', 'x', 'Ġannounced', 'Ġfirst', 'Ġtest', 'Ġflight', 'Ġwould', 'Ġtake', 'Ġplace', 'Ġde', 'cember', 'Ġpushing', 'Ġlaunch', 'Ġsecond', 'Ġlaunch', 'space', 'Ġtest', 'Ġprogram', 'Ġj', 'une', 'Ġmay', 'Ġoccasion', 'Ġfirst', 'Ġlaunch', 'Ġfal', 'con', 'Ġblock', 'Ġvariant', 'Ġdelay', 'Ġoct', 'ober', 'Ġannounced', 'Ġlaunch', 'Ġeventually', 'Ġpushed', 'Ġj', 'une', 'Ġmission', 'Ġused', 'Ġthree', 'Ġblock', 'Ġcores', 'Ġspace', 'x', 'Ġawarded', 'Ġlaunches', 'Ġphase', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'n', 'ssl', 'Ġcontracts', 'Ġincludes', 'Ġseveral', 'Ġlaunches', 'Ġvertical', 'Ġintegration', 'Ġfacility', 'Ġdevelopment', 'Ġlarger', 'Ġfair', 'ing', 'Ġpayload', 'Ġmission', 'Ġdepartment', 'Ġdefense', 'Ġincluded', 'Ġsmall', 'Ġspacecraft', 'Ġu', 'Ġmilitary', 'Ġn', 'asa', 'Ġresearch', 'Ġinstitutions']</t>
+          <t>['Ġregion', 'ars', 'Ġplans', 'Ġimprove', 'Ġglobal', 'x', 'press', 'Ġconnectivity', 'Â°', 'Ġnorth', 'Ġtwo', 'Ġhigh', 'capacity', 'Ġmulti', 'beam', 'Ġpayload', 'Ġplanned', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbits', 'Ġreliable', 'Ġcoverage', 'ars', 'Ġworked', 'Ġpartnership', 'Ġspace', 'way', 'os', 'Ġar', 'ctic', 'Ġsatellite', 'Ġbroadband', 'Ġmission', 'Ġsatellites', 'Ġcarrying', 'ars', 'Ġpayload', 'Ġmanufactured', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġinnovation', 'Ġsystems', 'ng', 'Ġlaunch', 'Ġscheduled', 'Ġglobal', 'Ġx', 'press', 'Ġexpansion', 'ars', 'ars', 'Ġwik', 'ipedia', 'Ġend', 'ars', 'Ġordered', 'Ġtwo', 'Ġsixth', 'Ġgeneration', 'Ġsatellites', 'Ġair', 'bus', 'Ġsatellites', 'Ġplanned', 'Ġoffer', 'Ġka', 'Ġl', 'band', 'Ġpayload', 'Ġadditional', 'Ġcapacity', 'Ġexisting', 'Ġglobal', 'Ġx', 'press', 'Ġnetworks', 'Ġannounced', 'Ġfirst', 'Ġsatellites', 'Ġwould', 'Ġlaunched', 'hi', 'Ġde', 'cember', 'ars', 'Ġparticipating', 'Ġtwo', 'Ġes', 'Ġart', 'es', 'Ġprograms', 'Ġir', 'Ġice', 'Ġir', 'Ġproject', 'Ġimprove', 'Ġtracking', 'Ġaircraft', 'Ġimprove', 'Ġcommunications', 'Ġaircraft', 'Ġair', 'Ġtra', 'f', 'ï', '¬', 'ģ', 'c', 'Ġcontrollers', 'ars', 'Ġprovide', 'Ġhigh', 'Ġcapacity', 'Ġsatellite', 'Ġcommunications', 'Ġlinks', 'Ġaircraft', 'Ġimprove', 'Ġdetection', 'Ġaircraft', 'Ġlocations', 'Ġtime', 'Ġspace', 'Ġice', 'ars', 'Ġcommunications', 'Ġevolution', 'Ġpartnership', 'Ġindustrial', 'Ġpartners', 'Ġintended', 'Ġidentify', 'Ġinnovative', 'Ġtechnologies', 'Ġexpand', 'Ġenhance', 'Ġcapabilities', 'Ġnext', 'Ġgeneration', 'Ġsatellite', 'ars', 'Ġir', 'idium', 'Ġfrequency', 'Ġbands', 'Ġab', 'ut', 'Ġthus', 'Ġsat', 'Ġradio', 'Ġability', 'Ġinterfere', 'Ġusually', 'Ġfar', 'Ġpowerful', 'ars', 'Ġradio', 'Ġdisrupt', 'Ġir', 'idium', 'Ġradio', 'âĢĵ', 'âĢĵ', 'Ġft', 'Ġaway', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġmobile', 'atellite', 'Ġservice', 'Ġsatellite', 'Ġphone', 'Ġaer', 'om', 'obile', 'Ġglobal', 'star', 'Ġglob', 'als', 'Ġgroup', 'Ġinter', 'put', 'nik', 'Ġir', 'idium', 'Ġcommunications', 'Ġlib', 'rest', 'ream', 'Ġmaritime', 'Ġsafety', 'Ġinformation', 'Ġnetworks', 'air', 'Ġorb', 'comm', 'Ġradi', 'ote', 'le', 'phone', 'es', 'Ġbroadband', 'Ġmaritime', 'Ġspace', 'Ġglobal', 'Ġth', 'ur', 'aya', 'Ġir', 'Ġice', 'Ġissues', 'Ġsee', 'Ġalso', 'ars']</t>
         </is>
       </c>
       <c r="C260" t="n">
@@ -3818,7 +3818,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>[':[', 'Ġgreen', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', 'Ġpayload', 'Ġproject', 'Ġpartly', 'Ġdeveloped', 'Ġu', 'Ġair', 'Ġforce', 'Ġdemonstrate', 'Ġless', 'oxic', 'Ġanother', 'Ġsecondary', 'Ġpayload', 'Ġmini', 'atur', 'ized', 'Ġdeep', 'Ġspace', 'Ġatomic', 'Ġclock', 'Ġexpected', 'Ġfacilitate', 'Ġautonomous', 'Ġnavigation', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', "'s", 'Ġdemonstration', 'Ġscience', 'Ġexperiments', 'Ġmass', 'Ġmeasure', 'Ġeffects', 'Ġlow', 'Ġfrequency', 'Ġradio', 'Ġwaves', 'Ġspace', 'Ġradiation', 'Ġb', 'rit', 'ish', 'orb', 'ital', 'Ġtest', 'Ġbed', 'Ġpayload', 'Ġhosting', 'Ġseveral', 'Ġcommercial', 'Ġmilitary', 'Ġexperiments', 'Ġsmall', 'Ġsatellites', 'Ġincluded', 'Ġprox', 'Ġbuilt', 'Ġge', 'org', 'ia', 'Ġtech', 'Ġstudents', 'Ġtest', 'printed', 'Ġthr', 'uster', 'Ġmini', 'atur', 'ized', 'Ġgy', 'ro', 'scope', 'Ġlights', 'ail', 'Ġplanetary', 'Ġsociety', 'culus', 'r', 'Ġnan', 'os', 'atellite', 'ich', 'igan', 'Ġtech', 'Ġcubes', 'ats', 'Ġu', 'Ġair', 'Ġforce', 'Ġacademy', 'Ġnaval', 'Ġpost', 'graduate', 'Ġschool', 'Ġunited', 'Ġstates', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġuniversity', 'Ġtex', 'Ġaust', 'Ġcal', 'ornia', 'Ġpoly', 'techn', 'ic', 'Ġstate', 'Ġuniversity', 'Ġcubes', 'Ġassembled', 'Ġstudents', 'Ġmer', 'r', 'itt', 'Ġisland', 'Ġhigh', 'Ġschool', 'Ġfl', 'ida', 'Ġblock', 'second', 'Ġstage', 'Ġallowed', 'Ġmultiple', 'Ġreign', 'itions', 'Ġplace', 'Ġmany', 'Ġpayload', 'Ġmultiple', 'Ġorbits', 'Ġlaunch', 'Ġplanned', 'Ġinclude', '000', 'Ġball', 'ast', 'Ġmass', 'Ġball', 'ast', 'Ġmass', 'Ġlater', 'Ġomitted', 'Ġtotal', 'Ġmass', 'Ġpayload', 'Ġstack', 'Ġn', 'asa', 'es', 'Ġresearch', 'Ġcenter', 'Ġproposed', 'Ġmars', 'Ġmission', 'Ġcalled', 'Ġred', 'Ġdragon', 'Ġwould', 'Ġuse', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġtrans', 'mart', 'ian', 'Ġinjection', 'Ġvehicle', 'Ġvariant', 'Ġdragon', 'Ġcapsule', 'Ġenter', 'Ġmart', 'ian', 'Ġatmosphere', 'Ġproposed', 'Ġscience', 'Ġobjectives', 'Ġdetect', 'Ġbios', 'ign', 'atures', 'Ġdrill', 'Ġft', 'Ġunderground', 'Ġeffort', 'Ġsample', 'Ġreservoirs', 'Ġwater', 'Ġice', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġmission', 'Ġn', 'asa', 'Ġcontracts', 'Ġsolar', 'Ġsystem', 'Ġtransport', 'Ġmissions', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġunited', 'Ġstates', 'Ġportal', 'Ġcompanies', 'Ġportal', 'Ġknown', 'Ġexist', 'Ġsurface', 'Ġmission', 'Ġcost', 'Ġprojected', 'Ġless', 'Ġus', 'Ġmillion', 'Ġincluding', 'Ġlaunch', 'Ġcost', 'Ġspace', 'x', 'Ġestimation', '000', 'âĢĵ']</t>
+          <t>['Ġwik', 'ipedia', 'Ġwide', 'band', 'Ġglobal', 'Ġsat', 'p', 'rel', 'iminary', 'Ġfull', 'Ġyear', 'Ġresults', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'ï', '¬', 'ģ', 'ces', 'ars', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġus', 'ars', 'v', 'ias', 'Ġcompletes', 'Ġacquisition', 'ars', 'Ġv', 'ias', 'Ġmay', 'Ġretrieved', 'Ġj', 'uly', 'prop', 'osed', 'Ġamendments', 'Ġconvention', 'Ġinternational', 'Ġmobile', 'Ġsatellite', 'Ġorganization', 'im', ')"', 'Ġinternational', 'Ġcivil', 'Ġaviation', 'Ġorganization', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'agar', 'Ġdavid', 'Ġhar', 'ris', 'Ġr', 'ed', '.).', 'Ġprivat', 'isation', 'ars', 'Ġspecial', 'Ġproblems', '".', 'Ġinternational', 'Ġorganisations', 'Ġspace', 'Ġlaw', 'Ġproceedings', 'Ġthird', 'Ġcoll', 'oqu', 'ium', 'Ġper', 'ug', 'ia', 'aly', 'âĢĵ', 'Ġmay', 'âĢĵ', 'Ġj', 'athan', 'Ġhig', 'gins', 'Ġsatellite', 'Ġnews', 'g', 'athering', 'Ġfocal', 'Ġpress', 'Ġp', 'Ġgod', 'win', 'Ġmatt', 'hew', 'Ġde', 'cember', 'inter', 'view', 'Ġroy', 'Ġgib', 'son', 'Ġoral', 'Ġhistory', 'Ġeuro', 'pe', 'Ġspace', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġp', 'Ġretrieved', 'Ġj', 'une', 'Ġj', 'athan', 'Ġhig', 'gins', 'Ġp', 'oll', 'ars', 'Ġsense', 'Ġsat', 'Ġsatell', 'et', 'oday', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'private', 'Ġequity', 'Ġorbits', 'ars', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġbuys', 'Ġstrat', 'os', 'Ġglobal', 'Ġwashing', 'ton', 'Ġbusiness', 'Ġjournal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'Ġsand', 'le', 'Ġp', 'aul', 'Ġapr', 'il', 'ars', 'Ġtake', 'Ġstake', 'Ġtracking', 'Ġco', 'Ġsky', 'wave', 'uters', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ars', 'Ġgrabs', 'Ġmacro', 'bert', 'Ġengineering', 'Ġprize', 'Ġmars', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C261" t="n">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>['000', 'âĢĵ', 'Ġsurface', 'Ġmars', 'Ġsoft', 'Ġretro', 'prop', 'ulsive', 'Ġlanding', 'Ġfollowing', 'Ġlimited', 'Ġatmospheric', 'Ġde', 'celer', 'ation', 'Ġusing', 'Ġparachute', 'Ġheat', 'Ġshield', 'Ġbeyond', 'Ġred', 'Ġdragon', 'Ġconcept', 'Ġspace', 'x', 'Ġseeing', 'Ġpotential', 'Ġfal', 'con', 'Ġheavy', 'Ġdragon', 'Ġcarry', 'Ġscience', 'Ġpayload', 'Ġacross', 'Ġmuch', 'Ġsolar', 'Ġsystem', 'Ġparticularly', 'Ġj', 'upiter', "'s", 'Ġmoon', 'Ġeuro', 'pa', 'Ġspace', 'x', 'Ġannounced', 'Ġprop', 'ulsive', 'Ġlanding', 'Ġdragon', 'Ġwould', 'Ġdeveloped', 'Ġcapsule', 'Ġwould', 'Ġreceive', 'Ġlanding', 'Ġlegs', 'Ġconsequently', 'Ġred', 'Ġdragon', 'Ġmissions', 'Ġmars', 'Ġcanceled', 'Ġfavor', 'Ġstarship', 'Ġlarger', 'Ġvehicle', 'Ġusing', 'Ġdifferent', 'Ġlanding', 'Ġtechnology', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġinitial', 'Ġmodules', 'Ġlunar', 'Ġgateway', 'Ġpower', 'Ġpropulsion', 'Ġelement', 'ppe', 'Ġhabit', 'ation', 'Ġlogistics', 'Ġoutpost', 'h', 'alo', ').[', 'Ġdecrease', 'Ġcomplexity', 'Ġn', 'asa', 'Ġannounced', 'Ġfe', 'b', 'ruary', 'Ġlaunching', 'Ġfirst', 'Ġtwo', 'Ġelements', 'Ġsingle', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġtargeting', 'Ġlaunch', 'Ġdate', 'Ġearlier', 'mber', 'Ġswitching', 'Ġmerged', 'Ġlaunch', 'Ġn', 'asa', 'Ġlisted', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġp', 'pe', 'Ġlone', 'Ġlaunch', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġfirst', 'Ġaward', 'Ġres', 'upp', 'ly', 'Ġmission', 'Ġlunar', 'Ġgateway', 'Ġplacing', 'Ġnew', 'Ġdragon', 'Ġspacecraft', 'Ġtransl', 'un', 'ar', 'Ġinjection', 'Ġorbit', 'Ġn', 'asa', 'Ġchose', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġvehicle', 'Ġpsyche', 'Ġmission', 'Ġmetallic', 'Ġasteroid', 'Ġlaunched', 'Ġoct', 'ober', 'Ġcontract', 'Ġworth', 'Ġus', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġinitially', 'Ġtargeted', 'Ġlaunched', 'Ġsl', 'Ġrocket', 'Ġhowever', 'Ġdue', 'Ġextensive', 'Ġdelays', 'Ġn', 'asa', 'Ġawarded', 'Ġlaunch', 'Ġcontract', 'Ġspace', 'x', 'Ġfully', 'Ġexpend', 'able', 'Ġfal', 'con', 'Ġheavy', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġcomparison', 'Ġorbital', 'Ġlaunchers', 'Ġfamilies', 'Ġspace', 'x', 'Ġmars', 'Ġtransportation', 'Ġinfrastructure', 'Ġsat', 'urn', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġreused', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', 'Ġheavy', 'Ġlift', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġarchived', 'Ġlunar', 'Ġmissions', 'Ġpsyche', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġreferences', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġsheet', 'z', 'ichael']</t>
+          <t>['Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'making', 'Ġthings', 'Ġbetter', 'Ġï', '¬', 'ģ', 'n', 'al', 'ists', 'Ġannounced', 'Ġb', 'rit', "'s", 'Ġtop', 'Ġengineering', 'Ġaward', 'Ġnews', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġreferences', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġends', 'Ġservice', 'Ġyears', 'ara', 'org', 'Ġarchived', 'Ġoriginal', 'Ġris', 'htm', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmarch', 'Ġlaunch', 'cs', 'Ġes', 'ars', 'Ġspace', 'sky', 'rocket', 'de', 'ars', 'Ġprovides', 'Ġtwo', 'way', 'Ġdata', 'Ġmessaging', 'Ġcommunication', 'Ġservices', 'ars', 'esa', 'ars', 'Ġagreement', 'Ġimprove', 'Ġsatellite', 'Ġmobile', 'Ġphone', 'Ġdata', 'Ġservices', 'http', 'esa', 'Ġes', 'int', 'ars', 'Ġarchived', 'Ġoriginal', 'ww', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'global', 'Ġx', 'press', 'ars', 'Ġaviation', 'ars', 'euro', 'pe', 'Ġaviation', 'Ġnetwork', 'ars', 'ars', 'Ġpartners', 'Ġisot', 'rop', 'ic', 'Ġsystems', 'Ġdevelop', 'Ġnext', 'gen', 'Ġka', 'band', 'Ġmobility', 'Ġantenna', 'http', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'ars', 'Ġpan', 'asonic', 'Ġpartner', 'ï', '¬', 'Ĥ', 'ight', 'Ġconnectivity', 'uters', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ars', 'Ġpan', 'asonic', 'Ġannounce', 'Ġstrategic', 'Ġcollaboration', 'Ġquick', 'Ġfacts', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġï', '¬', 'ģ', 'rm', 'Ġbehind', 'Ġmal', 'ays', 'ia', 'Ġairlines', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġbreakthrough', 'Ġnews', 'Ġmarch', 'Ġash', 'ton', 'Ġch', 'ris', 'Ġbru', 'ce', 'Ġal', 'Ġsh', 'uster', 'Ġcoll', 'edge', 'Ġg', 'ary', 'Ġdick', 'inson', 'Ġmark', 'Ġse', 'pt', 'ember', 'Ġsearch', 'Ġjournal', 'Ġnavigation', 'Ġroyal', 'Ġinstitute', 'Ġnavigation', 'âĢĵ', 'Ġsatellite', 'Ġoperator', 'ars', 'Ġagrees', 'Ġbillion', 'Ġtakeover', 'Ġguardian', 'Ġmarch', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C262" t="n">
@@ -3844,7 +3844,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>['Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', 'Ġsays', 'Ġnew', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġcr', 'ushes', 'Ġcompetition', 'Ġcost', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmay', 'fal', 'con', 'Ġheavy', 'Ġspace', 'x', 'Ġretrieved', 'Ġapr', 'il', 'Ġhar', 'wood', 'iam', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġputs', 'Ġspectacular', 'Ġshow', 'Ġmaiden', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġ', 'ight', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġah', 'mad', 'ase', 'er', 'mar', 'Ġah', 'med', 'Ġk', 'amara', 'Ġah', 'med', 'Ġlim', 'Ġg', 'ab', 'riel', 'Ġmag', 'owan', 'Ġca', 'lin', 'dor', 'ova', 'Ġbl', 'aga', 'se', 'ee', 'Ġche', 'ung', 'Ġwhite', 'Ġtom', 'Ġmars', 'Ġsociety', 'Ġinspiration', 'Ġmars', 'Ġinternational', 'Ġstudent', 'Ġdesign', 'Ġcompetition', 'Ġmars', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġde', 'cember', 'Ġ"-', 'ĠÂ°', 'f', 'Ġcase', 'Ġdeep', 'Ġcry', 'Ġincreases', 'Ġdensity', 'Ġampl', 'ï', '¬', 'ģ', 'es', 'Ġrocket', 'Ġperformance', 'Ġfirst', 'Ġtime', 'Ġanyone', 'Ġgone', 'Ġlow', 'Ġchilled', 'ĠÂ°', 'f', 'ĠÂ°', 'f', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'fal', 'con', 'Ġoverview', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'el', 'Ġmus', 'k', "'s", 'Ġhuge', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġset', 'Ġlaunch', 'ment', 'Ġnews', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġaug', 'ust', 'Ġar', 'abs', 'Ġmission', 'Ġg', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġse', 'pt', 'ember', 'air', 'Ġforce', 'Ġcert', 'ï', '¬', 'ģ', 'ed', 'Ġfal', 'con', 'Ġheavy', 'Ġnational', 'Ġsecurity', 'Ġlaunch', 'Ġwork', 'Ġneeded', 'Ġmeet', 'Ġrequired', 'Ġorbits', 'Ġspac', 'en', 'ews', 'Ġarchived']</t>
+          <t>['Ġaug', 'ust', 'Ġgovernment', 'Ġset', 'Ġapprove', 'Ġbillion', 'ars', 'Ġbuy', 'Ġbloom', 'berg', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġf', 'ild', 'es', 'Ġnic', 'mber', 'ars', 'Ġrejects', 'Ġactivist', 'Ġeffort', 'Ġthwart', 'Ġbillion', 'Ġtakeover', 'htt', 'Ġfinancial', 'Ġtimes', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'ars', 'Ġdel', 'ists', 'Ġstock', 'Ġexchange', 'Ġbuy', 'Ġspac', 'en', 'ews', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'ars', 'Ġwik', 'ipedia', 'private', 'Ġequity', 'Ġgiants', 'Ġtake', 'Ġcontrol', 'ars', 'Ġhedge', 'Ġfunds', 'Ġfold', 'Ġte', 'legraph', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ason', 'Ġrainbow', 'mber', 'v', 'ias', 'Ġbuying', 'ars', 'Ġbillion', 'Ġdeal', 'sp', 'ac', 'ene', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', 'Ġsim', 'Ġshar', 'wood', 'mber', 'space', 'Ġbroadband', 'ï', '¬', 'ģ', 'Ġv', 'ias', 'Ġacqu', 'ires', 'Ġrival', 'ars', 'ht', 'Ġregister', 'Ġretrieved', 'mber', 'Ġprovision', 'ally', 'Ġclears', 'Ġsatellite', 'Ġcomm', 'Ġdeal', 'Ġfollowing', 'depth', 'Ġreview', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'administ', 'rative', 'Ġtimetable', 'Ġgovernment', 'Ġpublishing', 'Ġservice', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'Ġmay', 'Ġrevised', 'Ġstatutory', 'Ġdeadline', 'Ġfollowing', 'Ġextension', 'Ġfre', 'eman', 'ike', 'Ġmay', 'c', 'arl', 'bad', "'s", 'Ġv', 'ias', 'Ġboosts', 'Ġsatellite', 'Ġinternet', 'Ġfootprint', 'Ġglobally', 'Ġcompletion', 'ars', 'Ġacquisition', 'ition', 'Ġsan', 'Ġdie', 'go', 'Ġunion', 'ribune', 'Ġrainbow', 'Ġj', 'ason', 'Ġmay', 'atellite', 'Ġoperators', 'Ġv', 'ias', 'ars', 'Ġcomplete', 'Ġmerger', 'Ġdeal', 'h', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'une', 'priv', 'acy', 'Ġpolicy', 'ars', 'Ġretrieved', 'Ġmarch', 'Ġcity', 'Ġroad', 'Ġl', 'ondon', 'Ġunited', 'Ġkingdom', 'g', 'md', 'ss', 'Ġweather', 'Ġweather', 'g', 'md', 'ss', 'org', 'Ġretrieved', 'Ġapr', 'il']</t>
         </is>
       </c>
       <c r="C263" t="n">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġpas', 'z', 'tor', 'el', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'x', "'s", 'Ġnew', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġunlikely', 'Ġcarry', 'Ġastronauts', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'mus', 'k', 'Ġunve', 'ils', 'Ġrevised', 'Ġversion', 'Ġgiant', 'Ġinter', 'plan', 'etary', 'Ġlaunch', 'Ġsystem', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġinterview', 'Ġel', 'Ġmus', 'k', 'Ġmus', 'k', 'html', 'Ġh', 'obb', 'ys', 'pace', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġel', 'Ġk', 'oen', 'igs', 'mann', 'Ġh', 'ans', 'Ġg', 'ure', 'vich', 'Ġaug', 'ust', 'Ġfal', 'con', 'Ġlaunch', 'Ġvehicle', 'Ġattempt', 'Ġmaking', 'Ġaccess', 'Ġspace', 'Ġaffordable', 'Ġreliable', 'Ġpleasant', 'di', 'th', 'Ġannual', 'ia', 'us', 'u', 'Ġconference', 'Ġsmall', 'Ġsatellites', 'Ġlog', 'Ġut', 'ah', 'Ġut', 'ah', 'Ġstate', 'Ġuniversity', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġg', 'ask', 'ill', 'Ġbr', 'addock', 'Ġoct', 'ober', 'space', 'x', 'Ġreveals', 'Ġfal', 'con', 'Ġhall', 'ow', 'een', 'Ġdate', 'nas', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', 'Ġenters', 'Ġrealm', 'Ġheavy', 'lift', 'Ġrocket', 'ry', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġwall', 'ike', 'Ġj', 'uly', 'space', 'x', "'s", 'Ġbig', 'Ġnew', 'Ġrocket', 'Ġmay', 'Ġcrash', 'st', 'Ġflight', 'Ġel', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġmus', 'k', 'Ġel', 'Ġj', 'uly', 'Ġel', 'Ġmus', 'k', 'Ġiss', 'Ġr', 'Ġconference', 'video', 'Ġiss', 'Ġr', 'Ġconference', 'Ġwashing']</t>
+          <t>['ars', 'Ġretrieved', 'Ġoct', 'ober', 'ars', 'enter', 'prise', 'Ġservices', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġf', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'global', 'Ġmobile', 'Ġbroadband', 'ars', 'Ġretrieved', 'Ġmarch', 'trans', 'forming', 'Ġsatellite', 'Ġnews', 'g', 'athering', 'Ġtext', 'false', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'one', 'Ġworld', 'Ġone', 'Ġnumber', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġwik', 'ipedia', 'Ġprovides', 'eyes', 'Ġears', 'Ġoil', 'Ġrigs', 'en', 'text', 'false', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'low', 'cost', 'Ġhand', 'held', 'Ġfixed', 'Ġvoice', 'Ġservices', 'ars', 'ces', 'aces', 'ars', 'Ġsatellite', 'Ġsystem', 'Ġworks', 'Ġw', 'cc', 'lp', 'Ġarchived', 'Ġoriginal', 'Ġn', 'ex', 'asp', 'pg', 'id', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġglobal', 'Ġx', 'press', 'Ġcoverage', 'low', 'res', 'pdf', 'ars', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'mar', 'itime', 'Ġsolution', 'Ġoverview', 'sh', 'ane', 'Ġro', 'ss', 'b', 'acher', 'dig', 'itals', 'hip', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġhen', 'ry', 'Ġc', 'aleb', 'mber', 'arian', 'e', 'Ġlaunches', 'Ġsatellites', 'ars', 'sp', 'ac', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', 'air', 'bus', 'built', 'ars', 'Ġsatellite', 'Ġbreaks', 'Ġworld', 'Ġrecord', 'Ġmission', 'Ġlifespan', 'ion', 'lif', 'es', 'pan', 'Ġvia', 'Ġsatellite', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'ars', 'Ġnational', 'Ġspace', 'Ġscience', 'Ġdata', 'Ġcenter', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgo', 'Ġgiant', 'Ġcomm']</t>
         </is>
       </c>
       <c r="C264" t="n">
@@ -3870,7 +3870,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>['ton', 'Ġu', 'Ġevent', 'Ġoccurs', '00', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'Ġlot', 'Ġrisk', 'Ġassociated', 'Ġfal', 'con', 'Ġheavy', 'Ġreal', 'Ġgood', 'Ġchance', 'Ġvehicle', 'Ġmake', 'Ġorbit', 'Ġ...', 'Ġhope', 'Ġmakes', 'Ġfar', 'Ġenough', 'Ġaway', 'Ġpad', 'Ġcause', 'Ġpad', 'Ġdamage', 'Ġwould', 'Ġconsider', 'Ġeven', 'Ġwin', 'Ġhonest', 'Ġ...', 'Ġthink', 'Ġfal', 'con', 'Ġheavy', 'Ġgoing', 'Ġgreat', 'Ġvehicle', 'Ġmuch', 'Ġreally', 'Ġimpossible', 'Ġtest', 'Ġground', "'ll", 'Ġbest', 'Ġ...', 'Ġactually', 'Ġended', 'Ġway', 'Ġharder', 'Ġfal', 'con', 'Ġheavy', 'Ġthought', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsounds', 'Ġreal', 'Ġeasy', 'Ġstick', 'Ġtwo', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstages', 'Ġstrap', 'Ġboosters', 'Ġhard', 'Ġeverything', 'Ġchanges', 'Ġloads', 'Ġchange', 'Ġaer', 'odynamics', 'Ġtotally', 'Ġchange', 'Ġtripled', 'Ġvibration', 'Ġac', 'oust', 'ics', 'Ġbreak', 'Ġqual', 'ï', '¬', 'ģ', 'cation', 'Ġlevels', 'Ġhardware', 'Ġredesign', 'Ġcenter', 'Ġcore', 'Ġair', 'frame', 'Ġseparation', 'Ġsystems', 'Ġ...', 'Ġreally', 'Ġway', 'Ġway', 'ï', '¬', 'ģ', 'cult', 'Ġoriginally', 'Ġthought', 'Ġpretty', 'Ġnaive', 'Ġ...', 'Ġoptimized', "'s", 'Ġtimes', 'Ġpayload', 'Ġcapability', 'Ġfal', 'con', '."', 'Ġmus', 'k', 'Ġel', 'Ġde', 'cember', 'j', 'une', 'Ġse', 'pt', 'ember', 'Ġupdate', 'http', 'space', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġbo', 'oz', 'er', 'Ġr', 'Ġmarch', 'rocket', 'us', 'ability', 'Ġdriver', 'Ġeconomic', 'Ġgrowth', 'http', 'hes', 'p', 'Ġspace', 'Ġreview', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'Ġmus', 'k', 'Ġel', 'Ġaug', 'ust', 'trans', 'cript', 'Ġel', 'Ġmus', 'k', 'Ġfuture', 'Ġspace', 'x', 'web', 'arch', 'iv', 'Ġshit', 'el', 'ons', 'ays', 'Ġmars', 'Ġsociety', 'Ġconference', 'Ġboulder', 'Ġcolor', 'ado', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'f']</t>
+          <t>['Ġsatellite', 'Ġnews', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'Ġc', 'aleb', 'Ġhen', 'ry', 'Ġj', 'une', 'ars', 'Ġsatellite', 'Ġrel', 'ocating', 'Ġcover', 'Ġmiddle', 'Ġeast', 'ia', 'Ġvia', 'Ġsatellite', 'Ġretrieved', 'Ġde', 'cember', 'ils', 'Ġpro', 'ton', 'Ġsuccessfully', 'Ġlaunches', 'ars', 'Ġsatellite', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'fl', 'aw', 'less', 'Ġlaunch', 'Ġal', 'phas', 'Ġtelecom', 'atellite', 'Ġes', 'Ġj', 'uly', 'Ġsatellites', 'ars', 'Ġretrieved', 'Ġjan', 'uary', 'ars', ')"', 'Ġspace', 'sky', 'rocket', 'de', 'Ġretrieved', 'Ġjan', 'uary', 'ars', 'Ġbegins', 'Ġglobal', 'Ġx', 'press', 'Ġroll', '09', 'Ġnews', 'Ġde', 'cember', 'ars', 'Ġinternational', 'Ġlaunch', 'Ġservices', 'Ġde', 'cember', 'ars', 'Ġwik', 'ipedia', 'ars', 'Ġlaunches', 'Ġsecond', 'Ġglobal', 'Ġx', 'press', 'Ġsatellite', 'Ġment', 'Ġnews', 'Ġfe', 'b', 'ruary', 'Ġmission', 'mission', 'ars', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ars', 'Ġpurchase', 'Ġfourth', 'ars', 'Ġsatellite', 'Ġbo', 'e', 'ing', 'press', 'Ġrelease', 'ars', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġmission', 'Ġspace', 'Ġx', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ars', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġsuccessful', 'Ġlaunch', 'ars', 'atell', 'ites', 'ars', 'Ġretrieved', 'Ġde', 'cember', 'Ġï', '¬', 'ģ', 'r', 'st', 'ars', 'Ġspacecraft', 'Ġscheduled', 'Ġlaunch', 'ub', 'ishi', 'Ġheavy', 'Ġindustries', 'hi', 'Ġend', 'Ġsecond', 'Ġfollow', '."', 'ars', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġsuccessful', 'Ġlaunch', 'Ġworld']</t>
         </is>
       </c>
       <c r="C265" t="n">
@@ -3883,7 +3883,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>['dragon', 'Ġpreparing', 'Ġiss', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġmarch', 'space', 'x', 'Ġaims', 'Ġdebut', 'Ġnew', 'Ġversion', 'Ġfal', 'con', 'Ġsummer', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġspace', 'x', 'Ġde', 'cember', 'fal', 'con', 'Ġheavy', 'Ġinter', 'stage', 'Ġpre', 'pped', 'Ġrocket', 'Ġfactory', 'Ġf', 'h', 'Ġï', '¬', 'Ĥ', 'ies', 'Ġnext', 'Ġyear', 'Ġpowerful', 'Ġoperational', 'Ġrocket', 'Ġworld', 'Ġfactor', 'Ġtwo', 'ht', 'Ġinst', 'agram', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'fal', 'con', 'Ġheavy', 'Ġtest', 'Ġstand', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġmay', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġmay', 'space', 'x', 'Ġproves', 'Ġfal', 'con', 'Ġheavy', 'Ġindeed', 'Ġreal', 'Ġrocket', 'Ġtest', 'Ġï', '¬', 'ģ', 'ring', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'space', 'x', 'Ġmay', 'first', 'Ġstatic', 'Ġï', '¬', 'ģ', 'Ġtest', 'Ġfal', 'con', 'Ġheavy', 'Ġcenter', 'Ġcore', 'Ġcompleted', 'Ġmc', 'greg', 'Ġrocket', 'Ġdevelopment', 'Ġfacility', 'Ġlast', 'Ġweek', 'weet', 'Ġretrieved', 'Ġmay', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġse', 'pt', 'ember', 'fal', 'con', 'Ġheavy', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġcores', 'Ġcompleted', 'Ġtesting', 'Ġrocket', 'Ġdevelopment', 'Ġfacility', 'Ġmc', 'greg', 'Ġtex', 'Ġ01', 'weet', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġperforms', 'Ġcrucial', 'Ġtest', 'Ġï', '¬', 'ģ', 'Ġfal', 'con', 'Ġheavy', 'Ġpotentially', 'Ġpaving', 'Ġway', 'Ġlaunch', 'ww', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'u', 'Ġspace', 'x', 'Ġbuild', 'Ġheavy', 'lift', 'Ġlow', 'cost', 'Ġrocket', 'uters', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'x', 'Ġannounces', 'Ġlaunch', 'Ġdate', 'Ġworld', "'s", 'Ġpowerful']</t>
+          <t>["'s", 'Ġadvanced', 'Ġsatellite', 'ars', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġsuccessfully', 'Ġlaunched', 'ars', "'s", 'Ġlatest', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġlast', 'Ġnight', 'Ġlaunch', 'Ġpad', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', '."', 'æµ', '·', 'äº', 'ĭ', 'åį', '«', 'æĺ', 'Ł', 'çĶ', 'µ', 'è¯', 'Ŀ', 'åı', '·', 'æ', '®', 'µ', 'æ', 'Ĭ', 'ķ', 'â', '¼', 'Ĭ', 'ä½¿', 'â', '½', '¤', 'Ġch', 'inese', 'hu', 'Ġnews', 'Ġj', 'uly', 'global', 'Ġx', 'press', 'Ġseamless', 'Ġsatellite', 'Ġbroadband', 'ars', 'Ġal', 'x', 'press', 'ars', 'global', 'Ġexpress', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'bel', 'gian', 'Ġcourt', 'Ġpunches', 'Ġhole', 'ars', "'s", 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġspac', 'en', 'ews', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'successful', 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġshows', 'Ġe', 'Ġtrack', 'Ġlaunch', 'ars', 'Ġaviation', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġde', 'utsche', 'Ġtele', 'k', 'om', 'Ġcomplete', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġspac', 'en', 'ews', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'euro', 'pe', 'Ġaviation', 'Ġnetwork', 'ean', 'ï', '¬', 'Ĥ', 'ight', 'Ġbroadband', 'Ġavailable', 'Ġthousands', 'Ġairline', 'Ġpassengers', 'ars', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ã¶', 'Ġjan', 'uary', 'euro', 'pe', "'s", 'Ġfastest', 'ï', '¬', 'Ĥ', 'ight', 'Ġwi', 'fi', 'Ġservice', 'Ġexpands', 'Ġcoverage', 'http', 'Ġft', 'n', 'news', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ars', 'Ġservices', 'ars', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġretrieved', 'Ġmarch', 'voice', 'ars', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġwik', 'ipedia', 'phone', 'Ġoverview', 'ars', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmarch', 'Ġservices', 'Ġglance', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġse']</t>
         </is>
       </c>
       <c r="C266" t="n">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>['Ġrocket', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġse', 'pt', 'ember', 'first', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġscheduled', 'Ġspring', 'http', 'sp', 'ac', 'ene', 'Ġspac', 'en', 'ews', 'Ġarchived', 'http', 'web', 'archive', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'launch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'http', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġseeks', 'Ġaccelerate', 'Ġfal', 'con', 'Ġproduction', 'Ġlaunch', 'Ġrates', 'Ġyear', 'year', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġaug', 'ust', 'pad', 'Ġhardware', 'Ġchanges', 'Ġpreview', 'Ġnew', 'Ġera', 'Ġspace', 'Ġcoast', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'space', 'x', 'Ġpushing', 'Ġback', 'Ġtarget', 'Ġlaunch', 'Ġdate', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmars', 'Ġmission', 'Ġverge', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġoct', 'ober', 'launch', 'Ġschedule', 'Ġe', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'deb', 'ut', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġplanned', 'Ġearly', 'Ġnext', 'Ġyear', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġpl', 'ait', 'Ġphil', 'Ġde', 'cember', 'el', 'Ġmus', 'k', 'Ġroad', 'ster', 'Ġmars', 'Ġwire', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'mus', 'k', 'Ġsays', 'es', 'la', 'Ġcar', 'Ġï', '¬', 'Ĥ', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġspac', 'en', 'ews', 'Ġde', 'cember', 'Ġarchived', 'w', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde']</t>
+          <t>['Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'ars', 'Ġb', 'ars', 'Ġretrieved', 'Ġj', 'une', 'mission', 'Ġboost', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'Ġp', 'aves', 'Ġway', 'Ġwide', 'Ġhigh', 'Ġspeed', 'Ġdata', 'Ġcommunications', 'Ġeuro', 'pa', 'web', 'Ġportal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'new', 'Ġsatellites', 'Ġeuro', 'pe', 'Ġcommission', 'Ġstarts', 'Ġselection', 'Ġprocedure', 'Ġoperators', 'Ġpan', 'euro', 'pe', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'Ġeuro', 'pa', 'web', 'Ġportal', 'Ġretrieved', 'Ġapr', 'il', 'euro', 'pe', 'Ġcommission', 'Ġp', 'aves', 'Ġway', 'Ġeuro', 'pe', 'Ġmobile', 'Ġsatellite', 'Ġservices', 'press', 'Ġrelease', 'Ġeuro', 'pe', 'Ġcommission', 'Ġmay', 'mobile', 'Ġsatellite', 'Ġservices', 'Ġeuro', 'pe', 'Ġfrequently', 'Ġasked', 'Ġquestions', 'Ġeuro', 'pa', 'web', 'Ġportal', 'Ġretrieved', 'Ġapr', 'il', 'Ġfel', 'ix', 'Ġb', 'ate', 'Ġmay', 'ars', 'Ġsolar', 'Ġwin', 'Ġspectrum', 'Ġrights', 'uters', 'Ġretrieved', 'Ġapr', 'il', 'pan', 'euro', 'pe', 'Ġnumbers', 'Ġservices', 'Ġeuro', 'pe', 'Ġcommission', 'Ġretrieved', 'Ġapr', 'il', 'euro', 'pas', 'Ġhell', 'ass', 'Ġskyrocket', 'de', 'Ġretrieved', 'Ġmay', 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġone', 'Ġgiant', 'Ġstep', 'Ġcloser', 'ars', 'Ġaviation', 'Ġretrieved', 'Ġmarch', 'ï', '¬', 'Ĥ', 'ight', 'Ġwifi', 'Ġbattle', 'Ġeuro', 'pe', 'Ġtakes', 'Ġfinancial', 'Ġtimes', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'bel', 'gian', 'Ġcourt', 'Ġpunches', 'Ġhole', 'ars', "'s", 'Ġeuro', 'pe', 'Ġaviation', 'Ġnetwork', 'Ġspac', 'en', 'ews', 'Ġmarch', 'ars', 'Ġorders', 'Ġï', '¬', 'ģ', 'f', 'th', 'Ġglobal', 'Ġx', 'press', 'Ġsatellite', 'Ġth', 'ales', 'Ġal', 'en', 'ia', 'Ġspace', 'Ġspac', 'en', 'ews', 'Ġj', 'une', 'ars', 'Ġce', 'Ġhints', 'Ġadvanced', 'Ġglobal', 'Ġx', 'press', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġmarch', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġbuild', 'Ġtwo', 'Ġtriple', 'pay', 'load', 'Ġsatellites', 'Ġspace', 'way', 'Ġspace', 'x', 'Ġlaunch', 'htt', 'Ġace', 'x', 'launch', 'Ġspac', 'en', 'ews', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'ars']</t>
         </is>
       </c>
       <c r="C267" t="n">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>['cember', 'Ġkn', 'app', 'lex', 'Ġde', 'cember', 'el', 'Ġmus', 'k', 'Ġshows', 'Ġphotos', 'es', 'la', 'Ġroad', 'ster', 'Ġgetting', 'Ġpre', 'pped', 'Ġgo', 'Ġmars', 'Ġforb', 'es', 'Ġarchived', 'web', 'ar', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġke', 'lly', 'Ġem', 'Ġjan', 'uary', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġstatus', 'Ġupdates', 'Ġtargeting', 'Ġfr', 'iday', 'Ġtest', 'Ġï', '¬', 'ģ', 'Ġk', 'sc', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', '001', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġjan', 'uary', 'Ġshutdown', 'Ġmeans', 'Ġspace', 'x', "'t", 'Ġtest', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġcreating', 'Ġdelays', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'ap', 'atos', 'ennis', 'Ġjan', 'uary', 'Ġ01', 'Ġhistoric', 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġfire', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'el', 'mus', 'k', 'Ġjan', 'uary', 'aim', 'ing', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfal', 'con', 'Ġheavy', 'Ġfe', 'b', 'ruary', 'Ġap', 'ollo', 'Ġlaunch', 'pad', 'Ġcape', 'Ġk', 'enn', 'edy', 'Ġeasy', 'Ġviewing', 'Ġpublic', 'Ġcause', 'way', 'weet', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġfe', 'b', 'ruary', 'continue', 'Ġmonitor', 'Ġupper', 'Ġlevel', 'Ġwind', 'ar', 'Ġnew', 'Ġest', 'Ġut', 'c', 'weet', 'Ġvia', 'Ġtwitter', 'el', 'mus', 'k', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġside', 'Ġcores', 'Ġlanded', 'Ġspace', 'x', "'s", 'Ġlanding', 'Ġzones', 'weet', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġlanded', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġtwo', 'Ġboosters', 'Ġcore', 'Ġclipped', 'Ġdrone', 'Ġship', 'Ġmph', 'Ġg', 'iz', 'mod', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmiddle', 'Ġbooster', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġfailed', 'Ġland', 'Ġdrone', 'Ġship']</t>
+          <t>['Ġawards', 'Ġcontract', 'Ġair', 'bus', 'ars', 'hi', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'ars', 'Ġsatellite', 'ars', 'ars', 'Ġwik', 'ipedia', 'atellite', 'Ġcommunication', 'Ġair', 'Ġtra', 'f', 'ï', '¬', 'ģ', 'c', 'Ġmanagement', 'iris', ')"', 'Ġes', 'int', 'esa', 'Ġusing', 'ars', 'Ġir', 'Ġopen', 'Ġskies', 'Ġav', 'ionics', 'Ġaviation', 'today', 'Ġmarch', 'ice', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġretrieved', 'Ġmarch', 'ars', 'Ġinterference', 'Ġinformation', 'ars', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmarch', 'ï', '¬', 'ģ', 'cial', 'Ġwebsite', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C268" t="n">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>['ww', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', "'s", 'es', 'la', 'shot', 'Ġmars', 'Ġorbit', "'t", 'Ġreach', 'Ġasteroid', 'Ġbelt', 'Ġclaimed', 'ww', 'Ġus', 'k', 'ars', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġyear', 'Ġcolossal', 'Ġspace', 'x', 'Ġrocket', "'s", 'Ġdebut', 'Ġfal', 'con', 'Ġheavy', 'high', 'Ġvalue', 'Ġuses', 'Ġdespite', 'Ġskepticism', 'case', 'html', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġar', 'abs', 'Ġreset', 'uesday', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmarch', 'r', 'ides', 'hare', 'Ġmission', 'Ġu', 'Ġmilitary', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġsecond', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġoct', 'ober', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġaug', 'ust', 'ses', 'Ġagrees', 'Ġlaunch', 'Ġsatellite', 'ï', '¬', 'Ĥ', 'ight', 'proven', 'Ġfal', 'con', 'Ġrocket', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'mber', 'ars', 'Ġjuggling', 'Ġtwo', 'Ġlaunches', 'Ġsays', 'Ġspace', 'x', 'Ġreturn', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġj', 'une', 'Ġwatt', 'les', 'Ġjack', 'ie', 'mber', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġreturns', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġthree', 'Ġyears', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunches', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġmission', 'Ġus', 'Ġspace', 'Ġforce', 'sp', 'Ġspace', 'Ġjan', 'uary', 'Ġarchived']</t>
+          <t>['Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġrendering', 'Ġfully', 'Ġdeployed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġnames', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'ng', 'st', 'âĢĵ', 'Ġmission', 'Ġtype', 'Ġastronomy', 'Ġoperator', 'Ġst', 'sci', 'n', 'asa', ')[', 'Ġes', 'Ġc', 'sa', 'Ġcos', 'par', 'Ġid', 'Ġsat', 'cat', 'Ġwebsite', 'ï', '¬', 'ģ', 'cial', 'Ġwebsite', 'Ġweb', 'bt', 'el', 'esc', 'ope', 'org', 'Ġmission', 'Ġduration', 'Ġyear', 'Ġmonths', 'Ġdays', 'el', 'apsed', 'âģ', 'Ħ', 'Ġyears', 'primary', 'Ġmission', ')[', 'Ġyears', 'planned', 'Ġyears', 'expected', 'Ġspacecraft', 'Ġproperties', 'Ġmanufacturer', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġlaunch', 'Ġmass', 'Ġdimensions', 'Ġft', 'Ġsun', 'shield', 'Ġpower', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġde', 'cember', 'Ġrocket', 'ri', 'ane', 'Ġe', 'ca', 'Ġlaunch', 'Ġsite', 'Ġcentre', 'Ġspatial', 'Ġguy', 'ana', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġcontractor', 'rian', 'esp', 'ace', 'Ġentered', 'Ġservice', 'Ġj', 'uly', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġsun', 'âĢĵ', 'earth', 'Ġorbit', 'Ġregime', 'Ġh', 'alo', 'Ġorbit', 'Ġper', 'aps', 'Ġaltitude', '000', '000', 'Ġap', 'aps', 'Ġaltitude', '000', '000', 'Ġperiod', 'Ġmonths', 'Ġmain', 'Ġtelescope', 'Ġtype', 'Ġk', 'ors', 'ch', 'Ġtelescope', 'Ġdiameter', 'Ġft', 'Ġfocal', 'Ġlength', 'Ġft', 'Ġfocal', 'Ġratio', 'Ġcollecting', 'Ġarea', 'Ġwavelengths', 'âĢĵ', 'ĠÎ¼', 'orange', 'Ġmid', 'inf', 'rared', 'Ġtrans', 'p', 'ond', 'ers', 'Ġband', 'band', 'Ġtele', 'metry', 'Ġtele', 'command', 'Ġka', 'band', 'Ġscience', 'Ġdata', 'link', 'Ġbandwidth', 'band', 'Ġk', 'bit', 'band', 'Ġk', 'bit', 'Ġka', 'band', 'bit', 'Ġinstruments', 'Ġf', 'gs', 'nir', 'iss', 'Ġmir', 'Ġn', 'irc', 'Ġn', 'ir', 'spec', 'Ġelements', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'Ġspacecraft', 'bus', 'Ġsun', 'shield', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmission', 'Ġlogo', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', 'Ġspace', 'Ġtelescope', 'Ġspecifically', 'Ġdesigned', 'Ġconduct', 'Ġinfrared', 'Ġastronomy', 'Ġhigh', 'resolution', 'Ġhigh', 'ensitivity', 'Ġinstruments', 'Ġallow', 'Ġview', 'Ġobjects', 'Ġold']</t>
         </is>
       </c>
       <c r="C269" t="n">
@@ -3935,7 +3935,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>['h', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'v', 'ias', 'Ġameric', 'Ġsuccessfully', 'Ġlaunched', 'Ġv', 'ias', 'Ġmay', 'n', 'asa', 'Ġhead', 'Ġrules', 'Ġspace', 'x', 'Ġrockets', 'Ġmoon', 'Ġmission', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġj', 'uly', 'n', 'asa', "'s", 'Ġdaunting', 'Ġlist', 'Ġsending', 'Ġpeople', 'Ġback', 'Ġmoon', 'htt', 'Ġverge', 'Ġarchived', 'ary', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'Ġn', 'asa', 'Ġtries', 'Ġland', 'Ġmoon', 'Ġplenty', 'Ġrockets', 'Ġchoose', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'n', 'asa', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġfinal', 'ize', 'Ġmoon', 'Ġoutpost', 'Ġliving', 'Ġquarters', 'Ġcontract', 'n', 'asa', 'g', 'Ġn', 'asa', 'press', 'Ġrelease', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġselects', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġlunar', 'Ġrover', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'fal', 'con', 'Ġheavy', 'Ġoverview', 'Ġspace', 'x', 'Ġarchived', 'Ġe', 'avy', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'space', 'x', 'Ġannounces', 'Ġlaunch', 'Ġdate', 'Ġworld', "'s", 'Ġpowerful', 'Ġrocket', 'Ġspace', 'ref', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'oct', 'aw', 'eb', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'land', 'ing', 'Ġlegs', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġk', 'mer', 'Ġk', 'en', 'Ġjan', 'uary', 'fal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġbooster', 'Ġrecovery', 'Ġfeatured', 'Ġcool', 'Ġnew', 'Ġspace', 'x', 'Ġanimation', 'Ġuniverse', 'Ġtoday', 'Ġarchived']</t>
+          <t>['Ġdistant', 'Ġfaint', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġenables', 'Ġinvestigations', 'Ġacross', 'Ġmany', 'Ġfields', 'Ġastronomy', 'Ġcos', 'mology', 'Ġobservation', 'Ġfirst', 'Ġstars', 'Ġformation', 'Ġfirst', 'Ġgalaxies', 'Ġdetailed', 'Ġatmospheric', 'Ġcharacterization', 'Ġpotentially', 'Ġhabitable', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġu', 'Ġnational', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġadministration', 'n', 'asa', 'Ġled', 'Ġweb', 'b', "'s", 'Ġdesign', 'Ġdevelopment', 'Ġpartnered', 'Ġtwo', 'Ġmain', 'Ġagencies', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'esa', 'adian', 'Ġspace', 'Ġagency', 'cs', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'gs', 'fc', 'ary', 'land', 'Ġmanaged', 'Ġtelescope', 'Ġdevelopment', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġb', 'alt', 'imore', 'Ġhom', 'ew', 'ood', 'Ġcampus', 'Ġjohn', 'Ġhop', 'kins', 'Ġuniversity', 'Ġcurrently', 'Ġoperates', 'Ġweb', 'b', 'Ġprimary', 'Ġcontractor', 'Ġproject', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġtelescope', 'Ġnamed', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', 'Ġadministrator', 'Ġn', 'asa', 'Ġmercury', 'Ġgem', 'ini', 'Ġap', 'ollo', 'Ġprograms', 'Ġweb', 'b', 'Ġlaunched', 'Ġde', 'cember', 'ri', 'ane', 'Ġrocket', 'Ġk', 'ou', 'Ġfrench', 'Ġgu', 'iana', 'Ġarrived', 'Ġsun', 'âĢĵ', 'earth', 'Ġlag', 'range', 'Ġpoint', 'Ġjan', 'uary', 'Ġfirst', 'Ġweb', 'b', 'Ġimage', 'Ġreleased', 'Ġpublic', 'Ġvia', 'Ġpress', 'Ġconference', 'Ġj', 'uly', 'Ġweb', 'b', "'s", 'Ġprimary', 'Ġmirror', 'Ġconsists', 'Ġhex', 'agonal', 'Ġmirror', 'Ġsegments', 'Ġmade', 'Ġgold', 'pl', 'ated', 'Ġb', 'ery', 'ium', 'Ġcombined', 'Ġcreate', 'meter', 'iameter', 'Ġft', 'Ġmirror', 'Ġcompared', 'Ġhub', 'ble', "'s", 'Ġft', 'Ġgives', 'Ġweb', 'b', 'Ġlight', 'collect', 'ing', 'Ġarea', 'Ġsquare', 'Ġmeters', 'Ġtimes', 'Ġhub', 'ble', 'Ġunlike', 'Ġhub', 'ble', 'Ġobserves', 'Ġnear', 'Ġultraviolet', 'Ġvisible', 'ĠÂµ', 'Ġnear', 'Ġinfrared', 'âĢĵ', 'Ġspect', 'ra', 'Ġweb', 'b', 'Ġobserves', 'Ġlower', 'Ġfrequency', 'Ġrange', 'Ġlong', 'wa', 'velength', 'Ġvisible', 'Ġlight', 'red', 'Ġmid', 'inf', 'rared', 'âĢĵ', 'ĠÂµ', 'Ġtelescope', 'Ġmust', 'Ġkept', 'Ġextremely', 'Ġcold', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', 'Ġinfrared', 'Ġlight', 'Ġemitted', 'Ġtelescope']</t>
         </is>
       </c>
       <c r="C270" t="n">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġn', 'ield', 'Ġge', 'orge', 'Ġc', 'ap', 'ril', 'Ġdraft', 'Ġenvironmental', 'Ġimpact', 'Ġstatement', 'Ġspace', 'x', 'Ġtex', 'Ġlaunch', 'Ġsite', 'report', 'Ġvol', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'ï', '¬', 'ģ', 'ce', 'Ġcommercial', 'Ġspace', 'Ġtransportation', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġsim', 'berg', 'Ġrand', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', 'Ġspace', 'x', "'s", 'Ġreusable', 'Ġrocket', 'Ġplans', 'Ġpopular', 'Ġmechanics', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'f', 'iche', 'Ġtechnique', 'Ġfal', 'con', 'Ġheavy', 'technical', 'Ġdata', 'Ġsheet', 'Ġfal', 'con', 'Ġheavy', '].', 'Ġes', 'pace', 'Ġexploration', 'Ġfrench', 'Ġj', 'une', 'Ġpp', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġk', 'sc', 'Ġjan', 'uary', 'Ġut', 'c', ')"', 'forum', 'n', 'Ġretrieved', 'Ġjan', 'uary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'seeking', 'Ġhuman', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġprogram', 'Ġworthy', 'Ġgreat', 'Ġnation', 'na', 'Ġn', 'asa', 'Ġoct', 'ober', 'Ġarchived', 'http', 'Ġreport', 'pdf', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', 'Ġenters', 'Ġrealm', 'Ġheavy', 'lift', 'Ġrocket', 'ry', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'Ġexploration', 'Ġtechnologies', 'Ġcorporation', 'Ġfal', 'con', 'Ġheavy', 'Ġal', 'con', 'heavy', 'Ġspace', 'x', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġbroch', 'ure', 'Ġarchived', 'Ġoriginal', 'Ġace', 'x', 'bro', 'ch', 'ure', 'pdf', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġpress', 'Ġconference', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch']</t>
+          <t>['Ġinterfere', 'Ġcollected', 'Ġlight', 'Ġdeployed', 'Ġsolar', 'Ġorbit', 'Ġnear', 'Ġsun', 'âĢĵ', 'earth', 'Ġlag', 'range', 'Ġpoint', 'Ġmillion', 'Ġkilometers', '000', 'Ġmi', 'Ġearth', 'Ġfive', 'layer', 'Ġsun', 'shield', 'Ġprotects', 'Ġwarming', 'Ġsun', 'Ġearth', 'Ġmoon', 'Ġinitial', 'Ġdesigns', 'Ġtelescope', 'Ġnamed', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġbegan', 'Ġtwo', 'Ġconcept', 'Ġstudies', 'Ġcommissioned', 'Ġpotential', 'Ġlaunch', 'Ġbillion', 'Ġbudget', 'Ġprogram', 'Ġplagued', 'Ġenormous', 'Ġcost', 'Ġoverrun', 'Ġdelays', 'Ġmajor', 'Ġredesign', 'Ġled', 'Ġcurrent', 'Ġapproach', 'Ġconstruction', 'Ġcompleted', 'Ġtotal', 'Ġcost', 'Ġus', 'Ġbillion', 'Ġhigh', 'stakes', 'Ġnature', 'Ġlaunch', 'Ġtelescope', "'s", 'Ġcomplexity', 'Ġremarked', 'Ġupon', 'Ġmedia', 'Ġscientists', 'Ġengineers', 'Ġj', 'uly', 'Ġastronomers', 'Ġreported', 'Ġfirst', 'Ġyear', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġoperations', 'Ġconsiderable', 'Ġsuccess', 'Ġmass', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġhalf', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġweb', 'b', 'Ġft', ')-', 'iameter', 'Ġgold', 'co', 'ated', 'Ġb', 'ery', 'ium', 'Ġprimary', 'Ġmirror', 'Ġmade', 'Ġseparate', 'Ġhex', 'agonal', 'Ġmirrors', 'Ġmirror', 'Ġpolished', 'Ġarea', 'Ġft', 'Ġft', 'Ġobscured', 'Ġsecondary', 'Ġsupport', 'Ġstr', 'uts', 'Ġgiving', 'Ġtotal', 'Ġcollecting', 'Ġarea', 'Ġft', 'Ġtimes', 'Ġlarger', 'Ġcollecting', 'Ġarea', 'Ġhub', 'ble', "'s", 'Ġft', 'Ġdiameter', 'Ġmirror', 'Ġcollecting', 'Ġarea', 'Ġft', 'Ġmirror', 'Ġgold', 'Ġcoating', 'Ġprovide', 'Ġinfrared', 'Ġreflect', 'ivity', 'Ġcovered', 'Ġthin', 'Ġlayer', 'Ġglass', 'Ġdurability', 'Ġweb', 'b', 'Ġdesigned', 'Ġprimarily', 'Ġnear', 'inf', 'rared', 'Ġastronomy', 'Ġalso', 'Ġsee', 'Ġorange', 'Ġred', 'Ġvisible', 'Ġlight', 'Ġwell', 'Ġmid', 'inf', 'rared', 'Ġregion', 'Ġdepending', 'Ġinstrument', 'Ġused', 'Ġdetect', 'Ġobjects', 'Ġtimes', 'Ġf', 'ter', 'Ġhub', 'ble', 'Ġobjects', 'Ġmuch', 'Ġearlier', 'Ġhistory', 'Ġuniverse', 'Ġback', 'Ġred', 'shift', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime', 'Ġbig', 'Ġbang', ').[', 'Ġcomparison', 'Ġearliest', 'Ġstars', 'Ġthought', 'Ġformed', 'âĢĵ', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime']</t>
         </is>
       </c>
       <c r="C271" t="n">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġapr', 'il', 'fe', 'ibility', 'Ġdragon', 'derived', 'Ġmars', 'Ġland', 'er', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġhuman', 'pre', 'c', 'ursor', 'Ġinvestigations', 'htt', 'net', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġmay', 'cap', 'abilities', 'Ġservices', 'Ġbout', 'cap', 'abilities', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġties', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmarch', 'el', 'mus', 'k', 'Ġfe', 'b', 'ruary', 'side', 'Ġboosters', 'Ġlanding', 'Ġdrones', 'hips', 'Ġcenter', 'Ġexpended', 'Ġperformance', 'Ġpenalty', 'Ġfully', 'Ġexpended', 'Ġcost', 'Ġslightly', 'Ġhigher', 'Ġexpended', 'Ġaround', 'Ġmillion', 'weet', 'Ġvia', 'Ġtwitter', 'Ġmus', 'k', 'Ġel', 'Ġse', 'pt', 'ember', 'Ġbecoming', 'Ġmulti', 'planet', 'Ġspecies', 'video', 'Ġad', 'elaide', 'Ġaust', 'ral', 'ia', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġyoutube', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġjan', 'uary', 'mus', 'k', 'Ġambition', 'Ġspace', 'x', 'Ġaim', 'Ġfully', 'Ġreusable', 'Ġfal', 'con', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'fair', 'ing', 'Ġrecovery', 'Ġattempts', 'Ġspace', 'xf', 'le', 'et', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmarch', 'space', 'x', 'Ġï', '¬', 'Ĥ', 'ies', 'Ġrocket', 'Ġsecond', 'Ġtime', 'Ġhistoric', 'Ġtest', 'Ġcost', 'cutting', 'Ġtechnology', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'mus', 'k', 'Ġmarch', 'consider', 'ing', 'Ġtrying', 'Ġbring', 'Ġupper', 'Ġstage', 'Ġback', 'Ġfal', 'con', 'Ġheavy', 'Ġdemo', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġfull', 'us', 'ability', 'Ġodds', 'Ġsuccess', 'Ġlow', 'Ġmaybe', 'Ġworth', 'Ġshot', 'weet', 'Ġretrieved', 'Ġj', 'une', 'Ġvia', 'Ġtwitter', 'ula', 'Ġdelta', 'Ġiv', 'Ġreference', 'Ġpage', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġe', 'ts', 'elta', 'iv', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġstr', 'ick', 'land', 'Ġjohn', 'Ġk', 'se', 'pt', 'ember', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġbooster', 'http']</t>
+          <t>['Ġfirst', 'Ġgalaxies', 'Ġmay', 'Ġformed', 'Ġaround', 'Ġred', 'shift', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime', 'Ġhub', 'ble', 'Ġunable', 'Ġsee', 'Ġback', 'Ġearly', 'Ġz', 'âī', 'Ī', 'gal', 'axy', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime', ').[', 'Ġfeatures', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġrough', 'Ġplot', 'Ġearth', "'s", 'Ġatmospheric', 'Ġabsorption', 'Ġopacity', 'Ġvarious', 'Ġwavelengths', 'Ġelectromagnetic', 'Ġradiation', 'Ġincluding', 'Ġvisible', 'Ġlight', 'Ġdesign', 'Ġemphasizes', 'Ġnear', 'Ġmid', 'inf', 'rared', 'Ġseveral', 'Ġreasons', 'Ġhigh', 'red', 'shift', 'Ġearly', 'Ġdistant', 'Ġobjects', 'Ġvisible', 'Ġemissions', 'Ġshifted', 'Ġinfrared', 'Ġtherefore', 'Ġlight', 'Ġobserved', 'Ġtoday', 'Ġvia', 'Ġinfrared', 'Ġastronomy', 'Ġinfrared', 'Ġlight', 'Ġpasses', 'Ġeasily', 'Ġdust', 'Ġclouds', 'Ġvisible', 'Ġlight', 'Ġcolder', 'Ġobjects', 'Ġdebris', 'Ġdisks', 'Ġplanets', 'Ġemit', 'Ġstrongly', 'Ġinfrared', 'Ġinfrared', 'Ġbands', 'ï', '¬', 'ģ', 'cult', 'Ġstudy', 'Ġground', 'Ġexisting', 'Ġspace', 'Ġtelescopes', 'Ġhub', 'ble', 'Ġground', 'based', 'Ġtelescopes', 'Ġmust', 'Ġlook', 'Ġearth', "'s", 'Ġatmosphere', 'Ġopaque', 'Ġmany', 'Ġinfrared', 'Ġbands', 'see', 'Ġfigure', 'Ġright', 'Ġeven', 'Ġatmosphere', 'Ġtransparent', 'Ġmany', 'Ġtarget', 'Ġchemical', 'Ġcompounds', 'Ġwater', 'Ġcarbon', 'Ġdioxide', 'Ġmethane', 'Ġalso', 'Ġexist', 'Ġearth', "'s", 'Ġatmosphere', 'Ġvastly', 'Ġcompl', 'icating', 'Ġanalysis', 'Ġexisting', 'Ġspace', 'Ġtelescopes', 'Ġhub', 'ble', 'Ġcannot', 'Ġstudy', 'Ġbands', 'Ġsince', 'Ġmirrors', 'Ġinsufficient', 'ly', 'Ġcool', 'Ġhub', 'ble', 'Ġmirror', 'Ġmaintained', 'ĠÂ°', 'c', 'Ġk', 'ĠÂ°', 'f', '])', 'Ġmeans', 'Ġtelescope', 'Ġradi', 'ates', 'Ġstrongly', 'Ġrelevant', 'Ġinfrared', 'Ġbands', 'Ġweb', 'b', 'Ġalso', 'Ġobserve', 'Ġobjects', 'Ġsolar', 'Ġsystem', 'Ġangle', 'Â°', 'Ġsun', 'Ġapparent', 'Ġangular', 'Ġrate', 'Ġmotion', 'Ġless', '03', 'Ġarc', 'Ġseconds', 'Ġper', 'Ġsecond', 'Ġincludes', 'Ġmars', 'Ġj', 'upiter', 'Ġsat', 'urn', 'Ġur', 'anus', 'Ġne', 'pt', 'une', 'Ġpl', 'uto', 'Ġsatellites', 'ets', 'Ġasteroids', 'Ġminor', 'Ġplanets', 'Ġbeyond', 'Ġorbit', 'Ġmars', 'Ġweb', 'b', 'Ġnear', 'ir', 'Ġmid', 'ir', 'Ġsensitivity', 'Ġable', 'Ġobserve', 'Ġvirtually', 'Ġknown', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġobjects', 'Ġaddition', 'Ġobserve', 'Ġopportun', 'istic', 'Ġun', 'planned', 'Ġtargets', 'Ġwithin', 'Ġhours', 'Ġdecision']</t>
         </is>
       </c>
       <c r="C272" t="n">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>['n', 'ss', 'Ġnational', 'Ġspace', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'x', 'Ġannounces', 'Ġlaunch', 'Ġdate', 'Ġworld', "'s", 'Ġpowerful', 'Ġrocket', 'Ġspace', 'x', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'el', 'mus', 'k', 'Ġmay', 'Ġf', 'h', 'Ġexpend', 'able', 'Ġperformance', 'Ġinclude', 'Ġcross', 'feed', '?"', 'Ġcross', 'Ġfeed', 'Ġwould', 'Ġhelp', 'Ġperformance', 'Ġneeded', 'Ġnumbers', 'weet', 'Ġretrieved', 'Ġj', 'une', 'Ġvia', 'Ġtwitter', 'Ġenvironmental', 'Ġimpact', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', '?"', 'Ġscience', 'Ġfocus', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'avis', 'Ġj', 'ason', 'let', "'s", 'Ġtalk', 'Ġel', 'Ġmus', 'k', 'Ġlaunching', 'es', 'la', 'Ġspace', 'Ġplanetary', 'Ġsociety', 'Ġretrieved', 'Ġoct', 'ober', 'Ġpur', 'due', 'Ġuniversity', 'Ġfe', 'b', 'ruary', 'tes', 'la', 'Ġspace', 'Ġcould', 'Ġcarry', 'Ġbacteria', 'Ġearth', 'phy', 'Ġphys', 'org', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'z', 'ond', 'Ġdavid', 'Ġfe', 'b', 'ruary', 'es', 'la', 'Ġroad', 'ster', 'Ġcould', 'Ġdirt', 'iest', 'Ġman', 'made', 'Ġobject', 'Ġspace', 'Ġnew', 'las', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ad', 'option', 'Ġenvironmental', 'Ġassessment', 'Ġfinding', 'Ġsign', 'ï', '¬', 'ģ', 'c', 'ant', 'Ġimpact', 'Ġboost', 'back', 'Ġlanding', 'Ġfal', 'con', 'Ġheavy', 'Ġboosters', 'Ġlanding', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfl', 'ida', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġtestimony', 'Ġel', 'Ġmus', 'k', 'Ġmay', 'space', 'Ġshuttle', 'Ġfuture', 'Ġspace', 'Ġlaunch', 'Ġvehicles', 'Ġspace', 'ref', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une']</t>
+          <t>['Ġsuper', 'nov', 'ae', 'Ġgamma', 'Ġray', 'Ġbursts', 'Ġthree', 'quarter', 'Ġview', 'Ġtop', 'Ġbottom', 'sun', 'facing', 'Ġside', 'Ġlocation', 'Ġorbit', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġtest', 'Ġunit', 'Ġsun', 'shield', 'Ġstacked', 'Ġexpanded', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġfacility', 'Ġcal', 'ornia', 'Ġweb', 'b', 'Ġoperates', 'Ġh', 'alo', 'Ġorbit', 'Ġcircling', 'Ġaround', 'Ġpoint', 'Ġspace', 'Ġknown', 'Ġsun', 'âĢĵ', 'earth', 'Ġlag', 'range', 'Ġpoint', 'Ġapproximately', '000', '000', 'Ġmi', 'Ġbeyond', 'Ġearth', "'s", 'Ġorbit', 'Ġaround', 'Ġsun', 'Ġactual', 'Ġposition', 'Ġvaries', '000', '000', '000', 'âĢĵ', '000', 'Ġmi', 'Ġorbits', 'Ġkeeping', 'Ġearth', 'Ġmoon', "'s", 'Ġshadow', 'Ġway', 'Ġcomparison', 'Ġhub', 'ble', 'Ġorbits', 'Ġmi', 'Ġearth', "'s", 'Ġsurface', 'Ġmoon', 'Ġroughly', '000', '000', 'Ġmi', 'Ġearth', 'Ġobjects', 'Ġnear', 'Ġsun', 'âĢĵ', 'earth', 'Ġpoint', 'Ġorbit', 'Ġsun', 'Ġsynchron', 'Ġearth', 'Ġallowing', 'Ġtelescope', 'Ġremain', 'Ġroughly', 'Ġconstant', 'Ġdistance', 'Ġcontinuous', 'Ġorientation', 'Ġsun', 'shield', 'Ġequipment', 'Ġbus', 'Ġtoward', 'Ġsun', 'Ġearth', 'Ġmoon', 'Ġcombined', 'Ġwide', 'Ġshadow', 'avoid', 'ing', 'Ġorbit', 'Ġtelescope', 'Ġsimultaneously', 'Ġblock', 'Ġincoming', 'Ġheat', 'Ġlight', 'Ġthree', 'Ġbodies', 'Ġavoid', 'Ġeven', 'Ġsmallest', 'Ġchanges', 'Ġtemperature', 'Ġearth', 'Ġmoon', 'Ġshadows', 'Ġwould', 'Ġaffect', 'Ġstructure', 'Ġyet', 'Ġstill', 'Ġmaintain', 'Ġuninterrupted', 'Ġsolar', 'Ġpower', 'Ġearth', 'Ġcommunications', 'Ġsun', 'facing', 'Ġside', 'Ġarrangement', 'Ġkeeps', 'Ġtemperature', 'Ġspacecraft', 'Ġconstant', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', 'Ġnecessary', 'Ġfaint', 'Ġinfrared', 'Ġmake', 'Ġobservations', 'Ġinfrared', 'Ġspectrum', 'Ġweb', 'b', 'Ġmust', 'Ġkept', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', ');', 'Ġotherwise', 'Ġinfrared', 'Ġradiation', 'Ġtelescope', 'Ġwould', 'Ġoverwhelm', 'Ġinstruments', 'Ġlarge', 'Ġsun', 'shield', 'Ġblocks', 'Ġlight', 'Ġheat', 'Ġsun', 'Ġearth', 'Ġmoon', 'Ġposition', 'Ġnear', 'Ġsun', 'âĢĵ', 'earth', 'Ġkeeps', 'Ġthree', 'Ġbodies', 'Ġside', 'Ġspacecraft', 'Ġtimes', 'Ġh', 'alo', 'Ġorbit', 'Ġaround', 'Ġpoint', 'Ġavoids', 'Ġshadow', 'Ġearth', 'Ġmoon', 'Ġmaintaining', 'Ġconstant', 'Ġenvironment', 'Ġsun', 'shield', 'Ġsolar', 'Ġarrays', 'Ġresulting', 'Ġstable', 'Ġtemperature', 'Ġstructures', 'Ġdark', 'Ġside', 'Ġcritical']</t>
         </is>
       </c>
       <c r="C273" t="n">
@@ -3987,7 +3987,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>['iet', 'zen', 'Ġfrank', 'Ġmarch', 'sp', 'ac', 'el', 'ift', 'Ġwashing', 'ton', 'Ġinternational', 'Ġspace', 'Ġtransportation', 'Ġassociation', 'Ġfal', 'tering', 'Ġmyth', 'Ġus', '000', 'Ġper', 'Ġpound', 'Ġw', 'html', 'id', 'Ġspace', 'ref', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'cap', 'abilities', 'Ġservices', 'mber', 'Ġarchived', 'Ġoriginal', 'cap', 'abilities', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmarch', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'cap', 'abilities', 'Ġj', 'uly', 'space', 'x', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'cap', 'abilities', 'Ġservices', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġdod', 'son', 'Ġg', 'ere', 'l', 'le', 'Ġj', 'uly', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġpace', 'tel', 'esc', 'ope', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'elta', 'Ġiv', 'Ġul', 'al', 'aunch', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġv', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġset', 'Ġlaunch', 'Ġmassive', 'Ġsatellite', 'Ġj', 'uly', 'nd', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġdays', 'es', 'lar', 'ati', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ars', 'Ġjuggling', 'Ġtwo', 'Ġlaunches', 'Ġsays', 'Ġspace', 'x', 'Ġreturn', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'http', 'sp', 'ac', 'en', 'ews', 'c', 'Ġspac', 'en', 'ews', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġde', 'cember', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġset', 'Ġfal', 'con', 'Ġheavy', 'Ġdebut', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary']</t>
+          <t>['Ġmaintaining', 'Ġprecise', 'Ġalignment', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġfive', 'layer', 'Ġsun', 'shield', 'Ġlayer', 'Ġthin', 'Ġhuman', 'Ġhair', 'Ġmade', 'Ġk', 'apt', 'Ġfilm', 'Ġcoated', 'Ġaluminum', 'Ġsides', 'Ġlayer', 'oped', 'Ġsilicon', 'Ġsun', 'facing', 'Ġside', 'Ġtwo', 'Ġhottest', 'Ġlayers', 'Ġreflect', 'Ġsun', "'s", 'Ġheat', 'Ġback', 'Ġspace', 'Ġaccidental', 'Ġtears', 'Ġdelicate', 'Ġfilm', 'Ġstructure', 'Ġdeployment', 'Ġtesting', 'Ġled', 'Ġdelays', 'Ġtelescope', 'Ġsun', 'shield', 'Ġdesigned', 'Ġfolded', 'Ġtwelve', 'Ġtimes', 'concert', 'ina', 'Ġstyle', 'Ġwould', 'Ġfit', 'Ġwithin', 'ri', 'ane', 'Ġrocket', "'s", 'Ġpayload', 'Ġfair', 'ing', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġlong', 'Ġshield', "'s", 'Ġfully', 'Ġdeployed', 'Ġdimensions', 'Ġplanned', 'Ġft', 'Ġkeeping', 'Ġwithin', 'Ġshadow', 'Ġsun', 'shield', 'Ġlimits', 'Ġfield', 'Ġregard', 'Ġweb', 'b', 'Ġgiven', 'Ġtime', 'Ġtelescope', 'Ġsee', 'Ġpercent', 'Ġone', 'Ġposition', 'Ġsee', 'Ġperiod', 'Ġmonths', 'Ġweb', 'b', "'s", 'Ġprimary', 'Ġmirror', 'Ġft', ')-', 'iameter', 'Ġgold', 'co', 'ated', 'Ġb', 'ery', 'ium', 'Ġreflect', 'Ġcollecting', 'Ġarea', 'Ġft', 'Ġdesigned', 'Ġsingle', 'Ġlarge', 'Ġmirror', 'Ġwould', 'Ġlarge', 'Ġexisting', 'Ġlaunch', 'Ġvehicles', 'Ġmirror', 'Ġtherefore', 'Ġcomposed', 'Ġhex', 'agonal', 'Ġsegments', 'Ġsun', 'shield', 'Ġprotection', 'Ġoptics', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġengineers', 'Ġcleaning', 'Ġtest', 'Ġmirror', 'Ġcarbon', 'Ġdioxide', 'Ġsnow', 'Ġmain', 'Ġmirror', 'Ġassembly', 'Ġfront', 'Ġprimary', 'Ġmirrors', 'Ġattached', 'mber', 'Ġdiff', 'raction', 'Ġspikes', 'Ġdue', 'Ġmirror', 'Ġsegments', 'Ġspider', 'Ġcolor', 'coded', 'Ġtechnique', 'Ġpioneered', 'Ġguid', 'Ġhorn', 'art', 'uro', 'Ġunfolded', 'Ġtelescope', 'Ġlaunched', 'Ġimage', 'Ġplane', 'Ġwave', 'front', 'Ġsensing', 'Ġphase', 'Ġretrieval', 'Ġused', 'Ġposition', 'Ġmirror', 'Ġsegments', 'Ġcorrect', 'Ġlocation', 'Ġusing', 'Ġprecise', 'Ġactu', 'ators', 'Ġsubsequent', 'Ġinitial', 'Ġconfiguration', 'Ġneed', 'Ġoccasional', 'Ġupdates', 'Ġevery', 'Ġdays', 'Ġretain', 'Ġoptimal', 'Ġfocus', 'Ġunlike', 'Ġterrestrial', 'Ġtelescopes', 'Ġexample', 'Ġke', 'ck', 'Ġtelescopes', 'Ġcontinually', 'Ġadjust', 'Ġmirror', 'Ġsegments', 'Ġusing', 'Ġactive', 'Ġoptics', 'Ġovercome', 'Ġeffects', 'Ġgravitational', 'Ġwind', 'Ġloading']</t>
         </is>
       </c>
       <c r="C274" t="n">
@@ -4000,7 +4000,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>['Ġgovernment', 'opened', 'Ġspace', 'x', 'Ġsought', 'Ġtwo', 'Ġfal', 'con', 'Ġheavy', 'Ġpermits', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'two', 'months', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'draft', 'Ġenvironmental', 'Ġassessment', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġlaunches', 'Ġk', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'Ġfederal', 'Ġaviation', 'Ġadministration', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġoct', 'ober', 'fal', 'con', 'heavy', 'block', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'tes', 'la', 'Ġroad', 'ster', 'aka', 'Ġstar', 'man', '017', ')"', 'sd', 'j', 'pl', 'n', 'asa', 'gov', 'Ġn', 'asa', 'Ġmarch', 'Ġarchived', 'Ġmand', '=-', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġroar', 'Ġthunder', 'Ġcarries', 'Ġspace', 'x', "'s", 'Ġambition', 'Ġorbit', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġde', 'cember', 'pay', 'load', 'Ġmidnight', 'Ġcherry', 'es', 'la', 'Ġroad', 'ster', 'Ġplaying', 'Ġspace', 'Ġodd', 'ity', 'Ġdestination', 'Ġmars', 'Ġorbit', 'Ġdeep', 'Ġspace', 'Ġbillion', 'Ġyears', "'t", 'Ġblow', 'Ġascent', 'weet', 'Ġretrieved', 'Ġde', 'cember', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġde', 'cember', 'Ġred', 'Ġcar', 'Ġred', 'Ġplanet', 'weet', 'Ġretrieved', 'Ġjan', 'uary', 'Ġvia', 'Ġtwitter', 'Ġapr', 'il', 'launch', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġpushed', 'Ġth', 'ursday', 'Ġw', 'l', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'ar', 'abs', 'Ġgun']</t>
+          <t>['Ġweb', 'b', 'Ġtelescope', 'Ġuses', 'Ġsmall', 'Ġact', 'uation', 'Ġmotors', 'Ġposition', 'Ġadjust', 'Ġoptics', 'Ġactu', 'ators', 'Ġposition', 'Ġmirror', 'Ġnan', 'ometer', 'Ġaccuracy', 'Ġweb', 'b', "'s", 'Ġoptical', 'Ġdesign', 'Ġthree', 'mir', 'ror', 'ast', 'igmat', 'Ġmakes', 'Ġuse', 'Ġcurved', 'Ġsecondary', 'Ġtert', 'iary', 'Ġmirrors', 'Ġdeliver', 'Ġimages', 'Ġfree', 'Ġoptical', 'Ġab', 'err', 'ations', 'Ġwide', 'Ġfield', 'Ġsecondary', 'Ġmirror', 'Ġft', 'Ġdiameter', 'Ġaddition', 'Ġfine', 'Ġsteering', 'Ġmirror', 'Ġadjust', 'Ġposition', 'Ġmany', 'Ġtimes', 'Ġper', 'Ġsecond', 'Ġprovide', 'Ġimage', 'Ġstabilization', 'Ġphotographs', 'Ġtaken', 'Ġweb', 'b', 'Ġspikes', 'Ġplus', 'Ġtwo', 'Ġf', 'ter', 'Ġones', 'Ġdue', 'Ġspider', 'Ġsupporting', 'Ġsecondary', 'Ġmirror', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', 'Ġframework', 'Ġprovides', 'Ġelectrical', 'Ġpower', 'Ġcomputing', 'Ġresources', 'Ġcooling', 'Ġcapability', 'Ġwell', 'Ġstructural', 'Ġstability', 'Ġweb', 'b', 'Ġtelescope', 'Ġmade', 'Ġbonded', 'Ġgraph', 'ite', 'ep', 'oxy', 'Ġcomposite', 'Ġattached', 'Ġunderside', 'Ġweb', 'b', "'s", 'Ġtelescope', 'Ġstructure', 'im', 'Ġholds', 'Ġfour', 'Ġscience', 'Ġinstruments', 'Ġguide', 'Ġcamera', 'Ġn', 'irc', 'near', 'Ġinfrared', 'Ġcamera', 'Ġinfrared', 'Ġim', 'ager', 'Ġspectral', 'Ġcoverage', 'Ġranging', 'Ġedge', 'Ġvisible', 'ĠÎ¼', 'Ġnear', 'Ġinfrared', 'Ġsensors', 'Ġmeg', 'ap', 'ixels', 'Ġn', 'irc', 'Ġserves', 'Ġobserv', 'atory', "'s", 'Ġwave', 'front', 'Ġsensor', 'Ġrequired', 'Ġwave', 'front', 'Ġsensing', 'Ġcontrol', 'Ġactivities', 'Ġused', 'Ġalign', 'Ġfocus', 'Ġmain', 'Ġmirror', 'Ġsegments', 'Ġn', 'irc', 'Ġbuilt', 'Ġteam', 'Ġled', 'Ġuniversity', 'ri', 'zona', 'Ġprincipal', 'Ġinvestigator', 'Ġmar', 'cia', 'Ġj', 'Ġn', 'ir', 'spec', 'near', 'Ġinfrared', 'Ġspect', 'rog', 'raph', 'Ġperforms', 'Ġspect', 'rosc', 'opy', 'Ġwavelength', 'Ġrange', 'Ġbuilt', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġest', 'ec', 'Ġnet', 'lands', 'Ġleading', 'Ġdevelopment', 'Ġteam', 'Ġincludes', 'Ġmembers', 'Ġair', 'bus', 'Ġdefence', 'Ġspace', 'tt', 'ob', 'run', 'n', 'Ġfried', 'rich', 'sh', 'af', 'en', 'Ġg', 'erman', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġpier', 'Ġfer', 'ruit', 'Ã©', 'co', 'le', 'Ġnorm', 'ale', 'Ġsup', 'Ã©', 'rie', 'ure', 'Ġde', 'Ġl', 'yon', 'Ġn', 'ir', 'spec', 'Ġproject', 'Ġscientist', 'Ġn', 'ir', 'spec', 'Ġdesign', 'Ġprovides', 'Ġthree', 'Ġobserving', 'Ġmodes', 'Ġlow', 'resolution', 'Ġmode', 'Ġusing', 'Ġprism', 'Ġr', 'Ġmulti', 'object', 'Ġmode', 'Ġr', '00', 'Ġintegral', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġunit']</t>
         </is>
       </c>
       <c r="C275" t="n">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>['ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'ar', 'abs', 'Ġce', 'Ġfal', 'con', 'Ġheavy', 'Ġgives', 'Ġsatellite', 'Ġextra', 'Ġlife', 'Ġspac', 'en', 'ews', 'Ġapr', 'il', 'Ġarchived', 'Ġra', 'life', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġapr', 'il', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'space', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġsuccessful', 'Ġcommercial', 'Ġdebut', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'n', 'asa', 'Ġlooking', 'Ġlaunch', 'Ġdelayed', 'Ġspace', 'Ġscience', 'Ġmissions', 'Ġearly', 'Ġar', 'ly', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġgra', 'ham', 'iam', 'Ġapr', 'il', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunches', 'Ġar', 'abs', 'nas', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġke', 'lly', 'Ġem', 'Ġapr', 'il', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġcore', 'Ġbooster', 'Ġlost', 'Ġrough', 'Ġseas', 'Ġen', 'Ġroute', 'Ġport', 'aver', 'al', 'Ġfl', 'ida', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġapr', 'il', 'fal', 'con', 'Ġheavy', 'Ġstar', 'link', 'Ġheadline', 'Ġspace', 'x', "'s", 'Ġupcoming', 'Ġmanifest', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'space', 'x', 'Ġlaunch', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'n', 'asa', 'k', 'enn', 'edy', 'Ġspace', 'Ġcenter', 'pm', 'Ġyoutube', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'rocket', 'Ġlaunch', 'Ġviewing', 'Ġcape', 'aver', 'al', 'Ġwatch', 'Ġview', 'Ġsee', 'las', 'Ġdelta', 'Ġfal', 'con', 'Ġlaunches', 'Ġviewing', 'html', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'une', 'pre', 'view', 'Ġsucceed', 'Ġfail', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġtest', 'Ġsure', '..."', 'Ġplanetary']</t>
+          <t>['Ġlong', 'sl', 'Ġspect', 'rosc', 'opy', 'Ġmode', 'Ġswitching', 'Ġmodes', 'Ġdone', 'Ġoperating', 'Ġwavelength', 'Ġpre', 'selection', 'Ġmechanism', 'Ġcalled', 'Ġfilter', 'Ġwheel', 'Ġassembly', 'Ġselecting', 'Ġcorresponding', 'Ġdisp', 'ersive', 'Ġelement', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġinstruments', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġn', 'irc', 'Ġwrapped', 'Ġcalibration', 'Ġassembly', 'Ġone', 'Ġcomponent', 'Ġn', 'ir', 'spec', 'Ġinstrument', 'Ġmir', 'pr', 'ism', 'Ġgr', 'ating', 'Ġusing', 'Ġgr', 'ating', 'Ġwheel', 'Ġassembly', 'Ġmechanism', 'Ġmechanisms', 'Ġbased', 'Ġsuccessful', 'oph', 'ot', 'Ġwheel', 'Ġmechanisms', 'Ġinfrared', 'Ġspace', 'Ġobserv', 'atory', 'Ġmulti', 'object', 'Ġmode', 'Ġrelies', 'Ġcomplex', 'Ġmicro', 'sh', 'utter', 'Ġmechanism', 'Ġallow', 'Ġsimultaneous', 'Ġobservations', 'Ġhundreds', 'Ġindividual', 'Ġobjects', 'Ġanywhere', 'Ġn', 'ir', 'spec', "'s", 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġview', 'Ġtwo', 'Ġsensors', 'Ġmeg', 'ap', 'ixels', 'Ġmir', 'mid', 'inf', 'rared', 'Ġinstrument', 'Ġmeasures', 'Ġmid', 'long', 'inf', 'rared', 'Ġwavelength', 'Ġrange', 'Ġcontains', 'Ġmid', 'inf', 'rared', 'Ġcamera', 'Ġimaging', 'Ġspect', 'rom', 'eter', 'Ġmir', 'Ġdeveloped', 'Ġcollaboration', 'Ġn', 'asa', 'Ġconsortium', 'Ġeuro', 'pe', 'Ġcountries', 'Ġled', 'Ġge', 'orge', 'Ġr', 'ie', 'ke', 'un', 'iversity', 'ri', 'zona', 'Ġg', 'illian', 'Ġwr', 'ight', 'Ġastronomy', 'Ġtechnology', 'Ġcentre', 'Ġed', 'inburgh', 'Ġsc', 'ot', 'land', ').[', 'Ġtemperature', 'Ġmir', 'Ġmust', 'Ġexceed', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', '):', 'Ġhelium', 'Ġgas', 'Ġmechanical', 'Ġcooler', 'ited', 'Ġwarm', 'Ġside', 'Ġenvironmental', 'Ġshield', 'Ġprovides', 'Ġcooling', 'Ġf', 'gs', 'nir', 'iss', 'fine', 'Ġguidance', 'Ġsensor', 'Ġnear', 'Ġinfrared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'Ġled', 'adian', 'Ġspace', 'Ġagency', 'Ġproject', 'Ġscientist', 'Ġjohn', 'Ġh', 'utch', 'ings', 'z', 'berg', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġresearch', 'Ġcentre', 'Ġused', 'Ġstabilize', 'Ġline', 'sight', 'Ġobserv', 'atory', 'Ġscience', 'Ġobservations', 'Ġmeasurements', 'Ġused', 'Ġcontrol', 'Ġoverall', 'Ġorientation', 'Ġspacecraft', 'Ġdrive', 'Ġï', '¬', 'ģ', 'ne', 'Ġsteering', 'Ġmirror', 'Ġimage', 'Ġstabilization', 'adian', 'Ġspace', 'Ġagency', 'Ġalso', 'Ġprovided', 'Ġnear', 'Ġinfrared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'nir', 'iss', 'Ġmodule', 'Ġastronomical', 'Ġimaging', 'Ġspect', 'rosc', 'opy', 'ĠÎ¼', 'Ġwavelength', 'Ġrange', 'Ġled', 'Ġprincipal', 'Ġinvestigator', 'Ġren', 'Ã©', 'yon', 'Ġunivers', 'itÃ©', 'Ġde', 'Ġmont', 'rÃ©', 'al']</t>
         </is>
       </c>
       <c r="C276" t="n">
@@ -4026,7 +4026,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>['Ġsociety', 'Ġarchived', 'web', 'arch', 'iv', 'Ġe', 'w', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'lights', 'ail', 'Ġplanetary', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgreen', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', ')"', 'Ġages', 'td', 'green', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'green', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', ')"', 'Ġball', 'Ġaerospace', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġgreen', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'gp', 'im', ')"', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġcorp', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdeep', 'Ġspace', 'Ġatomic', 'Ġclock', 'ds', 'ac', 'Ġoverview', 'Ġarchived', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġn', 'asa', 'Ġaccessed', 'Ġde', 'cember', 'Ġgeneral', 'Ġatom', 'ics', 'Ġcompletes', 'Ġready', 'launch', 'Ġtesting', 'Ġorbital', 'Ġtest', 'Ġbed', 'Ġsatellite', 'Ġarchived', 'h', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġgeneral', 'Ġatom', 'ics', 'Ġelectromagnetic', 'Ġsystems', 'Ġpress', 'Ġrelease', 'Ġapr', 'il', 'space', 'x', 'Ġawarded', 'Ġtwo', 'Ġe', 'el', 'v', 'class', 'Ġmissions', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'http', 'space', 'Ġspace', 'x', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'form', 'os', 'Ġcosmic', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'oc', 'ulus', 'r', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'r', 'htm', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'fal', 'con', 'Ġoverloaded', 'Ġknowledge', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġscheduled', 'Ġoct', 'ober', 'Ġspace', 'ï', '¬', 'Ĥ', 'ights', 'Ġnews', 'Ġarchived', 'htt']</t>
+          <t>['Ġalthough', 'Ġoften', 'Ġreferred', 'Ġtogether', 'Ġunit', 'Ġn', 'ir', 'iss', 'Ġserve', 'Ġentirely', 'Ġdifferent', 'Ġpurposes', 'Ġone', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġinstrument', 'Ġpart', 'Ġobserv', 'atory', "'s", 'Ġsupport', 'Ġinfrastructure', 'Ġn', 'irc', 'Ġmir', 'Ġfeature', 'Ġstar', 'light', 'blocking', 'Ġcoron', 'agraph', 'Ġobservation', 'Ġfaint', 'Ġtargets', 'Ġextras', 'olar', 'Ġplanets', 'Ġcircumst', 'ellar', 'Ġdisks', 'Ġclose', 'Ġbright', 'Ġstars', 'Ġspacecraft', 'Ġbus', 'Ġprimary', 'Ġsupport', 'Ġcomponent', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġhosting', 'Ġmultitude', 'Ġcomputing', 'Ġcommunication', 'Ġelectric', 'Ġpower', 'Ġpropulsion', 'Ġstructural', 'Ġparts', 'Ġalong', 'Ġsun', 'shield', 'Ġforms', 'Ġspacecraft', 'Ġelement', 'Ġspace', 'Ġtelescope', 'Ġspacecraft', 'Ġbus', 'Ġsun', 'facing', 'warm', 'Ġside', 'Ġsun', 'shield', 'Ġoperates', 'Ġtemperature', 'ĠÂ°', 'c', 'Ġstructure', 'Ġspacecraft', 'Ġbus', 'Ġmass', 'Ġmust', 'Ġsupport', 'Ġspace', 'Ġtelescope', 'Ġmade', 'Ġprimarily', 'Ġgraph', 'ite', 'Ġcomposite', 'Ġmaterial', 'Ġassembly', 'Ġcompleted', 'Ġcal', 'ornia', 'Ġintegrated', 'Ġrest', 'Ġspace', 'Ġtelescope', 'Ġleading', 'Ġspacecraft', 'Ġbus', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġdiagram', 'Ġspacecraft', 'Ġbus', 'Ġsolar', 'Ġpanel', 'Ġgreen', 'Ġlight', 'Ġpurple', 'Ġpanels', 'Ġradi', 'ators', 'Ġcomparison', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġprimary', 'Ġmirror', 'Ġlaunch', 'Ġspacecraft', 'Ġbus', 'Ġrotate', 'Ġtelescope', 'Ġpointing', 'Ġprecision', 'Ġone', 'Ġarc', 'second', 'Ġisol', 'ates', 'Ġvibration', 'Ġtwo', 'Ġweb', 'b', 'Ġtwo', 'Ġpairs', 'Ġrocket', 'Ġengines', 'one', 'Ġpair', 'Ġredundancy', 'Ġmake', 'Ġcourse', 'Ġcorrections', 'Ġway', 'Ġstation', 'Ġkeeping', 'Ġmaintaining', 'Ġcorrect', 'Ġposition', 'Ġh', 'alo', 'Ġorbit', 'Ġeight', 'Ġsmaller', 'Ġthr', 'usters', 'Ġused', 'Ġattitude', 'Ġcontrol', 'Ġcorrect', 'Ġpointing', 'Ġspacecraft', 'Ġengines', 'Ġuse', 'Ġhyd', 'raz', 'ine', 'Ġfuel', 'Ġlit', 'ers', 'Ġu', 'Ġgallons', 'Ġlaunch', 'init', 'rogen', 'Ġtet', 'rox', 'ide', 'Ġoxid', 'izer', 'Ġlit', 'ers', 'Ġu', 'Ġgallons', 'Ġlaunch', ').[', 'Ġweb', 'b', 'Ġintended', 'Ġserv', 'iced', 'Ġspace', 'Ġcrew', 'ed', 'Ġmission', 'Ġrepair', 'Ġupgrade', 'Ġobserv', 'atory', 'Ġdone', 'Ġhub', 'ble', 'Ġwould', 'Ġcurrently', 'Ġpossible', 'Ġaccording', 'Ġn']</t>
         </is>
       </c>
       <c r="C277" t="n">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġcenter', 'Ġcore', 'Ġnarrowly', 'Ġmiss', 'Ġinverse', 'Ġj', 'une', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'uss', 'f', 'Ġspace', 'Ġforce', 'Ġsuccessfully', 'Ġcompletes', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'ero', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'air', 'Ġforce', 'Ġawards', 'Ġmillion', 'Ġlaunch', 'Ġservice', 'Ġcontracts', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġwins', 'Ġpotential', 'Ġus', 'Ġmillion', 'Ġcontract', 'Ġus', 'af', 'Ġn', 'ro', 'Ġsatellite', 'Ġlaunch', 'Ġservices', 'http', 'Ġh', 'services', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġr', 'v', 'ices', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'us', 'Ġspace', 'Ġforce', 'Ġtet', 'ra', 'Ġsatellite', 'Ġprepared', 'Ġlaunch', 'month', 'Ġintegration', 'Ġpar', 'abolic', 'Ġarc', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġse', 'pt', 'ember', 'space', 'x', "'s", 'Ġnext', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġslips', 'ww', 'es', 'lar', 'ati', 'Ġarchived', 'web', 'Ġed', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'uss', 'f', 'Ġcentre', 'Ġcore', 'Ġlacks', 'Ġlanding', 'Ġgear', 'Ġgrid', 'Ġï', '¬', 'ģ', 'ns', 'Ġtwitter', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġthree', 'year', 'Ġwait', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġcould', 'Ġlaunch', 'Ġlater', 'Ġmonth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġcore', 'Ġstage', 'Ġexpended', 'Ġus', 'sf', 'Ġrocket', "'s", 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġreturned', 'Ġnear', 'sim', 'ultane', 'ous', 'Ġland', 'ings', 'Ġspace', 'x', "'s", 'Ġrecovery', 'Ġzone', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation']</t>
+          <t>['asa', 'Ġassociate', 'Ġadministrator', 'Ġth', 'omas', 'Ġz', 'urb', 'uc', 'hen', 'Ġdespite', 'Ġbest', 'Ġefforts', 'Ġunc', 'rew', 'ed', 'Ġremote', 'Ġmission', 'Ġfound', 'Ġbeyond', 'Ġcurrent', 'Ġtechnology', 'Ġtime', 'Ġweb', 'b', 'Ġdesigned', 'Ġlong', 'Ġweb', 'b', 'Ġtesting', 'Ġperiod', 'Ġn', 'asa', 'Ġofficials', 'Ġreferred', 'Ġidea', 'Ġservicing', 'Ġmission', 'Ġplans', 'Ġannounced', 'Ġsince', 'Ġsuccessful', 'Ġlaunch', 'Ġn', 'asa', 'Ġstated', 'Ġnevertheless', 'Ġlimited', 'Ġaccommodation', 'Ġmade', 'Ġfacilitate', 'Ġfuture', 'Ġservicing', 'Ġmissions', 'Ġaccommodations', 'Ġincluded', 'Ġprecise', 'Ġguidance', 'Ġmarkers', 'Ġform', 'Ġcrosses', 'Ġsurface', 'Ġweb', 'b', 'Ġuse', 'Ġremote', 'Ġservicing', 'Ġmissions', 'Ġwell', 'Ġrefill', 'able', 'Ġfuel', 'Ġtanks', 'Ġremovable', 'Ġheat', 'Ġprotect', 'ors', 'Ġaccessible', 'Ġattachment', 'Ġpoints', 'Ġil', 'ana', 'vs', 'ky', 'Ġv', 'ick', 'Ġbal', 'z', 'ano', 'Ġwrite', 'Ġweb', 'b', 'Ġuses', 'Ġmodified', 'Ġversion', 'Ġjavascript', 'Ġcalled', 'Ġn', 'omb', 'Ġscript', 'e', 'ase', '00', 'e', 'Ġoperations', 'Ġfollows', 'Ġec', 'ascript', 'Ġstandard', 'allows', 'Ġmodular', 'Ġdesign', 'Ġflow', 'board', 'Ġscripts', 'Ġcall', 'Ġlower', 'level', 'Ġscripts', 'Ġdefined', 'Ġfunctions', '".', 'Ġj', 'w', 'st', 'Ġscience', 'Ġoperations', 'Ġdriven', 'instead', 'Ġbinary', 'Ġcommand', 'Ġblocks', 'board', 'Ġscripts', 'Ġwritten', 'Ġcustomized', 'Ġversion', 'Ġjavascript', 'Ġscript', 'Ġinterpreter', 'Ġrun', 'Ġflight', 'Ġsoftware', 'Ġwritten', 'Ġprogramming', 'Ġlanguage', 'Ġc', '++', 'Ġflight', 'Ġsoftware', 'Ġoperates', 'Ġspacecraft', 'Ġscience', 'Ġdesire', 'Ġlarge', 'Ġinfrared', 'Ġspace', 'Ġtelescope', 'Ġtraces', 'Ġback', 'Ġdecades', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġinfrared', 'Ġtelescope', 'Ġfacility', 'later', 'Ġcalled', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'Ġplanned', 'Ġspace', 'Ġshuttle', 'Ġdevelopment', 'Ġpotential', 'Ġinfrared', 'Ġastronomy', 'Ġacknowledged', 'Ġtime', 'Ġunlike', 'Ġground', 'Ġtelescopes', 'Ġspace', 'Ġobserv', 'atories', 'Ġfree', 'Ġatmospheric', 'Ġabsorption', 'Ġinfrared', 'Ġlight', 'Ġspace', 'Ġobserv', 'atories', 'Ġopened', 'new', 'Ġastronomers', 'Ġservicing', 'Ġsoftware', 'Ġcomparison', 'Ġtelescopes', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġprimary', 'Ġmirror', 'Ġsize', 'Ġcomparison', 'Ġweb', 'b', 'Ġhub', 'ble', 'Ġten', 'uous', 'Ġatmosphere', 'Ġnominal', 'Ġflight', 'Ġaltitude', 'Ġmeasurable', 'Ġabsorption', 'Ġdetectors', 'Ġoperating', 'Ġwavelengths', 'ĠÂµ', 'ĠÂµ', 'Ġachieve', 'Ġhigh', 'Ġradi', 'ometric', 'Ġsensitivity', 'Ġg', 'cc', 'arthy', 'Ġg', 'Ġw', 'Ġaut', 'io', 'Ġhowever', 'Ġinfrared', 'Ġtelescopes', 'Ġdisadvantage', 'Ġneed', 'Ġstay', 'Ġextremely', 'Ġcold', 'Ġlonger']</t>
         </is>
       </c>
       <c r="C278" t="n">
@@ -4052,7 +4052,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>['Ġmilitary', 'Ġspokesperson', 'Ġsaid', 'Ġfal', 'con', 'Ġheavy', "'s", 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġus', 'sf', 'Ġmission', 'Ġwould', 'Ġtarget', 'Ġlanding', 'Ġtwo', 'Ġspace', 'x', 'Ġdrone', 'Ġships', 'Ġï', '¬', 'Ĥ', 'ating', 'range', 'l', 'antic', 'Ġocean', '."', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġmay', 'launch', 'Ġn', 'asa', "'s", 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġdelayed', 'Ġlate', 'Ġse', 'pt', 'ember', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'se', 'pt', 'ember', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'one', 'Ġmissions', 'Ġus', 'sf', 'Ġtent', 'atively', 'Ġscheduled', 'Ġlate', 'Ġj', 'une', 'Ġpostponed', 'Ġind', 'e', 'ï', '¬', 'ģ', 'n', 'itely', 'Ġ...', 'Ġdelays', 'Ġupcoming', 'Ġfal', 'con', 'Ġheavy', 'Ġmissions', 'Ġcaused', 'Ġpayload', 'Ġissues', '."', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġoct', 'ober', 'space', 'x', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġthree', 'Ġyears', 'Ġeyes', 'Ġlate', 'oct', 'ober', 'Ġlif', 'ff', 'two', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġthree', 'year', 'Ġwait', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġcould', 'Ġlaunch', 'Ġlater', 'Ġmonth', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġspace', 'Ġforce', 'Ġsaid', 'Ġmission', 'Ġmilitary', 'Ġsays', 'Ġlaunch', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġlike', 'Ġus', 'sf', 'Ġcurrently', 'Ġscheduled', 'Ġjan', 'uary', '."', 'space', 'Ġnews', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'mber', 'Ġcl', 'ark', 'Ġstep', 'hen', 'fal', 'con', 'Ġheavy', 'Ġrocket', 'Ġlaunch', 'Ġpad', 'Ġone', 'Ġspace', 'x', "'s", 'Ġcomplex', 'Ġmissions', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'Ġnext', 'Ġmilitary', 'Ġmission', 'Ġï', '¬', 'Ĥ', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġnamed', 'Ġlaunch', 'Ġl', 'pe', 'Ġspacecraft', 'Ġspace', 'Ġforce', 'Ġcommunications', 'Ġsatellite', 'Ġtandem', 'Ġlaunch', 'Ġscheduled', 'Ġjan', 'uary', 'Ġuse', 'Ġfal', 'con', 'Ġheavy', 'Ġside', 'Ġboosters', 'Ġï', '¬', 'Ĥ', 'Ġus', 'sf', 'Ġmission']</t>
+          <t>['Ġwavelength', 'Ġinfrared', 'Ġcolder', 'Ġneed', 'Ġbackground', 'Ġheat', 'Ġdevice', 'Ġoverwhel', 'ms', 'Ġdetectors', 'Ġmaking', 'Ġeffectively', 'Ġblind', 'Ġovercome', 'Ġcareful', 'Ġspacecraft', 'Ġdesign', 'Ġparticular', 'Ġplacing', 'Ġtelescope', 'Ġde', 'war', 'Ġextremely', 'Ġcold', 'Ġsubstance', 'Ġliquid', 'Ġhelium', 'Ġcool', 'ant', 'Ġslowly', 'Ġvapor', 'ize', 'Ġlimiting', 'Ġlifetime', 'Ġinstrument', 'Ġshort', 'Ġmonths', 'Ġyears', 'Ġcases', 'Ġpossible', 'Ġmaintain', 'Ġtemperature', 'Ġlow', 'Ġenough', 'Ġdesign', 'Ġspacecraft', 'Ġenable', 'Ġnear', 'inf', 'rared', 'Ġobservations', 'Ġwithout', 'Ġsupply', 'Ġcool', 'ant', 'Ġextended', 'Ġmissions', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'Ġwide', 'field', 'Ġinfrared', 'Ġsurvey', 'Ġexplorer', 'Ġoperated', 'Ġreduced', 'Ġcapacity', 'Ġcool', 'ant', 'Ġdepletion', 'Ġanother', 'Ġexample', 'Ġhub', 'ble', "'s", 'Ġnear', 'Ġinfrared', 'Ġcamera', 'Ġmulti', 'object', 'Ġspect', 'rom', 'eter', 'nic', 'mos', 'Ġinstrument', 'Ġstarted', 'Ġusing', 'Ġblock', 'Ġnitrogen', 'Ġice', 'Ġdepleted', 'Ġcouple', 'Ġyears', 'Ġreplaced', 'Ġsts', 'Ġservicing', 'Ġmission', 'Ġcry', 'oc', 'ool', 'er', 'Ġworked', 'Ġcontinuously', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdesigned', 'Ġcool', 'Ġwithout', 'Ġde', 'war', 'Ġusing', 'Ġcombination', 'Ġsun', 'shield', 'Ġradi', 'ators', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'Ġusing', 'Ġadditional', 'Ġcry', 'oc', 'ool', 'er', 'Ġselected', 'Ġspace', 'Ġtelescopes', 'Ġinstruments', 'Ġname', 'Ġlaunch', 'Ġyear', 'Ġwavelength', 'Î¼', 'Ġaperture', 'Ġcooling', 'Ġspac', 'el', 'ab', 'Ġinfrared', 'Ġtelescope', 'irt', 'âĢĵ', 'Ġhelium', 'Ġinfrared', 'Ġspace', 'Ġobserv', 'atory', 'âĢĵ', 'Ġhelium', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġimaging', 'Ġspect', 'rog', 'raph', 'st', 'âĢĵ', '03', 'Ġpassive', 'Ġhub', 'ble', 'Ġnear', 'Ġinfrared', 'Ġcamera', 'Ġmulti', 'object', 'Ġspect', 'rom', 'eter', 'nic', 'mos', 'âĢĵ', 'Ġnitrogen', 'Ġlater', 'Ġcry', 'oc', 'ool', 'er', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'âĢĵ', 'Ġhelium', 'Ġhub', 'ble', 'Ġwide', 'Ġfield', 'Ġcamera', 'âĢĵ', 'Ġpassive', 'Ġtherm', 'oe', 'lect', 'ric', 'sc', 'hel', 'Ġspace', 'Ġobserv', 'atory', 'âĢĵ', 'Ġhelium', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'âĢĵ', 'Ġpassive', 'Ġcry', 'oc', 'ool', 'er', 'mir']</t>
         </is>
       </c>
       <c r="C279" t="n">
@@ -4065,7 +4065,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>['Ġassuming', 'Ġsuccessful', 'Ġrecovery', 'Ġlanding', 'Ġzones', 'Ġcape', 'aver', 'al', 'Ġspace', 'Ġforce', 'Ġstation', 'Ġspace', 'Ġforce', 'Ġsaid', '."', 'fal', 'con', 'Ġheavy', 'Ġcould', 'Ġlaunch', 'Ġthree', 'Ġu', 'Ġspace', 'Ġforce', 'Ġmissions', 'Ġspac', 'en', 'ews', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġoct', 'ober', 'v', 'ias', 'Ġameric', 'Ġar', 'ct', 'urus', 'Ġnext', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġrainbow', 'Ġj', 'ason', 'Ġse', 'pt', 'ember', 'next', 'Ġcommercial', 'Ġfal', 'con', 'Ġheavy', 'Ġmission', 'Ġlaunch', 'Ġdebut', 'str', 'Ġsatellite', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'application', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'str', 'Ġb', 'erm', 'uda', 'Ġattachment', 'Ġnarrative', 'fc', 'str', 'Ġb', 'erm', 'uda', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'ar', 'abs', 'Ġfal', 'con', 'Ġheavy', 'Ġmission', 'Ġslated', 'Ġde', 'cember', 'âĢĵ', 'jan', 'uary', 'Ġtimeframe', 'Ġspac', 'en', 'ews', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'v', 'ias', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġnext', 'gen', 'Ġbroadband', 'Ġsatellite', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'v', 'ias', 'Ġspace', 'x', 'Ġenter', 'Ġcontract', 'Ġfuture', 'Ġv', 'ias', 'Ġsatellite', 'Ġlaunch', 'Ġv', 'ias', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġb', 'aylor', 'ichael', 'fal', 'con', 'Ġheavy', 'Ġe', 'ch', 'ost', 'ar', 'j', 'upiter', ')"', 'Ġtails', 'Ġarchived', 'Ġn', 'ches', 'details', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġmay', 'j', 'upiter', 'Ġe', 'ch', 'ost', 'ar', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay']</t>
+          <t>['Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmajor', 'Ġmilestones', 'Ġyear', 'Ġmilestone', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġproject', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġproposed', 'mir', 'ror', 'Ġsize', 'Ġnexus', 'Ġspace', 'Ġtelescope', 'Ġprecursor', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġcancelled', 'Ġproposed', 'Ġproject', 'Ġrenamed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'mir', 'ror', 'Ġsize', 'Ġreduced', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġawarded', 'Ġcontract', 'Ġbuild', 'Ġtelescope', 'Ġmemorandum', 'Ġunderstanding', 'Ġsigned', 'Ġn', 'asa', 'Ġmission', 'Ġcritical', 'Ġdesign', 'Ġreview', 'Ġpassed', 'Ġproposed', 'Ġcancellation', 'Ġfinal', 'Ġassembly', 'Ġcompleted', 'Ġde', 'cember', 'Ġlaunch', 'Ġweb', 'b', "'s", 'Ġdelays', 'Ġcost', 'Ġincreases', 'Ġcompared', 'Ġpredecessor', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġhub', 'ble', 'Ġformally', 'Ġstarted', 'Ġestimated', 'Ġdevelopment', 'Ġcost', 'Ġus', 'Ġmillion', 'equ', 'ivalent', '09', '000', 'Ġtime', 'Ġsent', 'Ġorbit', 'Ġcost', 'Ġfour', 'Ġtimes', 'Ġaddition', 'Ġnew', 'Ġinstruments', 'Ġservicing', 'Ġmissions', 'Ġincreased', 'Ġcost', 'Ġleast', 'Ġbillion', 'equ', 'ivalent', '000', 'Ġdiscussions', 'Ġhub', 'ble', 'Ġfollow', 'Ġstarted', 'Ġserious', 'Ġplanning', 'Ġbegan', 'Ġearly', 'Ġhi', 'z', 'Ġtelescope', 'Ġconcept', 'Ġdeveloped', ':[', 'Ġfully', 'Ġbaffled', 'b', 'Ġft', 'Ġaperture', 'Ġinfrared', 'Ġtelescope', 'Ġwould', 'Ġrec', 'ede', 'Ġorbit', 'Ġastronomical', 'Ġunit', 'Ġdistant', 'Ġorbit', 'Ġwould', 'Ġbenefited', 'Ġreduced', 'Ġlight', 'Ġnoise', 'Ġz', 'odiac', 'al', 'Ġearly', 'Ġplans', 'Ġcalled', 'Ġnexus', 'Ġprecursor', 'Ġtelescope', 'Ġmission', 'Ġcorrecting', 'Ġflawed', 'Ġoptics', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'h', 'st', 'Ġfirst', 'Ġyears', 'Ġplayed', 'Ġsignificant', 'Ġrole', 'Ġbirth', 'Ġweb', 'b', 'Ġn', 'asa', 'Ġconducted', 'Ġspace', 'Ġshuttle', 'Ġmission', 'Ġreplaced', 'Ġh', 'st', "'s", 'Ġcamera', 'Ġinstalled', 'Ġretro', 'fit', 'Ġimaging', 'Ġspect', 'rog', 'raph', 'Ġcompensate', 'Ġspherical', 'Ġaber', 'ration', 'Ġprimary', 'Ġmirror', 'Ġh', 'st', 'Ġbeyond', 'Ġcommittee', 'Ġformed', 'Ġstudy', 'Ġpossible', 'Ġmissions', 'Ġprograms', 'Ġoptical', 'ult', 'raviolet', 'Ġastronomy', 'Ġspace', 'Ġfirst', 'Ġdecades', 'st', 'Ġcentury', '."[', 'Ġembold', 'ened', 'Ġh', 'st', "'s", 'Ġsuccess', 'Ġreport', 'Ġexplored', 'Ġconcept', 'Ġlarger', 'Ġmuch', 'Ġcolder', 'Ġinfrared', 'sensitive', 'Ġtelescope', 'Ġcould', 'Ġreach', 'Ġback', 'Ġcosmic', 'Ġtime', 'Ġbirth', 'Ġfirst', 'Ġgalaxies', 'Ġhigh']</t>
         </is>
       </c>
       <c r="C280" t="n">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>['n', 'asa', 'Ġcontinues', 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġn', 'asa', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġpsyche', 'Ġmission', 'nas', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġus', 'sf', 'Ġnext', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'air', 'Ġforce', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġspace', 'x', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'contract', 'Ġaug', 'Ġdefense', 'gov', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'space', 'Ġexploration', 'Ġtechnologies', 'Ġcorp', '.,', 'Ġhaw', 'th', 'orne', 'Ġcal', 'ornia', 'Ġawarded', '07', 'Ġbilateral', 'Ġmod', 'ï', '¬', 'ģ', 'cation', 'p', '0000', 'Ġpreviously', 'Ġawarded', 'Ġspace', 'Ġforce', 'Ġcontract', 'Ġfa', 'c', '000', '...', 'Ġ...', 'Ġtotal', 'Ġcumulative', 'Ġface', 'Ġvalue', 'Ġcontract', '07', '."', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'ms', 'r', 'Ġintegrated', 'Ġmaster', 'Ġschedule', 'ï', '¬', 'ģ', 'ce', 'Ġsafety', 'Ġmission', 'Ġassurance', 'Ġn', 'asa', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'n', 'asa', 'g', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġmarg', 'etta', 'Ġro', 'bert', 'Ġse', 'pt', 'ember', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġgoes', 'u', 'Ġmission', 'Ġss', 'ion', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġmission', 'w', 'press', 'Ġrelease', 'Ġn', 'asa', 'Ġj', 'uly']</t>
+          <t>['priority', 'Ġscience', 'Ġgoal', 'Ġbeyond', 'Ġh', 'st', "'s", 'Ġcapability', 'Ġwarm', 'Ġtelescope', 'Ġblinded', 'Ġinfrared', 'Ġemission', 'Ġoptical', 'Ġsystem', 'Ġaddition', 'Ġrecommendations', 'Ġextend', 'Ġh', 'st', 'Ġmission', 'Ġdevelop', 'Ġtechnologies', 'Ġfinding', 'Ġplanets', 'Ġaround', 'Ġstars', 'Ġn', 'asa', 'Ġembraced', 'Ġchief', 'Ġrecommendation', 'Ġh', 'st', 'Ġbeyond', 'Ġlarge', 'Ġcold', 'Ġspace', 'Ġtelescope', 'rad', 'atively', 'Ġcooled', 'Ġfar', 'ĠÂ°', 'c', 'Ġbegan', 'Ġplanning', 'Ġprocess', 'Ġfuture', 'Ġweb', 'b', 'Ġtelescope', 'Ġdevelopment', 'Ġhistory', 'Ġbackground', 'development', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġearly', 'Ġfull', 'scale', 'Ġmodel', 'Ġdisplay', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġpreparation', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġdec', 'adal', 'Ġsurvey', 'Ġliterature', 'Ġreview', 'Ġproduced', 'Ġunited', 'Ġstates', 'Ġnational', 'Ġresearch', 'Ġcouncil', 'Ġincludes', 'Ġidentifying', 'Ġresearch', 'Ġpriorities', 'Ġmaking', 'Ġrecommendations', 'Ġupcoming', 'Ġdecade', 'Ġincluded', 'Ġdevelopment', 'Ġscientific', 'Ġprogram', 'Ġbecame', 'Ġknown', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġadvancements', 'Ġrelevant', 'Ġtechnologies', 'Ġn', 'asa', 'Ġmatured', 'Ġstudying', 'Ġbirth', 'Ġgalaxies', 'Ġyoung', 'Ġuniverse', 'Ġsearching', 'Ġplanets', 'Ġaround', 'Ġstars', 'Ġprime', 'Ġgoals', 'Ġcoales', 'ced', 'orig', 'ins', 'Ġh', 'st', 'Ġbeyond', 'Ġbecame', 'Ġprominent', 'Ġhoped', 'Ġng', 'st', 'Ġreceived', 'Ġhighest', 'Ġranking', 'Ġdec', 'adal', 'Ġsurvey', 'Ġadministrator', 'Ġn', 'asa', 'Ġdan', 'Ġgold', 'Ġcoined', 'Ġphrase', 'f', 'aster', 'Ġbetter', 'Ġcheaper', '",', 'Ġopted', 'Ġnext', 'Ġbig', 'Ġparadigm', 'Ġshift', 'Ġastronomy', 'Ġnamely', 'Ġbreaking', 'Ġbarrier', 'Ġsingle', 'Ġmirror', 'Ġmeant', 'Ġgoing', 'el', 'im', 'inate', 'Ġmoving', 'Ġparts', 'learn', 'Ġlive', 'Ġmoving', 'Ġparts', 'e', 'Ġsegment', 'ed', 'Ġoptics', 'Ġgoal', 'Ġreduce', 'Ġmass', 'Ġdensity', 'Ġten', 'fold', 'Ġsilicon', 'Ġcarb', 'ide', 'Ġthin', 'Ġlayer', 'Ġglass', 'Ġtop', 'Ġfirst', 'Ġlooked', 'Ġb', 'ery', 'ium', 'Ġselected', 'Ġmid', 'Ġera', 'f', 'aster', 'Ġbetter', 'Ġcheaper', 'Ġproduced', 'Ġng', 'st', 'Ġconcept', 'Ġft', 'Ġaperture', 'Ġflown', 'Ġroughly', 'Ġestimated', 'Ġcost', 'Ġus', 'Ġmillion', 'Ġn', 'asa', 'Ġworked', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġconduct', 'Ġtechnical', 'Ġrequirement', 'Ġcost', 'Ġstudies', 'Ġthree', 'Ġdifferent', 'Ġconcepts', 'Ġselected', 'Ġlock', 'heed']</t>
         </is>
       </c>
       <c r="C281" t="n">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'ion', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġflagship', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġinches', 'Ġforward', 'Ġshack', 'led', 'Ġearth', 'Ġsuper', 'cl', 'uster', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'n', 'asa', 'Ġuse', 'Ġcommercial', 'Ġlaunch', 'Ġvehicle', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġspac', 'en', 'ews', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġde', 'cember', 'Ġcol', 'ap', 'rete', 'Ġanth', 'ony', 'Ġaug', 'ust', 'vi', 'per', 'Ġlunar', 'Ġwater', 'Ġreconnaissance', 'Ġmission', 'sc', 'ie', 'Ġac', 'pdf', 'Ġn', 'asa', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'n', 'asa', 'Ġrepl', 'ans', 'Ġcl', 'ps', 'Ġdelivery', 'Ġv', 'iper', 'Ġreduce', 'Ġrisk', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġcol', 'ap', 'rete', 'Ġanth', 'ony', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġselects', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġlunar', 'Ġrover', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġselects', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', "'s", 'Ġv', 'iper', 'Ġlunar', 'Ġrover', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġassessments', 'Ġmajor', 'Ġprojects', 'Ġapr', 'il', 'pdf', 'Ġus', 'Ġgovernment', 'Ġaccountability', 'ï', '¬', 'ģ', 'ce', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'n', 'asa', 'Ġplans', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtwo', 'Ġgateway', 'Ġelements', 'Ġrocket', 'space', 'f', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember']</t>
+          <t>['Ġmart', 'Ġtr', 'w', 'Ġpreliminary', 'Ġconcept', 'Ġstudies', 'Ġlaunch', 'Ġtime', 'Ġplanned', 'Ġlaunch', 'Ġdate', 'Ġpushed', 'Ġback', 'Ġmany', 'Ġtimes', 'see', 'Ġtable', 'Ġproject', 'Ġrenamed', 'Ġn', 'asa', "'s", 'Ġsecond', 'Ġadministrator', 'âĢĵ', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', '06', 'âĢĵ', ').[', 'Ġweb', 'b', 'Ġled', 'Ġagency', 'Ġap', 'ollo', 'Ġprogram', 'Ġestablished', 'Ġscientific', 'Ġresearch', 'Ġcore', 'Ġn', 'asa', 'Ġactivity', 'Ġn', 'asa', 'Ġawarded', 'Ġtr', 'w', 'Ġus', 'Ġmillion', 'Ġprime', 'Ġcontract', 'Ġweb', 'b', 'Ġdesign', 'Ġcalled', 'Ġde', 'sc', 'oped', 'Ġft', 'Ġprimary', 'Ġmirror', 'Ġlaunch', 'Ġdate', 'Ġlater', 'Ġyear', 'Ġtr', 'w', 'Ġacquired', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġhostile', 'Ġbid', 'Ġbecame', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġtechnology', 'Ġdevelopment', 'Ġmanaged', 'Ġn', 'asa', "'s", 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġgreen', 'belt', 'ary', 'land', 'Ġjohn', 'Ġc', 'ather', 'Ġproject', 'Ġscientist', 'Ġprimary', 'Ġcontractor', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġaerospace', 'Ġsystems', 'Ġresponsible', 'Ġdeveloping', 'Ġbuilding', 'Ġspacecraft', 'Ġelement', 'Ġincluded', 'Ġsatellite', 'Ġbus', 'Ġsun', 'shield', 'Ġdeploy', 'able', 'Ġtower', 'Ġassembly', 'ta', 'Ġconnects', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'Ġspacecraft', 'Ġbus', 'Ġmid', 'Ġboom', 'Ġassembly', 'mb', 'Ġhelps', 'Ġdeploy', 'Ġlarge', 'Ġsun', 'shield', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġsub', 'cont', 'racted', 'Ġdevelop', 'Ġbuild', 'te', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', ').[', 'Ġcost', 'Ġgrowth', 'Ġrevealed', 'Ġspring', 'Ġled', 'Ġaug', 'ust', 'plan', 'ning', 'Ġprimary', 'Ġtechnical', 'Ġoutcomes', 'plan', 'ning', 'Ġsignificant', 'Ġchanges', 'Ġintegration', 'Ġtest', 'Ġplans', 'month', 'Ġlaunch', 'Ġdelay', 'Ġelimination', 'Ġsystem', 'level', 'Ġtesting', 'Ġobserv', 'atory', 'Ġmodes', 'Ġearly', 'Ġdevelopment', 'Ġrepl', 'ning', 'âĢĵ', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġj', 'w', 'st', 'Ġmirror', 'Ġsegment', 'Ġmirror', 'Ġsegments', 'Ġundergoing', 'Ġcry', 'ogenic', 'Ġtests', 'Ġx', 'ray', 'Ġcry', 'ogenic', 'Ġfacility', 'Ġmarsh', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġassembled', 'Ġtelescope', 'Ġfollowing', 'Ġenvironmental', 'Ġtesting', 'Ġwavelength', 'Ġshorter', 'ĠÂµ', 'Ġmajor', 'Ġfeatures', 'Ġobserv', 'atory', 'Ġunchanged', 'Ġfollowing', 'plan', 'ning']</t>
         </is>
       </c>
       <c r="C282" t="n">
@@ -4104,7 +4104,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>['Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġpot', 'ter', 'Ġse', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġawards', 'Ġcontract', 'Ġlaunch', 'Ġinitial', 'Ġelements', 'Ġlunar', 'Ġoutpost', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'Ġnews', 'mber', 'Ġarchived', 'eway', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'press', 'Ġrelease', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'uly', 'n', 'asa', 'Ġintroduces', 'Ġnew', 'Ġwider', 'Ġset', 'Ġeyes', 'Ġuniverse', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'web', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'uly', 'Ġobserv', 'atory', 'Ġbegin', 'Ġoperations', 'Ġtravelling', 'Ġgravitational', 'Ġbalance', 'Ġpoint', 'Ġknown', 'Ġearth', 'sun', 'sc', 'ig', 'u', 'ys', 'pace', 'Ġapr', 'il', 'ast', 'rob', 'otic', 'Ġlaunching', 'Ġdebut', 'Ġland', 'er', 'Ġvul', 'Ġsaid', 'Ġtoday', 'Ġpurchasing', 'Ġfal', 'con', 'Ġheavy', 'Ġthird', 'Ġland', 'er', 'Ġmission', 'Ġmoon', 'Ġmission', 'Ġlaunch', 'Ġast', 'rob', 'otic', 'Ġland', 'er', 'Ġmoon', "'s", 'Ġsouth', 'Ġpole', 'weet', 'Ġvia', 'Ġtwitter', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'n', 'asa', 'Ġplanning', 'Ġspend', 'Ġbillion', 'Ġspace', 'Ġstation', 'Ġde', 'orbit', 'Ġmodule', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġplans', 'Ġstart', 'Ġwork', 'Ġyear', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġgateway', 'Ġlogistics', 'Ġmission', 'Ġion', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġmarch', 'Ġcl', 'ark', 'Ġstep', 'hen', 'n', 'asa', 'Ġpicks', 'Ġspace', 'x', 'Ġdeliver', 'Ġcargo', 'Ġgateway', 'Ġstation', 'Ġlunar', 'Ġorbit', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġsheet', 'z', 'ichael', 'Ġmarch', 'space', 'x', "'s", 'Ġpowerful', 'Ġrocket', 'Ġsend', 'Ġn', 'asa', 'Ġcargo']</t>
+          <t>['Ġproject', 'Ġindependently', 'Ġreviewed', 'Ġapr', 'il', 'plan', 'Ġlife', 'cycle', 'Ġcost', 'Ġproject', 'Ġestimated', 'Ġbillion', 'Ġcomprised', 'Ġapproximately', 'Ġbillion', 'Ġdesign', 'Ġdevelopment', 'Ġlaunch', 'Ġcommission', 'ing', 'Ġapproximately', 'Ġus', 'Ġbillion', 'Ġten', 'Ġyears', 'Ġoperations', 'Ġes', 'Ġagreed', 'Ġcontributing', 'ĠâĤ¬', 'Ġmillion', 'Ġincluding', 'Ġlaunch', 'adian', 'Ġspace', 'Ġagency', 'Ġpledged', 'Ġmillion', 'Ġdelivered', 'Ġcontributions', 'Ġequipment', 'Ġpoint', 'Ġtelescope', 'Ġdetect', 'Ġatmospheric', 'Ġconditions', 'Ġdistant', 'Ġplanets', 'Ġjan', 'uary', 'Ġnine', 'Ġten', 'Ġtechnology', 'Ġdevelopment', 'Ġitems', 'Ġproject', 'Ġsuccessfully', 'Ġpassed', 'Ġnon', 'adv', 'ocate', 'Ġreview', 'Ġtechnologies', 'Ġdeemed', 'Ġsufficiently', 'Ġmature', 'Ġretire', 'Ġsignificant', 'Ġrisks', 'Ġproject', 'Ġremaining', 'Ġtechnology', 'Ġdevelopment', 'Ġitem', 'Ġmir', 'Ġcry', 'oc', 'ool', 'er', 'Ġcompleted', 'Ġtechnology', 'aturation', 'Ġmilestone', 'Ġapr', 'il', 'Ġtechnology', 'Ġreview', 'Ġrepresented', 'Ġbeginning', 'Ġstep', 'Ġprocess', 'Ġultimately', 'Ġmoved', 'Ġproject', 'Ġdetailed', 'Ġdesign', 'Ġphase', 'phase', 'Ġc', 'Ġmay', 'Ġcosts', 'Ġstill', 'Ġtarget', 'Ġmarch', 'Ġproject', 'Ġsuccessfully', 'Ġcompleted', 'Ġpreliminary', 'Ġdesign', 'Ġreview', 'Ġapr', 'il', 'Ġproject', 'Ġpassed', 'Ġnon', 'adv', 'ocate', 'Ġreview', 'Ġpassed', 'Ġreviews', 'Ġinclude', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'Ġreview', 'Ġmarch', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'Ġreview', 'Ġcompleted', 'Ġoct', 'ober', 'Ġsun', 'shield', 'Ġreview', 'Ġcompleted', 'Ġjan', 'uary', 'Ġapr', 'il', 'Ġtelescope', 'Ġpassed', 'Ġtechnical', 'Ġportion', 'Ġmission', 'Ġcritical', 'Ġdesign', 'Ġreview', 'Ġpassing', 'Ġsign', 'ified', 'Ġintegrated', 'Ġobserv', 'atory', 'Ġmeet', 'Ġscience', 'Ġengineering', 'Ġrequirements', 'Ġmission', 'Ġencomp', 'assed', 'Ġprevious', 'Ġdesign', 'Ġreviews', 'Ġproject', 'Ġschedule', 'Ġunderwent', 'Ġreview', 'Ġmonths', 'Ġfollowing', 'Ġprocess', 'Ġcalled', 'Ġindependent', 'Ġcomprehensive', 'Ġreview', 'Ġpanel', 'Ġled', 'plan', 'Ġmission', 'Ġaiming', 'Ġlaunch', 'Ġlate', 'Ġcost', 'runs', 'Ġimpacting', 'Ġprojects', 'Ġthough', 'Ġweb', 'b', 'Ġremained', 'Ġschedule', 'Ġweb', 'b', 'Ġproject', 'Ġfinal', 'Ġdesign', 'Ġfabrication', 'Ġphase', 'phase', 'Ġc', 'Ġassembly', 'Ġhex', 'agonal', 'Ġsegments', 'Ġprimary', 'Ġmirror', 'Ġdone', 'Ġvia', 'Ġrobotic', 'Ġarm', 'Ġbegan', 'mber', 'Ġcompleted', 'Ġfe', 'b', 'ruary', 'Ġsecondary', 'Ġmirror', 'Ġinstalled', 'Ġmarch']</t>
         </is>
       </c>
       <c r="C283" t="n">
@@ -4117,7 +4117,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>['Ġmoon', "'s", 'Ġorbit', 'Ġsupply', 'Ġastronauts', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'space', 'x', 'Ġwins', 'Ġn', 'asa', 'Ġcommercial', 'Ġcargo', 'Ġcontract', 'Ġlunar', 'Ġgateway', 'Ġspac', 'en', 'ews', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġj', 'une', 'ar', 'abs', 'Ġfal', 'con', 'Ġheavy', 'Ġmission', 'Ġslated', 'Ġde', 'cember', 'âĢĵ', 'jan', 'uary', 'Ġtimeframe', 'Ġe', 'frame', 'Ġspac', 'en', 'ews', 'Ġarchived', 'time', 'frame', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'herty', 'Ġca', 'lin', 'Ġj', 'une', 'first', 'Ġever', 'Ġcommercial', 'Ġlaunch', 'Ġvia', 'Ġel', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġcould', 'Ġhappen', 'Ġend', 'Ġyear', 'Ġexpress', 'co', 'uk', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġannounces', 'Ġfirst', 'Ġcommercial', 'Ġcontract', 'Ġlaunch', 'Ġred', 'Ġorbit', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġde', 'cember', 'int', 'els', 'Ġsigns', 'Ġfirst', 'Ġcommercial', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġagreement', 'Ġspace', 'x', 'http', 'sp', 'ac', 'press', 'Ġrelease', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġment', 'space', 'x', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġde', 'cember', 'fal', 'con', 'Ġspace', 'x', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġj', 'uly', 'ars', 'Ġbooks', 'Ġfal', 'con', 'Ġheavy', 'Ġthree', 'Ġlaunches', 'http', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġes', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'ars', 'Ġshifts', 'Ġsatellite', 'Ġspace', 'x', 'rian', 'esp', 'ace', 'http', 'sp', 'ac', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġx', 'arian', 'esp', 'ace', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġde', 'cember', 'Ġk', 'bs', 'Ġgun', 'ter', 'ars', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une']</t>
+          <t>['Ġfinal', 'Ġconstruction', 'Ġweb', 'b', 'Ġtelescope', 'Ġcompleted', 'mber', 'Ġextensive', 'Ġtesting', 'Ġprocedures', 'Ġbegan', 'Ġdetailed', 'Ġdesign', 'Ġconstruction', 'âĢĵ', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmarch', 'Ġn', 'asa', 'Ġdelayed', 'Ġweb', 'b', "'s", 'Ġlaunch', 'Ġadditional', 'Ġyears', 'Ġmay', 'Ġtelescope', "'s", 'Ġsun', 'shield', 'Ġripped', 'Ġpractice', 'Ġdeployment', 'Ġsun', 'shield', "'s", 'Ġcables', 'Ġsufficiently', 'Ġtighten', 'Ġj', 'une', 'Ġn', 'asa', 'Ġdelayed', 'Ġlaunch', 'Ġadditional', 'Ġmonths', 'Ġmarch', 'Ġbased', 'Ġassessment', 'Ġindependent', 'Ġreview', 'Ġboard', 'Ġconvened', 'Ġfailed', 'Ġmarch', 'Ġtest', 'Ġdeployment', 'Ġreview', 'Ġidentified', 'Ġweb', 'b', 'Ġlaunch', 'Ġdeployment', 'Ġpotential', 'Ġsingle', 'point', 'Ġfailures', 'Ġtasks', 'Ġalternative', 'Ġmeans', 'Ġrecovery', 'Ġunsuccessful', 'Ġtherefore', 'Ġsucceed', 'Ġtelescope', 'Ġwork', 'Ġaug', 'ust', 'Ġmechanical', 'Ġintegration', 'Ġtelescope', 'Ġcompleted', 'Ġsomething', 'Ġscheduled', 'Ġdone', 'Ġyears', 'Ġconstruction', 'Ġcompleted', 'Ġweb', 'b', 'Ġunderwent', 'Ġfinal', 'Ġtests', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġfactory', 'Ġred', 'ondo', 'Ġbeach', 'Ġcal', 'ornia', 'Ġship', 'Ġcarrying', 'Ġtelescope', 'Ġleft', 'Ġcal', 'ornia', 'Ġse', 'pt', 'ember', 'Ġpassed', 'Ġpan', 'ama', 'Ġcanal', 'Ġarrived', 'Ġfrench', 'Ġgu', 'iana', 'Ġoct', 'ober', 'Ġn', 'asa', "'s", 'Ġlifetime', 'Ġcost', 'Ġproject', 'Ġexpected', 'Ġbillion', 'Ġbillion', 'Ġspent', 'Ġspacecraft', 'Ġdesign', 'Ġdevelopment', 'Ġmillion', 'Ġplanned', 'Ġsupport', 'Ġfive', 'Ġyears', 'Ġmission', 'Ġoperations', 'Ġrepresentatives', 'Ġes', 'Ġc', 'sa', 'Ġstated', 'Ġproject', 'Ġcontributions', 'Ġamount', 'Ġapproximately', 'ĠâĤ¬', 'Ġmillion', 'Ġca', 'Ġmillion', 'Ġrespectively', 'Ġstudy', 'Ġspace', 'Ġscience', 'Ġboard', 'Ġestimated', 'Ġbuild', 'Ġnext', 'generation', 'Ġinfrared', 'Ġobserv', 'atory', 'Ġorbit', 'Ġwould', 'Ġcost', 'Ġbillion', 'Ġdollars', 'Ġdollars', ').[', 'Ġcame', 'Ġclose', 'Ġfinal', 'Ġcost', 'Ġweb', 'b', 'Ġfirst', 'Ġn', 'asa', 'Ġdesign', 'Ġconsidered', 'Ġlate', 'Ġmodest', 'Ġaiming', 'Ġbillion', 'Ġprice', 'Ġtag', 'Ġyears', 'Ġconstruction', 'Ġtime', 'Ġdesign', 'Ġexpanded', 'Ġadded', 'Ġfunding', 'Ġconting', 'encies', 'Ġscheduling', 'Ġdelays', 'Ġproject', 'Ġentered', 'Ġpreliminary', 'Ġdesign', 'Ġreview', 'Ġformally', 'Ġconfirmed', 'Ġconstruction', 'Ġbillion', 'Ġalready', 'Ġspent', 'Ġdeveloping', 'Ġtelescope']</t>
         </is>
       </c>
       <c r="C284" t="n">
@@ -4130,7 +4130,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġj', 'une', 'Ġdavid', 'Ġle', 'ard', 'Ġapr', 'il', 'space', 'craft', 'Ġpowered', 'green', 'Ġpropell', 'ant', 'Ġlaunch', 'htt', 'Ġspace', 'Ġarchived', 'http', 'Ġss', 'ion', 'gp', 'im', 'html', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'space', 'x', 'Ġoffers', 'Ġlarge', 'Ġrockets', 'Ġsmall', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'ds', 'ac', 'deep', 'Ġspace', 'Ġatomic', 'Ġclock', ')"', 'Ġn', 'asa', 'Ġearth', 'Ġobservation', 'Ġresources', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'Ġgr', 'uss', 'ike', 'Ġapr', 'il', 'space', 'x', 'Ġsends', 'Ġair', 'Ġforce', 'Ġoutline', 'Ġfal', 'con', 'Ġheavy', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'avis', 'Ġj', 'ason', 'Ġmay', 'lights', 'ail', 'Ġlaunch', 'Ġslips', 'Ġfall', 'Ġplanetary', 'Ġsociety', 'Ġarchived', 'web', 'arc', 'launch', 'sl', 'ip', 'html', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'space', 'Ġforce', 'Ġawards', 'Ġnational', 'Ġsecurity', 'Ġspace', 'Ġlaunch', 'Ġphase', 'Ġlaunch', 'Ġservice', 'Ġcontracts', 'Ġu', 'la', 'Ġspace', 'x', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'green', 'Ġpropell', 'ant', 'Ġinfusion', 'Ġmission', 'Ġproject', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'deep', 'Ġspace', 'Ġatomic', 'Ġclock', 'Ġjet', 'Ġpropulsion', 'Ġlaboratory', 'Ġn', 'asa', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'une', 'space', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġblock', 'Ġrockets', 'Ġtargets', 'mber']</t>
+          <t>['Ġtotal', 'Ġbudget', 'Ġestimated', 'Ġbillion', 'equ', 'ivalent', 'Ġbillion', ').[', 'Ġsummer', 'Ġmission', 'Ġpassed', 'Ġcritical', 'Ġdesign', 'Ġreview', 'Ġexcellent', 'Ġgrades', 'Ġtechnical', 'Ġmatters', 'Ġschedule', 'Ġcost', 'Ġslips', 'Ġtime', 'Ġprompted', 'ary', 'land', 'Ġu', 'Ġsenator', 'Ġbar', 'bara', 'ik', 'uls', 'ki', 'Ġcall', 'Ġexternal', 'Ġreview', 'Ġproject', 'Ġindependent', 'Ġcomprehensive', 'Ġreview', 'Ġpanel', 'ic', 'r', 'p', 'Ġchaired', 'Ġj', 'Ġcas', 'ani', 'Ġfound', 'Ġearliest', 'Ġpossible', 'Ġlaunch', 'Ġdate', 'Ġlate', 'Ġextra', 'Ġcost', 'Ġbillion', 'Ġtotal', 'Ġbillion', 'Ġalso', 'Ġpointed', 'Ġwould', 'Ġrequired', 'Ġextra', 'Ġfunding', 'Ġf', 'Ġf', 'Ġlater', 'Ġlaunch', 'Ġdate', 'Ġwould', 'Ġlead', 'Ġhigher', 'Ġtotal', 'Ġcost', 'Ġj', 'uly', 'Ġunited', 'Ġstates', 'Ġhouse', 'Ġrepresentatives', 'Ġappropriations', 'Ġcommittee', 'Ġcommerce', 'Ġjustice', 'Ġscience', 'Ġmoved', 'Ġcancel', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġproject', 'Ġproposing', 'Ġf', 'Ġbudget', 'Ġremoved', 'Ġus', 'Ġbillion', 'Ġn', 'asa', "'s", 'Ġoverall', 'Ġbudget', 'Ġroughly', 'Ġone', 'Ġquarter', 'Ġbillion', 'Ġspent', 'Ġhardware', 'Ġproduction', 'Ġbudget', 'Ġproposal', 'Ġapproved', 'Ġsubcommittee', 'Ġvote', 'Ġfollowing', 'Ġday', 'Ġcommittee', 'Ġcharged', 'Ġproject', 'bill', 'ions', 'Ġdollars', 'Ġbudget', 'Ġplagued', 'Ġpoor', 'Ġmanagement', '".[', 'Ġresponse', 'Ġameric', 'Ġastronomical', 'Ġsociety', 'Ġissued', 'Ġstatement', 'Ġsupport', 'Ġsenator', 'ik', 'uls', 'ki', 'Ġnumber', 'Ġeditor', 'ials', 'Ġsupporting', 'Ġweb', 'b', 'Ġappeared', 'Ġinternational', 'Ġpress', 'mber', 'Ġcongress', 'Ġreversed', 'Ġplans', 'Ġcancel', 'Ġweb', 'b', 'Ġinstead', 'Ġcapped', 'Ġadditional', 'Ġfunding', 'Ġcomplete', 'Ġproject', 'Ġbillion', 'Ġcost', 'Ġschedule', 'Ġissues', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġprogression', 'Ġestimates', 'Ġschedule', 'Ġcost', 'Ġalong', 'Ġmajor', 'Ġmilestones', 'Ġyear', 'Ġplanned', 'Ġlaunch', 'Ġbudget', 'Ġplan', 'billion', 'Ġus', 'Ġpreliminary', 'Ġdesign', 'Ġreview', 'Ġcritical', 'Ġdesign', 'Ġreview']</t>
         </is>
       </c>
       <c r="C285" t="n">
@@ -4143,7 +4143,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>['Ġlaunch', 'Ġdebut', 'es', 'lar', 'ati', 'Ġretrieved', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġsurprise', 'Ġfal', 'con', 'Ġheavy', 'Ġbooster', 'Ġlanding', 'Ġsmash', 'Ġdistance', 'Ġrecord', 'Ġj', 'une', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġwall', 'ike', 'Ġj', 'uly', 'red', 'Ġdragon', 'Ġmission', 'Ġmull', 'ed', 'Ġcheap', 'Ġsearch', 'Ġmars', 'Ġlife', 'Ġspace', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġmay', 'fal', 'con', 'Ġheavy', 'Ġen', 'ab', 'ler', 'Ġdragon', 'Ġsolar', 'Ġsystem', 'Ġexplorer', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'el', 'Ġmus', 'k', 'Ġsuggests', 'Ġspace', 'x', 'Ġscra', 'pping', 'Ġplans', 'Ġland', 'Ġdragon', 'Ġcapsules', 'Ġmars', 'Ġverge', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'w', 'Ġj', 'uly', 'Ġcl', 'ark', 'Ġstep', 'hen', 'n', 'asa', 'Ġchooses', 'Ġmax', 'ar', 'Ġbuild', 'Ġkey', 'stone', 'Ġmodule', 'Ġlunar', 'Ġgateway', 'Ġstation', 'http', 'Ġway', 'station', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'ion', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġplans', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtwo', 'Ġgateway', 'Ġelements', 'Ġrocket', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġone', 'Ġpreceding', 'Ġsentences', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ass', 'ess', 'ments', 'Ġmajor', 'Ġprojects', 'Ġg', 'ao', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'psy', 'che', 'Ġspacecraft', 'Ġseparates', 'Ġfal', 'con', 'Ġheavy', 'Ġsecond', 'Ġstage', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġn', 'asa', 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsh', 'ie', 'ber', 'Ġj', 'athan', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġwins']</t>
+          <t>['Ġâī¥', 'Ġmarch', 'Ġdec', 'Ġsimilar', 'Ġissues', 'Ġaffected', 'Ġmajor', 'Ġn', 'asa', 'Ġprojects', 'Ġhub', 'ble', 'Ġtelescope', 'Ġscientists', 'Ġexpressed', 'Ġconcerns', 'Ġgrowing', 'Ġcosts', 'Ġschedule', 'Ġdelays', 'Ġweb', 'b', 'Ġtelescope', 'Ġworrying', 'Ġbudget', 'Ġmight', 'Ġcompeting', 'Ġspace', 'Ġscience', 'Ġprograms', 'Ġnature', 'Ġarticle', 'Ġdescribed', 'Ġweb', 'b', 'Ġtelescope', 'Ġate', 'Ġastronomy', '".[', 'Ġn', 'asa', 'Ġcontinued', 'Ġdefend', 'Ġbudget', 'Ġtimeline', 'Ġprogram', 'Ġcongress', 'Ġg', 'reg', 'ory', 'Ġl', 'Ġrob', 'inson', 'Ġappointed', 'Ġnew', 'Ġdirector', 'Ġweb', 'b', 'Ġprogram', 'Ġrob', 'inson', 'Ġcredited', 'Ġraising', 'Ġprogram', "'s", 'Ġschedule', 'Ġefficiency', 'Ġmany', 'Ġmeasures', 'Ġcompleted', 'Ġtime', 'Ġrole', 'Ġimproving', 'Ġperformance', 'Ġweb', 'b', 'Ġprogram', 'Ġrob', 'ins', 'ons', "'s", 'Ġsupervisor', 'Ġth', 'omas', 'Ġz', 'urb', 'uc', 'hen', 'Ġcalled', 'Ġeffective', 'Ġleader', 'Ġmission', 'Ġever', 'Ġseen', 'Ġhistory', 'Ġn', 'asa', '."[', 'Ġj', 'uly', 'Ġweb', 'b', "'s", 'Ġcommission', 'ing', 'Ġprocess', 'Ġcomplete', 'Ġbegan', 'Ġtransmitting', 'Ġfirst', 'Ġdata', 'Ġrob', 'inson', 'Ġretired', 'Ġfollowing', 'year', 'Ġcareer', 'Ġn', 'asa', 'Ġmarch', 'Ġn', 'asa', 'Ġpushed', 'Ġback', 'Ġlaunch', 'Ġmay', 'Ġlater', 'Ġfinal', 'Ġcost', 'Ġestimate', 'Ġcome', 'Ġnew', 'Ġlaunch', 'Ġwindow', 'Ġdetermined', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġmission', 'Ġcost', 'Ġcap', 'Ġincreased', 'Ġus', 'Ġmillion', 'Ġlaunch', 'Ġwindows', 'Ġpaused', 'Ġdue', 'Ġcov', 'id', 'Ġpand', 'emic', 'Ġweb', 'b', 'Ġfinally', 'Ġlaunched', 'Ġend', 'Ġtotal', 'Ġbudget', 'Ġus', 'Ġbillion', 'Ġn', 'asa', 'Ġes', 'Ġc', 'sa', 'Ġcollaborated', 'Ġtelescope', 'Ġsince', 'Ġes', "'s", 'Ġparticipation', 'Ġconstruction', 'Ġlaunch', 'Ġapproved', 'Ġmembers', 'Ġagreement', 'Ġsigned', 'Ġes', 'Ġn', 'asa', 'Ġexchange', 'Ġfull', 'Ġpartnership', 'Ġrepresentation', 'Ġaccess', 'Ġobserv', 'atory', 'Ġastronomers', 'Ġes', 'Ġproviding', 'Ġn', 'ir', 'spec', 'Ġinstrument', 'Ġoptical', 'Ġbench', 'Ġassembly', 'Ġmir', 'Ġinstrument', 'ri', 'ane', 'Ġe', 'ca', 'Ġlauncher']</t>
         </is>
       </c>
       <c r="C286" t="n">
@@ -4156,7 +4156,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>['Ġmillion', 'Ġlaunch', 'Ġcontract', 'Ġexplore', 'Ġpsyche', "'s", 'Ġheavy', 'Ġmetal', 'Ġasteroid', 'Ġtech', 'cr', 'unch', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmoon', 'Ġmar', 'ie', 'lla', 'Ġfe', 'b', 'ruary', 'n', 'asa', "'s", 'Ġpsyche', 'Ġasteroid', 'Ġmission', 'Ġuse', 'Ġspace', 'x', 'Ġfal', 'con', 'Ġheavy', 'Ġrocket', 'Ġeng', 'ad', 'get', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġpot', 'ter', 'Ġse', 'Ġj', 'uly', 'n', 'asa', 'Ġawards', 'Ġlaunch', 'Ġservices', 'Ġcontract', 'Ġeuro', 'pa', 'Ġcl', 'ipper', 'Ġmission', 'Ġion', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġfal', 'con', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġheavy', 'ï', '¬', 'ģ', 'cial', 'Ġpage', 'Ġfal', 'con', 'Ġheavy', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġanimation', 'Ġfe', 'b', 'ruary', 'Ġel', 'Ġmus', 'k', 'Ġfal', 'con', 'Ġheavy', 'Ġchange', 'Ġspace', 'Ġtravel', 'Ġverge', 'Ġyoutube', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġmanpower', 'Ġsupport', 'Ġc', 'sa', 'Ġprovided', 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġnear', 'inf', 'rared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'Ġmanpower', 'Ġsupport', 'Ġoperations', 'Ġseveral', 'Ġthousand', 'Ġscientists', 'Ġengineers', 'Ġtechnicians', 'Ġspanning', 'Ġcountries', 'Ġcontributed', 'Ġbuild', 'Ġtest', 'Ġintegration', 'Ġtotal', 'Ġcompanies', 'Ġgovernment', 'Ġagencies', 'Ġacademic', 'Ġinstitutions', 'Ġparticipated', 'Ġpre', 'launch', 'Ġproject', 'Ġunited', 'Ġstates', 'Ġeuro', 'pe', 'Ġcountries', 'including', 'Ġfr', 'ance', 'Ġg', 'erman', 'ada', 'Ġcountries', 'Ġn', 'asa', 'Ġpartners', 'Ġaust', 'ral', 'ia', 'Ġinvolved', 'Ġpost', 'launch', 'Ġoperation', 'Ġparticipating', 'Ġcountries', 'Ġaust', 'ria', 'Ġbel', 'g', 'ium', 'ada', 'Ġpartnership', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġc', 'zech', 'Ġrepublic', 'Ġden', 'mark', 'Ġfin', 'land', 'Ġfr', 'ance', 'Ġg', 'erman', 'Ġg', 'ree', 'ce', 'Ġire', 'land', 'aly', 'Ġlux', 'em', 'bourg', 'Ġnet', 'lands', 'way', 'Ġport', 'ugal', 'Ġsp', 'Ġsw', 'eden', 'Ġsw', 'itzerland', 'Ġunited', 'Ġkingdom', 'Ġunited', 'Ġstates', 'Ġn', 'asa', 'Ġadministrator', 'âĢĵ', 'Ġse', 'ke', 'efe', 'Ġmade', 'Ġdecision', 'Ġname', 'Ġtelescope', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', 'Ġadministrator', 'Ġn', 'asa', 'Ġmercury', 'Ġgem', 'ini', 'Ġmuch', 'Ġap', 'ollo', 'Ġprograms', 'Ġconcerns', 'Ġraised', 'Ġaround', 'Ġweb', 'b', "'s", 'Ġpossible', 'Ġrole', 'Ġlav', 'ender', 'Ġscare', 'Ġmid', 'th', 'century', 'Ġpersecution', 'Ġu', 'Ġgovernment', 'Ġtargeting', 'Ġhomosexuals', 'Ġfederal', 'Ġn', 'asa', 'Ġreleased', 'Ġreport', 'Ġinvestigation', 'Ġbased', 'Ġexamination', '000', 'Ġdocuments', 'Ġreport', 'Ġfound', 'Ġavailable', 'Ġevidence', 'Ġdirectly', 'Ġlinks', 'Ġweb', 'b', 'Ġactions', 'Ġfollow', 'Ġrelated', 'Ġfiring', 'Ġindividuals', 'Ġsexual', 'Ġorientation', '",', 'Ġeither', 'Ġtime', 'Ġstate', 'Ġdepartment', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġfour', 'Ġkey', 'Ġgoals', 'Ġsearch', 'Ġlight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstars', 'Ġgalaxies', 'Ġformed', 'Ġuniverse', 'Ġbig', 'Ġbang', 'Ġstudy', 'Ġgalaxy', 'Ġformation', 'Ġevolution', 'Ġunderstand', 'Ġstar', 'Ġformation', 'Ġplanet', 'Ġformation', 'Ġstudy', 'Ġplanetary', 'Ġsystems', 'Ġorigins', 'Ġlife', 'Ġgoals', 'Ġaccomplished', 'Ġeffectively', 'Ġobservation', 'Ġnear', 'inf', 'rared', 'Ġlight', 'Ġrather', 'Ġlight']</t>
         </is>
       </c>
       <c r="C287" t="n">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>['Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlaunches', 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġfunction', 'Ġorbital', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġmanufacturer', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġus', 'Ġmillion', 'Ġn', 'ro', 'Ġus', 'Ġmillion', 'Ġsize', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġwidth', 'Ġft', 'Ġmass', '000', '000', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġdelta', 'Ġiv', 'Ġheavy', 'elta', 'h', 'Ġexpend', 'able', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġlargest', 'Ġtype', 'Ġdelta', 'Ġiv', 'Ġfamily', 'Ġworld', "'s", 'Ġthird', 'Ġhighest', 'capacity', 'Ġlaunch', 'Ġvehicle', 'Ġoperation', 'Ġbehind', 'Ġn', 'asa', "'s", 'Ġspace', 'Ġlaunch', 'Ġsystem', 'Ġspace', 'x', "'s", 'Ġfal', 'con', 'Ġheavy', 'Ġclosely', 'Ġfollowed', 'Ġcasc', "'s", 'Ġlong', 'Ġmarch', 'Ġmanufactured', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'ula', 'Ġfirst', 'Ġlaunched', 'Ġu', 'la', 'Ġretire', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġj', 'une', 'Ġone', 'Ġflight', 'Ġremains', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġconsists', 'Ġcentral', 'Ġcommon', 'Ġbooster', 'Ġcore', 'Ġtwo', 'Ġadditional', 'Ġliquid', 'Ġrocket', 'Ġboosters', 'Ġinstead', 'Ġsolid', 'Ġrocket', 'Ġmotors', 'Ġused', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġversions', 'Ġlift', 'Ġthree', 'Ġcores', 'Ġoperate', 'Ġfull', 'Ġthrust', 'Ġseconds', 'Ġlater', 'Ġcenter', 'Ġcore', 'Ġthrott', 'les', 'Ġconserve', 'Ġfuel', 'Ġbooster', 'Ġseparation', 'Ġtwo', 'Ġside', 'Ġboosters', 'Ġburn', 'Ġseconds', 'Ġlaunch', 'Ġseparated', 'Ġcore', 'Ġbooster', 'Ġthrott', 'les', 'Ġback', 'Ġfull', 'Ġthrust', 'Ġcore', 'Ġburns', 'Ġseconds', 'Ġlater', 'Ġsecond', 'Ġstage', 'Ġcompletes', 'Ġascent', 'Ġlaunch', 'Ġvehicle', 'Ġuses', 'Ġthree', 'Ġengines', 'Ġone', 'Ġcentral', 'Ġcore', 'Ġone', 'Ġbooster', 'Ġlast', 'Ġseconds', 'Ġcountdown', 'Ġhydrogen', 'Ġfuel', 'Ġflows', 'Ġengines', 'Ġupwards', 'Ġalong', 'Ġbooster', 'Ġbody', 'Ġignition', 'Ġhydrogen', 'Ġinfl', 'ames', 'Ġmaking', 'Ġcharacteristic', 'Ġfireball', 'Ġcharred', 'Ġlook', 'Ġbooster', 'Ġdelta', 'Ġiv', 'Ġline', 'Ġrockets', 'Ġdeveloped', 'Ġmc', 'nell', 'Ġdou', 'glas', 'Ġprogram', 'Ġlater', 'Ġtransferred', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġpowerful', 'Ġmember', 'Ġline', 'Ġalso', 'Ġincludes', 'Ġsmaller', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlift', 'Ġlow', 'Ġearth', 'Ġorbit']</t>
+          <t>['Ġvisible', 'Ġpart', 'Ġspectrum', 'Ġreason', 'Ġweb', 'b', "'s", 'Ġinstruments', 'Ġmeasure', 'Ġvisible', 'Ġultraviolet', 'Ġlight', 'Ġlike', 'Ġhub', 'ble', 'Ġtelescope', 'Ġmuch', 'Ġgreater', 'Ġcapacity', 'Ġperform', 'Ġinfrared', 'Ġastronomy', 'Ġweb', 'b', 'Ġsensitive', 'Ġrange', 'Ġwavelengths', 'ĠÂµ', 'cor', 'respond', 'ing', 'Ġrespectively', 'Ġorange', 'Ġlight', 'Ġdeep', 'Ġinfrared', 'Ġradiation', 'ĠâĪĴ', 'ĠÂ°', 'c', 'Ġweb', 'b', 'Ġmay', 'Ġused', 'Ġgather', 'Ġinformation', 'Ġdim', 'ming', 'Ġlight', 'Ġstar', 'Ġk', 'ic', 'Ġdiscovered', 'Ġabnormal', 'Ġlight', 'cur', 'Ġproperties', 'Ġadditionally', 'Ġable', 'Ġtell', 'Ġex', 'oplan', 'et', 'Ġmethane', 'Ġatmosphere', 'Ġallowing', 'Ġastronomers', 'Ġdetermine', 'Ġwhether', 'Ġmethane', 'Ġweb', 'b', 'Ġorbits', 'Ġsun', 'Ġnear', 'Ġsecond', 'Ġlag', 'range', 'Ġpoint', 'Ġsun', 'âĢĵ', 'earth', 'Ġsystem', '000', '000', 'Ġmi', 'Ġfarther', 'Ġsun', 'Ġearth', "'s", 'Ġorbit', 'Ġfour', 'Ġtimes', 'Ġfarther', 'Ġmoon', "'s", 'Ġorbit', 'Ġnormally', 'Ġobject', 'Ġcircling', 'Ġsun', 'Ġfarther', 'Ġearth', 'Ġwould', 'Ġtake', 'Ġlonger', 'Ġnaming', 'Ġconcerns', 'Ġmission', 'Ġgoals', 'Ġorbit', 'Ġdesign', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġweb', 'b', 'Ġexactly', 'Ġpoint', 'Ġcircles', 'Ġaround', 'Ġh', 'alo', 'Ġorbit', 'Ġalternative', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġviews', 'Ġcar', 'ina', 'Ġneb', 'ula', 'Ġcomparing', 'Ġultraviolet', 'Ġvisible', 'top', 'Ġinfrared', 'bottom', 'Ġastronomy', 'Ġfar', 'Ġstars', 'Ġvisible', 'Ġlatter', 'Ġone', 'Ġyear', 'Ġcomplete', 'Ġorbit', 'Ġnear', 'Ġpoint', 'Ġcombined', 'Ġgravitational', 'Ġpull', 'Ġearth', 'Ġsun', 'Ġallow', 'Ġspacecraft', 'Ġorbit', 'Ġsun', 'Ġtime', 'Ġtakes', 'Ġearth', 'Ġstaying', 'Ġclose', 'Ġearth', 'Ġallows', 'Ġdata', 'Ġrates', 'Ġmuch', 'Ġfaster', 'Ġgiven', 'Ġsize', 'Ġantenna', 'Ġtelescope', 'Ġcircles', 'Ġsun', 'âĢĵ', 'earth', 'Ġpoint', 'Ġh', 'alo', 'Ġorbit', 'Ġinclined', 'Ġrespect', 'Ġe', 'cl', 'ipt', 'ic', 'Ġradius', 'Ġvarying', '000', '000', 'Ġmi', '000', '000', 'Ġmi', 'Ġtakes', 'Ġhalf', 'Ġyear', 'Ġcomplete', 'Ġsince', 'Ġequilibrium', 'Ġpoint', 'Ġgravitational', 'Ġpull', 'Ġh', 'alo', 'Ġorbit', 'Ġorbit', 'Ġusual', 'Ġsense', 'Ġspacecraft', 'Ġactually', 'Ġorbit', 'Ġaround', 'Ġsun', 'Ġh', 'alo', 'Ġorbit', 'Ġthought']</t>
         </is>
       </c>
       <c r="C288" t="n">
@@ -4182,7 +4182,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>['Ġge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'g', ').[', 'Ġliquid', 'fuel', 'ed', 'Ġlaunch', 'Ġvehicle', 'Ġconsisting', 'Ġupper', 'Ġstage', 'Ġone', 'Ġmain', 'Ġbooster', 'Ġtwo', 'Ġstrap', 'Ġboosters', 'Ġfirst', 'Ġlaunch', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġcarried', 'Ġboiler', 'plate', 'Ġpayload', 'Ġpartial', 'Ġfailure', 'Ġcav', 'itation', 'Ġliquid', 'oxy', 'gen', 'Ġpropell', 'ant', 'Ġlines', 'Ġcaused', 'Ġshutdown', 'Ġhistory', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġstages', 'Ġcapacity', 'Ġpayload', 'Ġle', 'Ġmass', 'Ġpayload', 'Ġg', 'Ġmass', 'Ġassociated', 'Ġrockets', 'Ġfamily', 'Ġdelta', 'Ġcomparable', 'Ġlong', 'Ġmarch', 'Ġfal', 'con', 'Ġheavy', 'Ġpro', 'ton', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġproduction', 'Ġended', 'Ġlaunch', 'Ġsites', 'Ġcape', 'aver', 'al', 'Ġv', 'enberg', 'Ġtotal', 'Ġlaunches', 'Ġsuccess', 'es', 'Ġpartial', 'Ġfailure', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġde', 'cember', 'usa', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġj', 'une', 'Ġtype', 'Ġpassengers', 'c', 'argo', 'Ġn', 'ro', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġpayload', 'k', 'enn', 'en', 'ion', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'Ġboosters', 'Ġboosters', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġempty', 'Ġmass', '000', '000', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġboosters', 'Ġeight', 'Ġseconds', 'Ġearly', 'Ġcore', 'Ġengine', 'Ġnine', 'Ġseconds', 'Ġearly', 'Ġresulted', 'Ġlower', 'Ġstaging', 'Ġvelocity', 'Ġsecond', 'Ġstage', 'Ġunable', 'Ġcompensate', 'Ġpayload', 'Ġleft', 'Ġlower', 'Ġintended', 'Ġorbit', 'Ġfirst', 'Ġoperational', 'Ġpayload', 'sp', 'Ġsatellite', 'Ġsuccessfully', 'Ġlaunched', 'Ġused', 'Ġlaunch', 'Ġfive', 'Ġvisual', 'Ġelectronic', 'Ġreconnaissance', 'Ġsatellites', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'n', 'ro', 'Ġde', 'cember', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġused', 'Ġlaunch', 'Ġun', 'crew', 'ed', 'Ġtest', 'Ġflight', 'ion', 'Ġspacecraft', 'Ġdesignated', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġseveral', 'Ġdelays', 'Ġmission', 'Ġsuccessfully', 'Ġlaunched', '05', 'Ġut', 'c', 'Ġde', 'cember', 'Ġaug', 'ust', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġadditional', 'Ġstar', 'Ġthird', 'Ġstage', 'Ġused', 'Ġlaunch', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'Ġellipt', 'ical', 'Ġhel', 'oc', 'entric', 'Ġorbit']</t>
+          <t>['Ġcontrolled', 'Ġdrifting', 'Ġremain', 'Ġvicinity', 'Ġpoint', 'Ġrequires', 'Ġstation', 'keeping', 'Ġaround', 'Ġper', 'Ġyear', 'Ġtotal', 'ĠâĪ', 'Ĩ', 'v', 'Ġbudget', 'Ġtwo', 'Ġsets', 'Ġthr', 'usters', 'Ġconstitute', 'Ġobserv', 'atory', "'s", 'Ġpropulsion', 'Ġsystem', 'Ġthr', 'usters', 'Ġlocated', 'Ġsolely', 'Ġsun', 'facing', 'Ġside', 'Ġobserv', 'atory', 'Ġstation', 'keeping', 'Ġoperations', 'Ġdesigned', 'Ġslightly', 'Ġunders', 'h', 'oot', 'Ġrequired', 'Ġamount', 'Ġthrust', 'Ġorder', 'Ġavoid', 'Ġpushing', 'Ġweb', 'b', 'Ġbeyond', 'Ġsemi', 'stable', 'Ġpoint', 'Ġsituation', 'Ġwould', 'Ġunre', 'cover', 'able', 'Ġr', 'andy', 'Ġk', 'imble', 'Ġintegration', 'Ġtest', 'Ġproject', 'Ġscientist', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġcompared', 'Ġprecise', 'Ġstation', 'keeping', 'Ġweb', 'b', 'sis', 'ph', 'us', 'Ġ[...]', 'Ġrolling', 'Ġrock', 'Ġgentle', 'Ġslope', 'Ġnear', 'Ġtop', 'Ġhill', 'Ġnever', 'Ġwant', 'Ġroll', 'Ġcrest', 'Ġget', 'Ġaway', '".[', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġinfrared', 'Ġobservations', 'Ġsee', 'Ġobjects', 'Ġhidden', 'Ġvisible', 'Ġlight', 'Ġshown', 'Ġatmospheric', 'Ġwindows', 'Ġinfrared', 'Ġmuch', 'Ġtype', 'Ġlight', 'Ġblocked', 'Ġviewed', 'Ġearth', "'s", 'Ġsurface', 'Ġwould', 'Ġlike', 'Ġlooking', 'Ġrainbow', 'Ġseeing', 'Ġone', 'Ġcolor', 'Ġanimation', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġtrajectory', 'Ġtop', 'Ġview', 'Ġside', 'Ġview', 'Ġside', 'Ġview', 'Ġsun', 'Ġweb', 'b', 'Ġformal', 'Ġsuccessor', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'h', 'st', 'Ġsince', 'Ġprimary', 'Ġemphasis', 'Ġinfrared', 'Ġastronomy', 'Ġalso', 'Ġsuccessor', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'Ġweb', 'b', 'Ġfar', 'Ġsurpass', 'Ġtelescopes', 'Ġable', 'Ġsee', 'Ġmany', 'Ġmuch', 'Ġolder', 'Ġstars', 'Ġgalaxies', 'Ġobserving', 'Ġinfrared', 'Ġspectrum', 'Ġkey', 'Ġtechnique', 'Ġachieving', 'Ġcos', 'ological', 'Ġred', 'shift', 'Ġbetter', 'Ġpenet', 'rates', 'Ġobsc', 'uring', 'Ġdust', 'Ġgas', 'Ġallows', 'Ġobservation', 'Ġdim', 'mer', 'Ġcooler', 'Ġobjects', 'Ġsince', 'Ġwater', 'Ġvapor', 'Ġcarbon', 'Ġdioxide', 'Ġearth', "'s", 'Ġatmosphere', 'Ġstrongly', 'Ġabsorbs', 'Ġinfrared', 'Ġground', 'based', 'Ġinfrared', 'Ġastronomy', 'Ġlimited', 'Ġnarrow', 'Ġwavelength', 'Ġranges', 'Ġatmosphere', 'Ġabsorbs', 'Ġless', 'Ġstrongly', 'Ġadditionally', 'Ġatmosphere', 'Ġradi', 'ates', 'Ġinfrared', 'Ġspectrum', 'Ġoften', 'Ġoverwhelming', 'Ġlight', 'Ġobject', 'Ġobserved', 'Ġmakes', 'Ġspace', 'Ġtelescope', 'Ġpreferable', 'Ġinfrared', 'Ġobservation', 'Ġdistant', 'Ġobject', 'Ġyounger', 'Ġappears']</t>
         </is>
       </c>
       <c r="C289" t="n">
@@ -4195,7 +4195,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>['Ġmay', 'Ġfinal', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġcore', 'Ġboosters', 'Ġfinished', 'Ġconstruction', 'Ġofficially', 'Ġending', 'Ġdelta', 'Ġiv', 'Ġproduction', 'Ġmaking', 'Ġway', 'Ġvul', 'Ġlaunch', 'Ġvehicle', 'Ġcapacity', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Â°', 'Ġlow', 'Ġearth', 'Ġorbit', 'iss', 'Â°', 'Ġge', 'os', 'ynchronous', 'Ġtransfer', 'Ġorbit', 'g', '):', 'Ġcapabilities', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġpowered', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġtotal', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '04', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġfirst', 'Ġstage', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', 'Ġpowered', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġsea', 'Ġlevel', 'Ġvacuum', '04', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'dc', 'ss', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġgross', 'Ġmass', 'Ġpropell', 'ant', 'Ġmass', '010', 'Ġpowered', 'Ġmaximum', 'Ġthrust', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġburn', 'Ġtime', 'Ġseconds', 'Ġpropell', 'ant', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'ge', '):', 'Ġlunar', 'Ġtransfer', 'Ġorbit', 'l', '):', '000', '000', 'Ġmars', 'Ġtransfer', 'Ġorbit', '000', '000', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġdelta', 'Ġiv', 'Ġheavy', "'s", 'Ġtotal', 'Ġmass', 'Ġlaunch', 'Ġapproximately', '000', '000', 'Ġproduce', 'Ġaround', '000', '000', 'Ġthrust', 'Ġpower', 'Ġrocket', 'Ġsky', 'ward', 'Ġlif', 'ff', 'hide', 'Ġflight', 'Ġdate', 'Ġpayload', 'Ġmass']</t>
+          <t>['Ġlight', 'Ġtaken', 'Ġlonger', 'Ġreach', 'Ġhuman', 'Ġobservers', 'Ġuniverse', 'Ġexpanding', 'Ġlight', 'Ġtravels', 'Ġbecomes', 'Ġred', 'sh', 'ifted', 'Ġobjects', 'Ġextreme', 'Ġdistances', 'Ġtherefore', 'Ġeasier', 'Ġsee', 'Ġviewed', 'Ġinfrared', 'Ġweb', 'b', "'s", 'Ġinfrared', 'Ġcapabilities', 'Ġexpected', 'Ġlet', 'Ġsee', 'Ġback', 'Ġtime', 'Ġfirst', 'Ġgalaxies', 'Ġforming', 'Ġhundred', 'Ġmillion', 'Ġyears', 'Ġbig', 'Ġbang', 'Ġinfrared', 'Ġradiation', 'Ġpass', 'Ġfreely', 'Ġregions', 'Ġcosmic', 'Ġdust', 'Ġscatter', 'Ġvisible', 'Ġlight', 'Ġobservations', 'Ġinfrared', 'Ġallow', 'Ġstudy', 'Ġobjects', 'Ġregions', 'Ġspace', 'Ġwould', 'Ġobscured', 'Ġgas', 'Ġdust', 'Ġvisible', 'Ġspectrum', 'Ġinfrared', 'Ġastronomy', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmolecular', 'Ġclouds', 'Ġstars', 'Ġborn', 'Ġcircumst', 'ellar', 'Ġdisks', 'Ġgive', 'Ġrise', 'Ġplanets', 'Ġcores', 'Ġactive', 'Ġgalaxies', 'Ġrelatively', 'Ġcool', 'Ġobjects', 'tem', 'per', 'atures', 'Ġless', 'Ġseveral', 'Ġthousand', 'Ġdegrees', 'Ġemit', 'Ġradiation', 'Ġprimarily', 'Ġinfrared', 'Ġdescribed', 'Ġplan', 'ck', "'s", 'Ġlaw', 'Ġresult', 'Ġobjects', 'Ġcooler', 'Ġstars', 'Ġbetter', 'Ġstudied', 'Ġinfrared', 'Ġincludes', 'Ġclouds', 'Ġinterstellar', 'Ġmedium', 'Ġbrown', 'Ġdwar', 'fs', 'Ġplanets', 'Ġsolar', 'Ġsystems', 'ets', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġobjects', 'Ġobserved', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'mir', ').[', 'Ġmissions', 'Ġinfrared', 'Ġastronomy', 'Ġimpacted', 'Ġweb', 'b', 'Ġdevelopment', 'Ġsp', 'itzer', 'Ġwil', 'kinson', 'Ġmicrowave', 'ot', 'ropy', 'Ġprobe', 'w', 'map', ').[', 'Ġsp', 'itzer', 'Ġshowed', 'Ġimportance', 'Ġmid', 'inf', 'rared', 'Ġhelpful', 'Ġtasks', 'Ġobserving', 'Ġdust', 'Ġdisks', 'Ġaround', 'Ġstars', 'Ġalso', 'Ġw', 'map', 'Ġprobe', 'Ġshowed', 'Ġuniverse', 'lit', 'Ġred', 'shift', 'Ġundersc', 'oring', 'Ġimportance', 'Ġmid', 'inf', 'rared', 'Ġmissions', 'Ġlaunched', 'Ġearly', 'Ġtime', 'Ġinfluence', 'Ġweb', 'b', 'Ġdevelopment', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'sts', 'ci', 'Ġb', 'alt', 'imore', 'ary', 'land', 'Ġhom', 'ew', 'ood', 'Ġcampus', 'Ġjohn', 'Ġhop', 'kins', 'Ġuniversity', 'Ġselected', 'Ġscience', 'Ġoperations', 'Ġcenter', 'oc', 'Ġweb', 'b', 'Ġinitial', 'Ġbudget', 'Ġus', 'Ġmillion', 'Ġintended', 'Ġsupport', 'Ġoperations', 'Ġfirst', 'Ġyear', 'Ġlaunch']</t>
         </is>
       </c>
       <c r="C290" t="n">
@@ -4208,7 +4208,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>['Ġlaunch', 'Ġsite', 'Ġoutcome', 'Ġde', 'cember', 'Ġdemos', 'Ġspark', 'ie', 'Ġr', 'alph', 'ie', 'Ġpounds', 'Ġkilograms', 'Ġcape', 'aver', 'al', 'Ġpartial', 'Ġfailure', 'mber', 'sp', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'Ġpounds', 'Ġkilograms', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġjan', 'uary', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'mber', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġjan', 'uary', 'Ġk', 'enn', 'en', 'usa', 'Ġpounds', '000', 'Ġkilograms', 'Ġv', 'enberg', 'Ġsuccess', 'Ġj', 'une', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġaug', 'ust', 'Ġk', 'enn', 'en', 'usa', 'Ġpounds', '000', 'Ġkilograms', 'Ġv', 'enberg', 'Ġsuccess', 'Ġde', 'cember', 'ion', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġpounds', '000', 'Ġkilograms', 'b', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġj', 'une', 'ion', 'Ġmentor', 'usa', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġaug', 'ust', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'c', 'Ġpounds', 'Ġkilograms', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġjan', 'uary', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġv', 'enberg', 'Ġsuccess', 'Ġde', 'cember', 'ion', 'Ġmentor', 'usa', 'Ġn', 'rol', ')[', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġapr', 'il', 'Ġk', 'enn', 'en', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġv', 'enberg', 'Ġsuccess', 'Ġse', 'pt', 'ember', 'Ġk', 'enn', 'en', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġv', 'enberg', 'Ġsuccess', 'Ġj', 'une', 'ion', 'Ġmentor', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġcape', 'aver', 'al', 'Ġsuccess', 'Ġmissions', 'Ġthirteen', 'Ġsixteen', 'Ġannounced', 'Ġnational', 'Ġreconnaissance', 'Ġoffice', 'Ġfinal', 'Ġfive', 'Ġmissions', 'Ġincluding', 'Ġmodifications', 'Ġu', 'la', 'Ġawarded', 'Ġbillion', 'Ġus', 'Ġmillion', 'Ġper', 'Ġlaunch', 'Ġcompared', 'Ġfal', 'con', 'Ġheavy', 'Ġlaunch', 'Ġprice', 'Ġj', 'une']</t>
+          <t>['Ġcapacity', 'Ġst', 'sci', 'Ġresponsible', 'Ġscientific', 'Ġoperation', 'Ġtelescope', 'Ġdelivery', 'Ġdata', 'Ġproducts', 'Ġastronomical', 'Ġcommunity', 'Ġdata', 'Ġtransmitted', 'Ġweb', 'b', 'Ġground', 'Ġvia', 'Ġn', 'asa', 'Ġdeep', 'Ġspace', 'Ġnetwork', 'Ġprocessed', 'Ġcalibrated', 'Ġst', 'sci', 'Ġdistributed', 'Ġonline', 'Ġastronomers', 'Ġworldwide', 'Ġsimilar', 'Ġhub', 'ble', 'Ġoperated', 'Ġanyone', 'Ġanywhere', 'Ġworld', 'Ġallowed', 'Ġsubmit', 'Ġproposals', 'Ġobservations', 'Ġyear', 'Ġseveral', 'Ġcommittees', 'Ġastronomers', 'Ġpeer', 'Ġreview', 'Ġsubmitted', 'Ġproposals', 'Ġselect', 'Ġprojects', 'Ġobserve', 'Ġcoming', 'Ġyear', 'Ġauthors', 'Ġchosen', 'Ġproposals', 'Ġtypically', 'Ġone', 'Ġyear', 'Ġprivate', 'Ġaccess', 'Ġnew', 'Ġobservations', 'Ġdata', 'Ġbecome', 'Ġpublicly', 'Ġavailable', 'Ġdownload', 'Ġanyone', 'Ġonline', 'Ġarchive', 'Ġst', 'sci', 'Ġbandwidth', 'Ġdigital', 'Ġthroughput', 'Ġsatellite', 'Ġdesigned', 'Ġoperate', 'Ġgig', 'ab', 'Ġdata', 'Ġper', 'Ġday', 'Ġlength', 'Ġmission', 'equ', 'ivalent', 'Ġsustained', 'Ġrate', 'Ġdata', 'Ġprocessing', 'Ġtelescope', 'Ġdone', 'Ġconventional', 'Ġsingle', 'board', 'Ġcomputers', 'Ġdigit', 'ization', 'Ġanalog', 'Ġdata', 'Ġinstruments', 'Ġperformed', 'Ġcustom', 'Ġside', 'car', 'ic', 'system', 'Ġimage', 'Ġdigit', 'ization', 'Ġenhancement', 'Ġcontrol', 'Ġretrieval', 'Ġapplication', 'Ġspecific', 'Ġintegrated', 'Ġcircuit', 'Ġn', 'asa', 'Ġstated', 'Ġside', 'car', 'ic', 'Ġinclude', 'Ġfunctions', 'Ġinstrument', 'Ġpackage', 'Ġconsume', 'Ġmill', 'iw', 'atts', 'Ġpower', 'Ġsince', 'Ġconversion', 'Ġmust', 'Ġdone', 'Ġclose', 'Ġdetectors', 'Ġcold', 'Ġside', 'Ġtelescope', 'Ġlow', 'Ġpower', 'Ġdiss', 'ipation', 'Ġcrucial', 'Ġmaintaining', 'Ġlow', 'Ġtemperature', 'Ġrequired', 'Ġoptimal', 'Ġoperation', 'Ġground', 'Ġsupport', 'Ġoperations', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġstrike', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmirror', 'Ġsegment', 'Ġsuffered', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġstrike', 'Ġlarge', 'Ġdust', 'ote', 'sized', 'Ġparticle', 'Ġmay', 'Ġfifth', 'Ġlargest', 'Ġstrike', 'Ġsince', 'Ġlaunch', 'Ġreported', 'Ġj', 'une', 'Ġrequired', 'Ġengineers', 'Ġcompensate', 'Ġstrike', 'Ġusing', 'Ġmirror', 'Ġactu', 'ator', 'Ġdespite', 'Ġstrike', 'Ġn', 'asa', 'Ġcharacterization', 'Ġreport', 'Ġstates', 'Ġj', 'w', 'st', 'Ġobserving', 'Ġmodes', 'Ġreviewed', 'Ġconfirmed', 'Ġready', 'Ġscience', 'Ġuse', 'Ġj', 'uly', 'Ġlaunch', 'design', 'ated', 'ri', 'ane', 'Ġflight', 'Ġtook', 'Ġplace']</t>
         </is>
       </c>
       <c r="C291" t="n">
@@ -4221,7 +4221,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>['Ġone', 'Ġremains', 'Ġu', 'la', 'Ġret', 'ires', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlaunch', 'Ġhistory', 'Ġfuture', 'Ġlaunches', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġflight', 'Ġdate', 'Ġlaunch', 'Ġsite', 'Ġpayload', 'Ġmass', 'Ġorbit', 'Ġcustomer', 'Ġlaunch', 'Ġoutcome', 'Ġmarch', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġgeo', 'Ġus', 'Ġn', 'ro', 'Ġplanned', 'Ġreconnaissance', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'n', 'al', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġdelta', 'Ġrocket', 'Ġfamily', 'per', 'formed', 'Ġlower', 'Ġorbit', 'Ġplanned', 'Ġb', 'ï', '¬', 'ģ', 'cially', 'Ġreported', 'Ġmass', '000', 'Ġincludes', 'Ġlaunch', 'Ġabort', 'Ġsystem', 'las', 'Ġreach', 'Ġorbit', 'Ġexcludes', 'Ġresidual', 'Ġmass', 'Ġupper', 'Ġstage', 'Ġreach', 'Ġorbit', 'Ġlikely', 'Ġoffset', 'ting', 'Ġmass', 'Ġlas', 'Ġc', 'Ġstar', 'Ġupper', 'Ġstage', 'Ġcurrent', 'Ġlong', 'Ġmarch', 'ge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġlong', 'Ġmarch', 'low', 'Ġearth', 'Ġorbit', 'Ġlong', 'Ġmarch', 'ge', 'ost', 'ation', 'ary', 'Ġtransfer', 'Ġorbit', 'Ġfal', 'con', 'Ġheavy', 'Ġpro', 'ton', 'Ġdevelopment', 'Ġang', 'ara', 'ri', 'ane', 'Ġnew', 'Ġgl', 'enn', 'Ġvul', 'Ġcent', 'aur', 'Ġretired', 'Ġcancelled', 'ri', 'ane', 'ret', 'ired', 'las', 'Ġheavy', 'prop', 'osed', 'Ġnever', 'Ġdeveloped', 'Ġsat', 'urn', 'ret', 'ired', 'Ġtitan', 'ret', 'ired', 'Ġtitan', 'Ġiv', 'ret', 'ired', 'Ġheavy', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġcomparison', 'Ġorbital', 'Ġrocket', 'Ġengines', 'Ġcomparison', 'Ġspace', 'Ġstation', 'Ġcargo', 'Ġvehicles', 'Ġcomparable', 'Ġvehicles', 'Ġsee', 'Ġalso', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'Ġnational', 'Ġlaunch', 'Ġsystem', 'âĢĵ', 'Ġstudy', 'ula', 'Ġce', 'ory', 'Ġbr', 'uno', 'Ġtwitter', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'elta', 'Ġiv', 'Ġheavy', 'Ġgoes', 'Ġus', "'s", 'Ġcurrent', 'Ġfuture', 'Ġretirement', 'Ġdelta', 'Ġiv', 'Ġmedium', 'Ġdelta', 'elta', 'Ġiv', 'Ġheavy', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'elta', 'Ġiv', 'Ġpayload', 'Ġplanner', "'s", 'Ġguide', 'Ġj', 'une', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'mission', 'Ġstatus', 'Ġcenter', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'Ġu', 'la', 'Ġdelta', 'heavy', 'Ġcurrently', 'Ġworld', "'s", 'Ġlargest', 'Ġrocket', 'Ġproviding', 'Ġnation', 'Ġreliable', 'Ġproven', 'Ġheavy', 'Ġlift']</t>
+          <t>['Ġscheduled', 'Ġut', 'c', 'Ġde', 'cember', 'ri', 'ane', 'Ġrocket', 'Ġlifted', 'Ġgu', 'iana', 'Ġspace', 'Ġcentre', 'Ġfrench', 'Ġgu', 'iana', 'Ġtelescope', 'Ġconfirmed', 'Ġreceiving', 'Ġpower', 'Ġstarting', 'Ġtwo', 'week', 'Ġdeployment', 'Ġphase', 'Ġparts', 'Ġtraveling', 'Ġtarget', 'Ġtelescope', 'Ġreleased', 'Ġupper', 'Ġstage', 'Ġminutes', 'Ġseconds', 'Ġlaunch', 'Ġbeginning', 'day', 'Ġadjustment', 'Ġplace', 'Ġtelescope', 'Ġl', 'iss', 'aj', 'ous', 'Ġorbit', 'Ġaround', 'Ġlag', 'range', 'Ġpoint', 'Ġtelescope', 'Ġlaunched', 'Ġslightly', 'Ġless', 'Ġspeed', 'Ġneeded', 'Ġreach', 'Ġfinal', 'Ġorbit', 'Ġslowed', 'Ġtravelled', 'Ġaway', 'Ġearth', 'Ġorder', 'Ġreach', 'Ġvelocity', 'Ġneeded', 'Ġenter', 'Ġorbit', 'Ġtelescope', 'Ġreached', 'Ġjan', 'uary', 'Ġflight', 'Ġincluded', 'Ġthree', 'Ġplanned', 'Ġcourse', 'Ġcorrections', 'Ġadjust', 'Ġspeed', 'Ġdirection', 'Ġobserv', 'atory', 'Ġcould', 'Ġrecover', 'th', 'rust', 'going', 'Ġslowly', 'Ġcould', 'Ġrecover', 'Ġoverth', 'rust', 'going', 'Ġfast', 'Ġprotect', 'Ġhighly', 'Ġinstruments', 'Ġsun', 'shield', 'Ġmust', 'Ġremain', 'Ġtelescope', 'Ġsun', 'Ġspacecraft', 'Ġcould', 'Ġturn', 'Ġaround', 'Ġuse', 'Ġthr', 'usters', 'Ġslow', 'Ġorbit', 'Ġunstable', 'Ġj', 'w', 'st', 'Ġneeds', 'Ġuse', 'Ġpropell', 'ant', 'Ġmaintain', 'Ġh', 'alo', 'Ġorbit', 'Ġaround', 'known', 'Ġstation', 'keeping', 'Ġprevent', 'Ġtelescope', 'Ġdrifting', 'Ġaway', 'Ġorbital', 'Ġposition', 'Ġdesigned', 'Ġcarry', 'Ġenough', 'Ġpropell', 'ant', 'Ġyears', 'Ġprecision', 'ri', 'ane', 'Ġlaunch', 'Ġfirst', 'Ġmid', 'course', 'Ġcorrection', 'Ġcredited', 'Ġsaving', 'Ġenough', 'Ġonboard', 'Ġfuel', 'Ġj', 'w', 'st', 'Ġmay', 'Ġable', 'Ġmaintain', 'Ġorbit', 'Ġaround', 'Ġyears', 'Ġspace', 'Ġcalled', 'Ġlaunch', 'fl', 'aw', 'less', '".[', 'Ġlaunch', 'Ġcommission', 'ing', 'Ġlaunch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġdiagram', 'Ġweb', 'b', 'Ġinside', 'ri', 'ane', 'ri', 'ane', 'Ġweb', 'b', 'Ġlaunch', 'Ġpad', 'ri', 'ane', 'Ġcontaining', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlifting', 'Ġlaunch', 'Ġpad', 'ri', 'ane', 'Ġcontaining', 'Ġweb', 'b', 'Ġmoments', 'Ġlift', 'Ġweb', 'b', 'Ġseen', 'Ġcry', 'ote', 'chn', 'ic', 'Ġupper', 'Ġstage', 'Ġshortly', 'Ġseparation', 'Ġapproximately', 'Ġminutes', 'Ġlaunch', 'Ġpart', 'Ġearth', 'Ġgulf', 'Ġad', 'en', 'Ġvisible', 'Ġbackground', 'Ġimage', 'Ġweb', 'b']</t>
         </is>
       </c>
       <c r="C292" t="n">
@@ -4234,7 +4234,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>['Ġcapability', 'Ġcountry', "'s", 'Ġnational', 'Ġsecurity', 'Ġpayload', 'Ġeast', 'Ġwest', 'Ġcoasts', '."', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġfe', 'b', 'ruary', 'fal', 'con', 'Ġheavy', 'Ġspace', 'x', "'s", 'Ġbig', 'Ġnew', 'Ġrocket', 'Ġsucceeds', 'Ġfirst', 'Ġtest', 'Ġlaunch', 'Ġl', 'Ġnew', 'ork', 'Ġtimes', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfal', 'con', 'Ġheavy', 'Ġcapable', 'Ġlifting', '000', 'Ġpounds', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġrocket', 'Ġtoday', '."', 'bo', 'e', 'ing', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġachieves', 'Ġmajor', 'Ġtest', 'Ġobjectives', 'Ġfirst', 'Ġflight', 'Ġarchived', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġbo', 'e', 'ing', 'Ġaccessed', 'Ġmarch', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġaug', 'ust', 'ula', 'Ġlaunch', 'Ġdelta', 'Ġheavy', 'th', 'Ġmission', 'Ġfour', 'Ġgo', 'Ġrocket', 'Ġretired', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'elta', 'heavy', 'Ġlikely', 'Ġheading', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġtop', 'Ġsecret', 'Ġpayload', 'space', 'ï', '¬', 'Ĥ', 'igh', 'Ġad', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġer', 'ic', 'Ġber', 'ger', 'Ġjan', 'uary', 'Ġmassive', 'Ġrocket', 'Ġcreates', 'Ġï', '¬', 'ģ', 'ball', 'Ġlaunches', "'s", 'Ġdesign', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġapr', 'il', 'elta', 'Ġiv', 'Ġheavy', 'Ġpowerful', 'Ġlaunch', 'Ġvehicle', 'Ġspace', 'Ġretrieved', 'Ġj', 'uly', 'elta', 'heavy', 'Ġinvestigation', 'Ġident', 'ï', '¬', 'ģ', 'es', 'Ġrocket', "'s", 'Ġproblem', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'second', 'Ġstage', 'Ġign', 'ites', 'Ġfirst', 'Ġstage', 'Ġfalls', 'Ġaway', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'elta', 'Ġiv', 'Ġpark', 'er', 'Ġsolar', 'Ġprobe', 'Ġker', 'olar', 'pro', 'Ġul', 'al', 'aunch', 'Ġretrieved', 'Ġde', 'cember', 'ula', "'s", 'Ġdelta', 'Ġrocket', 'Ġassembly', 'Ġline', 'Ġfalls', 'Ġsilent', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġreferences', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġwik', 'ipedia', 'elta', 'Ġiv', 'Ġlaunch', 'Ġservices', 'Ġuser', "'s", 'Ġguide', 'Ġj', 'une', 'j', 'une', 'pdf', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġj', 'une', 'Ġpp']</t>
+          <t>['Ġreleased', 'Ġrocket', 'Ġupper', 'Ġstage', 'Ġminutes', 'Ġflawless', 'Ġlaunch', 'Ġstarting', 'Ġminutes', 'Ġlaunch', 'Ġcontinuing', 'Ġdays', 'Ġweb', 'b', 'Ġbegan', 'Ġprocess', 'Ġdeploying', 'Ġsolar', 'Ġarray', 'Ġantenna', 'Ġsun', 'shield', 'Ġmirrors', 'Ġnearly', 'Ġdeployment', 'Ġactions', 'Ġcommanded', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġb', 'alt', 'imore', 'ary', 'land', 'Ġexcept', 'Ġtwo', 'Ġearly', 'Ġautomatic', 'Ġsteps', 'Ġsolar', 'Ġpanel', 'Ġunfolding', 'Ġcommunication', 'Ġantenna', 'Ġmission', 'Ġdesigned', 'Ġgive', 'Ġground', 'Ġcontrollers', 'Ġflexibility', 'Ġchange', 'Ġmodify', 'Ġdeployment', 'Ġsequence', 'Ġcase', 'Ġproblems', 'Ġest', 'Ġde', 'cember', 'Ġhours', 'Ġlaunch', 'Ġtelescope', "'s", 'Ġpair', 'Ġprimary', 'Ġrockets', 'Ġbegan', 'Ġfiring', 'Ġminutes', 'Ġmake', 'Ġfirst', 'Ġthree', 'Ġplanned', 'Ġmid', 'course', 'Ġcorrections', 'Ġday', 'Ġtwo', 'Ġhigh', 'Ġgain', 'Ġcommunication', 'Ġantenna', 'Ġdeployed', 'Ġautomatically', 'Ġtransit', 'Ġstructural', 'Ġdeployment', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġstructural', 'Ġdeployment', 'Ġtimeline', 'Ġstructural', 'Ġdeployment', 'Ġsequence', 'Ġde', 'cember', 'Ġhours', 'Ġlaunch', 'Ġweb', 'b', "'s", 'Ġrockets', 'Ġfired', 'Ġnine', 'Ġminutes', 'Ġseconds', 'Ġmake', 'Ġsecond', 'Ġthree', 'Ġmid', 'course', 'Ġcorrections', 'Ġtelescope', 'Ġarrive', 'Ġdestination', 'Ġde', 'cember', 'Ġthree', 'Ġdays', 'Ġlaunch', 'Ġmission', 'Ġcontrollers', 'Ġbegan', 'Ġmulti', 'day', 'Ġdeployment', 'Ġweb', 'b', "'s", 'important', 'Ġsun', 'shield', 'Ġde', 'cember', 'Ġcontrollers', 'Ġsuccessfully', 'Ġcompleted', 'Ġtwo', 'Ġsteps', 'Ġunp', 'acking', 'Ġobserv', 'atory', 'Ġfirst', 'Ġcommands', 'Ġdeployed', 'Ġaft', 'mom', 'ent', 'um', 'Ġflap', '",', 'Ġdevice', 'Ġprovides', 'Ġbalance', 'Ġsolar', 'Ġpressure', 'Ġsun', 'shield', 'Ġsaving', 'Ġfuel', 'Ġreducing', 'Ġneed', 'Ġthr', 'uster', 'Ġfiring', 'Ġmaintain', 'Ġweb', 'b', "'s", 'Ġorientation', 'Ġde', 'cember', 'Ġground', 'Ġteam', 'Ġextended', 'Ġtwo', 'Ġtelesc', 'oping', 'mid', 'Ġbo', 'oms', 'Ġleft', 'Ġright', 'Ġsides', 'Ġobserv', 'atory', 'Ġleft', 'Ġside', 'Ġdeployed', 'Ġhours', 'Ġminutes', 'Ġright', 'Ġside', 'Ġtook', 'Ġhours', 'Ġminutes', 'Ġcommands', 'Ġseparate', 'Ġtension', 'Ġmembranes', 'Ġfollowed', 'Ġjan', 'uary', 'Ġsuccessful', 'Ġjan', 'uary', 'Ġmission', 'Ġcontrol', 'Ġsuccessfully', 'Ġdeployed', 'Ġtelescope', "'s", 'Ġsecondary', 'Ġmirror', 'Ġlocked', 'Ġplace', 'Ġtolerance', 'Ġone', 'Ġhalf', 'Ġmill', 'imeters', 'Ġlast', 'Ġstep', 'Ġstructural', 'Ġdeployment', 'Ġunfold', 'Ġwings']</t>
         </is>
       </c>
       <c r="C293" t="n">
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>['âĢĵ', 'âĢĵ', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'elta', 'Ġiv', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'Ġretrieved', 'Ġj', 'uly', 'Ġray', 'Ġde', 'cember', 'Ġheavy', 'Ġtriple', 'sized', 'Ġdelta', 'Ġrocket', 'Ġdebut', 'web', 'arc', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġview', 'html', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'live', 'Ġcoverage', 'Ġlaunch', 'Ġdelta', 'heavy', 'Ġrocket', 'Ġset', 'Ġearly', 'aturday', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġk', 'bs', 'Ġgun', 'ter', 'elta', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġretrieved', 'Ġmarch', 'n', 'asa', 'ion', 'Ġexploration', 'Ġflight', 'Ġtest', 'Ġpress', 'Ġkit', 'Ġn', 'asa', 'Ġde', 'cember', 'Ġp', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'launch', 'Ġschedule', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'launch', 'Ġmission', 'Ġexecution', 'Ġforecast', 'th', 'Ġweather', 'Ġsquadron', 'Ġpat', 'rick', 'Ġair', 'Ġforce', 'Ġbase', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'elta', 'heavy', 'Ġrocket', 'Ġlifts', 'Ġn', 'ro', 'Ġsatellite', 'sp', 'ac', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġray', 'Ġj', 'une', 'sur', 'illance', 'Ġsatellite', 'Ġlaunching', 'Ġth', 'ursday', 'Ġatop', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġrocket', 'rocket', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'air', 'Ġforce', 'Ġawards', 'Ġu', 'la', 'Ġus', 'Ġbillion', 'Ġcontract', 'Ġcomplete', 'Ġï', '¬', 'ģ', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġn', 'ro', 'Ġmissions', 'h', 'missions', 'Ġspac', 'en', 'ews', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'n', 'ssl', 'Ġphase', 'Ġindustry', 'Ġday', 'Ġspace', 'Ġsystems', 'Ġcommand', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġdelta', 'Ġiv', 'Ġbooster', 'Ġintegration', 'Ġanother', 'Ġstep', 'Ġtoward', 'Ġfirst', 'ion', 'Ġflight', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġprimary', 'Ġmirror', 'Ġpanel', 'Ġconsists', 'Ġthree', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġfolded', 'Ġallow', 'Ġspace', 'Ġtelescope', 'Ġinstalled', 'Ġfair', 'ing', 'ri', 'ane', 'Ġrocket', 'Ġlaunch', 'Ġtelescope', 'Ġjan', 'uary', 'Ġn', 'asa', 'Ġdeployed', 'Ġlocked', 'Ġplace', 'Ġport', 'side', 'Ġwing', 'Ġjan', 'uary', 'Ġstar', 'board', 'side', 'Ġmirror', 'Ġwing', 'Ġsuccessfully', 'Ġcompleted', 'Ġstructural', 'Ġdeployment', 'Ġjan', 'uary', '00', 'Ġeastern', 'Ġstandard', 'Ġtime', 'Ġnearly', 'Ġmonth', 'Ġlaunch', 'Ġthird', 'Ġfinal', 'Ġcourse', 'Ġcorrection', 'Ġtook', 'Ġplace', 'Ġinserting', 'Ġweb', 'b', 'Ġplanned', 'Ġh', 'alo', 'Ġorbit', 'Ġaround', 'Ġsun', 'âĢĵ', 'Ġearth', 'Ġpoint', 'Ġmir', 'Ġinstrument', 'Ġfour', 'Ġobserving', 'Ġmodes', 'âĢĶ', 'im', 'aging', 'Ġlow', 'resolution', 'Ġspect', 'rosc', 'opy', 'Ġmedium', 'resolution', 'Ġspect', 'rosc', 'opy', 'Ġcoron', 'agraph', 'ic', 'Ġimaging', 'ĠâĢ', 'ľ', 'Ġaug', 'Ġmechanism', 'Ġsupports', 'Ġmedium', 'resolution', 'Ġspect', 'rosc', 'opy', 'Ġexhibited', 'Ġappears', 'Ġincreased', 'Ġfriction', 'Ġsetup', 'Ġscience', 'Ġobservation', 'Ġmechanism', 'Ġgr', 'ating', 'Ġwheel', 'Ġallows', 'Ġscientists', 'Ġselect', 'Ġshort', 'Ġmedium', 'Ġlonger', 'Ġwavelengths', 'Ġmaking', 'Ġobservations', 'Ġusing', 'Ġmode', 'âĢ', 'Ŀ', 'Ġsaid', 'Ġn', 'asa', 'Ġpress', 'Ġstatement', 'Ġjan', 'uary', 'Ġstill', 'Ġtransit', 'Ġmirror', 'Ġalignment', 'Ġbegan', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġsecondary', 'Ġmirror', 'Ġmoved', 'Ġaway', 'Ġprotective', 'Ġlaunch', 'Ġpositions', 'Ġtook', 'Ġdays', 'Ġactu', 'ator', 'Ġmotors', 'Ġdesigned', 'Ġfine', 'une', 'Ġmirror', 'Ġpositions', 'Ġmicroscopic', 'Ġcommission', 'ing', 'Ġtesting', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġanimation', 'Ġweb', 'b', "'s", 'Ġh', 'alo', 'Ġorbit', 'Ġaccuracy', 'Ġnan', 'ometer', 'Ġincrements', 'Ġmust', 'Ġmove', 'Ġmillion', 'Ġincrements', 'Ġmm', 'Ġinitial', 'Ġalignment', 'Ġmirror', 'Ġalignment', 'Ġrequires', 'Ġmirror', 'Ġsegments', 'Ġsecondary', 'Ġmirror', 'Ġpositioned', 'Ġwithin', 'Ġnan', 'ometers', 'Ġn', 'asa', 'Ġcompares', 'Ġrequired', 'Ġaccuracy', 'Ġanalogy', 'Ġweb', 'b', 'Ġprimary', 'Ġmirror', 'Ġsize', 'Ġunited', 'Ġstates', 'mir', 'ror', 'Ġsegment', 'Ġwould', 'Ġsize', 'Ġtex', 'Ġteam', 'Ġwould', 'Ġneed', 'Ġline', 'Ġheight', 'Ġtex', 'sized', 'Ġsegments', 'Ġaccuracy', 'Ġinches', '".[', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmirror']</t>
         </is>
       </c>
       <c r="C294" t="n">
@@ -4260,7 +4260,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>['01', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġwik', 'ipedia', 'b', 'ss', '048', 'Ġï', '¬', 'ģ', 'r', 'st', 'b', 'ss', 'Ġsatellites', 'Ġpassing', 'Ġcy', 'gn', 'us', 'Ġse', 'pt', 'ember', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'red', 'irect', 'ed', 'Ġg', 'ss', 'ap', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'sb', 'ss', 'Ġsystem', 'Ġplanned', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġconstellation', 'Ġsatellites', 'Ġsupporting', 'Ġground', 'Ġinfrastructure', 'Ġimprove', 'Ġability', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'od', 'Ġdetect', 'Ġtrack', 'Ġspace', 'Ġobjects', 'Ġorbit', 'Ġaround', 'Ġearth', 'Ġprimary', 'b', 'ss', 'Ġcontractor', 'Ġbo', 'e', 'ing', 'Ġcharacter', 'izes', 'Ġorbiting', 'Ġspace', 'Ġobjects', 'pot', 'ential', 'Ġfuture', 'Ġthreats', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġassets', '".[', 'b', 'ss', 'Ġdevelopment', 'Ġwork', 'Ġconducted', 'Ġcoordination', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġgroup', 'Ġspace', 'Ġsuperiority', 'Ġsystems', 'Ġwing', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'Ġcommander', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġgroup', 'Ġbelieves', 'b', 'ss', 'Ġsatellite', 'Ġoperations', 'Ġcenter', 'Ġtransform', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġproviding', 'Ġgateway', 'Ġresponsive', 'Ġtask', 'able', 'Ġsensor', 'Ġcapability', 'Ġkey', 'Ġenabling', 'Ġevent', 'driven', 'Ġoperations', 'Ġconcept', 'Ġfuture', '".[', 'Ġfirst', 'path', 'finder', 'Ġsatellite', 'b', 'ss', 'Ġsystem', 'sb', 'ss', 'Ġaka', 'Ġus', 'Ġcos', 'par', '048', 'Ġsat', 'cat', 'Ġsuccessfully', 'Ġplaced', 'Ġorbit', 'Ġboard', 'Ġmin', 'otaur', 'Ġiv', 'Ġrocket', 'Ġse', 'pt', 'ember', 'Ġoriginally', 'Ġlaunch', 'Ġscheduled', 'Ġde', 'cember', 'Ġres', 'ched', 'uled', 'Ġspring', 'Ġdelayed', 'Ġoct', 'ober', 'Ġlaunch', 'Ġdelays', 'Ġcaused', 'Ġproblems', 'Ġbooster', 'Ġsatellite', 'Ġlaunch', 'Ġexpected', 'Ġj', 'uly', 'Ġalso', 'Ġpostponed', 'Ġprogram', 'Ġcost', 'Ġmillion', 'Ġincluding', 'Ġsatellite', 'Ġpayload', 'Ġlaunch', 'Ġground', 'Ġsupport', 'Ġsatellite', 'Ġpayload', 'Ġcontracts', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġapproximately', 'Ġtotal', 'Ġdesigned', 'Ġexamine', 'Ġevery', 'Ġspacecraft', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġleast', 'b', 'ss', 'Ġpath', 'finder', 'Ġsatellite', 'Ġtelescope', 'Ġtwo', 'Ġaxis', 'Ġg', 'im', 'bal', 'Ġmeg', 'apixel', 'Ġimage', 'Ġsensor', 'Ġprojected', 'Ġmission', 'Ġduration', 'Ġfive', 'Ġhalf', 'Ġyears', 'Ġfirst', 'Ġtwo', 'Ġg', 'ss', 'ap', 'Ġspacecraft', 'Ġlaunched', 'Ġtwo', 'Ġlaunched']</t>
+          <t>['Ġalignment', 'Ġanimations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġsegment', 'Ġimage', 'Ġident', 'ï', '¬', 'ģ', 'cation', 'Ġmirror', 'Ġsegments', 'Ġmoved', 'Ġdetermine', 'Ġsegment', 'Ġcreates', 'Ġsegment', 'Ġimage', 'Ġmatching', 'Ġmirror', 'Ġsegments', 'Ġrespective', 'Ġimages', 'Ġmirrors', 'Ġtilted', 'Ġbring', 'Ġimages', 'Ġnear', 'Ġcommon', 'Ġpoint', 'Ġanalysis', 'Ġsegment', 'Ġalignment', 'Ġbegins', 'Ġdef', 'ocusing', 'Ġsegment', 'Ġimages', 'Ġmoving', 'Ġsecondary', 'Ġmirror', 'Ġslightly', 'Ġmathematical', 'Ġanalysis', 'Ġcalled', 'Ġphase', 'Ġretrieval', 'Ġapplied', 'Ġdef', 'ocused', 'Ġimages', 'Ġdetermine', 'Ġprecise', 'Ġpositioning', 'Ġerrors', 'Ġsegments', 'Ġadjustments', 'Ġsegments', 'Ġresult', 'Ġwell', 'correct', 'ed', 'tel', 'esc', 'opes', '".', 'Ġhowever', 'Ġsegments', 'Ġstill', 'Ġwork', 'Ġtogether', 'Ġsingle', 'Ġmirror', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġimage', 'Ġstacking', 'Ġput', 'Ġlight', 'Ġsingle', 'Ġplace', 'Ġsegment', 'Ġimage', 'Ġmust', 'Ġstacked', 'Ġtop', 'Ġone', 'Ġanother', 'Ġimage', 'Ġstacking', 'Ġstep', 'Ġindividual', 'Ġsegment', 'Ġimages', 'Ġmoved', 'Ġfall', 'Ġprecisely', 'Ġcenter', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġproduce', 'Ġone', 'Ġun', 'ï', '¬', 'ģ', 'ed', 'Ġimage', 'Ġprocess', 'Ġprepares', 'Ġtelescope', 'Ġcoarse', 'Ġph', 'asing', 'Ġtelescope', 'Ġalignment', 'Ġinstrument', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġview', 'Ġï', '¬', 'ģ', 'ne', 'Ġph', 'asing', 'Ġtelescope', 'Ġwell', 'Ġaligned', 'Ġone', 'Ġplace', 'Ġn', 'irc', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġview', 'Ġalignment', 'Ġmust', 'Ġextended', 'Ġrest', 'Ġinstruments', 'Ġmirror', 'Ġalignment', 'Ġcomplex', 'Ġoperation', 'Ġsplit', 'Ġseven', 'Ġphases', 'Ġrepeatedly', 'Ġrehears', 'ed', 'Ġusing', 'Ġscale', 'Ġmodel', 'Ġtelescope', 'Ġmirrors', 'Ġreached', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'Ġn', 'irc', 'Ġtargeted', 'th', 'Ġmagnitude', 'Ġstar', 'Ġ', 'urs', 'Ġmajor', 'Ġn', 'irc', 'Ġtook', 'Ġimages', 'Ġused', 'Ġwide', 'ranging', 'Ġimages', 'Ġdetermine', 'Ġsegment', 'Ġmain', 'Ġmirror', 'Ġinitially', 'Ġpointed', 'Ġfirst', 'Ġindividual', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġgreatly', 'Ġmis', 'aligned', 'Ġimage', 'Ġcontained', 'Ġseparate', 'Ġblurry', 'Ġimages', 'Ġstar', 'Ġfield', 'Ġcontaining', 'Ġimage', 'Ġtarget', 'Ġstar', 'Ġimages', 'Ġmatched', 'Ġrespective', 'Ġmirror', 'Ġsegments', 'Ġsegments', 'Ġbrought', 'Ġapproximate', 'Ġalignment', 'Ġcentered']</t>
         </is>
       </c>
       <c r="C295" t="n">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>['Ġaug', 'ust', 'usa', 'Ġus', 'Ġfirst', 'Ġtwo', 'Ġbuilt', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'Ġcapabilities', 'Ġdevelopment', 'Ġconstruction', 'Ġbudgets', 'Ġclassified', 'Ġoperate', 'near', 'ge', 'os', 'ynchronous', 'Ġorbit', '",', 'Ġfirst', 'Ġlaunch', 'Ġscheduled', 'Ġj', 'uly', 'Ġaboard', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġdelta', 'Ġiv', 'Ġlaunch', 'Ġvehicle', 'Ġpath', 'finder', 'Ġsatellite', 'Ġge', 'os', 'ynchronous', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġprogram', '01', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġwik', 'ipedia', 'Ġeven', 'Ġtesting', 'Ġprocess', 'Ġsatellites', 'Ġpressed', 'Ġearly', 'Ġservice', 'Ġfulfill', 'Ġcritical', 'Ġneeds', 'Ġse', 'pt', 'ember', 'Ġthird', 'Ġfourth', 'Ġsatellites', 'Ġdeclared', 'Ġoperational', 'Ġtwo', 'Ġsatellites', 'g', 'ss', 'ap', 'Ġg', 'ss', 'ap', 'Ġsuccessfully', 'Ġlaunched', 'Ġjan', 'uary', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġus', 'Ġapproached', 'Ġtwo', 'Ġch', 'inese', 'Ġsatellites', 'Ġgeo', 'Ġexamine', 'Ġclosely', 'Ġch', 'inese', 'Ġresearchers', 'Ġreported', 'Ġobserved', 'Ġinstances', 'Ġus', 'Ġsatellites', 'Ġapproached', 'Ġch', 'inese', 'Ġones', 'Ġaug', 'ust', 'Ġspace', 'Ġsystems', 'Ġcommand', 'Ġannounced', 'Ġretirement', 'Ġg', 'ss', 'ap', 'Ġsatellite', 'Ġfirst', 'Ġconstellation', 'Ġdecom', 'mission', 'ed', 'Ġsubsequent', 'Ġtransfer', 'Ġgraveyard', 'Ġorbit', 'Ġmoreover', 'Ġrevealed', 'Ġtwo', 'Ġsatellites', 'Ġordered', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġkeep', 'Ġdemand', 'Ġg', 'ss', 'ap', 'Ġassets', 'Ġlaunches', 'Ġnew', 'Ġsatellites', 'Ġplanned', 'Ġrespectively', 'Ġspacecraft', 'Ġfirst', 'Ġconstellation', 'Ġlaunched', 'Ġpairs', 'Ġair', 'Ġforce', 'Ġspace', 'Ġsurveillance', 'Ġsystem', 'ite', 'x', 'bo', 'e', 'ing', 'Ġball', 'Ġaerospace', 'Ġachieve', 'Ġnew', 'Ġmilestone', 'b', 'ss', 'Ġprogram', 'Ġl', 'Ġbo', 'e', 'ing', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'bo', 'e', 'ing', 'Ġcompletes', 'Ġhardware', 'Ġinstallation', 'b', 'ss', 'Ġsatellite', 'Ġoperations', 'Ġcenter', 'web', 'arch', 'Ġbo', 'e', 'ing', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'min', 'otaur', 'Ġiv', 'Ġv', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'v', 'enberg', 'Ġlaunches', 'Ġmin', 'otaur', 'Ġiv', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext']</t>
+          <t>['Ġstar', 'Ġ("', 'se', 'gment', 'Ġimage', 'Ġidentification', '").', 'Ġsegment', 'Ġindividually', 'Ġcorrected', 'Ġmajor', 'Ġfocusing', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġerrors', 'Ġusing', 'Ġtechnique', 'Ġcalled', 'Ġphase', 'Ġretrieval', 'Ġresulting', 'Ġseparate', 'Ġgood', 'Ġquality', 'Ġimages', 'Ġmirror', 'Ġsegments', 'Ġ("', 'se', 'gment', 'Ġalignment', '").', 'Ġimages', 'Ġsegment', 'Ġmoved', 'Ġprecisely', 'Ġoverlap', 'Ġcreate', 'Ġsingle', 'Ġimage', 'Ġ("', 'image', 'Ġstacking', '").', 'Ġmirrors', 'Ġpositioned', 'Ġalmost', 'Ġcorrect', 'Ġimages', 'Ġfine', 'Ġtuned', 'Ġoperational', 'Ġaccuracy', 'Ġnan', 'ometers', 'Ġless', 'Ġone', 'Ġwavelength', 'Ġlight', 'Ġdetected', 'Ġtechnique', 'Ġcalled', 'Ġdispersed', 'Ġfringe', 'Ġsensing', 'Ġused', 'Ġcompare', 'Ġimages', 'Ġpair', 'ings', 'Ġmirrors', 'Ġallowing', 'Ġerrors', 'Ġcorrected', 'Ġ("', 'co', 'arse', 'Ġph', 'asing', '"),', 'Ġintroduced', 'Ġlight', 'Ġdef', 'ocus', 'Ġsegment', "'s", 'Ġimage', 'Ġallowing', 'Ġdetection', 'Ġcorrection', 'Ġalmost', 'Ġremaining', 'Ġerrors', 'Ġ("', 'fine', 'Ġph', 'asing', '").', 'Ġtwo', 'Ġprocesses', 'Ġrepeated', 'Ġthree', 'Ġtimes', 'Ġfine', 'Ġph', 'asing', 'Ġroutinely', 'Ġchecked', 'Ġthroughout', 'Ġtelescope', "'s", 'Ġoperation', 'Ġthree', 'Ġrounds', 'Ġcoarse', 'Ġfine', 'Ġph', 'asing', 'Ġtelescope', 'Ġwell', 'Ġaligned', 'Ġone', 'Ġplace', 'Ġn', 'irc', 'Ġfield', 'Ġview', 'Ġmeasurements', 'Ġmade', 'Ġvarious', 'Ġpoints', 'Ġcaptured', 'Ġimage', 'Ġacross', 'Ġinstruments', 'Ġcorrections', 'Ġcalculated', 'Ġdetected', 'Ġvariations', 'Ġintensity', 'Ġgiving', 'Ġwell', 'aligned', 'Ġoutcome', 'Ġacross', 'Ġinstruments', 'Ġ("', 'tel', 'esc', 'ope', 'Ġalignment', 'Ġinstrument', 'Ġfields', 'Ġview', '").', 'Ġfinally', 'Ġlast', 'Ġround', 'Ġfine', 'Ġph', 'asing', 'Ġchecks', 'Ġimage', 'Ġquality', 'Ġinstruments', 'Ġperformed', 'Ġensure', 'Ġsmall', 'Ġresidual', 'Ġerrors', 'Ġremaining', 'Ġprevious', 'Ġsteps', 'Ġcorrected', 'Ġ("', 'iter', 'ate', 'Ġalignment', 'Ġfinal', 'Ġcorrection', '").', 'Ġtelescope', "'s", 'Ġmirror', 'Ġsegments', 'Ġaligned', 'Ġable', 'Ġcapture', 'Ġprecise', 'Ġfocused', 'Ġimages', 'Ġpreparation', 'Ġalignment', 'Ġn', 'asa', 'Ġannounced', 'Ġut', 'c', 'Ġfe', 'b', 'ruary', 'Ġn', 'irc', 'Ġdetected', 'Ġtelescope', "'s", 'Ġfirst', 'Ġphotons', 'although', 'Ġyet', 'Ġcomplete', 'Ġimages', ').[', 'Ġfe', 'b', 'ruary', 'Ġn', 'asa', 'Ġannounced', 'Ġtelescope', 'Ġalmost', 'Ġcompleted', 'Ġphase', 'Ġalignment', 'Ġevery', 'Ġsegment', 'Ġprimary', 'Ġmirror', 'Ġlocated', 'Ġim', 'aged', 'Ġtarget', 'Ġstar', 'Ġsegments', 'Ġbrought', 'Ġapproximate', 'Ġalignment', 'Ġphase', 'Ġalignment', 'Ġcompleted', 'Ġfe', 'b', 'ruary', 'Ġweek', 'Ġlater', 'Ġphases', 'Ġalso', 'Ġcompleted']</t>
         </is>
       </c>
       <c r="C296" t="n">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>['Ġsource', 'Ġpublic', 'Ġdomain', 'bo', 'e', 'ing', 'b', 'ss', 'Ġsystem', 'Ġprogressing', 'Ġtoward', 'st', 'Ġlaunch', 'Ġbo', 'e', 'ing', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'laun', 'cher', 'Ġissues', 'Ġblamed', 'month', 'b', 'ss', 'Ġslip', 'Ġspace', 'Ġnews', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġbo', 'e', 'ing', 'Ġteam', 'Ġships', 'Ġfirst', 'b', 'ss', 'Ġspacecraft', 'Ġlaunch', 'Ġsite', 'launch', 'Ġdelayed', 'Ġsatellite', 'Ġwatch', 'Ġspace', 'Ġdebris', 'ahoo', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġic', 'cam', 'delay', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'Ġsee', 'Ġalso', 'Ġreferences', '01', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġwik', 'ipedia', 'space', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġe', 'sb', 'ss', 'Ġball', 'Ġaerospace', 'Ġretrieved', 'mber', 'Ġneighborhood', 'Ġwatch', 'Ġspace', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġaug', 'ust', 'ler', 'Ġamy', 'Ġfe', 'b', 'ruary', 'us', 'af', 'Ġreveals', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġnew', 'Ġsatellite', 'web', 'arch', 'iv', 'Ġaviation', 'Ġweek', 'Ġsap', 'ce', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhar', 'per', 'Ġj', 'Ġj', 'uly', 'air', 'Ġforce', 'Ġlaunching', 'Ġsatellites', 'Ġsatellites', 'http', 'str', 'Ġstripes', 'Ġstars', 'Ġstripes', 'Ġretrieved', 'Ġj', 'uly', 'Ġgr', 'uss', 'ike', 'Ġse', 'pt', 'ember', 'space', 'Ġsurveillance', 'ats', 'Ġpressed', 'Ġearly', 'Ġservice', 'http', 'sp', 'Ġspac', 'en', 'ews', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġes', 'pin', 'osa', 'Ġshell', 'ie', 'anne', 'Ġse', 'pt', 'ember', 'two', 'Ġnew', 'Ġsatellites', 'Ġoperational', 'Ġexpand', 'Ġu', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġaf', 'sp', 'c', 'af', 'mil', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġpublic', 'Ġaffairs', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgra', 'ham', 'iam', 'Ġjan', 'uary', 'ula', "'s", 'las', 'Ġlaunches', 'Ġmission', 'Ġspace', 'Ġforce', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġw', 'er', 'ner', 'Ġdeb', 'ra']</t>
+          <t>['Ġmeant', 'Ġsegments', 'Ġworking', 'Ġunison', 'Ġhowever', 'Ġphases', 'Ġcomplete', 'Ġsegments', 'Ġstill', 'Ġacting', 'Ġsmaller', 'Ġtelescopes', 'Ġrather', 'Ġone', 'Ġlarger', 'Ġone', 'Ġtime', 'Ġprimary', 'Ġmirror', 'Ġcommissioned', 'Ġhundreds', 'Ġinstrument', 'Ġcommission', 'ing', 'Ġcalibration', 'Ġtasks', 'Ġalso', 'Ġongoing', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġphase', 'Ġinterim', 'Ġimage', 'Ġannot', 'ated', 'Ġrelated', 'Ġmirror', 'Ġsegments', 'Ġtook', 'Ġimage', 'Ġphase', 'Ġannot', 'ated', 'Ġcompletion', 'Ġimage', 'Ġphase', 'Ġcompletion', 'Ġshowing', 'Ġeffects', 'Ġsegment', 'Ġalignment', 'Ġphase', 'Ġcompletion', 'Ġshowing', 'Ġsegments', 'st', 'acked', 'Ġsingle', 'Ġimage', 'Ġstar', 'mass', 'Ġcaptured', 'Ġn', 'irc', 'Ġinstrument', 'sel', 'ï', '¬', 'ģ', 'e', 'Ġtaken', 'Ġn', 'irc', 'Ġalignment', 'Ġprocess', 'Ġimage', 'Ġcomparison', 'old', 'Ġsp', 'itzer', 'Ġnew', 'Ġalignment', 'Ġn', 'asa', 'esa', 'cs', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'Ġsensors', 'Ġweb', 'b', 'âĢ', 'Ļ', 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġweb', 'b', 'Ġobserving', 'Ġtime', 'Ġallocated', 'Ġgeneral', 'Ġobservers', 'go', 'Ġprogram', 'Ġguaranteed', 'Ġtime', 'Ġobservations', 'g', 'Ġprogram', 'Ġdirector', "'s", 'Ġdiscretionary', 'Ġearly', 'Ġrelease', 'Ġscience', 'dd', 'ers', 'Ġprogram', 'Ġg', 'Ġprogram', 'Ġprovides', 'Ġguaranteed', 'Ġobserving', 'Ġtime', 'Ġscientists', 'Ġdeveloped', 'Ġhardware', 'Ġsoftware', 'Ġcomponents', 'Ġobserv', 'atory', 'Ġgo', 'Ġprogram', 'Ġprovides', 'Ġastronomers', 'Ġallocation', 'Ġobservation', 'Ġtime', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġopportunity', 'Ġapply', 'Ġobserving', 'Ġtime', 'Ġrepresent', 'Ġbulk', 'Ġobserving', 'Ġtime', 'Ġgo', 'Ġprograms', 'Ġselected', 'Ġpeer', 'Ġreview', 'Ġtime', 'Ġallocation', 'Ġcommittee', 'ac', 'Ġsimilar', 'Ġproposal', 'Ġreview', 'Ġprocess', 'Ġused', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'mber', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġannounced', 'Ġselection', 'Ġdirector', "'s", 'Ġdiscretionary', 'Ġearly', 'Ġrelease', 'Ġscience', 'dd', 'ers', 'Ġprograms', 'Ġchosen', 'Ġcompetitive', 'Ġproposal', 'Ġprocess', 'Ġobservations', 'Ġprograms', 'Ġearly', 'Ġrelease', 'Ġobservations', 'ero', ')[', 'Ġobtained', 'Ġfirst', 'Ġfive', 'Ġmonths', 'Ġweb', 'b', 'Ġscience', 'Ġoperations', 'Ġend', 'Ġcommission', 'ing', 'Ġperiod', 'Ġtotal', 'Ġhours', 'Ġobserving', 'Ġtime', 'Ġawarded', 'Ġprograms', 'Ġspan', 'Ġscience', 'Ġtopics', 'Ġincluding', 'Ġsolar', 'Ġsystem', 'Ġex', 'oplan', 'ets', 'Ġstars', 'Ġstar', 'Ġformation', 'Ġnearby', 'Ġdistant', 'Ġgalaxies', 'Ġgravitational', 'Ġlenses']</t>
         </is>
       </c>
       <c r="C297" t="n">
@@ -4299,7 +4299,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>['Ġj', 'une', 'orbit', 'Ġgame', 'Ġcat', 'Ġmouse', 'Ġclose', 'Ġapproaches', 'Ġprompt', 'Ġcalls', 'Ġcommunications', 'Ġnorms', 'Ġspac', 'en', 'ews', 'Ġtam', 'im', 'Ġbab', 'Ġmay', 'us', 'Ġconducted', 'Ġmissions', 'Ġch', 'ina', "'s", 'Ġsatellites', 'Ġyears', 'Ġclaims', 'Ġch', 'inese', 'Ġstudy', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġaug', 'ust', 'u', 'Ġde', 'activ', 'ates', 'Ġg', 'ss', 'ap', 'Ġsurveillance', 'Ġsatellite', 'Ġtwo', 'Ġnew', 'Ġones', 'Ġworks', 'Ġretrieved', 'Ġaug', 'ust', 'ley', 'Ġg', 'reg', 'Ġaug', 'ust', 'space', 'Ġforce', 'Ġde', 'activ', 'ates', 'Ġone', 'Ġspace', 'Ġsurveillance', 'Ġsatellite', 'Ġsets', 'Ġplans', 'Ġtwo', 'Ġair', 'Ġspace', 'Ġforces', 'Ġmagazine', 'Ġretrieved', 'Ġaug', 'ust', 'Ġretrieved']</t>
+          <t>['Ġqu', 'ars', 'Ġ', 'ers', 'Ġprograms', 'Ġuse', 'Ġtotal', 'Ġhours', 'Ġobserving', 'Ġtime', 'Ġtelescope', 'Ġincluding', 'Ġweb', 'b', 'Ġobserving', 'heads', 'Ġslew', 'Ġtime', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprograms', 'Ġname', 'Ġprincipal', 'Ġinvestigator', 'Ġcategory', 'Ġobservation', 'Ġtime', 'hours', 'Ġradi', 'ative', 'Ġfeedback', 'Ġmassive', 'Ġstars', 'Ġtraced', 'Ġmult', 'iband', 'Ġimaging', 'Ġspect', 'rosc', 'opic', 'Ġmosa', 'ics', 'liv', 'ier', 'Ġb', 'ern', 'Ã©', 'Ġstellar', 'Ġphysics', 'Ġice', 'age', 'Ġchemical', 'Ġevolution', 'Ġ', 'ices', 'Ġstar', 'Ġformation', 'Ġmel', 'issa', 'cc', 'l', 'ure', 'Ġstellar', 'Ġphysics', 'Ġlooking', 'Ġglass', 'Ġj', 'w', 'st', 'Ġexploration', 'Ġgalaxy', 'Ġformation', 'Ġevolution', 'Ġcosmic', 'Ġdawn', 'Ġpresent', 'Ġday', 'mm', 'Ġtre', 'u', 'Ġgalaxies', 'Ġj', 'w', 'st', 'Ġstudy', 'Ġstar', 'burst', 'agn', 'Ġconnection', 'Ġmerging', 'Ġl', 'ir', 'gs', 'Ġle', 'e', 'Ġarm', 'us', 'Ġgalaxies', 'Ġresolved', 'Ġstellar', 'Ġpopulations', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'aniel', 'Ġstellar', 'Ġpopulations', 'Ġimaging', 'Ġspect', 'rosc', 'opy', 'Ġqu', 'asar', 'Ġhosts', 'Ġj', 'w', 'st', 'Ġanalyzed', 'Ġpowerful', 'Ġnew', 'Ġps', 'f', 'Ġdecom', 'position', 'Ġspectral', 'Ġanalysis', 'Ġpackage', 'Ġdomin', 'ika', 'Ġw', 'yle', 'z', 'al', 'ek', 'Ġmassive', 'Ġblack', 'Ġholes', 'Ġgalaxies', 'Ġcosmic', 'Ġevolution', 'Ġearly', 'Ġrelease', 'Ġscience', 'ce', 'ers', 'Ġsurvey', 'Ġste', 'ven', 'Ġfin', 'kel', 'stein', 'Ġgalaxies', 'Ġestablishing', 'Ġextreme', 'Ġdynamic', 'Ġrange', 'Ġj', 'w', 'st', 'Ġdecoding', 'Ġsmoke', 'Ġsignals', 'Ġglare', 'Ġwolf', 'ray', 'et', 'Ġbinary', 'Ġr', 'yan', 'Ġl', 'au', 'Ġstellar', 'Ġphysics', 'Ġtemplates', 'Ġtargeting', 'Ġextremely', 'Ġmagn', 'ï', '¬', 'ģ', 'ed', 'Ġpan', 'chrom', 'atic', 'Ġlens', 'ed', 'Ġarcs', 'Ġextended', 'Ġstar', 'Ġformation', 'Ġj', 'ane', 'Ġrig', 'Ġgalaxies', 'Ġnuclear', 'Ġdynamics', 'Ġnearby', 'Ġse', 'f', 'ert', 'Ġn', 'ir', 'spec', 'Ġintegral', 'Ġfield', 'Ġspect', 'rosc', 'opy', 'Ġmist', 'Ġbent', 'z', 'Ġmassive', 'Ġblack', 'Ġholes', 'Ġgalaxies', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'et', 'Ġcommunity', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġn', 'atalie', 'Ġbat', 'al', 'ha', 'Ġplanets', 'Ġplanet', 'Ġformation', 'Ġ', 'ers', 'Ġobservations', 'Ġj', 'ov', 'ian', 'Ġsystem', 'Ġdemonstration', 'Ġj', 'w', 'st', "'s", 'Ġcapabilities', 'Ġsolar', 'Ġsystem', 'Ġscience', 'Ġde', 'Ġp', 'ater', 'Ġsolar', 'Ġsystem', 'Ġhigh', 'Ġcontrast', 'Ġimaging', 'Ġex', 'oplan', 'ets', 'Ġex', 'oplan']</t>
         </is>
       </c>
       <c r="C298" t="n">
@@ -4312,7 +4312,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>['Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġrendering', 'Ġfully', 'Ġdeployed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġnames', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'ng', 'st', 'âĢĵ', 'Ġmission', 'Ġtype', 'Ġastronomy', 'Ġoperator', 'Ġst', 'sci', 'n', 'asa', ')[', 'Ġes', 'Ġc', 'sa', 'Ġcos', 'par', 'Ġid', 'Ġsat', 'cat', 'Ġwebsite', 'ï', '¬', 'ģ', 'cial', 'Ġwebsite', 'Ġweb', 'bt', 'el', 'esc', 'ope', 'org', 'Ġmission', 'Ġduration', 'Ġyear', 'Ġmonths', 'Ġdays', 'el', 'apsed', 'âģ', 'Ħ', 'Ġyears', 'primary', 'Ġmission', ')[', 'Ġyears', 'planned', 'Ġyears', 'expected', 'Ġspacecraft', 'Ġproperties', 'Ġmanufacturer', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġlaunch', 'Ġmass', 'Ġdimensions', 'Ġft', 'Ġsun', 'shield', 'Ġpower', 'Ġstart', 'Ġmission', 'Ġlaunch', 'Ġdate', 'Ġde', 'cember', 'Ġrocket', 'ri', 'ane', 'Ġe', 'ca', 'Ġlaunch', 'Ġsite', 'Ġcentre', 'Ġspatial', 'Ġguy', 'ana', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġcontractor', 'rian', 'esp', 'ace', 'Ġentered', 'Ġservice', 'Ġj', 'uly', 'Ġorbital', 'Ġparameters', 'Ġreference', 'Ġsystem', 'Ġsun', 'âĢĵ', 'earth', 'Ġorbit', 'Ġregime', 'Ġh', 'alo', 'Ġorbit', 'Ġper', 'aps', 'Ġaltitude', '000', '000', 'Ġap', 'aps', 'Ġaltitude', '000', '000', 'Ġperiod', 'Ġmonths', 'Ġmain', 'Ġtelescope', 'Ġtype', 'Ġk', 'ors', 'ch', 'Ġtelescope', 'Ġdiameter', 'Ġft', 'Ġfocal', 'Ġlength', 'Ġft', 'Ġfocal', 'Ġratio', 'Ġcollecting', 'Ġarea', 'Ġwavelengths', 'âĢĵ', 'ĠÎ¼', 'orange', 'Ġmid', 'inf', 'rared', 'Ġtrans', 'p', 'ond', 'ers', 'Ġband', 'band', 'Ġtele', 'metry', 'Ġtele', 'command', 'Ġka', 'band', 'Ġscience', 'Ġdata', 'link', 'Ġbandwidth', 'band', 'Ġk', 'bit', 'band', 'Ġk', 'bit', 'Ġka', 'band', 'bit', 'Ġinstruments', 'Ġf', 'gs', 'nir', 'iss', 'Ġmir', 'Ġn', 'irc', 'Ġn', 'ir', 'spec', 'Ġelements', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'Ġspacecraft', 'bus', 'Ġsun', 'shield', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmission', 'Ġlogo', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', 'Ġspace', 'Ġtelescope', 'Ġspecifically', 'Ġdesigned', 'Ġconduct', 'Ġinfrared', 'Ġastronomy', 'Ġhigh', 'resolution', 'Ġhigh', 'ensitivity', 'Ġinstruments', 'Ġallow', 'Ġview', 'Ġobjects', 'Ġold']</t>
+          <t>['etary', 'Ġsystems', 'Ġj', 'w', 'st', 'asha', 'Ġh', 'ink', 'ley', 'Ġplanets', 'Ġplanet', 'Ġformation', 'Ġgo', 'Ġcycle', '000', 'Ġhours', 'Ġobservation', 'Ġtime', 'Ġavailable', 'Ġallocate', 'Ġproposals', 'Ġsubmitted', 'Ġrequesting', 'Ġtotal', 'Ġhours', 'Ġobservation', 'Ġtime', 'Ġselection', 'Ġcycle', 'Ġgo', 'Ġprograms', 'Ġannounced', 'Ġmarch', 'Ġprograms', 'Ġapproved', 'Ġincluded', 'Ġlarge', 'Ġprograms', 'Ġtreasury', 'Ġprograms', 'Ġproducing', 'Ġdata', 'Ġpublic', 'Ġaccess', 'Ġcycle', 'Ġgo', 'Ġprogram', 'Ġannounced', 'Ġmay', 'Ġweb', 'b', 'Ġscience', 'Ġobservations', 'Ġnom', 'inally', 'Ġscheduled', 'Ġweekly', 'Ġincrements', 'Ġobservation', 'Ġplan', 'Ġevery', 'Ġweek', 'Ġpublished', 'ond', 'ays', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġfinished', 'Ġcommission', 'ing', 'Ġactivities', 'Ġready', 'Ġbegin', 'Ġfull', 'Ġscientific', 'Ġoperations', 'Ġj', 'uly', 'Ġexceptions', 'Ġexperiment', 'Ġdata', 'Ġkept', 'Ġprivate', 'Ġone', 'Ġyear', 'Ġexclusive', 'Ġuse', 'Ġscientists', 'Ġrunning', 'Ġparticular', 'Ġexperiment', 'Ġgeneral', 'Ġobserver', 'Ġprogram', 'Ġscientific', 'Ġresults', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġhub', 'ble', 'Ġcompared', 'Ġweb', 'b', ')[', 'Ġdeep', 'Ġfield', 'Ġgalaxy', 'Ġcluster', 'Ġsm', 'acs', 'Ġone', 'Ġyear', 'Ġraw', 'Ġdata', 'Ġreleased', 'Ġpublic', 'Ġfirst', 'Ġfull', 'color', 'Ġimages', 'Ġspect', 'rosc', 'opic', 'Ġdata', 'Ġreleased', 'Ġj', 'uly', 'Ġalso', 'Ġmarked', 'Ġofficial', 'Ġbeginning', 'Ġweb', 'b', "'s", 'Ġgeneral', 'Ġscience', 'Ġoperations', 'Ġunited', 'Ġstates', 'Ġpresident', 'Ġjo', 'e', 'Ġbid', 'en', 'Ġrevealed', 'Ġfirst', 'Ġimage', 'Ġweb', 'b', "'s", 'Ġfirst', 'Ġdeep', 'Ġfield', 'Ġj', 'uly', 'Ġadditional', 'Ġreleases', 'Ġaround', 'Ġtime', 'Ġcar', 'ina', 'Ġneb', 'ula', 'Ġyoung', 'Ġstar', 'forming', 'Ġregion', 'Ġcalled', 'Ġng', 'c', 'Ġdisplaying', 'cos', 'mic', 'Ġcliffs', 'Ġlight', 'years', 'Ġearth', 'p', 'b', 'Ġincluding', 'Ġanalysis', 'Ġatmosphere', 'Ġevidence', 'Ġwater', 'Ġaround', 'Ġgiant', 'Ġgas', 'Ġplanet', 'Ġorbiting', 'Ġdistant', 'Ġstar', 'Ġlight', 'years', 'Ġearth', 'Ġsouthern', 'Ġring', 'Ġneb', 'ula', 'Ġclouds', 'Ġgas', 'Ġdust', 'Ġexpelled', 'Ġdying', 'Ġstar', 'Ġlight', 'years', 'Ġearth', 'Ġstep', 'han', "'s", 'Ġquint', 'et', 'Ġvisual', 'Ġdisplay', 'Ġï', '¬', 'ģ', 'Ġgalaxies', 'Ġcoll', 'iding', 'Ġgas', 'Ġdust', 'Ġclouds', 'Ġcreating', 'Ġnew', 'Ġstars', 'Ġfour', 'Ġcentral', 'Ġgalaxies', 'Ġmillion', 'Ġlight', 'years', 'Ġearth', 'Ġsm', 'acs', 'Ġj', '07', 'Ġgalaxy', 'Ġcluster', 'Ġred']</t>
         </is>
       </c>
       <c r="C299" t="n">
@@ -4325,7 +4325,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>['Ġdistant', 'Ġfaint', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġenables', 'Ġinvestigations', 'Ġacross', 'Ġmany', 'Ġfields', 'Ġastronomy', 'Ġcos', 'mology', 'Ġobservation', 'Ġfirst', 'Ġstars', 'Ġformation', 'Ġfirst', 'Ġgalaxies', 'Ġdetailed', 'Ġatmospheric', 'Ġcharacterization', 'Ġpotentially', 'Ġhabitable', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġu', 'Ġnational', 'Ġaer', 'aut', 'ics', 'Ġspace', 'Ġadministration', 'n', 'asa', 'Ġled', 'Ġweb', 'b', "'s", 'Ġdesign', 'Ġdevelopment', 'Ġpartnered', 'Ġtwo', 'Ġmain', 'Ġagencies', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'esa', 'adian', 'Ġspace', 'Ġagency', 'cs', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'gs', 'fc', 'ary', 'land', 'Ġmanaged', 'Ġtelescope', 'Ġdevelopment', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġb', 'alt', 'imore', 'Ġhom', 'ew', 'ood', 'Ġcampus', 'Ġjohn', 'Ġhop', 'kins', 'Ġuniversity', 'Ġcurrently', 'Ġoperates', 'Ġweb', 'b', 'Ġprimary', 'Ġcontractor', 'Ġproject', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġtelescope', 'Ġnamed', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', 'Ġadministrator', 'Ġn', 'asa', 'Ġmercury', 'Ġgem', 'ini', 'Ġap', 'ollo', 'Ġprograms', 'Ġweb', 'b', 'Ġlaunched', 'Ġde', 'cember', 'ri', 'ane', 'Ġrocket', 'Ġk', 'ou', 'Ġfrench', 'Ġgu', 'iana', 'Ġarrived', 'Ġsun', 'âĢĵ', 'earth', 'Ġlag', 'range', 'Ġpoint', 'Ġjan', 'uary', 'Ġfirst', 'Ġweb', 'b', 'Ġimage', 'Ġreleased', 'Ġpublic', 'Ġvia', 'Ġpress', 'Ġconference', 'Ġj', 'uly', 'Ġweb', 'b', "'s", 'Ġprimary', 'Ġmirror', 'Ġconsists', 'Ġhex', 'agonal', 'Ġmirror', 'Ġsegments', 'Ġmade', 'Ġgold', 'pl', 'ated', 'Ġb', 'ery', 'ium', 'Ġcombined', 'Ġcreate', 'meter', 'iameter', 'Ġft', 'Ġmirror', 'Ġcompared', 'Ġhub', 'ble', "'s", 'Ġft', 'Ġgives', 'Ġweb', 'b', 'Ġlight', 'collect', 'ing', 'Ġarea', 'Ġsquare', 'Ġmeters', 'Ġtimes', 'Ġhub', 'ble', 'Ġunlike', 'Ġhub', 'ble', 'Ġobserves', 'Ġnear', 'Ġultraviolet', 'Ġvisible', 'ĠÂµ', 'Ġnear', 'Ġinfrared', 'âĢĵ', 'Ġspect', 'ra', 'Ġweb', 'b', 'Ġobserves', 'Ġlower', 'Ġfrequency', 'Ġrange', 'Ġlong', 'wa', 'velength', 'Ġvisible', 'Ġlight', 'red', 'Ġmid', 'inf', 'rared', 'âĢĵ', 'ĠÂµ', 'Ġtelescope', 'Ġmust', 'Ġkept', 'Ġextremely', 'Ġcold', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', 'Ġinfrared', 'Ġlight', 'Ġemitted', 'Ġtelescope']</t>
+          <t>['shift', 'Ġdistant', 'Ġbackground', 'Ġgalaxies', 'Ġwhose', 'Ġimages', 'Ġdistorted', 'Ġmagn', 'ï', '¬', 'ģ', 'ed', 'Ġdue', 'Ġgravitational', 'Ġlens', 'ing', 'Ġcluster', 'Ġimage', 'Ġcalled', 'Ġweb', 'b', "'s", 'Ġfirst', 'Ġdeep', 'Ġfield', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġpresented', 'Ġimages', 'Ġj', 'upiter', 'Ġrelated', 'Ġareas', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġincluding', 'Ġinfrared', 'Ġviews', 'Ġpre', 'print', 'Ġreleased', 'Ġaround', 'Ġtime', 'Ġn', 'asa', 'Ġes', 'Ġc', 'sa', 'Ġscientists', 'Ġstated', 'almost', 'Ġacross', 'Ġboard', 'Ġscience', 'Ġperformance', 'Ġj', 'w', 'st', 'Ġbetter', 'Ġexpected', '".', 'Ġdocument', 'Ġdescribed', 'Ġseries', 'Ġobservations', 'Ġcommission', 'ing', 'Ġinstruments', 'Ġcaptured', 'Ġspect', 'ra', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'ets', 'Ġprecision', 'Ġbetter', 'Ġper', 'Ġdata', 'Ġpoint', 'Ġtracked', 'Ġmoving', 'Ġobjects', 'Ġspeeds', 'Ġtwice', 'Ġfast', 'Ġrequirement', 'Ġalso', 'Ġobtained', 'Ġspect', 'ra', 'Ġhundreds', 'Ġstars', 'Ġsimultaneously', 'Ġdense', 'Ġfield', 'Ġtowards', 'Ġmil', 'ky', 'Ġway', 'Ġgalactic', 'Ġcenter', 'Ġtargets', 'Ġincluded', ':[', 'Ġmoving', 'Ġtargets', 'Ġj', 'upiter', 'including', 'Ġrings', 'Ġmoons', 'Ġeuro', 'pa', 'Ġmet', 'Ġasteroids', 'Ġr', 'oman', 'Ġpe', 'ith', 'Ġten', 'zing', 'Ġr', 'ump', 'el', 'st', 'il', 'z', 'Ġk', 'le', 'op', 'atra', 'Ġst', 'ear', 'ns', 'Ġwil', 'son', 'har', 'rington', 'Ġn', 'irc', 'Ġgr', 'ism', 'Ġtime', 'series', 'Ġn', 'ir', 'iss', 'oss', 'Ġn', 'ir', 'spec', 'Ġbots', 'Ġmode', 'Ġj', 'upiter', 'sized', 'Ġplanet', 'Ġn', 'ir', 'iss', 'Ġaperture', 'Ġmask', 'ing', 'Ġinter', 'fer', 'ometry', 'ami', '):', 'Ġclear', 'Ġdetection', 'Ġlow', 'mass', 'Ġcompanion', 'Ġstar', 'Ġab', 'ad', 'us', 'Ġc', 'Ġseparation', 'Ġarc', 'seconds', 'Ġprimary', 'Ġfirst', 'Ġfull', 'color', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġobservation', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdemonstration', 'Ġspace', 'Ġmir', 'Ġlow', 'resolution', 'Ġspect', 'rosc', 'opy', 'l', 'rs', '):', 'Ġhot', 'Ġsuper', 'earth', 'Ġplanet', 'Ġaround', 'Ġbright', 'war', 'f', 'Ġstar', 'red', 'ar', 'w', 'f', 'Ġstar', ')[', 'Ġwithin', 'Ġtwo', 'Ġweeks', 'Ġfirst', 'Ġweb', 'b', 'Ġimages', 'Ġseveral', 'Ġpre', 'print', 'Ġpapers', 'Ġdescribed', 'Ġwide', 'Ġrange', 'Ġhigh', 'Ġred', 'shift', 'Ġlumin', 'ous', 'pres', 'umably', 'Ġlarge', 'Ġgalaxies', 'Ġbelieved', 'Ġdate', 'Ġmillion', 'Ġyears', 'z']</t>
         </is>
       </c>
       <c r="C300" t="n">
@@ -4338,7 +4338,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>['Ġinterfere', 'Ġcollected', 'Ġlight', 'Ġdeployed', 'Ġsolar', 'Ġorbit', 'Ġnear', 'Ġsun', 'âĢĵ', 'earth', 'Ġlag', 'range', 'Ġpoint', 'Ġmillion', 'Ġkilometers', '000', 'Ġmi', 'Ġearth', 'Ġfive', 'layer', 'Ġsun', 'shield', 'Ġprotects', 'Ġwarming', 'Ġsun', 'Ġearth', 'Ġmoon', 'Ġinitial', 'Ġdesigns', 'Ġtelescope', 'Ġnamed', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġbegan', 'Ġtwo', 'Ġconcept', 'Ġstudies', 'Ġcommissioned', 'Ġpotential', 'Ġlaunch', 'Ġbillion', 'Ġbudget', 'Ġprogram', 'Ġplagued', 'Ġenormous', 'Ġcost', 'Ġoverrun', 'Ġdelays', 'Ġmajor', 'Ġredesign', 'Ġled', 'Ġcurrent', 'Ġapproach', 'Ġconstruction', 'Ġcompleted', 'Ġtotal', 'Ġcost', 'Ġus', 'Ġbillion', 'Ġhigh', 'stakes', 'Ġnature', 'Ġlaunch', 'Ġtelescope', "'s", 'Ġcomplexity', 'Ġremarked', 'Ġupon', 'Ġmedia', 'Ġscientists', 'Ġengineers', 'Ġj', 'uly', 'Ġastronomers', 'Ġreported', 'Ġfirst', 'Ġyear', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġoperations', 'Ġconsiderable', 'Ġsuccess', 'Ġmass', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġhalf', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġweb', 'b', 'Ġft', ')-', 'iameter', 'Ġgold', 'co', 'ated', 'Ġb', 'ery', 'ium', 'Ġprimary', 'Ġmirror', 'Ġmade', 'Ġseparate', 'Ġhex', 'agonal', 'Ġmirrors', 'Ġmirror', 'Ġpolished', 'Ġarea', 'Ġft', 'Ġft', 'Ġobscured', 'Ġsecondary', 'Ġsupport', 'Ġstr', 'uts', 'Ġgiving', 'Ġtotal', 'Ġcollecting', 'Ġarea', 'Ġft', 'Ġtimes', 'Ġlarger', 'Ġcollecting', 'Ġarea', 'Ġhub', 'ble', "'s", 'Ġft', 'Ġdiameter', 'Ġmirror', 'Ġcollecting', 'Ġarea', 'Ġft', 'Ġmirror', 'Ġgold', 'Ġcoating', 'Ġprovide', 'Ġinfrared', 'Ġreflect', 'ivity', 'Ġcovered', 'Ġthin', 'Ġlayer', 'Ġglass', 'Ġdurability', 'Ġweb', 'b', 'Ġdesigned', 'Ġprimarily', 'Ġnear', 'inf', 'rared', 'Ġastronomy', 'Ġalso', 'Ġsee', 'Ġorange', 'Ġred', 'Ġvisible', 'Ġlight', 'Ġwell', 'Ġmid', 'inf', 'rared', 'Ġregion', 'Ġdepending', 'Ġinstrument', 'Ġused', 'Ġdetect', 'Ġobjects', 'Ġtimes', 'Ġf', 'ter', 'Ġhub', 'ble', 'Ġobjects', 'Ġmuch', 'Ġearlier', 'Ġhistory', 'Ġuniverse', 'Ġback', 'Ġred', 'shift', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime', 'Ġbig', 'Ġbang', ').[', 'Ġcomparison', 'Ġearliest', 'Ġstars', 'Ġthought', 'Ġformed', 'âĢĵ', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime']</t>
+          <t>['Ġmillion', 'Ġyears', 'Ġbig', 'Ġbang', 'Ġfar', 'Ġearlier', 'Ġpreviously', 'Ġknown', 'Ġaug', 'ust', 'Ġn', 'asa', 'Ġreleased', 'Ġlarge', 'Ġmosaic', 'Ġimage', 'Ġindividual', 'Ġframes', 'Ġtaken', 'Ġnear', 'Ġinfrared', 'Ġcamera', 'n', 'irc', 'Ġweb', 'b', 'Ġnumerous', 'Ġearly', 'Ġgalaxies', 'Ġearly', 'Ġgalaxies', 'Ġobserved', 'Ġweb', 'b', 'Ġlike', 'Ġce', 'ers', 'Ġestimated', 'Ġred', 'shift', 'Ġapproximately', 'Ġz', 'Ġcorresponding', 'Ġmillion', 'Ġyears', 'Ġbig', 'Ġbang', 'Ġhigh', 'Ġred', 'shift', 'Ġgalaxy', 'Ġse', 'pt', 'ember', 'Ġprim', 'ordial', 'Ġblack', 'Ġholes', 'Ġproposed', 'Ġexplaining', 'Ġunexpectedly', 'Ġlarge', 'Ġearly', 'Ġgalaxies', 'Ġj', 'une', 'Ġdetection', 'Ġorganic', 'Ġmolecules', 'Ġbillion', 'Ġlight', 'years', 'Ġaway', 'Ġgalaxy', 'Ġcalled', 'pt', '04', 'Ġusing', 'Ġweb', 'b', 'Ġtelescope', 'Ġannounced', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġcelebrated', 'Ġfirst', 'Ġyear', 'Ġoperations', 'Ġrelease', 'Ġweb', 'b', 'âĢ', 'Ļ', 'Ġimage', 'Ġsmall', 'Ġstar', 'forming', 'Ġregion', 'Ġr', 'ho', 'phi', 'uchi', 'Ġcloud', 'Ġcomplex', 'Ġlight', 'Ġyears', 'Ġaway', 'Ġfirst', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġreleased', 'Ġj', 'uly', 'Ġcosmic', 'Ġcliffs', 'Ġcar', 'ina', 'Ġneb', 'ula', 'ng', 'c', 'n', 'irc', 'Ġcar', 'ina', 'Ġneb', 'ula', 'ng', 'c', 'mir', 'Ġsouthern', 'Ġring', 'Ġneb', 'ula', 'ng', 'c', 'Ġleft', 'Ġn', 'irc', 'Ġright', 'Ġmir', 'Ġweb', 'b', "'s", 'Ġfirst', 'Ġdeep', 'Ġfield', 'sm', 'acs', 'Ġ07', 'Ġleft', 'Ġmir', 'Ġright', 'Ġn', 'irc', 'Ġstep', 'han', "'s", 'Ġquint', 'et', 'n', 'irc', 'mir', 'Ġcomposite', 'Ġgallery', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġspectrum', 'p', 'b', 'Ġmedia', 'Ġrelated', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'imedia', 'Ġcommons', 'Ġspacecraft', 'Ġattitude', 'Ġcontrol', 'Ġprocess', 'Ġcontrolling', 'Ġorientation', 'Ġaerospace', 'Ġvehicle', 'Ġtimeline', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlib', 'ration', 'Ġpoint', 'Ġorbit', 'Ġqu', 'iper', 'iod', 'ic', 'Ġorbit', 'Ġaround', 'Ġlag', 'range', 'Ġpoint', 'Ġlist', 'Ġdeep', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġlist', 'Ġlargest', 'Ġinfrared', 'Ġtelescopes', 'Ġlist', 'Ġlargest', 'Ġoptical', 'ï', '¬', 'Ĥ', 'ect', 'ing', 'Ġtelescopes', 'Ġlist', 'Ġspace', 'Ġtelescopes', 'Ġn', 'ancy', 'Ġgrace', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġplanned', 'Ġlaunch', 'Ġlater', 'Ġmay', 'Ġnew', 'Ġworlds', 'Ġmission', 'prop', 'osed', 'Ġocc', 'ul']</t>
         </is>
       </c>
       <c r="C301" t="n">
@@ -4351,7 +4351,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>['Ġfirst', 'Ġgalaxies', 'Ġmay', 'Ġformed', 'Ġaround', 'Ġred', 'shift', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime', 'Ġhub', 'ble', 'Ġunable', 'Ġsee', 'Ġback', 'Ġearly', 'Ġz', 'âī', 'Ī', 'gal', 'axy', 'Ġmillion', 'Ġyears', 'Ġcosmic', 'Ġtime', ').[', 'Ġfeatures', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġrough', 'Ġplot', 'Ġearth', "'s", 'Ġatmospheric', 'Ġabsorption', 'Ġopacity', 'Ġvarious', 'Ġwavelengths', 'Ġelectromagnetic', 'Ġradiation', 'Ġincluding', 'Ġvisible', 'Ġlight', 'Ġdesign', 'Ġemphasizes', 'Ġnear', 'Ġmid', 'inf', 'rared', 'Ġseveral', 'Ġreasons', 'Ġhigh', 'red', 'shift', 'Ġearly', 'Ġdistant', 'Ġobjects', 'Ġvisible', 'Ġemissions', 'Ġshifted', 'Ġinfrared', 'Ġtherefore', 'Ġlight', 'Ġobserved', 'Ġtoday', 'Ġvia', 'Ġinfrared', 'Ġastronomy', 'Ġinfrared', 'Ġlight', 'Ġpasses', 'Ġeasily', 'Ġdust', 'Ġclouds', 'Ġvisible', 'Ġlight', 'Ġcolder', 'Ġobjects', 'Ġdebris', 'Ġdisks', 'Ġplanets', 'Ġemit', 'Ġstrongly', 'Ġinfrared', 'Ġinfrared', 'Ġbands', 'ï', '¬', 'ģ', 'cult', 'Ġstudy', 'Ġground', 'Ġexisting', 'Ġspace', 'Ġtelescopes', 'Ġhub', 'ble', 'Ġground', 'based', 'Ġtelescopes', 'Ġmust', 'Ġlook', 'Ġearth', "'s", 'Ġatmosphere', 'Ġopaque', 'Ġmany', 'Ġinfrared', 'Ġbands', 'see', 'Ġfigure', 'Ġright', 'Ġeven', 'Ġatmosphere', 'Ġtransparent', 'Ġmany', 'Ġtarget', 'Ġchemical', 'Ġcompounds', 'Ġwater', 'Ġcarbon', 'Ġdioxide', 'Ġmethane', 'Ġalso', 'Ġexist', 'Ġearth', "'s", 'Ġatmosphere', 'Ġvastly', 'Ġcompl', 'icating', 'Ġanalysis', 'Ġexisting', 'Ġspace', 'Ġtelescopes', 'Ġhub', 'ble', 'Ġcannot', 'Ġstudy', 'Ġbands', 'Ġsince', 'Ġmirrors', 'Ġinsufficient', 'ly', 'Ġcool', 'Ġhub', 'ble', 'Ġmirror', 'Ġmaintained', 'ĠÂ°', 'c', 'Ġk', 'ĠÂ°', 'f', '])', 'Ġmeans', 'Ġtelescope', 'Ġradi', 'ates', 'Ġstrongly', 'Ġrelevant', 'Ġinfrared', 'Ġbands', 'Ġweb', 'b', 'Ġalso', 'Ġobserve', 'Ġobjects', 'Ġsolar', 'Ġsystem', 'Ġangle', 'Â°', 'Ġsun', 'Ġapparent', 'Ġangular', 'Ġrate', 'Ġmotion', 'Ġless', '03', 'Ġarc', 'Ġseconds', 'Ġper', 'Ġsecond', 'Ġincludes', 'Ġmars', 'Ġj', 'upiter', 'Ġsat', 'urn', 'Ġur', 'anus', 'Ġne', 'pt', 'une', 'Ġpl', 'uto', 'Ġsatellites', 'ets', 'Ġasteroids', 'Ġminor', 'Ġplanets', 'Ġbeyond', 'Ġorbit', 'Ġmars', 'Ġweb', 'b', 'Ġnear', 'ir', 'Ġmid', 'ir', 'Ġsensitivity', 'Ġable', 'Ġobserve', 'Ġvirtually', 'Ġknown', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġobjects', 'Ġaddition', 'Ġobserve', 'Ġopportun', 'istic', 'Ġun', 'planned', 'Ġtargets', 'Ġwithin', 'Ġhours', 'Ġdecision']</t>
+          <t>['ter', 'Ġj', 'w', 'st', 'Ġphysical', 'Ġcos', 'mology', 'Ġbranch', 'Ġcos', 'mology', 'Ġstudies', 'Ġmathematical', 'Ġmodels', 'Ġuniverse', 'Ġsatellite', 'Ġbus', 'Ġmain', 'Ġbody', 'Ġstructural', 'Ġcomponent', 'Ġsatellite', 'Ġsolar', 'Ġpanels', 'Ġspacecraft', 'Ġphot', 'ov', 'olt', 'aic', 'Ġsolar', 'Ġpanels', 'Ġspacecraft', 'Ġoperating', 'Ġinner', 'Ġsolar', 'Ġsystem', 'Ġspacecraft', 'Ġdesign', 'Ġspacecraft', 'Ġthermal', 'Ġcontrol', 'Ġprocess', 'Ġkeeping', 'Ġparts', 'Ġspacecraft', 'Ġwithin', 'Ġacceptable', 'Ġtemperature', 'Ġranges', 'Ġj', 'w', 'st', 'Ġdesigned', 'Ġrequirement', 'Ġtrack', 'Ġobjects', 'Ġmove', 'Ġfast', 'Ġmars', 'Ġmaximum', 'Ġapparent', 'Ġspeed', 'Ġmas', 'Ġvalue', 'Ġgiven', 'Ġtechnical', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'cation', 'e', 'Ġnominal', 'Ġvalue', 'Ġcommission', 'ing', 'Ġvarious', 'Ġasteroids', 'Ġobserved', 'Ġdetermine', 'Ġactual', 'Ġlimitation', 'Ġspeed', 'Ġobjects', 'Ġturned', 'Ġmas', 'Ġtwice', 'Ġnominal', 'Ġvalue', 'Ġtracking', 'Ġrates', 'âĢĵ', 'Ġmas', 'Ġshowed', 'Ġaccur', 'acies', 'Ġsimilar', 'Ġtracking', 'Ġslower', 'Ġtargets', 'Ġthus', 'Ġtelescope', 'Ġable', 'Ġobserve', 'Ġalso', 'Ġnear', 'earth', 'Ġasteroids', 'ne', 'ets', 'Ġcloser', 'Ġper', 'hel', 'ion', 'Ġinterstellar', 'Ġobjects', ']:', 'Ġlater', 'Ġexperience', 'Ġgained', 'Ġtracking', 'Ġspeed', 'Ġlimit', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġset', 'Ġmas', 'Ġroutine', 'Ġobservations', 'Ġhigher', 'Ġrates', 'Ġmas', 'Ġalso', 'Ġpossible', 'Ġspecial', 'Ġrequest', 'Ġneeds', 'Ġmultiple', 'Ġguide', 'Ġstars', 'Ġend', 'Ġintroduces', 'Ġcomplexity', 'ef', 'ï', '¬', 'ģ', 'ci', 'ency', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġobservation', 'Ġsuper', 'fast', 'Ġrate', 'Ġdart', 'Ġimpact', 'Ġexperiment', 'Ġse', 'pt', 'ember', 'Ġb', 'b', 'af', 'ï', '¬', 'Ĥ', 'ed', '",', 'Ġcontext', 'Ġmeans', 'Ġenclosed', 'Ġtube', 'Ġsimilar', 'Ġmanner', 'Ġconventional', 'Ġoptical', 'Ġtelescope', 'Ġhelps', 'Ġstop', 'Ġstray', 'Ġlight', 'Ġentering', 'Ġtelescope', 'Ġside', 'Ġactual', 'Ġexample', 'Ġsee', 'Ġfollowing', 'Ġlink', 'Ġfren', 'iere', 'Ġe', 'r', 'first', 'order', 'Ġdesign', 'Ġoptical', 'Ġb', 'af', 'ï', '¬', 'Ĥ', 'es', '".', 'Ġsociety', 'Ġphoto', 'opt', 'ical', 'Ġinstrument', 'ation', 'Ġengineers', 'sp', 'ie', 'Ġconference', 'Ġseries', 'Ġfirst', 'order', 'Ġdesign', 'Ġoptical', 'Ġb', 'af', 'ï', '¬', 'Ĥ', 'es', 'Ġradiation', 'Ġscattering', 'Ġoptical', 'Ġsystems', 'Ġvol', 'Ġpp', 'âĢĵ', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġc', 'Ġmirror', 'Ġsegment']</t>
         </is>
       </c>
       <c r="C302" t="n">
@@ -4364,7 +4364,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>['Ġsuper', 'nov', 'ae', 'Ġgamma', 'Ġray', 'Ġbursts', 'Ġthree', 'quarter', 'Ġview', 'Ġtop', 'Ġbottom', 'sun', 'facing', 'Ġside', 'Ġlocation', 'Ġorbit', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġtest', 'Ġunit', 'Ġsun', 'shield', 'Ġstacked', 'Ġexpanded', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġfacility', 'Ġcal', 'ornia', 'Ġweb', 'b', 'Ġoperates', 'Ġh', 'alo', 'Ġorbit', 'Ġcircling', 'Ġaround', 'Ġpoint', 'Ġspace', 'Ġknown', 'Ġsun', 'âĢĵ', 'earth', 'Ġlag', 'range', 'Ġpoint', 'Ġapproximately', '000', '000', 'Ġmi', 'Ġbeyond', 'Ġearth', "'s", 'Ġorbit', 'Ġaround', 'Ġsun', 'Ġactual', 'Ġposition', 'Ġvaries', '000', '000', '000', 'âĢĵ', '000', 'Ġmi', 'Ġorbits', 'Ġkeeping', 'Ġearth', 'Ġmoon', "'s", 'Ġshadow', 'Ġway', 'Ġcomparison', 'Ġhub', 'ble', 'Ġorbits', 'Ġmi', 'Ġearth', "'s", 'Ġsurface', 'Ġmoon', 'Ġroughly', '000', '000', 'Ġmi', 'Ġearth', 'Ġobjects', 'Ġnear', 'Ġsun', 'âĢĵ', 'earth', 'Ġpoint', 'Ġorbit', 'Ġsun', 'Ġsynchron', 'Ġearth', 'Ġallowing', 'Ġtelescope', 'Ġremain', 'Ġroughly', 'Ġconstant', 'Ġdistance', 'Ġcontinuous', 'Ġorientation', 'Ġsun', 'shield', 'Ġequipment', 'Ġbus', 'Ġtoward', 'Ġsun', 'Ġearth', 'Ġmoon', 'Ġcombined', 'Ġwide', 'Ġshadow', 'avoid', 'ing', 'Ġorbit', 'Ġtelescope', 'Ġsimultaneously', 'Ġblock', 'Ġincoming', 'Ġheat', 'Ġlight', 'Ġthree', 'Ġbodies', 'Ġavoid', 'Ġeven', 'Ġsmallest', 'Ġchanges', 'Ġtemperature', 'Ġearth', 'Ġmoon', 'Ġshadows', 'Ġwould', 'Ġaffect', 'Ġstructure', 'Ġyet', 'Ġstill', 'Ġmaintain', 'Ġuninterrupted', 'Ġsolar', 'Ġpower', 'Ġearth', 'Ġcommunications', 'Ġsun', 'facing', 'Ġside', 'Ġarrangement', 'Ġkeeps', 'Ġtemperature', 'Ġspacecraft', 'Ġconstant', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', 'Ġnecessary', 'Ġfaint', 'Ġinfrared', 'Ġmake', 'Ġobservations', 'Ġinfrared', 'Ġspectrum', 'Ġweb', 'b', 'Ġmust', 'Ġkept', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', ');', 'Ġotherwise', 'Ġinfrared', 'Ġradiation', 'Ġtelescope', 'Ġwould', 'Ġoverwhelm', 'Ġinstruments', 'Ġlarge', 'Ġsun', 'shield', 'Ġblocks', 'Ġlight', 'Ġheat', 'Ġsun', 'Ġearth', 'Ġmoon', 'Ġposition', 'Ġnear', 'Ġsun', 'âĢĵ', 'earth', 'Ġkeeps', 'Ġthree', 'Ġbodies', 'Ġside', 'Ġspacecraft', 'Ġtimes', 'Ġh', 'alo', 'Ġorbit', 'Ġaround', 'Ġpoint', 'Ġavoids', 'Ġshadow', 'Ġearth', 'Ġmoon', 'Ġmaintaining', 'Ġconstant', 'Ġenvironment', 'Ġsun', 'shield', 'Ġsolar', 'Ġarrays', 'Ġresulting', 'Ġstable', 'Ġtemperature', 'Ġstructures', 'Ġdark', 'Ġside', 'Ġcritical']</t>
+          <t>['Ġpositioned', 'Ġouter', 'Ġring', 'Ġsegments', 'Ġlocated', 'clock', 'Ġnumber', 'Ġclock', 'Ġface', 'Ġviewing', 'Ġprimary', 'Ġmirror', 'Ġface', 'Ġstar', 'Ġapproximately', 'Ġlight', 'years', 'Ġaway', 'Ġconstellation', 'Ġ', 'urs', 'Ġmajor', 'Ġstar', 'Ġspectral', 'Ġtype', 'Ġstar', 'Ġhigh', 'Ġproper', 'Ġmotion', 'Ġe', 'mass', 'Ġj', 'Ġalso', 'Ġknown', 'Ġun', 'sw', 'v', 'Ġty', 'c', 'Ġstar', 'Ġconstellation', 'Ġdr', 'aco', 'Ġmil', 'ky', 'Ġway', 'Ġlocated', 'Ġalmost', '000', 'Ġlight', 'Ġyears', 'Ġaway', 'Ġearth', 'Ġwithin', 'Ġdegree', 'Ġnorth', 'Ġe', 'cl', 'ipt', 'ic', 'Ġpole', 'Ġvisual', 'Ġapparent', 'Ġmagnitude', 'Ġmakes', 'Ġmuch', 'Ġfaint', 'Ġobserved', 'Ġnaked', 'Ġeye', 'Ġcooler', 'Ġsun', 'Ġtimes', 'Ġbrighter', 'Ġvisible', 'Ġlight', 'Ġconsequently', 'Ġsun', 'like', 'Ġstar', 'Ġmotion', 'Ġvector', 'Ġdirection', 'Ġsun', 'n', 'asa', 'Ġj', 'w', 'st', 'Ġpartners', 'Ġweb', 'b', 'Ġproject', '?"', 'Ġart', 'ners', 'Ġn', 'asa', 'Ġarchived', 'q', 'html', 'part', 'ners', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġke', 'l', 'Ġth', 'omas', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġcel', 'est', 'rak', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġfull', 'Ġgeneral', 'Ġpublic', 'Ġweb', 'b', 'Ġtelescope', 'n', 'asa', 'Ġml', 'h', 'owl', 'ong', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġsays', 'Ġweb', 'b', "'s", 'Ġexcess', 'Ġfuel', 'Ġlikely', 'Ġextend', 'Ġlifetime', 'Ġexpectations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', ')"', 'Ġn', 'id', 'Ġn', 'asa', 'Ġspace', 'Ġscience', 'Ġdata', 'Ġcoordinated', 'Ġarchive', 'Ġretrieved', 'Ġfe', 'b', 'ruary']</t>
         </is>
       </c>
       <c r="C303" t="n">
@@ -4377,7 +4377,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>['Ġmaintaining', 'Ġprecise', 'Ġalignment', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġfive', 'layer', 'Ġsun', 'shield', 'Ġlayer', 'Ġthin', 'Ġhuman', 'Ġhair', 'Ġmade', 'Ġk', 'apt', 'Ġfilm', 'Ġcoated', 'Ġaluminum', 'Ġsides', 'Ġlayer', 'oped', 'Ġsilicon', 'Ġsun', 'facing', 'Ġside', 'Ġtwo', 'Ġhottest', 'Ġlayers', 'Ġreflect', 'Ġsun', "'s", 'Ġheat', 'Ġback', 'Ġspace', 'Ġaccidental', 'Ġtears', 'Ġdelicate', 'Ġfilm', 'Ġstructure', 'Ġdeployment', 'Ġtesting', 'Ġled', 'Ġdelays', 'Ġtelescope', 'Ġsun', 'shield', 'Ġdesigned', 'Ġfolded', 'Ġtwelve', 'Ġtimes', 'concert', 'ina', 'Ġstyle', 'Ġwould', 'Ġfit', 'Ġwithin', 'ri', 'ane', 'Ġrocket', "'s", 'Ġpayload', 'Ġfair', 'ing', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġlong', 'Ġshield', "'s", 'Ġfully', 'Ġdeployed', 'Ġdimensions', 'Ġplanned', 'Ġft', 'Ġkeeping', 'Ġwithin', 'Ġshadow', 'Ġsun', 'shield', 'Ġlimits', 'Ġfield', 'Ġregard', 'Ġweb', 'b', 'Ġgiven', 'Ġtime', 'Ġtelescope', 'Ġsee', 'Ġpercent', 'Ġone', 'Ġposition', 'Ġsee', 'Ġperiod', 'Ġmonths', 'Ġweb', 'b', "'s", 'Ġprimary', 'Ġmirror', 'Ġft', ')-', 'iameter', 'Ġgold', 'co', 'ated', 'Ġb', 'ery', 'ium', 'Ġreflect', 'Ġcollecting', 'Ġarea', 'Ġft', 'Ġdesigned', 'Ġsingle', 'Ġlarge', 'Ġmirror', 'Ġwould', 'Ġlarge', 'Ġexisting', 'Ġlaunch', 'Ġvehicles', 'Ġmirror', 'Ġtherefore', 'Ġcomposed', 'Ġhex', 'agonal', 'Ġsegments', 'Ġsun', 'shield', 'Ġprotection', 'Ġoptics', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġengineers', 'Ġcleaning', 'Ġtest', 'Ġmirror', 'Ġcarbon', 'Ġdioxide', 'Ġsnow', 'Ġmain', 'Ġmirror', 'Ġassembly', 'Ġfront', 'Ġprimary', 'Ġmirrors', 'Ġattached', 'mber', 'Ġdiff', 'raction', 'Ġspikes', 'Ġdue', 'Ġmirror', 'Ġsegments', 'Ġspider', 'Ġcolor', 'coded', 'Ġtechnique', 'Ġpioneered', 'Ġguid', 'Ġhorn', 'art', 'uro', 'Ġunfolded', 'Ġtelescope', 'Ġlaunched', 'Ġimage', 'Ġplane', 'Ġwave', 'front', 'Ġsensing', 'Ġphase', 'Ġretrieval', 'Ġused', 'Ġposition', 'Ġmirror', 'Ġsegments', 'Ġcorrect', 'Ġlocation', 'Ġusing', 'Ġprecise', 'Ġactu', 'ators', 'Ġsubsequent', 'Ġinitial', 'Ġconfiguration', 'Ġneed', 'Ġoccasional', 'Ġupdates', 'Ġevery', 'Ġdays', 'Ġretain', 'Ġoptimal', 'Ġfocus', 'Ġunlike', 'Ġterrestrial', 'Ġtelescopes', 'Ġexample', 'Ġke', 'ck', 'Ġtelescopes', 'Ġcontinually', 'Ġadjust', 'Ġmirror', 'Ġsegments', 'Ġusing', 'Ġactive', 'Ġoptics', 'Ġovercome', 'Ġeffects', 'Ġgravitational', 'Ġwind', 'Ġloading']</t>
+          <t>['bb', 'Ġkey', 'Ġfacts', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġn', 'asa', 'Ġretrieved', 'Ġapr', 'il', 'j', 'w', 'st', 'Ġorbit', 'Ġj', 'w', 'st', 'Ġuser', 'Ġdocumentation', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġtelescope', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġuser', 'Ġdocumentation', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġreferences', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmos', 'k', 'owitz', 'Ġcl', 'ara', 'Ġde', 'cember', 'Ġj', 'w', 'st', 'Ġchanging', 'Ġview', 'Ġuniverse', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsparked', 'Ġnew', 'Ġera', 'Ġastronomy', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġarchived', 'http', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'bye', 'ennis', 'Ġaug', 'ust', 'Ġweb', 'b', 'Ġtelescope', 'Ġexpanded', 'Ġuniverse', 'Ġnew', 'Ġimages', 'Ġj', 'upiter', 'Ġgalactic', 'Ġsurvey', 'Ġspring', 'Ġforth', 'Ġn', 'asa', "'s", 'Ġnew', 'Ġobserv', 'atory', 'Ġcosmic', 'Ġaffairs', 'Ġcorrespondent', 'Ġconfess', 'es', "'t", 'Ġanticipate', 'Ġpower', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġaug', 'ust', 'Ġweb', 'b', 'Ġtelescope', 'Ġastonishing', 'Ġuniverse', 'Ġeven', 'Ġnew', 'Ġtool', "'t", 'Ġeverything', "'s", 'Ġcapturing', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlight', 'Ġemitted', 'Ġbig', 'Ġbang', 'Ġalready', 'Ġrevealing', 'Ġwonders', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'call', 'aghan', 'Ġj', 'athan', 'Ġjan', 'uary', 'j', 'w', 'st', 'Ġherald', 'Ġnew', 'Ġdawn', 'Ġex', 'oplan', 'et', 'Ġscience', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġopening', 'Ġexciting', 'Ġnew', 'Ġchapter', 'Ġstudy', 'Ġex', 'oplan', 'ets', 'Ġsearch', 'Ġlife', 'Ġbeyond', 'Ġearth', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġretrieved', 'Ġjan', 'uary']</t>
         </is>
       </c>
       <c r="C304" t="n">
@@ -4390,7 +4390,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>['Ġweb', 'b', 'Ġtelescope', 'Ġuses', 'Ġsmall', 'Ġact', 'uation', 'Ġmotors', 'Ġposition', 'Ġadjust', 'Ġoptics', 'Ġactu', 'ators', 'Ġposition', 'Ġmirror', 'Ġnan', 'ometer', 'Ġaccuracy', 'Ġweb', 'b', "'s", 'Ġoptical', 'Ġdesign', 'Ġthree', 'mir', 'ror', 'ast', 'igmat', 'Ġmakes', 'Ġuse', 'Ġcurved', 'Ġsecondary', 'Ġtert', 'iary', 'Ġmirrors', 'Ġdeliver', 'Ġimages', 'Ġfree', 'Ġoptical', 'Ġab', 'err', 'ations', 'Ġwide', 'Ġfield', 'Ġsecondary', 'Ġmirror', 'Ġft', 'Ġdiameter', 'Ġaddition', 'Ġfine', 'Ġsteering', 'Ġmirror', 'Ġadjust', 'Ġposition', 'Ġmany', 'Ġtimes', 'Ġper', 'Ġsecond', 'Ġprovide', 'Ġimage', 'Ġstabilization', 'Ġphotographs', 'Ġtaken', 'Ġweb', 'b', 'Ġspikes', 'Ġplus', 'Ġtwo', 'Ġf', 'ter', 'Ġones', 'Ġdue', 'Ġspider', 'Ġsupporting', 'Ġsecondary', 'Ġmirror', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', 'Ġframework', 'Ġprovides', 'Ġelectrical', 'Ġpower', 'Ġcomputing', 'Ġresources', 'Ġcooling', 'Ġcapability', 'Ġwell', 'Ġstructural', 'Ġstability', 'Ġweb', 'b', 'Ġtelescope', 'Ġmade', 'Ġbonded', 'Ġgraph', 'ite', 'ep', 'oxy', 'Ġcomposite', 'Ġattached', 'Ġunderside', 'Ġweb', 'b', "'s", 'Ġtelescope', 'Ġstructure', 'im', 'Ġholds', 'Ġfour', 'Ġscience', 'Ġinstruments', 'Ġguide', 'Ġcamera', 'Ġn', 'irc', 'near', 'Ġinfrared', 'Ġcamera', 'Ġinfrared', 'Ġim', 'ager', 'Ġspectral', 'Ġcoverage', 'Ġranging', 'Ġedge', 'Ġvisible', 'ĠÎ¼', 'Ġnear', 'Ġinfrared', 'Ġsensors', 'Ġmeg', 'ap', 'ixels', 'Ġn', 'irc', 'Ġserves', 'Ġobserv', 'atory', "'s", 'Ġwave', 'front', 'Ġsensor', 'Ġrequired', 'Ġwave', 'front', 'Ġsensing', 'Ġcontrol', 'Ġactivities', 'Ġused', 'Ġalign', 'Ġfocus', 'Ġmain', 'Ġmirror', 'Ġsegments', 'Ġn', 'irc', 'Ġbuilt', 'Ġteam', 'Ġled', 'Ġuniversity', 'ri', 'zona', 'Ġprincipal', 'Ġinvestigator', 'Ġmar', 'cia', 'Ġj', 'Ġn', 'ir', 'spec', 'near', 'Ġinfrared', 'Ġspect', 'rog', 'raph', 'Ġperforms', 'Ġspect', 'rosc', 'opy', 'Ġwavelength', 'Ġrange', 'Ġbuilt', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġest', 'ec', 'Ġnet', 'lands', 'Ġleading', 'Ġdevelopment', 'Ġteam', 'Ġincludes', 'Ġmembers', 'Ġair', 'bus', 'Ġdefence', 'Ġspace', 'tt', 'ob', 'run', 'n', 'Ġfried', 'rich', 'sh', 'af', 'en', 'Ġg', 'erman', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġpier', 'Ġfer', 'ruit', 'Ã©', 'co', 'le', 'Ġnorm', 'ale', 'Ġsup', 'Ã©', 'rie', 'ure', 'Ġde', 'Ġl', 'yon', 'Ġn', 'ir', 'spec', 'Ġproject', 'Ġscientist', 'Ġn', 'ir', 'spec', 'Ġdesign', 'Ġprovides', 'Ġthree', 'Ġobserving', 'Ġmodes', 'Ġlow', 'resolution', 'Ġmode', 'Ġusing', 'Ġprism', 'Ġr', 'Ġmulti', 'object', 'Ġmode', 'Ġr', '00', 'Ġintegral', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġunit']</t>
+          <t>['Ġfisher', 'Ġal', 'ise', 'Ġpin', 'ol', 'Ġnat', 'asha', 'Ġbet', 'z', 'Ġl', 'aura', 'Ġj', 'uly', 'president', 'Ġbid', 'en', 'Ġreveals', 'Ġfirst', 'Ġimage', 'Ġn', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġn', 'asa', 'Ġarchived', 'Ġscope', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'par', 'ison', 'Ġweb', 'b', 'Ġhub', 'ble', 'Ġtelescope', 'Ġweb', 'b', 'n', 'asa', 'j', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'Ġmill', 'er', 'Ġk', 'rina', 'Ġj', 'uly', 'Ġyear', 'Ġcosmic', 'Ġwonder', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġnew', 'Ġimage', 'Ġn', 'asa', 'Ġcommemor', 'ates', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġanniversary', 'Ġscience', 'Ġpowerful', 'Ġobserv', 'atory', 'Ġever', 'Ġsent', 'Ġspace', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġl', 'allo', 'Ġmatt', 'hew', 'exper', 'ience', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġyears', 'Ġarchetype', '".', 'Ġoptical', 'Ġengineering', '):', 'Ġ01', 'âĢĵ', '01', 'âĢĵ', 'Ġar', 'x', 'iv', '03', '0002', '03', '0002', 'l', 'mir', 'rors', 'Ġweb', 'b', 'n', 'asa', 'Ġweb', 'b', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'uly', 'Ġdeeper', 'Ġb', 'rian', 'Ġk', 'ober', 'lein', 'Ġbri', 'ank', 'ober', 'lein', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġscientists', 'Ġweb', 'b', 'Ġtelescope', 'n', 'asa', 'Ġts', 'html', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġshel', 'ton', 'Ġmarch', 'sh', 'attering', 'Ġcosmic', 'Ġdistance', 'Ġrecord', 'http', 'news', 'al', 'ale', 'Ġuniversity', 'Ġarchived', 'http', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'hub', 'ble', 'Ġbreaks', 'Ġcosmic', 'Ġdistance', 'Ġrecord', 'Ġsp', 'acet', 'el', 'esc', 'ope', 'org', 'Ġmarch', 'ic']</t>
         </is>
       </c>
       <c r="C305" t="n">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>['Ġlong', 'sl', 'Ġspect', 'rosc', 'opy', 'Ġmode', 'Ġswitching', 'Ġmodes', 'Ġdone', 'Ġoperating', 'Ġwavelength', 'Ġpre', 'selection', 'Ġmechanism', 'Ġcalled', 'Ġfilter', 'Ġwheel', 'Ġassembly', 'Ġselecting', 'Ġcorresponding', 'Ġdisp', 'ersive', 'Ġelement', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġinstruments', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġn', 'irc', 'Ġwrapped', 'Ġcalibration', 'Ġassembly', 'Ġone', 'Ġcomponent', 'Ġn', 'ir', 'spec', 'Ġinstrument', 'Ġmir', 'pr', 'ism', 'Ġgr', 'ating', 'Ġusing', 'Ġgr', 'ating', 'Ġwheel', 'Ġassembly', 'Ġmechanism', 'Ġmechanisms', 'Ġbased', 'Ġsuccessful', 'oph', 'ot', 'Ġwheel', 'Ġmechanisms', 'Ġinfrared', 'Ġspace', 'Ġobserv', 'atory', 'Ġmulti', 'object', 'Ġmode', 'Ġrelies', 'Ġcomplex', 'Ġmicro', 'sh', 'utter', 'Ġmechanism', 'Ġallow', 'Ġsimultaneous', 'Ġobservations', 'Ġhundreds', 'Ġindividual', 'Ġobjects', 'Ġanywhere', 'Ġn', 'ir', 'spec', "'s", 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġview', 'Ġtwo', 'Ġsensors', 'Ġmeg', 'ap', 'ixels', 'Ġmir', 'mid', 'inf', 'rared', 'Ġinstrument', 'Ġmeasures', 'Ġmid', 'long', 'inf', 'rared', 'Ġwavelength', 'Ġrange', 'Ġcontains', 'Ġmid', 'inf', 'rared', 'Ġcamera', 'Ġimaging', 'Ġspect', 'rom', 'eter', 'Ġmir', 'Ġdeveloped', 'Ġcollaboration', 'Ġn', 'asa', 'Ġconsortium', 'Ġeuro', 'pe', 'Ġcountries', 'Ġled', 'Ġge', 'orge', 'Ġr', 'ie', 'ke', 'un', 'iversity', 'ri', 'zona', 'Ġg', 'illian', 'Ġwr', 'ight', 'Ġastronomy', 'Ġtechnology', 'Ġcentre', 'Ġed', 'inburgh', 'Ġsc', 'ot', 'land', ').[', 'Ġtemperature', 'Ġmir', 'Ġmust', 'Ġexceed', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'ĠÂ°', 'f', '):', 'Ġhelium', 'Ġgas', 'Ġmechanical', 'Ġcooler', 'ited', 'Ġwarm', 'Ġside', 'Ġenvironmental', 'Ġshield', 'Ġprovides', 'Ġcooling', 'Ġf', 'gs', 'nir', 'iss', 'fine', 'Ġguidance', 'Ġsensor', 'Ġnear', 'Ġinfrared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'Ġled', 'adian', 'Ġspace', 'Ġagency', 'Ġproject', 'Ġscientist', 'Ġjohn', 'Ġh', 'utch', 'ings', 'z', 'berg', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġresearch', 'Ġcentre', 'Ġused', 'Ġstabilize', 'Ġline', 'sight', 'Ġobserv', 'atory', 'Ġscience', 'Ġobservations', 'Ġmeasurements', 'Ġused', 'Ġcontrol', 'Ġoverall', 'Ġorientation', 'Ġspacecraft', 'Ġdrive', 'Ġï', '¬', 'ģ', 'ne', 'Ġsteering', 'Ġmirror', 'Ġimage', 'Ġstabilization', 'adian', 'Ġspace', 'Ġagency', 'Ġalso', 'Ġprovided', 'Ġnear', 'Ġinfrared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'nir', 'iss', 'Ġmodule', 'Ġastronomical', 'Ġimaging', 'Ġspect', 'rosc', 'opy', 'ĠÎ¼', 'Ġwavelength', 'Ġrange', 'Ġled', 'Ġprincipal', 'Ġinvestigator', 'Ġren', 'Ã©', 'yon', 'Ġunivers', 'itÃ©', 'Ġde', 'Ġmont', 'rÃ©', 'al']</t>
+          <t>['04', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'es', 'ch', 'Ġp', '.;', 'Ġb', 'ram', 'mer', 'Ġg', '.;', 'Ġvan', 'Ġp', '.;', 'Ġet', 'Ġal', 'arch', 'Ġremarkably', 'Ġlumin', 'ous', 'Ġgalaxy', 'Ġz', 'Ġmeasured', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġgr', 'ism', 'Ġspect', 'rosc', 'opy', '".', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġar', 'x', 'iv', '03', '00', 'kinson', 'Ġn', 'ancy', 'hub', 'ble', 'Ġlooked', 'Ġback', 'Ġtime', 'Ġfar', 'Ġstill', "'t", 'Ġfind', 'Ġfirst', 'Ġstars', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġvia', 'Ġscience', 'alert', 'inf', 'rared', 'Ġastronomy', 'Ġearth', 'Ġorbit', 'Ġinfrared', 'Ġprocessing', 'Ġanalysis', 'Ġcenter', 'Ġn', 'asa', 'Ġsp', 'itzer', 'Ġscience', 'Ġcenter', 'Ġcal', 'ornia', 'Ġinstitute', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'http', 'ip', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġfisher', 'Ġal', 'ise', 'Ġj', 'uly', 'bb', 'Ġimages', 'Ġj', 'upiter', 'Ġavailable', 'Ġcommission', 'ing', 'Ġdata', 'mission', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġaug', 'ust', 'Ġrig', 'Ġj', 'ane', 'Ġper', 'rin', 'Ġmarsh', 'cel', 'w', 'ichael', 'Ġk', 'imble', 'Ġr', 'andy', 'Ġfried', 'man', 'Ġsc', 'ott', 'Ġl', 'allo', 'Ġmatt', 'yon', 'Ġren', 'Ã©', 'Ġfe', 'berg', 'Ġle', 'e', 'Ġfer', 'ruit', 'Ġpier', 'Ġgl', 'asse', 'Ġal', 'ist', 'air', 'Ġr', 'ie', 'ke', 'Ġmar', 'cia', 'Ġr', 'ie', 'ke', 'Ġge', 'orge', 'Ġet', 'Ġal', 'Ġscience', 'Ġperformance', 'Ġj', 'w', 'st', 'Ġcharacterized', 'Ġcommission', 'ing', '".', 'Ġpublications', 'Ġastronomical', 'Ġsociety', 'Ġpac', 'ï', '¬', 'ģ', 'c', '):', '001', 'Ġar', 'x', 'iv', '05', '05', 'Ġth', 'add', 'eus', 'Ġc', 'es', 'ari', 'Ġfe', 'b', 'ruary', 'breaking', 'Ġtracking', 'Ġspeed', 'Ġlimit', 'Ġweb', 'b', 'blog', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs']</t>
         </is>
       </c>
       <c r="C306" t="n">
@@ -4416,7 +4416,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>['Ġalthough', 'Ġoften', 'Ġreferred', 'Ġtogether', 'Ġunit', 'Ġn', 'ir', 'iss', 'Ġserve', 'Ġentirely', 'Ġdifferent', 'Ġpurposes', 'Ġone', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġinstrument', 'Ġpart', 'Ġobserv', 'atory', "'s", 'Ġsupport', 'Ġinfrastructure', 'Ġn', 'irc', 'Ġmir', 'Ġfeature', 'Ġstar', 'light', 'blocking', 'Ġcoron', 'agraph', 'Ġobservation', 'Ġfaint', 'Ġtargets', 'Ġextras', 'olar', 'Ġplanets', 'Ġcircumst', 'ellar', 'Ġdisks', 'Ġclose', 'Ġbright', 'Ġstars', 'Ġspacecraft', 'Ġbus', 'Ġprimary', 'Ġsupport', 'Ġcomponent', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġhosting', 'Ġmultitude', 'Ġcomputing', 'Ġcommunication', 'Ġelectric', 'Ġpower', 'Ġpropulsion', 'Ġstructural', 'Ġparts', 'Ġalong', 'Ġsun', 'shield', 'Ġforms', 'Ġspacecraft', 'Ġelement', 'Ġspace', 'Ġtelescope', 'Ġspacecraft', 'Ġbus', 'Ġsun', 'facing', 'warm', 'Ġside', 'Ġsun', 'shield', 'Ġoperates', 'Ġtemperature', 'ĠÂ°', 'c', 'Ġstructure', 'Ġspacecraft', 'Ġbus', 'Ġmass', 'Ġmust', 'Ġsupport', 'Ġspace', 'Ġtelescope', 'Ġmade', 'Ġprimarily', 'Ġgraph', 'ite', 'Ġcomposite', 'Ġmaterial', 'Ġassembly', 'Ġcompleted', 'Ġcal', 'ornia', 'Ġintegrated', 'Ġrest', 'Ġspace', 'Ġtelescope', 'Ġleading', 'Ġspacecraft', 'Ġbus', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġdiagram', 'Ġspacecraft', 'Ġbus', 'Ġsolar', 'Ġpanel', 'Ġgreen', 'Ġlight', 'Ġpurple', 'Ġpanels', 'Ġradi', 'ators', 'Ġcomparison', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġprimary', 'Ġmirror', 'Ġlaunch', 'Ġspacecraft', 'Ġbus', 'Ġrotate', 'Ġtelescope', 'Ġpointing', 'Ġprecision', 'Ġone', 'Ġarc', 'second', 'Ġisol', 'ates', 'Ġvibration', 'Ġtwo', 'Ġweb', 'b', 'Ġtwo', 'Ġpairs', 'Ġrocket', 'Ġengines', 'one', 'Ġpair', 'Ġredundancy', 'Ġmake', 'Ġcourse', 'Ġcorrections', 'Ġway', 'Ġstation', 'Ġkeeping', 'Ġmaintaining', 'Ġcorrect', 'Ġposition', 'Ġh', 'alo', 'Ġorbit', 'Ġeight', 'Ġsmaller', 'Ġthr', 'usters', 'Ġused', 'Ġattitude', 'Ġcontrol', 'Ġcorrect', 'Ġpointing', 'Ġspacecraft', 'Ġengines', 'Ġuse', 'Ġhyd', 'raz', 'ine', 'Ġfuel', 'Ġlit', 'ers', 'Ġu', 'Ġgallons', 'Ġlaunch', 'init', 'rogen', 'Ġtet', 'rox', 'ide', 'Ġoxid', 'izer', 'Ġlit', 'ers', 'Ġu', 'Ġgallons', 'Ġlaunch', ').[', 'Ġweb', 'b', 'Ġintended', 'Ġserv', 'iced', 'Ġspace', 'Ġcrew', 'ed', 'Ġmission', 'Ġrepair', 'Ġupgrade', 'Ġobserv', 'atory', 'Ġdone', 'Ġhub', 'ble', 'Ġwould', 'Ġcurrently', 'Ġpossible', 'Ġaccording', 'Ġn']</t>
+          <t>['Ġretrieved', 'Ġfe', 'b', 'ruary', 'technical', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ally', 'Ġsolar', 'Ġsystem', 'Ġobservations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġorbit', 'Ġes', 'ign', 'orbit', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġaug', 'ust', 'Ġsun', 'shield', 'Ġn', 'asa', 'gov', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdra', 'ke', 'Ġn', 'adia', 'Ġapr', 'il', 'hub', 'ble', 'Ġstill', 'Ġw', 'ows', 'Ġwait', 'Ġtill', 'Ġsee', "'s", 'Ġnext', 'http', 'Ġnational', 'Ġgeographic', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġapr', 'il', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'sun', 'shield', 'Ġcoat', 'ings', 'Ġweb', 'b', 'n', 'asa', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġcl', 'ery', 'aniel', 'Ġmarch', 'n', 'asa', 'Ġannounces', 'Ġdelays', 'Ġgiant', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġmor', 'ring', 'Ġfrank', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġsun', 'sh', 'ade', 'Ġfolding', 'Ġdeployment', 'Ġtest', 'av', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġpp', 'âĢĵ', 'Ġiss', 'n', 'Ġ000', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġfisher', 'Ġal', 'ise', 'Ġde', 'cember', 'bb', 'Ġready', 'Ġsun', 'shield', 'Ġdeployment', 'Ġcooldown', 'http', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġn']</t>
         </is>
       </c>
       <c r="C307" t="n">
@@ -4429,7 +4429,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>['asa', 'Ġassociate', 'Ġadministrator', 'Ġth', 'omas', 'Ġz', 'urb', 'uc', 'hen', 'Ġdespite', 'Ġbest', 'Ġefforts', 'Ġunc', 'rew', 'ed', 'Ġremote', 'Ġmission', 'Ġfound', 'Ġbeyond', 'Ġcurrent', 'Ġtechnology', 'Ġtime', 'Ġweb', 'b', 'Ġdesigned', 'Ġlong', 'Ġweb', 'b', 'Ġtesting', 'Ġperiod', 'Ġn', 'asa', 'Ġofficials', 'Ġreferred', 'Ġidea', 'Ġservicing', 'Ġmission', 'Ġplans', 'Ġannounced', 'Ġsince', 'Ġsuccessful', 'Ġlaunch', 'Ġn', 'asa', 'Ġstated', 'Ġnevertheless', 'Ġlimited', 'Ġaccommodation', 'Ġmade', 'Ġfacilitate', 'Ġfuture', 'Ġservicing', 'Ġmissions', 'Ġaccommodations', 'Ġincluded', 'Ġprecise', 'Ġguidance', 'Ġmarkers', 'Ġform', 'Ġcrosses', 'Ġsurface', 'Ġweb', 'b', 'Ġuse', 'Ġremote', 'Ġservicing', 'Ġmissions', 'Ġwell', 'Ġrefill', 'able', 'Ġfuel', 'Ġtanks', 'Ġremovable', 'Ġheat', 'Ġprotect', 'ors', 'Ġaccessible', 'Ġattachment', 'Ġpoints', 'Ġil', 'ana', 'vs', 'ky', 'Ġv', 'ick', 'Ġbal', 'z', 'ano', 'Ġwrite', 'Ġweb', 'b', 'Ġuses', 'Ġmodified', 'Ġversion', 'Ġjavascript', 'Ġcalled', 'Ġn', 'omb', 'Ġscript', 'e', 'ase', '00', 'e', 'Ġoperations', 'Ġfollows', 'Ġec', 'ascript', 'Ġstandard', 'allows', 'Ġmodular', 'Ġdesign', 'Ġflow', 'board', 'Ġscripts', 'Ġcall', 'Ġlower', 'level', 'Ġscripts', 'Ġdefined', 'Ġfunctions', '".', 'Ġj', 'w', 'st', 'Ġscience', 'Ġoperations', 'Ġdriven', 'instead', 'Ġbinary', 'Ġcommand', 'Ġblocks', 'board', 'Ġscripts', 'Ġwritten', 'Ġcustomized', 'Ġversion', 'Ġjavascript', 'Ġscript', 'Ġinterpreter', 'Ġrun', 'Ġflight', 'Ġsoftware', 'Ġwritten', 'Ġprogramming', 'Ġlanguage', 'Ġc', '++', 'Ġflight', 'Ġsoftware', 'Ġoperates', 'Ġspacecraft', 'Ġscience', 'Ġdesire', 'Ġlarge', 'Ġinfrared', 'Ġspace', 'Ġtelescope', 'Ġtraces', 'Ġback', 'Ġdecades', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġinfrared', 'Ġtelescope', 'Ġfacility', 'later', 'Ġcalled', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'Ġplanned', 'Ġspace', 'Ġshuttle', 'Ġdevelopment', 'Ġpotential', 'Ġinfrared', 'Ġastronomy', 'Ġacknowledged', 'Ġtime', 'Ġunlike', 'Ġground', 'Ġtelescopes', 'Ġspace', 'Ġobserv', 'atories', 'Ġfree', 'Ġatmospheric', 'Ġabsorption', 'Ġinfrared', 'Ġlight', 'Ġspace', 'Ġobserv', 'atories', 'Ġopened', 'new', 'Ġastronomers', 'Ġservicing', 'Ġsoftware', 'Ġcomparison', 'Ġtelescopes', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġprimary', 'Ġmirror', 'Ġsize', 'Ġcomparison', 'Ġweb', 'b', 'Ġhub', 'ble', 'Ġten', 'uous', 'Ġatmosphere', 'Ġnominal', 'Ġflight', 'Ġaltitude', 'Ġmeasurable', 'Ġabsorption', 'Ġdetectors', 'Ġoperating', 'Ġwavelengths', 'ĠÂµ', 'ĠÂµ', 'Ġachieve', 'Ġhigh', 'Ġradi', 'ometric', 'Ġsensitivity', 'Ġg', 'cc', 'arthy', 'Ġg', 'Ġw', 'Ġaut', 'io', 'Ġhowever', 'Ġinfrared', 'Ġtelescopes', 'Ġdisadvantage', 'Ġneed', 'Ġstay', 'Ġextremely', 'Ġcold', 'Ġlonger']</t>
+          <t>['Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġwave', 'front', 'Ġsensing', 'Ġcontrol', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'ke', 'ck', 'Ġke', 'ck', 'Ġtelescopes', 'Ġn', 'Ġw', 'Ġke', 'ck', 'Ġobserv', 'atory', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'uly', 'Ġmall', 'one', 'e', 'Ġl', 'aura', 'Ġoct', 'ober', 'n', 'asa', "'s", 'Ġbiggest', 'Ġtelescope', 'Ġever', 'Ġprepares', 'Ġlaunch', 'Ġwired', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'mir', 'ror', 'Ġmirror', 'âĢ¦', 'Ġway', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'j', 'w', 'st', 'Ġmirrors', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'os', 'Ġj', 'athan', 'Ġmarch', 'j', 'ames', 'Ġweb', 'b', 'fully', 'Ġfocused', 'Ġtelescope', 'Ġbeats', 'Ġexpectations', 'ht', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'j', 'w', 'st', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', ')"', 'Ġn', 'asa', 'Ġarchived', 'Ġl', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġnear', 'Ġinfrared', 'Ġcamera', 'Ġst', 'sci', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'n', 'irc', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġuniversity', 'ri', 'zona', 'Ġarchived', 'Ġ', 'iz', 'ona', 'edu', 'n', 'irc', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'j', 'w', 'st', 'Ġcurrent', 'Ġstatus', 'Ġview', 'status', 'html', 'Ġst', 'sci', 'Ġarchived', 'Ġoriginal', 'Ġl', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'nir', 'spec', 'Ġnear', 'inf', 'rared', 'Ġspect', 'rog', 'raph', 'Ġj', 'w', 'st']</t>
         </is>
       </c>
       <c r="C308" t="n">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>['Ġwavelength', 'Ġinfrared', 'Ġcolder', 'Ġneed', 'Ġbackground', 'Ġheat', 'Ġdevice', 'Ġoverwhel', 'ms', 'Ġdetectors', 'Ġmaking', 'Ġeffectively', 'Ġblind', 'Ġovercome', 'Ġcareful', 'Ġspacecraft', 'Ġdesign', 'Ġparticular', 'Ġplacing', 'Ġtelescope', 'Ġde', 'war', 'Ġextremely', 'Ġcold', 'Ġsubstance', 'Ġliquid', 'Ġhelium', 'Ġcool', 'ant', 'Ġslowly', 'Ġvapor', 'ize', 'Ġlimiting', 'Ġlifetime', 'Ġinstrument', 'Ġshort', 'Ġmonths', 'Ġyears', 'Ġcases', 'Ġpossible', 'Ġmaintain', 'Ġtemperature', 'Ġlow', 'Ġenough', 'Ġdesign', 'Ġspacecraft', 'Ġenable', 'Ġnear', 'inf', 'rared', 'Ġobservations', 'Ġwithout', 'Ġsupply', 'Ġcool', 'ant', 'Ġextended', 'Ġmissions', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'Ġwide', 'field', 'Ġinfrared', 'Ġsurvey', 'Ġexplorer', 'Ġoperated', 'Ġreduced', 'Ġcapacity', 'Ġcool', 'ant', 'Ġdepletion', 'Ġanother', 'Ġexample', 'Ġhub', 'ble', "'s", 'Ġnear', 'Ġinfrared', 'Ġcamera', 'Ġmulti', 'object', 'Ġspect', 'rom', 'eter', 'nic', 'mos', 'Ġinstrument', 'Ġstarted', 'Ġusing', 'Ġblock', 'Ġnitrogen', 'Ġice', 'Ġdepleted', 'Ġcouple', 'Ġyears', 'Ġreplaced', 'Ġsts', 'Ġservicing', 'Ġmission', 'Ġcry', 'oc', 'ool', 'er', 'Ġworked', 'Ġcontinuously', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdesigned', 'Ġcool', 'Ġwithout', 'Ġde', 'war', 'Ġusing', 'Ġcombination', 'Ġsun', 'shield', 'Ġradi', 'ators', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'Ġusing', 'Ġadditional', 'Ġcry', 'oc', 'ool', 'er', 'Ġselected', 'Ġspace', 'Ġtelescopes', 'Ġinstruments', 'Ġname', 'Ġlaunch', 'Ġyear', 'Ġwavelength', 'Î¼', 'Ġaperture', 'Ġcooling', 'Ġspac', 'el', 'ab', 'Ġinfrared', 'Ġtelescope', 'irt', 'âĢĵ', 'Ġhelium', 'Ġinfrared', 'Ġspace', 'Ġobserv', 'atory', 'âĢĵ', 'Ġhelium', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġimaging', 'Ġspect', 'rog', 'raph', 'st', 'âĢĵ', '03', 'Ġpassive', 'Ġhub', 'ble', 'Ġnear', 'Ġinfrared', 'Ġcamera', 'Ġmulti', 'object', 'Ġspect', 'rom', 'eter', 'nic', 'mos', 'âĢĵ', 'Ġnitrogen', 'Ġlater', 'Ġcry', 'oc', 'ool', 'er', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'âĢĵ', 'Ġhelium', 'Ġhub', 'ble', 'Ġwide', 'Ġfield', 'Ġcamera', 'âĢĵ', 'Ġpassive', 'Ġtherm', 'oe', 'lect', 'ric', 'sc', 'hel', 'Ġspace', 'Ġobserv', 'atory', 'âĢĵ', 'Ġhelium', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'âĢĵ', 'Ġpassive', 'Ġcry', 'oc', 'ool', 'er', 'mir']</t>
+          <t>['Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'web', 'arch', 'Ġh', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'mir', 'Ġspect', 'rom', 'eter', 'Ġng', 'st', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'j', 'w', 'st', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'mir', ')"', 'Ġn', 'asa', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'j', 'w', 'st', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbanks', 'Ġk', 'im', 'ber', 'ly', 'Ġl', 'arson', 'Ġmel', 'ora', 'Ġay', 'mer', 'gen', 'Ġc', 'ag', 'ay', 'Ġz', 'hang', 'Ġb', 'urt', 'Ġangel', 'Ġge', 'orge', 'Ġz', '.;', 'Ġcull', 'um', 'Ġmart', 'Ġj', 'eds', '.).', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'Ġcooler', 'Ġsystems', 'Ġengineering', 'Ġproceedings', 'Ġsp', 'ie', 'Ġmodeling', 'Ġsystems', 'Ġengineering', 'Ġproject', 'Ġmanagement', 'Ġastronomy', '017', 'api', 'se', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fig', 'Ġcooler', 'Ġarchitecture', 'Ġoverview', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'j', 'w', 'st', 'Ġready', 'Ġlaunch', 'Ġamazing', 'Ġscience', 'Ġplanetary', 'Ġsociety', 'Ġretrieved', 'Ġaug', 'ust', 'yon', 'Ġren', 'Ã©', 'Ġh', 'utch', 'ings', 'Ġjohn', 'Ġb', '.;', 'aul', 'ieu', 'Ġmath', 'ilde', 'Ġal', 'bert', 'Ġlo', 'ic', 'Ġl', 'af', 'ren', 'Ã¨re', 'Ġdavid', 'ott', 'Ġch', 'ris', 'Ġtou', 'ah', 'ri', 'Ġdr', 'iss', 'Ġrow', 'lands', 'Ġne', 'il', 'Ġmic', 'al', 'Ġfull', 'erton', 'lex', 'Ġw', '.;', 'Ġvol', 'k', 'Ġke', 'vin', 'Ġmart', 'el', 'rÃ©', 'Ġr', '.;', 'Ġch', 'ayer', 'Ġpier', 'iv', 'aram', 'ak', 'rish', 'nan', 'Ġab', 'raham', 'Ġro', 'berto', 'Ġfer', 'ra', 'se', 'Ġl', 'aura', 'Ġj', 'ay', 'aw', 'ard', 'h', 'ana', 'Ġray', 'Ġjohn', 'stone', 'Ġdou', 'g', 'yer', 'ichael', 'Ġpip']</t>
         </is>
       </c>
       <c r="C309" t="n">
@@ -4455,7 +4455,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>['Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmajor', 'Ġmilestones', 'Ġyear', 'Ġmilestone', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġproject', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġproposed', 'mir', 'ror', 'Ġsize', 'Ġnexus', 'Ġspace', 'Ġtelescope', 'Ġprecursor', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġcancelled', 'Ġproposed', 'Ġproject', 'Ġrenamed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'mir', 'ror', 'Ġsize', 'Ġreduced', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġawarded', 'Ġcontract', 'Ġbuild', 'Ġtelescope', 'Ġmemorandum', 'Ġunderstanding', 'Ġsigned', 'Ġn', 'asa', 'Ġmission', 'Ġcritical', 'Ġdesign', 'Ġreview', 'Ġpassed', 'Ġproposed', 'Ġcancellation', 'Ġfinal', 'Ġassembly', 'Ġcompleted', 'Ġde', 'cember', 'Ġlaunch', 'Ġweb', 'b', "'s", 'Ġdelays', 'Ġcost', 'Ġincreases', 'Ġcompared', 'Ġpredecessor', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġhub', 'ble', 'Ġformally', 'Ġstarted', 'Ġestimated', 'Ġdevelopment', 'Ġcost', 'Ġus', 'Ġmillion', 'equ', 'ivalent', '09', '000', 'Ġtime', 'Ġsent', 'Ġorbit', 'Ġcost', 'Ġfour', 'Ġtimes', 'Ġaddition', 'Ġnew', 'Ġinstruments', 'Ġservicing', 'Ġmissions', 'Ġincreased', 'Ġcost', 'Ġleast', 'Ġbillion', 'equ', 'ivalent', '000', 'Ġdiscussions', 'Ġhub', 'ble', 'Ġfollow', 'Ġstarted', 'Ġserious', 'Ġplanning', 'Ġbegan', 'Ġearly', 'Ġhi', 'z', 'Ġtelescope', 'Ġconcept', 'Ġdeveloped', ':[', 'Ġfully', 'Ġbaffled', 'b', 'Ġft', 'Ġaperture', 'Ġinfrared', 'Ġtelescope', 'Ġwould', 'Ġrec', 'ede', 'Ġorbit', 'Ġastronomical', 'Ġunit', 'Ġdistant', 'Ġorbit', 'Ġwould', 'Ġbenefited', 'Ġreduced', 'Ġlight', 'Ġnoise', 'Ġz', 'odiac', 'al', 'Ġearly', 'Ġplans', 'Ġcalled', 'Ġnexus', 'Ġprecursor', 'Ġtelescope', 'Ġmission', 'Ġcorrecting', 'Ġflawed', 'Ġoptics', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'h', 'st', 'Ġfirst', 'Ġyears', 'Ġplayed', 'Ġsignificant', 'Ġrole', 'Ġbirth', 'Ġweb', 'b', 'Ġn', 'asa', 'Ġconducted', 'Ġspace', 'Ġshuttle', 'Ġmission', 'Ġreplaced', 'Ġh', 'st', "'s", 'Ġcamera', 'Ġinstalled', 'Ġretro', 'fit', 'Ġimaging', 'Ġspect', 'rog', 'raph', 'Ġcompensate', 'Ġspherical', 'Ġaber', 'ration', 'Ġprimary', 'Ġmirror', 'Ġh', 'st', 'Ġbeyond', 'Ġcommittee', 'Ġformed', 'Ġstudy', 'Ġpossible', 'Ġmissions', 'Ġprograms', 'Ġoptical', 'ult', 'raviolet', 'Ġastronomy', 'Ġspace', 'Ġfirst', 'Ġdecades', 'st', 'Ġcentury', '."[', 'Ġembold', 'ened', 'Ġh', 'st', "'s", 'Ġsuccess', 'Ġreport', 'Ġexplored', 'Ġconcept', 'Ġlarger', 'Ġmuch', 'Ġcolder', 'Ġinfrared', 'sensitive', 'Ġtelescope', 'Ġcould', 'Ġreach', 'Ġback', 'Ġcosmic', 'Ġtime', 'Ġbirth', 'Ġfirst', 'Ġgalaxies', 'Ġhigh']</t>
+          <t>['Ġjud', 'ith', 'Ġl', '.;', 'Ġsaw', 'ick', 'Ġmar', 'cin', 'Ġaug', 'ust', 'Ġclamp', 'Ġmark', 'Ġc', 'Ġf', 'az', 'io', 'Ġg', 'iov', 'anni', 'Ġg', 'Ġmac', 'ew', 'en', 'ard', 'sch', 'mann', 'Ġj', 'ac', 'ob', 'us', 'eds', '.).', 'Ġj', 'w', 'st', 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġnear', 'inf', 'rared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'nir', 'iss', '".', 'Ġproceedings', 'Ġsp', 'ie', 'Ġspace', 'Ġtelescopes', 'Ġinstrument', 'ation', 'Ġoptical', 'Ġinfrared', 'Ġmill', 'imeter', 'Ġwave', 'r', 'ui', 'Ġf', 'Ġfeatures', 'Ġtwo', 'Ġmodules', 'Ġinfrared', 'Ġcamera', 'Ġdedicated', 'Ġï', '¬', 'ģ', 'ne', 'Ġguiding', 'Ġobserv', 'atory', 'Ġscience', 'Ġcamera', 'Ġmodule', 'Ġnear', 'inf', 'rared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'nir', 'iss', ')"', 'Ġspacecraft', 'Ġbus', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'w', 'st', 'Ġobserv', 'atory', 'Ġn', 'asa', 'Ġarchived', 'w', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġobserv', 'atory', 'Ġspace', 'based', 'Ġportion', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsystem', 'Ġcomprised', 'Ġthree', 'Ġelements', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'ote', 'Ġincludes', 'Ġmirrors', 'Ġback', 'plane', 'Ġspacecraft', 'Ġelement', 'Ġincludes', 'Ġspacecraft', 'Ġbus', 'Ġsun', 'shield', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'integ', 'rated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', ')"', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ough', 'Ġsc', 'ott', 'Ġp', 'f', 'eb', 'ruary', 'prime', 'Ġuntold', 'Ġstory', 'Ġn', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsat', 'mag', 'azine', 'Ġsat', 'news', 'Ġarchived', 'Ġu', 'mber', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'Ġsl', 'oan', 'Ġje', 'ff']</t>
         </is>
       </c>
       <c r="C310" t="n">
@@ -4468,7 +4468,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>['priority', 'Ġscience', 'Ġgoal', 'Ġbeyond', 'Ġh', 'st', "'s", 'Ġcapability', 'Ġwarm', 'Ġtelescope', 'Ġblinded', 'Ġinfrared', 'Ġemission', 'Ġoptical', 'Ġsystem', 'Ġaddition', 'Ġrecommendations', 'Ġextend', 'Ġh', 'st', 'Ġmission', 'Ġdevelop', 'Ġtechnologies', 'Ġfinding', 'Ġplanets', 'Ġaround', 'Ġstars', 'Ġn', 'asa', 'Ġembraced', 'Ġchief', 'Ġrecommendation', 'Ġh', 'st', 'Ġbeyond', 'Ġlarge', 'Ġcold', 'Ġspace', 'Ġtelescope', 'rad', 'atively', 'Ġcooled', 'Ġfar', 'ĠÂ°', 'c', 'Ġbegan', 'Ġplanning', 'Ġprocess', 'Ġfuture', 'Ġweb', 'b', 'Ġtelescope', 'Ġdevelopment', 'Ġhistory', 'Ġbackground', 'development', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġearly', 'Ġfull', 'scale', 'Ġmodel', 'Ġdisplay', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġpreparation', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġdec', 'adal', 'Ġsurvey', 'Ġliterature', 'Ġreview', 'Ġproduced', 'Ġunited', 'Ġstates', 'Ġnational', 'Ġresearch', 'Ġcouncil', 'Ġincludes', 'Ġidentifying', 'Ġresearch', 'Ġpriorities', 'Ġmaking', 'Ġrecommendations', 'Ġupcoming', 'Ġdecade', 'Ġincluded', 'Ġdevelopment', 'Ġscientific', 'Ġprogram', 'Ġbecame', 'Ġknown', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġadvancements', 'Ġrelevant', 'Ġtechnologies', 'Ġn', 'asa', 'Ġmatured', 'Ġstudying', 'Ġbirth', 'Ġgalaxies', 'Ġyoung', 'Ġuniverse', 'Ġsearching', 'Ġplanets', 'Ġaround', 'Ġstars', 'Ġprime', 'Ġgoals', 'Ġcoales', 'ced', 'orig', 'ins', 'Ġh', 'st', 'Ġbeyond', 'Ġbecame', 'Ġprominent', 'Ġhoped', 'Ġng', 'st', 'Ġreceived', 'Ġhighest', 'Ġranking', 'Ġdec', 'adal', 'Ġsurvey', 'Ġadministrator', 'Ġn', 'asa', 'Ġdan', 'Ġgold', 'Ġcoined', 'Ġphrase', 'f', 'aster', 'Ġbetter', 'Ġcheaper', '",', 'Ġopted', 'Ġnext', 'Ġbig', 'Ġparadigm', 'Ġshift', 'Ġastronomy', 'Ġnamely', 'Ġbreaking', 'Ġbarrier', 'Ġsingle', 'Ġmirror', 'Ġmeant', 'Ġgoing', 'el', 'im', 'inate', 'Ġmoving', 'Ġparts', 'learn', 'Ġlive', 'Ġmoving', 'Ġparts', 'e', 'Ġsegment', 'ed', 'Ġoptics', 'Ġgoal', 'Ġreduce', 'Ġmass', 'Ġdensity', 'Ġten', 'fold', 'Ġsilicon', 'Ġcarb', 'ide', 'Ġthin', 'Ġlayer', 'Ġglass', 'Ġtop', 'Ġfirst', 'Ġlooked', 'Ġb', 'ery', 'ium', 'Ġselected', 'Ġmid', 'Ġera', 'f', 'aster', 'Ġbetter', 'Ġcheaper', 'Ġproduced', 'Ġng', 'st', 'Ġconcept', 'Ġft', 'Ġaperture', 'Ġflown', 'Ġroughly', 'Ġestimated', 'Ġcost', 'Ġus', 'Ġmillion', 'Ġn', 'asa', 'Ġworked', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġconduct', 'Ġtechnical', 'Ġrequirement', 'Ġcost', 'Ġstudies', 'Ġthree', 'Ġdifferent', 'Ġconcepts', 'Ġselected', 'Ġlock', 'heed']</t>
+          <t>['Ġoct', 'ober', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġspacecraft', 'Ġinches', 'Ġtowards', 'Ġfull', 'Ġassembly', 'Ġcompos', 'ites', 'Ġworld', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġpropulsion', 'prop', 'ulsion', 'Ġj', 'w', 'st', 'Ġuser', 'Ġdocumentation', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'mber', 'n', 'asa', 'Ġgives', 'Ġgreen', 'Ġlight', 'Ġfuel', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġce', 'tel', 'esc', 'ope', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġweb', 'b', 'Ġservice', 'able', 'Ġlike', 'Ġhub', 'ble', '?"', 'Ġ', 'erv', 'ice', 'able', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'rel', 'ief', 'Ġn', 'asa', "'s", 'Ġpowerful', 'Ġspace', 'Ġtelescope', 'Ġï', '¬', 'ģ', 'n', 'ishes', 'Ġrisky', 'Ġunfolding', 'Ġng', 'Ġscience', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġsm', 'ith', 'Ġmar', 'cia', 'Ġaug', 'ust', 'z', 'urb', 'uc', 'hen', 'Ġtaking', 'Ġone', 'Ġlast', 'Ġlook', 'Ġj', 'w', 'st', 'Ġservicing', 'Ġcompat', 'ibl', 'ity', 'sic', ']"', 'Ġv', 'icing', 'Ġspac', 'ep', 'olic', 'yon', 'line', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'scient', 'ists', 'Ġengineers', 'Ġpush', 'Ġservicing', 'Ġassembly', 'Ġfuture', 'Ġspace', 'Ġobserv', 'atories', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġce', 'ob', 'serv', 'atories', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġtransform', 'Ġï', '¬', 'ģ', 'n', 'al', 'Ġform', 'Ġverge', 'Ġarchived', 'Ġoy', 'ment', 'sequence', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'vs', 'ky', 'Ġil', 'ana', 'Ġbal', 'z', 'ano', 'Ġv', 'ick', 'j', 'w', 'st', 'Ġmaximizing', 'Ġe', 'f', 'ï']</t>
         </is>
       </c>
       <c r="C311" t="n">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>['Ġmart', 'Ġtr', 'w', 'Ġpreliminary', 'Ġconcept', 'Ġstudies', 'Ġlaunch', 'Ġtime', 'Ġplanned', 'Ġlaunch', 'Ġdate', 'Ġpushed', 'Ġback', 'Ġmany', 'Ġtimes', 'see', 'Ġtable', 'Ġproject', 'Ġrenamed', 'Ġn', 'asa', "'s", 'Ġsecond', 'Ġadministrator', 'âĢĵ', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', '06', 'âĢĵ', ').[', 'Ġweb', 'b', 'Ġled', 'Ġagency', 'Ġap', 'ollo', 'Ġprogram', 'Ġestablished', 'Ġscientific', 'Ġresearch', 'Ġcore', 'Ġn', 'asa', 'Ġactivity', 'Ġn', 'asa', 'Ġawarded', 'Ġtr', 'w', 'Ġus', 'Ġmillion', 'Ġprime', 'Ġcontract', 'Ġweb', 'b', 'Ġdesign', 'Ġcalled', 'Ġde', 'sc', 'oped', 'Ġft', 'Ġprimary', 'Ġmirror', 'Ġlaunch', 'Ġdate', 'Ġlater', 'Ġyear', 'Ġtr', 'w', 'Ġacquired', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġhostile', 'Ġbid', 'Ġbecame', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġtechnology', 'Ġdevelopment', 'Ġmanaged', 'Ġn', 'asa', "'s", 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġgreen', 'belt', 'ary', 'land', 'Ġjohn', 'Ġc', 'ather', 'Ġproject', 'Ġscientist', 'Ġprimary', 'Ġcontractor', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġaerospace', 'Ġsystems', 'Ġresponsible', 'Ġdeveloping', 'Ġbuilding', 'Ġspacecraft', 'Ġelement', 'Ġincluded', 'Ġsatellite', 'Ġbus', 'Ġsun', 'shield', 'Ġdeploy', 'able', 'Ġtower', 'Ġassembly', 'ta', 'Ġconnects', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'Ġspacecraft', 'Ġbus', 'Ġmid', 'Ġboom', 'Ġassembly', 'mb', 'Ġhelps', 'Ġdeploy', 'Ġlarge', 'Ġsun', 'shield', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġsub', 'cont', 'racted', 'Ġdevelop', 'Ġbuild', 'te', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', ').[', 'Ġcost', 'Ġgrowth', 'Ġrevealed', 'Ġspring', 'Ġled', 'Ġaug', 'ust', 'plan', 'ning', 'Ġprimary', 'Ġtechnical', 'Ġoutcomes', 'plan', 'ning', 'Ġsignificant', 'Ġchanges', 'Ġintegration', 'Ġtest', 'Ġplans', 'month', 'Ġlaunch', 'Ġdelay', 'Ġelimination', 'Ġsystem', 'level', 'Ġtesting', 'Ġobserv', 'atory', 'Ġmodes', 'Ġearly', 'Ġdevelopment', 'Ġrepl', 'ning', 'âĢĵ', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġj', 'w', 'st', 'Ġmirror', 'Ġsegment', 'Ġmirror', 'Ġsegments', 'Ġundergoing', 'Ġcry', 'ogenic', 'Ġtests', 'Ġx', 'ray', 'Ġcry', 'ogenic', 'Ġfacility', 'Ġmarsh', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġassembled', 'Ġtelescope', 'Ġfollowing', 'Ġenvironmental', 'Ġtesting', 'Ġwavelength', 'Ġshorter', 'ĠÂµ', 'Ġmajor', 'Ġfeatures', 'Ġobserv', 'atory', 'Ġunchanged', 'Ġfollowing', 'plan', 'ning']</t>
+          <t>['¬', 'ģ', 'ci', 'ency', 'Ġminimizing', 'Ġground', 'Ġsystems', 'Ġinternational', 'Ġsym', 'posium', 'Ġreducing', 'Ġcosts', 'Ġspacecraft', 'Ġground', 'Ġsystems', 'Ġoperations', 'Ġproceedings', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġgreenhouse', 'Ġmatt', 'hew', 'Ġstatus', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'Ġsystem', 'report', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'cc', 'arthy', 'Ġg', '.;', 'Ġaut', 'io', 'Ġg', 'Ġw', 'Ġinfrared', 'Ġdetector', 'Ġperformance', 'Ġshuttle', 'Ġinfrared', 'Ġtelescope', 'Ġfacility', 'irt', 'f', 'Ġlos', 'Ġangel', 'es', 'Ġtechnical', 'Ġsym', 'posium', 'Ġutilization', 'Ġinfrared', 'Ġdetectors', 'Ġvol', 'Ġsociety', 'Ġphotographic', 'Ġinstrument', 'ation', 'Ġengineers', 'Ġpp', 'âĢĵ', 'ui', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġcold', 'Ġgo', 'Ġcooler', 'Ġtested', 'Ġn', 'asa', 'Ġtelescope', 'Ġphys', 'org', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'sc', 'hel', 'Ġspace', 'Ġobserv', 'atory', 'Ġrelated', 'Ġmissions', 'sh', 'tml', 'Ġn', 'asa', 'Ġjet', 'Ġpropulsion', 'Ġlaboratory', 'Ġgodd', 'ard', 'Ġflight', 'Ġcenter', 'Ġcal', 'ornia', 'Ġinstitute', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġiso', '?"', 'Ġes', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'hub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġwide', 'Ġfield', 'Ġcamera', 'Ġn', 'asa', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ich', 'hardt', 'ony', 'arch', 'us', 'Ġastronomy', 'Ġnext', 'Ġbig', 'Ġthing', 'Ġbig', '?"', 'f', '01', 'Ġnature', '):', 'âĢĵ', 'ui', 'ads', 'abs', 'Ġdoi', '01']</t>
         </is>
       </c>
       <c r="C312" t="n">
@@ -4494,7 +4494,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>['Ġproject', 'Ġindependently', 'Ġreviewed', 'Ġapr', 'il', 'plan', 'Ġlife', 'cycle', 'Ġcost', 'Ġproject', 'Ġestimated', 'Ġbillion', 'Ġcomprised', 'Ġapproximately', 'Ġbillion', 'Ġdesign', 'Ġdevelopment', 'Ġlaunch', 'Ġcommission', 'ing', 'Ġapproximately', 'Ġus', 'Ġbillion', 'Ġten', 'Ġyears', 'Ġoperations', 'Ġes', 'Ġagreed', 'Ġcontributing', 'ĠâĤ¬', 'Ġmillion', 'Ġincluding', 'Ġlaunch', 'adian', 'Ġspace', 'Ġagency', 'Ġpledged', 'Ġmillion', 'Ġdelivered', 'Ġcontributions', 'Ġequipment', 'Ġpoint', 'Ġtelescope', 'Ġdetect', 'Ġatmospheric', 'Ġconditions', 'Ġdistant', 'Ġplanets', 'Ġjan', 'uary', 'Ġnine', 'Ġten', 'Ġtechnology', 'Ġdevelopment', 'Ġitems', 'Ġproject', 'Ġsuccessfully', 'Ġpassed', 'Ġnon', 'adv', 'ocate', 'Ġreview', 'Ġtechnologies', 'Ġdeemed', 'Ġsufficiently', 'Ġmature', 'Ġretire', 'Ġsignificant', 'Ġrisks', 'Ġproject', 'Ġremaining', 'Ġtechnology', 'Ġdevelopment', 'Ġitem', 'Ġmir', 'Ġcry', 'oc', 'ool', 'er', 'Ġcompleted', 'Ġtechnology', 'aturation', 'Ġmilestone', 'Ġapr', 'il', 'Ġtechnology', 'Ġreview', 'Ġrepresented', 'Ġbeginning', 'Ġstep', 'Ġprocess', 'Ġultimately', 'Ġmoved', 'Ġproject', 'Ġdetailed', 'Ġdesign', 'Ġphase', 'phase', 'Ġc', 'Ġmay', 'Ġcosts', 'Ġstill', 'Ġtarget', 'Ġmarch', 'Ġproject', 'Ġsuccessfully', 'Ġcompleted', 'Ġpreliminary', 'Ġdesign', 'Ġreview', 'Ġapr', 'il', 'Ġproject', 'Ġpassed', 'Ġnon', 'adv', 'ocate', 'Ġreview', 'Ġpassed', 'Ġreviews', 'Ġinclude', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'Ġreview', 'Ġmarch', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'Ġreview', 'Ġcompleted', 'Ġoct', 'ober', 'Ġsun', 'shield', 'Ġreview', 'Ġcompleted', 'Ġjan', 'uary', 'Ġapr', 'il', 'Ġtelescope', 'Ġpassed', 'Ġtechnical', 'Ġportion', 'Ġmission', 'Ġcritical', 'Ġdesign', 'Ġreview', 'Ġpassing', 'Ġsign', 'ified', 'Ġintegrated', 'Ġobserv', 'atory', 'Ġmeet', 'Ġscience', 'Ġengineering', 'Ġrequirements', 'Ġmission', 'Ġencomp', 'assed', 'Ġprevious', 'Ġdesign', 'Ġreviews', 'Ġproject', 'Ġschedule', 'Ġunderwent', 'Ġreview', 'Ġmonths', 'Ġfollowing', 'Ġprocess', 'Ġcalled', 'Ġindependent', 'Ġcomprehensive', 'Ġreview', 'Ġpanel', 'Ġled', 'plan', 'Ġmission', 'Ġaiming', 'Ġlaunch', 'Ġlate', 'Ġcost', 'runs', 'Ġimpacting', 'Ġprojects', 'Ġthough', 'Ġweb', 'b', 'Ġremained', 'Ġschedule', 'Ġweb', 'b', 'Ġproject', 'Ġfinal', 'Ġdesign', 'Ġfabrication', 'Ġphase', 'phase', 'Ġc', 'Ġassembly', 'Ġhex', 'agonal', 'Ġsegments', 'Ġprimary', 'Ġmirror', 'Ġdone', 'Ġvia', 'Ġrobotic', 'Ġarm', 'Ġbegan', 'mber', 'Ġcompleted', 'Ġfe', 'b', 'ruary', 'Ġsecondary', 'Ġmirror', 'Ġinstalled', 'Ġmarch']</t>
+          <t>['Ġpm', 'id', 'nexus', 'Ġspace', 'Ġtelescope', 'Ġmit', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġbrown', 'wayne', 'Ġbra', 'uk', 'us', 'ichael', 'n', 'asa', 'Ġn', 'asa', 'Ġes', 'Ġsign', 'Ġagreements', 'Ġfuture', 'Ġcooperation', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'Ġg', 'ur', 'Ġha', 'v', 'iv', 'tt', 'ig', 'Ġjan', 'uary', 'space', 'Ġchanging', 'Ġweb', 'b', 'Ġstart', 'Ġsays', 'Ġex', 'rael', 'Ġdawn', 'Ġtimes', 'rael', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'adv', 'anced', 'Ġconcepts', 'Ġstudies', 'Ġaperture', 'hi', 'z', 'Ġtelescope', 'Ġn', 'asa', 'Ġspace', 'Ġoptics', 'Ġmanufacturing', 'Ġtechnology', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'sts', 'ci', 'Ġj', 'w', 'st', 'Ġhistory', 'Ġarchived', 'Ġoriginal', 'Ġr', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġde', 'cember', 'ast', 'ron', 'Ġastroph', 'ysics', 'Ġnew', 'Ġmillennium', 'Ġ', 'xt', 'ng', 'st', 'htm', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġde', 'ck', 'liv', 'ier', 'Ġl', '.;', 'Ġmill', 'er', 'Ġdavid', 'Ġw', '.;', 'Ġmos', 'ier', 'Ġg', 'ary', 'Ġe', 'mult', 'idis', 'ciplinary', 'Ġanalysis', 'Ġnexus', 'Ġprecursor', 'Ġspace', 'Ġtelescope', 'Ġmac', 'ew', 'en', 'ard', 'ed', '.).', 'Ġhighly', 'Ġinnovative', 'Ġspace', 'Ġtelescope', 'Ġconcepts', 'Ġhighly', 'Ġinnovative', 'Ġspace', 'Ġtelescope', 'Ġconcepts', 'Ġvol', 'Ġp', 'Ġcites', 'eer', 'x', 'Ġ00', 'Ġarchived', 'w', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġbrown', 'Ġr', 'Ġpage', '03', 'Ġconf', '..', 'b', 'Ġscience', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', '03', 'h', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C313" t="n">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>['Ġfinal', 'Ġconstruction', 'Ġweb', 'b', 'Ġtelescope', 'Ġcompleted', 'mber', 'Ġextensive', 'Ġtesting', 'Ġprocedures', 'Ġbegan', 'Ġdetailed', 'Ġdesign', 'Ġconstruction', 'âĢĵ', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmarch', 'Ġn', 'asa', 'Ġdelayed', 'Ġweb', 'b', "'s", 'Ġlaunch', 'Ġadditional', 'Ġyears', 'Ġmay', 'Ġtelescope', "'s", 'Ġsun', 'shield', 'Ġripped', 'Ġpractice', 'Ġdeployment', 'Ġsun', 'shield', "'s", 'Ġcables', 'Ġsufficiently', 'Ġtighten', 'Ġj', 'une', 'Ġn', 'asa', 'Ġdelayed', 'Ġlaunch', 'Ġadditional', 'Ġmonths', 'Ġmarch', 'Ġbased', 'Ġassessment', 'Ġindependent', 'Ġreview', 'Ġboard', 'Ġconvened', 'Ġfailed', 'Ġmarch', 'Ġtest', 'Ġdeployment', 'Ġreview', 'Ġidentified', 'Ġweb', 'b', 'Ġlaunch', 'Ġdeployment', 'Ġpotential', 'Ġsingle', 'point', 'Ġfailures', 'Ġtasks', 'Ġalternative', 'Ġmeans', 'Ġrecovery', 'Ġunsuccessful', 'Ġtherefore', 'Ġsucceed', 'Ġtelescope', 'Ġwork', 'Ġaug', 'ust', 'Ġmechanical', 'Ġintegration', 'Ġtelescope', 'Ġcompleted', 'Ġsomething', 'Ġscheduled', 'Ġdone', 'Ġyears', 'Ġconstruction', 'Ġcompleted', 'Ġweb', 'b', 'Ġunderwent', 'Ġfinal', 'Ġtests', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġfactory', 'Ġred', 'ondo', 'Ġbeach', 'Ġcal', 'ornia', 'Ġship', 'Ġcarrying', 'Ġtelescope', 'Ġleft', 'Ġcal', 'ornia', 'Ġse', 'pt', 'ember', 'Ġpassed', 'Ġpan', 'ama', 'Ġcanal', 'Ġarrived', 'Ġfrench', 'Ġgu', 'iana', 'Ġoct', 'ober', 'Ġn', 'asa', "'s", 'Ġlifetime', 'Ġcost', 'Ġproject', 'Ġexpected', 'Ġbillion', 'Ġbillion', 'Ġspent', 'Ġspacecraft', 'Ġdesign', 'Ġdevelopment', 'Ġmillion', 'Ġplanned', 'Ġsupport', 'Ġfive', 'Ġyears', 'Ġmission', 'Ġoperations', 'Ġrepresentatives', 'Ġes', 'Ġc', 'sa', 'Ġstated', 'Ġproject', 'Ġcontributions', 'Ġamount', 'Ġapproximately', 'ĠâĤ¬', 'Ġmillion', 'Ġca', 'Ġmillion', 'Ġrespectively', 'Ġstudy', 'Ġspace', 'Ġscience', 'Ġboard', 'Ġestimated', 'Ġbuild', 'Ġnext', 'generation', 'Ġinfrared', 'Ġobserv', 'atory', 'Ġorbit', 'Ġwould', 'Ġcost', 'Ġbillion', 'Ġdollars', 'Ġdollars', ').[', 'Ġcame', 'Ġclose', 'Ġfinal', 'Ġcost', 'Ġweb', 'b', 'Ġfirst', 'Ġn', 'asa', 'Ġdesign', 'Ġconsidered', 'Ġlate', 'Ġmodest', 'Ġaiming', 'Ġbillion', 'Ġprice', 'Ġtag', 'Ġyears', 'Ġconstruction', 'Ġtime', 'Ġdesign', 'Ġexpanded', 'Ġadded', 'Ġfunding', 'Ġconting', 'encies', 'Ġscheduling', 'Ġdelays', 'Ġproject', 'Ġentered', 'Ġpreliminary', 'Ġdesign', 'Ġreview', 'Ġformally', 'Ġconfirmed', 'Ġconstruction', 'Ġbillion', 'Ġalready', 'Ġspent', 'Ġdeveloping', 'Ġtelescope']</t>
+          <t>['Ġjan', 'uary', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdress', 'ler', '.,', 'Ġed', 'expl', 'oration', 'Ġsearch', 'Ġorigins', 'Ġvision', 'Ġspace', 'Ġastronomy', 'Ġreport', 'h', 'st', 'Ġbeyond', 'Ġcommittee', 'Ġst', 'sci', 'edu', 'Ġassociation', 'Ġuniversities', 'Ġresearch', 'Ġastronomy', 'Ġarchived', 'Ġh', 'stand', 'yond', 'pdf', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġstock', 'man', 'Ġh', 'j', 'une', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġvisiting', 'Ġtime', 'Ġgalaxies', 'Ġyoung', '".', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġb', 'alt', 'imore', 'ary', 'land', 'Ġassociation', 'Ġuniversities', 'Ġresearch', 'Ġastronomy', 'Ġwashing', 'ton', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġsurvey', 'Ġcommittee', 'Ġboard', 'Ġphysics', 'Ġastronomy', 'Ġspace', 'Ġstudies', 'Ġboard', 'Ġcommission', 'Ġphysical', 'Ġsciences', 'Ġmathematics', 'Ġapplications', 'Ġnational', 'Ġresearch', 'Ġcouncil', 'Ġjan', 'uary', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġnew', 'Ġmillennium', 'n', 'ap', 'e', 'Ġdu', 'cat', 'alog', 'Ġwashing', 'ton', 'Ġnational', 'Ġacad', 'emies', 'Ġpress', 'Ġdoi', 'doi', 'Ġg', 'f', '070', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'sts', 'ci', 'Ġj', 'w', 'st', 'Ġhistory', 'Ġst', 'sci', 'edu', 'Ġarchived', 'Ġoriginal', 'Ġr', 'view', 'history', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'g', 'odd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġdesign', 'Ġg', 'es', 'op', 'b', 'Ġretrieved', 'Ġaug', 'ust', 'esa', 'Ġscience', 'Ġtechnology', 'Ġball', 'Ġaerospace', 'Ġdesign', 'Ġj', 'w', 'st', 'Ġarchived', 'Ġde', 'cember', 'Ġarchive', 'today', 'Ġsci', 'esa', 'int', 'Ġretrieved', 'Ġaug', 'ust', 'esa', 'Ġscience', 'Ġtechnology', 'Ġtr', 'w', 'Ġdesign', 'Ġj', 'w', 'st', 'Ġarchived', 'Ġde', 'cember', 'Ġarchive', 'today', 'Ġsci', 'esa', 'int', 'Ġretrieved', 'Ġaug', 'ust', 'esa', 'Ġscience', 'Ġtechnology', 'Ġlock', 'heed', 'mart', 'Ġdesign', 'Ġj', 'w', 'st', 'Ġarchived', 'Ġde', 'cember', 'Ġarchive', 'today', 'Ġsci', 'esa', 'int', 'Ġretrieved', 'Ġaug', 'ust', 'hub', 'bles', 'ite', 'Ġweb', 'b', 'Ġpast', 'Ġfuture']</t>
         </is>
       </c>
       <c r="C314" t="n">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>['Ġtotal', 'Ġbudget', 'Ġestimated', 'Ġbillion', 'equ', 'ivalent', 'Ġbillion', ').[', 'Ġsummer', 'Ġmission', 'Ġpassed', 'Ġcritical', 'Ġdesign', 'Ġreview', 'Ġexcellent', 'Ġgrades', 'Ġtechnical', 'Ġmatters', 'Ġschedule', 'Ġcost', 'Ġslips', 'Ġtime', 'Ġprompted', 'ary', 'land', 'Ġu', 'Ġsenator', 'Ġbar', 'bara', 'ik', 'uls', 'ki', 'Ġcall', 'Ġexternal', 'Ġreview', 'Ġproject', 'Ġindependent', 'Ġcomprehensive', 'Ġreview', 'Ġpanel', 'ic', 'r', 'p', 'Ġchaired', 'Ġj', 'Ġcas', 'ani', 'Ġfound', 'Ġearliest', 'Ġpossible', 'Ġlaunch', 'Ġdate', 'Ġlate', 'Ġextra', 'Ġcost', 'Ġbillion', 'Ġtotal', 'Ġbillion', 'Ġalso', 'Ġpointed', 'Ġwould', 'Ġrequired', 'Ġextra', 'Ġfunding', 'Ġf', 'Ġf', 'Ġlater', 'Ġlaunch', 'Ġdate', 'Ġwould', 'Ġlead', 'Ġhigher', 'Ġtotal', 'Ġcost', 'Ġj', 'uly', 'Ġunited', 'Ġstates', 'Ġhouse', 'Ġrepresentatives', 'Ġappropriations', 'Ġcommittee', 'Ġcommerce', 'Ġjustice', 'Ġscience', 'Ġmoved', 'Ġcancel', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġproject', 'Ġproposing', 'Ġf', 'Ġbudget', 'Ġremoved', 'Ġus', 'Ġbillion', 'Ġn', 'asa', "'s", 'Ġoverall', 'Ġbudget', 'Ġroughly', 'Ġone', 'Ġquarter', 'Ġbillion', 'Ġspent', 'Ġhardware', 'Ġproduction', 'Ġbudget', 'Ġproposal', 'Ġapproved', 'Ġsubcommittee', 'Ġvote', 'Ġfollowing', 'Ġday', 'Ġcommittee', 'Ġcharged', 'Ġproject', 'bill', 'ions', 'Ġdollars', 'Ġbudget', 'Ġplagued', 'Ġpoor', 'Ġmanagement', '".[', 'Ġresponse', 'Ġameric', 'Ġastronomical', 'Ġsociety', 'Ġissued', 'Ġstatement', 'Ġsupport', 'Ġsenator', 'ik', 'uls', 'ki', 'Ġnumber', 'Ġeditor', 'ials', 'Ġsupporting', 'Ġweb', 'b', 'Ġappeared', 'Ġinternational', 'Ġpress', 'mber', 'Ġcongress', 'Ġreversed', 'Ġplans', 'Ġcancel', 'Ġweb', 'b', 'Ġinstead', 'Ġcapped', 'Ġadditional', 'Ġfunding', 'Ġcomplete', 'Ġproject', 'Ġbillion', 'Ġcost', 'Ġschedule', 'Ġissues', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġprogression', 'Ġestimates', 'Ġschedule', 'Ġcost', 'Ġalong', 'Ġmajor', 'Ġmilestones', 'Ġyear', 'Ġplanned', 'Ġlaunch', 'Ġbudget', 'Ġplan', 'billion', 'Ġus', 'Ġpreliminary', 'Ġdesign', 'Ġreview', 'Ġcritical', 'Ġdesign', 'Ġreview']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġannounces', 'Ġcontract', 'Ġnext', 'generation', 'Ġspace', 'Ġtelescope', 'Ġnamed', 'Ġspace', 'Ġpioneer', 'Ġn', 'asa', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'tr', 'w', 'Ġselected', 'Ġj', 'w', 'st', 'Ġprime', 'Ġcontractor', 'Ġst', 'ci', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġjan', 'uary', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġcompletes', 'Ġfabrication', 'Ġsun', 'shield', 'Ġdeployment', 'Ġflight', 'Ġstructure', 'Ġj', 'w', 'st', 'Ġspace', 'Ġdaily', 'Ġde', 'cember', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'ather', 'Ġjohn', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', ')"', 'Ġnational', 'Ġacademy', 'Ġscience', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'euro', 'pe', 'Ġagreement', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'mir', 'Ġsigned', 'press', 'Ġrelease', 'Ġes', 'Ġmedia', 'Ġrelations', 'Ġservice', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ada', "'s", 'Ġcontribution', 'Ġn', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'ada', 'ca', 'adian', 'Ġspace', 'Ġagency', 'Ġj', 'une', 'Ġarchived', 'pe', 'html', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'adian', 'Ġspace', 'Ġagency', 'Ġdelivers', 'ada', "'s", 'Ġcontributions', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'space', 'tel', 'esc', 'ope', 'Ġspace', 'q', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'j', 'w', 'st', 'Ġpasses', 'nar', 'Ġst', 'sci', 'Ġarchived', 'Ġoriginal', 'Ġasses', 'nar', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'uly']</t>
         </is>
       </c>
       <c r="C315" t="n">
@@ -4533,7 +4533,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>['Ġâī¥', 'Ġmarch', 'Ġdec', 'Ġsimilar', 'Ġissues', 'Ġaffected', 'Ġmajor', 'Ġn', 'asa', 'Ġprojects', 'Ġhub', 'ble', 'Ġtelescope', 'Ġscientists', 'Ġexpressed', 'Ġconcerns', 'Ġgrowing', 'Ġcosts', 'Ġschedule', 'Ġdelays', 'Ġweb', 'b', 'Ġtelescope', 'Ġworrying', 'Ġbudget', 'Ġmight', 'Ġcompeting', 'Ġspace', 'Ġscience', 'Ġprograms', 'Ġnature', 'Ġarticle', 'Ġdescribed', 'Ġweb', 'b', 'Ġtelescope', 'Ġate', 'Ġastronomy', '".[', 'Ġn', 'asa', 'Ġcontinued', 'Ġdefend', 'Ġbudget', 'Ġtimeline', 'Ġprogram', 'Ġcongress', 'Ġg', 'reg', 'ory', 'Ġl', 'Ġrob', 'inson', 'Ġappointed', 'Ġnew', 'Ġdirector', 'Ġweb', 'b', 'Ġprogram', 'Ġrob', 'inson', 'Ġcredited', 'Ġraising', 'Ġprogram', "'s", 'Ġschedule', 'Ġefficiency', 'Ġmany', 'Ġmeasures', 'Ġcompleted', 'Ġtime', 'Ġrole', 'Ġimproving', 'Ġperformance', 'Ġweb', 'b', 'Ġprogram', 'Ġrob', 'ins', 'ons', "'s", 'Ġsupervisor', 'Ġth', 'omas', 'Ġz', 'urb', 'uc', 'hen', 'Ġcalled', 'Ġeffective', 'Ġleader', 'Ġmission', 'Ġever', 'Ġseen', 'Ġhistory', 'Ġn', 'asa', '."[', 'Ġj', 'uly', 'Ġweb', 'b', "'s", 'Ġcommission', 'ing', 'Ġprocess', 'Ġcomplete', 'Ġbegan', 'Ġtransmitting', 'Ġfirst', 'Ġdata', 'Ġrob', 'inson', 'Ġretired', 'Ġfollowing', 'year', 'Ġcareer', 'Ġn', 'asa', 'Ġmarch', 'Ġn', 'asa', 'Ġpushed', 'Ġback', 'Ġlaunch', 'Ġmay', 'Ġlater', 'Ġfinal', 'Ġcost', 'Ġestimate', 'Ġcome', 'Ġnew', 'Ġlaunch', 'Ġwindow', 'Ġdetermined', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġmission', 'Ġcost', 'Ġcap', 'Ġincreased', 'Ġus', 'Ġmillion', 'Ġlaunch', 'Ġwindows', 'Ġpaused', 'Ġdue', 'Ġcov', 'id', 'Ġpand', 'emic', 'Ġweb', 'b', 'Ġfinally', 'Ġlaunched', 'Ġend', 'Ġtotal', 'Ġbudget', 'Ġus', 'Ġbillion', 'Ġn', 'asa', 'Ġes', 'Ġc', 'sa', 'Ġcollaborated', 'Ġtelescope', 'Ġsince', 'Ġes', "'s", 'Ġparticipation', 'Ġconstruction', 'Ġlaunch', 'Ġapproved', 'Ġmembers', 'Ġagreement', 'Ġsigned', 'Ġes', 'Ġn', 'asa', 'Ġexchange', 'Ġfull', 'Ġpartnership', 'Ġrepresentation', 'Ġaccess', 'Ġobserv', 'atory', 'Ġastronomers', 'Ġes', 'Ġproviding', 'Ġn', 'ir', 'spec', 'Ġinstrument', 'Ġoptical', 'Ġbench', 'Ġassembly', 'Ġmir', 'Ġinstrument', 'ri', 'ane', 'Ġe', 'ca', 'Ġlauncher']</t>
+          <t>['Ġber', 'ger', 'Ġb', 'rian', 'Ġmay', 'n', 'asa', 'Ġadds', 'Ġdocking', 'Ġcapability', 'Ġnext', 'Ġspace', 'Ġobserv', 'atory', 'htt', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'uly', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsun', 'shield', 'Ġready', 'Ġfabric', 'ate', 'Ġab', 'ric', 'ate', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġpasses', 'Ġkey', 'Ġmission', 'Ġdesign', 'Ġreview', 'Ġmilestone', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġaug', 'ust', 'n', 'asa', 'Ġsays', 'Ġj', 'w', 'st', 'Ġcost', 'Ġcrunch', 'Ġimp', 'eding', 'Ġnew', 'Ġmissions', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġaug', 'ust', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġprimary', 'Ġmirror', 'Ġfully', 'Ġassembled', 'Ġn', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsecondary', 'Ġmirror', 'Ġinstalled', 'Ġn', 'asa', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'uh', 'Ġal', 'mber', 'n', 'asa', 'Ġbegins', 'Ġtesting', 'Ġenormous', 'Ġspace', 'Ġtelescope', 'Ġmade', 'Ġgold', 'Ġmirrors', 'Ġcope', 'gold', 'Ġguardian', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'n', 'asa', 'Ġcompletes', 'Ġweb', 'b', 'Ġtelescope', 'Ġreview', 'Ġcommits', 'Ġlaunch', 'Ġearly', 'n', 'asa', 'Ġn', 'asa', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġj', 'uly', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġce']</t>
         </is>
       </c>
       <c r="C316" t="n">
@@ -4546,7 +4546,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>['Ġmanpower', 'Ġsupport', 'Ġc', 'sa', 'Ġprovided', 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġnear', 'inf', 'rared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'Ġmanpower', 'Ġsupport', 'Ġoperations', 'Ġseveral', 'Ġthousand', 'Ġscientists', 'Ġengineers', 'Ġtechnicians', 'Ġspanning', 'Ġcountries', 'Ġcontributed', 'Ġbuild', 'Ġtest', 'Ġintegration', 'Ġtotal', 'Ġcompanies', 'Ġgovernment', 'Ġagencies', 'Ġacademic', 'Ġinstitutions', 'Ġparticipated', 'Ġpre', 'launch', 'Ġproject', 'Ġunited', 'Ġstates', 'Ġeuro', 'pe', 'Ġcountries', 'including', 'Ġfr', 'ance', 'Ġg', 'erman', 'ada', 'Ġcountries', 'Ġn', 'asa', 'Ġpartners', 'Ġaust', 'ral', 'ia', 'Ġinvolved', 'Ġpost', 'launch', 'Ġoperation', 'Ġparticipating', 'Ġcountries', 'Ġaust', 'ria', 'Ġbel', 'g', 'ium', 'ada', 'Ġpartnership', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġc', 'zech', 'Ġrepublic', 'Ġden', 'mark', 'Ġfin', 'land', 'Ġfr', 'ance', 'Ġg', 'erman', 'Ġg', 'ree', 'ce', 'Ġire', 'land', 'aly', 'Ġlux', 'em', 'bourg', 'Ġnet', 'lands', 'way', 'Ġport', 'ugal', 'Ġsp', 'Ġsw', 'eden', 'Ġsw', 'itzerland', 'Ġunited', 'Ġkingdom', 'Ġunited', 'Ġstates', 'Ġn', 'asa', 'Ġadministrator', 'âĢĵ', 'Ġse', 'ke', 'efe', 'Ġmade', 'Ġdecision', 'Ġname', 'Ġtelescope', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', 'Ġadministrator', 'Ġn', 'asa', 'Ġmercury', 'Ġgem', 'ini', 'Ġmuch', 'Ġap', 'ollo', 'Ġprograms', 'Ġconcerns', 'Ġraised', 'Ġaround', 'Ġweb', 'b', "'s", 'Ġpossible', 'Ġrole', 'Ġlav', 'ender', 'Ġscare', 'Ġmid', 'th', 'century', 'Ġpersecution', 'Ġu', 'Ġgovernment', 'Ġtargeting', 'Ġhomosexuals', 'Ġfederal', 'Ġn', 'asa', 'Ġreleased', 'Ġreport', 'Ġinvestigation', 'Ġbased', 'Ġexamination', '000', 'Ġdocuments', 'Ġreport', 'Ġfound', 'Ġavailable', 'Ġevidence', 'Ġdirectly', 'Ġlinks', 'Ġweb', 'b', 'Ġactions', 'Ġfollow', 'Ġrelated', 'Ġfiring', 'Ġindividuals', 'Ġsexual', 'Ġorientation', '",', 'Ġeither', 'Ġtime', 'Ġstate', 'Ġdepartment', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġfour', 'Ġkey', 'Ġgoals', 'Ġsearch', 'Ġlight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstars', 'Ġgalaxies', 'Ġformed', 'Ġuniverse', 'Ġbig', 'Ġbang', 'Ġstudy', 'Ġgalaxy', 'Ġformation', 'Ġevolution', 'Ġunderstand', 'Ġstar', 'Ġformation', 'Ġplanet', 'Ġformation', 'Ġstudy', 'Ġplanetary', 'Ġsystems', 'Ġorigins', 'Ġlife', 'Ġgoals', 'Ġaccomplished', 'Ġeffectively', 'Ġobservation', 'Ġnear', 'inf', 'rared', 'Ġlight', 'Ġrather', 'Ġlight']</t>
+          <t>['Ġgrilled', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġerrors', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'Ġcope', 'errors', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġtwo', 'Ġhalves', 'Ġhub', 'ble', "'s", 'Ġus', 'Ġbillion', 'Ġsuccessor', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġcome', 'Ġtogether', 'Ġyears', 'Ġwaiting', 'Ġbusiness', 'Ġinsider', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġse', 'pt', 'ember', 'Ġtwo', 'Ġdecades', 'Ġweb', 'b', 'Ġtelescope', 'Ġï', '¬', 'ģ', 'n', 'ished', 'Ġway', 'Ġlaunch', 'Ġsite', 'Ġna', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'Ġoct', 'ober', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarrives', 'Ġfrench', 'Ġgu', 'iana', 'Ġahead', 'Ġde', 'cember', 'Ġlaunch', 'f', 'rench', 'gu', 'iana', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġn', 'asa', 'Ġcongressional', 'Ġbudget', 'ï', '¬', 'ģ', 'cation', 'Ġn', 'asa', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġj', 'une', 'j', 'w', 'st', 'Ġlaunch', 'Ġslips', 'mber', 'Ġlips', 'n', 'ovember', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġoct', 'ober', 'Ġl', 'illy', 'Ġsim', 'mber', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'ng', 'st', ')"', 'Ġuniversity', 'Ġtor', 'onto', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'ng', 'st', 'Ġweekly', 'Ġmiss', 'ive', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'n', 'asa', 'Ġmod', 'ï', '¬', 'ģ', 'es', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġcontract', 'mber', 'Ġarchived', 'Ġl', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust']</t>
         </is>
       </c>
       <c r="C317" t="n">
@@ -4559,7 +4559,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>['Ġvisible', 'Ġpart', 'Ġspectrum', 'Ġreason', 'Ġweb', 'b', "'s", 'Ġinstruments', 'Ġmeasure', 'Ġvisible', 'Ġultraviolet', 'Ġlight', 'Ġlike', 'Ġhub', 'ble', 'Ġtelescope', 'Ġmuch', 'Ġgreater', 'Ġcapacity', 'Ġperform', 'Ġinfrared', 'Ġastronomy', 'Ġweb', 'b', 'Ġsensitive', 'Ġrange', 'Ġwavelengths', 'ĠÂµ', 'cor', 'respond', 'ing', 'Ġrespectively', 'Ġorange', 'Ġlight', 'Ġdeep', 'Ġinfrared', 'Ġradiation', 'ĠâĪĴ', 'ĠÂ°', 'c', 'Ġweb', 'b', 'Ġmay', 'Ġused', 'Ġgather', 'Ġinformation', 'Ġdim', 'ming', 'Ġlight', 'Ġstar', 'Ġk', 'ic', 'Ġdiscovered', 'Ġabnormal', 'Ġlight', 'cur', 'Ġproperties', 'Ġadditionally', 'Ġable', 'Ġtell', 'Ġex', 'oplan', 'et', 'Ġmethane', 'Ġatmosphere', 'Ġallowing', 'Ġastronomers', 'Ġdetermine', 'Ġwhether', 'Ġmethane', 'Ġweb', 'b', 'Ġorbits', 'Ġsun', 'Ġnear', 'Ġsecond', 'Ġlag', 'range', 'Ġpoint', 'Ġsun', 'âĢĵ', 'earth', 'Ġsystem', '000', '000', 'Ġmi', 'Ġfarther', 'Ġsun', 'Ġearth', "'s", 'Ġorbit', 'Ġfour', 'Ġtimes', 'Ġfarther', 'Ġmoon', "'s", 'Ġorbit', 'Ġnormally', 'Ġobject', 'Ġcircling', 'Ġsun', 'Ġfarther', 'Ġearth', 'Ġwould', 'Ġtake', 'Ġlonger', 'Ġnaming', 'Ġconcerns', 'Ġmission', 'Ġgoals', 'Ġorbit', 'Ġdesign', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġweb', 'b', 'Ġexactly', 'Ġpoint', 'Ġcircles', 'Ġaround', 'Ġh', 'alo', 'Ġorbit', 'Ġalternative', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġviews', 'Ġcar', 'ina', 'Ġneb', 'ula', 'Ġcomparing', 'Ġultraviolet', 'Ġvisible', 'top', 'Ġinfrared', 'bottom', 'Ġastronomy', 'Ġfar', 'Ġstars', 'Ġvisible', 'Ġlatter', 'Ġone', 'Ġyear', 'Ġcomplete', 'Ġorbit', 'Ġnear', 'Ġpoint', 'Ġcombined', 'Ġgravitational', 'Ġpull', 'Ġearth', 'Ġsun', 'Ġallow', 'Ġspacecraft', 'Ġorbit', 'Ġsun', 'Ġtime', 'Ġtakes', 'Ġearth', 'Ġstaying', 'Ġclose', 'Ġearth', 'Ġallows', 'Ġdata', 'Ġrates', 'Ġmuch', 'Ġfaster', 'Ġgiven', 'Ġsize', 'Ġantenna', 'Ġtelescope', 'Ġcircles', 'Ġsun', 'âĢĵ', 'earth', 'Ġpoint', 'Ġh', 'alo', 'Ġorbit', 'Ġinclined', 'Ġrespect', 'Ġe', 'cl', 'ipt', 'ic', 'Ġradius', 'Ġvarying', '000', '000', 'Ġmi', '000', '000', 'Ġmi', 'Ġtakes', 'Ġhalf', 'Ġyear', 'Ġcomplete', 'Ġsince', 'Ġequilibrium', 'Ġpoint', 'Ġgravitational', 'Ġpull', 'Ġh', 'alo', 'Ġorbit', 'Ġorbit', 'Ġusual', 'Ġsense', 'Ġspacecraft', 'Ġactually', 'Ġorbit', 'Ġaround', 'Ġsun', 'Ġh', 'alo', 'Ġorbit', 'Ġthought']</t>
+          <t>['Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'pro', 'blems', 'Ġj', 'w', 'st', 'Ġmay', 'Ġarchived', 'Ġproblems', 'j', 'w', 'st', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'ref', 'ocusing', 'Ġn', 'asa', "'s", 'Ġvision', 'Ġnature', '):', 'Ġmarch', '.).', 'Ġdoi', '01', 'Ġpm', 'id', 'pub', 'med', 'Ġcow', 'en', 'Ġr', 'Ġaug', 'ust', 'bb', 'Ġtelescope', 'Ġdelayed', 'Ġcosts', 'Ġrise', 'Ġbillion', 'web', 'ar', 'Ġscience', 'ins', 'ider', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'independent', 'Ġcomprehensive', 'Ġreview', 'Ġpanel', 'Ġfinal', 'Ġreport', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'os', 'Ġj', 'athan', 'Ġaug', 'ust', 'j', 'w', 'st', 'Ġprice', 'Ġtag', 'Ġput', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunched', 'Ġspring', 'Ġn', 'asa', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'n', 'asa', 'Ġdelays', 'Ġlaunch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'n', 'asa', 'Ġcompletes', 'Ġweb', 'b', 'Ġtelescope', 'Ġreview', 'Ġcommits', 'Ġlaunch', 'Ġearly', 'n', 'asa', 'Ġn', 'asa', 'gov', 'Ġn', 'asa', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġdelays', 'Ġlaunch', 'Ġweb', 'b', 'Ġtelescope', 'Ġearlier', 'Ġdec', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C318" t="n">
@@ -4572,7 +4572,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>['Ġcontrolled', 'Ġdrifting', 'Ġremain', 'Ġvicinity', 'Ġpoint', 'Ġrequires', 'Ġstation', 'keeping', 'Ġaround', 'Ġper', 'Ġyear', 'Ġtotal', 'ĠâĪ', 'Ĩ', 'v', 'Ġbudget', 'Ġtwo', 'Ġsets', 'Ġthr', 'usters', 'Ġconstitute', 'Ġobserv', 'atory', "'s", 'Ġpropulsion', 'Ġsystem', 'Ġthr', 'usters', 'Ġlocated', 'Ġsolely', 'Ġsun', 'facing', 'Ġside', 'Ġobserv', 'atory', 'Ġstation', 'keeping', 'Ġoperations', 'Ġdesigned', 'Ġslightly', 'Ġunders', 'h', 'oot', 'Ġrequired', 'Ġamount', 'Ġthrust', 'Ġorder', 'Ġavoid', 'Ġpushing', 'Ġweb', 'b', 'Ġbeyond', 'Ġsemi', 'stable', 'Ġpoint', 'Ġsituation', 'Ġwould', 'Ġunre', 'cover', 'able', 'Ġr', 'andy', 'Ġk', 'imble', 'Ġintegration', 'Ġtest', 'Ġproject', 'Ġscientist', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġcompared', 'Ġprecise', 'Ġstation', 'keeping', 'Ġweb', 'b', 'sis', 'ph', 'us', 'Ġ[...]', 'Ġrolling', 'Ġrock', 'Ġgentle', 'Ġslope', 'Ġnear', 'Ġtop', 'Ġhill', 'Ġnever', 'Ġwant', 'Ġroll', 'Ġcrest', 'Ġget', 'Ġaway', '".[', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġinfrared', 'Ġobservations', 'Ġsee', 'Ġobjects', 'Ġhidden', 'Ġvisible', 'Ġlight', 'Ġshown', 'Ġatmospheric', 'Ġwindows', 'Ġinfrared', 'Ġmuch', 'Ġtype', 'Ġlight', 'Ġblocked', 'Ġviewed', 'Ġearth', "'s", 'Ġsurface', 'Ġwould', 'Ġlike', 'Ġlooking', 'Ġrainbow', 'Ġseeing', 'Ġone', 'Ġcolor', 'Ġanimation', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġtrajectory', 'Ġtop', 'Ġview', 'Ġside', 'Ġview', 'Ġside', 'Ġview', 'Ġsun', 'Ġweb', 'b', 'Ġformal', 'Ġsuccessor', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'h', 'st', 'Ġsince', 'Ġprimary', 'Ġemphasis', 'Ġinfrared', 'Ġastronomy', 'Ġalso', 'Ġsuccessor', 'Ġsp', 'itzer', 'Ġspace', 'Ġtelescope', 'Ġweb', 'b', 'Ġfar', 'Ġsurpass', 'Ġtelescopes', 'Ġable', 'Ġsee', 'Ġmany', 'Ġmuch', 'Ġolder', 'Ġstars', 'Ġgalaxies', 'Ġobserving', 'Ġinfrared', 'Ġspectrum', 'Ġkey', 'Ġtechnique', 'Ġachieving', 'Ġcos', 'ological', 'Ġred', 'shift', 'Ġbetter', 'Ġpenet', 'rates', 'Ġobsc', 'uring', 'Ġdust', 'Ġgas', 'Ġallows', 'Ġobservation', 'Ġdim', 'mer', 'Ġcooler', 'Ġobjects', 'Ġsince', 'Ġwater', 'Ġvapor', 'Ġcarbon', 'Ġdioxide', 'Ġearth', "'s", 'Ġatmosphere', 'Ġstrongly', 'Ġabsorbs', 'Ġinfrared', 'Ġground', 'based', 'Ġinfrared', 'Ġastronomy', 'Ġlimited', 'Ġnarrow', 'Ġwavelength', 'Ġranges', 'Ġatmosphere', 'Ġabsorbs', 'Ġless', 'Ġstrongly', 'Ġadditionally', 'Ġatmosphere', 'Ġradi', 'ates', 'Ġinfrared', 'Ġspectrum', 'Ġoften', 'Ġoverwhelming', 'Ġlight', 'Ġobject', 'Ġobserved', 'Ġmakes', 'Ġspace', 'Ġtelescope', 'Ġpreferable', 'Ġinfrared', 'Ġobservation', 'Ġdistant', 'Ġobject', 'Ġyounger', 'Ġappears']</t>
+          <t>['Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'âĢĵ', 'cc', 'us', 'ker', 'Ġj', 'Ġj', 'Ġmuch', 'Ġreal', 'Ġmoney', 'Ġhistorical', 'Ġprice', 'Ġindex', 'Ġuse', 'Ġde', 'ï', '¬', 'Ĥ', 'ator', 'Ġmoney', 'Ġvalues', 'Ġeconomy', 'Ġunited', 'Ġstates', 'Ġadd', 'enda', 'Ġet', 'Ġcor', 'rig', 'enda', 'Ġameric', 'Ġantiqu', 'arian', 'Ġsociety', 'âĢĵ', 'cc', 'us', 'ker', 'Ġj', 'Ġj', 'Ġmuch', 'Ġreal', 'Ġmoney', 'Ġhistorical', 'Ġprice', 'Ġindex', 'Ġuse', 'Ġde', 'ï', '¬', 'Ĥ', 'ator', 'Ġmoney', 'Ġvalues', 'Ġeconomy', 'Ġunited', 'Ġstates', 'Ġameric', 'Ġantiqu', 'arian', 'Ġsociety', 'âĢĵ', 'Ġpresent', 'Ġfederal', 'Ġreserve', 'Ġbank', 'Ġmin', 'neapolis', 'consumer', 'Ġprice', 'Ġindex', 'est', 'imate', 'âĢĵ', 'Ġretrieved', 'Ġmay', 'ck', 'ie', 'Ġrob', 'Ġj', 'uly', 'n', 'asa', 'Ġï', '¬', 'ģ', 'gh', 'ts', 'Ġsave', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġguardian', 'Ġl', 'ondon', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'appropri', 'ations', 'Ġcommittee', 'Ġreleases', 'Ġfiscal', 'Ġyear', 'Ġcommerce', 'Ġjustice', 'Ġscience', 'Ġappropriations', 'Ġus', 'Ġhouse', 'Ġrepresentatives', 'Ġcommittee', 'Ġappropriations', 'Ġj', 'uly', 'Ġarchived', 'web', 'c', 'ument', 'id', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'us', 'Ġlawmakers', 'Ġvote', 'Ġkill', 'Ġhub', 'ble', 'Ġsuccessor', 'Ġspaced', 'aily', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'prop', 'osed', 'Ġn', 'asa', 'Ġbudget', 'Ġbill', 'Ġwould', 'Ġcancel', 'Ġmajor', 'Ġspace', 'Ġtelescope', 'Ġspace', 'Ġj', 'uly', 'Ġarchived', 'http', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġjan', 'uary', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġhardware', 'Ġentering', 'Ġkey', 'Ġtest', 'Ġphase', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġaug', 'ust', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġhand', 'Ġe']</t>
         </is>
       </c>
       <c r="C319" t="n">
@@ -4585,7 +4585,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>['Ġlight', 'Ġtaken', 'Ġlonger', 'Ġreach', 'Ġhuman', 'Ġobservers', 'Ġuniverse', 'Ġexpanding', 'Ġlight', 'Ġtravels', 'Ġbecomes', 'Ġred', 'sh', 'ifted', 'Ġobjects', 'Ġextreme', 'Ġdistances', 'Ġtherefore', 'Ġeasier', 'Ġsee', 'Ġviewed', 'Ġinfrared', 'Ġweb', 'b', "'s", 'Ġinfrared', 'Ġcapabilities', 'Ġexpected', 'Ġlet', 'Ġsee', 'Ġback', 'Ġtime', 'Ġfirst', 'Ġgalaxies', 'Ġforming', 'Ġhundred', 'Ġmillion', 'Ġyears', 'Ġbig', 'Ġbang', 'Ġinfrared', 'Ġradiation', 'Ġpass', 'Ġfreely', 'Ġregions', 'Ġcosmic', 'Ġdust', 'Ġscatter', 'Ġvisible', 'Ġlight', 'Ġobservations', 'Ġinfrared', 'Ġallow', 'Ġstudy', 'Ġobjects', 'Ġregions', 'Ġspace', 'Ġwould', 'Ġobscured', 'Ġgas', 'Ġdust', 'Ġvisible', 'Ġspectrum', 'Ġinfrared', 'Ġastronomy', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmolecular', 'Ġclouds', 'Ġstars', 'Ġborn', 'Ġcircumst', 'ellar', 'Ġdisks', 'Ġgive', 'Ġrise', 'Ġplanets', 'Ġcores', 'Ġactive', 'Ġgalaxies', 'Ġrelatively', 'Ġcool', 'Ġobjects', 'tem', 'per', 'atures', 'Ġless', 'Ġseveral', 'Ġthousand', 'Ġdegrees', 'Ġemit', 'Ġradiation', 'Ġprimarily', 'Ġinfrared', 'Ġdescribed', 'Ġplan', 'ck', "'s", 'Ġlaw', 'Ġresult', 'Ġobjects', 'Ġcooler', 'Ġstars', 'Ġbetter', 'Ġstudied', 'Ġinfrared', 'Ġincludes', 'Ġclouds', 'Ġinterstellar', 'Ġmedium', 'Ġbrown', 'Ġdwar', 'fs', 'Ġplanets', 'Ġsolar', 'Ġsystems', 'ets', 'Ġk', 'ui', 'per', 'Ġbelt', 'Ġobjects', 'Ġobserved', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'mir', ').[', 'Ġmissions', 'Ġinfrared', 'Ġastronomy', 'Ġimpacted', 'Ġweb', 'b', 'Ġdevelopment', 'Ġsp', 'itzer', 'Ġwil', 'kinson', 'Ġmicrowave', 'ot', 'ropy', 'Ġprobe', 'w', 'map', ').[', 'Ġsp', 'itzer', 'Ġshowed', 'Ġimportance', 'Ġmid', 'inf', 'rared', 'Ġhelpful', 'Ġtasks', 'Ġobserving', 'Ġdust', 'Ġdisks', 'Ġaround', 'Ġstars', 'Ġalso', 'Ġw', 'map', 'Ġprobe', 'Ġshowed', 'Ġuniverse', 'lit', 'Ġred', 'shift', 'Ġundersc', 'oring', 'Ġimportance', 'Ġmid', 'inf', 'rared', 'Ġmissions', 'Ġlaunched', 'Ġearly', 'Ġtime', 'Ġinfluence', 'Ġweb', 'b', 'Ġdevelopment', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'sts', 'ci', 'Ġb', 'alt', 'imore', 'ary', 'land', 'Ġhom', 'ew', 'ood', 'Ġcampus', 'Ġjohn', 'Ġhop', 'kins', 'Ġuniversity', 'Ġselected', 'Ġscience', 'Ġoperations', 'Ġcenter', 'oc', 'Ġweb', 'b', 'Ġinitial', 'Ġbudget', 'Ġus', 'Ġmillion', 'Ġintended', 'Ġsupport', 'Ġoperations', 'Ġfirst', 'Ġyear', 'Ġlaunch']</t>
+          <t>['Ġj', 'uly', 'Ġissues', 'Ġstatement', 'Ġproposed', 'Ġcancellation', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġameric', 'Ġastronomical', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ik', 'uls', 'ki', 'Ġstatement', 'Ġhouse', 'Ġappropriations', 'Ġsubcommittee', 'Ġtermination', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġspace', 'ref', 'Ġj', 'uly', 'Ġarchived', 'Ġe', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'way', 'Ġshuttle', 'Ġflight', 'Ġl', 'ref', 'op', 'inion', 'Ġnew', 'ork', 'Ġtimes', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhar', 'ro', 'ld', 'Ġj', 'uly', 'bad', 'Ġnews', 'ada', 'Ġu', 'Ġcould', 'Ġscrap', 'Ġnew', 'Ġspace', 'Ġtelescope', 'http', 'story', 'html', 'Ġv', 'ancouver', 'Ġsun', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġbudget', 'Ġplan', 'Ġsaves', 'Ġtelescope', 'Ġcuts', 'Ġspace', 'Ġtaxis', 'uters', 'mber', 'Ġarchived', 'web', 'arch', 'iv', 'Ġtre', 'af', '06', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'uly', 'Ġle', 'one', 'Ġdan', 'mber', 'n', 'asa', 'Ġacknowledges', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġcosts', 'Ġdelay', 'Ġscience', 'Ġmissions', 'missions', 'html', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmos', 'k', 'owitz', 'Ġcl', 'ara', 'Ġmarch', 'n', 'asa', 'Ġassures', 'Ġskeptical', 'Ġcongress', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġtrack', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġbill', 'ings', 'Ġle', 'e', 'Ġoct', 'ober', 'Ġtelescope', 'Ġate', 'Ġastronomy', 'Ġnature', '):', 'âĢĵ', 'Ġpm', 'id', 'Ġk', 'oren', 'Ġmar', 'ina', 'Ġde', 'cember', 'Ġextreme', 'Ġha', 'zing', 'Ġexpensive', 'Ġtelescope', 'Ġever', 'Ġbuilt', 'l', 'antic', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C320" t="n">
@@ -4598,7 +4598,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>['Ġcapacity', 'Ġst', 'sci', 'Ġresponsible', 'Ġscientific', 'Ġoperation', 'Ġtelescope', 'Ġdelivery', 'Ġdata', 'Ġproducts', 'Ġastronomical', 'Ġcommunity', 'Ġdata', 'Ġtransmitted', 'Ġweb', 'b', 'Ġground', 'Ġvia', 'Ġn', 'asa', 'Ġdeep', 'Ġspace', 'Ġnetwork', 'Ġprocessed', 'Ġcalibrated', 'Ġst', 'sci', 'Ġdistributed', 'Ġonline', 'Ġastronomers', 'Ġworldwide', 'Ġsimilar', 'Ġhub', 'ble', 'Ġoperated', 'Ġanyone', 'Ġanywhere', 'Ġworld', 'Ġallowed', 'Ġsubmit', 'Ġproposals', 'Ġobservations', 'Ġyear', 'Ġseveral', 'Ġcommittees', 'Ġastronomers', 'Ġpeer', 'Ġreview', 'Ġsubmitted', 'Ġproposals', 'Ġselect', 'Ġprojects', 'Ġobserve', 'Ġcoming', 'Ġyear', 'Ġauthors', 'Ġchosen', 'Ġproposals', 'Ġtypically', 'Ġone', 'Ġyear', 'Ġprivate', 'Ġaccess', 'Ġnew', 'Ġobservations', 'Ġdata', 'Ġbecome', 'Ġpublicly', 'Ġavailable', 'Ġdownload', 'Ġanyone', 'Ġonline', 'Ġarchive', 'Ġst', 'sci', 'Ġbandwidth', 'Ġdigital', 'Ġthroughput', 'Ġsatellite', 'Ġdesigned', 'Ġoperate', 'Ġgig', 'ab', 'Ġdata', 'Ġper', 'Ġday', 'Ġlength', 'Ġmission', 'equ', 'ivalent', 'Ġsustained', 'Ġrate', 'Ġdata', 'Ġprocessing', 'Ġtelescope', 'Ġdone', 'Ġconventional', 'Ġsingle', 'board', 'Ġcomputers', 'Ġdigit', 'ization', 'Ġanalog', 'Ġdata', 'Ġinstruments', 'Ġperformed', 'Ġcustom', 'Ġside', 'car', 'ic', 'system', 'Ġimage', 'Ġdigit', 'ization', 'Ġenhancement', 'Ġcontrol', 'Ġretrieval', 'Ġapplication', 'Ġspecific', 'Ġintegrated', 'Ġcircuit', 'Ġn', 'asa', 'Ġstated', 'Ġside', 'car', 'ic', 'Ġinclude', 'Ġfunctions', 'Ġinstrument', 'Ġpackage', 'Ġconsume', 'Ġmill', 'iw', 'atts', 'Ġpower', 'Ġsince', 'Ġconversion', 'Ġmust', 'Ġdone', 'Ġclose', 'Ġdetectors', 'Ġcold', 'Ġside', 'Ġtelescope', 'Ġlow', 'Ġpower', 'Ġdiss', 'ipation', 'Ġcrucial', 'Ġmaintaining', 'Ġlow', 'Ġtemperature', 'Ġrequired', 'Ġoptimal', 'Ġoperation', 'Ġground', 'Ġsupport', 'Ġoperations', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġstrike', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmirror', 'Ġsegment', 'Ġsuffered', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġstrike', 'Ġlarge', 'Ġdust', 'ote', 'sized', 'Ġparticle', 'Ġmay', 'Ġfifth', 'Ġlargest', 'Ġstrike', 'Ġsince', 'Ġlaunch', 'Ġreported', 'Ġj', 'une', 'Ġrequired', 'Ġengineers', 'Ġcompensate', 'Ġstrike', 'Ġusing', 'Ġmirror', 'Ġactu', 'ator', 'Ġdespite', 'Ġstrike', 'Ġn', 'asa', 'Ġcharacterization', 'Ġreport', 'Ġstates', 'Ġj', 'w', 'st', 'Ġobserving', 'Ġmodes', 'Ġreviewed', 'Ġconfirmed', 'Ġready', 'Ġscience', 'Ġuse', 'Ġj', 'uly', 'Ġlaunch', 'design', 'ated', 'ri', 'ane', 'Ġflight', 'Ġtook', 'Ġplace']</t>
+          <t>['Ġjan', 'uary', 'Ġco', 'hen', 'Ġben', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġengineer', 'Ġmade', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwork', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġiss', 'n', 'Ġ00', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġpot', 'ter', 'Ġse', 'Ġj', 'uly', 'n', 'asa', 'Ġweb', 'b', 'Ġprogram', 'Ġdirector', 'Ġg', 'reg', 'Ġrob', 'inson', 'Ġannounces', 'Ġretirement', 'Ġet', 'irement', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġw', 'ang', 'Ġj', 'en', 'Ġco', 'le', 'Ġste', 'Ġnorth', 'Ġk', 'Ġmarch', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġobserv', 'atory', 'Ġrequires', 'Ġtime', 'Ġtesting', 'Ġevaluation', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'os', 'Ġj', 'athan', 'Ġmarch', 'hub', 'ble', 'success', 'Ġfaces', 'Ġnew', 'Ġdelay', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġwit', 'ze', 'lex', 'andra', 'Ġmarch', 'n', 'asa', 'Ġreveals', 'Ġmajor', 'Ġdelay', 'billion', 'Ġhub', 'ble', 'Ġsuccessor', 'ht', 'Ġnature', '):', 'âĢĵ', 'Ġpm', 'id', 'ier', 'Ġcase', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġgot', 'Ġbest', 'Ġbudget', 'Ġdecade', 'http', 'plan', 'eta', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmarch', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'cor', 'av', 'irus', 'Ġpauses', 'Ġwork', 'Ġj', 'w', 'st', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'esa', 'Ġscience', 'Ġtechnology', 'Ġeuro', 'pe', "'s", 'Ġcontributions', 'Ġj', 'w', 'st', 'Ġmission', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'adian', 'Ġspace', 'Ġagency', 'eyes', 'Ġhub', 'ble', "'s", 'Ġsuccessor', 'ada', 'Ġdelivers', 'Ġcontribution', 'Ġworld', "'s"]</t>
         </is>
       </c>
       <c r="C321" t="n">
@@ -4611,7 +4611,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>['Ġscheduled', 'Ġut', 'c', 'Ġde', 'cember', 'ri', 'ane', 'Ġrocket', 'Ġlifted', 'Ġgu', 'iana', 'Ġspace', 'Ġcentre', 'Ġfrench', 'Ġgu', 'iana', 'Ġtelescope', 'Ġconfirmed', 'Ġreceiving', 'Ġpower', 'Ġstarting', 'Ġtwo', 'week', 'Ġdeployment', 'Ġphase', 'Ġparts', 'Ġtraveling', 'Ġtarget', 'Ġtelescope', 'Ġreleased', 'Ġupper', 'Ġstage', 'Ġminutes', 'Ġseconds', 'Ġlaunch', 'Ġbeginning', 'day', 'Ġadjustment', 'Ġplace', 'Ġtelescope', 'Ġl', 'iss', 'aj', 'ous', 'Ġorbit', 'Ġaround', 'Ġlag', 'range', 'Ġpoint', 'Ġtelescope', 'Ġlaunched', 'Ġslightly', 'Ġless', 'Ġspeed', 'Ġneeded', 'Ġreach', 'Ġfinal', 'Ġorbit', 'Ġslowed', 'Ġtravelled', 'Ġaway', 'Ġearth', 'Ġorder', 'Ġreach', 'Ġvelocity', 'Ġneeded', 'Ġenter', 'Ġorbit', 'Ġtelescope', 'Ġreached', 'Ġjan', 'uary', 'Ġflight', 'Ġincluded', 'Ġthree', 'Ġplanned', 'Ġcourse', 'Ġcorrections', 'Ġadjust', 'Ġspeed', 'Ġdirection', 'Ġobserv', 'atory', 'Ġcould', 'Ġrecover', 'th', 'rust', 'going', 'Ġslowly', 'Ġcould', 'Ġrecover', 'Ġoverth', 'rust', 'going', 'Ġfast', 'Ġprotect', 'Ġhighly', 'Ġinstruments', 'Ġsun', 'shield', 'Ġmust', 'Ġremain', 'Ġtelescope', 'Ġsun', 'Ġspacecraft', 'Ġcould', 'Ġturn', 'Ġaround', 'Ġuse', 'Ġthr', 'usters', 'Ġslow', 'Ġorbit', 'Ġunstable', 'Ġj', 'w', 'st', 'Ġneeds', 'Ġuse', 'Ġpropell', 'ant', 'Ġmaintain', 'Ġh', 'alo', 'Ġorbit', 'Ġaround', 'known', 'Ġstation', 'keeping', 'Ġprevent', 'Ġtelescope', 'Ġdrifting', 'Ġaway', 'Ġorbital', 'Ġposition', 'Ġdesigned', 'Ġcarry', 'Ġenough', 'Ġpropell', 'ant', 'Ġyears', 'Ġprecision', 'ri', 'ane', 'Ġlaunch', 'Ġfirst', 'Ġmid', 'course', 'Ġcorrection', 'Ġcredited', 'Ġsaving', 'Ġenough', 'Ġonboard', 'Ġfuel', 'Ġj', 'w', 'st', 'Ġmay', 'Ġable', 'Ġmaintain', 'Ġorbit', 'Ġaround', 'Ġyears', 'Ġspace', 'Ġcalled', 'Ġlaunch', 'fl', 'aw', 'less', '".[', 'Ġlaunch', 'Ġcommission', 'ing', 'Ġlaunch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġdiagram', 'Ġweb', 'b', 'Ġinside', 'ri', 'ane', 'ri', 'ane', 'Ġweb', 'b', 'Ġlaunch', 'Ġpad', 'ri', 'ane', 'Ġcontaining', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlifting', 'Ġlaunch', 'Ġpad', 'ri', 'ane', 'Ġcontaining', 'Ġweb', 'b', 'Ġmoments', 'Ġlift', 'Ġweb', 'b', 'Ġseen', 'Ġcry', 'ote', 'chn', 'ic', 'Ġupper', 'Ġstage', 'Ġshortly', 'Ġseparation', 'Ġapproximately', 'Ġminutes', 'Ġlaunch', 'Ġpart', 'Ġearth', 'Ġgulf', 'Ġad', 'en', 'Ġvisible', 'Ġbackground', 'Ġimage', 'Ġweb', 'b']</t>
+          <t>['Ġpowerful', 'Ġspace', 'Ġtelescope', 'adian', 'Ġspace', 'Ġagency', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġsp', 'Ġapr', 'il', 'Ġj', 'en', 'ner', 'Ġlyn', 'n', 'Ġj', 'une', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġinternational', 'Ġendeavor', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'inst', 'itutional', 'Ġpartners', 'Ġweb', 'b', 'n', 'asa', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġshepherd', 'ony', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġworld', "'s", 'Ġpowerful', 'Ġtelescope', 'Ġmakes', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcall', 'Ġaust', 'ral', 'ia', 'Ġchrist', 'mas', 'Ġday', 'Ġguardian', 'Ġarchived', 'Ġn', 'christ', 'mas', 'day', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfranc', 'Ġmatt', 'hew', 'Ġproblem', 'Ġnaming', 'Ġobserv', 'atories', 'Ġbig', 'ots', 'Ġforb', 'es', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġsavage', 'Ġdan', 'Ġjan', 'uary', 'Ġn', 'asa', 'Ġname', 'Ġtelescope', 'Ġdead', 'Ġpersecuted', 'Ġgay', 'Ġpeople', '?"', 'Ġstranger', 'Ġarchived', 'Ġple', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'Ġfisher', 'Ġal', 'ise', 'mber', 'n', 'asa', 'Ġshares', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġhistory', 'Ġreport', 'n', 'asa', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'dom', 'Ġb', 'rian', 'Ġc', 'n', 'asa', 'Ġhistorical', 'Ġinvestigation', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', "'s", 'Ġrelationship', 'Ġlav', 'ender', 'Ġscare', 'Ġfinal', 'Ġreport', 'Ġn', 'asa', 'gov', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġwit', 'ze', 'lex', 'andra', 'mber', 'n', 'asa', 'Ġreally', 'Ġreally', "'t", 'Ġrename', 'Ġweb', 'b', 'Ġtelescope', 'Ġdespite', 'Ġcommunity', 'Ġpush', 'back', 'Ġnature', 'Ġpm', 'id', '00', 'api', 'se', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C322" t="n">
@@ -4624,7 +4624,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>['Ġreleased', 'Ġrocket', 'Ġupper', 'Ġstage', 'Ġminutes', 'Ġflawless', 'Ġlaunch', 'Ġstarting', 'Ġminutes', 'Ġlaunch', 'Ġcontinuing', 'Ġdays', 'Ġweb', 'b', 'Ġbegan', 'Ġprocess', 'Ġdeploying', 'Ġsolar', 'Ġarray', 'Ġantenna', 'Ġsun', 'shield', 'Ġmirrors', 'Ġnearly', 'Ġdeployment', 'Ġactions', 'Ġcommanded', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġb', 'alt', 'imore', 'ary', 'land', 'Ġexcept', 'Ġtwo', 'Ġearly', 'Ġautomatic', 'Ġsteps', 'Ġsolar', 'Ġpanel', 'Ġunfolding', 'Ġcommunication', 'Ġantenna', 'Ġmission', 'Ġdesigned', 'Ġgive', 'Ġground', 'Ġcontrollers', 'Ġflexibility', 'Ġchange', 'Ġmodify', 'Ġdeployment', 'Ġsequence', 'Ġcase', 'Ġproblems', 'Ġest', 'Ġde', 'cember', 'Ġhours', 'Ġlaunch', 'Ġtelescope', "'s", 'Ġpair', 'Ġprimary', 'Ġrockets', 'Ġbegan', 'Ġfiring', 'Ġminutes', 'Ġmake', 'Ġfirst', 'Ġthree', 'Ġplanned', 'Ġmid', 'course', 'Ġcorrections', 'Ġday', 'Ġtwo', 'Ġhigh', 'Ġgain', 'Ġcommunication', 'Ġantenna', 'Ġdeployed', 'Ġautomatically', 'Ġtransit', 'Ġstructural', 'Ġdeployment', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġstructural', 'Ġdeployment', 'Ġtimeline', 'Ġstructural', 'Ġdeployment', 'Ġsequence', 'Ġde', 'cember', 'Ġhours', 'Ġlaunch', 'Ġweb', 'b', "'s", 'Ġrockets', 'Ġfired', 'Ġnine', 'Ġminutes', 'Ġseconds', 'Ġmake', 'Ġsecond', 'Ġthree', 'Ġmid', 'course', 'Ġcorrections', 'Ġtelescope', 'Ġarrive', 'Ġdestination', 'Ġde', 'cember', 'Ġthree', 'Ġdays', 'Ġlaunch', 'Ġmission', 'Ġcontrollers', 'Ġbegan', 'Ġmulti', 'day', 'Ġdeployment', 'Ġweb', 'b', "'s", 'important', 'Ġsun', 'shield', 'Ġde', 'cember', 'Ġcontrollers', 'Ġsuccessfully', 'Ġcompleted', 'Ġtwo', 'Ġsteps', 'Ġunp', 'acking', 'Ġobserv', 'atory', 'Ġfirst', 'Ġcommands', 'Ġdeployed', 'Ġaft', 'mom', 'ent', 'um', 'Ġflap', '",', 'Ġdevice', 'Ġprovides', 'Ġbalance', 'Ġsolar', 'Ġpressure', 'Ġsun', 'shield', 'Ġsaving', 'Ġfuel', 'Ġreducing', 'Ġneed', 'Ġthr', 'uster', 'Ġfiring', 'Ġmaintain', 'Ġweb', 'b', "'s", 'Ġorientation', 'Ġde', 'cember', 'Ġground', 'Ġteam', 'Ġextended', 'Ġtwo', 'Ġtelesc', 'oping', 'mid', 'Ġbo', 'oms', 'Ġleft', 'Ġright', 'Ġsides', 'Ġobserv', 'atory', 'Ġleft', 'Ġside', 'Ġdeployed', 'Ġhours', 'Ġminutes', 'Ġright', 'Ġside', 'Ġtook', 'Ġhours', 'Ġminutes', 'Ġcommands', 'Ġseparate', 'Ġtension', 'Ġmembranes', 'Ġfollowed', 'Ġjan', 'uary', 'Ġsuccessful', 'Ġjan', 'uary', 'Ġmission', 'Ġcontrol', 'Ġsuccessfully', 'Ġdeployed', 'Ġtelescope', "'s", 'Ġsecondary', 'Ġmirror', 'Ġlocked', 'Ġplace', 'Ġtolerance', 'Ġone', 'Ġhalf', 'Ġmill', 'imeters', 'Ġlast', 'Ġstep', 'Ġstructural', 'Ġdeployment', 'Ġunfold', 'Ġwings']</t>
+          <t>['mber', 'Ġmas', 'etti', 'Ġmag', 'gie', 'Ġk', 'rish', 'nam', 'ur', 'th', 'ita', 'j', 'w', 'st', 'Ġscience', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', "'s", 'Ġnext', 'Ġtelescope', 'Ġcould', 'Ġid', 'Ġalien', 'Ġmeg', 'ast', 'ruct', 'ures', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġz', 'immer', 'Ġcar', 'l', 'Ġj', 'uly', 'bb', 'Ġtelescope', 'Ġlook', 'Ġsigns', 'Ġlife', 'Ġway', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġquestion', 'Ġastronomers', 'Ġwant', 'Ġanswer', 'Ġex', 'oplan', 'ets', 'Ġatmosp', 'heres', 'Ġfriendly', 'Ġlife', '?"', 'Ġl', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġupdated', 'Ġst', 'ef', 'anie', 'Ġw', 'ald', 'ek', 'Ġlast', 'Ġmarch', 'n', 'asa', "'s", 'Ġnew', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġable', 'Ġsniff', 'Ġmethane', "'s", 'Ġtell', "'s", 'Ġsign', 'Ġlife', 'Ġspace', 'Ġretrieved', 'Ġaug', 'ust', 'bas', 'ics', 'Ġspace', 'Ġflight', 'Ġjet', 'Ġpropulsion', 'Ġlaboratory', 'Ġarchived', 'Ġp', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdich', 'mann', 'ald', 'Ġj', '.;', 'Ġal', 'ber', 'ding', 'Ġcass', 'andra', '.;', 'Ġway', 'ne', 'Ġh', 'Ġmay', 'station', 'keeping', 'Ġmon', 'te', 'Ġcar', 'lo', 'Ġsimulation', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'web', 'arch', 'pdf', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'nt', 'rs', 'n', 'asa', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgreenhouse', 'Ġmatt', 'Ġapr', 'il', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmission', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C323" t="n">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>['Ġprimary', 'Ġmirror', 'Ġpanel', 'Ġconsists', 'Ġthree', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġfolded', 'Ġallow', 'Ġspace', 'Ġtelescope', 'Ġinstalled', 'Ġfair', 'ing', 'ri', 'ane', 'Ġrocket', 'Ġlaunch', 'Ġtelescope', 'Ġjan', 'uary', 'Ġn', 'asa', 'Ġdeployed', 'Ġlocked', 'Ġplace', 'Ġport', 'side', 'Ġwing', 'Ġjan', 'uary', 'Ġstar', 'board', 'side', 'Ġmirror', 'Ġwing', 'Ġsuccessfully', 'Ġcompleted', 'Ġstructural', 'Ġdeployment', 'Ġjan', 'uary', '00', 'Ġeastern', 'Ġstandard', 'Ġtime', 'Ġnearly', 'Ġmonth', 'Ġlaunch', 'Ġthird', 'Ġfinal', 'Ġcourse', 'Ġcorrection', 'Ġtook', 'Ġplace', 'Ġinserting', 'Ġweb', 'b', 'Ġplanned', 'Ġh', 'alo', 'Ġorbit', 'Ġaround', 'Ġsun', 'âĢĵ', 'Ġearth', 'Ġpoint', 'Ġmir', 'Ġinstrument', 'Ġfour', 'Ġobserving', 'Ġmodes', 'âĢĶ', 'im', 'aging', 'Ġlow', 'resolution', 'Ġspect', 'rosc', 'opy', 'Ġmedium', 'resolution', 'Ġspect', 'rosc', 'opy', 'Ġcoron', 'agraph', 'ic', 'Ġimaging', 'ĠâĢ', 'ľ', 'Ġaug', 'Ġmechanism', 'Ġsupports', 'Ġmedium', 'resolution', 'Ġspect', 'rosc', 'opy', 'Ġexhibited', 'Ġappears', 'Ġincreased', 'Ġfriction', 'Ġsetup', 'Ġscience', 'Ġobservation', 'Ġmechanism', 'Ġgr', 'ating', 'Ġwheel', 'Ġallows', 'Ġscientists', 'Ġselect', 'Ġshort', 'Ġmedium', 'Ġlonger', 'Ġwavelengths', 'Ġmaking', 'Ġobservations', 'Ġusing', 'Ġmode', 'âĢ', 'Ŀ', 'Ġsaid', 'Ġn', 'asa', 'Ġpress', 'Ġstatement', 'Ġjan', 'uary', 'Ġstill', 'Ġtransit', 'Ġmirror', 'Ġalignment', 'Ġbegan', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġsecondary', 'Ġmirror', 'Ġmoved', 'Ġaway', 'Ġprotective', 'Ġlaunch', 'Ġpositions', 'Ġtook', 'Ġdays', 'Ġactu', 'ator', 'Ġmotors', 'Ġdesigned', 'Ġfine', 'une', 'Ġmirror', 'Ġpositions', 'Ġmicroscopic', 'Ġcommission', 'ing', 'Ġtesting', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġanimation', 'Ġweb', 'b', "'s", 'Ġh', 'alo', 'Ġorbit', 'Ġaccuracy', 'Ġnan', 'ometer', 'Ġincrements', 'Ġmust', 'Ġmove', 'Ġmillion', 'Ġincrements', 'Ġmm', 'Ġinitial', 'Ġalignment', 'Ġmirror', 'Ġalignment', 'Ġrequires', 'Ġmirror', 'Ġsegments', 'Ġsecondary', 'Ġmirror', 'Ġpositioned', 'Ġwithin', 'Ġnan', 'ometers', 'Ġn', 'asa', 'Ġcompares', 'Ġrequired', 'Ġaccuracy', 'Ġanalogy', 'Ġweb', 'b', 'Ġprimary', 'Ġmirror', 'Ġsize', 'Ġunited', 'Ġstates', 'mir', 'ror', 'Ġsegment', 'Ġwould', 'Ġsize', 'Ġtex', 'Ġteam', 'Ġwould', 'Ġneed', 'Ġline', 'Ġheight', 'Ġtex', 'sized', 'Ġsegments', 'Ġaccuracy', 'Ġinches', '".[', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmirror']</t>
+          <t>['j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġinitial', 'Ġmid', 'course', 'Ġcorrection', 'Ġmon', 'te', 'Ġcar', 'lo', 'Ġimplementation', 'Ġusing', 'Ġtask', 'Ġparallel', 'ism', 'Ġarchived', 'web', 'arch', 'iv', 'Ġmarch', 'Ġway', 'back', 'Ġmachine', 'Ġpropulsion', 'Ġsystem', 'Ġoverview', 'Ġj', 'Ġpet', 'ersen', 'Ġet', 'Ġal', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġk', 'imble', 'Ġr', 'andy', 'Ġde', 'cember', 'Ġwanted', 'Ġknow', 'Ġweb', 'b', "'s", 'Ġmid', 'course', 'Ġcorrections', '!"', 'Ġn', 'asa', 'Ġarchived', 'ctions', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ard', 'Ġr', 'ick', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', ')"', 'Ġarchived', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġn', 'asa', 'gov', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'inf', 'rared', 'Ġatmospheric', 'Ġwindows', 'Ġcool', 'Ġcosmos', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġaug', 'ust', 'inf', 'rared', 'Ġastronomy', 'Ġoverview', 'Ġn', 'asa', 'Ġinfrared', 'Ġastronomy', 'Ġprocessing', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'bb', 'Ġscience', 'Ġend', 'Ġdark', 'Ġages', 'Ġfirst', 'Ġlight', 'ion', 'ization', 'Ġv', 'ï', '¬', 'ģ', 'r', 'st', 'light', 'html', 'Ġn', 'asa', 'Ġarchived', 'Ġov', 'ï', '¬', 'ģ', 'r', 'st', 'light', 'html', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'ather', 'Ġjohn', 'Ġj', 'une', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', 'Ġscience', 'Ġsummary', 'sb', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġsavage', 'ald', 'Ġne', 'al', 'Ġn', 'ancy', 'Ġj', 'une', 'bb', 'Ġspacecraft', 'Ġscience', 'Ġoperations', 'Ġcenter', 'Ġcontract', 'Ġawarded', 'Ġn', 'asa']</t>
         </is>
       </c>
       <c r="C324" t="n">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>['Ġalignment', 'Ġanimations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġsegment', 'Ġimage', 'Ġident', 'ï', '¬', 'ģ', 'cation', 'Ġmirror', 'Ġsegments', 'Ġmoved', 'Ġdetermine', 'Ġsegment', 'Ġcreates', 'Ġsegment', 'Ġimage', 'Ġmatching', 'Ġmirror', 'Ġsegments', 'Ġrespective', 'Ġimages', 'Ġmirrors', 'Ġtilted', 'Ġbring', 'Ġimages', 'Ġnear', 'Ġcommon', 'Ġpoint', 'Ġanalysis', 'Ġsegment', 'Ġalignment', 'Ġbegins', 'Ġdef', 'ocusing', 'Ġsegment', 'Ġimages', 'Ġmoving', 'Ġsecondary', 'Ġmirror', 'Ġslightly', 'Ġmathematical', 'Ġanalysis', 'Ġcalled', 'Ġphase', 'Ġretrieval', 'Ġapplied', 'Ġdef', 'ocused', 'Ġimages', 'Ġdetermine', 'Ġprecise', 'Ġpositioning', 'Ġerrors', 'Ġsegments', 'Ġadjustments', 'Ġsegments', 'Ġresult', 'Ġwell', 'correct', 'ed', 'tel', 'esc', 'opes', '".', 'Ġhowever', 'Ġsegments', 'Ġstill', 'Ġwork', 'Ġtogether', 'Ġsingle', 'Ġmirror', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġimage', 'Ġstacking', 'Ġput', 'Ġlight', 'Ġsingle', 'Ġplace', 'Ġsegment', 'Ġimage', 'Ġmust', 'Ġstacked', 'Ġtop', 'Ġone', 'Ġanother', 'Ġimage', 'Ġstacking', 'Ġstep', 'Ġindividual', 'Ġsegment', 'Ġimages', 'Ġmoved', 'Ġfall', 'Ġprecisely', 'Ġcenter', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġproduce', 'Ġone', 'Ġun', 'ï', '¬', 'ģ', 'ed', 'Ġimage', 'Ġprocess', 'Ġprepares', 'Ġtelescope', 'Ġcoarse', 'Ġph', 'asing', 'Ġtelescope', 'Ġalignment', 'Ġinstrument', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġview', 'Ġï', '¬', 'ģ', 'ne', 'Ġph', 'asing', 'Ġtelescope', 'Ġwell', 'Ġaligned', 'Ġone', 'Ġplace', 'Ġn', 'irc', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġview', 'Ġalignment', 'Ġmust', 'Ġextended', 'Ġrest', 'Ġinstruments', 'Ġmirror', 'Ġalignment', 'Ġcomplex', 'Ġoperation', 'Ġsplit', 'Ġseven', 'Ġphases', 'Ġrepeatedly', 'Ġrehears', 'ed', 'Ġusing', 'Ġscale', 'Ġmodel', 'Ġtelescope', 'Ġmirrors', 'Ġreached', 'Ġ(âĪĴ', 'ĠÂ°', 'c', 'ĠâĪĴ', 'Ġn', 'irc', 'Ġtargeted', 'th', 'Ġmagnitude', 'Ġstar', 'Ġ', 'urs', 'Ġmajor', 'Ġn', 'irc', 'Ġtook', 'Ġimages', 'Ġused', 'Ġwide', 'ranging', 'Ġimages', 'Ġdetermine', 'Ġsegment', 'Ġmain', 'Ġmirror', 'Ġinitially', 'Ġpointed', 'Ġfirst', 'Ġindividual', 'Ġprimary', 'Ġmirror', 'Ġsegments', 'Ġgreatly', 'Ġmis', 'aligned', 'Ġimage', 'Ġcontained', 'Ġseparate', 'Ġblurry', 'Ġimages', 'Ġstar', 'Ġfield', 'Ġcontaining', 'Ġimage', 'Ġtarget', 'Ġstar', 'Ġimages', 'Ġmatched', 'Ġrespective', 'Ġmirror', 'Ġsegments', 'Ġsegments', 'Ġbrought', 'Ġapproximate', 'Ġalignment', 'Ġcentered']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'single', 'Ġboard', 'Ġcomputer', 'htm', 'Ġf', 'bo', 'Ġdaily', 'Ġissue', 'Ġf', 'bo', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'azing', 'Ġmini', 'atur', 'ized', 'side', 'car', 'Ġdrives', 'Ġweb', 'b', 'Ġtelescope', "'s", 'Ġsignal', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'utherland', 'Ġsc', 'ott', 'Ġj', 'une', 'bb', "'s", 'Ġprimary', 'Ġmirror', 'Ġhit', 'Ġmeteor', 'oid', 'Ġbuilt', 'Ġendure', 'Ġweather', 'Ġnetwork', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġhar', 'wood', 'iam', 'Ġj', 'une', 'bb', 'Ġtelescope', 'Ġstill', 'Ġperforming', 'Ġwell', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġimpact', 'Ġmirror', 'Ġsegment', 'Ġn', 'asa', 'Ġsays', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'ell', 'Ġel', 'izabeth', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġpicture', 'Ġshows', 'Ġnoticeable', 'Ġdamage', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġstrike', 'Ġcites', 'Ġn', 'asa', 'esa', 'cs', 'Ġjoint', 'Ġreport', 'Ġj', 'uly', 'Ġco', 'authors', 'Ġinstitutions', ']:', 'arian', 'e', 'Ġgoes', 'Ġhistory', 'Ġsuccessful', 'Ġlaunch', 'Ġweb', 'b', 'rian', 'esp', 'ace', 'press', 'Ġrelease', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġp', 'ino', 'Ġnat', 'asha', 'Ġf', 'iser', 'Ġal', 'ise', 'Ġbet', 'z', 'Ġl', 'aura', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġlaunches', 'Ġsee', 'Ġfirst', 'Ġgalaxies', 'Ġdistant', 'Ġworlds', 'Ġn', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunched', 'Ġest', 'aturday', 'dec', 'ri', 'ane', 'Ġrocket', 'Ġfrench', 'Ġgu', 'iana', 'Ġsouth', 'Ġameric', 'Ġes', 'istant', 'world', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C325" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>['Ġstar', 'Ġ("', 'se', 'gment', 'Ġimage', 'Ġidentification', '").', 'Ġsegment', 'Ġindividually', 'Ġcorrected', 'Ġmajor', 'Ġfocusing', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġerrors', 'Ġusing', 'Ġtechnique', 'Ġcalled', 'Ġphase', 'Ġretrieval', 'Ġresulting', 'Ġseparate', 'Ġgood', 'Ġquality', 'Ġimages', 'Ġmirror', 'Ġsegments', 'Ġ("', 'se', 'gment', 'Ġalignment', '").', 'Ġimages', 'Ġsegment', 'Ġmoved', 'Ġprecisely', 'Ġoverlap', 'Ġcreate', 'Ġsingle', 'Ġimage', 'Ġ("', 'image', 'Ġstacking', '").', 'Ġmirrors', 'Ġpositioned', 'Ġalmost', 'Ġcorrect', 'Ġimages', 'Ġfine', 'Ġtuned', 'Ġoperational', 'Ġaccuracy', 'Ġnan', 'ometers', 'Ġless', 'Ġone', 'Ġwavelength', 'Ġlight', 'Ġdetected', 'Ġtechnique', 'Ġcalled', 'Ġdispersed', 'Ġfringe', 'Ġsensing', 'Ġused', 'Ġcompare', 'Ġimages', 'Ġpair', 'ings', 'Ġmirrors', 'Ġallowing', 'Ġerrors', 'Ġcorrected', 'Ġ("', 'co', 'arse', 'Ġph', 'asing', '"),', 'Ġintroduced', 'Ġlight', 'Ġdef', 'ocus', 'Ġsegment', "'s", 'Ġimage', 'Ġallowing', 'Ġdetection', 'Ġcorrection', 'Ġalmost', 'Ġremaining', 'Ġerrors', 'Ġ("', 'fine', 'Ġph', 'asing', '").', 'Ġtwo', 'Ġprocesses', 'Ġrepeated', 'Ġthree', 'Ġtimes', 'Ġfine', 'Ġph', 'asing', 'Ġroutinely', 'Ġchecked', 'Ġthroughout', 'Ġtelescope', "'s", 'Ġoperation', 'Ġthree', 'Ġrounds', 'Ġcoarse', 'Ġfine', 'Ġph', 'asing', 'Ġtelescope', 'Ġwell', 'Ġaligned', 'Ġone', 'Ġplace', 'Ġn', 'irc', 'Ġfield', 'Ġview', 'Ġmeasurements', 'Ġmade', 'Ġvarious', 'Ġpoints', 'Ġcaptured', 'Ġimage', 'Ġacross', 'Ġinstruments', 'Ġcorrections', 'Ġcalculated', 'Ġdetected', 'Ġvariations', 'Ġintensity', 'Ġgiving', 'Ġwell', 'aligned', 'Ġoutcome', 'Ġacross', 'Ġinstruments', 'Ġ("', 'tel', 'esc', 'ope', 'Ġalignment', 'Ġinstrument', 'Ġfields', 'Ġview', '").', 'Ġfinally', 'Ġlast', 'Ġround', 'Ġfine', 'Ġph', 'asing', 'Ġchecks', 'Ġimage', 'Ġquality', 'Ġinstruments', 'Ġperformed', 'Ġensure', 'Ġsmall', 'Ġresidual', 'Ġerrors', 'Ġremaining', 'Ġprevious', 'Ġsteps', 'Ġcorrected', 'Ġ("', 'iter', 'ate', 'Ġalignment', 'Ġfinal', 'Ġcorrection', '").', 'Ġtelescope', "'s", 'Ġmirror', 'Ġsegments', 'Ġaligned', 'Ġable', 'Ġcapture', 'Ġprecise', 'Ġfocused', 'Ġimages', 'Ġpreparation', 'Ġalignment', 'Ġn', 'asa', 'Ġannounced', 'Ġut', 'c', 'Ġfe', 'b', 'ruary', 'Ġn', 'irc', 'Ġdetected', 'Ġtelescope', "'s", 'Ġfirst', 'Ġphotons', 'although', 'Ġyet', 'Ġcomplete', 'Ġimages', ').[', 'Ġfe', 'b', 'ruary', 'Ġn', 'asa', 'Ġannounced', 'Ġtelescope', 'Ġalmost', 'Ġcompleted', 'Ġphase', 'Ġalignment', 'Ġevery', 'Ġsegment', 'Ġprimary', 'Ġmirror', 'Ġlocated', 'Ġim', 'aged', 'Ġtarget', 'Ġstar', 'Ġsegments', 'Ġbrought', 'Ġapproximate', 'Ġalignment', 'Ġphase', 'Ġalignment', 'Ġcompleted', 'Ġfe', 'b', 'ruary', 'Ġweek', 'Ġlater', 'Ġphases', 'Ġalso', 'Ġcompleted']</t>
+          <t>['Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġtrack', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmission', 'Ġtimeline', 'Ġspace', 'Ġexplored', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunches', 'Ġfrench', 'Ġgu', 'iana', 'Ġbillion', 'Ġsuccessor', 'Ġhub', 'ble', 'Ġtelescope', 'Ġcapture', 'Ġlight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstars', 'Ġstudy', 'Ġdistant', 'Ġworlds', 'launch', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'live', 'Ġupdates', 'Ġweb', 'b', 'Ġtelescope', 'Ġlaunches', 'Ġlong', 'awaited', 'Ġjourney', 'Ġnew', 'ork', 'Ġtimes', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'bye', 'ennis', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunches', 'Ġjourney', 'Ġsee', 'Ġdawn', 'Ġstar', 'light', 'Ġastronomers', 'Ġj', 'ub', 'ilant', 'Ġspacecraft', 'Ġmade', 'Ġlaunch', 'pad', 'Ġfollowing', 'Ġdecades', 'Ġdelays', 'Ġcost', 'Ġoverrun', 'Ġweb', 'b', 'Ġset', 'Ġoffer', 'Ġnew', 'Ġkey', 'hole', 'Ġearliest', 'Ġmoments', 'Ġuniverse', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'l', 'iss', 'aj', 'ous', 'Ġorbit', 'Ġox', 'ford', 'Ġreference', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'j', 'w', 'st', 'Ġorbit', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġuser', 'Ġdocumentation', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'f', 'requently', 'Ġasked', 'Ġquestions', 'Ġlong', 'Ġweb', 'b', 'Ġmission', 'Ġlast', '?"', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġk', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C326" t="n">
@@ -4676,7 +4676,7 @@
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>['Ġmeant', 'Ġsegments', 'Ġworking', 'Ġunison', 'Ġhowever', 'Ġphases', 'Ġcomplete', 'Ġsegments', 'Ġstill', 'Ġacting', 'Ġsmaller', 'Ġtelescopes', 'Ġrather', 'Ġone', 'Ġlarger', 'Ġone', 'Ġtime', 'Ġprimary', 'Ġmirror', 'Ġcommissioned', 'Ġhundreds', 'Ġinstrument', 'Ġcommission', 'ing', 'Ġcalibration', 'Ġtasks', 'Ġalso', 'Ġongoing', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġphase', 'Ġinterim', 'Ġimage', 'Ġannot', 'ated', 'Ġrelated', 'Ġmirror', 'Ġsegments', 'Ġtook', 'Ġimage', 'Ġphase', 'Ġannot', 'ated', 'Ġcompletion', 'Ġimage', 'Ġphase', 'Ġcompletion', 'Ġshowing', 'Ġeffects', 'Ġsegment', 'Ġalignment', 'Ġphase', 'Ġcompletion', 'Ġshowing', 'Ġsegments', 'st', 'acked', 'Ġsingle', 'Ġimage', 'Ġstar', 'mass', 'Ġcaptured', 'Ġn', 'irc', 'Ġinstrument', 'sel', 'ï', '¬', 'ģ', 'e', 'Ġtaken', 'Ġn', 'irc', 'Ġalignment', 'Ġprocess', 'Ġimage', 'Ġcomparison', 'old', 'Ġsp', 'itzer', 'Ġnew', 'Ġalignment', 'Ġn', 'asa', 'esa', 'cs', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'Ġsensors', 'Ġweb', 'b', 'âĢ', 'Ļ', 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġweb', 'b', 'Ġobserving', 'Ġtime', 'Ġallocated', 'Ġgeneral', 'Ġobservers', 'go', 'Ġprogram', 'Ġguaranteed', 'Ġtime', 'Ġobservations', 'g', 'Ġprogram', 'Ġdirector', "'s", 'Ġdiscretionary', 'Ġearly', 'Ġrelease', 'Ġscience', 'dd', 'ers', 'Ġprogram', 'Ġg', 'Ġprogram', 'Ġprovides', 'Ġguaranteed', 'Ġobserving', 'Ġtime', 'Ġscientists', 'Ġdeveloped', 'Ġhardware', 'Ġsoftware', 'Ġcomponents', 'Ġobserv', 'atory', 'Ġgo', 'Ġprogram', 'Ġprovides', 'Ġastronomers', 'Ġallocation', 'Ġobservation', 'Ġtime', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġopportunity', 'Ġapply', 'Ġobserving', 'Ġtime', 'Ġrepresent', 'Ġbulk', 'Ġobserving', 'Ġtime', 'Ġgo', 'Ġprograms', 'Ġselected', 'Ġpeer', 'Ġreview', 'Ġtime', 'Ġallocation', 'Ġcommittee', 'ac', 'Ġsimilar', 'Ġproposal', 'Ġreview', 'Ġprocess', 'Ġused', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'mber', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġannounced', 'Ġselection', 'Ġdirector', "'s", 'Ġdiscretionary', 'Ġearly', 'Ġrelease', 'Ġscience', 'dd', 'ers', 'Ġprograms', 'Ġchosen', 'Ġcompetitive', 'Ġproposal', 'Ġprocess', 'Ġobservations', 'Ġprograms', 'Ġearly', 'Ġrelease', 'Ġobservations', 'ero', ')[', 'Ġobtained', 'Ġfirst', 'Ġfive', 'Ġmonths', 'Ġweb', 'b', 'Ġscience', 'Ġoperations', 'Ġend', 'Ġcommission', 'ing', 'Ġperiod', 'Ġtotal', 'Ġhours', 'Ġobserving', 'Ġtime', 'Ġawarded', 'Ġprograms', 'Ġspan', 'Ġscience', 'Ġtopics', 'Ġincluding', 'Ġsolar', 'Ġsystem', 'Ġex', 'oplan', 'ets', 'Ġstars', 'Ġstar', 'Ġformation', 'Ġnearby', 'Ġdistant', 'Ġgalaxies', 'Ġgravitational', 'Ġlenses']</t>
+          <t>['n', 'asa', 'Ġsays', 'Ġweb', 'b', "'s", 'Ġexcess', 'Ġfuel', 'Ġlikely', 'Ġextend', 'Ġlifetime', 'Ġexpectations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary', 'Ġhail', 'ri', 'ane', 'Ġrocket', 'Ġdoubled', 'Ġweb', 'b', 'Ġtelescope', "'s", 'Ġlifetime', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'os', 'Ġj', 'athan', 'Ġjan', 'uary', 'j', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġcompletes', 'Ġepic', 'Ġdeployment', 'Ġsequence', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġp', 'ult', 'ar', 'ova', 'ere', 'za', 'Ġde', 'cember', "'s", 'Ġtruly', 'Ġchrist', 'mas', "':", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'ulet', 'ide', 'Ġlaunch', 'Ġn', 'asa', 'joy', 'ed', 'Ġh', 'n', 'asa', 'action', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcamera', 'Ġcry', 'ote', 'chn', 'ic', 'Ġupper', 'Ġstage', 'Ġdec', 'Ġview', 'Ġnewly', 'Ġseparated', 'Ġj', 'w', 'st', 'Ġseen', 'Ġcry', 'ote', 'chn', 'ic', 'Ġupper', 'Ġstage', 'Ġarchived', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġp', 'ult', 'ar', 'ova', 'ere', 'za', 'Ġde', 'cember', "'s", 'Ġtruly', 'Ġchrist', 'mas', "':", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'ulet', 'ide', 'Ġlaunch', 'Ġn', 'asa', 'joy', 'ed', 'Ġh', 'n', 'asa', 'action', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdeployment', 'Ġsequence', 'nom', 'inal', 'Ġpp', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġwar', 'ren', 'Ġhay', 'gen', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġen', 'Ġroute', 'Ġdeployment', 'Ġsequence', 'Ġunderway', 'Ġce', 'way', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġjan', 'uary', 'n', 'asa', 'Ġthrilled', 'Ġweb']</t>
         </is>
       </c>
       <c r="C327" t="n">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>['Ġqu', 'ars', 'Ġ', 'ers', 'Ġprograms', 'Ġuse', 'Ġtotal', 'Ġhours', 'Ġobserving', 'Ġtime', 'Ġtelescope', 'Ġincluding', 'Ġweb', 'b', 'Ġobserving', 'heads', 'Ġslew', 'Ġtime', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprograms', 'Ġname', 'Ġprincipal', 'Ġinvestigator', 'Ġcategory', 'Ġobservation', 'Ġtime', 'hours', 'Ġradi', 'ative', 'Ġfeedback', 'Ġmassive', 'Ġstars', 'Ġtraced', 'Ġmult', 'iband', 'Ġimaging', 'Ġspect', 'rosc', 'opic', 'Ġmosa', 'ics', 'liv', 'ier', 'Ġb', 'ern', 'Ã©', 'Ġstellar', 'Ġphysics', 'Ġice', 'age', 'Ġchemical', 'Ġevolution', 'Ġ', 'ices', 'Ġstar', 'Ġformation', 'Ġmel', 'issa', 'cc', 'l', 'ure', 'Ġstellar', 'Ġphysics', 'Ġlooking', 'Ġglass', 'Ġj', 'w', 'st', 'Ġexploration', 'Ġgalaxy', 'Ġformation', 'Ġevolution', 'Ġcosmic', 'Ġdawn', 'Ġpresent', 'Ġday', 'mm', 'Ġtre', 'u', 'Ġgalaxies', 'Ġj', 'w', 'st', 'Ġstudy', 'Ġstar', 'burst', 'agn', 'Ġconnection', 'Ġmerging', 'Ġl', 'ir', 'gs', 'Ġle', 'e', 'Ġarm', 'us', 'Ġgalaxies', 'Ġresolved', 'Ġstellar', 'Ġpopulations', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'aniel', 'Ġstellar', 'Ġpopulations', 'Ġimaging', 'Ġspect', 'rosc', 'opy', 'Ġqu', 'asar', 'Ġhosts', 'Ġj', 'w', 'st', 'Ġanalyzed', 'Ġpowerful', 'Ġnew', 'Ġps', 'f', 'Ġdecom', 'position', 'Ġspectral', 'Ġanalysis', 'Ġpackage', 'Ġdomin', 'ika', 'Ġw', 'yle', 'z', 'al', 'ek', 'Ġmassive', 'Ġblack', 'Ġholes', 'Ġgalaxies', 'Ġcosmic', 'Ġevolution', 'Ġearly', 'Ġrelease', 'Ġscience', 'ce', 'ers', 'Ġsurvey', 'Ġste', 'ven', 'Ġfin', 'kel', 'stein', 'Ġgalaxies', 'Ġestablishing', 'Ġextreme', 'Ġdynamic', 'Ġrange', 'Ġj', 'w', 'st', 'Ġdecoding', 'Ġsmoke', 'Ġsignals', 'Ġglare', 'Ġwolf', 'ray', 'et', 'Ġbinary', 'Ġr', 'yan', 'Ġl', 'au', 'Ġstellar', 'Ġphysics', 'Ġtemplates', 'Ġtargeting', 'Ġextremely', 'Ġmagn', 'ï', '¬', 'ģ', 'ed', 'Ġpan', 'chrom', 'atic', 'Ġlens', 'ed', 'Ġarcs', 'Ġextended', 'Ġstar', 'Ġformation', 'Ġj', 'ane', 'Ġrig', 'Ġgalaxies', 'Ġnuclear', 'Ġdynamics', 'Ġnearby', 'Ġse', 'f', 'ert', 'Ġn', 'ir', 'spec', 'Ġintegral', 'Ġfield', 'Ġspect', 'rosc', 'opy', 'Ġmist', 'Ġbent', 'z', 'Ġmassive', 'Ġblack', 'Ġholes', 'Ġgalaxies', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'et', 'Ġcommunity', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġn', 'atalie', 'Ġbat', 'al', 'ha', 'Ġplanets', 'Ġplanet', 'Ġformation', 'Ġ', 'ers', 'Ġobservations', 'Ġj', 'ov', 'ian', 'Ġsystem', 'Ġdemonstration', 'Ġj', 'w', 'st', "'s", 'Ġcapabilities', 'Ġsolar', 'Ġsystem', 'Ġscience', 'Ġde', 'Ġp', 'ater', 'Ġsolar', 'Ġsystem', 'Ġhigh', 'Ġcontrast', 'Ġimaging', 'Ġex', 'oplan', 'ets', 'Ġex', 'oplan']</t>
+          <t>['b', 'Ġspace', 'Ġtelescope', 'Ġdeploy', 'Ġsun', 'Ġshield', 'Ġev', 'ades', 'Ġmany', 'Ġpotential', 'single', 'point', 'Ġfailures', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'g', 'imb', 'aled', 'Ġantenna', 'Ġassembly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġk', 'Ġde', 'cember', 'Ġfirst', 'Ġmid', 'course', 'Ġcorrection', 'Ġburn', 'Ġn', 'asa', 'Ġblogs', 'Ġarchived', 'web', 'arch', 'iv', 'Ġn', 'burn', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġk', 'Ġde', 'cember', 'bb', "'s", 'Ġsecond', 'Ġmid', 'course', 'Ġcorrection', 'Ġburn', 'blogs', 'nas', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġfisher', 'Ġal', 'ise', 'Ġde', 'cember', 'bb', "'s", 'Ġaft', 'Ġmomentum', 'Ġflap', 'Ġdeployed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġlyn', 'ch', 'Ġpat', 'rick', 'Ġde', 'cember', 'Ġweb', 'b', "'s", 'Ġmid', 'bo', 'oms', 'Ġextended', 'Ġsun', 'shield', 'Ġtakes', 'Ġshape', 'Ġe', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġes', 'shape', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġjan', 'uary', 'Ġlyn', 'ch', 'Ġpat', 'rick', 'Ġde', 'cember', 'first', 'Ġtwo', 'Ġsun', 'shield', 'Ġmid', 'bo', 'oms', 'Ġdeploy', 'blogs', 'na', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'secondary', 'Ġmirror', 'Ġdeployment', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'first', 'Ġtwo', 'Ġprimary', 'Ġmirror', 'Ġwings', 'Ġunfolds', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary']</t>
         </is>
       </c>
       <c r="C328" t="n">
@@ -4702,7 +4702,7 @@
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>['etary', 'Ġsystems', 'Ġj', 'w', 'st', 'asha', 'Ġh', 'ink', 'ley', 'Ġplanets', 'Ġplanet', 'Ġformation', 'Ġgo', 'Ġcycle', '000', 'Ġhours', 'Ġobservation', 'Ġtime', 'Ġavailable', 'Ġallocate', 'Ġproposals', 'Ġsubmitted', 'Ġrequesting', 'Ġtotal', 'Ġhours', 'Ġobservation', 'Ġtime', 'Ġselection', 'Ġcycle', 'Ġgo', 'Ġprograms', 'Ġannounced', 'Ġmarch', 'Ġprograms', 'Ġapproved', 'Ġincluded', 'Ġlarge', 'Ġprograms', 'Ġtreasury', 'Ġprograms', 'Ġproducing', 'Ġdata', 'Ġpublic', 'Ġaccess', 'Ġcycle', 'Ġgo', 'Ġprogram', 'Ġannounced', 'Ġmay', 'Ġweb', 'b', 'Ġscience', 'Ġobservations', 'Ġnom', 'inally', 'Ġscheduled', 'Ġweekly', 'Ġincrements', 'Ġobservation', 'Ġplan', 'Ġevery', 'Ġweek', 'Ġpublished', 'ond', 'ays', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġfinished', 'Ġcommission', 'ing', 'Ġactivities', 'Ġready', 'Ġbegin', 'Ġfull', 'Ġscientific', 'Ġoperations', 'Ġj', 'uly', 'Ġexceptions', 'Ġexperiment', 'Ġdata', 'Ġkept', 'Ġprivate', 'Ġone', 'Ġyear', 'Ġexclusive', 'Ġuse', 'Ġscientists', 'Ġrunning', 'Ġparticular', 'Ġexperiment', 'Ġgeneral', 'Ġobserver', 'Ġprogram', 'Ġscientific', 'Ġresults', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġhub', 'ble', 'Ġcompared', 'Ġweb', 'b', ')[', 'Ġdeep', 'Ġfield', 'Ġgalaxy', 'Ġcluster', 'Ġsm', 'acs', 'Ġone', 'Ġyear', 'Ġraw', 'Ġdata', 'Ġreleased', 'Ġpublic', 'Ġfirst', 'Ġfull', 'color', 'Ġimages', 'Ġspect', 'rosc', 'opic', 'Ġdata', 'Ġreleased', 'Ġj', 'uly', 'Ġalso', 'Ġmarked', 'Ġofficial', 'Ġbeginning', 'Ġweb', 'b', "'s", 'Ġgeneral', 'Ġscience', 'Ġoperations', 'Ġunited', 'Ġstates', 'Ġpresident', 'Ġjo', 'e', 'Ġbid', 'en', 'Ġrevealed', 'Ġfirst', 'Ġimage', 'Ġweb', 'b', "'s", 'Ġfirst', 'Ġdeep', 'Ġfield', 'Ġj', 'uly', 'Ġadditional', 'Ġreleases', 'Ġaround', 'Ġtime', 'Ġcar', 'ina', 'Ġneb', 'ula', 'Ġyoung', 'Ġstar', 'forming', 'Ġregion', 'Ġcalled', 'Ġng', 'c', 'Ġdisplaying', 'cos', 'mic', 'Ġcliffs', 'Ġlight', 'years', 'Ġearth', 'p', 'b', 'Ġincluding', 'Ġanalysis', 'Ġatmosphere', 'Ġevidence', 'Ġwater', 'Ġaround', 'Ġgiant', 'Ġgas', 'Ġplanet', 'Ġorbiting', 'Ġdistant', 'Ġstar', 'Ġlight', 'years', 'Ġearth', 'Ġsouthern', 'Ġring', 'Ġneb', 'ula', 'Ġclouds', 'Ġgas', 'Ġdust', 'Ġexpelled', 'Ġdying', 'Ġstar', 'Ġlight', 'years', 'Ġearth', 'Ġstep', 'han', "'s", 'Ġquint', 'et', 'Ġvisual', 'Ġdisplay', 'Ġï', '¬', 'ģ', 'Ġgalaxies', 'Ġcoll', 'iding', 'Ġgas', 'Ġdust', 'Ġclouds', 'Ġcreating', 'Ġnew', 'Ġstars', 'Ġfour', 'Ġcentral', 'Ġgalaxies', 'Ġmillion', 'Ġlight', 'years', 'Ġearth', 'Ġsm', 'acs', 'Ġj', '07', 'Ġgalaxy', 'Ġcluster', 'Ġred']</t>
+          <t>['Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'primary', 'Ġmirror', 'Ġwings', 'Ġdeployed', 'Ġmajor', 'Ġdeployments', 'Ġcomplete', 'plete', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary', 'rem', 'ark', 'ably', 'Ġn', 'asa', 'Ġcompleted', 'Ġdeployment', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġcans', 'ci', 'enc', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'space', 'Ġtelescope', "'s", 'gold', 'en', 'Ġeye', 'Ġopens', 'Ġlast', 'Ġmajor', 'Ġhurdle', 'Ġphys', 'org', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'bb', "'s", 'Ġjourney', 'Ġnearly', 'Ġcomplete', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġjan', 'uary', 'Ġmillion', 'mile', 'Ġjourney', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġreaches', 'Ġdestination', 'Ġtelescope', "'s", 'Ġsafe', 'Ġarrival', 'Ġrelief', 'Ġscientists', 'Ġplan', 'Ġspend', 'Ġnext', 'Ġyears', 'Ġusing', 'Ġstudy', 'Ġancient', 'Ġgalaxies', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'orb', 'ital', 'Ġinsertion', 'Ġburn', 'Ġsuccess', 'Ġweb', 'b', 'Ġarrives', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'bl', 'Ġblogs', 'n', 'asa', 'gov', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġruns', 'Ġtechnical', 'Ġissue', 'Ġind', 'ian', 'Ġexpress', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'bb', 'Ġmirror', 'Ġsegment', 'Ġdeployments', 'Ġcomplete', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'blogs', 'na', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'bb', 'Ġbegins', 'Ġmonths', 'long', 'Ġmirror', 'Ġalignment', 'Ġj', 'ames', 'Ġweb']</t>
         </is>
       </c>
       <c r="C329" t="n">
@@ -4715,7 +4715,7 @@
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>['shift', 'Ġdistant', 'Ġbackground', 'Ġgalaxies', 'Ġwhose', 'Ġimages', 'Ġdistorted', 'Ġmagn', 'ï', '¬', 'ģ', 'ed', 'Ġdue', 'Ġgravitational', 'Ġlens', 'ing', 'Ġcluster', 'Ġimage', 'Ġcalled', 'Ġweb', 'b', "'s", 'Ġfirst', 'Ġdeep', 'Ġfield', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġpresented', 'Ġimages', 'Ġj', 'upiter', 'Ġrelated', 'Ġareas', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġincluding', 'Ġinfrared', 'Ġviews', 'Ġpre', 'print', 'Ġreleased', 'Ġaround', 'Ġtime', 'Ġn', 'asa', 'Ġes', 'Ġc', 'sa', 'Ġscientists', 'Ġstated', 'almost', 'Ġacross', 'Ġboard', 'Ġscience', 'Ġperformance', 'Ġj', 'w', 'st', 'Ġbetter', 'Ġexpected', '".', 'Ġdocument', 'Ġdescribed', 'Ġseries', 'Ġobservations', 'Ġcommission', 'ing', 'Ġinstruments', 'Ġcaptured', 'Ġspect', 'ra', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'ets', 'Ġprecision', 'Ġbetter', 'Ġper', 'Ġdata', 'Ġpoint', 'Ġtracked', 'Ġmoving', 'Ġobjects', 'Ġspeeds', 'Ġtwice', 'Ġfast', 'Ġrequirement', 'Ġalso', 'Ġobtained', 'Ġspect', 'ra', 'Ġhundreds', 'Ġstars', 'Ġsimultaneously', 'Ġdense', 'Ġfield', 'Ġtowards', 'Ġmil', 'ky', 'Ġway', 'Ġgalactic', 'Ġcenter', 'Ġtargets', 'Ġincluded', ':[', 'Ġmoving', 'Ġtargets', 'Ġj', 'upiter', 'including', 'Ġrings', 'Ġmoons', 'Ġeuro', 'pa', 'Ġmet', 'Ġasteroids', 'Ġr', 'oman', 'Ġpe', 'ith', 'Ġten', 'zing', 'Ġr', 'ump', 'el', 'st', 'il', 'z', 'Ġk', 'le', 'op', 'atra', 'Ġst', 'ear', 'ns', 'Ġwil', 'son', 'har', 'rington', 'Ġn', 'irc', 'Ġgr', 'ism', 'Ġtime', 'series', 'Ġn', 'ir', 'iss', 'oss', 'Ġn', 'ir', 'spec', 'Ġbots', 'Ġmode', 'Ġj', 'upiter', 'sized', 'Ġplanet', 'Ġn', 'ir', 'iss', 'Ġaperture', 'Ġmask', 'ing', 'Ġinter', 'fer', 'ometry', 'ami', '):', 'Ġclear', 'Ġdetection', 'Ġlow', 'mass', 'Ġcompanion', 'Ġstar', 'Ġab', 'ad', 'us', 'Ġc', 'Ġseparation', 'Ġarc', 'seconds', 'Ġprimary', 'Ġfirst', 'Ġfull', 'color', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġobservation', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdemonstration', 'Ġspace', 'Ġmir', 'Ġlow', 'resolution', 'Ġspect', 'rosc', 'opy', 'l', 'rs', '):', 'Ġhot', 'Ġsuper', 'earth', 'Ġplanet', 'Ġaround', 'Ġbright', 'war', 'f', 'Ġstar', 'red', 'ar', 'w', 'f', 'Ġstar', ')[', 'Ġwithin', 'Ġtwo', 'Ġweeks', 'Ġfirst', 'Ġweb', 'b', 'Ġimages', 'Ġseveral', 'Ġpre', 'print', 'Ġpapers', 'Ġdescribed', 'Ġwide', 'Ġrange', 'Ġhigh', 'Ġred', 'shift', 'Ġlumin', 'ous', 'pres', 'umably', 'Ġlarge', 'Ġgalaxies', 'Ġbelieved', 'Ġdate', 'Ġmillion', 'Ġyears', 'z']</t>
+          <t>['b', 'Ġspace', 'Ġtelescope', 'blogs', 'n', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'phot', 'ons', 'Ġincoming', 'Ġweb', 'b', 'Ġteam', 'Ġbegins', 'Ġalign', 'ing', 'Ġtelescope', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'pe', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'follow', 'ing', 'Ġweb', 'b', "'s", 'Ġarrival', 'Ġtelescope', 'Ġcommission', 'ing', 'Ġset', 'Ġbegin', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġjan', 'uary', 'Ġarchived', 'set', 'begin', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsim', 'bad', 'Ġcentre', 'Ġde', 'n', 'Ã©', 'es', 'Ġastron', 'om', 'iques', 'Ġde', 'Ġstr', 'bourg', 'Ġretrieved', 'Ġjan', 'uary', 'v', 'ors', 'ky', 'Ġge', 'orge', 'Ġfe', 'b', 'ruary', 'bb', 'Ġspace', 'Ġtelescope', 'Ġsuccessfully', 'Ġsees', 'Ġfirst', 'Ġgl', 'immer', 'Ġlight', 'Ġgo', 'Ġhistory', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstar', 'Ġspotted', 'Ġbillion', 'Ġspace', 'Ġtelescope', 'Ġg', 'iz', 'mod', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhood', 'Ġab', 'Ġle', 'e', 'Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdetected', 'Ġfirst', 'Ġsignal', "'re", 'Ġwatching', 'Ġfuture', 'Ġunfold', 'Ġreal', 'Ġtime', 'Ġfut', 'ur', 'ism', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'phot', 'ons', 'Ġreceived', 'Ġweb', 'b', 'Ġsees', 'Ġfirst', 'Ġstar', 'Ġtimes', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'http', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġn', 'irc', 'Ġinstrument', "'s", 'Ġdetectors', 'Ġsaw', 'st', 'Ġphotons', 'Ġstar', 'light', 'nas', 'aw', 'eb', 'b', 'Ġyet', 'Ġready', 'Ġscience', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmany', 'Ġsteps', 'Ġcapture', 'Ġimages', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġunfocused', 'Ġused', 'Ġslowly', 'Ġï', '¬', 'ģ', 'ne', 'une', 'Ġoptics', 'Ġtwitter', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C330" t="n">
@@ -4728,7 +4728,7 @@
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>['Ġmillion', 'Ġyears', 'Ġbig', 'Ġbang', 'Ġfar', 'Ġearlier', 'Ġpreviously', 'Ġknown', 'Ġaug', 'ust', 'Ġn', 'asa', 'Ġreleased', 'Ġlarge', 'Ġmosaic', 'Ġimage', 'Ġindividual', 'Ġframes', 'Ġtaken', 'Ġnear', 'Ġinfrared', 'Ġcamera', 'n', 'irc', 'Ġweb', 'b', 'Ġnumerous', 'Ġearly', 'Ġgalaxies', 'Ġearly', 'Ġgalaxies', 'Ġobserved', 'Ġweb', 'b', 'Ġlike', 'Ġce', 'ers', 'Ġestimated', 'Ġred', 'shift', 'Ġapproximately', 'Ġz', 'Ġcorresponding', 'Ġmillion', 'Ġyears', 'Ġbig', 'Ġbang', 'Ġhigh', 'Ġred', 'shift', 'Ġgalaxy', 'Ġse', 'pt', 'ember', 'Ġprim', 'ordial', 'Ġblack', 'Ġholes', 'Ġproposed', 'Ġexplaining', 'Ġunexpectedly', 'Ġlarge', 'Ġearly', 'Ġgalaxies', 'Ġj', 'une', 'Ġdetection', 'Ġorganic', 'Ġmolecules', 'Ġbillion', 'Ġlight', 'years', 'Ġaway', 'Ġgalaxy', 'Ġcalled', 'pt', '04', 'Ġusing', 'Ġweb', 'b', 'Ġtelescope', 'Ġannounced', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġcelebrated', 'Ġfirst', 'Ġyear', 'Ġoperations', 'Ġrelease', 'Ġweb', 'b', 'âĢ', 'Ļ', 'Ġimage', 'Ġsmall', 'Ġstar', 'forming', 'Ġregion', 'Ġr', 'ho', 'phi', 'uchi', 'Ġcloud', 'Ġcomplex', 'Ġlight', 'Ġyears', 'Ġaway', 'Ġfirst', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġreleased', 'Ġj', 'uly', 'Ġcosmic', 'Ġcliffs', 'Ġcar', 'ina', 'Ġneb', 'ula', 'ng', 'c', 'n', 'irc', 'Ġcar', 'ina', 'Ġneb', 'ula', 'ng', 'c', 'mir', 'Ġsouthern', 'Ġring', 'Ġneb', 'ula', 'ng', 'c', 'Ġleft', 'Ġn', 'irc', 'Ġright', 'Ġmir', 'Ġweb', 'b', "'s", 'Ġfirst', 'Ġdeep', 'Ġfield', 'sm', 'acs', 'Ġ07', 'Ġleft', 'Ġmir', 'Ġright', 'Ġn', 'irc', 'Ġstep', 'han', "'s", 'Ġquint', 'et', 'n', 'irc', 'mir', 'Ġcomposite', 'Ġgallery', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġspectrum', 'p', 'b', 'Ġmedia', 'Ġrelated', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'imedia', 'Ġcommons', 'Ġspacecraft', 'Ġattitude', 'Ġcontrol', 'Ġprocess', 'Ġcontrolling', 'Ġorientation', 'Ġaerospace', 'Ġvehicle', 'Ġtimeline', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlib', 'ration', 'Ġpoint', 'Ġorbit', 'Ġqu', 'iper', 'iod', 'ic', 'Ġorbit', 'Ġaround', 'Ġlag', 'range', 'Ġpoint', 'Ġlist', 'Ġdeep', 'Ġï', '¬', 'ģ', 'e', 'ld', 'Ġlist', 'Ġlargest', 'Ġinfrared', 'Ġtelescopes', 'Ġlist', 'Ġlargest', 'Ġoptical', 'ï', '¬', 'Ĥ', 'ect', 'ing', 'Ġtelescopes', 'Ġlist', 'Ġspace', 'Ġtelescopes', 'Ġn', 'ancy', 'Ġgrace', 'Ġr', 'oman', 'Ġspace', 'Ġtelescope', 'Ġplanned', 'Ġlaunch', 'Ġlater', 'Ġmay', 'Ġnew', 'Ġworlds', 'Ġmission', 'prop', 'osed', 'Ġocc', 'ul']</t>
+          <t>['Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'bb', 'Ġteam', 'Ġbrings', 'Ġdots', 'Ġstar', 'light', 'Ġhex', 'agonal', 'Ġformation', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'bb', 'Ġmirror', 'Ġalignment', 'Ġcontinues', 'Ġsuccessfully', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'blogs', 'n', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfind', 'Ġfirst', 'Ġgalaxies', 'Ġweb', 'b', 'Ġpays', 'Ġattention', 'Ġdetail', 'Ġtheory', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġaug', 'ust', 'mass', 'Ġj', 'Ġfacts', 'Ġstar', 'Ġuniverse', 'Ġguide', 'Ġguide', 'Ġspace', 'Ġplanets', 'Ġrest', 'Ġuniverse', 'Ġuniverse', 'guide', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġk', 'l', 'ug', 'er', 'Ġje', 'ff', 'rey', 'Ġmarch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġtook', 'Ġbest', 'Ġpicture', 'Ġyet', 'ht', 'Ġtime', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'kinson', 'Ġn', 'ancy', 'Ġmay', 'Ġfinally', 'Ġcompare', 'Ġweb', 'b', 'Ġinfrared', 'Ġobserv', 'atories', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġ', 'erv', 'atories', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'bb', 'Ġfull', 'Ġfocus', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'bb', "'s", 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġprovides', 'Ġpreview', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'blog', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'c', 'alls', 'Ġproposals', 'Ġpolicy', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'select', 'ions', 'Ġmade', 'Ġj', 'w', 'st', 'Ġdirector', "'s", 'Ġdiscretionary']</t>
         </is>
       </c>
       <c r="C331" t="n">
@@ -4741,7 +4741,7 @@
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>['ter', 'Ġj', 'w', 'st', 'Ġphysical', 'Ġcos', 'mology', 'Ġbranch', 'Ġcos', 'mology', 'Ġstudies', 'Ġmathematical', 'Ġmodels', 'Ġuniverse', 'Ġsatellite', 'Ġbus', 'Ġmain', 'Ġbody', 'Ġstructural', 'Ġcomponent', 'Ġsatellite', 'Ġsolar', 'Ġpanels', 'Ġspacecraft', 'Ġphot', 'ov', 'olt', 'aic', 'Ġsolar', 'Ġpanels', 'Ġspacecraft', 'Ġoperating', 'Ġinner', 'Ġsolar', 'Ġsystem', 'Ġspacecraft', 'Ġdesign', 'Ġspacecraft', 'Ġthermal', 'Ġcontrol', 'Ġprocess', 'Ġkeeping', 'Ġparts', 'Ġspacecraft', 'Ġwithin', 'Ġacceptable', 'Ġtemperature', 'Ġranges', 'Ġj', 'w', 'st', 'Ġdesigned', 'Ġrequirement', 'Ġtrack', 'Ġobjects', 'Ġmove', 'Ġfast', 'Ġmars', 'Ġmaximum', 'Ġapparent', 'Ġspeed', 'Ġmas', 'Ġvalue', 'Ġgiven', 'Ġtechnical', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'cation', 'e', 'Ġnominal', 'Ġvalue', 'Ġcommission', 'ing', 'Ġvarious', 'Ġasteroids', 'Ġobserved', 'Ġdetermine', 'Ġactual', 'Ġlimitation', 'Ġspeed', 'Ġobjects', 'Ġturned', 'Ġmas', 'Ġtwice', 'Ġnominal', 'Ġvalue', 'Ġtracking', 'Ġrates', 'âĢĵ', 'Ġmas', 'Ġshowed', 'Ġaccur', 'acies', 'Ġsimilar', 'Ġtracking', 'Ġslower', 'Ġtargets', 'Ġthus', 'Ġtelescope', 'Ġable', 'Ġobserve', 'Ġalso', 'Ġnear', 'earth', 'Ġasteroids', 'ne', 'ets', 'Ġcloser', 'Ġper', 'hel', 'ion', 'Ġinterstellar', 'Ġobjects', ']:', 'Ġlater', 'Ġexperience', 'Ġgained', 'Ġtracking', 'Ġspeed', 'Ġlimit', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġset', 'Ġmas', 'Ġroutine', 'Ġobservations', 'Ġhigher', 'Ġrates', 'Ġmas', 'Ġalso', 'Ġpossible', 'Ġspecial', 'Ġrequest', 'Ġneeds', 'Ġmultiple', 'Ġguide', 'Ġstars', 'Ġend', 'Ġintroduces', 'Ġcomplexity', 'ef', 'ï', '¬', 'ģ', 'ci', 'ency', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġobservation', 'Ġsuper', 'fast', 'Ġrate', 'Ġdart', 'Ġimpact', 'Ġexperiment', 'Ġse', 'pt', 'ember', 'Ġb', 'b', 'af', 'ï', '¬', 'Ĥ', 'ed', '",', 'Ġcontext', 'Ġmeans', 'Ġenclosed', 'Ġtube', 'Ġsimilar', 'Ġmanner', 'Ġconventional', 'Ġoptical', 'Ġtelescope', 'Ġhelps', 'Ġstop', 'Ġstray', 'Ġlight', 'Ġentering', 'Ġtelescope', 'Ġside', 'Ġactual', 'Ġexample', 'Ġsee', 'Ġfollowing', 'Ġlink', 'Ġfren', 'iere', 'Ġe', 'r', 'first', 'order', 'Ġdesign', 'Ġoptical', 'Ġb', 'af', 'ï', '¬', 'Ĥ', 'es', '".', 'Ġsociety', 'Ġphoto', 'opt', 'ical', 'Ġinstrument', 'ation', 'Ġengineers', 'sp', 'ie', 'Ġconference', 'Ġseries', 'Ġfirst', 'order', 'Ġdesign', 'Ġoptical', 'Ġb', 'af', 'ï', '¬', 'Ĥ', 'es', 'Ġradiation', 'Ġscattering', 'Ġoptical', 'Ġsystems', 'Ġvol', 'Ġpp', 'âĢĵ', 'Ġsee', 'Ġalso', 'Ġnotes', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġc', 'Ġmirror', 'Ġsegment']</t>
+          <t>['Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'director', "'s", 'Ġdiscretionary', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprograms', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġad', 'ams', 'Ġet', 'Ġal', 'jan', 'uary', 'iscovery', 'Ġproperties', 'Ġultra', 'high', 'Ġred', 'shift', 'Ġgalaxies', 'Ġj', 'w', 'st', 'Ġer', 'Ġsm', 'acs', 'Ġ07', 'Ġfield', 'Ġmonthly', 'Ġnotices', 'Ġroyal', 'Ġastronomical', 'Ġsociety', '):', 'âĢĵ', 'Ġar', 'x', 'iv', 'doi', 'org', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġha', 'oj', 'ing', 'Ġet', 'Ġal', 'jan', 'uary', 'first', 'Ġbatch', 'âĢĵ', 'Ġcandidate', 'Ġobjects', 'Ġrevealed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġearly', 'Ġrelease', 'Ġobservations', 'Ġsm', 'acs', 'Ġ07', 'doi', 'org', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġletters', 'Ġar', 'x', 'iv', 'ui', 'ads', 'rad', 'ative', 'Ġfeedback', 'Ġmassive', 'Ġstars', 'Ġtraced', 'Ġmult', 'iband', 'Ġimaging', 'Ġspect', 'rosc', 'opic', 'Ġmosaic', 'Ġarchived', 'ber', 'ne', 'pdf', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'ice', 'age', 'Ġchemical', 'Ġevolution', 'Ġ', 'ices', 'Ġstar', 'Ġformation', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġlooking', 'Ġglass', 'Ġj', 'w', 'st', 'Ġexploration', 'Ġgalaxy', 'Ġformation', 'Ġevolution', 'Ġcosmic', 'Ġdawn', 'Ġpresent', 'Ġday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġj', 'w', 'st', 'Ġstudy', 'Ġstar', 'burst', 'agn', 'Ġconnection', 'Ġmerging', 'Ġl', 'ir', 'gs', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġresolved', 'Ġstellar', 'Ġpopulations', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġarchived', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C332" t="n">
@@ -4754,7 +4754,7 @@
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>['Ġpositioned', 'Ġouter', 'Ġring', 'Ġsegments', 'Ġlocated', 'clock', 'Ġnumber', 'Ġclock', 'Ġface', 'Ġviewing', 'Ġprimary', 'Ġmirror', 'Ġface', 'Ġstar', 'Ġapproximately', 'Ġlight', 'years', 'Ġaway', 'Ġconstellation', 'Ġ', 'urs', 'Ġmajor', 'Ġstar', 'Ġspectral', 'Ġtype', 'Ġstar', 'Ġhigh', 'Ġproper', 'Ġmotion', 'Ġe', 'mass', 'Ġj', 'Ġalso', 'Ġknown', 'Ġun', 'sw', 'v', 'Ġty', 'c', 'Ġstar', 'Ġconstellation', 'Ġdr', 'aco', 'Ġmil', 'ky', 'Ġway', 'Ġlocated', 'Ġalmost', '000', 'Ġlight', 'Ġyears', 'Ġaway', 'Ġearth', 'Ġwithin', 'Ġdegree', 'Ġnorth', 'Ġe', 'cl', 'ipt', 'ic', 'Ġpole', 'Ġvisual', 'Ġapparent', 'Ġmagnitude', 'Ġmakes', 'Ġmuch', 'Ġfaint', 'Ġobserved', 'Ġnaked', 'Ġeye', 'Ġcooler', 'Ġsun', 'Ġtimes', 'Ġbrighter', 'Ġvisible', 'Ġlight', 'Ġconsequently', 'Ġsun', 'like', 'Ġstar', 'Ġmotion', 'Ġvector', 'Ġdirection', 'Ġsun', 'n', 'asa', 'Ġj', 'w', 'st', 'Ġpartners', 'Ġweb', 'b', 'Ġproject', '?"', 'Ġart', 'ners', 'Ġn', 'asa', 'Ġarchived', 'q', 'html', 'part', 'ners', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġke', 'l', 'Ġth', 'omas', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġcel', 'est', 'rak', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġfull', 'Ġgeneral', 'Ġpublic', 'Ġweb', 'b', 'Ġtelescope', 'n', 'asa', 'Ġml', 'h', 'owl', 'ong', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġsays', 'Ġweb', 'b', "'s", 'Ġexcess', 'Ġfuel', 'Ġlikely', 'Ġextend', 'Ġlifetime', 'Ġexpectations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', ')"', 'Ġn', 'id', 'Ġn', 'asa', 'Ġspace', 'Ġscience', 'Ġdata', 'Ġcoordinated', 'Ġarchive', 'Ġretrieved', 'Ġfe', 'b', 'ruary']</t>
+          <t>['Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġdomin', 'ika', 'Ġw', 'yle', 'z', 'al', 'ek', 'Ġimaging', 'Ġspect', 'rosc', 'opy', 'Ġqu', 'asar', 'Ġhosts', 'Ġj', 'w', 'st', 'Ġanalyzed', 'Ġpowerful', 'Ġnew', 'Ġps', 'f', 'Ġdecom', 'position', 'Ġspectral', 'Ġanalysis', 'Ġpackage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġcosmic', 'Ġevolution', 'Ġearly', 'Ġrelease', 'Ġscience', 'ce', 'ers', 'Ġsurvey', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'establish', 'ing', 'Ġextreme', 'Ġdynamic', 'Ġrange', 'Ġj', 'w', 'st', 'Ġdecoding', 'Ġsmoke', 'Ġsignals', 'Ġglare', 'Ġwolf', 'ray', 'et', 'Ġbinary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'tem', 'plates', 'Ġtargeting', 'Ġextremely', 'Ġmagn', 'ï', '¬', 'ģ', 'ed', 'Ġpan', 'chrom', 'atic', 'Ġlens', 'ed', 'Ġarcs', 'Ġextended', 'Ġstar', 'Ġformation', 'Ġarchived', 'Ġrs', 'rig', 'pdf', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'nuclear', 'Ġdynamics', 'Ġnearby', 'Ġse', 'f', 'ert', 'Ġn', 'ir', 'spec', 'Ġintegral', 'Ġfield', 'Ġspect', 'rosc', 'opy', 'st', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'et', 'Ġcommunity', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'ers', 'Ġobservations', 'Ġj', 'ov', 'ian', 'Ġsystem', 'Ġdemonstration', 'Ġj', 'w', 'st', "'s", 'Ġcapabilities', 'Ġsolar', 'Ġsystem', 'Ġscience', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'high', 'Ġcontrast', 'Ġimaging', 'Ġex', 'oplan', 'ets', 'Ġex', 'oplan', 'etary', 'Ġsystems', 'Ġj', 'w', 'st', 'Ġdf', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'j', 'w', 'st', 'Ġcycle', 'Ġgeneral', 'Ġobserver', 'Ġsubmission', 'Ġstatistics', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'sts', 'ci', 'Ġannounces', 'Ġj', 'w', 'st', 'Ġcycle', 'Ġgeneral', 'Ġobserver', 'Ġprogram', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'sts', 'ci', 'Ġannounces', 'Ġj', 'w', 'st', 'Ġcycle', 'Ġgeneral', 'Ġobserver', 'Ġprogram', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġretrieved', 'Ġmay', 'ob', 'serving', 'Ġschedules']</t>
         </is>
       </c>
       <c r="C333" t="n">
@@ -4767,7 +4767,7 @@
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>['bb', 'Ġkey', 'Ġfacts', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġn', 'asa', 'Ġretrieved', 'Ġapr', 'il', 'j', 'w', 'st', 'Ġorbit', 'Ġj', 'w', 'st', 'Ġuser', 'Ġdocumentation', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġtelescope', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġuser', 'Ġdocumentation', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġreferences', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġmos', 'k', 'owitz', 'Ġcl', 'ara', 'Ġde', 'cember', 'Ġj', 'w', 'st', 'Ġchanging', 'Ġview', 'Ġuniverse', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsparked', 'Ġnew', 'Ġera', 'Ġastronomy', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġarchived', 'http', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'bye', 'ennis', 'Ġaug', 'ust', 'Ġweb', 'b', 'Ġtelescope', 'Ġexpanded', 'Ġuniverse', 'Ġnew', 'Ġimages', 'Ġj', 'upiter', 'Ġgalactic', 'Ġsurvey', 'Ġspring', 'Ġforth', 'Ġn', 'asa', "'s", 'Ġnew', 'Ġobserv', 'atory', 'Ġcosmic', 'Ġaffairs', 'Ġcorrespondent', 'Ġconfess', 'es', "'t", 'Ġanticipate', 'Ġpower', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġaug', 'ust', 'Ġweb', 'b', 'Ġtelescope', 'Ġastonishing', 'Ġuniverse', 'Ġeven', 'Ġnew', 'Ġtool', "'t", 'Ġeverything', "'s", 'Ġcapturing', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlight', 'Ġemitted', 'Ġbig', 'Ġbang', 'Ġalready', 'Ġrevealing', 'Ġwonders', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'call', 'aghan', 'Ġj', 'athan', 'Ġjan', 'uary', 'j', 'w', 'st', 'Ġherald', 'Ġnew', 'Ġdawn', 'Ġex', 'oplan', 'et', 'Ġscience', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġopening', 'Ġexciting', 'Ġnew', 'Ġchapter', 'Ġstudy', 'Ġex', 'oplan', 'ets', 'Ġsearch', 'Ġlife', 'Ġbeyond', 'Ġearth', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġretrieved', 'Ġjan', 'uary']</t>
+          <t>['ules', 'Ġst', 'sci', 'edu', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġc', 'es', 'ari', 'Ġth', 'add', 'eus', 'Ġcenter', 'Ġn', 'asa', 'âĢ', 'Ļ', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġj', 'uly', 'Ġlast', 'Ġn', 'asa', "'s", 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġfully', 'Ġready', 'Ġscience', 'Ġsc', 'itech', 'daily', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġbart', 'els', 'ghan', 'Ġde', 'cember', 'n', 'asa', 'Ġmay', 'Ġunlock', 'Ġfuture', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdata', 'Ġspace', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġch', 'ow', 'Ġden', 'ise', 'Ġj', 'ach', 'uan', 'Ġj', 'uly', 'photos', 'Ġpictures', 'Ġweb', 'b', 'Ġtelescope', 'Ġcompare', 'Ġhub', 'ble', "'s", 'Ġn', 'asa', "'s", 'Ġbillion', 'Ġtelescope', 'Ġpeers', 'Ġdeeper', 'Ġspace', 'Ġever', 'Ġrevealing', 'Ġpreviously', 'Ġundet', 'ect', 'able', 'Ġdetails', 'Ġcosmos', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġdel', 'iso', 'red', 'ith', 'Ġlong', 'red', 'ith', 'Ġrot', 'hen', 'berg', 'Ġnic', 'olas', 'Ġj', 'uly', 'hub', 'ble', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġimages', 'Ġsee', 'Ġdifference', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġgarner', 'Ġrob', 'Ġj', 'uly', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġdelivers', 'Ġdeepest', 'Ġinfrared', 'Ġimage', 'Ġuniverse', 'Ġyet', 'http', 'Ġn', 'iverse', 'yet', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'bye', 'ennis', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġtank', 'ers', 'ley', 'Ġj', 'uly', 'b', 'iden', 'Ġn', 'asa', 'Ġshare', 'Ġfirst', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġimage', 'Ġwhite', 'Ġhouse', 'onday', 'Ġhumanity', 'Ġgot', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġglimpse', 'Ġobserv', 'atory', 'Ġspace', 'Ġseeing', 'Ġcluster', 'Ġearly', 'Ġgalaxies', 'ny', 'time', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġpac', 'ucci', 'Ġfab', 'io', 'Ġj', 'uly', 'Ġtaking', 'Ġpictures', 'nothing', 'Ġchanged', 'Ġastronomy']</t>
         </is>
       </c>
       <c r="C334" t="n">
@@ -4780,7 +4780,7 @@
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>['Ġfisher', 'Ġal', 'ise', 'Ġpin', 'ol', 'Ġnat', 'asha', 'Ġbet', 'z', 'Ġl', 'aura', 'Ġj', 'uly', 'president', 'Ġbid', 'en', 'Ġreveals', 'Ġfirst', 'Ġimage', 'Ġn', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġn', 'asa', 'Ġarchived', 'Ġscope', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'par', 'ison', 'Ġweb', 'b', 'Ġhub', 'ble', 'Ġtelescope', 'Ġweb', 'b', 'n', 'asa', 'j', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'Ġmill', 'er', 'Ġk', 'rina', 'Ġj', 'uly', 'Ġyear', 'Ġcosmic', 'Ġwonder', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġnew', 'Ġimage', 'Ġn', 'asa', 'Ġcommemor', 'ates', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġanniversary', 'Ġscience', 'Ġpowerful', 'Ġobserv', 'atory', 'Ġever', 'Ġsent', 'Ġspace', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġl', 'allo', 'Ġmatt', 'hew', 'exper', 'ience', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġyears', 'Ġarchetype', '".', 'Ġoptical', 'Ġengineering', '):', 'Ġ01', 'âĢĵ', '01', 'âĢĵ', 'Ġar', 'x', 'iv', '03', '0002', '03', '0002', 'l', 'mir', 'rors', 'Ġweb', 'b', 'n', 'asa', 'Ġweb', 'b', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġj', 'uly', 'Ġdeeper', 'Ġb', 'rian', 'Ġk', 'ober', 'lein', 'Ġbri', 'ank', 'ober', 'lein', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġscientists', 'Ġweb', 'b', 'Ġtelescope', 'n', 'asa', 'Ġts', 'html', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġshel', 'ton', 'Ġmarch', 'sh', 'attering', 'Ġcosmic', 'Ġdistance', 'Ġrecord', 'http', 'news', 'al', 'ale', 'Ġuniversity', 'Ġarchived', 'http', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'hub', 'ble', 'Ġbreaks', 'Ġcosmic', 'Ġdistance', 'Ġrecord', 'Ġsp', 'acet', 'el', 'esc', 'ope', 'org', 'Ġmarch', 'ic']</t>
+          <t>['Ġdeep', 'ï', '¬', 'ģ', 'e', 'ld', 'Ġimages', 'empty', 'Ġregions', 'Ġweb', 'b', 'Ġspace', 'Ġtelescopes', 'Ġrevealing', 'Ġuniverse', 'Ġever', 'Ġthought', 'Ġpossible', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġko', 'oser', 'anda', 'Ġj', 'uly', 'hub', 'ble', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġimages', 'Ġcompared', 'Ġsee', 'Ġdifference', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġbuilds', 'Ġhub', 'ble', "'s", 'Ġlegacy', 'Ġstunning', 'Ġnew', 'Ġviews', 'Ġcosmos', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġtim', 'mer', 'Ġjohn', 'Ġj', 'uly', 'n', 'asa', 'Ġnames', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'ģ', 'Ġtargets', 'Ġweb', 'b', 'Ġimages', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'first', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'Ġv', 'bb', 'ï', '¬', 'ģ', 'r', 'st', 'images', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġstir', 'one', 'Ġsh', 'annon', 'Ġj', 'uly', 'g', 'aw', 'king', 'Ġawe', 'Ġuniverse', 'Ġtogether', 'ny', 'time', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'bye', 'ennis', 'Ġchang', 'Ġk', 'enn', 'eth', 'ok', 'ol', 'Ġj', 'osh', 'ua', 'Ġj', 'uly', 'bb', 'Ġtelescope', 'Ġreveals', 'Ġnew', 'Ġvision', 'Ġancient', 'Ġuniverse', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġj', 'uly', 'n', 'asa', 'Ġshows', 'Ġweb', 'b', "'s", 'Ġview', 'Ġsomething', 'Ġcloser', 'Ġhome', 'Ġj', 'upiter', 'Ġpowerful', 'Ġtelescope', 'Ġhelp', 'Ġscientists', 'Ġmake', 'Ġdiscoveries', 'Ġwithin', 'Ġsolar', 'Ġsystem', 'Ġwell', 'Ġbeyond', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġast', 'ud', 'illo', 'def', 'ru', 'Ġn', '.;', 'Ġclout', 'ier', 'Ġr', '.;', 'Ġw', 'ang', 'Ġx']</t>
         </is>
       </c>
       <c r="C335" t="n">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>['04', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'es', 'ch', 'Ġp', '.;', 'Ġb', 'ram', 'mer', 'Ġg', '.;', 'Ġvan', 'Ġp', '.;', 'Ġet', 'Ġal', 'arch', 'Ġremarkably', 'Ġlumin', 'ous', 'Ġgalaxy', 'Ġz', 'Ġmeasured', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġgr', 'ism', 'Ġspect', 'rosc', 'opy', '".', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġar', 'x', 'iv', '03', '00', 'kinson', 'Ġn', 'ancy', 'hub', 'ble', 'Ġlooked', 'Ġback', 'Ġtime', 'Ġfar', 'Ġstill', "'t", 'Ġfind', 'Ġfirst', 'Ġstars', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġvia', 'Ġscience', 'alert', 'inf', 'rared', 'Ġastronomy', 'Ġearth', 'Ġorbit', 'Ġinfrared', 'Ġprocessing', 'Ġanalysis', 'Ġcenter', 'Ġn', 'asa', 'Ġsp', 'itzer', 'Ġscience', 'Ġcenter', 'Ġcal', 'ornia', 'Ġinstitute', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'http', 'ip', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġfisher', 'Ġal', 'ise', 'Ġj', 'uly', 'bb', 'Ġimages', 'Ġj', 'upiter', 'Ġavailable', 'Ġcommission', 'ing', 'Ġdata', 'mission', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġaug', 'ust', 'Ġrig', 'Ġj', 'ane', 'Ġper', 'rin', 'Ġmarsh', 'cel', 'w', 'ichael', 'Ġk', 'imble', 'Ġr', 'andy', 'Ġfried', 'man', 'Ġsc', 'ott', 'Ġl', 'allo', 'Ġmatt', 'yon', 'Ġren', 'Ã©', 'Ġfe', 'berg', 'Ġle', 'e', 'Ġfer', 'ruit', 'Ġpier', 'Ġgl', 'asse', 'Ġal', 'ist', 'air', 'Ġr', 'ie', 'ke', 'Ġmar', 'cia', 'Ġr', 'ie', 'ke', 'Ġge', 'orge', 'Ġet', 'Ġal', 'Ġscience', 'Ġperformance', 'Ġj', 'w', 'st', 'Ġcharacterized', 'Ġcommission', 'ing', '".', 'Ġpublications', 'Ġastronomical', 'Ġsociety', 'Ġpac', 'ï', '¬', 'ģ', 'c', '):', '001', 'Ġar', 'x', 'iv', '05', '05', 'Ġth', 'add', 'eus', 'Ġc', 'es', 'ari', 'Ġfe', 'b', 'ruary', 'breaking', 'Ġtracking', 'Ġspeed', 'Ġlimit', 'Ġweb', 'b', 'blog', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs']</t>
+          <t>['.;', 'es', 'ke', 'Ġj', '.;', 'Ġr', '.;', 'Ġhell', 'ier', 'Ġc', '.;', 'Ġr', 'icker', 'Ġg', '.;', 'Ġv', 'anders', 'pe', 'k', 'Ġr', '.;', 'Ġl', 'atham', '.;', 'Ġse', 'ager', '.;', 'Ġwin', 'n', 'Ġj', 'Ġn', '.;', 'Ġet', 'Ġal', 'Ġapr', 'il', 'Ġhot', 'Ġterrestrial', 'Ġplanet', 'Ġorbiting', 'Ġbright', 'Ġdwarf', 'Ġunveiled', 'ess', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġar', 'x', 'iv', '09', 'Ġ01', '09', 'Ġiss', 'n', 'Ġ0004', 'api', 'se', 'man', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'uly', 'kinson', 'Ġn', 'ancy', 'Ġaug', 'ust', "'s", 'Ġlargest', 'Ġimage', 'Ġj', 'w', 'st', 'Ġtaken', 'Ġfar', 'w', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġwh', 'itt', 'Ġke', 'lly', 'Ġk', 'izer', 'Ġaug', 'ust', 'bb', "'s", 'Ġlargest', 'Ġimage', 'Ġgalaxies', 'Ġyet', 'Ġearth', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'ed', 'inburgh', 'Ġastronomers', 'Ġï', '¬', 'ģ', 'nd', 'Ġdistant', 'Ġgalaxy', 'Ġearly', 'Ġdata', 'Ġnew', 'Ġspace', 'Ġtelescope', 'Ġenabled', 'Ġed', 'inburgh', 'Ġastronomers', 'Ġlocate', 'Ġdistant', 'Ġgalaxy', 'Ġever', 'Ġfound', 'Ġuniversity', 'Ġed', 'inburgh', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġplan', 'ck', 'Ġcollaboration', 'plan', 'ck', 'Ġresults', 'Ġvi', 'Ġcos', 'ological', 'Ġparameters', '".', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġpage', 'see', 'Ġpage', 'Ġtable', 'age', 'gy', 'r', '",', 'Ġlast', 'Ġcolumn', 'Ġar', 'x', 'iv', '07', '06', 'ui', 'ads', 'doi', 'org', 'Ġsid', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġboy', 'uan', 'Ġb', 'rom', 'Ġvol', 'ker', 'Ġse', 'pt', 'ember', 'ac', 'celer', 'ating', 'Ġearly', 'Ġmassive', 'Ġgalaxy', 'Ġformation', 'Ġprim', 'ordial', 'Ġblack', 'Ġholes', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġletters', '):', 'Ġar', 'x', 'iv', 'Ġiss', 'n', 'Ġyuan', 'Ġgu', 'wen', 'Ġle', 'Ġle']</t>
         </is>
       </c>
       <c r="C336" t="n">
@@ -4806,7 +4806,7 @@
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġfe', 'b', 'ruary', 'technical', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ally', 'Ġsolar', 'Ġsystem', 'Ġobservations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġorbit', 'Ġes', 'ign', 'orbit', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġaug', 'ust', 'Ġsun', 'shield', 'Ġn', 'asa', 'gov', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdra', 'ke', 'Ġn', 'adia', 'Ġapr', 'il', 'hub', 'ble', 'Ġstill', 'Ġw', 'ows', 'Ġwait', 'Ġtill', 'Ġsee', "'s", 'Ġnext', 'http', 'Ġnational', 'Ġgeographic', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġapr', 'il', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'sun', 'shield', 'Ġcoat', 'ings', 'Ġweb', 'b', 'n', 'asa', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġcl', 'ery', 'aniel', 'Ġmarch', 'n', 'asa', 'Ġannounces', 'Ġdelays', 'Ġgiant', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġmor', 'ring', 'Ġfrank', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġsun', 'sh', 'ade', 'Ġfolding', 'Ġdeployment', 'Ġtest', 'av', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġpp', 'âĢĵ', 'Ġiss', 'n', 'Ġ000', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġfisher', 'Ġal', 'ise', 'Ġde', 'cember', 'bb', 'Ġready', 'Ġsun', 'shield', 'Ġdeployment', 'Ġcooldown', 'http', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġn']</t>
+          <t>['Ġw', 'ang', 'Ġw', 'ang', 'Ġbo', 'Ġw', 'ang', 'ying', 'Ġc', 'hen', 'Ġch', 'ao', 'n', 'Ġca', 'fu', 'Ġfan', 'zh', 'ong', 'Ġmarch', 'rap', 'id', 'ly', 'Ġgrowing', 'Ġprim', 'ordial', 'Ġblack', 'Ġholes', 'Ġseeds', 'Ġmassive', 'Ġhigh', 'red', 'shift', 'Ġj', 'w', 'st', 'Ġgalaxies', '".', 'Ġar', 'x', 'iv', '09', 'Ġ09', 'ast', 'ro', 'ph', 'co', 'Ġstr', 'ick', 'land', 'Ġash', 'ley', 'Ġj', 'une', 'bb', 'Ġtelescope', 'Ġdetects', 'Ġorganic', 'Ġmolecules', 'Ġdistant', 'Ġgalaxy', 'ht', 'Ġretrieved', 'Ġj', 'une', 'Ġgrey', 'Ġchar', 'les', 'Ġj', 'uly', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmarks', 'Ġfirst', 'Ġyear', 'Ġscience', 'Ġoperations', 'Ġper', 'ations', 'Ġair', 'Ġspace', 'Ġnews', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'athan', 'Ġp', 'Ġgard', 'ner', 'Ġet', 'Ġal', 'n', 'ovember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', '".', 'Ġspace', 'Ġscience', 'Ġreviews', '):', 'âĢĵ', 'Ġformal', 'Ġcase', 'Ġj', 'w', 'st', 'Ġscience', 'Ġpresented', 'Ġj', 'ason', 'Ġk', 'al', 'ir', 'ai', 'ap', 'ril', 'scient', 'ï', '¬', 'ģ', 'c', 'Ġdiscovery', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', '".', 'Ġcontemporary', 'Ġphysics', '):', 'âĢĵ', 'Ġar', 'x', 'iv', '05', '06', 'Ġreview', 'Ġj', 'w', 'st', 'Ġcapabilities', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġopportunities', 'Ġrig', 'Ġj', 'ane', 'Ġper', 'rin', 'Ġmarsh', 'cel', 'w', 'ichael', 'Ġk', 'imble', 'Ġr', 'andy', 'Ġfried', 'man', 'Ġsc', 'ott', 'Ġet', 'Ġal', 'Ġscience', 'Ġperformance', 'Ġj', 'w', 'st', 'Ġcharacterized', 'Ġcommission', 'ing', '".', 'Ġpublications', 'Ġastronomical', 'Ġsociety', 'Ġpac', 'ï', '¬', 'ģ', 'c', '):', '001', 'Ġar', 'x', 'iv', '05', '05', '001', 'r', 'ï', '¬', 'ģ', 'cial', 'Ġn', 'asa', 'Ġst', 'sci', 'Ġpe', 'org', 'Ġes', 'Ġfrench', 'Ġst', 'fr', 'Ġwebsite', 'Ġj', 'w', 'st', 'Ġn', 'asa', 'Ġtracking', 'Ġpage', 'Ġlaunch', 'Ġfinal', 'Ġcalibr', 'ations', 'Ġj', 'w', 'st', 'Ġn', 'asa', 'Ġpage', 'Ġtimeline', 'Ġdetails', 'Ġweb', 'b', 'Ġorbit', 'Ġcommunicating', 'Ġj', 'w', 'st', 'Ġtext', 'Ġcritical', 'Ġevents', 'Ġlaunching', 'Ġdeployment', 'Ġreading']</t>
         </is>
       </c>
       <c r="C337" t="n">
@@ -4819,7 +4819,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġwave', 'front', 'Ġsensing', 'Ġcontrol', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'ke', 'ck', 'Ġke', 'ck', 'Ġtelescopes', 'Ġn', 'Ġw', 'Ġke', 'ck', 'Ġobserv', 'atory', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'uly', 'Ġmall', 'one', 'e', 'Ġl', 'aura', 'Ġoct', 'ober', 'n', 'asa', "'s", 'Ġbiggest', 'Ġtelescope', 'Ġever', 'Ġprepares', 'Ġlaunch', 'Ġwired', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġj', 'une', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'mir', 'ror', 'Ġmirror', 'âĢ¦', 'Ġway', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'j', 'w', 'st', 'Ġmirrors', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'une', 'os', 'Ġj', 'athan', 'Ġmarch', 'j', 'ames', 'Ġweb', 'b', 'fully', 'Ġfocused', 'Ġtelescope', 'Ġbeats', 'Ġexpectations', 'ht', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'j', 'w', 'st', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', ')"', 'Ġn', 'asa', 'Ġarchived', 'Ġl', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġnear', 'Ġinfrared', 'Ġcamera', 'Ġst', 'sci', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'n', 'irc', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġuniversity', 'ri', 'zona', 'Ġarchived', 'Ġ', 'iz', 'ona', 'edu', 'n', 'irc', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'j', 'w', 'st', 'Ġcurrent', 'Ġstatus', 'Ġview', 'status', 'html', 'Ġst', 'sci', 'Ġarchived', 'Ġoriginal', 'Ġl', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'nir', 'spec', 'Ġnear', 'inf', 'rared', 'Ġspect', 'rog', 'raph', 'Ġj', 'w', 'st']</t>
+          <t>['Ġexternal', 'Ġlinks', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġj', 'w', 'st', 'Ġvideo', '031', '):', 'Ġhighlights', 'Ġtechnical', 'Ġengineering', 'Ġdetails', 'Ġj', 'w', 'st', 'Ġvideo', '012', '02', '):', 'st', 'Ġmonth', 'Ġlaunching', 'Ġdeployment', 'anim', 'ation', 'Ġj', 'w', 'st', 'Ġvideo', '008', '06', '):', 'st', 'Ġmonth', 'Ġlaunching', 'Ġdeployment', 'update', 'Ġj', 'w', 'st', 'Ġvideo', '003', '00', '):', 'nd', 'Ġmonth', 'Ġmirror', 'Ġalignment', 'Ġdetails', 'Ġj', 'w', 'st', 'Ġvideos', 'mission', 'Ġcontrol', 'Ġlive', 'Ġdeployment', 'Ġevents', 'Ġsuccessfully', 'Ġcompleted', '):', 'Ġlaunch', '005', '07', 'Ġdec', 'Ġseparation', '003', 'Ġdec', 'mir', 'ror', 'http', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsun', 'shield', 'Ġdeployment', 'Ġmission', 'Ġcontrol', 'Ġlive', 'Ġsun', 'shield', 'Ġ04', 'Ġjan', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsecondary', 'Ġmirror', 'Ġdeployment', 'Ġmission', 'Ġcontrol', 'Ġlive', 'Ġsecondary', 'Ġmirror', '08', 'Ġ05', 'Ġjan', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġprimary', 'Ġmirror', 'Ġdeployment', 'Ġmission', 'Ġcontrol', 'Ġlive', 'Ġprimary', 'Ġmirror', 'Ġ08', 'Ġjan', 'Ġnews', 'Ġupdate', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'Ġfull', 'Ġdeployment', 'Ġfinal', 'Ġdeployment', '08', 'Ġ08', 'Ġjan', 'Ġmedia', 'Ġb', 'rie', 'ï', '¬', 'ģ', 'ng', 'âĢ', 'Ļ', 'Ġnext', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarrival', '07', 'Ġjan', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġfirst', 'Ġphotos', 'Ġdata', 'Ġcalibr', 'ations', 'Ġexplained', 'Ġtest', 'ings', 'Ġcalibr', 'ations', 'Ġfirst', 'Ġthing', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġsee', 'Ġfirst', 'Ġlight', 'http', 'unknown', 'Ġcosmic', 'Ġtime', 'Ġmachine', 'net', 'ï', '¬', 'Ĥ', 'ix', 'Ġdocumentary', 'Ġdevelopment', 'Ġdeployment', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C338" t="n">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>['Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'web', 'arch', 'Ġh', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'mir', 'Ġspect', 'rom', 'eter', 'Ġng', 'st', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'j', 'w', 'st', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'mir', ')"', 'Ġn', 'asa', 'Ġarchived', 'ht', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'j', 'w', 'st', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbanks', 'Ġk', 'im', 'ber', 'ly', 'Ġl', 'arson', 'Ġmel', 'ora', 'Ġay', 'mer', 'gen', 'Ġc', 'ag', 'ay', 'Ġz', 'hang', 'Ġb', 'urt', 'Ġangel', 'Ġge', 'orge', 'Ġz', '.;', 'Ġcull', 'um', 'Ġmart', 'Ġj', 'eds', '.).', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'Ġcooler', 'Ġsystems', 'Ġengineering', 'Ġproceedings', 'Ġsp', 'ie', 'Ġmodeling', 'Ġsystems', 'Ġengineering', 'Ġproject', 'Ġmanagement', 'Ġastronomy', '017', 'api', 'se', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'fig', 'Ġcooler', 'Ġarchitecture', 'Ġoverview', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'j', 'w', 'st', 'Ġready', 'Ġlaunch', 'Ġamazing', 'Ġscience', 'Ġplanetary', 'Ġsociety', 'Ġretrieved', 'Ġaug', 'ust', 'yon', 'Ġren', 'Ã©', 'Ġh', 'utch', 'ings', 'Ġjohn', 'Ġb', '.;', 'aul', 'ieu', 'Ġmath', 'ilde', 'Ġal', 'bert', 'Ġlo', 'ic', 'Ġl', 'af', 'ren', 'Ã¨re', 'Ġdavid', 'ott', 'Ġch', 'ris', 'Ġtou', 'ah', 'ri', 'Ġdr', 'iss', 'Ġrow', 'lands', 'Ġne', 'il', 'Ġmic', 'al', 'Ġfull', 'erton', 'lex', 'Ġw', '.;', 'Ġvol', 'k', 'Ġke', 'vin', 'Ġmart', 'el', 'rÃ©', 'Ġr', '.;', 'Ġch', 'ayer', 'Ġpier', 'iv', 'aram', 'ak', 'rish', 'nan', 'Ġab', 'raham', 'Ġro', 'berto', 'Ġfer', 'ra', 'se', 'Ġl', 'aura', 'Ġj', 'ay', 'aw', 'ard', 'h', 'ana', 'Ġray', 'Ġjohn', 'stone', 'Ġdou', 'g', 'yer', 'ichael', 'Ġpip']</t>
+          <t>['Ġke', 'pler', 'Ġwik', 'ipedia', 'Ġke', 'pler', 'Ġartist', "'s", 'Ġconception', 'Ġsimultaneous', 'Ġtransit', 'Ġthree', 'Ġplanets', 'Ġke', 'pler', 'Ġobserved', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġspacecraft', 'Ġaug', 'Ġobservation', 'Ġdata', 'Ġepoch', 'Ġj', 'Ġequ', 'ox', 'Ġj', 'Ġconstellation', 'Ġcy', 'gn', 'us', 'Ġright', 'Ġasc', 'ension', 'h', 'Ġdecl', 'ination', 'Â°', 'âĢ²', '03', 'âĢ³', 'Ġapparent', 'Ġmagnitude', 'v', 'Ġcharacteristics', 'Ġspectral', 'Ġtype', 'Ġast', 'rom', 'etry', 'Ġproper', 'Ġmotion', 'Î¼', 'Ġra', 'ĠâĪĴ', '025', 'Ġmas', 'yr', 'Ġdec', '.:', 'ĠâĪĴ', '06', '029', 'Ġmas', 'yr', 'Ġpar', 'ax', 'ÏĢ', '01', 'Ġmas', 'Ġdistance', 'Ġly', 'Ġabsolute', 'Ġmagnitude', 'Ġdetails', 'Ġmass', '04', '005', 'âĺ', 'ī', 'Ġradius', '021', '025', 'Ġr', 'âĺ', 'ī', 'Ġsurface', 'Ġgravity', 'log', 'Ġg', '02', 'Ġtemperature', 'Ġmet', 'icity', 'fe', 'h', '06', '007', 'Ġdex', 'Ġrot', 'ational', 'Ġvelocity', 'v', 'Ġsin', 'Ġage', 'Ġdesign', 'ations', 'Ġk', 'ic', 'mass', 'Ġdatabase', 'Ġreferences', 'Ġsim', 'bad', 'Ġdata', 'Ġk', 'ic', 'Ġdata', 'Ġid', 'Ġke', 'pler', 'Ġcoordinates', 'h', 'Â°', 'âĢ²', 'âĢ³', 'Ġke', 'pler', 'Ġalso', 'Ġdesignated', 'mass', 'Ġsun', 'like', 'Ġstar', 'Ġslightly', 'Ġlarger', 'Ġsun', 'Ġconstellation', 'Ġcy', 'gn', 'us', 'Ġlocated', 'Ġlight', 'Ġyears', 'Ġearth', 'Ġlocated', 'Ġwithin', 'Ġfield', 'Ġvision', 'Ġke', 'pler', 'Ġspacecraft', 'Ġsatellite', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġmission', 'Ġuses', 'Ġdetect', 'Ġplanets', 'Ġmay', 'Ġtrans', 'iting', 'Ġstars', 'Ġannounced', 'Ġfe', 'b', 'ruary', 'Ġstar', 'Ġsystem', 'Ġamong', 'Ġcompact', 'Ġflatt', 'est', 'Ġsystems', 'Ġyet', 'Ġdiscovered', 'Ġfirst', 'Ġdiscovered', 'Ġcase', 'Ġstar', 'Ġsystem', 'Ġtrans', 'iting', 'Ġplanets', 'Ġdiscovered', 'Ġplanets', 'Ġlarger', 'Ġearth', 'Ġlarger', 'Ġones', 'Ġne', 'pt', 'une', "'s", 'Ġsize', 'Ġke', 'pler', 'Ġplanets', 'Ġdiscovered', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġmission']</t>
         </is>
       </c>
       <c r="C339" t="n">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>['Ġjud', 'ith', 'Ġl', '.;', 'Ġsaw', 'ick', 'Ġmar', 'cin', 'Ġaug', 'ust', 'Ġclamp', 'Ġmark', 'Ġc', 'Ġf', 'az', 'io', 'Ġg', 'iov', 'anni', 'Ġg', 'Ġmac', 'ew', 'en', 'ard', 'sch', 'mann', 'Ġj', 'ac', 'ob', 'us', 'eds', '.).', 'Ġj', 'w', 'st', 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġnear', 'inf', 'rared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'nir', 'iss', '".', 'Ġproceedings', 'Ġsp', 'ie', 'Ġspace', 'Ġtelescopes', 'Ġinstrument', 'ation', 'Ġoptical', 'Ġinfrared', 'Ġmill', 'imeter', 'Ġwave', 'r', 'ui', 'Ġf', 'Ġfeatures', 'Ġtwo', 'Ġmodules', 'Ġinfrared', 'Ġcamera', 'Ġdedicated', 'Ġï', '¬', 'ģ', 'ne', 'Ġguiding', 'Ġobserv', 'atory', 'Ġscience', 'Ġcamera', 'Ġmodule', 'Ġnear', 'inf', 'rared', 'Ġim', 'ager', 'Ġslit', 'less', 'Ġspect', 'rog', 'raph', 'nir', 'iss', ')"', 'Ġspacecraft', 'Ġbus', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'w', 'st', 'Ġobserv', 'atory', 'Ġn', 'asa', 'Ġarchived', 'w', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġde', 'cember', 'Ġobserv', 'atory', 'Ġspace', 'based', 'Ġportion', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsystem', 'Ġcomprised', 'Ġthree', 'Ġelements', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', 'Ġoptical', 'Ġtelescope', 'Ġelement', 'ote', 'Ġincludes', 'Ġmirrors', 'Ġback', 'plane', 'Ġspacecraft', 'Ġelement', 'Ġincludes', 'Ġspacecraft', 'Ġbus', 'Ġsun', 'shield', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'integ', 'rated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'im', ')"', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ough', 'Ġsc', 'ott', 'Ġp', 'f', 'eb', 'ruary', 'prime', 'Ġuntold', 'Ġstory', 'Ġn', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsat', 'mag', 'azine', 'Ġsat', 'news', 'Ġarchived', 'Ġu', 'mber', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'Ġsl', 'oan', 'Ġje', 'ff']</t>
+          <t>['Ġmission', 'Ġtasked', 'Ġdiscovering', 'Ġplanets', 'Ġtransit', 'Ġaround', 'Ġstars', 'Ġtransit', 'Ġmethod', 'Ġke', 'pler', 'Ġuses', 'Ġinvolves', 'Ġdetecting', 'Ġdips', 'Ġbrightness', 'Ġstars', 'Ġdips', 'Ġbrightness', 'Ġinterpreted', 'Ġplanets', 'Ġwhose', 'Ġorbits', 'Ġmove', 'Ġfront', 'Ġstars', 'Ġperspective', 'Ġearth', 'Ġke', 'pler', 'Ġfirst', 'Ġdiscovered', 'Ġex', 'oplan', 'etary', 'Ġsystem', 'Ġthree', 'Ġtrans', 'iting', 'Ġplanets', 'Ġke', 'pler', 'Ġnamed', 'Ġke', 'pler', 'Ġmission', 'th', 'Ġstar', 'Ġconfirmed', 'Ġplanets', 'Ġdiscovered', 'Ġke', 'pler', 'Ġfield', 'Ġview', 'Ġplanets', 'Ġnamed', 'Ġalphabet', 'ically', 'Ġstarting', 'Ġinner', 'Ġb', 'Ġc', 'Ġe', 'Ġf', 'Ġg', 'Ġdistingu', 'ishers', 'Ġtagged', 'Ġonto', 'Ġname', 'Ġhome', 'Ġstar', 'Ġke', 'pler', 'Ġg', 'type', 'Ġstar', 'Ġapproximately', 'Ġmass', 'Ġradius', 'Ġsun', 'Ġsurface', 'Ġtemperature', 'Ġestimated', 'Ġage', 'Ġaround', 'Ġbillion', 'Ġyears', 'Ġcomparison', 'Ġsun', 'Ġbillion', 'Ġyears', 'Ġsurface', 'Ġtemperature', 'Ġapparent', 'Ġmagnitude', 'Ġfaint', 'Ġseen', 'Ġnaked', 'Ġknown', 'Ġplanets', 'Ġtransit', 'Ġstar', 'Ġmeans', 'Ġplanets', 'Ġorbits', 'Ġappear', 'Ġcross', 'Ġfront', 'Ġstar', 'Ġviewed', 'Ġearth', "'s", 'Ġperspective', 'Ġincl', 'inations', 'Ġrelative', 'Ġearth', "'s", 'Ġline', 'Ġsight', 'Ġfar', 'Ġplane', 'Ġsight', 'Ġvary', 'Ġlittle', 'Ġdegree', 'Ġallows', 'Ġdirect', 'Ġmeasurements', 'Ġplanets', 'Ġperiods', 'Ġrelative', 'Ġdiam', 'eters', 'comp', 'ared', 'Ġhost', 'Ġstar', 'Ġmonitoring', 'Ġplanet', "'s", 'Ġtransit', 'Ġstar', 'Ġsimulations', 'Ġsuggest', 'Ġmean', 'Ġmutual', 'Ġincl', 'inations', 'Ġplanetary', 'Ġorbits', 'Â°', 'Ġmeaning', 'Ġsystem', 'Ġprobably', 'Ġcop', 'lan', 'ar', 'fl', 'atter', 'Ġsolar', 'Ġsystem', 'Ġcorresponding', 'Ġfigure', 'Â°', 'Ġestimated', 'Ġmasses', 'Ġplanets', 'Ġfall', 'Ġrange', 'Ġearth', 'Ġne', 'pt', 'une', 'Ġestimated', 'Ġdens', 'ities', 'Ġlower', 'Ġearth', 'Ġimply', 'Ġnone', 'Ġearth', 'like', 'Ġcomposition', 'Ġsignificant', 'Ġhydrogen', 'hel', 'ium', 'Ġatmosphere', 'Ġpredicted', 'Ġplanets', 'Ġc', 'Ġe', 'Ġf', 'Ġg', 'Ġplanet', 'Ġmay', 'Ġsurrounded', 'Ġsteam', 'Ġatmosphere', 'Ġperhaps', 'Ġhydrogen', 'Ġatmosphere']</t>
         </is>
       </c>
       <c r="C340" t="n">
@@ -4858,7 +4858,7 @@
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>['Ġoct', 'ober', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġspacecraft', 'Ġinches', 'Ġtowards', 'Ġfull', 'Ġassembly', 'Ġcompos', 'ites', 'Ġworld', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġde', 'cember', 'j', 'w', 'st', 'Ġpropulsion', 'prop', 'ulsion', 'Ġj', 'w', 'st', 'Ġuser', 'Ġdocumentation', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'mber', 'n', 'asa', 'Ġgives', 'Ġgreen', 'Ġlight', 'Ġfuel', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġce', 'tel', 'esc', 'ope', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġweb', 'b', 'Ġservice', 'able', 'Ġlike', 'Ġhub', 'ble', '?"', 'Ġ', 'erv', 'ice', 'able', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'rel', 'ief', 'Ġn', 'asa', "'s", 'Ġpowerful', 'Ġspace', 'Ġtelescope', 'Ġï', '¬', 'ģ', 'n', 'ishes', 'Ġrisky', 'Ġunfolding', 'Ġng', 'Ġscience', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġsm', 'ith', 'Ġmar', 'cia', 'Ġaug', 'ust', 'z', 'urb', 'uc', 'hen', 'Ġtaking', 'Ġone', 'Ġlast', 'Ġlook', 'Ġj', 'w', 'st', 'Ġservicing', 'Ġcompat', 'ibl', 'ity', 'sic', ']"', 'Ġv', 'icing', 'Ġspac', 'ep', 'olic', 'yon', 'line', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġfe', 'b', 'ruary', 'scient', 'ists', 'Ġengineers', 'Ġpush', 'Ġservicing', 'Ġassembly', 'Ġfuture', 'Ġspace', 'Ġobserv', 'atories', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġce', 'ob', 'serv', 'atories', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġtransform', 'Ġï', '¬', 'ģ', 'n', 'al', 'Ġform', 'Ġverge', 'Ġarchived', 'Ġoy', 'ment', 'sequence', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'vs', 'ky', 'Ġil', 'ana', 'Ġbal', 'z', 'ano', 'Ġv', 'ick', 'j', 'w', 'st', 'Ġmaximizing', 'Ġe', 'f', 'ï']</t>
+          <t>['Ġlow', 'Ġdens', 'ities', 'Ġlikely', 'Ġresult', 'Ġhigh', 'volume', 'Ġextended', 'Ġatmosp', 'heres', 'Ġsurround', 'Ġcores', 'Ġiron', 'Ġrock', 'Ġpossibly', 'Ġinner', 'Ġconstituents', 'Ġke', 'pler', 'Ġsystem', 'Ġtime', 'Ġdiscoveries', 'Ġcomprehens', 'ively', 'Ġunderstood', 'Ġextras', 'olar', 'Ġplanets', 'Ġsmaller', 'Ġne', 'pt', 'une', 'Ġcurrently', 'Ġobservations', 'Ġplace', 'Ġfirm', 'Ġconstraint', 'Ġmass', 'Ġplanet', 'Ġ(&lt;', 'Ġhowever', 'Ġformation', 'Ġevolution', 'Ġstudies', 'Ġindicate', 'Ġmass', 'Ġplanet', 'Ġmuch', 'Ġgreater', 'Ġke', 'pler', 'Ġplanets', 'Ġmay', 'Ġformed', 'Ġsitu', 'e', '.,', 'Ġobserved', 'Ġorbital', 'Ġlocations', 'Ġsitu', 'Ġmay', 'Ġstarted', 'Ġformation', 'Ġfarther', 'Ġaway', 'Ġstar', 'Ġmigrating', 'Ġinward', 'Ġgravitational', 'Ġinteractions', 'Ġg', 'ase', 'ous', 'Ġprot', 'oplan', 'etary', 'Ġdisk', 'Ġsecond', 'Ġscenario', 'Ġpredicts', 'Ġsubstantial', 'Ġfraction', 'Ġplanets', 'Ġmass', 'Ġregardless', 'Ġformation', 'Ġscenario', 'Ġg', 'ase', 'ous', 'Ġcomponent', 'Ġplanets', 'Ġn', 'omen', 'cl', 'ature', 'Ġhistory', 'Ġcharacteristics', 'Ġplanetary', 'Ġsystem', 'Ġke', 'pler', 'Ġwik', 'ipedia', 'Ġorbit', 'Ġke', 'pler', 'Ġplanets', 'Ġcomparison', 'Ġorbits', 'Ġplanets', 'Ġmercury', 'Ġven', 'us', 'Ġaccounts', 'Ġless', 'Ġmasses', 'Ġâī', 'Ī', 'Ġâī', 'Ī', 'Ġrad', 'ii', 'Ġdynam', 'ical', 'Ġsimulation', 'Ġshown', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġlikely', 'Ġundergone', 'Ġsubstantial', 'Ġinward', 'Ġmigration', 'Ġpast', 'Ġproducing', 'Ġobserved', 'Ġpattern', 'Ġlower', 'mass', 'Ġplanets', 'Ġtight', 'est', 'Ġorbits', 'Ġadditional', 'Ġyet', 'Ġunob', 'served', 'Ġgas', 'Ġgiant', 'Ġplanets', 'Ġwider', 'Ġorbit', 'Ġlikely', 'Ġnecessary', 'Ġmigration', 'Ġsmaller', 'Ġplanets', 'Ġproceed', 'Ġfar', 'Ġinward', 'Ġsystem', 'Ġamong', 'Ġcompact', 'Ġknown', 'Ġorbits', 'Ġplanets', 'Ġwould', 'Ġeasily', 'Ġfit', 'Ġinside', 'Ġorbit', 'Ġmercury', 'Ġslightly', 'Ġoutside', 'Ġdespite', 'Ġclose', 'Ġpacking', 'Ġorbits', 'Ġdynam', 'ical', 'Ġinteg', 'rations', 'Ġindicate', 'Ġke', 'pler', 'Ġsystem', 'Ġpotential', 'Ġstable', 'Ġtime', 'Ġscale', 'Ġbillions', 'Ġyears', 'Ġhowever', 'Ġmay', 'Ġapproaching', 'Ġinstability', 'Ġdue', 'Ġsecular', 'Ġresonance', 'Ġinvolving', 'Ġc', 'Ġhappens', 'Ġlikely', 'Ġbecome', 'Ġeccentric', 'Ġenough', 'Ġcoll', 'ides', 'Ġnone', 'Ġplanets', 'Ġlow', 'rat', 'io', 'Ġorbital', 'Ġreson', 'ances', 'Ġmultiple', 'Ġplanets', 'Ġgrav', 'itation', 'ally', 'Ġtug', 'Ġstabilize', "'s", 'Ġorbits', 'Ġresulting', 'Ġsimple', 'Ġratios', 'Ġorbital', 'Ġperiods']</t>
         </is>
       </c>
       <c r="C341" t="n">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>['¬', 'ģ', 'ci', 'ency', 'Ġminimizing', 'Ġground', 'Ġsystems', 'Ġinternational', 'Ġsym', 'posium', 'Ġreducing', 'Ġcosts', 'Ġspacecraft', 'Ġground', 'Ġsystems', 'Ġoperations', 'Ġproceedings', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġgreenhouse', 'Ġmatt', 'hew', 'Ġstatus', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġintegrated', 'Ġscience', 'Ġinstrument', 'Ġmodule', 'Ġsystem', 'report', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'cc', 'arthy', 'Ġg', '.;', 'Ġaut', 'io', 'Ġg', 'Ġw', 'Ġinfrared', 'Ġdetector', 'Ġperformance', 'Ġshuttle', 'Ġinfrared', 'Ġtelescope', 'Ġfacility', 'irt', 'f', 'Ġlos', 'Ġangel', 'es', 'Ġtechnical', 'Ġsym', 'posium', 'Ġutilization', 'Ġinfrared', 'Ġdetectors', 'Ġvol', 'Ġsociety', 'Ġphotographic', 'Ġinstrument', 'ation', 'Ġengineers', 'Ġpp', 'âĢĵ', 'ui', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġcold', 'Ġgo', 'Ġcooler', 'Ġtested', 'Ġn', 'asa', 'Ġtelescope', 'Ġphys', 'org', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'sc', 'hel', 'Ġspace', 'Ġobserv', 'atory', 'Ġrelated', 'Ġmissions', 'sh', 'tml', 'Ġn', 'asa', 'Ġjet', 'Ġpropulsion', 'Ġlaboratory', 'Ġgodd', 'ard', 'Ġflight', 'Ġcenter', 'Ġcal', 'ornia', 'Ġinstitute', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġiso', '?"', 'Ġes', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'hub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġwide', 'Ġfield', 'Ġcamera', 'Ġn', 'asa', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ich', 'hardt', 'ony', 'arch', 'us', 'Ġastronomy', 'Ġnext', 'Ġbig', 'Ġthing', 'Ġbig', '?"', 'f', '01', 'Ġnature', '):', 'âĢĵ', 'ui', 'ads', 'abs', 'Ġdoi', '01']</t>
+          <t>['Ġhowever', 'Ġclose', 'Ġratio', 'Ġcould', 'Ġconce', 'ivably', 'Ġplanets', 'Ġsystem', 'Ġtransit', 'Ġstar', 'Ġwould', 'Ġdetectable', 'Ġeffects', 'Ġgravity', 'Ġmotion', 'Ġvisible', 'Ġplanets', 'much', 'Ġne', 'pt', 'une', 'Ġdiscovered', 'Ġpresence', 'Ġadditional', 'Ġgas', 'Ġgiant', 'Ġplanets', 'Ġcurrently', 'Ġexcluded', 'Ġorbital', 'Ġradius', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġcompanion', 'Ġorder', 'Ġstar', 'Ġmass', 'Ġsem', 'im', 'ajor', 'Ġaxis', 'Ġorbital', 'Ġperiod', 'days', 'Ġeccentric', 'ity', 'Ġinclination', 'Ġradius', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '09', '001', '000', 'ĠâĪĴ', '0010', '045', 'ĠâĪĴ', '04', 'ĠâĪĴ', 'Â°', '07', 'ĠâĪĴ', '04', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '001', '00', 'ĠâĪĴ', '000', '026', '06', 'ĠâĪĴ', '013', 'ĠâĪĴ', 'Â°', '05', 'ĠâĪĴ', '06', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '001', '000', '004', '007', 'ĠâĪĴ', '002', 'ĠâĪĴ', 'Â°', '06', 'ĠâĪĴ', '07', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '002', '000', 'ĠâĪĴ', '00', '012', '006', 'ĠâĪĴ', '006', '02', 'ĠâĪĴ', '02', 'Â°', '07', 'ĠâĪĴ', '09', 'Ġr', 'ðŁ', 'ľ', '¨', 'ĠâĪĴ', 'ðŁ', 'ľ', '¨', '002', '00', 'ĠâĪĴ', '00', '013', '011', 'ĠâĪĴ', '009', '04', 'Â°']</t>
         </is>
       </c>
       <c r="C342" t="n">
@@ -4884,7 +4884,7 @@
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>['Ġpm', 'id', 'nexus', 'Ġspace', 'Ġtelescope', 'Ġmit', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġbrown', 'wayne', 'Ġbra', 'uk', 'us', 'ichael', 'n', 'asa', 'Ġn', 'asa', 'Ġes', 'Ġsign', 'Ġagreements', 'Ġfuture', 'Ġcooperation', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'Ġg', 'ur', 'Ġha', 'v', 'iv', 'tt', 'ig', 'Ġjan', 'uary', 'space', 'Ġchanging', 'Ġweb', 'b', 'Ġstart', 'Ġsays', 'Ġex', 'rael', 'Ġdawn', 'Ġtimes', 'rael', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'adv', 'anced', 'Ġconcepts', 'Ġstudies', 'Ġaperture', 'hi', 'z', 'Ġtelescope', 'Ġn', 'asa', 'Ġspace', 'Ġoptics', 'Ġmanufacturing', 'Ġtechnology', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'sts', 'ci', 'Ġj', 'w', 'st', 'Ġhistory', 'Ġarchived', 'Ġoriginal', 'Ġr', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġde', 'cember', 'ast', 'ron', 'Ġastroph', 'ysics', 'Ġnew', 'Ġmillennium', 'Ġ', 'xt', 'ng', 'st', 'htm', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġde', 'ck', 'liv', 'ier', 'Ġl', '.;', 'Ġmill', 'er', 'Ġdavid', 'Ġw', '.;', 'Ġmos', 'ier', 'Ġg', 'ary', 'Ġe', 'mult', 'idis', 'ciplinary', 'Ġanalysis', 'Ġnexus', 'Ġprecursor', 'Ġspace', 'Ġtelescope', 'Ġmac', 'ew', 'en', 'ard', 'ed', '.).', 'Ġhighly', 'Ġinnovative', 'Ġspace', 'Ġtelescope', 'Ġconcepts', 'Ġhighly', 'Ġinnovative', 'Ġspace', 'Ġtelescope', 'Ġconcepts', 'Ġvol', 'Ġp', 'Ġcites', 'eer', 'x', 'Ġ00', 'Ġarchived', 'w', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġbrown', 'Ġr', 'Ġpage', '03', 'Ġconf', '..', 'b', 'Ġscience', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', '03', 'h', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['04', 'ĠâĪĴ', '07', 'Ġr', 'ðŁ', 'ľ', '¨', 'ðŁ', 'ľ', '¨', '004', '0010', 'ĠâĪĴ', '000', '013', '011', 'ĠâĪĴ', '009', '05', 'ĠâĪĴ', '06', 'Â°', '06', 'ĠâĪĴ', '08', 'Ġr', 'ðŁ', 'ľ', '¨', 'Ġrelative', 'Ġsize', 'Ġpositions', 'Ġplanets', 'Ġke', 'pler', 'Ġinner', 'Ġsolar', 'Ġsystem', 'Ġcomparison', 'Ġdiam', 'eters', 'Ġplanets', 'Ġstars', 'Ġscaled', 'Ġfactor', 'Ġlist', 'Ġmulti', 'plan', 'etary', 'Ġsystems', 'Ġke', 'pler', 'Ġmission', 'Ġgl', 'ies', 'e', 'c', 'ri', 'Ġbrown', 'Ġg', '.;', 'Ġet', 'Ġal', 'ga', 'ia', 'Ġcollaboration', 'aug', 'ust', 'ga', 'ia', 'Ġdata', 'Ġrelease', 'Ġsummary', 'Ġcontents', 'Ġsurvey', 'Ġproperties', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġar', 'x', 'iv', '04', '09', 'ui', 'Ġga', 'ia', 'Ġrecord', 'Ġsource', 'Ġviz', 'ier', 'Ġl', 'iss', 'auer', 'Ġjack', 'Ġj', '.;', 'Ġet', 'Ġal', 'Ġclosely', 'Ġpacked', 'Ġsystem', 'Ġlow', 'mass', 'Ġlow', 'density', 'Ġplanets', 'Ġtrans', 'iting', 'Ġke', 'pler', '".', 'Ġnature', '):', 'âĢĵ', 'Ġar', 'x', 'iv', 'f', 'nature', '09', 'Ġpm', 'id', 'Ġn', 'ih', 'gov', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġke', 'pler', 'Ġwik', 'ipedia', 'Ġbed', 'ell', 'gan', 'Ġet', 'Ġal', 'ke', 'pler', 'Ġsolar', 'Ġtwin', 'Ġrev', 'ising', 'Ġmasses', 'Ġrad', 'ii', 'Ġbenchmark', 'Ġplanets', 'Ġvia', 'Ġprecise', 'Ġstellar', 'Ġcharacterization', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġar', 'x', 'iv', '06', 'htt', 'http', 'ke', 'pler', 'Ġpl', 'er', 'Ġsim', 'bad', 'Ġcentre', 'Ġde', 'n', 'Ã©', 'es', 'Ġastron', 'om', 'iques', 'Ġde', 'Ġstr', 'bourg', 'Ġretrieved', '05', '09', 'mass', 'Ġj', 'Ġsim', 'bad', 'Ġcentre', 'Ġde', 'n', 'Ã©', 'es', 'Ġastron', 'om', 'iques', 'Ġde', 'Ġstr']</t>
         </is>
       </c>
       <c r="C343" t="n">
@@ -4897,7 +4897,7 @@
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>['Ġjan', 'uary', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġdress', 'ler', '.,', 'Ġed', 'expl', 'oration', 'Ġsearch', 'Ġorigins', 'Ġvision', 'Ġspace', 'Ġastronomy', 'Ġreport', 'h', 'st', 'Ġbeyond', 'Ġcommittee', 'Ġst', 'sci', 'edu', 'Ġassociation', 'Ġuniversities', 'Ġresearch', 'Ġastronomy', 'Ġarchived', 'Ġh', 'stand', 'yond', 'pdf', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġstock', 'man', 'Ġh', 'j', 'une', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'Ġvisiting', 'Ġtime', 'Ġgalaxies', 'Ġyoung', '".', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġb', 'alt', 'imore', 'ary', 'land', 'Ġassociation', 'Ġuniversities', 'Ġresearch', 'Ġastronomy', 'Ġwashing', 'ton', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġsurvey', 'Ġcommittee', 'Ġboard', 'Ġphysics', 'Ġastronomy', 'Ġspace', 'Ġstudies', 'Ġboard', 'Ġcommission', 'Ġphysical', 'Ġsciences', 'Ġmathematics', 'Ġapplications', 'Ġnational', 'Ġresearch', 'Ġcouncil', 'Ġjan', 'uary', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġnew', 'Ġmillennium', 'n', 'ap', 'e', 'Ġdu', 'cat', 'alog', 'Ġwashing', 'ton', 'Ġnational', 'Ġacad', 'emies', 'Ġpress', 'Ġdoi', 'doi', 'Ġg', 'f', '070', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'sts', 'ci', 'Ġj', 'w', 'st', 'Ġhistory', 'Ġst', 'sci', 'edu', 'Ġarchived', 'Ġoriginal', 'Ġr', 'view', 'history', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'g', 'odd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġdesign', 'Ġg', 'es', 'op', 'b', 'Ġretrieved', 'Ġaug', 'ust', 'esa', 'Ġscience', 'Ġtechnology', 'Ġball', 'Ġaerospace', 'Ġdesign', 'Ġj', 'w', 'st', 'Ġarchived', 'Ġde', 'cember', 'Ġarchive', 'today', 'Ġsci', 'esa', 'int', 'Ġretrieved', 'Ġaug', 'ust', 'esa', 'Ġscience', 'Ġtechnology', 'Ġtr', 'w', 'Ġdesign', 'Ġj', 'w', 'st', 'Ġarchived', 'Ġde', 'cember', 'Ġarchive', 'today', 'Ġsci', 'esa', 'int', 'Ġretrieved', 'Ġaug', 'ust', 'esa', 'Ġscience', 'Ġtechnology', 'Ġlock', 'heed', 'mart', 'Ġdesign', 'Ġj', 'w', 'st', 'Ġarchived', 'Ġde', 'cember', 'Ġarchive', 'today', 'Ġsci', 'esa', 'int', 'Ġretrieved', 'Ġaug', 'ust', 'hub', 'bles', 'ite', 'Ġweb', 'b', 'Ġpast', 'Ġfuture']</t>
+          <t>['bourg', 'ichael', 'ew', 'hin', 'ney', 'Ġrac', 'hel', 'Ġh', 'oo', 'ver', 'rent', 'Ġj', 'Ġper', 'ro', 'tto', 'Ġfe', 'b', 'ruary', 'n', 'asa', "'s", 'Ġke', 'pler', 'Ġspacecraft', 'Ġdiscovers', 'Ġextraordinary', 'Ġnew', 'Ġplanetary', 'Ġsystem', 'Ġn', 'asa', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfr', 'aser', 'Ġc', 'Ġse', 'pt', 'ember', 'Ġold', 'Ġsun', '?"', 'Ġuniverse', 'Ġtoday', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfr', 'aser', 'Ġc', 'se', 'pt', 'ember', 'tem', 'perature', 'Ġsun', 'htt', 'Ġuniverse', 'Ġtoday', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġboy', 'le', 'Ġal', 'Ġfe', 'b', 'ruary', 'plan', 'etary', 'Ġsix', 'pack', 'Ġposes', 'Ġpuzzle', 'Ġcosmic', 'Ġlog', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġl', 'iss', 'auer', 'Ġjack', 'Ġj', '.;', 'Ġet', 'Ġal', 'Ġplanets', 'Ġknown', 'Ġorbit', 'Ġke', 'pler', 'Ġlow', 'Ġdens', 'ities', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġar', 'x', 'iv', 'angelo', 'Ġg', '.;', 'Ġbod', 'en', 'heimer', 'Ġp', 'Ġsitu', 'Ġsitu', 'Ġformation', 'Ġmodels', 'Ġke', 'pler', 'Ġplanets', '".', 'Ġastroph', 'ysical', 'Ġjournal', '):', 'Ġid', 'Ġpp', '.).', 'Ġar', 'x', 'iv', '06', '080', 'ar', 'x', 'iv', 'Ġg', 'abs', '06', '080', 'ui', 'ads', 'ab', 'Ġpus', 'id', 'Ġna', 'eye', 'Ġro', 'bert', 'Ġfe', 'b', 'ruary', 'ke', 'pler', "'s", 'Ġoutrageous', 'Ġsystem', 'Ġplanets', 'Ġtelescope', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġjohn', 'atson', 'Ġfe', 'b', 'ruary', 'Ġwealth', 'Ġworlds', 'Ġke', 'pler', 'Ġspacecraft', 'Ġfinds', 'Ġnew', 'Ġex', 'oplan', 'ets', 'Ġhints', 'htt', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhands', 'Ġr', 'lex', 'ander', 'Ġw', 'Ġde', 'hn', 'en', 'standing', 'Ġassembly', 'Ġke', 'pler', "'s", 'Ġcompact', 'Ġplanetary', 'Ġsystems', '",', 'ac', 'Ġhands', '.;', 'lex', 'ander', 'Ġr', 'Ġmight']</t>
         </is>
       </c>
       <c r="C344" t="n">
@@ -4910,7 +4910,7 @@
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġannounces', 'Ġcontract', 'Ġnext', 'generation', 'Ġspace', 'Ġtelescope', 'Ġnamed', 'Ġspace', 'Ġpioneer', 'Ġn', 'asa', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'tr', 'w', 'Ġselected', 'Ġj', 'w', 'st', 'Ġprime', 'Ġcontractor', 'Ġst', 'ci', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġjan', 'uary', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġcompletes', 'Ġfabrication', 'Ġsun', 'shield', 'Ġdeployment', 'Ġflight', 'Ġstructure', 'Ġj', 'w', 'st', 'Ġspace', 'Ġdaily', 'Ġde', 'cember', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'ather', 'Ġjohn', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', ')"', 'Ġnational', 'Ġacademy', 'Ġscience', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'euro', 'pe', 'Ġagreement', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'Ġmid', 'inf', 'rared', 'Ġinstrument', 'mir', 'Ġsigned', 'press', 'Ġrelease', 'Ġes', 'Ġmedia', 'Ġrelations', 'Ġservice', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'ada', "'s", 'Ġcontribution', 'Ġn', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'ada', 'ca', 'adian', 'Ġspace', 'Ġagency', 'Ġj', 'une', 'Ġarchived', 'pe', 'html', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'adian', 'Ġspace', 'Ġagency', 'Ġdelivers', 'ada', "'s", 'Ġcontributions', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'space', 'tel', 'esc', 'ope', 'Ġspace', 'q', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'j', 'w', 'st', 'Ġpasses', 'nar', 'Ġst', 'sci', 'Ġarchived', 'Ġoriginal', 'Ġasses', 'nar', 'Ġaug', 'ust', 'Ġretrieved', 'Ġj', 'uly']</t>
+          <t>['Ġgiants', 'Ġunseen', 'Ġj', 'upiter', 'mass', 'Ġplanets', 'Ġsculpt', 'ors', 'Ġtightly', 'packed', 'Ġplanetary', 'Ġsystems', '",', 'Ġmonthly', 'Ġnotices', 'Ġroyal', 'Ġastronomical', 'Ġsociety', '):', 'âĢĵ', 'Ġar', 'x', 'iv', '026', 'Ġb', '026', 'Ġcont', 'ras', 'Ġp', 'Ġgran', 'ados', 'Ġbo', 'ley', 'Ġc', 'Ġmarch', 'Ġdynamics', 'Ġtightly', 'packed', 'Ġplanetary', 'Ġsystems', 'Ġpresence', 'Ġouter', 'Ġplanet', 'Ġcase', 'Ġstudies', 'Ġusing', 'Ġke', 'pler', 'Ġke', 'pler', '".', 'Ġastronomical', 'Ġjournal', '):', 'Ġar', 'x', 'iv', '02', '01', 'http', 'Ġbec', 'ker', 'Ġj', 'ul', 'iet', 'te', 'Ġc', '.;', 'Ġad', 'ams', 'Ġf', 'red', 'Ġc', 'effects', 'Ġunseen', 'Ġadditional', 'Ġplanetary', 'Ġpert', 'ur', 'bers', 'Ġcompact', 'Ġextras', 'olar', 'Ġplanetary', 'Ġsystems', '",', 'Ġmonthly', 'Ġnotices', 'Ġroyal', 'Ġastronomical', 'Ġsociety', 'âĢĵ', 'Ġar', 'x', 'iv', '02', '07', '005', 'Ġpus', 'id', '005', 'Ġk', 'ub', 'ys', 'h', 'k', 'ina', '.;', 'Ġfoss', 'ati', 'Ġl', '.;', 'Ġmust', 'ill', 'Ġj', '.;', 'Ġcub', 'ill', 'os', 'Ġp', 'Ġe', '.;', 'av', 'ies', 'Ġb', '.;', 'Ġer', 'ka', 'ev', 'Ġn', 'Ġv', '.;', 'Ġjohn', 'stone', 'Ġc', 'Ġp', '.;', 'Ġk', 'lyak', 'ova', 'Ġk', 'Ġg', '.;', 'Ġlam', 'mer', 'Ġh', '.;', 'Ġlend', 'l', '.;', 'Ġod', 'ert', 'Ġp', 'Ġke', 'pler', 'Ġsystem', 'Ġevolution', 'Ġstellar', 'Ġhigh', 'energy', 'Ġemission', 'Ġinitial', 'Ġplanetary', 'Ġatmospheric', 'Ġmass', 'Ġfractions', '".', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġar', 'x', 'iv', '09', 'http', '003', '003', 'ï', '¬', 'ģ', 'cial', 'Ġrelease', 'Ġn', 'asa', "'s", 'Ġke', 'pler', 'Ġspacecraft', 'Ġdiscovers', 'Ġextraordinary', 'Ġnew', 'Ġplanetary', 'Ġsystem', 'Ġyoutube', 'Ġanimation', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġke', 'pler', 'Ġplanetary', 'Ġsystem', 'Ġorbits', 'Ġplanet', 'Ġsizes', 'Ġastronomers', 'Ġfind', 'pack', 'Ġplanets', 'Ġalien', 'Ġsolar', 'Ġsystem', 'Ġn', 'asa', 'Ġastronomy', 'Ġpicture', 'Ġday', 'Ġworlds', 'Ġke', 'pler', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C345" t="n">
@@ -4923,7 +4923,7 @@
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>['Ġber', 'ger', 'Ġb', 'rian', 'Ġmay', 'n', 'asa', 'Ġadds', 'Ġdocking', 'Ġcapability', 'Ġnext', 'Ġspace', 'Ġobserv', 'atory', 'htt', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'uly', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsun', 'shield', 'Ġready', 'Ġfabric', 'ate', 'Ġab', 'ric', 'ate', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġpasses', 'Ġkey', 'Ġmission', 'Ġdesign', 'Ġreview', 'Ġmilestone', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġaug', 'ust', 'n', 'asa', 'Ġsays', 'Ġj', 'w', 'st', 'Ġcost', 'Ġcrunch', 'Ġimp', 'eding', 'Ġnew', 'Ġmissions', 'http', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġaug', 'ust', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġprimary', 'Ġmirror', 'Ġfully', 'Ġassembled', 'Ġn', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsecondary', 'Ġmirror', 'Ġinstalled', 'Ġn', 'asa', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'uh', 'Ġal', 'mber', 'n', 'asa', 'Ġbegins', 'Ġtesting', 'Ġenormous', 'Ġspace', 'Ġtelescope', 'Ġmade', 'Ġgold', 'Ġmirrors', 'Ġcope', 'gold', 'Ġguardian', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'n', 'asa', 'Ġcompletes', 'Ġweb', 'b', 'Ġtelescope', 'Ġreview', 'Ġcommits', 'Ġlaunch', 'Ġearly', 'n', 'asa', 'Ġn', 'asa', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġj', 'uly', 'north', 'rop', 'Ġgr', 'um', 'man', 'Ġce']</t>
+          <t>['Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġlist', 'Ġtypes', 'Ġu', 'Ġreconnaissance', 'Ġsatellites', 'Ġdeployed', 'Ġonward', 'Ġaerial', 'Ġview', 'Ġos', 'ama', 'Ġbin', 'Ġlad', 'en', "'s", 'Ġcompound', 'Ġp', 'ak', 'istani', 'Ġcity', 'Ġab', 'bott', 'abad', 'Ġmade', 'Ġc', 'ia', 'Ġcor', 'ona', 'Ġsatellite', 'Ġreconnaissance', 'Ġsatellite', 'Ġreconnaissance', 'Ġsatellite', 'Ġintelligence', 'Ġsatellite', 'common', 'ly', 'Ġalthough', 'Ġun', 'offic', 'ially', 'Ġreferred', 'Ġsatellite', 'Ġearth', 'Ġobservation', 'Ġsatellite', 'Ġcommunications', 'Ġsatellite', 'Ġdeployed', 'Ġmilitary', 'Ġintelligence', 'Ġapplications', 'Ġfirst', 'Ġgeneration', 'Ġtype', 'e', '.,', 'Ġcor', 'ona', 'Ġz', 'en', 'Ġtook', 'Ġphotographs', 'Ġejected', 'isters', 'Ġphotographic', 'Ġfilm', 'Ġwould', 'Ġdescend', 'Ġback', 'Ġearth', "'s", 'Ġatmosphere', 'Ġcor', 'ona', 'Ġcapsules', 'Ġretrieved', 'Ġmid', 'air', 'Ġfloated', 'Ġparach', 'utes', 'Ġlater', 'Ġspacecraft', 'Ġdigital', 'Ġimaging', 'Ġsystems', 'Ġdownloaded', 'Ġimages', 'Ġvia', 'Ġencrypted', 'Ġradio', 'Ġlinks', 'Ġunited', 'Ġstates', 'Ġinformation', 'Ġavailable', 'Ġreconnaissance', 'Ġsatellites', 'Ġprograms', 'Ġexisted', 'Ġinformation', 'Ġdeclass', 'ified', 'Ġdue', 'Ġage', 'Ġinformation', 'Ġprograms', 'Ġtime', 'Ġstill', 'Ġclassified', 'Ġinformation', 'Ġsmall', 'Ġamount', 'Ġinformation', 'Ġavailable', 'Ġsubsequent', 'Ġmissions', 'date', 'Ġreconnaissance', 'Ġsatellite', 'Ġimages', 'Ġdeclass', 'ified', 'Ġoccasion', 'Ġleaked', 'Ġcase', 'Ġphotographs', 'Ġsent', 'Ġj', 'ane', "'s", 'Ġdefence', 'Ġweekly', 'Ġmarch', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġofficially', 'Ġordered', 'Ġdevelopment', 'Ġadvanced', 'Ġreconnaissance', 'Ġsatellite', 'Ġprovide', 'Ġcontinuous', 'Ġsurveillance', 'pre', 'selected', 'Ġareas', 'Ġearth', 'Ġorder', 'Ġdetermine', 'Ġstatus', 'Ġpotential', 'Ġenemy', 'âĢ', 'Ļ', 'Ġwar', 'making', 'Ġcapability', '".[', 'Ġseveral', 'Ġmajor', 'Ġtypes', 'Ġreconnaissance', 'Ġsatellite', 'Ġmissile', 'Ġearly', 'Ġwarning', 'Ġprovides', 'Ġwarning', 'Ġattack', 'Ġdetecting', 'Ġballistic', 'Ġmissile', 'Ġlaunches', 'Ġearliest', 'Ġknown', 'Ġmissile', 'Ġdefense', 'Ġalarm', 'Ġsystem', 'Ġnuclear', 'Ġexplosion', 'Ġdetection', 'Ġdetects', 'Ġnuclear', 'Ġdeton', 'ation', 'Ġspace', 'Ġvel', 'Ġearliest', 'Ġknown', 'Ġhistory', 'Ġtypes', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġu', 'Ġlac', 'rosse', 'Ġradar', 'Ġsatellite', 'Ġconstruction', 'Ġmodel', 'Ġg', 'erman', 'Ġsar', 'lu', 'pe', 'Ġreconnaissance', 'Ġsatellite', 'Ġinside', 'Ġcosmos', 'Ġrocket', 'Ġmicrowave', 'Ġinterception', 'r', 'hy', 'ol', 'ite', 'Ġelectronic', 'Ġreconnaissance', 'Ġsignals', 'Ġintelligence', 'Ġintercept', 'Ġstray', 'Ġradio', 'Ġwaves', 'Ġsol', 'rad', 'Ġearliest', 'Ġoptical', 'Ġimaging', 'Ġsurveillance', 'Ġearth', 'Ġimaging', 'Ġsatellites', 'Ġsatellite', 'Ġimages', 'Ġsurvey', 'Ġclose']</t>
         </is>
       </c>
       <c r="C346" t="n">
@@ -4936,7 +4936,7 @@
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>['Ġgrilled', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġerrors', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'Ġcope', 'errors', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġtwo', 'Ġhalves', 'Ġhub', 'ble', "'s", 'Ġus', 'Ġbillion', 'Ġsuccessor', 'Ġï', '¬', 'ģ', 'n', 'ally', 'Ġcome', 'Ġtogether', 'Ġyears', 'Ġwaiting', 'Ġbusiness', 'Ġinsider', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġse', 'pt', 'ember', 'Ġtwo', 'Ġdecades', 'Ġweb', 'b', 'Ġtelescope', 'Ġï', '¬', 'ģ', 'n', 'ished', 'Ġway', 'Ġlaunch', 'Ġsite', 'Ġna', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġwall', 'ike', 'Ġoct', 'ober', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarrives', 'Ġfrench', 'Ġgu', 'iana', 'Ġahead', 'Ġde', 'cember', 'Ġlaunch', 'f', 'rench', 'gu', 'iana', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġn', 'asa', 'Ġcongressional', 'Ġbudget', 'ï', '¬', 'ģ', 'cation', 'Ġn', 'asa', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġj', 'une', 'j', 'w', 'st', 'Ġlaunch', 'Ġslips', 'mber', 'Ġlips', 'n', 'ovember', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġoct', 'ober', 'Ġl', 'illy', 'Ġsim', 'mber', 'Ġnext', 'Ġgeneration', 'Ġspace', 'Ġtelescope', 'ng', 'st', ')"', 'Ġuniversity', 'Ġtor', 'onto', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'ng', 'st', 'Ġweekly', 'Ġmiss', 'ive', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġaug', 'ust', 'n', 'asa', 'Ġmod', 'ï', '¬', 'ģ', 'es', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġcontract', 'mber', 'Ġarchived', 'Ġl', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust']</t>
+          <t>['look', 'Ġtele', 'photo', 'Ġcor', 'ona', 'Ġearliest', 'Ġknown', 'Ġspectral', 'Ġimaging', 'Ġcommonplace', 'Ġradar', 'Ġimaging', 'Ġsurveillance', 'Ġspace', 'based', 'Ġrad', 'ars', 'Ġuse', 'Ġsynthetic', 'ap', 'ert', 'ure', 'Ġradar', 'Ġused', 'Ġnight', 'Ġcloud', 'Ġcover', 'Ġearliest', 'Ġknown', 'v', 'iet', 'Ġus', 'Ġseries', 'Ġexamples', 'Ġreconnaissance', 'Ġsatellite', 'Ġmissions', 'Ġhigh', 'Ġresolution', 'Ġphotography', 'im', 'int', 'Ġmeasurement', 'Ġsignature', 'Ġintelligence', 'mas', 'int', 'Ġcommunications', 'Ġeaves', 'dropping', 'ig', 'int', 'Ġcovert', 'Ġcommunications', 'Ġmonitoring', 'Ġnuclear', 'Ġtest', 'Ġban', 'Ġcompliance', 'see', 'Ġnational', 'Ġtechnical', 'Ġmeans', 'Ġdetection', 'Ġmissile', 'Ġlaunches', 'Ġaug', 'ust', 'Ġthought', 'billion', 'Ġhigh', 'powered', 'Ġsatellite', 'Ġcapable', 'Ġsnapping', 'Ġpictures', 'Ġdetailed', 'Ġenough', 'Ġdistinguish', 'Ġmake', 'Ġmodel', 'Ġautomobile', 'Ġhundreds', 'Ġmiles', '"[', 'Ġlaunched', 'Ġcal', 'ornia', "'s", 'Ġv', 'enberg', 'Ġair', 'Ġforce', 'Ġbase', 'Ġusing', 'Ġdelta', 'Ġiv', 'Ġheavy', 'Ġlauncher', 'Ġameric', "'s", 'Ġhighest', 'pay', 'load', 'Ġspace', 'Ġlaunch', 'Ġvehicle', 'Ġtime', 'Ġfe', 'b', 'ruary', 'Ġr', 'ussian', 'Ġk', 'os', 'mos', 'Ġoriginally', 'Ġlaunched', 'Ġused', 'Ġnaval', 'Ġmissile', 'Ġtargeting', 'Ġmade', 'Ġuncontrolled', 'Ġatmospheric', 'Ġentry', 'v', 'iet', 'Ġled', 'Ġameric', 'Ġfears', 'Ġbomber', 'Ġgap', 'Ġgaining', 'Ġsatellite', 'Ġphotography', 'Ġunited', 'Ġstates', 'Ġintelligence', 'Ġagencies', 'Ġable', 'Ġstate', 'Ġcertainty', 'Ġnew', 'Ġcomplexes', 'Ġestablished', 'Ġus', 'sr', 'Ġpast', 'Ġyear', '".', 'Ġpresident', 'Ġly', 'nd', 'Ġb', 'Ġjohn', 'son', 'Ġtold', 'Ġgathering', ':[', "'t", 'Ġwant', 'Ġquoted', 'Ġ...', "'ve", 'Ġspent', 'Ġbillion', 'Ġspace', 'Ġprogram', 'Ġnothing', 'Ġelse', 'Ġcome', 'Ġexcept', 'Ġknowledge', 'Ġgained', 'Ġspace', 'Ġphotography', 'Ġwould', 'Ġworth', 'Ġten', 'Ġtimes', 'Ġwhole', 'Ġprogram', 'Ġcost', 'Ġmissions', 'Ġbenefits', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġtonight', 'Ġknow', 'Ġmany', 'Ġmissiles', 'Ġenemy', 'Ġturned', 'Ġguesses', 'Ġway', 'Ġthings', "'t", 'Ġneed', 'Ġbuilding', 'Ġthings', "'t", 'Ġneed', 'Ġbuild', 'Ġharbor', 'ing', 'Ġfears', "'t", 'Ġneed', 'Ġharbor', 'Ġstate', 'Ġunion', 'Ġaddress', 'Ġpresident', 'Ġj', 'im', 'Ġcar', 'ter', 'Ġexplained', 'Ġhumanity', 'Ġbenefited', 'Ġpresence', 'Ġameric', 'Ġsatellites', ':[', 'Ġsatellites']</t>
         </is>
       </c>
       <c r="C347" t="n">
@@ -4949,7 +4949,7 @@
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>['Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'pro', 'blems', 'Ġj', 'w', 'st', 'Ġmay', 'Ġarchived', 'Ġproblems', 'j', 'w', 'st', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġaug', 'ust', 'ref', 'ocusing', 'Ġn', 'asa', "'s", 'Ġvision', 'Ġnature', '):', 'Ġmarch', '.).', 'Ġdoi', '01', 'Ġpm', 'id', 'pub', 'med', 'Ġcow', 'en', 'Ġr', 'Ġaug', 'ust', 'bb', 'Ġtelescope', 'Ġdelayed', 'Ġcosts', 'Ġrise', 'Ġbillion', 'web', 'ar', 'Ġscience', 'ins', 'ider', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'independent', 'Ġcomprehensive', 'Ġreview', 'Ġpanel', 'Ġfinal', 'Ġreport', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'os', 'Ġj', 'athan', 'Ġaug', 'ust', 'j', 'w', 'st', 'Ġprice', 'Ġtag', 'Ġput', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġj', 'une', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunched', 'Ġspring', 'Ġn', 'asa', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'n', 'asa', 'Ġdelays', 'Ġlaunch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'n', 'asa', 'Ġcompletes', 'Ġweb', 'b', 'Ġtelescope', 'Ġreview', 'Ġcommits', 'Ġlaunch', 'Ġearly', 'n', 'asa', 'Ġn', 'asa', 'gov', 'Ġn', 'asa', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', 'Ġdelays', 'Ġlaunch', 'Ġweb', 'b', 'Ġtelescope', 'Ġearlier', 'Ġdec', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['Ġexample', 'Ġenormously', 'Ġimportant', 'Ġstabil', 'izing', 'Ġworld', 'Ġaffairs', 'Ġthereby', 'Ġmake', 'Ġsignificant', 'Ġcontribution', 'Ġsecurity', 'Ġnations', 'Ġreconnaissance', 'Ġsatellites', 'Ġused', 'Ġenforce', 'Ġhuman', 'Ġrights', 'Ġsatellite', 'Ġsent', 'inel', 'Ġproject', 'Ġmonitors', 'Ġatrocities', 'Ġsu', 'dan', 'Ġsouth', 'Ġsu', 'dan', 'Ġadditionally', 'Ġcompanies', 'Ġge', 'oe', 'ye', 'Ġdigital', 'gl', 'obe', 'Ġprovided', 'Ġcommercial', 'Ġsatellite', 'Ġimagery', 'Ġsupport', 'Ġnatural', 'Ġdisaster', 'Ġresponse', 'Ġhumanitarian', 'Ġmissions', 'Ġsatellites', 'Ġcommonly', 'Ġseen', 'Ġfiction', 'Ġmilitary', 'Ġfiction', 'Ġworks', 'Ġfiction', 'Ġfocus', 'Ġspecifically', 'Ġsatellites', 'Ġinclude', 'mac', 'Ġproject', 'Ġenemy', 'Ġstate', 'Ġbody', 'Ġlies', 'Ġice', 'Ġstation', 'Ġz', 'ebra', 'Ġpar', 'man', 'u', 'Ġstory', 'Ġp', 'ok', 'hran', 'Ġpatriot', 'Ġgames', 'Ġaerial', 'Ġreconnaissance', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'u', '.)', 'Ġeuro', 'pe', 'Ġunion', 'Ġsatellite', 'Ġcentre', 'Ġlist', 'Ġintelligence', 'Ġgathering', 'Ġdisciplines', 'Ġlist', 'Ġk', 'os', 'mos', 'Ġsatellites', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'u', '.)', 'Ġsat', 'Ġmove', 'cor', 'ona', 'Ġhistory', 'Ġr', 'ona', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', '].', 'Ġarchived', 'Ġoriginal', 'Ġr', 'cor', 'ona', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'cor', 'ona', 'Ġprogram', 'Ġmission', 'Ġspacecraft', 'Ġlibrary', 'Ġarchived', 'Ġoriginal', 'http', 'space', 'j', 'pl', 'n', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġfiction', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġwr', 'ight', 'ichael', 'ron', 'Ġcar', 'oline', 'Ġrand', 'Ġde', 'cember', 'two', 'Ġyears', 'Ġmor', 'ison', 'Ġnew', 'ork', 'Ġtimes', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġer', 'ickson', 'Ġmark', 'Ġunknown', 'Ġtogether', 'Ġdod', 'Ġn', 'asa', 'Ġearly', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'http', 'Ġair', 'Ġuniversity', 'Ġpress', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġreconnaissance', 'Ġsatellite', 'Ġinf', 'ople', 'ase', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġnavy', "'s", 'Ġmissions', 'Ġspace', 'Ġu', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'nn', 'igan', 'Ġaug', 'ust']</t>
         </is>
       </c>
       <c r="C348" t="n">
@@ -4962,7 +4962,7 @@
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>['Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'âĢĵ', 'cc', 'us', 'ker', 'Ġj', 'Ġj', 'Ġmuch', 'Ġreal', 'Ġmoney', 'Ġhistorical', 'Ġprice', 'Ġindex', 'Ġuse', 'Ġde', 'ï', '¬', 'Ĥ', 'ator', 'Ġmoney', 'Ġvalues', 'Ġeconomy', 'Ġunited', 'Ġstates', 'Ġadd', 'enda', 'Ġet', 'Ġcor', 'rig', 'enda', 'Ġameric', 'Ġantiqu', 'arian', 'Ġsociety', 'âĢĵ', 'cc', 'us', 'ker', 'Ġj', 'Ġj', 'Ġmuch', 'Ġreal', 'Ġmoney', 'Ġhistorical', 'Ġprice', 'Ġindex', 'Ġuse', 'Ġde', 'ï', '¬', 'Ĥ', 'ator', 'Ġmoney', 'Ġvalues', 'Ġeconomy', 'Ġunited', 'Ġstates', 'Ġameric', 'Ġantiqu', 'arian', 'Ġsociety', 'âĢĵ', 'Ġpresent', 'Ġfederal', 'Ġreserve', 'Ġbank', 'Ġmin', 'neapolis', 'consumer', 'Ġprice', 'Ġindex', 'est', 'imate', 'âĢĵ', 'Ġretrieved', 'Ġmay', 'ck', 'ie', 'Ġrob', 'Ġj', 'uly', 'n', 'asa', 'Ġï', '¬', 'ģ', 'gh', 'ts', 'Ġsave', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġguardian', 'Ġl', 'ondon', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'appropri', 'ations', 'Ġcommittee', 'Ġreleases', 'Ġfiscal', 'Ġyear', 'Ġcommerce', 'Ġjustice', 'Ġscience', 'Ġappropriations', 'Ġus', 'Ġhouse', 'Ġrepresentatives', 'Ġcommittee', 'Ġappropriations', 'Ġj', 'uly', 'Ġarchived', 'web', 'c', 'ument', 'id', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'us', 'Ġlawmakers', 'Ġvote', 'Ġkill', 'Ġhub', 'ble', 'Ġsuccessor', 'Ġspaced', 'aily', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'prop', 'osed', 'Ġn', 'asa', 'Ġbudget', 'Ġbill', 'Ġwould', 'Ġcancel', 'Ġmajor', 'Ġspace', 'Ġtelescope', 'Ġspace', 'Ġj', 'uly', 'Ġarchived', 'http', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġber', 'gin', 'Ġch', 'ris', 'Ġjan', 'uary', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġhardware', 'Ġentering', 'Ġkey', 'Ġtest', 'Ġphase', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġaug', 'ust', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġhand', 'Ġe']</t>
+          <t>['monster', 'Ġrocket', 'Ġblast', 'Ġpac', 'ï', '¬', 'ģ', 'c', 'Ġcoast', 'Ġr', 'attle', 'Ġsouth', 'land', 'story', 'Ġlos', 'Ġangel', 'es', 'Ġtimes', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġmel', 'issa', 'Ġgold', 'Ġfe', 'b', 'ruary', 'fr', 'ag', 'ments', 'v', 'iet', 'era', 'Ġsatellite', 'Ġburn', 'Ġearth', "'s", 'Ġatmosphere', 'Ġmash', 'able', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'pp', 'en', 'heimer', 'Ġspace', 'Ġshuttle', 'Ġdecision', 'Ġts', 'htm', 'Ġn', 'asa', 'Ġpp', 'Ġstate', 'Ġunion', 'Ġannual', 'Ġmessage', 'Ġcongress', 'Ġstate', 'Ġunion', 'Ġaddress', 'Ġameric', 'Ġpresidency', 'Ġproject', 'Ġretrieved', 'Ġapr', 'il', 'commercial', 'Ġsatellite', 'Ġimagery', 'Ġcompanies', 'Ġpartner', 'Ġu', 'Ġgeological', 'Ġsurvey', 'Ġsupport', 'Ġinternational', 'Ġcharter', 'space', 'Ġmajor', 'Ġdisasters', 'Ġus', 'gs', 'Ġnews', 'room', 'Ġunited', 'Ġstates', 'Ġgeological', 'Ġsurvey', 'Ġretrieved', 'Ġapr', 'il', 'Ġk', 'upper', 'berg', 'Ġp', 'aul', 'Ġsatellites', 'Ġro', 'sen', 'Ġpublishing', 'Ġgroup', 'Ġric', 'hel', 'son', 'Ġje', 'ff', 'rey', 'Ġameric', "'s", 'Ġsecret', 'Ġeyes', 'Ġspace', 'Ġu', 'Ġkey', 'hole', 'Ġsatellite', 'Ġprogram', 'Ġhar', 'per', 'Ġrow', 'ris', 'Ġpat', 'Ġspies', 'Ġsurveillance', 'Ġsatellites', 'Ġwar', 'Ġpeace', 'Ġber', 'lin', 'Ġnew', 'ork', 'Ġspring', 'er', 'Ġch', 'iche', 'ster', 'Ġassociation', 'Ġpra', 'x', 'Ġpublishing', 'http', 'cl', 'c', 'Ġcl', 'c', 'Ġf', 'Ġintelligence', 'Ġresource', 'Ġprogram', 'Ġimagery', 'Ġintelligence', 'im', 'int', 'Ġir', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsatellite', 'Ġarchived', 'Ġh', 'tm', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'mis', 'rs', 'Ġreading', 'Ġexternal', 'Ġlinks', 'Ġreconnaissance', 'Ġsatellite', 'Ġwik', 'ipedia', 'Ġspac', 'ep', 'orts', 'Ġaround', 'Ġworld', 'Ġal', 'bar', 'Ġspace', 'Ġresearch', 'Ġcenter', 'Ġmilitary', 'Ġintelligence', 'Ġsatellites', 'Ġv', 'n', 'asa', 'Ġremote', 'Ġsensing', 'Ġtutorial', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C349" t="n">
@@ -4975,7 +4975,7 @@
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>['Ġj', 'uly', 'Ġissues', 'Ġstatement', 'Ġproposed', 'Ġcancellation', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġameric', 'Ġastronomical', 'Ġsociety', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'ik', 'uls', 'ki', 'Ġstatement', 'Ġhouse', 'Ġappropriations', 'Ġsubcommittee', 'Ġtermination', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġspace', 'ref', 'Ġj', 'uly', 'Ġarchived', 'Ġe', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'way', 'Ġshuttle', 'Ġflight', 'Ġl', 'ref', 'op', 'inion', 'Ġnew', 'ork', 'Ġtimes', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhar', 'ro', 'ld', 'Ġj', 'uly', 'bad', 'Ġnews', 'ada', 'Ġu', 'Ġcould', 'Ġscrap', 'Ġnew', 'Ġspace', 'Ġtelescope', 'http', 'story', 'html', 'Ġv', 'ancouver', 'Ġsun', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'n', 'asa', 'Ġbudget', 'Ġplan', 'Ġsaves', 'Ġtelescope', 'Ġcuts', 'Ġspace', 'Ġtaxis', 'uters', 'mber', 'Ġarchived', 'web', 'arch', 'iv', 'Ġtre', 'af', '06', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'uly', 'Ġle', 'one', 'Ġdan', 'mber', 'n', 'asa', 'Ġacknowledges', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġcosts', 'Ġdelay', 'Ġscience', 'Ġmissions', 'missions', 'html', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmos', 'k', 'owitz', 'Ġcl', 'ara', 'Ġmarch', 'n', 'asa', 'Ġassures', 'Ġskeptical', 'Ġcongress', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġtrack', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġbill', 'ings', 'Ġle', 'e', 'Ġoct', 'ober', 'Ġtelescope', 'Ġate', 'Ġastronomy', 'Ġnature', '):', 'âĢĵ', 'Ġpm', 'id', 'Ġk', 'oren', 'Ġmar', 'ina', 'Ġde', 'cember', 'Ġextreme', 'Ġha', 'zing', 'Ġexpensive', 'Ġtelescope', 'Ġever', 'Ġbuilt', 'l', 'antic', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved']</t>
+          <t>['09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġelectron', 'Ġelectron', 'Ġlaunching', 'Ġtrop', 'ics', 'Ġmanufacturer', 'Ġrocket', 'Ġlab', 'Ġcountry', 'Ġorigin', 'Ġnew', 'Ġzeal', 'Ġunited', 'Ġstates', 'Ġproject', 'Ġcost', 'Ġus', 'Ġmillion', 'Ġcost', 'Ġper', 'Ġlaunch', 'Ġmillion', 'Ġsize', 'Ġheight', 'Ġdiameter', 'Ġft', 'Ġmass', '000', 'Ġstages', 'âĢĵ', 'Ġcapacity', 'Ġpayload', 'Ġle', 'Ġmass', 'Ġoriginal', 'Ġupdated', 'Ġpayload', 'Ġmass', 'Ġoriginal', 'Ġupdated', 'Ġassociated', 'Ġrockets', 'Ġcomparable', 'Ġsh', 'av', 'Ġun', 'ha', 'Ġprime', 'Ġmi', 'ura', 'Ġrocket', 'Ġlab', 'Ġelectron', 'red', 'irect', 'ed', 'Ġelectron', 'rocket', '))', 'Ġelectron', 'Ġtwo', 'stage', 'Ġpartially', 'Ġrecover', 'able', 'Ġorbital', 'Ġlaunch', 'Ġvehicle', 'Ġdeveloped', 'Ġrocket', 'Ġlab', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġwholly', 'Ġowned', 'Ġnew', 'Ġzeal', 'Ġsubsidiary', 'Ġelectron', 'Ġdeveloped', 'Ġservice', 'Ġcommercial', 'Ġsmall', 'Ġsatellite', 'Ġlaunch', 'Ġmarket', 'Ġr', 'utherford', 'Ġengines', 'Ġfirst', 'Ġelectric', 'p', 'ump', 'fed', 'Ġengine', 'Ġpower', 'Ġorbital', 'class', 'Ġrocket', 'Ġelectron', 'Ġoften', 'Ġflown', 'Ġkick', 'stage', 'Ġrocket', 'Ġlab', "'s", 'Ġphoton', 'Ġspacecraft', 'Ġalthough', 'Ġrocket', 'Ġdesigned', 'Ġexpend', 'able', 'Ġrocket', 'Ġlab', 'Ġrecovered', 'Ġfirst', 'Ġstage', 'Ġtwice', 'Ġworking', 'Ġtowards', 'Ġcapability', 'using', 'Ġbooster', 'Ġflight', 'Ġbooster', 'Ġfeatured', 'Ġfirst', 'Ġhelicopter', 'Ġcatch', 'Ġrecovery', 'Ġattempt', 'Ġde', 'cember', 'Ġelectron', 'Ġcompleted', 'Ġflight', 'Ġqualification', 'Ġfirst', 'Ġrocket', 'Ġlaunched', 'Ġmay', 'Ġflight', 'Ġcalled', "'s", 'Ġtest', '",', 'Ġreaching', 'Ġspace', 'Ġachieving', 'Ġorbit', 'Ġdue', 'Ġglitch', 'Ġcommunication', 'Ġequipment', 'Ġground', 'Ġsecond', 'Ġflight', 'Ġjan', 'uary', 'Ġelectron', 'Ġreached', 'Ġorbit', 'Ġdeployed', 'Ġthree', 'Ġcubes', 'ats', 'Ġmission', 'Ġcalled', 'still', 'Ġtesting', '".[', 'Ġfirst', 'Ġcommercial', 'Ġlaunch', 'Ġelectron', 'Ġthird', 'Ġlaunch', 'Ġoverall', 'Ġoccurred', 'mber', 'Ġmission', 'Ġcalled', "'s", 'Ġbusiness', 'Ġtime', '".[', 'Ġsince', 'Ġelectron', 'Ġlaunched', 'Ġsuccessfully', 'Ġthirty', 'Ġtimes', 'Ġelectron', 'Ġuses', 'Ġtwo', 'Ġstages', 'Ġdiameter', 'Ġft', '))', 'Ġfilled', 'Ġpropell', 'ant', 'Ġmain', 'Ġbody', 'Ġrocket', 'Ġconstructed', 'Ġusing', 'Ġlightweight', 'Ġcarbon', 'Ġcomposite', 'Ġmaterial', 'Ġstages', 'Ġuse', 'Ġr', 'utherford', 'Ġrocket']</t>
         </is>
       </c>
       <c r="C350" t="n">
@@ -4988,7 +4988,7 @@
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>['Ġjan', 'uary', 'Ġco', 'hen', 'Ġben', 'Ġj', 'uly', 'Ġn', 'asa', 'Ġengineer', 'Ġmade', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwork', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġiss', 'n', 'Ġ00', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġpot', 'ter', 'Ġse', 'Ġj', 'uly', 'n', 'asa', 'Ġweb', 'b', 'Ġprogram', 'Ġdirector', 'Ġg', 'reg', 'Ġrob', 'inson', 'Ġannounces', 'Ġretirement', 'Ġet', 'irement', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġw', 'ang', 'Ġj', 'en', 'Ġco', 'le', 'Ġste', 'Ġnorth', 'Ġk', 'Ġmarch', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġobserv', 'atory', 'Ġrequires', 'Ġtime', 'Ġtesting', 'Ġevaluation', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'os', 'Ġj', 'athan', 'Ġmarch', 'hub', 'ble', 'success', 'Ġfaces', 'Ġnew', 'Ġdelay', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġwit', 'ze', 'lex', 'andra', 'Ġmarch', 'n', 'asa', 'Ġreveals', 'Ġmajor', 'Ġdelay', 'billion', 'Ġhub', 'ble', 'Ġsuccessor', 'ht', 'Ġnature', '):', 'âĢĵ', 'Ġpm', 'id', 'ier', 'Ġcase', 'Ġfe', 'b', 'ruary', 'n', 'asa', 'Ġgot', 'Ġbest', 'Ġbudget', 'Ġdecade', 'http', 'plan', 'eta', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġmarch', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'cor', 'av', 'irus', 'Ġpauses', 'Ġwork', 'Ġj', 'w', 'st', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġapr', 'il', 'esa', 'Ġscience', 'Ġtechnology', 'Ġeuro', 'pe', "'s", 'Ġcontributions', 'Ġj', 'w', 'st', 'Ġmission', 'Ġeuro', 'pe', 'Ġspace', 'Ġagency', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'adian', 'Ġspace', 'Ġagency', 'eyes', 'Ġhub', 'ble', "'s", 'Ġsuccessor', 'ada', 'Ġdelivers', 'Ġcontribution', 'Ġworld', "'s"]</t>
+          <t>['Ġengine', 'Ġfirst', 'Ġelectric', 'p', 'ump', 'fed', 'Ġengine', 'Ġpower', 'Ġorbital', 'Ġrocket', 'Ġelectric', 'Ġpumps', 'Ġpowered', 'Ġlithium', 'poly', 'mer', 'Ġbatteries', 'Ġsecond', 'Ġstage', 'Ġuses', 'Ġthree', 'Ġbatteries', 'hot', 'Ġswapped', '",', 'Ġtwo', 'Ġbatteries', 'Ġj', 'ett', 'ison', 'ed', 'Ġdepleted', 'Ġshed', 'Ġmass', 'Ġnine', 'Ġr', 'utherford', 'Ġengines', 'Ġfirst', 'Ġstage', 'Ġone', 'Ġvacuum', 'optim', 'ized', 'Ġversion', 'Ġsecond', 'Ġstage', 'Ġfirst', 'Ġstage', 'Ġengines', 'Ġdeliver', 'Ġkn', '000', 'Ġthrust', 'Ġsecond', 'Ġstage', 'Ġdelivers', 'Ġkn', 'Ġthrust', 'Ġalmost', 'Ġengines', 'Ġparts', 'Ġprinted', 'Ġsave', 'Ġtime', 'Ġmoney', 'Ġmanufacturing', 'Ġprocess', 'Ġrocket', 'Ġlab', 'Ġalso', 'Ġdeveloped', 'Ġoptional', 'Ġthird', 'Ġstage', 'Ġknown', 'kick', 'Ġstage', '",', 'Ġdesigned', 'Ġcircular', 'ize', 'Ġorbits', 'Ġsatellite', 'Ġpayload', 'Ġstage', 'Ġalso', 'Ġputs', 'Ġsatellites', 'Ġaccurate', 'Ġorbit', 'Ġless', 'Ġtime', 'Ġelectron', 'Ġkick', 'Ġstage', 'Ġequipped', 'Ġsingle', 'Ġcur', 'ie', 'Ġengine', 'Ġcapable', 'Ġperforming', 'Ġmultiple', 'Ġburns', 'Ġuses', 'Ġunspecified', 'green', 'Ġbip', 'ro', 'pell', 'ant', 'Ġprinted', 'Ġfirst', 'Ġused', 'Ġelectron', "'s", 'Ġsecond', 'Ġflight', 'Ġkick', 'Ġstage', 'Ġtransport', 'Ġpayload', 'Ġrocket', 'Ġlab', 'Ġalso', 'Ġdeveloped', 'Ġderivative', 'Ġspacecraft', 'Ġkick', 'Ġstage', 'Ġphoton', 'Ġintended', 'Ġuse', 'Ġlunar', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'Ġphoton', 'Ġcapable', 'Ġdelivering', 'Ġsmall', 'Ġpayload', 'Ġlunar', 'Ġorbit', 'Ġdesign', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġlaunch', 'Ġhistory', 'Ġstatus', 'Ġactive', 'Ġlaunch', 'Ġsites', 'Äģ', 'h', 'ia', 'active', 'Ġmars', 'active', 'Ġsax', 'av', 'ord', 'prop', 'osed', 'utherland', 'prop', 'osed', ')[', 'Ġtotal', 'Ġlaunches', 'Ġsuccess', 'es', 'Ġfailure', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġmay', 'Ġlast', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġse', 'pt', 'ember', 'active', 'Ġfirst', 'Ġstage', 'Ġheight', 'Ġft', 'Ġdiameter', 'Ġft', 'Ġpowered', 'Ġr', 'utherford', 'Ġmaximum', 'Ġthrust', 'Ġsea', 'Ġlevel', 'Ġkn', 'Ġvacuum', 'Ġkn', '000', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', '05', 'Ġpropell', 'ant', 'Ġsecond', 'Ġstage', 'Ġheight', 'Ġft', 'Ġdiameter']</t>
         </is>
       </c>
       <c r="C351" t="n">
@@ -5001,7 +5001,7 @@
       </c>
       <c r="B352" t="inlineStr">
         <is>
-          <t>['Ġpowerful', 'Ġspace', 'Ġtelescope', 'adian', 'Ġspace', 'Ġagency', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġsp', 'Ġapr', 'il', 'Ġj', 'en', 'ner', 'Ġlyn', 'n', 'Ġj', 'une', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġinternational', 'Ġendeavor', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'inst', 'itutional', 'Ġpartners', 'Ġweb', 'b', 'n', 'asa', 'Ġj', 'w', 'st', 'n', 'asa', 'gov', 'Ġretrieved', 'Ġaug', 'ust', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġshepherd', 'ony', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġworld', "'s", 'Ġpowerful', 'Ġtelescope', 'Ġmakes', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcall', 'Ġaust', 'ral', 'ia', 'Ġchrist', 'mas', 'Ġday', 'Ġguardian', 'Ġarchived', 'Ġn', 'christ', 'mas', 'day', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfranc', 'Ġmatt', 'hew', 'Ġproblem', 'Ġnaming', 'Ġobserv', 'atories', 'Ġbig', 'ots', 'Ġforb', 'es', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġsavage', 'Ġdan', 'Ġjan', 'uary', 'Ġn', 'asa', 'Ġname', 'Ġtelescope', 'Ġdead', 'Ġpersecuted', 'Ġgay', 'Ġpeople', '?"', 'Ġstranger', 'Ġarchived', 'Ġple', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġapr', 'il', 'Ġfisher', 'Ġal', 'ise', 'mber', 'n', 'asa', 'Ġshares', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġhistory', 'Ġreport', 'n', 'asa', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'dom', 'Ġb', 'rian', 'Ġc', 'n', 'asa', 'Ġhistorical', 'Ġinvestigation', 'Ġj', 'ames', 'Ġe', 'Ġweb', 'b', "'s", 'Ġrelationship', 'Ġlav', 'ender', 'Ġscare', 'Ġfinal', 'Ġreport', 'Ġn', 'asa', 'gov', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġwit', 'ze', 'lex', 'andra', 'mber', 'n', 'asa', 'Ġreally', 'Ġreally', "'t", 'Ġrename', 'Ġweb', 'b', 'Ġtelescope', 'Ġdespite', 'Ġcommunity', 'Ġpush', 'back', 'Ġnature', 'Ġpm', 'id', '00', 'api', 'se', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved']</t>
+          <t>['Ġft', 'Ġpowered', 'Ġr', 'utherford', 'Ġmaximum', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġpropell', 'ant', 'Ġkick', 'Ġstage', 'optional', 'Ġphoton', 'Ġpowered', 'Ġcur', 'ie', 'Ġmaximum', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġpropell', 'ant', 'Ġvisc', 'ous', 'Ġliquid', 'Ġmonop', 'ro', 'pell', 'ant', 'ap', 'Ġal', 'Ġkick', 'Ġstage', 'optional', 'Ġphoton', 'mod', 'ï', '¬', 'ģ', 'ed', 'Ġpowered', 'Ġhyper', 'cur', 'ie', 'Ġrocket', 'Ġlab', "'s", 'Ġelectron', 'Ġreturn', 'Ġphases', 'Ġelectron', 'Ġpayload', 'Ġfair', 'ing', 'Ġfeet', 'Ġinches', 'Ġlength', 'Ġfeet', 'Ġinches', 'Ġdiameter', 'Ġtotal', 'Ġmass', 'Ġmanufacturing', 'Ġcarbon', 'Ġcomposite', 'Ġcomponents', 'Ġmain', 'Ġflight', 'Ġstructure', 'Ġtraditionally', 'Ġrequired', 'Ġhours', 'Ġextensive', 'Ġhand', 'Ġlabor', 'Ġprocess', 'Ġlate', 'Ġrocket', 'Ġlab', 'Ġbrought', 'Ġnew', 'Ġrobotic', 'Ġmanufacturing', 'Ġcapability', 'Ġonline', 'Ġproduce', 'Ġcomposite', 'Ġparts', 'Ġelectron', 'Ġhours', 'Ġrobot', 'Ġnicknamed', 'ros', 'ie', 'Ġrobot', '",', 'Ġjets', 'ons', 'Ġcharacter', 'Ġprocess', 'Ġmake', 'Ġcarbon', 'Ġfiber', 'Ġstructures', 'Ġwell', 'Ġhandle', 'Ġcutting', 'Ġdrilling', 'Ġsand', 'ing', 'Ġparts', 'Ġready', 'Ġfinal', 'Ġassembly', 'Ġcompany', 'Ġobjective', 'mber', 'Ġreduce', 'Ġoverall', 'Ġelectron', 'Ġmanufacturing', 'Ġcycle', 'Ġseven', 'Ġdays', 'Ġr', 'utherford', 'Ġengine', 'Ġproduction', 'Ġmakes', 'Ġextensive', 'Ġuse', 'Ġadditive', 'Ġmanufacturing', 'Ġsince', 'Ġearliest', 'Ġflights', 'Ġelectron', 'Ġallows', 'Ġcapability', 'Ġscale', 'Ġproduction', 'Ġrelatively', 'Ġstraightforward', 'Ġmanner', 'Ġincreasing', 'Ġnumber', 'Ġcapability', 'Ġprinters', 'Ġaug', 'ust', 'Ġrocket', 'Ġlab', 'Ġannounced', 'Ġrecovery', 'Ġref', 'light', 'Ġplans', 'Ġfirst', 'Ġstage', 'Ġelectron', 'Ġalthough', 'Ġplans', 'Ġstarted', 'Ġinternally', 'Ġlate', 'Ġelectron', 'Ġoriginally', 'Ġdesigned', 'Ġreusable', 'Ġlaunch', 'Ġvehicle', 'Ġsmall', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġpursued', 'Ġdue', 'Ġincreased', 'Ġunderstanding', 'Ġelectron', "'s", 'Ġperformance', 'Ġbased', 'Ġanalysis', 'Ġprevious', 'Ġflights', 'Ġthough', 'Ġsensors', 'Ġvehicle', 'Ġaddition', 'us', 'ability', 'Ġpursued', 'Ġmeet', 'Ġlaunch', 'Ġdemands', 'Ġcounteract', 'Ġdecreased', 'Ġpayload', 'Ġcapacity', 'Ġcaused', 'Ġadded', 'Ġmass', 'Ġrecovery', 'Ġhardware', 'Ġperformance', 'Ġimprovements', 'Ġelectrons', 'Ġexpected', 'Ġearly', 'Ġphases', 'Ġrecovery', 'Ġincluded', 'Ġdata', 'Ġgathering', 'Ġsurviving', 'Ġatmospheric', 'entry', 'Ġalso', 'Ġknown', 'Ġwall', '".[', 'Ġnext', 'Ġphase', 'Ġrequire', 'Ġsuccessful', 'Ġdeployment']</t>
         </is>
       </c>
       <c r="C352" t="n">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="B353" t="inlineStr">
         <is>
-          <t>['mber', 'Ġmas', 'etti', 'Ġmag', 'gie', 'Ġk', 'rish', 'nam', 'ur', 'th', 'ita', 'j', 'w', 'st', 'Ġscience', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'n', 'asa', "'s", 'Ġnext', 'Ġtelescope', 'Ġcould', 'Ġid', 'Ġalien', 'Ġmeg', 'ast', 'ruct', 'ures', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġz', 'immer', 'Ġcar', 'l', 'Ġj', 'uly', 'bb', 'Ġtelescope', 'Ġlook', 'Ġsigns', 'Ġlife', 'Ġway', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġquestion', 'Ġastronomers', 'Ġwant', 'Ġanswer', 'Ġex', 'oplan', 'ets', 'Ġatmosp', 'heres', 'Ġfriendly', 'Ġlife', '?"', 'Ġl', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġupdated', 'Ġst', 'ef', 'anie', 'Ġw', 'ald', 'ek', 'Ġlast', 'Ġmarch', 'n', 'asa', "'s", 'Ġnew', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġable', 'Ġsniff', 'Ġmethane', "'s", 'Ġtell', "'s", 'Ġsign', 'Ġlife', 'Ġspace', 'Ġretrieved', 'Ġaug', 'ust', 'bas', 'ics', 'Ġspace', 'Ġflight', 'Ġjet', 'Ġpropulsion', 'Ġlaboratory', 'Ġarchived', 'Ġp', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġaug', 'ust', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġdich', 'mann', 'ald', 'Ġj', '.;', 'Ġal', 'ber', 'ding', 'Ġcass', 'andra', '.;', 'Ġway', 'ne', 'Ġh', 'Ġmay', 'station', 'keeping', 'Ġmon', 'te', 'Ġcar', 'lo', 'Ġsimulation', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'web', 'arch', 'pdf', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'nt', 'rs', 'n', 'asa', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgreenhouse', 'Ġmatt', 'Ġapr', 'il', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmission', 'Ġn', 'asa', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember']</t>
+          <t>['Ġaer', 'odynamic', 'Ġde', 'celer', 'ator', 'Ġball', 'ute', 'Ġslow', 'Ġbooster', 'Ġfollowed', 'Ġdeployment', 'Ġpar', 'af', 'oil', 'Ġconcluded', 'Ġtouchdown', 'Ġocean', 'Ġsuccessful', 'Ġtouchdown', 'Ġocean', 'Ġstage', 'Ġwould', 'Ġmoved', 'Ġonto', 'Ġship', 'Ġrefurb', 'ishment', 'Ġref', 'light', 'Ġrocket', 'Ġlab', 'Ġreleased', 'Ġinformation', 'Ġaer', 'odynamic', 'Ġde', 'celer', 'ator', 'Ġwould', 'Ġrequired', 'Ġslow', 'Ġbooster', 'Ġatmospheric', 'entry', 'Ġlate', 'Ġphases', 'Ġelectron', 'Ġreuse', 'Ġinvolve', 'Ġusing', 'Ġpar', 'af', 'oil', 'Ġmid', 'air', 'Ġretrieval', 'Ġhelicopter', 'Ġsuccessful', 'Ġmid', 'air', 'Ġretrieval', 'Ġhelicopter', 'Ġwould', 'Ġbring', 'Ġelectron', 'Ġship', 'Ġwould', 'Ġbring', 'Ġstage', 'Ġlaunch', 'Ġsite', 'Ġrefurb', 'ishment', 'Ġlaunch', 'Ġlater', 'Ġrocket', 'Ġlab', 'Ġabandoned', 'Ġplan', 'Ġcatch', 'Ġstage', 'Ġhelicopter', 'Ġuse', 'Ġocean', 'Ġlanding', 'Ġinstead', 'Ġone', 'Ġrecovered', 'Ġr', 'utherford', 'Ġengine', 'Ġpassed', 'Ġfive', 'Ġfull', 'duration', 'Ġhot', 'Ġfire', 'Ġtests', 'Ġdeclared', 'Ġready', 'Ġfly', 'Ġrocket', 'Ġlab', "'s", 'th', 'Ġelectron', 'Ġmission', 'Ġreused', 'Ġrefurb', 'ished', 'Ġr', 'utherford', 'Ġengine', 'Ġprevious', 'Ġflight', 'Ġproduction', 'us', 'ability', 'Ġaer', 'othermal', 'Ġde', 'celer', 'ator', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġmaximum', 'Ġthrust', 'Ġvacuum', 'Ġkn', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġimpulse', 'Ġpropell', 'ant', 'Ġun', 'spe', 'ci', 'ï', '¬', 'ģ', 'ed', 'Ġhyper', 'g', 'olic', 'Ġbip', 'ro', 'pell', 'ant', 'Ġrocket', 'Ġlab', 'Ġinvestigating', 'us', 'ability', 'Ġdecided', 'Ġpursue', 'Ġprop', 'ulsive', 'Ġrecovery', 'Ġlike', 'Ġspace', 'x', 'Ġinstead', 'Ġuse', 'Ġatmosphere', 'Ġslow', 'Ġbooster', 'Ġknown', 'aer', 'othermal', 'Ġde', 'celer', 'ator', 'Ġtechnology', 'Ġexact', 'Ġmethods', 'Ġused', 'Ġproprietary', 'Ġmay', 'Ġinclude', 'Ġkeeping', 'Ġproper', 'Ġorientation', 'ent', 'ering', 'Ġatmosphere', 'Ġelectron', 'Ġinitially', 'Ġpayload', 'Ġcapacity', 'âĢĵ', 'âĢĵ', 'Ġmi', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġpursuit', 'us', 'ability', 'Ġrocket', 'Ġlab', 'Ġmade', 'Ġchanges', 'Ġelectron', 'Ġflight', 'Ġ("', "'s", 'Ġfunny', 'Ġlooking', 'Ġc', 'actus', 'make', 'Ġrain', '")', 'Ġinstruments', 'Ġfirst', 'Ġstage', 'Ġneeded', 'Ġgather', 'Ġdata', 'Ġhelp', 'Ġref', 'light', 'Ġprogram', 'Ġflight', 'Ġ("', 'look', 'Ġhands', '")', 'Ġbrut', 'us', 'Ġinstrument', 'Ġcollected', 'Ġdata', 'Ġfirst', 'Ġstage', 'Ġstudy', 'entry', 'Ġdesigned', 'Ġable', 'Ġsurvive', 'Ġsplash', 'Ġocean', 'Ġflight', 'Ġ("']</t>
         </is>
       </c>
       <c r="C353" t="n">
@@ -5027,7 +5027,7 @@
       </c>
       <c r="B354" t="inlineStr">
         <is>
-          <t>['j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġinitial', 'Ġmid', 'course', 'Ġcorrection', 'Ġmon', 'te', 'Ġcar', 'lo', 'Ġimplementation', 'Ġusing', 'Ġtask', 'Ġparallel', 'ism', 'Ġarchived', 'web', 'arch', 'iv', 'Ġmarch', 'Ġway', 'back', 'Ġmachine', 'Ġpropulsion', 'Ġsystem', 'Ġoverview', 'Ġj', 'Ġpet', 'ersen', 'Ġet', 'Ġal', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġk', 'imble', 'Ġr', 'andy', 'Ġde', 'cember', 'Ġwanted', 'Ġknow', 'Ġweb', 'b', "'s", 'Ġmid', 'course', 'Ġcorrections', '!"', 'Ġn', 'asa', 'Ġarchived', 'ctions', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'ard', 'Ġr', 'ick', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', ')"', 'Ġarchived', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġn', 'asa', 'gov', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'inf', 'rared', 'Ġatmospheric', 'Ġwindows', 'Ġcool', 'Ġcosmos', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġaug', 'ust', 'inf', 'rared', 'Ġastronomy', 'Ġoverview', 'Ġn', 'asa', 'Ġinfrared', 'Ġastronomy', 'Ġprocessing', 'Ġcenter', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'bb', 'Ġscience', 'Ġend', 'Ġdark', 'Ġages', 'Ġfirst', 'Ġlight', 'ion', 'ization', 'Ġv', 'ï', '¬', 'ģ', 'r', 'st', 'light', 'html', 'Ġn', 'asa', 'Ġarchived', 'Ġov', 'ï', '¬', 'ģ', 'r', 'st', 'light', 'html', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'ather', 'Ġjohn', 'Ġj', 'une', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'j', 'w', 'st', 'Ġscience', 'Ġsummary', 'sb', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġsavage', 'ald', 'Ġne', 'al', 'Ġn', 'ancy', 'Ġj', 'une', 'bb', 'Ġspacecraft', 'Ġscience', 'Ġoperations', 'Ġcenter', 'Ġcontract', 'Ġawarded', 'Ġn', 'asa']</t>
+          <t>['running', 'Ġfingers', '")', 'Ġblock', 'Ġupdate', 'Ġfirst', 'Ġstage', 'Ġelectron', 'Ġallow', 'Ġfirst', 'Ġguided', 'entry', 'Ġfirst', 'Ġstage', 'Ġbooster', 'Ġupdates', 'Ġincluded', 'Ġadditional', 'Ġhardware', 'Ġguidance', 'Ġnavigation', 'Ġonboard', 'Ġflight', 'Ġcomputers', 'band', 'Ġtele', 'metry', 'Ġgather', 'Ġlivestream', 'Ġdata', 'Ġgathered', 'entry', 'Ġfirst', 'Ġstage', 'Ġalso', 'Ġreaction', 'Ġcontrol', 'Ġsystem', 'Ġorient', 'Ġbooster', 'Ġstage', 'Ġseparation', 'Ġfirst', 'Ġstage', 'Ġusing', 'Ġnew', 'Ġhardware', 'Ġinstalled', 'Ġflipped', 'Â°', 'Ġprepare', 'entry', 'Ġthroughout', 'entry', 'Ġstage', 'Ġguided', 'Ġthough', 'Ġatmosphere', 'Ġright', 'Ġorientation', 'Ġangle', 'Ġattack', 'Ġbase', 'Ġheat', 'Ġshield', 'Ġprotect', 'Ġbooster', 'Ġdestruction', 'Ġusing', 'Ġonboard', 'Ġcomputers', 'Ġbooster', 'Ġsuccessfully', 'Ġsurvived', 'Ġguided', 'entry', 'Ġdespite', 'Ġde', 'celer', 'ation', 'Ġhardware', 'Ġonboard', 'Ġdestruct', 'ively', 'Ġspl', 'ashed', 'Ġocean', 'Ġmph', 'Ġplanned', 'entry', 'Ġsuccessful', 'Ġrocket', 'Ġlab', 'Ġplans', 'Ġrecover', 'Ġstage', 'Ġinstead', 'Ġwanted', 'Ġdemonstrate', 'Ġability', 'Ġsuccessfully', 'enter', 'Ġflight', 'Ġ("', 'birds', 'Ġfeather', '")', 'Ġdemonstrated', 'Ġsimilar', 'Ġsuccess', 'Ġatmospheric', 'entry', 'Ġtests', 'Ġsimilar', 'Ġflight', 'Ġexpected', 'Ġfollowing', 'Ġflight', 'Ġ("', 'birds', 'Ġfeather', '"),', 'Ġmid', 'f', 'eb', 'ruary', 'Ġlow', 'Ġaltitude', 'Ġtests', 'Ġdone', 'Ġtest', 'Ġparach', 'utes', 'Ġapr', 'il', 'Ġrocket', 'Ġlab', 'Ġshared', 'Ġsuccessful', 'Ġdemonstration', 'Ġmid', 'air', 'Ġretrieval', 'Ġdone', 'Ġmarch', 'Ġelectron', 'Ġtest', 'Ġarticle', 'Ġdropped', 'Ġhelicopter', 'Ġdeployed', 'Ġparach', 'utes', 'Ġhelicopter', 'Ġcarrying', 'Ġlong', 'bo', 'om', 'Ġsn', 'agged', 'Ġdro', 'gue', 'Ġline', 'Ġparachute', 'Ġft', 'Ġdemonstrating', 'Ġsuccessful', 'Ġretrieval', 'Ġfollowing', 'Ġcatch', 'Ġtest', 'Ġarticle', 'Ġbrought', 'Ġback', 'Ġland', 'Ġflight', 'Ġ("', 'return', 'Ġsender', '"),', 'Ġfirst', 'Ġrecover', 'Ġfirst', 'Ġstage', 'Ġbooster', 'Ġsplash', 'Ġpac', 'ific', 'Ġocean', 'Ġrocket', 'Ġalso', 'Ġloft', 'ed', 'Ġthirty', 'Ġpayload', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġincluding', 'Ġtitanium', 'Ġmass', 'Ġsimulator', 'Ġshape', 'Ġgarden', 'Ġgn', 'ome', 'gn', 'ome', 'Ġch', 'om', 'ps', 'ki', 'Ġvideo', 'Ġgame', 'Ġhalf', 'life', 'Ġaug', 'ust', 'Ġrocket', 'Ġlab', 'Ġannounced', 'Ġincreased', 'Ġpayload', 'Ġelectron', 'âĢĵ', 'âĢĵ', 'Ġpayload', 'Ġcapacity', 'Ġincrease']</t>
         </is>
       </c>
       <c r="C354" t="n">
@@ -5040,7 +5040,7 @@
       </c>
       <c r="B355" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'single', 'Ġboard', 'Ġcomputer', 'htm', 'Ġf', 'bo', 'Ġdaily', 'Ġissue', 'Ġf', 'bo', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'azing', 'Ġmini', 'atur', 'ized', 'side', 'car', 'Ġdrives', 'Ġweb', 'b', 'Ġtelescope', "'s", 'Ġsignal', 'Ġn', 'asa', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'utherland', 'Ġsc', 'ott', 'Ġj', 'une', 'bb', "'s", 'Ġprimary', 'Ġmirror', 'Ġhit', 'Ġmeteor', 'oid', 'Ġbuilt', 'Ġendure', 'Ġweather', 'Ġnetwork', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġhar', 'wood', 'iam', 'Ġj', 'une', 'bb', 'Ġtelescope', 'Ġstill', 'Ġperforming', 'Ġwell', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġimpact', 'Ġmirror', 'Ġsegment', 'Ġn', 'asa', 'Ġsays', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'ell', 'Ġel', 'izabeth', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġpicture', 'Ġshows', 'Ġnoticeable', 'Ġdamage', 'Ġmic', 'rom', 'et', 'eor', 'oid', 'Ġstrike', 'Ġcites', 'Ġn', 'asa', 'esa', 'cs', 'Ġjoint', 'Ġreport', 'Ġj', 'uly', 'Ġco', 'authors', 'Ġinstitutions', ']:', 'arian', 'e', 'Ġgoes', 'Ġhistory', 'Ġsuccessful', 'Ġlaunch', 'Ġweb', 'b', 'rian', 'esp', 'ace', 'press', 'Ġrelease', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġp', 'ino', 'Ġnat', 'asha', 'Ġf', 'iser', 'Ġal', 'ise', 'Ġbet', 'z', 'Ġl', 'aura', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġtelescope', 'Ġlaunches', 'Ġsee', 'Ġfirst', 'Ġgalaxies', 'Ġdistant', 'Ġworlds', 'Ġn', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunched', 'Ġest', 'aturday', 'dec', 'ri', 'ane', 'Ġrocket', 'Ġfrench', 'Ġgu', 'iana', 'Ġsouth', 'Ġameric', 'Ġes', 'istant', 'world', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġde', 'cember']</t>
+          <t>['Ġmainly', 'Ġdue', 'Ġbattery', 'Ġadvancements', 'Ġincreased', 'Ġpayload', 'Ġcapacity', 'Ġallows', 'Ġoffset', 'Ġmass', 'Ġadded', 'Ġrecovery', 'Ġtechnology', 'Ġaddition', 'Ġpayload', 'Ġmass', 'Ġcould', 'Ġflown', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'Ġothers', 'Ġelectron', 'Ġexpended', 'Ġrocket', 'Ġlab', 'Ġalso', 'Ġannounced', 'Ġexpanded', 'Ġfair', 'ings', 'Ġft', 'Ġdiameter', 'Ġlarger', 'Ġstandard', 'Ġft', 'Ġlong', 'Ġft', 'Ġdiameter', 'Ġfair', 'ings', 'Ġstri', 'x', 'Î±', 'Ġmission', 'Ġsyn', 'spective', 'Ġde', 'cember', 'Ġused', 'Ġextended', 'Ġfair', 'ing', 'Ġrocket', 'Ġlab', 'Ġdeveloped', 'fts', 'Ġlaunches', 'Ġnew', 'Ġzeal', 'Ġdec', 'Ġfirst', 'Ġlaunch', 'Ġus', 'Ġused', 'Ġn', 'asa', 'Ġautonomous', 'Ġflight', 'Ġtermination', 'Ġunit', 'Ġvehicle', 'Ġmod', 'ï', '¬', 'ģ', 'cation', 'Ġhistory', 'Ġfair', 'ings', 'Ġautonomous', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtermination', 'Ġsystems', 'Ġapplications', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Äģ', 'h', 'ia', 'Ġlaunch', 'Ġsite', 'Ġconstruction', 'Ġelectron', 'Ġdesigned', 'Ġlaunch', 'âĢĵ', 'âĢĵ', 'Ġpayload', 'Ġmi', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġsuitable', 'Ġcubes', 'ats', 'Ġsmall', 'Ġpayload', 'Ġoct', 'ober', 'Ġrocket', 'Ġlab', 'Ġopened', 'Ġfactory', 'Ġlarge', 'Ġenough', 'Ġproduce', 'Ġrockets', 'Ġper', 'Ġyear', 'Ġaccording', 'Ġcompany', 'Ġcustomers', 'Ġmay', 'Ġchoose', 'Ġencaps', 'ulate', 'Ġspacecraft', 'Ġpayload', 'Ġfair', 'ings', 'Ġprovided', 'Ġcompany', 'Ġeasily', 'Ġattached', 'Ġrocket', 'Ġshortly', 'Ġlaunch', 'Ġstarting', 'Ġprice', 'Ġdelivering', 'Ġpayload', 'Ġorbit', 'Ġmillion', 'Ġper', 'Ġlaunch', 'Ġoffers', 'Ġdedicated', 'Ġservice', 'Ġprice', 'Ġpoint', 'Ġmoon', 'Ġexpress', 'Ġcontracted', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġlunar', 'Ġland', 'ers', 'multiple', 'Ġlaunches', 'Ġcontracted', 'Ġplanned', 'Ġmoon', 'Ġexpress', 'Ġoperations', 'Ġelectron', 'Ġcompete', 'Ġgoogle', 'Ġlunar', 'Ġprize', 'Ġnone', 'Ġcontenders', 'Ġmet', 'Ġprize', 'Ġdeadline', 'Ġcompetition', 'Ġclosed', 'Ġwithout', 'Ġwinner', 'Ġsometime', 'Ġclosure', 'Ġmoon', 'Ġexpress', 'Ġelectron', 'Ġlaunches', 'Ġremained', 'Ġscheduled', 'Ġfe', 'b', 'ruary', 'Ġlaunches', 'Ġmoon', 'Ġexpress', 'Ġusing', 'Ġelectron', 'Ġcanceled', 'Ġapr', 'il', 'Ġrocket', 'Ġlab', 'Ġannounced', 'Ġelectron', 'Ġderivative', 'Ġvehicle', 'Ġnamed', 'Ġhaste', 'hyp', 'erson', 'ic', 'Ġaccelerator', 'Ġsub', 'orb', 'ital', 'Ġtest', 'Ġelectron', 'Ġcapable', 'Ġdelivering', 'Ġsub', 'orb', 'ital', 'Ġtrajectory', 'Ġcustomers', 'Ġinclude', 'Ġdyn', 'etics']</t>
         </is>
       </c>
       <c r="C355" t="n">
@@ -5053,7 +5053,7 @@
       </c>
       <c r="B356" t="inlineStr">
         <is>
-          <t>['Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġtrack', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmission', 'Ġtimeline', 'Ġspace', 'Ġexplored', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġde', 'cember', 'n', 'asa', "'s", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunches', 'Ġfrench', 'Ġgu', 'iana', 'Ġbillion', 'Ġsuccessor', 'Ġhub', 'ble', 'Ġtelescope', 'Ġcapture', 'Ġlight', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstars', 'Ġstudy', 'Ġdistant', 'Ġworlds', 'launch', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'live', 'Ġupdates', 'Ġweb', 'b', 'Ġtelescope', 'Ġlaunches', 'Ġlong', 'awaited', 'Ġjourney', 'Ġnew', 'ork', 'Ġtimes', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'bye', 'ennis', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġlaunches', 'Ġjourney', 'Ġsee', 'Ġdawn', 'Ġstar', 'light', 'Ġastronomers', 'Ġj', 'ub', 'ilant', 'Ġspacecraft', 'Ġmade', 'Ġlaunch', 'pad', 'Ġfollowing', 'Ġdecades', 'Ġdelays', 'Ġcost', 'Ġoverrun', 'Ġweb', 'b', 'Ġset', 'Ġoffer', 'Ġnew', 'Ġkey', 'hole', 'Ġearliest', 'Ġmoments', 'Ġuniverse', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'l', 'iss', 'aj', 'ous', 'Ġorbit', 'Ġox', 'ford', 'Ġreference', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'j', 'w', 'st', 'Ġorbit', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġuser', 'Ġdocumentation', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'f', 'requently', 'Ġasked', 'Ġquestions', 'Ġlong', 'Ġweb', 'b', 'Ġmission', 'Ġlast', '?"', 'Ġn', 'asa', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġk', 'Ġde', 'cember']</t>
+          <t>['Ġusing', 'Ġrocket', 'Ġlaunch', 'Ġtest', 'Ġvehicles', 'Ġmach', 'b', 'Ġprogram', 'Ġfirst', 'Ġlaunch', 'Ġdynam', 'Ġoccurred', 'Ġj', 'une', 'Ġlaunch', 'Ġcomplex', 'Ġmid', 'atlantic', 'Ġregional', 'Ġspac', 'eport', 'Ġrocket', 'Ġlaunched', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġcomplex', 'Äģ', 'h', 'ia', 'Ġpeninsula', 'Ġnew', 'Ġzeal', 'Ġlaunch', 'Ġpad', "'s", 'Ġremote', 'Ġsparse', 'ly', 'Ġpopulated', 'Ġlocation', 'Ġintended', 'Ġenable', 'Ġhigh', 'Ġfrequency', 'Ġlaunches', 'Ġrocket', 'Ġlaunch', 'Ġpad', 'Ġprivately', 'Ġfunded', 'Ġfirst', 'Ġtime', 'Ġparts', 'Ġorbital', 'Ġlaunch', 'Ġoperation', 'Ġentirely', 'Ġrun', 'Ġprivate', 'Ġsector', 'Ġprivate', 'Ġspace', 'flight', 'Ġcompanies', 'Ġlease', 'Ġlaunch', 'Ġfacilities', 'Ġgovernment', 'Ġagencies', 'Ġlaunch', 'Ġsub', 'orb', 'ital', 'Ġrockets', ').[', 'Ġoct', 'ober', 'Ġrocket', 'Ġlab', 'Ġselected', 'Ġvirgin', 'ia', 'Ġspace', "'s", 'Ġmid', 'atlantic', 'Ġregional', 'Ġspac', 'eport', 'ars', 'Ġwall', 'ops', 'Ġflight', 'Ġfacility', 'Ġvirgin', 'ia', 'Ġfuture', 'Ġsecondary', 'Ġlaunch', 'Ġsite', 'Ġunited', 'Ġstates', 'Ġcalled', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġcomplex', 'Ġlaunch', 'Ġcomplex', 'Ġexpected', 'Ġserve', 'Ġgovernment', 'Ġcustomers', 'Ġfirst', 'Ġlaunch', 'Ġhappened', 'Ġjan', 'uary', 'Ġelectron', 'Ġrocket', 'Ġsuccessfully', 'Ġorb', 'ited', 'Ġsatellites', 'Ġadditionally', 'Ġspace', 'Ġagency', 'Ġgiving', 'Ġhigh', 'lands', 'Ġislands', 'Ġenterprise', 'Ġopportunity', 'Ġdevelop', 'Ġelectron', 'Ġlaunch', 'Ġpad', 'h', 'Ã', '²', 'ine', 'Ġpeninsula', 'utherland', 'Ġsc', 'ot', 'land', 'Ġlocation', 'Ġwould', 'Ġnamed', 'utherland', 'Ġspac', 'eport', 'Ġelectron', 'Ġflown', 'Ġtimes', 'Ġsince', 'Ġmay', 'Ġtotal', 'Ġsuccesses', 'Ġfailures', 'Ġinitial', 'Ġtest', 'Ġflight', 'Ġcalled', "'s", 'Ġtest', '",', 'Ġfailed', 'Ġdue', 'Ġglitch', 'Ġcommunication', 'Ġequipment', 'Ġground', 'Ġfollow', 'Ġmissions', 'Ġcalled', 'still', 'Ġtesting', '",', "'s", 'Ġbusiness', 'Ġtime', 'Ġone', "'s", 'Ġpick', 'ering', '",', 'Ġdelivered', 'Ġmultiple', 'Ġsmall', 'Ġpayload', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġaug', 'ust', 'Ġmission', 'Ġnamed', 'look', 'Ġhands', 'Ġsuccessfully', 'Ġdelivered', 'Ġfour', 'Ġsatellites', 'Ġoct', 'ober', 'Ġmission', 'Ġnamed', 'Ġcrow', 'Ġflies', 'Ġsuccessfully', 'Ġlaunched', 'Äģ', 'h', 'ia', 'Ġdeploying', 'Ġsmall', 'Ġsatellite', 'Ġkick', 'Ġstage', 'Ġparking', 'Ġj', 'uly', 'Ġth', 'ir', 'teenth', 'Ġelectron', 'Ġrocket', 'Ġlaunch', 'Ġfailed', 'Ġcustomer', 'Ġpayload', 'Ġboard', 'Ġfirst', 'Ġfailure', 'Ġmaiden', 'Ġflight', 'Ġmay']</t>
         </is>
       </c>
       <c r="C356" t="n">
@@ -5066,7 +5066,7 @@
       </c>
       <c r="B357" t="inlineStr">
         <is>
-          <t>['n', 'asa', 'Ġsays', 'Ġweb', 'b', "'s", 'Ġexcess', 'Ġfuel', 'Ġlikely', 'Ġextend', 'Ġlifetime', 'Ġexpectations', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary', 'Ġhail', 'ri', 'ane', 'Ġrocket', 'Ġdoubled', 'Ġweb', 'b', 'Ġtelescope', "'s", 'Ġlifetime', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'os', 'Ġj', 'athan', 'Ġjan', 'uary', 'j', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġcompletes', 'Ġepic', 'Ġdeployment', 'Ġsequence', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġp', 'ult', 'ar', 'ova', 'ere', 'za', 'Ġde', 'cember', "'s", 'Ġtruly', 'Ġchrist', 'mas', "':", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'ulet', 'ide', 'Ġlaunch', 'Ġn', 'asa', 'joy', 'ed', 'Ġh', 'n', 'asa', 'action', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcamera', 'Ġcry', 'ote', 'chn', 'ic', 'Ġupper', 'Ġstage', 'Ġdec', 'Ġview', 'Ġnewly', 'Ġseparated', 'Ġj', 'w', 'st', 'Ġseen', 'Ġcry', 'ote', 'chn', 'ic', 'Ġupper', 'Ġstage', 'Ġarchived', 'Ġde', 'cember', 'Ġway', 'back', 'Ġmachine', 'Ġp', 'ult', 'ar', 'ova', 'ere', 'za', 'Ġde', 'cember', "'s", 'Ġtruly', 'Ġchrist', 'mas', "':", 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'ulet', 'ide', 'Ġlaunch', 'Ġn', 'asa', 'joy', 'ed', 'Ġh', 'n', 'asa', 'action', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdeployment', 'Ġsequence', 'nom', 'inal', 'Ġpp', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġwar', 'ren', 'Ġhay', 'gen', 'Ġde', 'cember', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġen', 'Ġroute', 'Ġdeployment', 'Ġsequence', 'Ġunderway', 'Ġce', 'way', 'Ġn', 'asa', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġac', 'hen', 'bach', 'Ġjo', 'el', 'Ġjan', 'uary', 'n', 'asa', 'Ġthrilled', 'Ġweb']</t>
+          <t>['Ġtwentieth', 'Ġlaunch', 'Ġalso', 'Ġfailed', 'still', 'Ġtesting', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsuccessful', 'Ġlaunch', 'Ġel', 'ana', 'Ġone', "'s", 'Ġpick', 'ering', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġn', 'asa', 'sponsored', 'Ġlaunch', 'Ġn', 'rol', 'birds', 'Ġfeather', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġn', 'ro', 'sponsored', 'Ġlaunch', 'Ġsub', 'orb', 'ital', 'Ġlaunches', 'Ġlaunch', 'Ġsites', 'Ġlaunch', 'Ġhistory', 'Ġnotable', 'Ġlaunches', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġnational', 'Ġreconnaissance', 'ï', '¬', 'ģ', 'ce', 'n', 'ro', 'Ġpayload', 'Ġsuccessfully', 'Ġlaunched', 'Ġaboard', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġrocket', 'Ġlaunch', 'Ġcomplex', 'return', 'Ġsender', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġocean', 'Ġrecovery', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', "'s", 'Ġlittle', 'Ġch', 'ile', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġspace', 'Ġtest', 'Ġprogram', 'Ġcap', 'stone', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġmoon', 'Ġhaw', 'keye', 'Ġcluster', 'v', 'irgin', 'ia', 'Ġlaunch', 'Ġlovers', '",', 'Ġelectron', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġlaunch', 'Ġcomplex', 'Ġmid', 'atlantic', 'Ġregional', 'Ġspac', 'eport', 'Ġorbital', 'Ġlaunch', 'Ġfailure', 'Ġorbital', 'Ġlaunch', 'Ġsuccess', 'Ġsub', 'orb', 'ital', 'Ġlaunch', 'Ġfailure', 'Ġsub', 'orb', 'ital', 'Ġlaunch', 'Ġsuccess', 'Ġscheduled', 'Ġorbital', 'Ġmissions', 'Ġmah', 'ia', 'Ġmah', 'ia', 'Ġmars', 'Ġlaunch', 'Ġstatistics', 'Ġlaunch', 'Ġoutcomes', 'Ġlaunch', 'Ġsites', 'Ġbooster', 'Ġtests', 'Ġrecover', 'ies', 'Ġrocket', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'urations', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġattempt', 'Ġatmospheric', 'Ġtest', 'Ġsuccess', 'Ġocean', 'Ġrecovery', 'Ġsuccess', 'Ġaerial', 'Ġcapture', 'Ġpartial', 'Ġfailure', 'Ġblock', 'Ġblock', 'Ġupgrade', 'th', 'rust', 'ers', 'Ġblock', 'Ġupgrade', 'par', 'ach', 'ute', 'Ġblock', 'Ġupgrade', 'par', 'af', 'oil', 'Ġhaste', 'sub', 'orb', 'ital', 'Ġsmall', 'lift', 'Ġlaunch', 'Ġvehicle', 'Ġcomparison', 'Ġorbital', 'Ġlauncher', 'Ġfamilies', 'Ġcomparison', 'Ġorbital', 'Ġlaunch', 'Ġsystems', 'Ġfal', 'con', 'Ġfire', 'ï', '¬', 'Ĥ', 'Ġalpha', 'Ġmi', 'ura', 'Ġvector', 'r', 'rocket', 'Ġlab', 'Ġcelebrates', 'Ġrich', 'Ġten', 'year', 'Ġhistory', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġj', 'une', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'Ġgets', 'Ġsecond', 'Ġlaunch', 'Ġsite', 'Ġgears', 'Ġrapid', 'Ġflight', 'Ġcad', 'ence', 'ar', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġoct', 'ober', 'Ġbots', 'ford']</t>
         </is>
       </c>
       <c r="C357" t="n">
@@ -5079,7 +5079,7 @@
       </c>
       <c r="B358" t="inlineStr">
         <is>
-          <t>['b', 'Ġspace', 'Ġtelescope', 'Ġdeploy', 'Ġsun', 'Ġshield', 'Ġev', 'ades', 'Ġmany', 'Ġpotential', 'single', 'point', 'Ġfailures', 'Ġwashing', 'ton', 'Ġpost', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'g', 'imb', 'aled', 'Ġantenna', 'Ġassembly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġk', 'Ġde', 'cember', 'Ġfirst', 'Ġmid', 'course', 'Ġcorrection', 'Ġburn', 'Ġn', 'asa', 'Ġblogs', 'Ġarchived', 'web', 'arch', 'iv', 'Ġn', 'burn', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġk', 'Ġde', 'cember', 'bb', "'s", 'Ġsecond', 'Ġmid', 'course', 'Ġcorrection', 'Ġburn', 'blogs', 'nas', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġfisher', 'Ġal', 'ise', 'Ġde', 'cember', 'bb', "'s", 'Ġaft', 'Ġmomentum', 'Ġflap', 'Ġdeployed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġlyn', 'ch', 'Ġpat', 'rick', 'Ġde', 'cember', 'Ġweb', 'b', "'s", 'Ġmid', 'bo', 'oms', 'Ġextended', 'Ġsun', 'shield', 'Ġtakes', 'Ġshape', 'Ġe', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġes', 'shape', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġjan', 'uary', 'Ġlyn', 'ch', 'Ġpat', 'rick', 'Ġde', 'cember', 'first', 'Ġtwo', 'Ġsun', 'shield', 'Ġmid', 'bo', 'oms', 'Ġdeploy', 'blogs', 'na', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'secondary', 'Ġmirror', 'Ġdeployment', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'med', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'first', 'Ġtwo', 'Ġprimary', 'Ġmirror', 'Ġwings', 'Ġunfolds', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary']</t>
+          <t>['Ġend', 'Ġmay', 'rocket', 'Ġlab', 'Ġelectron', 'Ġr', 'utherford', 'Ġp', 'eter', 'Ġbeck', 'Ġstarted', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġplace', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġinsider', 'Ġretrieved', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'Ġelectron', "'s", 'Ġtest', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġsuccessfully', 'Ġmakes', 'Ġspace', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġbeck', 'Ġp', 'eter', 'ye', 'Ġtook', 'Ġus', 'Ġget', 'Ġorbit', 'Ġbelieve', 'Ġmuch', '!"', 'Ġtwitter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ye', 'Ġtook', 'Ġus', 'Ġmillion', 'Ġget', 'Ġorbit', 'Ġbelieve', 'Ġmuch', '!"', 'Ġv', 'ance', 'Ġash', 'lee', 'Ġfe', 'b', 'ruary', 'Ġsmall', 'Ġrocket', 'Ġmaker', 'Ġrunning', 'Ġdifferent', 'Ġkind', 'Ġspace', 'Ġrace', 'bl', 'Ġbloom', 'berg', 'Ġretrieved', 'Ġoct', 'ober', 'aven', 'port', 'Ġchrist', 'ian', 'Ġoct', 'ober', 'v', 'irgin', 'ia', 'Ġrocket', 'Ġlaunch', 'Ġsite', "'s", 'Ġgrow', 'Ġsuccessful', 'Ġstartup', 'Ġsince', 'Ġspace', 'x', 'Ġwashing', 'ton', 'Ġpost', 'Ġretrieved', 'Ġoct', 'ober', 'elect', 'ron', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġelectron', 'Ġdata', 'Ġsheet', 'Ġspace', 'Ġlaunch', 'Ġreport', 'mber', 'Ġretrieved', 'mber', 'Ġb', 'ennett', 'Ġj', 'ay', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġreveals', 'Ġsecret', 'Ġengine', 'kick', 'Ġstage', 'Ġelectron', 'Ġrocket', 'http', 'Ġpopular', 'Ġmechanics', 'Ġretrieved', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġincreases', 'Ġelectron', 'Ġpayload', 'Ġcapacity', 'Ġenabling', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'us', 'ability', 'roc', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġmay', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'uly', 'sc', 'ot', 'land', 'Ġsite', 'Ġselected', 'Ġlaunch', 'Ġbase', 'Ġlock', 'heed', 'Ġmart', 'Ġorb', 'ex', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġsee', 'Ġalso', 'Ġreferences', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġether', 'ington', 'arrell']</t>
         </is>
       </c>
       <c r="C358" t="n">
@@ -5092,7 +5092,7 @@
       </c>
       <c r="B359" t="inlineStr">
         <is>
-          <t>['Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'primary', 'Ġmirror', 'Ġwings', 'Ġdeployed', 'Ġmajor', 'Ġdeployments', 'Ġcomplete', 'plete', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġjan', 'uary', 'rem', 'ark', 'ably', 'Ġn', 'asa', 'Ġcompleted', 'Ġdeployment', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġcans', 'ci', 'enc', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'space', 'Ġtelescope', "'s", 'gold', 'en', 'Ġeye', 'Ġopens', 'Ġlast', 'Ġmajor', 'Ġhurdle', 'Ġphys', 'org', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġfisher', 'Ġal', 'ise', 'Ġjan', 'uary', 'bb', "'s", 'Ġjourney', 'Ġnearly', 'Ġcomplete', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'n', 'asa', 'Ġblogs', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġjan', 'uary', 'Ġmillion', 'mile', 'Ġjourney', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġreaches', 'Ġdestination', 'Ġtelescope', "'s", 'Ġsafe', 'Ġarrival', 'Ġrelief', 'Ġscientists', 'Ġplan', 'Ġspend', 'Ġnext', 'Ġyears', 'Ġusing', 'Ġstudy', 'Ġancient', 'Ġgalaxies', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'orb', 'ital', 'Ġinsertion', 'Ġburn', 'Ġsuccess', 'Ġweb', 'b', 'Ġarrives', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'bl', 'Ġblogs', 'n', 'asa', 'gov', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġruns', 'Ġtechnical', 'Ġissue', 'Ġind', 'ian', 'Ġexpress', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'bb', 'Ġmirror', 'Ġsegment', 'Ġdeployments', 'Ġcomplete', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'blogs', 'na', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'bb', 'Ġbegins', 'Ġmonths', 'long', 'Ġmirror', 'Ġalignment', 'Ġj', 'ames', 'Ġweb']</t>
+          <t>['Ġmay', 'rocket', 'Ġlab', 'Ġtests', 'Ġnew', 'Ġhyper', 'cur', 'ie', 'Ġengine', 'Ġpower', 'Ġdeep', 'Ġspace', 'Ġdelivery', 'Ġvehicle', 'Ġl', 'ivery', 'veh', 'icle', 'Ġtech', 'cr', 'unch', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'rocket', 'Ġlab', 'Ġp', 'eter', 'Ġbeck', 'Ġsmall', 'sat', 'Ġkeynote', 'Ġyoutube', 'Ġrocket', 'Ġlab', 'rocket', 'Ġlab', 'Ġcelebrates', 'Ġrich', 'Ġten', 'year', 'Ġhistory', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', 'view', 'Ġdetails', 'Ġretrieved', 'mber', 'elect', 'ron', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġapr', 'il', 'printed', 'Ġbattery', 'powered', 'Ġrocket', 'Ġengine', 'Ġpopular', 'Ġscience', 'Ġretrieved', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġmakes', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġbooster', 'Ġrecovery', 'Ġsuccessful', 'Ġlaunch', 'Ġtech', 'cr', 'unch', 'mber', 'Ġretrieved', 'mber', 'new', 'Ġzeal', 'Ġspace', 'Ġlaunch', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġprivate', 'Ġsite', 'Ġnews', 'Ġmay', 'Ġretrieved', 'Ġmay', 'new', 'Ġzeal', 'Ġtest', 'Ġrocket', 'Ġmakes', 'Ġspace', 'Ġorbit', 'Ġindependent', 'ie', 'Ġassociated', 'Ġpress', 'Ġmay', 'Ġretrieved', 'Ġmay', 'rocket', 'Ġlab', 'Ġcompletes', 'Ġpost', 'flight', 'Ġanalysis', 'Ġelectron', 'Ġtest', 'Ġrocket', 'Ġlab', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġr', 'yan', 'Ġh', 'olly', 'Ġjan', 'uary', 'blast', 'Ġrocket', 'Ġlab', 'Ġsuccessfully', 'Ġreaches', 'Ġorbit', 'Ġnew', 'Ġzeal', 'Ġherald', 'Ġretrieved', 'Ġjan', 'uary', 'Ġrocket', 'Ġlab', 'Ġus', 'mber', "'s", 'Ġbusiness', 'Ġtime', 'Ġlaunch', 'Ġretrieved', 'mber', 'Ġsm', 'yth', 'Ġjam', 'ie', 'Ġjan', 'uary', 'private', 'Ġgroup', 'world', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcheap', 'Ġrocket', 'Ġlaunch', 'Ġfinancial', 'Ġtimes', 'Ġretrieved', 'Ġjan', 'uary', 'launch', 'Ġweek', 'Ġarrives', 'Ġrocket', 'Ġlab', "'s", 'Ġelectron', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġbr', 'Ã¼', 'g', 'ge', 'bert', 'elect', 'ron', 'Ġb', 'de', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġbr']</t>
         </is>
       </c>
       <c r="C359" t="n">
@@ -5105,7 +5105,7 @@
       </c>
       <c r="B360" t="inlineStr">
         <is>
-          <t>['b', 'Ġspace', 'Ġtelescope', 'blogs', 'n', 'Ġjan', 'uary', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'phot', 'ons', 'Ġincoming', 'Ġweb', 'b', 'Ġteam', 'Ġbegins', 'Ġalign', 'ing', 'Ġtelescope', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'pe', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'follow', 'ing', 'Ġweb', 'b', "'s", 'Ġarrival', 'Ġtelescope', 'Ġcommission', 'ing', 'Ġset', 'Ġbegin', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġjan', 'uary', 'Ġarchived', 'set', 'begin', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsim', 'bad', 'Ġcentre', 'Ġde', 'n', 'Ã©', 'es', 'Ġastron', 'om', 'iques', 'Ġde', 'Ġstr', 'bourg', 'Ġretrieved', 'Ġjan', 'uary', 'v', 'ors', 'ky', 'Ġge', 'orge', 'Ġfe', 'b', 'ruary', 'bb', 'Ġspace', 'Ġtelescope', 'Ġsuccessfully', 'Ġsees', 'Ġfirst', 'Ġgl', 'immer', 'Ġlight', 'Ġgo', 'Ġhistory', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstar', 'Ġspotted', 'Ġbillion', 'Ġspace', 'Ġtelescope', 'Ġg', 'iz', 'mod', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhood', 'Ġab', 'Ġle', 'e', 'Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdetected', 'Ġfirst', 'Ġsignal', "'re", 'Ġwatching', 'Ġfuture', 'Ġunfold', 'Ġreal', 'Ġtime', 'Ġfut', 'ur', 'ism', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'phot', 'ons', 'Ġreceived', 'Ġweb', 'b', 'Ġsees', 'Ġfirst', 'Ġstar', 'Ġtimes', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'http', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġn', 'irc', 'Ġinstrument', "'s", 'Ġdetectors', 'Ġsaw', 'st', 'Ġphotons', 'Ġstar', 'light', 'nas', 'aw', 'eb', 'b', 'Ġyet', 'Ġready', 'Ġscience', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmany', 'Ġsteps', 'Ġcapture', 'Ġimages', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġunfocused', 'Ġused', 'Ġslowly', 'Ġï', '¬', 'ģ', 'ne', 'une', 'Ġoptics', 'Ġtwitter', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved']</t>
+          <t>['Ã¼', 'g', 'ge', 'bert', 'elect', 'ron', 'Ġpropulsion', 'Ġb', 'de', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'prop', 'ulsion', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġlaunch', 'Ġalso', 'Ġtested', 'Ġnew', 'Ġkick', 'Ġstage', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġcircular', 'izes', 'Ġorbit', 'Ġnew', 'Ġelectron', 'Ġkick', 'Ġstage', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġjan', 'uary', 'Ġretrieved', 'Ġmay', 'rocket', 'Ġlab', 'Ġincreases', 'Ġelectron', 'Ġpayload', 'Ġcapacity', 'Ġenabling', 'Ġinter', 'plan', 'etary', 'Ġmissions', 'us', 'ability', 'roc', 'Ġusability', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'ep', 'Ġrocket', 'Ġlab', 'Ġplan', 'Ġdeliver', 'Ġsatellites', 'Ġmoon', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġf', 'oust', 'Ġje', 'ff', 'mber', 'rocket', 'Ġlab', 'Ġintroduces', 'Ġrobotic', 'Ġmanufacturing', 'Ġsystem', 'Ġincrease', 'Ġelectron', 'Ġproduction', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġel', 'izabeth', 'ell', 'mber', 'space', 'x', 'Ġcompetitor', "'s", 'ros', 'ie', 'Ġrobot', 'Ġpump', 'Ġrocket', 'Ġparts', 'Ġevery', 'Ġhours', 'Ġforb', 'es', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġannounces', 'us', 'ability', 'Ġplans', 'Ġelectron', 'Ġrocket', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġj', 'uly', 'Ġbeck', 'Ġp', 'eter', 'Ġaug', 'ust', "'s", 'Ġrocket', 'Ġlab', 'Ġchanged', 'Ġmind', 'Ġreusable', 'Ġlaunch', 'inter', 'view', 'Ġinterviewed', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġattempt', 'Ġreuse', 'Ġelectron', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'uly', 'Ġsheet', 'z', 'ichael', 'Ġde', 'cember', 'rocket', 'Ġlab', 'pun', 'ched', 'Ġwall', '",', 'Ġce', 'Ġsays', 'Ġpassing', 'Ġkey', 'Ġmilestone', 'Ġeffort', 'Ġreuse', 'Ġrockets', 'Ġace', 'x', 'html', 'Ġretrieved', 'Ġj', 'uly', 'kinson']</t>
         </is>
       </c>
       <c r="C360" t="n">
@@ -5118,7 +5118,7 @@
       </c>
       <c r="B361" t="inlineStr">
         <is>
-          <t>['Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'bb', 'Ġteam', 'Ġbrings', 'Ġdots', 'Ġstar', 'light', 'Ġhex', 'agonal', 'Ġformation', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'bb', 'Ġmirror', 'Ġalignment', 'Ġcontinues', 'Ġsuccessfully', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'blogs', 'n', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġaug', 'ust', 'Ġfind', 'Ġfirst', 'Ġgalaxies', 'Ġweb', 'b', 'Ġpays', 'Ġattention', 'Ġdetail', 'Ġtheory', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġblogs', 'n', 'asa', 'gov', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġaug', 'ust', 'mass', 'Ġj', 'Ġfacts', 'Ġstar', 'Ġuniverse', 'Ġguide', 'Ġguide', 'Ġspace', 'Ġplanets', 'Ġrest', 'Ġuniverse', 'Ġuniverse', 'guide', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġk', 'l', 'ug', 'er', 'Ġje', 'ff', 'rey', 'Ġmarch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġtook', 'Ġbest', 'Ġpicture', 'Ġyet', 'ht', 'Ġtime', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'kinson', 'Ġn', 'ancy', 'Ġmay', 'Ġfinally', 'Ġcompare', 'Ġweb', 'b', 'Ġinfrared', 'Ġobserv', 'atories', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġ', 'erv', 'atories', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'bb', 'Ġfull', 'Ġfocus', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'bb', "'s", 'Ġfine', 'Ġguidance', 'Ġsensor', 'Ġprovides', 'Ġpreview', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'blog', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'c', 'alls', 'Ġproposals', 'Ġpolicy', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'select', 'ions', 'Ġmade', 'Ġj', 'w', 'st', 'Ġdirector', "'s", 'Ġdiscretionary']</t>
+          <t>['Ġ', 'ian', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġelectron', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġcompany', 'Ġpreviews', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġstage', 'Ġrecovery', 'http', 'Ġretrieved', 'Ġj', 'uly', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġaug', 'ust', 'small', 'Ġsatellite', 'Ġlauncher', 'Ġrocket', 'Ġlab', 'Ġunve', 'ils', 'Ġplans', 'Ġrecover', 'Ġrockets', 'Ġmid', 'air', 'Ġhelicopters', 'Ġverge', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġattempt', 'Ġfirst', 'Ġlaunch', 'printed', 'Ġengine', "'s", 'Ġalready', 'Ġflown', 'Ġspace', 'g', 'iz', 'mod', 'co', 'Ġg', 'iz', 'mod', 'Ġsheet', 'z', 'ichael', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġunve', 'ils', 'Ġplan', 'Ġland', 'Ġsmall', 'Ġrockets', 'Ġcatching', 'Ġhelicopter', 'Ġretrieved', 'Ġj', 'uly', 'Ġco', 'ï', '¬', 'ģ', 'e', 'ld', 'Ġcall', 'Ġse', 'pt', 'ember', 'rocket', 'Ġlab', 'Ġopens', 'Ġprivate', 'Ġorbital', 'Ġlaunch', 'Ġsite', 'Ġnew', 'Ġzeal', 'sp', 'Ġspace', 'Ġretrieved', 'Ġjan', 'uary', 'next', 'Ġgeneration', 'Ġelectron', 'Ġbooster', 'Ġpad', 'Ġrocket', 'Ġlab', "'s", 'th', 'Ġmission', 'Ġrocket', 'Ġlab', 'Ġus', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'elect', 'ron', 'Ġlaunches', 'Ġsmall', 'ats', 'Ġtest', 'Ġrocket', 'us', 'ability', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'uly', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'rocket', 'Ġlab', "'s", 'th', 'Ġlaunch', 'Ġtests', 'Ġbooster', 'Ġrecovery', 'Ġtechnology', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'amp', 'son', 'Ġben', 'Ġde', 'cember', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtests', 'entry', 'Ġrocket', 'Ġbooster', 'ero', 'Ġaerospace', 'Ġtesting', 'Ġinternational', 'Ġretrieved', 'Ġde', 'cember', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġlaunches', 'Ġn', 'ro', 'Ġsatellite', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġdeploy', 'Ġn', 'ro', 'Ġsatellite', 'th', 'Ġelectron', 'Ġmission', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'Ġf', 'letcher', 'Ġcol', 'Ġj', 'une', 'rocket', 'Ġlab', 'Ġlaunches', 'th', 'Ġelectron']</t>
         </is>
       </c>
       <c r="C361" t="n">
@@ -5131,7 +5131,7 @@
       </c>
       <c r="B362" t="inlineStr">
         <is>
-          <t>['Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'director', "'s", 'Ġdiscretionary', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprograms', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'web', 'arch', 'iv', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġde', 'cember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġad', 'ams', 'Ġet', 'Ġal', 'jan', 'uary', 'iscovery', 'Ġproperties', 'Ġultra', 'high', 'Ġred', 'shift', 'Ġgalaxies', 'Ġj', 'w', 'st', 'Ġer', 'Ġsm', 'acs', 'Ġ07', 'Ġfield', 'Ġmonthly', 'Ġnotices', 'Ġroyal', 'Ġastronomical', 'Ġsociety', '):', 'âĢĵ', 'Ġar', 'x', 'iv', 'doi', 'org', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġha', 'oj', 'ing', 'Ġet', 'Ġal', 'jan', 'uary', 'first', 'Ġbatch', 'âĢĵ', 'Ġcandidate', 'Ġobjects', 'Ġrevealed', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġearly', 'Ġrelease', 'Ġobservations', 'Ġsm', 'acs', 'Ġ07', 'doi', 'org', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġletters', 'Ġar', 'x', 'iv', 'ui', 'ads', 'rad', 'ative', 'Ġfeedback', 'Ġmassive', 'Ġstars', 'Ġtraced', 'Ġmult', 'iband', 'Ġimaging', 'Ġspect', 'rosc', 'opic', 'Ġmosaic', 'Ġarchived', 'ber', 'ne', 'pdf', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'ice', 'age', 'Ġchemical', 'Ġevolution', 'Ġ', 'ices', 'Ġstar', 'Ġformation', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġlooking', 'Ġglass', 'Ġj', 'w', 'st', 'Ġexploration', 'Ġgalaxy', 'Ġformation', 'Ġevolution', 'Ġcosmic', 'Ġdawn', 'Ġpresent', 'Ġday', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġj', 'w', 'st', 'Ġstudy', 'Ġstar', 'burst', 'agn', 'Ġconnection', 'Ġmerging', 'Ġl', 'ir', 'gs', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġresolved', 'Ġstellar', 'Ġpopulations', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġarchived', 'Ġoriginal']</t>
+          <t>['Ġcontinues', 'Ġwork', 'Ġfuture', 'Ġplans', 'nas', 'Ġretrieved', 'Ġj', 'uly', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġapr', 'il', 'rocket', 'Ġlab', 'Ġreports', 'Ġrecovery', 'Ġtest', 'Ġsuccess', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġelectron', 'Ġtest', 'Ġbooster', 'Ġrecovery', 'Ġspac', 'en', 'ews', 'mber', 'Ġretrieved', 'mber', 'rocket', 'Ġlab', 'Ġattempt', 'Ġelectron', 'Ġstage', 'Ġrecovery', 'Ġnext', 'Ġlaunch', 'Ġspac', 'en', 'ews', 'mber', 'Ġretrieved', 'mber', 'Ġr', 'yan', 'Ġjack', 'son', 'mber', 'half', 'life', 'Ġgarden', 'Ġgn', 'ome', 'Ġreaches', 'Ġspace', 'Ġaboard', 'Ġrocket', 'Ġlab', "'s", 'Ġelectron', 'http', 'Ġretrieved', 'mber', 'rocket', 'Ġlab', 'Ġlaunch', 'Ġpayload', 'Ġusers', 'Ġguide', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġaug', 'ust', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġready', 'Ġattempt', 'Ġelectron', 'Ġbooster', 'Ġrecovery', 'Ġspac', 'en', 'ews', 'cal', 'end', 'ario', 'Ġde', 'Ġlan', 'z', 'ient', 'os', 'Ġcosmos', 'Ġsp', 'anish', 'oci', 'aci', 'Ã³n', 'Ġaer', 'oes', 'p', 'acial', 'Ġcosmos', 'Ġjan', 'uary', 'Ġp', 'Ġretrieved', 'Ġde', 'cember', 'Ġowl', "'s", 'Ġnight', 'Ġbegins', 'Ġ[...]', 'Ġlan', 'z', 'ient', 'Ġdel', 'Ġsat', 'Ã©', 'lite', 'Ġstri', 'x', 'Î±', 'Ġsu', 'ama', 'Ã±o', 'Ġoblig', 'Ã³', 'Ġutil', 'iz', 'ar', 'Ġun', 'Ġco', 'ï', '¬', 'ģ', 'Ġextend', 'ida', 'rocket', 'Ġlab', 'Ġdeb', 'uts', 'Ġfully', 'Ġautonomous', 'Ġflight', 'Ġtermination', 'Ġsystem', 'Ġspace', 'ref', 'Ġde', 'cember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġn', 'asa', 'Ġsafety', 'Ġsystem', 'Ġenables', 'Ġrocket', 'Ġlab', 'Ġlaunch', 'Ġwall', 'ops', 'Ġjan', 'odd', 'Ġtim', 'Ġoct', 'ober', 'exclusive', 'Ġinside', 'Ġlook', 'Ġrocket', 'Ġlab', "'s", 'Ġsecret', 'Ġnew', 'Ġmega', 'Ġfactory', '!"', 'Ġeveryday', 'Ġastronaut', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'pay', 'load', 'Ġuser', "'s", 'Ġguide', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'roc', 'ke', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġjan']</t>
         </is>
       </c>
       <c r="C362" t="n">
@@ -5144,7 +5144,7 @@
       </c>
       <c r="B363" t="inlineStr">
         <is>
-          <t>['Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġdomin', 'ika', 'Ġw', 'yle', 'z', 'al', 'ek', 'Ġimaging', 'Ġspect', 'rosc', 'opy', 'Ġqu', 'asar', 'Ġhosts', 'Ġj', 'w', 'st', 'Ġanalyzed', 'Ġpowerful', 'Ġnew', 'Ġps', 'f', 'Ġdecom', 'position', 'Ġspectral', 'Ġanalysis', 'Ġpackage', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġcosmic', 'Ġevolution', 'Ġearly', 'Ġrelease', 'Ġscience', 'ce', 'ers', 'Ġsurvey', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'establish', 'ing', 'Ġextreme', 'Ġdynamic', 'Ġrange', 'Ġj', 'w', 'st', 'Ġdecoding', 'Ġsmoke', 'Ġsignals', 'Ġglare', 'Ġwolf', 'ray', 'et', 'Ġbinary', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'tem', 'plates', 'Ġtargeting', 'Ġextremely', 'Ġmagn', 'ï', '¬', 'ģ', 'ed', 'Ġpan', 'chrom', 'atic', 'Ġlens', 'ed', 'Ġarcs', 'Ġextended', 'Ġstar', 'Ġformation', 'Ġarchived', 'Ġrs', 'rig', 'pdf', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'nuclear', 'Ġdynamics', 'Ġnearby', 'Ġse', 'f', 'ert', 'Ġn', 'ir', 'spec', 'Ġintegral', 'Ġfield', 'Ġspect', 'rosc', 'opy', 'st', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'Ġtrans', 'iting', 'Ġex', 'oplan', 'et', 'Ġcommunity', 'Ġearly', 'Ġrelease', 'Ġscience', 'Ġprogram', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'ers', 'Ġobservations', 'Ġj', 'ov', 'ian', 'Ġsystem', 'Ġdemonstration', 'Ġj', 'w', 'st', "'s", 'Ġcapabilities', 'Ġsolar', 'Ġsystem', 'Ġscience', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'high', 'Ġcontrast', 'Ġimaging', 'Ġex', 'oplan', 'ets', 'Ġex', 'oplan', 'etary', 'Ġsystems', 'Ġj', 'w', 'st', 'Ġdf', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'j', 'w', 'st', 'Ġcycle', 'Ġgeneral', 'Ġobserver', 'Ġsubmission', 'Ġstatistics', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'sts', 'ci', 'Ġannounces', 'Ġj', 'w', 'st', 'Ġcycle', 'Ġgeneral', 'Ġobserver', 'Ġprogram', 'Ġarchived', 'w', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġmarch', 'sts', 'ci', 'Ġannounces', 'Ġj', 'w', 'st', 'Ġcycle', 'Ġgeneral', 'Ġobserver', 'Ġprogram', 'Ġspace', 'Ġtelescope', 'Ġscience', 'Ġinstitute', 'Ġretrieved', 'Ġmay', 'ob', 'serving', 'Ġschedules']</t>
+          <t>['uary', 'space', 'ï', '¬', 'Ĥ', 'ight', 'Ġstartup', 'Ġrocket', 'Ġlab', 'Ġsends', 'Ġelectron', 'Ġrocket', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtime', 'h', 'Ġverge', 'Ġretrieved', 'Ġjan', 'uary', 'Ġwall', 'ike', 'Ġjan', 'uary', 'ex', 'pri', 'ze', 'Ġgoogle', "'s", 'Ġmillion', 'Ġmoon', 'Ġrace', 'Ġends', 'Ġwinner', 'sp', 'Ġspace', 'Ġretrieved', 'Ġjan', 'uary', 'Ġmoon', 'Ġexpress', 'mo', 'one', 'x', 'Ġfe', 'b', 'ruary', 'Ġupcoming', 'Ġlaunch', 'Ġrocket', 'lab', 'Ġcontracted', 'Ġrocket', 'lab', 'Ġback', 'Ġattempt', 'Ġcurrently', 'Ġfocused', 'Ġefforts', 'Ġsupporting', 'Ġn', 'asa', 'Ġcommercial', 'Ġlunar', 'Ġpayload', 'Ġservices', 'cl', 'ps', 'Ġcontract', 'weet', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'rocket', 'Ġlab', 'Ġintroduces', 'Ġsub', 'orb', 'ital', 'Ġtest', 'bed', 'Ġrocket', 'Ġselected', 'Ġhyp', 'erson', 'ic', 'Ġtest', 'Ġflights', 'fl', 'ights', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'es', 'nic', 'Ġtre', 'vor', 'Ġj', 'une', 'launch', 'Ġroundup', 'Ġrocket', 'Ġlab', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġhaste', 'Ġmission', 'Ġspace', 'x', 'Ġlaunch', 'Ġsat', 'ria', 'Ġretrieved', 'Ġj', 'une', 'rocket', 'Ġlab', 'Ġselects', 'Ġwall', 'ops', 'Ġu', 'Ġlaunch', 'Ġsite', 'u', 'launch', 'site', 'Ġspac', 'en', 'ews', 'Ġoct', 'ober', 'Ġretrieved', 'Ġjan', 'uary', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġj', 'une', 'rocket', 'Ġlab', 'Ġï', '¬', 'Ĥ', 'ies', 'Ġnew', 'Ġzeal', 'Ġwork', 'Ġprogresses', 'Ġvirgin', 'ia', 'Ġlaunch', 'Ġpad', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'uly', 'Ġhar', 'wood', 'iam', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġsatellites', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġmission', 'Ġu', 'Ġsoil', 'Ġnews', 'Ġretrieved', 'Ġjan', 'uary', 'os', 'Ġj', 'athan', 'Ġj', 'uly', 'sc', 'ot', 'land', 'Ġhost', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġspac', 'eport', 'Ġent', 'Ġnews', 'Ġretrieved', 'Ġj', 'uly', 'utherland', 'Ġspac', 'eport', 'Ġsc', 'ot', 'land', 'Ġsp', 'acet', 'v', 'Ġretrieved', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġcompletes', 'Ġpost', 'flight', 'Ġanalysis', 'ly', 'sis', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġaug']</t>
         </is>
       </c>
       <c r="C363" t="n">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>['ules', 'Ġst', 'sci', 'edu', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġc', 'es', 'ari', 'Ġth', 'add', 'eus', 'Ġcenter', 'Ġn', 'asa', 'âĢ', 'Ļ', 'Ġgodd', 'ard', 'Ġspace', 'Ġflight', 'Ġj', 'uly', 'Ġlast', 'Ġn', 'asa', "'s", 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġfully', 'Ġready', 'Ġscience', 'Ġsc', 'itech', 'daily', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġbart', 'els', 'ghan', 'Ġde', 'cember', 'n', 'asa', 'Ġmay', 'Ġunlock', 'Ġfuture', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġdata', 'Ġspace', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġch', 'ow', 'Ġden', 'ise', 'Ġj', 'ach', 'uan', 'Ġj', 'uly', 'photos', 'Ġpictures', 'Ġweb', 'b', 'Ġtelescope', 'Ġcompare', 'Ġhub', 'ble', "'s", 'Ġn', 'asa', "'s", 'Ġbillion', 'Ġtelescope', 'Ġpeers', 'Ġdeeper', 'Ġspace', 'Ġever', 'Ġrevealing', 'Ġpreviously', 'Ġundet', 'ect', 'able', 'Ġdetails', 'Ġcosmos', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġdel', 'iso', 'red', 'ith', 'Ġlong', 'red', 'ith', 'Ġrot', 'hen', 'berg', 'Ġnic', 'olas', 'Ġj', 'uly', 'hub', 'ble', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġimages', 'Ġsee', 'Ġdifference', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġgarner', 'Ġrob', 'Ġj', 'uly', 'n', 'asa', "'s", 'Ġweb', 'b', 'Ġdelivers', 'Ġdeepest', 'Ġinfrared', 'Ġimage', 'Ġuniverse', 'Ġyet', 'http', 'Ġn', 'iverse', 'yet', 'Ġn', 'asa', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'bye', 'ennis', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġtank', 'ers', 'ley', 'Ġj', 'uly', 'b', 'iden', 'Ġn', 'asa', 'Ġshare', 'Ġfirst', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġimage', 'Ġwhite', 'Ġhouse', 'onday', 'Ġhumanity', 'Ġgot', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġglimpse', 'Ġobserv', 'atory', 'Ġspace', 'Ġseeing', 'Ġcluster', 'Ġearly', 'Ġgalaxies', 'ny', 'time', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġpac', 'ucci', 'Ġfab', 'io', 'Ġj', 'uly', 'Ġtaking', 'Ġpictures', 'nothing', 'Ġchanged', 'Ġastronomy']</t>
+          <t>['ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġaug', 'ust', 'tele', 'metry', 'Ġglitch', 'Ġkept', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġelectron', 'Ġrocket', 'Ġreaching', 'Ġorbit', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'ell', 'Ġel', 'izabeth', 'Ġaug', 'ust', 'rocket', 'Ġlab', 'Ġelectron', 'Ġbooster', 'Ġlaunches', 'Ġsatellites', 'Ġorbit', 'sp', 'ac', 'Ġspace', 'Ġretrieved', 'Ġaug', 'ust', 'Ġether', 'ington', 'arrell', 'Ġoct', 'ober', 'rocket', 'Ġlab', 'Ġsuccessfully', 'Ġlaunches', 'Ġï', '¬', 'ģ', 'f', 'th', 'Ġelectron', 'Ġrocket', 'Ġyear', 'tech', 'Ġtech', 'cr', 'unch', 'Ġretrieved', 'mber', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġj', 'uly', 'rocket', 'Ġlab', 'Ġelectron', 'Ġlaunch', 'Ġfails', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġj', 'uly', 'rocket', 'Ġlab', "'s", 'th', 'Ġelectron', 'Ġlaunch', 'Ġends', 'Ġfailure', 'Ġloss', 'Ġpayload', 'Ġtech', 'cr', 'unch', 'Ġmay', 'Ġretrieved', 'Ġmay', '09', 'Ġrocket', 'Ġlab', 'Ġelectron', 'Ġwik', 'ipedia', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġdelivers', 'Ġnan', 'os', 'atell', 'ites', 'Ġorbit', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsuccessful', 'Ġtest', 'Ġlaunch', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġde', 'cember', 'n', 'asa', 'Ġrocket', 'Ġlab', 'Ġpartner', 'Ġsuccessful', 'Ġsatellite', 'Ġlaunch', 'Ġnew', 'Ġzeal', 'h', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġj', 'une', 'Ġwall', 'ike', 'Ġjan', 'uary', 'rocket', 'Ġlab', 'Ġlaunches', 'Ġsatellite', 'Ġu', 'Ġsp', 'ys', 'Ġagency', 'Ġguides', 'Ġbooster', 'Ġback', 'Ġearth', 'Ġspace', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'return', 'Ġsender', 'Ġrocket', 'Ġlab', 'Ġus', 'Ġretrieved', 'Ġde', 'cember', 'Ġelectron', 'Ġwebsite', 'Ġrocket', 'lab', 'usa', 'Ġelectron', 'Ġpayload', 'Ġuser', "'s", 'Ġguide', 'Ġrocket', 'lab', 'usa', 'Ġcomputer', 'Ġsimulation', 'Ġelectron', 'Ġlaunch', 'Ġyoutube', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C364" t="n">
@@ -5170,7 +5170,7 @@
       </c>
       <c r="B365" t="inlineStr">
         <is>
-          <t>['Ġdeep', 'ï', '¬', 'ģ', 'e', 'ld', 'Ġimages', 'empty', 'Ġregions', 'Ġweb', 'b', 'Ġspace', 'Ġtelescopes', 'Ġrevealing', 'Ġuniverse', 'Ġever', 'Ġthought', 'Ġpossible', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġameric', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġko', 'oser', 'anda', 'Ġj', 'uly', 'hub', 'ble', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġimages', 'Ġcompared', 'Ġsee', 'Ġdifference', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġbuilds', 'Ġhub', 'ble', "'s", 'Ġlegacy', 'Ġstunning', 'Ġnew', 'Ġviews', 'Ġcosmos', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġtim', 'mer', 'Ġjohn', 'Ġj', 'uly', 'n', 'asa', 'Ġnames', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġï', '¬', 'ģ', 'Ġtargets', 'Ġweb', 'b', 'Ġimages', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'first', 'Ġimages', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġn', 'asa', 'Ġj', 'uly', 'Ġarchived', 'Ġv', 'bb', 'ï', '¬', 'ģ', 'r', 'st', 'images', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġstir', 'one', 'Ġsh', 'annon', 'Ġj', 'uly', 'g', 'aw', 'king', 'Ġawe', 'Ġuniverse', 'Ġtogether', 'ny', 'time', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'bye', 'ennis', 'Ġchang', 'Ġk', 'enn', 'eth', 'ok', 'ol', 'Ġj', 'osh', 'ua', 'Ġj', 'uly', 'bb', 'Ġtelescope', 'Ġreveals', 'Ġnew', 'Ġvision', 'Ġancient', 'Ġuniverse', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġchang', 'Ġk', 'enn', 'eth', 'Ġj', 'uly', 'n', 'asa', 'Ġshows', 'Ġweb', 'b', "'s", 'Ġview', 'Ġsomething', 'Ġcloser', 'Ġhome', 'Ġj', 'upiter', 'Ġpowerful', 'Ġtelescope', 'Ġhelp', 'Ġscientists', 'Ġmake', 'Ġdiscoveries', 'Ġwithin', 'Ġsolar', 'Ġsystem', 'Ġwell', 'Ġbeyond', 'Ġnew', 'ork', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġast', 'ud', 'illo', 'def', 'ru', 'Ġn', '.;', 'Ġclout', 'ier', 'Ġr', '.;', 'Ġw', 'ang', 'Ġx']</t>
+          <t>['Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġr', 'af', 'Ġmen', 'Ġhill', 'Ġlarge', 'Ġsite', 'Ġunited', 'Ġkingdom', 'Ġpart', 'Ġe', 'che', 'lon', 'Ġu', 'k', 'usa', 'Ġagreement', 'Ġg', 'erman', 'Ġmessage', 'Ġintercepted', 'Ġb', 'rit', 'ish', 'Ġworld', 'Ġwar', 'Ġsignaling', 'Ġg', 'erman', "'s", 'Ġunconditional', 'Ġsurrender', 'Ġsignals', 'Ġintelligence', 'red', 'irect', 'ed', 'Ġsig', 'int', 'Ġsignals', 'Ġintelligence', 'ig', 'int', 'Ġinterception', 'Ġsignals', 'Ġwhether', 'Ġcommunications', 'Ġpeople', 'communications', 'int', 'Ġelectronic', 'Ġsignals', 'Ġdirectly', 'Ġused', 'Ġcommunication', 'elect', 'ronic', 'Ġel', 'int', ').[', 'Ġsignals', 'Ġintelligence', 'Ġsubset', 'Ġintelligence', 'Ġcollection', 'Ġmanagement', 'Ġclassified', 'Ġsensitive', 'Ġinformation', 'Ġusually', 'Ġencrypted', 'Ġsignals', 'Ġintelligence', 'Ġturn', 'Ġinvolves', 'Ġuse', 'Ġcrypt', 'analysis', 'Ġdecipher', 'Ġmessages', 'Ġtraffic', 'Ġanalysis', 'âĢĶ', 'Ġstudy', 'Ġsignaling', 'Ġquantity', 'âĢĶ', 'Ġalso', 'Ġused', 'Ġintegrate', 'Ġinformation', 'Ġelectronic', 'Ġinterceptions', 'Ġappeared', 'Ġearly', 'Ġbo', 'er', 'Ġwar', 'âĢĵ', '02', 'Ġb', 'rit', 'ish', 'Ġroyal', 'Ġnavy', 'Ġinstalled', 'Ġwireless', 'Ġsets', 'Ġproduced', 'Ġmar', 'coni', 'Ġboard', 'Ġships', 'Ġlate', 'Ġb', 'rit', 'ish', 'Ġarmy', 'Ġused', 'Ġlimited', 'Ġwireless', 'Ġsignalling', 'Ġbo', 'ers', 'Ġcaptured', 'Ġwireless', 'Ġsets', 'Ġused', 'Ġmake', 'Ġvital', 'Ġtransmissions', 'Ġsince', 'Ġb', 'rit', 'ish', 'Ġpeople', 'Ġtransmitting', 'Ġtime', 'Ġspecial', 'Ġinterpretation', 'Ġsignals', 'Ġintercepted', 'Ġb', 'rit', 'ish', 'Ġnecessary', 'Ġbirth', 'Ġsignals', 'Ġintelligence', 'Ġmodern', 'Ġsense', 'Ġdates', 'Ġr', 'us', 'j', 'apan', 'ese', 'Ġwar', 'âĢĵ', '05', 'Ġr', 'ussian', 'Ġfleet', 'Ġprepared', 'Ġconflict', 'Ġj', 'apan', 'Ġb', 'rit', 'ish', 'Ġship', 'iana', 'Ġstationed', 'Ġcanal', 'Ġintercepted', 'Ġr', 'ussian', 'Ġnaval', 'Ġwireless', 'Ġsignals', 'Ġsent', 'Ġmobilization', 'Ġfleet', 'Ġfirst', 'Ġtime', 'Ġhistory', 'Ġcourse', 'Ġfirst', 'Ġworld', 'Ġwar', 'Ġnew', 'Ġmethod', 'Ġsignals', 'Ġintelligence', 'Ġreached', 'Ġmaturity', 'Ġfailure', 'Ġproperly', 'Ġprotect', 'Ġcommunications', 'Ġfatally', 'Ġcompromised', 'Ġr', 'ussian', 'Ġarmy', 'Ġadvance', 'Ġearly', 'Ġworld', 'Ġwar', 'Ġled', 'Ġdisastrous', 'Ġdefeat', 'Ġgerm', 'ans', 'Ġl', 'ud', 'endor', 'ff', 'Ġhind', 'enburg', 'Ġbattle', 'ann', 'enberg', 'Ġfrench', 'Ġintercept', 'Ġpersonnel', 'Ġcaptured', 'Ġmessage', 'Ġwritten', 'Ġnew', 'Ġcipher', 'Ġcrypt', 'analy', 'zed', 'Ġge', 'org', 'es', 'Ġpain', 'vin', 'Ġgave', 'Ġallies', 'Ġadvance', 'Ġwarning', 'Ġg', 'erman']</t>
         </is>
       </c>
       <c r="C365" t="n">
@@ -5183,7 +5183,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>['.;', 'es', 'ke', 'Ġj', '.;', 'Ġr', '.;', 'Ġhell', 'ier', 'Ġc', '.;', 'Ġr', 'icker', 'Ġg', '.;', 'Ġv', 'anders', 'pe', 'k', 'Ġr', '.;', 'Ġl', 'atham', '.;', 'Ġse', 'ager', '.;', 'Ġwin', 'n', 'Ġj', 'Ġn', '.;', 'Ġet', 'Ġal', 'Ġapr', 'il', 'Ġhot', 'Ġterrestrial', 'Ġplanet', 'Ġorbiting', 'Ġbright', 'Ġdwarf', 'Ġunveiled', 'ess', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġar', 'x', 'iv', '09', 'Ġ01', '09', 'Ġiss', 'n', 'Ġ0004', 'api', 'se', 'man', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġj', 'uly', 'kinson', 'Ġn', 'ancy', 'Ġaug', 'ust', "'s", 'Ġlargest', 'Ġimage', 'Ġj', 'w', 'st', 'Ġtaken', 'Ġfar', 'w', 'Ġuniverse', 'Ġtoday', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġwh', 'itt', 'Ġke', 'lly', 'Ġk', 'izer', 'Ġaug', 'ust', 'bb', "'s", 'Ġlargest', 'Ġimage', 'Ġgalaxies', 'Ġyet', 'Ġearth', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'ed', 'inburgh', 'Ġastronomers', 'Ġï', '¬', 'ģ', 'nd', 'Ġdistant', 'Ġgalaxy', 'Ġearly', 'Ġdata', 'Ġnew', 'Ġspace', 'Ġtelescope', 'Ġenabled', 'Ġed', 'inburgh', 'Ġastronomers', 'Ġlocate', 'Ġdistant', 'Ġgalaxy', 'Ġever', 'Ġfound', 'Ġuniversity', 'Ġed', 'inburgh', 'Ġaug', 'ust', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġaug', 'ust', 'Ġplan', 'ck', 'Ġcollaboration', 'plan', 'ck', 'Ġresults', 'Ġvi', 'Ġcos', 'ological', 'Ġparameters', '".', 'Ġastronomy', 'Ġastroph', 'ysics', 'Ġpage', 'see', 'Ġpage', 'Ġtable', 'age', 'gy', 'r', '",', 'Ġlast', 'Ġcolumn', 'Ġar', 'x', 'iv', '07', '06', 'ui', 'ads', 'doi', 'org', 'Ġsid', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġboy', 'uan', 'Ġb', 'rom', 'Ġvol', 'ker', 'Ġse', 'pt', 'ember', 'ac', 'celer', 'ating', 'Ġearly', 'Ġmassive', 'Ġgalaxy', 'Ġformation', 'Ġprim', 'ordial', 'Ġblack', 'Ġholes', 'Ġastroph', 'ysical', 'Ġjournal', 'Ġletters', '):', 'Ġar', 'x', 'iv', 'Ġiss', 'n', 'Ġyuan', 'Ġgu', 'wen', 'Ġle', 'Ġle']</t>
+          <t>['Ġspring', 'Ġoffensive', 'Ġhistory', 'Ġorigins', 'Ġdevelopment', 'Ġworld', 'Ġwar', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġz', 'immer', 'mann', 'Ġte', 'legram', 'Ġdec', 'oded', 'Ġroom', 'Ġb', 'rit', 'ish', 'Ġparticular', 'Ġbuilt', 'Ġgreat', 'Ġexpertise', 'Ġnewly', 'Ġemerging', 'Ġfield', 'Ġsignals', 'Ġintelligence', 'Ġcode', 'breaking', 'syn', 'onymous', 'Ġcrypt', 'analysis', 'Ġdeclaration', 'Ġwar', 'Ġb', 'rit', 'Ġcut', 'Ġg', 'erman', 'sea', 'Ġcables', 'Ġforced', 'Ġgerm', 'ans', 'Ġuse', 'Ġeither', 'Ġte', 'legraph', 'Ġline', 'Ġconnected', 'Ġb', 'rit', 'ish', 'Ġnetwork', 'Ġcould', 'Ġtapped', 'Ġradio', 'Ġb', 'rit', 'ish', 'Ġcould', 'Ġintercept', 'Ġrear', 'Ġadm', 'iral', 'Ġhen', 'ry', 'Ġol', 'iver', 'Ġappointed', 'Ġsir', 'Ġal', 'fred', 'Ġe', 'wing', 'Ġestablish', 'Ġinterception', 'Ġdec', 'ryption', 'Ġservice', 'Ġadm', 'ir', 'alty', 'Ġroom', 'Ġinterception', 'Ġservice', 'Ġknown', 'Ġservice', 'Ġtogether', 'Ġpost', 'Ġoffice', 'Ġmar', 'coni', 'Ġstations', 'Ġgrew', 'Ġrapidly', 'Ġpoint', 'Ġb', 'rit', 'ish', 'Ġcould', 'Ġintercept', 'Ġalmost', 'Ġofficial', 'Ġg', 'erman', 'Ġmessages', 'Ġg', 'erman', 'Ġfleet', 'Ġhabit', 'Ġday', 'Ġwireless', 'ing', 'Ġexact', 'Ġposition', 'Ġship', 'Ġgiving', 'Ġregular', 'Ġposition', 'Ġreports', 'Ġsea', 'Ġpossible', 'Ġbuild', 'Ġprecise', 'Ġpicture', 'Ġnormal', 'Ġoperation', 'Ġhigh', 'Ġseas', 'Ġfleet', 'Ġinfer', 'Ġroutes', 'Ġchose', 'Ġdefensive', 'Ġmine', 'fields', 'Ġplaced', 'Ġsafe', 'Ġships', 'Ġoperate', 'Ġwhenever', 'Ġchange', 'Ġnormal', 'Ġpattern', 'Ġseen', 'Ġimmediately', 'Ġsign', 'alled', 'Ġoperation', 'Ġtake', 'Ġplace', 'Ġwarning', 'Ġcould', 'Ġgiven', 'Ġdetailed', 'Ġinformation', 'Ġsubmarine', 'Ġmovements', 'Ġalso', 'Ġavailable', 'Ġuse', 'Ġradio', 'ce', 'iving', 'Ġequipment', 'Ġpinpoint', 'Ġlocation', 'Ġtransmitter', 'Ġalso', 'Ġdeveloped', 'Ġwar', 'Ġcaptain', 'Ġround', 'Ġworking', 'Ġmar', 'coni', 'Ġbegan', 'Ġcarrying', 'Ġexperiments', 'Ġdirection', 'finding', 'Ġradio', 'Ġequipment', 'Ġarmy', 'Ġfr', 'ance', 'Ġmay', 'Ġadm', 'ir', 'alty', 'Ġable', 'Ġtrack', 'Ġg', 'erman', 'Ġsubmarines', 'Ġcrossing', 'Ġnorth', 'Ġsea', 'Ġstations', 'Ġalso', 'Ġacted', 'Ġstations', 'Ġcollect', 'Ġg', 'erman', 'Ġmessages', 'Ġnew', 'Ġsection', 'Ġcreated', 'Ġwithin', 'Ġroom', 'Ġplot', 'Ġpositions', 'Ġships', 'Ġdirectional', 'Ġreports', 'Ġroom', 'Ġplayed', 'Ġimportant', 'Ġrole', 'Ġseveral', 'Ġnaval', 'Ġengagements', 'Ġwar', 'Ġnotably', 'Ġdetecting', 'Ġmajor', 'Ġg', 'erman', 'Ġsort', 'ies', 'Ġnorth', 'Ġsea', 'Ġbattle', 'gger', 'Ġbank']</t>
         </is>
       </c>
       <c r="C366" t="n">
@@ -5196,7 +5196,7 @@
       </c>
       <c r="B367" t="inlineStr">
         <is>
-          <t>['Ġw', 'ang', 'Ġw', 'ang', 'Ġbo', 'Ġw', 'ang', 'ying', 'Ġc', 'hen', 'Ġch', 'ao', 'n', 'Ġca', 'fu', 'Ġfan', 'zh', 'ong', 'Ġmarch', 'rap', 'id', 'ly', 'Ġgrowing', 'Ġprim', 'ordial', 'Ġblack', 'Ġholes', 'Ġseeds', 'Ġmassive', 'Ġhigh', 'red', 'shift', 'Ġj', 'w', 'st', 'Ġgalaxies', '".', 'Ġar', 'x', 'iv', '09', 'Ġ09', 'ast', 'ro', 'ph', 'co', 'Ġstr', 'ick', 'land', 'Ġash', 'ley', 'Ġj', 'une', 'bb', 'Ġtelescope', 'Ġdetects', 'Ġorganic', 'Ġmolecules', 'Ġdistant', 'Ġgalaxy', 'ht', 'Ġretrieved', 'Ġj', 'une', 'Ġgrey', 'Ġchar', 'les', 'Ġj', 'uly', 'j', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġmarks', 'Ġfirst', 'Ġyear', 'Ġscience', 'Ġoperations', 'Ġper', 'ations', 'Ġair', 'Ġspace', 'Ġnews', 'Ġretrieved', 'Ġj', 'uly', 'Ġj', 'athan', 'Ġp', 'Ġgard', 'ner', 'Ġet', 'Ġal', 'n', 'ovember', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', '".', 'Ġspace', 'Ġscience', 'Ġreviews', '):', 'âĢĵ', 'Ġformal', 'Ġcase', 'Ġj', 'w', 'st', 'Ġscience', 'Ġpresented', 'Ġj', 'ason', 'Ġk', 'al', 'ir', 'ai', 'ap', 'ril', 'scient', 'ï', '¬', 'ģ', 'c', 'Ġdiscovery', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', '".', 'Ġcontemporary', 'Ġphysics', '):', 'âĢĵ', 'Ġar', 'x', 'iv', '05', '06', 'Ġreview', 'Ġj', 'w', 'st', 'Ġcapabilities', 'Ġscient', 'ï', '¬', 'ģ', 'c', 'Ġopportunities', 'Ġrig', 'Ġj', 'ane', 'Ġper', 'rin', 'Ġmarsh', 'cel', 'w', 'ichael', 'Ġk', 'imble', 'Ġr', 'andy', 'Ġfried', 'man', 'Ġsc', 'ott', 'Ġet', 'Ġal', 'Ġscience', 'Ġperformance', 'Ġj', 'w', 'st', 'Ġcharacterized', 'Ġcommission', 'ing', '".', 'Ġpublications', 'Ġastronomical', 'Ġsociety', 'Ġpac', 'ï', '¬', 'ģ', 'c', '):', '001', 'Ġar', 'x', 'iv', '05', '05', '001', 'r', 'ï', '¬', 'ģ', 'cial', 'Ġn', 'asa', 'Ġst', 'sci', 'Ġpe', 'org', 'Ġes', 'Ġfrench', 'Ġst', 'fr', 'Ġwebsite', 'Ġj', 'w', 'st', 'Ġn', 'asa', 'Ġtracking', 'Ġpage', 'Ġlaunch', 'Ġfinal', 'Ġcalibr', 'ations', 'Ġj', 'w', 'st', 'Ġn', 'asa', 'Ġpage', 'Ġtimeline', 'Ġdetails', 'Ġweb', 'b', 'Ġorbit', 'Ġcommunicating', 'Ġj', 'w', 'st', 'Ġtext', 'Ġcritical', 'Ġevents', 'Ġlaunching', 'Ġdeployment', 'Ġreading']</t>
+          <t>['Ġsmall', 'Ġpart', 'Ġdue', 'Ġintercept', 'Ġallowed', 'Ġnavy', 'Ġposition', 'Ġships', 'Ġright', 'Ġplace', 'Ġplayed', 'Ġvital', 'Ġrole', 'Ġsubsequent', 'Ġnaval', 'Ġclashes', 'Ġincluding', 'Ġbattle', 'Ġj', 'ut', 'land', 'Ġb', 'rit', 'ish', 'Ġfleet', 'Ġsent', 'Ġintercept', 'Ġdirection', 'finding', 'Ġcapability', 'Ġallowed', 'Ġtracking', 'Ġlocation', 'Ġg', 'erman', 'Ġships', 'Ġsubmarines', 'Ġze', 'ppel', 'ins', 'Ġsystem', 'Ġsuccessful', 'Ġend', 'Ġwar', 'Ġmillion', 'Ġwords', 'Ġcomprising', 'Ġtotality', 'Ġg', 'erman', 'Ġwireless', 'Ġtransmission', 'Ġcourse', 'Ġwar', 'Ġintercepted', 'Ġoperators', 'st', 'ations', 'Ġdec', 'rypted', 'Ġhowever', 'Ġastonishing', 'Ġsuccess', 'Ġdecrypt', 'ing', 'Ġz', 'immer', 'mann', 'Ġte', 'legram', 'Ġte', 'legram', 'Ġg', 'erman', 'Ġforeign', 'Ġoffice', 'Ġsent', 'Ġvia', 'Ġwashing', 'ton', 'Ġambassador', 'rich', 'Ġvon', 'Ġe', 'ck', 'ard', 'x', 'ico', 'Ġimportance', 'Ġinterception', 'Ġdec', 'ryption', 'Ġfirmly', 'Ġestablished', 'Ġwartime', 'Ġexperience', 'Ġcountries', 'Ġestablished', 'Ġpermanent', 'Ġagencies', 'Ġdedicated', 'Ġtask', 'Ġinter', 'war', 'Ġperiod', 'Ġb', 'rit', 'ish', 'Ġcabinet', "'s", 'Ġsecret', 'Ġservice', 'Ġcommittee', 'Ġchaired', 'Ġlord', 'Ġcur', 'zon', 'Ġrecommended', 'Ġpeace', 'time', 'Ġcode', 'breaking', 'Ġagency', 'Ġcreated', 'Ġgovernment', 'Ġcode', 'Ġcy', 'pher', 'Ġschool', 'Ġfirst', 'Ġpeace', 'time', 'Ġcode', 'breaking', 'Ġagency', 'Ġpublic', 'Ġfunction', 'Ġadvise', 'Ġsecurity', 'Ġcodes', 'Ġpostwar', 'Ġconsolidation', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġmark', 'Ġcol', 'ossus', 'Ġcomputer', 'Ġten', 'Ġcol', 'oss', 'Ġworld', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġprogram', 'mable', 'Ġelectronic', 'Ġcomputers', 'Ġbuilt', 'Ġbreak', 'Ġg', 'erman', 'Ġcodes', 'Ġunit', 'Ġsig', 'int', 'Ġunit', 'rael', 'Ġintelligence', 'Ġcorps', 'Ġbase', 'Ġmount', 'Ġav', 'ital', 'Ġg', 'olan', 'Ġheights', 'Ġcy', 'p', 'Ġused', 'Ġgovernment', 'Ġdepartments', 'Ġassist', 'Ġprovision', '",', 'Ġalso', 'Ġsecret', 'Ġdirective', 'study', 'Ġmethods', 'Ġcy', 'pher', 'Ġcommunications', 'Ġused', 'Ġforeign', 'Ġpowers', '".[', 'Ġofficially', 'Ġformed', 'mber', 'Ġproduced', 'Ġfirst', 'Ġdecrypt', 'Ġoct', 'ober', 'Ġworking', 'Ġdiplomatic', 'Ġcodes', 'Ġc', 'ip', 'Ġcountries', 'Ġtackling', 'Ġdiplomatic', 'Ġcrypt', 'os', 'ystem', 'Ġus', 'Ġcipher', 'Ġbureau', 'Ġestablished', 'Ġachieved', 'Ġsuccess', 'Ġwashing', 'ton', 'Ġnaval', 'Ġconference', 'Ġcrypt', 'analysis']</t>
         </is>
       </c>
       <c r="C367" t="n">
@@ -5209,7 +5209,7 @@
       </c>
       <c r="B368" t="inlineStr">
         <is>
-          <t>['Ġexternal', 'Ġlinks', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġwik', 'ipedia', 'Ġj', 'w', 'st', 'Ġvideo', '031', '):', 'Ġhighlights', 'Ġtechnical', 'Ġengineering', 'Ġdetails', 'Ġj', 'w', 'st', 'Ġvideo', '012', '02', '):', 'st', 'Ġmonth', 'Ġlaunching', 'Ġdeployment', 'anim', 'ation', 'Ġj', 'w', 'st', 'Ġvideo', '008', '06', '):', 'st', 'Ġmonth', 'Ġlaunching', 'Ġdeployment', 'update', 'Ġj', 'w', 'st', 'Ġvideo', '003', '00', '):', 'nd', 'Ġmonth', 'Ġmirror', 'Ġalignment', 'Ġdetails', 'Ġj', 'w', 'st', 'Ġvideos', 'mission', 'Ġcontrol', 'Ġlive', 'Ġdeployment', 'Ġevents', 'Ġsuccessfully', 'Ġcompleted', '):', 'Ġlaunch', '005', '07', 'Ġdec', 'Ġseparation', '003', 'Ġdec', 'mir', 'ror', 'http', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsun', 'shield', 'Ġdeployment', 'Ġmission', 'Ġcontrol', 'Ġlive', 'Ġsun', 'shield', 'Ġ04', 'Ġjan', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġsecondary', 'Ġmirror', 'Ġdeployment', 'Ġmission', 'Ġcontrol', 'Ġlive', 'Ġsecondary', 'Ġmirror', '08', 'Ġ05', 'Ġjan', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġprimary', 'Ġmirror', 'Ġdeployment', 'Ġmission', 'Ġcontrol', 'Ġlive', 'Ġprimary', 'Ġmirror', 'Ġ08', 'Ġjan', 'Ġnews', 'Ġupdate', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', "'s", 'Ġfull', 'Ġdeployment', 'Ġfinal', 'Ġdeployment', '08', 'Ġ08', 'Ġjan', 'Ġmedia', 'Ġb', 'rie', 'ï', '¬', 'ģ', 'ng', 'âĢ', 'Ļ', 'Ġnext', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġarrival', '07', 'Ġjan', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġtelescope', 'Ġfirst', 'Ġphotos', 'Ġdata', 'Ġcalibr', 'ations', 'Ġexplained', 'Ġtest', 'ings', 'Ġcalibr', 'ations', 'Ġfirst', 'Ġthing', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġsee', 'Ġfirst', 'Ġlight', 'http', 'unknown', 'Ġcosmic', 'Ġtime', 'Ġmachine', 'net', 'ï', '¬', 'Ĥ', 'ix', 'Ġdocumentary', 'Ġdevelopment', 'Ġdeployment', 'Ġj', 'ames', 'Ġweb', 'b', 'Ġspace', 'Ġtelescope', 'Ġretrieved']</t>
+          <t>['bert', 'Ġyard', 'ley', 'Ġsecretary', 'Ġwar', 'Ġhen', 'ry', 'Ġl', 'Ġstim', 'son', 'Ġclosed', 'Ġus', 'Ġcipher', 'Ġbureau', 'Ġwords', 'gent', 'le', 'men', 'Ġread', "'s", 'Ġmail', '."', 'Ġuse', 'Ġsig', 'int', 'Ġeven', 'Ġgreater', 'Ġimplications', 'Ġworld', 'Ġwar', 'Ġcombined', 'Ġeffort', 'Ġintercept', 'Ġcrypt', 'analysis', 'Ġwhole', 'Ġb', 'rit', 'ish', 'Ġforces', 'Ġworld', 'Ġwar', 'Ġcame', 'Ġcode', 'Ġname', 'ult', 'ra', '",', 'Ġmanaged', 'Ġgovernment', 'Ġcode', 'Ġcy', 'pher', 'Ġschool', 'Ġb', 'let', 'ch', 'ley', 'Ġpark', 'Ġproperly', 'Ġused', 'Ġg', 'erman', 'Ġen', 'igma', 'Ġlore', 'nz', 'Ġc', 'ip', 'Ġvirtually', 'Ġun', 'break', 'able', 'Ġflaws', 'Ġg', 'erman', 'Ġcryptographic', 'Ġprocedures', 'Ġpoor', 'Ġdiscipline', 'Ġamong', 'Ġpersonnel', 'Ġcarrying', 'Ġcreated', 'Ġvulnerabilities', 'Ġmade', 'Ġb', 'let', 'ch', 'ley', "'s", 'Ġattacks', 'Ġfeasible', 'Ġb', 'let', 'ch', 'ley', "'s", 'Ġwork', 'Ġessential', 'Ġdefeating', 'Ġu', 'boats', 'Ġbattle', 'l', 'antic', 'Ġb', 'rit', 'ish', 'Ġnaval', 'Ġvictories', 'Ġbattle', 'Ġcape', 'Ġmat', 'apan', 'Ġbattle', 'Ġnorth', 'Ġcape', 'Ġultra', 'Ġexerted', 'Ġpowerful', 'Ġeffect', 'Ġnorth', 'Ġaf', 'rican', 'Ġdesert', 'Ġcampaign', 'Ġg', 'erman', 'Ġforces', 'Ġgeneral', 'Ġer', 'win', 'Ġr', 'ommel', 'Ġgeneral', 'Ġsir', 'Ġcla', 'ude', 'uchin', 'leck', 'Ġwrote', 'Ġultra', 'rom', 'mel', 'Ġwould', 'Ġcertainly', 'Ġgot', 'Ġca', 'iro', '".', 'Ġultra', 'Ġdecrypt', 'Ġfeatured', 'Ġprominently', 'Ġstory', 'Ġoperation', 'Ġsal', 'Ġal', 'Ã¡', 'sy', "'s", 'Ġmission', 'Ġacross', 'Ġdesert', 'Ġbehind', 'Ġallied', 'Ġlines', 'Ġprior', 'Ġnorm', 'andy', 'Ġland', 'ings', 'day', 'Ġj', 'une', 'Ġallies', 'Ġknew', 'Ġlocations', 'Ġtwo', 'Ġg', 'erman', "'s", 'Ġfifty', 'eight', 'Ġwestern', 'Ġfront', 'Ġdivisions', 'Ġwin', 'ston', 'Ġchurch', 'ill', 'Ġreported', 'Ġtold', 'Ġking', 'Ġge', 'orge', 'Ġvi', 'Ġthanks', 'Ġsecret', 'Ġweapon', 'Ġgeneral', 'Ġmen', 'z', 'ies', 'Ġput', 'Ġuse', 'Ġfronts', 'Ġwar', '!"', 'Ġsupreme', 'Ġallied', 'Ġcommander', 'Ġdw', 'ight', 'Ġe', 'isen', 'hower', 'Ġend', 'Ġwar', 'Ġdescribed', 'Ġultra', 'dec', 'isive', 'Ġallied', 'Ġvictory', 'Ġofficial', 'Ġhistorian', 'Ġb', 'rit', 'ish', 'Ġintelligence', 'Ġworld', 'Ġwar', 'Ġsir', 'Ġhar', 'ry', 'Ġh', 'ins', 'ley', 'Ġargued', 'Ġultra', 'Ġshortened', 'Ġwar', 'Ġless', 'Ġtwo', 'Ġyears', 'Ġprobably', 'Ġfour', 'Ġyears', '";', 'Ġabsence', 'Ġultra', 'Ġuncertain', 'Ġwar', 'Ġwould', 'Ġended', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġdefined']</t>
         </is>
       </c>
       <c r="C368" t="n">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="B369" t="inlineStr">
         <is>
-          <t>['Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'b', 'irs', 'Ġsystems', 'Ġgeo', 'Ġlow', 'Ġcomponents', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'sb', 'irs', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġsystem', 'Ġintended', 'Ġmeet', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġinfrared', 'Ġspace', 'Ġsurveillance', 'Ġneeds', 'Ġfirst', 'Ġtwo', 'Ġthree', 'Ġdecades', 'st', 'Ġcentury', 'b', 'irs', 'Ġprogram', 'Ġdesigned', 'Ġprovide', 'Ġkey', 'Ġcapabilities', 'Ġareas', 'Ġmissile', 'Ġwarning', 'Ġmissile', 'Ġdefense', 'Ġbattles', 'pace', 'Ġcharacterization', 'Ġtechnical', 'Ġintelligence', 'Ġvia', 'Ġsatellites', 'Ġge', 'os', 'ynchronous', 'Ġearth', 'Ġorbit', 'ge', 'Ġsensors', 'Ġhosted', 'Ġsatellites', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'Ġground', 'based', 'Ġdata', 'Ġprocessing', 'Ġcontrol', 'Ġtotal', 'Ġtwelve', 'Ġsatellites', 'Ġcarrying', 'b', 'irs', 'Ġst', 'ss', 'Ġpayload', 'Ġlaunched', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'Ġst', 'ss', 'rr', 'usa', 'Ġst', 'ss', 'Ġdemo', 'usa', 'Ġst', 'ss', 'Ġdemo', 'usa', 'Ġmanufacturing', 'Ġcontract', 'b', 'irs', 'b', 'irs', 'Ġawarded', 'Ġfunding', 'b', 'irs', 'b', 'irs', 'Ġcanceled', 'Ġbased', 'Ġexperiences', 'Ġlaunching', 'Ġshort', 'range', 'Ġtheater', 'Ġmissiles', 'Ġpers', 'ian', 'Ġgulf', 'Ġwar', 'Ġu', 'Ġdepartment', 'Ġdefense', 'od', 'Ġconcluded', 'Ġexpanded', 'Ġtheater', 'Ġmissile', 'Ġwarning', 'Ġcapabilities', 'Ġneeded', 'Ġbegan', 'Ġplanning', 'Ġimproved', 'Ġinfrared', 'Ġsatellite', 'Ġsensor', 'Ġcapability', 'Ġwould', 'Ġsupport', 'Ġlong', 'range', 'Ġstrategic', 'Ġshort', 'range', 'Ġtheater', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġdefense', 'Ġoperations', 'Ġdod', 'Ġstudied', 'Ġconsolid', 'ating', 'Ġvarious', 'Ġinfrared', 'Ġspace', 'Ġrequirements', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġdefense', 'Ġtechnical', 'Ġintelligence', 'Ġbattles', 'pace', 'Ġcharacterization', 'Ġselected', 'b', 'irs', 'Ġreplace', 'Ġenhance', 'Ġcapabilities', 'Ġprovided', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'sp', 'sp', 'Ġsatellites']</t>
+          <t>['Ġterm', 'sign', 'als', 'Ġintelligence', 'Ġcategory', 'Ġintelligence', 'Ġcomprising', 'Ġeither', 'Ġindividually', 'Ġcombination', 'Ġcommunications', 'Ġintelligence', 'int', 'Ġelectronic', 'Ġintelligence', 'el', 'int', 'Ġforeign', 'Ġinstrument', 'ation', 'Ġsignals', 'Ġintelligence', 'f', 'int', 'Ġhowever', 'Ġtransmitted', 'Ġworld', 'Ġwar', 'Ġtechnical', 'Ġdefinitions', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġoste', 'Ġoste', 'Ġclass', 'Ġel', 'int', 'elect', 'ronic', 'Ġsignals', 'Ġintelligence', 'Ġreconnaissance', 'Ġship', 'Ġg', 'erman', 'Ġnavy', 'Ġsatellite', 'Ġground', 'Ġstation', 'utch', 'Ġnational', 'e', 'Ġsig', 'int', 'Ġorganis', 'ie', 'n', 'Ġintelligence', 'Ġderived', 'Ġcommunications', 'Ġelectronic', 'Ġforeign', 'Ġinstrument', 'ation', 'Ġsignals', 'Ġbroad', 'Ġfield', 'Ġsig', 'int', 'Ġmany', 'Ġsub', 'dis', 'cipl', 'ines', 'Ġtwo', 'Ġmain', 'Ġones', 'Ġcommunications', 'Ġintelligence', 'int', 'Ġelectronic', 'Ġintelligence', 'el', 'int', 'Ġcollection', 'Ġsystem', 'Ġknow', 'Ġlook', 'Ġparticular', 'Ġsignal', 'system', '",', 'Ġcontext', 'Ġseveral', 'Ġnuances', 'Ġtargeting', 'Ġprocess', 'Ġdeveloping', 'Ġcollection', 'Ġrequirements', 'Ġintelligence', 'Ġneed', 'Ġconsidered', 'Ġallocation', 'Ġintelligence', 'Ġresources', 'Ġwithin', 'Ġdepartment', 'Ġdefense', 'Ġcollection', 'Ġrequirements', 'Ġful', 'ï', '¬', 'ģ', 'Ġessential', 'Ġelements', 'Ġinformation', 'Ġintelligence', 'Ġneeds', 'Ġcommander', 'Ġagency', 'Ġestablished', 'Ġintelligence', 'Ġneed', 'Ġvalidated', 'Ġappropriate', 'Ġallocation', 'Ġintelligence', 'Ġresources', 'Ġrequirement', 'Ġful', 'ï', '¬', 'ģ', 'Ġessential', 'Ġelements', 'Ġinformation', 'Ġintelligence', 'Ġneeds', 'Ġintelligence', 'Ġconsumer', '."[', 'Ġfirst', 'Ġatmospheric', 'Ġconditions', 'Ġsun', 'sp', 'ots', 'Ġtarget', "'s", 'Ġtransmission', 'Ġschedule', 'Ġantenna', 'Ġcharacteristics', 'Ġfactors', 'Ġcreate', 'Ġuncertainty', 'Ġgiven', 'Ġsignal', 'Ġintercept', 'Ġsensor', 'Ġable', 'ar', 'Ġsignal', 'Ġinterest', 'Ġeven', 'Ġgeographically', 'Ġfixed', 'Ġtarget', 'Ġopponent', 'Ġmaking', 'Ġattempt', 'Ġevade', 'Ġinterception', 'Ġbasic', 'Ġcounter', 'measures', 'Ġinterception', 'Ġinclude', 'Ġfrequent', 'Ġchanging', 'Ġradio', 'Ġfrequency', 'Ġpolarization', 'Ġtransmission', 'Ġcharacteristics', 'Ġintercept', 'Ġaircraft', 'Ġcould', 'Ġget', 'Ġground', 'Ġcarry', 'Ġantennas', 'Ġreceivers', 'Ġevery', 'Ġpossible', 'Ġfrequency', 'Ġsignal', 'Ġtype', 'Ġdeal', 'Ġcounter', 'measures', 'Ġsecond', 'Ġlocating', 'Ġtransmitter', "'s", 'Ġposition', 'Ġusually', 'Ġpart', 'Ġsig', 'int', 'Ġtri', 'ang', 'ulation', 'Ġsophisticated', 'Ġradio', 'Ġlocation', 'Ġtechniques', 'Ġtime', 'Ġarrival', 'Ġmethods', 'Ġrequire', 'Ġmultiple', 'Ġreceiving', 'Ġpoints', 'Ġdifferent', 'Ġlocations', 'Ġreceivers', 'Ġsend', 'Ġlocation', 'relevant', 'Ġinformation', 'Ġcentral', 'Ġpoint', 'Ġperhaps', 'Ġdistributed', 'Ġsystem', 'Ġparticipate', 'Ġinformation', 'Ġcorrelated']</t>
         </is>
       </c>
       <c r="C369" t="n">
@@ -5235,7 +5235,7 @@
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>['Ġbuilt', 'Ġinfrared', 'Ġdetectors', 'Ġsense', 'Ġmissile', 'Ġpl', 'umes', 'Ġproviding', 'Ġearly', 'Ġwarning', 'Ġlong', 'range', 'Ġballistic', 'Ġmissile', 'Ġlaunches', 'Ġyears', 'Ġdod', 'Ġpreviously', 'Ġattempted', 'Ġreplace', 'sp', 'Ġadvanced', 'Ġwarning', 'Ġsystem', 'Ġearly', 'Ġboost', 'Ġsurveillance', 'Ġtracking', 'Ġsystem', 'Ġlate', 'Ġfollow', 'Ġearly', 'Ġwarning', 'Ġsystem', 'Ġearly', 'Ġaccording', 'Ġgovernment', 'Ġaccountability', 'Ġoffice', 'Ġattempts', 'Ġfailed', 'Ġdue', 'Ġimmature', 'Ġtechnology', 'Ġhigh', 'Ġcost', 'Ġaffordability', 'Ġissues', 'b', 'irs', 'Ġuse', 'Ġsophisticated', 'Ġinfrared', 'Ġtechnologies', 'sp', 'Ġenhance', 'Ġdetection', 'Ġstrategic', 'Ġtheater', 'Ġballistic', 'Ġmissile', 'Ġlaunches', 'Ġperformance', 'Ġmissile', 'tracking', 'Ġfunction', 'Ġbackground', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'b', 'irs', 'Ġhigh', 'Ġgeo', 'Ġoriginal', 'Ġcontract', 'Ġconsisted', 'b', 'irs', 'Ġsatellite', 'Ġsensors', 'b', 'irs', 'Ġgeo', 'Ġsensors', 'Ġsatellites', 'Ġoption', 'Ġtotal', 'Ġge', 'os', 'Ġcomplement', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġplanned', 'Ġpart', 'Ġprogram', 'sb', 'irs', 'low', 'Ġmoved', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'st', 'ss', 'Ġprogram', 'b', 'irs', 'Ġcontinues', 'Ġstruggle', 'Ġcost', 'Ġoverrun', 'Ġn', 'unn', 'cc', 'urdy', 'Ġbreaches', 'Ġoccurring', 'Ġse', 'pt', 'ember', 'Ġexpected', 'Ġproject', 'Ġcost', 'Ġincreased', 'Ġus', 'Ġbillion', 'Ġde', 'cember', 'Ġfollowing', 'Ġthird', 'b', 'irs', 'Ġn', 'unn', 'cc', 'urdy', 'Ġviolation', 'Ġgovernment', 'Ġdecided', 'Ġcompete', 'b', 'irs', 'b', 'irs', 'Ġoption', 'b', 'irs', 'Ġcontingent', 'Ġbased', 'Ġperformance', 'Ġfirst', 'Ġj', 'une', 'Ġlock', 'heed', 'Ġmart', 'Ġannounced', 'Ġawarded', 'Ġcontract', 'Ġthird', 'b', 'irs', 'Ġpayload', 'Ġthird', 'b', 'irs', 'Ġgeo', 'Ġsatellite', 'Ġassociated', 'Ġground', 'Ġequipment', 'Ġmodifications', 'Ġj', 'uly', 'Ġlock', 'heed', 'Ġmart', 'Ġawarded', 'Ġus', 'Ġmillion', 'Ġpayment', 'Ġus', 'af', 'Ġtowards', 'Ġpurchase', 'Ġfourth', 'Ġsatellite', 'Ġfirst', 'b', 'irs', 'Ġgeo', 'Ġsatellite', 'b', 'irs', 'Ġprogram', 'b', 'irs', 'Ġsuccessfully', 'Ġlaunched', 'Ġcape', 'aver', 'al', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġmay', 'Ġj', 'une', 'Ġlock', 'heed', 'Ġmart', 'Ġcontracted']</t>
+          <t>['Ġlocation', 'Ġcomputed', 'Ġmodern', 'Ġsig', 'int', 'Ġsystems', 'Ġtherefore', 'Ġsubstantial', 'Ġcommunications', 'Ġamong', 'Ġintercept', 'Ġplatforms', 'Ġeven', 'Ġplatforms', 'Ġclandestine', 'Ġstill', 'Ġbroadcast', 'Ġinformation', 'Ġtelling', 'Ġlook', 'Ġsignals', 'Ġunited', 'Ġstates', 'Ġtargeting', 'Ġsystem', 'Ġdevelopment', 'Ġlate', 'Ġp', 'sts', 'Ġconstantly', 'Ġsends', 'Ġinformation', 'Ġhelps', 'Ġintercept', 'ors', 'Ġproperly', 'Ġaim', 'Ġantennas', 'Ġdisciplines', 'Ġshared', 'Ġacross', 'Ġbranches', 'Ġtargeting', 'Ġneed', 'Ġmultiple', 'Ġcoordinated', 'Ġreceivers', 'Ġintercept', 'Ġmanagement', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġsimpl', 'ï', '¬', 'ģ', 'ed', 'Ġspectrum', 'Ġanaly', 'zer', 'Ġdisplay', 'Ġsuper', 'heter', 'ody', 'ned', 'Ġamplitude', 'Ġmod', 'ulated', 'Ġsignals', 'Ġtune', 'Ġreceivers', 'Ġlarger', 'Ġintercept', 'Ġaircraft', 'board', 'Ġcapability', 'Ġtarget', 'Ġanalysis', 'Ġplanning', 'Ġothers', 'Ġguard', 'rail', 'Ġcompletely', 'Ġground', 'Ġdirection', 'Ġguard', 'rail', 'Ġaircraft', 'Ġfairly', 'Ġsmall', 'Ġusually', 'Ġwork', 'Ġunits', 'Ġthree', 'Ġcover', 'Ġtactical', 'Ġsig', 'int', 'Ġrequirement', 'Ġwhereas', 'Ġlarger', 'Ġaircraft', 'Ġtend', 'Ġassigned', 'Ġstrategic', 'national', 'Ġmissions', 'Ġdetailed', 'Ġprocess', 'Ġtargeting', 'Ġbegins', 'Ġsomeone', 'Ġdecide', 'Ġvalue', 'Ġcollecting', 'Ġinformation', 'Ġsomething', 'Ġwould', 'Ġpossible', 'Ġdirect', 'Ġsignals', 'Ġintelligence', 'Ġcollection', 'Ġmajor', 'Ġsports', 'Ġevent', 'Ġsystems', 'Ġwould', 'Ġcapture', 'Ġgreat', 'Ġdeal', 'Ġnoise', 'Ġnews', 'Ġsignals', 'Ġperhaps', 'Ġannouncements', 'Ġstadium', 'Ġhowever', 'Ġanti', 'terrorist', 'Ġorganization', 'Ġbelieved', 'Ġsmall', 'Ġgroup', 'Ġwould', 'Ġtrying', 'Ġcoordinate', 'Ġefforts', 'Ġusing', 'Ġshort', 'range', 'Ġun', 'licensed', 'Ġradios', 'Ġevent', 'Ġsig', 'int', 'Ġtargeting', 'Ġradios', 'Ġtype', 'Ġwould', 'Ġreasonable', 'Ġtargeting', 'Ġwould', 'Ġknow', 'Ġstadium', 'Ġradios', 'Ġmight', 'Ġlocated', 'Ġexact', 'Ġfrequency', 'Ġusing', 'Ġfunctions', 'Ġsubsequent', 'Ġsteps', 'Ġsignal', 'Ġdetection', 'Ġdirection', 'Ġfinding', 'Ġdecision', 'Ġtarget', 'Ġmade', 'Ġvarious', 'Ġinterception', 'Ġpoints', 'Ġneed', 'Ġcooperate', 'Ġsince', 'Ġresources', 'Ġlimited', 'Ġknowing', 'Ġinterception', 'Ġequipment', 'Ġuse', 'Ġbecomes', 'Ġeasier', 'Ġtarget', 'Ġcountry', 'Ġbuys', 'Ġrad', 'ars', 'Ġradios', 'Ġknown', 'Ġmanufacturers', 'Ġgiven', 'Ġmilitary', 'Ġaid', 'Ġnational', 'Ġintelligence', 'Ġservices', 'Ġkeep', 'Ġlibraries', 'Ġdevices', 'Ġmanufactured', 'Ġcountry', 'Ġothers', 'Ġuse', 'Ġvariety', 'Ġtechniques', 'Ġlearn', 'Ġequipment', 'Ġacquired', 'Ġgiven', 'Ġcountry', 'Ġknowledge', 'Ġphysics', 'Ġelectronic', 'Ġengineering', 'Ġnarrow', 'Ġproblem', 'Ġtypes', 'Ġequipment', 'Ġmight', 'Ġuse', 'Ġintelligence', 'Ġaircraft', 'Ġflying', 'Ġwell', 'Ġoutside', 'Ġborders', 'Ġanother', 'Ġcountry', 'Ġlisten', 'Ġlong', 'range', 'Ġsearch']</t>
         </is>
       </c>
       <c r="C370" t="n">
@@ -5248,7 +5248,7 @@
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>['Ġus', 'af', 'Ġbuild', 'b', 'irs', 'b', 'irs', 'Ġcost', 'Ġus', 'Ġbillion', 'Ġbudget', 'Ġalloc', 'ates', 'Ġbillion', 'b', 'irs', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'b', 'irs', 'Ġhigh', 'also', 'Ġsimply', 'Ġreferred', 'sb', 'irs', '")', 'Ġconsist', 'Ġfour', 'Ġdedicated', 'Ġsatellites', 'Ġoperating', 'Ġge', 'os', 'ynchronous', 'Ġearth', 'Ġorbit', 'Ġsensors', 'Ġtwo', 'Ġhost', 'Ġsatellites', 'Ġoperating', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'b', 'irs', 'Ġhigh', 'Ġreplace', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'sp', 'Ġsatellites', 'Ġintended', 'Ġprimarily', 'Ġprovide', 'Ġenhanced', 'Ġstrategic', 'Ġtheater', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġcapabilities', 'b', 'irs', 'Ġhigh', 'Ġgeo', 'Ġlaunched', 'Ġmay', 'Ġtwo', 'b', 'irs', 'Ġsensors', 'Ġhosted', 'Ġtwo', 'Ġclassified', 'Ġsatellites', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'Ġalready', 'Ġlaunched', 'Ġprobably', 'Ġpart', 'usa', 'usa', 'Ġlaunches', 'Ġus', 'Ġus', 'Ġbelieved', 'Ġanalysts', 'Ġel', 'int', 'Ġsatellites', 'Ġfamily', 'Ġjump', 'seat', 'Ġtrumpet', 'Ġtrumpet', 'Ġreported', 'Ġcarried', 'Ġinfrared', 'Ġsensor', 'Ġcalled', 'Ġheritage', 'Ġprime', 'Ġcontractor', 'b', 'irs', 'Ġlock', 'heed', 'Ġmart', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġmajor', 'Ġsubcontract', 'Ġlock', 'heed', 'Ġmart', 'Ġalso', 'Ġprovides', 'Ġsatellite', 'b', 'irs', 'Ġgeo', 'Ġsystem', "'s", 'Ġexpected', 'Ġdeployment', 'Ġdelayed', 'Ġde', 'cember', 'Ġproblems', 'Ġlock', 'heed', "'s", 'Ġwork', 'manship', 'Ġsystem', 'Ġcomponents', 'Ġincluding', 'Ġunresolved', 'Ġsoftware', 'Ġmalf', 'unctions', 'Ġseveral', 'Ġbroken', 'Ġsolder', 'Ġjoints', 'Ġsubcontract', 'Ġproc', 'ured', 'Ġgy', 'ro', 'scope', 'Ġassembly', 'Ġfirst', 'Ġspacecraft', 'Ġbuilt', 'Ġfeared', 'Ġlaunch', 'Ġpostp', 'onement', 'Ġlate', 'Ġwould', 'Ġlead', 'Ġconflict', 'Ġplanned', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġjun', 'Ġspacecraft', 'Ġmars', 'Ġscience', 'Ġlaboratory', 'Ġwould', 'Ġuse', 'Ġlaunch', 'Ġfacility', 'Ġhowever', 'Ġfirst', 'Ġgeo', 'Ġlaunch', 'b', 'irs', 'Ġsuccessfully', 'Ġconducted', 'Ġmay', 'b', 'irs', 'Ġhigh', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'b', 'irs', 'Ġlow', 'Ġaccording', 'uters', 'Ġreport', 'Ġfirst', 'Ġtwo', 'b', 'irs', 'Ġgeo', 'Ġsatellites', 'Ġstarted', 'Ġoperations', 'b', 'irs', 'Ġlaunched', 'Ġjan', 'uary', 'b', 'irs', 'Ġsuccessfully', 'Ġdeployed', 'Ġjan', 'uary']</t>
+          <t>['Ġrad', 'ars', 'Ġshort', 'range', 'Ġfire', 'Ġcontrol', 'Ġrad', 'ars', 'Ġwould', 'Ġused', 'Ġmobile', 'Ġair', 'Ġdefense', 'Ġsoldiers', 'Ġscouting', 'Ġfront', 'Ġlines', 'Ġanother', 'Ġarmy', 'Ġknow', 'Ġside', 'Ġusing', 'Ġradios', 'Ġmust', 'Ġportable', 'Ġhuge', 'Ġantennas', 'Ġeven', 'Ġsignal', 'Ġhuman', 'Ġcommunications', 'Ġradio', 'Ġintelligence', 'Ġcollection', 'Ġspecialists', 'Ġknow', 'Ġexists', 'Ġtargeting', 'Ġfunction', 'Ġdescribed', 'Ġlearns', 'Ġcountry', 'Ġradar', 'Ġoperates', 'Ġcertain', 'Ġfrequency', 'Ġrange', 'Ġfirst', 'Ġstep', 'Ġuse', 'Ġsensitive', 'Ġreceiver', 'Ġone', 'Ġantennas', 'Ġlisten', 'Ġevery', 'Ġdirection', 'Ġfind', 'Ġarea', 'Ġradar', 'Ġoperating', 'Ġradar', 'Ġknown', 'Ġarea', 'Ġnext', 'Ġstep', 'Ġfind', 'Ġlocation', 'Ġoperators', 'Ġknow', 'Ġprobable', 'Ġfrequencies', 'Ġtransmissions', 'Ġinterest', 'Ġmay', 'Ġuse', 'Ġset', 'Ġreceivers', 'Ġpreset', 'Ġfrequencies', 'Ġinterest', 'Ġfrequency', 'hor', 'izontal', 'Ġaxis', 'Ġversus', 'Ġpower', 'vert', 'ical', 'Ġaxis', 'Ġproduced', 'Ġtransmitter', 'Ġfiltering', 'Ġsignals', 'Ġadd', 'Ġinformation', 'Ġtransmitted', 'Ġreceived', 'Ġenergy', 'Ġparticular', 'Ġfrequency', 'Ġmay', 'Ġstart', 'Ġrecorder', 'Ġalert', 'Ġhuman', 'Ġlisten', 'Ġsignals', 'Ġintellig', 'ible', 'e', '.,', 'int', 'Ġfrequency', 'Ġknown', 'Ġoperators', 'Ġmay', 'Ġlook', 'Ġpower', 'Ġprimary', 'Ġside', 'band', 'Ġfrequencies', 'Ġusing', 'Ġspectrum', 'Ġanaly', 'zer', 'Ġinformation', 'Ġspectrum', 'Ġanaly', 'zer', 'Ġused', 'Ġtune', 'Ġreceivers', 'Ġsignals', 'Ġinterest', 'Ġexample', 'Ġsimplified', 'Ġspectrum', 'Ġactual', 'Ġinformation', 'Ġsignal', 'Ġdetection', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġhypothetical', 'Ġdisplays', 'Ġfour', 'Ġspectrum', 'Ġanaly', 'zers', 'Ġconnected', 'Ġdirectional', 'Ġantennas', 'Ġtransmitter', 'Ġbearing', 'Ġdegrees', 'Ġreal', 'world', 'Ġtransmit', 'ters', 'Ġreceivers', 'Ġusually', 'Ġdirectional', 'Ġfigure', 'Ġleft', 'Ġassume', 'Ġdisplay', 'Ġconnected', 'Ġspectrum', 'Ġanaly', 'zer', 'Ġconnected', 'Ġdirectional', 'Ġantenna', 'Ġaimed', 'Ġindicated', 'Ġdirection', 'Ġspread', 'spect', 'rum', 'Ġcommunications', 'Ġelectronic', 'Ġtechnique', 'Ġdefeat', 'Ġlooking', 'Ġparticular', 'Ġfrequencies', 'Ġspectrum', 'Ġanalysis', 'Ġused', 'Ġdifferent', 'Ġway', 'Ġidentify', 'Ġfrequencies', 'Ġjammed', 'Ġuse', 'Ġearliest', 'Ġstill', 'Ġcommon', 'Ġmeans', 'Ġdirection', 'Ġfinding', 'Ġuse', 'Ġdirectional', 'Ġantennas', 'Ġg', 'oni', 'ometers', 'Ġline', 'Ġdrawn', 'Ġreceiver', 'Ġposition', 'Ġsignal', 'Ġinterest', 'see', 'Ġknowing', 'Ġcompass', 'Ġbearing', 'Ġsingle', 'Ġpoint', 'Ġtransmitter']</t>
         </is>
       </c>
       <c r="C371" t="n">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="B372" t="inlineStr">
         <is>
-          <t>['Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġrequested', 'Ġbillion', 'Ġfiscal', 'Ġyear', 'b', 'irs', 'Ġfunds', 'Ġadvance', 'Ġprocurement', 'b', 'irs', 'Ġmillion', 'Ġfunding', 'Ġprovided', 'b', 'irs', 'Ġfiscal', 'Ġyear', 'Ġfunding', 'b', 'irs', 'Ġeliminated', 'Ġfavor', 'Ġnew', 'Ġprogram', 'Ġng', 'op', 'ir', 'next', 'Ġgeneration', 'Ġoverhead', 'Ġpersistent', 'Ġinfrared', 'Ġplans', 'Ġremained', 'Ġlaunch', 'b', 'irs', 'b', 'irs', 'b', 'irs', 'Ġsuccessfully', 'Ġlaunched', 'Ġmay', 'b', 'irs', 'Ġsuccessfully', 'Ġlaunched', 'Ġaug', 'ust', 'b', 'irs', 'Ġlow', 'Ġcontract', 'Ġmanaged', 'Ġmissile', 'Ġdefense', 'Ġagency', 'Ġrenamed', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'st', 'ss', 'b', 'irs', 'Ġlow', 'Ġprogram', 'Ġoriginally', 'Ġexpected', 'Ġconsist', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġprimary', 'Ġpurpose', 'b', 'irs', 'Ġlow', 'Ġtracking', 'Ġballistic', 'Ġmissiles', 'Ġdiscrimination', 'Ġwarheads', 'Ġobjects', 'Ġdec', 'oys', 'Ġseparate', 'Ġmissile', 'Ġbodies', 'Ġthroughout', 'Ġmiddle', 'Ġportion', 'Ġflights', 'Ġsystem', 'Ġtwo', 'Ġmajor', 'Ġsensors', 'Ġcoordinated', 'board', 'Ġcomputer', 'Ġscanning', 'Ġinfrared', 'Ġsensor', 'Ġdesigned', 'Ġacquire', 'Ġballistic', 'Ġmissiles', 'Ġearly', 'Ġstages', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtracking', 'Ġinfrared', 'Ġsensor', 'Ġdesigned', 'Ġfollow', 'Ġmissiles', 'Ġwarheads', 'Ġobjects', 'Ġdebris', 'Ġdec', 'oys', 'Ġmiddle', 'Ġlater', 'Ġstages', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtracking', 'Ġsensor', 'Ġwould', 'Ġcooled', 'Ġlow', 'Ġtemperatures', 'b', 'irs', 'Ġlow', "'s", 'Ġoriginal', 'Ġdeployment', 'Ġschedule', 'Ġdate', 'Ġcapabilities', 'Ġsaid', 'Ġneeded', 'Ġnational', 'Ġmissile', 'Ġdefense', 'Ġsystem', 'Ġmissile', 'Ġdefense', 'Ġagency', 'Ġassessed', 'Ġprograms', 'Ġneeded', 'Ġnational', 'Ġballistic', 'Ġmissile', 'Ġdefense', 'Ġsystem', 'Ġfound', 'Ġlacking', 'Ġrelatively', 'Ġnew', 'Ġarena', 'Ġspace', 'Ġdecided', 'Ġabsorb', 'b', 'irs', 'Ġlow', 'Ġconstellation', 'Ġearly', 'Ġstages', 'Ġdevelopment', 'Ġrenamed', 'Ġprogram', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'st', 'ss', 'Ġtransition', 'Ġchanged', 'Ġdirection', 'Ġprogram', 'Ġsomewhat', 'Ġoverall', 'Ġmission', 'Ġremained', 'Ġdetection', 'Ġtracking', 'Ġballistic', 'Ġmissiles', 'Ġphases', 'Ġflight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġfe', 'b', 'ruary', 'Ġend', 'b', 'irs', 'Ġair', 'Ġforce', 'Ġsays', "'s", 'Ġtime', 'Ġmove', 'http']</t>
+          <t>['Ġlocate', 'Ġbearings', 'Ġmultiple', 'Ġpoints', 'Ġusing', 'Ġg', 'oni', 'ometry', 'Ġplotted', 'Ġmap', 'Ġtransmitter', 'Ġlocated', 'Ġpoint', 'Ġbearings', 'Ġintersect', 'Ġsimplest', 'Ġcase', 'Ġtarget', 'Ġmay', 'Ġtry', 'Ġconfuse', 'Ġlisteners', 'Ġmultiple', 'Ġtransmit', 'ters', 'Ġgiving', 'Ġsignal', 'Ġdifferent', 'Ġlocations', 'Ġswitching', 'Ġpattern', 'Ġknown', 'Ġuser', 'Ġapparently', 'Ġrandom', 'Ġlistener', 'Ġindividual', 'Ġdirectional', 'Ġantennas', 'Ġmanually', 'Ġautomatically', 'Ġturned', 'Ġfind', 'Ġsignal', 'Ġdirection', 'Ġmay', 'Ġslow', 'Ġsignal', 'Ġshort', 'Ġduration', 'Ġone', 'Ġalternative', 'Ġw', 'ull', 'en', 'ber', 'Ġarray', 'Ġtechnique', 'Ġmethod', 'Ġseveral', 'Ġconcent', 'ric', 'Ġrings', 'Ġantenna', 'Ġelements', 'Ġsimultaneously', 'Ġreceive', 'Ġsignal', 'Ġbest', 'Ġbearing', 'Ġideally', 'Ġclearly', 'Ġsingle', 'Ġantenna', 'Ġsmall', 'Ġset', 'Ġw', 'ull', 'en', 'ber', 'Ġarrays', 'Ġhigh', 'frequency', 'Ġsignals', 'Ġenormous', 'Ġreferred', 'ele', 'phant', 'Ġcages', 'Ġusers', 'Ġalternative', 'Ġtun', 'able', 'Ġdirectional', 'Ġantennas', 'Ġlarge', 'Ġomn', 'id', 'irection', 'al', 'Ġarrays', 'Ġw', 'ull', 'en', 'ber', 'Ġmeasure', 'Ġtime', 'Ġarrival', 'Ġsignal', 'Ġmultiple', 'Ġpoints', 'Ġusing', 'Ġsimilar', 'Ġmethod', 'Ġprecise', 'Ġtime', 'Ġsynchronization', 'Ġreceivers', 'Ġground', 'Ġstations', 'Ġships', 'Ġaircraft', 'Ġsatellites', 'Ġgiving', 'Ġgreat', 'Ġflexibility', 'Ġmodern', 'Ġanti', 'rad', 'iation', 'Ġmissiles', 'Ġhome', 'Ġattack', 'Ġtransmit', 'ters', 'Ġmilitary', 'Ġantennas', 'Ġrarely', 'Ġsafe', 'Ġdistance', 'Ġuser', 'Ġtransmitter', 'Ġlocations', 'Ġknown', 'Ġusage', 'Ġpatterns', 'Ġmay', 'Ġemerge', 'Ġinf', 'erences', 'Ġmay', 'Ġdrawn', 'Ġtraffic', 'Ġanalysis', 'Ġdiscipline', 'Ġdrawing', 'Ġpatterns', 'Ġinformation', 'Ġflow', 'Ġamong', 'Ġset', 'Ġsend', 'ers', 'Ġreceivers', 'Ġwhether', 'Ġsend', 'ers', 'Ġreceivers', 'Ġdesignated', 'Ġlocation', 'Ġdetermined', 'Ġdirection', 'Ġfinding', 'Ġadd', 'res', 'see', 'Ġsender', 'Ġident', 'ifications', 'Ġmessage', 'Ġeven', 'Ġmas', 'int', 'Ġtechniques', 'finger', 'print', 'ing', 'Ġtransmit', 'ters', 'Ġoperators', 'Ġmessage', 'Ġcontent', 'Ġsender', 'Ġreceiver', 'Ġnecessary', 'Ġtraffic', 'Ġanalysis', 'Ġalthough', 'Ġinformation', 'Ġhelpful', 'Ġexample', 'Ġcertain', 'Ġtype', 'Ġradio', 'Ġknown', 'Ġused', 'Ġtank', 'Ġunits', 'Ġeven', 'Ġposition', 'Ġprecisely', 'Ġdetermined', 'Ġdirection', 'Ġfinding', 'Ġmay', 'Ġassumed', 'Ġtank', 'Ġunit', 'Ġgeneral', 'Ġarea', 'Ġsignal', 'Ġowner', 'Ġtransmitter', 'Ġassume', 'Ġsomeone', 'Ġlistening', 'Ġmight', 'Ġset', 'Ġtank', 'Ġcounter', 'measures', 'Ġinterception', 'Ġdirection', 'ï', '¬', 'ģ', 'nd', 'ing', 'Ġtra', 'f', 'ï', '¬', 'ģ', 'c', 'Ġanalysis']</t>
         </is>
       </c>
       <c r="C372" t="n">
@@ -5274,7 +5274,7 @@
       </c>
       <c r="B373" t="inlineStr">
         <is>
-          <t>['b', 'irs', 'Ġlow', 'space', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'Ġoriginal', 'b', 'irs', 'Ġlow', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'Ġreferences', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'intelligence', 'Ġauthorization', 'Ġact', 'Ġfiscal', 'Ġyear', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'high', 'house', 'Ġreport', ')"', 'Ġu', 'Ġgovernment', 'Ġprinting', 'ï', '¬', 'ģ', 'ce', 'Ġmay', 'space', 'Ġbased', 'Ġinfrared', 'Ġsystem', 'Ġhigh', 'Ġprogram', 'Ġalternative', 'web', 'ar', 'Ġgovernment', 'Ġaccountability', 'ï', '¬', 'ģ', 'ce', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'r', 'html', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġfact', 'Ġsheet', 'Ġspace', 'Ġbased', 'Ġinfrared', 'Ġsystem', 'Ġc', 'di', 'org', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'contract', 'Ġmay', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġmay', 'Ġretrieved', 'mber', 'u', 'Ġair', 'Ġforce', 'Ġawards', 'Ġlock', 'heed', 'Ġmart', 'Ġus', 'billion', 'Ġcontract', 'b', 'irs', 'Ġfollow', 'Ġspacecraft', 'Ġlock', 'heed', 'Ġmart', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġv', 'orman', 'Ġj', 'ul', 'ie', 'Ġj', 'uly', 'lock', 'heed', 'Ġgets', 'Ġus', 'Ġmillion', 'Ġu', 'Ġsatellite', 'Ġpayment', 'http', 'uters', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'sb', 'irs', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'press', 'Ġrelease', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġretrieved', 'mber', 'sb', 'irs', 'Ġgeo', 'Ġcontract', 'Ġawarded', 'Ġlos', 'Ġangel', 'es', 'Ġair', 'Ġforce', 'Ġbase', 'Ġu', 'Ġair', 'Ġforce', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'u', 'Ġair', 'Ġforce', 'Ġawards', 'Ġlock', 'heed', 'Ġmart', 'Ġcontract', 'Ġnext', 'Ġtwo', 'b', 'irs', 'Ġmissile', 'Ġdefense', 'Ġearly', 'Ġwarning', 'Ġsatellites', 'Ġb', 'irs', 'html', 'Ġlock', 'heed', 'mart', 'press', 'Ġrelease', 'Ġlock', 'heed', 'Ġmart', 'Ġj', 'une', 'Ġretrieved', 'mber']</t>
+          <t>['Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġradios', 'Ġarea', 'Ġwants', 'Ġside', 'Ġbelieve', 'Ġactual', 'Ġtanks', 'Ġpart', 'Ġoperation', 'Ġqu', 'icks', 'ilver', 'Ġpart', 'Ġdeception', 'Ġplan', 'Ġinvasion', 'Ġeuro', 'pe', 'Ġbattle', 'Ġnorm', 'andy', 'Ġradio', 'Ġtransmissions', 'Ġsimulated', 'Ġheadquarters', 'Ġsubordinate', 'Ġunits', 'Ġfictitious', 'Ġfirst', 'Ġunited', 'Ġstates', 'Ġarmy', 'Ġgroup', 'f', 'us', 'ag', 'Ġcommanded', 'Ġge', 'orge', 'Ġp', 'atton', 'Ġmake', 'Ġg', 'erman', 'Ġdefense', 'Ġthink', 'Ġmain', 'Ġinvasion', 'Ġcome', 'Ġanother', 'Ġlocation', 'Ġlike', 'Ġmanner', 'Ġfake', 'Ġradio', 'Ġtransmissions', 'Ġj', 'apan', 'ese', 'Ġaircraft', 'Ġcarriers', 'Ġbattle', 'Ġpearl', 'Ġharbor', 'Ġmade', 'Ġj', 'apan', 'ese', 'Ġlocal', 'Ġwaters', 'Ġattacking', 'Ġships', 'Ġmoved', 'Ġstrict', 'Ġradio', 'Ġsilence', 'Ġtraffic', 'Ġanalysis', 'Ġneed', 'Ġfocus', 'Ġhuman', 'Ġcommunications', 'Ġexample', 'Ġsequence', 'Ġradar', 'Ġsignal', 'Ġfollowed', 'Ġexchange', 'Ġtargeting', 'Ġdata', 'Ġconfirmation', 'Ġfollowed', 'Ġobservation', 'Ġartillery', 'Ġfire', 'Ġmay', 'Ġidentify', 'Ġautomated', 'Ġcounter', 'b', 'attery', 'Ġsystem', 'Ġradio', 'Ġsignal', 'Ġtriggers', 'Ġnavig', 'ational', 'acons', 'Ġcould', 'Ġlanding', 'Ġaid', 'Ġsystem', 'Ġairst', 'rip', 'Ġhelicopter', 'Ġpad', 'Ġintended', 'Ġlow', 'profile', 'Ġpatterns', 'Ġemerge', 'Ġknowing', 'Ġradio', 'Ġsignal', 'Ġcertain', 'Ġcharacteristics', 'Ġoriginating', 'Ġfixed', 'Ġheadquarters', 'Ġmay', 'Ġstrongly', 'Ġsuggestive', 'Ġparticular', 'Ġunit', 'Ġsoon', 'Ġmove', 'Ġregular', 'Ġbase', 'Ġcontents', 'Ġmessage', 'Ġneed', 'Ġknown', 'Ġinfer', 'Ġmovement', 'Ġart', 'Ġwell', 'Ġscience', 'Ġtraffic', 'Ġanalysis', 'Ġexpert', 'Ġanalysts', 'Ġdevelop', 'Ġsense', 'Ġreal', 'Ġdeceptive', 'Ġhar', 'ry', 'Ġkid', 'der', 'Ġexample', 'Ġone', 'Ġstar', 'Ġcrypt', 'analy', 'sts', 'Ġworld', 'Ġwar', 'Ġstar', 'Ġhidden', 'Ġbehind', 'Ġsecret', 'Ġcurtain', 'Ġsig', 'int', 'Ġgenerating', 'Ġelectronic', 'Ġorder', 'Ġbattle', 'e', 'ob', 'Ġrequires', 'Ġidentifying', 'Ġsig', 'int', 'Ġemit', 'ters', 'Ġarea', 'Ġinterest', 'Ġdetermining', 'Ġgeographic', 'Ġlocation', 'Ġrange', 'Ġmobility', 'Ġcharacter', 'izing', 'Ġsignals', 'Ġpossible', 'Ġdetermining', 'Ġrole', 'Ġbroader', 'Ġorganizational', 'Ġorder', 'Ġbattle', 'Ġe', 'ob', 'Ġcovers', 'int', 'Ġel', 'int', 'Ġdefense', 'Ġintelligence', 'Ġagency', 'Ġmaintains', 'Ġe', 'ob', 'Ġlocation', 'Ġjoint', 'Ġspectrum', 'Ġcenter', 'Ġdefense', 'Ġinformation', 'Ġsystems', 'Ġagency', 'Ġsupplements', 'Ġlocation', 'Ġdatabase', 'Ġfive', 'Ġtechnical', 'Ġdatabases', 'Ġfr', 'rs', 'Ġfrequency', 'Ġresource', 'Ġrecord', 'Ġsystem', 'Ġbackground', 'Ġenvironment', 'Ġinformation', 'Ġspectrum', 'Ġcert', 'ï', '¬', 'ģ', 'cation', 'Ġsystem']</t>
         </is>
       </c>
       <c r="C373" t="n">
@@ -5287,7 +5287,7 @@
       </c>
       <c r="B374" t="inlineStr">
         <is>
-          <t>['od', 'Ġreleases', 'Ġfiscal', 'Ġyear', 'Ġbudget', 'Ġproposal', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'rocket', 'Ġblasts', 'Ġmissile', 'warning', 'Ġsatellite', 'uters', 'Ġmay', 'u', 'Ġair', 'Ġforce', 'Ġawards', 'Ġlock', 'heed', 'Ġmart', 'Ġus', 'billion', 'Ġcontract', 'b', 'irs', 'Ġfollow', 'Ġspacecraft', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'mol', 'c', 'zan', 'Ġsat', 'obs', 'Ġmessage', 'Ġse', 'pt', 'ember', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'mol', 'c', 'zan', 'Ġsat', 'obs', 'Ġmessage', 'Ġfe', 'b', 'ruary', 'Ġcap', 'acc', 'io', 'ony', 'Ġse', 'pt', 'ember', 'del', 'ivery', 'Ġdelayed', 'Ġlock', 'heed', 'Ġmart', "'s", 'Ġearly', 'Ġwarning', 'Ġsatellite', '".', 'Ġbloom', 'berg', 'Ġth', 'om', 'pson', 'Ġlore', 'n', 'Ġb', 'Ġlaunch', 'Ġpriority', 'Ġmissile', 'Ġwarning', 'Ġcome', 'Ġfirst', 'Ġlex', 'ington', 'Ġinstitute', 'Ġoct', 'ober', 'lock', 'heed', 'Ġwins', 'Ġus', 'Ġbillion', 'Ġdeal', 'Ġu', 'Ġmissile', 'warning', 'Ġsatellites', 'uters', 'Ġj', 'une', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'press', 'Ġrelease', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'Ġrich', 'ards', 'Ġde', 'rek', 'Ġjan', 'uary', 'var', 'ious', 'Ġissues', 'Ġprompt', 'hour', 'Ġscrub', 'las', 'b', 'irs', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġinsider', 'Ġretrieved', 'mber', 'Ġcl', 'ark', 'Ġstep', 'hen', 'u', 'Ġmilitary', 'Ġsatellite', 'Ġlaunched', 'Ġfort', 'ify', 'Ġmissile', 'Ġattacks', 'space', 'ï', '¬', 'Ĥ', 'igh', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġoct', 'ober', 'production', 'Ġnew', 'Ġmissile', 'Ġwarning', 'Ġsatellites', 'Ġlikely', 'Ġdelayed', 'Ġbudget', 'Ġimp', 'asse', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', 'las', 'Ġrocket', 'Ġlaunches', 'b', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġus', 'Ġspace', 'Ġforce', 'ww', 'Ġspace', 'Ġmay', 'Ġretrieved', 'Ġj', 'une']</t>
+          <t>['Ġequipment', 'Ġtac', 'db', 'Ġplatform', 'Ġlists', 'Ġsorted', 'Ġn', 'omen', 'cl', 'ature', 'Ġcontain', 'Ġlinks', 'Ġc', 'e', 'Ġequipment', 'Ġcomplement', 'Ġplatform', 'Ġlinks', 'Ġparam', 'etric', 'Ġdata', 'Ġpiece', 'Ġequipment', 'Ġmilitary', 'Ġunit', 'Ġlists', 'Ġsubordinate', 'Ġunits', 'Ġequipment', 'Ġused', 'Ġunit', 'Ġexample', 'Ġseveral', 'Ġvoice', 'Ġtransmit', 'ters', 'Ġmight', 'Ġidentified', 'Ġcommand', 'Ġnet', 'e', '.,', 'Ġtop', 'Ġcommander', 'Ġdirect', 'Ġreports', 'Ġtank', 'Ġbattalion', 'Ġtank', 'heavy', 'Ġtask', 'Ġforce', 'Ġanother', 'Ġset', 'Ġtransmit', 'ters', 'Ġmight', 'Ġidentify', 'Ġlog', 'istic', 'Ġnet', 'Ġunit', 'Ġinventory', 'Ġel', 'int', 'Ġsources', 'Ġmight', 'Ġidentify', 'Ġmedium', 'Ġlong', 'range', 'Ġcounter', 'art', 'illery', 'Ġrad', 'ars', 'Ġgiven', 'Ġarea', 'Ġsignals', 'Ġintelligence', 'Ġunits', 'Ġidentify', 'Ġchanges', 'Ġe', 'ob', 'Ġmight', 'Ġindicate', 'Ġenemy', 'Ġunit', 'Ġmovement', 'Ġchanges', 'Ġcommand', 'Ġrelationships', 'Ġincreases', 'Ġdecreases', 'Ġcapability', 'Ġusing', 'int', 'Ġgathering', 'Ġmethod', 'Ġenables', 'Ġintelligence', 'Ġofficer', 'Ġproduce', 'Ġelectronic', 'Ġorder', 'Ġbattle', 'Ġtraffic', 'Ġanalysis', 'Ġcontent', 'Ġanalysis', 'Ġamong', 'Ġseveral', 'Ġenemy', 'Ġunits', 'Ġexample', 'Ġfollowing', 'Ġmessages', 'Ġintercepted', 'Ġelectronic', 'Ġorder', 'Ġbattle', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġe', 'ob', 'Ġrelated', 'Ġdata', 'Ġï', '¬', 'Ĥ', 'ow', 'Ġrequesting', 'Ġpermission', 'Ġproceed', 'Ġcheckpoint', 'Ġx', 'Ġapproved', 'Ġplease', 'Ġreport', 'Ġarrival', 'Ġminutes', 'Ġlater', 'Ġvehicles', 'Ġarrived', 'Ġcheckpoint', 'Ġx', 'Ġsequence', 'Ġshows', 'Ġtwo', 'Ġunits', 'Ġbattlefield', 'Ġunit', 'Ġmobile', 'Ġunit', 'Ġhigher', 'Ġhierarchical', 'Ġlevel', 'Ġperhaps', 'Ġcommand', 'Ġpost', 'Ġone', 'Ġalso', 'Ġunderstand', 'Ġunit', 'Ġmoved', 'Ġone', 'Ġpoint', 'Ġanother', 'Ġdistant', 'Ġminutes', 'Ġvehicle', 'Ġregular', 'Ġreports', 'Ġperiod', 'Ġtime', 'Ġmight', 'Ġreveal', 'Ġpatrol', 'Ġpattern', 'Ġdirection', 'finding', 'Ġradio', 'Ġfrequency', 'Ġmas', 'int', 'Ġcould', 'Ġhelp', 'Ġconfirm', 'Ġtraffic', 'Ġdeception', 'Ġe', 'ob', 'Ġbuildup', 'Ġprocess', 'Ġdivided', 'Ġfollowing', 'Ġsignal', 'Ġseparation', 'Ġmeasurements', 'Ġoptimization', 'Ġdata', 'Ġfusion', 'Ġnetworks', 'Ġbuild', 'Ġseparation', 'Ġintercepted', 'Ġspectrum', 'Ġsignals', 'Ġintercepted', 'Ġsensor', 'Ġmust', 'Ġtake', 'Ġplace', 'Ġextremely', 'Ġsmall', 'Ġperiod', 'Ġtime', 'Ġorder', 'Ġseparate', 'Ġdifferent', 'Ġsignals', 'Ġdifferent', 'Ġtransmit', 'ters', 'Ġbattlefield', 'Ġcomplexity', 'Ġseparation', 'Ġprocess', 'Ġdepends', 'Ġcomplexity', 'Ġtransmission', 'Ġmethods', 'Ġhopping', 'Ġtime', 'division', 'Ġmultiple', 'Ġaccess', 'td', ')).', 'Ġgathering', 'Ġclust', 'ering', 'Ġdata', 'Ġsensor', 'Ġmeasurements', 'Ġdirection', 'Ġsignals']</t>
         </is>
       </c>
       <c r="C374" t="n">
@@ -5300,7 +5300,7 @@
       </c>
       <c r="B375" t="inlineStr">
         <is>
-          <t>['las', 'b', 'irs', 'Ġgeo', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġu', 'Ġspace', 'Ġforce', 'h', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġaug', 'ust', 'Ġl', 'isa', 'odd', 'ers', 'Ġaug', 'b', 'irs', 'Ġlaunch', 'Ġcloses', 'Ġtwo', 'Ġdecades', 'Ġprogress', 'Ġmissile', 'Ġwarning', 'Ġtracking', 'Ġdetection', 'Ġnext', 'gen', 'Ġop', 'ir', 'Ġtake', 'Ġhelm', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġlow', 'Ġrisk', 'Ġmissing', 'Ġinitial', 'Ġdeployment', 'Ġdate', 'Ġu', 'Ġgeneral', 'Ġaccounting', 'ï', '¬', 'ģ', 'ce', 'Ġfe', 'b', 'ruary', 'Ġfact', 'Ġsheets', 'Ġspace', 'Ġbased', 'Ġinfrared', 'Ġsystems', 'Ġspace', 'Ġbased', 'Ġinfrared', 'Ġsystems', 'Ġtactical', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġu', 'Ġstrategic', 'Ġcommand', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
+          <t>['Ġoptimized', 'Ġget', 'Ġmuch', 'Ġaccurate', 'Ġbasic', 'Ġmeasurements', 'Ġstandard', 'Ġdirection', 'Ġfinding', 'Ġsensor', 'Ġcalculating', 'Ġlarger', 'Ġsamples', 'Ġsensor', "'s", 'Ġoutput', 'Ġdata', 'Ġnear', 'Ġreal', 'time', 'Ġtogether', 'Ġhistorical', 'Ġinformation', 'Ġsignals', 'Ġbetter', 'Ġresults', 'Ġachieved', 'Ġdata', 'Ġfusion', 'Ġcorrelates', 'Ġdata', 'Ġsamples', 'Ġdifferent', 'Ġfrequencies', 'Ġsensor', 'Ġconfirmed', 'Ġdirection', 'Ġfinding', 'Ġradio', 'frequency', 'Ġmas', 'int', 'Ġem', 'itter', 'Ġmobile', 'Ġdirection', 'Ġfinding', 'Ġdiscovering', 'Ġrepetitive', 'Ġpattern', 'Ġmovement', 'Ġlimited', 'Ġvalue', 'Ġdetermining', 'Ġsensor', 'Ġunique', 'Ġmas', 'int', 'Ġbecomes', 'Ġinformative', 'Ġindividual', 'Ġtransmit', 'ters', 'Ġantennas', 'Ġmay', 'Ġunique', 'Ġside', 'Ġlob', 'es', 'Ġunintentional', 'Ġradiation', 'Ġpulse', 'Ġtiming', 'Ġetc', 'Ġnetwork', 'Ġbuild', 'Ġanalysis', 'Ġemit', 'ters', 'communication', 'Ġtransmit', 'ters', 'Ġtarget', 'Ġregion', 'Ġsufficient', 'Ġperiod', 'Ġtime', 'Ġenables', 'Ġcreation', 'Ġcommunications', 'Ġflows', 'Ġbattlefield', 'int', 'communications', 'Ġintelligence', 'Ġsub', 'category', 'Ġsignals', 'Ġintelligence', 'Ġengages', 'Ġdealing', 'Ġmessages', 'Ġvoice', 'Ġinformation', 'Ġderived', 'Ġinterception', 'Ġforeign', 'Ġcommunications', 'int', 'Ġcommonly', 'Ġreferred', 'Ġsig', 'int', 'Ġcause', 'Ġconfusion', 'Ġtalking', 'Ġbroader', 'Ġintelligence', 'Ġdisciplines', 'Ġus', 'Ġjoint', 'Ġchiefs', 'Ġstaff', 'Ġdefines', 'technical', 'Ġinformation', 'Ġintelligence', 'Ġderived', 'Ġforeign', 'Ġcommunications', 'Ġintended', 'Ġrecipients', '".[', 'Ġcommunications', 'Ġintelligence', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'int', 'Ġdefined', 'Ġcommunications', 'Ġamong', 'Ġpeople', 'Ġreveal', 'Ġfollowing', 'Ġtransmitting', 'Ġlocated', 'Ġtransmitter', 'Ġmoving', 'Ġreport', 'Ġmay', 'Ġgive', 'Ġplot', 'Ġsignal', 'Ġlocation', 'Ġknown', 'Ġorganizational', 'Ġfunction', 'Ġtransmitter', 'Ġtime', 'Ġduration', 'Ġtransmission', 'Ġschedule', 'Ġperiodic', 'Ġtransmission', 'Ġfrequencies', 'Ġtechnical', 'Ġcharacteristics', 'Ġtransmission', 'Ġtransmission', 'Ġencrypted', 'Ġdec', 'rypted', 'Ġpossible', 'Ġintercept', 'Ġeither', 'Ġoriginally', 'Ġtransmitted', 'Ġcle', 'art', 'ext', 'Ġobtain', 'Ġcrypt', 'analysis', 'Ġlanguage', 'Ġcommunication', 'Ġtranslation', 'Ġneeded', 'Ġaddresses', 'Ġsignal', 'Ġgeneral', 'Ġbroadcast', 'Ġaddresses', 'Ġretri', 'ev', 'able', 'Ġmessage', 'Ġstations', 'Ġmay', 'Ġalso', 'int', 'Ġcon', 'ï', '¬', 'ģ', 'rm', 'ation', 'Ġmessage', 'Ġresponse', 'Ġmessage', 'Ġel', 'int', 'Ġnavigation', 'Ġbeacon']</t>
         </is>
       </c>
       <c r="C375" t="n">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="B376" t="inlineStr">
         <is>
-          <t>['Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġya', 'ogan', 'Ġé', 'ģ', '¥', 'æĦ', 'Ł', 'åį', '«', 'æĺ', 'Ł', 'Ã¡', 'og', 'Ç', 'İ', 'n', 'Ġmodel', 'Ġya', 'ogan', 'Ġprogram', 'Ġoverview', 'Ġcountry', 'Ġpeople', "'s", 'Ġrepublic', 'Ġch', 'ina', 'Ġorganization', 'Ġch', 'ina', 'Ġacademy', 'Ġspace', 'Ġtechnology', 'cast', 'Ġpurpose', 'Ġreconnaissance', 'Ġstatus', 'Ġactive', 'Ġprogram', 'Ġhistory', 'Ġfirst', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġapr', 'il', 'Ġsuccesses', 'Ġfailures', 'Ġlaunch', 'Ġsite', 'Ġvehicle', 'Ġinformation', 'Ġlaunch', 'Ġvehicle', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġlong', 'Ġmarch', 'Ġya', 'ogan', 'Ġya', 'ogan', 'sim', 'pl', 'ified', 'Ġch', 'inese', 'Ġé', 'ģ', '¥', 'æĦ', 'Ł', 'åį', '«', 'æĺ', 'Ł', 'Ġtraditional', 'Ġch', 'inese', 'Ġé', 'ģ', 'Ļ', 'æĦ', 'Ł', 'è¡', 'ŀ', 'æĺ', 'Ł', 'Ġp', 'iny', 'Ã¡', 'og', 'Ç', 'İ', 'n', 'Ġlit', 'remote', 'Ġsensing', 'Ġsatellite', "')", 'Ġcover', 'Ġname', 'Ġused', 'Ġpeople', "'s", 'Ġrepublic', 'Ġch', 'ina', 'Ġrefer', 'Ġmilitary', 'Ġreconnaissance', 'Ġsatellites', 'Ġya', 'ogan', 'Ġsatellites', 'Ġlargely', 'Ġknown', 'Ġprimarily', 'Ġsupport', 'Ġpeople', "'s", 'Ġliberation', 'Ġarmy', "'s", 'Ġstrategic', 'Ġsupport', 'Ġforce', 'pl', 'ass', 'f', 'Ġformerly', 'Ġaerospace', 'Ġreconnaissance', 'Ġbureau', 'Ġsecond', 'Ġdepartment', 'Ġgeneral', 'Ġstaff', 'Ġya', 'ogan', 'Ġsatellites', 'Ġsuccessor', 'Ġprogram', 'Ġfan', 'h', 'ui', 'Ġsh', 'ix', 'ing', 'f', 'sw', 'Ġrecover', 'able', 'Ġreconnaissance', 'Ġsatellite', 'Ġprogram', 'Ġunlike', 'Ġpredecessor', 'Ġincludes', 'Ġvariety', 'Ġclasses', 'Ġutilizing', 'Ġvarious', 'Ġmeans', 'Ġremote', 'Ġsensing', 'Ġoptical', 'Ġreconnaissance', 'Ġsynthetic', 'ap', 'ert', 'ure', 'Ġradar', 'ar', 'Ġelectronic', 'Ġintelligence', 'el', 'int', 'Ġmaritime', 'Ġsurveillance', 'Ġya', 'ogan', 'Ġsatellites', 'Ġlaunched', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'Ġsh', 'xi', 'Ġprovince', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'Ġinner', 'ong', 'olia', 'Ġautonomous', 'Ġregion', 'Ġx', 'ich', 'ang', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'ich', 'uan', 'Ġprovince', 'Ġalthough', 'Ġindividual', 'Ġya', 'ogan', 'Ġsatellites', 'Ġoften', 'Ġreferred', 'Ġnumber', 'Ġya', 'ogan', 'Ġch', 'inese', 'Ġmilitary', 'Ġreconnaissance', 'Ġsatellites', 'Ġtypically', 'Ġcategorized', 'Ġmilitary', 'Ġj', 'ian', 'bing', 'Ġdesignation', 'Ġj', 'ian', 'bing', 'Ġtranslates', 'point', 'Ġsoldier', '",', 'v', 'anguard', '",', 'p', 'ione', 'er', 'Ġentered', 'Ġuse', 'Ġsatellite', 'Ġdesign', 'ations', 'Ġch', 'ina', "'s", 'Ġfirst', 'Ġseries', 'Ġreconnaissance', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġseries', 'Ġfirst', 'Ġya', 'ogan', 'Ġsatellite', 'Ġya', 'ogan', 'Ġone', 'Ġthree', 'Ġj', 'ian', 'bing', 'Ġseries', 'Ġsatellites', 'Ġfollowing', 'Ġfinal', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġseries', 'Ġj', 'ian', 'bing', 'Ġdesign', 'ations', 'Ġsecret']</t>
+          <t>['Ġactivated', 'Ġrather', 'Ġaddition', 'Ġaddress', 'Ġident', 'ï', '¬', 'ģ', 'er', 'Ġmay', 'Ġinformation', 'Ġlocation', 'Ġsignal', 'Ġcharacteristics', 'Ġrespond', 'er', 'Ġbasic', 'int', 'Ġtechnique', 'Ġlisten', 'Ġvoice', 'Ġcommunications', 'Ġusually', 'Ġradio', 'Ġpossibly', 'le', 'aking', 'Ġtele', 'phones', 'Ġwiret', 'aps', 'Ġvoice', 'Ġcommunications', 'Ġencrypted', 'Ġtraffic', 'Ġanalysis', 'Ġmay', 'Ġstill', 'Ġgive', 'Ġinformation', 'Ġsecond', 'Ġworld', 'Ġwar', 'Ġsecurity', 'Ġunited', 'Ġstates', 'Ġused', 'Ġnative', 'Ġameric', 'Ġvolunteer', 'Ġcommun', 'icators', 'Ġknown', 'Ġcode', 'Ġtalk', 'ers', 'Ġused', 'Ġlanguages', 'Ġnav', 'ajo', 'anche', 'Ġcho', 'ct', 'aw', 'Ġwould', 'Ġunderstood', 'Ġpeople', 'Ġeven', 'Ġu', 'Ġeven', 'Ġwithin', 'Ġuncommon', 'Ġlanguages', 'Ġcode', 'Ġtalk', 'ers', 'Ġused', 'Ġspecialized', 'Ġcodes', 'ter', 'fly', 'Ġmight', 'Ġspecific', 'Ġj', 'apan', 'ese', 'Ġaircraft', 'Ġb', 'rit', 'ish', 'Ġforces', 'Ġmade', 'Ġlimited', 'Ġuse', 'Ġwel', 'sh', 'Ġspeakers', 'Ġreason', 'Ġmodern', 'Ġelectronic', 'Ġencryption', 'Ġaway', 'Ġneed', 'Ġarmies', 'Ġuse', 'Ġobscure', 'Ġlanguages', 'Ġlikely', 'Ġgroups', 'Ġmight', 'Ġuse', 'Ġrare', 'Ġdialect', 'Ġoutside', 'Ġethnic', 'Ġgroup', 'Ġwould', 'Ġunderstand', 'Ġmor', 'se', 'Ġcode', 'Ġinterception', 'Ġimportant', 'Ġmor', 'se', 'Ġcode', 'Ġte', 'legraph', 'Ġobsolete', 'Ġwestern', 'Ġworld', 'Ġalthough', 'Ġpossibly', 'Ġused', 'Ġspecial', 'Ġoperations', 'Ġforces', 'Ġforces', 'Ġhowever', 'Ġportable', 'Ġcryptographic', 'Ġequipment', 'Ġspecialists', 'Ġscan', 'Ġradio', 'Ġfrequencies', 'Ġcharacter', 'Ġsequences', 'Ġelectronic', 'Ġmail', 'Ġgiven', 'Ġdigital', 'Ġcommunications', 'Ġlink', 'Ġcarry', 'Ġthousands', 'Ġmillions', 'Ġvoice', 'Ġcommunications', 'Ġespecially', 'Ġdeveloped', 'Ġcountries', 'Ġwithout', 'Ġaddressing', 'Ġlegality', 'Ġactions', 'Ġproblem', 'Ġidentifying', 'Ġchannel', 'Ġcontains', 'Ġconversation', 'Ġbecomes', 'Ġmuch', 'Ġsimpler', 'Ġfirst', 'Ġthing', 'Ġintercepted', 'Ġsignaling', 'Ġchannel', 'Ġcarries', 'Ġinformation', 'Ġset', 'Ġtelephone', 'Ġcalls', 'Ġcivilian', 'Ġmany', 'Ġmilitary', 'Ġuse', 'Ġchannel', 'Ġcarry', 'Ġmessages', 'Ġsignaling', 'Ġsystem', 'Ġprotocols', 'Ġvoice', 'Ġinterception', 'Ġtext', 'Ġinterception', 'Ġsignaling', 'Ġchannel', 'Ġinterception', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġretrospective', 'Ġanalysis', 'Ġtelephone', 'Ġcalls', 'Ġmade', 'Ġcall', 'Ġdetail', 'Ġrecord', 'Ġused', 'Ġbilling', 'Ġcalls', 'Ġpart', 'Ġcommunications', 'Ġsecurity', 'Ġtrue', 'Ġintelligence', 'Ġcollection', 'Ġsig', 'int', 'Ġunits', 'Ġstill', 'Ġmay', 'Ġresponsibility', 'Ġmonitoring', 'Ġone', "'s", 'Ġcommunications', 'Ġelectronic', 'Ġemissions', 'Ġavoid', 'Ġproviding', 'Ġintelligence', 'Ġenemy', 'Ġexample', 'Ġsecurity', 'Ġmonitor', 'Ġmay', 'Ġhear', 'Ġindividual', 'Ġtransmitting', 'Ġinappropriate', 'Ġinformation', 'Ġun', 'encrypted', 'Ġradio', 'Ġnetwork', 'Ġsimply', 'Ġone', 'Ġauthorized', 'Ġtype']</t>
         </is>
       </c>
       <c r="C376" t="n">
@@ -5326,7 +5326,7 @@
       </c>
       <c r="B377" t="inlineStr">
         <is>
-          <t>['Ġya', 'ogan', 'Ġnumbers', 'Ġofficially', 'Ġused', 'Ġj', 'ian', 'bing', 'Ġdesign', 'ations', 'Ġlater', 'Ġclasses', 'Ġstill', 'Ġremains', 'Ġunknown', 'Ġpublic', 'Ġch', 'inese', 'Ġsynthetic', 'ap', 'ert', 'ure', 'Ġradar', 'ar', 'Ġch', 'inese', 'Ġp', 'iny', 'Ġh', 'Ã©', 'ch', 'Ã©', 'ng', 'Ġk', 'Ç', 'Ĵ', 'ng', 'j', 'Ã', '¬', 'ng', 'Ġl', 'Ã©', 'id', 'Ã¡', 'Ġsensor', 'Ġdevelopment', 'Ġbegan', 'Ġlate', 'Ġelectronic', 'Ġresearch', 'Ġinstitute', 'Ġch', 'ina', 'Ġacademy', 'Ġsciences', 'cas', 'Ġresulting', 'Ġtesting', 'Ġfirst', 'Ġairborne', 'Ġx', 'band', 'Ġmono', 'p', 'olar', 'ization', 'Ġsar', 'Ġcollection', 'Ġcas', 'Ġintroduced', 'Ġfirst', 'Ġoperational', 'Ġreal', 'time', 'Ġairborne', 'Ġsar', 'Ġsystem', 'Ġmonitor', 'Ġflooding', 'Ġtransmit', 'Ġcollected', 'Ġdata', 'Ġground', 'Ġstations', 'Ġpreliminary', 'Ġresearch', 'Ġdevelopment', 'Ġch', 'ina', "'s", 'Ġfirst', 'generation', 'Ġspace', 'based', 'Ġsar', 'Ġsystem', 'Ġbegan', 'Ġsometime', 'Ġdevelopment', 'Ġbeginning', 'Ġfull', 'Ġhigh', 'resolution', 'Ġspace', 'based', 'Ġsar', 'Ġcollection', 'bit', 'iously', 'Ġpursued', 'Ġpl', 'Ġpotential', 'Ġcontributions', 'weather', 'Ġtargeting', 'Ġnaval', 'Ġforces', 'ai', 'wan', 'Ġstra', 'Ġj', 'ian', 'bing', 'Ġseries', 'Ġsatellites', 'ab', 'bre', 'vi', 'ated', 'Ġch', 'ina', "'s", 'Ġfirst', 'Ġspace', 'based', 'Ġsynthetic', 'ap', 'ert', 'ure', 'Ġradar', 'ar', 'Ġsatellites', 'Ġfirst', 'Ġsatellites', 'Ġya', 'ogan', 'Ġprogram', 'Ġdevelopment', 'Ġproduction', 'Ġj', 'ian', 'bing', 'Ġseries', 'Ġsatellites', 'Ġentirely', 'Ġfunded', 'Ġpeople', "'s", 'Ġliberation', 'Ġarmy', 'pl', 'Ġability', 'Ġpenetrate', 'Ġseemingly', 'Ġconstant', 'Ġcloud', 'Ġcover', 'Ġpresent', 'Ġsouthern', 'Ġprovinces', 'ib', 'et', 'ich', 'uan', 'un', 'nan', 'Ġgu', 'ang', 'xi', 'Ġgu', 'g', 'ong', 'Ġha', 'Ġchallenges', 'Ġtraditional', 'Ġoptical', 'Ġcollection', 'Ġregions', 'Ġpl', 'Ġalso', 'Ġbelieves', 'Ġpotential', 'Ġwar', 'Ġsar', 'Ġcollection', 'Ġcapabilities', 'Ġvital', 'Ġinformation', 'Ġdominance', 'Ġmapping', 'Ġterrain', 'Ġidentifying', 'Ġtargets', 'Ġcloud', 'Ġcover', 'Ġrain', 'Ġfog', 'Ġdust', 'Ġpotentially', 'Ġmonitoring', 'Ġenemy', 'Ġsubmarines', 'Ġshallow', 'Ġwaters', 'Ġtargets', 'Ġsubter', 'ranean', 'Ġfacilities', 'Ġmay', 'Ġfinalized', 'Ġdesigns', 'Ġapproved', 'Ġdevelopment', 'Ġbegan', 'Ġearnest', 'Ġapproval', 'Ġstate', 'Ġscience', 'Ġtechnology', 'Ġcommittee', 'st', 'c', 'Ġcommission', 'Ġscience', 'Ġtechnology', 'Ġindustry', 'Ġnational', 'Ġdefense', 'cost', 'ind', ').[', 'Ġch', 'ina', 'Ġacademy', 'Ġscience', 'cas', 'Ġinstitute', 'Ġelectronics', 'Ġbuilt', 'Ġsar', 'Ġinstruments', 'Ġonboard', 'Ġj', 'ian', 'bing', 'Ġsatellites', 'Ġcraft', 'Ġdesigned']</t>
+          <t>['Ġinformation', 'Ġgiven', 'Ġimmediately', 'Ġcalling', 'Ġattention', 'Ġviolation', 'Ġwould', 'Ġcreate', 'Ġeven', 'Ġgreater', 'Ġsecurity', 'Ġrisk', 'Ġmonitor', 'Ġcall', 'Ġone', 'Ġbead', 'window', 'Ġcodes', 'Ġused', 'Ġaust', 'ral', 'ia', 'ada', 'Ġnew', 'Ġzeal', 'Ġunited', 'Ġkingdom', 'Ġunited', 'Ġstates', 'Ġnations', 'Ġworking', 'Ġprocedures', 'Ġstandard', 'Ġbead', 'window', 'Ġcodes', 'b', 'ead', 'window', '")', 'Ġinclude', 'Ġposition', 'Ġdisclosing', 'Ġinsecure', 'Ġinappropriate', 'Ġway', 'friendly', 'Ġenemy', 'Ġposition', 'Ġmovement', 'Ġintended', 'Ġmovement', 'Ġposition', 'Ġcourse', 'Ġspeed', 'Ġaltitude', 'Ġdestination', 'Ġair', 'Ġsea', 'Ġground', 'Ġelement', 'Ġunit', 'Ġforce', '."', 'Ġcapabilities', 'friendly', 'Ġenemy', 'Ġcapabilities', 'Ġlimitations', 'Ġforce', 'Ġcompositions', 'Ġsign', 'ï', '¬', 'ģ', 'c', 'ant', 'Ġcasualties', 'Ġspecial', 'Ġequipment', 'Ġweapons', 'Ġsystems', 'Ġsensors', 'Ġunits', 'Ġpersonnel', 'Ġpercentages', 'Ġfuel', 'Ġammunition', 'Ġremaining', '."', 'Ġoperations', 'friendly', 'Ġenemy', 'Ġoperation', 'Ġintentions', 'Ġprogress', 'Ġresults', 'Ġoperational', 'Ġlog', 'istic', 'Ġintentions', 'Ġmission', 'Ġparticipants', 'Ġï', '¬', 'Ĥ', 'ying', 'Ġprogrammes', 'Ġmission', 'Ġsituation', 'Ġreports', 'Ġresults', 'Ġfriendly', 'Ġenemy', 'Ġoperations', 'Ġassault', 'Ġobjectives', '."', 'Ġelectronic', 'Ġwarfare', 'ew', '):', 'friendly', 'Ġenemy', 'Ġelectronic', 'Ġwarfare', 'ew', 'Ġeman', 'ations', 'Ġcontrol', 'em', 'con', 'Ġintentions', 'Ġprogress', 'Ġresults', 'Ġintention', 'Ġemploy', 'Ġelectronic', 'Ġcounter', 'measures', 'Ġresults', 'Ġfriendly', 'Ġenemy', 'Ġobjectives', 'Ġresults', 'Ġfriendly', 'Ġenemy', 'Ġelectronic', 'Ġresults', 'Ġelectronic', 'Ġsupport', 'Ġmeasures', 'act', 'ical', 'Ġsig', 'int', 'esm', ');', 'Ġpresent', 'Ġintended', 'Ġem', 'con', 'Ġpolicy', 'Ġequipment', 'Ġaffected', 'Ġem', 'con', 'Ġpolicy', '."', 'Ġfriendly', 'Ġenemy', 'Ġkey', 'Ġpersonnel', 'move', 'ment', 'Ġidentity', 'Ġfriendly', 'Ġenemy', 'ï', '¬', 'ģ', 'cers', 'Ġvisitors', 'Ġcommanders', 'Ġmovement', 'Ġkey', 'Ġmaintenance', 'Ġpersonnel', 'Ġindicating', 'Ġequipment', 'Ġlimitations', '."', 'Ġcommunications', 'Ġsecurity', 'sec', '):', 'friendly', 'Ġenemy', 'sec', 'Ġbreaches', 'Ġlinkage', 'Ġcodes', 'Ġcod', 'ew', 'ords', 'Ġplain', 'Ġlanguage', 'Ġcompromise', 'Ġchanging', 'Ġfrequencies', 'Ġlinkage', 'Ġline', 'Ġnumber', 'circ', 'uit', 'Ġdesign', 'ators', 'Ġlinkage', 'Ġchanging', 'Ġcall', 'Ġsigns', 'Ġprevious', 'Ġcall', 'Ġsigns', 'Ġunits', 'Ġcompromise', 'Ġencrypted', 'class', 'ï', '¬', 'ģ', 'ed', 'Ġcall', 'Ġsigns', 'Ġincorrect', 'Ġauthentication', 'Ġprocedure', '."', 'Ġwrong', 'Ġcircuit', 'appropriate', 'Ġtransmission', 'Ġinformation', 'Ġrequested', 'Ġtransmitted', 'Ġtransmitted', 'Ġpassed', 'Ġsubject', 'Ġcircuit', 'Ġeither', 'Ġrequires', 'Ġgreater', 'Ġsecurity', 'Ġprotection', 'Ġappropriate', 'Ġpurpose', 'Ġcircuit', 'Ġprovided', '."', 'Ġcodes', 'Ġappropriate']</t>
         </is>
       </c>
       <c r="C377" t="n">
@@ -5339,7 +5339,7 @@
       </c>
       <c r="B378" t="inlineStr">
         <is>
-          <t>['Ġsh', 'ghai', 'Ġacademy', 'Ġspace', 'flight', 'Ġtechnology', 'ast', 'Ġalso', 'Ġdevelops', 'Ġlong', 'Ġmarch', 'Ġlaunch', 'Ġvehicle', 'Ġdevelopers', 'Ġinvolved', 'Ġproject', 'Ġch', 'ina', 'Ġacademy', 'Ġspace', 'Ġtechnology', 'cast', 'th', 'Ġspace', 'Ġacademy', 'st', 'th', 'Ġinstit', 'utes', 'Ġch', 'ina', 'Ġelectronics', 'Ġtechnology', 'Ġgroup', 'Ġcorporation', 'c', 'etc', ")'", 'Ġnan', 'jing', 'Ġresearch', 'Ġinstitute', 'Ġelectronic', 'Ġtechnology', 'known', 'Ġalso', 'th', 'Ġinstitute', 'Ġsouthwest', 'Ġinstitute', 'Ġelectronic', 'Ġequipment', 'sw', 'ie', 'e', 'th', 'Ġinstitute', 'ijing', 'Ġuniversity', 'Ġaer', 'aut', 'ics', 'Ġastronaut', 'ics', 'ast', 'Ġalso', 'Ġdeveloper', 'Ġf', 'eng', 'un', 'Ġseries', 'Ġweather', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġsatellites', 'Ġbuilt', 'Ġsh', 'ghai', 'Ġacademy', 'Ġspace', 'flight', 'Ġtechnology', 'ast', 'Ġlaunched', 'Ġsatellite', 'Ġlaunch', 'Ġcenter', 'Ġprovide', 'Ġmilitary', 'Ġanalysts', 'Ġsynthetic', 'rad', 'ar', 'Ġimagery', 'Ġpurportedly', 'Ġspatial', 'Ġresolution', 'Ġsharp', 'Ġmeters', 'Ġl', 'band', 'âĢĵ', 'Ġsatellites', 'Ġconfirmed', 'Ġelectronic', 'Ġmotor', 'powered', 'Ġsolar', 'Ġpanel', 'Ġexpanded', 'Ġcontracted', 'Ġground', 'Ġcontrol', 'Ġstation', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġsatellites', 'Ġreported', 'Ġmass', 'Ġkilograms', 'Ġorbital', 'Ġinclination', 'Ġapproximately', 'Â°', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġtwo', 'Ġoperational', 'Ġsatellites', 'Ġenjoys', 'Ġtwice', 'Ġdaily', 'Ġrevisit', 'Ġrate', 'Â°', 'Ġviewing', 'Ġangle', 'Ġapr', 'il', 'Ġaug', 'ust', 'Ġch', 'ina', 'Ġlaunched', 'Ġthree', 'Ġj', 'ian', 'bing', 'Ġsar', 'Ġsatellites', 'Ġlast', 'Ġtwo', 'Ġremain', 'Ġoperation', 'Ġya', 'ogan', 'Ġlaunched', 'Ġapr', 'il', 'Ġreportedly', 'Ġbroke', 'Ġaround', 'Ġfe', 'b', 'ruary', 'Ġalmost', 'Ġfour', 'Ġyears', 'Ġlaunch', 'Ġdue', 'Ġsmall', 'Ġnumber', 'Ġpieces', 'Ġlow', 'Ġorbital', 'Ġspeeds', 'Ġbreakup', 'Ġlikely', 'Ġdue', 'Ġinternal', 'Ġexplosion', 'Ġhigh', 'speed', 'Ġcollision', 'Ġya', 'ogan', 'Ġlaunched', 'mber', 'Ġsimilar', 'Ġorbit', 'Ġappears', 'Ġmodern', 'ized', 'Ġsuccessor', 'Ġj', 'ian', 'bing', 'Ġseries', 'Ġsar', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġya', 'ogan', 'Ġsatellites', 'Ġmilitary', 'Ġdesign', 'ations', 'Ġbeginning', 'Ġch', 'inese', 'Ġmilitary', 'Ġradar', 'Ġreconnaissance', 'Ġsatellites', 'Ġbuilt', 'ast', 'Ġorbital', 'Ġperiod', 'Ġminutes', 'Ġside', 'looking', 'Ġradar', 'Ġsystem', 'Ġdesigned', 'Ġinstitute', 'Ġelectronics', 'Ġch', 'inese', 'Ġacademy', 'Ġsciences', 'Ġj', 'uly', 'Ġch', 'ina', 'Ġlaunched', 'Ġfour', 'Ġj', 'ian', 'bing', 'Ġradar']</t>
+          <t>['Ġsituation', 'Ġmay', 'Ġde', 'ï', '¬', 'ģ', 'ned', 'Ġcommander', 'Ġexample', 'Ġj', 'apan', 'ese', 'Ġnavy', 'Ġpoor', 'Ġpractice', 'Ġidentified', 'Ġkey', 'Ġperson', "'s", 'Ġmovement', 'Ġlow', 'security', 'Ġcrypt', 'os', 'ystem', 'Ġmade', 'Ġpossible', 'Ġoperation', 'Ġvengeance', 'Ġinterception', 'Ġdeath', 'Ġcombined', 'Ġfleet', 'Ġcommander', 'Ġadm', 'iral', 'oku', 'amoto', 'Ġmonitoring', 'Ġfriendly', 'Ġcommunications', 'Ġelectronic', 'Ġsignals', 'Ġintelligence', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġelectronic', 'Ġsignals', 'Ġintelligence', 'el', 'int', 'Ġrefers', 'Ġuse', 'Ġelectronic', 'Ġsensors', 'Ġprimary', 'Ġfocus', 'Ġlies', 'Ġnon', 'communications', 'Ġsignals', 'Ġintelligence', 'Ġjoint', 'Ġchiefs', 'Ġstaff', 'Ġdefine', 'technical', 'Ġge', 'ol', 'ocation', 'Ġintelligence', 'Ġderived', 'Ġforeign', 'Ġnon', 'communications', 'Ġelectromagnetic', 'Ġradi', 'ations', 'Ġemanating', 'Ġsources', 'Ġnuclear', 'Ġdeton', 'ations', 'Ġradioactive', 'Ġsources', '."[', 'Ġsignal', 'Ġidentification', 'Ġperformed', 'Ġanalyzing', 'Ġcollected', 'Ġparameters', 'Ġspecific', 'Ġsignal', 'Ġeither', 'Ġmatching', 'Ġknown', 'Ġcriteria', 'Ġrecording', 'Ġpossible', 'Ġnew', 'Ġem', 'itter', 'Ġel', 'int', 'Ġdata', 'Ġusually', 'Ġhighly', 'Ġclassified', 'Ġprotected', 'Ġdata', 'Ġgathered', 'Ġtypically', 'Ġpertinent', 'Ġelectronics', 'Ġopponent', "'s", 'Ġdefense', 'Ġnetwork', 'Ġespecially', 'Ġelectronic', 'Ġparts', 'Ġrad', 'ars', 'Ġsurface', 'air', 'Ġmissile', 'Ġsystems', 'Ġaircraft', 'Ġetc', 'Ġel', 'int', 'Ġused', 'Ġdetect', 'Ġships', 'Ġaircraft', 'Ġradar', 'Ġelectromagnetic', 'Ġradiation', 'Ġcommanders', 'Ġmake', 'Ġchoices', 'Ġusing', 'Ġradar', 'em', 'con', 'Ġintermitt', 'ently', 'Ġusing', 'Ġusing', 'Ġexpecting', 'Ġavoid', 'Ġdefenses', 'Ġel', 'int', 'Ġcollected', 'Ġground', 'Ġstations', 'Ġnear', 'Ġopponent', "'s", 'Ġterritory', 'Ġships', 'Ġcoast', 'Ġaircraft', 'Ġnear', 'Ġairspace', 'Ġsatellite', 'Ġcombining', 'Ġsources', 'Ġinformation', 'Ġel', 'int', 'Ġallows', 'Ġtraffic', 'Ġanalysis', 'Ġperformed', 'Ġelectronic', 'Ġemissions', 'Ġcontain', 'Ġhuman', 'Ġencoded', 'Ġmessages', 'Ġmethod', 'Ġanalysis', 'Ġdiffers', 'Ġsig', 'int', 'Ġhuman', 'Ġencoded', 'Ġmessage', 'Ġelectronic', 'Ġtransmission', 'Ġanalyzed', 'Ġel', 'int', 'Ġinterest', 'Ġtype', 'Ġelectronic', 'Ġtransmission', 'Ġlocation', 'Ġexample', 'Ġbattle', 'l', 'antic', 'Ġworld', 'Ġwar', 'Ġultra', 'int', 'Ġalways', 'Ġavailable', 'Ġb', 'let', 'ch', 'ley', 'Ġpark', 'Ġalways', 'Ġable', 'Ġread', 'Ġu', 'boat', 'Ġen', 'igma', 'Ġtraffic', 'Ġhigh', 'frequency', 'Ġdirection', 'Ġfinding', 'Ġstill', 'Ġable', 'Ġdetect', 'Ġu', 'boats', 'Ġanalysis', 'Ġradio', 'Ġtransmissions', 'Ġpositions', 'Ġtri', 'ang', 'ulation', 'Ġdirection', 'Ġlocated', 'Ġtwo', 'Ġsystems', 'Ġadm', 'ir']</t>
         </is>
       </c>
       <c r="C378" t="n">
@@ -5352,7 +5352,7 @@
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>['Ġsatellites', 'Ġfirst', 'Ġlaunched', 'Ġapr', 'il', 'Ġlatest', 'mber', 'Ġmass', 'Ġkilograms', 'Ġpounds', 'Ġthird', 'Ġsatellite', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġlaunched', 'Ġoct', 'ober', 'Ġorbit', 'Ġlowered', 'Ġapr', 'il', 'Ġj', 'uly', 'Ġconsequently', 'Ġunderwent', 'Ġuncontrolled', 'Ġdecay', 'ent', 'ering', 'Ġatmosphere', 'Ġclasses', 'Ġsynthetic', 'ap', 'ert', 'ure', 'Ġradar', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġlaunch', 'mber', 'Ġalthough', 'Ġj', 'ian', 'bing', 'Ġdesignation', 'Ġstill', 'Ġunknown', 'Ġlatest', 'Ġclass', 'Ġsar', 'Ġreconnaissance', 'Ġsatellites', 'Ġch', 'ina', 'Ġlaunched', 'Ġthree', 'Ġsatellites', 'Ġmodern', 'ized', 'Ġsuccessor', 'Ġclass', 'Ġj', 'ian', 'bing', 'Ġj', 'ian', 'bing', 'Ġclasses', 'Ġsar', 'Ġreconnaissance', 'Ġsatellites', 'Ġclass', 'Ġuses', 'Ġorbit', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġlikely', 'Ġdifferent', 'Ġdesign', 'Ġaccording', 'Ġpublished', 'Ġillustrations', 'Ġsecond', 'Ġsatellite', 'Ġclass', 'Ġya', 'ogan', 'Ġfailed', 'Ġreach', 'Ġorbit', 'Ġmay', 'Ġlikely', 'Ġreplacement', 'Ġya', 'ogan', 'r', 'Ġlaunched', 'Ġyear', 'Ġhalf', 'Ġlater', 'Ġused', 'Ġdifferent', 'Ġlaunch', 'Ġsite', 'Ġinstead', 'Ġhigher', 'Ġorbit', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġya', 'ogan', 'Ġsatellites', 'Ġmilitary', 'Ġdesign', 'ations', 'Ġbeginning', 'Ġprovides', 'Ġch', 'inese', 'Ġmilitary', 'Ġoptical', 'Ġimaging', 'Ġcapabilities', 'Ġcompliment', 'Ġj', 'ian', 'bing', 'Ġclass', "'s", 'Ġsar', 'Ġreconnaissance', 'Ġcapabilities', 'Ġreported', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġresolution', 'Ġmeters', 'Ġj', 'ian', 'bing', 'Ġsatellites', 'Ġdeveloped', 'Ġcast', 'Ġbased', 'Ġcast', 'Ġsatellites', 'Ġbus', 'Ġoriginally', 'Ġdeveloped', 'Ġch', 'ina', 'Ġspaces', 'Ġcompany', 'Ġj', 'ian', 'bing', 'Ġsatellites', 'Ġimage', 'Ġearth', 'Ġspatial', 'Ġresolution', 'Ġapproximately', 'Ġmeters', 'Ġtransmit', 'Ġvia', 'Ġx', 'band', 'Ġreceiving', 'Ġtele', 'metry', 'Ġtracking', 'Ġcommand', 'Ġsignals', 'band', 'Ġj', 'uly', 'Ġch', 'ina', 'Ġindividually', 'Ġlaunched', 'Ġya', 'ogan', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġfirst', 'Ġsatellite', 'Ġlaunched', 'Ġmay', 'Ġlatest', 'Ġmay', 'Ġbol', 'iv', 'ian', 'Ġagency', 'Ġspace', 'Ġactivities', 'Ġsigned', 'Ġus', 'Ġmillion', 'Ġdeal', 'Ġch', 'ina', 'Ġgreat', 'Ġwall', 'Ġindustries', 'Ġco', 'Ġlaunch', 'Ġv', 'enezuel', 'Ġremote', 'ensing', 'Ġsatellite', 'Ġmay', 'Ġmarking', 'Ġch', 'ina', "'s", 'Ġfirst', 'Ġexport']</t>
+          <t>['alty', 'Ġable', 'Ġuse', 'Ġinformation', 'Ġplot', 'Ġcourses', 'Ġtook', 'Ġconv', 'oys', 'Ġaway', 'Ġhigh', 'Ġconcentrations', 'Ġu', 'boats', 'Ġel', 'int', 'Ġdisciplines', 'Ġinclude', 'Ġintercept', 'ing', 'Ġanalyzing', 'Ġenemy', 'Ġweapons', 'Ġcontrol', 'Ġsignals', 'Ġidentification', 'Ġfriend', 'Ġfoe', 'Ġresponses', 'Ġtrans', 'p', 'ond', 'ers', 'Ġaircraft', 'Ġused', 'Ġdistinguish', 'Ġenemy', 'Ġcraft', 'Ġfriendly', 'Ġones', 'Ġcommon', 'Ġarea', 'Ġel', 'int', 'Ġintercept', 'ing', 'Ġrad', 'ars', 'Ġlearning', 'Ġlocations', 'Ġoperating', 'Ġprocedures', 'Ġattacking', 'Ġforces', 'Ġmay', 'Ġable', 'Ġavoid', 'Ġcoverage', 'Ġcertain', 'Ġrad', 'ars', 'Ġknowing', 'Ġcharacteristics', 'Ġelectronic', 'Ġwarfare', 'Ġunits', 'Ġmay', 'Ġjam', 'Ġrad', 'ars', 'Ġsend', 'Ġdeceptive', 'Ġsignals', 'Ġconfusing', 'Ġradar', 'Ġelectronically', 'Ġcalled', 'soft', 'Ġkill', '",', 'Ġmilitary', 'Ġunits', 'Ġalso', 'Ġsend', 'Ġspecialized', 'Ġmissiles', 'Ġrad', 'ars', 'Ġbomb', 'Ġget', 'hard', 'Ġkill', '".', 'Ġmodern', 'Ġair', 'air', 'Ġmissiles', 'Ġalso', 'Ġradar', 'Ġh', 'oming', 'Ġguidance', 'Ġsystems', 'Ġparticularly', 'Ġuse', 'Ġlarge', 'Ġairborne', 'Ġrad', 'ars', 'Ġknowing', 'Ġsurface', 'air', 'Ġmissile', 'Ġanti', 'air', 'craft', 'Ġartillery', 'Ġsystem', 'Ġtype', 'Ġmeans', 'Ġair', 'Ġraids', 'Ġplotted', 'Ġavoid', 'Ġheavily', 'Ġdefended', 'Ġareas', 'Ġfly', 'Ġflight', 'Ġprofile', 'Ġgive', 'Ġaircraft', 'Ġbest', 'Ġchance', 'Ġev', 'ading', 'Ġground', 'Ġfire', 'Ġfighter', 'Ġpatrols', 'Ġalso', 'Ġallows', 'Ġjam', 'ming', 'Ġspoof', 'ing', 'Ġenemy', "'s", 'Ġdefense', 'Ġnetwork', 'see', 'Ġelectronic', 'Ġwarfare', 'Ġgood', 'Ġelectronic', 'Ġintelligence', 'Ġimportant', 'Ġstealth', 'Ġoperations', 'Ġstealth', 'Ġaircraft', 'Ġtotally', 'Ġundet', 'ect', 'able', 'Ġneed', 'Ġknow', 'Ġareas', 'Ġavoid', 'Ġsimilarly', 'Ġconventional', 'Ġaircraft', 'Ġneed', 'Ġknow', 'Ġfixed', 'Ġsemi', 'mobile', 'Ġair', 'Ġdefense', 'Ġsystems', 'Ġshut', 'Ġfly', 'Ġaround', 'Ġcomplementary', 'Ġrelationship', 'int', 'Ġrole', 'Ġair', 'Ġwarfare', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġelectronic', 'Ġsupport', 'Ġmeasures', 'esm', 'Ġelectronic', 'Ġsurveillance', 'Ġmeasures', 'Ġel', 'int', 'Ġtechniques', 'Ġusing', 'Ġvarious', 'Ġelectronic', 'Ġsurveillance', 'Ġsystems', 'Ġterm', 'Ġused', 'Ġspecific', 'Ġcontext', 'Ġtactical', 'Ġwarfare', 'Ġes', 'Ġgive', 'Ġinformation', 'Ġneeded', 'Ġelectronic', 'Ġattack', 'ea', 'Ġjam', 'ming', 'Ġdirectional', 'Ġbearings', 'comp', 'ass', 'Ġangle', 'Ġtarget', 'Ġsignals', 'Ġintercept', 'Ġradio', 'Ġdirection', 'Ġfinding', 'rd', 'f', 'Ġsystems', 'Ġcritically', 'Ġimportant', 'Ġworld', 'Ġwar', 'Ġbattle', 'l', 'antic', 'Ġr', 'df', 'Ġoriginally', 'Ġapplied', 'Ġcommunications', 'Ġbroad', 'ened', 'Ġsystems', 'Ġalso', 'Ġtake', 'Ġel', 'int', 'Ġradar', 'Ġbandwidth', 'Ġlower', 'Ġfrequency', 'Ġcommunications', 'Ġsystems']</t>
         </is>
       </c>
       <c r="C379" t="n">
@@ -5365,7 +5365,7 @@
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>['Ġreconnaissance', 'Ġsatellite', 'Ġbased', 'Ġdesign', 'Ġj', 'ian', 'bing', 'Ġsatellites', 'Ġlaunched', 'Ġse', 'pt', 'ember', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġya', 'ogan', 'Ġsatellites', 'Ġmilitary', 'Ġdesign', 'ations', 'Ġbeginning', 'Ġprovides', 'Ġch', 'inese', 'Ġmilitary', 'Ġoptical', 'Ġimaging', 'Ġcapabilities', 'Ġlikely', 'Ġsuccessor', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġthought', 'Ġorbit', 'Ġmuch', 'Ġhigher', 'Ġaltitude', 'Ġindicating', 'Ġsatellites', 'Ġclass', 'Ġlower', 'resolution', 'Ġmapping', 'Ġarea', 'Ġsurveillance', 'Ġoptical', 'Ġpayload', 'Ġya', 'ogan', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġdeveloped', 'Ġchang', 'ch', 'un', 'Ġinstitute', 'Ġoptics', 'Ġfine', 'Ġmechanics', 'Ġphysics', 'Ġch', 'ina', 'Ġlaunched', 'Ġfive', 'Ġindividual', 'Ġya', 'ogan', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġfirst', 'Ġlaunched', 'Ġde', 'cember', 'Ġlatest', 'Ġaug', 'ust', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġya', 'ogan', 'Ġsatellites', 'Ġmilitary', 'Ġdesign', 'ations', 'Ġbeginning', 'Ġprovides', 'Ġch', 'inese', 'Ġmilitary', 'Ġoptical', 'Ġimaging', 'Ġcapabilities', 'Ġbelieved', 'Ġalso', 'Ġbased', 'Ġcast', 'Ġsatellite', 'Ġbus', 'Ġlike', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġthree', 'Ġj', 'ian', 'bing', 'class', 'Ġsatellites', 'Ġbuilt', 'Ġcast', 'Ġcarrying', 'Ġoptical', 'Ġimaging', 'Ġsystem', 'Ġx', 'ian', 'Ġinstitute', 'Ġoptics', 'Ġprecision', 'Ġmechanics', 'Ġindividually', 'Ġlaunched', 'Ġfirst', 'Ġlaunched', 'Ġde', 'cember', 'Ġreported', 'Ġlast', 'Ġclass', 'Ġse', 'pt', 'ember', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġya', 'ogan', 'Ġsatellites', 'Ġmilitary', 'Ġdesign', 'ations', 'Ġbeginning', 'Ġprovides', 'Ġch', 'inese', 'Ġmilitary', 'Ġoptical', 'Ġimaging', 'Ġcapabilities', 'Ġmay', 'Ġch', 'ina', 'Ġlaunched', 'Ġtwo', 'Ġindividually', 'Ġlaunched', 'Ġya', 'ogan', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġfirst', 'Ġlaunched', 'Ġmay', 'Ġlatest', 'mber', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġya', 'ogan', 'Ġsatellites', 'Ġmilitary', 'Ġdesign', 'ations', 'Ġbeginning', 'Ġmilitary', 'Ġoptical', 'Ġreconnaissance', 'Ġsatellites', 'Ġresponse', 'ai', 'wan', 'ese', 'Ġpresident', 'Ġle', 'e', 'eng', 'h', 'ui', "'s", 'Ġvisit', 'Ġunited', 'Ġstates', 'Ġpr', 'c', 'Ġinitiated', 'Ġthird', 'ai', 'wan', 'Ġstra', 'Ġcrisis', 'Ġconducting', 'Ġhigh', 'profile', 'Ġmissile', 'Ġtests', 'Ġamphib', 'ious', 'Ġlanding', 'Ġdrills', 'Ġtroop', 'Ġstaging', 'Ġprovince', 'Ġacross', 'Ġstra', 'Ġisland', 'ai', 'wan', 'Ġunited', 'Ġstates', 'Ġgovernment', 'Ġresponded', 'Ġpr', 'c', "'s", 'Ġescalation', 'Ġdeploying', 'Ġlargest', 'Ġameric', 'Ġshow', 'Ġforce']</t>
+          <t>['Ġgiving', 'Ġbirth', 'Ġfamily', 'Ġn', 'ato', 'Ġes', 'Ġsystems', 'Ġship', 'board', 'Ġus', 'Ġsystems', 'Ġcomparable', 'Ġairborne', 'Ġunits', 'Ġe', 'Ġalso', 'Ġcalled', 'Ġelectronic', 'Ġcounter', 'measures', 'Ġes', 'Ġprovides', 'Ġinformation', 'Ġneeded', 'Ġelectronic', 'Ġcounter', 'counter', 'Ġmeasures', 'Ġunderstanding', 'Ġspoof', 'ing', 'Ġjam', 'ming', 'Ġmode', 'Ġone', 'Ġchange', 'Ġone', "'s", 'Ġradar', 'Ġcharacteristics', 'Ġavoid', 'acon', 'ing', 'Ġcombined', 'Ġintelligence', 'Ġelectronic', 'Ġwarfare', 'Ġlearning', 'Ġcharacteristics', 'Ġenemy', 'Ġnavigation', 'Ġaids', 'Ġradio', 'acons', 'Ġret', 'rans', 'mitting', 'Ġincorrect', 'Ġinformation', 'Ġf', 'int', 'foreign', 'Ġinstrument', 'ation', 'Ġsignals', 'Ġintelligence', 'Ġsub', 'category', 'Ġsig', 'int', 'Ġmonitoring', 'Ġprimarily', 'Ġnon', 'human', 'Ġcommunication', 'Ġforeign', 'Ġinstrument', 'ation', 'Ġsignals', 'Ġinclude', 'Ġlimited', 'Ġtele', 'metry', 'tel', 'int', 'Ġtracking', 'Ġsystems', 'Ġvideo', 'Ġdata', 'Ġlinks', 'Ġtel', 'int', 'Ġimportant', 'Ġpart', 'Ġnational', 'Ġmeans', 'Ġtechnical', 'Ġverification', 'Ġarms', 'Ġcontrol', 'Ġstill', 'Ġresearch', 'Ġlevel', 'Ġtechniques', 'Ġdescribed', 'Ġcounter', 'el', 'int', 'Ġwould', 'Ġpart', 'Ġse', 'ad', 'Ġcampaign', 'Ġmay', 'Ġinformative', 'Ġcompare', 'Ġcontrast', 'Ġcounter', 'el', 'int', 'Ġsignals', 'Ġintelligence', 'Ġmeasurement', 'Ġsignature', 'Ġintelligence', 'mas', 'int', 'Ġclosely', 'Ġsometimes', 'Ġconfusing', 'ly', 'Ġrelated', 'Ġsignals', 'Ġintelligence', 'Ġdisciplines', 'Ġcommunications', 'Ġelectronic', 'Ġintelligence', 'Ġfocus', 'Ġinformation', 'Ġsignals', 'int', 'Ġdetecting', 'Ġspeech', 'Ġvoice', 'Ġcommunication', 'Ġel', 'int', 'Ġmeasuring', 'Ġfrequency', 'Ġpulse', 'Ġrepetition', 'Ġrate', 'Ġcharacteristics', 'Ġradar', 'Ġmas', 'int', 'Ġalso', 'Ġworks', 'Ġcollected', 'Ġsignals', 'Ġanalysis', 'Ġdiscipline', 'Ġhowever', 'Ġunique', 'Ġmas', 'int', 'Ġsensors', 'Ġtypically', 'Ġworking', 'Ġdifferent', 'Ġregions', 'Ġdomains', 'Ġelectromagnetic', 'Ġspectrum', 'Ġinfrared', 'Ġmagnetic', 'Ġfields', 'Ġn', 'sa', 'Ġagencies', 'Ġmas', 'int', 'Ġgroups', 'Ġcentral', 'Ġmas', 'int', 'Ġoffice', 'Ġdefense', 'Ġintelligence', 'Ġagency', 'ia', 'Ġel', 'int', 'Ġes', 'Ġel', 'int', 'acon', 'ing', 'Ġforeign', 'Ġinstrument', 'ation', 'Ġsignals', 'Ġintelligence', 'Ġcounter', 'el', 'int', 'Ġsig', 'int', 'Ġversus', 'Ġmas', 'int', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġmodel', 'Ġg', 'erman', 'Ġsar', 'lu', 'pe', 'Ġreconnaissance', 'Ġsatellite', 'Ġinside', 'v', 'iet', 'Ġcosmos', 'Ġrocket', 'int', 'Ġel', 'int', 'Ġfocus', 'Ġintentionally', 'Ġtransmitted', 'Ġpart', 'Ġsignal', 'Ġmas', 'int', 'Ġfocuses', 'Ġunintentionally', 'Ġtransmitted', 'Ġinformation', 'Ġexample', 'Ġgiven', 'Ġradar', 'Ġantenna', 'Ġsidel', 'ob', 'es', 'Ġemanating', 'Ġdirection']</t>
         </is>
       </c>
       <c r="C380" t="n">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="B381" t="inlineStr">
         <is>
-          <t>['Ġsince', 'Ġv', 'iet', 'nam', 'Ġwar', 'Ġincluding', 'Ġsending', 'Ġtwo', 'Ġameric', 'Ġcarrier', 'Ġbattle', 'Ġgroups', 'Ġeffectively', 'Ġforced', 'Ġpr', 'c', 'Ġsince', 'Ġpl', 'Ġcommitted', 'Ġdesign', 'Ġfield', 'Ġadvanced', 'Ġant', 'ish', 'ip', 'Ġmissile', 'Ġsystems', 'Ġincluding', 'ong', 'Ġf', 'eng', 'Ġdeployed', 'Ġnearly', 'Ġsixty', 'Ġmaritime', 'Ġsurveillance', 'Ġsatellites', 'Ġusing', 'Ġelectronic', 'Ġintelligence', 'el', 'int', 'Ġlocate', 'Ġidentify', 'Ġtrack', 'Ġadvers', 'arial', 'Ġvessels', 'Ġsupport', 'Ġtargeting', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġya', 'ogan', 'Ġsatellites', 'Ġmilitary', 'Ġdesign', 'ations', 'Ġbeginning', 'Ġconsist', 'Ġone', 'Ġprimary', 'Ġsatellite', 'Ġtwo', 'Ġsub', 'atell', 'ites', 'Ġlaunched', 'Ġtriple', 'ts', 'Ġsatellites', 'Ġreportedly', 'Ġperform', 'Ġocean', 'Ġnaval', 'Ġsurveillance', 'Ġmission', 'Ġsimilar', 'Ġunited', 'Ġstates', 'Ġnaval', 'Ġocean', 'Ġsurveillance', 'Ġsystem', 'n', 'oss', 'Ġpar', 'c', 'ae', 'Ġdespite', 'Ġch', 'inese', 'Ġstate', 'media', "'s", 'Ġinsistence', 'Ġdesigned', 'conduct', 'Ġelectromagnetic', 'Ġenvironmental', 'Ġmonitoring', 'Ġrelated', 'Ġtechnology', 'Ġtests', '".[', 'Ġtriple', 'Ġgroups', 'Ġlikely', 'Ġfly', 'Ġloose', 'Ġformation', 'Ġlocate', 'Ġradio', 'Ġemit', 'ters', 'Ġusing', 'Ġdifference', 'Ġtime', 'Ġarrival', 'Ġradio', 'Ġsignals', 'Ġdifferent', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġsatellites', 'Ġbased', 'Ġcast', 'Ġsatellites', 'Ġbus', 'Ġmass', 'Ġkilograms', 'Ġpounds', 'Ġorbital', 'Ġperiod', 'Ġminutes', 'Ġle', 'Ġmay', 'Ġnine', 'Ġlaunches', 'Ġj', 'ian', 'bing', 'Ġtriple', 'ts', 'tw', 'enty', 'seven', 'Ġtotal', 'Ġsatellites', 'Ġfirst', 'Ġtriple', 'Ġlaunching', 'Ġmarch', 'Ġlatest', 'Ġmarch', 'Ġelectro', 'opt', 'ical', 'Ġelectronic', 'Ġintelligence', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġch', 'u', 'ang', 'x', 'sim', 'pl', 'ified', 'Ġch', 'inese', 'Ġå', 'Ī', 'Ľ', 'æĸ', '°', 'Ġtraditional', 'Ġch', 'inese', 'Ġå', 'ī', 'µ', 'æĸ', '°', 'Ġp', 'iny', 'Ġlit', 'inn', 'ovation', "')", 'Ġclass', 'Ġsatellites', 'Ġknown', 'Ġya', 'ogan', 'Ġsatellites', 'Ġlaunched', 'Ġx', 'ich', 'ang', 'Ġstill', 'Ġlargely', 'Ġshrouded', 'Ġsecrecy', 'Ġpurpose', 'Ġspeculated', 'Ġel', 'int', 'Ġnature', 'Ġtriple', 'Ġlaunches', 'Ġsimilar', 'Ġsatellites', 'Ġj', 'ian', 'bing', 'Ġclass', 'Ġname', 'Ġmilitary', 'Ġdesignation', 'Ġlaunch', 'Ġfunction', 'Ġorbit', 'Ġorbital', 'ps', 'Ġinclination', 'Ġcos', 'par', 'id', 'Ġya', 'ogan', 'Ġapr', 'il', 'Ġsar', 'Â°', '09', '015', 'Ġya', 'ogan', 'Ġmay', 'Ġe']</t>
+          <t>['Ġmain', 'Ġantenna', 'Ġaimed', 'Ġrad', 'int', 'rad', 'ar', 'Ġintelligence', 'Ġdiscipline', 'Ġinvolves', 'Ġlearning', 'Ġrecognize', 'Ġradar', 'Ġprimary', 'Ġsignal', 'Ġcaptured', 'Ġel', 'int', 'Ġsidel', 'ob', 'es', 'Ġperhaps', 'Ġcaptured', 'Ġmain', 'Ġel', 'int', 'Ġsensor', 'Ġlikely', 'Ġsensor', 'Ġaimed', 'Ġsides', 'Ġradio', 'Ġantenna', 'Ġmas', 'int', 'Ġassociated', 'int', 'Ġmight', 'Ġinvolve', 'Ġdetection', 'Ġcommon', 'Ġbackground', 'Ġsounds', 'Ġexpected', 'Ġhuman', 'Ġvoice', 'Ġcommunications', 'Ġexample', 'Ġgiven', 'Ġradio', 'Ġsignal', 'Ġcomes', 'Ġradio', 'Ġused', 'Ġtank', 'Ġintercept', 'Ġhear', 'Ġengine', 'Ġnoise', 'Ġhigher', 'Ġvoice', 'Ġfrequency', 'Ġvoice', 'Ġmodulation', 'Ġusually', 'Ġuses', 'Ġeven', 'Ġthough', 'Ġvoice', 'Ġconversation', 'Ġmeaningful', 'Ġmas', 'int', 'Ġmight', 'Ġsuggest', 'Ġdeception', 'Ġcoming', 'Ġreal', 'Ġtank', 'Ġsee', 'Ġdiscussion', 'Ġsig', 'int', 'capt', 'ured', 'Ġinformation', 'Ġmas', 'int', 'Ġflavor', 'Ġdetermining', 'Ġfrequency', 'Ġreceiver', 'Ġtuned', 'Ġdetecting', 'Ġfrequency', 'Ġbeat', 'Ġfrequency', 'Ġoscill', 'ator', 'Ġsuper', 'heter', 'ody', 'ne', 'Ġreceiver', 'Ġsince', 'Ġinvention', 'Ġradio', 'Ġinternational', 'Ġconsensus', 'Ġradio', 'waves', 'Ġone', "'s", 'Ġproperty', 'Ġthus', 'Ġinterception', 'Ġillegal', 'Ġhowever', 'Ġnational', 'Ġlaws', 'Ġallowed', 'Ġcollect', 'Ġstore', 'Ġprocess', 'Ġradio', 'Ġtraffic', 'Ġpurposes', 'Ġmonitoring', 'Ġtraffic', 'Ġcables', 'e', 'Ġtelephone', 'Ġinternet', 'Ġfar', 'Ġcontroversial', 'Ġsince', 'Ġtime', 'Ġrequires', 'Ġphysical', 'Ġaccess', 'Ġcable', 'Ġthereby', 'Ġviolating', 'Ġownership', 'Ġexpected', 'Ġprivacy', 'Ġcentral', 'Ġintelligence', 'Ġagency', 'Ġdirector', 'ate', 'Ġscience', 'Ġtechnology', 'Ġco', 'intel', 'pro', 'Ġe', 'che', 'lon', 'Ġforeign', 'Ġintelligence', 'Ġsurveillance', 'Ġact', 'Ġamendments', 'Ġact', 'Ġge', 'osp', 'atial', 'Ġintelligence', 'Ġhuman', 'Ġintelligence', 'esp', 'ionage', 'Ġimagery', 'Ġintelligence', 'Ġintelligence', 'Ġbranch', 'adian', 'Ġforces', 'Ġlist', 'Ġintelligence', 'Ġgathering', 'Ġdisciplines', 'Ġlistening', 'Ġstation', 'Ġopen', 'source', 'Ġintelligence', 'Ġradio', 'Ġreconnaissance', 'Ġplatoon', 'Ġr', 'af', 'Ġintelligence', 'Ġsignals', 'Ġintelligence', 'Ġalliances', 'Ġnations', 'Ġindustries', 'Ġsignals', 'Ġintelligence', 'Ġoperational', 'Ġplatforms', 'Ġnation', 'Ġcurrent', 'Ġcollection', 'Ġsystems', 'Ġlegality', 'Ġsee', 'Ġalso', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'ot', 'Ġtemp', 'est', 'Ġus', 'Ġsignals', 'Ġintelligence', 'Ġcold', 'Ġwar', 'Ġven', 'ona', 'Ġz', 'ir', 'con', 'Ġsatellite', 'Ġv', 'ulkan', 'Ġï', '¬', 'ģ', 'les', 'Ġleak', 'sign', 'als', 'Ġintelligence', 'ig', 'int', 'Ġoverview', 'Ġn', 'sa', 'gov', 'Ġhome', 'Ġsignals', 'Ġintelligence', 'Ġoverview', 'Ġretrieved', 'Ġde', 'cember', 'national', 'Ġsecurity', 'Ġagency', 'central', 'Ġsecurity', 'Ġservice', 'Ġsignals', 'Ġintelligence', 'Ġoverview', 'Ġchap', 'man']</t>
         </is>
       </c>
       <c r="C381" t="n">
@@ -5391,7 +5391,7 @@
       </c>
       <c r="B382" t="inlineStr">
         <is>
-          <t>['Â°', '019', 'Ġya', 'ogan', 'mber', 'Ġsar', 'Â°', '055', 'Ġya', 'ogan', 'Ġde', 'cember', 'Ġe', 'Â°', '06', 'Ġya', 'ogan', 'Ġde', 'cember', 'Ġe', 'Â°', 'Ġya', 'ogan', 'Ġapr', 'il', 'Ġsar', 'Â°', '021', 'Ġya', 'ogan', 'Ġde', 'cember', 'Ġe', 'Â°', '06', 'Ġya', 'ogan', 'Ġde', 'cember', 'Ġe', 'Â°', '07', 'Ġya', 'ogan', 'Ġmarch', 'Ġel', 'int', 'Ġle', 'Â°', '009', 'Ġya', 'ogan', 'Ġle', 'Â°', '009', 'b', 'Ġya', 'ogan', 'Ġle', 'Â°', '009', 'c', 'Ġya', 'ogan', 'Ġaug', 'ust', 'Ġsar', 'Â°', 'Ġya', 'ogan', 'Ġse', 'pt', 'ember', 'Ġe', 'Â°', '047', 'Ġya', 'ogan', 'mber', 'Ġe', 'Â°', 'b', 'Ġya', 'ogan', 'mber', 'Ġsar', 'Â°', '07', 'Ġya', 'ogan', 'Ġmay', 'Ġe', 'Â°', '021', 'Ġya', 'ogan', 'Ġmay', 'Ġe', '04', 'Â°', '029', 'Ġya', 'ogan', 'mber', 'Ġel', 'int', 'Ġle', 'Â°', '011', 'Ġya', 'ogan', 'b', 'Ġle', 'Â°', '012', 'b', 'Ġya', 'ogan', 'c', 'Ġle', 'Â°', '013']</t>
+          <t>['b', 'rit', 'ish', 'Ġuse', 'dirty', 'Ġtricks', 'Ġexternal', 'Ġpolicy', 'Ġprior', 'ww', 'Ġwar', 'Ġhistory', '):', 'âĢĵ', 'http', 'Ġiss', 'n', 'Ġ09', 'Ġj', 'st', '014', 'Ġcompare', 'Ġle', 'e', 'Ġbar', 'th', 'ol', 'omew', 'radio', 'Ġspies', 'Ġepisodes', 'Ġether', 'Ġwars', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġoct', 'ober', 'Ġearly', 'Ġbo', 'er', 'Ġwar', 'Ġroyal', 'Ġnavy', 'Ġsouth', 'Ġaf', 'rica', 'Ġappears', 'Ġused', 'Ġwireless', 'Ġsets', 'Ġinherited', 'Ġroyal', 'Ġengineers', 'Ġsignal', 'Ġneutral', 'Ġport', 'Ġlou', 'ren', 'co', 'Ġmar', 'ques', 'information', 'Ġrelative', 'Ġenemy', 'Ġalbeit', 'Ġviolation', 'Ġinternational', 'Ġlaw', 'Ġ[...]', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġuse', 'Ġradio', 'Ġintelligence', 'Ġpurposes', 'Ġdepended', 'Ġcourse', 'Ġinability', 'Ġothers', 'Ġintercept', 'Ġsignals', 'Ġb', 'rit', 'ish', 'Ġpart', 'Ġworld', 'Ġwireless', 'Ġcapability', '."', 'Ġreport', 'iana', 'Ġr', 'ussian', 'Ġsignals', 'Ġintercepted', 'Ġjan', 'uary', 'Ġnaval', 'Ġlibrary', 'Ġministry', 'Ġdefence', 'Ġl', 'ondon', 'Ġdou', 'glas', 'Ġl', 'Ġwheel', 'er', 'Ġguide', 'Ġhistory', 'Ġintelligence', 'âĢĵ', 'Ġjournal', 'Ġu', 'Ġintelligence', 'Ġstudies', 'Ġwink', 'ler', 'Ġj', 'athan', 'ed', 'j', 'uly', 'information', 'Ġwarfare', 'Ġworld', 'Ġwar', '".', 'Ġjournal', 'Ġmilitary', 'Ġhistory', '):', 'âĢĵ', 'Ġbees', 'ly', 'Ġpat', 'rick', 'Ġroom', 'Ġb', 'rit', 'ish', 'Ġnaval', 'Ġintelligence', 'âĢĵ', 'Ġlong', 'Ġacre', 'Ġl', 'ondon', 'Ġham', 'ish', 'Ġham', 'ilton', 'Ġlives', 'ey', 'Ġanth', 'ony', 'Ġhistorical', 'las', 'Ġworld', 'Ġwar', 'Ġone', 'Ġh', 'olt', 'Ġnew', 'ork', 'Ġp', 'code', 'Ġbreaking', 'Ġwireless', 'Ġintercept', 'Ġjohn', 'son', 'Ġjohn', 'Ġevolution', 'Ġb', 'rit', 'ish', 'Ġsig', 'int', 'âĢĵ', 'Ġh', 'Ġp', 'Ġsm', 'ith', 'ichael', 'Ġfirst', 'Ġcold', 'Ġwar', '".', 'Ġsm', 'ith', 'ichael', 'Ġ', 'ers', 'k', 'ine', 'Ġr', 'alph', 'eds', '.).', 'Ġaction', 'Ġday']</t>
         </is>
       </c>
       <c r="C382" t="n">
@@ -5404,7 +5404,7 @@
       </c>
       <c r="B383" t="inlineStr">
         <is>
-          <t>['c', 'Ġya', 'ogan', 'Ġse', 'pt', 'ember', 'Ġel', 'int', 'Ġle', 'Â°', '046', 'Ġya', 'ogan', 'b', 'Ġle', 'Â°', '046', 'b', 'Ġya', 'ogan', 'c', 'Ġle', 'Â°', '046', 'c', 'Ġya', 'ogan', 'Ġoct', 'ober', 'Ġsar', 'Â°', '059', 'Ġya', 'ogan', 'mber', 'Ġe', '04', 'Â°', 'Ġsatellites', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġname', 'Ġmilitary', 'Ġdesignation', 'Ġlaunch', 'Ġfunction', 'Ġorbit', 'Ġorbital', 'ps', 'Ġinclination', 'Ġcos', 'par', 'id', 'Ġya', 'ogan', 'Ġaug', 'ust', 'Ġel', 'int', 'Ġle', 'Â°', '09', '047', 'Ġya', 'ogan', 'b', 'Ġle', 'Â°', '047', 'b', 'Ġya', 'ogan', 'c', 'Ġle', 'Â°', '047', 'c', 'Ġya', 'ogan', 'Ġse', 'pt', 'ember', 'Ġe', 'Â°', '05', 'Ġya', 'ogan', 'Ġoct', 'ober', 'Ġe', '07', 'Â°', '06', 'Ġya', 'ogan', 'mber', 'Ġsar', 'Â°', 'Ġ01', '07', 'Ġya', 'ogan', 'mber', 'Ġe', 'Â°', '07', 'Ġya', 'ogan', 'Ġde', 'cember', 'Ġel', 'int', 'Ġle', 'Â°', '080', 'Ġya', 'ogan', 'b', 'Ġle', 'Â°', '080', 'b', 'Ġya', 'ogan', 'c', 'Ġle', 'Â°', '080', 'c', 'Ġya', 'ogan', 'Ġde', 'cember', 'Ġe', 'Â°', '088', 'Ġya', 'ogan']</t>
+          <t>['Ġb', 'let', 'ch', 'ley', 'Ġpark', 'Ġbreaking', 'Ġen', 'igma', 'Ġcode', 'Ġbirth', 'Ġmodern', 'Ġcomputer', 'Ġb', 'antam', 'Ġpress', 'Ġpp', 'âĢĵ', 'Ġg', 'annon', 'Ġp', 'aul', 'Ġinside', 'Ġroom', 'Ġcode', 'breakers', 'Ġworld', 'Ġwar', 'Ġ', 'ian', 'Ġpublishing', 'Ġdavid', 'Ġal', 'v', 'arez', 'Ġameric', 'Ġdiplomatic', 'Ġcrypt', 'analysis', 'Ġreferences', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'Ġgross', 'Ġk', 'uno', 'ichael', 'Ġro', 'l', 'ke', 'r', 'Ã¡s', 'Ġz', 'bor', 'ay', 'Ġoperation', 'Ġsal', 'Ġal', 'Ã¡', 'sy', "'s", 'Ġdaring', 'Ġmission', 'Ġdesert', 'Ġwar', 'Ġbel', 'lev', 'ille', 'Ã¼', 'n', 'chen', 'Ġwinter', 'Ġf', 'Ġw', 'Ġultra', 'Ġsecret', 'Ġnew', 'ork', 'Ġhar', 'per', 'Ġrow', 'Ġpp', '06', '01', 'Ġh', 'ins', 'ley', 'Ġsir', 'Ġhar', 'ry', '],', 'ï', '¬', 'Ĥ', 'u', 'ence', 'Ġultra', 'Ġsecond', 'Ġworld', 'Ġwar', 'Ġretrieved', 'Ġj', 'uly', 'Ġus', 'Ġdepartment', 'Ġdefense', 'Ġj', 'uly', 'j', 'oint', 'Ġpublication', '02', 'Ġdepartment', 'Ġdefense', 'Ġdictionary', 'Ġmilitary', 'Ġassociated', 'Ġterms', 'Ġarchived', 'Ġoriginal', 'http', 'tic', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'pre', 'cision', 'Ġsig', 'int', 'Ġtargeting', 'Ġsystem', 'p', 'sts', ')"', 'Ġintelligence', 'Ġresearch', 'Ġprogram', 'Ġfederation', 'Ġameric', 'Ġscientists', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'Ġn', 'sa', 'gov', 'Ġwhit', 'lock', 'Ġdu', 'ane', 'aut', 'umn', 'Ġsilent', 'Ġwar', 'Ġj', 'apan', 'ese', 'Ġnavy', 'Ġnaval', 'Ġwar', 'Ġcollege', 'Ġreview', '):', 'âĢĵ', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġmilitary', 'Ġintelligence', 'mi', 'Ġbattalion', 'aug', 'ust', 'war', 'ï', '¬', 'ģ', 'gh', 'ter', 'Ġguide', 'Ġintelligence', 'htt', 'Ġrc', 'htm', 'Ġjoint', 'Ġspectrum', 'Ġcenter', 'us', 'Ġdefense', 'Ġinformation', 'Ġservices', 'Ġagency', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġoct', 'ober', 'Ġk', 'essler', 'tto', 'ig', 'int']</t>
         </is>
       </c>
       <c r="C383" t="n">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="B384" t="inlineStr">
         <is>
-          <t>['Ġaug', 'ust', 'Ġe', '01', 'Â°', '040', 'Ġya', 'ogan', 'mber', 'Ġe', 'Â°', 'Ġya', 'ogan', 'mber', 'Ġsar', 'Â°', '06', 'Ġya', 'ogan', 'Ġmay', 'Ġe', 'Â°', '029', 'Ġya', 'ogan', 'Ġse', 'pt', 'ember', 'Ġel', 'int', 'Ġle', '03', 'Â°', '05', 'Ġya', 'ogan', 'b', 'Ġle', '04', 'Â°', '05', 'b', 'Ġya', 'ogan', 'c', 'Ġle', 'Â°', '05', 'c', 'Ġya', 'ogan', 'mber', 'Ġel', 'int', 'Ġle', '04', 'Â°', '075', 'Ġya', 'ogan', 'b', 'Ġle', '05', 'Â°', '075', 'b', 'Ġya', 'ogan', 'c', 'Ġle', '04', 'Â°', '075', 'c', 'Ġya', 'ogan', 'Ġde', 'cember', 'Ġel', 'int', 'Ġle', '05', 'Â°', '08', 'Ġya', 'ogan', 'b', 'Ġle', 'Â°', '08', 'b', 'Ġya', 'ogan', 'c', 'Ġle', '05', 'Â°', '08', 'c', 'Ġya', 'ogan', 'Ġjan', 'uary', 'Ġel', 'int', 'Ġle', 'Â°', '011', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġname', 'Ġmilitary', 'Ġdesignation', 'Ġlaunch', 'Ġfunction', 'Ġorbit', 'Ġorbital', 'ps', 'Ġinclination', 'Ġcos', 'par', 'id', 'Ġya', 'ogan', 'b', 'Ġle', '04', 'Â°', '011', 'b', 'Ġya', 'ogan', 'c', 'Ġle']</t>
+          <t>['Ġchange', 'Ġdetection', 'Ġapproach', 'Ġdynamic', 'Ġdatabase', 'Ġe', 'f', 'ï', '¬', 'ģ', 'ci', 'ently', 'Ġconvert', 'Ġmassive', 'Ġquantities', 'Ġsensor', 'Ġdata', 'Ġaction', 'able', 'Ġinformation', 'Ġtactical', 'Ġcommanders', 'Ġdefense', 'Ġadvanced', 'Ġresearch', 'Ġprojects', 'Ġagency', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġter', 'ry', 'us', 'Ġnaval', 'Ġresearch', 'Ġlaboratory', 'Ġnetwork', 'ed', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'Ġem', 'itter', 'Ġident', 'ï', '¬', 'ģ', 'cation', 'Ġfleet', 'Ġbattle', 'Ġexperiment', 'Ġj', 'ul', 'iet', 'Ġreview', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġcombined', 'Ġboard', 'c', 'ce', 'b', 'jan', 'uary', 'Ġcommunications', 'Ġinstructions', 'Ġradio', 'Ġte', 'legraph', 'Ġprocedure', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġoct', 'ober', 'Ġjan', 'uary', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġus', 'Ġarmy', 'Ġj', 'uly', 'chapter', 'acon', 'ing', 'Ġintrusion', 'Ġjam', 'ming', 'Ġinterference', 'Ġreporting', 'Ġfield', 'Ġmanual', 'âĢĵ', 'Ġcommunications', 'Ġtechniques', 'Ġelectronic', 'âĢĵ', 'Ġretrieved', 'Ġoct', 'ober', 'Ġinter', 'agency', 'Ġop', 'sec', 'Ġsupport', 'Ġstaff', 'oss', 'may', 'oper', 'ations', 'Ġsecurity', 'Ġintelligence', 'Ġthreat', 'Ġhand', 'book', 'Ġsection', 'Ġintelligence', 'Ġcollection', 'Ġactivities', 'Ġdisciplines', 'oss', 'Ġsection', 'Ġretrieved', 'Ġoct', 'ober', 'Ġsignals', 'Ġintelligence', 'Ġwik', 'ipedia', 'radio', 'Ġregulations', 'Ġboard', 'u', 'itu', 'int', 'Ġb', 'ford', 'Ġj', 'ames', 'Ġbody', 'Ġsecrets', 'Ġameric', "'s", 'Ġn', 'sa', 'Ġb', 'rit', "'s", 'Ġeaves', 'drop', 'Ġworld', 'century', 'Ġl', 'ondon', 'Ġbol', 'ton', 'Ġmatt', 'de', 'cember', 'Ġtall', 'inn', 'Ġcables', 'Ġglimpse', 'Ġtall', 'inn', "'s", 'Ġsecret', 'Ġhistory', 'Ġespionage', 'Ġlonely', 'Ġplanet', 'Ġmagazine', 'Ġiss', 'n', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġj', '.;', 'Ġhar', 'ris', 'Ġb', '.;', 'Ġking', 'Ġwel', 'ch', 'Ġh', 'Ġw', '.,', 'Ġed', '].', 'Ġelectronic', 'Ġcounter', 'measures', 'Ġlos', 'Ġalt', 'os', 'Ġca', 'Ġpeninsula', '00', 'Ġg', 'annon', 'Ġp', 'aul', '].']</t>
         </is>
       </c>
       <c r="C384" t="n">
@@ -5430,7 +5430,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>['04', 'Â°', '011', 'c', 'Ġya', 'ogan', 'Ġapr', 'il', 'Ġel', 'int', 'Ġle', 'Â°', '034', 'Ġya', 'ogan', 'Ġle', 'Â°', '034', 'b', 'Ġya', 'ogan', 'Ġle', 'Â°', '034', 'c', 'Ġya', 'ogan', 'Ġunknown', 'Ġoct', 'ober', 'Ġe', 'Â°', '07', 'Ġya', 'ogan', 'b', 'Ġunknown', 'Â°', '07', 'b', 'Ġya', 'ogan', 'Ġmay', 'Ġsar', 'launch', 'Ġfailure', 'Ġya', 'ogan', 'Ġj', 'uly', 'Ġel', 'int', 'Ġle', 'Â°', '045', 'Ġya', 'ogan', 'b', 'Ġle', 'Â°', '045', 'b', 'Ġya', 'ogan', 'c', 'Ġle', '03', 'Â°', '045', 'c', 'Ġya', 'ogan', 'Ġmarch', 'Ġel', 'int', 'Ġle', '05', 'Â°', '021', 'Ġya', 'ogan', 'b', 'Ġle', '04', 'Â°', '021', 'b', 'Ġya', 'ogan', 'c', 'Ġle', '03', 'Â°', '021', 'c', 'Ġya', 'ogan', 'Ġoct', 'ober', 'Ġel', 'int', 'Ġle', '02', '02', 'Â°', '07', 'Ġya', 'ogan', 'b', 'Ġle', '04', 'Â°', '07', 'b', 'Ġya', 'ogan', 'c', 'Ġle', 'Â°', '07', 'c', 'Ġya', 'ogan', 'r', 'Ġde', 'cember', 'Ġsar', 'Â°', 'Ġya', 'ogan', 'Ġjan', 'uary', 'Ġel', 'int', 'Ġle', 'Â°']</t>
+          <t>['Ġcol', 'ossus', 'Ġb', 'let', 'ch', 'ley', 'Ġpark', "'s", 'Ġgreatest', 'Ġsecret', 'Ġl', 'ondon', 'l', 'antic', 'Ġbooks', 'dist', 'ur', 'bing', 'v', 'iet', 'Ġtransmissions', 'Ġaug', 'ust', 'Ġmuseum', 'Ġoccupations', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'une', 'Ġwest', 'Ġnig', 'el', 'Ġsig', 'int', 'Ġsecrets', 'Ġsignals', 'Ġintelligence', 'Ġwar', 'Ġtoday', 'iam', 'Ġmor', 'row', 'Ġnew', 'ork', 'Ġmedia', 'Ġrelated', 'Ġsig', 'int', 'Ġwik', 'imedia', 'Ġcommons', 'Ġpart', 'Ġiv', 'Ġarticles', 'Ġevolution', 'Ġarmy', 'Ġsignal', 'Ġcorps', 'int', 'Ġsig', 'int', 'Ġn', 'sa', 'Ġarchived', 'Ġfe', 'b', 'ruary', 'Ġway', 'back', 'Ġmachine', 'Ġn', 'sa', "'s", 'Ġoverview', 'Ġsig', 'int', 'Ġarchived', 'http', 'Ġaug', 'ust', 'Ġway', 'back', 'Ġmachine', 'Ġus', 'af', 'Ġpamphlet', 'Ġsources', 'Ġintelligence', 'Ġg', 'erman', 'Ġsig', 'int', 'int', 'Ġintelligence', 'Ġprograms', 'Ġsystems', 'Ġu', 'Ġintelligence', 'Ġcommunity', 'Ġje', 'ff', 'rey', 'Ġric', 'hel', 'son', 'Ġj', 'nd', 'ry', 'sp', 'oc', 'Ġsecrets', 'Ġsignals', 'Ġintelligence', 'Ġcold', 'Ġwar', 'Ġbeyond', 'Ġmatt', 'hew', 'Ġaid', 'Ġet', 'Ġal', 'bo', 'Ġmaritime', 'Ġsig', 'int', 'Ġarchitecture', 'Ġtechnical', 'Ġstandards', 'Ġhand', 'book', 'Ġretrieved', 'Ġreading', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C385" t="n">
@@ -5443,7 +5443,7 @@
       </c>
       <c r="B386" t="inlineStr">
         <is>
-          <t>['007', 'Ġya', 'ogan', 'Ġle', 'Â°', '007', 'b', 'Ġya', 'ogan', 'f', 'f', 'Ġle', 'Â°', '007', 'c', 'Ġya', 'ogan', 'Ġfe', 'b', 'ruary', 'Ġel', 'int', 'Ġle', 'Â°', '014', 'Ġya', 'ogan', 'Ġle', 'Â°', '014', 'b', 'Ġya', 'ogan', 'Ġle', 'Â°', '014', 'c', 'Ġya', 'ogan', 'Ġmarch', 'Ġel', 'int', 'Ġle', 'Â°', '020', 'b', 'Ġya', 'ogan', 'Ġle', 'Â°', '020', 'c', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġname', 'Ġmilitary', 'Ġdesignation', 'Ġlaunch', 'Ġfunction', 'Ġorbit', 'Ġorbital', 'ps', 'Ġinclination', 'Ġcos', 'par', 'id', 'Ġya', 'ogan', 'Ġle', 'Â°', '020', 'Ġya', 'ogan', 'Ġunknown', 'Ġapr', 'il', 'Ġe', 'Ġle', 'Â°', 'Ġya', 'ogan', 'Ġmay', 'Ġel', 'int', 'Ġle', '05', 'Â°', 'Ġya', 'ogan', 'b', 'Ġle', '05', 'Â°', 'b', 'Ġya', 'ogan', 'c', 'Ġle', '03', 'Â°', 'c', 'Ġya', 'ogan', 'Ġj', 'une', 'Ġel', 'int', 'Ġle', '05', 'Â°', '055', 'Ġya', 'ogan', 'b', 'Ġle', '05', 'Â°', '055', 'b', 'Ġya', 'ogan', 'c', 'Ġle', '05', 'Â°', '055', 'Ġya', 'ogan', 'Ġj', 'uly', 'Ġel', 'int', 'Ġle', 'Â°']</t>
+          <t>['01', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġwik', 'ipedia', 'b', 'ss', '048', 'Ġï', '¬', 'ģ', 'r', 'st', 'b', 'ss', 'Ġsatellites', 'Ġpassing', 'Ġcy', 'gn', 'us', 'Ġse', 'pt', 'ember', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'red', 'irect', 'ed', 'Ġg', 'ss', 'ap', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'sb', 'ss', 'Ġsystem', 'Ġplanned', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġconstellation', 'Ġsatellites', 'Ġsupporting', 'Ġground', 'Ġinfrastructure', 'Ġimprove', 'Ġability', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'od', 'Ġdetect', 'Ġtrack', 'Ġspace', 'Ġobjects', 'Ġorbit', 'Ġaround', 'Ġearth', 'Ġprimary', 'b', 'ss', 'Ġcontractor', 'Ġbo', 'e', 'ing', 'Ġcharacter', 'izes', 'Ġorbiting', 'Ġspace', 'Ġobjects', 'pot', 'ential', 'Ġfuture', 'Ġthreats', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġassets', '".[', 'b', 'ss', 'Ġdevelopment', 'Ġwork', 'Ġconducted', 'Ġcoordination', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġgroup', 'Ġspace', 'Ġsuperiority', 'Ġsystems', 'Ġwing', 'Ġspace', 'Ġmissile', 'Ġsystems', 'Ġcenter', 'Ġcommander', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġgroup', 'Ġbelieves', 'b', 'ss', 'Ġsatellite', 'Ġoperations', 'Ġcenter', 'Ġtransform', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġproviding', 'Ġgateway', 'Ġresponsive', 'Ġtask', 'able', 'Ġsensor', 'Ġcapability', 'Ġkey', 'Ġenabling', 'Ġevent', 'driven', 'Ġoperations', 'Ġconcept', 'Ġfuture', '".[', 'Ġfirst', 'path', 'finder', 'Ġsatellite', 'b', 'ss', 'Ġsystem', 'sb', 'ss', 'Ġaka', 'Ġus', 'Ġcos', 'par', '048', 'Ġsat', 'cat', 'Ġsuccessfully', 'Ġplaced', 'Ġorbit', 'Ġboard', 'Ġmin', 'otaur', 'Ġiv', 'Ġrocket', 'Ġse', 'pt', 'ember', 'Ġoriginally', 'Ġlaunch', 'Ġscheduled', 'Ġde', 'cember', 'Ġres', 'ched', 'uled', 'Ġspring', 'Ġdelayed', 'Ġoct', 'ober', 'Ġlaunch', 'Ġdelays', 'Ġcaused', 'Ġproblems', 'Ġbooster', 'Ġsatellite', 'Ġlaunch', 'Ġexpected', 'Ġj', 'uly', 'Ġalso', 'Ġpostponed', 'Ġprogram', 'Ġcost', 'Ġmillion', 'Ġincluding', 'Ġsatellite', 'Ġpayload', 'Ġlaunch', 'Ġground', 'Ġsupport', 'Ġsatellite', 'Ġpayload', 'Ġcontracts', 'Ġball', 'Ġaerospace', 'Ġtechnologies', 'Ġapproximately', 'Ġtotal', 'Ġdesigned', 'Ġexamine', 'Ġevery', 'Ġspacecraft', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġleast', 'b', 'ss', 'Ġpath', 'finder', 'Ġsatellite', 'Ġtelescope', 'Ġtwo', 'Ġaxis', 'Ġg', 'im', 'bal', 'Ġmeg', 'apixel', 'Ġimage', 'Ġsensor', 'Ġprojected', 'Ġmission', 'Ġduration', 'Ġfive', 'Ġhalf', 'Ġyears', 'Ġfirst', 'Ġtwo', 'Ġg', 'ss', 'ap', 'Ġspacecraft', 'Ġlaunched', 'Ġtwo', 'Ġlaunched']</t>
         </is>
       </c>
       <c r="C386" t="n">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="B387" t="inlineStr">
         <is>
-          <t>['Ġya', 'ogan', 'b', 'Ġle', '04', 'Â°', 'b', 'Ġya', 'ogan', 'c', 'Ġle', '03', 'Â°', 'c', 'Ġya', 'ogan', 'Ġunknown', 'mber', 'Ġsig', 'int', 'Â°', 'Ġya', 'ogan', 'b', 'Ġunknown', 'Â°', 'b', 'Ġya', 'ogan', 'Ġunknown', 'mber', 'Ġunknown', 'Ġle', 'Â°', 'Ġya', 'ogan', 'b', 'Ġunknown', 'Ġle', 'Â°', 'b', 'Ġya', 'ogan', 'c', 'Ġunknown', 'Ġle', 'Â°', 'c', 'Ġya', 'ogan', 'Ġunknown', 'Ġmarch', 'Ġe', 'Ġle', 'Â°', '027', 'Ġya', 'ogan', 'Ġ02', 'Ġunknown', 'Ġj', 'une', 'Ġel', 'int', 'Ġle', 'Â°', '07', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', '08', 'b', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', '09', 'c', 'Ġya', 'ogan', 'Ġ03', 'Ġunknown', 'Ġj', 'uly', 'Ġel', 'int', 'Ġle', 'Â°', '088', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', '088', 'b', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', '088', 'c', 'Ġya', 'ogan', 'Ġ04', 'Ġunknown', 'Ġaug', 'ust', 'Ġel', 'int', 'Ġle', 'Â°', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'b', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'c', 'Ġya', 'ogan', 'Ġunknown', 'Ġse', 'pt']</t>
+          <t>['Ġaug', 'ust', 'usa', 'Ġus', 'Ġfirst', 'Ġtwo', 'Ġbuilt', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'Ġcapabilities', 'Ġdevelopment', 'Ġconstruction', 'Ġbudgets', 'Ġclassified', 'Ġoperate', 'near', 'ge', 'os', 'ynchronous', 'Ġorbit', '",', 'Ġfirst', 'Ġlaunch', 'Ġscheduled', 'Ġj', 'uly', 'Ġaboard', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġdelta', 'Ġiv', 'Ġlaunch', 'Ġvehicle', 'Ġpath', 'finder', 'Ġsatellite', 'Ġge', 'os', 'ynchronous', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġprogram', '01', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġwik', 'ipedia', 'Ġeven', 'Ġtesting', 'Ġprocess', 'Ġsatellites', 'Ġpressed', 'Ġearly', 'Ġservice', 'Ġfulfill', 'Ġcritical', 'Ġneeds', 'Ġse', 'pt', 'ember', 'Ġthird', 'Ġfourth', 'Ġsatellites', 'Ġdeclared', 'Ġoperational', 'Ġtwo', 'Ġsatellites', 'g', 'ss', 'ap', 'Ġg', 'ss', 'ap', 'Ġsuccessfully', 'Ġlaunched', 'Ġjan', 'uary', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġus', 'Ġapproached', 'Ġtwo', 'Ġch', 'inese', 'Ġsatellites', 'Ġgeo', 'Ġexamine', 'Ġclosely', 'Ġch', 'inese', 'Ġresearchers', 'Ġreported', 'Ġobserved', 'Ġinstances', 'Ġus', 'Ġsatellites', 'Ġapproached', 'Ġch', 'inese', 'Ġones', 'Ġaug', 'ust', 'Ġspace', 'Ġsystems', 'Ġcommand', 'Ġannounced', 'Ġretirement', 'Ġg', 'ss', 'ap', 'Ġsatellite', 'Ġfirst', 'Ġconstellation', 'Ġdecom', 'mission', 'ed', 'Ġsubsequent', 'Ġtransfer', 'Ġgraveyard', 'Ġorbit', 'Ġmoreover', 'Ġrevealed', 'Ġtwo', 'Ġsatellites', 'Ġordered', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġkeep', 'Ġdemand', 'Ġg', 'ss', 'ap', 'Ġassets', 'Ġlaunches', 'Ġnew', 'Ġsatellites', 'Ġplanned', 'Ġrespectively', 'Ġspacecraft', 'Ġfirst', 'Ġconstellation', 'Ġlaunched', 'Ġpairs', 'Ġair', 'Ġforce', 'Ġspace', 'Ġsurveillance', 'Ġsystem', 'ite', 'x', 'bo', 'e', 'ing', 'Ġball', 'Ġaerospace', 'Ġachieve', 'Ġnew', 'Ġmilestone', 'b', 'ss', 'Ġprogram', 'Ġl', 'Ġbo', 'e', 'ing', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'bo', 'e', 'ing', 'Ġcompletes', 'Ġhardware', 'Ġinstallation', 'b', 'ss', 'Ġsatellite', 'Ġoperations', 'Ġcenter', 'web', 'arch', 'Ġbo', 'e', 'ing', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'min', 'otaur', 'Ġiv', 'Ġv', 'Ġorbital', 'Ġsciences', 'Ġcorporation', 'v', 'enberg', 'Ġlaunches', 'Ġmin', 'otaur', 'Ġiv', 'th', 'Ġspace', 'Ġwing', 'Ġpublic', 'Ġaffairs', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġarticle', 'Ġincorporates', 'Ġtext']</t>
         </is>
       </c>
       <c r="C387" t="n">
@@ -5469,7 +5469,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>['ember', 'Ġsar', 'Â°', 'Ġya', 'ogan', 'Ġ05', 'Ġunknown', 'Ġse', 'pt', 'ember', 'Ġel', 'int', 'Ġle', 'Â°', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġname', 'Ġmilitary', 'Ġdesignation', 'Ġlaunch', 'Ġfunction', 'Ġorbit', 'Ġorbital', 'ps', 'Ġinclination', 'Ġcos', 'par', 'id', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'b', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'c', 'Ġya', 'ogan', 'Ġunknown', 'Ġse', 'pt', 'ember', 'Ġunknown', 'Ġle', 'Â°', 'Ġya', 'ogan', 'b', 'Ġunknown', 'Ġle', 'Â°', 'b', 'Ġya', 'ogan', 'c', 'Ġunknown', 'Ġle', 'Â°', 'c', 'Ġya', 'ogan', 'Ġ02', 'Ġunknown', 'Ġoct', 'ober', 'Ġel', 'int', 'Ġle', 'Â°', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'b', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'c', 'Ġya', 'ogan', 'Ġunknown', 'mber', 'Ġunknown', 'Ġle', '080', 'Â°', 'Ġya', 'ogan', 'Ġ03', 'Ġunknown', 'mber', 'Ġel', 'int', 'Ġle', 'Â°', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'b', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'c', 'Ġya', 'ogan', 'Ġ04', 'Ġunknown', 'Ġde', 'cember', 'Ġel', 'int', 'Ġle', 'Â°', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'b', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'c']</t>
+          <t>['Ġsource', 'Ġpublic', 'Ġdomain', 'bo', 'e', 'ing', 'b', 'ss', 'Ġsystem', 'Ġprogressing', 'Ġtoward', 'st', 'Ġlaunch', 'Ġbo', 'e', 'ing', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'laun', 'cher', 'Ġissues', 'Ġblamed', 'month', 'b', 'ss', 'Ġslip', 'Ġspace', 'Ġnews', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'Ġbo', 'e', 'ing', 'Ġteam', 'Ġships', 'Ġfirst', 'b', 'ss', 'Ġspacecraft', 'Ġlaunch', 'Ġsite', 'launch', 'Ġdelayed', 'Ġsatellite', 'Ġwatch', 'Ġspace', 'Ġdebris', 'ahoo', 'Ġnews', 'Ġarchived', 'Ġoriginal', 'Ġic', 'cam', 'delay', 'Ġj', 'uly', 'Ġretrieved', 'Ġjan', 'uary', 'Ġsee', 'Ġalso', 'Ġreferences', '01', 'Ġspace', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġwik', 'ipedia', 'space', 'Ġbased', 'Ġspace', 'Ġsurveillance', 'Ġe', 'sb', 'ss', 'Ġball', 'Ġaerospace', 'Ġretrieved', 'mber', 'Ġneighborhood', 'Ġwatch', 'Ġspace', 'Ġaviation', 'Ġweek', 'Ġspace', 'Ġtechnology', 'Ġaug', 'ust', 'ler', 'Ġamy', 'Ġfe', 'b', 'ruary', 'us', 'af', 'Ġreveals', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġnew', 'Ġsatellite', 'web', 'arch', 'iv', 'Ġaviation', 'Ġweek', 'Ġsap', 'ce', 'Ġtechnology', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġhar', 'per', 'Ġj', 'Ġj', 'uly', 'air', 'Ġforce', 'Ġlaunching', 'Ġsatellites', 'Ġsatellites', 'http', 'str', 'Ġstripes', 'Ġstars', 'Ġstripes', 'Ġretrieved', 'Ġj', 'uly', 'Ġgr', 'uss', 'ike', 'Ġse', 'pt', 'ember', 'space', 'Ġsurveillance', 'ats', 'Ġpressed', 'Ġearly', 'Ġservice', 'http', 'sp', 'Ġspac', 'en', 'ews', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġes', 'pin', 'osa', 'Ġshell', 'ie', 'anne', 'Ġse', 'pt', 'ember', 'two', 'Ġnew', 'Ġsatellites', 'Ġoperational', 'Ġexpand', 'Ġu', 'Ġspace', 'Ġsituational', 'Ġawareness', 'Ġaf', 'sp', 'c', 'af', 'mil', 'Ġair', 'Ġforce', 'Ġspace', 'Ġcommand', 'Ġpublic', 'Ġaffairs', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgra', 'ham', 'iam', 'Ġjan', 'uary', 'ula', "'s", 'las', 'Ġlaunches', 'Ġmission', 'Ġspace', 'Ġforce', 'Ġnas', 'asp', 'ace', 'flight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġw', 'er', 'ner', 'Ġdeb', 'ra']</t>
         </is>
       </c>
       <c r="C388" t="n">
@@ -5482,7 +5482,7 @@
       </c>
       <c r="B389" t="inlineStr">
         <is>
-          <t>['Ġya', 'ogan', 'Ġunknown', 'Ġjan', 'uary', 'Ġunknown', 'Ġle', 'Â°', '006', 'c', 'Ġya', 'ogan', 'Ġunknown', 'Ġmarch', 'Ġunknown', 'Ġle', 'Â°', '048', 'Ġya', 'ogan', 'Ġ05', 'Ġunknown', 'Ġj', 'uly', 'Ġel', 'int', 'Ġle', 'Â°', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'c', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Â°', 'e', 'Ġya', 'ogan', 'Ġ01', 'Ġunknown', 'Ġaug', 'ust', 'Ġel', 'int', 'Ġle', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Ġya', 'ogan', 'Ġunknown', 'Ġle', 'Ġtable', 'Ġdata', 'Ġsourced', 'Ġpreviously', 'Ġcited', 'Ġreferences', 'c', 'als', 'ky', 'Ġc', 'als', 'ky', 'Ġc', 'als', 'ky', 'Ġretrieved', 'mber', 'real', 'Ġtime', 'Ġsatellite', 'Ġtracking', 'Ġret', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġmay', 'Ġretrieved', 'Ġoct', 'ober', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġch', 'ina', 'Ġportal', 'Ġus', 'sr', 'Ġr', 'ussia', 'Ġk', 'os', 'mos', 'atellite', 'Ġunited', 'Ġstates', 'Ġn', 'oss', 'Ġsee', 'Ġalso', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'Ġfr', 'ance', 'Ġce', 'res', 'atellite', 'Ġcl', 'ark', 'Ġstep', 'hen', 'Ġjan', 'uary', 'ch', 'ina', 'Ġlaunches', 'Ġmilitary', 'Ġsatellite', 'Ġtrio', 'Ġorbit', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'orbit', 'Ġoriginal', 'Ġoct', 'ober', 'Ġj', 'athan', 'cd', 'owell', 'planet', 'Ġapr', 'il', 'Ġj', 'ian', 'bing', 'Ġ03', 'Ġradar', 'Ġsatellite', 'Ġcover', 'Ġname', 'Ġya', 'ogan', 'ent', 'ered', 'Ġ00', 'Ġut', 'c', 'Ġapr', 'Ġsouth', 'l', 'antic', 'Ġlaunched', 'Ġoct', 'Ġoperated', 'Ġfe', 'b', 'Ġorbit', 'Ġlowered', 'Ġapr', 'j', 'ul', 'Ġunderwent', 'Ġuncontrolled', 'Ġdecay', 'Ġsince', 'Ġj', 'ul', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġvia', 'Ġtwitter', 'Ġcost', 'ello', 'Ġjohn', 'cre', 'yn', 'olds', 'Ġjo', 'e', 'oct', 'ober', 'ch']</t>
+          <t>['Ġj', 'une', 'orbit', 'Ġgame', 'Ġcat', 'Ġmouse', 'Ġclose', 'Ġapproaches', 'Ġprompt', 'Ġcalls', 'Ġcommunications', 'Ġnorms', 'Ġspac', 'en', 'ews', 'Ġtam', 'im', 'Ġbab', 'Ġmay', 'us', 'Ġconducted', 'Ġmissions', 'Ġch', 'ina', "'s", 'Ġsatellites', 'Ġyears', 'Ġclaims', 'Ġch', 'inese', 'Ġstudy', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġaug', 'ust', 'u', 'Ġde', 'activ', 'ates', 'Ġg', 'ss', 'ap', 'Ġsurveillance', 'Ġsatellite', 'Ġtwo', 'Ġnew', 'Ġones', 'Ġworks', 'Ġretrieved', 'Ġaug', 'ust', 'ley', 'Ġg', 'reg', 'Ġaug', 'ust', 'space', 'Ġforce', 'Ġde', 'activ', 'ates', 'Ġone', 'Ġspace', 'Ġsurveillance', 'Ġsatellite', 'Ġsets', 'Ġplans', 'Ġtwo', 'Ġair', 'Ġspace', 'Ġforces', 'Ġmagazine', 'Ġretrieved', 'Ġaug', 'ust', 'Ġretrieved']</t>
         </is>
       </c>
       <c r="C389" t="n">
@@ -5495,7 +5495,7 @@
       </c>
       <c r="B390" t="inlineStr">
         <is>
-          <t>['ina', "'s", 'Ġstrategic', 'Ġsupport', 'Ġforce', 'Ġforce', 'Ġnew', 'Ġera', 'Ġch', 'ina', 'Ġstrategic', 'Ġperspectives', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġj', 'une', 'Ġvia', 'Ġnational', 'Ġdefense', 'Ġuniversity', 'Ġbarb', 'osa', 'Ġru', 'Ġc', 'Ġapr', 'il', 'ch', 'inese', 'Ġlaunch', 'Ġya', 'ogan', 'ix', 'ing', 'Ġremote', 'Ġsensing', 'Ġsatellite', 'ite', 'Ġnas', 'asp', 'ace', 'ï', '¬', 'Ĥ', 'ight', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'å¹', '´', 'â', '½', 'ī', 'â', '½', 'ĩ', 'éģ', '¥', 'æĦ', 'Ł', 'åį', '«', 'æĺ', 'Ł', 'â', '¼', 'Ģ', 'åı', '·', 'æĪ', 'Ĳ', 'åĬ', 'Ł', 'åı', 'ĳ', 'å°', 'Ħ', 'htm', 'x', 'h', 'uan', 'et', 'Ġx', 'h', 'uan', 'et', 'Ġapr', 'il', 'Ġarchived', 'Ġoriginal', 'htm', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'ch', 'ina', 'Ġlaunches', 'Ġsatellite', 'ell', 'ite', 'ian', 'Ġsurve', 'ying', 'Ġmapping', 'Ġmagazine', 'Ġde', 'cember', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'j', 'ian', 'bing', 'ya', 'ogan', 'ix', 'ing', 'Ġsynthetic', 'Ġaperture', 'Ġradar', 'ino', 'Ġdefense', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġraft', 'j', 'ian', 'bing', 'asp', 'Ġapr', 'il', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġde', 'cember', 'ya', 'ogan', ')"', 'htt', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġcliff', 'Ġro', 'ger', 'Ġready', 'Ġtakeoff', 'Ġch', 'ina', "'s", 'Ġadvancing', 'Ġaerospace', 'Ġindustry', 'Ġch', 'ad', 'Ġj', 'Ġr', 'Ġoh', 'land', 'Ġdavid', 'ang', 'Ġu', '.-', 'ch', 'ina', 'Ġeconomic', 'Ġsecurity', 'Ġreview', 'Ġcommission', 'Ġrand', 'Ġcorporation', 'Ġnational', 'Ġsecurity', 'Ġresearch', 'Ġdivision', 'anta', 'Ġmon', 'ica', 'Ġca', 'Ġrand', 'Ġnational', 'Ġsecurity', 'Ġresearch', 'Ġdivision', 'cl', 'c', 'ya', 'ogan', 'ix', 'ing', 'remote', 'Ġsensing', 'Ġsatellite', ')"', 'Ġch', 'ina', 'Ġspace', 'Ġreport', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj']</t>
+          <t>['Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'b', 'irs', 'Ġsystems', 'Ġgeo', 'Ġlow', 'Ġcomponents', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'sb', 'irs', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'Ġsystem', 'Ġintended', 'Ġmeet', 'Ġunited', 'Ġstates', 'Ġdepartment', 'Ġdefense', 'Ġinfrared', 'Ġspace', 'Ġsurveillance', 'Ġneeds', 'Ġfirst', 'Ġtwo', 'Ġthree', 'Ġdecades', 'st', 'Ġcentury', 'b', 'irs', 'Ġprogram', 'Ġdesigned', 'Ġprovide', 'Ġkey', 'Ġcapabilities', 'Ġareas', 'Ġmissile', 'Ġwarning', 'Ġmissile', 'Ġdefense', 'Ġbattles', 'pace', 'Ġcharacterization', 'Ġtechnical', 'Ġintelligence', 'Ġvia', 'Ġsatellites', 'Ġge', 'os', 'ynchronous', 'Ġearth', 'Ġorbit', 'ge', 'Ġsensors', 'Ġhosted', 'Ġsatellites', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'Ġground', 'based', 'Ġdata', 'Ġprocessing', 'Ġcontrol', 'Ġtotal', 'Ġtwelve', 'Ġsatellites', 'Ġcarrying', 'b', 'irs', 'Ġst', 'ss', 'Ġpayload', 'Ġlaunched', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'b', 'irs', 'usa', 'Ġst', 'ss', 'rr', 'usa', 'Ġst', 'ss', 'Ġdemo', 'usa', 'Ġst', 'ss', 'Ġdemo', 'usa', 'Ġmanufacturing', 'Ġcontract', 'b', 'irs', 'b', 'irs', 'Ġawarded', 'Ġfunding', 'b', 'irs', 'b', 'irs', 'Ġcanceled', 'Ġbased', 'Ġexperiences', 'Ġlaunching', 'Ġshort', 'range', 'Ġtheater', 'Ġmissiles', 'Ġpers', 'ian', 'Ġgulf', 'Ġwar', 'Ġu', 'Ġdepartment', 'Ġdefense', 'od', 'Ġconcluded', 'Ġexpanded', 'Ġtheater', 'Ġmissile', 'Ġwarning', 'Ġcapabilities', 'Ġneeded', 'Ġbegan', 'Ġplanning', 'Ġimproved', 'Ġinfrared', 'Ġsatellite', 'Ġsensor', 'Ġcapability', 'Ġwould', 'Ġsupport', 'Ġlong', 'range', 'Ġstrategic', 'Ġshort', 'range', 'Ġtheater', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġdefense', 'Ġoperations', 'Ġdod', 'Ġstudied', 'Ġconsolid', 'ating', 'Ġvarious', 'Ġinfrared', 'Ġspace', 'Ġrequirements', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġdefense', 'Ġtechnical', 'Ġintelligence', 'Ġbattles', 'pace', 'Ġcharacterization', 'Ġselected', 'b', 'irs', 'Ġreplace', 'Ġenhance', 'Ġcapabilities', 'Ġprovided', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'sp', 'sp', 'Ġsatellites']</t>
         </is>
       </c>
       <c r="C390" t="n">
@@ -5508,7 +5508,7 @@
       </c>
       <c r="B391" t="inlineStr">
         <is>
-          <t>['une', 'ya', 'ogan', 'Ġerupt', 'Ġpts', 'Ġarms', 'Ġcontrol', 'k', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'web', 'arch', 'iv', 'Ġg', 'er', 'upt', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġw', 'ade', 'Ġmark', 'Ġastronaut', 'ix', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'cd', 'owell', 'Ġj', 'athan', 'planet', 'Ġapr', 'il', 'j', 'ian', 'bing', 'Ġ03', 'Ġdecay', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġvia', 'Ġtwitter', 'Ġk', 'bs', 'Ġgun', 'ter', 'ya', 'ogan', 'r', 'ya', 'ogan', 'htm', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġse', 'pt', 'ember', 'ya', 'ogan', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'ya', 'ogan', ')"', 'sp', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġw', 'ade', 'Ġmark', 'Ġastronaut', 'ix', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġk', 'bs', 'Ġgun', 'ter', 'ya', 'ogan', ')"', 'sp', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', 'ya', 'ogan', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġw', 'ade', 'Ġmark', 'Ġastronaut', 'ix', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly']</t>
+          <t>['Ġbuilt', 'Ġinfrared', 'Ġdetectors', 'Ġsense', 'Ġmissile', 'Ġpl', 'umes', 'Ġproviding', 'Ġearly', 'Ġwarning', 'Ġlong', 'range', 'Ġballistic', 'Ġmissile', 'Ġlaunches', 'Ġyears', 'Ġdod', 'Ġpreviously', 'Ġattempted', 'Ġreplace', 'sp', 'Ġadvanced', 'Ġwarning', 'Ġsystem', 'Ġearly', 'Ġboost', 'Ġsurveillance', 'Ġtracking', 'Ġsystem', 'Ġlate', 'Ġfollow', 'Ġearly', 'Ġwarning', 'Ġsystem', 'Ġearly', 'Ġaccording', 'Ġgovernment', 'Ġaccountability', 'Ġoffice', 'Ġattempts', 'Ġfailed', 'Ġdue', 'Ġimmature', 'Ġtechnology', 'Ġhigh', 'Ġcost', 'Ġaffordability', 'Ġissues', 'b', 'irs', 'Ġuse', 'Ġsophisticated', 'Ġinfrared', 'Ġtechnologies', 'sp', 'Ġenhance', 'Ġdetection', 'Ġstrategic', 'Ġtheater', 'Ġballistic', 'Ġmissile', 'Ġlaunches', 'Ġperformance', 'Ġmissile', 'tracking', 'Ġfunction', 'Ġbackground', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'b', 'irs', 'Ġhigh', 'Ġgeo', 'Ġoriginal', 'Ġcontract', 'Ġconsisted', 'b', 'irs', 'Ġsatellite', 'Ġsensors', 'b', 'irs', 'Ġgeo', 'Ġsensors', 'Ġsatellites', 'Ġoption', 'Ġtotal', 'Ġge', 'os', 'Ġcomplement', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġplanned', 'Ġpart', 'Ġprogram', 'sb', 'irs', 'low', 'Ġmoved', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'st', 'ss', 'Ġprogram', 'b', 'irs', 'Ġcontinues', 'Ġstruggle', 'Ġcost', 'Ġoverrun', 'Ġn', 'unn', 'cc', 'urdy', 'Ġbreaches', 'Ġoccurring', 'Ġse', 'pt', 'ember', 'Ġexpected', 'Ġproject', 'Ġcost', 'Ġincreased', 'Ġus', 'Ġbillion', 'Ġde', 'cember', 'Ġfollowing', 'Ġthird', 'b', 'irs', 'Ġn', 'unn', 'cc', 'urdy', 'Ġviolation', 'Ġgovernment', 'Ġdecided', 'Ġcompete', 'b', 'irs', 'b', 'irs', 'Ġoption', 'b', 'irs', 'Ġcontingent', 'Ġbased', 'Ġperformance', 'Ġfirst', 'Ġj', 'une', 'Ġlock', 'heed', 'Ġmart', 'Ġannounced', 'Ġawarded', 'Ġcontract', 'Ġthird', 'b', 'irs', 'Ġpayload', 'Ġthird', 'b', 'irs', 'Ġgeo', 'Ġsatellite', 'Ġassociated', 'Ġground', 'Ġequipment', 'Ġmodifications', 'Ġj', 'uly', 'Ġlock', 'heed', 'Ġmart', 'Ġawarded', 'Ġus', 'Ġmillion', 'Ġpayment', 'Ġus', 'af', 'Ġtowards', 'Ġpurchase', 'Ġfourth', 'Ġsatellite', 'Ġfirst', 'b', 'irs', 'Ġgeo', 'Ġsatellite', 'b', 'irs', 'Ġprogram', 'b', 'irs', 'Ġsuccessfully', 'Ġlaunched', 'Ġcape', 'aver', 'al', 'las', 'Ġlaunch', 'Ġvehicle', 'Ġmay', 'Ġj', 'une', 'Ġlock', 'heed', 'Ġmart', 'Ġcontracted']</t>
         </is>
       </c>
       <c r="C391" t="n">
@@ -5521,7 +5521,7 @@
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>['ya', 'ogan', ')"', 'sp', 'ac', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġk', 'bs', 'Ġgun', 'ter', 'Ġj', 'uly', 'ya', 'ogan', ')"', 'space', 'sk', 'yr', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'ai', 'wan', "'s", 'Ġpresident', 'Ġspeaks', 'Ġcor', 'nell', 'Ġreunion', 'Ġweekend', 'Ġcor', 'nell', 'Ġuniversity', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'u', 'Ġaircraft', 'Ġcarrier', 'ia', 'r', 'outine', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġlin', 'Ġj', 'enn', 'ifer', 'Ġmarch', 'u', 'Ġconsiders', 'Ġrisking', 'Ġch', 'ina', "'s", 'Ġwrath', 'ai', 'wan', 'Ġn', 'im', 'itz', 'Ġcould', 'Ġsail', 'ai', 'wan', 'Ġstra', 'Ġch', 'ina', 'Ġcalling', 'b', 'razen', '."', 'Ġph', 'ilipp', 'ine', 'Ġdaily', 'Ġinquire', 'r', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'su', 'Ġchi', 'ai', 'wan', "'s", 'Ġrelations', 'Ġmainland', 'Ġch', 'ina', 'Ġtail', 'Ġw', 'agging', 'Ġtwo', 'Ġdogs', 'Ġrout', 'ledge', 'Ġp', '040', 'Ġsu', 'ivan', 'Ġdan', 'Ġmay', 'balance', 'ia', 'Ġcalls', 'pr', 'ong', 'ed', 'Ġstrategy', 'Ġhill', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'uly', 'Ġreferences', 'Ġya', 'ogan', 'Ġwik', 'ipedia', 'could', 'Ġch', 'ina', 'Ġseize', 'Ġoccupy', 'ai', 'wan', 'Ġmilit', 'arily', '?"', 'Ġchin', 'ap', 'ower', 'Ġcenter', 'Ġstrategic', 'Ġinternational', 'Ġstudies', 'Ġmay', 'Ġarchived', 'Ġn', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'uly', 'Ġch', 'inese', 'Ġmaritime', 'Ġsurveillance', 'Ġsystem', 'Ġse', 'pt', 'ember', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġmarch', 'Ġbl', 'izzard', 'Ġtim', 'othy', 'Ġj', 'Ġpl', 'Ġad', 'f', 'Ġlessons', 'Ġfuture', 'Ġmaritime', 'Ġstrategy', 'Ġsecurity', 'Ġchallenges', '):']</t>
+          <t>['Ġus', 'af', 'Ġbuild', 'b', 'irs', 'b', 'irs', 'Ġcost', 'Ġus', 'Ġbillion', 'Ġbudget', 'Ġalloc', 'ates', 'Ġbillion', 'b', 'irs', 'Ġunited', 'Ġstates', 'Ġspace', 'Ġforce', 'b', 'irs', 'Ġhigh', 'also', 'Ġsimply', 'Ġreferred', 'sb', 'irs', '")', 'Ġconsist', 'Ġfour', 'Ġdedicated', 'Ġsatellites', 'Ġoperating', 'Ġge', 'os', 'ynchronous', 'Ġearth', 'Ġorbit', 'Ġsensors', 'Ġtwo', 'Ġhost', 'Ġsatellites', 'Ġoperating', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'b', 'irs', 'Ġhigh', 'Ġreplace', 'Ġdefense', 'Ġsupport', 'Ġprogram', 'sp', 'Ġsatellites', 'Ġintended', 'Ġprimarily', 'Ġprovide', 'Ġenhanced', 'Ġstrategic', 'Ġtheater', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġcapabilities', 'b', 'irs', 'Ġhigh', 'Ġgeo', 'Ġlaunched', 'Ġmay', 'Ġtwo', 'b', 'irs', 'Ġsensors', 'Ġhosted', 'Ġtwo', 'Ġclassified', 'Ġsatellites', 'Ġhighly', 'Ġellipt', 'ical', 'Ġorbit', 'Ġalready', 'Ġlaunched', 'Ġprobably', 'Ġpart', 'usa', 'usa', 'Ġlaunches', 'Ġus', 'Ġus', 'Ġbelieved', 'Ġanalysts', 'Ġel', 'int', 'Ġsatellites', 'Ġfamily', 'Ġjump', 'seat', 'Ġtrumpet', 'Ġtrumpet', 'Ġreported', 'Ġcarried', 'Ġinfrared', 'Ġsensor', 'Ġcalled', 'Ġheritage', 'Ġprime', 'Ġcontractor', 'b', 'irs', 'Ġlock', 'heed', 'Ġmart', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġmajor', 'Ġsubcontract', 'Ġlock', 'heed', 'Ġmart', 'Ġalso', 'Ġprovides', 'Ġsatellite', 'b', 'irs', 'Ġgeo', 'Ġsystem', "'s", 'Ġexpected', 'Ġdeployment', 'Ġdelayed', 'Ġde', 'cember', 'Ġproblems', 'Ġlock', 'heed', "'s", 'Ġwork', 'manship', 'Ġsystem', 'Ġcomponents', 'Ġincluding', 'Ġunresolved', 'Ġsoftware', 'Ġmalf', 'unctions', 'Ġseveral', 'Ġbroken', 'Ġsolder', 'Ġjoints', 'Ġsubcontract', 'Ġproc', 'ured', 'Ġgy', 'ro', 'scope', 'Ġassembly', 'Ġfirst', 'Ġspacecraft', 'Ġbuilt', 'Ġfeared', 'Ġlaunch', 'Ġpostp', 'onement', 'Ġlate', 'Ġwould', 'Ġlead', 'Ġconflict', 'Ġplanned', 'Ġlaunches', 'Ġn', 'asa', "'s", 'Ġjun', 'Ġspacecraft', 'Ġmars', 'Ġscience', 'Ġlaboratory', 'Ġwould', 'Ġuse', 'Ġlaunch', 'Ġfacility', 'Ġhowever', 'Ġfirst', 'Ġgeo', 'Ġlaunch', 'b', 'irs', 'Ġsuccessfully', 'Ġconducted', 'Ġmay', 'b', 'irs', 'Ġhigh', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'b', 'irs', 'Ġlow', 'Ġaccording', 'uters', 'Ġreport', 'Ġfirst', 'Ġtwo', 'b', 'irs', 'Ġgeo', 'Ġsatellites', 'Ġstarted', 'Ġoperations', 'b', 'irs', 'Ġlaunched', 'Ġjan', 'uary', 'b', 'irs', 'Ġsuccessfully', 'Ġdeployed', 'Ġjan', 'uary']</t>
         </is>
       </c>
       <c r="C392" t="n">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>['âĢĵ', 'Ġj', 'st', 'Ġvia', 'Ġj', 'st', 'ate', 'rew', 'Ġmarch', 'ch', 'ina', 'Ġdeploy', 'Ġsurveillance', 'Ġsatellites', 'Ġj', 'anes', 'Ġdefense', 'Ġarchived', 'web', 'Ġoriginal', 'Ġj', 'uly', 'Ġastronaut', 'ix', 'Ġarchived', 'htt', 'Ġoriginal', 'Ġmarch', 'ya', 'ogan', ')"', 'Ġgun', 'ter', "'s", 'Ġspace', 'Ġpage', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġretrieved']</t>
+          <t>['Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġrequested', 'Ġbillion', 'Ġfiscal', 'Ġyear', 'b', 'irs', 'Ġfunds', 'Ġadvance', 'Ġprocurement', 'b', 'irs', 'Ġmillion', 'Ġfunding', 'Ġprovided', 'b', 'irs', 'Ġfiscal', 'Ġyear', 'Ġfunding', 'b', 'irs', 'Ġeliminated', 'Ġfavor', 'Ġnew', 'Ġprogram', 'Ġng', 'op', 'ir', 'next', 'Ġgeneration', 'Ġoverhead', 'Ġpersistent', 'Ġinfrared', 'Ġplans', 'Ġremained', 'Ġlaunch', 'b', 'irs', 'b', 'irs', 'b', 'irs', 'Ġsuccessfully', 'Ġlaunched', 'Ġmay', 'b', 'irs', 'Ġsuccessfully', 'Ġlaunched', 'Ġaug', 'ust', 'b', 'irs', 'Ġlow', 'Ġcontract', 'Ġmanaged', 'Ġmissile', 'Ġdefense', 'Ġagency', 'Ġrenamed', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'st', 'ss', 'b', 'irs', 'Ġlow', 'Ġprogram', 'Ġoriginally', 'Ġexpected', 'Ġconsist', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġprimary', 'Ġpurpose', 'b', 'irs', 'Ġlow', 'Ġtracking', 'Ġballistic', 'Ġmissiles', 'Ġdiscrimination', 'Ġwarheads', 'Ġobjects', 'Ġdec', 'oys', 'Ġseparate', 'Ġmissile', 'Ġbodies', 'Ġthroughout', 'Ġmiddle', 'Ġportion', 'Ġflights', 'Ġsystem', 'Ġtwo', 'Ġmajor', 'Ġsensors', 'Ġcoordinated', 'board', 'Ġcomputer', 'Ġscanning', 'Ġinfrared', 'Ġsensor', 'Ġdesigned', 'Ġacquire', 'Ġballistic', 'Ġmissiles', 'Ġearly', 'Ġstages', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtracking', 'Ġinfrared', 'Ġsensor', 'Ġdesigned', 'Ġfollow', 'Ġmissiles', 'Ġwarheads', 'Ġobjects', 'Ġdebris', 'Ġdec', 'oys', 'Ġmiddle', 'Ġlater', 'Ġstages', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtracking', 'Ġsensor', 'Ġwould', 'Ġcooled', 'Ġlow', 'Ġtemperatures', 'b', 'irs', 'Ġlow', "'s", 'Ġoriginal', 'Ġdeployment', 'Ġschedule', 'Ġdate', 'Ġcapabilities', 'Ġsaid', 'Ġneeded', 'Ġnational', 'Ġmissile', 'Ġdefense', 'Ġsystem', 'Ġmissile', 'Ġdefense', 'Ġagency', 'Ġassessed', 'Ġprograms', 'Ġneeded', 'Ġnational', 'Ġballistic', 'Ġmissile', 'Ġdefense', 'Ġsystem', 'Ġfound', 'Ġlacking', 'Ġrelatively', 'Ġnew', 'Ġarena', 'Ġspace', 'Ġdecided', 'Ġabsorb', 'b', 'irs', 'Ġlow', 'Ġconstellation', 'Ġearly', 'Ġstages', 'Ġdevelopment', 'Ġrenamed', 'Ġprogram', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'st', 'ss', 'Ġtransition', 'Ġchanged', 'Ġdirection', 'Ġprogram', 'Ġsomewhat', 'Ġoverall', 'Ġmission', 'Ġremained', 'Ġdetection', 'Ġtracking', 'Ġballistic', 'Ġmissiles', 'Ġphases', 'Ġflight', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġportal', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġfe', 'b', 'ruary', 'Ġend', 'b', 'irs', 'Ġair', 'Ġforce', 'Ġsays', "'s", 'Ġtime', 'Ġmove', 'http']</t>
         </is>
       </c>
       <c r="C393" t="n">
@@ -5547,7 +5547,7 @@
       </c>
       <c r="B394" t="inlineStr">
         <is>
-          <t>['Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġstar', 'link', 'Ġsatellites', 'Ġstacked', 'Ġtogether', 'Ġdeployment', 'Ġmay', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġoperator', 'Ġspace', 'x', 'Ġapplications', 'Ġinternet', 'Ġservice', 'Ġwebsite', 'Ġstar', 'link', 'st', 'arl', 'Ġink', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġspacecraft', 'Ġtype', 'Ġsmall', 'Ġsatellite', 'Ġlaunch', 'Ġmass', 'Ġmini', 'Ġequipment', 'Ġka', 'Ġe', 'band', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġlaser', 'Ġtrans', 'p', 'ond', 'ers', 'Ġunits', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġregime', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġproduction', 'Ġstatus', 'Ġactive', 'Ġstar', 'link', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'Ġoperated', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġspace', 'x', 'Ġproviding', 'Ġcoverage', 'Ġcountries', 'Ġalso', 'Ġaims', 'Ġglobal', 'Ġmobile', 'Ġphone', 'Ġservice', 'Ġspace', 'x', 'Ġstarted', 'Ġlaunching', 'Ġstar', 'link', 'Ġsatellites', 'Ġaug', 'ust', 'Ġstar', 'link', 'Ġconsists', '000', 'Ġmass', 'produced', 'Ġsmall', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcommunicate', 'Ġdesignated', 'Ġground', 'Ġtrans', 'ce', 'ivers', 'Ġtotal', 'Ġnearly', '000', 'Ġsatellites', 'Ġplanned', 'Ġdeployed', 'Ġpossible', 'Ġlater', 'Ġextension', '000', 'Ġspace', 'x', 'Ġannounced', 'Ġreaching', 'Ġmillion', 'Ġsubscribers', 'Ġde', 'cember', 'Ġmillion', 'Ġsubscribers', 'Ġmay', 'Ġspace', 'x', 'Ġsatellite', 'Ġdevelopment', 'Ġfacility', 'Ġred', 'mond', 'Ġwashing', 'ton', 'Ġhouses', 'Ġstar', 'link', 'Ġresearch', 'Ġdevelopment', 'Ġmanufacturing', 'Ġorbit', 'Ġcontrol', 'Ġteams', 'Ġcost', 'Ġdecade', 'long', 'Ġproject', 'Ġdesign', 'Ġbuild', 'Ġdeploy', 'Ġconstellation', 'Ġestimated', 'Ġspace', 'x', 'Ġmay', 'Ġleast', 'Ġus', 'Ġbillion', 'equ', 'ivalent', 'Ġus', 'Ġbillion', ').[', 'Ġspace', 'x', 'Ġexpects', 'Ġbillion', 'Ġrevenue', 'Ġsatellite', 'Ġconstellation', 'Ġrevenues', 'Ġlaunch', 'Ġbusiness', 'Ġexpected', 'Ġreach', 'Ġbillion', 'Ġyear', 'Ġastronomers', 'Ġraised', 'Ġconcerns', 'Ġeffect', 'Ġconstellation', 'Ġground', 'based', 'Ġastronomy', 'Ġsatellites', 'Ġadd', 'Ġalready', 'Ġcongest', 'ed', 'Ġorbital', 'Ġspace', 'x', 'Ġattempted', 'Ġmitigate', 'Ġastron', 'ometric', 'Ġinterference', 'Ġconcerns', 'Ġmeasures', 'Ġreduce', 'Ġbrightness', 'Ġoperation']</t>
+          <t>['b', 'irs', 'Ġlow', 'space', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'Ġoriginal', 'b', 'irs', 'Ġlow', 'Ġspace', 'Ġtracking', 'Ġsurveillance', 'Ġsystem', 'Ġreferences', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'intelligence', 'Ġauthorization', 'Ġact', 'Ġfiscal', 'Ġyear', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'high', 'house', 'Ġreport', ')"', 'Ġu', 'Ġgovernment', 'Ġprinting', 'ï', '¬', 'ģ', 'ce', 'Ġmay', 'space', 'Ġbased', 'Ġinfrared', 'Ġsystem', 'Ġhigh', 'Ġprogram', 'Ġalternative', 'web', 'ar', 'Ġgovernment', 'Ġaccountability', 'ï', '¬', 'ģ', 'ce', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'r', 'html', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġfact', 'Ġsheet', 'Ġspace', 'Ġbased', 'Ġinfrared', 'Ġsystem', 'Ġc', 'di', 'org', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'contract', 'Ġmay', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġmay', 'Ġretrieved', 'mber', 'u', 'Ġair', 'Ġforce', 'Ġawards', 'Ġlock', 'heed', 'Ġmart', 'Ġus', 'billion', 'Ġcontract', 'b', 'irs', 'Ġfollow', 'Ġspacecraft', 'Ġlock', 'heed', 'Ġmart', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġv', 'orman', 'Ġj', 'ul', 'ie', 'Ġj', 'uly', 'lock', 'heed', 'Ġgets', 'Ġus', 'Ġmillion', 'Ġu', 'Ġsatellite', 'Ġpayment', 'http', 'uters', 'united', 'Ġlaunch', 'Ġalliance', 'Ġmarks', 'th', 'Ġsuccessful', 'Ġlaunch', 'Ġdelivering', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'sb', 'irs', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'press', 'Ġrelease', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġmay', 'Ġretrieved', 'mber', 'sb', 'irs', 'Ġgeo', 'Ġcontract', 'Ġawarded', 'Ġlos', 'Ġangel', 'es', 'Ġair', 'Ġforce', 'Ġbase', 'Ġu', 'Ġair', 'Ġforce', 'Ġj', 'une', 'Ġretrieved', 'Ġjan', 'uary', 'u', 'Ġair', 'Ġforce', 'Ġawards', 'Ġlock', 'heed', 'Ġmart', 'Ġcontract', 'Ġnext', 'Ġtwo', 'b', 'irs', 'Ġmissile', 'Ġdefense', 'Ġearly', 'Ġwarning', 'Ġsatellites', 'Ġb', 'irs', 'html', 'Ġlock', 'heed', 'mart', 'press', 'Ġrelease', 'Ġlock', 'heed', 'Ġmart', 'Ġj', 'une', 'Ġretrieved', 'mber']</t>
         </is>
       </c>
       <c r="C394" t="n">
@@ -5560,7 +5560,7 @@
       </c>
       <c r="B395" t="inlineStr">
         <is>
-          <t>['Ġsatellites', 'Ġequipped', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġallowing', 'Ġorbit', 'Ġraise', 'Ġstation', 'keep', 'Ġde', 'orbit', 'Ġend', 'Ġlife', 'Ġadditionally', 'Ġsatellites', 'Ġdesigned', 'Ġautonom', 'ously', 'Ġsmoothly', 'Ġavoid', 'Ġcollisions', 'Ġbased', 'Ġupl', 'ink', 'ed', 'Ġtracking', 'Ġdata', 'Ġconst', 'ell', 'ations', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellites', 'Ġfirst', 'Ġconceptual', 'ized', 'Ġmid', 'Ġpart', 'Ġstrategic', 'Ġdefense', 'Ġinitiative', 'Ġculminating', 'Ġbrilliant', 'Ġpe', 'b', 'bles', 'Ġweapons', 'Ġstaged', 'Ġorbit', 'Ġintercept', 'Ġballistic', 'Ġmissiles', 'Ġshort', 'Ġnotice', 'Ġpotential', 'Ġlow', 'lat', 'ency', 'Ġcommunication', 'Ġalso', 'Ġrecognized', 'Ġdevelopment', 'sh', 'oots', 'Ġled', 'Ġnumerous', 'Ġcommercial', 'Ġmeg', 'acon', 'st', 'ell', 'ations', 'Ġusing', 'Ġaround', 'Ġsatellites', 'Ġcel', 'est', 'ron', 'Ġtel', 'edes', 'ic', 'Ġir', 'idium', 'Ġglobal', 'star', 'Ġhowever', 'Ġentities', 'Ġentered', 'Ġbankruptcy', 'Ġdot', 'Ġbubble', 'Ġburst', 'Ġdue', 'Ġpart', 'Ġexcessive', 'Ġlaunch', 'Ġcosts', 'Ġtime', 'Ġl', 'arry', 'iam', 'Ġspace', 'x', 'Ġstrategic', 'Ġrelations', 'Ġformer', 'Ġtel', 'edes', 'ic', "'s", 'internet', 'Ġprogram', 'Ġopened', 'Ġspace', 'x', 'Ġwashing', 'ton', 'Ġoffice', 'Ġj', 'une', 'Ġspace', 'x', 'Ġacquired', 'Ġstake', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'st', 'l', 'Ġpart', 'shared', 'Ġstrategic', 'Ġhistory', 'Ġbackground', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġsatellite', 'Ġdevelopment', 'Ġfacility', 'Ġred', 'mond', 'Ġwashing', 'ton', 'Ġuse', 'Ġmid', 'Ġvision', '".[', 'st', 'l', 'Ġtime', 'Ġworking', 'Ġextend', 'Ġinternet', 'Ġspace', 'Ġhowever', 'Ġspace', 'x', "'s", 'Ġstake', 'Ġeventually', 'Ġsold', 'Ġback', 'Ġe', 'ads', 'Ġast', 'rium', 'Ġcompany', 'Ġbecame', 'Ġfocused', 'Ġnavigation', 'Ġearth', 'Ġobservation', 'Ġearly', 'Ġel', 'Ġmus', 'k', 'Ġg', 'reg', 'Ġw', 'ler', 'Ġworking', 'Ġtogether', 'Ġplanning', 'Ġconstellation', 'Ġaround', 'Ġsatellites', 'Ġcalled', 'Ġworld', 'vu', 'Ġwould', 'Ġtimes', 'Ġsize', 'Ġlargest', 'Ġir', 'idium', 'Ġsatellite', 'Ġconstellation', 'Ġhowever', 'Ġdiscussions', 'Ġbroke', 'Ġj', 'une', 'Ġspace', 'x', 'Ġinstead', 'Ġfiled', 'u', 'Ġapplication', 'Ġvia', 'way', 'Ġtelecom', 'Ġregulator', 'Ġname', 'Ġsteam', 'Ġspace', 'x', 'Ġconfirmed', 'Ġconnection', 'Ġapplication', 'Ġlicense', 'Ġstar', 'link', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġspace', 'x', 'Ġtrademark', 'ed', 'Ġname', 'Ġstar', 'link', 'Ġunited', 'Ġstates', 'Ġsatellite', 'Ġbroadband', 'Ġnetwork']</t>
+          <t>['od', 'Ġreleases', 'Ġfiscal', 'Ġyear', 'Ġbudget', 'Ġproposal', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'rocket', 'Ġblasts', 'Ġmissile', 'warning', 'Ġsatellite', 'uters', 'Ġmay', 'u', 'Ġair', 'Ġforce', 'Ġawards', 'Ġlock', 'heed', 'Ġmart', 'Ġus', 'billion', 'Ġcontract', 'b', 'irs', 'Ġfollow', 'Ġspacecraft', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'mol', 'c', 'zan', 'Ġsat', 'obs', 'Ġmessage', 'Ġse', 'pt', 'ember', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġwik', 'ipedia', 'mol', 'c', 'zan', 'Ġsat', 'obs', 'Ġmessage', 'Ġfe', 'b', 'ruary', 'Ġcap', 'acc', 'io', 'ony', 'Ġse', 'pt', 'ember', 'del', 'ivery', 'Ġdelayed', 'Ġlock', 'heed', 'Ġmart', "'s", 'Ġearly', 'Ġwarning', 'Ġsatellite', '".', 'Ġbloom', 'berg', 'Ġth', 'om', 'pson', 'Ġlore', 'n', 'Ġb', 'Ġlaunch', 'Ġpriority', 'Ġmissile', 'Ġwarning', 'Ġcome', 'Ġfirst', 'Ġlex', 'ington', 'Ġinstitute', 'Ġoct', 'ober', 'lock', 'heed', 'Ġwins', 'Ġus', 'Ġbillion', 'Ġdeal', 'Ġu', 'Ġmissile', 'warning', 'Ġsatellites', 'uters', 'Ġj', 'une', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'b', 'irs', 'Ġgeo', 'Ġflight', 'Ġsatellite', 'Ġorbit', 'Ġu', 'Ġair', 'Ġforce', 'press', 'Ġrelease', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġjan', 'uary', 'Ġretrieved', 'mber', 'Ġrich', 'ards', 'Ġde', 'rek', 'Ġjan', 'uary', 'var', 'ious', 'Ġissues', 'Ġprompt', 'hour', 'Ġscrub', 'las', 'b', 'irs', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġinsider', 'Ġretrieved', 'mber', 'Ġcl', 'ark', 'Ġstep', 'hen', 'u', 'Ġmilitary', 'Ġsatellite', 'Ġlaunched', 'Ġfort', 'ify', 'Ġmissile', 'Ġattacks', 'space', 'ï', '¬', 'Ĥ', 'igh', 'Ġspace', 'ï', '¬', 'Ĥ', 'ight', 'Ġretrieved', 'Ġjan', 'uary', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġoct', 'ober', 'production', 'Ġnew', 'Ġmissile', 'Ġwarning', 'Ġsatellites', 'Ġlikely', 'Ġdelayed', 'Ġbudget', 'Ġimp', 'asse', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'mber', 'las', 'Ġrocket', 'Ġlaunches', 'b', 'irs', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġus', 'Ġspace', 'Ġforce', 'ww', 'Ġspace', 'Ġmay', 'Ġretrieved', 'Ġj', 'une']</t>
         </is>
       </c>
       <c r="C395" t="n">
@@ -5573,7 +5573,7 @@
       </c>
       <c r="B396" t="inlineStr">
         <is>
-          <t>['Ġname', 'Ġinspired', 'Ġnovel', 'Ġfault', 'Ġstars', 'Ġstar', 'link', 'Ġpublicly', 'Ġannounced', 'Ġjan', 'uary', 'Ġopening', 'Ġspace', 'x', 'Ġsatellite', 'Ġdevelopment', 'Ġfacility', 'Ġred', 'mond', 'Ġwashing', 'ton', 'Ġopening', 'Ġmus', 'k', 'Ġstated', 'Ġstill', 'Ġsignificant', 'Ġun', 'met', 'Ġdemand', 'Ġworldwide', 'Ġlow', 'cost', 'Ġbroadband', 'Ġstar', 'link', 'Ġwould', 'Ġtarget', 'Ġbandwidth', 'Ġcarry', 'Ġback', 'haul', 'Ġcommunications', 'Ġtraffic', 'Ġlocal', 'Ġinternet', 'Ġtraffic', 'Ġhigh', 'density', 'Ġcities', 'Ġmus', 'k', 'Ġstated', 'Ġpositive', 'Ġcash', 'Ġflow', 'Ġselling', 'Ġsatellite', 'Ġinternet', 'Ġservices', 'Ġwould', 'Ġnecessary', 'Ġfund', 'Ġmars', 'Ġplans', 'Ġfurthermore', 'Ġspace', 'x', 'Ġlong', 'term', 'Ġplans', 'Ġdevelop', 'Ġdeploy', 'Ġversion', 'Ġsatellite', 'Ġcommunication', 'Ġsystem', 'Ġserve', 'Ġmars', 'Ġstarting', 'Ġengineers', 'Ġcompany', 'Ġoperated', '000', 'Ġft', 'Ġleased', 'Ġspace', 'Ġjan', 'uary', 'Ġtaken', '000', 'Ġft', 'Ġsecond', 'Ġfacility', 'Ġred', 'mond', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġconsolidated', 'Ġse', 'attle', 'area', 'Ġoperations', 'Ġmove', 'Ġlarger', 'Ġthree', 'building', 'Ġfacility', 'Ġred', 'mond', 'Ġridge', 'Ġcorporate', 'Ġcenter', 'Ġsupport', 'Ġsatellite', 'Ġmanufacturing', 'Ġaddition', 'Ġj', 'uly', 'Ġspace', 'x', 'Ġacquired', 'Ġadditional', '000', 'Ġft', 'Ġcreative', 'Ġspace', 'Ġir', 'vine', 'Ġcal', 'ornia', 'orange', 'Ġcounty', ').[', 'Ġir', 'vine', 'Ġoffice', 'Ġwould', 'Ġinclude', 'Ġsignal', 'Ġprocessing', 'Ġr', 'f', 'ic', 'ic', 'Ġdevelopment', 'Ġsatellite', 'Ġprogram', 'Ġoct', 'ober', 'Ġsatellite', 'Ġdivision', 'Ġfocusing', 'Ġsignificant', 'Ġbusiness', 'Ġchallenge', 'Ġachieving', 'Ġsufficiently', 'Ġlow', 'cost', 'Ġdesign', 'Ġuser', 'Ġequipment', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġsaid', 'Ġproject', 'Ġremained', 'design', 'Ġphase', 'Ġcompany', 'Ġseeks', 'Ġtackle', 'Ġissues', 'Ġrelated', 'Ġuser', 'termin', 'al', 'Ġcost', '".[', 'mber', 'Ġspace', 'x', 'Ġfiled', 'Ġapplication', 'non', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'ng', 'Ġsatellite', 'Ġsystem', 'Ġfixed', 'atellite', 'Ġservice', 'Ġusing', 'Ġka', 'Ġfrequency', 'Ġbands', '".[', 'Ġmarch', 'Ġspace', 'x', 'Ġfiled', 'Ġplans', 'Ġfield', 'Ġsecond', 'Ġorbital', 'Ġshell', 'v', 'band', 'Ġsatellites', 'Ġnon', 'ge', 'os', 'ynchronous', 'Ġorbits', 'Ġprovide', 'Ġcommunications', 'Ġservices', 'Ġelectromagnetic', 'Ġspectrum', 'Ġpreviously', 'Ġheavily', 'Ġemployed', 'Ġcommercial', 'Ġcommunications', 'Ġservices']</t>
+          <t>['las', 'b', 'irs', 'Ġgeo', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġj', 'uly', 'united', 'Ġlaunch', 'Ġalliance', 'Ġsuccessfully', 'Ġlaunches', 'Ġmissile', 'Ġwarning', 'Ġsatellite', 'Ġu', 'Ġspace', 'Ġforce', 'h', 'Ġunited', 'Ġlaunch', 'Ġalliance', 'Ġretrieved', 'Ġaug', 'ust', 'Ġl', 'isa', 'odd', 'ers', 'Ġaug', 'b', 'irs', 'Ġlaunch', 'Ġcloses', 'Ġtwo', 'Ġdecades', 'Ġprogress', 'Ġmissile', 'Ġwarning', 'Ġtracking', 'Ġdetection', 'Ġnext', 'gen', 'Ġop', 'ir', 'Ġtake', 'Ġhelm', 'Ġspace', 'based', 'Ġinfrared', 'Ġsystem', 'Ġlow', 'Ġrisk', 'Ġmissing', 'Ġinitial', 'Ġdeployment', 'Ġdate', 'Ġu', 'Ġgeneral', 'Ġaccounting', 'ï', '¬', 'ģ', 'ce', 'Ġfe', 'b', 'ruary', 'Ġfact', 'Ġsheets', 'Ġspace', 'Ġbased', 'Ġinfrared', 'Ġsystems', 'Ġspace', 'Ġbased', 'Ġinfrared', 'Ġsystems', 'Ġtactical', 'Ġballistic', 'Ġmissile', 'Ġwarning', 'Ġu', 'Ġstrategic', 'Ġcommand', 'Ġretrieved', 'Ġexternal', 'Ġlinks']</t>
         </is>
       </c>
       <c r="C396" t="n">
@@ -5586,7 +5586,7 @@
       </c>
       <c r="B397" t="inlineStr">
         <is>
-          <t>['Ġcalled', 'low', 'Ġearth', 'Ġorbit', 'v', 'le', 'Ġconstellation', '",', 'Ġcomprised', 'Ġsatellites', 'Ġorbit', 'Ġmi', 'Ġaltitude', 'Ġsmaller', 'Ġoriginally', 'Ġplanned', 'Ġgroup', 'Ġsatellites', 'Ġwould', 'Ġoperate', 'Ġka', 'Ġk', 'u', 'bands', 'Ġorbit', 'Ġmi', 'Ġaltitude', 'Ġspace', 'x', 'Ġwithdrawn', 'Ġplans', 'Ġfield', 'atellite', 'Ġv', 'band', 'Ġsystem', 'Ġsupers', 'eding', 'Ġcomprehensive', 'Ġdesign', 'Ġsecond', 'generation', 'Ġstar', 'link', 'Ġnetwork', 'Ġse', 'pt', 'ember', 'Ġruled', 'Ġhalf', 'Ġconstellation', 'Ġmust', 'Ġorbit', 'Ġwithin', 'Ġyears', 'Ġcomply', 'Ġlicensing', 'Ġterms', 'Ġfull', 'Ġsystem', 'Ġorbit', 'Ġwithin', 'Ġnine', 'Ġyears', 'Ġdate', 'Ġlicense', 'Ġspace', 'x', 'Ġfiled', 'Ġdocuments', 'Ġlate', 'Ġclarify', 'Ġspace', 'Ġdebris', 'Ġmitigation', 'Ġplan', 'Ġcompany', 'Ġdesign', 'Ġphase', 'âĢĵ', 'Ġstart', 'Ġdevelopment', 'Ġphase', 'âĢĵ', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġlifts', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġfl', 'ida', 'Ġdelivering', 'Ġstar', 'link', 'Ġsatellites', 'Ġorbit', 'mber', 'im', 'plement', 'Ġoperations', 'Ġplan', 'Ġorderly', 'Ġde', 'orbit', 'Ġsatellites', 'Ġnearing', 'Ġend', 'Ġuseful', 'Ġlives', 'rough', 'ly', 'Ġfive', 'Ġseven', 'Ġyears', 'Ġrate', 'Ġfar', 'Ġfaster', 'Ġrequired', 'Ġinternational', 'Ġstandards', 'atell', 'ites', 'Ġde', 'orbit', 'Ġprop', 'uls', 'ively', 'Ġmoving', 'Ġdisposal', 'Ġorbit', 'enter', 'Ġearth', "'s", 'Ġatmosphere', 'Ġwithin', 'Ġapproximately', 'Ġone', 'Ġyear', 'Ġcompletion', 'Ġmission', '."[', 'Ġmarch', 'Ġgranted', 'Ġspace', 'x', 'Ġapproval', 'Ġinitial', 'Ġsatellites', 'Ġconditions', 'Ġspace', 'x', 'Ġwould', 'Ġneed', 'Ġobtain', 'Ġseparate', 'Ġapproval', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', ').[', 'Ġsupported', 'Ġn', 'asa', 'Ġrequest', 'Ġask', 'Ġspace', 'x', 'Ġachieve', 'Ġeven', 'Ġhigher', 'Ġlevel', 'Ġde', 'orb', 'iting', 'Ġreliability', 'Ġstandard', 'Ġn', 'asa', 'Ġpreviously', 'Ġused', 'Ġreliably', 'Ġde', 'orb', 'iting', 'Ġsatellites', 'Ġmissions', 'Ġcomplete', 'Ġmay', 'Ġspace', 'x', 'Ġexpected', 'Ġtotal', 'Ġcost', 'Ġdevelopment', 'Ġbuild', 'Ġconstellation', 'Ġapproach', 'Ġbillion']</t>
+          <t>['Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġstar', 'link', 'Ġsatellites', 'Ġstacked', 'Ġtogether', 'Ġdeployment', 'Ġmay', 'Ġmanufacturer', 'Ġspace', 'x', 'Ġcountry', 'Ġorigin', 'Ġunited', 'Ġstates', 'Ġoperator', 'Ġspace', 'x', 'Ġapplications', 'Ġinternet', 'Ġservice', 'Ġwebsite', 'Ġstar', 'link', 'st', 'arl', 'Ġink', 'Ġspe', 'ci', 'ï', '¬', 'ģ', 'c', 'ations', 'Ġspacecraft', 'Ġtype', 'Ġsmall', 'Ġsatellite', 'Ġlaunch', 'Ġmass', 'Ġmini', 'Ġequipment', 'Ġka', 'Ġe', 'band', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġlaser', 'Ġtrans', 'p', 'ond', 'ers', 'Ġunits', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġregime', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsun', 'syn', 'chron', 'ous', 'Ġorbit', 'Ġproduction', 'Ġstatus', 'Ġactive', 'Ġstar', 'link', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'Ġoperated', 'Ġameric', 'Ġaerospace', 'Ġcompany', 'Ġspace', 'x', 'Ġproviding', 'Ġcoverage', 'Ġcountries', 'Ġalso', 'Ġaims', 'Ġglobal', 'Ġmobile', 'Ġphone', 'Ġservice', 'Ġspace', 'x', 'Ġstarted', 'Ġlaunching', 'Ġstar', 'link', 'Ġsatellites', 'Ġaug', 'ust', 'Ġstar', 'link', 'Ġconsists', '000', 'Ġmass', 'produced', 'Ġsmall', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġcommunicate', 'Ġdesignated', 'Ġground', 'Ġtrans', 'ce', 'ivers', 'Ġtotal', 'Ġnearly', '000', 'Ġsatellites', 'Ġplanned', 'Ġdeployed', 'Ġpossible', 'Ġlater', 'Ġextension', '000', 'Ġspace', 'x', 'Ġannounced', 'Ġreaching', 'Ġmillion', 'Ġsubscribers', 'Ġde', 'cember', 'Ġmillion', 'Ġsubscribers', 'Ġmay', 'Ġspace', 'x', 'Ġsatellite', 'Ġdevelopment', 'Ġfacility', 'Ġred', 'mond', 'Ġwashing', 'ton', 'Ġhouses', 'Ġstar', 'link', 'Ġresearch', 'Ġdevelopment', 'Ġmanufacturing', 'Ġorbit', 'Ġcontrol', 'Ġteams', 'Ġcost', 'Ġdecade', 'long', 'Ġproject', 'Ġdesign', 'Ġbuild', 'Ġdeploy', 'Ġconstellation', 'Ġestimated', 'Ġspace', 'x', 'Ġmay', 'Ġleast', 'Ġus', 'Ġbillion', 'equ', 'ivalent', 'Ġus', 'Ġbillion', ').[', 'Ġspace', 'x', 'Ġexpects', 'Ġbillion', 'Ġrevenue', 'Ġsatellite', 'Ġconstellation', 'Ġrevenues', 'Ġlaunch', 'Ġbusiness', 'Ġexpected', 'Ġreach', 'Ġbillion', 'Ġyear', 'Ġastronomers', 'Ġraised', 'Ġconcerns', 'Ġeffect', 'Ġconstellation', 'Ġground', 'based', 'Ġastronomy', 'Ġsatellites', 'Ġadd', 'Ġalready', 'Ġcongest', 'ed', 'Ġorbital', 'Ġspace', 'x', 'Ġattempted', 'Ġmitigate', 'Ġastron', 'ometric', 'Ġinterference', 'Ġconcerns', 'Ġmeasures', 'Ġreduce', 'Ġbrightness', 'Ġoperation']</t>
         </is>
       </c>
       <c r="C397" t="n">
@@ -5599,7 +5599,7 @@
       </c>
       <c r="B398" t="inlineStr">
         <is>
-          <t>['equ', 'ivalent', '000', '000', ').[', 'Ġmid', 'Ġspace', 'x', 'organized', 'Ġsatellite', 'Ġdevelopment', 'Ġdivision', 'Ġred', 'mond', 'Ġterminated', 'Ġseveral', 'Ġmembers', 'Ġsenior', 'Ġmanagement', 'mber', 'Ġspace', 'x', 'Ġreceived', 'Ġu', 'Ġregulatory', 'Ġapproval', 'Ġdeploy', 'Ġv', 'band', 'Ġbroadband', 'Ġsatellites', 'Ġaddition', 'Ġapproved', 'Ġearlier', 'Ġhowever', 'Ġv', 'band', 'Ġplans', 'Ġsubsequently', 'Ġwithdrawn', 'Ġtime', 'Ġspace', 'x', 'Ġalso', 'Ġmade', 'Ġnew', 'Ġregulatory', 'Ġfilings', 'Ġu', 'Ġrequest', 'Ġability', 'Ġalter', 'Ġpreviously', 'Ġgranted', 'Ġlicense', 'Ġorder', 'Ġoperate', 'Ġapproximately', 'Ġka', 'ku', 'band', 'Ġsatellites', 'Ġapproved', 'Ġoperation', 'Ġmi', 'new', 'Ġlower', 'Ġshell', 'Ġconstellation', 'Ġorbital', 'Ġaltitude', 'Ġsatellites', 'Ġwould', 'Ġeffectively', 'Ġoperate', 'Ġthird', 'Ġorbital', 'Ġshell', 'Ġmi', 'Ġorbit', 'Ġhigher', 'Ġlower', 'Ġorbits', 'Ġapproximately', 'Ġmi', 'Ġapproximately', 'Ġmi', 'Ġwould', 'Ġused', 'Ġlater', 'Ġconsiderably', 'Ġlarger', 'Ġdeployment', 'Ġsatellites', 'Ġbecomes', 'Ġpossible', 'Ġlater', 'Ġyears', 'Ġdeployment', 'Ġprocess', 'Ġapproved', 'Ġrequest', 'Ġapr', 'il', 'Ġgiving', 'Ġapproval', 'Ġplace', 'Ġnearly', '000', 'Ġsatellites', 'Ġthree', 'Ġorbital', 'Ġshells', 'Ġinitially', 'Ġapproximately', 'Ġmi', 'Ġaltitude', 'Ġshell', 'Ġsubsequently', 'Ġplacing', 'Ġapproximately', 'Ġka', 'band', 'Ġspectrum', 'Ġsatellites', 'Ġmi', 'Ġapproximately', 'Ġv', 'band', 'Ġsatellites', 'Ġtotal', 'Ġnearly', '000', 'Ġsatellites', 'Ġplanned', 'Ġdeployed', 'Ġpossible', 'Ġlater', 'Ġextension', '000', 'Ġfe', 'b', 'ruary', 'Ġsister', 'Ġcompany', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġservices', 'Ġinc', '.,', 'Ġfiled', 'Ġrequest', 'Ġreceive', 'Ġlicense', 'Ġoperation', 'Ġmillion', 'Ġfixed', 'Ġsatellite', 'Ġearth', 'Ġstations', 'Ġwould', 'Ġcommunicate', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'ng', 'Ġsatellite', 'Ġstar', 'link', 'Ġsystem', 'Ġlaunching', 'Ġtwo', 'Ġtest', 'Ġsatellites', 'Ġfe', 'b', 'ruary', 'Ġfirst', 'Ġbatch', 'Ġoperational', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġmay', 'Ġj', 'une', 'Ġspace', 'x', 'Ġapplied', 'Ġlicense', 'Ġtest', 'Ġground', 'Ġterminals', 'Ġnationwide', 'Ġacross']</t>
+          <t>['Ġsatellites', 'Ġequipped', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġallowing', 'Ġorbit', 'Ġraise', 'Ġstation', 'keep', 'Ġde', 'orbit', 'Ġend', 'Ġlife', 'Ġadditionally', 'Ġsatellites', 'Ġdesigned', 'Ġautonom', 'ously', 'Ġsmoothly', 'Ġavoid', 'Ġcollisions', 'Ġbased', 'Ġupl', 'ink', 'ed', 'Ġtracking', 'Ġdata', 'Ġconst', 'ell', 'ations', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellites', 'Ġfirst', 'Ġconceptual', 'ized', 'Ġmid', 'Ġpart', 'Ġstrategic', 'Ġdefense', 'Ġinitiative', 'Ġculminating', 'Ġbrilliant', 'Ġpe', 'b', 'bles', 'Ġweapons', 'Ġstaged', 'Ġorbit', 'Ġintercept', 'Ġballistic', 'Ġmissiles', 'Ġshort', 'Ġnotice', 'Ġpotential', 'Ġlow', 'lat', 'ency', 'Ġcommunication', 'Ġalso', 'Ġrecognized', 'Ġdevelopment', 'sh', 'oots', 'Ġled', 'Ġnumerous', 'Ġcommercial', 'Ġmeg', 'acon', 'st', 'ell', 'ations', 'Ġusing', 'Ġaround', 'Ġsatellites', 'Ġcel', 'est', 'ron', 'Ġtel', 'edes', 'ic', 'Ġir', 'idium', 'Ġglobal', 'star', 'Ġhowever', 'Ġentities', 'Ġentered', 'Ġbankruptcy', 'Ġdot', 'Ġbubble', 'Ġburst', 'Ġdue', 'Ġpart', 'Ġexcessive', 'Ġlaunch', 'Ġcosts', 'Ġtime', 'Ġl', 'arry', 'iam', 'Ġspace', 'x', 'Ġstrategic', 'Ġrelations', 'Ġformer', 'Ġtel', 'edes', 'ic', "'s", 'internet', 'Ġprogram', 'Ġopened', 'Ġspace', 'x', 'Ġwashing', 'ton', 'Ġoffice', 'Ġj', 'une', 'Ġspace', 'x', 'Ġacquired', 'Ġstake', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'st', 'l', 'Ġpart', 'shared', 'Ġstrategic', 'Ġhistory', 'Ġbackground', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġsatellite', 'Ġdevelopment', 'Ġfacility', 'Ġred', 'mond', 'Ġwashing', 'ton', 'Ġuse', 'Ġmid', 'Ġvision', '".[', 'st', 'l', 'Ġtime', 'Ġworking', 'Ġextend', 'Ġinternet', 'Ġspace', 'Ġhowever', 'Ġspace', 'x', "'s", 'Ġstake', 'Ġeventually', 'Ġsold', 'Ġback', 'Ġe', 'ads', 'Ġast', 'rium', 'Ġcompany', 'Ġbecame', 'Ġfocused', 'Ġnavigation', 'Ġearth', 'Ġobservation', 'Ġearly', 'Ġel', 'Ġmus', 'k', 'Ġg', 'reg', 'Ġw', 'ler', 'Ġworking', 'Ġtogether', 'Ġplanning', 'Ġconstellation', 'Ġaround', 'Ġsatellites', 'Ġcalled', 'Ġworld', 'vu', 'Ġwould', 'Ġtimes', 'Ġsize', 'Ġlargest', 'Ġir', 'idium', 'Ġsatellite', 'Ġconstellation', 'Ġhowever', 'Ġdiscussions', 'Ġbroke', 'Ġj', 'une', 'Ġspace', 'x', 'Ġinstead', 'Ġfiled', 'u', 'Ġapplication', 'Ġvia', 'way', 'Ġtelecom', 'Ġregulator', 'Ġname', 'Ġsteam', 'Ġspace', 'x', 'Ġconfirmed', 'Ġconnection', 'Ġapplication', 'Ġlicense', 'Ġstar', 'link', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġspace', 'x', 'Ġtrademark', 'ed', 'Ġname', 'Ġstar', 'link', 'Ġunited', 'Ġstates', 'Ġsatellite', 'Ġbroadband', 'Ġnetwork']</t>
         </is>
       </c>
       <c r="C398" t="n">
@@ -5612,7 +5612,7 @@
       </c>
       <c r="B399" t="inlineStr">
         <is>
-          <t>['Ġunited', 'Ġstates', 'Ġwashing', 'ton', 'Ġstate', 'Ġspace', 'x', 'Ġemployee', 'Ġhomes', 'Ġaircraft', 'borne', 'Ġantenna', 'Ġoperation', 'Ġfour', 'Ġdistributed', 'Ġunited', 'Ġstates', 'Ġair', 'fields', 'Ġwell', 'Ġfive', 'Ġground', 'ground', 'Ġtest', 'Ġlocations', 'Ġlate', 'Ġspace', 'x', 'Ġtransitioning', 'Ġsatellite', 'Ġefforts', 'Ġresearch', 'Ġdevelopment', 'Ġmanufacturing', 'Ġplanned', 'Ġfirst', 'Ġlaunch', 'Ġlarge', 'Ġgroup', 'Ġsatellites', 'Ġorbit', 'Ġclear', 'Ġneed', 'Ġachieve', 'Ġaverage', 'Ġlaunch', 'Ġrate', 'Ġhigh', 'performance', 'Ġlow', 'cost', 'Ġspacecraft', 'Ġbuilt', 'Ġlaunched', 'Ġevery', 'Ġmonth', 'Ġnext', 'Ġmonths', 'Ġget', 'Ġsatellites', 'Ġlaunched', 'Ġsupport', 'Ġspectrum', 'Ġallocation', 'Ġlicense', 'Ġassignment', 'Ġspace', 'x', 'Ġsaid', 'Ġmeet', 'Ġdeadline', 'Ġhalf', 'Ġconstellation', 'Ġorbit', 'Ġwithin', 'Ġyears', 'Ġauthorization', '...', 'Ġfull', 'Ġsystem', 'Ġnine', 'Ġyears', '".[', 'Ġoct', 'ober', 'Ġunited', 'Ġstates', 'Ġsubmitted', 'Ġfilings', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', 'Ġspace', 'x', "'s", 'Ġbehalf', 'Ġarrange', 'Ġspectrum', '000', 'Ġadditional', 'Ġstar', 'link', 'Ġsatellites', 'Ġsupplement', '000', 'Ġstar', 'link', 'Ġsatellites', 'Ġalready', 'Ġapproved', 'Ġmonth', 'Ġmus', 'k', 'Ġpublicly', 'Ġtested', 'Ġstar', 'link', 'Ġnetwork', 'Ġusing', 'Ġinternet', 'Ġconnection', 'Ġrouted', 'Ġnetwork', 'Ġpost', 'Ġfirst', 'Ġtweet', 'Ġsocial', 'Ġmedia', 'Ġsite', 'Ġtwitter', 'Ġfirst', 'Ġlaunches', 'âĢĵ', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġearly', 'Ġstar', 'link', 'Ġuser', 'Ġterminal', 'Ġdish', 'Ġshipped', 'Ġearly', 'mber', 'Ġstar', 'link', 'Ġbeta', 'Ġinternet', 'Ġservice', 'Ġopened', 'Ġpublic', 'Ġstar', 'link', 'Ġbeta', 'Ġtesters', 'Ġreported', 'Ġspeeds', 'Ġmeg', 'ab', 'Ġper', 'Ġsecond', 'Ġrange', 'Ġannounced', 'Ġpublic', 'Ġbeta', 'Ġtest', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġopened', 'Ġpre', 'orders', 'Ġpublic', 'Ġspace', 'x', 'Ġcompleted', 'Ġraising', 'Ġadditional', 'Ġbillion', 'Ġequity', 'Ġfinancing', 'Ġprevious', 'Ġmonths', 'Ġsupport', 'Ġcapital', 'intensive', 'Ġphase', 'Ġoperational', 'Ġfielding', 'Ġstar', 'link', 'Ġplus', 'Ġdevelopment', 'Ġstarship', 'Ġlaunch', 'Ġsystem', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġclarified', 'Ġalready', 'Ġtested', 'Ġtwo', 'Ġgenerations', 'Ġstar', 'link', 'Ġtechnology', 'Ġsecond', 'Ġone', 'Ġless', 'Ġexpensive', 'Ġfirst', 'Ġthird', 'Ġgeneration', 'Ġlaser', 'Ġinter', 'atellite', 'Ġlinks', 'Ġexpected', 'Ġbegin', 'Ġlaunching', 'Ġnext', 'Ġmonths']</t>
+          <t>['Ġname', 'Ġinspired', 'Ġnovel', 'Ġfault', 'Ġstars', 'Ġstar', 'link', 'Ġpublicly', 'Ġannounced', 'Ġjan', 'uary', 'Ġopening', 'Ġspace', 'x', 'Ġsatellite', 'Ġdevelopment', 'Ġfacility', 'Ġred', 'mond', 'Ġwashing', 'ton', 'Ġopening', 'Ġmus', 'k', 'Ġstated', 'Ġstill', 'Ġsignificant', 'Ġun', 'met', 'Ġdemand', 'Ġworldwide', 'Ġlow', 'cost', 'Ġbroadband', 'Ġstar', 'link', 'Ġwould', 'Ġtarget', 'Ġbandwidth', 'Ġcarry', 'Ġback', 'haul', 'Ġcommunications', 'Ġtraffic', 'Ġlocal', 'Ġinternet', 'Ġtraffic', 'Ġhigh', 'density', 'Ġcities', 'Ġmus', 'k', 'Ġstated', 'Ġpositive', 'Ġcash', 'Ġflow', 'Ġselling', 'Ġsatellite', 'Ġinternet', 'Ġservices', 'Ġwould', 'Ġnecessary', 'Ġfund', 'Ġmars', 'Ġplans', 'Ġfurthermore', 'Ġspace', 'x', 'Ġlong', 'term', 'Ġplans', 'Ġdevelop', 'Ġdeploy', 'Ġversion', 'Ġsatellite', 'Ġcommunication', 'Ġsystem', 'Ġserve', 'Ġmars', 'Ġstarting', 'Ġengineers', 'Ġcompany', 'Ġoperated', '000', 'Ġft', 'Ġleased', 'Ġspace', 'Ġjan', 'uary', 'Ġtaken', '000', 'Ġft', 'Ġsecond', 'Ġfacility', 'Ġred', 'mond', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġconsolidated', 'Ġse', 'attle', 'area', 'Ġoperations', 'Ġmove', 'Ġlarger', 'Ġthree', 'building', 'Ġfacility', 'Ġred', 'mond', 'Ġridge', 'Ġcorporate', 'Ġcenter', 'Ġsupport', 'Ġsatellite', 'Ġmanufacturing', 'Ġaddition', 'Ġj', 'uly', 'Ġspace', 'x', 'Ġacquired', 'Ġadditional', '000', 'Ġft', 'Ġcreative', 'Ġspace', 'Ġir', 'vine', 'Ġcal', 'ornia', 'orange', 'Ġcounty', ').[', 'Ġir', 'vine', 'Ġoffice', 'Ġwould', 'Ġinclude', 'Ġsignal', 'Ġprocessing', 'Ġr', 'f', 'ic', 'ic', 'Ġdevelopment', 'Ġsatellite', 'Ġprogram', 'Ġoct', 'ober', 'Ġsatellite', 'Ġdivision', 'Ġfocusing', 'Ġsignificant', 'Ġbusiness', 'Ġchallenge', 'Ġachieving', 'Ġsufficiently', 'Ġlow', 'cost', 'Ġdesign', 'Ġuser', 'Ġequipment', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġsaid', 'Ġproject', 'Ġremained', 'design', 'Ġphase', 'Ġcompany', 'Ġseeks', 'Ġtackle', 'Ġissues', 'Ġrelated', 'Ġuser', 'termin', 'al', 'Ġcost', '".[', 'mber', 'Ġspace', 'x', 'Ġfiled', 'Ġapplication', 'non', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'ng', 'Ġsatellite', 'Ġsystem', 'Ġfixed', 'atellite', 'Ġservice', 'Ġusing', 'Ġka', 'Ġfrequency', 'Ġbands', '".[', 'Ġmarch', 'Ġspace', 'x', 'Ġfiled', 'Ġplans', 'Ġfield', 'Ġsecond', 'Ġorbital', 'Ġshell', 'v', 'band', 'Ġsatellites', 'Ġnon', 'ge', 'os', 'ynchronous', 'Ġorbits', 'Ġprovide', 'Ġcommunications', 'Ġservices', 'Ġelectromagnetic', 'Ġspectrum', 'Ġpreviously', 'Ġheavily', 'Ġemployed', 'Ġcommercial', 'Ġcommunications', 'Ġservices']</t>
         </is>
       </c>
       <c r="C399" t="n">
@@ -5625,7 +5625,7 @@
       </c>
       <c r="B400" t="inlineStr">
         <is>
-          <t>['Ġmuch', 'Ġless', 'Ġexpensive', 'Ġearlier', 'Ġversions', '".[', 'mber', 'Ġinnovation', 'Ġscience', 'Ġeconomic', 'Ġdevelopment', 'ada', 'Ġannounced', 'Ġregulatory', 'Ġapproval', 'Ġstar', 'link', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġconstellation', 'Ġinitially', 'Ġawarded', 'Ġspace', 'x', 'Ġmillion', 'Ġworth', 'Ġfederal', 'Ġsubsidies', 'Ġsupport', 'Ġrural', 'Ġbroadband', 'Ġcustomers', 'Ġcompany', "'s", 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġnetwork', 'Ġspace', 'x', 'Ġsubsidies', 'Ġbring', 'Ġservice', 'Ġcustomers', 'Ġu', 'Ġstates', 'Ġmillion', 'Ġaid', 'Ġpackage', 'Ġrevoked', 'Ġaug', 'ust', 'Ġstating', 'Ġstar', 'link', 'failed', 'Ġdemonstrate', 'Ġability', 'Ġdeliver', 'Ġpromised', 'Ġservice', 'Ġspace', 'x', 'Ġlater', 'Ġappealed', 'Ġdecision', 'Ġsaying', 'Ġmet', 'Ġsurpassed', 'Ġr', 'Ġdeployment', 'Ġrequirements', 'Ġexisted', 'Ġbidding', 'Ġcreated', 'new', 'Ġstandards', 'Ġbidder', 'Ġcould', 'Ġmeet', 'Ġtoday', '".[', 'Ġmarch', 'Ġspace', 'x', 'Ġsubmitted', 'Ġapplication', 'Ġmobile', 'Ġvariations', 'Ġterminal', 'Ġvehicles', 'Ġvessels', 'Ġaircraft', 'Ġmay', 'Ġspace', 'x', 'Ġannounced', 'Ġagreements', 'Ġgoogle', 'Ġcloud', 'Ġplatform', 'Ġmicro', 'soft', 'Ġaz', 'ure', 'Ġprovide', 'ground', 'Ġcompute', 'Ġnetworking', 'Ġservices', 'Ġstar', 'link', 'Ġv', 'ias', 'Ġmade', 'Ġlegal', 'Ġattempt', 'Ġtemporarily', 'Ġhalt', 'Ġstar', 'link', 'Ġlaunches', 'Ġj', 'une', 'Ġspace', 'x', 'Ġapplied', 'Ġuse', 'Ġmobile', 'Ġstar', 'link', 'Ġtrans', 'ce', 'ivers', 'Ġlaunch', 'Ġvehicles', 'Ġflying', 'Ġearth', 'Ġorbit', 'Ġpreviously', 'Ġtested', 'Ġhigh', 'alt', 'itude', 'Ġlow', 'vel', 'ocity', 'Ġmobile', 'Ġuse', 'Ġrocket', 'Ġprototype', 'Ġmay', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġsold', 'Ġstar', 'link', 'Ġpre', 'orders', 'Ġind', 'ia', 'Ġannounced', 'Ġsan', 'jay', 'Ġb', 'h', 'arg', 'ava', 'Ġworked', 'Ġmus', 'k', 'Ġpart', 'Ġteam', 'Ġfounded', 'Ġelectronic', 'Ġpayment', 'Ġfirm', 'Ġpay', 'pal', 'Ġwould', 'Ġhead', 'Ġtech', 'Ġbillionaire', 'Ġentrepreneur', "'s", 'Ġstar', 'link', 'Ġsatellite', 'Ġbroadband', 'Ġventure', 'Ġind', 'ia', 'Ġthree', 'Ġmonths', 'Ġlater', 'Ġb', 'h', 'arg', 'ava', 'Ġresigned', 'Ġpersonal', 'Ġreasons', 'Ġfollowing', 'Ġind', 'ian', 'Ġgovernment', 'Ġordering', 'Ġspace', 'x', 'Ġhalt', 'Ġselling', 'Ġpre', 'orders', 'Ġstar', 'link', 'Ġservice', 'Ġspace', 'x', 'Ġgains', 'Ġregulatory', 'Ġapproval', 'Ġproviding', 'Ġsatellite', 'Ġinternet', 'Ġservices', 'Ġcountry', 'Ġspace', 'x', 'Ġannounced', 'Ġstar', 'link', 'Ġbusiness', 'Ġservice', 'Ġtier', 'Ġhigher', 'Ġperformance', 'Ġedition', 'Ġservice', 'Ġprovides', 'Ġlarger', 'Ġhigh', 'performance', 'Ġantenna', 'Ġlisted', 'Ġspeeds', 'bit', 'Ġcost', 'Ġantenna', 'Ġmonthly', 'Ġservice']</t>
+          <t>['Ġcalled', 'low', 'Ġearth', 'Ġorbit', 'v', 'le', 'Ġconstellation', '",', 'Ġcomprised', 'Ġsatellites', 'Ġorbit', 'Ġmi', 'Ġaltitude', 'Ġsmaller', 'Ġoriginally', 'Ġplanned', 'Ġgroup', 'Ġsatellites', 'Ġwould', 'Ġoperate', 'Ġka', 'Ġk', 'u', 'bands', 'Ġorbit', 'Ġmi', 'Ġaltitude', 'Ġspace', 'x', 'Ġwithdrawn', 'Ġplans', 'Ġfield', 'atellite', 'Ġv', 'band', 'Ġsystem', 'Ġsupers', 'eding', 'Ġcomprehensive', 'Ġdesign', 'Ġsecond', 'generation', 'Ġstar', 'link', 'Ġnetwork', 'Ġse', 'pt', 'ember', 'Ġruled', 'Ġhalf', 'Ġconstellation', 'Ġmust', 'Ġorbit', 'Ġwithin', 'Ġyears', 'Ġcomply', 'Ġlicensing', 'Ġterms', 'Ġfull', 'Ġsystem', 'Ġorbit', 'Ġwithin', 'Ġnine', 'Ġyears', 'Ġdate', 'Ġlicense', 'Ġspace', 'x', 'Ġfiled', 'Ġdocuments', 'Ġlate', 'Ġclarify', 'Ġspace', 'Ġdebris', 'Ġmitigation', 'Ġplan', 'Ġcompany', 'Ġdesign', 'Ġphase', 'âĢĵ', 'Ġstart', 'Ġdevelopment', 'Ġphase', 'âĢĵ', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġfal', 'con', 'Ġlifts', 'Ġcape', 'aver', 'al', 'Ġair', 'Ġforce', 'Ġstation', 'cc', 'af', 'Ġfl', 'ida', 'Ġdelivering', 'Ġstar', 'link', 'Ġsatellites', 'Ġorbit', 'mber', 'im', 'plement', 'Ġoperations', 'Ġplan', 'Ġorderly', 'Ġde', 'orbit', 'Ġsatellites', 'Ġnearing', 'Ġend', 'Ġuseful', 'Ġlives', 'rough', 'ly', 'Ġfive', 'Ġseven', 'Ġyears', 'Ġrate', 'Ġfar', 'Ġfaster', 'Ġrequired', 'Ġinternational', 'Ġstandards', 'atell', 'ites', 'Ġde', 'orbit', 'Ġprop', 'uls', 'ively', 'Ġmoving', 'Ġdisposal', 'Ġorbit', 'enter', 'Ġearth', "'s", 'Ġatmosphere', 'Ġwithin', 'Ġapproximately', 'Ġone', 'Ġyear', 'Ġcompletion', 'Ġmission', '."[', 'Ġmarch', 'Ġgranted', 'Ġspace', 'x', 'Ġapproval', 'Ġinitial', 'Ġsatellites', 'Ġconditions', 'Ġspace', 'x', 'Ġwould', 'Ġneed', 'Ġobtain', 'Ġseparate', 'Ġapproval', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', ').[', 'Ġsupported', 'Ġn', 'asa', 'Ġrequest', 'Ġask', 'Ġspace', 'x', 'Ġachieve', 'Ġeven', 'Ġhigher', 'Ġlevel', 'Ġde', 'orb', 'iting', 'Ġreliability', 'Ġstandard', 'Ġn', 'asa', 'Ġpreviously', 'Ġused', 'Ġreliably', 'Ġde', 'orb', 'iting', 'Ġsatellites', 'Ġmissions', 'Ġcomplete', 'Ġmay', 'Ġspace', 'x', 'Ġexpected', 'Ġtotal', 'Ġcost', 'Ġdevelopment', 'Ġbuild', 'Ġconstellation', 'Ġapproach', 'Ġbillion']</t>
         </is>
       </c>
       <c r="C400" t="n">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="B401" t="inlineStr">
         <is>
-          <t>['Ġservice', 'Ġincludes', 'Ġpriorit', 'ized', 'Ġsupport', 'Ġdeliveries', 'Ġadvertised', 'Ġbegin', 'Ġsecond', 'Ġquarter', 'Ġalso', 'Ġapproved', 'Ġlicensing', 'Ġstar', 'link', 'Ġservices', 'Ġboats', 'Ġaircraft', 'Ġmoving', 'Ġvehicles', 'Ġstar', 'link', 'Ġterminal', 'Ġproduction', 'Ġdelayed', 'âĢĵ', 'present', 'Ġglobal', 'Ġchip', 'Ġshortage', 'Ġled', '000', 'Ġsubscribers', 'Ġfirst', 'Ġtwo', 'Ġmonths', 'Ġsoon', 'Ġresolved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġannounced', 'Ġstar', 'link', 'Ġsatellites', 'Ġactivated', 'Ġu', 'k', 'raine', 'Ġrequest', 'Ġu', 'k', 'rain', 'ian', 'Ġgovernment', 'Ġreplace', 'Ġinternet', 'Ġservices', 'Ġdestroyed', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġmay', 'Ġstar', 'link', 'Ġentered', 'Ġph', 'ilipp', 'ine', 'Ġmarket', 'Ġcompany', "'s", 'Ġfirst', 'Ġdeployment', 'ia', 'Ġdue', 'Ġlandmark', 'Ġlegislative', 'Ġchange', 'ra', 'Ġpublic', 'Ġservices', 'Ġact', 'foreign', 'Ġallowance', 'Ġcompany', 'Ġownership', 'Ġregards', 'Ġutility', 'Ġentities', 'Ġinternet', 'Ġtel', 'co', 'Ġcompanies', 'Ġstar', 'link', 'Ġable', 'Ġobtain', 'Ġprovisional', 'Ġpermission', 'Ġcountry', "'s", 'Ġdepartment', 'Ġinformation', 'Ġcommunication', 'Ġtechnologies', 'dict', 'Ġnational', 'Ġtelecommunications', 'Ġcommission', 'nt', 'c', 'Ġdepartment', 'Ġtrade', 'Ġindustry', 'ti', 'Ġsoon', 'Ġbegan', 'Ġcommercial', 'Ġservices', 'Ġaimed', 'Ġregions', 'Ġlower', 'Ġinternet', 'Ġconnectivity', 'Ġcommercial', 'Ġservice', 'âĢĵ', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġnumber', 'Ġstar', 'link', 'Ġsubscribers', 'Ġtime', 'Ġmonth', 'Ġnumber', 'Ġsubscribers', 'Ġsource', 'Ġfe', 'b', 'ruary', '000', 'Ġj', 'une', '000', 'Ġfe', 'b', 'ruary', '000', 'Ġmay', '000', 'Ġj', 'une', '000', 'Ġse', 'pt', 'ember', '000', 'Ġde', 'cember', '000', '000', 'Ġmay', '000', 'Ġalso', 'Ġmay', 'Ġch', 'inese', 'Ġmilitary', 'Ġresearchers', 'Ġpublished', 'Ġarticle', 'Ġpeer', 'reviewed', 'Ġjournal', 'Ġdescribing', 'Ġstrategy', 'Ġdestroying', 'Ġstar', 'link', 'Ġconstellation', 'Ġthreaten', 'Ġnational', 'Ġresearchers', 'Ġspecifically', 'Ġhighlight', 'Ġconcerns', 'Ġreported', 'Ġstar', 'link', 'Ġmilitary', 'Ġcapabilities', 'Ġmus', 'k', 'Ġlater', 'Ġannounced', 'st', 'arl', 'ink', 'Ġmeant', 'Ġpeaceful', 'Ġuse', '...', 'Ġmend', 'Ġfault', 'Ġstars', '",', 'Ġreferencing', 'Ġquote', 'Ġj', 'ul', 'ius', 'Ġca', 'esar', 'men', 'Ġtime', 'Ġmasters', 'Ġf', 'ates', 'Ġfault', 'Ġdear', 'Ġbrut', 'us', 'Ġstars']</t>
+          <t>['equ', 'ivalent', '000', '000', ').[', 'Ġmid', 'Ġspace', 'x', 'organized', 'Ġsatellite', 'Ġdevelopment', 'Ġdivision', 'Ġred', 'mond', 'Ġterminated', 'Ġseveral', 'Ġmembers', 'Ġsenior', 'Ġmanagement', 'mber', 'Ġspace', 'x', 'Ġreceived', 'Ġu', 'Ġregulatory', 'Ġapproval', 'Ġdeploy', 'Ġv', 'band', 'Ġbroadband', 'Ġsatellites', 'Ġaddition', 'Ġapproved', 'Ġearlier', 'Ġhowever', 'Ġv', 'band', 'Ġplans', 'Ġsubsequently', 'Ġwithdrawn', 'Ġtime', 'Ġspace', 'x', 'Ġalso', 'Ġmade', 'Ġnew', 'Ġregulatory', 'Ġfilings', 'Ġu', 'Ġrequest', 'Ġability', 'Ġalter', 'Ġpreviously', 'Ġgranted', 'Ġlicense', 'Ġorder', 'Ġoperate', 'Ġapproximately', 'Ġka', 'ku', 'band', 'Ġsatellites', 'Ġapproved', 'Ġoperation', 'Ġmi', 'new', 'Ġlower', 'Ġshell', 'Ġconstellation', 'Ġorbital', 'Ġaltitude', 'Ġsatellites', 'Ġwould', 'Ġeffectively', 'Ġoperate', 'Ġthird', 'Ġorbital', 'Ġshell', 'Ġmi', 'Ġorbit', 'Ġhigher', 'Ġlower', 'Ġorbits', 'Ġapproximately', 'Ġmi', 'Ġapproximately', 'Ġmi', 'Ġwould', 'Ġused', 'Ġlater', 'Ġconsiderably', 'Ġlarger', 'Ġdeployment', 'Ġsatellites', 'Ġbecomes', 'Ġpossible', 'Ġlater', 'Ġyears', 'Ġdeployment', 'Ġprocess', 'Ġapproved', 'Ġrequest', 'Ġapr', 'il', 'Ġgiving', 'Ġapproval', 'Ġplace', 'Ġnearly', '000', 'Ġsatellites', 'Ġthree', 'Ġorbital', 'Ġshells', 'Ġinitially', 'Ġapproximately', 'Ġmi', 'Ġaltitude', 'Ġshell', 'Ġsubsequently', 'Ġplacing', 'Ġapproximately', 'Ġka', 'band', 'Ġspectrum', 'Ġsatellites', 'Ġmi', 'Ġapproximately', 'Ġv', 'band', 'Ġsatellites', 'Ġtotal', 'Ġnearly', '000', 'Ġsatellites', 'Ġplanned', 'Ġdeployed', 'Ġpossible', 'Ġlater', 'Ġextension', '000', 'Ġfe', 'b', 'ruary', 'Ġsister', 'Ġcompany', 'Ġspace', 'x', 'Ġspace', 'x', 'Ġservices', 'Ġinc', '.,', 'Ġfiled', 'Ġrequest', 'Ġreceive', 'Ġlicense', 'Ġoperation', 'Ġmillion', 'Ġfixed', 'Ġsatellite', 'Ġearth', 'Ġstations', 'Ġwould', 'Ġcommunicate', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'ng', 'Ġsatellite', 'Ġstar', 'link', 'Ġsystem', 'Ġlaunching', 'Ġtwo', 'Ġtest', 'Ġsatellites', 'Ġfe', 'b', 'ruary', 'Ġfirst', 'Ġbatch', 'Ġoperational', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġmay', 'Ġj', 'une', 'Ġspace', 'x', 'Ġapplied', 'Ġlicense', 'Ġtest', 'Ġground', 'Ġterminals', 'Ġnationwide', 'Ġacross']</t>
         </is>
       </c>
       <c r="C401" t="n">
@@ -5651,7 +5651,7 @@
       </c>
       <c r="B402" t="inlineStr">
         <is>
-          <t>['lings', '."', 'Ġsuggesting', 'Ġstar', 'link', 'Ġcould', 'Ġenforce', 'Ġpeace', 'Ġtaking', 'Ġstrategic', 'Ġinitiative', 'Ġhead', 'Ġr', 'ussia', "'s", 'Ġspace', 'Ġagency', 'mit', 'ry', 'Ġro', 'go', 'zin', 'Ġearlier', 'Ġwarned', 'Ġmus', 'k', 'Ġanswer', 'Ġadult', 'Ġway', 'Ġel', 'Ġmatter', 'Ġplay', 'Ġspace', 'x', 'Ġunveiled', 'Ġnew', 'Ġvariants', 'Ġstar', 'link', 'Ġservice', 'Ġmay', 'Ġspace', 'x', 'Ġrolled', 'Ġstar', 'link', 'Ġservice', 'Ġlets', 'Ġcustomers', 'Ġpay', 'Ġskip', 'Ġwait', 'lists', 'Ġconnect', 'Ġbroadband', 'Ġsatellites', 'Ġwithout', 'Ġfixed', 'Ġaddress', 'Ġalthough', 'Ġconnection', 'Ġspeeds', 'Ġusers', 'Ġpriorit', 'ized', 'Ġj', 'uly', 'Ġspace', 'x', 'Ġannounced', 'Ġstar', 'link', 'Ġmaritime', 'Ġhelp', 'Ġsupport', 'Ġusers', 'Ġcompanies', 'Ġocean', 'Ġworking', 'Ġwater', 'Ġunable', 'Ġwork', 'Ġland', 'Ġadvertised', 'Ġspeed', 'Ġservice', 'Ġset', 'bit', 'Ġhowever', 'Ġcomes', 'Ġone', 'Ġtime', 'Ġprice', '000', 'Ġtwo', 'Ġuser', 'Ġterminals', '000', 'Ġmonthly', 'Ġprice', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġsecured', 'Ġfirst', 'Ġcontract', 'Ġservices', 'Ġpassenger', 'Ġshipping', 'Ġindustry', 'Ġroyal', 'Ġcar', 'ib', 'bean', 'Ġgroup', 'Ġadded', 'Ġstar', 'link', 'Ġinternet', 'Ġfreedom', 'Ġseas', 'Ġplans', 'Ġoffer', 'Ġservice', 'Ġships', 'Ġroyal', 'Ġcar', 'ib', 'bean', 'Ġinternational', 'Ġcelebrity', 'Ġcru', 'ises', 'Ġsil', 'verse', 'Ġcru', 'ises', 'Ġbrands', 'Ġmarch', 'Ġstar', 'link', 'Ġservices', 'Ġprivate', 'Ġjet', 'Ġcharter', 'Ġflights', 'Ġus', 'Ġexpected', 'Ġbegin', 'Ġlate', 'Ġhaw', 'ai', 'ian', 'Ġairlines', 'Ġcontracted', 'Ġprovide', 'st', 'arl', 'ink', 'Ġservices', 'Ġtrans', 'pac', 'ific', 'Ġflights', 'Ġhaw', 'aii', '."[', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġsent', 'Ġemail', 'Ġusers', 'Ġpre', 'orders', 'Ġservice', 'Ġcalled', 'Ġbest', 'Ġeffort', 'Ġallows', 'Ġstill', 'Ġwaiting', 'Ġfull', 'Ġcapacity', 'Ġcell', 'Ġreceive', 'Ġunused', 'Ġbandwidth', 'Ġcell', 'Ġstill', 'Ġwaiting', 'Ġlist', 'Ġpriorit', 'ized', 'Ġservice', 'Ġprice', 'Ġequipment', 'Ġresidential', 'Ġservice', 'Ġcoming', 'Ġper', 'Ġmonth', 'Ġde', 'cember', 'Ġmonthly', 'Ġdata', 'Ġcap', 'Ġintroduced', 'Ġsubscribers', 'Ġaccording', 'Ġinternet', 'Ġanalysis', 'Ġcompany', 'ok', 'la', 'Ġstar', 'link', 'Ġspeeds', 'Ġdegraded', 'Ġfirst', 'Ġhalf', 'Ġcustomers', 'Ġsigned', 'Ġservice', 'Ġspace', 'x', 'Ġsaid', 'Ġstar', 'link', 'Ġspeeds']</t>
+          <t>['Ġunited', 'Ġstates', 'Ġwashing', 'ton', 'Ġstate', 'Ġspace', 'x', 'Ġemployee', 'Ġhomes', 'Ġaircraft', 'borne', 'Ġantenna', 'Ġoperation', 'Ġfour', 'Ġdistributed', 'Ġunited', 'Ġstates', 'Ġair', 'fields', 'Ġwell', 'Ġfive', 'Ġground', 'ground', 'Ġtest', 'Ġlocations', 'Ġlate', 'Ġspace', 'x', 'Ġtransitioning', 'Ġsatellite', 'Ġefforts', 'Ġresearch', 'Ġdevelopment', 'Ġmanufacturing', 'Ġplanned', 'Ġfirst', 'Ġlaunch', 'Ġlarge', 'Ġgroup', 'Ġsatellites', 'Ġorbit', 'Ġclear', 'Ġneed', 'Ġachieve', 'Ġaverage', 'Ġlaunch', 'Ġrate', 'Ġhigh', 'performance', 'Ġlow', 'cost', 'Ġspacecraft', 'Ġbuilt', 'Ġlaunched', 'Ġevery', 'Ġmonth', 'Ġnext', 'Ġmonths', 'Ġget', 'Ġsatellites', 'Ġlaunched', 'Ġsupport', 'Ġspectrum', 'Ġallocation', 'Ġlicense', 'Ġassignment', 'Ġspace', 'x', 'Ġsaid', 'Ġmeet', 'Ġdeadline', 'Ġhalf', 'Ġconstellation', 'Ġorbit', 'Ġwithin', 'Ġyears', 'Ġauthorization', '...', 'Ġfull', 'Ġsystem', 'Ġnine', 'Ġyears', '".[', 'Ġoct', 'ober', 'Ġunited', 'Ġstates', 'Ġsubmitted', 'Ġfilings', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', 'Ġspace', 'x', "'s", 'Ġbehalf', 'Ġarrange', 'Ġspectrum', '000', 'Ġadditional', 'Ġstar', 'link', 'Ġsatellites', 'Ġsupplement', '000', 'Ġstar', 'link', 'Ġsatellites', 'Ġalready', 'Ġapproved', 'Ġmonth', 'Ġmus', 'k', 'Ġpublicly', 'Ġtested', 'Ġstar', 'link', 'Ġnetwork', 'Ġusing', 'Ġinternet', 'Ġconnection', 'Ġrouted', 'Ġnetwork', 'Ġpost', 'Ġfirst', 'Ġtweet', 'Ġsocial', 'Ġmedia', 'Ġsite', 'Ġtwitter', 'Ġfirst', 'Ġlaunches', 'âĢĵ', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġearly', 'Ġstar', 'link', 'Ġuser', 'Ġterminal', 'Ġdish', 'Ġshipped', 'Ġearly', 'mber', 'Ġstar', 'link', 'Ġbeta', 'Ġinternet', 'Ġservice', 'Ġopened', 'Ġpublic', 'Ġstar', 'link', 'Ġbeta', 'Ġtesters', 'Ġreported', 'Ġspeeds', 'Ġmeg', 'ab', 'Ġper', 'Ġsecond', 'Ġrange', 'Ġannounced', 'Ġpublic', 'Ġbeta', 'Ġtest', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġopened', 'Ġpre', 'orders', 'Ġpublic', 'Ġspace', 'x', 'Ġcompleted', 'Ġraising', 'Ġadditional', 'Ġbillion', 'Ġequity', 'Ġfinancing', 'Ġprevious', 'Ġmonths', 'Ġsupport', 'Ġcapital', 'intensive', 'Ġphase', 'Ġoperational', 'Ġfielding', 'Ġstar', 'link', 'Ġplus', 'Ġdevelopment', 'Ġstarship', 'Ġlaunch', 'Ġsystem', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġclarified', 'Ġalready', 'Ġtested', 'Ġtwo', 'Ġgenerations', 'Ġstar', 'link', 'Ġtechnology', 'Ġsecond', 'Ġone', 'Ġless', 'Ġexpensive', 'Ġfirst', 'Ġthird', 'Ġgeneration', 'Ġlaser', 'Ġinter', 'atellite', 'Ġlinks', 'Ġexpected', 'Ġbegin', 'Ġlaunching', 'Ġnext', 'Ġmonths']</t>
         </is>
       </c>
       <c r="C402" t="n">
@@ -5664,7 +5664,7 @@
       </c>
       <c r="B403" t="inlineStr">
         <is>
-          <t>['Ġimprove', 'Ġsatellites', 'Ġdeployed', 'Ġde', 'cember', 'Ġissued', 'Ġapproval', 'Ġspace', 'x', 'Ġlaunch', 'Ġinitial', 'Ġsatellites', 'Ġsecond', 'generation', 'Ġconstellation', 'Ġthree', 'Ġlow', 'earth', 'orbit', 'Ġorbital', 'Ġshells', 'Ġaltitude', 'Ġoverall', 'Ġspace', 'x', 'Ġrequested', 'Ġapproval', 'Ġmany', 'Ġsatellites', 'Ġapproximately', '000', 'âĢĵ', 'Ġaltitude', 'Ġshells', 'Ġplus', '000', 'âĢĵ', 'Ġshells', 'Ġnearly', '04', 'âĢĵ', 'km', 'Ġshells', 'Ġhowever', 'Ġnoted', 'Ġnet', 'Ġincrease', 'Ġapproved', 'orbit', 'Ġsatellites', 'Ġspace', 'x', 'Ġsince', 'Ġspace', 'x', 'Ġlonger', 'Ġplanning', 'Ġdeploy', 'Ġv', 'band', 'Ġsatellites', 'Ġmi', 'Ġaltitude', 'Ġpreviously', 'Ġauthorized', 'Ġmarch', 'Ġcompany', 'Ġreported', 'Ġmanufacturing', 'Ġstar', 'link', 'Ġmini', 'Ġsatellites', 'Ġper', 'Ġday', 'Ġwell', 'Ġthousands', 'Ġusers', 'Ġterminals', 'Ġmini', 'Ġstar', 'link', 'Ġsatellite', 'Ġfeatures', 'Ġassembled', 'Ġsmaller', 'Ġform', 'Ġfactor', 'Ġlarger', 'ats', 'Ġsatellites', 'Ġrequire', 'meter', 'iameter', 'Ġstarship', 'Ġorder', 'Ġlaunch', 'Ġstar', 'link', 'Ġbusiness', 'Ġunit', 'Ġsingle', 'Ġcash', 'flow', 'positive', 'Ġquarter', 'Ġexpecting', 'Ġprofitable', 'Ġj', 'une', 'Ġlicense', 'Ġoffer', 'Ġinternet', 'Ġservices', 'Ġz', 'amb', 'ia', 'Ġgranted', 'Ġstar', 'link', 'Ġz', 'amb', 'ian', 'Ġgovernment', 'Ġelectronic', 'Ġgovernment', 'Ġdivision', 'Ġsmart', 'Ġz', 'amb', 'ia', 'Ġfollowing', 'Ġcompletion', 'Ġmany', 'Ġprosperous', 'Ġtrial', 'Ġprojects', 'Ġthroughout', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġantenna', 'Ġdish', 'user', 'Ġterminal', 'Ġassembled', 'Ġstar', 'link', 'Ġwifi', 'Ġrouter', 'Ġj', 'uly', 'ong', 'ol', 'ian', 'Ġgovernment', 'Ġissued', 'Ġtwo', 'Ġlicenses', 'Ġspace', 'x', 'Ġprovide', 'Ġinternet', 'Ġaccess', 'Ġcountry', 'Ġstar', 'link', 'Ġprovides', 'Ġsatellite', 'based', 'Ġinternet', 'Ġconnectivity', 'Ġunders', 'erved', 'Ġareas', 'Ġplanet', 'Ġwell', 'Ġcompetitive', 'ly', 'Ġpriced', 'Ġservice', 'Ġurban', 'ized', 'Ġareas', 'Ġunited', 'Ġstates', 'Ġstar', 'link', 'Ġcharged', 'Ġlaunch', 'Ġone', 'time', 'Ġhardware', 'Ġfee', 'Ġuser', 'Ġterminal', 'Ġper', 'Ġmonth', 'Ġinternet', 'Ġservice', 'Ġfixed', 'Ġservice', 'Ġaddress', 'Ġlocation', 'Ġadditional', 'Ġper', 'Ġmonth', 'Ġallows', 'Ġuser', 'Ġterminal', 'Ġmove', 'Ġbeyond', 'Ġfixed', 'Ġlocation', 'st', 'arl', 'ink', 'Ġservice', 'Ġspeeds', 'Ġdep', 'rior', 'itized']</t>
+          <t>['Ġmuch', 'Ġless', 'Ġexpensive', 'Ġearlier', 'Ġversions', '".[', 'mber', 'Ġinnovation', 'Ġscience', 'Ġeconomic', 'Ġdevelopment', 'ada', 'Ġannounced', 'Ġregulatory', 'Ġapproval', 'Ġstar', 'link', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġconstellation', 'Ġinitially', 'Ġawarded', 'Ġspace', 'x', 'Ġmillion', 'Ġworth', 'Ġfederal', 'Ġsubsidies', 'Ġsupport', 'Ġrural', 'Ġbroadband', 'Ġcustomers', 'Ġcompany', "'s", 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġnetwork', 'Ġspace', 'x', 'Ġsubsidies', 'Ġbring', 'Ġservice', 'Ġcustomers', 'Ġu', 'Ġstates', 'Ġmillion', 'Ġaid', 'Ġpackage', 'Ġrevoked', 'Ġaug', 'ust', 'Ġstating', 'Ġstar', 'link', 'failed', 'Ġdemonstrate', 'Ġability', 'Ġdeliver', 'Ġpromised', 'Ġservice', 'Ġspace', 'x', 'Ġlater', 'Ġappealed', 'Ġdecision', 'Ġsaying', 'Ġmet', 'Ġsurpassed', 'Ġr', 'Ġdeployment', 'Ġrequirements', 'Ġexisted', 'Ġbidding', 'Ġcreated', 'new', 'Ġstandards', 'Ġbidder', 'Ġcould', 'Ġmeet', 'Ġtoday', '".[', 'Ġmarch', 'Ġspace', 'x', 'Ġsubmitted', 'Ġapplication', 'Ġmobile', 'Ġvariations', 'Ġterminal', 'Ġvehicles', 'Ġvessels', 'Ġaircraft', 'Ġmay', 'Ġspace', 'x', 'Ġannounced', 'Ġagreements', 'Ġgoogle', 'Ġcloud', 'Ġplatform', 'Ġmicro', 'soft', 'Ġaz', 'ure', 'Ġprovide', 'ground', 'Ġcompute', 'Ġnetworking', 'Ġservices', 'Ġstar', 'link', 'Ġv', 'ias', 'Ġmade', 'Ġlegal', 'Ġattempt', 'Ġtemporarily', 'Ġhalt', 'Ġstar', 'link', 'Ġlaunches', 'Ġj', 'une', 'Ġspace', 'x', 'Ġapplied', 'Ġuse', 'Ġmobile', 'Ġstar', 'link', 'Ġtrans', 'ce', 'ivers', 'Ġlaunch', 'Ġvehicles', 'Ġflying', 'Ġearth', 'Ġorbit', 'Ġpreviously', 'Ġtested', 'Ġhigh', 'alt', 'itude', 'Ġlow', 'vel', 'ocity', 'Ġmobile', 'Ġuse', 'Ġrocket', 'Ġprototype', 'Ġmay', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġsold', 'Ġstar', 'link', 'Ġpre', 'orders', 'Ġind', 'ia', 'Ġannounced', 'Ġsan', 'jay', 'Ġb', 'h', 'arg', 'ava', 'Ġworked', 'Ġmus', 'k', 'Ġpart', 'Ġteam', 'Ġfounded', 'Ġelectronic', 'Ġpayment', 'Ġfirm', 'Ġpay', 'pal', 'Ġwould', 'Ġhead', 'Ġtech', 'Ġbillionaire', 'Ġentrepreneur', "'s", 'Ġstar', 'link', 'Ġsatellite', 'Ġbroadband', 'Ġventure', 'Ġind', 'ia', 'Ġthree', 'Ġmonths', 'Ġlater', 'Ġb', 'h', 'arg', 'ava', 'Ġresigned', 'Ġpersonal', 'Ġreasons', 'Ġfollowing', 'Ġind', 'ian', 'Ġgovernment', 'Ġordering', 'Ġspace', 'x', 'Ġhalt', 'Ġselling', 'Ġpre', 'orders', 'Ġstar', 'link', 'Ġservice', 'Ġspace', 'x', 'Ġgains', 'Ġregulatory', 'Ġapproval', 'Ġproviding', 'Ġsatellite', 'Ġinternet', 'Ġservices', 'Ġcountry', 'Ġspace', 'x', 'Ġannounced', 'Ġstar', 'link', 'Ġbusiness', 'Ġservice', 'Ġtier', 'Ġhigher', 'Ġperformance', 'Ġedition', 'Ġservice', 'Ġprovides', 'Ġlarger', 'Ġhigh', 'performance', 'Ġantenna', 'Ġlisted', 'Ġspeeds', 'bit', 'Ġcost', 'Ġantenna', 'Ġmonthly', 'Ġservice']</t>
         </is>
       </c>
       <c r="C403" t="n">
@@ -5677,7 +5677,7 @@
       </c>
       <c r="B404" t="inlineStr">
         <is>
-          <t>['Ġcompared', 'Ġfixed', 'Ġusers', 'Ġarea', 'Ġfixed', 'Ġusers', 'Ġtold', 'Ġexpect', 'Ġtypical', 'Ġthroughput', 'Ġlatency', 'Ġms', 'Ġstudy', 'Ġfound', 'Ġusers', 'Ġaveraged', 'Ġdownload', 'Ġspeeds', 'Ġhigher', 'Ġperformance', 'Ġversion', 'Ġservice', 'st', 'arl', 'ink', 'Ġbusiness', 'Ġadvert', 'ises', 'Ġspeeds', 'bit', 'Ġexchange', 'Ġcostly', 'Ġuser', 'Ġterminal', 'Ġmonthly', 'Ġservice', 'Ġanother', 'Ġservice', 'Ġcalled', 'Ġstar', 'link', 'Ġmaritime', 'Ġbecame', 'Ġavailable', 'Ġj', 'uly', 'Ġproviding', 'Ġinternet', 'Ġaccess', 'Ġopen', 'Ġocean', 'Ġspeeds', 'bit', 'Ġrequiring', 'Ġpurchase', 'Ġmaritime', 'grade', '000', 'Ġuser', 'Ġterminal', '000', 'Ġmonthly', 'Ġservice', 'Ġsales', 'Ġcapped', 'Ġhundred', 'Ġfixed', 'Ġusers', 'Ġper', 'service', 'Ġcell', 'Ġarea', 'Ġdue', 'Ġlimited', 'Ġwireless', 'Ġcapacity', 'Ġstar', 'link', 'Ġalternatively', 'Ġoffers', 'Ġbest', 'Ġeffort', 'Ġservice', 'Ġtier', 'Ġallowing', 'Ġhomes', 'Ġcapped', 'Ġareas', 'Ġreceive', 'Ġcurrent', 'Ġunused', 'Ġbandwidth', 'Ġcell', 'Ġwaiting', 'Ġlist', 'Ġpriorit', 'ized', 'Ġservice', 'Ġprice', 'Ġequipment', 'Ġresidential', 'Ġservice', 'Ġper', 'Ġmonth', 'Ġimprove', 'Ġservice', 'Ġquality', 'Ġdensely', 'Ġpopulated', 'Ġareas', 'Ġstar', 'link', 'Ġintroduced', 'Ġmonthly', 'Ġdata', 'Ġcap', 'Ġnon', 'business', 'Ġusers', 'Ġbecame', 'Ġenforced', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġlowered', 'Ġmonthly', 'Ġservice', 'Ġcosts', 'Ġusers', 'Ġselect', 'Ġcountries', 'Ġexample', 'Ġusers', 'Ġb', 'razil', 'Ġch', 'ile', 'Ġsaw', 'Ġmonthly', 'Ġfee', 'Ġdecreases', 'Ġfe', 'b', 'ruary', 'Ġreported', 'Ġstar', 'link', '000', 'Ġsubscribers', 'Ġaust', 'ral', 'ia', 'Ġmay', 'Ġstar', 'link', 'Ġreported', 'Ġmillion', 'Ġactive', 'Ġsubscribers', 'Ġfuture', 'Ġservice', 'mobile', 'Ġus', 'Ġspace', 'x', 'Ġpartnering', 'Ġadd', 'Ġsatellite', 'Ġcellular', 'Ġservice', 'Ġcapability', 'Ġstar', 'link', 'Ġsatellites', 'Ġprovide', 'Ġdead', 'zone', 'Ġcell', 'Ġphone', 'Ġcoverage', 'Ġacross', 'Ġus', 'Ġusing', 'Ġexisting', 'Ġmid', 'band', 'Ġspectrum', 'mobile', 'Ġowns', 'Ġcell', 'Ġcoverage', 'Ġbegin', 'Ġmessaging', 'Ġexpand', 'Ġinclude', 'Ġvoice', 'Ġlimited', 'Ġdata', 'Ġservices', 'Ġlater', 'Ġtesting', 'Ġbegin', 'mobile', 'Ġplans', 'Ġconnect', 'Ġstar', 'link', 'Ġsatellites', 'Ġvia', 'Ġexisting', 'Ġmobile', 'Ġdevices', 'Ġunlike', 'Ġprevious', 'Ġgenerations', 'Ġsatellite', 'Ġphones', 'Ġused', 'Ġspecialized', 'Ġradios', 'Ġmod', 'ems', 'Ġantennas', 'Ġconnect', 'Ġsatellites', 'Ġhigher', 'Ġorbits', 'Ġbandwidth', 'Ġlimited', 'Ġapproximately', 'Ġmeg', 'ab', 'Ġper', 'Ġsecond', 'Ġtotal']</t>
+          <t>['Ġservice', 'Ġincludes', 'Ġpriorit', 'ized', 'Ġsupport', 'Ġdeliveries', 'Ġadvertised', 'Ġbegin', 'Ġsecond', 'Ġquarter', 'Ġalso', 'Ġapproved', 'Ġlicensing', 'Ġstar', 'link', 'Ġservices', 'Ġboats', 'Ġaircraft', 'Ġmoving', 'Ġvehicles', 'Ġstar', 'link', 'Ġterminal', 'Ġproduction', 'Ġdelayed', 'âĢĵ', 'present', 'Ġglobal', 'Ġchip', 'Ġshortage', 'Ġled', '000', 'Ġsubscribers', 'Ġfirst', 'Ġtwo', 'Ġmonths', 'Ġsoon', 'Ġresolved', 'Ġfe', 'b', 'ruary', 'Ġmus', 'k', 'Ġannounced', 'Ġstar', 'link', 'Ġsatellites', 'Ġactivated', 'Ġu', 'k', 'raine', 'Ġrequest', 'Ġu', 'k', 'rain', 'ian', 'Ġgovernment', 'Ġreplace', 'Ġinternet', 'Ġservices', 'Ġdestroyed', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġmay', 'Ġstar', 'link', 'Ġentered', 'Ġph', 'ilipp', 'ine', 'Ġmarket', 'Ġcompany', "'s", 'Ġfirst', 'Ġdeployment', 'ia', 'Ġdue', 'Ġlandmark', 'Ġlegislative', 'Ġchange', 'ra', 'Ġpublic', 'Ġservices', 'Ġact', 'foreign', 'Ġallowance', 'Ġcompany', 'Ġownership', 'Ġregards', 'Ġutility', 'Ġentities', 'Ġinternet', 'Ġtel', 'co', 'Ġcompanies', 'Ġstar', 'link', 'Ġable', 'Ġobtain', 'Ġprovisional', 'Ġpermission', 'Ġcountry', "'s", 'Ġdepartment', 'Ġinformation', 'Ġcommunication', 'Ġtechnologies', 'dict', 'Ġnational', 'Ġtelecommunications', 'Ġcommission', 'nt', 'c', 'Ġdepartment', 'Ġtrade', 'Ġindustry', 'ti', 'Ġsoon', 'Ġbegan', 'Ġcommercial', 'Ġservices', 'Ġaimed', 'Ġregions', 'Ġlower', 'Ġinternet', 'Ġconnectivity', 'Ġcommercial', 'Ġservice', 'âĢĵ', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġnumber', 'Ġstar', 'link', 'Ġsubscribers', 'Ġtime', 'Ġmonth', 'Ġnumber', 'Ġsubscribers', 'Ġsource', 'Ġfe', 'b', 'ruary', '000', 'Ġj', 'une', '000', 'Ġfe', 'b', 'ruary', '000', 'Ġmay', '000', 'Ġj', 'une', '000', 'Ġse', 'pt', 'ember', '000', 'Ġde', 'cember', '000', '000', 'Ġmay', '000', 'Ġalso', 'Ġmay', 'Ġch', 'inese', 'Ġmilitary', 'Ġresearchers', 'Ġpublished', 'Ġarticle', 'Ġpeer', 'reviewed', 'Ġjournal', 'Ġdescribing', 'Ġstrategy', 'Ġdestroying', 'Ġstar', 'link', 'Ġconstellation', 'Ġthreaten', 'Ġnational', 'Ġresearchers', 'Ġspecifically', 'Ġhighlight', 'Ġconcerns', 'Ġreported', 'Ġstar', 'link', 'Ġmilitary', 'Ġcapabilities', 'Ġmus', 'k', 'Ġlater', 'Ġannounced', 'st', 'arl', 'ink', 'Ġmeant', 'Ġpeaceful', 'Ġuse', '...', 'Ġmend', 'Ġfault', 'Ġstars', '",', 'Ġreferencing', 'Ġquote', 'Ġj', 'ul', 'ius', 'Ġca', 'esar', 'men', 'Ġtime', 'Ġmasters', 'Ġf', 'ates', 'Ġfault', 'Ġdear', 'Ġbrut', 'us', 'Ġstars']</t>
         </is>
       </c>
       <c r="C404" t="n">
@@ -5690,7 +5690,7 @@
       </c>
       <c r="B405" t="inlineStr">
         <is>
-          <t>['Ġsplit', 'Ġacross', 'Ġlarge', 'Ġcell', 'Ġcoverage', 'Ġarea', 'Ġlimited', 'Ġapproximately', '000', 'Ġvoice', 'Ġcall', 'ers', 'Ġcell', 'Ġsize', 'Ġsingle', 'Ġcoverage', 'Ġcell', 'Ġyet', 'Ġpublicly', 'Ġreleased', 'Ġsatellites', 'Ġmeters', 'Ġlong', 'Ġantenna', 'Ġwould', 'Ġfold', 'rough', 'ly', 'Ġsquare', 'Ġmeters', '".[', 'Ġmarch', 'Ġspace', 'x', 'Ġconfirmed', 'Ġremain', 'Ġtrack', 'Ġbegin', 'Ġtesting', 'Ġservice', 'Ġapr', 'il', 'Ġone', 'formerly', 'Ġv', 'od', 'af', 'one', 'Ġnew', 'Ġzeal', 'Ġannounced', 'Ġwould', 'Ġpartnering', 'Ġspace', 'x', "'s", 'Ġstar', 'link', 'Ġprovide', 'Ġmobile', 'Ġnetwork', 'Ġcoverage', 'Ġnew', 'Ġzeal', 'Ġsm', 'Ġtext', 'Ġservice', 'Ġexpected', 'Ġbegin', 'Ġvoice', 'Ġdata', 'Ġfunctionality', 'Ġcoming', 'Ġj', 'uly', 'Ġopt', 'us', 'Ġaust', 'ral', 'ia', 'Ġannounced', 'Ġsimilar', 'Ġpartnership', 'Ġservices', 'Ġsatellite', 'Ġinternet', 'Ġsatellite', 'Ġcellular', 'Ġservice', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġel', 'Ġmus', 'k', 'Ġfour', 'star', 'Ġgeneral', 'Ġter', 'rence', 'Ġj', "'s", 'h', 'augh', 'ness', 'Ġapr', 'il', 'Ġfuture', 'Ġsecretary', 'Ġdefense', 'Ġresearch', 'Ġengineering', 'ichael', 'Ġgr', 'ï', '¬', 'ģ', 'n', 'Ġmeets', 'Ġel', 'Ġmus', 'k', 'Ġl', 'arry', 'iam', 'Ġformer', 'Ġtel', 'edes', 'ic', 'Ġspace', 'x', 'Ġalso', 'Ġdesigns', 'Ġbuilds', 'Ġlaunches', 'Ġcustomized', 'Ġmilitary', 'Ġsatellites', 'Ġbased', 'Ġvariants', 'Ġstar', 'link', 'Ġsatellite', 'Ġbus', 'Ġlargest', 'Ġpublicly', 'Ġknown', 'Ġcustomer', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'da', 'da', 'Ġformed', 'Ġpart', 'Ġtrump', 'Ġadministration', 'Ġeffort', 'Ġresurrect', 'agan', 'era', 'Ġstrategic', 'Ġdefense', 'Ġinitiative', 'di', ').[', 'da', 'Ġacceler', 'ates', 'Ġdevelopment', 'Ġmissile', 'Ġdefense', 'Ġcapabilities', 'Ġusing', 'Ġindustry', 'proc', 'ured', 'Ġlow', 'cost', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġplatforms', 'Ġprogram', 'Ġconceived', 'Ġinstituted', 'Ġsecretary', 'Ġdefense', 'r', 'e', 'ichael', 'Ġgr', 'iffin', 'Ġdecades', 'Ġearlier', 'Ġjoined', 'Ġmus', 'k', 'Ġtrip', 'Ġr', 'ussia', 'Ġexamine', 'Ġpart', 'Ġspace', 'x', "'s", 'Ġfounding', ').[', 'Ġmonths', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġannounced', 'Ġspace', 'x', 'Ġchief', 'Ġoperating', 'Ġofficer', 'Ġshot', 'well', 'Ġasked', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġgiven', 'Ġnature', 'Ġprogram', 'Ġwhether', 'Ġspace', 'x', 'Ġwould', 'Ġlaunch', 'Ġweapons', 'Ġspace', 'Ġus', 'Ġmilitary', 'Ġaffirmed', 'Ġwould', "'s", 'Ġdefense', 'Ġcountry', '."[']</t>
+          <t>['lings', '."', 'Ġsuggesting', 'Ġstar', 'link', 'Ġcould', 'Ġenforce', 'Ġpeace', 'Ġtaking', 'Ġstrategic', 'Ġinitiative', 'Ġhead', 'Ġr', 'ussia', "'s", 'Ġspace', 'Ġagency', 'mit', 'ry', 'Ġro', 'go', 'zin', 'Ġearlier', 'Ġwarned', 'Ġmus', 'k', 'Ġanswer', 'Ġadult', 'Ġway', 'Ġel', 'Ġmatter', 'Ġplay', 'Ġspace', 'x', 'Ġunveiled', 'Ġnew', 'Ġvariants', 'Ġstar', 'link', 'Ġservice', 'Ġmay', 'Ġspace', 'x', 'Ġrolled', 'Ġstar', 'link', 'Ġservice', 'Ġlets', 'Ġcustomers', 'Ġpay', 'Ġskip', 'Ġwait', 'lists', 'Ġconnect', 'Ġbroadband', 'Ġsatellites', 'Ġwithout', 'Ġfixed', 'Ġaddress', 'Ġalthough', 'Ġconnection', 'Ġspeeds', 'Ġusers', 'Ġpriorit', 'ized', 'Ġj', 'uly', 'Ġspace', 'x', 'Ġannounced', 'Ġstar', 'link', 'Ġmaritime', 'Ġhelp', 'Ġsupport', 'Ġusers', 'Ġcompanies', 'Ġocean', 'Ġworking', 'Ġwater', 'Ġunable', 'Ġwork', 'Ġland', 'Ġadvertised', 'Ġspeed', 'Ġservice', 'Ġset', 'bit', 'Ġhowever', 'Ġcomes', 'Ġone', 'Ġtime', 'Ġprice', '000', 'Ġtwo', 'Ġuser', 'Ġterminals', '000', 'Ġmonthly', 'Ġprice', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġsecured', 'Ġfirst', 'Ġcontract', 'Ġservices', 'Ġpassenger', 'Ġshipping', 'Ġindustry', 'Ġroyal', 'Ġcar', 'ib', 'bean', 'Ġgroup', 'Ġadded', 'Ġstar', 'link', 'Ġinternet', 'Ġfreedom', 'Ġseas', 'Ġplans', 'Ġoffer', 'Ġservice', 'Ġships', 'Ġroyal', 'Ġcar', 'ib', 'bean', 'Ġinternational', 'Ġcelebrity', 'Ġcru', 'ises', 'Ġsil', 'verse', 'Ġcru', 'ises', 'Ġbrands', 'Ġmarch', 'Ġstar', 'link', 'Ġservices', 'Ġprivate', 'Ġjet', 'Ġcharter', 'Ġflights', 'Ġus', 'Ġexpected', 'Ġbegin', 'Ġlate', 'Ġhaw', 'ai', 'ian', 'Ġairlines', 'Ġcontracted', 'Ġprovide', 'st', 'arl', 'ink', 'Ġservices', 'Ġtrans', 'pac', 'ific', 'Ġflights', 'Ġhaw', 'aii', '."[', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġsent', 'Ġemail', 'Ġusers', 'Ġpre', 'orders', 'Ġservice', 'Ġcalled', 'Ġbest', 'Ġeffort', 'Ġallows', 'Ġstill', 'Ġwaiting', 'Ġfull', 'Ġcapacity', 'Ġcell', 'Ġreceive', 'Ġunused', 'Ġbandwidth', 'Ġcell', 'Ġstill', 'Ġwaiting', 'Ġlist', 'Ġpriorit', 'ized', 'Ġservice', 'Ġprice', 'Ġequipment', 'Ġresidential', 'Ġservice', 'Ġcoming', 'Ġper', 'Ġmonth', 'Ġde', 'cember', 'Ġmonthly', 'Ġdata', 'Ġcap', 'Ġintroduced', 'Ġsubscribers', 'Ġaccording', 'Ġinternet', 'Ġanalysis', 'Ġcompany', 'ok', 'la', 'Ġstar', 'link', 'Ġspeeds', 'Ġdegraded', 'Ġfirst', 'Ġhalf', 'Ġcustomers', 'Ġsigned', 'Ġservice', 'Ġspace', 'x', 'Ġsaid', 'Ġstar', 'link', 'Ġspeeds']</t>
         </is>
       </c>
       <c r="C405" t="n">
@@ -5703,7 +5703,7 @@
       </c>
       <c r="B406" t="inlineStr">
         <is>
-          <t>['Ġoct', 'ober', 'da', 'Ġawarded', 'Ġspace', 'x', 'Ġinitial', 'Ġmillion', 'Ġdual', 'use', 'Ġcontract', 'Ġdevelop', 'Ġsatellites', 'Ġdetect', 'Ġtrack', 'Ġballistic', 'Ġhyp', 'erson', 'ic', 'Ġmissiles', 'Ġfirst', 'Ġbatch', 'Ġsatellites', 'Ġoriginally', 'Ġscheduled', 'Ġlaunch', 'Ġse', 'pt', 'ember', 'Ġform', 'Ġpart', 'Ġtracking', 'Ġlayer', 'Ġtr', 'anche', 'Ġspace', 'Ġforce', "'s", 'Ġnational', 'Ġdefense', 'Ġspace', 'Ġarchitecture', 'Ġlaunch', 'Ġschedule', 'Ġslipped', 'Ġmultiple', 'Ġtimes', 'Ġeventually', 'Ġlaunched', 'Ġapr', 'il', 'Ġn', 'ds', 'Ġcomposed', 'Ġseven', 'Ġlayers', 'Ġspecific', 'Ġfunctions', 'Ġdata', 'Ġtransport', 'Ġbattle', 'Ġmanagement', 'Ġmissile', 'Ġtracking', 'Ġcustody', 'weapons', 'Ġtargeting', 'Ġsatellite', 'Ġnavigation', 'Ġdeterrence', 'Ġground', 'Ġsupport', 'Ġhistorically', 'Ġspace', 'based', 'Ġmissile', 'Ġdefense', 'Ġconcepts', 'Ġexpensive', 'Ġreusable', 'Ġlaunch', 'Ġsystems', 'Ġmit', 'igated', 'Ġcosts', 'Ġaccording', 'Ġcongressional', 'Ġbudget', 'Ġoffice', 'Ġanalysis', 'Ġns', 'da', 'Ġlever', 'ages', 'Ġexisting', 'Ġcommercial', 'Ġsatellite', 'Ġbus', 'Ġdevelopment', 'Ġstar', 'link', 'Ġreduce', 'Ġcosts', 'Ġincluding', 'Ġfree', 'space', 'Ġoptical', 'Ġlaser', 'Ġterminals', 'Ġsecure', 'Ġcommand', 'Ġcontrol', 'Ġmesh', 'Ġnetwork', 'Ġmissile', 'Ġdefense', 'Ġreview', 'Ġnotes', 'Ġspace', 'based', 'Ġsensing', 'Ġenables', 'impro', 'ved', 'Ġtracking', 'Ġpotentially', 'Ġtargeting', 'Ġadvanced', 'Ġthreats', 'Ġincluding', 'Ġhyp', 'erson', 'ic', 'Ġcruise', 'Ġmissiles', '".[', 'Ġhowever', 'Ġunion', 'Ġconcerned', 'Ġscientists', 'Ġwarns', 'Ġdevelopments', 'Ġcould', 'Ġescalate', 'Ġtensions', 'Ġr', 'ussia', 'Ġch', 'ina', 'Ġcalled', 'Ġproject', 'fund', 'ament', 'ally', 'Ġcar', 'negie', 'Ġend', 'owment', 'Ġinternational', 'Ġpeace', 'Ġlater', 'Ġadvocated', 'Ġtreaty', 'Ġhalting', 'Ġdevelopment', 'Ġprevent', 'Ġarms', 'Ġrace', 'Ġspace', 'Ġsince', 'Ġstar', 'link', "'s", 'Ġmilitary', 'Ġsatellite', 'Ġdevelopment', 'Ġoverseen', 'Ġinternally', 'Ġspace', 'x', 'Ġretired', 'Ġfour', 'star', 'Ġgeneral', 'Ġter', 'rence', 'Ġj', "'s", 'h', 'augh', 'ness', 'Ġadvocated', 'Ġunited', 'Ġstates', 'Ġsenate', 'Ġcommittee', 'Ġarmed', 'Ġservices', 'Ġlayered', 'Ġcapability', 'Ġlethal', 'Ġfollow', 'Ġincorporates', 'Ġmachine', 'Ġlearning', 'Ġartificial', 'Ġintelligence', 'Ġgather', 'Ġact', 'Ġupon', 'Ġsensor', 'Ġdata', 'Ġquickly', 'Ġspace', 'x', 'Ġawarded', 'Ġcontract', 'Ġlarger', 'Ġtr', 'anche', 'Ġawards', 'Ġgoing', 'ork', 'Ġspace', 'Ġsystems', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġsystems', '].', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġannounced', 'Ġst', 'arsh', 'ield', 'Ġprogram', 'Ġincorporate', 'Ġmilitary', 'Ġgovernment', 'Ġentity', 'Ġpayload', 'Ġboard', 'Ġcustomized', 'Ġsatellite', 'Ġbus', 'pot', 'entially', 'Ġbased', 'Ġstar', 'link', 'Ġblock', 'Ġtechnology', ']).', 'Ġsatellites', 'Ġheavier', 'Ġtwice', 'Ġarea', 'Ġsingle', 'Ġstar', 'link', 'Ġtwo', 'Ġpair', 'Ġsolar', 'Ġarrays', 'Ġopposed', 'Ġone', 'Ġstar', 'link', 'Ġblock', 'Ġv']</t>
+          <t>['Ġimprove', 'Ġsatellites', 'Ġdeployed', 'Ġde', 'cember', 'Ġissued', 'Ġapproval', 'Ġspace', 'x', 'Ġlaunch', 'Ġinitial', 'Ġsatellites', 'Ġsecond', 'generation', 'Ġconstellation', 'Ġthree', 'Ġlow', 'earth', 'orbit', 'Ġorbital', 'Ġshells', 'Ġaltitude', 'Ġoverall', 'Ġspace', 'x', 'Ġrequested', 'Ġapproval', 'Ġmany', 'Ġsatellites', 'Ġapproximately', '000', 'âĢĵ', 'Ġaltitude', 'Ġshells', 'Ġplus', '000', 'âĢĵ', 'Ġshells', 'Ġnearly', '04', 'âĢĵ', 'km', 'Ġshells', 'Ġhowever', 'Ġnoted', 'Ġnet', 'Ġincrease', 'Ġapproved', 'orbit', 'Ġsatellites', 'Ġspace', 'x', 'Ġsince', 'Ġspace', 'x', 'Ġlonger', 'Ġplanning', 'Ġdeploy', 'Ġv', 'band', 'Ġsatellites', 'Ġmi', 'Ġaltitude', 'Ġpreviously', 'Ġauthorized', 'Ġmarch', 'Ġcompany', 'Ġreported', 'Ġmanufacturing', 'Ġstar', 'link', 'Ġmini', 'Ġsatellites', 'Ġper', 'Ġday', 'Ġwell', 'Ġthousands', 'Ġusers', 'Ġterminals', 'Ġmini', 'Ġstar', 'link', 'Ġsatellite', 'Ġfeatures', 'Ġassembled', 'Ġsmaller', 'Ġform', 'Ġfactor', 'Ġlarger', 'ats', 'Ġsatellites', 'Ġrequire', 'meter', 'iameter', 'Ġstarship', 'Ġorder', 'Ġlaunch', 'Ġstar', 'link', 'Ġbusiness', 'Ġunit', 'Ġsingle', 'Ġcash', 'flow', 'positive', 'Ġquarter', 'Ġexpecting', 'Ġprofitable', 'Ġj', 'une', 'Ġlicense', 'Ġoffer', 'Ġinternet', 'Ġservices', 'Ġz', 'amb', 'ia', 'Ġgranted', 'Ġstar', 'link', 'Ġz', 'amb', 'ian', 'Ġgovernment', 'Ġelectronic', 'Ġgovernment', 'Ġdivision', 'Ġsmart', 'Ġz', 'amb', 'ia', 'Ġfollowing', 'Ġcompletion', 'Ġmany', 'Ġprosperous', 'Ġtrial', 'Ġprojects', 'Ġthroughout', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġantenna', 'Ġdish', 'user', 'Ġterminal', 'Ġassembled', 'Ġstar', 'link', 'Ġwifi', 'Ġrouter', 'Ġj', 'uly', 'ong', 'ol', 'ian', 'Ġgovernment', 'Ġissued', 'Ġtwo', 'Ġlicenses', 'Ġspace', 'x', 'Ġprovide', 'Ġinternet', 'Ġaccess', 'Ġcountry', 'Ġstar', 'link', 'Ġprovides', 'Ġsatellite', 'based', 'Ġinternet', 'Ġconnectivity', 'Ġunders', 'erved', 'Ġareas', 'Ġplanet', 'Ġwell', 'Ġcompetitive', 'ly', 'Ġpriced', 'Ġservice', 'Ġurban', 'ized', 'Ġareas', 'Ġunited', 'Ġstates', 'Ġstar', 'link', 'Ġcharged', 'Ġlaunch', 'Ġone', 'time', 'Ġhardware', 'Ġfee', 'Ġuser', 'Ġterminal', 'Ġper', 'Ġmonth', 'Ġinternet', 'Ġservice', 'Ġfixed', 'Ġservice', 'Ġaddress', 'Ġlocation', 'Ġadditional', 'Ġper', 'Ġmonth', 'Ġallows', 'Ġuser', 'Ġterminal', 'Ġmove', 'Ġbeyond', 'Ġfixed', 'Ġlocation', 'st', 'arl', 'ink', 'Ġservice', 'Ġspeeds', 'Ġdep', 'rior', 'itized']</t>
         </is>
       </c>
       <c r="C406" t="n">
@@ -5716,7 +5716,7 @@
       </c>
       <c r="B407" t="inlineStr">
         <is>
-          <t>['Ġstar', 'link', 'Ġdesigned', 'Ġconsumer', 'Ġcommercial', 'Ġuse', 'Ġst', 'arsh', 'ield', 'Ġdesigned', 'Ġus', 'Ġgovernment', 'Ġuse', 'Ġinitial', 'Ġfocus', 'Ġthree', 'Ġareas', 'Ġnamely', 'Ġearth', 'Ġobservation', 'Ġcommunications', 'Ġhosting', 'Ġpayload', 'Ġmilitary', 'Ġsatellites', 'Ġst', 'arsh', 'ield', 'Ġprogram', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġvital', 'Ġk', 'l', 'itsch', 'ko', 'Ġmayor', 'Ġk', 'iv', 'Ġbrother', 'Ġw', 'lad', 'imir', 'Ġk', 'l', 'itsch', 'ko', 'Ġstar', 'link', 'Ġterminals', 'Ġshipped', 'Ġk', 'iv', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġdesigned', 'Ġmeet', 'Ġdiverse', 'Ġmission', 'Ġrequirements', 'Ġst', 'arsh', 'ield', 'Ġsatellites', 'Ġadvertised', 'Ġcapable', 'Ġintegrating', 'Ġwide', 'Ġvariety', 'Ġpayload', 'Ġoffering', 'Ġunique', 'Ġversatility', 'Ġusers', 'Ġst', 'arsh', 'ield', 'Ġsatellites', 'Ġcompatible', 'Ġinter', 'connect', 'Ġexisting', 'Ġcommercial', 'Ġstar', 'link', 'Ġsatellites', 'Ġvia', 'Ġoptical', 'Ġinter', 'atellite', 'Ġlinks', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġdeployed', 'Ġfour', 'Ġnational', 'Ġsecurity', 'Ġsatellites', 'Ġus', 'Ġgovernment', 'Ġtransporter', 'Ġrides', 'hare', 'Ġmission', 'Ġyear', 'Ġlaunched', 'Ġanother', 'Ġgroup', 'Ġfour', 'Ġu', 'Ġsatellites', 'Ġsingle', 'orbit', 'Ġspare', 'Ġglobal', 'star', 'Ġsatellite', 'Ġpurpose', 'Ġdisclosed', 'Ġtime', 'Ġlaunch', 'Ġconsidered', 'Ġlikely', 'Ġeither', 'Ġtechnical', 'Ġdemonstration', 'Ġcommunications', 'Ġearth', 'Ġobservation', 'Ġsignals', 'Ġintelligence', 'Ġsuspected', 'Ġper', 'Ġimages', 'Ġtwo', 'Ġspace', 'x', 'built', 'Ġstar', 'link', 'Ġderived', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġtr', 'anche', 'Ġflight', 'Ġtracking', 'Ġlayer', 'Ġinfrared', 'Ġimaging', 'Ġsatellites', 'Ġlaunched', 'Ġapr', 'il', 'Ġalso', 'Ġbased', 'Ġst', 'arsh', 'ield', 'Ġsatellite', 'Ġbus', 'Ġtests', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'af', 'rl', 'Ġdemonstrated', 'bit', 'Ġdata', 'Ġlink', 'Ġstar', 'link', 'ech', 'craft', 'Ġhur', 'Ġaircraft', 'Ġflight', 'Ġadditionally', 'Ġlate', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġsuccessfully', 'Ġtested', 'Ġconnection', 'Ġstar', 'link', 'Ġguns', 'hip', 'Ġair', 'Ġforce', 'Ġutilized', 'Ġstar', 'link', 'Ġsupport', 'Ġadvanced', 'Ġbattlefield', 'Ġmanagement', 'Ġsystem', 'Ġlive', 'fire', 'Ġexercise', 'Ġdemonstrated', 'Ġstar', 'link', 'Ġconnected', 'var', 'iety', 'Ġair', 'Ġterrestrial', 'Ġassets', 'Ġincluding', 'Ġbo', 'e', 'ing', 'Ġstrat', 'ot', 'ank', 'er', 'Ġexpert', 'Ġbattlefield', 'Ġcommunications', 'Ġth', 'omas', 'Ġwell', 'ington', 'Ġargues', 'Ġstar', 'link', 'Ġsignals', 'Ġuse', 'Ġnarrow', 'Ġfocused', 'Ġbeams', 'Ġless', 'Ġvulnerable', 'Ġinterference', 'Ġjam', 'ming', 'Ġenemy', 'Ġwartime']</t>
+          <t>['Ġcompared', 'Ġfixed', 'Ġusers', 'Ġarea', 'Ġfixed', 'Ġusers', 'Ġtold', 'Ġexpect', 'Ġtypical', 'Ġthroughput', 'Ġlatency', 'Ġms', 'Ġstudy', 'Ġfound', 'Ġusers', 'Ġaveraged', 'Ġdownload', 'Ġspeeds', 'Ġhigher', 'Ġperformance', 'Ġversion', 'Ġservice', 'st', 'arl', 'ink', 'Ġbusiness', 'Ġadvert', 'ises', 'Ġspeeds', 'bit', 'Ġexchange', 'Ġcostly', 'Ġuser', 'Ġterminal', 'Ġmonthly', 'Ġservice', 'Ġanother', 'Ġservice', 'Ġcalled', 'Ġstar', 'link', 'Ġmaritime', 'Ġbecame', 'Ġavailable', 'Ġj', 'uly', 'Ġproviding', 'Ġinternet', 'Ġaccess', 'Ġopen', 'Ġocean', 'Ġspeeds', 'bit', 'Ġrequiring', 'Ġpurchase', 'Ġmaritime', 'grade', '000', 'Ġuser', 'Ġterminal', '000', 'Ġmonthly', 'Ġservice', 'Ġsales', 'Ġcapped', 'Ġhundred', 'Ġfixed', 'Ġusers', 'Ġper', 'service', 'Ġcell', 'Ġarea', 'Ġdue', 'Ġlimited', 'Ġwireless', 'Ġcapacity', 'Ġstar', 'link', 'Ġalternatively', 'Ġoffers', 'Ġbest', 'Ġeffort', 'Ġservice', 'Ġtier', 'Ġallowing', 'Ġhomes', 'Ġcapped', 'Ġareas', 'Ġreceive', 'Ġcurrent', 'Ġunused', 'Ġbandwidth', 'Ġcell', 'Ġwaiting', 'Ġlist', 'Ġpriorit', 'ized', 'Ġservice', 'Ġprice', 'Ġequipment', 'Ġresidential', 'Ġservice', 'Ġper', 'Ġmonth', 'Ġimprove', 'Ġservice', 'Ġquality', 'Ġdensely', 'Ġpopulated', 'Ġareas', 'Ġstar', 'link', 'Ġintroduced', 'Ġmonthly', 'Ġdata', 'Ġcap', 'Ġnon', 'business', 'Ġusers', 'Ġbecame', 'Ġenforced', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġlowered', 'Ġmonthly', 'Ġservice', 'Ġcosts', 'Ġusers', 'Ġselect', 'Ġcountries', 'Ġexample', 'Ġusers', 'Ġb', 'razil', 'Ġch', 'ile', 'Ġsaw', 'Ġmonthly', 'Ġfee', 'Ġdecreases', 'Ġfe', 'b', 'ruary', 'Ġreported', 'Ġstar', 'link', '000', 'Ġsubscribers', 'Ġaust', 'ral', 'ia', 'Ġmay', 'Ġstar', 'link', 'Ġreported', 'Ġmillion', 'Ġactive', 'Ġsubscribers', 'Ġfuture', 'Ġservice', 'mobile', 'Ġus', 'Ġspace', 'x', 'Ġpartnering', 'Ġadd', 'Ġsatellite', 'Ġcellular', 'Ġservice', 'Ġcapability', 'Ġstar', 'link', 'Ġsatellites', 'Ġprovide', 'Ġdead', 'zone', 'Ġcell', 'Ġphone', 'Ġcoverage', 'Ġacross', 'Ġus', 'Ġusing', 'Ġexisting', 'Ġmid', 'band', 'Ġspectrum', 'mobile', 'Ġowns', 'Ġcell', 'Ġcoverage', 'Ġbegin', 'Ġmessaging', 'Ġexpand', 'Ġinclude', 'Ġvoice', 'Ġlimited', 'Ġdata', 'Ġservices', 'Ġlater', 'Ġtesting', 'Ġbegin', 'mobile', 'Ġplans', 'Ġconnect', 'Ġstar', 'link', 'Ġsatellites', 'Ġvia', 'Ġexisting', 'Ġmobile', 'Ġdevices', 'Ġunlike', 'Ġprevious', 'Ġgenerations', 'Ġsatellite', 'Ġphones', 'Ġused', 'Ġspecialized', 'Ġradios', 'Ġmod', 'ems', 'Ġantennas', 'Ġconnect', 'Ġsatellites', 'Ġhigher', 'Ġorbits', 'Ġbandwidth', 'Ġlimited', 'Ġapproximately', 'Ġmeg', 'ab', 'Ġper', 'Ġsecond', 'Ġtotal']</t>
         </is>
       </c>
       <c r="C407" t="n">
@@ -5729,7 +5729,7 @@
       </c>
       <c r="B408" t="inlineStr">
         <is>
-          <t>['Ġsatellites', 'Ġflying', 'Ġhigher', 'Ġorbits', 'Ġstar', 'link', 'Ġactivated', 'Ġfirst', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġrequest', 'Ġu', 'k', 'rain', 'ian', 'Ġu', 'k', 'raine', "'s", 'Ġmilitary', 'Ġgovernment', 'Ġrapidly', 'Ġbecame', 'Ġdependent', 'Ġstar', 'link', 'Ġmaintain', 'Ġinternet', 'Ġstar', 'link', 'Ġused', 'Ġu', 'k', 'raine', 'Ġcommunication', 'Ġkeeping', 'Ġtouch', 'Ġoutside', 'Ġworld', 'Ġkeeping', 'Ġenergy', 'Ġinfrastructure', 'Ġworking', 'Ġservice', 'Ġalso', 'Ġnotably', 'Ġused', 'Ġwarfare', 'Ġstar', 'link', 'Ġused', 'Ġconnecting', 'Ġcombat', 'Ġdrones', 'Ġnaval', 'Ġdrones', 'Ġartillery', 'Ġfire', 'Ġcoordination', 'Ġsystems', 'Ġattacks', 'Ġr', 'ussian', 'Ġspace', 'x', 'Ġexpressed', 'Ġreservations', 'Ġoffensive', 'Ġuse', 'Ġstar', 'link', 'Ġu', 'k', 'raine', 'Ġbeyond', 'Ġmilitary', 'Ġcommunications', 'Ġrestricted', 'Ġstar', 'link', 'Ġcommunication', 'Ġtechnology', 'Ġmilitary', 'Ġuse', 'Ġweapon', 'Ġsystems', 'Ġspace', 'x', 'Ġhowever', 'Ġkept', 'Ġservice', 'Ġonline', 'Ġuse', 'Ġattacking', 'Ġr', 'ussian', 'Ġtargets', 'Ġcriticized', 'Ġk', 'remlin', 'Ġmus', 'k', 'Ġwarned', 'Ġservice', 'Ġcosting', 'Ġmillion', 'Ġper', 'Ġmonth', 'Ġu', 'k', 'rain', 'ian', 'Ġofficial', 'Ġestimated', 'Ġspace', 'x', "'s", 'Ġcontributions', 'Ġmillion', 'Ġj', 'une', 'Ġdod', 'Ġsigned', 'Ġcontract', 'Ġspace', 'x', 'Ġfinance', 'Ġstar', 'link', 'Ġuse', 'Ġu', 'k', 'raine', 'Ġorder', 'Ġoffer', 'Ġsatellite', 'Ġservices', 'Ġnation', 'state', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', 'Ġregulations', 'Ġlong', 'standing', 'Ġinternational', 'Ġtreaties', 'Ġrequire', 'Ġlanding', 'Ġrights', 'Ġgranted', 'Ġcountry', 'Ġjurisdiction', 'Ġwithin', 'Ġcountry', 'Ġnational', 'Ġcommunications', 'Ġregulators', 'Ġresult', 'Ġeven', 'Ġthough', 'Ġstar', 'link', 'Ġnetwork', 'Ġnear', 'global', 'Ġreach', 'Ġlat', 'itudes', 'Ġapproximately', 'Â°', 'Ġbroadband', 'Ġservices', 'Ġprovided', 'Ġcountries', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġalso', 'Ġbusiness', 'Ġoperation', 'Ġeconomic', 'Ġconsiderations', 'Ġmay', 'Ġmake', 'Ġmilitary', 'Ġcommunications', 'Ġuse', 'Ġu', 'k', 'raine', 'Ġavailability', 'Ġregulatory', 'Ġapproval', 'Ġcountry', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġavailability', 'Ġcountry', 'Ġapproved', 'Ġactivated', 'Ġactivated', 'Ġunknown', 'Ġdifference', 'Ġcountries', 'Ġstar', 'link', 'Ġservice', 'Ġoffered', 'Ġorder', 'Ġsoon', 'Ġexample', 'Ġspace', 'x', 'Ġformally', 'Ġrequested', 'Ġauthorization', 'ada', 'Ġj', 'une', 'adian', 'Ġregulatory', 'Ġauthority', 'Ġapproved', 'mber', 'Ġspace', 'x', 'Ġrolled', 'Ġservice', 'Ġtwo', 'Ġmonths', 'Ġlater', 'Ġjan', 'uary', 'Ġse', 'pt', 'ember', 'Ġstar']</t>
+          <t>['Ġsplit', 'Ġacross', 'Ġlarge', 'Ġcell', 'Ġcoverage', 'Ġarea', 'Ġlimited', 'Ġapproximately', '000', 'Ġvoice', 'Ġcall', 'ers', 'Ġcell', 'Ġsize', 'Ġsingle', 'Ġcoverage', 'Ġcell', 'Ġyet', 'Ġpublicly', 'Ġreleased', 'Ġsatellites', 'Ġmeters', 'Ġlong', 'Ġantenna', 'Ġwould', 'Ġfold', 'rough', 'ly', 'Ġsquare', 'Ġmeters', '".[', 'Ġmarch', 'Ġspace', 'x', 'Ġconfirmed', 'Ġremain', 'Ġtrack', 'Ġbegin', 'Ġtesting', 'Ġservice', 'Ġapr', 'il', 'Ġone', 'formerly', 'Ġv', 'od', 'af', 'one', 'Ġnew', 'Ġzeal', 'Ġannounced', 'Ġwould', 'Ġpartnering', 'Ġspace', 'x', "'s", 'Ġstar', 'link', 'Ġprovide', 'Ġmobile', 'Ġnetwork', 'Ġcoverage', 'Ġnew', 'Ġzeal', 'Ġsm', 'Ġtext', 'Ġservice', 'Ġexpected', 'Ġbegin', 'Ġvoice', 'Ġdata', 'Ġfunctionality', 'Ġcoming', 'Ġj', 'uly', 'Ġopt', 'us', 'Ġaust', 'ral', 'ia', 'Ġannounced', 'Ġsimilar', 'Ġpartnership', 'Ġservices', 'Ġsatellite', 'Ġinternet', 'Ġsatellite', 'Ġcellular', 'Ġservice', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġel', 'Ġmus', 'k', 'Ġfour', 'star', 'Ġgeneral', 'Ġter', 'rence', 'Ġj', "'s", 'h', 'augh', 'ness', 'Ġapr', 'il', 'Ġfuture', 'Ġsecretary', 'Ġdefense', 'Ġresearch', 'Ġengineering', 'ichael', 'Ġgr', 'ï', '¬', 'ģ', 'n', 'Ġmeets', 'Ġel', 'Ġmus', 'k', 'Ġl', 'arry', 'iam', 'Ġformer', 'Ġtel', 'edes', 'ic', 'Ġspace', 'x', 'Ġalso', 'Ġdesigns', 'Ġbuilds', 'Ġlaunches', 'Ġcustomized', 'Ġmilitary', 'Ġsatellites', 'Ġbased', 'Ġvariants', 'Ġstar', 'link', 'Ġsatellite', 'Ġbus', 'Ġlargest', 'Ġpublicly', 'Ġknown', 'Ġcustomer', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'da', 'da', 'Ġformed', 'Ġpart', 'Ġtrump', 'Ġadministration', 'Ġeffort', 'Ġresurrect', 'agan', 'era', 'Ġstrategic', 'Ġdefense', 'Ġinitiative', 'di', ').[', 'da', 'Ġacceler', 'ates', 'Ġdevelopment', 'Ġmissile', 'Ġdefense', 'Ġcapabilities', 'Ġusing', 'Ġindustry', 'proc', 'ured', 'Ġlow', 'cost', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġplatforms', 'Ġprogram', 'Ġconceived', 'Ġinstituted', 'Ġsecretary', 'Ġdefense', 'r', 'e', 'ichael', 'Ġgr', 'iffin', 'Ġdecades', 'Ġearlier', 'Ġjoined', 'Ġmus', 'k', 'Ġtrip', 'Ġr', 'ussia', 'Ġexamine', 'Ġpart', 'Ġspace', 'x', "'s", 'Ġfounding', ').[', 'Ġmonths', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġannounced', 'Ġspace', 'x', 'Ġchief', 'Ġoperating', 'Ġofficer', 'Ġshot', 'well', 'Ġasked', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġgiven', 'Ġnature', 'Ġprogram', 'Ġwhether', 'Ġspace', 'x', 'Ġwould', 'Ġlaunch', 'Ġweapons', 'Ġspace', 'Ġus', 'Ġmilitary', 'Ġaffirmed', 'Ġwould', "'s", 'Ġdefense', 'Ġcountry', '."[']</t>
         </is>
       </c>
       <c r="C408" t="n">
@@ -5742,7 +5742,7 @@
       </c>
       <c r="B409" t="inlineStr">
         <is>
-          <t>['link', 'Ġservices', 'Ġoffer', 'Ġcountries', 'Ġapplications', 'Ġpending', 'Ġregulatory', 'Ġapproval', 'Ġmany', 'Ġj', 'apan', "'s", 'Ġmajor', 'Ġmobile', 'Ġprovider', 'Ġk', 'dd', 'Ġannounced', 'Ġpartnership', 'Ġspace', 'x', 'Ġbegin', 'Ġoffering', 'Ġexpanded', 'Ġconnectivity', 'Ġrural', 'Ġmobile', 'Ġcustomers', 'Ġvia', 'Ġremote', 'Ġmobile', 'Ġtowers', 'Ġapr', 'il', 'Ġhaw', 'ai', 'ian', 'Ġairlines', 'Ġannounced', 'Ġagreement', 'Ġstar', 'link', 'Ġprovide', 'Ġfree', 'Ġinternet', 'Ġaccess', 'Ġaircraft', 'Ġbecoming', 'Ġfirst', 'Ġairline', 'Ġuse', 'Ġstar', 'link', 'Ġj', 'uly', 'Ġstar', 'link', 'Ġinternet', 'Ġservice', 'Ġavailable', 'Ġcountries', 'Ġmarkets', 'Ġmay', 'Ġannounced', 'Ġregulatory', 'Ġapproval', 'Ġgranted', 'Ġnig', 'eria', 'Ġmo', 'z', 'amb', 'ique', 'Ġph', 'ilipp', 'ines', 'Ġcommercial', 'Ġavailability', 'Ġbegan', 'Ġfe', 'b', 'ruary', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcountries', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġnorth', 'Ġameric', 'Ġunited', 'Ġstates', 'Ġpu', 'erto', 'Ġr', 'ico', 'Ġunited', 'Ġstates', 'Ġvirgin', 'Ġislands', 'Ġlimited', 'Ġtrials', 'Ġaug', 'ust', 'Ġpublic', 'Ġbeta', 'mber', 'Ġfirst', 'Ġauthorized', 'Ġregion', 'Ġapproved', 'Ġspace', 'x', "'s", 'Ġproposed', 'Ġmod', 'ï', '¬', 'ģ', 'cation', 'Ġlicense', 'Ġnorth', 'Ġameric', 'ada', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġunited', 'Ġkingdom', 'Ġpit', 'cair', 'n', 'Ġislands', 'Ġjan', 'uary', 'Ġservice', 'Ġexpanded', 'Ġpit', 'cair', 'n', 'Ġislands', 'mber', 'Ġeuro', 'pe', 'Ġg', 'erman', 'Ġmarch', 'ce', 'ania', 'Ġnew', 'Ġzeal', 'Ġapr', 'il', 'ce', 'ania', 'Ġaust', 'ral', 'ia', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġfr', 'ance', 'Ġsaint', 'Ġmart', 'Ġsaint', 'Ġbar', 'th', 'Ã©', 'le', 'Ġgu', 'adel', 'ou', 'pe', 'Ġmart', 'ique', 'Ġoriginal', 'Ġdebut', 'Ġmay', 'Ġrevoked', 'Ġapr', 'il', 'approved', 'Ġj', 'une', 'Ġapproval', 'Ġoriginally', 'Ġgiven', 'Ġfe', 'b', 'ruary', 'Ġcon', 'se', 'il', 'Ã©t', 'Ġann', 'ull', 'ed', 'Ġdecision', 'Ġapr', 'il', 'Ġdue', 'Ġlack', 'Ġpublic', 'Ġconsultation', 'Ġapproval', 'Ġgiven', 'Ġconsultation', 'Ġcompleted', 'Ġj', 'une', 'Ġservice', 'Ġexpanded', 'Ġsaint', 'Ġmart', 'Ġsaint', 'Ġbar', 'th', 'Ã©', 'le', 'Ġj', 'uly', 'Ġservice', 'Ġexpanded', 'Ġmart', 'ique', 'Ġgu', 'adel', 'ou', 'pe', 'Ġse', 'pt', 'ember']</t>
+          <t>['Ġoct', 'ober', 'da', 'Ġawarded', 'Ġspace', 'x', 'Ġinitial', 'Ġmillion', 'Ġdual', 'use', 'Ġcontract', 'Ġdevelop', 'Ġsatellites', 'Ġdetect', 'Ġtrack', 'Ġballistic', 'Ġhyp', 'erson', 'ic', 'Ġmissiles', 'Ġfirst', 'Ġbatch', 'Ġsatellites', 'Ġoriginally', 'Ġscheduled', 'Ġlaunch', 'Ġse', 'pt', 'ember', 'Ġform', 'Ġpart', 'Ġtracking', 'Ġlayer', 'Ġtr', 'anche', 'Ġspace', 'Ġforce', "'s", 'Ġnational', 'Ġdefense', 'Ġspace', 'Ġarchitecture', 'Ġlaunch', 'Ġschedule', 'Ġslipped', 'Ġmultiple', 'Ġtimes', 'Ġeventually', 'Ġlaunched', 'Ġapr', 'il', 'Ġn', 'ds', 'Ġcomposed', 'Ġseven', 'Ġlayers', 'Ġspecific', 'Ġfunctions', 'Ġdata', 'Ġtransport', 'Ġbattle', 'Ġmanagement', 'Ġmissile', 'Ġtracking', 'Ġcustody', 'weapons', 'Ġtargeting', 'Ġsatellite', 'Ġnavigation', 'Ġdeterrence', 'Ġground', 'Ġsupport', 'Ġhistorically', 'Ġspace', 'based', 'Ġmissile', 'Ġdefense', 'Ġconcepts', 'Ġexpensive', 'Ġreusable', 'Ġlaunch', 'Ġsystems', 'Ġmit', 'igated', 'Ġcosts', 'Ġaccording', 'Ġcongressional', 'Ġbudget', 'Ġoffice', 'Ġanalysis', 'Ġns', 'da', 'Ġlever', 'ages', 'Ġexisting', 'Ġcommercial', 'Ġsatellite', 'Ġbus', 'Ġdevelopment', 'Ġstar', 'link', 'Ġreduce', 'Ġcosts', 'Ġincluding', 'Ġfree', 'space', 'Ġoptical', 'Ġlaser', 'Ġterminals', 'Ġsecure', 'Ġcommand', 'Ġcontrol', 'Ġmesh', 'Ġnetwork', 'Ġmissile', 'Ġdefense', 'Ġreview', 'Ġnotes', 'Ġspace', 'based', 'Ġsensing', 'Ġenables', 'impro', 'ved', 'Ġtracking', 'Ġpotentially', 'Ġtargeting', 'Ġadvanced', 'Ġthreats', 'Ġincluding', 'Ġhyp', 'erson', 'ic', 'Ġcruise', 'Ġmissiles', '".[', 'Ġhowever', 'Ġunion', 'Ġconcerned', 'Ġscientists', 'Ġwarns', 'Ġdevelopments', 'Ġcould', 'Ġescalate', 'Ġtensions', 'Ġr', 'ussia', 'Ġch', 'ina', 'Ġcalled', 'Ġproject', 'fund', 'ament', 'ally', 'Ġcar', 'negie', 'Ġend', 'owment', 'Ġinternational', 'Ġpeace', 'Ġlater', 'Ġadvocated', 'Ġtreaty', 'Ġhalting', 'Ġdevelopment', 'Ġprevent', 'Ġarms', 'Ġrace', 'Ġspace', 'Ġsince', 'Ġstar', 'link', "'s", 'Ġmilitary', 'Ġsatellite', 'Ġdevelopment', 'Ġoverseen', 'Ġinternally', 'Ġspace', 'x', 'Ġretired', 'Ġfour', 'star', 'Ġgeneral', 'Ġter', 'rence', 'Ġj', "'s", 'h', 'augh', 'ness', 'Ġadvocated', 'Ġunited', 'Ġstates', 'Ġsenate', 'Ġcommittee', 'Ġarmed', 'Ġservices', 'Ġlayered', 'Ġcapability', 'Ġlethal', 'Ġfollow', 'Ġincorporates', 'Ġmachine', 'Ġlearning', 'Ġartificial', 'Ġintelligence', 'Ġgather', 'Ġact', 'Ġupon', 'Ġsensor', 'Ġdata', 'Ġquickly', 'Ġspace', 'x', 'Ġawarded', 'Ġcontract', 'Ġlarger', 'Ġtr', 'anche', 'Ġawards', 'Ġgoing', 'ork', 'Ġspace', 'Ġsystems', 'Ġlock', 'heed', 'Ġmart', 'Ġspace', 'Ġnorth', 'rop', 'Ġgr', 'um', 'man', 'Ġspace', 'Ġsystems', '].', 'Ġde', 'cember', 'Ġspace', 'x', 'Ġannounced', 'Ġst', 'arsh', 'ield', 'Ġprogram', 'Ġincorporate', 'Ġmilitary', 'Ġgovernment', 'Ġentity', 'Ġpayload', 'Ġboard', 'Ġcustomized', 'Ġsatellite', 'Ġbus', 'pot', 'entially', 'Ġbased', 'Ġstar', 'link', 'Ġblock', 'Ġtechnology', ']).', 'Ġsatellites', 'Ġheavier', 'Ġtwice', 'Ġarea', 'Ġsingle', 'Ġstar', 'link', 'Ġtwo', 'Ġpair', 'Ġsolar', 'Ġarrays', 'Ġopposed', 'Ġone', 'Ġstar', 'link', 'Ġblock', 'Ġv']</t>
         </is>
       </c>
       <c r="C409" t="n">
@@ -5755,7 +5755,7 @@
       </c>
       <c r="B410" t="inlineStr">
         <is>
-          <t>['Ġeuro', 'pe', 'Ġaust', 'ria', 'Ġmay', 'Ġeuro', 'pe', 'Ġnet', 'lands', 'Ġmay', 'Ġeuro', 'pe', 'Ġbel', 'g', 'ium', 'Ġmay', 'Ġeuro', 'pe', 'Ġire', 'land', 'Ġlimited', 'Ġtrials', 'Ġapr', 'il', 'Ġpublic', 'Ġbeta', 'Ġj', 'uly', 'Ġeuro', 'pe', 'Ġden', 'mark', 'Ġj', 'uly', 'Ġeuro', 'pe', 'Ġport', 'ugal', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'Ġsw', 'itzerland', 'Ġaug', 'ust', 'Ġsouth', 'Ġameric', 'Ġch', 'ile', 'Ġeas', 'ter', 'Ġisland', 'Ġlimited', 'Ġtrials', 'Ġj', 'uly', 'Ġpublic', 'Ġbeta', 'Ġse', 'pt', 'ember', 'Ġservice', 'Ġexpanded', 'Ġeas', 'ter', 'Ġisland', 'mber', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġeuro', 'pe', 'Ġpol', 'Ġse', 'pt', 'ember', 'Ġeuro', 'pe', 'aly', 'Ġse', 'pt', 'ember', 'Ġeuro', 'pe', 'Ġc', 'zech', 'Ġrepublic', 'Ġse', 'pt', 'ember', 'Ġeuro', 'pe', 'Ġsw', 'eden', 'Ġoct', 'ober', 'Ġnorth', 'Ġameric', 'x', 'ico', 'mber', 'Ġeuro', 'pe', 'Ġcro', 'ia', 'mber', 'Ġeuro', 'pe', 'Ġlith', 'uania', 'Ġde', 'cember', 'Ġeuro', 'pe', 'Ġsp', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġsl', 'ov', 'akia', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġsl', 'oven', 'ia', 'Ġjan', 'uary', 'ce', 'ania', 'Ġtong', 'Ġfe', 'b', 'ruary', 'Ġemergency', 'Ġrelief', 'Ġprovided', 'Ġone', 'Ġmonth', 'Ġhung', 'Ġtong', 'âĢĵ', 'Ġhung', 'Ġha', 'ap', 'ai', 'Ġeruption', 'Ġtsunami', 'Ġground', 'Ġstation', 'Ġestablished', 'Ġneighboring', 'Ġmonths', 'Ġsouth', 'Ġameric', 'Ġb', 'razil', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġbul', 'gar', 'ia', 'Ġfe', 'b', 'ruary', 'Ġeuro', 'pe', 'Ġu', 'k', 'raine', 'Ġfe', 'b', 'ruary', 'Ġinitially', 'Ġsupplied', 'Ġemergency', 'Ġrelief', 'Ġresponse', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġsee', 'Ġstar', 'link', 'Ġsatellite', 'Ġservices', 'Ġu', 'k', 'raine', 'Ġeuro', 'pe', 'Ġr', 'oman', 'ia', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġg', 'ree', 'ce', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġlat', 'via', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġhung', 'ary', 'Ġmay', 'Ġeuro', 'pe', 'Ġnorth', 'aced', 'onia', 'Ġj', 'une', 'Ġeuro', 'pe', 'Ġlux']</t>
+          <t>['Ġstar', 'link', 'Ġdesigned', 'Ġconsumer', 'Ġcommercial', 'Ġuse', 'Ġst', 'arsh', 'ield', 'Ġdesigned', 'Ġus', 'Ġgovernment', 'Ġuse', 'Ġinitial', 'Ġfocus', 'Ġthree', 'Ġareas', 'Ġnamely', 'Ġearth', 'Ġobservation', 'Ġcommunications', 'Ġhosting', 'Ġpayload', 'Ġmilitary', 'Ġsatellites', 'Ġst', 'arsh', 'ield', 'Ġprogram', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġvital', 'Ġk', 'l', 'itsch', 'ko', 'Ġmayor', 'Ġk', 'iv', 'Ġbrother', 'Ġw', 'lad', 'imir', 'Ġk', 'l', 'itsch', 'ko', 'Ġstar', 'link', 'Ġterminals', 'Ġshipped', 'Ġk', 'iv', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġdesigned', 'Ġmeet', 'Ġdiverse', 'Ġmission', 'Ġrequirements', 'Ġst', 'arsh', 'ield', 'Ġsatellites', 'Ġadvertised', 'Ġcapable', 'Ġintegrating', 'Ġwide', 'Ġvariety', 'Ġpayload', 'Ġoffering', 'Ġunique', 'Ġversatility', 'Ġusers', 'Ġst', 'arsh', 'ield', 'Ġsatellites', 'Ġcompatible', 'Ġinter', 'connect', 'Ġexisting', 'Ġcommercial', 'Ġstar', 'link', 'Ġsatellites', 'Ġvia', 'Ġoptical', 'Ġinter', 'atellite', 'Ġlinks', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġdeployed', 'Ġfour', 'Ġnational', 'Ġsecurity', 'Ġsatellites', 'Ġus', 'Ġgovernment', 'Ġtransporter', 'Ġrides', 'hare', 'Ġmission', 'Ġyear', 'Ġlaunched', 'Ġanother', 'Ġgroup', 'Ġfour', 'Ġu', 'Ġsatellites', 'Ġsingle', 'orbit', 'Ġspare', 'Ġglobal', 'star', 'Ġsatellite', 'Ġpurpose', 'Ġdisclosed', 'Ġtime', 'Ġlaunch', 'Ġconsidered', 'Ġlikely', 'Ġeither', 'Ġtechnical', 'Ġdemonstration', 'Ġcommunications', 'Ġearth', 'Ġobservation', 'Ġsignals', 'Ġintelligence', 'Ġsuspected', 'Ġper', 'Ġimages', 'Ġtwo', 'Ġspace', 'x', 'built', 'Ġstar', 'link', 'Ġderived', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġtr', 'anche', 'Ġflight', 'Ġtracking', 'Ġlayer', 'Ġinfrared', 'Ġimaging', 'Ġsatellites', 'Ġlaunched', 'Ġapr', 'il', 'Ġalso', 'Ġbased', 'Ġst', 'arsh', 'ield', 'Ġsatellite', 'Ġbus', 'Ġtests', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġresearch', 'Ġlaboratory', 'af', 'rl', 'Ġdemonstrated', 'bit', 'Ġdata', 'Ġlink', 'Ġstar', 'link', 'ech', 'craft', 'Ġhur', 'Ġaircraft', 'Ġflight', 'Ġadditionally', 'Ġlate', 'Ġunited', 'Ġstates', 'Ġair', 'Ġforce', 'Ġsuccessfully', 'Ġtested', 'Ġconnection', 'Ġstar', 'link', 'Ġguns', 'hip', 'Ġair', 'Ġforce', 'Ġutilized', 'Ġstar', 'link', 'Ġsupport', 'Ġadvanced', 'Ġbattlefield', 'Ġmanagement', 'Ġsystem', 'Ġlive', 'fire', 'Ġexercise', 'Ġdemonstrated', 'Ġstar', 'link', 'Ġconnected', 'var', 'iety', 'Ġair', 'Ġterrestrial', 'Ġassets', 'Ġincluding', 'Ġbo', 'e', 'ing', 'Ġstrat', 'ot', 'ank', 'er', 'Ġexpert', 'Ġbattlefield', 'Ġcommunications', 'Ġth', 'omas', 'Ġwell', 'ington', 'Ġargues', 'Ġstar', 'link', 'Ġsignals', 'Ġuse', 'Ġnarrow', 'Ġfocused', 'Ġbeams', 'Ġless', 'Ġvulnerable', 'Ġinterference', 'Ġjam', 'ming', 'Ġenemy', 'Ġwartime']</t>
         </is>
       </c>
       <c r="C410" t="n">
@@ -5768,7 +5768,7 @@
       </c>
       <c r="B411" t="inlineStr">
         <is>
-          <t>['em', 'bourg', 'Ġj', 'uly', 'Ġnorth', 'Ġameric', 'Ġdomin', 'ican', 'Ġrepublic', 'Ġj', 'uly', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġeuro', 'pe', 'Ġmold', 'ova', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'Ġest', 'onia', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'way', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'Ġmalt', 'Ġse', 'pt', 'ember', 'ia', 'Ġir', 'Ġse', 'pt', 'ember', 'Ġactivated', 'Ġresponse', 'Ġir', 'anian', 'Ġcensorship', 'Ġresult', 'Ġir', 'anian', 'Ġprotests', 'Ġcompulsory', 'ia', 'Ġj', 'apan', 'Ġoct', 'ober', 'Ġfirst', 'ia', 'Ġnorth', 'Ġameric', 'Ġj', 'ama', 'ica', 'Ġoct', 'ober', 'Ġeuro', 'pe', 'Ġfin', 'land', 'mber', 'Ġsouth', 'Ġameric', 'Ġper', 'u', 'Ġjan', 'uary', 'Ġaf', 'rica', 'Ġnig', 'eria', 'Ġjan', 'uary', 'Ġfirst', 'Ġaf', 'rica', 'Ġsouth', 'Ġameric', 'Ġcol', 'omb', 'ia', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġic', 'eland', 'Ġfe', 'b', 'ruary', 'Ġaf', 'rica', 'Ġr', 'w', 'anda', 'Ġfe', 'b', 'ruary', 'ia', 'Ġph', 'ilipp', 'ines', 'Ġfe', 'b', 'ruary', 'Ġsecond', 'ia', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsoutheast', 'ia', 'Ġnorth', 'Ġameric', 'Ġha', 'iti', 'Ġmarch', 'Ġsouth', 'Ġameric', 'Ġec', 'uador', 'Ġmarch', 'Ġnorth', 'Ġameric', 'Ġel', 'Ġsalv', 'ador', 'Ġapr', 'il', 'Ġnorth', 'Ġameric', 'Ġpan', 'ama', 'Ġmay', 'Ġaf', 'rica', 'Ġmo', 'z', 'amb', 'ique', 'Ġj', 'une', 'Ġsouth', 'Ġameric', 'Ġtr', 'idad', 'Ġtob', 'ago', 'Ġj', 'une', 'Ġeuro', 'pe', 'Ġcy', 'prus', 'Ġj', 'uly', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġnorth', 'Ġameric', 'Ġgu', 'atem', 'ala', 'Ġj', 'uly', 'Ġaf', 'rica', 'Ġk', 'en', 'ya', 'Ġj', 'uly', 'ia', 'Ġmal', 'ays', 'ia', 'Ġj', 'uly', 'Ġsecond', 'Ġsoutheast', 'ia', 'Ġaf', 'rica', 'Ġmal', 'awi', 'Ġj', 'uly', 'Ġnorth', 'Ġameric', 'Ġb', 'ah', 'amas', 'Ġaug', 'ust']</t>
+          <t>['Ġsatellites', 'Ġflying', 'Ġhigher', 'Ġorbits', 'Ġstar', 'link', 'Ġactivated', 'Ġfirst', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġrequest', 'Ġu', 'k', 'rain', 'ian', 'Ġu', 'k', 'raine', "'s", 'Ġmilitary', 'Ġgovernment', 'Ġrapidly', 'Ġbecame', 'Ġdependent', 'Ġstar', 'link', 'Ġmaintain', 'Ġinternet', 'Ġstar', 'link', 'Ġused', 'Ġu', 'k', 'raine', 'Ġcommunication', 'Ġkeeping', 'Ġtouch', 'Ġoutside', 'Ġworld', 'Ġkeeping', 'Ġenergy', 'Ġinfrastructure', 'Ġworking', 'Ġservice', 'Ġalso', 'Ġnotably', 'Ġused', 'Ġwarfare', 'Ġstar', 'link', 'Ġused', 'Ġconnecting', 'Ġcombat', 'Ġdrones', 'Ġnaval', 'Ġdrones', 'Ġartillery', 'Ġfire', 'Ġcoordination', 'Ġsystems', 'Ġattacks', 'Ġr', 'ussian', 'Ġspace', 'x', 'Ġexpressed', 'Ġreservations', 'Ġoffensive', 'Ġuse', 'Ġstar', 'link', 'Ġu', 'k', 'raine', 'Ġbeyond', 'Ġmilitary', 'Ġcommunications', 'Ġrestricted', 'Ġstar', 'link', 'Ġcommunication', 'Ġtechnology', 'Ġmilitary', 'Ġuse', 'Ġweapon', 'Ġsystems', 'Ġspace', 'x', 'Ġhowever', 'Ġkept', 'Ġservice', 'Ġonline', 'Ġuse', 'Ġattacking', 'Ġr', 'ussian', 'Ġtargets', 'Ġcriticized', 'Ġk', 'remlin', 'Ġmus', 'k', 'Ġwarned', 'Ġservice', 'Ġcosting', 'Ġmillion', 'Ġper', 'Ġmonth', 'Ġu', 'k', 'rain', 'ian', 'Ġofficial', 'Ġestimated', 'Ġspace', 'x', "'s", 'Ġcontributions', 'Ġmillion', 'Ġj', 'une', 'Ġdod', 'Ġsigned', 'Ġcontract', 'Ġspace', 'x', 'Ġfinance', 'Ġstar', 'link', 'Ġuse', 'Ġu', 'k', 'raine', 'Ġorder', 'Ġoffer', 'Ġsatellite', 'Ġservices', 'Ġnation', 'state', 'Ġinternational', 'Ġtele', 'communication', 'Ġunion', 'itu', 'Ġregulations', 'Ġlong', 'standing', 'Ġinternational', 'Ġtreaties', 'Ġrequire', 'Ġlanding', 'Ġrights', 'Ġgranted', 'Ġcountry', 'Ġjurisdiction', 'Ġwithin', 'Ġcountry', 'Ġnational', 'Ġcommunications', 'Ġregulators', 'Ġresult', 'Ġeven', 'Ġthough', 'Ġstar', 'link', 'Ġnetwork', 'Ġnear', 'global', 'Ġreach', 'Ġlat', 'itudes', 'Ġapproximately', 'Â°', 'Ġbroadband', 'Ġservices', 'Ġprovided', 'Ġcountries', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġalso', 'Ġbusiness', 'Ġoperation', 'Ġeconomic', 'Ġconsiderations', 'Ġmay', 'Ġmake', 'Ġmilitary', 'Ġcommunications', 'Ġuse', 'Ġu', 'k', 'raine', 'Ġavailability', 'Ġregulatory', 'Ġapproval', 'Ġcountry', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġavailability', 'Ġcountry', 'Ġapproved', 'Ġactivated', 'Ġactivated', 'Ġunknown', 'Ġdifference', 'Ġcountries', 'Ġstar', 'link', 'Ġservice', 'Ġoffered', 'Ġorder', 'Ġsoon', 'Ġexample', 'Ġspace', 'x', 'Ġformally', 'Ġrequested', 'Ġauthorization', 'ada', 'Ġj', 'une', 'adian', 'Ġregulatory', 'Ġauthority', 'Ġapproved', 'mber', 'Ġspace', 'x', 'Ġrolled', 'Ġservice', 'Ġtwo', 'Ġmonths', 'Ġlater', 'Ġjan', 'uary', 'Ġse', 'pt', 'ember', 'Ġstar']</t>
         </is>
       </c>
       <c r="C411" t="n">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="B412" t="inlineStr">
         <is>
-          <t>['Ġinternet', 'Ġcommunication', 'Ġsatellites', 'Ġexpected', 'Ġsmall', 'sat', 'class', 'Ġlb', 'mass', 'Ġintended', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġaltitude', 'Ġapproximately', 'Ġmi', 'Ġaccording', 'Ġearly', 'Ġpublic', 'Ġreleases', 'Ġinformation', 'Ġevent', 'Ġfirst', 'Ġlarge', 'Ġdeployment', 'Ġsatellites', 'Ġmay', 'Ġspace', 'x', 'Ġdecided', 'Ġplace', 'Ġsatellites', 'Ġrelatively', 'Ġlow', 'Ġmi', 'Ġdue', 'Ġconcerns', 'Ġspace', 'Ġenvironment', 'Ġinitial', 'Ġplans', 'Ġjan', 'uary', 'Ġconstellation', 'Ġmade', 'Ġapproximately', '000', 'Ġcross', 'linked', 'Ġsatellites', 'Ġtwice', 'Ġmany', 'Ġoperational', 'Ġsatellites', 'Ġorbit', 'Ġjan', 'uary', 'Ġsatellites', 'Ġemploy', 'Ġoptical', 'Ġinter', 'atellite', 'Ġlinks', 'Ġphased', 'Ġarray', 'Ġbeam', 'forming', 'Ġdigital', 'Ġprocessing', 'Ġtechnologies', 'Ġka', 'Ġmicrowave', 'Ġbands', 'super', 'Ġhigh', 'Ġfrequency', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġaccording', 'Ġdocuments', 'Ġfiled', 'Ġu', 'Ġf', 'cc', 'Ġspecifics', 'Ġphased', 'Ġarray', 'Ġtechnologies', 'Ġdisclosed', 'Ġpart', 'Ġfrequency', 'Ġapplication', 'Ġspace', 'x', 'Ġenforced', 'Ġconfidentiality', 'Ġregarding', 'Ġdetails', 'Ġoptical', 'Ġinter', 'atellite', 'Ġlinks', 'Ġearly', 'Ġsatellites', 'Ġlaunched', 'Ġwithout', 'Ġlaser', 'Ġlinks', 'Ġinter', 'atellite', 'Ġlaser', 'Ġlinks', 'Ġsuccessfully', 'Ġtested', 'Ġlate', 'Ġsatellites', 'Ġmass', 'produced', 'Ġmuch', 'Ġlower', 'Ġcost', 'Ġper', 'Ġunit', 'Ġcapability', 'Ġpreviously', 'Ġexisting', 'Ġsatellites', 'Ġmus', 'k', 'Ġsaid', "'re", 'Ġgoing', 'Ġtry', 'Ġsatellites', "'ve", 'Ġdone', 'Ġrockets', '."[', 'Ġorder', 'Ġrevolution', 'ize', 'Ġspace', 'Ġaddress', 'Ġsatellites', 'Ġrockets', '."[', 'small', 'er', 'Ġsatellites', 'Ġcrucial', 'Ġlowering', 'Ġcost', 'Ġspace', 'based', 'Ġinternet', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġasked', 'Ġconsider', 'Ġfuture', 'Ġinnovative', 'Ġuses', 'Ġka', 'band', 'Ġspectrum', 'Ġcommits', 'Ġcommunications', 'Ġregulations', 'Ġwould', 'Ġcreate', 'Ġbarriers', 'Ġentry', 'Ġsince', 'Ġspace', 'x', 'Ġnew', 'Ġent', 'rant', 'Ġsatellite', 'Ġcommunications', 'Ġmarket', 'Ġspace', 'x', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcommunications', 'Ġsatellite', 'Ġconstellation', 'Ġoperate', 'Ġhigh', 'frequency', 'Ġbands', 'Ġsteer', 'able', 'Ġearth', 'Ġstation', 'Ġtransmit', 'Ġantennas', 'Ġwould', 'Ġwider', 'Ġgeographic', 'Ġimpact', 'Ġsignificantly', 'Ġlower', 'Ġsatellite', 'Ġalt', 'itudes', 'Ġmagn', 'ify', 'Ġimpact', 'Ġaggregate', 'Ġinterference', 'Ġterrestrial', 'Ġinternet', 'Ġtraffic', 'Ġvia', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġminimum', 'Ġtheoretical']</t>
+          <t>['link', 'Ġservices', 'Ġoffer', 'Ġcountries', 'Ġapplications', 'Ġpending', 'Ġregulatory', 'Ġapproval', 'Ġmany', 'Ġj', 'apan', "'s", 'Ġmajor', 'Ġmobile', 'Ġprovider', 'Ġk', 'dd', 'Ġannounced', 'Ġpartnership', 'Ġspace', 'x', 'Ġbegin', 'Ġoffering', 'Ġexpanded', 'Ġconnectivity', 'Ġrural', 'Ġmobile', 'Ġcustomers', 'Ġvia', 'Ġremote', 'Ġmobile', 'Ġtowers', 'Ġapr', 'il', 'Ġhaw', 'ai', 'ian', 'Ġairlines', 'Ġannounced', 'Ġagreement', 'Ġstar', 'link', 'Ġprovide', 'Ġfree', 'Ġinternet', 'Ġaccess', 'Ġaircraft', 'Ġbecoming', 'Ġfirst', 'Ġairline', 'Ġuse', 'Ġstar', 'link', 'Ġj', 'uly', 'Ġstar', 'link', 'Ġinternet', 'Ġservice', 'Ġavailable', 'Ġcountries', 'Ġmarkets', 'Ġmay', 'Ġannounced', 'Ġregulatory', 'Ġapproval', 'Ġgranted', 'Ġnig', 'eria', 'Ġmo', 'z', 'amb', 'ique', 'Ġph', 'ilipp', 'ines', 'Ġcommercial', 'Ġavailability', 'Ġbegan', 'Ġfe', 'b', 'ruary', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcountries', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġnorth', 'Ġameric', 'Ġunited', 'Ġstates', 'Ġpu', 'erto', 'Ġr', 'ico', 'Ġunited', 'Ġstates', 'Ġvirgin', 'Ġislands', 'Ġlimited', 'Ġtrials', 'Ġaug', 'ust', 'Ġpublic', 'Ġbeta', 'mber', 'Ġfirst', 'Ġauthorized', 'Ġregion', 'Ġapproved', 'Ġspace', 'x', "'s", 'Ġproposed', 'Ġmod', 'ï', '¬', 'ģ', 'cation', 'Ġlicense', 'Ġnorth', 'Ġameric', 'ada', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġunited', 'Ġkingdom', 'Ġpit', 'cair', 'n', 'Ġislands', 'Ġjan', 'uary', 'Ġservice', 'Ġexpanded', 'Ġpit', 'cair', 'n', 'Ġislands', 'mber', 'Ġeuro', 'pe', 'Ġg', 'erman', 'Ġmarch', 'ce', 'ania', 'Ġnew', 'Ġzeal', 'Ġapr', 'il', 'ce', 'ania', 'Ġaust', 'ral', 'ia', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġfr', 'ance', 'Ġsaint', 'Ġmart', 'Ġsaint', 'Ġbar', 'th', 'Ã©', 'le', 'Ġgu', 'adel', 'ou', 'pe', 'Ġmart', 'ique', 'Ġoriginal', 'Ġdebut', 'Ġmay', 'Ġrevoked', 'Ġapr', 'il', 'approved', 'Ġj', 'une', 'Ġapproval', 'Ġoriginally', 'Ġgiven', 'Ġfe', 'b', 'ruary', 'Ġcon', 'se', 'il', 'Ã©t', 'Ġann', 'ull', 'ed', 'Ġdecision', 'Ġapr', 'il', 'Ġdue', 'Ġlack', 'Ġpublic', 'Ġconsultation', 'Ġapproval', 'Ġgiven', 'Ġconsultation', 'Ġcompleted', 'Ġj', 'une', 'Ġservice', 'Ġexpanded', 'Ġsaint', 'Ġmart', 'Ġsaint', 'Ġbar', 'th', 'Ã©', 'le', 'Ġj', 'uly', 'Ġservice', 'Ġexpanded', 'Ġmart', 'ique', 'Ġgu', 'adel', 'ou', 'pe', 'Ġse', 'pt', 'ember']</t>
         </is>
       </c>
       <c r="C412" t="n">
@@ -5794,7 +5794,7 @@
       </c>
       <c r="B413" t="inlineStr">
         <is>
-          <t>['Ġround', 'trip', 'Ġlatency', 'Ġleast', 'Ġmilliseconds', 'ms', 'Ġuser', 'Ġground', 'Ġgateway', 'Ġpractice', 'Ġcurrent', 'Ġsatellites', 'Ġlat', 'encies', 'Ġms', 'Ġstar', 'link', 'Ġsatellites', 'Ġorbiting', 'âģ', 'Ħ', 'âģ', 'Ħ', 'Ġheight', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġthus', 'Ġoffer', 'Ġpractical', 'Ġearth', 'sat', 'Ġlat', 'encies', 'Ġaround', 'Ġms', 'Ġcomparable', 'Ġexisting', 'Ġcable', 'Ġfiber', 'Ġnetworks', 'Ġsystem', 'Ġuse', 'Ġpeer', 'ope', 'er', 'Ġprotocol', 'Ġclaimed', 'sim', 'pler', 'Ġalso', 'Ġincorporate', 'Ġend', 'end', 'Ġencryption', 'Ġnative', 'ly', 'Ġtechnology', 'Ġsatellite', 'Ġhardware', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġboard', 'Ġmember', 'Ġste', 'Ġjur', 'ts', 'Ġholding', 'Ġstar', 'link', 'Ġuser', 'Ġterminal', 'Ġj', 'une', 'Ġstar', 'link', 'Ġsatellites', 'Ġuse', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġk', 'rypt', 'Ġarg', 'Ġgas', 'Ġreaction', 'Ġmass', 'Ġorbit', 'Ġraising', 'Ġstation', 'Ġkeeping', 'Ġk', 'rypt', 'Ġhall', 'Ġthr', 'usters', 'Ġtend', 'Ġexhibit', 'Ġsignificantly', 'Ġhigher', 'Ġerosion', 'Ġflow', 'Ġchannel', 'Ġcompared', 'Ġsimilar', 'Ġelectric', 'Ġpropulsion', 'Ġsystem', 'Ġoperated', 'Ġxen', 'Ġk', 'rypt', 'Ġmuch', 'Ġabundant', 'Ġlower', 'Ġmarket', 'Ġprice', 'Ġspace', 'x', 'Ġclaims', 'nd', 'Ġgeneration', 'Ġthr', 'uster', 'Ġusing', 'Ġarg', 'Ġthrust', 'Ġspecific', 'Ġimpulse', 'Ġk', 'rypt', 'Ġfueled', 'Ġthr', 'uster', 'Ġsystem', 'Ġdirectly', 'Ġconnect', 'Ġsatellites', 'Ġhands', 'ets', 'like', 'Ġconst', 'ell', 'ations', 'Ġir', 'idium', 'Ġglobal', 'star', 'Ġth', 'ur', 'aya', 'ars', 'Ġinstead', 'Ġlinked', 'Ġflat', 'Ġuser', 'Ġterminals', 'Ġsize', 'Ġpizza', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġtrack', 'Ġsatellites', 'Ġterminals', 'Ġmounted', 'Ġanywhere', 'Ġlong', 'Ġsee', 'Ġincludes', 'Ġfast', 'moving', 'Ġobjects', 'Ġlike', 'Ġtrains', 'Ġphotographs', 'Ġcustomer', 'Ġantennas', 'Ġfirst', 'Ġseen', 'Ġinternet', 'Ġj', 'une', 'Ġsupporting', 'Ġearlier', 'Ġstatements', 'Ġspace', 'x', 'Ġce', 'Ġmus', 'k', 'Ġterminals', 'Ġwould', 'Ġlook', 'Ġlike', 'uf', 'Ġstick', 'Ġstar', 'link', 'Ġterminal', 'Ġmotors', 'Ġself', 'adjust', 'Ġoptimal', 'Ġangle', 'Ġview', 'Ġantenna', 'Ġknown', 'Ġinternally', 'ishy', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġlaunched', 'Ġpaid', 'Ġbeta', 'Ġservice', 'Ġu', 'Ġcalled', 'better', 'Ġnothing', 'Ġbeta', '",', 'Ġcharging', 'equ', 'ivalent', 'Ġuser']</t>
+          <t>['Ġeuro', 'pe', 'Ġaust', 'ria', 'Ġmay', 'Ġeuro', 'pe', 'Ġnet', 'lands', 'Ġmay', 'Ġeuro', 'pe', 'Ġbel', 'g', 'ium', 'Ġmay', 'Ġeuro', 'pe', 'Ġire', 'land', 'Ġlimited', 'Ġtrials', 'Ġapr', 'il', 'Ġpublic', 'Ġbeta', 'Ġj', 'uly', 'Ġeuro', 'pe', 'Ġden', 'mark', 'Ġj', 'uly', 'Ġeuro', 'pe', 'Ġport', 'ugal', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'Ġsw', 'itzerland', 'Ġaug', 'ust', 'Ġsouth', 'Ġameric', 'Ġch', 'ile', 'Ġeas', 'ter', 'Ġisland', 'Ġlimited', 'Ġtrials', 'Ġj', 'uly', 'Ġpublic', 'Ġbeta', 'Ġse', 'pt', 'ember', 'Ġservice', 'Ġexpanded', 'Ġeas', 'ter', 'Ġisland', 'mber', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġeuro', 'pe', 'Ġpol', 'Ġse', 'pt', 'ember', 'Ġeuro', 'pe', 'aly', 'Ġse', 'pt', 'ember', 'Ġeuro', 'pe', 'Ġc', 'zech', 'Ġrepublic', 'Ġse', 'pt', 'ember', 'Ġeuro', 'pe', 'Ġsw', 'eden', 'Ġoct', 'ober', 'Ġnorth', 'Ġameric', 'x', 'ico', 'mber', 'Ġeuro', 'pe', 'Ġcro', 'ia', 'mber', 'Ġeuro', 'pe', 'Ġlith', 'uania', 'Ġde', 'cember', 'Ġeuro', 'pe', 'Ġsp', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġsl', 'ov', 'akia', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġsl', 'oven', 'ia', 'Ġjan', 'uary', 'ce', 'ania', 'Ġtong', 'Ġfe', 'b', 'ruary', 'Ġemergency', 'Ġrelief', 'Ġprovided', 'Ġone', 'Ġmonth', 'Ġhung', 'Ġtong', 'âĢĵ', 'Ġhung', 'Ġha', 'ap', 'ai', 'Ġeruption', 'Ġtsunami', 'Ġground', 'Ġstation', 'Ġestablished', 'Ġneighboring', 'Ġmonths', 'Ġsouth', 'Ġameric', 'Ġb', 'razil', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġbul', 'gar', 'ia', 'Ġfe', 'b', 'ruary', 'Ġeuro', 'pe', 'Ġu', 'k', 'raine', 'Ġfe', 'b', 'ruary', 'Ġinitially', 'Ġsupplied', 'Ġemergency', 'Ġrelief', 'Ġresponse', 'Ġr', 'ussian', 'Ġinvasion', 'Ġu', 'k', 'raine', 'Ġsee', 'Ġstar', 'link', 'Ġsatellite', 'Ġservices', 'Ġu', 'k', 'raine', 'Ġeuro', 'pe', 'Ġr', 'oman', 'ia', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġg', 'ree', 'ce', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġlat', 'via', 'Ġapr', 'il', 'Ġeuro', 'pe', 'Ġhung', 'ary', 'Ġmay', 'Ġeuro', 'pe', 'Ġnorth', 'aced', 'onia', 'Ġj', 'une', 'Ġeuro', 'pe', 'Ġlux']</t>
         </is>
       </c>
       <c r="C413" t="n">
@@ -5807,7 +5807,7 @@
       </c>
       <c r="B414" t="inlineStr">
         <is>
-          <t>['Ġterminal', 'Ġexpected', 'Ġservice', 'Ġlatency', 'Ġms', 'Ġms', 'Ġnext', 'Ġseveral', 'Ġmonths', '".[', 'Ġjan', 'uary', 'Ġpaid', 'Ġbeta', 'Ġservice', 'Ġextended', 'Ġcontinents', 'Ġstarting', 'Ġunited', 'Ġkingdom', 'Ġlarger', 'Ġhigh', 'performance', 'Ġversion', 'Ġantenna', 'Ġavailable', 'Ġuse', 'Ġstar', 'link', 'Ġbusiness', 'Ġservice', 'Ġtier', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġapplied', 'Ġpermission', 'Ġput', 'Ġterminals', 'Ġships', 'Ġexpectation', 'Ġentering', 'Ġmaritime', 'Ġmarket', 'Ġfuture', 'Ġaug', 'ust', 'Ġresponse', 'Ġopen', 'Ġinvitation', 'Ġspace', 'x', 'Ġterminal', 'Ġexamined', 'Ġsecurity', 'Ġcommunity', 'Ġsecurity', 'Ġspecialist', 'Ġl', 'enn', 'ert', 'Ġw', 'ou', 'ters', 'Ġpresented', 'Ġseveral', 'Ġtechnical', 'Ġarchitecture', 'Ġdetails', 'current', 'Ġstar', 'link', 'Ġterminals', 'Ġmain', 'Ġcontrol', 'Ġunit', 'Ġdish', 'Ġst', 'micro', 'elect', 'ronics', 'Ġcustom', 'Ġdesigned', 'Ġchip', 'Ġcod', 'en', 'amed', 'Ġcats', 'Ġquad', 'core', 'Ġarm', 'Ġcortex', 'based', 'Ġcontrol', 'Ġprocessor', 'Ġrunning', 'Ġlinux', 'Ġkernel', 'Ġbooted', 'Ġusing', 'Ġu', 'boot', 'Ġmain', 'Ġprocessor', 'Ġuses', 'Ġseveral', 'Ġcustom', 'Ġchips', 'Ġdigital', 'Ġbeam', 'Ġformer', 'Ġnamed', 'Ġsh', 'ir', 'az', 'Ġfront', 'end', 'Ġmodule', 'Ġnamed', 'Ġpuls', 'ar', 'ad', 'Ġmain', 'Ġcontrol', 'Ġunit', 'Ġcontrols', 'Ġarray', 'Ġdigital', 'Ġbeam', 'form', 'ers', 'Ġbeam', 'former', 'Ġcontrols', 'Ġfront', 'end', 'Ġmodules', 'Ġaddition', 'Ġterminal', 'Ġreceiver', 'Ġmotor', 'Ġcontrollers', 'Ġsynchron', 'ous', 'Ġclock', 'Ġgeneration', 'Ġpower', 'Ġether', 'net', 'Ġcircuits', 'Ġmanufactured', 'Ġspace', 'x', 'Ġmade', 'Ġapplications', 'Ġleast', 'Ġground', 'Ġstations', 'Ġunited', 'Ġstates', 'Ġj', 'uly', 'Ġapprovals', 'Ġfive', 'Ġfive', 'Ġstates', 'Ġtill', 'Ġfe', 'b', 'ruary', 'Ġstar', 'link', 'Ġused', 'Ġka', 'band', 'Ġconnect', 'Ġground', 'Ġstations', 'Ġlaunch', 'Ġmini', 'Ġadded', 'Ġfrequencies', 'Ġband', 'Ġrange', 'Ġtypical', 'Ġground', 'Ġstation', 'Ġright', 'Ġnine', 'Ġantennas', 'Ġf', 'enced', 'Ġarea', 'Ġaccording', 'Ġfiling', 'Ġspace', 'x', "'s", 'Ġground', 'Ġstations', 'Ġwould', 'Ġalso', 'Ġinstalled', 'site', 'Ġgoogle', 'Ġdata', 'cent', 'ers', 'Ġworldwide', 'Ġuser', 'Ġterminals', 'Ġground', 'Ġstations', 'Ġsatellite', 'Ġrevisions', 'Ġmicro', 'sat', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġmicro', 'sat', 'Ġmicro', 'sat', 'b', 'Ġoriginally', 'Ġslated', 'Ġlaunched', 'Ġmi', 'Ġcircular', 'Ġorbits', 'Ġapproximately', 'Â°', 'Ġinclination', 'Ġinclude', 'Ġpan']</t>
+          <t>['em', 'bourg', 'Ġj', 'uly', 'Ġnorth', 'Ġameric', 'Ġdomin', 'ican', 'Ġrepublic', 'Ġj', 'uly', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġeuro', 'pe', 'Ġmold', 'ova', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'Ġest', 'onia', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'way', 'Ġaug', 'ust', 'Ġeuro', 'pe', 'Ġmalt', 'Ġse', 'pt', 'ember', 'ia', 'Ġir', 'Ġse', 'pt', 'ember', 'Ġactivated', 'Ġresponse', 'Ġir', 'anian', 'Ġcensorship', 'Ġresult', 'Ġir', 'anian', 'Ġprotests', 'Ġcompulsory', 'ia', 'Ġj', 'apan', 'Ġoct', 'ober', 'Ġfirst', 'ia', 'Ġnorth', 'Ġameric', 'Ġj', 'ama', 'ica', 'Ġoct', 'ober', 'Ġeuro', 'pe', 'Ġfin', 'land', 'mber', 'Ġsouth', 'Ġameric', 'Ġper', 'u', 'Ġjan', 'uary', 'Ġaf', 'rica', 'Ġnig', 'eria', 'Ġjan', 'uary', 'Ġfirst', 'Ġaf', 'rica', 'Ġsouth', 'Ġameric', 'Ġcol', 'omb', 'ia', 'Ġjan', 'uary', 'Ġeuro', 'pe', 'Ġic', 'eland', 'Ġfe', 'b', 'ruary', 'Ġaf', 'rica', 'Ġr', 'w', 'anda', 'Ġfe', 'b', 'ruary', 'ia', 'Ġph', 'ilipp', 'ines', 'Ġfe', 'b', 'ruary', 'Ġsecond', 'ia', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġsoutheast', 'ia', 'Ġnorth', 'Ġameric', 'Ġha', 'iti', 'Ġmarch', 'Ġsouth', 'Ġameric', 'Ġec', 'uador', 'Ġmarch', 'Ġnorth', 'Ġameric', 'Ġel', 'Ġsalv', 'ador', 'Ġapr', 'il', 'Ġnorth', 'Ġameric', 'Ġpan', 'ama', 'Ġmay', 'Ġaf', 'rica', 'Ġmo', 'z', 'amb', 'ique', 'Ġj', 'une', 'Ġsouth', 'Ġameric', 'Ġtr', 'idad', 'Ġtob', 'ago', 'Ġj', 'une', 'Ġeuro', 'pe', 'Ġcy', 'prus', 'Ġj', 'uly', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġcontinent', 'Ġcountry', 'ter', 'rit', 'ory', 'Ġdebut', 'Ġnotes', 'Ġnorth', 'Ġameric', 'Ġgu', 'atem', 'ala', 'Ġj', 'uly', 'Ġaf', 'rica', 'Ġk', 'en', 'ya', 'Ġj', 'uly', 'ia', 'Ġmal', 'ays', 'ia', 'Ġj', 'uly', 'Ġsecond', 'Ġsoutheast', 'ia', 'Ġaf', 'rica', 'Ġmal', 'awi', 'Ġj', 'uly', 'Ġnorth', 'Ġameric', 'Ġb', 'ah', 'amas', 'Ġaug', 'ust']</t>
         </is>
       </c>
       <c r="C414" t="n">
@@ -5820,7 +5820,7 @@
       </c>
       <c r="B415" t="inlineStr">
         <is>
-          <t>['chrom', 'atic', 'Ġvideo', 'Ġim', 'ager', 'Ġcameras', 'Ġfilm', 'Ġimages', 'Ġearth', 'Ġsatellite', 'Ġtwo', 'Ġsatellites', 'micro', 'sat', 'micro', 'sat', 'b', 'Ġmeant', 'Ġlaunched', 'Ġtogether', 'Ġsecondary', 'Ġpayload', 'Ġone', 'Ġir', 'idium', 'Ġnext', 'Ġflights', 'Ġinstead', 'Ġused', 'Ġground', 'based', 'Ġtests', 'Ġtime', 'Ġj', 'une', 'Ġannouncement', 'Ġspace', 'x', 'Ġstated', 'Ġplans', 'Ġlaunch', 'Ġfirst', 'Ġtwo', 'Ġdemonstration', 'Ġsatellites', 'Ġtarget', 'Ġdate', 'Ġsubsequently', 'Ġmoved', 'Ġspace', 'x', 'Ġbegan', 'Ġflight', 'Ġtesting', 'Ġsatellite', 'Ġtechnologies', 'Ġlaunch', 'Ġtwo', 'Ġtest', 'Ġsatellites', 'Ġtwo', 'Ġidentical', 'Ġsatellites', 'Ġcalled', 'Ġmicro', 'sat', 'Ġmicro', 'sat', 'b', 'Ġdevelopment', 'Ġrenamed', 'Ġtint', 'Ġtint', 'Ġupon', 'Ġorbital', 'Ġdeployment', 'Ġfe', 'b', 'ruary', 'Ġsatellites', 'Ġlaunched', 'Ġfal', 'con', 'Ġrocket', 'Ġpig', 'gy', 'pack', 'Ġpayload', 'Ġlaunching', 'Ġsatellite', 'Ġtint', 'Ġinserted', 'Ġmi', 'Ġorbit', 'Ġper', 'Ġfilings', 'Ġintended', 'Ġraise', 'Ġmi', 'Ġorbit', 'Ġoperational', 'Ġaltitude', 'Ġstar', 'link', 'Ġle', 'Ġsatellites', 'Ġper', 'Ġearliest', 'Ġregulatory', 'Ġfilings', 'Ġstayed', 'Ġclose', 'Ġoriginal', 'Ġorbits', 'Ġspace', 'x', 'Ġannounced', 'mber', 'Ġwould', 'Ġlike', 'Ġoperate', 'Ġinitial', 'Ġshell', 'Ġsatellites', 'Ġconstellation', 'Ġmi', 'Ġorbital', 'Ġaltitude', 'Ġaltitude', 'Ġsimilar', 'Ġorbits', 'Ġtint', 'Ġstayed', 'Ġsatellites', 'Ġorbit', 'Ġcircular', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġmi', 'Ġaltitude', 'Ġhigh', 'cl', 'ination', 'Ġorbit', 'Ġplanned', 'Ġtwelve', 'month', 'Ġduration', 'Ġsatellites', 'Ġcommunicate', 'Ġthree', 'Ġtesting', 'Ġground', 'Ġstations', 'Ġwashing', 'ton', 'Ġstate', 'Ġcal', 'ornia', 'Ġshort', 'term', 'Ġexperiments', 'Ġless', 'Ġten', 'Ġminutes', 'Ġduration', 'Ġroughly', 'Ġdaily', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġmay', 'Ġfollowing', 'Ġflat', 'panel', 'Ġdesign', 'Ġmultiple', 'Ġhigh', 'put', 'Ġantennas', 'Ġsingle', 'Ġsolar', 'Ġarray', 'Ġmass', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġusing', 'Ġk', 'rypt', 'Ġreaction', 'Ġmass', 'Ġposition', 'Ġadjustment', 'Ġorbit', 'Ġaltitude', 'Ġmaintenance', 'Ġde', 'orbit', 'Ġstar', 'Ġtracker', 'Ġnavigation', 'Ġsystem', 'Ġprecision', 'Ġpointing', 'Ġable', 'Ġuse', 'Ġdepartment', 'Ġdefense', 'provided', 'Ġdebris', 'Ġdata', 'Ġautonom', 'ously', 'Ġavoid', 'Ġcollision']</t>
+          <t>['Ġinternet', 'Ġcommunication', 'Ġsatellites', 'Ġexpected', 'Ġsmall', 'sat', 'class', 'Ġlb', 'mass', 'Ġintended', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġaltitude', 'Ġapproximately', 'Ġmi', 'Ġaccording', 'Ġearly', 'Ġpublic', 'Ġreleases', 'Ġinformation', 'Ġevent', 'Ġfirst', 'Ġlarge', 'Ġdeployment', 'Ġsatellites', 'Ġmay', 'Ġspace', 'x', 'Ġdecided', 'Ġplace', 'Ġsatellites', 'Ġrelatively', 'Ġlow', 'Ġmi', 'Ġdue', 'Ġconcerns', 'Ġspace', 'Ġenvironment', 'Ġinitial', 'Ġplans', 'Ġjan', 'uary', 'Ġconstellation', 'Ġmade', 'Ġapproximately', '000', 'Ġcross', 'linked', 'Ġsatellites', 'Ġtwice', 'Ġmany', 'Ġoperational', 'Ġsatellites', 'Ġorbit', 'Ġjan', 'uary', 'Ġsatellites', 'Ġemploy', 'Ġoptical', 'Ġinter', 'atellite', 'Ġlinks', 'Ġphased', 'Ġarray', 'Ġbeam', 'forming', 'Ġdigital', 'Ġprocessing', 'Ġtechnologies', 'Ġka', 'Ġmicrowave', 'Ġbands', 'super', 'Ġhigh', 'Ġfrequency', 'Ġextremely', 'Ġhigh', 'Ġfrequency', 'Ġaccording', 'Ġdocuments', 'Ġfiled', 'Ġu', 'Ġf', 'cc', 'Ġspecifics', 'Ġphased', 'Ġarray', 'Ġtechnologies', 'Ġdisclosed', 'Ġpart', 'Ġfrequency', 'Ġapplication', 'Ġspace', 'x', 'Ġenforced', 'Ġconfidentiality', 'Ġregarding', 'Ġdetails', 'Ġoptical', 'Ġinter', 'atellite', 'Ġlinks', 'Ġearly', 'Ġsatellites', 'Ġlaunched', 'Ġwithout', 'Ġlaser', 'Ġlinks', 'Ġinter', 'atellite', 'Ġlaser', 'Ġlinks', 'Ġsuccessfully', 'Ġtested', 'Ġlate', 'Ġsatellites', 'Ġmass', 'produced', 'Ġmuch', 'Ġlower', 'Ġcost', 'Ġper', 'Ġunit', 'Ġcapability', 'Ġpreviously', 'Ġexisting', 'Ġsatellites', 'Ġmus', 'k', 'Ġsaid', "'re", 'Ġgoing', 'Ġtry', 'Ġsatellites', "'ve", 'Ġdone', 'Ġrockets', '."[', 'Ġorder', 'Ġrevolution', 'ize', 'Ġspace', 'Ġaddress', 'Ġsatellites', 'Ġrockets', '."[', 'small', 'er', 'Ġsatellites', 'Ġcrucial', 'Ġlowering', 'Ġcost', 'Ġspace', 'based', 'Ġinternet', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġasked', 'Ġconsider', 'Ġfuture', 'Ġinnovative', 'Ġuses', 'Ġka', 'band', 'Ġspectrum', 'Ġcommits', 'Ġcommunications', 'Ġregulations', 'Ġwould', 'Ġcreate', 'Ġbarriers', 'Ġentry', 'Ġsince', 'Ġspace', 'x', 'Ġnew', 'Ġent', 'rant', 'Ġsatellite', 'Ġcommunications', 'Ġmarket', 'Ġspace', 'x', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġorbit', 'Ġcommunications', 'Ġsatellite', 'Ġconstellation', 'Ġoperate', 'Ġhigh', 'frequency', 'Ġbands', 'Ġsteer', 'able', 'Ġearth', 'Ġstation', 'Ġtransmit', 'Ġantennas', 'Ġwould', 'Ġwider', 'Ġgeographic', 'Ġimpact', 'Ġsignificantly', 'Ġlower', 'Ġsatellite', 'Ġalt', 'itudes', 'Ġmagn', 'ify', 'Ġimpact', 'Ġaggregate', 'Ġinterference', 'Ġterrestrial', 'Ġinternet', 'Ġtraffic', 'Ġvia', 'Ġge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġminimum', 'Ġtheoretical']</t>
         </is>
       </c>
       <c r="C415" t="n">
@@ -5833,7 +5833,7 @@
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>['Ġaltitude', 'Ġmi', 'Ġcomponents', 'Ġdesign', 'Ġquickly', 'Ġburn', 'Ġearth', "'s", 'Ġatmosphere', 'Ġend', 'Ġsatellite', "'s", 'Ġlif', 'ecycle', '".', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'mber', 'Ġfollowing', 'Ġadditional', 'Ġcharacteristics', 'Ġcomponents', 'Ġdesign', 'Ġcompletely', 'Ġdemise', 'Ġburn', 'Ġearth', "'s", 'Ġatmosphere', 'Ġend', 'Ġsatellite', "'s", 'Ġlife', 'Ġka', 'band', 'Ġadded', 'Ġmass', 'Ġone', 'Ġnumbered', 'Ġcalled', 'arks', 'Ġal', 'bed', 'Ġreduced', 'Ġusing', 'Ġspecial', 'Ġcoating', 'Ġmethod', 'Ġabandoned', 'Ġdue', 'Ġthermal', 'Ġissues', 'Ġir', 'Ġtint', 'test', 'oper', 'ational', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'Ġninth', 'Ġlaunch', 'Ġaug', 'ust', 'Ġvis', 'ors', 'Ġblock', 'Ġsunlight', 'ï', '¬', 'Ĥ', 'ect', 'ing', 'Ġparts', 'Ġsatellite', 'Ġreduce', 'Ġal', 'bed', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'Ġjan', 'uary', 'Ġfollowing', 'Ġadditional', 'Ġcharacteristics', 'Ġlasers', 'Ġinter', 'atellite', 'Ġcommunication', 'Ġmass', 'Ġvis', 'ors', 'Ġblocked', 'Ġsunlight', 'Ġremoved', 'Ġsatellites', 'Ġlaunched', 'Ġse', 'pt', 'ember', 'Ġonwards', 'Ġsatellites', 'Ġbuses', 'Ġtwo', 'Ġsolar', 'Ġarrays', 'Ġderived', 'Ġstar', 'link', 'Ġmilitary', 'Ġuse', 'Ġhost', 'Ġclassified', 'Ġgovernment', 'Ġmilitary', 'Ġpayload', 'Ġspace', 'x', 'Ġpreparing', 'Ġproduction', 'Ġstar', 'link', 'Ġsatellites', 'Ġearly', 'Ġaccording', 'Ġmus', 'k', 'Ġstar', 'link', 'Ġsatellites', 'Ġorder', 'Ġmagnitude', 'Ġbetter', 'Ġstar', 'link', 'Ġterms', 'Ġcommunications', 'Ġbandwidth', 'Ġspace', 'x', 'Ġhoped', 'Ġbegin', 'Ġlaunching', 'Ġstar', 'link', 'Ġmay', 'Ġspace', 'x', 'Ġsaid', 'Ġpublicly', 'Ġsatellites', 'Ġsecond', 'generation', 'Ġconstellation', 'Ġwould', 'Ġneed', 'Ġlaunched', 'Ġstarship', 'Ġlarge', 'Ġfit', 'Ġinside', 'Ġfal', 'con', 'Ġfair', 'ing', 'Ġhowever', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġmade', 'Ġformal', 'Ġregulatory', 'Ġfilings', 'Ġindicated', 'Ġwould', 'Ġbuild', 'Ġsatellites', 'Ġsecond', 'generation', 'Ġconstellation', 'Ġtwo', 'Ġdifferent', 'Ġtechnically', 'Ġidentical', 'Ġform', 'Ġfactors', 'Ġone', 'Ġphysical', 'Ġstructures', 'Ġtailored', 'Ġlaunching', 'Ġfal', 'con', 'Ġone', 'Ġtailored', 'Ġlaunching', 'Ġstarship', 'Ġstar', 'link', 'Ġlarger', 'Ġheavier', 'Ġstar', 'link', 'Ġsatellites', 'Ġstar', 'link', 'Ġsecond', 'generation', 'Ġsatellites', 'Ġplanned']</t>
+          <t>['Ġround', 'trip', 'Ġlatency', 'Ġleast', 'Ġmilliseconds', 'ms', 'Ġuser', 'Ġground', 'Ġgateway', 'Ġpractice', 'Ġcurrent', 'Ġsatellites', 'Ġlat', 'encies', 'Ġms', 'Ġstar', 'link', 'Ġsatellites', 'Ġorbiting', 'âģ', 'Ħ', 'âģ', 'Ħ', 'Ġheight', 'Ġge', 'ost', 'ation', 'ary', 'Ġorbits', 'Ġthus', 'Ġoffer', 'Ġpractical', 'Ġearth', 'sat', 'Ġlat', 'encies', 'Ġaround', 'Ġms', 'Ġcomparable', 'Ġexisting', 'Ġcable', 'Ġfiber', 'Ġnetworks', 'Ġsystem', 'Ġuse', 'Ġpeer', 'ope', 'er', 'Ġprotocol', 'Ġclaimed', 'sim', 'pler', 'Ġalso', 'Ġincorporate', 'Ġend', 'end', 'Ġencryption', 'Ġnative', 'ly', 'Ġtechnology', 'Ġsatellite', 'Ġhardware', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġspace', 'x', 'Ġboard', 'Ġmember', 'Ġste', 'Ġjur', 'ts', 'Ġholding', 'Ġstar', 'link', 'Ġuser', 'Ġterminal', 'Ġj', 'une', 'Ġstar', 'link', 'Ġsatellites', 'Ġuse', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġk', 'rypt', 'Ġarg', 'Ġgas', 'Ġreaction', 'Ġmass', 'Ġorbit', 'Ġraising', 'Ġstation', 'Ġkeeping', 'Ġk', 'rypt', 'Ġhall', 'Ġthr', 'usters', 'Ġtend', 'Ġexhibit', 'Ġsignificantly', 'Ġhigher', 'Ġerosion', 'Ġflow', 'Ġchannel', 'Ġcompared', 'Ġsimilar', 'Ġelectric', 'Ġpropulsion', 'Ġsystem', 'Ġoperated', 'Ġxen', 'Ġk', 'rypt', 'Ġmuch', 'Ġabundant', 'Ġlower', 'Ġmarket', 'Ġprice', 'Ġspace', 'x', 'Ġclaims', 'nd', 'Ġgeneration', 'Ġthr', 'uster', 'Ġusing', 'Ġarg', 'Ġthrust', 'Ġspecific', 'Ġimpulse', 'Ġk', 'rypt', 'Ġfueled', 'Ġthr', 'uster', 'Ġsystem', 'Ġdirectly', 'Ġconnect', 'Ġsatellites', 'Ġhands', 'ets', 'like', 'Ġconst', 'ell', 'ations', 'Ġir', 'idium', 'Ġglobal', 'star', 'Ġth', 'ur', 'aya', 'ars', 'Ġinstead', 'Ġlinked', 'Ġflat', 'Ġuser', 'Ġterminals', 'Ġsize', 'Ġpizza', 'Ġphased', 'Ġarray', 'Ġantennas', 'Ġtrack', 'Ġsatellites', 'Ġterminals', 'Ġmounted', 'Ġanywhere', 'Ġlong', 'Ġsee', 'Ġincludes', 'Ġfast', 'moving', 'Ġobjects', 'Ġlike', 'Ġtrains', 'Ġphotographs', 'Ġcustomer', 'Ġantennas', 'Ġfirst', 'Ġseen', 'Ġinternet', 'Ġj', 'une', 'Ġsupporting', 'Ġearlier', 'Ġstatements', 'Ġspace', 'x', 'Ġce', 'Ġmus', 'k', 'Ġterminals', 'Ġwould', 'Ġlook', 'Ġlike', 'uf', 'Ġstick', 'Ġstar', 'link', 'Ġterminal', 'Ġmotors', 'Ġself', 'adjust', 'Ġoptimal', 'Ġangle', 'Ġview', 'Ġantenna', 'Ġknown', 'Ġinternally', 'ishy', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġlaunched', 'Ġpaid', 'Ġbeta', 'Ġservice', 'Ġu', 'Ġcalled', 'better', 'Ġnothing', 'Ġbeta', '",', 'Ġcharging', 'equ', 'ivalent', 'Ġuser']</t>
         </is>
       </c>
       <c r="C416" t="n">
@@ -5846,7 +5846,7 @@
       </c>
       <c r="B417" t="inlineStr">
         <is>
-          <t>['Ġlaunch', 'Ġstarship', 'Ġfollowing', 'Ġlasers', 'Ġinter', 'atellite', 'Ġcommunication', 'Ġmass', 'Ġlength', 'Ġft', 'Ġimprovements', 'Ġreduce', 'Ġbrightness', 'Ġincluding', 'Ġuse', 'Ġdie', 'lect', 'ric', 'Ġmirror', '016', 'Ġinitially', 'Ġlicensed', 'Ġsatellites', ':[', 'Ġstar', 'link', 'Ġsatellites', 'Ġalso', 'Ġinclude', 'Ġapproximately', 'Ġsquare', 'Ġmeter', 'Ġantenna', 'Ġwould', 'Ġallow', 'mobile', 'Ġsubscribers', 'Ġable', 'Ġcommunicate', 'Ġdirectly', 'Ġvia', 'Ġsatellite', 'Ġregular', 'Ġmobile', 'Ġdevices', 'Ġimplemented', 'Ġvia', 'Ġg', 'erman', 'licensed', 'Ġhosted', 'Ġpayload', 'Ġdeveloped', 'Ġtogether', 'Ġspace', 'x', "'s", 'Ġsubsidiary', 'Ġswarm', 'Ġtechnologies', 'mobile', 'Ġhardware', 'Ġsupplemental', 'Ġexisting', 'Ġk', 'u', 'band', 'Ġka', 'band', 'Ġsystems', 'Ġinter', 'atellite', 'Ġlaser', 'Ġlinks', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġgeneration', 'Ġsatellites', 'Ġlaunching', 'Ġmid', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġred', 'efined', 'Ġearly', 'Ġdifferent', 'Ġb', 'uss', 'es', 'Ġbus', 'planned', 'Ġmass', 'Ġroughly', 'Ġdimensions', 'Ġmass', 'Ġcurrent', 'Ġsatellites', 'Ġbus', 'initial', 'Ġdeployment', 'sometimes', 'Ġcalled', 'Ġmini', '"[', ']),', 'Ġmass', 'Ġmeasuring', 'Ġft', 'Ġft', 'Ġtotal', 'Ġarray', 'Ġft', 'Ġsolar', 'Ġarrays', 'Ġnumber', 'Ġcould', 'Ġoffer', 'Ġaround', 'Ġtimes', 'Ġusable', 'Ġbandwidth', 'Ġper', 'Ġsatellite', 'Ġsmaller', 'Ġstar', 'link', "'s", 'Ġoriginal', 'Ġones', 'Ġlaunched', 'Ġexisting', 'Ġrockets', 'Ġfour', 'Ġtimes', 'Ġcapacity', 'Ġground', 'Ġstation', 'Ġincrease', 'Ġspeed', 'Ġcapacity', 'Ġdue', 'Ġe', 'f', 'ï', '¬', 'ģ', 'cient', 'Ġarray', 'Ġantennas', 'Ġuse', 'Ġradio', 'Ġfrequencies', 'Ġband', 'Ġrange', 'oper', 'ational', 'Ġst', 'arsh', 'ield', 'oper', 'ational', 'initial', 'Ġdeployment', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġconstellation', 'Ġphase', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġorbital', 'Ġshell', 'Ġorbits', 'Ġtherefore', 'Ġsatellites', 'Ġaltitude', 'Ġbus', 'Ġstarship', 'planned', 'Ġmass', 'Ġfe', 'b', 'ruary', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġsuccessfully', 'Ġlaunched', 'Ġstar', 'link', 'Ġsatellites', 'Ġorbit', 'Ġincluding', 'Ġprototypes', 'Ġsatellites', 'Ġlater', 'Ġfailed', 'Ġde', 'orb', 'ited', 'Ġentering', 'Ġoperational', 'Ġservice']</t>
+          <t>['Ġterminal', 'Ġexpected', 'Ġservice', 'Ġlatency', 'Ġms', 'Ġms', 'Ġnext', 'Ġseveral', 'Ġmonths', '".[', 'Ġjan', 'uary', 'Ġpaid', 'Ġbeta', 'Ġservice', 'Ġextended', 'Ġcontinents', 'Ġstarting', 'Ġunited', 'Ġkingdom', 'Ġlarger', 'Ġhigh', 'performance', 'Ġversion', 'Ġantenna', 'Ġavailable', 'Ġuse', 'Ġstar', 'link', 'Ġbusiness', 'Ġservice', 'Ġtier', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġapplied', 'Ġpermission', 'Ġput', 'Ġterminals', 'Ġships', 'Ġexpectation', 'Ġentering', 'Ġmaritime', 'Ġmarket', 'Ġfuture', 'Ġaug', 'ust', 'Ġresponse', 'Ġopen', 'Ġinvitation', 'Ġspace', 'x', 'Ġterminal', 'Ġexamined', 'Ġsecurity', 'Ġcommunity', 'Ġsecurity', 'Ġspecialist', 'Ġl', 'enn', 'ert', 'Ġw', 'ou', 'ters', 'Ġpresented', 'Ġseveral', 'Ġtechnical', 'Ġarchitecture', 'Ġdetails', 'current', 'Ġstar', 'link', 'Ġterminals', 'Ġmain', 'Ġcontrol', 'Ġunit', 'Ġdish', 'Ġst', 'micro', 'elect', 'ronics', 'Ġcustom', 'Ġdesigned', 'Ġchip', 'Ġcod', 'en', 'amed', 'Ġcats', 'Ġquad', 'core', 'Ġarm', 'Ġcortex', 'based', 'Ġcontrol', 'Ġprocessor', 'Ġrunning', 'Ġlinux', 'Ġkernel', 'Ġbooted', 'Ġusing', 'Ġu', 'boot', 'Ġmain', 'Ġprocessor', 'Ġuses', 'Ġseveral', 'Ġcustom', 'Ġchips', 'Ġdigital', 'Ġbeam', 'Ġformer', 'Ġnamed', 'Ġsh', 'ir', 'az', 'Ġfront', 'end', 'Ġmodule', 'Ġnamed', 'Ġpuls', 'ar', 'ad', 'Ġmain', 'Ġcontrol', 'Ġunit', 'Ġcontrols', 'Ġarray', 'Ġdigital', 'Ġbeam', 'form', 'ers', 'Ġbeam', 'former', 'Ġcontrols', 'Ġfront', 'end', 'Ġmodules', 'Ġaddition', 'Ġterminal', 'Ġreceiver', 'Ġmotor', 'Ġcontrollers', 'Ġsynchron', 'ous', 'Ġclock', 'Ġgeneration', 'Ġpower', 'Ġether', 'net', 'Ġcircuits', 'Ġmanufactured', 'Ġspace', 'x', 'Ġmade', 'Ġapplications', 'Ġleast', 'Ġground', 'Ġstations', 'Ġunited', 'Ġstates', 'Ġj', 'uly', 'Ġapprovals', 'Ġfive', 'Ġfive', 'Ġstates', 'Ġtill', 'Ġfe', 'b', 'ruary', 'Ġstar', 'link', 'Ġused', 'Ġka', 'band', 'Ġconnect', 'Ġground', 'Ġstations', 'Ġlaunch', 'Ġmini', 'Ġadded', 'Ġfrequencies', 'Ġband', 'Ġrange', 'Ġtypical', 'Ġground', 'Ġstation', 'Ġright', 'Ġnine', 'Ġantennas', 'Ġf', 'enced', 'Ġarea', 'Ġaccording', 'Ġfiling', 'Ġspace', 'x', "'s", 'Ġground', 'Ġstations', 'Ġwould', 'Ġalso', 'Ġinstalled', 'site', 'Ġgoogle', 'Ġdata', 'cent', 'ers', 'Ġworldwide', 'Ġuser', 'Ġterminals', 'Ġground', 'Ġstations', 'Ġsatellite', 'Ġrevisions', 'Ġmicro', 'sat', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġmicro', 'sat', 'Ġmicro', 'sat', 'b', 'Ġoriginally', 'Ġslated', 'Ġlaunched', 'Ġmi', 'Ġcircular', 'Ġorbits', 'Ġapproximately', 'Â°', 'Ġinclination', 'Ġinclude', 'Ġpan']</t>
         </is>
       </c>
       <c r="C417" t="n">
@@ -5859,7 +5859,7 @@
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>['Ġmarch', 'Ġspace', 'x', 'Ġreported', 'Ġproducing', 'Ġsatellites', 'Ġper', 'Ġday', 'Ġdeployment', 'Ġfirst', 'Ġsatellites', 'Ġplanned', 'Ġorbital', 'Ġplanes', 'Ġsatellites', 'Ġrequested', 'Ġlower', 'Ġminimum', 'Ġelevation', 'Ġangle', 'Ġbeams', 'Ġimprove', 'Ġreception', 'Â°', 'Ġrather', 'Â°', 'Ġtwo', 'Ġorbital', 'Ġshells', ']:', 'Ġspace', 'x', 'Ġlaunched', 'Ġfirst', 'Ġsatellites', 'Ġconstellation', 'Ġmay', 'Ġmi', 'Ġorbit', 'Ġexpected', 'Ġlaunches', 'Ġtime', 'Ġsatellites', 'Ġcontinuous', 'Ġcoverage', 'Ġstar', 'link', 'Ġsatellites', 'Ġalso', 'Ġplanned', 'Ġlaunch', 'Ġstarship', 'development', 'Ġrocket', 'Ġspace', 'x', 'Ġmuch', 'Ġlarger', 'Ġpayload', 'Ġcapability', 'Ġinitial', 'Ġannouncement', 'Ġincluded', 'Ġplans', 'Ġlaunch', 'Ġstar', 'link', 'version', 'Ġsatellites', 'Ġtime', 'Ġcurrent', 'Ġplans', 'Ġcall', 'Ġstarship', 'Ġlaunch', 'Ġvehicle', 'Ġused', 'Ġlaunch', 'Ġfewer', 'Ġmuch', 'Ġlarger', 'Ġstar', 'link', 'Ġversion', 'Ġcontains', 'Ġfirst', 'Ġgeneration', 'Ġsatellites', 'Ġtint', 'Ġtint', 'Ġtest', 'Ġsatellites', 'Ġincluded', 'Ġlaunches', 'Ġconstellation', 'Ġdesign', 'Ġstatus', 'Ġfirst', 'Ġgeneration', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġphase', 'Ġgroup', 'Ġdesignation', 'Ġorbital', 'Ġshells', 'Ġorbital', 'Ġplanes', 'Ġcommitted', 'Ġcompletion', 'Ġdate', 'Ġdeployed', 'Ġsatellites', 'Ġj', 'une', 'Ġaltitude', 'Ġauthorized', 'Ġsatellites', 'Ġincl', 'Ġnation', 'Ġcount', 'Ġsatellites', 'Ġper', 'Ġhalf', 'Ġfull', 'Ġactive', 'Ġdecaying', 'Ġde', 'orb', 'ited', 'Ġgroup', 'Ġmi', 'Â°', 'Ġmarch', 'aim', 'ed', 'Ġaug', 'ust', 'ach', 'ieved', ')[', 'Ġmarch', 'Ġgroup', 'Ġmi', 'Â°', 'Ġgroup', 'Ġmi', 'Â°', 'Ġgroup', 'Ġmi', 'Â°', 'Ġmi', 'Â°', 'Ġmi', ')[', 'Â°', 'mber', 'mber', 'Ġmi', ')[', 'Â°', 'Ġmi', ')[', 'Â°', 'Ġspace', 'x', 'Ġplans', 'Ġabandon']</t>
+          <t>['chrom', 'atic', 'Ġvideo', 'Ġim', 'ager', 'Ġcameras', 'Ġfilm', 'Ġimages', 'Ġearth', 'Ġsatellite', 'Ġtwo', 'Ġsatellites', 'micro', 'sat', 'micro', 'sat', 'b', 'Ġmeant', 'Ġlaunched', 'Ġtogether', 'Ġsecondary', 'Ġpayload', 'Ġone', 'Ġir', 'idium', 'Ġnext', 'Ġflights', 'Ġinstead', 'Ġused', 'Ġground', 'based', 'Ġtests', 'Ġtime', 'Ġj', 'une', 'Ġannouncement', 'Ġspace', 'x', 'Ġstated', 'Ġplans', 'Ġlaunch', 'Ġfirst', 'Ġtwo', 'Ġdemonstration', 'Ġsatellites', 'Ġtarget', 'Ġdate', 'Ġsubsequently', 'Ġmoved', 'Ġspace', 'x', 'Ġbegan', 'Ġflight', 'Ġtesting', 'Ġsatellite', 'Ġtechnologies', 'Ġlaunch', 'Ġtwo', 'Ġtest', 'Ġsatellites', 'Ġtwo', 'Ġidentical', 'Ġsatellites', 'Ġcalled', 'Ġmicro', 'sat', 'Ġmicro', 'sat', 'b', 'Ġdevelopment', 'Ġrenamed', 'Ġtint', 'Ġtint', 'Ġupon', 'Ġorbital', 'Ġdeployment', 'Ġfe', 'b', 'ruary', 'Ġsatellites', 'Ġlaunched', 'Ġfal', 'con', 'Ġrocket', 'Ġpig', 'gy', 'pack', 'Ġpayload', 'Ġlaunching', 'Ġsatellite', 'Ġtint', 'Ġinserted', 'Ġmi', 'Ġorbit', 'Ġper', 'Ġfilings', 'Ġintended', 'Ġraise', 'Ġmi', 'Ġorbit', 'Ġoperational', 'Ġaltitude', 'Ġstar', 'link', 'Ġle', 'Ġsatellites', 'Ġper', 'Ġearliest', 'Ġregulatory', 'Ġfilings', 'Ġstayed', 'Ġclose', 'Ġoriginal', 'Ġorbits', 'Ġspace', 'x', 'Ġannounced', 'mber', 'Ġwould', 'Ġlike', 'Ġoperate', 'Ġinitial', 'Ġshell', 'Ġsatellites', 'Ġconstellation', 'Ġmi', 'Ġorbital', 'Ġaltitude', 'Ġaltitude', 'Ġsimilar', 'Ġorbits', 'Ġtint', 'Ġstayed', 'Ġsatellites', 'Ġorbit', 'Ġcircular', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġmi', 'Ġaltitude', 'Ġhigh', 'cl', 'ination', 'Ġorbit', 'Ġplanned', 'Ġtwelve', 'month', 'Ġduration', 'Ġsatellites', 'Ġcommunicate', 'Ġthree', 'Ġtesting', 'Ġground', 'Ġstations', 'Ġwashing', 'ton', 'Ġstate', 'Ġcal', 'ornia', 'Ġshort', 'term', 'Ġexperiments', 'Ġless', 'Ġten', 'Ġminutes', 'Ġduration', 'Ġroughly', 'Ġdaily', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġmay', 'Ġfollowing', 'Ġflat', 'panel', 'Ġdesign', 'Ġmultiple', 'Ġhigh', 'put', 'Ġantennas', 'Ġsingle', 'Ġsolar', 'Ġarray', 'Ġmass', 'Ġhall', 'effect', 'Ġthr', 'usters', 'Ġusing', 'Ġk', 'rypt', 'Ġreaction', 'Ġmass', 'Ġposition', 'Ġadjustment', 'Ġorbit', 'Ġaltitude', 'Ġmaintenance', 'Ġde', 'orbit', 'Ġstar', 'Ġtracker', 'Ġnavigation', 'Ġsystem', 'Ġprecision', 'Ġpointing', 'Ġable', 'Ġuse', 'Ġdepartment', 'Ġdefense', 'provided', 'Ġdebris', 'Ġdata', 'Ġautonom', 'ously', 'Ġavoid', 'Ġcollision']</t>
         </is>
       </c>
       <c r="C418" t="n">
@@ -5872,7 +5872,7 @@
       </c>
       <c r="B419" t="inlineStr">
         <is>
-          <t>['Ġapproved', 'Ġphase', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġearly', 'Ġdesigns', 'Ġphase', 'Ġsatellites', 'Ġalt', 'itudes', 'Ġaround', 'âĢĵ', 'âĢĵ', 'Ġmi', 'Ġspace', 'x', 'Ġinitially', 'Ġrequested', 'Ġlower', 'Ġfirst', 'Ġsatellites', 'Ġapr', 'il', 'Ġrequested', 'Ġlower', 'Ġhigher', 'Ġsatellite', 'Ġorbits', 'Ġmi', ').[', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġmodified', 'Ġarchitecture', 'Ġstar', 'link', 'Ġnetwork', 'Ġspace', 'x', 'Ġsubmitted', 'Ġapplication', 'Ġproposing', 'Ġoperate', 'Ġsatellites', 'Ġlower', 'Ġorbits', 'Ġfirst', 'Ġphase', 'Ġpreviously', 'Ġauthorized', 'Ġfirst', 'Ġphase', 'Ġstill', 'Ġinclude', 'Ġsatellites', 'Ġfirst', 'Ġshell', 'Ġorbiting', 'Ġmi', 'Ġplanes', 'Ġinclined', 'Â°', 'Ġchange', 'Ġfirst', 'Ġshell', 'Ġconstellation', 'Ġlaunched', 'Ġlargely', 'Ġspace', 'x', 'Ġalso', 'Ġapplied', 'Ġunited', 'Ġstates', 'Ġuse', 'Ġe', 'band', 'Ġconstellation', 'Ġapproved', 'Ġapplication', 'Ġapr', 'il', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġreleased', 'Ġnew', 'Ġgroup', 'Ġstar', 'link', 'Ġsatellites', 'Ġfirst', 'Ġstar', 'link', 'Ġsatellites', 'Ġpolar', 'Ġorbits', 'Ġlaunch', 'Ġsurpassed', 'ro', "'s", 'Ġrecord', 'Ġlaunching', 'Ġsatellites', 'Ġone', 'Ġmission', 'Ġtaking', '025', 'Ġcumulative', 'Ġnumber', 'Ġsatellites', 'Ġdeployed', 'Ġstar', 'link', 'Ġdate', 'Ġfe', 'b', 'ruary', 'Ġsatellites', 'Ġlaunched', 'Ġstar', 'link', 'Ġgroup', 'Ġg', 'rated', 'Ġge', 'om', 'agnetic', 'Ġstorm', 'Ġoccurred', 'Ġfe', 'b', 'ruary', 'Ġcaused', 'Ġatmosphere', 'Ġwarm', 'Ġdensity', 'Ġlow', 'Ġdeployment', 'Ġalt', 'itudes', 'Ġincrease', 'Ġpredictions', 'Ġsatellites', 'Ġmight', 'Ġlost', 'Ġdue', 'Ġdrag', 'Ġevent', 'Ġsatellites', 'ent', 'ered', 'Ġatmosphere', 'Ġfe', 'b', 'ruary', 'Ġremaining', 'Ġable', 'Ġraise', 'Ġorbits', 'Ġavoid', 'Ġloss', 'Ġdue', 'Ġstorm', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġfe', 'b', 'Ġlaunch', 'Ġplus', 'Ġhours', 'Ġsignal', 'Ġpollution', 'second', 'Ġexposure', 'Ġimage', 'Ġtaken', 'Ġbl', 'anco', 'Ġfour', 'meter', "')", 'Ġtelescope', 'Ġcer', 'ro', 'l', 'olo', 'Ġinter', 'amer', 'ican', 'Ġobserv', 'atory', 'mber', 'Ġmarch', 'Ġspace', 'x', 'Ġsubmitted', 'Ġapplication', 'Ġadd', 'Ġv', 'band', 'Ġpayload', 'Ġsecond', 'Ġgeneration', 'Ġsatellites', 'Ġrather', 'Ġfly', 'Ġphase', 'Ġv', 'band', 'Ġsatellites']</t>
+          <t>['Ġaltitude', 'Ġmi', 'Ġcomponents', 'Ġdesign', 'Ġquickly', 'Ġburn', 'Ġearth', "'s", 'Ġatmosphere', 'Ġend', 'Ġsatellite', "'s", 'Ġlif', 'ecycle', '".', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'mber', 'Ġfollowing', 'Ġadditional', 'Ġcharacteristics', 'Ġcomponents', 'Ġdesign', 'Ġcompletely', 'Ġdemise', 'Ġburn', 'Ġearth', "'s", 'Ġatmosphere', 'Ġend', 'Ġsatellite', "'s", 'Ġlife', 'Ġka', 'band', 'Ġadded', 'Ġmass', 'Ġone', 'Ġnumbered', 'Ġcalled', 'arks', 'Ġal', 'bed', 'Ġreduced', 'Ġusing', 'Ġspecial', 'Ġcoating', 'Ġmethod', 'Ġabandoned', 'Ġdue', 'Ġthermal', 'Ġissues', 'Ġir', 'Ġtint', 'test', 'oper', 'ational', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'Ġninth', 'Ġlaunch', 'Ġaug', 'ust', 'Ġvis', 'ors', 'Ġblock', 'Ġsunlight', 'ï', '¬', 'Ĥ', 'ect', 'ing', 'Ġparts', 'Ġsatellite', 'Ġreduce', 'Ġal', 'bed', 'Ġstar', 'link', 'Ġsatellites', 'Ġlaunched', 'Ġsince', 'Ġjan', 'uary', 'Ġfollowing', 'Ġadditional', 'Ġcharacteristics', 'Ġlasers', 'Ġinter', 'atellite', 'Ġcommunication', 'Ġmass', 'Ġvis', 'ors', 'Ġblocked', 'Ġsunlight', 'Ġremoved', 'Ġsatellites', 'Ġlaunched', 'Ġse', 'pt', 'ember', 'Ġonwards', 'Ġsatellites', 'Ġbuses', 'Ġtwo', 'Ġsolar', 'Ġarrays', 'Ġderived', 'Ġstar', 'link', 'Ġmilitary', 'Ġuse', 'Ġhost', 'Ġclassified', 'Ġgovernment', 'Ġmilitary', 'Ġpayload', 'Ġspace', 'x', 'Ġpreparing', 'Ġproduction', 'Ġstar', 'link', 'Ġsatellites', 'Ġearly', 'Ġaccording', 'Ġmus', 'k', 'Ġstar', 'link', 'Ġsatellites', 'Ġorder', 'Ġmagnitude', 'Ġbetter', 'Ġstar', 'link', 'Ġterms', 'Ġcommunications', 'Ġbandwidth', 'Ġspace', 'x', 'Ġhoped', 'Ġbegin', 'Ġlaunching', 'Ġstar', 'link', 'Ġmay', 'Ġspace', 'x', 'Ġsaid', 'Ġpublicly', 'Ġsatellites', 'Ġsecond', 'generation', 'Ġconstellation', 'Ġwould', 'Ġneed', 'Ġlaunched', 'Ġstarship', 'Ġlarge', 'Ġfit', 'Ġinside', 'Ġfal', 'con', 'Ġfair', 'ing', 'Ġhowever', 'Ġaug', 'ust', 'Ġspace', 'x', 'Ġmade', 'Ġformal', 'Ġregulatory', 'Ġfilings', 'Ġindicated', 'Ġwould', 'Ġbuild', 'Ġsatellites', 'Ġsecond', 'generation', 'Ġconstellation', 'Ġtwo', 'Ġdifferent', 'Ġtechnically', 'Ġidentical', 'Ġform', 'Ġfactors', 'Ġone', 'Ġphysical', 'Ġstructures', 'Ġtailored', 'Ġlaunching', 'Ġfal', 'con', 'Ġone', 'Ġtailored', 'Ġlaunching', 'Ġstarship', 'Ġstar', 'link', 'Ġlarger', 'Ġheavier', 'Ġstar', 'link', 'Ġsatellites', 'Ġstar', 'link', 'Ġsecond', 'generation', 'Ġsatellites', 'Ġplanned']</t>
         </is>
       </c>
       <c r="C419" t="n">
@@ -5885,7 +5885,7 @@
       </c>
       <c r="B420" t="inlineStr">
         <is>
-          <t>['Ġoriginally', 'Ġplanned', 'Ġauthorized', 'Ġrequest', 'Ġsubject', 'Ġapproval', 'Ġphase', 'Ġgroup', 'Ġdesignation', 'Ġorbital', 'Ġshells', 'Ġorbital', 'Ġplanes', 'Ġcommitted', 'Ġcompletion', 'Ġdate', 'Ġdeployed', 'Ġsatellites', 'Ġaug', 'ust', 'Ġaltitude', 'Ġplanned', 'Ġsatellites', 'Ġincl', 'Ġnation', 'Ġcount', 'Ġsatellites', 'Ġper', 'Ġhalf', 'Ġfull', 'Ġactive', 'Ġdecaying', 'Ġde', 'orb', 'ited', 'Ġgroup', 'Ġmi', 'b', 'Â°', 'Ġde', 'cember', 'Ġde', 'cember', 'Ġgroup', 'Ġmi', 'b', 'Â°', 'Ġmi', 'b', 'Â°', 'Ġspace', 'x', 'Ġabandoned', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġproposed', 'Ġamendment', 'Ġb', 'Ġlimited', 'Ġphase', 'Ġsatellites', 'Ġacross', 'Ġshells', 'Ġunknown', 'Ġstarship', 'Ġable', 'Ġlaunch', 'Ġsecond', 'Ġgeneration', 'Ġsatellites', 'Ġspace', 'x', 'Ġmodified', 'Ġoriginal', 'Ġblueprint', 'Ġsmaller', 'Ġcompact', 'Ġone', 'Ġnamed', 'Ġmini', '".', 'Ġadjustment', 'Ġallowed', 'Ġfal', 'con', 'Ġtransport', 'Ġsatellites', 'Ġthough', 'Ġmany', 'Ġorbit', 'Ġfirst', 'Ġset', 'Ġsatellites', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġcommitted', 'Ġreducing', 'Ġdebris', 'Ġkeeping', 'Ġstar', 'link', 'Ġtension', 'Ġrods', 'Ġhold', 'Ġmini', 'atell', 'ites', 'Ġtogether', 'Ġattached', 'Ġfal', 'con', 'Ġsecond', 'Ġstage', 'Ġtension', 'Ġrods', 'Ġdiscarded', 'Ġorbit', 'Ġlaunching', 'Ġearlier', 'Ġversions', 'Ġstar', 'link', 'Ġsatellites', 'Ġobservations', 'Ġconfirm', 'Ġmini', 'atell', 'ites', 'Ġhost', 'Ġtwo', 'Ġsolar', 'Ġpanels', 'Ġlike', 'Ġstarship', 'Ġsatellites', 'Ġplanned', 'Ġlarge', 'Ġnumber', 'Ġsatellites', 'Ġmet', 'Ġcriticism', 'Ġastronomical', 'Ġcommunity', 'Ġconcerns', 'Ġlight', 'Ġastronomers', 'Ġclaim', 'Ġnumber', 'Ġvisible', 'Ġsatellites', 'number', 'Ġvisible', 'Ġstars', 'Ġbrightness', 'Ġoptical', 'Ġradio', 'Ġwavelengths', 'Ġseverely', 'Ġimpact', 'Ġscientific', 'Ġobservations', 'Ġastronomers', 'Ġschedule', 'Ġobservations', 'Ġavoid', 'Ġpointing', 'Ġsatellites', 'Ġcurrently', 'Ġorbit', 'getting', 'Ġdifficult', 'Ġsatellites', 'Ġcome', 'Ġonline', 'Ġinternational', 'Ġastronomical', 'Ġunion', 'Ġnational', 'Ġradio', 'Ġastronomy', 'Ġobserv', 'atory', 'Ġsquare', 'Ġkilomet', 'Ġarray', 'Ġorganization', 'Ġreleased', 'Ġofficial', 'Ġstatements', 'Ġexpressing', 'Ġconcern', 'mber', 'Ġfour', 'meter', "')", 'Ġbl', 'anco', 'Ġtelescope', 'Ġcer', 'ro', 'l', 'olo', 'Ġinter', 'amer', 'ican', 'Ġobserv', 'atory', 'ct', 'io', 'Ġrecorded', 'Ġstrong', 'Ġsignal', 'Ġloss', 'Ġappearance']</t>
+          <t>['Ġlaunch', 'Ġstarship', 'Ġfollowing', 'Ġlasers', 'Ġinter', 'atellite', 'Ġcommunication', 'Ġmass', 'Ġlength', 'Ġft', 'Ġimprovements', 'Ġreduce', 'Ġbrightness', 'Ġincluding', 'Ġuse', 'Ġdie', 'lect', 'ric', 'Ġmirror', '016', 'Ġinitially', 'Ġlicensed', 'Ġsatellites', ':[', 'Ġstar', 'link', 'Ġsatellites', 'Ġalso', 'Ġinclude', 'Ġapproximately', 'Ġsquare', 'Ġmeter', 'Ġantenna', 'Ġwould', 'Ġallow', 'mobile', 'Ġsubscribers', 'Ġable', 'Ġcommunicate', 'Ġdirectly', 'Ġvia', 'Ġsatellite', 'Ġregular', 'Ġmobile', 'Ġdevices', 'Ġimplemented', 'Ġvia', 'Ġg', 'erman', 'licensed', 'Ġhosted', 'Ġpayload', 'Ġdeveloped', 'Ġtogether', 'Ġspace', 'x', "'s", 'Ġsubsidiary', 'Ġswarm', 'Ġtechnologies', 'mobile', 'Ġhardware', 'Ġsupplemental', 'Ġexisting', 'Ġk', 'u', 'band', 'Ġka', 'band', 'Ġsystems', 'Ġinter', 'atellite', 'Ġlaser', 'Ġlinks', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġgeneration', 'Ġsatellites', 'Ġlaunching', 'Ġmid', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġred', 'efined', 'Ġearly', 'Ġdifferent', 'Ġb', 'uss', 'es', 'Ġbus', 'planned', 'Ġmass', 'Ġroughly', 'Ġdimensions', 'Ġmass', 'Ġcurrent', 'Ġsatellites', 'Ġbus', 'initial', 'Ġdeployment', 'sometimes', 'Ġcalled', 'Ġmini', '"[', ']),', 'Ġmass', 'Ġmeasuring', 'Ġft', 'Ġft', 'Ġtotal', 'Ġarray', 'Ġft', 'Ġsolar', 'Ġarrays', 'Ġnumber', 'Ġcould', 'Ġoffer', 'Ġaround', 'Ġtimes', 'Ġusable', 'Ġbandwidth', 'Ġper', 'Ġsatellite', 'Ġsmaller', 'Ġstar', 'link', "'s", 'Ġoriginal', 'Ġones', 'Ġlaunched', 'Ġexisting', 'Ġrockets', 'Ġfour', 'Ġtimes', 'Ġcapacity', 'Ġground', 'Ġstation', 'Ġincrease', 'Ġspeed', 'Ġcapacity', 'Ġdue', 'Ġe', 'f', 'ï', '¬', 'ģ', 'cient', 'Ġarray', 'Ġantennas', 'Ġuse', 'Ġradio', 'Ġfrequencies', 'Ġband', 'Ġrange', 'oper', 'ational', 'Ġst', 'arsh', 'ield', 'oper', 'ational', 'initial', 'Ġdeployment', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġconstellation', 'Ġphase', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġorbital', 'Ġshell', 'Ġorbits', 'Ġtherefore', 'Ġsatellites', 'Ġaltitude', 'Ġbus', 'Ġstarship', 'planned', 'Ġmass', 'Ġfe', 'b', 'ruary', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġsuccessfully', 'Ġlaunched', 'Ġstar', 'link', 'Ġsatellites', 'Ġorbit', 'Ġincluding', 'Ġprototypes', 'Ġsatellites', 'Ġlater', 'Ġfailed', 'Ġde', 'orb', 'ited', 'Ġentering', 'Ġoperational', 'Ġservice']</t>
         </is>
       </c>
       <c r="C420" t="n">
@@ -5898,7 +5898,7 @@
       </c>
       <c r="B421" t="inlineStr">
         <is>
-          <t>['Ġwhite', 'Ġlines', 'Ġdec', 'Ġshot', 'right', 'Ġimage', 'Ġimage', 'Ġnoise', 'Ġcorrelated', 'Ġtransit', 'Ġstar', 'link', 'Ġsatellite', 'Ġtrain', 'Ġlaunched', 'Ġweek', 'Ġearlier', 'Ġsecond', 'Ġgeneration', 'Ġimpact', 'Ġastronomy', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ã¼', 'bing', 'en', 'Ġg', 'erman', 'Ġstar', 'link', 'Ġseen', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġtim', 'el', 'apse', 'Ġrecently', 'Ġdeployed', 'Ġspace', 'x', 'Ġrepresentatives', 'Ġmus', 'k', 'Ġclaimed', 'Ġsatellites', 'Ġminimal', 'Ġimpact', 'Ġeasily', 'Ġmit', 'igated', 'Ġpixel', 'Ġmask', 'ing', 'Ġimage', 'Ġstacking', 'Ġhowever', 'Ġprofessional', 'Ġastronomers', 'Ġdisputed', 'Ġclaims', 'Ġbased', 'Ġinitial', 'Ġobservation', 'Ġstar', 'link', 'Ġsatellites', 'Ġfirst', 'Ġlaunch', 'Ġshortly', 'Ġdeployment', 'Ġlaunch', 'Ġlater', 'Ġstatements', 'Ġtwitter', 'Ġmus', 'k', 'Ġstated', 'Ġspace', 'x', 'Ġwork', 'Ġreducing', 'Ġal', 'bed', 'Ġsatellites', 'Ġprovide', 'demand', 'Ġorientation', 'Ġadjustments', 'Ġastronomical', 'Ġexperiments', 'Ġone', 'Ġstar', 'link', 'Ġsatellite', 'st', 'arl', 'ink', 'arks', 'Ġlaunched', 'Ġexperimental', 'Ġcoating', 'Ġreduce', 'Ġal', 'bed', 'Ġreduction', 'Ġg', 'band', 'Ġmagnitude', 'Ġmagnitude', '%).', 'Ġdespite', 'Ġmeasures', 'Ġastronomers', 'Ġfound', 'Ġsatellites', 'Ġstill', 'Ġbright', 'Ġthus', 'Ġmaking', 'arks', 'Ġessentially', 'dead', 'Ġend', '".[', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġwrote', 'Ġfiling', 'Ġwould', 'Ġtest', 'Ġnew', 'Ġmethods', 'Ġmitigating', 'Ġlight', 'Ġpollution', 'Ġalso', 'Ġprovide', 'Ġaccess', 'Ġsatellite', 'Ġtracking', 'Ġdata', 'Ġastronomers', 'better', 'Ġcoordinate', 'Ġobservations', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġannounced', 'Ġcompany', 'Ġwould', 'Ġintroduce', 'Ġnew', 'Ġsun', 'sh', 'ade', 'Ġdesigned', 'Ġreduce', 'Ġbrightness', 'Ġstar', 'link', 'Ġsatellites', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġsatellites', 'Ġsun', 'sh', 'ade', 'Ġoct', 'ober', 'Ġanalysis', 'Ġfound', 'Ġmarginally', 'Ġf', 'ter', 'arks', 'Ġjan', 'uary', 'Ġstudy', 'Ġpinned', 'Ġbrightness', 'Ġoriginal', 'Ġdesign', 'Ġaccording', 'Ġmay', 'Ġstudy', 'Ġlarge', 'Ġnumber', 'Ġfast', 'moving', 'Ġtransmitting', 'Ġstations', 'e', 'Ġsatellites', 'Ġcause', 'Ġinterference', 'Ġnew', 'Ġanalysis', 'Ġmethods', 'Ġcould', 'Ġmitigate', 'Ġeffects', 'Ġdata', 'Ġloss', 'Ġinevitable', 'Ġincreasing', 'Ġtime', 'Ġneeded', 'Ġstudy', 'Ġlimiting', 'Ġoverall', 'Ġamount', 'Ġscience', 'Ġdone', '".[', 'Ġfe', 'b', 'ruary', 'Ġinternational', 'Ġastronomical', 'Ġunion', 'Ġestablished', 'Ġcenter', 'Ġhelp', 'Ġastronomers']</t>
+          <t>['Ġmarch', 'Ġspace', 'x', 'Ġreported', 'Ġproducing', 'Ġsatellites', 'Ġper', 'Ġday', 'Ġdeployment', 'Ġfirst', 'Ġsatellites', 'Ġplanned', 'Ġorbital', 'Ġplanes', 'Ġsatellites', 'Ġrequested', 'Ġlower', 'Ġminimum', 'Ġelevation', 'Ġangle', 'Ġbeams', 'Ġimprove', 'Ġreception', 'Â°', 'Ġrather', 'Â°', 'Ġtwo', 'Ġorbital', 'Ġshells', ']:', 'Ġspace', 'x', 'Ġlaunched', 'Ġfirst', 'Ġsatellites', 'Ġconstellation', 'Ġmay', 'Ġmi', 'Ġorbit', 'Ġexpected', 'Ġlaunches', 'Ġtime', 'Ġsatellites', 'Ġcontinuous', 'Ġcoverage', 'Ġstar', 'link', 'Ġsatellites', 'Ġalso', 'Ġplanned', 'Ġlaunch', 'Ġstarship', 'development', 'Ġrocket', 'Ġspace', 'x', 'Ġmuch', 'Ġlarger', 'Ġpayload', 'Ġcapability', 'Ġinitial', 'Ġannouncement', 'Ġincluded', 'Ġplans', 'Ġlaunch', 'Ġstar', 'link', 'version', 'Ġsatellites', 'Ġtime', 'Ġcurrent', 'Ġplans', 'Ġcall', 'Ġstarship', 'Ġlaunch', 'Ġvehicle', 'Ġused', 'Ġlaunch', 'Ġfewer', 'Ġmuch', 'Ġlarger', 'Ġstar', 'link', 'Ġversion', 'Ġcontains', 'Ġfirst', 'Ġgeneration', 'Ġsatellites', 'Ġtint', 'Ġtint', 'Ġtest', 'Ġsatellites', 'Ġincluded', 'Ġlaunches', 'Ġconstellation', 'Ġdesign', 'Ġstatus', 'Ġfirst', 'Ġgeneration', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġphase', 'Ġgroup', 'Ġdesignation', 'Ġorbital', 'Ġshells', 'Ġorbital', 'Ġplanes', 'Ġcommitted', 'Ġcompletion', 'Ġdate', 'Ġdeployed', 'Ġsatellites', 'Ġj', 'une', 'Ġaltitude', 'Ġauthorized', 'Ġsatellites', 'Ġincl', 'Ġnation', 'Ġcount', 'Ġsatellites', 'Ġper', 'Ġhalf', 'Ġfull', 'Ġactive', 'Ġdecaying', 'Ġde', 'orb', 'ited', 'Ġgroup', 'Ġmi', 'Â°', 'Ġmarch', 'aim', 'ed', 'Ġaug', 'ust', 'ach', 'ieved', ')[', 'Ġmarch', 'Ġgroup', 'Ġmi', 'Â°', 'Ġgroup', 'Ġmi', 'Â°', 'Ġgroup', 'Ġmi', 'Â°', 'Ġmi', 'Â°', 'Ġmi', ')[', 'Â°', 'mber', 'mber', 'Ġmi', ')[', 'Â°', 'Ġmi', ')[', 'Â°', 'Ġspace', 'x', 'Ġplans', 'Ġabandon']</t>
         </is>
       </c>
       <c r="C421" t="n">
@@ -5911,7 +5911,7 @@
       </c>
       <c r="B422" t="inlineStr">
         <is>
-          <t>['Ġdeal', 'Ġadverse', 'Ġeffects', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'Ġstar', 'link', 'Ġwork', 'Ġinclude', 'Ġdevelopment', 'Ġsoftware', 'Ġtools', 'Ġastronomers', 'Ġadvancement', 'Ġnational', 'Ġinternational', 'Ġpolicies', 'Ġcommunity', 'Ġoutreach', 'Ġwork', 'Ġindustry', 'Ġrelevant', 'Ġtechnologies', 'Ġj', 'une', 'Ġreleased', 'Ġwebsite', 'Ġastronomers', 'Ġdeal', 'Ġadverse', 'Ġeffects', 'Ġvia', 'Ġsatellite', 'Ġtracking', 'Ġenable', 'Ġastronomers', 'Ġable', 'Ġtrack', 'Ġsatellites', 'Ġable', 'Ġavoid', 'Ġtime', 'Ġminimal', 'Ġimpact', 'Ġcurrent', 'Ġwork', 'Ġfirst', 'Ġbatch', 'Ġgeneration', 'Ġspacecraft', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġsatellites', 'Ġreferred', 'mini', 'Ġsmaller', 'Ġfull', 'sized', 'Ġgen', 'Ġspacecraft', 'Ġcome', 'Ġlater', 'Ġspace', 'x', 'Ġuses', 'Ġbrightness', 'Ġmitigation', 'Ġgen', 'Ġincludes', 'Ġmirror', 'like', 'Ġsurface', 'Ġreflects', 'Ġsunlight', 'Ġback', 'Ġspace', 'Ġorient', 'Ġsolar', 'Ġpanels', 'Ġobservers', 'Ġground', 'Ġsee', 'Ġdark', 'Ġsides', 'Ġmin', 'Ġf', 'ter', 'Ġgen', 'Ġspacecraft', 'Ġdespite', 'Ġfour', 'Ġtimes', 'Ġlarge', 'Ġaccording', 'Ġobservational', 'Ġstudy', 'Ġpublished', 'Ġj', 'une', 'Ġbright', 'Ġgen', 'Ġplaced', 'Ġfinal', 'Ġorbit', 'Ġmin', 'Ġappear', 'Ġtimes', 'Ġbrighter', 'Ġreach', 'Ġtarget', 'Ġorbit', 'Ġlarge', 'Ġnumber', 'Ġsatellites', 'Ġemployed', 'Ġstar', 'link', 'Ġmay', 'Ġcreate', 'Ġlong', 'term', 'Ġdanger', 'Ġspace', 'Ġdebris', 'Ġresulting', 'Ġplacing', 'Ġthousands', 'Ġsatellites', 'Ġorbit', 'Ġrisk', 'Ġcausing', 'Ġsatellite', 'Ġcollision', 'Ġpotentially', 'Ġtriggering', 'Ġphenomenon', 'Ġknown', 'Ġk', 'essler', 'Ġsyndrome', 'Ġspace', 'x', 'Ġsaid', 'Ġsatellites', 'Ġlaunched', 'Ġlower', 'Ġaltitude', 'Ġfailed', 'Ġsatellites', 'Ġexpected', 'Ġde', 'orbit', 'Ġwithin', 'Ġfive', 'Ġyears', 'Ġwithout', 'Ġearly', 'Ġprogram', 'Ġnear', 'miss', 'Ġoccurred', 'Ġspace', 'x', 'Ġmove', 'Ġsatellite', '000', 'Ġchance', 'Ġcoll', 'iding', 'Ġeuro', 'pe', 'Ġone', 'Ġten', 'Ġtimes', 'Ġhigher', 'Ġes', "'s", 'Ġthreshold', 'Ġavoidance', 'Ġmaneuvers', 'Ġspace', 'x', 'Ġsubsequently', 'Ġfixed', 'Ġissue', 'Ġp', 'aging', 'Ġsystem', 'Ġdisrupted', 'Ġemails', 'Ġes', 'Ġspace', 'x', 'Ġes', 'Ġsaid', 'Ġplans', 'Ġinvest', 'Ġtechnologies', 'Ġautomate', 'Ġsatellite', 'Ġcollision', 'Ġavoidance', 'Ġch', 'inese', 'Ġauthorities', 'Ġlodged', 'Ġcomplaint', 'Ġunited', 'Ġnations', 'Ġsaying', 'Ġspace', 'Ġstation', 'Ġperformed', 'Ġev', 'asive', 'Ġmaneuvers', 'Ġyear', 'Ġavoid', 'Ġincreased', 'Ġrisk', 'Ġsatellite', 'Ġcollision', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġsatellites', 'Ġdocument', 'Ġch', 'inese', 'Ġdelegates', 'Ġsaid', 'Ġcontinuously', 'Ġmaneuver', 'ing']</t>
+          <t>['Ġapproved', 'Ġphase', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġearly', 'Ġdesigns', 'Ġphase', 'Ġsatellites', 'Ġalt', 'itudes', 'Ġaround', 'âĢĵ', 'âĢĵ', 'Ġmi', 'Ġspace', 'x', 'Ġinitially', 'Ġrequested', 'Ġlower', 'Ġfirst', 'Ġsatellites', 'Ġapr', 'il', 'Ġrequested', 'Ġlower', 'Ġhigher', 'Ġsatellite', 'Ġorbits', 'Ġmi', ').[', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġmodified', 'Ġarchitecture', 'Ġstar', 'link', 'Ġnetwork', 'Ġspace', 'x', 'Ġsubmitted', 'Ġapplication', 'Ġproposing', 'Ġoperate', 'Ġsatellites', 'Ġlower', 'Ġorbits', 'Ġfirst', 'Ġphase', 'Ġpreviously', 'Ġauthorized', 'Ġfirst', 'Ġphase', 'Ġstill', 'Ġinclude', 'Ġsatellites', 'Ġfirst', 'Ġshell', 'Ġorbiting', 'Ġmi', 'Ġplanes', 'Ġinclined', 'Â°', 'Ġchange', 'Ġfirst', 'Ġshell', 'Ġconstellation', 'Ġlaunched', 'Ġlargely', 'Ġspace', 'x', 'Ġalso', 'Ġapplied', 'Ġunited', 'Ġstates', 'Ġuse', 'Ġe', 'band', 'Ġconstellation', 'Ġapproved', 'Ġapplication', 'Ġapr', 'il', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġreleased', 'Ġnew', 'Ġgroup', 'Ġstar', 'link', 'Ġsatellites', 'Ġfirst', 'Ġstar', 'link', 'Ġsatellites', 'Ġpolar', 'Ġorbits', 'Ġlaunch', 'Ġsurpassed', 'ro', "'s", 'Ġrecord', 'Ġlaunching', 'Ġsatellites', 'Ġone', 'Ġmission', 'Ġtaking', '025', 'Ġcumulative', 'Ġnumber', 'Ġsatellites', 'Ġdeployed', 'Ġstar', 'link', 'Ġdate', 'Ġfe', 'b', 'ruary', 'Ġsatellites', 'Ġlaunched', 'Ġstar', 'link', 'Ġgroup', 'Ġg', 'rated', 'Ġge', 'om', 'agnetic', 'Ġstorm', 'Ġoccurred', 'Ġfe', 'b', 'ruary', 'Ġcaused', 'Ġatmosphere', 'Ġwarm', 'Ġdensity', 'Ġlow', 'Ġdeployment', 'Ġalt', 'itudes', 'Ġincrease', 'Ġpredictions', 'Ġsatellites', 'Ġmight', 'Ġlost', 'Ġdue', 'Ġdrag', 'Ġevent', 'Ġsatellites', 'ent', 'ered', 'Ġatmosphere', 'Ġfe', 'b', 'ruary', 'Ġremaining', 'Ġable', 'Ġraise', 'Ġorbits', 'Ġavoid', 'Ġloss', 'Ġdue', 'Ġstorm', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġfe', 'b', 'Ġlaunch', 'Ġplus', 'Ġhours', 'Ġsignal', 'Ġpollution', 'second', 'Ġexposure', 'Ġimage', 'Ġtaken', 'Ġbl', 'anco', 'Ġfour', 'meter', "')", 'Ġtelescope', 'Ġcer', 'ro', 'l', 'olo', 'Ġinter', 'amer', 'ican', 'Ġobserv', 'atory', 'mber', 'Ġmarch', 'Ġspace', 'x', 'Ġsubmitted', 'Ġapplication', 'Ġadd', 'Ġv', 'band', 'Ġpayload', 'Ġsecond', 'Ġgeneration', 'Ġsatellites', 'Ġrather', 'Ġfly', 'Ġphase', 'Ġv', 'band', 'Ġsatellites']</t>
         </is>
       </c>
       <c r="C422" t="n">
@@ -5924,7 +5924,7 @@
       </c>
       <c r="B423" t="inlineStr">
         <is>
-          <t>['Ġstar', 'link', 'Ġsatellites', 'Ġposed', 'Ġrisk', 'Ġcollision', 'Ġtwo', 'Ġclose', 'Ġencounters', 'Ġsatellites', 'Ġj', 'uly', 'Ġoct', 'ober', 'Ġconstituted', 'Ġdangers', 'Ġlife', 'Ġhealth', 'Ġastronauts', 'Ġaboard', 'Ġch', 'inese', 'iang', 'ong', 'Ġspace', 'Ġstation', 'Ġreported', 'Ġissues', 'Ġplus', 'Ġcurrent', 'Ġplans', 'Ġextension', 'Ġconstellation', 'Ġmotivated', 'Ġformal', 'Ġletter', 'Ġnational', 'Ġtelecommunications', 'Ġinformation', 'Ġadministration', 'nt', 'ia', 'Ġbehalf', 'Ġn', 'asa', 'Ġn', 'sf', 'Ġsubmitted', 'Ġfe', 'b', 'ruary', 'Ġwarning', 'Ġpotential', 'Ġimpact', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġincreased', 'Ġcollision', 'Ġrisk', 'Ġimpact', 'Ġscience', 'Ġmissions', 'Ġrocket', 'Ġlaunches', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġradio', 'Ġfrequencies', 'Ġspace', 'x', 'Ġsatellites', 'Ġmaneuver', 'Ġprobability', 'Ġcollision', 'Ġgreater', 'âĪĴ', '000', 'Ġchance', 'Ġcollision', 'Ġopposed', 'Ġindustry', 'Ġstandard', 'âĪĴ', '000', 'Ġchance', 'Ġcollision', ').[', 'Ġspace', 'x', 'Ġbudget', 'ed', 'Ġsufficient', 'Ġpropell', 'ant', 'Ġaccommodate', 'Ġapproximately', '000', 'Ġprop', 'ulsive', 'Ġmaneuvers', 'Ġlife', 'Ġsatellite', 'Ġincluding', 'Ġbudget', 'Ġapproximately', 'Ġcollision', 'Ġavoidance', 'Ġmaneuvers', 'Ġper', 'Ġsatellite', 'Ġtime', 'Ġperiod', 'Ġmay', 'Ġaverage', 'Ġstar', 'link', 'Ġsatellite', 'Ġconducted', 'Ġfewer', 'Ġthree', 'Ġcollision', 'avoid', 'ance', 'Ġmaneuvers', 'Ġpreceding', 'Ġmonths', 'Ġmaneuvers', 'Ġperformed', 'Ġavoid', 'Ġk', 'os', 'mos', '08', 'Ġdebris', 'Ġaddition', 'ew', 'eb', 'Ġconstellation', 'Ġannounced', 'Ġnearly', 'Ġconcurrently', 'Ġspace', 'x', 'Ġconstellation', 'Ġproposal', 'amsung', 'Ġoutlined', 'atellite', 'Ġconstellation', 'Ġorbiting', 'Ġmi', 'Ġcould', 'Ġprovide', 'Ġz', 'ett', 'abyte', 'Ġper', 'Ġmonth', 'Ġcapacity', 'Ġworldwide', 'Ġequivalent', 'Ġgig', 'abytes', 'Ġper', 'Ġmonth', 'Ġbillion', 'Ġusers', 'Ġinternet', 'Ġdata', 'Ġpublic', 'Ġinformation', 'Ġreleased', 'amsung', 'Ġconstellation', 'Ġtel', 'es', 'Ġannounced', 'Ġsmaller', 'Ġsatellite', 'Ġconstellation', 'Ġplans', 'Ġdeliver', 'Ġinitial', 'Ġservice', 'azon', 'Ġannounced', 'Ġlarge', 'Ġbroadband', 'Ġinternet', 'Ġsatellite', 'Ġconstellation', 'Ġapr', 'il', 'Ġplanning', 'Ġlaunch', 'Ġsatellites', 'Ġnext', 'Ġdecade', 'Ġcompany', 'Ġcalls', 'project', 'Ġk', 'ui', 'per', '",', 'Ġsatellite', 'Ġconstellation', 'Ġwork', 'Ġconcert', 'azon', "'s", 'Ġpreviously', 'Ġannounced', 'Ġlarge', 'Ġnetwork', 'Ġtwelve', 'Ġsatellite', 'Ġground', 'Ġstation', 'Ġfacilities', 'Ġground', 'Ġstation', 'Ġunit', '")', 'Ġannounced', 'mber', 'Ġfe', 'b', 'ruary']</t>
+          <t>['Ġoriginally', 'Ġplanned', 'Ġauthorized', 'Ġrequest', 'Ġsubject', 'Ġapproval', 'Ġphase', 'Ġgroup', 'Ġdesignation', 'Ġorbital', 'Ġshells', 'Ġorbital', 'Ġplanes', 'Ġcommitted', 'Ġcompletion', 'Ġdate', 'Ġdeployed', 'Ġsatellites', 'Ġaug', 'ust', 'Ġaltitude', 'Ġplanned', 'Ġsatellites', 'Ġincl', 'Ġnation', 'Ġcount', 'Ġsatellites', 'Ġper', 'Ġhalf', 'Ġfull', 'Ġactive', 'Ġdecaying', 'Ġde', 'orb', 'ited', 'Ġgroup', 'Ġmi', 'b', 'Â°', 'Ġde', 'cember', 'Ġde', 'cember', 'Ġgroup', 'Ġmi', 'b', 'Â°', 'Ġmi', 'b', 'Â°', 'Ġspace', 'x', 'Ġabandoned', 'Ġcon', 'ï', '¬', 'ģ', 'g', 'uration', 'Ġproposed', 'Ġamendment', 'Ġb', 'Ġlimited', 'Ġphase', 'Ġsatellites', 'Ġacross', 'Ġshells', 'Ġunknown', 'Ġstarship', 'Ġable', 'Ġlaunch', 'Ġsecond', 'Ġgeneration', 'Ġsatellites', 'Ġspace', 'x', 'Ġmodified', 'Ġoriginal', 'Ġblueprint', 'Ġsmaller', 'Ġcompact', 'Ġone', 'Ġnamed', 'Ġmini', '".', 'Ġadjustment', 'Ġallowed', 'Ġfal', 'con', 'Ġtransport', 'Ġsatellites', 'Ġthough', 'Ġmany', 'Ġorbit', 'Ġfirst', 'Ġset', 'Ġsatellites', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġcommitted', 'Ġreducing', 'Ġdebris', 'Ġkeeping', 'Ġstar', 'link', 'Ġtension', 'Ġrods', 'Ġhold', 'Ġmini', 'atell', 'ites', 'Ġtogether', 'Ġattached', 'Ġfal', 'con', 'Ġsecond', 'Ġstage', 'Ġtension', 'Ġrods', 'Ġdiscarded', 'Ġorbit', 'Ġlaunching', 'Ġearlier', 'Ġversions', 'Ġstar', 'link', 'Ġsatellites', 'Ġobservations', 'Ġconfirm', 'Ġmini', 'atell', 'ites', 'Ġhost', 'Ġtwo', 'Ġsolar', 'Ġpanels', 'Ġlike', 'Ġstarship', 'Ġsatellites', 'Ġplanned', 'Ġlarge', 'Ġnumber', 'Ġsatellites', 'Ġmet', 'Ġcriticism', 'Ġastronomical', 'Ġcommunity', 'Ġconcerns', 'Ġlight', 'Ġastronomers', 'Ġclaim', 'Ġnumber', 'Ġvisible', 'Ġsatellites', 'number', 'Ġvisible', 'Ġstars', 'Ġbrightness', 'Ġoptical', 'Ġradio', 'Ġwavelengths', 'Ġseverely', 'Ġimpact', 'Ġscientific', 'Ġobservations', 'Ġastronomers', 'Ġschedule', 'Ġobservations', 'Ġavoid', 'Ġpointing', 'Ġsatellites', 'Ġcurrently', 'Ġorbit', 'getting', 'Ġdifficult', 'Ġsatellites', 'Ġcome', 'Ġonline', 'Ġinternational', 'Ġastronomical', 'Ġunion', 'Ġnational', 'Ġradio', 'Ġastronomy', 'Ġobserv', 'atory', 'Ġsquare', 'Ġkilomet', 'Ġarray', 'Ġorganization', 'Ġreleased', 'Ġofficial', 'Ġstatements', 'Ġexpressing', 'Ġconcern', 'mber', 'Ġfour', 'meter', "')", 'Ġbl', 'anco', 'Ġtelescope', 'Ġcer', 'ro', 'l', 'olo', 'Ġinter', 'amer', 'ican', 'Ġobserv', 'atory', 'ct', 'io', 'Ġrecorded', 'Ġstrong', 'Ġsignal', 'Ġloss', 'Ġappearance']</t>
         </is>
       </c>
       <c r="C423" t="n">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="B424" t="inlineStr">
         <is>
-          <t>['Ġfinancial', 'Ġanalysts', 'Ġquestioned', 'Ġestablished', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġcommunications', 'Ġsatellite', 'Ġfleet', 'Ġoperators', 'Ġintended', 'Ġrespond', 'Ġcompetitive', 'Ġthreat', 'Ġspace', 'x', 'ew', 'eb', 'Ġle', 'Ġcommunication', 'Ġsatellites', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġindicated', 'Ġdevelopment', 'Ġcontinues', 'Ġbusiness', 'Ġcase', 'Ġlong', 'term', 'Ġrollout', 'Ġoperational', 'Ġsatellite', 'Ġnetwork', 'Ġstill', 'Ġearly', 'Ġphase', 'Ġoct', 'ober', 'Ġexpectation', 'Ġlarge', 'Ġincreases', 'Ġsatellite', 'Ġnetwork', 'Ġcapacity', 'Ġemerging', 'Ġlower', 'alt', 'itude', 'Ġbroadband', 'Ġconst', 'ell', 'ations', 'Ġcaused', 'Ġmarket', 'Ġplayers', 'Ġcancel', 'Ġplanned', 'Ġinvestments', 'Ġnew', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġbroadband', 'Ġcommunications', 'Ġsatellites', 'Ġspace', 'x', 'Ġchallenged', 'Ġregarding', 'Ġstar', 'link', 'Ġfe', 'b', 'ruary', 'Ġnational', 'Ġrural', 'Ġelectric', 'Ġcooperative', 'Ġassociation', 'n', 'ca', 'Ġpolitical', 'Ġinterest', 'Ġgroup', 'Ġrepresenting', 'Ġtraditional', 'Ġrural', 'Ġinternet', 'Ġservice', 'Ġproviders', 'Ġurged', 'Ġu', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'actively', 'Ġaggressively', 'Ġthought', 'fully', 'Ġvet', 'Ġsubsidy', 'Ġapplications', 'Ġspace', 'x', 'Ġbroadband', 'Ġproviders', 'Ġtime', 'Ġspace', 'x', 'Ġprovision', 'ally', 'Ġmillion', 'Ġcommitment', 'Ġprovide', 'Ġservice', 'Ġapproximately', '000', 'Ġlocations', 'Ġstates', 'Ġpart', 'Ġrural', 'Ġdigital', 'Ġopportunity', 'Ġfund', 'rd', ').[', 'Ġn', 'ca', 'Ġcriticisms', 'Ġincluded', 'Ġfunding', 'Ġallocation', 'Ġstar', 'link', 'Ġwould', 'Ġinclude', 'Ġservice', 'Ġlocations', 'âĢĶ', 'Ġhar', 'lem', 'Ġterminals', 'Ġnew', 'ark', 'Ġliberty', 'Ġinternational', 'Ġairport', 'iami', 'Ġinternational', 'Ġairport', 'âĢĶ', 'Ġrural', 'Ġspace', 'x', 'Ġplanning', 'Ġbuild', 'Ġinfrastructure', 'Ġserve', 'Ġcustomers', 'Ġrequest', 'Ġservice', 'Ġwithout', 'Ġsubsidy', 'Ġadditionally', 'Ġmat', 'hes', 'Ġchief', 'Ġexecutive', 'Ġofficer', 'Ġn', 'ca', 'Ġvoiced', 'Ġconcern', 'Ġtechnologies', 'Ġyet', 'Ġproven', 'Ġmeet', 'Ġhigh', 'Ġspeeds', 'Ġrequired', 'Ġaward', 'Ġcategory', 'Ġstar', 'link', 'Ġspecifically', 'Ġcriticized', 'Ġstill', 'Ġbeta', 'Ġtesting', 'Ġun', 'proven', 'Ġtechnology', 'Ġstar', 'link', 'Ġdeployed', 'Ġworldwide', 'Ġencountered', 'Ġtrademark', 'Ġconflicts', 'Ġcountries', 'x', 'ico', 'ew', 'eb', 'Ġsatellite', 'Ġconstellation', 'Ġsatellite', 'Ġconstellation', 'Ġproject', 'Ġbegan', 'Ġoperational', 'Ġdeployment', 'Ġsatellites', 'Ġcompetition', 'Ġmarket', 'Ġeffects', 'Ġsimilar', 'Ġcompetitive', 'Ġsystems', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġch', 'ina', 'Ġnational', 'Ġsatellite', 'Ġinternet', 'Ġproject', 'Ġplanned', 'Ġsatellite', 'Ġinternet', 'Ġoffering', 'Ġch', 'inese', 'Ġmarket', 'Ġk', 'ui', 'per', 'Ġsystems', 'Ġplanned', 'Ġle', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'azon']</t>
+          <t>['Ġwhite', 'Ġlines', 'Ġdec', 'Ġshot', 'right', 'Ġimage', 'Ġimage', 'Ġnoise', 'Ġcorrelated', 'Ġtransit', 'Ġstar', 'link', 'Ġsatellite', 'Ġtrain', 'Ġlaunched', 'Ġweek', 'Ġearlier', 'Ġsecond', 'Ġgeneration', 'Ġimpact', 'Ġastronomy', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ã¼', 'bing', 'en', 'Ġg', 'erman', 'Ġstar', 'link', 'Ġseen', 'Ġhub', 'ble', 'Ġspace', 'Ġtelescope', 'Ġtim', 'el', 'apse', 'Ġrecently', 'Ġdeployed', 'Ġspace', 'x', 'Ġrepresentatives', 'Ġmus', 'k', 'Ġclaimed', 'Ġsatellites', 'Ġminimal', 'Ġimpact', 'Ġeasily', 'Ġmit', 'igated', 'Ġpixel', 'Ġmask', 'ing', 'Ġimage', 'Ġstacking', 'Ġhowever', 'Ġprofessional', 'Ġastronomers', 'Ġdisputed', 'Ġclaims', 'Ġbased', 'Ġinitial', 'Ġobservation', 'Ġstar', 'link', 'Ġsatellites', 'Ġfirst', 'Ġlaunch', 'Ġshortly', 'Ġdeployment', 'Ġlaunch', 'Ġlater', 'Ġstatements', 'Ġtwitter', 'Ġmus', 'k', 'Ġstated', 'Ġspace', 'x', 'Ġwork', 'Ġreducing', 'Ġal', 'bed', 'Ġsatellites', 'Ġprovide', 'demand', 'Ġorientation', 'Ġadjustments', 'Ġastronomical', 'Ġexperiments', 'Ġone', 'Ġstar', 'link', 'Ġsatellite', 'st', 'arl', 'ink', 'arks', 'Ġlaunched', 'Ġexperimental', 'Ġcoating', 'Ġreduce', 'Ġal', 'bed', 'Ġreduction', 'Ġg', 'band', 'Ġmagnitude', 'Ġmagnitude', '%).', 'Ġdespite', 'Ġmeasures', 'Ġastronomers', 'Ġfound', 'Ġsatellites', 'Ġstill', 'Ġbright', 'Ġthus', 'Ġmaking', 'arks', 'Ġessentially', 'dead', 'Ġend', '".[', 'Ġapr', 'il', 'Ġspace', 'x', 'Ġwrote', 'Ġfiling', 'Ġwould', 'Ġtest', 'Ġnew', 'Ġmethods', 'Ġmitigating', 'Ġlight', 'Ġpollution', 'Ġalso', 'Ġprovide', 'Ġaccess', 'Ġsatellite', 'Ġtracking', 'Ġdata', 'Ġastronomers', 'better', 'Ġcoordinate', 'Ġobservations', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġannounced', 'Ġcompany', 'Ġwould', 'Ġintroduce', 'Ġnew', 'Ġsun', 'sh', 'ade', 'Ġdesigned', 'Ġreduce', 'Ġbrightness', 'Ġstar', 'link', 'Ġsatellites', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġsatellites', 'Ġsun', 'sh', 'ade', 'Ġoct', 'ober', 'Ġanalysis', 'Ġfound', 'Ġmarginally', 'Ġf', 'ter', 'arks', 'Ġjan', 'uary', 'Ġstudy', 'Ġpinned', 'Ġbrightness', 'Ġoriginal', 'Ġdesign', 'Ġaccording', 'Ġmay', 'Ġstudy', 'Ġlarge', 'Ġnumber', 'Ġfast', 'moving', 'Ġtransmitting', 'Ġstations', 'e', 'Ġsatellites', 'Ġcause', 'Ġinterference', 'Ġnew', 'Ġanalysis', 'Ġmethods', 'Ġcould', 'Ġmitigate', 'Ġeffects', 'Ġdata', 'Ġloss', 'Ġinevitable', 'Ġincreasing', 'Ġtime', 'Ġneeded', 'Ġstudy', 'Ġlimiting', 'Ġoverall', 'Ġamount', 'Ġscience', 'Ġdone', '".[', 'Ġfe', 'b', 'ruary', 'Ġinternational', 'Ġastronomical', 'Ġunion', 'Ġestablished', 'Ġcenter', 'Ġhelp', 'Ġastronomers']</t>
         </is>
       </c>
       <c r="C424" t="n">
@@ -5950,7 +5950,7 @@
       </c>
       <c r="B425" t="inlineStr">
         <is>
-          <t>['Ġsubsidiary', 'Ġhug', 'hes', 'Ġnetwork', 'Ġsystems', 'Ġcurrent', 'Ġbroadband', 'Ġsatellite', 'Ġprovider', 'Ġproviding', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġcellular', 'Ġback', 'haul', 'Ġairborne', 'Ġantennas', 'Ġv', 'ias', 'Ġinc', 'Ġcurrent', 'Ġbroadband', 'Ġsatellite', 'Ġprovider', 'Ġproviding', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġground', 'Ġmobile', 'Ġairborne', 'Ġantennas', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġconstellation', 'Ġprovides', 'Ġaccess', 'Ġmobile', 'Ġphone', 'Ġoperators', 'Ġinternet', 'Ġservice', 'Ġproviders', 'Ġcovers', 'Ġequ', 'atorial', 'Ġregion', 'Ġast', 'Ġspac', 'em', 'obile', 'Ġsatellite', 'Ġconstellation', 'Ġworking', 'Ġlarge', 'Ġmobile', 'Ġnetwork', 'Ġoperators', 'Ġv', 'od', 'af', 'one', 'Ġorange', 'Ġr', 'ak', 'uten', 'Ġtel', 'est', 'ra', 'Ġtele', 'f', 'Ã³n', 'ica', 'Ġetc', 'Ġobjective', 'Ġprovide', 'Ġbroadband', 'Ġinternet', 'Ġcoverage', 'Ġexisting', 'Ġun', 'mod', 'ï', '¬', 'ģ', 'ed', 'Ġmobile', 'Ġphones', 'Ġorb', 'comm', 'Ġoperational', 'Ġconstellation', 'Ġused', 'Ġprovide', 'Ġglobal', 'Ġasset', 'Ġmonitoring', 'Ġmessaging', 'Ġservices', 'Ġconstellation', 'Ġle', 'Ġcommunications', 'Ġsatellites', 'Ġorbiting', 'Ġglobal', 'star', 'Ġoperational', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġsatellite', 'Ġconstellation', 'Ġsatellite', 'Ġphone', 'Ġlow', 'speed', 'Ġdata', 'Ġcommunications', 'Ġcovering', 'Ġworld', "'s", 'Ġland', 'mass', 'Ġir', 'idium', 'Ġoperational', 'Ġconstellation', 'Ġcross', 'linked', 'Ġsatellites', 'Ġpolar', 'Ġorbit', 'Ġused', 'Ġprovide', 'Ġsatellite', 'Ġphone', 'Ġlow', 'speed', 'Ġdata', 'Ġservices', 'Ġentire', 'Ġsurface', 'Ġearth', 'Ġlyn', 'k', 'Ġglobal', 'Ġsatellite', 'Ġconstellation', 'Ġobjective', 'Ġcoverage', 'Ġtraditional', 'Ġlow', 'cost', 'Ġmobile', 'Ġdevices', 'Ġtel', 'edes', 'ic', 'Ġformer', 'Ġventure', 'Ġaccomplish', 'Ġbroadband', 'Ġsatellite', 'Ġinternet', 'Ġservices', 'Ġproject', 'Ġl', 'oon', 'Ġformer', 'Ġconcept', 'Ġprovide', 'Ġinternet', 'Ġaccess', 'Ġvia', 'Ġballoons', 'Ġstrat', 'osphere', 'st', 'arl', 'ink', 'Ġgroup', 'Ġfal', 'con', 'Ġblock', 'Ġeveryday', 'Ġastronaut', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġmay', 'space', 'x', 'Ġce', 'Ġel', 'Ġmus', 'k', 'Ġreveals', 'Ġnext', 'generation', 'Ġstar', 'link', 'Ġsatellite', 'Ġdetails', 'w', 'es', 'lar', 'ati', 'Ġretrieved', 'Ġj', 'une', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġlaunch', 'Ġtwo', 'Ġspace', 'Ġinternet', 'Ġsatellites', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġnearly', '000', 'Ġaz', 'watch', 'live', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġk', 'ol', 'od', 'ny', 'Ġl', 'ora', 'Ġaug', 'ust', 'space', 'x', 'mobile', 'Ġteam', 'Ġuse', 'Ġstar', 'link', 'Ġsatellites', 'end', 'Ġmobile', 'Ġdead', 'Ġzones', 'Ġretrieved', 'Ġaug', 'ust']</t>
+          <t>['Ġdeal', 'Ġadverse', 'Ġeffects', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'Ġstar', 'link', 'Ġwork', 'Ġinclude', 'Ġdevelopment', 'Ġsoftware', 'Ġtools', 'Ġastronomers', 'Ġadvancement', 'Ġnational', 'Ġinternational', 'Ġpolicies', 'Ġcommunity', 'Ġoutreach', 'Ġwork', 'Ġindustry', 'Ġrelevant', 'Ġtechnologies', 'Ġj', 'une', 'Ġreleased', 'Ġwebsite', 'Ġastronomers', 'Ġdeal', 'Ġadverse', 'Ġeffects', 'Ġvia', 'Ġsatellite', 'Ġtracking', 'Ġenable', 'Ġastronomers', 'Ġable', 'Ġtrack', 'Ġsatellites', 'Ġable', 'Ġavoid', 'Ġtime', 'Ġminimal', 'Ġimpact', 'Ġcurrent', 'Ġwork', 'Ġfirst', 'Ġbatch', 'Ġgeneration', 'Ġspacecraft', 'Ġlaunched', 'Ġfe', 'b', 'ruary', 'Ġsatellites', 'Ġreferred', 'mini', 'Ġsmaller', 'Ġfull', 'sized', 'Ġgen', 'Ġspacecraft', 'Ġcome', 'Ġlater', 'Ġspace', 'x', 'Ġuses', 'Ġbrightness', 'Ġmitigation', 'Ġgen', 'Ġincludes', 'Ġmirror', 'like', 'Ġsurface', 'Ġreflects', 'Ġsunlight', 'Ġback', 'Ġspace', 'Ġorient', 'Ġsolar', 'Ġpanels', 'Ġobservers', 'Ġground', 'Ġsee', 'Ġdark', 'Ġsides', 'Ġmin', 'Ġf', 'ter', 'Ġgen', 'Ġspacecraft', 'Ġdespite', 'Ġfour', 'Ġtimes', 'Ġlarge', 'Ġaccording', 'Ġobservational', 'Ġstudy', 'Ġpublished', 'Ġj', 'une', 'Ġbright', 'Ġgen', 'Ġplaced', 'Ġfinal', 'Ġorbit', 'Ġmin', 'Ġappear', 'Ġtimes', 'Ġbrighter', 'Ġreach', 'Ġtarget', 'Ġorbit', 'Ġlarge', 'Ġnumber', 'Ġsatellites', 'Ġemployed', 'Ġstar', 'link', 'Ġmay', 'Ġcreate', 'Ġlong', 'term', 'Ġdanger', 'Ġspace', 'Ġdebris', 'Ġresulting', 'Ġplacing', 'Ġthousands', 'Ġsatellites', 'Ġorbit', 'Ġrisk', 'Ġcausing', 'Ġsatellite', 'Ġcollision', 'Ġpotentially', 'Ġtriggering', 'Ġphenomenon', 'Ġknown', 'Ġk', 'essler', 'Ġsyndrome', 'Ġspace', 'x', 'Ġsaid', 'Ġsatellites', 'Ġlaunched', 'Ġlower', 'Ġaltitude', 'Ġfailed', 'Ġsatellites', 'Ġexpected', 'Ġde', 'orbit', 'Ġwithin', 'Ġfive', 'Ġyears', 'Ġwithout', 'Ġearly', 'Ġprogram', 'Ġnear', 'miss', 'Ġoccurred', 'Ġspace', 'x', 'Ġmove', 'Ġsatellite', '000', 'Ġchance', 'Ġcoll', 'iding', 'Ġeuro', 'pe', 'Ġone', 'Ġten', 'Ġtimes', 'Ġhigher', 'Ġes', "'s", 'Ġthreshold', 'Ġavoidance', 'Ġmaneuvers', 'Ġspace', 'x', 'Ġsubsequently', 'Ġfixed', 'Ġissue', 'Ġp', 'aging', 'Ġsystem', 'Ġdisrupted', 'Ġemails', 'Ġes', 'Ġspace', 'x', 'Ġes', 'Ġsaid', 'Ġplans', 'Ġinvest', 'Ġtechnologies', 'Ġautomate', 'Ġsatellite', 'Ġcollision', 'Ġavoidance', 'Ġch', 'inese', 'Ġauthorities', 'Ġlodged', 'Ġcomplaint', 'Ġunited', 'Ġnations', 'Ġsaying', 'Ġspace', 'Ġstation', 'Ġperformed', 'Ġev', 'asive', 'Ġmaneuvers', 'Ġyear', 'Ġavoid', 'Ġincreased', 'Ġrisk', 'Ġsatellite', 'Ġcollision', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstar', 'link', 'Ġsatellites', 'Ġdocument', 'Ġch', 'inese', 'Ġdelegates', 'Ġsaid', 'Ġcontinuously', 'Ġmaneuver', 'ing']</t>
         </is>
       </c>
       <c r="C425" t="n">
@@ -5963,7 +5963,7 @@
       </c>
       <c r="B426" t="inlineStr">
         <is>
-          <t>['cd', 'owell', 'Ġj', 'athan', 'Ġmay', 'st', 'arl', 'ink', 'Ġlaunch', 'Ġstatistics', 'Ġplanet', 'Ġretrieved', 'Ġmay', 'Ġspace', 'x', 'space', 'x', 'Ġde', 'cember', 'st', 'arl', 'ink', '000', '000', 'Ġactive', 'Ġsubscribers', 'tw', 'weet', 'Ġretrieved', 'Ġmarch', 'Ġvia', 'Ġtwitter', 'Ġstar', 'link', 'thank', 'Ġcustomers', 'Ġaround', 'Ġworld', '!"', 'Ġ07', 'Ġtwitter', 'Ġretrieved', 'Ġmay', 'Ġb', 'aylor', 'ichael', 'Ġmay', 'Ġblock', 'Ġspace', 'x', 'Ġincrease', 'Ġlaunch', 'Ġcad', 'ence', 'Ġlower', 'Ġprices', 'ww', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġsystem', 'Ġdesigned', 'Ġimprove', 'Ġglobal', 'Ġinternet', 'Ġaccess', 'Ġutilizing', 'Ġthousands', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġstated', 'Ġted', 'Ġtalk', 'Ġlast', 'Ġmonth', 'Ġexpects', 'Ġconstellation', 'Ġcost', 'Ġleast', 'Ġus', 'Ġbillion', 'Ġtherefore', 'Ġreducing', 'Ġlaunch', 'Ġcosts', 'Ġvital', '."', 'Ġwink', 'ler', 'Ġro', 'lf', 'e', 'Ġpas', 'z', 'tor', 'Ġjan', 'uary', 'exclusive', 'Ġpeek', 'Ġspace', 'x', 'Ġdata', 'Ġshows', 'Ġloss', 'Ġheavy', 'Ġexpectations', 'Ġnascent', 'Ġinternet', 'Ġservice', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġether', 'ington', 'arrell', 'space', 'x', 'Ġhopes', 'Ġsatellite', 'Ġinternet', 'Ġbusiness', 'Ġpad', 'Ġthin', 'Ġrocket', 'Ġlaunch', 'Ġmargins', 'tech', 'cr', 'Ġtech', 'cr', 'unch', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġsatellites', 'Ġharm', 'Ġastronomy', "'s", 'Ġknow', 'Ġnational', 'Ġgeographic', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'j', 'ason', 'Ġreport', 'Ġimpacts', 'Ġlarge', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'Ġnational', 'Ġscience', 'Ġfoundation', 'Ġretrieved', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġapr', 'il', 'ast', 'ron', 'omy', 'Ġdiscussion', 'Ġnational', 'Ġacademy', 'Ġsciences', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'st', 'arl', 'ink', 'Ġblock', 'Ġspace', 'sky', 'rocket', 'de', 'Ġarchived', 'http', 'Ġoriginal']</t>
+          <t>['Ġstar', 'link', 'Ġsatellites', 'Ġposed', 'Ġrisk', 'Ġcollision', 'Ġtwo', 'Ġclose', 'Ġencounters', 'Ġsatellites', 'Ġj', 'uly', 'Ġoct', 'ober', 'Ġconstituted', 'Ġdangers', 'Ġlife', 'Ġhealth', 'Ġastronauts', 'Ġaboard', 'Ġch', 'inese', 'iang', 'ong', 'Ġspace', 'Ġstation', 'Ġreported', 'Ġissues', 'Ġplus', 'Ġcurrent', 'Ġplans', 'Ġextension', 'Ġconstellation', 'Ġmotivated', 'Ġformal', 'Ġletter', 'Ġnational', 'Ġtelecommunications', 'Ġinformation', 'Ġadministration', 'nt', 'ia', 'Ġbehalf', 'Ġn', 'asa', 'Ġn', 'sf', 'Ġsubmitted', 'Ġfe', 'b', 'ruary', 'Ġwarning', 'Ġpotential', 'Ġimpact', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġincreased', 'Ġcollision', 'Ġrisk', 'Ġimpact', 'Ġscience', 'Ġmissions', 'Ġrocket', 'Ġlaunches', 'Ġinternational', 'Ġspace', 'Ġstation', 'Ġradio', 'Ġfrequencies', 'Ġspace', 'x', 'Ġsatellites', 'Ġmaneuver', 'Ġprobability', 'Ġcollision', 'Ġgreater', 'âĪĴ', '000', 'Ġchance', 'Ġcollision', 'Ġopposed', 'Ġindustry', 'Ġstandard', 'âĪĴ', '000', 'Ġchance', 'Ġcollision', ').[', 'Ġspace', 'x', 'Ġbudget', 'ed', 'Ġsufficient', 'Ġpropell', 'ant', 'Ġaccommodate', 'Ġapproximately', '000', 'Ġprop', 'ulsive', 'Ġmaneuvers', 'Ġlife', 'Ġsatellite', 'Ġincluding', 'Ġbudget', 'Ġapproximately', 'Ġcollision', 'Ġavoidance', 'Ġmaneuvers', 'Ġper', 'Ġsatellite', 'Ġtime', 'Ġperiod', 'Ġmay', 'Ġaverage', 'Ġstar', 'link', 'Ġsatellite', 'Ġconducted', 'Ġfewer', 'Ġthree', 'Ġcollision', 'avoid', 'ance', 'Ġmaneuvers', 'Ġpreceding', 'Ġmonths', 'Ġmaneuvers', 'Ġperformed', 'Ġavoid', 'Ġk', 'os', 'mos', '08', 'Ġdebris', 'Ġaddition', 'ew', 'eb', 'Ġconstellation', 'Ġannounced', 'Ġnearly', 'Ġconcurrently', 'Ġspace', 'x', 'Ġconstellation', 'Ġproposal', 'amsung', 'Ġoutlined', 'atellite', 'Ġconstellation', 'Ġorbiting', 'Ġmi', 'Ġcould', 'Ġprovide', 'Ġz', 'ett', 'abyte', 'Ġper', 'Ġmonth', 'Ġcapacity', 'Ġworldwide', 'Ġequivalent', 'Ġgig', 'abytes', 'Ġper', 'Ġmonth', 'Ġbillion', 'Ġusers', 'Ġinternet', 'Ġdata', 'Ġpublic', 'Ġinformation', 'Ġreleased', 'amsung', 'Ġconstellation', 'Ġtel', 'es', 'Ġannounced', 'Ġsmaller', 'Ġsatellite', 'Ġconstellation', 'Ġplans', 'Ġdeliver', 'Ġinitial', 'Ġservice', 'azon', 'Ġannounced', 'Ġlarge', 'Ġbroadband', 'Ġinternet', 'Ġsatellite', 'Ġconstellation', 'Ġapr', 'il', 'Ġplanning', 'Ġlaunch', 'Ġsatellites', 'Ġnext', 'Ġdecade', 'Ġcompany', 'Ġcalls', 'project', 'Ġk', 'ui', 'per', '",', 'Ġsatellite', 'Ġconstellation', 'Ġwork', 'Ġconcert', 'azon', "'s", 'Ġpreviously', 'Ġannounced', 'Ġlarge', 'Ġnetwork', 'Ġtwelve', 'Ġsatellite', 'Ġground', 'Ġstation', 'Ġfacilities', 'Ġground', 'Ġstation', 'Ġunit', '")', 'Ġannounced', 'mber', 'Ġfe', 'b', 'ruary']</t>
         </is>
       </c>
       <c r="C426" t="n">
@@ -5976,7 +5976,7 @@
       </c>
       <c r="B427" t="inlineStr">
         <is>
-          <t>['mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġtel', 'edes', 'ic', 'Ġplays', 'Ġlast', 'Ġcard', 'Ġleaves', 'Ġgame', '."', 'Ġoct', 'ober', 'Ġway', 'back', 'Ġmachine', 'Ġspace', 'Ġnews', 'Ġj', 'uly', 'Ġg', 'ild', 'er', 'Ġge', 'orge', 'Ġoct', 'ober', 'light', 'Ġspeed', 'Ġtrap', 'Ġahead', 'Ġl', 'Ġforb', 'es', 'space', 'x', 'Ġwash', 'Ġops', 'Ġexecutive', 'Ġlaunching', 'Ġconsulting', 'Ġfirm', 'Ġspac', 'en', 'ews', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġj', 'une', 'space', 'Ġtakes', 'Ġpercent', 'Ġstake', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'sp', 'Ġspace', 'Ġnews', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtransfer', 'Ġsensor', 'Ġdata', 'Ġspace', 'Ġusing', 'b', 'undle', 'Ġprotocol', 'Ġarchived', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġpress', 'Ġrelease', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'Ġse', 'pt', 'ember', 'ead', 'Ġast', 'rium', 'Ġsigns', 'Ġagreement', 'Ġacquire', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'Ġlimited', 'Ġuniversity', 'Ġsur', 'rey', '."', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġuniversity', 'Ġsur', 'rey', 'Ġapr', 'il', 'Ġwink', 'ler', 'Ġro', 'lf', 'e', 'mber', 'el', 'Ġmus', 'k', "'s", 'Ġnext', 'Ġmission', 'Ġinternet', 'Ġsatellites', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġf', 'ern', 'hol', 'z', 'Ġtim', 'Ġj', 'une', 'inside', 'Ġrace', 'Ġcreate', 'Ġnext', 'Ġgeneration', 'Ġsatellite', 'Ġinternet', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'application', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'Ġspace', 'Ġexploration', 'Ġholdings', 'c', 'Ġtechnical', 'Ġattachment', 'f', 'cc', 'mber', 'Ġp', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġboy', 'le', 'Ġal', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġseeks', 'Ġtrademark', 'Ġname', 'st', 'arl', 'ink', 'Ġsatellite', 'Ġbroadband', 'Ġnetwork', 'Ġgeek', 'wire', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġind', 'ian', 'apolis', 'Ġauthor', 'Ġjohn', 'Ġgreen', 'Ġinspired', 'Ġone', 'Ġel']</t>
+          <t>['Ġfinancial', 'Ġanalysts', 'Ġquestioned', 'Ġestablished', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġcommunications', 'Ġsatellite', 'Ġfleet', 'Ġoperators', 'Ġintended', 'Ġrespond', 'Ġcompetitive', 'Ġthreat', 'Ġspace', 'x', 'ew', 'eb', 'Ġle', 'Ġcommunication', 'Ġsatellites', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġindicated', 'Ġdevelopment', 'Ġcontinues', 'Ġbusiness', 'Ġcase', 'Ġlong', 'term', 'Ġrollout', 'Ġoperational', 'Ġsatellite', 'Ġnetwork', 'Ġstill', 'Ġearly', 'Ġphase', 'Ġoct', 'ober', 'Ġexpectation', 'Ġlarge', 'Ġincreases', 'Ġsatellite', 'Ġnetwork', 'Ġcapacity', 'Ġemerging', 'Ġlower', 'alt', 'itude', 'Ġbroadband', 'Ġconst', 'ell', 'ations', 'Ġcaused', 'Ġmarket', 'Ġplayers', 'Ġcancel', 'Ġplanned', 'Ġinvestments', 'Ġnew', 'Ġge', 'os', 'ynchronous', 'Ġorbit', 'Ġbroadband', 'Ġcommunications', 'Ġsatellites', 'Ġspace', 'x', 'Ġchallenged', 'Ġregarding', 'Ġstar', 'link', 'Ġfe', 'b', 'ruary', 'Ġnational', 'Ġrural', 'Ġelectric', 'Ġcooperative', 'Ġassociation', 'n', 'ca', 'Ġpolitical', 'Ġinterest', 'Ġgroup', 'Ġrepresenting', 'Ġtraditional', 'Ġrural', 'Ġinternet', 'Ġservice', 'Ġproviders', 'Ġurged', 'Ġu', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'actively', 'Ġaggressively', 'Ġthought', 'fully', 'Ġvet', 'Ġsubsidy', 'Ġapplications', 'Ġspace', 'x', 'Ġbroadband', 'Ġproviders', 'Ġtime', 'Ġspace', 'x', 'Ġprovision', 'ally', 'Ġmillion', 'Ġcommitment', 'Ġprovide', 'Ġservice', 'Ġapproximately', '000', 'Ġlocations', 'Ġstates', 'Ġpart', 'Ġrural', 'Ġdigital', 'Ġopportunity', 'Ġfund', 'rd', ').[', 'Ġn', 'ca', 'Ġcriticisms', 'Ġincluded', 'Ġfunding', 'Ġallocation', 'Ġstar', 'link', 'Ġwould', 'Ġinclude', 'Ġservice', 'Ġlocations', 'âĢĶ', 'Ġhar', 'lem', 'Ġterminals', 'Ġnew', 'ark', 'Ġliberty', 'Ġinternational', 'Ġairport', 'iami', 'Ġinternational', 'Ġairport', 'âĢĶ', 'Ġrural', 'Ġspace', 'x', 'Ġplanning', 'Ġbuild', 'Ġinfrastructure', 'Ġserve', 'Ġcustomers', 'Ġrequest', 'Ġservice', 'Ġwithout', 'Ġsubsidy', 'Ġadditionally', 'Ġmat', 'hes', 'Ġchief', 'Ġexecutive', 'Ġofficer', 'Ġn', 'ca', 'Ġvoiced', 'Ġconcern', 'Ġtechnologies', 'Ġyet', 'Ġproven', 'Ġmeet', 'Ġhigh', 'Ġspeeds', 'Ġrequired', 'Ġaward', 'Ġcategory', 'Ġstar', 'link', 'Ġspecifically', 'Ġcriticized', 'Ġstill', 'Ġbeta', 'Ġtesting', 'Ġun', 'proven', 'Ġtechnology', 'Ġstar', 'link', 'Ġdeployed', 'Ġworldwide', 'Ġencountered', 'Ġtrademark', 'Ġconflicts', 'Ġcountries', 'x', 'ico', 'ew', 'eb', 'Ġsatellite', 'Ġconstellation', 'Ġsatellite', 'Ġconstellation', 'Ġproject', 'Ġbegan', 'Ġoperational', 'Ġdeployment', 'Ġsatellites', 'Ġcompetition', 'Ġmarket', 'Ġeffects', 'Ġsimilar', 'Ġcompetitive', 'Ġsystems', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġch', 'ina', 'Ġnational', 'Ġsatellite', 'Ġinternet', 'Ġproject', 'Ġplanned', 'Ġsatellite', 'Ġinternet', 'Ġoffering', 'Ġch', 'inese', 'Ġmarket', 'Ġk', 'ui', 'per', 'Ġsystems', 'Ġplanned', 'Ġle', 'Ġsatellite', 'Ġinternet', 'Ġconstellation', 'azon']</t>
         </is>
       </c>
       <c r="C427" t="n">
@@ -5989,7 +5989,7 @@
       </c>
       <c r="B428" t="inlineStr">
         <is>
-          <t>['Ġmus', 'k', "'s", 'Ġgrand', 'Ġideas', 'Ġind', 'ian', 'apolis', 'Ġstar', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġoct', 'ober', 'shot', 'well', 'Ġsays', 'Ġspace', 'x', 'h', 'oming', 'Ġcause', 'Ġfal', 'con', 'Ġpad', 'Ġexplosion', 'http', 'sp', 'Ġspac', 'en', 'ews', 'Ġarchived', 'http', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġoct', 'ober', 'types', 'Ġbroadband', 'Ġconnections', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgates', 'Ġdomin', 'ic', 'Ġjan', 'uary', 'el', 'Ġmus', 'k', 'outs', 'Ġlaunch', 'space', 'x', 'Ġse', 'attle', 'Ġse', 'attle', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġse', 'attle', 'Ġcliff', 'Ġjan', 'uary', 'Ġarchived', 'h', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'mus', 'k', 'Ġreiter', 'ates', 'Ġplans', 'Ġtesting', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'const', 'ruction', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġprototype', 'Ġspaceship', 'Ġprogress', "'re", 'Ġactually', 'Ġbuilding', 'Ġship', 'Ġright', '",', 'Ġsaid', 'Ġthink', "'ll", 'Ġprobably', 'Ġable', 'Ġshort', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġshort', 'Ġsort', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġprobably', 'Ġsometime', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġhalf', 'Ġnext', 'Ġyear', '."', 'space', 'x', 'Ġbuild', 'Ġstar', 'link', 'like', 'Ġconstellation', 'Ġaround', 'Ġmars', 'Ġpresident', 'Ġsays', 'Ġfut', 'ur', 'ism', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġboy', 'le', 'Ġal', 'Ġjan', 'uary', 'space', 'x', 'Ġadds', 'Ġbig', 'Ġnew', 'Ġlab', 'Ġsatellite', 'Ġdevelopment', 'Ġoperation', 'Ġse', 'attle', 'Ġarea', 'Ġgeek', 'wire', 'Ġarchived', 'Ġn', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'Ġboy', 'le', 'Ġal', 'Ġoct', 'ober', 'space', 'x', 'Ġreorgan', 'izes', 'Ġstar', 'link', 'Ġsatellite', 'Ġoperation']</t>
+          <t>['Ġsubsidiary', 'Ġhug', 'hes', 'Ġnetwork', 'Ġsystems', 'Ġcurrent', 'Ġbroadband', 'Ġsatellite', 'Ġprovider', 'Ġproviding', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġcellular', 'Ġback', 'haul', 'Ġairborne', 'Ġantennas', 'Ġv', 'ias', 'Ġinc', 'Ġcurrent', 'Ġbroadband', 'Ġsatellite', 'Ġprovider', 'Ġproviding', 'Ġï', '¬', 'ģ', 'x', 'ed', 'Ġground', 'Ġmobile', 'Ġairborne', 'Ġantennas', 'Ġmedium', 'Ġearth', 'Ġorbit', 'Ġconstellation', 'Ġprovides', 'Ġaccess', 'Ġmobile', 'Ġphone', 'Ġoperators', 'Ġinternet', 'Ġservice', 'Ġproviders', 'Ġcovers', 'Ġequ', 'atorial', 'Ġregion', 'Ġast', 'Ġspac', 'em', 'obile', 'Ġsatellite', 'Ġconstellation', 'Ġworking', 'Ġlarge', 'Ġmobile', 'Ġnetwork', 'Ġoperators', 'Ġv', 'od', 'af', 'one', 'Ġorange', 'Ġr', 'ak', 'uten', 'Ġtel', 'est', 'ra', 'Ġtele', 'f', 'Ã³n', 'ica', 'Ġetc', 'Ġobjective', 'Ġprovide', 'Ġbroadband', 'Ġinternet', 'Ġcoverage', 'Ġexisting', 'Ġun', 'mod', 'ï', '¬', 'ģ', 'ed', 'Ġmobile', 'Ġphones', 'Ġorb', 'comm', 'Ġoperational', 'Ġconstellation', 'Ġused', 'Ġprovide', 'Ġglobal', 'Ġasset', 'Ġmonitoring', 'Ġmessaging', 'Ġservices', 'Ġconstellation', 'Ġle', 'Ġcommunications', 'Ġsatellites', 'Ġorbiting', 'Ġglobal', 'star', 'Ġoperational', 'Ġlow', 'Ġearth', 'Ġorbit', 'le', 'Ġsatellite', 'Ġconstellation', 'Ġsatellite', 'Ġphone', 'Ġlow', 'speed', 'Ġdata', 'Ġcommunications', 'Ġcovering', 'Ġworld', "'s", 'Ġland', 'mass', 'Ġir', 'idium', 'Ġoperational', 'Ġconstellation', 'Ġcross', 'linked', 'Ġsatellites', 'Ġpolar', 'Ġorbit', 'Ġused', 'Ġprovide', 'Ġsatellite', 'Ġphone', 'Ġlow', 'speed', 'Ġdata', 'Ġservices', 'Ġentire', 'Ġsurface', 'Ġearth', 'Ġlyn', 'k', 'Ġglobal', 'Ġsatellite', 'Ġconstellation', 'Ġobjective', 'Ġcoverage', 'Ġtraditional', 'Ġlow', 'cost', 'Ġmobile', 'Ġdevices', 'Ġtel', 'edes', 'ic', 'Ġformer', 'Ġventure', 'Ġaccomplish', 'Ġbroadband', 'Ġsatellite', 'Ġinternet', 'Ġservices', 'Ġproject', 'Ġl', 'oon', 'Ġformer', 'Ġconcept', 'Ġprovide', 'Ġinternet', 'Ġaccess', 'Ġvia', 'Ġballoons', 'Ġstrat', 'osphere', 'st', 'arl', 'ink', 'Ġgroup', 'Ġfal', 'con', 'Ġblock', 'Ġeveryday', 'Ġastronaut', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġmay', 'space', 'x', 'Ġce', 'Ġel', 'Ġmus', 'k', 'Ġreveals', 'Ġnext', 'generation', 'Ġstar', 'link', 'Ġsatellite', 'Ġdetails', 'w', 'es', 'lar', 'ati', 'Ġretrieved', 'Ġj', 'une', 'Ġgr', 'ush', 'Ġlore', 'n', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġlaunch', 'Ġtwo', 'Ġspace', 'Ġinternet', 'Ġsatellites', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġnearly', '000', 'Ġaz', 'watch', 'live', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġk', 'ol', 'od', 'ny', 'Ġl', 'ora', 'Ġaug', 'ust', 'space', 'x', 'mobile', 'Ġteam', 'Ġuse', 'Ġstar', 'link', 'Ġsatellites', 'end', 'Ġmobile', 'Ġdead', 'Ġzones', 'Ġretrieved', 'Ġaug', 'ust']</t>
         </is>
       </c>
       <c r="C428" t="n">
@@ -6002,7 +6002,7 @@
       </c>
       <c r="B429" t="inlineStr">
         <is>
-          <t>['Ġreportedly', 'Ġhigh', 'level', 'Ġï', '¬', 'ģ', 'rings', 'Ġgeek', 'wire', 'Ġarchived', 'web', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'mber', 'space', 'x', 'Ġexpands', 'Ġnew', 'ï', '¬', 'ģ', 'ce', 'Ġspace', 'Ġorange', 'Ġcounty', 'Ġcal', 'ornia', 'es', 'lar', 'ati', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'open', 'Ġpositions', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġoct', 'ober', 'space', 'x', "'s", 'Ġshot', 'well', 'Ġfal', 'con', 'Ġinquiry', 'Ġdiscounts', 'Ġreused', 'Ġrockets', 'Ġsilicon', 'Ġvalley', "'s", 'Ġtest', 'fail', 'Ġethos', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġselected', 'Ġapplication', 'Ġlisting', 'Ġfile', 'Ġinternational', 'Ġbureau', 'Ġapplication', 'Ġfiling', 'Ġreporting', 'Ġsystem', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġmarch', 'Ġgets', 'Ġï', '¬', 'ģ', 'Ġnew', 'Ġapplications', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'htt', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġasks', 'Ġmake', 'Ġexception', 'Ġle', 'Ġconst', 'ell', 'ations', 'Ġconnect', 'Ġameric', 'Ġfund', 'Ġdecisions', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'Ġgrants', 'Ġpartial', 'Ġapproval', 'Ġstar', 'link', 'Ġsecond', 'generation', 'Ġconstellation', 'http', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġde', 'cember', 'dating', 'Ġrules', 'Ġorbit', 'Ġfixed', 'atellite', 'Ġservice', 'Ġconst', 'ell', 'ations', 'Ġse', 'pt', 'ember', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġbro', 'kin', 'Ġj', 'Ġoct', 'ober', 'space', 'x', 'ew', 'eb', 'Ġbroadband', 'Ġsatellites', 'Ġraise', 'Ġfears', 'Ġspace', 'Ġdebris', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober']</t>
+          <t>['cd', 'owell', 'Ġj', 'athan', 'Ġmay', 'st', 'arl', 'ink', 'Ġlaunch', 'Ġstatistics', 'Ġplanet', 'Ġretrieved', 'Ġmay', 'Ġspace', 'x', 'space', 'x', 'Ġde', 'cember', 'st', 'arl', 'ink', '000', '000', 'Ġactive', 'Ġsubscribers', 'tw', 'weet', 'Ġretrieved', 'Ġmarch', 'Ġvia', 'Ġtwitter', 'Ġstar', 'link', 'thank', 'Ġcustomers', 'Ġaround', 'Ġworld', '!"', 'Ġ07', 'Ġtwitter', 'Ġretrieved', 'Ġmay', 'Ġb', 'aylor', 'ichael', 'Ġmay', 'Ġblock', 'Ġspace', 'x', 'Ġincrease', 'Ġlaunch', 'Ġcad', 'ence', 'Ġlower', 'Ġprices', 'ww', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġsystem', 'Ġdesigned', 'Ġimprove', 'Ġglobal', 'Ġinternet', 'Ġaccess', 'Ġutilizing', 'Ġthousands', 'Ġsatellites', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġspace', 'x', 'Ġpresident', 'Ġshot', 'well', 'Ġstated', 'Ġted', 'Ġtalk', 'Ġlast', 'Ġmonth', 'Ġexpects', 'Ġconstellation', 'Ġcost', 'Ġleast', 'Ġus', 'Ġbillion', 'Ġtherefore', 'Ġreducing', 'Ġlaunch', 'Ġcosts', 'Ġvital', '."', 'Ġwink', 'ler', 'Ġro', 'lf', 'e', 'Ġpas', 'z', 'tor', 'Ġjan', 'uary', 'exclusive', 'Ġpeek', 'Ġspace', 'x', 'Ġdata', 'Ġshows', 'Ġloss', 'Ġheavy', 'Ġexpectations', 'Ġnascent', 'Ġinternet', 'Ġservice', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġsee', 'Ġalso', 'Ġreferences', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġether', 'ington', 'arrell', 'space', 'x', 'Ġhopes', 'Ġsatellite', 'Ġinternet', 'Ġbusiness', 'Ġpad', 'Ġthin', 'Ġrocket', 'Ġlaunch', 'Ġmargins', 'tech', 'cr', 'Ġtech', 'cr', 'unch', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġsatellites', 'Ġharm', 'Ġastronomy', "'s", 'Ġknow', 'Ġnational', 'Ġgeographic', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'j', 'ason', 'Ġreport', 'Ġimpacts', 'Ġlarge', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'Ġnational', 'Ġscience', 'Ġfoundation', 'Ġretrieved', 'Ġoct', 'ober', 'Ġspace', 'x', 'Ġapr', 'il', 'ast', 'ron', 'omy', 'Ġdiscussion', 'Ġnational', 'Ġacademy', 'Ġsciences', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġapr', 'il', 'st', 'arl', 'ink', 'Ġblock', 'Ġspace', 'sky', 'rocket', 'de', 'Ġarchived', 'http', 'Ġoriginal']</t>
         </is>
       </c>
       <c r="C429" t="n">
@@ -6015,7 +6015,7 @@
       </c>
       <c r="B430" t="inlineStr">
         <is>
-          <t>['Ġauthor', 'izes', 'Ġspace', 'x', 'Ġprovide', 'Ġbroadband', 'Ġsatellite', 'Ġservices', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbro', 'kin', 'Ġj', 'Ġmarch', 'Ġapproves', 'Ġspace', 'x', 'Ġplan', 'Ġlaunch', 'Ġbroadband', 'Ġsatellites', 'ar', 'st', 'ec', 'Ġwork', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġmarch', 'Ġapproves', 'Ġspace', 'x', 'Ġconstellation', 'Ġdenies', 'Ġwaiver', 'Ġeasier', 'Ġdeployment', 'Ġdeadline', 'Ġment', 'dead', 'line', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'author', 'izing', 'Ġspace', 'x', 'Ġv', 'band', 'Ġconstellation', 'Ġdeployment', 'Ġoperation', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġbro', 'kin', 'Ġj', 'Ġmarch', 'Ġtells', 'Ġspace', 'x', 'Ġdeploy', 'Ġbroadband', 'Ġsatellites', 'ar', 'st', 'ec', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġapr', 'il', 'onew', 'eb', 'Ġspace', 'x', 'Ġsatellites', 'Ġdodged', 'Ġpotential', 'Ġcollision', 'Ġorbit', 'v', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġwil', 'ts', 'hire', 'iam', '.,', 'Ġed', 'mber', 'application', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'Ġspace', 'Ġexploration', 'Ġholdings', 'c', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'space', 'Ġexploration', 'Ġholdings', 'c', 'Ġseeks', 'Ġmodify', 'Ġk', 'u', 'ka', 'band', 'Ġng', 'Ġlicense', 'Ġrelocate', 'Ġsatellites', 'Ġpreviously', 'Ġauthorized', 'Ġoperate', 'Ġaltitude', 'Ġmi', 'Ġaltitude', 'Ġmi', 'Ġmake', 'Ġrelated', 'Ġchanges', 'Ġoperations', 'Ġsatellites', 'Ġnew', 'Ġlower', 'Ġshell', 'Ġconstellation', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'space', 'x', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġsatellite']</t>
+          <t>['mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġtel', 'edes', 'ic', 'Ġplays', 'Ġlast', 'Ġcard', 'Ġleaves', 'Ġgame', '."', 'Ġoct', 'ober', 'Ġway', 'back', 'Ġmachine', 'Ġspace', 'Ġnews', 'Ġj', 'uly', 'Ġg', 'ild', 'er', 'Ġge', 'orge', 'Ġoct', 'ober', 'light', 'Ġspeed', 'Ġtrap', 'Ġahead', 'Ġl', 'Ġforb', 'es', 'space', 'x', 'Ġwash', 'Ġops', 'Ġexecutive', 'Ġlaunching', 'Ġconsulting', 'Ġfirm', 'Ġspac', 'en', 'ews', 'Ġmarch', 'Ġretrieved', 'Ġde', 'cember', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġj', 'une', 'space', 'Ġtakes', 'Ġpercent', 'Ġstake', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'sp', 'Ġspace', 'Ġnews', 'Ġsatellite', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġtransfer', 'Ġsensor', 'Ġdata', 'Ġspace', 'Ġusing', 'b', 'undle', 'Ġprotocol', 'Ġarchived', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġpress', 'Ġrelease', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'Ġse', 'pt', 'ember', 'ead', 'Ġast', 'rium', 'Ġsigns', 'Ġagreement', 'Ġacquire', 'Ġsur', 'rey', 'Ġsatellite', 'Ġtechnology', 'Ġlimited', 'Ġuniversity', 'Ġsur', 'rey', '."', 'Ġapr', 'il', 'Ġway', 'back', 'Ġmachine', 'Ġuniversity', 'Ġsur', 'rey', 'Ġapr', 'il', 'Ġwink', 'ler', 'Ġro', 'lf', 'e', 'mber', 'el', 'Ġmus', 'k', "'s", 'Ġnext', 'Ġmission', 'Ġinternet', 'Ġsatellites', 'Ġwall', 'Ġstreet', 'Ġjournal', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġf', 'ern', 'hol', 'z', 'Ġtim', 'Ġj', 'une', 'inside', 'Ġrace', 'Ġcreate', 'Ġnext', 'Ġgeneration', 'Ġsatellite', 'Ġinternet', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'application', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'Ġspace', 'Ġexploration', 'Ġholdings', 'c', 'Ġtechnical', 'Ġattachment', 'f', 'cc', 'mber', 'Ġp', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġboy', 'le', 'Ġal', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġseeks', 'Ġtrademark', 'Ġname', 'st', 'arl', 'ink', 'Ġsatellite', 'Ġbroadband', 'Ġnetwork', 'Ġgeek', 'wire', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġind', 'ian', 'apolis', 'Ġauthor', 'Ġjohn', 'Ġgreen', 'Ġinspired', 'Ġone', 'Ġel']</t>
         </is>
       </c>
       <c r="C430" t="n">
@@ -6028,7 +6028,7 @@
       </c>
       <c r="B431" t="inlineStr">
         <is>
-          <t>['Ġsystem', 'Ġattachment', 'Ġtechnical', 'Ġinformation', 'Ġsupplement', 'Ġschedule', 'Ġu', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'mber', 'Ġarchived', '000', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġapr', 'il', 'ks', 'Ġlower', 'Ġorbit', 'Ġstar', 'link', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'lower', 'Ġorbit', 'Ġnearly', 'Ġproposed', 'Ġbroadband', 'Ġsatellites', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġsaid', 'Ġapr', 'il', 'Ġcorrect', 'Ġspace', 'x', 'Ġchanging', 'Ġplans', 'Ġorbit', 'Ġsatellites', 'Ġmi', 'Ġinstead', 'Ġmi', 'Ġspace', 'x', 'Ġsays', 'Ġadjustment', 'Ġrequested', 'Ġmonths', 'Ġago', 'Ġmake', 'Ġsafer', 'Ġspace', 'Ġenvironment', 'Ġsince', 'Ġdefunct', 'Ġsatellites', 'Ġlower', 'Ġaltitude', 'Ġwould', 'enter', 'Ġearth', "'s", 'Ġatmosphere', 'Ġï', '¬', 'ģ', 'Ġyears', 'Ġeven', 'Ġwithout', 'Ġpropulsion', 'Ġlower', 'Ġorbit', 'Ġalso', 'Ġmeans', 'Ġdistance', 'Ġstar', 'link', 'Ġcompeting', 'Ġinternet', 'Ġconst', 'ell', 'ations', 'Ġproposed', 'ew', 'eb', 'Ġtel', 'es', 'Ġapproval', 'Ġallows', 'Ġsatellite', 'Ġcompanies', 'Ġprovide', 'Ġcommunications', 'Ġservices', 'Ġunited', 'Ġstates', 'Ġagency', 'Ġgranted', 'Ġspace', 'x', 'Ġmarket', 'Ġaccess', 'Ġmarch', 'Ġsatellites', 'Ġusing', 'Ġk', 'u', 'band', 'Ġka', 'band', 'Ġspectrum', 'Ġauthorized', 'Ġv', 'band', 'Ġsatellites', 'mber', 'Ġspace', 'x', "'s", 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġplans', 'Ġapply', 'Ġsmaller', 'Ġtwo', 'Ġconst', 'ell', 'ations', '."', 'space', 'x', 'Ġsub', 'mits', 'Ġpaperwork', '000', 'Ġstar', 'link', 'Ġsatellites', 'Ġoct', 'ober', 'Ġarchived', 'Ġtell', 'ites', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'space', 'x', 'Ġservices', 'Ġapplication', 'Ġblanket', 'licensed', 'Ġearth', 'Ġstations', 'Ġf', 'cc', 'report', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'st', 'arl', 'ink', 'Ġpress', 'Ġkit', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġform', 'Ġapplication', 'Ġnew', 'Ġmod']</t>
+          <t>['Ġmus', 'k', "'s", 'Ġgrand', 'Ġideas', 'Ġind', 'ian', 'apolis', 'Ġstar', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġoct', 'ober', 'shot', 'well', 'Ġsays', 'Ġspace', 'x', 'h', 'oming', 'Ġcause', 'Ġfal', 'con', 'Ġpad', 'Ġexplosion', 'http', 'sp', 'Ġspac', 'en', 'ews', 'Ġarchived', 'http', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġoct', 'ober', 'types', 'Ġbroadband', 'Ġconnections', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġgates', 'Ġdomin', 'ic', 'Ġjan', 'uary', 'el', 'Ġmus', 'k', 'outs', 'Ġlaunch', 'space', 'x', 'Ġse', 'attle', 'Ġse', 'attle', 'Ġtimes', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġjan', 'uary', 'Ġspace', 'x', 'Ġse', 'attle', 'Ġcliff', 'Ġjan', 'uary', 'Ġarchived', 'h', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġmarch', 'mus', 'k', 'Ġreiter', 'ates', 'Ġplans', 'Ġtesting', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġmarch', 'const', 'ruction', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġprototype', 'Ġspaceship', 'Ġprogress', "'re", 'Ġactually', 'Ġbuilding', 'Ġship', 'Ġright', '",', 'Ġsaid', 'Ġthink', "'ll", 'Ġprobably', 'Ġable', 'Ġshort', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġshort', 'Ġsort', 'Ġï', '¬', 'Ĥ', 'ights', 'Ġprobably', 'Ġsometime', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġhalf', 'Ġnext', 'Ġyear', '."', 'space', 'x', 'Ġbuild', 'Ġstar', 'link', 'like', 'Ġconstellation', 'Ġaround', 'Ġmars', 'Ġpresident', 'Ġsays', 'Ġfut', 'ur', 'ism', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġapr', 'il', 'Ġboy', 'le', 'Ġal', 'Ġjan', 'uary', 'space', 'x', 'Ġadds', 'Ġbig', 'Ġnew', 'Ġlab', 'Ġsatellite', 'Ġdevelopment', 'Ġoperation', 'Ġse', 'attle', 'Ġarea', 'Ġgeek', 'wire', 'Ġarchived', 'Ġn', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmay', 'Ġboy', 'le', 'Ġal', 'Ġoct', 'ober', 'space', 'x', 'Ġreorgan', 'izes', 'Ġstar', 'link', 'Ġsatellite', 'Ġoperation']</t>
         </is>
       </c>
       <c r="C431" t="n">
@@ -6041,7 +6041,7 @@
       </c>
       <c r="B432" t="inlineStr">
         <is>
-          <t>['ï', '¬', 'ģ', 'ed', 'Ġradio', 'Ġstation', 'Ġpart', 'Ġrules', 'Ġexperimental', 'Ġradio', 'Ġservice', 'Ġ05', 'ex', 'cn', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġarchived', 'Ġe', 'seq', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', '05', 'ex', 'cn', 'Ġapplication', 'Ġquestion', 'Ġpurpose', 'Ġexperiment', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'uly', 'space', 'x', 'Ġseeks', 'Ġexperimental', 'Ġauthority', 'Ġtwo', 'Ġtypes', 'Ġtesting', 'Ġtotal', 'Ġuser', 'Ġterminals', 'ixed', 'Ġtwo', 'Ġtypes', 'Ġantennas', 'Ġtest', 'Ġmultiple', 'Ġdevices', 'Ġnumber', 'Ġgeographically', 'Ġdispersed', 'Ġlocations', 'Ġthroughout', 'Ġunited', 'Ġstates', 'Ġphased', 'Ġarray', 'Ġuser', 'Ġterminals', 'Ġdeployed', 'Ġwithin', 'Ġstate', 'Ġwashing', 'ton', 'Ġhomes', 'Ġspace', 'x', 'Ġemployees', 'Ġongoing', 'Ġtesting', 'Ġauthority', 'Ġwould', 'Ġenable', 'Ġspace', 'x', 'Ġobtain', 'Ġcritical', 'Ġdata', 'Ġregarding', 'Ġoperational', 'Ġperformance', 'Ġuser', 'Ġterminals', 'Ġspace', 'x', 'Ġng', 'Ġsystem', '."', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġform', 'Ġapplication', 'Ġnew', 'Ġmodified', 'Ġradio', 'Ġstation', 'Ġpart', 'Ġrules', 'Ġexperimental', 'Ġradio', 'Ġservice', 'Ġ05', 'ex', 'cn', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'application', 'Ġquestion', 'Ġpurpose', 'Ġexperiment', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'space', 'x', 'Ġseeks', 'Ġexperimental', 'Ġauthorization', 'Ġtest', 'Ġactivities', 'Ġ...', 'Ġtests', 'Ġdesigned', 'Ġdemonstrate', 'Ġability', 'Ġtransmit', 'Ġreceive', 'Ġinformation', 'Ġï', '¬', 'ģ', 'Ġground', 'Ġsites', 'Ġfour', 'Ġground', 'Ġsites', 'Ġairborne', 'Ġaircraft', 'Ġ("', 'ground', 'air', '")', 'Ġ...', 'Ġapplication', 'Ġseeks', 'Ġuse', 'Ġearth', 'Ġstation', 'Ġtransmit', 'Ġsignals', 'Ġspace', 'x', 'Ġsatellites', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġground', 'Ġlater', 'Ġmoving', 'Ġaircraft', '."', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġapr', 'il', 'space', 'x', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdedicated', 'Ġstar', 'link', 'Ġlaunch']</t>
+          <t>['Ġreportedly', 'Ġhigh', 'level', 'Ġï', '¬', 'ģ', 'rings', 'Ġgeek', 'wire', 'Ġarchived', 'web', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'mber', 'space', 'x', 'Ġexpands', 'Ġnew', 'ï', '¬', 'ģ', 'ce', 'Ġspace', 'Ġorange', 'Ġcounty', 'Ġcal', 'ornia', 'es', 'lar', 'ati', 'Ġj', 'uly', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'open', 'Ġpositions', 'Ġspace', 'x', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġde', 'Ġse', 'ld', 'ing', 'Ġp', 'eter', 'Ġb', 'Ġoct', 'ober', 'space', 'x', "'s", 'Ġshot', 'well', 'Ġfal', 'con', 'Ġinquiry', 'Ġdiscounts', 'Ġreused', 'Ġrockets', 'Ġsilicon', 'Ġvalley', "'s", 'Ġtest', 'fail', 'Ġethos', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġselected', 'Ġapplication', 'Ġlisting', 'Ġfile', 'Ġinternational', 'Ġbureau', 'Ġapplication', 'Ġfiling', 'Ġreporting', 'Ġsystem', 'mber', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġmarch', 'Ġgets', 'Ġï', '¬', 'ģ', 'Ġnew', 'Ġapplications', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġsatellite', 'Ġconst', 'ell', 'ations', 'htt', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġjan', 'uary', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġasks', 'Ġmake', 'Ġexception', 'Ġle', 'Ġconst', 'ell', 'ations', 'Ġconnect', 'Ġameric', 'Ġfund', 'Ġdecisions', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġmay', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġde', 'cember', 'Ġgrants', 'Ġpartial', 'Ġapproval', 'Ġstar', 'link', 'Ġsecond', 'generation', 'Ġconstellation', 'http', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġde', 'cember', 'dating', 'Ġrules', 'Ġorbit', 'Ġfixed', 'atellite', 'Ġservice', 'Ġconst', 'ell', 'ations', 'Ġse', 'pt', 'ember', 'Ġp', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġbro', 'kin', 'Ġj', 'Ġoct', 'ober', 'space', 'x', 'ew', 'eb', 'Ġbroadband', 'Ġsatellites', 'Ġraise', 'Ġfears', 'Ġspace', 'Ġdebris', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober']</t>
         </is>
       </c>
       <c r="C432" t="n">
@@ -6054,7 +6054,7 @@
       </c>
       <c r="B433" t="inlineStr">
         <is>
-          <t>['Ġannounced', 'Ġmass', 'Ġproduction', 'Ġbegins', 'http', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġsub', 'mits', 'Ġpaperwork', '000', 'Ġstar', 'link', 'Ġsatellites', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġoct', 'ober', 'ending', 'Ġtweet', 'Ġspace', 'Ġvia', 'Ġstar', 'link', 'Ġsatellite', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'Ġmat', 'hew', 'son', 'Ġsam', 'antha', 'mber', 'space', 'x', 'Ġopens', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġpublic', 'Ġbeta', 'Ġtesters', 'http', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'space', 'x', "'s", 'Ġstar', 'link', 'Ġinternet', 'Ġspeeds', 'Ġconsistently', 'Ġtopping', 'Ġel', 'Ġmus', 'k', 'Ġsays', 'Ġbiggest', 'Ġchallenge', 'Ġslashing', 'Ġus', 'front', 'Ġcost', 'Ġusers', 'Ġbusiness', 'Ġinsider', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', 'Ġopens', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġpre', 'orders', 'Ġpublic', 'Ġeng', 'ad', 'get', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġapr', 'il', 'space', 'x', 'Ġadds', 'Ġlatest', 'Ġfunding', 'Ġround', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġapr', 'il', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġraises', 'Ġbillion', 'Ġfunding', 'uters', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'ed', 'ised', 'ca', 'mber', 'Ġ".', 'space', 'x', 'Ġjoining', 'Ġeffort', 'Ġhelp', 'Ġget', 'ad', 'ians', 'Ġconnected', 'Ġhigh', 'speed', 'Ġinternet', 'Ġregulatory', 'Ġapproval', 'space', 'x', 'st', 'arl', 'ink', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġconstellation', 'Ġgranted', '!"', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'space', 'x', "'s", 'Ġstar', 'link', 'Ġwins', 'Ġnearly', 'Ġus', 'Ġmillion', 'Ġsubsidies', 'Ġbring', 'Ġinternet', 'Ġrural', 'Ġareas', 'Ġde', 'cember']</t>
+          <t>['Ġauthor', 'izes', 'Ġspace', 'x', 'Ġprovide', 'Ġbroadband', 'Ġsatellite', 'Ġservices', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġmarch', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġbro', 'kin', 'Ġj', 'Ġmarch', 'Ġapproves', 'Ġspace', 'x', 'Ġplan', 'Ġlaunch', 'Ġbroadband', 'Ġsatellites', 'ar', 'st', 'ec', 'Ġwork', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġmarch', 'Ġapproves', 'Ġspace', 'x', 'Ġconstellation', 'Ġdenies', 'Ġwaiver', 'Ġeasier', 'Ġdeployment', 'Ġdeadline', 'Ġment', 'dead', 'line', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmay', 'author', 'izing', 'Ġspace', 'x', 'Ġv', 'band', 'Ġconstellation', 'Ġdeployment', 'Ġoperation', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġbro', 'kin', 'Ġj', 'Ġmarch', 'Ġtells', 'Ġspace', 'x', 'Ġdeploy', 'Ġbroadband', 'Ġsatellites', 'ar', 'st', 'ec', 'Ġar', 'Ġtechn', 'ica', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'Ġrou', 'lette', 'Ġjo', 'ey', 'Ġapr', 'il', 'onew', 'eb', 'Ġspace', 'x', 'Ġsatellites', 'Ġdodged', 'Ġpotential', 'Ġcollision', 'Ġorbit', 'v', 'Ġverge', 'Ġarchived', 'Ġoriginal', 'Ġapr', 'il', 'Ġretrieved', 'Ġapr', 'il', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġwil', 'ts', 'hire', 'iam', '.,', 'Ġed', 'mber', 'application', 'Ġfixed', 'Ġsatellite', 'Ġservice', 'Ġspace', 'Ġexploration', 'Ġholdings', 'c', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'space', 'Ġexploration', 'Ġholdings', 'c', 'Ġseeks', 'Ġmodify', 'Ġk', 'u', 'ka', 'band', 'Ġng', 'Ġlicense', 'Ġrelocate', 'Ġsatellites', 'Ġpreviously', 'Ġauthorized', 'Ġoperate', 'Ġaltitude', 'Ġmi', 'Ġaltitude', 'Ġmi', 'Ġmake', 'Ġrelated', 'Ġchanges', 'Ġoperations', 'Ġsatellites', 'Ġnew', 'Ġlower', 'Ġshell', 'Ġconstellation', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'space', 'x', 'Ġnon', 'ge', 'ost', 'ation', 'ary', 'Ġsatellite']</t>
         </is>
       </c>
       <c r="C433" t="n">
@@ -6067,7 +6067,7 @@
       </c>
       <c r="B434" t="inlineStr">
         <is>
-          <t>['Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġfing', 'Ġj', 'Ġaug', 'ust', 'Ġrejects', 'Ġstar', 'link', 'Ġrequest', 'Ġnearly', 'Ġmillion', 'Ġbroadband', 'Ġsubsidies', 'http', 'Ġeng', 'ad', 'get', 'Ġretrieved', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġappeals', 'Ġrejection', 'Ġgrant', 'Ġcalls', 'Ġreversal', 'gross', 'ly', 'Ġunfair', 'Ġar', 'Ġtechn', 'ica', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'application', 'Ġblanket', 'licensed', 'Ġearth', 'Ġstations', 'Ġmotion', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġal', 'v', 'arez', 'Ġsim', 'Ġmarch', 'st', 'arl', 'ink', 'Ġapplication', 'Ġreveal', 'Ġplans', 'Ġsatellite', 'Ġinternet', 'Ġmoving', 'Ġvehicles', 'h', 'es', 'lar', 'ati', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'vet', 'Ġj', 'ordan', 'Ġmay', 'google', 'Ġwins', 'Ġcloud', 'Ġdeal', 'Ġel', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġstar', 'link', 'Ġinternet', 'Ġconnectivity', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'v', 'ias', 'Ġasks', 'Ġhalt', 'Ġstar', 'link', 'Ġlaunches', 'Ġseeks', 'Ġcourt', 'Ġruling', 'Ġspac', 'en', 'ews', 'Ġmay', 'Ġarchived', 'Ġg', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'uly', 'space', 'x', 'Ġsays', 'Ġstarship', 'Ġbeat', 'pl', 'asma', 'Ġblackout', 'Ġstar', 'link', 'Ġantennas', 'ww', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġrainbow', 'Ġj', 'ason', 'Ġjan', 'uary', 'st', 'arl', 'ink', "'s", 'Ġhead', 'Ġind', 'ia', 'Ġresign', 'Ġspace', 'x', 'Ġrefunds', 'Ġpre', 'orders', 'sp', 'ac', 'en', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'san', 'jay', 'Ġb', 'h', 'arg', 'ava', 'Ġhead', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġsatellite', 'Ġbroadband', 'Ġventure', 'Ġind', 'ia', 'Ġeconomic', 'Ġtimes', 'Ġretrieved', 'Ġoct', 'ober', 'Ġp', 'orter', 'Ġj', 'Ġfe', 'b', 'ruary', 'space', 'x', "'s", 'Ġnew', 'Ġstar', 'link', 'Ġbusiness', 'Ġtier', 'Ġpromises', 'mb', 'ps']</t>
+          <t>['Ġsystem', 'Ġattachment', 'Ġtechnical', 'Ġinformation', 'Ġsupplement', 'Ġschedule', 'Ġu', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'mber', 'Ġarchived', '000', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġhen', 'ry', 'Ġc', 'aleb', 'Ġapr', 'il', 'ks', 'Ġlower', 'Ġorbit', 'Ġstar', 'link', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'lower', 'Ġorbit', 'Ġnearly', 'Ġproposed', 'Ġbroadband', 'Ġsatellites', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġsaid', 'Ġapr', 'il', 'Ġcorrect', 'Ġspace', 'x', 'Ġchanging', 'Ġplans', 'Ġorbit', 'Ġsatellites', 'Ġmi', 'Ġinstead', 'Ġmi', 'Ġspace', 'x', 'Ġsays', 'Ġadjustment', 'Ġrequested', 'Ġmonths', 'Ġago', 'Ġmake', 'Ġsafer', 'Ġspace', 'Ġenvironment', 'Ġsince', 'Ġdefunct', 'Ġsatellites', 'Ġlower', 'Ġaltitude', 'Ġwould', 'enter', 'Ġearth', "'s", 'Ġatmosphere', 'Ġï', '¬', 'ģ', 'Ġyears', 'Ġeven', 'Ġwithout', 'Ġpropulsion', 'Ġlower', 'Ġorbit', 'Ġalso', 'Ġmeans', 'Ġdistance', 'Ġstar', 'link', 'Ġcompeting', 'Ġinternet', 'Ġconst', 'ell', 'ations', 'Ġproposed', 'ew', 'eb', 'Ġtel', 'es', 'Ġapproval', 'Ġallows', 'Ġsatellite', 'Ġcompanies', 'Ġprovide', 'Ġcommunications', 'Ġservices', 'Ġunited', 'Ġstates', 'Ġagency', 'Ġgranted', 'Ġspace', 'x', 'Ġmarket', 'Ġaccess', 'Ġmarch', 'Ġsatellites', 'Ġusing', 'Ġk', 'u', 'band', 'Ġka', 'band', 'Ġspectrum', 'Ġauthorized', 'Ġv', 'band', 'Ġsatellites', 'mber', 'Ġspace', 'x', "'s", 'Ġmod', 'ï', '¬', 'ģ', 'ed', 'Ġplans', 'Ġapply', 'Ġsmaller', 'Ġtwo', 'Ġconst', 'ell', 'ations', '."', 'space', 'x', 'Ġsub', 'mits', 'Ġpaperwork', '000', 'Ġstar', 'link', 'Ġsatellites', 'Ġoct', 'ober', 'Ġarchived', 'Ġtell', 'ites', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'space', 'x', 'Ġservices', 'Ġapplication', 'Ġblanket', 'licensed', 'Ġearth', 'Ġstations', 'Ġf', 'cc', 'report', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'st', 'arl', 'ink', 'Ġpress', 'Ġkit', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġform', 'Ġapplication', 'Ġnew', 'Ġmod']</t>
         </is>
       </c>
       <c r="C434" t="n">
@@ -6080,7 +6080,7 @@
       </c>
       <c r="B435" t="inlineStr">
         <is>
-          <t>['Ġmonth', 'Ġnew', 'Ġantenna', 'Ġcarries', 'Ġupfront', 'Ġcost', 'Ġverge', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġfe', 'b', 'ruary', 'st', 'arl', 'ink', 'Ġbusiness', 'Ġstar', 'link', 'Ġretrieved', 'Ġmarch', 'Ġrainbow', 'Ġj', 'ason', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġsec', 'ures', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcruise', 'Ġline', 'Ġcustomer', 'Ġroyal', 'Ġcar', 'ib', 'bean', 'sp', 'ac', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġdeliveries', 'Ġslow', 'Ġamid', 'Ġchip', 'Ġshortage', 'Ġfed', 'ex', 'Ġdelays', 'Ġmagazine', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'space', 'x', 'Ġsays', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġservice', '000', 'Ġusers', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'http', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġpresident', 'Ġsays', 'Ġstar', 'link', 'Ġglobal', 'Ġsatellite', 'Ġbroad', 'brand', 'Ġservice', 'Ġlive', 'Ġse', 'pt', 'ember', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġstar', 'link', 'Ġmission', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'web', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'st', 'arl', 'ink', '000', 'Ġsubs', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġstar', 'link', 'st', 'arl', 'ink', 'Ġmay', 'thank', 'Ġcustomers', 'Ġaround', 'Ġworld', 'twitter', 'weet', 'Ġvia', 'Ġtwitter', 'st', 'arl', 'ink', 'Ġset', 'Ġdeliver', 'Ġbreakthrough', 'Ġinternet', 'Ġservices', 'Ġph', 'Ġsoon', 'Ġmay', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstep', 'hen', 'Ġc', 'hen', 'Ġmay', 'ch', 'ina', 'Ġmilitary', 'Ġmust', 'Ġable', 'Ġdestroy', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġsatellites', 'Ġthreaten', 'Ġnational', 'Ġsecurity', 'Ġscientists', 'Ġren', 'Ġyuan', 'zhen', 'Ġj', 'ng', 'Ġl', 'u', 'ao', 'bing', 'Ġh', 'ong', 'wei', 'Ġsun', 'Ġsh', 'u', 'yan', 'Ġdevelopment', 'Ġstatus', 'Ġstar', 'link', 'Ġcounter', 'measures', 'Ġmodern', 'Ġdefense', 'Ġtechnology', '):', 'âĢĵ', 'Ġarchived']</t>
+          <t>['ï', '¬', 'ģ', 'ed', 'Ġradio', 'Ġstation', 'Ġpart', 'Ġrules', 'Ġexperimental', 'Ġradio', 'Ġservice', 'Ġ05', 'ex', 'cn', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġarchived', 'Ġe', 'seq', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', '05', 'ex', 'cn', 'Ġapplication', 'Ġquestion', 'Ġpurpose', 'Ġexperiment', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'uly', 'space', 'x', 'Ġseeks', 'Ġexperimental', 'Ġauthority', 'Ġtwo', 'Ġtypes', 'Ġtesting', 'Ġtotal', 'Ġuser', 'Ġterminals', 'ixed', 'Ġtwo', 'Ġtypes', 'Ġantennas', 'Ġtest', 'Ġmultiple', 'Ġdevices', 'Ġnumber', 'Ġgeographically', 'Ġdispersed', 'Ġlocations', 'Ġthroughout', 'Ġunited', 'Ġstates', 'Ġphased', 'Ġarray', 'Ġuser', 'Ġterminals', 'Ġdeployed', 'Ġwithin', 'Ġstate', 'Ġwashing', 'ton', 'Ġhomes', 'Ġspace', 'x', 'Ġemployees', 'Ġongoing', 'Ġtesting', 'Ġauthority', 'Ġwould', 'Ġenable', 'Ġspace', 'x', 'Ġobtain', 'Ġcritical', 'Ġdata', 'Ġregarding', 'Ġoperational', 'Ġperformance', 'Ġuser', 'Ġterminals', 'Ġspace', 'x', 'Ġng', 'Ġsystem', '."', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġform', 'Ġapplication', 'Ġnew', 'Ġmodified', 'Ġradio', 'Ġstation', 'Ġpart', 'Ġrules', 'Ġexperimental', 'Ġradio', 'Ġservice', 'Ġ05', 'ex', 'cn', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'application', 'Ġquestion', 'Ġpurpose', 'Ġexperiment', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġj', 'uly', 'space', 'x', 'Ġseeks', 'Ġexperimental', 'Ġauthorization', 'Ġtest', 'Ġactivities', 'Ġ...', 'Ġtests', 'Ġdesigned', 'Ġdemonstrate', 'Ġability', 'Ġtransmit', 'Ġreceive', 'Ġinformation', 'Ġï', '¬', 'ģ', 'Ġground', 'Ġsites', 'Ġfour', 'Ġground', 'Ġsites', 'Ġairborne', 'Ġaircraft', 'Ġ("', 'ground', 'air', '")', 'Ġ...', 'Ġapplication', 'Ġseeks', 'Ġuse', 'Ġearth', 'Ġstation', 'Ġtransmit', 'Ġsignals', 'Ġspace', 'x', 'Ġsatellites', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġground', 'Ġlater', 'Ġmoving', 'Ġaircraft', '."', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġapr', 'il', 'space', 'x', "'s", 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġdedicated', 'Ġstar', 'link', 'Ġlaunch']</t>
         </is>
       </c>
       <c r="C435" t="n">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'Ġmay', 'Ġpass', 'ant', 'Ġrab', 'ie', 'Ġmay', 'ch', 'inese', 'Ġresearchers', 'Ġpublish', 'Ġstrategy', 'Ġdestroy', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġel', 'Ġmus', 'k', 'el', 'mus', 'k', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġmeant', 'Ġpeaceful', 'Ġuse', '...', 'Ġhelp', 'Ġmend', 'Ġfault', 'Ġstars', 'weet', 'Ġvia', 'Ġtwitter', 'Ġed', 'Ġbrown', 'e', 'Ġse', 'pt', 'ember', 'fact', 'Ġcheck', 'Ġk', 'remlin', 'Ġthreaten', 'Ġdestroy', 'Ġstar', 'link', 'Ġsatellites', '?"', 'ww', 'Ġnews', 'week', 'st', 'arl', 'ink', "'s", 'Ġservice', 'Ġlets', 'Ġusers', 'Ġjump', 'Ġline', 'Ġprice', 'Ġspac', 'en', 'ews', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġdun', 'phy', 'Ġch', 'ris', 'Ġj', 'uly', 'st', 'arl', 'ink', 'Ġboats', 'Ġspace', 'x', 'Ġannounces', 'Ġstar', 'link', 'Ġmaritime', 'Ġeye', 'po', 'pping', 'Ġprice', 'Ġg', 'price', 'Ġmobile', 'Ġinternet', 'Ġresource', 'Ġcenter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġstar', 'link', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ming', 'Ġdan', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġintroduces', 'Ġbest', 'Ġeffort', 'Ġservice', 'Ġmobile', 'Ġinternet', 'Ġresource', 'Ġcenter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'help', 'Ġcenter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġannounces', 'Ġmonthly', 'Ġcap', 'Ġusers', 'Ġgo', 'Ġget', 'Ġslower', 'Ġspeeds', 'Ġar', 'ste', 'chn', 'ica', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġbro', 'kin', 'Ġj', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġgetting', 'Ġlot', 'Ġslower', 'Ġpeople', 'Ġuse', 'Ġspeed', 'Ġtests', 'Ġshow', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġsays', 'Ġtest', 'Ġstar', 'link', 'âĢ', 'Ļ', 'Ġsatellite', 'cell', 'Ġservice', 'mobile', 'Ġyear', 'Ġmarch', 'st', 'arl', 'ink', 'Ġconnectivity', 'Ġeffective', 'Ġprovinces', 'Ġmut', 'ati', 'Ġl', 'us', 'ak', 'imes', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'une', 'st', 'arl', 'ink', 'Ġsec', 'ures', 'Ġlicence', 'Ġoperate', 'Ġz', 'amb', 'ia', 'Ġcomm', 'update', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'Ġmus', 'k']</t>
+          <t>['Ġannounced', 'Ġmass', 'Ġproduction', 'Ġbegins', 'http', 'es', 'lar', 'ati', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġapr', 'il', 'space', 'x', 'Ġsub', 'mits', 'Ġpaperwork', '000', 'Ġstar', 'link', 'Ġsatellites', 'Ġoct', 'ober', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġoct', 'ober', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġoct', 'ober', 'ending', 'Ġtweet', 'Ġspace', 'Ġvia', 'Ġstar', 'link', 'Ġsatellite', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'Ġmat', 'hew', 'son', 'Ġsam', 'antha', 'mber', 'space', 'x', 'Ġopens', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġpublic', 'Ġbeta', 'Ġtesters', 'http', 'Ġspace', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġmarch', 'space', 'x', "'s", 'Ġstar', 'link', 'Ġinternet', 'Ġspeeds', 'Ġconsistently', 'Ġtopping', 'Ġel', 'Ġmus', 'k', 'Ġsays', 'Ġbiggest', 'Ġchallenge', 'Ġslashing', 'Ġus', 'front', 'Ġcost', 'Ġusers', 'Ġbusiness', 'Ġinsider', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'mber', 'space', 'x', 'Ġopens', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġpre', 'orders', 'Ġpublic', 'Ġeng', 'ad', 'get', 'Ġarchived', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġf', 'oust', 'Ġje', 'ff', 'Ġapr', 'il', 'space', 'x', 'Ġadds', 'Ġlatest', 'Ġfunding', 'Ġround', 'Ġspac', 'en', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġapr', 'il', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġraises', 'Ġbillion', 'Ġfunding', 'uters', 'Ġarchived', 'Ġoriginal', 'Ġaug', 'ust', 'Ġretrieved', 'Ġapr', 'il', 'ed', 'ised', 'ca', 'mber', 'Ġ".', 'space', 'x', 'Ġjoining', 'Ġeffort', 'Ġhelp', 'Ġget', 'ad', 'ians', 'Ġconnected', 'Ġhigh', 'speed', 'Ġinternet', 'Ġregulatory', 'Ġapproval', 'space', 'x', 'st', 'arl', 'ink', 'Ġlow', 'Ġearth', 'Ġorbit', 'Ġsatellite', 'Ġconstellation', 'Ġgranted', '!"', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'space', 'x', "'s", 'Ġstar', 'link', 'Ġwins', 'Ġnearly', 'Ġus', 'Ġmillion', 'Ġsubsidies', 'Ġbring', 'Ġinternet', 'Ġrural', 'Ġareas', 'Ġde', 'cember']</t>
         </is>
       </c>
       <c r="C436" t="n">
@@ -6106,7 +6106,7 @@
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>["'s", 'Ġstar', 'link', 'Ġgiven', 'Ġlicense', 'Ġoperate', 'Ġz', 'amb', 'ia', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġlaunch', 'Ġsatellite', 'Ġinternet', 'Ġservice', 'ong', 'olia', 'uters', 'Ġj', 'uly', 'Ġstar', 'link', '?"', 'Ġtech', 'Ġtarget', 'Ġaug', 'ust', 'Ġretrieved', 'Ġjan', 'uary', 'Ġc', 'atherine', 'cn', 'ally', 'Ġmarch', 'space', 'x', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġreview', 'Ġreviews', 'org', 'Ġretrieved', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġapr', 'il', 'Ġ"@', 'er', 'day', 'ast', 'ron', 'aut', 'hes', 'etz', 'weet', 'z', 'Ġyeah', 'Ġfully', 'Ġmobile', 'Ġlater', 'Ġyear', 'Ġmove', 'Ġanywhere', 'Ġuse', 'Ġtruck', 'Ġmotion', 'Ġneed', 'Ġsatellite', 'Ġlaunches', 'Ġachieve', 'Ġcompete', 'Ġcoverage', 'Ġkey', 'Ġsoftware', 'Ġupgrades', '003', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'call', 'aghan', 'Ġj', 'athan', 'Ġoct', 'ober', 'space', 'x', 'Ġreveals', 'Ġmonthly', 'Ġcost', 'Ġstar', 'link', 'Ġinternet', 'better', 'Ġnothing', 'Ġbeta', 'Ġforb', 'es', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'broad', 'band', 'Ġgen', 'ie', 'Ġawards', 'Ġbest', 'Ġinternet', 'Ġproviders', 'Ġar', 'ds', 'Ġretrieved', 'Ġj', 'uly', 'Ġhar', 'per', 'Ġz', 'ach', 'ary', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġexpensive', 'Ġprice', 'Ġdrop', 'Ġturbo', 'Ġspeed', 'Ġwi', 'ï', '¬', 'ģ', 'Ġretrieved', 'Ġoct', 'ober', 'Ġr', 'icker', 'Ġth', 'omas', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġlowers', 'Ġmonthly', 'Ġinternet', 'Ġprices', 'Ġpercent', 'Ġverge', 'Ġretrieved', 'Ġoct', 'ober', 'Ġsam', 'ios', 'Ġz', 'oe', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġnear', '000', 'Ġaust', 'ral', 'ian', 'Ġcustomers', 'Ġsy', 'ney', 'Ġmorning', 'Ġherald', 'Ġretrieved', 'Ġmarch', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġaug', 'ust', 'get']</t>
+          <t>['Ġarchived', 'Ġoriginal', 'Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'Ġfing', 'Ġj', 'Ġaug', 'ust', 'Ġrejects', 'Ġstar', 'link', 'Ġrequest', 'Ġnearly', 'Ġmillion', 'Ġbroadband', 'Ġsubsidies', 'http', 'Ġeng', 'ad', 'get', 'Ġretrieved', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġappeals', 'Ġrejection', 'Ġgrant', 'Ġcalls', 'Ġreversal', 'gross', 'ly', 'Ġunfair', 'Ġar', 'Ġtechn', 'ica', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'application', 'Ġblanket', 'licensed', 'Ġearth', 'Ġstations', 'Ġmotion', 'Ġfederal', 'Ġcommunications', 'Ġcommission', 'Ġarchived', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġal', 'v', 'arez', 'Ġsim', 'Ġmarch', 'st', 'arl', 'ink', 'Ġapplication', 'Ġreveal', 'Ġplans', 'Ġsatellite', 'Ġinternet', 'Ġmoving', 'Ġvehicles', 'h', 'es', 'lar', 'ati', 'Ġarchived', 'web', 'arch', 'Ġoriginal', 'Ġmarch', 'Ġretrieved', 'Ġmarch', 'vet', 'Ġj', 'ordan', 'Ġmay', 'google', 'Ġwins', 'Ġcloud', 'Ġdeal', 'Ġel', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġstar', 'link', 'Ġinternet', 'Ġconnectivity', 'Ġarchived', 'Ġoriginal', 'Ġmay', 'v', 'ias', 'Ġasks', 'Ġhalt', 'Ġstar', 'link', 'Ġlaunches', 'Ġseeks', 'Ġcourt', 'Ġruling', 'Ġspac', 'en', 'ews', 'Ġmay', 'Ġarchived', 'Ġg', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġmay', 'Ġr', 'alph', 'Ġer', 'ic', 'Ġj', 'uly', 'space', 'x', 'Ġsays', 'Ġstarship', 'Ġbeat', 'pl', 'asma', 'Ġblackout', 'Ġstar', 'link', 'Ġantennas', 'ww', 'Ġarchived', 'Ġoriginal', 'Ġj', 'uly', 'Ġretrieved', 'Ġj', 'uly', 'Ġrainbow', 'Ġj', 'ason', 'Ġjan', 'uary', 'st', 'arl', 'ink', "'s", 'Ġhead', 'Ġind', 'ia', 'Ġresign', 'Ġspace', 'x', 'Ġrefunds', 'Ġpre', 'orders', 'sp', 'ac', 'en', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'san', 'jay', 'Ġb', 'h', 'arg', 'ava', 'Ġhead', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġsatellite', 'Ġbroadband', 'Ġventure', 'Ġind', 'ia', 'Ġeconomic', 'Ġtimes', 'Ġretrieved', 'Ġoct', 'ober', 'Ġp', 'orter', 'Ġj', 'Ġfe', 'b', 'ruary', 'space', 'x', "'s", 'Ġnew', 'Ġstar', 'link', 'Ġbusiness', 'Ġtier', 'Ġpromises', 'mb', 'ps']</t>
         </is>
       </c>
       <c r="C437" t="n">
@@ -6119,7 +6119,7 @@
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>['Ġwireless', 'Ġspace', 'x', 'mobile', 'Ġwant', 'Ġoffer', 'Ġzero', 'g', 'Ġcoverage', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġaug', 'ust', 'mobile', 'Ġwinning', 'Ġrace', 'Ġmid', 'band', 'Ġlight', 'Ġreading', 'mber', 'Ġretrieved', 'Ġaug', 'ust', 'space', 'x', 'Ġone', 'Ġretrieved', 'Ġj', 'uly', 'Ġpull', 'ar', 'st', 'reck', 'er', 'Ġtom', 'Ġapr', 'il', 'one', 'ks', 'Ġdeal', 'Ġspace', 'x', 'Ġprovide', 'Ġmobile', 'Ġcoverage', 'htt', 'Ġstuff', 'Ġretrieved', 'Ġj', 'uly', 'together', 'Ġopt', 'us', 'Ġspace', 'x', 'Ġplan', 'Ġcover', 'Ġaust', 'ral', 'ia', 'Ġpop', 'kin', 'Ġg', 'ab', 'riel', 'Ġjan', 'uary', 'dec', 'ades', 'agan', "'s", 'star', 'Ġwars', ",'", 'Ġtrump', 'Ġcalls', 'Ġmissile', 'Ġdefenses', 'Ġwould', 'Ġblast', 'Ġwarheads', 'Ġp', 'om', 'pe', 'ike', 'Ġjan', 'uary', 'nuclear', 'Ġweapons', 'Ġch', 'ina', 'Ġstrategic', 'Ġdefense', 'Ġinitiative', 'Ġcentury', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġapr', 'il', 'space', 'Ġdevelopment', 'Ġagency', 'Ġhuge', 'Ġwin', 'Ġgr', 'ï', '¬', 'ģ', 'n', 'Ġwar', 'Ġstatus', 'Ġquo', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'enn', 'eth', 'Ġchang', 'Ġmay', 'ent', 'reprene', 'ur', 'Ġtries', 'Ġmid', 'Ġtouch', 'Ġspace', 'Ġnew', 'ork', 'Ġtimes', 'ny', 'Ġnew', 'ork', 'Ġtimes', 'Ġtre', 'v', 'ith', 'ick', 'Ġj', 'ose', 'ph', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġexec', 'Ġsays', 'Ġcompany', 'Ġwould', 'Ġlaunch', 'Ġweapon', 'Ġspace', 'defense', 'Ġcountry', 'Ġretrieved', 'Ġjan', 'uary', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġoct', 'ober', 'l', 'har', 'ris', 'Ġspace', 'x', 'Ġwin', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġcontracts', 'Ġbuild', 'Ġmissile', 'warning', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġde', 'cember', 'Ġmach', 'Ġv', 'iv', 'ienne', 'Ġj', 'une', 'us', 'Ġmilitary', 'Ġplaces', 'Ġbet', 'Ġle', 'Ġspace', 'Ġsecurity', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġapr', 'il', 'space', 'x', 'Ġlaunches', 'Ġsatellites', 'Ġu', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'space', 'Ġsand', 'ra']</t>
+          <t>['Ġmonth', 'Ġnew', 'Ġantenna', 'Ġcarries', 'Ġupfront', 'Ġcost', 'Ġverge', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġspace', 'x', 'Ġfe', 'b', 'ruary', 'st', 'arl', 'ink', 'Ġbusiness', 'Ġstar', 'link', 'Ġretrieved', 'Ġmarch', 'Ġrainbow', 'Ġj', 'ason', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġsec', 'ures', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġcruise', 'Ġline', 'Ġcustomer', 'Ġroyal', 'Ġcar', 'ib', 'bean', 'sp', 'ac', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġdeliveries', 'Ġslow', 'Ġamid', 'Ġchip', 'Ġshortage', 'Ġfed', 'ex', 'Ġdelays', 'Ġmagazine', 'Ġjan', 'uary', 'Ġretrieved', 'Ġjan', 'uary', 'space', 'x', 'Ġsays', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġservice', '000', 'Ġusers', 'Ġfe', 'b', 'ruary', 'Ġarchived', 'http', 'Ġoriginal', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'space', 'x', 'Ġpresident', 'Ġsays', 'Ġstar', 'link', 'Ġglobal', 'Ġsatellite', 'Ġbroad', 'brand', 'Ġservice', 'Ġlive', 'Ġse', 'pt', 'ember', 'Ġj', 'une', 'Ġarchived', 'Ġoriginal', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'Ġstar', 'link', 'Ġmission', 'Ġspace', 'x', 'Ġmay', 'Ġarchived', 'web', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġyoutube', 'st', 'arl', 'ink', '000', 'Ġsubs', 'Ġse', 'pt', 'ember', 'Ġarchived', 'Ġoriginal', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġstar', 'link', 'st', 'arl', 'ink', 'Ġmay', 'thank', 'Ġcustomers', 'Ġaround', 'Ġworld', 'twitter', 'weet', 'Ġvia', 'Ġtwitter', 'st', 'arl', 'ink', 'Ġset', 'Ġdeliver', 'Ġbreakthrough', 'Ġinternet', 'Ġservices', 'Ġph', 'Ġsoon', 'Ġmay', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġstep', 'hen', 'Ġc', 'hen', 'Ġmay', 'ch', 'ina', 'Ġmilitary', 'Ġmust', 'Ġable', 'Ġdestroy', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġsatellites', 'Ġthreaten', 'Ġnational', 'Ġsecurity', 'Ġscientists', 'Ġren', 'Ġyuan', 'zhen', 'Ġj', 'ng', 'Ġl', 'u', 'ao', 'bing', 'Ġh', 'ong', 'wei', 'Ġsun', 'Ġsh', 'u', 'yan', 'Ġdevelopment', 'Ġstatus', 'Ġstar', 'link', 'Ġcounter', 'measures', 'Ġmodern', 'Ġdefense', 'Ġtechnology', '):', 'âĢĵ', 'Ġarchived']</t>
         </is>
       </c>
       <c r="C438" t="n">
@@ -6132,7 +6132,7 @@
       </c>
       <c r="B439" t="inlineStr">
         <is>
-          <t>['Ġer', 'win', 'Ġdec', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'âĢ', 'Ļ', 'Ġï', '¬', 'ģ', 'r', 'st', 'Ġlaunch', 'Ġslips', 'Ġmarch', 'Ġdue', 'Ġsatellite', 'Ġglitch', 'http', 'hyp', 'erson', 'ic', 'Ġmissile', 'Ġdefense', 'Ġissues', 'Ġcongress', 'Ġcongressional', 'Ġresearch', 'Ġservice', 'Ġjan', 'uary', 'Ġretrieved', 'Ġj', 'une', 'war', 'ï', '¬', 'ģ', 'gh', 'ter', 'Ġcouncil', 'Ġguides', 'Ġcapability', 'Ġdevelopment', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġment', 'agency', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġmarch', 'Ġretrieved', 'Ġj', 'une', 'cost', 'Ġimplementing', 'Ġrecommendations', 'Ġmissile', 'Ġdefense', 'Ġreview', 'Ġcongressional', 'Ġbudget', 'ï', '¬', 'ģ', 'ce', 'Ġjan', 'uary', 'Ġretrieved', 'Ġde', 'cember', 'Ġmach', 'Ġv', 'iv', 'ienne', 'Ġj', 'une', 'us', 'Ġmilitary', 'Ġplaces', 'Ġbet', 'Ġle', 'Ġspace', 'Ġsecurity', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġretrieved', 'Ġde', 'cember', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġmissile', 'Ġdefense', 'Ġreview', 'ï', '¬', 'ģ', 'ce', 'Ġsecretary', 'Ġdefense', 'mber', 'Ġretrieved', 'Ġj', 'une', 'space', 'based', 'Ġmissile', 'Ġdefense', 'Ġunion', 'Ġconcerned', 'Ġscientists', 'Ġaug', 'ust', 'Ġretrieved', 'Ġde', 'cember', 'appro', 'aching', 'Ġthird', 'Ġrail', 'Ġtr', 'ilateral', 'Ġtreaty', 'Ġprohibit', 'Ġspace', 'based', 'Ġmissile', 'Ġdefenses', 'Ġcar', 'negie', 'Ġend', 'owment', 'Ġinternational', 'Ġpeace', 'Ġde', 'cember', 'Ġretrieved', 'mber', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġwashing', 'ton', 'Ġoutsider', 'Ġcourts', 'Ġmilitary', 'Ġbusiness', 'Ġwall', 'Ġstreet', 'Ġjournal', 'mber', 'Ġretrieved', 'Ġde', 'cember', 'nd', 'ia', 'Ġappoint', 'Ġmembers', 'Ġboard', 'Ġgo', 'v', 'con', 'Ġwire', 'Ġoct', 'ober', 'Ġretrieved', 'Ġde', 'cember', 'statement', 'Ġgeneral', 'Ġter', 'rence', 'Ġj', "'s", 'h', 'aug', 'ness', 'Ġsenate', 'Ġarmed', 'Ġservices', 'Ġcommittee', 'ar', 'Ġu', 'Ġsenate', 'Ġfe', 'b', 'ruary', 'Ġretrieved', 'mber', 'space', 'Ġdevelopment', 'Ġagency', 'Ġmakes', 'Ġawards', 'Ġsatellites', 'Ġbuild', 'Ġtr', 'anche', 'Ġtransport', 'Ġlay', 'e', 'Ġu', 'Ġdepartment', 'Ġdefense', 'Ġretrieved', 'Ġaug', 'ust', 'usa', 'Ġ...', 'Ġ...', 'st', 'arsh', 'ield', 'Ġsupporting', 'Ġnational', 'Ġsecurity', 'Ġspace', 'x']</t>
+          <t>['Ġoriginal', 'Ġmay', 'Ġpass', 'ant', 'Ġrab', 'ie', 'Ġmay', 'ch', 'inese', 'Ġresearchers', 'Ġpublish', 'Ġstrategy', 'Ġdestroy', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġel', 'Ġmus', 'k', 'el', 'mus', 'k', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġmeant', 'Ġpeaceful', 'Ġuse', '...', 'Ġhelp', 'Ġmend', 'Ġfault', 'Ġstars', 'weet', 'Ġvia', 'Ġtwitter', 'Ġed', 'Ġbrown', 'e', 'Ġse', 'pt', 'ember', 'fact', 'Ġcheck', 'Ġk', 'remlin', 'Ġthreaten', 'Ġdestroy', 'Ġstar', 'link', 'Ġsatellites', '?"', 'ww', 'Ġnews', 'week', 'st', 'arl', 'ink', "'s", 'Ġservice', 'Ġlets', 'Ġusers', 'Ġjump', 'Ġline', 'Ġprice', 'Ġspac', 'en', 'ews', 'Ġmay', 'Ġretrieved', 'Ġmay', 'Ġdun', 'phy', 'Ġch', 'ris', 'Ġj', 'uly', 'st', 'arl', 'ink', 'Ġboats', 'Ġspace', 'x', 'Ġannounces', 'Ġstar', 'link', 'Ġmaritime', 'Ġeye', 'po', 'pping', 'Ġprice', 'Ġg', 'price', 'Ġmobile', 'Ġinternet', 'Ġresource', 'Ġcenter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġstar', 'link', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'ming', 'Ġdan', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġintroduces', 'Ġbest', 'Ġeffort', 'Ġservice', 'Ġmobile', 'Ġinternet', 'Ġresource', 'Ġcenter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'help', 'Ġcenter', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġannounces', 'Ġmonthly', 'Ġcap', 'Ġusers', 'Ġgo', 'Ġget', 'Ġslower', 'Ġspeeds', 'Ġar', 'ste', 'chn', 'ica', 'mber', 'Ġretrieved', 'Ġjan', 'uary', 'Ġbro', 'kin', 'Ġj', 'Ġse', 'pt', 'ember', 'st', 'arl', 'ink', 'Ġgetting', 'Ġlot', 'Ġslower', 'Ġpeople', 'Ġuse', 'Ġspeed', 'Ġtests', 'Ġshow', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġspace', 'x', 'Ġsays', 'Ġtest', 'Ġstar', 'link', 'âĢ', 'Ļ', 'Ġsatellite', 'cell', 'Ġservice', 'mobile', 'Ġyear', 'Ġmarch', 'st', 'arl', 'ink', 'Ġconnectivity', 'Ġeffective', 'Ġprovinces', 'Ġmut', 'ati', 'Ġl', 'us', 'ak', 'imes', 'Ġapr', 'il', 'Ġretrieved', 'Ġj', 'une', 'st', 'arl', 'ink', 'Ġsec', 'ures', 'Ġlicence', 'Ġoperate', 'Ġz', 'amb', 'ia', 'Ġcomm', 'update', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'Ġmus', 'k']</t>
         </is>
       </c>
       <c r="C439" t="n">
@@ -6145,7 +6145,7 @@
       </c>
       <c r="B440" t="inlineStr">
         <is>
-          <t>['Ġde', 'cember', 'Ġretrieved', 'Ġde', 'cember', 'space', 'x', 'Ġreleases', 'st', 'arsh', 'ield', 'Ġsatellite', 'Ġservices', 'Ġdesigned', 'Ġgovernment', 'Ġuse', 'Ġsupport', 'Ġnational', 'Ġsecurity', 'htt', 'mus', 'k', "'s", 'Ġspace', 'x', 'Ġwins', 'Ġpent', 'agon', 'Ġaward', 'Ġmissile', 'Ġtracking', 'Ġsatellites', 'uters', 'Ġoct', 'ober', 'Ġj', 'athan', 'cd', 'owell', 'planet', 'Ġj', 'une', 'space', 'track', 'Ġcon', 'ï', '¬', 'ģ', 'r', 'ms', 'Ġpresence', 'Ġfour', 'Ġsecret', 'Ġpayload', 'Ġglobal', 'star', 'Ġfal', 'con', 'Ġlaunch', 'Ġus', 'Ġus', 'Ġcatalog', 'Ġorbital', 'Ġdata', 'Ġavailable', 'Ġone', 'Ġpiece', 'Ġdebris', 'Ġprobably', 'Ġstar', 'link', 'style', 'Ġtension', 'Ġrod', '?"', 'weet', 'Ġvia', 'Ġtwitter', 'c', 'gb', 'ass', 'Ġj', 'une', 'Ġfour', 'Ġclass', 'ï', '¬', 'ģ', 'ed', 'Ġsatellites', 'Ġlaunched', 'Ġtogether', 'Ġglobal', 'star', 'Ġfal', 'con', 'Ġrocket', 'Ġyesterday', 'Ġdetected', 'Ġorbit', 'Ġdeg', 'Ġinclination', 'weet', 'Ġvia', 'Ġtwitter', 'space', 'x', 'Ġlaunches', 'Ġglobal', 'star', 'Ġsatellite', 'Ġmysterious', 'Ġfal', 'con', 'Ġmission', 'Ġj', 'une', 'tr', 'anche', 'Ġï', '¬', 'Ĥ', 'ight', 'Ġtracking', 'Ġlayer', 'ats', 'Ġmatches', 'orbit', 'Ġimages', 'Ġreleased', 'Ġst', 'arsh', 'ield', 'Ġpage', 'Ġst', 'arsh', 'ield', 'ats', 'Ġtwitter', 'Ġretrieved', 'Ġj', 'une', 'tracking', 'Ġlayer', 'Ġtr', 'anche', 'Ġw', 'f', 'ov', 'Ġ...', 'Ġx', 'htm', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġoct', 'ober', 'space', 'x', 'Ġplans', 'Ġstart', 'Ġoffering', 'Ġstar', 'link', 'Ġbroadband', 'Ġservices', 'sp', 'Ġspac', 'en', 'ews', 'Ġarchived', 'http', 'Ġ', 'ices', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġinsin', 'na', 'Ġval', 'erie', 'Ġjan', 'uary', 'Ġair', 'Ġforce', 'Ġtested', 'Ġadvanced', 'Ġbattle', 'Ġmanagement', 'Ġsystem', "'s", 'Ġworked', "'t", 'Ġdef', 'ensen', 'ews', 'Ġarchived', 'Ġoriginal', 'Ġjan', 'uary', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'Ġrich', 'Ġg', 'illian', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġstar', 'link', 'Ġimpress', 'es', 'Ġair', 'Ġforce', 'Ġweapons', 'Ġbuyer', 'Ġbig', 'Ġlive', 'fire', 'Ġexercise', 'Ġinvestors', 'Ġarchived']</t>
+          <t>["'s", 'Ġstar', 'link', 'Ġgiven', 'Ġlicense', 'Ġoperate', 'Ġz', 'amb', 'ia', 'Ġj', 'une', 'Ġretrieved', 'Ġj', 'une', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġlaunch', 'Ġsatellite', 'Ġinternet', 'Ġservice', 'ong', 'olia', 'uters', 'Ġj', 'uly', 'Ġstar', 'link', '?"', 'Ġtech', 'Ġtarget', 'Ġaug', 'ust', 'Ġretrieved', 'Ġjan', 'uary', 'Ġc', 'atherine', 'cn', 'ally', 'Ġmarch', 'space', 'x', 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġreview', 'Ġreviews', 'org', 'Ġretrieved', 'Ġapr', 'il', 'Ġmus', 'k', 'Ġel', 'el', 'mus', 'k', 'Ġapr', 'il', 'Ġ"@', 'er', 'day', 'ast', 'ron', 'aut', 'hes', 'etz', 'weet', 'z', 'Ġyeah', 'Ġfully', 'Ġmobile', 'Ġlater', 'Ġyear', 'Ġmove', 'Ġanywhere', 'Ġuse', 'Ġtruck', 'Ġmotion', 'Ġneed', 'Ġsatellite', 'Ġlaunches', 'Ġachieve', 'Ġcompete', 'Ġcoverage', 'Ġkey', 'Ġsoftware', 'Ġupgrades', '003', 'weet', 'Ġarchived', 'Ġoriginal', 'Ġoct', 'ober', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'Ġvia', 'Ġtwitter', 'call', 'aghan', 'Ġj', 'athan', 'Ġoct', 'ober', 'space', 'x', 'Ġreveals', 'Ġmonthly', 'Ġcost', 'Ġstar', 'link', 'Ġinternet', 'better', 'Ġnothing', 'Ġbeta', 'Ġforb', 'es', 'Ġarchived', 'Ġoriginal', 'mber', 'Ġretrieved', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġwik', 'ipedia', 'broad', 'band', 'Ġgen', 'ie', 'Ġawards', 'Ġbest', 'Ġinternet', 'Ġproviders', 'Ġar', 'ds', 'Ġretrieved', 'Ġj', 'uly', 'Ġhar', 'per', 'Ġz', 'ach', 'ary', 'Ġoct', 'ober', 'Ġstar', 'link', 'Ġexpensive', 'Ġprice', 'Ġdrop', 'Ġturbo', 'Ġspeed', 'Ġwi', 'ï', '¬', 'ģ', 'Ġretrieved', 'Ġoct', 'ober', 'Ġr', 'icker', 'Ġth', 'omas', 'Ġaug', 'ust', 'st', 'arl', 'ink', 'Ġlowers', 'Ġmonthly', 'Ġinternet', 'Ġprices', 'Ġpercent', 'Ġverge', 'Ġretrieved', 'Ġoct', 'ober', 'Ġsam', 'ios', 'Ġz', 'oe', 'Ġfe', 'b', 'ruary', 'el', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġnear', '000', 'Ġaust', 'ral', 'ian', 'Ġcustomers', 'Ġsy', 'ney', 'Ġmorning', 'Ġherald', 'Ġretrieved', 'Ġmarch', 'Ġber', 'ger', 'Ġer', 'ic', 'Ġaug', 'ust', 'get']</t>
         </is>
       </c>
       <c r="C440" t="n">
@@ -6158,7 +6158,7 @@
       </c>
       <c r="B441" t="inlineStr">
         <is>
-          <t>['Ġoriginal', 'mber', 'Ġretrieved', 'Ġse', 'pt', 'ember', 'Ġel', 'Ġmus', 'k', "'s", 'Ġsatellites', 'Ġsaved', 'Ġu', 'k', 'raine', 'Ġchanged', 'Ġwarfare', 'utm', 'id', 'Ġeconomist', 'Ġiss', 'n', 'Ġ00', '06', 'Ġretrieved', 'Ġj', 'une', 'ese', 'ac', 'Ġmarch', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġkeep', 'Ġu', 'k', 'raine', 'Ġonline', '?"', 'Ġreason', 'Ġreason', 'Ġretrieved', 'Ġmarch', 'Ġel', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'x', "'s", 'Ġstar', 'link', 'Ġsatellites', 'Ġactive', 'Ġu', 'k', 'raine', 'Ġrequest', 'Ġembattled', 'Ġcountry', "'s", 'Ġleaders', 'h', 'Ġindependent', 'Ġfe', 'b', 'ruary', 'Ġ"@', 'el', 'mus', 'k', 'Ġtry', 'Ġcolon', 'ize', 'Ġmars', 'Ġr', 'ussia', 'Ġtry', 'Ġoccupy', 'Ġu', 'k', 'raine', 'Ġrockets', 'Ġsuccessfully', 'Ġland', 'Ġspace', 'Ġr', 'ussian', 'Ġrockets', 'Ġattack', 'Ġu', 'k', 'rain', 'ian', 'Ġcivil', 'Ġpeople', 'Ġask', 'Ġprovide', 'Ġu', 'k', 'raine', 'Ġstar', 'link', 'Ġstations', 'Ġaddress', 'Ġsane', 'Ġr', 'uss', 'ians', 'Ġstand', 'Ġtwitter', 'Ġfe', 'b', 'ruary', 'abb', 'agh', 'Ġdan', 'Ġfe', 'b', 'ruary', 'f', 'ury', 'Ġu', 'k', 'raine', 'Ġel', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġlimits', 'Ġstar', 'link', 'Ġuse', 'Ġdrones', 'Ġones', 'el', 'mus', 'k', 'Ġguardian', 'Ġiss', 'n', 'Ġretrieved', 'Ġmay', 'Ġel', 'Ġmus', 'k', "'s", 'Ġsatellites', 'Ġsaved', 'Ġu', 'k', 'raine', 'Ġchanged', 'Ġwarfare', 'utm', 'id', 'Ġeconomist', 'Ġiss', 'n', 'Ġ00', '06', 'Ġretrieved', 'Ġj', 'une', 'Ġel', 'Ġmus', 'k', "'s", 'Ġstar', 'link', 'Ġsatellite', 'Ġinternet', 'Ġkeeps', 'Ġu', 'k', 'raine', 'Ġonline', 'Ġk', 'iv', 'Ġindependent', 'Ġse', 'pt', 'ember', 'Ġretrieved', 'Ġj', 'une', 'Ġfrank', 'Ġfe', 'b', 'ruary', 'mus', 'k', 'Ġdeputy', "'s", 'Ġwords', 'Ġstar', 'link', 'weapon', 'ization', 'Ġvex', 'Ġu', 'k', 'raine', 'ap', 'news', 'c', 'Ġassociated', 'Ġpress', 'Ġretrieved', 'Ġapr', 'il', 'k', 'rieg', 'Ġder', 'Ġu', 'k', 'raine', 'Ġdie', 'Ġer', 'fol', 'gs', 'ges', 'ch', 'ich', 'te', 'Ġder', 'Ġu', 'k', 'rain', 'isc', 'hen', 'Ġart', 'iller', 'ie', 'Ġyoutube', 'Ġel', 'Ġmus', 'k', "'s", 'Ġsatellites', 'Ġsaved', 'Ġu', 'k', 'raine', 'Ġchanged', 'Ġwarfare', 'utm']</t>
+          <t>['Ġwireless', 'Ġspace', 'x', 'mobile', 'Ġwant', 'Ġoffer', 'Ġzero', 'g', 'Ġcoverage', 'http', 'Ġar', 'Ġtechn', 'ica', 'Ġretrieved', 'Ġaug', 'ust', 'mobile', 'Ġwinning', 'Ġrace', 'Ġmid', 'band', 'Ġlight', 'Ġreading', 'mber', 'Ġretrieved', 'Ġaug', 'ust', 'space', 'x', 'Ġone', 'Ġretrieved', 'Ġj', 'uly', 'Ġpull', 'ar', 'st', 'reck', 'er', 'Ġtom', 'Ġapr', 'il', 'one', 'ks', 'Ġdeal', 'Ġspace', 'x', 'Ġprovide', 'Ġmobile', 'Ġcoverage', 'htt', 'Ġstuff', 'Ġretrieved', 'Ġj', 'uly', 'together', 'Ġopt', 'us', 'Ġspace', 'x', 'Ġplan', 'Ġcover', 'Ġaust', 'ral', 'ia', 'Ġpop', 'kin', 'Ġg', 'ab', 'riel', 'Ġjan', 'uary', 'dec', 'ades', 'agan', "'s", 'star', 'Ġwars', ",'", 'Ġtrump', 'Ġcalls', 'Ġmissile', 'Ġdefenses', 'Ġwould', 'Ġblast', 'Ġwarheads', 'Ġp', 'om', 'pe', 'ike', 'Ġjan', 'uary', 'nuclear', 'Ġweapons', 'Ġch', 'ina', 'Ġstrategic', 'Ġdefense', 'Ġinitiative', 'Ġcentury', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġapr', 'il', 'space', 'Ġdevelopment', 'Ġagency', 'Ġhuge', 'Ġwin', 'Ġgr', 'ï', '¬', 'ģ', 'n', 'Ġwar', 'Ġstatus', 'Ġquo', 'Ġretrieved', 'Ġjan', 'uary', 'Ġk', 'enn', 'eth', 'Ġchang', 'Ġmay', 'ent', 'reprene', 'ur', 'Ġtries', 'Ġmid', 'Ġtouch', 'Ġspace', 'Ġnew', 'ork', 'Ġtimes', 'ny', 'Ġnew', 'ork', 'Ġtimes', 'Ġtre', 'v', 'ith', 'ick', 'Ġj', 'ose', 'ph', 'Ġse', 'pt', 'ember', 'space', 'x', 'Ġexec', 'Ġsays', 'Ġcompany', 'Ġwould', 'Ġlaunch', 'Ġweapon', 'Ġspace', 'defense', 'Ġcountry', 'Ġretrieved', 'Ġjan', 'uary', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġoct', 'ober', 'l', 'har', 'ris', 'Ġspace', 'x', 'Ġwin', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġcontracts', 'Ġbuild', 'Ġmissile', 'warning', 'Ġsatellites', 'Ġspac', 'en', 'ews', 'Ġretrieved', 'Ġde', 'cember', 'Ġmach', 'Ġv', 'iv', 'ienne', 'Ġj', 'une', 'us', 'Ġmilitary', 'Ġplaces', 'Ġbet', 'Ġle', 'Ġspace', 'Ġsecurity', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'Ġretrieved', 'Ġde', 'cember', 'Ġarticle', 'Ġincorporates', 'Ġtext', 'Ġsource', 'Ġpublic', 'Ġdomain', 'Ġer', 'win', 'Ġsand', 'ra', 'Ġapr', 'il', 'space', 'x', 'Ġlaunches', 'Ġsatellites', 'Ġu', 'Ġspace', 'Ġdevelopment', 'Ġagency', 'space', 'Ġsand', 'ra']</t>
         </is>
       </c>
       <c r="C441" t="n">
@@ -6171,7 +6171,7 @@
       </c>
       <c r="B442" t="inlineStr">
         <is>
-          <t>['id', 'Ġeconomist', 'Ġiss', 'n', 'Ġ00', '06', 'Ġretrieved', 'Ġj', 'une', 'utton', 'Ġhi', 'Ġfe', 'b', 'ruary', 'st', 'arl', 'ink', 'Ġlimits', 'Ġu', 'k', 'raine', "'s", 'Ġmaritime', 'Ġdrones', 'Ġtime', 'Ġnew', 'Ġr', 'ussian', 'Ġthreat', 'http', 'Ġnaval', 'Ġnews', 'Ġretrieved', 'Ġfe', 'b', 'ruary', 'n', 'lex', 'Ġoct', 'ober', 'el', 'Ġmus', 'k', 'Ġsays', 'Ġspace', 'x', 'Ġkeep', 'Ġfunding', 'Ġstar', 'link', 'Ġinternet', 'Ġu', 'k', 'raine', 'ww', 'Ġe', 'Ġguardian', 'Ġiss', 'n', 'Ġretrieved', 'Ġj', 'une', 'Ġcap', 'acc', 'io', 'Ġanth', 'ony', 'el', 'Ġmus', 'k', "'s", 'Ġspace', 'x', 'Ġwins', 'Ġpent', 'agon', 'Ġdeal', 'Ġstar', 'link', 'Ġu', 'k', 'raine', 'Ġbloom', 'berg', 'ste', 'ven', 'Ġse', 'ag', 'al', 'Ġcalling', 'Ġcircus', 'Ġr', 'ussian', 'Ġtelevision', 'break', 'Ġfake', ')"', 'Ġworld', 'Ġyoutube', 'Ġfe', 'b', 'ruary', 'Ġfrank', 'Ġfe', 'b', 'ruary', 'mus', 'k', 'Ġdeputy', "'s", 'Ġwords', 'Ġstar', 'link', 'weapon', 'ization', 'Ġvex', 'Ġu'